<commit_message>
Add/update progress report for 9/05/2025 by Avichal
</commit_message>
<xml_diff>
--- a/PR&IR.xlsx
+++ b/PR&IR.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28730"/>
-  <workbookPr defaultThemeVersion="202300"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jayshil.singh\Desktop\Personal Files\CS415_A3\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\avichal avneel nath\Documents\Semester 7\CS415\A3\CS415_A3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{804CE9A9-4F24-4029-A552-382870E1B724}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF990874-22CD-41B1-9A17-D8CB24080417}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{BFA1E21A-08FA-4F02-8C25-33C81C8EE970}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{BFA1E21A-08FA-4F02-8C25-33C81C8EE970}"/>
   </bookViews>
   <sheets>
     <sheet name="Avichal" sheetId="1" r:id="rId1"/>
@@ -24,23 +24,12 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="21">
   <si>
     <t>Date</t>
   </si>
@@ -89,16 +78,52 @@
   <si>
     <t>Date Resolved</t>
   </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Developed core features of Enrollment Services module: course enrollment functionality, enrolled courses view, and course drop with validation. Integrated basic routing and tested module using </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial Unicode MS"/>
+        <family val="2"/>
+      </rPr>
+      <t>run_enrollment_services.py</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>.</t>
+    </r>
+  </si>
+  <si>
+    <t>Completed</t>
+  </si>
+  <si>
+    <t>Connect Enrollment with Fees &amp; Holds and Profile modules</t>
+  </si>
+  <si>
+    <t>Implemented drop course validation logic; routing structure established and tested successfully</t>
+  </si>
+  <si>
+    <t>AAN</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
-    <numFmt numFmtId="170" formatCode="h"/>
-    <numFmt numFmtId="171" formatCode="d/mm/yyyy;@"/>
+    <numFmt numFmtId="164" formatCode="h"/>
+    <numFmt numFmtId="165" formatCode="d/mm/yyyy;@"/>
   </numFmts>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -111,6 +136,12 @@
       <color theme="1"/>
       <name val="Times New Roman"/>
       <family val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial Unicode MS"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -133,16 +164,17 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="170" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="14" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="171" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -152,7 +184,7 @@
       <numFmt numFmtId="30" formatCode="@"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="171" formatCode="d/mm/yyyy;@"/>
+      <numFmt numFmtId="165" formatCode="d/mm/yyyy;@"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="30" formatCode="@"/>
@@ -161,49 +193,10 @@
       <numFmt numFmtId="30" formatCode="@"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="171" formatCode="d/mm/yyyy;@"/>
+      <numFmt numFmtId="165" formatCode="d/mm/yyyy;@"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="30" formatCode="@"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <name val="Times New Roman"/>
-        <family val="1"/>
-        <scheme val="none"/>
-      </font>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="171" formatCode="d/mm/yyyy;@"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="170" formatCode="h"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="14" formatCode="0.00%"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="19" formatCode="m/d/yyyy"/>
     </dxf>
     <dxf>
       <font>
@@ -230,7 +223,7 @@
       <numFmt numFmtId="30" formatCode="@"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="170" formatCode="h"/>
+      <numFmt numFmtId="164" formatCode="h"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="14" formatCode="0.00%"/>
@@ -239,7 +232,7 @@
       <numFmt numFmtId="30" formatCode="@"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="19" formatCode="m/d/yyyy"/>
+      <numFmt numFmtId="166" formatCode="m/d/yyyy"/>
     </dxf>
     <dxf>
       <font>
@@ -266,7 +259,7 @@
       <numFmt numFmtId="30" formatCode="@"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="170" formatCode="h"/>
+      <numFmt numFmtId="164" formatCode="h"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="14" formatCode="0.00%"/>
@@ -275,22 +268,7 @@
       <numFmt numFmtId="30" formatCode="@"/>
     </dxf>
     <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <name val="Times New Roman"/>
-        <family val="1"/>
-        <scheme val="none"/>
-      </font>
+      <numFmt numFmtId="166" formatCode="m/d/yyyy"/>
     </dxf>
     <dxf>
       <font>
@@ -317,7 +295,7 @@
       <numFmt numFmtId="30" formatCode="@"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="170" formatCode="h"/>
+      <numFmt numFmtId="164" formatCode="h"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="14" formatCode="0.00%"/>
@@ -326,7 +304,61 @@
       <numFmt numFmtId="30" formatCode="@"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="19" formatCode="m/d/yyyy"/>
+      <numFmt numFmtId="165" formatCode="d/mm/yyyy;@"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Times New Roman"/>
+        <family val="1"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="h"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="14" formatCode="0.00%"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="166" formatCode="m/d/yyyy"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Times New Roman"/>
+        <family val="1"/>
+        <scheme val="none"/>
+      </font>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -342,7 +374,7 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{9FACB7F7-F35A-492E-AAF4-C8AD07A65A4F}" name="Table1" displayName="Table1" ref="A1:H100" totalsRowShown="0" headerRowDxfId="28">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{9FACB7F7-F35A-492E-AAF4-C8AD07A65A4F}" name="Table1" displayName="Table1" ref="A1:H100" totalsRowShown="0" headerRowDxfId="34">
   <autoFilter ref="A1:H100" xr:uid="{9FACB7F7-F35A-492E-AAF4-C8AD07A65A4F}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
@@ -354,14 +386,14 @@
     <filterColumn colId="7" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="8">
-    <tableColumn id="1" xr3:uid="{022F0CCA-D3AD-4C41-96AC-23A1F1ACD784}" name="Date" dataDxfId="34"/>
-    <tableColumn id="2" xr3:uid="{37EC747A-FF52-4BB8-9E7B-6658170B560E}" name="Member Name" dataDxfId="33"/>
+    <tableColumn id="1" xr3:uid="{022F0CCA-D3AD-4C41-96AC-23A1F1ACD784}" name="Date" dataDxfId="33"/>
+    <tableColumn id="2" xr3:uid="{37EC747A-FF52-4BB8-9E7B-6658170B560E}" name="Member Name" dataDxfId="32"/>
     <tableColumn id="3" xr3:uid="{595E07A7-B79C-490D-94F8-CC8A9548AAAE}" name="Task/Activity"/>
     <tableColumn id="4" xr3:uid="{399451D6-2EBE-4B51-8C25-09283BEE7B49}" name="Status"/>
-    <tableColumn id="5" xr3:uid="{951691AA-F5B7-4E87-94DD-56C88DDA7F01}" name="% Complete" dataDxfId="32"/>
-    <tableColumn id="6" xr3:uid="{5173E32D-1D51-4EE1-B4EB-015C386C7E1D}" name="Hours Worked Today" dataDxfId="31"/>
-    <tableColumn id="7" xr3:uid="{9793C2C7-1239-4777-8672-318111FFC5D8}" name="Next Steps" dataDxfId="30"/>
-    <tableColumn id="8" xr3:uid="{46550E96-F4E9-4167-888B-2889A1FA646A}" name="Notes/Comments" dataDxfId="29"/>
+    <tableColumn id="5" xr3:uid="{951691AA-F5B7-4E87-94DD-56C88DDA7F01}" name="% Complete" dataDxfId="31"/>
+    <tableColumn id="6" xr3:uid="{5173E32D-1D51-4EE1-B4EB-015C386C7E1D}" name="Hours Worked Today" dataDxfId="30"/>
+    <tableColumn id="7" xr3:uid="{9793C2C7-1239-4777-8672-318111FFC5D8}" name="Next Steps" dataDxfId="29"/>
+    <tableColumn id="8" xr3:uid="{46550E96-F4E9-4167-888B-2889A1FA646A}" name="Notes/Comments" dataDxfId="28"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium26" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -380,21 +412,21 @@
     <filterColumn colId="7" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="8">
-    <tableColumn id="1" xr3:uid="{80182F43-8CEA-4E5A-AE23-4E131CE1B1B1}" name="Date" dataDxfId="7"/>
-    <tableColumn id="2" xr3:uid="{55A78D6C-890A-4502-A184-DEEFF14BB82E}" name="Member Name" dataDxfId="26"/>
+    <tableColumn id="1" xr3:uid="{80182F43-8CEA-4E5A-AE23-4E131CE1B1B1}" name="Date" dataDxfId="26"/>
+    <tableColumn id="2" xr3:uid="{55A78D6C-890A-4502-A184-DEEFF14BB82E}" name="Member Name" dataDxfId="25"/>
     <tableColumn id="3" xr3:uid="{57B9A516-E930-4C06-A589-24182A37BA85}" name="Task/Activity"/>
     <tableColumn id="4" xr3:uid="{A7CD18E8-808E-43EA-A960-7EDF2D2AB452}" name="Status"/>
-    <tableColumn id="5" xr3:uid="{A9BAB96D-D5FD-4C0D-A277-6E052D27EC3A}" name="% Complete" dataDxfId="25"/>
-    <tableColumn id="6" xr3:uid="{4EBDEBD4-A02D-4266-88BC-5E6088167CE4}" name="Hours Worked Today" dataDxfId="24"/>
-    <tableColumn id="7" xr3:uid="{88484166-6833-4A6B-B292-081E908E7876}" name="Next Steps" dataDxfId="23"/>
-    <tableColumn id="8" xr3:uid="{65034E84-46C0-4115-A351-A3C28C7B9EE1}" name="Notes/Comments" dataDxfId="22"/>
+    <tableColumn id="5" xr3:uid="{A9BAB96D-D5FD-4C0D-A277-6E052D27EC3A}" name="% Complete" dataDxfId="24"/>
+    <tableColumn id="6" xr3:uid="{4EBDEBD4-A02D-4266-88BC-5E6088167CE4}" name="Hours Worked Today" dataDxfId="23"/>
+    <tableColumn id="7" xr3:uid="{88484166-6833-4A6B-B292-081E908E7876}" name="Next Steps" dataDxfId="22"/>
+    <tableColumn id="8" xr3:uid="{65034E84-46C0-4115-A351-A3C28C7B9EE1}" name="Notes/Comments" dataDxfId="21"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium26" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{D9A2FBFA-47C8-4A27-8A35-991BC77E93AD}" name="Table14" displayName="Table14" ref="A1:H100" totalsRowShown="0" headerRowDxfId="21">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{D9A2FBFA-47C8-4A27-8A35-991BC77E93AD}" name="Table14" displayName="Table14" ref="A1:H100" totalsRowShown="0" headerRowDxfId="20">
   <autoFilter ref="A1:H100" xr:uid="{D9A2FBFA-47C8-4A27-8A35-991BC77E93AD}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
@@ -406,21 +438,21 @@
     <filterColumn colId="7" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="8">
-    <tableColumn id="1" xr3:uid="{9DF80C4D-D075-4428-A54F-FD6AD093D08C}" name="Date" dataDxfId="20"/>
-    <tableColumn id="2" xr3:uid="{EBFC72C6-272F-4910-98B7-AD481D68F5CF}" name="Member Name" dataDxfId="19"/>
+    <tableColumn id="1" xr3:uid="{9DF80C4D-D075-4428-A54F-FD6AD093D08C}" name="Date" dataDxfId="19"/>
+    <tableColumn id="2" xr3:uid="{EBFC72C6-272F-4910-98B7-AD481D68F5CF}" name="Member Name" dataDxfId="18"/>
     <tableColumn id="3" xr3:uid="{9F5B3984-7002-4FEA-8B81-D2D8284783D7}" name="Task/Activity"/>
     <tableColumn id="4" xr3:uid="{5F85F44B-886F-440F-9E69-8335A039C2E6}" name="Status"/>
-    <tableColumn id="5" xr3:uid="{AF0043ED-9EF2-470B-9735-7321011714BA}" name="% Complete" dataDxfId="18"/>
-    <tableColumn id="6" xr3:uid="{4F961AD8-B86B-411C-BB04-8D7EE4DD134D}" name="Hours Worked Today" dataDxfId="17"/>
-    <tableColumn id="7" xr3:uid="{34EBB1FC-FFD7-47AB-A959-A220B742401C}" name="Next Steps" dataDxfId="16"/>
-    <tableColumn id="8" xr3:uid="{128DAA9E-15FB-4BB9-B76B-4A920C859038}" name="Notes/Comments" dataDxfId="15"/>
+    <tableColumn id="5" xr3:uid="{AF0043ED-9EF2-470B-9735-7321011714BA}" name="% Complete" dataDxfId="17"/>
+    <tableColumn id="6" xr3:uid="{4F961AD8-B86B-411C-BB04-8D7EE4DD134D}" name="Hours Worked Today" dataDxfId="16"/>
+    <tableColumn id="7" xr3:uid="{34EBB1FC-FFD7-47AB-A959-A220B742401C}" name="Next Steps" dataDxfId="15"/>
+    <tableColumn id="8" xr3:uid="{128DAA9E-15FB-4BB9-B76B-4A920C859038}" name="Notes/Comments" dataDxfId="14"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium26" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{646C4EC7-41A3-4570-9D38-06D55FDE20F6}" name="Table15" displayName="Table15" ref="A1:H100" totalsRowShown="0" headerRowDxfId="14">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{646C4EC7-41A3-4570-9D38-06D55FDE20F6}" name="Table15" displayName="Table15" ref="A1:H100" totalsRowShown="0" headerRowDxfId="13">
   <autoFilter ref="A1:H100" xr:uid="{646C4EC7-41A3-4570-9D38-06D55FDE20F6}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
@@ -432,14 +464,14 @@
     <filterColumn colId="7" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="8">
-    <tableColumn id="1" xr3:uid="{13D6CE41-CF73-478C-B7F6-3B0C25C48DFD}" name="Date" dataDxfId="13"/>
-    <tableColumn id="2" xr3:uid="{E468B109-F9F1-48D8-BECE-0F7015DD8D95}" name="Member Name" dataDxfId="12"/>
+    <tableColumn id="1" xr3:uid="{13D6CE41-CF73-478C-B7F6-3B0C25C48DFD}" name="Date" dataDxfId="12"/>
+    <tableColumn id="2" xr3:uid="{E468B109-F9F1-48D8-BECE-0F7015DD8D95}" name="Member Name" dataDxfId="11"/>
     <tableColumn id="3" xr3:uid="{279E5366-E900-45EE-80D9-5446A85E61AD}" name="Task/Activity"/>
     <tableColumn id="4" xr3:uid="{63D996BE-E8E2-4186-8CD4-49EAB9AA8847}" name="Status"/>
-    <tableColumn id="5" xr3:uid="{2FF82CF3-E17A-4896-9C9C-7339D28CD4A7}" name="% Complete" dataDxfId="11"/>
-    <tableColumn id="6" xr3:uid="{67DCB379-6881-4BBC-A633-BD51853A9B6B}" name="Hours Worked Today" dataDxfId="10"/>
-    <tableColumn id="7" xr3:uid="{91C8F225-F251-45F2-BC41-843547B77A6F}" name="Next Steps" dataDxfId="9"/>
-    <tableColumn id="8" xr3:uid="{EEAB1D68-5668-4B1F-8473-D3A49DA7E015}" name="Notes/Comments" dataDxfId="8"/>
+    <tableColumn id="5" xr3:uid="{2FF82CF3-E17A-4896-9C9C-7339D28CD4A7}" name="% Complete" dataDxfId="10"/>
+    <tableColumn id="6" xr3:uid="{67DCB379-6881-4BBC-A633-BD51853A9B6B}" name="Hours Worked Today" dataDxfId="9"/>
+    <tableColumn id="7" xr3:uid="{91C8F225-F251-45F2-BC41-843547B77A6F}" name="Next Steps" dataDxfId="8"/>
+    <tableColumn id="8" xr3:uid="{EEAB1D68-5668-4B1F-8473-D3A49DA7E015}" name="Notes/Comments" dataDxfId="7"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium26" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -821,32 +853,32 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{37EAA098-74C6-4411-B7E2-26AD2DCBC3F0}">
-  <dimension ref="A1:H1"/>
+  <dimension ref="A1:H2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="K1" sqref="K1:T100"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C10" sqref="C10:C11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="8.7265625" style="1"/>
-    <col min="2" max="2" width="15.54296875" style="2" customWidth="1"/>
-    <col min="3" max="3" width="13.36328125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.08984375" style="3" customWidth="1"/>
-    <col min="6" max="6" width="20.90625" style="4" customWidth="1"/>
-    <col min="7" max="7" width="12.1796875" style="2" customWidth="1"/>
-    <col min="8" max="8" width="17.36328125" style="2" customWidth="1"/>
-    <col min="11" max="11" width="9.1796875" customWidth="1"/>
-    <col min="12" max="12" width="13.26953125" customWidth="1"/>
-    <col min="13" max="13" width="11.453125" customWidth="1"/>
-    <col min="14" max="14" width="17.453125" customWidth="1"/>
-    <col min="16" max="16" width="9.1796875" customWidth="1"/>
-    <col min="18" max="18" width="16.54296875" customWidth="1"/>
-    <col min="19" max="19" width="14.7265625" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="16.90625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.5703125" style="2" customWidth="1"/>
+    <col min="3" max="3" width="58" customWidth="1"/>
+    <col min="5" max="5" width="13.140625" style="3" customWidth="1"/>
+    <col min="6" max="6" width="20.85546875" style="4" customWidth="1"/>
+    <col min="7" max="7" width="34.85546875" style="2" customWidth="1"/>
+    <col min="8" max="8" width="43.42578125" style="2" customWidth="1"/>
+    <col min="11" max="11" width="9.140625" customWidth="1"/>
+    <col min="12" max="12" width="13.28515625" customWidth="1"/>
+    <col min="13" max="13" width="11.42578125" customWidth="1"/>
+    <col min="14" max="14" width="17.42578125" customWidth="1"/>
+    <col min="16" max="16" width="9.140625" customWidth="1"/>
+    <col min="18" max="18" width="16.5703125" customWidth="1"/>
+    <col min="19" max="19" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="16.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
@@ -870,6 +902,32 @@
       </c>
       <c r="H1" s="7" t="s">
         <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A2" s="1">
+        <v>45786</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="C2" t="s">
+        <v>16</v>
+      </c>
+      <c r="D2" t="s">
+        <v>17</v>
+      </c>
+      <c r="E2" s="3">
+        <v>1</v>
+      </c>
+      <c r="F2" s="9">
+        <v>4</v>
+      </c>
+      <c r="G2" t="s">
+        <v>18</v>
+      </c>
+      <c r="H2" t="s">
+        <v>19</v>
       </c>
     </row>
   </sheetData>
@@ -885,13 +943,13 @@
       <formula1>1</formula1>
       <formula2>24</formula2>
     </dataValidation>
-    <dataValidation type="list" errorStyle="warning" showInputMessage="1" showErrorMessage="1" errorTitle="Select Status" error="Fill in Status to proccessd " sqref="D2:D16" xr:uid="{C06F6745-3BEF-4E36-9959-47AACC93D371}">
+    <dataValidation type="list" errorStyle="warning" showInputMessage="1" showErrorMessage="1" errorTitle="Select Status" error="Fill in Status to proccessd " sqref="D3:D16" xr:uid="{C06F6745-3BEF-4E36-9959-47AACC93D371}">
       <formula1>"To Do,In Progress,Completed,Blocked"</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <ignoredErrors>
-    <ignoredError sqref="D2:D6 D7:D16" listDataValidation="1"/>
+    <ignoredError sqref="D3:D6 D7:D16" listDataValidation="1"/>
   </ignoredErrors>
   <tableParts count="1">
     <tablePart r:id="rId1"/>
@@ -903,23 +961,23 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3BDA6702-5DDF-42FB-988E-13FBEB26F5C9}">
   <dimension ref="A1:H100"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I34" sqref="I34"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="7.7265625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="17.26953125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.6328125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.5703125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="9" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.81640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="23.6328125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="13.36328125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="19.1796875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="23.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="19.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
@@ -945,15 +1003,13 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="8"/>
       <c r="B2" s="2"/>
       <c r="E2" s="3"/>
-      <c r="F2" s="4"/>
       <c r="G2" s="2"/>
-      <c r="H2" s="2"/>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="8"/>
       <c r="B3" s="2"/>
       <c r="E3" s="3"/>
@@ -961,7 +1017,7 @@
       <c r="G3" s="2"/>
       <c r="H3" s="2"/>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="8"/>
       <c r="B4" s="2"/>
       <c r="E4" s="3"/>
@@ -969,7 +1025,7 @@
       <c r="G4" s="2"/>
       <c r="H4" s="2"/>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="8"/>
       <c r="B5" s="2"/>
       <c r="E5" s="3"/>
@@ -977,7 +1033,7 @@
       <c r="G5" s="2"/>
       <c r="H5" s="2"/>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="8"/>
       <c r="B6" s="2"/>
       <c r="E6" s="3"/>
@@ -985,7 +1041,7 @@
       <c r="G6" s="2"/>
       <c r="H6" s="2"/>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="8"/>
       <c r="B7" s="2"/>
       <c r="E7" s="3"/>
@@ -993,7 +1049,7 @@
       <c r="G7" s="2"/>
       <c r="H7" s="2"/>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="8"/>
       <c r="B8" s="2"/>
       <c r="E8" s="3"/>
@@ -1001,7 +1057,7 @@
       <c r="G8" s="2"/>
       <c r="H8" s="2"/>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="8"/>
       <c r="B9" s="2"/>
       <c r="E9" s="3"/>
@@ -1009,7 +1065,7 @@
       <c r="G9" s="2"/>
       <c r="H9" s="2"/>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="8"/>
       <c r="B10" s="2"/>
       <c r="E10" s="3"/>
@@ -1017,7 +1073,7 @@
       <c r="G10" s="2"/>
       <c r="H10" s="2"/>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="8"/>
       <c r="B11" s="2"/>
       <c r="E11" s="3"/>
@@ -1025,7 +1081,7 @@
       <c r="G11" s="2"/>
       <c r="H11" s="2"/>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="8"/>
       <c r="B12" s="2"/>
       <c r="E12" s="3"/>
@@ -1033,7 +1089,7 @@
       <c r="G12" s="2"/>
       <c r="H12" s="2"/>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="8"/>
       <c r="B13" s="2"/>
       <c r="E13" s="3"/>
@@ -1041,7 +1097,7 @@
       <c r="G13" s="2"/>
       <c r="H13" s="2"/>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" s="8"/>
       <c r="B14" s="2"/>
       <c r="E14" s="3"/>
@@ -1049,7 +1105,7 @@
       <c r="G14" s="2"/>
       <c r="H14" s="2"/>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" s="8"/>
       <c r="B15" s="2"/>
       <c r="E15" s="3"/>
@@ -1057,7 +1113,7 @@
       <c r="G15" s="2"/>
       <c r="H15" s="2"/>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" s="8"/>
       <c r="B16" s="2"/>
       <c r="E16" s="3"/>
@@ -1065,7 +1121,7 @@
       <c r="G16" s="2"/>
       <c r="H16" s="2"/>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" s="8"/>
       <c r="B17" s="2"/>
       <c r="E17" s="3"/>
@@ -1073,7 +1129,7 @@
       <c r="G17" s="2"/>
       <c r="H17" s="2"/>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" s="8"/>
       <c r="B18" s="2"/>
       <c r="E18" s="3"/>
@@ -1081,7 +1137,7 @@
       <c r="G18" s="2"/>
       <c r="H18" s="2"/>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" s="8"/>
       <c r="B19" s="2"/>
       <c r="E19" s="3"/>
@@ -1089,7 +1145,7 @@
       <c r="G19" s="2"/>
       <c r="H19" s="2"/>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" s="8"/>
       <c r="B20" s="2"/>
       <c r="E20" s="3"/>
@@ -1097,7 +1153,7 @@
       <c r="G20" s="2"/>
       <c r="H20" s="2"/>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" s="8"/>
       <c r="B21" s="2"/>
       <c r="E21" s="3"/>
@@ -1105,7 +1161,7 @@
       <c r="G21" s="2"/>
       <c r="H21" s="2"/>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" s="8"/>
       <c r="B22" s="2"/>
       <c r="E22" s="3"/>
@@ -1113,7 +1169,7 @@
       <c r="G22" s="2"/>
       <c r="H22" s="2"/>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" s="8"/>
       <c r="B23" s="2"/>
       <c r="E23" s="3"/>
@@ -1121,7 +1177,7 @@
       <c r="G23" s="2"/>
       <c r="H23" s="2"/>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24" s="8"/>
       <c r="B24" s="2"/>
       <c r="E24" s="3"/>
@@ -1129,7 +1185,7 @@
       <c r="G24" s="2"/>
       <c r="H24" s="2"/>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25" s="8"/>
       <c r="B25" s="2"/>
       <c r="E25" s="3"/>
@@ -1137,7 +1193,7 @@
       <c r="G25" s="2"/>
       <c r="H25" s="2"/>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26" s="8"/>
       <c r="B26" s="2"/>
       <c r="E26" s="3"/>
@@ -1145,7 +1201,7 @@
       <c r="G26" s="2"/>
       <c r="H26" s="2"/>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A27" s="8"/>
       <c r="B27" s="2"/>
       <c r="E27" s="3"/>
@@ -1153,7 +1209,7 @@
       <c r="G27" s="2"/>
       <c r="H27" s="2"/>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A28" s="8"/>
       <c r="B28" s="2"/>
       <c r="E28" s="3"/>
@@ -1161,7 +1217,7 @@
       <c r="G28" s="2"/>
       <c r="H28" s="2"/>
     </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A29" s="8"/>
       <c r="B29" s="2"/>
       <c r="E29" s="3"/>
@@ -1169,7 +1225,7 @@
       <c r="G29" s="2"/>
       <c r="H29" s="2"/>
     </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A30" s="8"/>
       <c r="B30" s="2"/>
       <c r="E30" s="3"/>
@@ -1177,7 +1233,7 @@
       <c r="G30" s="2"/>
       <c r="H30" s="2"/>
     </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A31" s="8"/>
       <c r="B31" s="2"/>
       <c r="E31" s="3"/>
@@ -1185,7 +1241,7 @@
       <c r="G31" s="2"/>
       <c r="H31" s="2"/>
     </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A32" s="8"/>
       <c r="B32" s="2"/>
       <c r="E32" s="3"/>
@@ -1193,7 +1249,7 @@
       <c r="G32" s="2"/>
       <c r="H32" s="2"/>
     </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A33" s="8"/>
       <c r="B33" s="2"/>
       <c r="E33" s="3"/>
@@ -1201,7 +1257,7 @@
       <c r="G33" s="2"/>
       <c r="H33" s="2"/>
     </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A34" s="8"/>
       <c r="B34" s="2"/>
       <c r="E34" s="3"/>
@@ -1209,7 +1265,7 @@
       <c r="G34" s="2"/>
       <c r="H34" s="2"/>
     </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A35" s="8"/>
       <c r="B35" s="2"/>
       <c r="E35" s="3"/>
@@ -1217,7 +1273,7 @@
       <c r="G35" s="2"/>
       <c r="H35" s="2"/>
     </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A36" s="8"/>
       <c r="B36" s="2"/>
       <c r="E36" s="3"/>
@@ -1225,7 +1281,7 @@
       <c r="G36" s="2"/>
       <c r="H36" s="2"/>
     </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A37" s="8"/>
       <c r="B37" s="2"/>
       <c r="E37" s="3"/>
@@ -1233,7 +1289,7 @@
       <c r="G37" s="2"/>
       <c r="H37" s="2"/>
     </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A38" s="8"/>
       <c r="B38" s="2"/>
       <c r="E38" s="3"/>
@@ -1241,7 +1297,7 @@
       <c r="G38" s="2"/>
       <c r="H38" s="2"/>
     </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A39" s="8"/>
       <c r="B39" s="2"/>
       <c r="E39" s="3"/>
@@ -1249,7 +1305,7 @@
       <c r="G39" s="2"/>
       <c r="H39" s="2"/>
     </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A40" s="8"/>
       <c r="B40" s="2"/>
       <c r="E40" s="3"/>
@@ -1257,7 +1313,7 @@
       <c r="G40" s="2"/>
       <c r="H40" s="2"/>
     </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A41" s="8"/>
       <c r="B41" s="2"/>
       <c r="E41" s="3"/>
@@ -1265,7 +1321,7 @@
       <c r="G41" s="2"/>
       <c r="H41" s="2"/>
     </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A42" s="8"/>
       <c r="B42" s="2"/>
       <c r="E42" s="3"/>
@@ -1273,7 +1329,7 @@
       <c r="G42" s="2"/>
       <c r="H42" s="2"/>
     </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A43" s="8"/>
       <c r="B43" s="2"/>
       <c r="E43" s="3"/>
@@ -1281,7 +1337,7 @@
       <c r="G43" s="2"/>
       <c r="H43" s="2"/>
     </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A44" s="8"/>
       <c r="B44" s="2"/>
       <c r="E44" s="3"/>
@@ -1289,7 +1345,7 @@
       <c r="G44" s="2"/>
       <c r="H44" s="2"/>
     </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A45" s="8"/>
       <c r="B45" s="2"/>
       <c r="E45" s="3"/>
@@ -1297,7 +1353,7 @@
       <c r="G45" s="2"/>
       <c r="H45" s="2"/>
     </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A46" s="8"/>
       <c r="B46" s="2"/>
       <c r="E46" s="3"/>
@@ -1305,7 +1361,7 @@
       <c r="G46" s="2"/>
       <c r="H46" s="2"/>
     </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A47" s="8"/>
       <c r="B47" s="2"/>
       <c r="E47" s="3"/>
@@ -1313,7 +1369,7 @@
       <c r="G47" s="2"/>
       <c r="H47" s="2"/>
     </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A48" s="8"/>
       <c r="B48" s="2"/>
       <c r="E48" s="3"/>
@@ -1321,7 +1377,7 @@
       <c r="G48" s="2"/>
       <c r="H48" s="2"/>
     </row>
-    <row r="49" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A49" s="8"/>
       <c r="B49" s="2"/>
       <c r="E49" s="3"/>
@@ -1329,7 +1385,7 @@
       <c r="G49" s="2"/>
       <c r="H49" s="2"/>
     </row>
-    <row r="50" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A50" s="8"/>
       <c r="B50" s="2"/>
       <c r="E50" s="3"/>
@@ -1337,7 +1393,7 @@
       <c r="G50" s="2"/>
       <c r="H50" s="2"/>
     </row>
-    <row r="51" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A51" s="8"/>
       <c r="B51" s="2"/>
       <c r="E51" s="3"/>
@@ -1345,7 +1401,7 @@
       <c r="G51" s="2"/>
       <c r="H51" s="2"/>
     </row>
-    <row r="52" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A52" s="8"/>
       <c r="B52" s="2"/>
       <c r="E52" s="3"/>
@@ -1353,7 +1409,7 @@
       <c r="G52" s="2"/>
       <c r="H52" s="2"/>
     </row>
-    <row r="53" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A53" s="8"/>
       <c r="B53" s="2"/>
       <c r="E53" s="3"/>
@@ -1361,7 +1417,7 @@
       <c r="G53" s="2"/>
       <c r="H53" s="2"/>
     </row>
-    <row r="54" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A54" s="8"/>
       <c r="B54" s="2"/>
       <c r="E54" s="3"/>
@@ -1369,7 +1425,7 @@
       <c r="G54" s="2"/>
       <c r="H54" s="2"/>
     </row>
-    <row r="55" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A55" s="8"/>
       <c r="B55" s="2"/>
       <c r="E55" s="3"/>
@@ -1377,7 +1433,7 @@
       <c r="G55" s="2"/>
       <c r="H55" s="2"/>
     </row>
-    <row r="56" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A56" s="8"/>
       <c r="B56" s="2"/>
       <c r="E56" s="3"/>
@@ -1385,7 +1441,7 @@
       <c r="G56" s="2"/>
       <c r="H56" s="2"/>
     </row>
-    <row r="57" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A57" s="8"/>
       <c r="B57" s="2"/>
       <c r="E57" s="3"/>
@@ -1393,7 +1449,7 @@
       <c r="G57" s="2"/>
       <c r="H57" s="2"/>
     </row>
-    <row r="58" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A58" s="8"/>
       <c r="B58" s="2"/>
       <c r="E58" s="3"/>
@@ -1401,7 +1457,7 @@
       <c r="G58" s="2"/>
       <c r="H58" s="2"/>
     </row>
-    <row r="59" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A59" s="8"/>
       <c r="B59" s="2"/>
       <c r="E59" s="3"/>
@@ -1409,7 +1465,7 @@
       <c r="G59" s="2"/>
       <c r="H59" s="2"/>
     </row>
-    <row r="60" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A60" s="8"/>
       <c r="B60" s="2"/>
       <c r="E60" s="3"/>
@@ -1417,7 +1473,7 @@
       <c r="G60" s="2"/>
       <c r="H60" s="2"/>
     </row>
-    <row r="61" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A61" s="8"/>
       <c r="B61" s="2"/>
       <c r="E61" s="3"/>
@@ -1425,7 +1481,7 @@
       <c r="G61" s="2"/>
       <c r="H61" s="2"/>
     </row>
-    <row r="62" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A62" s="8"/>
       <c r="B62" s="2"/>
       <c r="E62" s="3"/>
@@ -1433,7 +1489,7 @@
       <c r="G62" s="2"/>
       <c r="H62" s="2"/>
     </row>
-    <row r="63" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A63" s="8"/>
       <c r="B63" s="2"/>
       <c r="E63" s="3"/>
@@ -1441,7 +1497,7 @@
       <c r="G63" s="2"/>
       <c r="H63" s="2"/>
     </row>
-    <row r="64" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A64" s="8"/>
       <c r="B64" s="2"/>
       <c r="E64" s="3"/>
@@ -1449,7 +1505,7 @@
       <c r="G64" s="2"/>
       <c r="H64" s="2"/>
     </row>
-    <row r="65" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A65" s="8"/>
       <c r="B65" s="2"/>
       <c r="E65" s="3"/>
@@ -1457,7 +1513,7 @@
       <c r="G65" s="2"/>
       <c r="H65" s="2"/>
     </row>
-    <row r="66" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A66" s="8"/>
       <c r="B66" s="2"/>
       <c r="E66" s="3"/>
@@ -1465,7 +1521,7 @@
       <c r="G66" s="2"/>
       <c r="H66" s="2"/>
     </row>
-    <row r="67" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A67" s="8"/>
       <c r="B67" s="2"/>
       <c r="E67" s="3"/>
@@ -1473,7 +1529,7 @@
       <c r="G67" s="2"/>
       <c r="H67" s="2"/>
     </row>
-    <row r="68" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A68" s="8"/>
       <c r="B68" s="2"/>
       <c r="E68" s="3"/>
@@ -1481,7 +1537,7 @@
       <c r="G68" s="2"/>
       <c r="H68" s="2"/>
     </row>
-    <row r="69" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A69" s="8"/>
       <c r="B69" s="2"/>
       <c r="E69" s="3"/>
@@ -1489,7 +1545,7 @@
       <c r="G69" s="2"/>
       <c r="H69" s="2"/>
     </row>
-    <row r="70" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A70" s="8"/>
       <c r="B70" s="2"/>
       <c r="E70" s="3"/>
@@ -1497,7 +1553,7 @@
       <c r="G70" s="2"/>
       <c r="H70" s="2"/>
     </row>
-    <row r="71" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A71" s="8"/>
       <c r="B71" s="2"/>
       <c r="E71" s="3"/>
@@ -1505,7 +1561,7 @@
       <c r="G71" s="2"/>
       <c r="H71" s="2"/>
     </row>
-    <row r="72" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A72" s="8"/>
       <c r="B72" s="2"/>
       <c r="E72" s="3"/>
@@ -1513,7 +1569,7 @@
       <c r="G72" s="2"/>
       <c r="H72" s="2"/>
     </row>
-    <row r="73" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A73" s="8"/>
       <c r="B73" s="2"/>
       <c r="E73" s="3"/>
@@ -1521,7 +1577,7 @@
       <c r="G73" s="2"/>
       <c r="H73" s="2"/>
     </row>
-    <row r="74" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A74" s="8"/>
       <c r="B74" s="2"/>
       <c r="E74" s="3"/>
@@ -1529,7 +1585,7 @@
       <c r="G74" s="2"/>
       <c r="H74" s="2"/>
     </row>
-    <row r="75" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A75" s="8"/>
       <c r="B75" s="2"/>
       <c r="E75" s="3"/>
@@ -1537,7 +1593,7 @@
       <c r="G75" s="2"/>
       <c r="H75" s="2"/>
     </row>
-    <row r="76" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="76" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A76" s="8"/>
       <c r="B76" s="2"/>
       <c r="E76" s="3"/>
@@ -1545,7 +1601,7 @@
       <c r="G76" s="2"/>
       <c r="H76" s="2"/>
     </row>
-    <row r="77" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="77" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A77" s="8"/>
       <c r="B77" s="2"/>
       <c r="E77" s="3"/>
@@ -1553,7 +1609,7 @@
       <c r="G77" s="2"/>
       <c r="H77" s="2"/>
     </row>
-    <row r="78" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="78" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A78" s="8"/>
       <c r="B78" s="2"/>
       <c r="E78" s="3"/>
@@ -1561,7 +1617,7 @@
       <c r="G78" s="2"/>
       <c r="H78" s="2"/>
     </row>
-    <row r="79" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="79" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A79" s="8"/>
       <c r="B79" s="2"/>
       <c r="E79" s="3"/>
@@ -1569,7 +1625,7 @@
       <c r="G79" s="2"/>
       <c r="H79" s="2"/>
     </row>
-    <row r="80" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="80" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A80" s="8"/>
       <c r="B80" s="2"/>
       <c r="E80" s="3"/>
@@ -1577,7 +1633,7 @@
       <c r="G80" s="2"/>
       <c r="H80" s="2"/>
     </row>
-    <row r="81" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="81" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A81" s="8"/>
       <c r="B81" s="2"/>
       <c r="E81" s="3"/>
@@ -1585,7 +1641,7 @@
       <c r="G81" s="2"/>
       <c r="H81" s="2"/>
     </row>
-    <row r="82" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="82" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A82" s="8"/>
       <c r="B82" s="2"/>
       <c r="E82" s="3"/>
@@ -1593,7 +1649,7 @@
       <c r="G82" s="2"/>
       <c r="H82" s="2"/>
     </row>
-    <row r="83" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="83" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A83" s="8"/>
       <c r="B83" s="2"/>
       <c r="E83" s="3"/>
@@ -1601,7 +1657,7 @@
       <c r="G83" s="2"/>
       <c r="H83" s="2"/>
     </row>
-    <row r="84" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="84" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A84" s="8"/>
       <c r="B84" s="2"/>
       <c r="E84" s="3"/>
@@ -1609,7 +1665,7 @@
       <c r="G84" s="2"/>
       <c r="H84" s="2"/>
     </row>
-    <row r="85" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="85" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A85" s="8"/>
       <c r="B85" s="2"/>
       <c r="E85" s="3"/>
@@ -1617,7 +1673,7 @@
       <c r="G85" s="2"/>
       <c r="H85" s="2"/>
     </row>
-    <row r="86" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="86" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A86" s="8"/>
       <c r="B86" s="2"/>
       <c r="E86" s="3"/>
@@ -1625,7 +1681,7 @@
       <c r="G86" s="2"/>
       <c r="H86" s="2"/>
     </row>
-    <row r="87" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="87" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A87" s="8"/>
       <c r="B87" s="2"/>
       <c r="E87" s="3"/>
@@ -1633,7 +1689,7 @@
       <c r="G87" s="2"/>
       <c r="H87" s="2"/>
     </row>
-    <row r="88" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="88" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A88" s="8"/>
       <c r="B88" s="2"/>
       <c r="E88" s="3"/>
@@ -1641,7 +1697,7 @@
       <c r="G88" s="2"/>
       <c r="H88" s="2"/>
     </row>
-    <row r="89" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="89" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A89" s="8"/>
       <c r="B89" s="2"/>
       <c r="E89" s="3"/>
@@ -1649,7 +1705,7 @@
       <c r="G89" s="2"/>
       <c r="H89" s="2"/>
     </row>
-    <row r="90" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="90" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A90" s="8"/>
       <c r="B90" s="2"/>
       <c r="E90" s="3"/>
@@ -1657,7 +1713,7 @@
       <c r="G90" s="2"/>
       <c r="H90" s="2"/>
     </row>
-    <row r="91" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="91" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A91" s="8"/>
       <c r="B91" s="2"/>
       <c r="E91" s="3"/>
@@ -1665,7 +1721,7 @@
       <c r="G91" s="2"/>
       <c r="H91" s="2"/>
     </row>
-    <row r="92" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="92" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A92" s="8"/>
       <c r="B92" s="2"/>
       <c r="E92" s="3"/>
@@ -1673,7 +1729,7 @@
       <c r="G92" s="2"/>
       <c r="H92" s="2"/>
     </row>
-    <row r="93" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="93" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A93" s="8"/>
       <c r="B93" s="2"/>
       <c r="E93" s="3"/>
@@ -1681,7 +1737,7 @@
       <c r="G93" s="2"/>
       <c r="H93" s="2"/>
     </row>
-    <row r="94" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="94" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A94" s="8"/>
       <c r="B94" s="2"/>
       <c r="E94" s="3"/>
@@ -1689,7 +1745,7 @@
       <c r="G94" s="2"/>
       <c r="H94" s="2"/>
     </row>
-    <row r="95" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="95" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A95" s="8"/>
       <c r="B95" s="2"/>
       <c r="E95" s="3"/>
@@ -1697,7 +1753,7 @@
       <c r="G95" s="2"/>
       <c r="H95" s="2"/>
     </row>
-    <row r="96" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="96" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A96" s="8"/>
       <c r="B96" s="2"/>
       <c r="E96" s="3"/>
@@ -1705,7 +1761,7 @@
       <c r="G96" s="2"/>
       <c r="H96" s="2"/>
     </row>
-    <row r="97" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="97" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A97" s="8"/>
       <c r="B97" s="2"/>
       <c r="E97" s="3"/>
@@ -1713,7 +1769,7 @@
       <c r="G97" s="2"/>
       <c r="H97" s="2"/>
     </row>
-    <row r="98" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="98" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A98" s="8"/>
       <c r="B98" s="2"/>
       <c r="E98" s="3"/>
@@ -1721,7 +1777,7 @@
       <c r="G98" s="2"/>
       <c r="H98" s="2"/>
     </row>
-    <row r="99" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="99" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A99" s="8"/>
       <c r="B99" s="2"/>
       <c r="E99" s="3"/>
@@ -1729,7 +1785,7 @@
       <c r="G99" s="2"/>
       <c r="H99" s="2"/>
     </row>
-    <row r="100" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="100" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A100" s="8"/>
       <c r="B100" s="2"/>
       <c r="E100" s="3"/>
@@ -1739,10 +1795,10 @@
     </row>
   </sheetData>
   <dataValidations count="4">
-    <dataValidation type="list" errorStyle="warning" showInputMessage="1" showErrorMessage="1" errorTitle="Select Status" error="Fill in Status to proccessd " sqref="D2:D16" xr:uid="{45147164-8A29-4CAF-A2DB-395497B89382}">
+    <dataValidation type="list" errorStyle="warning" showInputMessage="1" showErrorMessage="1" errorTitle="Select Status" error="Fill in Status to proccessd " sqref="D3:D16" xr:uid="{45147164-8A29-4CAF-A2DB-395497B89382}">
       <formula1>"To Do,In Progress,Completed,Blocked"</formula1>
     </dataValidation>
-    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F2:F100" xr:uid="{22EE2D3D-9C8A-455C-B524-020B4CD90E60}">
+    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F3:F100" xr:uid="{22EE2D3D-9C8A-455C-B524-020B4CD90E60}">
       <formula1>1</formula1>
       <formula2>24</formula2>
     </dataValidation>
@@ -1756,7 +1812,7 @@
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <ignoredErrors>
-    <ignoredError sqref="D2:D100" listDataValidation="1"/>
+    <ignoredError sqref="D3:D100" listDataValidation="1"/>
   </ignoredErrors>
   <tableParts count="1">
     <tablePart r:id="rId1"/>
@@ -1772,19 +1828,19 @@
       <selection activeCell="D2" sqref="D2:D100"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="7.7265625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="17.26953125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.6328125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="7.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.5703125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="9" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.81640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="23.6328125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="13.36328125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="19.1796875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="23.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="19.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
@@ -1810,7 +1866,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="1"/>
       <c r="B2" s="2"/>
       <c r="E2" s="3"/>
@@ -1818,7 +1874,7 @@
       <c r="G2" s="2"/>
       <c r="H2" s="2"/>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="1"/>
       <c r="B3" s="2"/>
       <c r="E3" s="3"/>
@@ -1826,7 +1882,7 @@
       <c r="G3" s="2"/>
       <c r="H3" s="2"/>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="1"/>
       <c r="B4" s="2"/>
       <c r="E4" s="3"/>
@@ -1834,7 +1890,7 @@
       <c r="G4" s="2"/>
       <c r="H4" s="2"/>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="1"/>
       <c r="B5" s="2"/>
       <c r="E5" s="3"/>
@@ -1842,7 +1898,7 @@
       <c r="G5" s="2"/>
       <c r="H5" s="2"/>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="1"/>
       <c r="B6" s="2"/>
       <c r="E6" s="3"/>
@@ -1850,7 +1906,7 @@
       <c r="G6" s="2"/>
       <c r="H6" s="2"/>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="1"/>
       <c r="B7" s="2"/>
       <c r="E7" s="3"/>
@@ -1858,7 +1914,7 @@
       <c r="G7" s="2"/>
       <c r="H7" s="2"/>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="1"/>
       <c r="B8" s="2"/>
       <c r="E8" s="3"/>
@@ -1866,7 +1922,7 @@
       <c r="G8" s="2"/>
       <c r="H8" s="2"/>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="1"/>
       <c r="B9" s="2"/>
       <c r="E9" s="3"/>
@@ -1874,7 +1930,7 @@
       <c r="G9" s="2"/>
       <c r="H9" s="2"/>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="1"/>
       <c r="B10" s="2"/>
       <c r="E10" s="3"/>
@@ -1882,7 +1938,7 @@
       <c r="G10" s="2"/>
       <c r="H10" s="2"/>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="1"/>
       <c r="B11" s="2"/>
       <c r="E11" s="3"/>
@@ -1890,7 +1946,7 @@
       <c r="G11" s="2"/>
       <c r="H11" s="2"/>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="1"/>
       <c r="B12" s="2"/>
       <c r="E12" s="3"/>
@@ -1898,7 +1954,7 @@
       <c r="G12" s="2"/>
       <c r="H12" s="2"/>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="1"/>
       <c r="B13" s="2"/>
       <c r="E13" s="3"/>
@@ -1906,7 +1962,7 @@
       <c r="G13" s="2"/>
       <c r="H13" s="2"/>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" s="1"/>
       <c r="B14" s="2"/>
       <c r="E14" s="3"/>
@@ -1914,7 +1970,7 @@
       <c r="G14" s="2"/>
       <c r="H14" s="2"/>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" s="1"/>
       <c r="B15" s="2"/>
       <c r="E15" s="3"/>
@@ -1922,7 +1978,7 @@
       <c r="G15" s="2"/>
       <c r="H15" s="2"/>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" s="1"/>
       <c r="B16" s="2"/>
       <c r="E16" s="3"/>
@@ -1930,7 +1986,7 @@
       <c r="G16" s="2"/>
       <c r="H16" s="2"/>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" s="1"/>
       <c r="B17" s="2"/>
       <c r="E17" s="3"/>
@@ -1938,7 +1994,7 @@
       <c r="G17" s="2"/>
       <c r="H17" s="2"/>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" s="1"/>
       <c r="B18" s="2"/>
       <c r="E18" s="3"/>
@@ -1946,7 +2002,7 @@
       <c r="G18" s="2"/>
       <c r="H18" s="2"/>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" s="1"/>
       <c r="B19" s="2"/>
       <c r="E19" s="3"/>
@@ -1954,7 +2010,7 @@
       <c r="G19" s="2"/>
       <c r="H19" s="2"/>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" s="1"/>
       <c r="B20" s="2"/>
       <c r="E20" s="3"/>
@@ -1962,7 +2018,7 @@
       <c r="G20" s="2"/>
       <c r="H20" s="2"/>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" s="1"/>
       <c r="B21" s="2"/>
       <c r="E21" s="3"/>
@@ -1970,7 +2026,7 @@
       <c r="G21" s="2"/>
       <c r="H21" s="2"/>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" s="1"/>
       <c r="B22" s="2"/>
       <c r="E22" s="3"/>
@@ -1978,7 +2034,7 @@
       <c r="G22" s="2"/>
       <c r="H22" s="2"/>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" s="1"/>
       <c r="B23" s="2"/>
       <c r="E23" s="3"/>
@@ -1986,7 +2042,7 @@
       <c r="G23" s="2"/>
       <c r="H23" s="2"/>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24" s="1"/>
       <c r="B24" s="2"/>
       <c r="E24" s="3"/>
@@ -1994,7 +2050,7 @@
       <c r="G24" s="2"/>
       <c r="H24" s="2"/>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25" s="1"/>
       <c r="B25" s="2"/>
       <c r="E25" s="3"/>
@@ -2002,7 +2058,7 @@
       <c r="G25" s="2"/>
       <c r="H25" s="2"/>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26" s="1"/>
       <c r="B26" s="2"/>
       <c r="E26" s="3"/>
@@ -2010,7 +2066,7 @@
       <c r="G26" s="2"/>
       <c r="H26" s="2"/>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A27" s="1"/>
       <c r="B27" s="2"/>
       <c r="E27" s="3"/>
@@ -2018,7 +2074,7 @@
       <c r="G27" s="2"/>
       <c r="H27" s="2"/>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A28" s="1"/>
       <c r="B28" s="2"/>
       <c r="E28" s="3"/>
@@ -2026,7 +2082,7 @@
       <c r="G28" s="2"/>
       <c r="H28" s="2"/>
     </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A29" s="1"/>
       <c r="B29" s="2"/>
       <c r="E29" s="3"/>
@@ -2034,7 +2090,7 @@
       <c r="G29" s="2"/>
       <c r="H29" s="2"/>
     </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A30" s="1"/>
       <c r="B30" s="2"/>
       <c r="E30" s="3"/>
@@ -2042,7 +2098,7 @@
       <c r="G30" s="2"/>
       <c r="H30" s="2"/>
     </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A31" s="1"/>
       <c r="B31" s="2"/>
       <c r="E31" s="3"/>
@@ -2050,7 +2106,7 @@
       <c r="G31" s="2"/>
       <c r="H31" s="2"/>
     </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A32" s="1"/>
       <c r="B32" s="2"/>
       <c r="E32" s="3"/>
@@ -2058,7 +2114,7 @@
       <c r="G32" s="2"/>
       <c r="H32" s="2"/>
     </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A33" s="1"/>
       <c r="B33" s="2"/>
       <c r="E33" s="3"/>
@@ -2066,7 +2122,7 @@
       <c r="G33" s="2"/>
       <c r="H33" s="2"/>
     </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A34" s="1"/>
       <c r="B34" s="2"/>
       <c r="E34" s="3"/>
@@ -2074,7 +2130,7 @@
       <c r="G34" s="2"/>
       <c r="H34" s="2"/>
     </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A35" s="1"/>
       <c r="B35" s="2"/>
       <c r="E35" s="3"/>
@@ -2082,7 +2138,7 @@
       <c r="G35" s="2"/>
       <c r="H35" s="2"/>
     </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A36" s="1"/>
       <c r="B36" s="2"/>
       <c r="E36" s="3"/>
@@ -2090,7 +2146,7 @@
       <c r="G36" s="2"/>
       <c r="H36" s="2"/>
     </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A37" s="1"/>
       <c r="B37" s="2"/>
       <c r="E37" s="3"/>
@@ -2098,7 +2154,7 @@
       <c r="G37" s="2"/>
       <c r="H37" s="2"/>
     </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A38" s="1"/>
       <c r="B38" s="2"/>
       <c r="E38" s="3"/>
@@ -2106,7 +2162,7 @@
       <c r="G38" s="2"/>
       <c r="H38" s="2"/>
     </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A39" s="1"/>
       <c r="B39" s="2"/>
       <c r="E39" s="3"/>
@@ -2114,7 +2170,7 @@
       <c r="G39" s="2"/>
       <c r="H39" s="2"/>
     </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A40" s="1"/>
       <c r="B40" s="2"/>
       <c r="E40" s="3"/>
@@ -2122,7 +2178,7 @@
       <c r="G40" s="2"/>
       <c r="H40" s="2"/>
     </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A41" s="1"/>
       <c r="B41" s="2"/>
       <c r="E41" s="3"/>
@@ -2130,7 +2186,7 @@
       <c r="G41" s="2"/>
       <c r="H41" s="2"/>
     </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A42" s="1"/>
       <c r="B42" s="2"/>
       <c r="E42" s="3"/>
@@ -2138,7 +2194,7 @@
       <c r="G42" s="2"/>
       <c r="H42" s="2"/>
     </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A43" s="1"/>
       <c r="B43" s="2"/>
       <c r="E43" s="3"/>
@@ -2146,7 +2202,7 @@
       <c r="G43" s="2"/>
       <c r="H43" s="2"/>
     </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A44" s="1"/>
       <c r="B44" s="2"/>
       <c r="E44" s="3"/>
@@ -2154,7 +2210,7 @@
       <c r="G44" s="2"/>
       <c r="H44" s="2"/>
     </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A45" s="1"/>
       <c r="B45" s="2"/>
       <c r="E45" s="3"/>
@@ -2162,7 +2218,7 @@
       <c r="G45" s="2"/>
       <c r="H45" s="2"/>
     </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A46" s="1"/>
       <c r="B46" s="2"/>
       <c r="E46" s="3"/>
@@ -2170,7 +2226,7 @@
       <c r="G46" s="2"/>
       <c r="H46" s="2"/>
     </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A47" s="1"/>
       <c r="B47" s="2"/>
       <c r="E47" s="3"/>
@@ -2178,7 +2234,7 @@
       <c r="G47" s="2"/>
       <c r="H47" s="2"/>
     </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A48" s="1"/>
       <c r="B48" s="2"/>
       <c r="E48" s="3"/>
@@ -2186,7 +2242,7 @@
       <c r="G48" s="2"/>
       <c r="H48" s="2"/>
     </row>
-    <row r="49" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A49" s="1"/>
       <c r="B49" s="2"/>
       <c r="E49" s="3"/>
@@ -2194,7 +2250,7 @@
       <c r="G49" s="2"/>
       <c r="H49" s="2"/>
     </row>
-    <row r="50" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A50" s="1"/>
       <c r="B50" s="2"/>
       <c r="E50" s="3"/>
@@ -2202,7 +2258,7 @@
       <c r="G50" s="2"/>
       <c r="H50" s="2"/>
     </row>
-    <row r="51" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A51" s="1"/>
       <c r="B51" s="2"/>
       <c r="E51" s="3"/>
@@ -2210,7 +2266,7 @@
       <c r="G51" s="2"/>
       <c r="H51" s="2"/>
     </row>
-    <row r="52" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A52" s="1"/>
       <c r="B52" s="2"/>
       <c r="E52" s="3"/>
@@ -2218,7 +2274,7 @@
       <c r="G52" s="2"/>
       <c r="H52" s="2"/>
     </row>
-    <row r="53" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A53" s="1"/>
       <c r="B53" s="2"/>
       <c r="E53" s="3"/>
@@ -2226,7 +2282,7 @@
       <c r="G53" s="2"/>
       <c r="H53" s="2"/>
     </row>
-    <row r="54" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A54" s="1"/>
       <c r="B54" s="2"/>
       <c r="E54" s="3"/>
@@ -2234,7 +2290,7 @@
       <c r="G54" s="2"/>
       <c r="H54" s="2"/>
     </row>
-    <row r="55" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A55" s="1"/>
       <c r="B55" s="2"/>
       <c r="E55" s="3"/>
@@ -2242,7 +2298,7 @@
       <c r="G55" s="2"/>
       <c r="H55" s="2"/>
     </row>
-    <row r="56" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A56" s="1"/>
       <c r="B56" s="2"/>
       <c r="E56" s="3"/>
@@ -2250,7 +2306,7 @@
       <c r="G56" s="2"/>
       <c r="H56" s="2"/>
     </row>
-    <row r="57" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A57" s="1"/>
       <c r="B57" s="2"/>
       <c r="E57" s="3"/>
@@ -2258,7 +2314,7 @@
       <c r="G57" s="2"/>
       <c r="H57" s="2"/>
     </row>
-    <row r="58" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A58" s="1"/>
       <c r="B58" s="2"/>
       <c r="E58" s="3"/>
@@ -2266,7 +2322,7 @@
       <c r="G58" s="2"/>
       <c r="H58" s="2"/>
     </row>
-    <row r="59" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A59" s="1"/>
       <c r="B59" s="2"/>
       <c r="E59" s="3"/>
@@ -2274,7 +2330,7 @@
       <c r="G59" s="2"/>
       <c r="H59" s="2"/>
     </row>
-    <row r="60" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A60" s="1"/>
       <c r="B60" s="2"/>
       <c r="E60" s="3"/>
@@ -2282,7 +2338,7 @@
       <c r="G60" s="2"/>
       <c r="H60" s="2"/>
     </row>
-    <row r="61" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A61" s="1"/>
       <c r="B61" s="2"/>
       <c r="E61" s="3"/>
@@ -2290,7 +2346,7 @@
       <c r="G61" s="2"/>
       <c r="H61" s="2"/>
     </row>
-    <row r="62" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A62" s="1"/>
       <c r="B62" s="2"/>
       <c r="E62" s="3"/>
@@ -2298,7 +2354,7 @@
       <c r="G62" s="2"/>
       <c r="H62" s="2"/>
     </row>
-    <row r="63" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A63" s="1"/>
       <c r="B63" s="2"/>
       <c r="E63" s="3"/>
@@ -2306,7 +2362,7 @@
       <c r="G63" s="2"/>
       <c r="H63" s="2"/>
     </row>
-    <row r="64" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A64" s="1"/>
       <c r="B64" s="2"/>
       <c r="E64" s="3"/>
@@ -2314,7 +2370,7 @@
       <c r="G64" s="2"/>
       <c r="H64" s="2"/>
     </row>
-    <row r="65" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A65" s="1"/>
       <c r="B65" s="2"/>
       <c r="E65" s="3"/>
@@ -2322,7 +2378,7 @@
       <c r="G65" s="2"/>
       <c r="H65" s="2"/>
     </row>
-    <row r="66" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A66" s="1"/>
       <c r="B66" s="2"/>
       <c r="E66" s="3"/>
@@ -2330,7 +2386,7 @@
       <c r="G66" s="2"/>
       <c r="H66" s="2"/>
     </row>
-    <row r="67" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A67" s="1"/>
       <c r="B67" s="2"/>
       <c r="E67" s="3"/>
@@ -2338,7 +2394,7 @@
       <c r="G67" s="2"/>
       <c r="H67" s="2"/>
     </row>
-    <row r="68" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A68" s="1"/>
       <c r="B68" s="2"/>
       <c r="E68" s="3"/>
@@ -2346,7 +2402,7 @@
       <c r="G68" s="2"/>
       <c r="H68" s="2"/>
     </row>
-    <row r="69" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A69" s="1"/>
       <c r="B69" s="2"/>
       <c r="E69" s="3"/>
@@ -2354,7 +2410,7 @@
       <c r="G69" s="2"/>
       <c r="H69" s="2"/>
     </row>
-    <row r="70" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A70" s="1"/>
       <c r="B70" s="2"/>
       <c r="E70" s="3"/>
@@ -2362,7 +2418,7 @@
       <c r="G70" s="2"/>
       <c r="H70" s="2"/>
     </row>
-    <row r="71" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A71" s="1"/>
       <c r="B71" s="2"/>
       <c r="E71" s="3"/>
@@ -2370,7 +2426,7 @@
       <c r="G71" s="2"/>
       <c r="H71" s="2"/>
     </row>
-    <row r="72" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A72" s="1"/>
       <c r="B72" s="2"/>
       <c r="E72" s="3"/>
@@ -2378,7 +2434,7 @@
       <c r="G72" s="2"/>
       <c r="H72" s="2"/>
     </row>
-    <row r="73" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A73" s="1"/>
       <c r="B73" s="2"/>
       <c r="E73" s="3"/>
@@ -2386,7 +2442,7 @@
       <c r="G73" s="2"/>
       <c r="H73" s="2"/>
     </row>
-    <row r="74" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A74" s="1"/>
       <c r="B74" s="2"/>
       <c r="E74" s="3"/>
@@ -2394,7 +2450,7 @@
       <c r="G74" s="2"/>
       <c r="H74" s="2"/>
     </row>
-    <row r="75" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A75" s="1"/>
       <c r="B75" s="2"/>
       <c r="E75" s="3"/>
@@ -2402,7 +2458,7 @@
       <c r="G75" s="2"/>
       <c r="H75" s="2"/>
     </row>
-    <row r="76" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="76" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A76" s="1"/>
       <c r="B76" s="2"/>
       <c r="E76" s="3"/>
@@ -2410,7 +2466,7 @@
       <c r="G76" s="2"/>
       <c r="H76" s="2"/>
     </row>
-    <row r="77" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="77" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A77" s="1"/>
       <c r="B77" s="2"/>
       <c r="E77" s="3"/>
@@ -2418,7 +2474,7 @@
       <c r="G77" s="2"/>
       <c r="H77" s="2"/>
     </row>
-    <row r="78" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="78" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A78" s="1"/>
       <c r="B78" s="2"/>
       <c r="E78" s="3"/>
@@ -2426,7 +2482,7 @@
       <c r="G78" s="2"/>
       <c r="H78" s="2"/>
     </row>
-    <row r="79" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="79" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A79" s="1"/>
       <c r="B79" s="2"/>
       <c r="E79" s="3"/>
@@ -2434,7 +2490,7 @@
       <c r="G79" s="2"/>
       <c r="H79" s="2"/>
     </row>
-    <row r="80" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="80" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A80" s="1"/>
       <c r="B80" s="2"/>
       <c r="E80" s="3"/>
@@ -2442,7 +2498,7 @@
       <c r="G80" s="2"/>
       <c r="H80" s="2"/>
     </row>
-    <row r="81" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="81" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A81" s="1"/>
       <c r="B81" s="2"/>
       <c r="E81" s="3"/>
@@ -2450,7 +2506,7 @@
       <c r="G81" s="2"/>
       <c r="H81" s="2"/>
     </row>
-    <row r="82" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="82" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A82" s="1"/>
       <c r="B82" s="2"/>
       <c r="E82" s="3"/>
@@ -2458,7 +2514,7 @@
       <c r="G82" s="2"/>
       <c r="H82" s="2"/>
     </row>
-    <row r="83" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="83" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A83" s="1"/>
       <c r="B83" s="2"/>
       <c r="E83" s="3"/>
@@ -2466,7 +2522,7 @@
       <c r="G83" s="2"/>
       <c r="H83" s="2"/>
     </row>
-    <row r="84" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="84" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A84" s="1"/>
       <c r="B84" s="2"/>
       <c r="E84" s="3"/>
@@ -2474,7 +2530,7 @@
       <c r="G84" s="2"/>
       <c r="H84" s="2"/>
     </row>
-    <row r="85" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="85" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A85" s="1"/>
       <c r="B85" s="2"/>
       <c r="E85" s="3"/>
@@ -2482,7 +2538,7 @@
       <c r="G85" s="2"/>
       <c r="H85" s="2"/>
     </row>
-    <row r="86" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="86" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A86" s="1"/>
       <c r="B86" s="2"/>
       <c r="E86" s="3"/>
@@ -2490,7 +2546,7 @@
       <c r="G86" s="2"/>
       <c r="H86" s="2"/>
     </row>
-    <row r="87" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="87" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A87" s="1"/>
       <c r="B87" s="2"/>
       <c r="E87" s="3"/>
@@ -2498,7 +2554,7 @@
       <c r="G87" s="2"/>
       <c r="H87" s="2"/>
     </row>
-    <row r="88" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="88" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A88" s="1"/>
       <c r="B88" s="2"/>
       <c r="E88" s="3"/>
@@ -2506,7 +2562,7 @@
       <c r="G88" s="2"/>
       <c r="H88" s="2"/>
     </row>
-    <row r="89" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="89" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A89" s="1"/>
       <c r="B89" s="2"/>
       <c r="E89" s="3"/>
@@ -2514,7 +2570,7 @@
       <c r="G89" s="2"/>
       <c r="H89" s="2"/>
     </row>
-    <row r="90" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="90" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A90" s="1"/>
       <c r="B90" s="2"/>
       <c r="E90" s="3"/>
@@ -2522,7 +2578,7 @@
       <c r="G90" s="2"/>
       <c r="H90" s="2"/>
     </row>
-    <row r="91" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="91" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A91" s="1"/>
       <c r="B91" s="2"/>
       <c r="E91" s="3"/>
@@ -2530,7 +2586,7 @@
       <c r="G91" s="2"/>
       <c r="H91" s="2"/>
     </row>
-    <row r="92" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="92" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A92" s="1"/>
       <c r="B92" s="2"/>
       <c r="E92" s="3"/>
@@ -2538,7 +2594,7 @@
       <c r="G92" s="2"/>
       <c r="H92" s="2"/>
     </row>
-    <row r="93" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="93" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A93" s="1"/>
       <c r="B93" s="2"/>
       <c r="E93" s="3"/>
@@ -2546,7 +2602,7 @@
       <c r="G93" s="2"/>
       <c r="H93" s="2"/>
     </row>
-    <row r="94" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="94" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A94" s="1"/>
       <c r="B94" s="2"/>
       <c r="E94" s="3"/>
@@ -2554,7 +2610,7 @@
       <c r="G94" s="2"/>
       <c r="H94" s="2"/>
     </row>
-    <row r="95" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="95" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A95" s="1"/>
       <c r="B95" s="2"/>
       <c r="E95" s="3"/>
@@ -2562,7 +2618,7 @@
       <c r="G95" s="2"/>
       <c r="H95" s="2"/>
     </row>
-    <row r="96" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="96" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A96" s="1"/>
       <c r="B96" s="2"/>
       <c r="E96" s="3"/>
@@ -2570,7 +2626,7 @@
       <c r="G96" s="2"/>
       <c r="H96" s="2"/>
     </row>
-    <row r="97" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="97" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A97" s="1"/>
       <c r="B97" s="2"/>
       <c r="E97" s="3"/>
@@ -2578,7 +2634,7 @@
       <c r="G97" s="2"/>
       <c r="H97" s="2"/>
     </row>
-    <row r="98" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="98" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A98" s="1"/>
       <c r="B98" s="2"/>
       <c r="E98" s="3"/>
@@ -2586,7 +2642,7 @@
       <c r="G98" s="2"/>
       <c r="H98" s="2"/>
     </row>
-    <row r="99" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="99" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A99" s="1"/>
       <c r="B99" s="2"/>
       <c r="E99" s="3"/>
@@ -2594,7 +2650,7 @@
       <c r="G99" s="2"/>
       <c r="H99" s="2"/>
     </row>
-    <row r="100" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="100" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A100" s="1"/>
       <c r="B100" s="2"/>
       <c r="E100" s="3"/>
@@ -2637,19 +2693,19 @@
       <selection activeCell="D2" sqref="D2:D100"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="7.7265625" customWidth="1"/>
-    <col min="2" max="2" width="17.26953125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.6328125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="7.7109375" customWidth="1"/>
+    <col min="2" max="2" width="17.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.5703125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="9" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.81640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="23.6328125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="13.36328125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="19.1796875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="23.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="19.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
@@ -2675,7 +2731,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="1"/>
       <c r="B2" s="2"/>
       <c r="E2" s="3"/>
@@ -2683,7 +2739,7 @@
       <c r="G2" s="2"/>
       <c r="H2" s="2"/>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="1"/>
       <c r="B3" s="2"/>
       <c r="E3" s="3"/>
@@ -2691,7 +2747,7 @@
       <c r="G3" s="2"/>
       <c r="H3" s="2"/>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="1"/>
       <c r="B4" s="2"/>
       <c r="E4" s="3"/>
@@ -2699,7 +2755,7 @@
       <c r="G4" s="2"/>
       <c r="H4" s="2"/>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="1"/>
       <c r="B5" s="2"/>
       <c r="E5" s="3"/>
@@ -2707,7 +2763,7 @@
       <c r="G5" s="2"/>
       <c r="H5" s="2"/>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="1"/>
       <c r="B6" s="2"/>
       <c r="E6" s="3"/>
@@ -2715,7 +2771,7 @@
       <c r="G6" s="2"/>
       <c r="H6" s="2"/>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="1"/>
       <c r="B7" s="2"/>
       <c r="E7" s="3"/>
@@ -2723,7 +2779,7 @@
       <c r="G7" s="2"/>
       <c r="H7" s="2"/>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="1"/>
       <c r="B8" s="2"/>
       <c r="E8" s="3"/>
@@ -2731,7 +2787,7 @@
       <c r="G8" s="2"/>
       <c r="H8" s="2"/>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="1"/>
       <c r="B9" s="2"/>
       <c r="E9" s="3"/>
@@ -2739,7 +2795,7 @@
       <c r="G9" s="2"/>
       <c r="H9" s="2"/>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="1"/>
       <c r="B10" s="2"/>
       <c r="E10" s="3"/>
@@ -2747,7 +2803,7 @@
       <c r="G10" s="2"/>
       <c r="H10" s="2"/>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="1"/>
       <c r="B11" s="2"/>
       <c r="E11" s="3"/>
@@ -2755,7 +2811,7 @@
       <c r="G11" s="2"/>
       <c r="H11" s="2"/>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="1"/>
       <c r="B12" s="2"/>
       <c r="E12" s="3"/>
@@ -2763,7 +2819,7 @@
       <c r="G12" s="2"/>
       <c r="H12" s="2"/>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="1"/>
       <c r="B13" s="2"/>
       <c r="E13" s="3"/>
@@ -2771,7 +2827,7 @@
       <c r="G13" s="2"/>
       <c r="H13" s="2"/>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" s="1"/>
       <c r="B14" s="2"/>
       <c r="E14" s="3"/>
@@ -2779,7 +2835,7 @@
       <c r="G14" s="2"/>
       <c r="H14" s="2"/>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" s="1"/>
       <c r="B15" s="2"/>
       <c r="E15" s="3"/>
@@ -2787,7 +2843,7 @@
       <c r="G15" s="2"/>
       <c r="H15" s="2"/>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" s="1"/>
       <c r="B16" s="2"/>
       <c r="E16" s="3"/>
@@ -2795,7 +2851,7 @@
       <c r="G16" s="2"/>
       <c r="H16" s="2"/>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" s="1"/>
       <c r="B17" s="2"/>
       <c r="E17" s="3"/>
@@ -2803,7 +2859,7 @@
       <c r="G17" s="2"/>
       <c r="H17" s="2"/>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" s="1"/>
       <c r="B18" s="2"/>
       <c r="E18" s="3"/>
@@ -2811,7 +2867,7 @@
       <c r="G18" s="2"/>
       <c r="H18" s="2"/>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" s="1"/>
       <c r="B19" s="2"/>
       <c r="E19" s="3"/>
@@ -2819,7 +2875,7 @@
       <c r="G19" s="2"/>
       <c r="H19" s="2"/>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" s="1"/>
       <c r="B20" s="2"/>
       <c r="E20" s="3"/>
@@ -2827,7 +2883,7 @@
       <c r="G20" s="2"/>
       <c r="H20" s="2"/>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" s="1"/>
       <c r="B21" s="2"/>
       <c r="E21" s="3"/>
@@ -2835,7 +2891,7 @@
       <c r="G21" s="2"/>
       <c r="H21" s="2"/>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" s="1"/>
       <c r="B22" s="2"/>
       <c r="E22" s="3"/>
@@ -2843,7 +2899,7 @@
       <c r="G22" s="2"/>
       <c r="H22" s="2"/>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" s="1"/>
       <c r="B23" s="2"/>
       <c r="E23" s="3"/>
@@ -2851,7 +2907,7 @@
       <c r="G23" s="2"/>
       <c r="H23" s="2"/>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24" s="1"/>
       <c r="B24" s="2"/>
       <c r="E24" s="3"/>
@@ -2859,7 +2915,7 @@
       <c r="G24" s="2"/>
       <c r="H24" s="2"/>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25" s="1"/>
       <c r="B25" s="2"/>
       <c r="E25" s="3"/>
@@ -2867,7 +2923,7 @@
       <c r="G25" s="2"/>
       <c r="H25" s="2"/>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26" s="1"/>
       <c r="B26" s="2"/>
       <c r="E26" s="3"/>
@@ -2875,7 +2931,7 @@
       <c r="G26" s="2"/>
       <c r="H26" s="2"/>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A27" s="1"/>
       <c r="B27" s="2"/>
       <c r="E27" s="3"/>
@@ -2883,7 +2939,7 @@
       <c r="G27" s="2"/>
       <c r="H27" s="2"/>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A28" s="1"/>
       <c r="B28" s="2"/>
       <c r="E28" s="3"/>
@@ -2891,7 +2947,7 @@
       <c r="G28" s="2"/>
       <c r="H28" s="2"/>
     </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A29" s="1"/>
       <c r="B29" s="2"/>
       <c r="E29" s="3"/>
@@ -2899,7 +2955,7 @@
       <c r="G29" s="2"/>
       <c r="H29" s="2"/>
     </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A30" s="1"/>
       <c r="B30" s="2"/>
       <c r="E30" s="3"/>
@@ -2907,7 +2963,7 @@
       <c r="G30" s="2"/>
       <c r="H30" s="2"/>
     </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A31" s="1"/>
       <c r="B31" s="2"/>
       <c r="E31" s="3"/>
@@ -2915,7 +2971,7 @@
       <c r="G31" s="2"/>
       <c r="H31" s="2"/>
     </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A32" s="1"/>
       <c r="B32" s="2"/>
       <c r="E32" s="3"/>
@@ -2923,7 +2979,7 @@
       <c r="G32" s="2"/>
       <c r="H32" s="2"/>
     </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A33" s="1"/>
       <c r="B33" s="2"/>
       <c r="E33" s="3"/>
@@ -2931,7 +2987,7 @@
       <c r="G33" s="2"/>
       <c r="H33" s="2"/>
     </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A34" s="1"/>
       <c r="B34" s="2"/>
       <c r="E34" s="3"/>
@@ -2939,7 +2995,7 @@
       <c r="G34" s="2"/>
       <c r="H34" s="2"/>
     </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A35" s="1"/>
       <c r="B35" s="2"/>
       <c r="E35" s="3"/>
@@ -2947,7 +3003,7 @@
       <c r="G35" s="2"/>
       <c r="H35" s="2"/>
     </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A36" s="1"/>
       <c r="B36" s="2"/>
       <c r="E36" s="3"/>
@@ -2955,7 +3011,7 @@
       <c r="G36" s="2"/>
       <c r="H36" s="2"/>
     </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A37" s="1"/>
       <c r="B37" s="2"/>
       <c r="E37" s="3"/>
@@ -2963,7 +3019,7 @@
       <c r="G37" s="2"/>
       <c r="H37" s="2"/>
     </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A38" s="1"/>
       <c r="B38" s="2"/>
       <c r="E38" s="3"/>
@@ -2971,7 +3027,7 @@
       <c r="G38" s="2"/>
       <c r="H38" s="2"/>
     </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A39" s="1"/>
       <c r="B39" s="2"/>
       <c r="E39" s="3"/>
@@ -2979,7 +3035,7 @@
       <c r="G39" s="2"/>
       <c r="H39" s="2"/>
     </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A40" s="1"/>
       <c r="B40" s="2"/>
       <c r="E40" s="3"/>
@@ -2987,7 +3043,7 @@
       <c r="G40" s="2"/>
       <c r="H40" s="2"/>
     </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A41" s="1"/>
       <c r="B41" s="2"/>
       <c r="E41" s="3"/>
@@ -2995,7 +3051,7 @@
       <c r="G41" s="2"/>
       <c r="H41" s="2"/>
     </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A42" s="1"/>
       <c r="B42" s="2"/>
       <c r="E42" s="3"/>
@@ -3003,7 +3059,7 @@
       <c r="G42" s="2"/>
       <c r="H42" s="2"/>
     </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A43" s="1"/>
       <c r="B43" s="2"/>
       <c r="E43" s="3"/>
@@ -3011,7 +3067,7 @@
       <c r="G43" s="2"/>
       <c r="H43" s="2"/>
     </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A44" s="1"/>
       <c r="B44" s="2"/>
       <c r="E44" s="3"/>
@@ -3019,7 +3075,7 @@
       <c r="G44" s="2"/>
       <c r="H44" s="2"/>
     </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A45" s="1"/>
       <c r="B45" s="2"/>
       <c r="E45" s="3"/>
@@ -3027,7 +3083,7 @@
       <c r="G45" s="2"/>
       <c r="H45" s="2"/>
     </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A46" s="1"/>
       <c r="B46" s="2"/>
       <c r="E46" s="3"/>
@@ -3035,7 +3091,7 @@
       <c r="G46" s="2"/>
       <c r="H46" s="2"/>
     </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A47" s="1"/>
       <c r="B47" s="2"/>
       <c r="E47" s="3"/>
@@ -3043,7 +3099,7 @@
       <c r="G47" s="2"/>
       <c r="H47" s="2"/>
     </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A48" s="1"/>
       <c r="B48" s="2"/>
       <c r="E48" s="3"/>
@@ -3051,7 +3107,7 @@
       <c r="G48" s="2"/>
       <c r="H48" s="2"/>
     </row>
-    <row r="49" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A49" s="1"/>
       <c r="B49" s="2"/>
       <c r="E49" s="3"/>
@@ -3059,7 +3115,7 @@
       <c r="G49" s="2"/>
       <c r="H49" s="2"/>
     </row>
-    <row r="50" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A50" s="1"/>
       <c r="B50" s="2"/>
       <c r="E50" s="3"/>
@@ -3067,7 +3123,7 @@
       <c r="G50" s="2"/>
       <c r="H50" s="2"/>
     </row>
-    <row r="51" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A51" s="1"/>
       <c r="B51" s="2"/>
       <c r="E51" s="3"/>
@@ -3075,7 +3131,7 @@
       <c r="G51" s="2"/>
       <c r="H51" s="2"/>
     </row>
-    <row r="52" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A52" s="1"/>
       <c r="B52" s="2"/>
       <c r="E52" s="3"/>
@@ -3083,7 +3139,7 @@
       <c r="G52" s="2"/>
       <c r="H52" s="2"/>
     </row>
-    <row r="53" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A53" s="1"/>
       <c r="B53" s="2"/>
       <c r="E53" s="3"/>
@@ -3091,7 +3147,7 @@
       <c r="G53" s="2"/>
       <c r="H53" s="2"/>
     </row>
-    <row r="54" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A54" s="1"/>
       <c r="B54" s="2"/>
       <c r="E54" s="3"/>
@@ -3099,7 +3155,7 @@
       <c r="G54" s="2"/>
       <c r="H54" s="2"/>
     </row>
-    <row r="55" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A55" s="1"/>
       <c r="B55" s="2"/>
       <c r="E55" s="3"/>
@@ -3107,7 +3163,7 @@
       <c r="G55" s="2"/>
       <c r="H55" s="2"/>
     </row>
-    <row r="56" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A56" s="1"/>
       <c r="B56" s="2"/>
       <c r="E56" s="3"/>
@@ -3115,7 +3171,7 @@
       <c r="G56" s="2"/>
       <c r="H56" s="2"/>
     </row>
-    <row r="57" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A57" s="1"/>
       <c r="B57" s="2"/>
       <c r="E57" s="3"/>
@@ -3123,7 +3179,7 @@
       <c r="G57" s="2"/>
       <c r="H57" s="2"/>
     </row>
-    <row r="58" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A58" s="1"/>
       <c r="B58" s="2"/>
       <c r="E58" s="3"/>
@@ -3131,7 +3187,7 @@
       <c r="G58" s="2"/>
       <c r="H58" s="2"/>
     </row>
-    <row r="59" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A59" s="1"/>
       <c r="B59" s="2"/>
       <c r="E59" s="3"/>
@@ -3139,7 +3195,7 @@
       <c r="G59" s="2"/>
       <c r="H59" s="2"/>
     </row>
-    <row r="60" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A60" s="1"/>
       <c r="B60" s="2"/>
       <c r="E60" s="3"/>
@@ -3147,7 +3203,7 @@
       <c r="G60" s="2"/>
       <c r="H60" s="2"/>
     </row>
-    <row r="61" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A61" s="1"/>
       <c r="B61" s="2"/>
       <c r="E61" s="3"/>
@@ -3155,7 +3211,7 @@
       <c r="G61" s="2"/>
       <c r="H61" s="2"/>
     </row>
-    <row r="62" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A62" s="1"/>
       <c r="B62" s="2"/>
       <c r="E62" s="3"/>
@@ -3163,7 +3219,7 @@
       <c r="G62" s="2"/>
       <c r="H62" s="2"/>
     </row>
-    <row r="63" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A63" s="1"/>
       <c r="B63" s="2"/>
       <c r="E63" s="3"/>
@@ -3171,7 +3227,7 @@
       <c r="G63" s="2"/>
       <c r="H63" s="2"/>
     </row>
-    <row r="64" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A64" s="1"/>
       <c r="B64" s="2"/>
       <c r="E64" s="3"/>
@@ -3179,7 +3235,7 @@
       <c r="G64" s="2"/>
       <c r="H64" s="2"/>
     </row>
-    <row r="65" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A65" s="1"/>
       <c r="B65" s="2"/>
       <c r="E65" s="3"/>
@@ -3187,7 +3243,7 @@
       <c r="G65" s="2"/>
       <c r="H65" s="2"/>
     </row>
-    <row r="66" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A66" s="1"/>
       <c r="B66" s="2"/>
       <c r="E66" s="3"/>
@@ -3195,7 +3251,7 @@
       <c r="G66" s="2"/>
       <c r="H66" s="2"/>
     </row>
-    <row r="67" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A67" s="1"/>
       <c r="B67" s="2"/>
       <c r="E67" s="3"/>
@@ -3203,7 +3259,7 @@
       <c r="G67" s="2"/>
       <c r="H67" s="2"/>
     </row>
-    <row r="68" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A68" s="1"/>
       <c r="B68" s="2"/>
       <c r="E68" s="3"/>
@@ -3211,7 +3267,7 @@
       <c r="G68" s="2"/>
       <c r="H68" s="2"/>
     </row>
-    <row r="69" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A69" s="1"/>
       <c r="B69" s="2"/>
       <c r="E69" s="3"/>
@@ -3219,7 +3275,7 @@
       <c r="G69" s="2"/>
       <c r="H69" s="2"/>
     </row>
-    <row r="70" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A70" s="1"/>
       <c r="B70" s="2"/>
       <c r="E70" s="3"/>
@@ -3227,7 +3283,7 @@
       <c r="G70" s="2"/>
       <c r="H70" s="2"/>
     </row>
-    <row r="71" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A71" s="1"/>
       <c r="B71" s="2"/>
       <c r="E71" s="3"/>
@@ -3235,7 +3291,7 @@
       <c r="G71" s="2"/>
       <c r="H71" s="2"/>
     </row>
-    <row r="72" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A72" s="1"/>
       <c r="B72" s="2"/>
       <c r="E72" s="3"/>
@@ -3243,7 +3299,7 @@
       <c r="G72" s="2"/>
       <c r="H72" s="2"/>
     </row>
-    <row r="73" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A73" s="1"/>
       <c r="B73" s="2"/>
       <c r="E73" s="3"/>
@@ -3251,7 +3307,7 @@
       <c r="G73" s="2"/>
       <c r="H73" s="2"/>
     </row>
-    <row r="74" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A74" s="1"/>
       <c r="B74" s="2"/>
       <c r="E74" s="3"/>
@@ -3259,7 +3315,7 @@
       <c r="G74" s="2"/>
       <c r="H74" s="2"/>
     </row>
-    <row r="75" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A75" s="1"/>
       <c r="B75" s="2"/>
       <c r="E75" s="3"/>
@@ -3267,7 +3323,7 @@
       <c r="G75" s="2"/>
       <c r="H75" s="2"/>
     </row>
-    <row r="76" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="76" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A76" s="1"/>
       <c r="B76" s="2"/>
       <c r="E76" s="3"/>
@@ -3275,7 +3331,7 @@
       <c r="G76" s="2"/>
       <c r="H76" s="2"/>
     </row>
-    <row r="77" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="77" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A77" s="1"/>
       <c r="B77" s="2"/>
       <c r="E77" s="3"/>
@@ -3283,7 +3339,7 @@
       <c r="G77" s="2"/>
       <c r="H77" s="2"/>
     </row>
-    <row r="78" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="78" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A78" s="1"/>
       <c r="B78" s="2"/>
       <c r="E78" s="3"/>
@@ -3291,7 +3347,7 @@
       <c r="G78" s="2"/>
       <c r="H78" s="2"/>
     </row>
-    <row r="79" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="79" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A79" s="1"/>
       <c r="B79" s="2"/>
       <c r="E79" s="3"/>
@@ -3299,7 +3355,7 @@
       <c r="G79" s="2"/>
       <c r="H79" s="2"/>
     </row>
-    <row r="80" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="80" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A80" s="1"/>
       <c r="B80" s="2"/>
       <c r="E80" s="3"/>
@@ -3307,7 +3363,7 @@
       <c r="G80" s="2"/>
       <c r="H80" s="2"/>
     </row>
-    <row r="81" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="81" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A81" s="1"/>
       <c r="B81" s="2"/>
       <c r="E81" s="3"/>
@@ -3315,7 +3371,7 @@
       <c r="G81" s="2"/>
       <c r="H81" s="2"/>
     </row>
-    <row r="82" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="82" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A82" s="1"/>
       <c r="B82" s="2"/>
       <c r="E82" s="3"/>
@@ -3323,7 +3379,7 @@
       <c r="G82" s="2"/>
       <c r="H82" s="2"/>
     </row>
-    <row r="83" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="83" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A83" s="1"/>
       <c r="B83" s="2"/>
       <c r="E83" s="3"/>
@@ -3331,7 +3387,7 @@
       <c r="G83" s="2"/>
       <c r="H83" s="2"/>
     </row>
-    <row r="84" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="84" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A84" s="1"/>
       <c r="B84" s="2"/>
       <c r="E84" s="3"/>
@@ -3339,7 +3395,7 @@
       <c r="G84" s="2"/>
       <c r="H84" s="2"/>
     </row>
-    <row r="85" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="85" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A85" s="1"/>
       <c r="B85" s="2"/>
       <c r="E85" s="3"/>
@@ -3347,7 +3403,7 @@
       <c r="G85" s="2"/>
       <c r="H85" s="2"/>
     </row>
-    <row r="86" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="86" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A86" s="1"/>
       <c r="B86" s="2"/>
       <c r="E86" s="3"/>
@@ -3355,7 +3411,7 @@
       <c r="G86" s="2"/>
       <c r="H86" s="2"/>
     </row>
-    <row r="87" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="87" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A87" s="1"/>
       <c r="B87" s="2"/>
       <c r="E87" s="3"/>
@@ -3363,7 +3419,7 @@
       <c r="G87" s="2"/>
       <c r="H87" s="2"/>
     </row>
-    <row r="88" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="88" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A88" s="1"/>
       <c r="B88" s="2"/>
       <c r="E88" s="3"/>
@@ -3371,7 +3427,7 @@
       <c r="G88" s="2"/>
       <c r="H88" s="2"/>
     </row>
-    <row r="89" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="89" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A89" s="1"/>
       <c r="B89" s="2"/>
       <c r="E89" s="3"/>
@@ -3379,7 +3435,7 @@
       <c r="G89" s="2"/>
       <c r="H89" s="2"/>
     </row>
-    <row r="90" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="90" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A90" s="1"/>
       <c r="B90" s="2"/>
       <c r="E90" s="3"/>
@@ -3387,7 +3443,7 @@
       <c r="G90" s="2"/>
       <c r="H90" s="2"/>
     </row>
-    <row r="91" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="91" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A91" s="1"/>
       <c r="B91" s="2"/>
       <c r="E91" s="3"/>
@@ -3395,7 +3451,7 @@
       <c r="G91" s="2"/>
       <c r="H91" s="2"/>
     </row>
-    <row r="92" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="92" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A92" s="1"/>
       <c r="B92" s="2"/>
       <c r="E92" s="3"/>
@@ -3403,7 +3459,7 @@
       <c r="G92" s="2"/>
       <c r="H92" s="2"/>
     </row>
-    <row r="93" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="93" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A93" s="1"/>
       <c r="B93" s="2"/>
       <c r="E93" s="3"/>
@@ -3411,7 +3467,7 @@
       <c r="G93" s="2"/>
       <c r="H93" s="2"/>
     </row>
-    <row r="94" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="94" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A94" s="1"/>
       <c r="B94" s="2"/>
       <c r="E94" s="3"/>
@@ -3419,7 +3475,7 @@
       <c r="G94" s="2"/>
       <c r="H94" s="2"/>
     </row>
-    <row r="95" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="95" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A95" s="1"/>
       <c r="B95" s="2"/>
       <c r="E95" s="3"/>
@@ -3427,7 +3483,7 @@
       <c r="G95" s="2"/>
       <c r="H95" s="2"/>
     </row>
-    <row r="96" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="96" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A96" s="1"/>
       <c r="B96" s="2"/>
       <c r="E96" s="3"/>
@@ -3435,7 +3491,7 @@
       <c r="G96" s="2"/>
       <c r="H96" s="2"/>
     </row>
-    <row r="97" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="97" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A97" s="1"/>
       <c r="B97" s="2"/>
       <c r="E97" s="3"/>
@@ -3443,7 +3499,7 @@
       <c r="G97" s="2"/>
       <c r="H97" s="2"/>
     </row>
-    <row r="98" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="98" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A98" s="1"/>
       <c r="B98" s="2"/>
       <c r="E98" s="3"/>
@@ -3451,7 +3507,7 @@
       <c r="G98" s="2"/>
       <c r="H98" s="2"/>
     </row>
-    <row r="99" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="99" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A99" s="1"/>
       <c r="B99" s="2"/>
       <c r="E99" s="3"/>
@@ -3459,7 +3515,7 @@
       <c r="G99" s="2"/>
       <c r="H99" s="2"/>
     </row>
-    <row r="100" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="100" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A100" s="1"/>
       <c r="B100" s="2"/>
       <c r="E100" s="3"/>
@@ -3502,21 +3558,21 @@
       <selection activeCell="P21" sqref="P21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.08984375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.81640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.81640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="19.453125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.6328125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.6328125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.5703125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="9" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="17.90625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="17.85546875" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="17" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="19.1796875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="19.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="7" t="s">
         <v>8</v>
       </c>
@@ -3548,7 +3604,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="2"/>
       <c r="B2" s="8"/>
       <c r="D2" s="2"/>
@@ -3556,7 +3612,7 @@
       <c r="I2" s="8"/>
       <c r="J2" s="2"/>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="2"/>
       <c r="B3" s="8"/>
       <c r="D3" s="2"/>
@@ -3564,7 +3620,7 @@
       <c r="I3" s="8"/>
       <c r="J3" s="2"/>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="2"/>
       <c r="B4" s="8"/>
       <c r="D4" s="2"/>
@@ -3572,7 +3628,7 @@
       <c r="I4" s="8"/>
       <c r="J4" s="2"/>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" s="2"/>
       <c r="B5" s="8"/>
       <c r="D5" s="2"/>
@@ -3580,7 +3636,7 @@
       <c r="I5" s="8"/>
       <c r="J5" s="2"/>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" s="2"/>
       <c r="B6" s="8"/>
       <c r="D6" s="2"/>
@@ -3588,7 +3644,7 @@
       <c r="I6" s="8"/>
       <c r="J6" s="2"/>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" s="2"/>
       <c r="B7" s="8"/>
       <c r="D7" s="2"/>
@@ -3596,7 +3652,7 @@
       <c r="I7" s="8"/>
       <c r="J7" s="2"/>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" s="2"/>
       <c r="B8" s="8"/>
       <c r="D8" s="2"/>
@@ -3604,7 +3660,7 @@
       <c r="I8" s="8"/>
       <c r="J8" s="2"/>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" s="2"/>
       <c r="B9" s="8"/>
       <c r="D9" s="2"/>
@@ -3612,7 +3668,7 @@
       <c r="I9" s="8"/>
       <c r="J9" s="2"/>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" s="2"/>
       <c r="B10" s="8"/>
       <c r="D10" s="2"/>
@@ -3620,7 +3676,7 @@
       <c r="I10" s="8"/>
       <c r="J10" s="2"/>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" s="2"/>
       <c r="B11" s="8"/>
       <c r="D11" s="2"/>
@@ -3628,7 +3684,7 @@
       <c r="I11" s="8"/>
       <c r="J11" s="2"/>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" s="2"/>
       <c r="B12" s="8"/>
       <c r="D12" s="2"/>
@@ -3636,7 +3692,7 @@
       <c r="I12" s="8"/>
       <c r="J12" s="2"/>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" s="2"/>
       <c r="B13" s="8"/>
       <c r="D13" s="2"/>
@@ -3644,7 +3700,7 @@
       <c r="I13" s="8"/>
       <c r="J13" s="2"/>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" s="2"/>
       <c r="B14" s="8"/>
       <c r="D14" s="2"/>
@@ -3652,7 +3708,7 @@
       <c r="I14" s="8"/>
       <c r="J14" s="2"/>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" s="2"/>
       <c r="B15" s="8"/>
       <c r="D15" s="2"/>
@@ -3660,7 +3716,7 @@
       <c r="I15" s="8"/>
       <c r="J15" s="2"/>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" s="2"/>
       <c r="B16" s="8"/>
       <c r="D16" s="2"/>
@@ -3668,7 +3724,7 @@
       <c r="I16" s="8"/>
       <c r="J16" s="2"/>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17" s="2"/>
       <c r="B17" s="8"/>
       <c r="D17" s="2"/>
@@ -3676,7 +3732,7 @@
       <c r="I17" s="8"/>
       <c r="J17" s="2"/>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18" s="2"/>
       <c r="B18" s="8"/>
       <c r="D18" s="2"/>
@@ -3684,7 +3740,7 @@
       <c r="I18" s="8"/>
       <c r="J18" s="2"/>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A19" s="2"/>
       <c r="B19" s="8"/>
       <c r="D19" s="2"/>
@@ -3692,7 +3748,7 @@
       <c r="I19" s="8"/>
       <c r="J19" s="2"/>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A20" s="2"/>
       <c r="B20" s="8"/>
       <c r="D20" s="2"/>
@@ -3700,7 +3756,7 @@
       <c r="I20" s="8"/>
       <c r="J20" s="2"/>
     </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A21" s="2"/>
       <c r="B21" s="8"/>
       <c r="D21" s="2"/>
@@ -3708,7 +3764,7 @@
       <c r="I21" s="8"/>
       <c r="J21" s="2"/>
     </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A22" s="2"/>
       <c r="B22" s="8"/>
       <c r="D22" s="2"/>
@@ -3716,7 +3772,7 @@
       <c r="I22" s="8"/>
       <c r="J22" s="2"/>
     </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A23" s="2"/>
       <c r="B23" s="8"/>
       <c r="D23" s="2"/>
@@ -3724,7 +3780,7 @@
       <c r="I23" s="8"/>
       <c r="J23" s="2"/>
     </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A24" s="2"/>
       <c r="B24" s="8"/>
       <c r="D24" s="2"/>
@@ -3732,7 +3788,7 @@
       <c r="I24" s="8"/>
       <c r="J24" s="2"/>
     </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A25" s="2"/>
       <c r="B25" s="8"/>
       <c r="D25" s="2"/>
@@ -3740,7 +3796,7 @@
       <c r="I25" s="8"/>
       <c r="J25" s="2"/>
     </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A26" s="2"/>
       <c r="B26" s="8"/>
       <c r="D26" s="2"/>
@@ -3748,7 +3804,7 @@
       <c r="I26" s="8"/>
       <c r="J26" s="2"/>
     </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A27" s="2"/>
       <c r="B27" s="8"/>
       <c r="D27" s="2"/>
@@ -3756,7 +3812,7 @@
       <c r="I27" s="8"/>
       <c r="J27" s="2"/>
     </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A28" s="2"/>
       <c r="B28" s="8"/>
       <c r="D28" s="2"/>
@@ -3764,7 +3820,7 @@
       <c r="I28" s="8"/>
       <c r="J28" s="2"/>
     </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A29" s="2"/>
       <c r="B29" s="8"/>
       <c r="D29" s="2"/>
@@ -3772,7 +3828,7 @@
       <c r="I29" s="8"/>
       <c r="J29" s="2"/>
     </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A30" s="2"/>
       <c r="B30" s="8"/>
       <c r="D30" s="2"/>
@@ -3780,7 +3836,7 @@
       <c r="I30" s="8"/>
       <c r="J30" s="2"/>
     </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A31" s="2"/>
       <c r="B31" s="8"/>
       <c r="D31" s="2"/>
@@ -3788,7 +3844,7 @@
       <c r="I31" s="8"/>
       <c r="J31" s="2"/>
     </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A32" s="2"/>
       <c r="B32" s="8"/>
       <c r="D32" s="2"/>
@@ -3796,7 +3852,7 @@
       <c r="I32" s="8"/>
       <c r="J32" s="2"/>
     </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A33" s="2"/>
       <c r="B33" s="8"/>
       <c r="D33" s="2"/>
@@ -3804,7 +3860,7 @@
       <c r="I33" s="8"/>
       <c r="J33" s="2"/>
     </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A34" s="2"/>
       <c r="B34" s="8"/>
       <c r="D34" s="2"/>
@@ -3812,7 +3868,7 @@
       <c r="I34" s="8"/>
       <c r="J34" s="2"/>
     </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A35" s="2"/>
       <c r="B35" s="8"/>
       <c r="D35" s="2"/>
@@ -3820,7 +3876,7 @@
       <c r="I35" s="8"/>
       <c r="J35" s="2"/>
     </row>
-    <row r="36" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A36" s="2"/>
       <c r="B36" s="8"/>
       <c r="D36" s="2"/>
@@ -3828,7 +3884,7 @@
       <c r="I36" s="8"/>
       <c r="J36" s="2"/>
     </row>
-    <row r="37" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A37" s="2"/>
       <c r="B37" s="8"/>
       <c r="D37" s="2"/>
@@ -3836,7 +3892,7 @@
       <c r="I37" s="8"/>
       <c r="J37" s="2"/>
     </row>
-    <row r="38" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A38" s="2"/>
       <c r="B38" s="8"/>
       <c r="D38" s="2"/>
@@ -3844,7 +3900,7 @@
       <c r="I38" s="8"/>
       <c r="J38" s="2"/>
     </row>
-    <row r="39" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A39" s="2"/>
       <c r="B39" s="8"/>
       <c r="D39" s="2"/>
@@ -3852,7 +3908,7 @@
       <c r="I39" s="8"/>
       <c r="J39" s="2"/>
     </row>
-    <row r="40" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A40" s="2"/>
       <c r="B40" s="8"/>
       <c r="D40" s="2"/>
@@ -3860,7 +3916,7 @@
       <c r="I40" s="8"/>
       <c r="J40" s="2"/>
     </row>
-    <row r="41" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A41" s="2"/>
       <c r="B41" s="8"/>
       <c r="D41" s="2"/>
@@ -3868,7 +3924,7 @@
       <c r="I41" s="8"/>
       <c r="J41" s="2"/>
     </row>
-    <row r="42" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A42" s="2"/>
       <c r="B42" s="8"/>
       <c r="D42" s="2"/>
@@ -3876,7 +3932,7 @@
       <c r="I42" s="8"/>
       <c r="J42" s="2"/>
     </row>
-    <row r="43" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A43" s="2"/>
       <c r="B43" s="8"/>
       <c r="D43" s="2"/>
@@ -3884,7 +3940,7 @@
       <c r="I43" s="8"/>
       <c r="J43" s="2"/>
     </row>
-    <row r="44" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A44" s="2"/>
       <c r="B44" s="8"/>
       <c r="D44" s="2"/>
@@ -3892,7 +3948,7 @@
       <c r="I44" s="8"/>
       <c r="J44" s="2"/>
     </row>
-    <row r="45" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A45" s="2"/>
       <c r="B45" s="8"/>
       <c r="D45" s="2"/>
@@ -3900,7 +3956,7 @@
       <c r="I45" s="8"/>
       <c r="J45" s="2"/>
     </row>
-    <row r="46" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A46" s="2"/>
       <c r="B46" s="8"/>
       <c r="D46" s="2"/>
@@ -3908,7 +3964,7 @@
       <c r="I46" s="8"/>
       <c r="J46" s="2"/>
     </row>
-    <row r="47" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A47" s="2"/>
       <c r="B47" s="8"/>
       <c r="D47" s="2"/>
@@ -3916,7 +3972,7 @@
       <c r="I47" s="8"/>
       <c r="J47" s="2"/>
     </row>
-    <row r="48" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A48" s="2"/>
       <c r="B48" s="8"/>
       <c r="D48" s="2"/>
@@ -3924,7 +3980,7 @@
       <c r="I48" s="8"/>
       <c r="J48" s="2"/>
     </row>
-    <row r="49" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A49" s="2"/>
       <c r="B49" s="8"/>
       <c r="D49" s="2"/>
@@ -3932,7 +3988,7 @@
       <c r="I49" s="8"/>
       <c r="J49" s="2"/>
     </row>
-    <row r="50" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A50" s="2"/>
       <c r="B50" s="8"/>
       <c r="D50" s="2"/>
@@ -3940,7 +3996,7 @@
       <c r="I50" s="8"/>
       <c r="J50" s="2"/>
     </row>
-    <row r="51" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A51" s="2"/>
       <c r="B51" s="8"/>
       <c r="D51" s="2"/>
@@ -3948,7 +4004,7 @@
       <c r="I51" s="8"/>
       <c r="J51" s="2"/>
     </row>
-    <row r="52" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A52" s="2"/>
       <c r="B52" s="8"/>
       <c r="D52" s="2"/>
@@ -3956,7 +4012,7 @@
       <c r="I52" s="8"/>
       <c r="J52" s="2"/>
     </row>
-    <row r="53" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A53" s="2"/>
       <c r="B53" s="8"/>
       <c r="D53" s="2"/>
@@ -3964,7 +4020,7 @@
       <c r="I53" s="8"/>
       <c r="J53" s="2"/>
     </row>
-    <row r="54" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A54" s="2"/>
       <c r="B54" s="8"/>
       <c r="D54" s="2"/>
@@ -3972,7 +4028,7 @@
       <c r="I54" s="8"/>
       <c r="J54" s="2"/>
     </row>
-    <row r="55" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A55" s="2"/>
       <c r="B55" s="8"/>
       <c r="D55" s="2"/>
@@ -3980,7 +4036,7 @@
       <c r="I55" s="8"/>
       <c r="J55" s="2"/>
     </row>
-    <row r="56" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A56" s="2"/>
       <c r="B56" s="8"/>
       <c r="D56" s="2"/>
@@ -3988,7 +4044,7 @@
       <c r="I56" s="8"/>
       <c r="J56" s="2"/>
     </row>
-    <row r="57" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A57" s="2"/>
       <c r="B57" s="8"/>
       <c r="D57" s="2"/>
@@ -3996,7 +4052,7 @@
       <c r="I57" s="8"/>
       <c r="J57" s="2"/>
     </row>
-    <row r="58" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A58" s="2"/>
       <c r="B58" s="8"/>
       <c r="D58" s="2"/>
@@ -4004,7 +4060,7 @@
       <c r="I58" s="8"/>
       <c r="J58" s="2"/>
     </row>
-    <row r="59" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A59" s="2"/>
       <c r="B59" s="8"/>
       <c r="D59" s="2"/>
@@ -4012,7 +4068,7 @@
       <c r="I59" s="8"/>
       <c r="J59" s="2"/>
     </row>
-    <row r="60" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A60" s="2"/>
       <c r="B60" s="8"/>
       <c r="D60" s="2"/>
@@ -4020,7 +4076,7 @@
       <c r="I60" s="8"/>
       <c r="J60" s="2"/>
     </row>
-    <row r="61" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A61" s="2"/>
       <c r="B61" s="8"/>
       <c r="D61" s="2"/>
@@ -4028,7 +4084,7 @@
       <c r="I61" s="8"/>
       <c r="J61" s="2"/>
     </row>
-    <row r="62" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A62" s="2"/>
       <c r="B62" s="8"/>
       <c r="D62" s="2"/>
@@ -4036,7 +4092,7 @@
       <c r="I62" s="8"/>
       <c r="J62" s="2"/>
     </row>
-    <row r="63" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A63" s="2"/>
       <c r="B63" s="8"/>
       <c r="D63" s="2"/>
@@ -4044,7 +4100,7 @@
       <c r="I63" s="8"/>
       <c r="J63" s="2"/>
     </row>
-    <row r="64" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A64" s="2"/>
       <c r="B64" s="8"/>
       <c r="D64" s="2"/>
@@ -4052,7 +4108,7 @@
       <c r="I64" s="8"/>
       <c r="J64" s="2"/>
     </row>
-    <row r="65" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A65" s="2"/>
       <c r="B65" s="8"/>
       <c r="D65" s="2"/>
@@ -4060,7 +4116,7 @@
       <c r="I65" s="8"/>
       <c r="J65" s="2"/>
     </row>
-    <row r="66" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A66" s="2"/>
       <c r="B66" s="8"/>
       <c r="D66" s="2"/>
@@ -4068,7 +4124,7 @@
       <c r="I66" s="8"/>
       <c r="J66" s="2"/>
     </row>
-    <row r="67" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A67" s="2"/>
       <c r="B67" s="8"/>
       <c r="D67" s="2"/>
@@ -4076,7 +4132,7 @@
       <c r="I67" s="8"/>
       <c r="J67" s="2"/>
     </row>
-    <row r="68" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A68" s="2"/>
       <c r="B68" s="8"/>
       <c r="D68" s="2"/>
@@ -4084,7 +4140,7 @@
       <c r="I68" s="8"/>
       <c r="J68" s="2"/>
     </row>
-    <row r="69" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A69" s="2"/>
       <c r="B69" s="8"/>
       <c r="D69" s="2"/>
@@ -4092,7 +4148,7 @@
       <c r="I69" s="8"/>
       <c r="J69" s="2"/>
     </row>
-    <row r="70" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A70" s="2"/>
       <c r="B70" s="8"/>
       <c r="D70" s="2"/>
@@ -4100,7 +4156,7 @@
       <c r="I70" s="8"/>
       <c r="J70" s="2"/>
     </row>
-    <row r="71" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A71" s="2"/>
       <c r="B71" s="8"/>
       <c r="D71" s="2"/>
@@ -4108,7 +4164,7 @@
       <c r="I71" s="8"/>
       <c r="J71" s="2"/>
     </row>
-    <row r="72" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A72" s="2"/>
       <c r="B72" s="8"/>
       <c r="D72" s="2"/>
@@ -4116,7 +4172,7 @@
       <c r="I72" s="8"/>
       <c r="J72" s="2"/>
     </row>
-    <row r="73" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A73" s="2"/>
       <c r="B73" s="8"/>
       <c r="D73" s="2"/>
@@ -4124,7 +4180,7 @@
       <c r="I73" s="8"/>
       <c r="J73" s="2"/>
     </row>
-    <row r="74" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A74" s="2"/>
       <c r="B74" s="8"/>
       <c r="D74" s="2"/>
@@ -4132,7 +4188,7 @@
       <c r="I74" s="8"/>
       <c r="J74" s="2"/>
     </row>
-    <row r="75" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A75" s="2"/>
       <c r="B75" s="8"/>
       <c r="D75" s="2"/>
@@ -4140,7 +4196,7 @@
       <c r="I75" s="8"/>
       <c r="J75" s="2"/>
     </row>
-    <row r="76" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="76" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A76" s="2"/>
       <c r="B76" s="8"/>
       <c r="D76" s="2"/>
@@ -4148,7 +4204,7 @@
       <c r="I76" s="8"/>
       <c r="J76" s="2"/>
     </row>
-    <row r="77" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="77" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A77" s="2"/>
       <c r="B77" s="8"/>
       <c r="D77" s="2"/>
@@ -4156,7 +4212,7 @@
       <c r="I77" s="8"/>
       <c r="J77" s="2"/>
     </row>
-    <row r="78" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="78" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A78" s="2"/>
       <c r="B78" s="8"/>
       <c r="D78" s="2"/>
@@ -4164,7 +4220,7 @@
       <c r="I78" s="8"/>
       <c r="J78" s="2"/>
     </row>
-    <row r="79" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="79" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A79" s="2"/>
       <c r="B79" s="8"/>
       <c r="D79" s="2"/>
@@ -4172,7 +4228,7 @@
       <c r="I79" s="8"/>
       <c r="J79" s="2"/>
     </row>
-    <row r="80" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="80" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A80" s="2"/>
       <c r="B80" s="8"/>
       <c r="D80" s="2"/>
@@ -4180,7 +4236,7 @@
       <c r="I80" s="8"/>
       <c r="J80" s="2"/>
     </row>
-    <row r="81" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="81" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A81" s="2"/>
       <c r="B81" s="8"/>
       <c r="D81" s="2"/>
@@ -4188,7 +4244,7 @@
       <c r="I81" s="8"/>
       <c r="J81" s="2"/>
     </row>
-    <row r="82" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="82" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A82" s="2"/>
       <c r="B82" s="8"/>
       <c r="D82" s="2"/>
@@ -4196,7 +4252,7 @@
       <c r="I82" s="8"/>
       <c r="J82" s="2"/>
     </row>
-    <row r="83" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="83" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A83" s="2"/>
       <c r="B83" s="8"/>
       <c r="D83" s="2"/>
@@ -4204,7 +4260,7 @@
       <c r="I83" s="8"/>
       <c r="J83" s="2"/>
     </row>
-    <row r="84" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="84" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A84" s="2"/>
       <c r="B84" s="8"/>
       <c r="D84" s="2"/>
@@ -4212,7 +4268,7 @@
       <c r="I84" s="8"/>
       <c r="J84" s="2"/>
     </row>
-    <row r="85" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="85" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A85" s="2"/>
       <c r="B85" s="8"/>
       <c r="D85" s="2"/>
@@ -4220,7 +4276,7 @@
       <c r="I85" s="8"/>
       <c r="J85" s="2"/>
     </row>
-    <row r="86" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="86" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A86" s="2"/>
       <c r="B86" s="8"/>
       <c r="D86" s="2"/>
@@ -4228,7 +4284,7 @@
       <c r="I86" s="8"/>
       <c r="J86" s="2"/>
     </row>
-    <row r="87" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="87" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A87" s="2"/>
       <c r="B87" s="8"/>
       <c r="D87" s="2"/>
@@ -4236,7 +4292,7 @@
       <c r="I87" s="8"/>
       <c r="J87" s="2"/>
     </row>
-    <row r="88" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="88" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A88" s="2"/>
       <c r="B88" s="8"/>
       <c r="D88" s="2"/>
@@ -4244,7 +4300,7 @@
       <c r="I88" s="8"/>
       <c r="J88" s="2"/>
     </row>
-    <row r="89" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="89" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A89" s="2"/>
       <c r="B89" s="8"/>
       <c r="D89" s="2"/>
@@ -4252,7 +4308,7 @@
       <c r="I89" s="8"/>
       <c r="J89" s="2"/>
     </row>
-    <row r="90" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="90" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A90" s="2"/>
       <c r="B90" s="8"/>
       <c r="D90" s="2"/>
@@ -4260,7 +4316,7 @@
       <c r="I90" s="8"/>
       <c r="J90" s="2"/>
     </row>
-    <row r="91" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="91" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A91" s="2"/>
       <c r="B91" s="8"/>
       <c r="D91" s="2"/>
@@ -4268,7 +4324,7 @@
       <c r="I91" s="8"/>
       <c r="J91" s="2"/>
     </row>
-    <row r="92" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="92" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A92" s="2"/>
       <c r="B92" s="8"/>
       <c r="D92" s="2"/>
@@ -4276,7 +4332,7 @@
       <c r="I92" s="8"/>
       <c r="J92" s="2"/>
     </row>
-    <row r="93" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="93" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A93" s="2"/>
       <c r="B93" s="8"/>
       <c r="D93" s="2"/>
@@ -4284,7 +4340,7 @@
       <c r="I93" s="8"/>
       <c r="J93" s="2"/>
     </row>
-    <row r="94" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="94" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A94" s="2"/>
       <c r="B94" s="8"/>
       <c r="D94" s="2"/>
@@ -4292,7 +4348,7 @@
       <c r="I94" s="8"/>
       <c r="J94" s="2"/>
     </row>
-    <row r="95" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="95" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A95" s="2"/>
       <c r="B95" s="8"/>
       <c r="D95" s="2"/>
@@ -4300,7 +4356,7 @@
       <c r="I95" s="8"/>
       <c r="J95" s="2"/>
     </row>
-    <row r="96" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="96" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A96" s="2"/>
       <c r="B96" s="8"/>
       <c r="D96" s="2"/>
@@ -4308,7 +4364,7 @@
       <c r="I96" s="8"/>
       <c r="J96" s="2"/>
     </row>
-    <row r="97" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="97" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A97" s="2"/>
       <c r="B97" s="8"/>
       <c r="D97" s="2"/>
@@ -4316,7 +4372,7 @@
       <c r="I97" s="8"/>
       <c r="J97" s="2"/>
     </row>
-    <row r="98" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="98" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A98" s="2"/>
       <c r="B98" s="8"/>
       <c r="D98" s="2"/>
@@ -4324,7 +4380,7 @@
       <c r="I98" s="8"/>
       <c r="J98" s="2"/>
     </row>
-    <row r="99" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="99" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A99" s="2"/>
       <c r="B99" s="8"/>
       <c r="D99" s="2"/>
@@ -4332,7 +4388,7 @@
       <c r="I99" s="8"/>
       <c r="J99" s="2"/>
     </row>
-    <row r="100" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="100" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A100" s="2"/>
       <c r="B100" s="8"/>
       <c r="D100" s="2"/>

</xml_diff>

<commit_message>
Add/update progress report for 10/05/2025 Sat by Avichal
</commit_message>
<xml_diff>
--- a/PR&IR.xlsx
+++ b/PR&IR.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\avichal avneel nath\Documents\Semester 7\CS415\A3\CS415_A3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF990874-22CD-41B1-9A17-D8CB24080417}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EDE79E87-F0BA-4616-B75B-DE25CFC30F54}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{BFA1E21A-08FA-4F02-8C25-33C81C8EE970}"/>
   </bookViews>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="24">
   <si>
     <t>Date</t>
   </si>
@@ -114,6 +114,17 @@
   <si>
     <t>AAN</t>
   </si>
+  <si>
+    <t>Resolved TemplateNotFound errors by relocating templates directory to root.
+Integrated Bootstrap and Font Awesome into Fees &amp; Holds UI for improved layout and clarity.
+Installed SQL Server and SQL Server Management Studio (SSMS), verified successful setup</t>
+  </si>
+  <si>
+    <t>setup backend logic for course enrollment</t>
+  </si>
+  <si>
+    <t>All major issues addressed. Application UI improved and backend setup completed with SQL Server and SSMS installation.</t>
+  </si>
 </sst>
 </file>
 
@@ -164,7 +175,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -174,7 +185,11 @@
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -853,10 +868,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{37EAA098-74C6-4411-B7E2-26AD2DCBC3F0}">
-  <dimension ref="A1:H2"/>
+  <dimension ref="A1:H28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10:C11"/>
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -894,7 +909,7 @@
       <c r="E1" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="7" t="s">
+      <c r="F1" s="10" t="s">
         <v>5</v>
       </c>
       <c r="G1" s="7" t="s">
@@ -920,7 +935,7 @@
       <c r="E2" s="3">
         <v>1</v>
       </c>
-      <c r="F2" s="9">
+      <c r="F2" s="11">
         <v>4</v>
       </c>
       <c r="G2" t="s">
@@ -929,6 +944,104 @@
       <c r="H2" t="s">
         <v>19</v>
       </c>
+    </row>
+    <row r="3" spans="1:8" ht="120" x14ac:dyDescent="0.25">
+      <c r="A3" s="1">
+        <v>45787</v>
+      </c>
+      <c r="C3" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="D3" t="s">
+        <v>17</v>
+      </c>
+      <c r="E3" s="3">
+        <v>1</v>
+      </c>
+      <c r="F3" s="11">
+        <v>3</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="H3" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="F4" s="11"/>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="F5" s="11"/>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="F6" s="11"/>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="F7" s="11"/>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="F8" s="11"/>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="F9" s="11"/>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="F10" s="11"/>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="F11" s="11"/>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="F12" s="11"/>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="F13" s="11"/>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="F14" s="11"/>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="F15" s="11"/>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="F16" s="11"/>
+    </row>
+    <row r="17" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F17" s="11"/>
+    </row>
+    <row r="18" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F18" s="11"/>
+    </row>
+    <row r="19" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F19" s="11"/>
+    </row>
+    <row r="20" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F20" s="11"/>
+    </row>
+    <row r="21" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F21" s="11"/>
+    </row>
+    <row r="22" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F22" s="11"/>
+    </row>
+    <row r="23" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F23" s="11"/>
+    </row>
+    <row r="24" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F24" s="11"/>
+    </row>
+    <row r="25" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F25" s="11"/>
+    </row>
+    <row r="26" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F26" s="11"/>
+    </row>
+    <row r="27" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F27" s="11"/>
+    </row>
+    <row r="28" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F28" s="11"/>
     </row>
   </sheetData>
   <dataValidations count="4">
@@ -948,11 +1061,12 @@
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
   <ignoredErrors>
-    <ignoredError sqref="D3:D6 D7:D16" listDataValidation="1"/>
+    <ignoredError sqref="D4:D6 D7:D16" listDataValidation="1"/>
   </ignoredErrors>
   <tableParts count="1">
-    <tablePart r:id="rId1"/>
+    <tablePart r:id="rId2"/>
   </tableParts>
 </worksheet>
 </file>

</xml_diff>

<commit_message>
Add/update progress report for 10/05/2025 Sat by Shivya
</commit_message>
<xml_diff>
--- a/PR&IR.xlsx
+++ b/PR&IR.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26026"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\avichal avneel nath\Documents\Semester 7\CS415\A3\CS415_A3\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SHIVYA KUMAR\Desktop\new415\CS415_A3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EDE79E87-F0BA-4616-B75B-DE25CFC30F54}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{01652070-29DC-4F77-A0F0-F5C7EB06AF3A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{BFA1E21A-08FA-4F02-8C25-33C81C8EE970}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{BFA1E21A-08FA-4F02-8C25-33C81C8EE970}"/>
   </bookViews>
   <sheets>
     <sheet name="Avichal" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="32">
   <si>
     <t>Date</t>
   </si>
@@ -125,6 +125,30 @@
   <si>
     <t>All major issues addressed. Application UI improved and backend setup completed with SQL Server and SSMS installation.</t>
   </si>
+  <si>
+    <t>Shivya Kumar</t>
+  </si>
+  <si>
+    <t>Convert UI for login, homepage and student profile</t>
+  </si>
+  <si>
+    <t>In Progress</t>
+  </si>
+  <si>
+    <t>Continue converting UI and setting route</t>
+  </si>
+  <si>
+    <t>I was unable to run the app locally, so I created a folder named run_main_app.py with the required code Once I did that I was able to start the Flask server successfully</t>
+  </si>
+  <si>
+    <t>Added header and footer to the remaining UIs, and converted UI for enrollment page.</t>
+  </si>
+  <si>
+    <t>Solve my routes and fix UI</t>
+  </si>
+  <si>
+    <t>I added my routes in the same file run_main_app.py</t>
+  </si>
 </sst>
 </file>
 
@@ -134,7 +158,7 @@
     <numFmt numFmtId="164" formatCode="h"/>
     <numFmt numFmtId="165" formatCode="d/mm/yyyy;@"/>
   </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="3">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -175,7 +199,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -189,6 +213,11 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
@@ -870,30 +899,30 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{37EAA098-74C6-4411-B7E2-26AD2DCBC3F0}">
   <dimension ref="A1:H28"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col min="1" max="1" width="10.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.5703125" style="2" customWidth="1"/>
+    <col min="1" max="1" width="10.3984375" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.59765625" style="2" customWidth="1"/>
     <col min="3" max="3" width="58" customWidth="1"/>
-    <col min="5" max="5" width="13.140625" style="3" customWidth="1"/>
-    <col min="6" max="6" width="20.85546875" style="4" customWidth="1"/>
-    <col min="7" max="7" width="34.85546875" style="2" customWidth="1"/>
-    <col min="8" max="8" width="43.42578125" style="2" customWidth="1"/>
-    <col min="11" max="11" width="9.140625" customWidth="1"/>
-    <col min="12" max="12" width="13.28515625" customWidth="1"/>
-    <col min="13" max="13" width="11.42578125" customWidth="1"/>
-    <col min="14" max="14" width="17.42578125" customWidth="1"/>
-    <col min="16" max="16" width="9.140625" customWidth="1"/>
-    <col min="18" max="18" width="16.5703125" customWidth="1"/>
-    <col min="19" max="19" width="14.7109375" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="16.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.09765625" style="3" customWidth="1"/>
+    <col min="6" max="6" width="20.8984375" style="4" customWidth="1"/>
+    <col min="7" max="7" width="34.8984375" style="2" customWidth="1"/>
+    <col min="8" max="8" width="43.3984375" style="2" customWidth="1"/>
+    <col min="11" max="11" width="9.09765625" customWidth="1"/>
+    <col min="12" max="12" width="13.296875" customWidth="1"/>
+    <col min="13" max="13" width="11.3984375" customWidth="1"/>
+    <col min="14" max="14" width="17.3984375" customWidth="1"/>
+    <col min="16" max="16" width="9.09765625" customWidth="1"/>
+    <col min="18" max="18" width="16.59765625" customWidth="1"/>
+    <col min="19" max="19" width="14.69921875" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="16.8984375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" ht="15.75">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
@@ -919,7 +948,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="15.75" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:8" ht="15.75">
       <c r="A2" s="1">
         <v>45786</v>
       </c>
@@ -945,7 +974,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="3" spans="1:8" ht="120" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" ht="120">
       <c r="A3" s="1">
         <v>45787</v>
       </c>
@@ -968,79 +997,79 @@
         <v>23</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" ht="15">
       <c r="F4" s="11"/>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" ht="15">
       <c r="F5" s="11"/>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" ht="15">
       <c r="F6" s="11"/>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" ht="15">
       <c r="F7" s="11"/>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" ht="15">
       <c r="F8" s="11"/>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" ht="15">
       <c r="F9" s="11"/>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" ht="15">
       <c r="F10" s="11"/>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" ht="15">
       <c r="F11" s="11"/>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8" ht="15">
       <c r="F12" s="11"/>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8" ht="15">
       <c r="F13" s="11"/>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8" ht="15">
       <c r="F14" s="11"/>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8" ht="15">
       <c r="F15" s="11"/>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8" ht="15">
       <c r="F16" s="11"/>
     </row>
-    <row r="17" spans="6:6" x14ac:dyDescent="0.25">
+    <row r="17" spans="6:6" ht="15">
       <c r="F17" s="11"/>
     </row>
-    <row r="18" spans="6:6" x14ac:dyDescent="0.25">
+    <row r="18" spans="6:6" ht="15">
       <c r="F18" s="11"/>
     </row>
-    <row r="19" spans="6:6" x14ac:dyDescent="0.25">
+    <row r="19" spans="6:6">
       <c r="F19" s="11"/>
     </row>
-    <row r="20" spans="6:6" x14ac:dyDescent="0.25">
+    <row r="20" spans="6:6">
       <c r="F20" s="11"/>
     </row>
-    <row r="21" spans="6:6" x14ac:dyDescent="0.25">
+    <row r="21" spans="6:6">
       <c r="F21" s="11"/>
     </row>
-    <row r="22" spans="6:6" x14ac:dyDescent="0.25">
+    <row r="22" spans="6:6">
       <c r="F22" s="11"/>
     </row>
-    <row r="23" spans="6:6" x14ac:dyDescent="0.25">
+    <row r="23" spans="6:6">
       <c r="F23" s="11"/>
     </row>
-    <row r="24" spans="6:6" x14ac:dyDescent="0.25">
+    <row r="24" spans="6:6">
       <c r="F24" s="11"/>
     </row>
-    <row r="25" spans="6:6" x14ac:dyDescent="0.25">
+    <row r="25" spans="6:6">
       <c r="F25" s="11"/>
     </row>
-    <row r="26" spans="6:6" x14ac:dyDescent="0.25">
+    <row r="26" spans="6:6">
       <c r="F26" s="11"/>
     </row>
-    <row r="27" spans="6:6" x14ac:dyDescent="0.25">
+    <row r="27" spans="6:6">
       <c r="F27" s="11"/>
     </row>
-    <row r="28" spans="6:6" x14ac:dyDescent="0.25">
+    <row r="28" spans="6:6">
       <c r="F28" s="11"/>
     </row>
   </sheetData>
@@ -1073,25 +1102,25 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3BDA6702-5DDF-42FB-988E-13FBEB26F5C9}">
-  <dimension ref="A1:H100"/>
+  <dimension ref="A1:I100"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H2" sqref="H2"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="H3" sqref="H3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col min="1" max="1" width="9.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="17.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.8984375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.296875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="63" customWidth="1"/>
     <col min="4" max="4" width="9" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.85546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="23.5703125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="13.42578125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="19.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.8984375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="23.59765625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="21.796875" customWidth="1"/>
+    <col min="8" max="8" width="116.3984375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" ht="15.6">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
@@ -1117,21 +1146,60 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A2" s="8"/>
-      <c r="B2" s="2"/>
-      <c r="E2" s="3"/>
-      <c r="G2" s="2"/>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A3" s="8"/>
-      <c r="B3" s="2"/>
-      <c r="E3" s="3"/>
-      <c r="F3" s="4"/>
-      <c r="G3" s="2"/>
-      <c r="H3" s="2"/>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9">
+      <c r="A2" s="15">
+        <v>45786</v>
+      </c>
+      <c r="B2" s="13" t="s">
+        <v>24</v>
+      </c>
+      <c r="C2" s="12" t="s">
+        <v>25</v>
+      </c>
+      <c r="D2" s="12" t="s">
+        <v>26</v>
+      </c>
+      <c r="E2" s="14">
+        <v>0.9</v>
+      </c>
+      <c r="F2" s="16">
+        <v>8</v>
+      </c>
+      <c r="G2" s="13" t="s">
+        <v>27</v>
+      </c>
+      <c r="H2" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="I2" s="13"/>
+    </row>
+    <row r="3" spans="1:9">
+      <c r="A3" s="8">
+        <v>45787</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="C3" t="s">
+        <v>29</v>
+      </c>
+      <c r="D3" t="s">
+        <v>26</v>
+      </c>
+      <c r="E3" s="16">
+        <v>90</v>
+      </c>
+      <c r="F3" s="16">
+        <v>8</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="H3" s="2" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9">
       <c r="A4" s="8"/>
       <c r="B4" s="2"/>
       <c r="E4" s="3"/>
@@ -1139,7 +1207,7 @@
       <c r="G4" s="2"/>
       <c r="H4" s="2"/>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" ht="15">
       <c r="A5" s="8"/>
       <c r="B5" s="2"/>
       <c r="E5" s="3"/>
@@ -1147,7 +1215,7 @@
       <c r="G5" s="2"/>
       <c r="H5" s="2"/>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" ht="15">
       <c r="A6" s="8"/>
       <c r="B6" s="2"/>
       <c r="E6" s="3"/>
@@ -1155,7 +1223,7 @@
       <c r="G6" s="2"/>
       <c r="H6" s="2"/>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" ht="15">
       <c r="A7" s="8"/>
       <c r="B7" s="2"/>
       <c r="E7" s="3"/>
@@ -1163,7 +1231,7 @@
       <c r="G7" s="2"/>
       <c r="H7" s="2"/>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" ht="15">
       <c r="A8" s="8"/>
       <c r="B8" s="2"/>
       <c r="E8" s="3"/>
@@ -1171,7 +1239,7 @@
       <c r="G8" s="2"/>
       <c r="H8" s="2"/>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" ht="15">
       <c r="A9" s="8"/>
       <c r="B9" s="2"/>
       <c r="E9" s="3"/>
@@ -1179,7 +1247,7 @@
       <c r="G9" s="2"/>
       <c r="H9" s="2"/>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" ht="15">
       <c r="A10" s="8"/>
       <c r="B10" s="2"/>
       <c r="E10" s="3"/>
@@ -1187,7 +1255,7 @@
       <c r="G10" s="2"/>
       <c r="H10" s="2"/>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" ht="15">
       <c r="A11" s="8"/>
       <c r="B11" s="2"/>
       <c r="E11" s="3"/>
@@ -1195,7 +1263,7 @@
       <c r="G11" s="2"/>
       <c r="H11" s="2"/>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9" ht="15">
       <c r="A12" s="8"/>
       <c r="B12" s="2"/>
       <c r="E12" s="3"/>
@@ -1203,7 +1271,7 @@
       <c r="G12" s="2"/>
       <c r="H12" s="2"/>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9" ht="15">
       <c r="A13" s="8"/>
       <c r="B13" s="2"/>
       <c r="E13" s="3"/>
@@ -1211,7 +1279,7 @@
       <c r="G13" s="2"/>
       <c r="H13" s="2"/>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:9" ht="15">
       <c r="A14" s="8"/>
       <c r="B14" s="2"/>
       <c r="E14" s="3"/>
@@ -1219,7 +1287,7 @@
       <c r="G14" s="2"/>
       <c r="H14" s="2"/>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:9" ht="15">
       <c r="A15" s="8"/>
       <c r="B15" s="2"/>
       <c r="E15" s="3"/>
@@ -1227,7 +1295,7 @@
       <c r="G15" s="2"/>
       <c r="H15" s="2"/>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:9" ht="15">
       <c r="A16" s="8"/>
       <c r="B16" s="2"/>
       <c r="E16" s="3"/>
@@ -1235,7 +1303,7 @@
       <c r="G16" s="2"/>
       <c r="H16" s="2"/>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:8" ht="15">
       <c r="A17" s="8"/>
       <c r="B17" s="2"/>
       <c r="E17" s="3"/>
@@ -1243,7 +1311,7 @@
       <c r="G17" s="2"/>
       <c r="H17" s="2"/>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:8" ht="15">
       <c r="A18" s="8"/>
       <c r="B18" s="2"/>
       <c r="E18" s="3"/>
@@ -1251,7 +1319,7 @@
       <c r="G18" s="2"/>
       <c r="H18" s="2"/>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:8" ht="15">
       <c r="A19" s="8"/>
       <c r="B19" s="2"/>
       <c r="E19" s="3"/>
@@ -1259,7 +1327,7 @@
       <c r="G19" s="2"/>
       <c r="H19" s="2"/>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:8" ht="15">
       <c r="A20" s="8"/>
       <c r="B20" s="2"/>
       <c r="E20" s="3"/>
@@ -1267,7 +1335,7 @@
       <c r="G20" s="2"/>
       <c r="H20" s="2"/>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:8" ht="15">
       <c r="A21" s="8"/>
       <c r="B21" s="2"/>
       <c r="E21" s="3"/>
@@ -1275,7 +1343,7 @@
       <c r="G21" s="2"/>
       <c r="H21" s="2"/>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:8" ht="15">
       <c r="A22" s="8"/>
       <c r="B22" s="2"/>
       <c r="E22" s="3"/>
@@ -1283,7 +1351,7 @@
       <c r="G22" s="2"/>
       <c r="H22" s="2"/>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:8" ht="15">
       <c r="A23" s="8"/>
       <c r="B23" s="2"/>
       <c r="E23" s="3"/>
@@ -1291,7 +1359,7 @@
       <c r="G23" s="2"/>
       <c r="H23" s="2"/>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:8" ht="15">
       <c r="A24" s="8"/>
       <c r="B24" s="2"/>
       <c r="E24" s="3"/>
@@ -1299,7 +1367,7 @@
       <c r="G24" s="2"/>
       <c r="H24" s="2"/>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:8" ht="15">
       <c r="A25" s="8"/>
       <c r="B25" s="2"/>
       <c r="E25" s="3"/>
@@ -1307,7 +1375,7 @@
       <c r="G25" s="2"/>
       <c r="H25" s="2"/>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:8">
       <c r="A26" s="8"/>
       <c r="B26" s="2"/>
       <c r="E26" s="3"/>
@@ -1315,7 +1383,7 @@
       <c r="G26" s="2"/>
       <c r="H26" s="2"/>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:8">
       <c r="A27" s="8"/>
       <c r="B27" s="2"/>
       <c r="E27" s="3"/>
@@ -1323,7 +1391,7 @@
       <c r="G27" s="2"/>
       <c r="H27" s="2"/>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:8">
       <c r="A28" s="8"/>
       <c r="B28" s="2"/>
       <c r="E28" s="3"/>
@@ -1331,7 +1399,7 @@
       <c r="G28" s="2"/>
       <c r="H28" s="2"/>
     </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:8">
       <c r="A29" s="8"/>
       <c r="B29" s="2"/>
       <c r="E29" s="3"/>
@@ -1339,7 +1407,7 @@
       <c r="G29" s="2"/>
       <c r="H29" s="2"/>
     </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:8">
       <c r="A30" s="8"/>
       <c r="B30" s="2"/>
       <c r="E30" s="3"/>
@@ -1347,7 +1415,7 @@
       <c r="G30" s="2"/>
       <c r="H30" s="2"/>
     </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:8">
       <c r="A31" s="8"/>
       <c r="B31" s="2"/>
       <c r="E31" s="3"/>
@@ -1355,7 +1423,7 @@
       <c r="G31" s="2"/>
       <c r="H31" s="2"/>
     </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:8">
       <c r="A32" s="8"/>
       <c r="B32" s="2"/>
       <c r="E32" s="3"/>
@@ -1363,7 +1431,7 @@
       <c r="G32" s="2"/>
       <c r="H32" s="2"/>
     </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:8">
       <c r="A33" s="8"/>
       <c r="B33" s="2"/>
       <c r="E33" s="3"/>
@@ -1371,7 +1439,7 @@
       <c r="G33" s="2"/>
       <c r="H33" s="2"/>
     </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:8">
       <c r="A34" s="8"/>
       <c r="B34" s="2"/>
       <c r="E34" s="3"/>
@@ -1379,7 +1447,7 @@
       <c r="G34" s="2"/>
       <c r="H34" s="2"/>
     </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:8">
       <c r="A35" s="8"/>
       <c r="B35" s="2"/>
       <c r="E35" s="3"/>
@@ -1387,7 +1455,7 @@
       <c r="G35" s="2"/>
       <c r="H35" s="2"/>
     </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:8">
       <c r="A36" s="8"/>
       <c r="B36" s="2"/>
       <c r="E36" s="3"/>
@@ -1395,7 +1463,7 @@
       <c r="G36" s="2"/>
       <c r="H36" s="2"/>
     </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:8">
       <c r="A37" s="8"/>
       <c r="B37" s="2"/>
       <c r="E37" s="3"/>
@@ -1403,7 +1471,7 @@
       <c r="G37" s="2"/>
       <c r="H37" s="2"/>
     </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:8">
       <c r="A38" s="8"/>
       <c r="B38" s="2"/>
       <c r="E38" s="3"/>
@@ -1411,7 +1479,7 @@
       <c r="G38" s="2"/>
       <c r="H38" s="2"/>
     </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:8">
       <c r="A39" s="8"/>
       <c r="B39" s="2"/>
       <c r="E39" s="3"/>
@@ -1419,7 +1487,7 @@
       <c r="G39" s="2"/>
       <c r="H39" s="2"/>
     </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:8">
       <c r="A40" s="8"/>
       <c r="B40" s="2"/>
       <c r="E40" s="3"/>
@@ -1427,7 +1495,7 @@
       <c r="G40" s="2"/>
       <c r="H40" s="2"/>
     </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:8">
       <c r="A41" s="8"/>
       <c r="B41" s="2"/>
       <c r="E41" s="3"/>
@@ -1435,7 +1503,7 @@
       <c r="G41" s="2"/>
       <c r="H41" s="2"/>
     </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:8">
       <c r="A42" s="8"/>
       <c r="B42" s="2"/>
       <c r="E42" s="3"/>
@@ -1443,7 +1511,7 @@
       <c r="G42" s="2"/>
       <c r="H42" s="2"/>
     </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:8">
       <c r="A43" s="8"/>
       <c r="B43" s="2"/>
       <c r="E43" s="3"/>
@@ -1451,7 +1519,7 @@
       <c r="G43" s="2"/>
       <c r="H43" s="2"/>
     </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:8">
       <c r="A44" s="8"/>
       <c r="B44" s="2"/>
       <c r="E44" s="3"/>
@@ -1459,7 +1527,7 @@
       <c r="G44" s="2"/>
       <c r="H44" s="2"/>
     </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:8">
       <c r="A45" s="8"/>
       <c r="B45" s="2"/>
       <c r="E45" s="3"/>
@@ -1467,7 +1535,7 @@
       <c r="G45" s="2"/>
       <c r="H45" s="2"/>
     </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:8">
       <c r="A46" s="8"/>
       <c r="B46" s="2"/>
       <c r="E46" s="3"/>
@@ -1475,7 +1543,7 @@
       <c r="G46" s="2"/>
       <c r="H46" s="2"/>
     </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:8">
       <c r="A47" s="8"/>
       <c r="B47" s="2"/>
       <c r="E47" s="3"/>
@@ -1483,7 +1551,7 @@
       <c r="G47" s="2"/>
       <c r="H47" s="2"/>
     </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:8">
       <c r="A48" s="8"/>
       <c r="B48" s="2"/>
       <c r="E48" s="3"/>
@@ -1491,7 +1559,7 @@
       <c r="G48" s="2"/>
       <c r="H48" s="2"/>
     </row>
-    <row r="49" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:8">
       <c r="A49" s="8"/>
       <c r="B49" s="2"/>
       <c r="E49" s="3"/>
@@ -1499,7 +1567,7 @@
       <c r="G49" s="2"/>
       <c r="H49" s="2"/>
     </row>
-    <row r="50" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:8">
       <c r="A50" s="8"/>
       <c r="B50" s="2"/>
       <c r="E50" s="3"/>
@@ -1507,7 +1575,7 @@
       <c r="G50" s="2"/>
       <c r="H50" s="2"/>
     </row>
-    <row r="51" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:8">
       <c r="A51" s="8"/>
       <c r="B51" s="2"/>
       <c r="E51" s="3"/>
@@ -1515,7 +1583,7 @@
       <c r="G51" s="2"/>
       <c r="H51" s="2"/>
     </row>
-    <row r="52" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:8">
       <c r="A52" s="8"/>
       <c r="B52" s="2"/>
       <c r="E52" s="3"/>
@@ -1523,7 +1591,7 @@
       <c r="G52" s="2"/>
       <c r="H52" s="2"/>
     </row>
-    <row r="53" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:8">
       <c r="A53" s="8"/>
       <c r="B53" s="2"/>
       <c r="E53" s="3"/>
@@ -1531,7 +1599,7 @@
       <c r="G53" s="2"/>
       <c r="H53" s="2"/>
     </row>
-    <row r="54" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:8">
       <c r="A54" s="8"/>
       <c r="B54" s="2"/>
       <c r="E54" s="3"/>
@@ -1539,7 +1607,7 @@
       <c r="G54" s="2"/>
       <c r="H54" s="2"/>
     </row>
-    <row r="55" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:8">
       <c r="A55" s="8"/>
       <c r="B55" s="2"/>
       <c r="E55" s="3"/>
@@ -1547,7 +1615,7 @@
       <c r="G55" s="2"/>
       <c r="H55" s="2"/>
     </row>
-    <row r="56" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:8">
       <c r="A56" s="8"/>
       <c r="B56" s="2"/>
       <c r="E56" s="3"/>
@@ -1555,7 +1623,7 @@
       <c r="G56" s="2"/>
       <c r="H56" s="2"/>
     </row>
-    <row r="57" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:8">
       <c r="A57" s="8"/>
       <c r="B57" s="2"/>
       <c r="E57" s="3"/>
@@ -1563,7 +1631,7 @@
       <c r="G57" s="2"/>
       <c r="H57" s="2"/>
     </row>
-    <row r="58" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:8">
       <c r="A58" s="8"/>
       <c r="B58" s="2"/>
       <c r="E58" s="3"/>
@@ -1571,7 +1639,7 @@
       <c r="G58" s="2"/>
       <c r="H58" s="2"/>
     </row>
-    <row r="59" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:8">
       <c r="A59" s="8"/>
       <c r="B59" s="2"/>
       <c r="E59" s="3"/>
@@ -1579,7 +1647,7 @@
       <c r="G59" s="2"/>
       <c r="H59" s="2"/>
     </row>
-    <row r="60" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:8">
       <c r="A60" s="8"/>
       <c r="B60" s="2"/>
       <c r="E60" s="3"/>
@@ -1587,7 +1655,7 @@
       <c r="G60" s="2"/>
       <c r="H60" s="2"/>
     </row>
-    <row r="61" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:8">
       <c r="A61" s="8"/>
       <c r="B61" s="2"/>
       <c r="E61" s="3"/>
@@ -1595,7 +1663,7 @@
       <c r="G61" s="2"/>
       <c r="H61" s="2"/>
     </row>
-    <row r="62" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:8">
       <c r="A62" s="8"/>
       <c r="B62" s="2"/>
       <c r="E62" s="3"/>
@@ -1603,7 +1671,7 @@
       <c r="G62" s="2"/>
       <c r="H62" s="2"/>
     </row>
-    <row r="63" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:8">
       <c r="A63" s="8"/>
       <c r="B63" s="2"/>
       <c r="E63" s="3"/>
@@ -1611,7 +1679,7 @@
       <c r="G63" s="2"/>
       <c r="H63" s="2"/>
     </row>
-    <row r="64" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:8">
       <c r="A64" s="8"/>
       <c r="B64" s="2"/>
       <c r="E64" s="3"/>
@@ -1619,7 +1687,7 @@
       <c r="G64" s="2"/>
       <c r="H64" s="2"/>
     </row>
-    <row r="65" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:8">
       <c r="A65" s="8"/>
       <c r="B65" s="2"/>
       <c r="E65" s="3"/>
@@ -1627,7 +1695,7 @@
       <c r="G65" s="2"/>
       <c r="H65" s="2"/>
     </row>
-    <row r="66" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:8">
       <c r="A66" s="8"/>
       <c r="B66" s="2"/>
       <c r="E66" s="3"/>
@@ -1635,7 +1703,7 @@
       <c r="G66" s="2"/>
       <c r="H66" s="2"/>
     </row>
-    <row r="67" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:8">
       <c r="A67" s="8"/>
       <c r="B67" s="2"/>
       <c r="E67" s="3"/>
@@ -1643,7 +1711,7 @@
       <c r="G67" s="2"/>
       <c r="H67" s="2"/>
     </row>
-    <row r="68" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:8">
       <c r="A68" s="8"/>
       <c r="B68" s="2"/>
       <c r="E68" s="3"/>
@@ -1651,7 +1719,7 @@
       <c r="G68" s="2"/>
       <c r="H68" s="2"/>
     </row>
-    <row r="69" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:8">
       <c r="A69" s="8"/>
       <c r="B69" s="2"/>
       <c r="E69" s="3"/>
@@ -1659,7 +1727,7 @@
       <c r="G69" s="2"/>
       <c r="H69" s="2"/>
     </row>
-    <row r="70" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:8">
       <c r="A70" s="8"/>
       <c r="B70" s="2"/>
       <c r="E70" s="3"/>
@@ -1667,7 +1735,7 @@
       <c r="G70" s="2"/>
       <c r="H70" s="2"/>
     </row>
-    <row r="71" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:8">
       <c r="A71" s="8"/>
       <c r="B71" s="2"/>
       <c r="E71" s="3"/>
@@ -1675,7 +1743,7 @@
       <c r="G71" s="2"/>
       <c r="H71" s="2"/>
     </row>
-    <row r="72" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:8">
       <c r="A72" s="8"/>
       <c r="B72" s="2"/>
       <c r="E72" s="3"/>
@@ -1683,7 +1751,7 @@
       <c r="G72" s="2"/>
       <c r="H72" s="2"/>
     </row>
-    <row r="73" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:8">
       <c r="A73" s="8"/>
       <c r="B73" s="2"/>
       <c r="E73" s="3"/>
@@ -1691,7 +1759,7 @@
       <c r="G73" s="2"/>
       <c r="H73" s="2"/>
     </row>
-    <row r="74" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:8">
       <c r="A74" s="8"/>
       <c r="B74" s="2"/>
       <c r="E74" s="3"/>
@@ -1699,7 +1767,7 @@
       <c r="G74" s="2"/>
       <c r="H74" s="2"/>
     </row>
-    <row r="75" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:8">
       <c r="A75" s="8"/>
       <c r="B75" s="2"/>
       <c r="E75" s="3"/>
@@ -1707,7 +1775,7 @@
       <c r="G75" s="2"/>
       <c r="H75" s="2"/>
     </row>
-    <row r="76" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:8">
       <c r="A76" s="8"/>
       <c r="B76" s="2"/>
       <c r="E76" s="3"/>
@@ -1715,7 +1783,7 @@
       <c r="G76" s="2"/>
       <c r="H76" s="2"/>
     </row>
-    <row r="77" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:8">
       <c r="A77" s="8"/>
       <c r="B77" s="2"/>
       <c r="E77" s="3"/>
@@ -1723,7 +1791,7 @@
       <c r="G77" s="2"/>
       <c r="H77" s="2"/>
     </row>
-    <row r="78" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:8">
       <c r="A78" s="8"/>
       <c r="B78" s="2"/>
       <c r="E78" s="3"/>
@@ -1731,7 +1799,7 @@
       <c r="G78" s="2"/>
       <c r="H78" s="2"/>
     </row>
-    <row r="79" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:8">
       <c r="A79" s="8"/>
       <c r="B79" s="2"/>
       <c r="E79" s="3"/>
@@ -1739,7 +1807,7 @@
       <c r="G79" s="2"/>
       <c r="H79" s="2"/>
     </row>
-    <row r="80" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:8">
       <c r="A80" s="8"/>
       <c r="B80" s="2"/>
       <c r="E80" s="3"/>
@@ -1747,7 +1815,7 @@
       <c r="G80" s="2"/>
       <c r="H80" s="2"/>
     </row>
-    <row r="81" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:8">
       <c r="A81" s="8"/>
       <c r="B81" s="2"/>
       <c r="E81" s="3"/>
@@ -1755,7 +1823,7 @@
       <c r="G81" s="2"/>
       <c r="H81" s="2"/>
     </row>
-    <row r="82" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:8">
       <c r="A82" s="8"/>
       <c r="B82" s="2"/>
       <c r="E82" s="3"/>
@@ -1763,7 +1831,7 @@
       <c r="G82" s="2"/>
       <c r="H82" s="2"/>
     </row>
-    <row r="83" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:8">
       <c r="A83" s="8"/>
       <c r="B83" s="2"/>
       <c r="E83" s="3"/>
@@ -1771,7 +1839,7 @@
       <c r="G83" s="2"/>
       <c r="H83" s="2"/>
     </row>
-    <row r="84" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:8">
       <c r="A84" s="8"/>
       <c r="B84" s="2"/>
       <c r="E84" s="3"/>
@@ -1779,7 +1847,7 @@
       <c r="G84" s="2"/>
       <c r="H84" s="2"/>
     </row>
-    <row r="85" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:8">
       <c r="A85" s="8"/>
       <c r="B85" s="2"/>
       <c r="E85" s="3"/>
@@ -1787,7 +1855,7 @@
       <c r="G85" s="2"/>
       <c r="H85" s="2"/>
     </row>
-    <row r="86" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:8">
       <c r="A86" s="8"/>
       <c r="B86" s="2"/>
       <c r="E86" s="3"/>
@@ -1795,7 +1863,7 @@
       <c r="G86" s="2"/>
       <c r="H86" s="2"/>
     </row>
-    <row r="87" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:8">
       <c r="A87" s="8"/>
       <c r="B87" s="2"/>
       <c r="E87" s="3"/>
@@ -1803,7 +1871,7 @@
       <c r="G87" s="2"/>
       <c r="H87" s="2"/>
     </row>
-    <row r="88" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:8">
       <c r="A88" s="8"/>
       <c r="B88" s="2"/>
       <c r="E88" s="3"/>
@@ -1811,7 +1879,7 @@
       <c r="G88" s="2"/>
       <c r="H88" s="2"/>
     </row>
-    <row r="89" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:8">
       <c r="A89" s="8"/>
       <c r="B89" s="2"/>
       <c r="E89" s="3"/>
@@ -1819,7 +1887,7 @@
       <c r="G89" s="2"/>
       <c r="H89" s="2"/>
     </row>
-    <row r="90" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:8">
       <c r="A90" s="8"/>
       <c r="B90" s="2"/>
       <c r="E90" s="3"/>
@@ -1827,7 +1895,7 @@
       <c r="G90" s="2"/>
       <c r="H90" s="2"/>
     </row>
-    <row r="91" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:8">
       <c r="A91" s="8"/>
       <c r="B91" s="2"/>
       <c r="E91" s="3"/>
@@ -1835,7 +1903,7 @@
       <c r="G91" s="2"/>
       <c r="H91" s="2"/>
     </row>
-    <row r="92" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:8">
       <c r="A92" s="8"/>
       <c r="B92" s="2"/>
       <c r="E92" s="3"/>
@@ -1843,7 +1911,7 @@
       <c r="G92" s="2"/>
       <c r="H92" s="2"/>
     </row>
-    <row r="93" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:8">
       <c r="A93" s="8"/>
       <c r="B93" s="2"/>
       <c r="E93" s="3"/>
@@ -1851,7 +1919,7 @@
       <c r="G93" s="2"/>
       <c r="H93" s="2"/>
     </row>
-    <row r="94" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:8">
       <c r="A94" s="8"/>
       <c r="B94" s="2"/>
       <c r="E94" s="3"/>
@@ -1859,7 +1927,7 @@
       <c r="G94" s="2"/>
       <c r="H94" s="2"/>
     </row>
-    <row r="95" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:8">
       <c r="A95" s="8"/>
       <c r="B95" s="2"/>
       <c r="E95" s="3"/>
@@ -1867,7 +1935,7 @@
       <c r="G95" s="2"/>
       <c r="H95" s="2"/>
     </row>
-    <row r="96" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:8">
       <c r="A96" s="8"/>
       <c r="B96" s="2"/>
       <c r="E96" s="3"/>
@@ -1875,7 +1943,7 @@
       <c r="G96" s="2"/>
       <c r="H96" s="2"/>
     </row>
-    <row r="97" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:8">
       <c r="A97" s="8"/>
       <c r="B97" s="2"/>
       <c r="E97" s="3"/>
@@ -1883,7 +1951,7 @@
       <c r="G97" s="2"/>
       <c r="H97" s="2"/>
     </row>
-    <row r="98" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:8">
       <c r="A98" s="8"/>
       <c r="B98" s="2"/>
       <c r="E98" s="3"/>
@@ -1891,7 +1959,7 @@
       <c r="G98" s="2"/>
       <c r="H98" s="2"/>
     </row>
-    <row r="99" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:8">
       <c r="A99" s="8"/>
       <c r="B99" s="2"/>
       <c r="E99" s="3"/>
@@ -1899,7 +1967,7 @@
       <c r="G99" s="2"/>
       <c r="H99" s="2"/>
     </row>
-    <row r="100" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:8">
       <c r="A100" s="8"/>
       <c r="B100" s="2"/>
       <c r="E100" s="3"/>
@@ -1926,7 +1994,7 @@
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <ignoredErrors>
-    <ignoredError sqref="D3:D100" listDataValidation="1"/>
+    <ignoredError sqref="D4:D100" listDataValidation="1"/>
   </ignoredErrors>
   <tableParts count="1">
     <tablePart r:id="rId1"/>
@@ -1942,19 +2010,19 @@
       <selection activeCell="D2" sqref="D2:D100"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col min="1" max="1" width="7.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="17.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="7.69921875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.296875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.59765625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="9" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.85546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="23.5703125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="13.42578125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="19.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.8984375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="23.59765625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.3984375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="19.09765625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" ht="15.75">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
@@ -1980,7 +2048,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" ht="15">
       <c r="A2" s="1"/>
       <c r="B2" s="2"/>
       <c r="E2" s="3"/>
@@ -1988,7 +2056,7 @@
       <c r="G2" s="2"/>
       <c r="H2" s="2"/>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" ht="15">
       <c r="A3" s="1"/>
       <c r="B3" s="2"/>
       <c r="E3" s="3"/>
@@ -1996,7 +2064,7 @@
       <c r="G3" s="2"/>
       <c r="H3" s="2"/>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" ht="15">
       <c r="A4" s="1"/>
       <c r="B4" s="2"/>
       <c r="E4" s="3"/>
@@ -2004,7 +2072,7 @@
       <c r="G4" s="2"/>
       <c r="H4" s="2"/>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" ht="15">
       <c r="A5" s="1"/>
       <c r="B5" s="2"/>
       <c r="E5" s="3"/>
@@ -2012,7 +2080,7 @@
       <c r="G5" s="2"/>
       <c r="H5" s="2"/>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" ht="15">
       <c r="A6" s="1"/>
       <c r="B6" s="2"/>
       <c r="E6" s="3"/>
@@ -2020,7 +2088,7 @@
       <c r="G6" s="2"/>
       <c r="H6" s="2"/>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" ht="15">
       <c r="A7" s="1"/>
       <c r="B7" s="2"/>
       <c r="E7" s="3"/>
@@ -2028,7 +2096,7 @@
       <c r="G7" s="2"/>
       <c r="H7" s="2"/>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" ht="15">
       <c r="A8" s="1"/>
       <c r="B8" s="2"/>
       <c r="E8" s="3"/>
@@ -2036,7 +2104,7 @@
       <c r="G8" s="2"/>
       <c r="H8" s="2"/>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" ht="15">
       <c r="A9" s="1"/>
       <c r="B9" s="2"/>
       <c r="E9" s="3"/>
@@ -2044,7 +2112,7 @@
       <c r="G9" s="2"/>
       <c r="H9" s="2"/>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" ht="15">
       <c r="A10" s="1"/>
       <c r="B10" s="2"/>
       <c r="E10" s="3"/>
@@ -2052,7 +2120,7 @@
       <c r="G10" s="2"/>
       <c r="H10" s="2"/>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" ht="15">
       <c r="A11" s="1"/>
       <c r="B11" s="2"/>
       <c r="E11" s="3"/>
@@ -2060,7 +2128,7 @@
       <c r="G11" s="2"/>
       <c r="H11" s="2"/>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8" ht="15">
       <c r="A12" s="1"/>
       <c r="B12" s="2"/>
       <c r="E12" s="3"/>
@@ -2068,7 +2136,7 @@
       <c r="G12" s="2"/>
       <c r="H12" s="2"/>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8" ht="15">
       <c r="A13" s="1"/>
       <c r="B13" s="2"/>
       <c r="E13" s="3"/>
@@ -2076,7 +2144,7 @@
       <c r="G13" s="2"/>
       <c r="H13" s="2"/>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8" ht="15">
       <c r="A14" s="1"/>
       <c r="B14" s="2"/>
       <c r="E14" s="3"/>
@@ -2084,7 +2152,7 @@
       <c r="G14" s="2"/>
       <c r="H14" s="2"/>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8" ht="15">
       <c r="A15" s="1"/>
       <c r="B15" s="2"/>
       <c r="E15" s="3"/>
@@ -2092,7 +2160,7 @@
       <c r="G15" s="2"/>
       <c r="H15" s="2"/>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8" ht="15">
       <c r="A16" s="1"/>
       <c r="B16" s="2"/>
       <c r="E16" s="3"/>
@@ -2100,7 +2168,7 @@
       <c r="G16" s="2"/>
       <c r="H16" s="2"/>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:8" ht="15">
       <c r="A17" s="1"/>
       <c r="B17" s="2"/>
       <c r="E17" s="3"/>
@@ -2108,7 +2176,7 @@
       <c r="G17" s="2"/>
       <c r="H17" s="2"/>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:8" ht="15">
       <c r="A18" s="1"/>
       <c r="B18" s="2"/>
       <c r="E18" s="3"/>
@@ -2116,7 +2184,7 @@
       <c r="G18" s="2"/>
       <c r="H18" s="2"/>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:8" ht="15">
       <c r="A19" s="1"/>
       <c r="B19" s="2"/>
       <c r="E19" s="3"/>
@@ -2124,7 +2192,7 @@
       <c r="G19" s="2"/>
       <c r="H19" s="2"/>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:8" ht="15">
       <c r="A20" s="1"/>
       <c r="B20" s="2"/>
       <c r="E20" s="3"/>
@@ -2132,7 +2200,7 @@
       <c r="G20" s="2"/>
       <c r="H20" s="2"/>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:8" ht="15">
       <c r="A21" s="1"/>
       <c r="B21" s="2"/>
       <c r="E21" s="3"/>
@@ -2140,7 +2208,7 @@
       <c r="G21" s="2"/>
       <c r="H21" s="2"/>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:8" ht="15">
       <c r="A22" s="1"/>
       <c r="B22" s="2"/>
       <c r="E22" s="3"/>
@@ -2148,7 +2216,7 @@
       <c r="G22" s="2"/>
       <c r="H22" s="2"/>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:8" ht="15">
       <c r="A23" s="1"/>
       <c r="B23" s="2"/>
       <c r="E23" s="3"/>
@@ -2156,7 +2224,7 @@
       <c r="G23" s="2"/>
       <c r="H23" s="2"/>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:8" ht="15">
       <c r="A24" s="1"/>
       <c r="B24" s="2"/>
       <c r="E24" s="3"/>
@@ -2164,7 +2232,7 @@
       <c r="G24" s="2"/>
       <c r="H24" s="2"/>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:8" ht="15">
       <c r="A25" s="1"/>
       <c r="B25" s="2"/>
       <c r="E25" s="3"/>
@@ -2172,7 +2240,7 @@
       <c r="G25" s="2"/>
       <c r="H25" s="2"/>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:8" ht="15">
       <c r="A26" s="1"/>
       <c r="B26" s="2"/>
       <c r="E26" s="3"/>
@@ -2180,7 +2248,7 @@
       <c r="G26" s="2"/>
       <c r="H26" s="2"/>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:8" ht="15">
       <c r="A27" s="1"/>
       <c r="B27" s="2"/>
       <c r="E27" s="3"/>
@@ -2188,7 +2256,7 @@
       <c r="G27" s="2"/>
       <c r="H27" s="2"/>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:8" ht="15">
       <c r="A28" s="1"/>
       <c r="B28" s="2"/>
       <c r="E28" s="3"/>
@@ -2196,7 +2264,7 @@
       <c r="G28" s="2"/>
       <c r="H28" s="2"/>
     </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:8" ht="15">
       <c r="A29" s="1"/>
       <c r="B29" s="2"/>
       <c r="E29" s="3"/>
@@ -2204,7 +2272,7 @@
       <c r="G29" s="2"/>
       <c r="H29" s="2"/>
     </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:8" ht="15">
       <c r="A30" s="1"/>
       <c r="B30" s="2"/>
       <c r="E30" s="3"/>
@@ -2212,7 +2280,7 @@
       <c r="G30" s="2"/>
       <c r="H30" s="2"/>
     </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:8" ht="15">
       <c r="A31" s="1"/>
       <c r="B31" s="2"/>
       <c r="E31" s="3"/>
@@ -2220,7 +2288,7 @@
       <c r="G31" s="2"/>
       <c r="H31" s="2"/>
     </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:8" ht="15">
       <c r="A32" s="1"/>
       <c r="B32" s="2"/>
       <c r="E32" s="3"/>
@@ -2228,7 +2296,7 @@
       <c r="G32" s="2"/>
       <c r="H32" s="2"/>
     </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:8" ht="15">
       <c r="A33" s="1"/>
       <c r="B33" s="2"/>
       <c r="E33" s="3"/>
@@ -2236,7 +2304,7 @@
       <c r="G33" s="2"/>
       <c r="H33" s="2"/>
     </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:8" ht="15">
       <c r="A34" s="1"/>
       <c r="B34" s="2"/>
       <c r="E34" s="3"/>
@@ -2244,7 +2312,7 @@
       <c r="G34" s="2"/>
       <c r="H34" s="2"/>
     </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:8" ht="15">
       <c r="A35" s="1"/>
       <c r="B35" s="2"/>
       <c r="E35" s="3"/>
@@ -2252,7 +2320,7 @@
       <c r="G35" s="2"/>
       <c r="H35" s="2"/>
     </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:8" ht="15">
       <c r="A36" s="1"/>
       <c r="B36" s="2"/>
       <c r="E36" s="3"/>
@@ -2260,7 +2328,7 @@
       <c r="G36" s="2"/>
       <c r="H36" s="2"/>
     </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:8" ht="15">
       <c r="A37" s="1"/>
       <c r="B37" s="2"/>
       <c r="E37" s="3"/>
@@ -2268,7 +2336,7 @@
       <c r="G37" s="2"/>
       <c r="H37" s="2"/>
     </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:8" ht="15">
       <c r="A38" s="1"/>
       <c r="B38" s="2"/>
       <c r="E38" s="3"/>
@@ -2276,7 +2344,7 @@
       <c r="G38" s="2"/>
       <c r="H38" s="2"/>
     </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:8" ht="15">
       <c r="A39" s="1"/>
       <c r="B39" s="2"/>
       <c r="E39" s="3"/>
@@ -2284,7 +2352,7 @@
       <c r="G39" s="2"/>
       <c r="H39" s="2"/>
     </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:8" ht="15">
       <c r="A40" s="1"/>
       <c r="B40" s="2"/>
       <c r="E40" s="3"/>
@@ -2292,7 +2360,7 @@
       <c r="G40" s="2"/>
       <c r="H40" s="2"/>
     </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:8" ht="15">
       <c r="A41" s="1"/>
       <c r="B41" s="2"/>
       <c r="E41" s="3"/>
@@ -2300,7 +2368,7 @@
       <c r="G41" s="2"/>
       <c r="H41" s="2"/>
     </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:8" ht="15">
       <c r="A42" s="1"/>
       <c r="B42" s="2"/>
       <c r="E42" s="3"/>
@@ -2308,7 +2376,7 @@
       <c r="G42" s="2"/>
       <c r="H42" s="2"/>
     </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:8" ht="15">
       <c r="A43" s="1"/>
       <c r="B43" s="2"/>
       <c r="E43" s="3"/>
@@ -2316,7 +2384,7 @@
       <c r="G43" s="2"/>
       <c r="H43" s="2"/>
     </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:8" ht="15">
       <c r="A44" s="1"/>
       <c r="B44" s="2"/>
       <c r="E44" s="3"/>
@@ -2324,7 +2392,7 @@
       <c r="G44" s="2"/>
       <c r="H44" s="2"/>
     </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:8" ht="15">
       <c r="A45" s="1"/>
       <c r="B45" s="2"/>
       <c r="E45" s="3"/>
@@ -2332,7 +2400,7 @@
       <c r="G45" s="2"/>
       <c r="H45" s="2"/>
     </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:8" ht="15">
       <c r="A46" s="1"/>
       <c r="B46" s="2"/>
       <c r="E46" s="3"/>
@@ -2340,7 +2408,7 @@
       <c r="G46" s="2"/>
       <c r="H46" s="2"/>
     </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:8" ht="15">
       <c r="A47" s="1"/>
       <c r="B47" s="2"/>
       <c r="E47" s="3"/>
@@ -2348,7 +2416,7 @@
       <c r="G47" s="2"/>
       <c r="H47" s="2"/>
     </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:8" ht="15">
       <c r="A48" s="1"/>
       <c r="B48" s="2"/>
       <c r="E48" s="3"/>
@@ -2356,7 +2424,7 @@
       <c r="G48" s="2"/>
       <c r="H48" s="2"/>
     </row>
-    <row r="49" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:8" ht="15">
       <c r="A49" s="1"/>
       <c r="B49" s="2"/>
       <c r="E49" s="3"/>
@@ -2364,7 +2432,7 @@
       <c r="G49" s="2"/>
       <c r="H49" s="2"/>
     </row>
-    <row r="50" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:8" ht="15">
       <c r="A50" s="1"/>
       <c r="B50" s="2"/>
       <c r="E50" s="3"/>
@@ -2372,7 +2440,7 @@
       <c r="G50" s="2"/>
       <c r="H50" s="2"/>
     </row>
-    <row r="51" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:8" ht="15">
       <c r="A51" s="1"/>
       <c r="B51" s="2"/>
       <c r="E51" s="3"/>
@@ -2380,7 +2448,7 @@
       <c r="G51" s="2"/>
       <c r="H51" s="2"/>
     </row>
-    <row r="52" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:8" ht="15">
       <c r="A52" s="1"/>
       <c r="B52" s="2"/>
       <c r="E52" s="3"/>
@@ -2388,7 +2456,7 @@
       <c r="G52" s="2"/>
       <c r="H52" s="2"/>
     </row>
-    <row r="53" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:8" ht="15">
       <c r="A53" s="1"/>
       <c r="B53" s="2"/>
       <c r="E53" s="3"/>
@@ -2396,7 +2464,7 @@
       <c r="G53" s="2"/>
       <c r="H53" s="2"/>
     </row>
-    <row r="54" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:8" ht="15">
       <c r="A54" s="1"/>
       <c r="B54" s="2"/>
       <c r="E54" s="3"/>
@@ -2404,7 +2472,7 @@
       <c r="G54" s="2"/>
       <c r="H54" s="2"/>
     </row>
-    <row r="55" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:8" ht="15">
       <c r="A55" s="1"/>
       <c r="B55" s="2"/>
       <c r="E55" s="3"/>
@@ -2412,7 +2480,7 @@
       <c r="G55" s="2"/>
       <c r="H55" s="2"/>
     </row>
-    <row r="56" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:8" ht="15">
       <c r="A56" s="1"/>
       <c r="B56" s="2"/>
       <c r="E56" s="3"/>
@@ -2420,7 +2488,7 @@
       <c r="G56" s="2"/>
       <c r="H56" s="2"/>
     </row>
-    <row r="57" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:8" ht="15">
       <c r="A57" s="1"/>
       <c r="B57" s="2"/>
       <c r="E57" s="3"/>
@@ -2428,7 +2496,7 @@
       <c r="G57" s="2"/>
       <c r="H57" s="2"/>
     </row>
-    <row r="58" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:8" ht="15">
       <c r="A58" s="1"/>
       <c r="B58" s="2"/>
       <c r="E58" s="3"/>
@@ -2436,7 +2504,7 @@
       <c r="G58" s="2"/>
       <c r="H58" s="2"/>
     </row>
-    <row r="59" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:8" ht="15">
       <c r="A59" s="1"/>
       <c r="B59" s="2"/>
       <c r="E59" s="3"/>
@@ -2444,7 +2512,7 @@
       <c r="G59" s="2"/>
       <c r="H59" s="2"/>
     </row>
-    <row r="60" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:8" ht="15">
       <c r="A60" s="1"/>
       <c r="B60" s="2"/>
       <c r="E60" s="3"/>
@@ -2452,7 +2520,7 @@
       <c r="G60" s="2"/>
       <c r="H60" s="2"/>
     </row>
-    <row r="61" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:8" ht="15">
       <c r="A61" s="1"/>
       <c r="B61" s="2"/>
       <c r="E61" s="3"/>
@@ -2460,7 +2528,7 @@
       <c r="G61" s="2"/>
       <c r="H61" s="2"/>
     </row>
-    <row r="62" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:8" ht="15">
       <c r="A62" s="1"/>
       <c r="B62" s="2"/>
       <c r="E62" s="3"/>
@@ -2468,7 +2536,7 @@
       <c r="G62" s="2"/>
       <c r="H62" s="2"/>
     </row>
-    <row r="63" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:8" ht="15">
       <c r="A63" s="1"/>
       <c r="B63" s="2"/>
       <c r="E63" s="3"/>
@@ -2476,7 +2544,7 @@
       <c r="G63" s="2"/>
       <c r="H63" s="2"/>
     </row>
-    <row r="64" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:8" ht="15">
       <c r="A64" s="1"/>
       <c r="B64" s="2"/>
       <c r="E64" s="3"/>
@@ -2484,7 +2552,7 @@
       <c r="G64" s="2"/>
       <c r="H64" s="2"/>
     </row>
-    <row r="65" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:8" ht="15">
       <c r="A65" s="1"/>
       <c r="B65" s="2"/>
       <c r="E65" s="3"/>
@@ -2492,7 +2560,7 @@
       <c r="G65" s="2"/>
       <c r="H65" s="2"/>
     </row>
-    <row r="66" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:8" ht="15">
       <c r="A66" s="1"/>
       <c r="B66" s="2"/>
       <c r="E66" s="3"/>
@@ -2500,7 +2568,7 @@
       <c r="G66" s="2"/>
       <c r="H66" s="2"/>
     </row>
-    <row r="67" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:8" ht="15">
       <c r="A67" s="1"/>
       <c r="B67" s="2"/>
       <c r="E67" s="3"/>
@@ -2508,7 +2576,7 @@
       <c r="G67" s="2"/>
       <c r="H67" s="2"/>
     </row>
-    <row r="68" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:8" ht="15">
       <c r="A68" s="1"/>
       <c r="B68" s="2"/>
       <c r="E68" s="3"/>
@@ -2516,7 +2584,7 @@
       <c r="G68" s="2"/>
       <c r="H68" s="2"/>
     </row>
-    <row r="69" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:8" ht="15">
       <c r="A69" s="1"/>
       <c r="B69" s="2"/>
       <c r="E69" s="3"/>
@@ -2524,7 +2592,7 @@
       <c r="G69" s="2"/>
       <c r="H69" s="2"/>
     </row>
-    <row r="70" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:8" ht="15">
       <c r="A70" s="1"/>
       <c r="B70" s="2"/>
       <c r="E70" s="3"/>
@@ -2532,7 +2600,7 @@
       <c r="G70" s="2"/>
       <c r="H70" s="2"/>
     </row>
-    <row r="71" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:8" ht="15">
       <c r="A71" s="1"/>
       <c r="B71" s="2"/>
       <c r="E71" s="3"/>
@@ -2540,7 +2608,7 @@
       <c r="G71" s="2"/>
       <c r="H71" s="2"/>
     </row>
-    <row r="72" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:8" ht="15">
       <c r="A72" s="1"/>
       <c r="B72" s="2"/>
       <c r="E72" s="3"/>
@@ -2548,7 +2616,7 @@
       <c r="G72" s="2"/>
       <c r="H72" s="2"/>
     </row>
-    <row r="73" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:8" ht="15">
       <c r="A73" s="1"/>
       <c r="B73" s="2"/>
       <c r="E73" s="3"/>
@@ -2556,7 +2624,7 @@
       <c r="G73" s="2"/>
       <c r="H73" s="2"/>
     </row>
-    <row r="74" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:8" ht="15">
       <c r="A74" s="1"/>
       <c r="B74" s="2"/>
       <c r="E74" s="3"/>
@@ -2564,7 +2632,7 @@
       <c r="G74" s="2"/>
       <c r="H74" s="2"/>
     </row>
-    <row r="75" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:8" ht="15">
       <c r="A75" s="1"/>
       <c r="B75" s="2"/>
       <c r="E75" s="3"/>
@@ -2572,7 +2640,7 @@
       <c r="G75" s="2"/>
       <c r="H75" s="2"/>
     </row>
-    <row r="76" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:8" ht="15">
       <c r="A76" s="1"/>
       <c r="B76" s="2"/>
       <c r="E76" s="3"/>
@@ -2580,7 +2648,7 @@
       <c r="G76" s="2"/>
       <c r="H76" s="2"/>
     </row>
-    <row r="77" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:8" ht="15">
       <c r="A77" s="1"/>
       <c r="B77" s="2"/>
       <c r="E77" s="3"/>
@@ -2588,7 +2656,7 @@
       <c r="G77" s="2"/>
       <c r="H77" s="2"/>
     </row>
-    <row r="78" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:8" ht="15">
       <c r="A78" s="1"/>
       <c r="B78" s="2"/>
       <c r="E78" s="3"/>
@@ -2596,7 +2664,7 @@
       <c r="G78" s="2"/>
       <c r="H78" s="2"/>
     </row>
-    <row r="79" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:8" ht="15">
       <c r="A79" s="1"/>
       <c r="B79" s="2"/>
       <c r="E79" s="3"/>
@@ -2604,7 +2672,7 @@
       <c r="G79" s="2"/>
       <c r="H79" s="2"/>
     </row>
-    <row r="80" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:8" ht="15">
       <c r="A80" s="1"/>
       <c r="B80" s="2"/>
       <c r="E80" s="3"/>
@@ -2612,7 +2680,7 @@
       <c r="G80" s="2"/>
       <c r="H80" s="2"/>
     </row>
-    <row r="81" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:8" ht="15">
       <c r="A81" s="1"/>
       <c r="B81" s="2"/>
       <c r="E81" s="3"/>
@@ -2620,7 +2688,7 @@
       <c r="G81" s="2"/>
       <c r="H81" s="2"/>
     </row>
-    <row r="82" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:8" ht="15">
       <c r="A82" s="1"/>
       <c r="B82" s="2"/>
       <c r="E82" s="3"/>
@@ -2628,7 +2696,7 @@
       <c r="G82" s="2"/>
       <c r="H82" s="2"/>
     </row>
-    <row r="83" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:8" ht="15">
       <c r="A83" s="1"/>
       <c r="B83" s="2"/>
       <c r="E83" s="3"/>
@@ -2636,7 +2704,7 @@
       <c r="G83" s="2"/>
       <c r="H83" s="2"/>
     </row>
-    <row r="84" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:8" ht="15">
       <c r="A84" s="1"/>
       <c r="B84" s="2"/>
       <c r="E84" s="3"/>
@@ -2644,7 +2712,7 @@
       <c r="G84" s="2"/>
       <c r="H84" s="2"/>
     </row>
-    <row r="85" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:8" ht="15">
       <c r="A85" s="1"/>
       <c r="B85" s="2"/>
       <c r="E85" s="3"/>
@@ -2652,7 +2720,7 @@
       <c r="G85" s="2"/>
       <c r="H85" s="2"/>
     </row>
-    <row r="86" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:8" ht="15">
       <c r="A86" s="1"/>
       <c r="B86" s="2"/>
       <c r="E86" s="3"/>
@@ -2660,7 +2728,7 @@
       <c r="G86" s="2"/>
       <c r="H86" s="2"/>
     </row>
-    <row r="87" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:8" ht="15">
       <c r="A87" s="1"/>
       <c r="B87" s="2"/>
       <c r="E87" s="3"/>
@@ -2668,7 +2736,7 @@
       <c r="G87" s="2"/>
       <c r="H87" s="2"/>
     </row>
-    <row r="88" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:8">
       <c r="A88" s="1"/>
       <c r="B88" s="2"/>
       <c r="E88" s="3"/>
@@ -2676,7 +2744,7 @@
       <c r="G88" s="2"/>
       <c r="H88" s="2"/>
     </row>
-    <row r="89" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:8">
       <c r="A89" s="1"/>
       <c r="B89" s="2"/>
       <c r="E89" s="3"/>
@@ -2684,7 +2752,7 @@
       <c r="G89" s="2"/>
       <c r="H89" s="2"/>
     </row>
-    <row r="90" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:8">
       <c r="A90" s="1"/>
       <c r="B90" s="2"/>
       <c r="E90" s="3"/>
@@ -2692,7 +2760,7 @@
       <c r="G90" s="2"/>
       <c r="H90" s="2"/>
     </row>
-    <row r="91" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:8">
       <c r="A91" s="1"/>
       <c r="B91" s="2"/>
       <c r="E91" s="3"/>
@@ -2700,7 +2768,7 @@
       <c r="G91" s="2"/>
       <c r="H91" s="2"/>
     </row>
-    <row r="92" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:8">
       <c r="A92" s="1"/>
       <c r="B92" s="2"/>
       <c r="E92" s="3"/>
@@ -2708,7 +2776,7 @@
       <c r="G92" s="2"/>
       <c r="H92" s="2"/>
     </row>
-    <row r="93" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:8">
       <c r="A93" s="1"/>
       <c r="B93" s="2"/>
       <c r="E93" s="3"/>
@@ -2716,7 +2784,7 @@
       <c r="G93" s="2"/>
       <c r="H93" s="2"/>
     </row>
-    <row r="94" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:8">
       <c r="A94" s="1"/>
       <c r="B94" s="2"/>
       <c r="E94" s="3"/>
@@ -2724,7 +2792,7 @@
       <c r="G94" s="2"/>
       <c r="H94" s="2"/>
     </row>
-    <row r="95" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:8">
       <c r="A95" s="1"/>
       <c r="B95" s="2"/>
       <c r="E95" s="3"/>
@@ -2732,7 +2800,7 @@
       <c r="G95" s="2"/>
       <c r="H95" s="2"/>
     </row>
-    <row r="96" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:8">
       <c r="A96" s="1"/>
       <c r="B96" s="2"/>
       <c r="E96" s="3"/>
@@ -2740,7 +2808,7 @@
       <c r="G96" s="2"/>
       <c r="H96" s="2"/>
     </row>
-    <row r="97" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:8">
       <c r="A97" s="1"/>
       <c r="B97" s="2"/>
       <c r="E97" s="3"/>
@@ -2748,7 +2816,7 @@
       <c r="G97" s="2"/>
       <c r="H97" s="2"/>
     </row>
-    <row r="98" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:8">
       <c r="A98" s="1"/>
       <c r="B98" s="2"/>
       <c r="E98" s="3"/>
@@ -2756,7 +2824,7 @@
       <c r="G98" s="2"/>
       <c r="H98" s="2"/>
     </row>
-    <row r="99" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:8">
       <c r="A99" s="1"/>
       <c r="B99" s="2"/>
       <c r="E99" s="3"/>
@@ -2764,7 +2832,7 @@
       <c r="G99" s="2"/>
       <c r="H99" s="2"/>
     </row>
-    <row r="100" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:8">
       <c r="A100" s="1"/>
       <c r="B100" s="2"/>
       <c r="E100" s="3"/>
@@ -2807,19 +2875,19 @@
       <selection activeCell="D2" sqref="D2:D100"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col min="1" max="1" width="7.7109375" customWidth="1"/>
-    <col min="2" max="2" width="17.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="7.69921875" customWidth="1"/>
+    <col min="2" max="2" width="17.296875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.59765625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="9" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.85546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="23.5703125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="13.42578125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="19.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.8984375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="23.59765625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.3984375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="19.09765625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" ht="15.75">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
@@ -2845,7 +2913,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" ht="15">
       <c r="A2" s="1"/>
       <c r="B2" s="2"/>
       <c r="E2" s="3"/>
@@ -2853,7 +2921,7 @@
       <c r="G2" s="2"/>
       <c r="H2" s="2"/>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" ht="15">
       <c r="A3" s="1"/>
       <c r="B3" s="2"/>
       <c r="E3" s="3"/>
@@ -2861,7 +2929,7 @@
       <c r="G3" s="2"/>
       <c r="H3" s="2"/>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" ht="15">
       <c r="A4" s="1"/>
       <c r="B4" s="2"/>
       <c r="E4" s="3"/>
@@ -2869,7 +2937,7 @@
       <c r="G4" s="2"/>
       <c r="H4" s="2"/>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" ht="15">
       <c r="A5" s="1"/>
       <c r="B5" s="2"/>
       <c r="E5" s="3"/>
@@ -2877,7 +2945,7 @@
       <c r="G5" s="2"/>
       <c r="H5" s="2"/>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" ht="15">
       <c r="A6" s="1"/>
       <c r="B6" s="2"/>
       <c r="E6" s="3"/>
@@ -2885,7 +2953,7 @@
       <c r="G6" s="2"/>
       <c r="H6" s="2"/>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" ht="15">
       <c r="A7" s="1"/>
       <c r="B7" s="2"/>
       <c r="E7" s="3"/>
@@ -2893,7 +2961,7 @@
       <c r="G7" s="2"/>
       <c r="H7" s="2"/>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" ht="15">
       <c r="A8" s="1"/>
       <c r="B8" s="2"/>
       <c r="E8" s="3"/>
@@ -2901,7 +2969,7 @@
       <c r="G8" s="2"/>
       <c r="H8" s="2"/>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" ht="15">
       <c r="A9" s="1"/>
       <c r="B9" s="2"/>
       <c r="E9" s="3"/>
@@ -2909,7 +2977,7 @@
       <c r="G9" s="2"/>
       <c r="H9" s="2"/>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" ht="15">
       <c r="A10" s="1"/>
       <c r="B10" s="2"/>
       <c r="E10" s="3"/>
@@ -2917,7 +2985,7 @@
       <c r="G10" s="2"/>
       <c r="H10" s="2"/>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" ht="15">
       <c r="A11" s="1"/>
       <c r="B11" s="2"/>
       <c r="E11" s="3"/>
@@ -2925,7 +2993,7 @@
       <c r="G11" s="2"/>
       <c r="H11" s="2"/>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8" ht="15">
       <c r="A12" s="1"/>
       <c r="B12" s="2"/>
       <c r="E12" s="3"/>
@@ -2933,7 +3001,7 @@
       <c r="G12" s="2"/>
       <c r="H12" s="2"/>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8" ht="15">
       <c r="A13" s="1"/>
       <c r="B13" s="2"/>
       <c r="E13" s="3"/>
@@ -2941,7 +3009,7 @@
       <c r="G13" s="2"/>
       <c r="H13" s="2"/>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8" ht="15">
       <c r="A14" s="1"/>
       <c r="B14" s="2"/>
       <c r="E14" s="3"/>
@@ -2949,7 +3017,7 @@
       <c r="G14" s="2"/>
       <c r="H14" s="2"/>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8" ht="15">
       <c r="A15" s="1"/>
       <c r="B15" s="2"/>
       <c r="E15" s="3"/>
@@ -2957,7 +3025,7 @@
       <c r="G15" s="2"/>
       <c r="H15" s="2"/>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8" ht="15">
       <c r="A16" s="1"/>
       <c r="B16" s="2"/>
       <c r="E16" s="3"/>
@@ -2965,7 +3033,7 @@
       <c r="G16" s="2"/>
       <c r="H16" s="2"/>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:8" ht="15">
       <c r="A17" s="1"/>
       <c r="B17" s="2"/>
       <c r="E17" s="3"/>
@@ -2973,7 +3041,7 @@
       <c r="G17" s="2"/>
       <c r="H17" s="2"/>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:8" ht="15">
       <c r="A18" s="1"/>
       <c r="B18" s="2"/>
       <c r="E18" s="3"/>
@@ -2981,7 +3049,7 @@
       <c r="G18" s="2"/>
       <c r="H18" s="2"/>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:8" ht="15">
       <c r="A19" s="1"/>
       <c r="B19" s="2"/>
       <c r="E19" s="3"/>
@@ -2989,7 +3057,7 @@
       <c r="G19" s="2"/>
       <c r="H19" s="2"/>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:8" ht="15">
       <c r="A20" s="1"/>
       <c r="B20" s="2"/>
       <c r="E20" s="3"/>
@@ -2997,7 +3065,7 @@
       <c r="G20" s="2"/>
       <c r="H20" s="2"/>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:8" ht="15">
       <c r="A21" s="1"/>
       <c r="B21" s="2"/>
       <c r="E21" s="3"/>
@@ -3005,7 +3073,7 @@
       <c r="G21" s="2"/>
       <c r="H21" s="2"/>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:8" ht="15">
       <c r="A22" s="1"/>
       <c r="B22" s="2"/>
       <c r="E22" s="3"/>
@@ -3013,7 +3081,7 @@
       <c r="G22" s="2"/>
       <c r="H22" s="2"/>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:8" ht="15">
       <c r="A23" s="1"/>
       <c r="B23" s="2"/>
       <c r="E23" s="3"/>
@@ -3021,7 +3089,7 @@
       <c r="G23" s="2"/>
       <c r="H23" s="2"/>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:8" ht="15">
       <c r="A24" s="1"/>
       <c r="B24" s="2"/>
       <c r="E24" s="3"/>
@@ -3029,7 +3097,7 @@
       <c r="G24" s="2"/>
       <c r="H24" s="2"/>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:8" ht="15">
       <c r="A25" s="1"/>
       <c r="B25" s="2"/>
       <c r="E25" s="3"/>
@@ -3037,7 +3105,7 @@
       <c r="G25" s="2"/>
       <c r="H25" s="2"/>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:8" ht="15">
       <c r="A26" s="1"/>
       <c r="B26" s="2"/>
       <c r="E26" s="3"/>
@@ -3045,7 +3113,7 @@
       <c r="G26" s="2"/>
       <c r="H26" s="2"/>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:8" ht="15">
       <c r="A27" s="1"/>
       <c r="B27" s="2"/>
       <c r="E27" s="3"/>
@@ -3053,7 +3121,7 @@
       <c r="G27" s="2"/>
       <c r="H27" s="2"/>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:8" ht="15">
       <c r="A28" s="1"/>
       <c r="B28" s="2"/>
       <c r="E28" s="3"/>
@@ -3061,7 +3129,7 @@
       <c r="G28" s="2"/>
       <c r="H28" s="2"/>
     </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:8" ht="15">
       <c r="A29" s="1"/>
       <c r="B29" s="2"/>
       <c r="E29" s="3"/>
@@ -3069,7 +3137,7 @@
       <c r="G29" s="2"/>
       <c r="H29" s="2"/>
     </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:8" ht="15">
       <c r="A30" s="1"/>
       <c r="B30" s="2"/>
       <c r="E30" s="3"/>
@@ -3077,7 +3145,7 @@
       <c r="G30" s="2"/>
       <c r="H30" s="2"/>
     </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:8" ht="15">
       <c r="A31" s="1"/>
       <c r="B31" s="2"/>
       <c r="E31" s="3"/>
@@ -3085,7 +3153,7 @@
       <c r="G31" s="2"/>
       <c r="H31" s="2"/>
     </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:8" ht="15">
       <c r="A32" s="1"/>
       <c r="B32" s="2"/>
       <c r="E32" s="3"/>
@@ -3093,7 +3161,7 @@
       <c r="G32" s="2"/>
       <c r="H32" s="2"/>
     </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:8" ht="15">
       <c r="A33" s="1"/>
       <c r="B33" s="2"/>
       <c r="E33" s="3"/>
@@ -3101,7 +3169,7 @@
       <c r="G33" s="2"/>
       <c r="H33" s="2"/>
     </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:8" ht="15">
       <c r="A34" s="1"/>
       <c r="B34" s="2"/>
       <c r="E34" s="3"/>
@@ -3109,7 +3177,7 @@
       <c r="G34" s="2"/>
       <c r="H34" s="2"/>
     </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:8" ht="15">
       <c r="A35" s="1"/>
       <c r="B35" s="2"/>
       <c r="E35" s="3"/>
@@ -3117,7 +3185,7 @@
       <c r="G35" s="2"/>
       <c r="H35" s="2"/>
     </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:8" ht="15">
       <c r="A36" s="1"/>
       <c r="B36" s="2"/>
       <c r="E36" s="3"/>
@@ -3125,7 +3193,7 @@
       <c r="G36" s="2"/>
       <c r="H36" s="2"/>
     </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:8" ht="15">
       <c r="A37" s="1"/>
       <c r="B37" s="2"/>
       <c r="E37" s="3"/>
@@ -3133,7 +3201,7 @@
       <c r="G37" s="2"/>
       <c r="H37" s="2"/>
     </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:8" ht="15">
       <c r="A38" s="1"/>
       <c r="B38" s="2"/>
       <c r="E38" s="3"/>
@@ -3141,7 +3209,7 @@
       <c r="G38" s="2"/>
       <c r="H38" s="2"/>
     </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:8" ht="15">
       <c r="A39" s="1"/>
       <c r="B39" s="2"/>
       <c r="E39" s="3"/>
@@ -3149,7 +3217,7 @@
       <c r="G39" s="2"/>
       <c r="H39" s="2"/>
     </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:8" ht="15">
       <c r="A40" s="1"/>
       <c r="B40" s="2"/>
       <c r="E40" s="3"/>
@@ -3157,7 +3225,7 @@
       <c r="G40" s="2"/>
       <c r="H40" s="2"/>
     </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:8" ht="15">
       <c r="A41" s="1"/>
       <c r="B41" s="2"/>
       <c r="E41" s="3"/>
@@ -3165,7 +3233,7 @@
       <c r="G41" s="2"/>
       <c r="H41" s="2"/>
     </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:8" ht="15">
       <c r="A42" s="1"/>
       <c r="B42" s="2"/>
       <c r="E42" s="3"/>
@@ -3173,7 +3241,7 @@
       <c r="G42" s="2"/>
       <c r="H42" s="2"/>
     </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:8" ht="15">
       <c r="A43" s="1"/>
       <c r="B43" s="2"/>
       <c r="E43" s="3"/>
@@ -3181,7 +3249,7 @@
       <c r="G43" s="2"/>
       <c r="H43" s="2"/>
     </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:8" ht="15">
       <c r="A44" s="1"/>
       <c r="B44" s="2"/>
       <c r="E44" s="3"/>
@@ -3189,7 +3257,7 @@
       <c r="G44" s="2"/>
       <c r="H44" s="2"/>
     </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:8" ht="15">
       <c r="A45" s="1"/>
       <c r="B45" s="2"/>
       <c r="E45" s="3"/>
@@ -3197,7 +3265,7 @@
       <c r="G45" s="2"/>
       <c r="H45" s="2"/>
     </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:8" ht="15">
       <c r="A46" s="1"/>
       <c r="B46" s="2"/>
       <c r="E46" s="3"/>
@@ -3205,7 +3273,7 @@
       <c r="G46" s="2"/>
       <c r="H46" s="2"/>
     </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:8" ht="15">
       <c r="A47" s="1"/>
       <c r="B47" s="2"/>
       <c r="E47" s="3"/>
@@ -3213,7 +3281,7 @@
       <c r="G47" s="2"/>
       <c r="H47" s="2"/>
     </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:8" ht="15">
       <c r="A48" s="1"/>
       <c r="B48" s="2"/>
       <c r="E48" s="3"/>
@@ -3221,7 +3289,7 @@
       <c r="G48" s="2"/>
       <c r="H48" s="2"/>
     </row>
-    <row r="49" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:8" ht="15">
       <c r="A49" s="1"/>
       <c r="B49" s="2"/>
       <c r="E49" s="3"/>
@@ -3229,7 +3297,7 @@
       <c r="G49" s="2"/>
       <c r="H49" s="2"/>
     </row>
-    <row r="50" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:8" ht="15">
       <c r="A50" s="1"/>
       <c r="B50" s="2"/>
       <c r="E50" s="3"/>
@@ -3237,7 +3305,7 @@
       <c r="G50" s="2"/>
       <c r="H50" s="2"/>
     </row>
-    <row r="51" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:8" ht="15">
       <c r="A51" s="1"/>
       <c r="B51" s="2"/>
       <c r="E51" s="3"/>
@@ -3245,7 +3313,7 @@
       <c r="G51" s="2"/>
       <c r="H51" s="2"/>
     </row>
-    <row r="52" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:8" ht="15">
       <c r="A52" s="1"/>
       <c r="B52" s="2"/>
       <c r="E52" s="3"/>
@@ -3253,7 +3321,7 @@
       <c r="G52" s="2"/>
       <c r="H52" s="2"/>
     </row>
-    <row r="53" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:8" ht="15">
       <c r="A53" s="1"/>
       <c r="B53" s="2"/>
       <c r="E53" s="3"/>
@@ -3261,7 +3329,7 @@
       <c r="G53" s="2"/>
       <c r="H53" s="2"/>
     </row>
-    <row r="54" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:8" ht="15">
       <c r="A54" s="1"/>
       <c r="B54" s="2"/>
       <c r="E54" s="3"/>
@@ -3269,7 +3337,7 @@
       <c r="G54" s="2"/>
       <c r="H54" s="2"/>
     </row>
-    <row r="55" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:8" ht="15">
       <c r="A55" s="1"/>
       <c r="B55" s="2"/>
       <c r="E55" s="3"/>
@@ -3277,7 +3345,7 @@
       <c r="G55" s="2"/>
       <c r="H55" s="2"/>
     </row>
-    <row r="56" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:8" ht="15">
       <c r="A56" s="1"/>
       <c r="B56" s="2"/>
       <c r="E56" s="3"/>
@@ -3285,7 +3353,7 @@
       <c r="G56" s="2"/>
       <c r="H56" s="2"/>
     </row>
-    <row r="57" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:8" ht="15">
       <c r="A57" s="1"/>
       <c r="B57" s="2"/>
       <c r="E57" s="3"/>
@@ -3293,7 +3361,7 @@
       <c r="G57" s="2"/>
       <c r="H57" s="2"/>
     </row>
-    <row r="58" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:8" ht="15">
       <c r="A58" s="1"/>
       <c r="B58" s="2"/>
       <c r="E58" s="3"/>
@@ -3301,7 +3369,7 @@
       <c r="G58" s="2"/>
       <c r="H58" s="2"/>
     </row>
-    <row r="59" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:8" ht="15">
       <c r="A59" s="1"/>
       <c r="B59" s="2"/>
       <c r="E59" s="3"/>
@@ -3309,7 +3377,7 @@
       <c r="G59" s="2"/>
       <c r="H59" s="2"/>
     </row>
-    <row r="60" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:8" ht="15">
       <c r="A60" s="1"/>
       <c r="B60" s="2"/>
       <c r="E60" s="3"/>
@@ -3317,7 +3385,7 @@
       <c r="G60" s="2"/>
       <c r="H60" s="2"/>
     </row>
-    <row r="61" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:8" ht="15">
       <c r="A61" s="1"/>
       <c r="B61" s="2"/>
       <c r="E61" s="3"/>
@@ -3325,7 +3393,7 @@
       <c r="G61" s="2"/>
       <c r="H61" s="2"/>
     </row>
-    <row r="62" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:8" ht="15">
       <c r="A62" s="1"/>
       <c r="B62" s="2"/>
       <c r="E62" s="3"/>
@@ -3333,7 +3401,7 @@
       <c r="G62" s="2"/>
       <c r="H62" s="2"/>
     </row>
-    <row r="63" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:8" ht="15">
       <c r="A63" s="1"/>
       <c r="B63" s="2"/>
       <c r="E63" s="3"/>
@@ -3341,7 +3409,7 @@
       <c r="G63" s="2"/>
       <c r="H63" s="2"/>
     </row>
-    <row r="64" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:8" ht="15">
       <c r="A64" s="1"/>
       <c r="B64" s="2"/>
       <c r="E64" s="3"/>
@@ -3349,7 +3417,7 @@
       <c r="G64" s="2"/>
       <c r="H64" s="2"/>
     </row>
-    <row r="65" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:8" ht="15">
       <c r="A65" s="1"/>
       <c r="B65" s="2"/>
       <c r="E65" s="3"/>
@@ -3357,7 +3425,7 @@
       <c r="G65" s="2"/>
       <c r="H65" s="2"/>
     </row>
-    <row r="66" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:8" ht="15">
       <c r="A66" s="1"/>
       <c r="B66" s="2"/>
       <c r="E66" s="3"/>
@@ -3365,7 +3433,7 @@
       <c r="G66" s="2"/>
       <c r="H66" s="2"/>
     </row>
-    <row r="67" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:8" ht="15">
       <c r="A67" s="1"/>
       <c r="B67" s="2"/>
       <c r="E67" s="3"/>
@@ -3373,7 +3441,7 @@
       <c r="G67" s="2"/>
       <c r="H67" s="2"/>
     </row>
-    <row r="68" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:8" ht="15">
       <c r="A68" s="1"/>
       <c r="B68" s="2"/>
       <c r="E68" s="3"/>
@@ -3381,7 +3449,7 @@
       <c r="G68" s="2"/>
       <c r="H68" s="2"/>
     </row>
-    <row r="69" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:8" ht="15">
       <c r="A69" s="1"/>
       <c r="B69" s="2"/>
       <c r="E69" s="3"/>
@@ -3389,7 +3457,7 @@
       <c r="G69" s="2"/>
       <c r="H69" s="2"/>
     </row>
-    <row r="70" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:8" ht="15">
       <c r="A70" s="1"/>
       <c r="B70" s="2"/>
       <c r="E70" s="3"/>
@@ -3397,7 +3465,7 @@
       <c r="G70" s="2"/>
       <c r="H70" s="2"/>
     </row>
-    <row r="71" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:8" ht="15">
       <c r="A71" s="1"/>
       <c r="B71" s="2"/>
       <c r="E71" s="3"/>
@@ -3405,7 +3473,7 @@
       <c r="G71" s="2"/>
       <c r="H71" s="2"/>
     </row>
-    <row r="72" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:8" ht="15">
       <c r="A72" s="1"/>
       <c r="B72" s="2"/>
       <c r="E72" s="3"/>
@@ -3413,7 +3481,7 @@
       <c r="G72" s="2"/>
       <c r="H72" s="2"/>
     </row>
-    <row r="73" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:8" ht="15">
       <c r="A73" s="1"/>
       <c r="B73" s="2"/>
       <c r="E73" s="3"/>
@@ -3421,7 +3489,7 @@
       <c r="G73" s="2"/>
       <c r="H73" s="2"/>
     </row>
-    <row r="74" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:8" ht="15">
       <c r="A74" s="1"/>
       <c r="B74" s="2"/>
       <c r="E74" s="3"/>
@@ -3429,7 +3497,7 @@
       <c r="G74" s="2"/>
       <c r="H74" s="2"/>
     </row>
-    <row r="75" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:8" ht="15">
       <c r="A75" s="1"/>
       <c r="B75" s="2"/>
       <c r="E75" s="3"/>
@@ -3437,7 +3505,7 @@
       <c r="G75" s="2"/>
       <c r="H75" s="2"/>
     </row>
-    <row r="76" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:8" ht="15">
       <c r="A76" s="1"/>
       <c r="B76" s="2"/>
       <c r="E76" s="3"/>
@@ -3445,7 +3513,7 @@
       <c r="G76" s="2"/>
       <c r="H76" s="2"/>
     </row>
-    <row r="77" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:8" ht="15">
       <c r="A77" s="1"/>
       <c r="B77" s="2"/>
       <c r="E77" s="3"/>
@@ -3453,7 +3521,7 @@
       <c r="G77" s="2"/>
       <c r="H77" s="2"/>
     </row>
-    <row r="78" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:8" ht="15">
       <c r="A78" s="1"/>
       <c r="B78" s="2"/>
       <c r="E78" s="3"/>
@@ -3461,7 +3529,7 @@
       <c r="G78" s="2"/>
       <c r="H78" s="2"/>
     </row>
-    <row r="79" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:8" ht="15">
       <c r="A79" s="1"/>
       <c r="B79" s="2"/>
       <c r="E79" s="3"/>
@@ -3469,7 +3537,7 @@
       <c r="G79" s="2"/>
       <c r="H79" s="2"/>
     </row>
-    <row r="80" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:8" ht="15">
       <c r="A80" s="1"/>
       <c r="B80" s="2"/>
       <c r="E80" s="3"/>
@@ -3477,7 +3545,7 @@
       <c r="G80" s="2"/>
       <c r="H80" s="2"/>
     </row>
-    <row r="81" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:8" ht="15">
       <c r="A81" s="1"/>
       <c r="B81" s="2"/>
       <c r="E81" s="3"/>
@@ -3485,7 +3553,7 @@
       <c r="G81" s="2"/>
       <c r="H81" s="2"/>
     </row>
-    <row r="82" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:8" ht="15">
       <c r="A82" s="1"/>
       <c r="B82" s="2"/>
       <c r="E82" s="3"/>
@@ -3493,7 +3561,7 @@
       <c r="G82" s="2"/>
       <c r="H82" s="2"/>
     </row>
-    <row r="83" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:8" ht="15">
       <c r="A83" s="1"/>
       <c r="B83" s="2"/>
       <c r="E83" s="3"/>
@@ -3501,7 +3569,7 @@
       <c r="G83" s="2"/>
       <c r="H83" s="2"/>
     </row>
-    <row r="84" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:8" ht="15">
       <c r="A84" s="1"/>
       <c r="B84" s="2"/>
       <c r="E84" s="3"/>
@@ -3509,7 +3577,7 @@
       <c r="G84" s="2"/>
       <c r="H84" s="2"/>
     </row>
-    <row r="85" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:8" ht="15">
       <c r="A85" s="1"/>
       <c r="B85" s="2"/>
       <c r="E85" s="3"/>
@@ -3517,7 +3585,7 @@
       <c r="G85" s="2"/>
       <c r="H85" s="2"/>
     </row>
-    <row r="86" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:8" ht="15">
       <c r="A86" s="1"/>
       <c r="B86" s="2"/>
       <c r="E86" s="3"/>
@@ -3525,7 +3593,7 @@
       <c r="G86" s="2"/>
       <c r="H86" s="2"/>
     </row>
-    <row r="87" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:8" ht="15">
       <c r="A87" s="1"/>
       <c r="B87" s="2"/>
       <c r="E87" s="3"/>
@@ -3533,7 +3601,7 @@
       <c r="G87" s="2"/>
       <c r="H87" s="2"/>
     </row>
-    <row r="88" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:8">
       <c r="A88" s="1"/>
       <c r="B88" s="2"/>
       <c r="E88" s="3"/>
@@ -3541,7 +3609,7 @@
       <c r="G88" s="2"/>
       <c r="H88" s="2"/>
     </row>
-    <row r="89" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:8">
       <c r="A89" s="1"/>
       <c r="B89" s="2"/>
       <c r="E89" s="3"/>
@@ -3549,7 +3617,7 @@
       <c r="G89" s="2"/>
       <c r="H89" s="2"/>
     </row>
-    <row r="90" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:8">
       <c r="A90" s="1"/>
       <c r="B90" s="2"/>
       <c r="E90" s="3"/>
@@ -3557,7 +3625,7 @@
       <c r="G90" s="2"/>
       <c r="H90" s="2"/>
     </row>
-    <row r="91" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:8">
       <c r="A91" s="1"/>
       <c r="B91" s="2"/>
       <c r="E91" s="3"/>
@@ -3565,7 +3633,7 @@
       <c r="G91" s="2"/>
       <c r="H91" s="2"/>
     </row>
-    <row r="92" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:8">
       <c r="A92" s="1"/>
       <c r="B92" s="2"/>
       <c r="E92" s="3"/>
@@ -3573,7 +3641,7 @@
       <c r="G92" s="2"/>
       <c r="H92" s="2"/>
     </row>
-    <row r="93" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:8">
       <c r="A93" s="1"/>
       <c r="B93" s="2"/>
       <c r="E93" s="3"/>
@@ -3581,7 +3649,7 @@
       <c r="G93" s="2"/>
       <c r="H93" s="2"/>
     </row>
-    <row r="94" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:8">
       <c r="A94" s="1"/>
       <c r="B94" s="2"/>
       <c r="E94" s="3"/>
@@ -3589,7 +3657,7 @@
       <c r="G94" s="2"/>
       <c r="H94" s="2"/>
     </row>
-    <row r="95" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:8">
       <c r="A95" s="1"/>
       <c r="B95" s="2"/>
       <c r="E95" s="3"/>
@@ -3597,7 +3665,7 @@
       <c r="G95" s="2"/>
       <c r="H95" s="2"/>
     </row>
-    <row r="96" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:8">
       <c r="A96" s="1"/>
       <c r="B96" s="2"/>
       <c r="E96" s="3"/>
@@ -3605,7 +3673,7 @@
       <c r="G96" s="2"/>
       <c r="H96" s="2"/>
     </row>
-    <row r="97" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:8">
       <c r="A97" s="1"/>
       <c r="B97" s="2"/>
       <c r="E97" s="3"/>
@@ -3613,7 +3681,7 @@
       <c r="G97" s="2"/>
       <c r="H97" s="2"/>
     </row>
-    <row r="98" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:8">
       <c r="A98" s="1"/>
       <c r="B98" s="2"/>
       <c r="E98" s="3"/>
@@ -3621,7 +3689,7 @@
       <c r="G98" s="2"/>
       <c r="H98" s="2"/>
     </row>
-    <row r="99" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:8">
       <c r="A99" s="1"/>
       <c r="B99" s="2"/>
       <c r="E99" s="3"/>
@@ -3629,7 +3697,7 @@
       <c r="G99" s="2"/>
       <c r="H99" s="2"/>
     </row>
-    <row r="100" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:8">
       <c r="A100" s="1"/>
       <c r="B100" s="2"/>
       <c r="E100" s="3"/>
@@ -3672,21 +3740,21 @@
       <selection activeCell="P21" sqref="P21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col min="1" max="1" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="19.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.5703125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.09765625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.8984375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.8984375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19.3984375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.59765625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.59765625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="9" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="17.85546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="17.8984375" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="17" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="19.140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="19.09765625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" ht="15.75">
       <c r="A1" s="7" t="s">
         <v>8</v>
       </c>
@@ -3718,7 +3786,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" ht="15">
       <c r="A2" s="2"/>
       <c r="B2" s="8"/>
       <c r="D2" s="2"/>
@@ -3726,7 +3794,7 @@
       <c r="I2" s="8"/>
       <c r="J2" s="2"/>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" ht="15">
       <c r="A3" s="2"/>
       <c r="B3" s="8"/>
       <c r="D3" s="2"/>
@@ -3734,7 +3802,7 @@
       <c r="I3" s="8"/>
       <c r="J3" s="2"/>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" ht="15">
       <c r="A4" s="2"/>
       <c r="B4" s="8"/>
       <c r="D4" s="2"/>
@@ -3742,7 +3810,7 @@
       <c r="I4" s="8"/>
       <c r="J4" s="2"/>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" ht="15">
       <c r="A5" s="2"/>
       <c r="B5" s="8"/>
       <c r="D5" s="2"/>
@@ -3750,7 +3818,7 @@
       <c r="I5" s="8"/>
       <c r="J5" s="2"/>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" ht="15">
       <c r="A6" s="2"/>
       <c r="B6" s="8"/>
       <c r="D6" s="2"/>
@@ -3758,7 +3826,7 @@
       <c r="I6" s="8"/>
       <c r="J6" s="2"/>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10" ht="15">
       <c r="A7" s="2"/>
       <c r="B7" s="8"/>
       <c r="D7" s="2"/>
@@ -3766,7 +3834,7 @@
       <c r="I7" s="8"/>
       <c r="J7" s="2"/>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10" ht="15">
       <c r="A8" s="2"/>
       <c r="B8" s="8"/>
       <c r="D8" s="2"/>
@@ -3774,7 +3842,7 @@
       <c r="I8" s="8"/>
       <c r="J8" s="2"/>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10" ht="15">
       <c r="A9" s="2"/>
       <c r="B9" s="8"/>
       <c r="D9" s="2"/>
@@ -3782,7 +3850,7 @@
       <c r="I9" s="8"/>
       <c r="J9" s="2"/>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:10" ht="15">
       <c r="A10" s="2"/>
       <c r="B10" s="8"/>
       <c r="D10" s="2"/>
@@ -3790,7 +3858,7 @@
       <c r="I10" s="8"/>
       <c r="J10" s="2"/>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:10" ht="15">
       <c r="A11" s="2"/>
       <c r="B11" s="8"/>
       <c r="D11" s="2"/>
@@ -3798,7 +3866,7 @@
       <c r="I11" s="8"/>
       <c r="J11" s="2"/>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:10" ht="15">
       <c r="A12" s="2"/>
       <c r="B12" s="8"/>
       <c r="D12" s="2"/>
@@ -3806,7 +3874,7 @@
       <c r="I12" s="8"/>
       <c r="J12" s="2"/>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:10" ht="15">
       <c r="A13" s="2"/>
       <c r="B13" s="8"/>
       <c r="D13" s="2"/>
@@ -3814,7 +3882,7 @@
       <c r="I13" s="8"/>
       <c r="J13" s="2"/>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:10" ht="15">
       <c r="A14" s="2"/>
       <c r="B14" s="8"/>
       <c r="D14" s="2"/>
@@ -3822,7 +3890,7 @@
       <c r="I14" s="8"/>
       <c r="J14" s="2"/>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:10" ht="15">
       <c r="A15" s="2"/>
       <c r="B15" s="8"/>
       <c r="D15" s="2"/>
@@ -3830,7 +3898,7 @@
       <c r="I15" s="8"/>
       <c r="J15" s="2"/>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:10" ht="15">
       <c r="A16" s="2"/>
       <c r="B16" s="8"/>
       <c r="D16" s="2"/>
@@ -3838,7 +3906,7 @@
       <c r="I16" s="8"/>
       <c r="J16" s="2"/>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:10" ht="15">
       <c r="A17" s="2"/>
       <c r="B17" s="8"/>
       <c r="D17" s="2"/>
@@ -3846,7 +3914,7 @@
       <c r="I17" s="8"/>
       <c r="J17" s="2"/>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:10" ht="15">
       <c r="A18" s="2"/>
       <c r="B18" s="8"/>
       <c r="D18" s="2"/>
@@ -3854,7 +3922,7 @@
       <c r="I18" s="8"/>
       <c r="J18" s="2"/>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:10" ht="15">
       <c r="A19" s="2"/>
       <c r="B19" s="8"/>
       <c r="D19" s="2"/>
@@ -3862,7 +3930,7 @@
       <c r="I19" s="8"/>
       <c r="J19" s="2"/>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:10" ht="15">
       <c r="A20" s="2"/>
       <c r="B20" s="8"/>
       <c r="D20" s="2"/>
@@ -3870,7 +3938,7 @@
       <c r="I20" s="8"/>
       <c r="J20" s="2"/>
     </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:10" ht="15">
       <c r="A21" s="2"/>
       <c r="B21" s="8"/>
       <c r="D21" s="2"/>
@@ -3878,7 +3946,7 @@
       <c r="I21" s="8"/>
       <c r="J21" s="2"/>
     </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:10" ht="15">
       <c r="A22" s="2"/>
       <c r="B22" s="8"/>
       <c r="D22" s="2"/>
@@ -3886,7 +3954,7 @@
       <c r="I22" s="8"/>
       <c r="J22" s="2"/>
     </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:10" ht="15">
       <c r="A23" s="2"/>
       <c r="B23" s="8"/>
       <c r="D23" s="2"/>
@@ -3894,7 +3962,7 @@
       <c r="I23" s="8"/>
       <c r="J23" s="2"/>
     </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:10" ht="15">
       <c r="A24" s="2"/>
       <c r="B24" s="8"/>
       <c r="D24" s="2"/>
@@ -3902,7 +3970,7 @@
       <c r="I24" s="8"/>
       <c r="J24" s="2"/>
     </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:10" ht="15">
       <c r="A25" s="2"/>
       <c r="B25" s="8"/>
       <c r="D25" s="2"/>
@@ -3910,7 +3978,7 @@
       <c r="I25" s="8"/>
       <c r="J25" s="2"/>
     </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:10">
       <c r="A26" s="2"/>
       <c r="B26" s="8"/>
       <c r="D26" s="2"/>
@@ -3918,7 +3986,7 @@
       <c r="I26" s="8"/>
       <c r="J26" s="2"/>
     </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:10">
       <c r="A27" s="2"/>
       <c r="B27" s="8"/>
       <c r="D27" s="2"/>
@@ -3926,7 +3994,7 @@
       <c r="I27" s="8"/>
       <c r="J27" s="2"/>
     </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:10">
       <c r="A28" s="2"/>
       <c r="B28" s="8"/>
       <c r="D28" s="2"/>
@@ -3934,7 +4002,7 @@
       <c r="I28" s="8"/>
       <c r="J28" s="2"/>
     </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:10">
       <c r="A29" s="2"/>
       <c r="B29" s="8"/>
       <c r="D29" s="2"/>
@@ -3942,7 +4010,7 @@
       <c r="I29" s="8"/>
       <c r="J29" s="2"/>
     </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:10">
       <c r="A30" s="2"/>
       <c r="B30" s="8"/>
       <c r="D30" s="2"/>
@@ -3950,7 +4018,7 @@
       <c r="I30" s="8"/>
       <c r="J30" s="2"/>
     </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:10">
       <c r="A31" s="2"/>
       <c r="B31" s="8"/>
       <c r="D31" s="2"/>
@@ -3958,7 +4026,7 @@
       <c r="I31" s="8"/>
       <c r="J31" s="2"/>
     </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:10">
       <c r="A32" s="2"/>
       <c r="B32" s="8"/>
       <c r="D32" s="2"/>
@@ -3966,7 +4034,7 @@
       <c r="I32" s="8"/>
       <c r="J32" s="2"/>
     </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:10">
       <c r="A33" s="2"/>
       <c r="B33" s="8"/>
       <c r="D33" s="2"/>
@@ -3974,7 +4042,7 @@
       <c r="I33" s="8"/>
       <c r="J33" s="2"/>
     </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:10">
       <c r="A34" s="2"/>
       <c r="B34" s="8"/>
       <c r="D34" s="2"/>
@@ -3982,7 +4050,7 @@
       <c r="I34" s="8"/>
       <c r="J34" s="2"/>
     </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:10">
       <c r="A35" s="2"/>
       <c r="B35" s="8"/>
       <c r="D35" s="2"/>
@@ -3990,7 +4058,7 @@
       <c r="I35" s="8"/>
       <c r="J35" s="2"/>
     </row>
-    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:10">
       <c r="A36" s="2"/>
       <c r="B36" s="8"/>
       <c r="D36" s="2"/>
@@ -3998,7 +4066,7 @@
       <c r="I36" s="8"/>
       <c r="J36" s="2"/>
     </row>
-    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:10">
       <c r="A37" s="2"/>
       <c r="B37" s="8"/>
       <c r="D37" s="2"/>
@@ -4006,7 +4074,7 @@
       <c r="I37" s="8"/>
       <c r="J37" s="2"/>
     </row>
-    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:10">
       <c r="A38" s="2"/>
       <c r="B38" s="8"/>
       <c r="D38" s="2"/>
@@ -4014,7 +4082,7 @@
       <c r="I38" s="8"/>
       <c r="J38" s="2"/>
     </row>
-    <row r="39" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:10">
       <c r="A39" s="2"/>
       <c r="B39" s="8"/>
       <c r="D39" s="2"/>
@@ -4022,7 +4090,7 @@
       <c r="I39" s="8"/>
       <c r="J39" s="2"/>
     </row>
-    <row r="40" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:10">
       <c r="A40" s="2"/>
       <c r="B40" s="8"/>
       <c r="D40" s="2"/>
@@ -4030,7 +4098,7 @@
       <c r="I40" s="8"/>
       <c r="J40" s="2"/>
     </row>
-    <row r="41" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:10">
       <c r="A41" s="2"/>
       <c r="B41" s="8"/>
       <c r="D41" s="2"/>
@@ -4038,7 +4106,7 @@
       <c r="I41" s="8"/>
       <c r="J41" s="2"/>
     </row>
-    <row r="42" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:10">
       <c r="A42" s="2"/>
       <c r="B42" s="8"/>
       <c r="D42" s="2"/>
@@ -4046,7 +4114,7 @@
       <c r="I42" s="8"/>
       <c r="J42" s="2"/>
     </row>
-    <row r="43" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:10">
       <c r="A43" s="2"/>
       <c r="B43" s="8"/>
       <c r="D43" s="2"/>
@@ -4054,7 +4122,7 @@
       <c r="I43" s="8"/>
       <c r="J43" s="2"/>
     </row>
-    <row r="44" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:10">
       <c r="A44" s="2"/>
       <c r="B44" s="8"/>
       <c r="D44" s="2"/>
@@ -4062,7 +4130,7 @@
       <c r="I44" s="8"/>
       <c r="J44" s="2"/>
     </row>
-    <row r="45" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:10">
       <c r="A45" s="2"/>
       <c r="B45" s="8"/>
       <c r="D45" s="2"/>
@@ -4070,7 +4138,7 @@
       <c r="I45" s="8"/>
       <c r="J45" s="2"/>
     </row>
-    <row r="46" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:10">
       <c r="A46" s="2"/>
       <c r="B46" s="8"/>
       <c r="D46" s="2"/>
@@ -4078,7 +4146,7 @@
       <c r="I46" s="8"/>
       <c r="J46" s="2"/>
     </row>
-    <row r="47" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:10">
       <c r="A47" s="2"/>
       <c r="B47" s="8"/>
       <c r="D47" s="2"/>
@@ -4086,7 +4154,7 @@
       <c r="I47" s="8"/>
       <c r="J47" s="2"/>
     </row>
-    <row r="48" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:10">
       <c r="A48" s="2"/>
       <c r="B48" s="8"/>
       <c r="D48" s="2"/>
@@ -4094,7 +4162,7 @@
       <c r="I48" s="8"/>
       <c r="J48" s="2"/>
     </row>
-    <row r="49" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:10">
       <c r="A49" s="2"/>
       <c r="B49" s="8"/>
       <c r="D49" s="2"/>
@@ -4102,7 +4170,7 @@
       <c r="I49" s="8"/>
       <c r="J49" s="2"/>
     </row>
-    <row r="50" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:10">
       <c r="A50" s="2"/>
       <c r="B50" s="8"/>
       <c r="D50" s="2"/>
@@ -4110,7 +4178,7 @@
       <c r="I50" s="8"/>
       <c r="J50" s="2"/>
     </row>
-    <row r="51" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:10">
       <c r="A51" s="2"/>
       <c r="B51" s="8"/>
       <c r="D51" s="2"/>
@@ -4118,7 +4186,7 @@
       <c r="I51" s="8"/>
       <c r="J51" s="2"/>
     </row>
-    <row r="52" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:10">
       <c r="A52" s="2"/>
       <c r="B52" s="8"/>
       <c r="D52" s="2"/>
@@ -4126,7 +4194,7 @@
       <c r="I52" s="8"/>
       <c r="J52" s="2"/>
     </row>
-    <row r="53" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:10">
       <c r="A53" s="2"/>
       <c r="B53" s="8"/>
       <c r="D53" s="2"/>
@@ -4134,7 +4202,7 @@
       <c r="I53" s="8"/>
       <c r="J53" s="2"/>
     </row>
-    <row r="54" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:10">
       <c r="A54" s="2"/>
       <c r="B54" s="8"/>
       <c r="D54" s="2"/>
@@ -4142,7 +4210,7 @@
       <c r="I54" s="8"/>
       <c r="J54" s="2"/>
     </row>
-    <row r="55" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:10">
       <c r="A55" s="2"/>
       <c r="B55" s="8"/>
       <c r="D55" s="2"/>
@@ -4150,7 +4218,7 @@
       <c r="I55" s="8"/>
       <c r="J55" s="2"/>
     </row>
-    <row r="56" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:10">
       <c r="A56" s="2"/>
       <c r="B56" s="8"/>
       <c r="D56" s="2"/>
@@ -4158,7 +4226,7 @@
       <c r="I56" s="8"/>
       <c r="J56" s="2"/>
     </row>
-    <row r="57" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:10">
       <c r="A57" s="2"/>
       <c r="B57" s="8"/>
       <c r="D57" s="2"/>
@@ -4166,7 +4234,7 @@
       <c r="I57" s="8"/>
       <c r="J57" s="2"/>
     </row>
-    <row r="58" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:10">
       <c r="A58" s="2"/>
       <c r="B58" s="8"/>
       <c r="D58" s="2"/>
@@ -4174,7 +4242,7 @@
       <c r="I58" s="8"/>
       <c r="J58" s="2"/>
     </row>
-    <row r="59" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:10">
       <c r="A59" s="2"/>
       <c r="B59" s="8"/>
       <c r="D59" s="2"/>
@@ -4182,7 +4250,7 @@
       <c r="I59" s="8"/>
       <c r="J59" s="2"/>
     </row>
-    <row r="60" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:10">
       <c r="A60" s="2"/>
       <c r="B60" s="8"/>
       <c r="D60" s="2"/>
@@ -4190,7 +4258,7 @@
       <c r="I60" s="8"/>
       <c r="J60" s="2"/>
     </row>
-    <row r="61" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:10">
       <c r="A61" s="2"/>
       <c r="B61" s="8"/>
       <c r="D61" s="2"/>
@@ -4198,7 +4266,7 @@
       <c r="I61" s="8"/>
       <c r="J61" s="2"/>
     </row>
-    <row r="62" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:10">
       <c r="A62" s="2"/>
       <c r="B62" s="8"/>
       <c r="D62" s="2"/>
@@ -4206,7 +4274,7 @@
       <c r="I62" s="8"/>
       <c r="J62" s="2"/>
     </row>
-    <row r="63" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:10">
       <c r="A63" s="2"/>
       <c r="B63" s="8"/>
       <c r="D63" s="2"/>
@@ -4214,7 +4282,7 @@
       <c r="I63" s="8"/>
       <c r="J63" s="2"/>
     </row>
-    <row r="64" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:10">
       <c r="A64" s="2"/>
       <c r="B64" s="8"/>
       <c r="D64" s="2"/>
@@ -4222,7 +4290,7 @@
       <c r="I64" s="8"/>
       <c r="J64" s="2"/>
     </row>
-    <row r="65" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:10">
       <c r="A65" s="2"/>
       <c r="B65" s="8"/>
       <c r="D65" s="2"/>
@@ -4230,7 +4298,7 @@
       <c r="I65" s="8"/>
       <c r="J65" s="2"/>
     </row>
-    <row r="66" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:10">
       <c r="A66" s="2"/>
       <c r="B66" s="8"/>
       <c r="D66" s="2"/>
@@ -4238,7 +4306,7 @@
       <c r="I66" s="8"/>
       <c r="J66" s="2"/>
     </row>
-    <row r="67" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:10">
       <c r="A67" s="2"/>
       <c r="B67" s="8"/>
       <c r="D67" s="2"/>
@@ -4246,7 +4314,7 @@
       <c r="I67" s="8"/>
       <c r="J67" s="2"/>
     </row>
-    <row r="68" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:10">
       <c r="A68" s="2"/>
       <c r="B68" s="8"/>
       <c r="D68" s="2"/>
@@ -4254,7 +4322,7 @@
       <c r="I68" s="8"/>
       <c r="J68" s="2"/>
     </row>
-    <row r="69" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:10">
       <c r="A69" s="2"/>
       <c r="B69" s="8"/>
       <c r="D69" s="2"/>
@@ -4262,7 +4330,7 @@
       <c r="I69" s="8"/>
       <c r="J69" s="2"/>
     </row>
-    <row r="70" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:10">
       <c r="A70" s="2"/>
       <c r="B70" s="8"/>
       <c r="D70" s="2"/>
@@ -4270,7 +4338,7 @@
       <c r="I70" s="8"/>
       <c r="J70" s="2"/>
     </row>
-    <row r="71" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:10">
       <c r="A71" s="2"/>
       <c r="B71" s="8"/>
       <c r="D71" s="2"/>
@@ -4278,7 +4346,7 @@
       <c r="I71" s="8"/>
       <c r="J71" s="2"/>
     </row>
-    <row r="72" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:10">
       <c r="A72" s="2"/>
       <c r="B72" s="8"/>
       <c r="D72" s="2"/>
@@ -4286,7 +4354,7 @@
       <c r="I72" s="8"/>
       <c r="J72" s="2"/>
     </row>
-    <row r="73" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:10">
       <c r="A73" s="2"/>
       <c r="B73" s="8"/>
       <c r="D73" s="2"/>
@@ -4294,7 +4362,7 @@
       <c r="I73" s="8"/>
       <c r="J73" s="2"/>
     </row>
-    <row r="74" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:10">
       <c r="A74" s="2"/>
       <c r="B74" s="8"/>
       <c r="D74" s="2"/>
@@ -4302,7 +4370,7 @@
       <c r="I74" s="8"/>
       <c r="J74" s="2"/>
     </row>
-    <row r="75" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:10">
       <c r="A75" s="2"/>
       <c r="B75" s="8"/>
       <c r="D75" s="2"/>
@@ -4310,7 +4378,7 @@
       <c r="I75" s="8"/>
       <c r="J75" s="2"/>
     </row>
-    <row r="76" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:10">
       <c r="A76" s="2"/>
       <c r="B76" s="8"/>
       <c r="D76" s="2"/>
@@ -4318,7 +4386,7 @@
       <c r="I76" s="8"/>
       <c r="J76" s="2"/>
     </row>
-    <row r="77" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:10">
       <c r="A77" s="2"/>
       <c r="B77" s="8"/>
       <c r="D77" s="2"/>
@@ -4326,7 +4394,7 @@
       <c r="I77" s="8"/>
       <c r="J77" s="2"/>
     </row>
-    <row r="78" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:10">
       <c r="A78" s="2"/>
       <c r="B78" s="8"/>
       <c r="D78" s="2"/>
@@ -4334,7 +4402,7 @@
       <c r="I78" s="8"/>
       <c r="J78" s="2"/>
     </row>
-    <row r="79" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:10">
       <c r="A79" s="2"/>
       <c r="B79" s="8"/>
       <c r="D79" s="2"/>
@@ -4342,7 +4410,7 @@
       <c r="I79" s="8"/>
       <c r="J79" s="2"/>
     </row>
-    <row r="80" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:10">
       <c r="A80" s="2"/>
       <c r="B80" s="8"/>
       <c r="D80" s="2"/>
@@ -4350,7 +4418,7 @@
       <c r="I80" s="8"/>
       <c r="J80" s="2"/>
     </row>
-    <row r="81" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:10">
       <c r="A81" s="2"/>
       <c r="B81" s="8"/>
       <c r="D81" s="2"/>
@@ -4358,7 +4426,7 @@
       <c r="I81" s="8"/>
       <c r="J81" s="2"/>
     </row>
-    <row r="82" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:10">
       <c r="A82" s="2"/>
       <c r="B82" s="8"/>
       <c r="D82" s="2"/>
@@ -4366,7 +4434,7 @@
       <c r="I82" s="8"/>
       <c r="J82" s="2"/>
     </row>
-    <row r="83" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:10">
       <c r="A83" s="2"/>
       <c r="B83" s="8"/>
       <c r="D83" s="2"/>
@@ -4374,7 +4442,7 @@
       <c r="I83" s="8"/>
       <c r="J83" s="2"/>
     </row>
-    <row r="84" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:10">
       <c r="A84" s="2"/>
       <c r="B84" s="8"/>
       <c r="D84" s="2"/>
@@ -4382,7 +4450,7 @@
       <c r="I84" s="8"/>
       <c r="J84" s="2"/>
     </row>
-    <row r="85" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:10">
       <c r="A85" s="2"/>
       <c r="B85" s="8"/>
       <c r="D85" s="2"/>
@@ -4390,7 +4458,7 @@
       <c r="I85" s="8"/>
       <c r="J85" s="2"/>
     </row>
-    <row r="86" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:10">
       <c r="A86" s="2"/>
       <c r="B86" s="8"/>
       <c r="D86" s="2"/>
@@ -4398,7 +4466,7 @@
       <c r="I86" s="8"/>
       <c r="J86" s="2"/>
     </row>
-    <row r="87" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:10">
       <c r="A87" s="2"/>
       <c r="B87" s="8"/>
       <c r="D87" s="2"/>
@@ -4406,7 +4474,7 @@
       <c r="I87" s="8"/>
       <c r="J87" s="2"/>
     </row>
-    <row r="88" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:10">
       <c r="A88" s="2"/>
       <c r="B88" s="8"/>
       <c r="D88" s="2"/>
@@ -4414,7 +4482,7 @@
       <c r="I88" s="8"/>
       <c r="J88" s="2"/>
     </row>
-    <row r="89" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:10">
       <c r="A89" s="2"/>
       <c r="B89" s="8"/>
       <c r="D89" s="2"/>
@@ -4422,7 +4490,7 @@
       <c r="I89" s="8"/>
       <c r="J89" s="2"/>
     </row>
-    <row r="90" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:10">
       <c r="A90" s="2"/>
       <c r="B90" s="8"/>
       <c r="D90" s="2"/>
@@ -4430,7 +4498,7 @@
       <c r="I90" s="8"/>
       <c r="J90" s="2"/>
     </row>
-    <row r="91" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:10">
       <c r="A91" s="2"/>
       <c r="B91" s="8"/>
       <c r="D91" s="2"/>
@@ -4438,7 +4506,7 @@
       <c r="I91" s="8"/>
       <c r="J91" s="2"/>
     </row>
-    <row r="92" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:10">
       <c r="A92" s="2"/>
       <c r="B92" s="8"/>
       <c r="D92" s="2"/>
@@ -4446,7 +4514,7 @@
       <c r="I92" s="8"/>
       <c r="J92" s="2"/>
     </row>
-    <row r="93" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:10">
       <c r="A93" s="2"/>
       <c r="B93" s="8"/>
       <c r="D93" s="2"/>
@@ -4454,7 +4522,7 @@
       <c r="I93" s="8"/>
       <c r="J93" s="2"/>
     </row>
-    <row r="94" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:10">
       <c r="A94" s="2"/>
       <c r="B94" s="8"/>
       <c r="D94" s="2"/>
@@ -4462,7 +4530,7 @@
       <c r="I94" s="8"/>
       <c r="J94" s="2"/>
     </row>
-    <row r="95" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:10">
       <c r="A95" s="2"/>
       <c r="B95" s="8"/>
       <c r="D95" s="2"/>
@@ -4470,7 +4538,7 @@
       <c r="I95" s="8"/>
       <c r="J95" s="2"/>
     </row>
-    <row r="96" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:10">
       <c r="A96" s="2"/>
       <c r="B96" s="8"/>
       <c r="D96" s="2"/>
@@ -4478,7 +4546,7 @@
       <c r="I96" s="8"/>
       <c r="J96" s="2"/>
     </row>
-    <row r="97" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:10">
       <c r="A97" s="2"/>
       <c r="B97" s="8"/>
       <c r="D97" s="2"/>
@@ -4486,7 +4554,7 @@
       <c r="I97" s="8"/>
       <c r="J97" s="2"/>
     </row>
-    <row r="98" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:10">
       <c r="A98" s="2"/>
       <c r="B98" s="8"/>
       <c r="D98" s="2"/>
@@ -4494,7 +4562,7 @@
       <c r="I98" s="8"/>
       <c r="J98" s="2"/>
     </row>
-    <row r="99" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:10">
       <c r="A99" s="2"/>
       <c r="B99" s="8"/>
       <c r="D99" s="2"/>
@@ -4502,7 +4570,7 @@
       <c r="I99" s="8"/>
       <c r="J99" s="2"/>
     </row>
-    <row r="100" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:10">
       <c r="A100" s="2"/>
       <c r="B100" s="8"/>
       <c r="D100" s="2"/>

</xml_diff>

<commit_message>
Updated my part of the PR&IR.xlsx file
</commit_message>
<xml_diff>
--- a/PR&IR.xlsx
+++ b/PR&IR.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SHIVYA KUMAR\Desktop\new415\CS415_A3\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\yashp\Documents\CS415\CS415_A3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{01652070-29DC-4F77-A0F0-F5C7EB06AF3A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{12BDB62A-F46C-4707-A947-1DB9D8B92BFE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{BFA1E21A-08FA-4F02-8C25-33C81C8EE970}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="2" xr2:uid="{BFA1E21A-08FA-4F02-8C25-33C81C8EE970}"/>
   </bookViews>
   <sheets>
     <sheet name="Avichal" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="36">
   <si>
     <t>Date</t>
   </si>
@@ -149,6 +149,18 @@
   <si>
     <t>I added my routes in the same file run_main_app.py</t>
   </si>
+  <si>
+    <t>YPP</t>
+  </si>
+  <si>
+    <t>Converted all assigned dart-flutter files to html/css/js files respectively.</t>
+  </si>
+  <si>
+    <t>Fix my route error and make my local host runnable.</t>
+  </si>
+  <si>
+    <t>N/A</t>
+  </si>
 </sst>
 </file>
 
@@ -158,7 +170,7 @@
     <numFmt numFmtId="164" formatCode="h"/>
     <numFmt numFmtId="165" formatCode="d/mm/yyyy;@"/>
   </numFmts>
-  <fonts count="3">
+  <fonts count="4">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -178,16 +190,29 @@
       <name val="Arial Unicode MS"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFCAEDFB"/>
+        <bgColor rgb="FFCAEDFB"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -195,11 +220,26 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF61CBF3"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF61CBF3"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF61CBF3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF61CBF3"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -219,6 +259,11 @@
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="14" fontId="3" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="3" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="10" fontId="3" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="3" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -276,7 +321,7 @@
       <numFmt numFmtId="30" formatCode="@"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="166" formatCode="m/d/yyyy"/>
+      <numFmt numFmtId="19" formatCode="m/d/yyyy"/>
     </dxf>
     <dxf>
       <font>
@@ -312,7 +357,7 @@
       <numFmt numFmtId="30" formatCode="@"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="166" formatCode="m/d/yyyy"/>
+      <numFmt numFmtId="19" formatCode="m/d/yyyy"/>
     </dxf>
     <dxf>
       <font>
@@ -384,7 +429,7 @@
       <numFmt numFmtId="30" formatCode="@"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="166" formatCode="m/d/yyyy"/>
+      <numFmt numFmtId="19" formatCode="m/d/yyyy"/>
     </dxf>
     <dxf>
       <font>
@@ -903,26 +948,26 @@
       <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8"/>
+  <sheetFormatPr defaultRowHeight="14"/>
   <cols>
-    <col min="1" max="1" width="10.3984375" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.59765625" style="2" customWidth="1"/>
+    <col min="1" max="1" width="10.4140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.58203125" style="2" customWidth="1"/>
     <col min="3" max="3" width="58" customWidth="1"/>
-    <col min="5" max="5" width="13.09765625" style="3" customWidth="1"/>
-    <col min="6" max="6" width="20.8984375" style="4" customWidth="1"/>
-    <col min="7" max="7" width="34.8984375" style="2" customWidth="1"/>
-    <col min="8" max="8" width="43.3984375" style="2" customWidth="1"/>
-    <col min="11" max="11" width="9.09765625" customWidth="1"/>
-    <col min="12" max="12" width="13.296875" customWidth="1"/>
-    <col min="13" max="13" width="11.3984375" customWidth="1"/>
-    <col min="14" max="14" width="17.3984375" customWidth="1"/>
-    <col min="16" max="16" width="9.09765625" customWidth="1"/>
-    <col min="18" max="18" width="16.59765625" customWidth="1"/>
-    <col min="19" max="19" width="14.69921875" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="16.8984375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.08203125" style="3" customWidth="1"/>
+    <col min="6" max="6" width="20.9140625" style="4" customWidth="1"/>
+    <col min="7" max="7" width="34.9140625" style="2" customWidth="1"/>
+    <col min="8" max="8" width="43.4140625" style="2" customWidth="1"/>
+    <col min="11" max="11" width="9.08203125" customWidth="1"/>
+    <col min="12" max="12" width="13.33203125" customWidth="1"/>
+    <col min="13" max="13" width="11.4140625" customWidth="1"/>
+    <col min="14" max="14" width="17.4140625" customWidth="1"/>
+    <col min="16" max="16" width="9.08203125" customWidth="1"/>
+    <col min="18" max="18" width="16.58203125" customWidth="1"/>
+    <col min="19" max="19" width="14.6640625" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="16.9140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="15.75">
+    <row r="1" spans="1:8" ht="15.5">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
@@ -948,7 +993,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="15.75">
+    <row r="2" spans="1:8">
       <c r="A2" s="1">
         <v>45786</v>
       </c>
@@ -974,7 +1019,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="3" spans="1:8" ht="120">
+    <row r="3" spans="1:8" ht="112">
       <c r="A3" s="1">
         <v>45787</v>
       </c>
@@ -997,49 +1042,49 @@
         <v>23</v>
       </c>
     </row>
-    <row r="4" spans="1:8" ht="15">
+    <row r="4" spans="1:8">
       <c r="F4" s="11"/>
     </row>
-    <row r="5" spans="1:8" ht="15">
+    <row r="5" spans="1:8">
       <c r="F5" s="11"/>
     </row>
-    <row r="6" spans="1:8" ht="15">
+    <row r="6" spans="1:8">
       <c r="F6" s="11"/>
     </row>
-    <row r="7" spans="1:8" ht="15">
+    <row r="7" spans="1:8">
       <c r="F7" s="11"/>
     </row>
-    <row r="8" spans="1:8" ht="15">
+    <row r="8" spans="1:8">
       <c r="F8" s="11"/>
     </row>
-    <row r="9" spans="1:8" ht="15">
+    <row r="9" spans="1:8">
       <c r="F9" s="11"/>
     </row>
-    <row r="10" spans="1:8" ht="15">
+    <row r="10" spans="1:8">
       <c r="F10" s="11"/>
     </row>
-    <row r="11" spans="1:8" ht="15">
+    <row r="11" spans="1:8">
       <c r="F11" s="11"/>
     </row>
-    <row r="12" spans="1:8" ht="15">
+    <row r="12" spans="1:8">
       <c r="F12" s="11"/>
     </row>
-    <row r="13" spans="1:8" ht="15">
+    <row r="13" spans="1:8">
       <c r="F13" s="11"/>
     </row>
-    <row r="14" spans="1:8" ht="15">
+    <row r="14" spans="1:8">
       <c r="F14" s="11"/>
     </row>
-    <row r="15" spans="1:8" ht="15">
+    <row r="15" spans="1:8">
       <c r="F15" s="11"/>
     </row>
-    <row r="16" spans="1:8" ht="15">
+    <row r="16" spans="1:8">
       <c r="F16" s="11"/>
     </row>
-    <row r="17" spans="6:6" ht="15">
+    <row r="17" spans="6:6">
       <c r="F17" s="11"/>
     </row>
-    <row r="18" spans="6:6" ht="15">
+    <row r="18" spans="6:6">
       <c r="F18" s="11"/>
     </row>
     <row r="19" spans="6:6">
@@ -1104,23 +1149,23 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3BDA6702-5DDF-42FB-988E-13FBEB26F5C9}">
   <dimension ref="A1:I100"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="H3" sqref="H3"/>
+    <sheetView topLeftCell="G1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:H3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8"/>
+  <sheetFormatPr defaultRowHeight="14"/>
   <cols>
-    <col min="1" max="1" width="9.8984375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="17.296875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.9140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.33203125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="63" customWidth="1"/>
     <col min="4" max="4" width="9" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.8984375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="23.59765625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="21.796875" customWidth="1"/>
-    <col min="8" max="8" width="116.3984375" customWidth="1"/>
+    <col min="5" max="5" width="14.9140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="23.58203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="21.83203125" customWidth="1"/>
+    <col min="8" max="8" width="116.4140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="15.6">
+    <row r="1" spans="1:9" ht="15.5">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
@@ -1207,7 +1252,7 @@
       <c r="G4" s="2"/>
       <c r="H4" s="2"/>
     </row>
-    <row r="5" spans="1:9" ht="15">
+    <row r="5" spans="1:9">
       <c r="A5" s="8"/>
       <c r="B5" s="2"/>
       <c r="E5" s="3"/>
@@ -1215,7 +1260,7 @@
       <c r="G5" s="2"/>
       <c r="H5" s="2"/>
     </row>
-    <row r="6" spans="1:9" ht="15">
+    <row r="6" spans="1:9">
       <c r="A6" s="8"/>
       <c r="B6" s="2"/>
       <c r="E6" s="3"/>
@@ -1223,7 +1268,7 @@
       <c r="G6" s="2"/>
       <c r="H6" s="2"/>
     </row>
-    <row r="7" spans="1:9" ht="15">
+    <row r="7" spans="1:9">
       <c r="A7" s="8"/>
       <c r="B7" s="2"/>
       <c r="E7" s="3"/>
@@ -1231,7 +1276,7 @@
       <c r="G7" s="2"/>
       <c r="H7" s="2"/>
     </row>
-    <row r="8" spans="1:9" ht="15">
+    <row r="8" spans="1:9">
       <c r="A8" s="8"/>
       <c r="B8" s="2"/>
       <c r="E8" s="3"/>
@@ -1239,7 +1284,7 @@
       <c r="G8" s="2"/>
       <c r="H8" s="2"/>
     </row>
-    <row r="9" spans="1:9" ht="15">
+    <row r="9" spans="1:9">
       <c r="A9" s="8"/>
       <c r="B9" s="2"/>
       <c r="E9" s="3"/>
@@ -1247,7 +1292,7 @@
       <c r="G9" s="2"/>
       <c r="H9" s="2"/>
     </row>
-    <row r="10" spans="1:9" ht="15">
+    <row r="10" spans="1:9">
       <c r="A10" s="8"/>
       <c r="B10" s="2"/>
       <c r="E10" s="3"/>
@@ -1255,7 +1300,7 @@
       <c r="G10" s="2"/>
       <c r="H10" s="2"/>
     </row>
-    <row r="11" spans="1:9" ht="15">
+    <row r="11" spans="1:9">
       <c r="A11" s="8"/>
       <c r="B11" s="2"/>
       <c r="E11" s="3"/>
@@ -1263,7 +1308,7 @@
       <c r="G11" s="2"/>
       <c r="H11" s="2"/>
     </row>
-    <row r="12" spans="1:9" ht="15">
+    <row r="12" spans="1:9">
       <c r="A12" s="8"/>
       <c r="B12" s="2"/>
       <c r="E12" s="3"/>
@@ -1271,7 +1316,7 @@
       <c r="G12" s="2"/>
       <c r="H12" s="2"/>
     </row>
-    <row r="13" spans="1:9" ht="15">
+    <row r="13" spans="1:9">
       <c r="A13" s="8"/>
       <c r="B13" s="2"/>
       <c r="E13" s="3"/>
@@ -1279,7 +1324,7 @@
       <c r="G13" s="2"/>
       <c r="H13" s="2"/>
     </row>
-    <row r="14" spans="1:9" ht="15">
+    <row r="14" spans="1:9">
       <c r="A14" s="8"/>
       <c r="B14" s="2"/>
       <c r="E14" s="3"/>
@@ -1287,7 +1332,7 @@
       <c r="G14" s="2"/>
       <c r="H14" s="2"/>
     </row>
-    <row r="15" spans="1:9" ht="15">
+    <row r="15" spans="1:9">
       <c r="A15" s="8"/>
       <c r="B15" s="2"/>
       <c r="E15" s="3"/>
@@ -1295,7 +1340,7 @@
       <c r="G15" s="2"/>
       <c r="H15" s="2"/>
     </row>
-    <row r="16" spans="1:9" ht="15">
+    <row r="16" spans="1:9">
       <c r="A16" s="8"/>
       <c r="B16" s="2"/>
       <c r="E16" s="3"/>
@@ -1303,7 +1348,7 @@
       <c r="G16" s="2"/>
       <c r="H16" s="2"/>
     </row>
-    <row r="17" spans="1:8" ht="15">
+    <row r="17" spans="1:8">
       <c r="A17" s="8"/>
       <c r="B17" s="2"/>
       <c r="E17" s="3"/>
@@ -1311,7 +1356,7 @@
       <c r="G17" s="2"/>
       <c r="H17" s="2"/>
     </row>
-    <row r="18" spans="1:8" ht="15">
+    <row r="18" spans="1:8">
       <c r="A18" s="8"/>
       <c r="B18" s="2"/>
       <c r="E18" s="3"/>
@@ -1319,7 +1364,7 @@
       <c r="G18" s="2"/>
       <c r="H18" s="2"/>
     </row>
-    <row r="19" spans="1:8" ht="15">
+    <row r="19" spans="1:8">
       <c r="A19" s="8"/>
       <c r="B19" s="2"/>
       <c r="E19" s="3"/>
@@ -1327,7 +1372,7 @@
       <c r="G19" s="2"/>
       <c r="H19" s="2"/>
     </row>
-    <row r="20" spans="1:8" ht="15">
+    <row r="20" spans="1:8">
       <c r="A20" s="8"/>
       <c r="B20" s="2"/>
       <c r="E20" s="3"/>
@@ -1335,7 +1380,7 @@
       <c r="G20" s="2"/>
       <c r="H20" s="2"/>
     </row>
-    <row r="21" spans="1:8" ht="15">
+    <row r="21" spans="1:8">
       <c r="A21" s="8"/>
       <c r="B21" s="2"/>
       <c r="E21" s="3"/>
@@ -1343,7 +1388,7 @@
       <c r="G21" s="2"/>
       <c r="H21" s="2"/>
     </row>
-    <row r="22" spans="1:8" ht="15">
+    <row r="22" spans="1:8">
       <c r="A22" s="8"/>
       <c r="B22" s="2"/>
       <c r="E22" s="3"/>
@@ -1351,7 +1396,7 @@
       <c r="G22" s="2"/>
       <c r="H22" s="2"/>
     </row>
-    <row r="23" spans="1:8" ht="15">
+    <row r="23" spans="1:8">
       <c r="A23" s="8"/>
       <c r="B23" s="2"/>
       <c r="E23" s="3"/>
@@ -1359,7 +1404,7 @@
       <c r="G23" s="2"/>
       <c r="H23" s="2"/>
     </row>
-    <row r="24" spans="1:8" ht="15">
+    <row r="24" spans="1:8">
       <c r="A24" s="8"/>
       <c r="B24" s="2"/>
       <c r="E24" s="3"/>
@@ -1367,7 +1412,7 @@
       <c r="G24" s="2"/>
       <c r="H24" s="2"/>
     </row>
-    <row r="25" spans="1:8" ht="15">
+    <row r="25" spans="1:8">
       <c r="A25" s="8"/>
       <c r="B25" s="2"/>
       <c r="E25" s="3"/>
@@ -2006,23 +2051,23 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9FD6A201-8E63-4A9E-A683-19506CB489E3}">
   <dimension ref="A1:H100"/>
   <sheetViews>
-    <sheetView topLeftCell="A63" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2:D100"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8"/>
+  <sheetFormatPr defaultRowHeight="14"/>
   <cols>
-    <col min="1" max="1" width="7.69921875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="17.296875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.59765625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="8.75" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.58203125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="9" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.8984375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="23.59765625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="13.3984375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="19.09765625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.9140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="23.58203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.4140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="19.08203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="15.75">
+    <row r="1" spans="1:8" ht="15.5">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
@@ -2048,15 +2093,33 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="15">
-      <c r="A2" s="1"/>
-      <c r="B2" s="2"/>
-      <c r="E2" s="3"/>
-      <c r="F2" s="4"/>
-      <c r="G2" s="2"/>
-      <c r="H2" s="2"/>
-    </row>
-    <row r="3" spans="1:8" ht="15">
+    <row r="2" spans="1:8">
+      <c r="A2" s="17">
+        <v>45939</v>
+      </c>
+      <c r="B2" s="18" t="s">
+        <v>32</v>
+      </c>
+      <c r="C2" s="19" t="s">
+        <v>33</v>
+      </c>
+      <c r="D2" s="19" t="s">
+        <v>17</v>
+      </c>
+      <c r="E2" s="20">
+        <v>1</v>
+      </c>
+      <c r="F2" s="21">
+        <v>3</v>
+      </c>
+      <c r="G2" s="18" t="s">
+        <v>34</v>
+      </c>
+      <c r="H2" s="18" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8">
       <c r="A3" s="1"/>
       <c r="B3" s="2"/>
       <c r="E3" s="3"/>
@@ -2064,7 +2127,7 @@
       <c r="G3" s="2"/>
       <c r="H3" s="2"/>
     </row>
-    <row r="4" spans="1:8" ht="15">
+    <row r="4" spans="1:8">
       <c r="A4" s="1"/>
       <c r="B4" s="2"/>
       <c r="E4" s="3"/>
@@ -2072,7 +2135,7 @@
       <c r="G4" s="2"/>
       <c r="H4" s="2"/>
     </row>
-    <row r="5" spans="1:8" ht="15">
+    <row r="5" spans="1:8">
       <c r="A5" s="1"/>
       <c r="B5" s="2"/>
       <c r="E5" s="3"/>
@@ -2080,7 +2143,7 @@
       <c r="G5" s="2"/>
       <c r="H5" s="2"/>
     </row>
-    <row r="6" spans="1:8" ht="15">
+    <row r="6" spans="1:8">
       <c r="A6" s="1"/>
       <c r="B6" s="2"/>
       <c r="E6" s="3"/>
@@ -2088,7 +2151,7 @@
       <c r="G6" s="2"/>
       <c r="H6" s="2"/>
     </row>
-    <row r="7" spans="1:8" ht="15">
+    <row r="7" spans="1:8">
       <c r="A7" s="1"/>
       <c r="B7" s="2"/>
       <c r="E7" s="3"/>
@@ -2096,7 +2159,7 @@
       <c r="G7" s="2"/>
       <c r="H7" s="2"/>
     </row>
-    <row r="8" spans="1:8" ht="15">
+    <row r="8" spans="1:8">
       <c r="A8" s="1"/>
       <c r="B8" s="2"/>
       <c r="E8" s="3"/>
@@ -2104,7 +2167,7 @@
       <c r="G8" s="2"/>
       <c r="H8" s="2"/>
     </row>
-    <row r="9" spans="1:8" ht="15">
+    <row r="9" spans="1:8">
       <c r="A9" s="1"/>
       <c r="B9" s="2"/>
       <c r="E9" s="3"/>
@@ -2112,7 +2175,7 @@
       <c r="G9" s="2"/>
       <c r="H9" s="2"/>
     </row>
-    <row r="10" spans="1:8" ht="15">
+    <row r="10" spans="1:8">
       <c r="A10" s="1"/>
       <c r="B10" s="2"/>
       <c r="E10" s="3"/>
@@ -2120,7 +2183,7 @@
       <c r="G10" s="2"/>
       <c r="H10" s="2"/>
     </row>
-    <row r="11" spans="1:8" ht="15">
+    <row r="11" spans="1:8">
       <c r="A11" s="1"/>
       <c r="B11" s="2"/>
       <c r="E11" s="3"/>
@@ -2128,7 +2191,7 @@
       <c r="G11" s="2"/>
       <c r="H11" s="2"/>
     </row>
-    <row r="12" spans="1:8" ht="15">
+    <row r="12" spans="1:8">
       <c r="A12" s="1"/>
       <c r="B12" s="2"/>
       <c r="E12" s="3"/>
@@ -2136,7 +2199,7 @@
       <c r="G12" s="2"/>
       <c r="H12" s="2"/>
     </row>
-    <row r="13" spans="1:8" ht="15">
+    <row r="13" spans="1:8">
       <c r="A13" s="1"/>
       <c r="B13" s="2"/>
       <c r="E13" s="3"/>
@@ -2144,7 +2207,7 @@
       <c r="G13" s="2"/>
       <c r="H13" s="2"/>
     </row>
-    <row r="14" spans="1:8" ht="15">
+    <row r="14" spans="1:8">
       <c r="A14" s="1"/>
       <c r="B14" s="2"/>
       <c r="E14" s="3"/>
@@ -2152,7 +2215,7 @@
       <c r="G14" s="2"/>
       <c r="H14" s="2"/>
     </row>
-    <row r="15" spans="1:8" ht="15">
+    <row r="15" spans="1:8">
       <c r="A15" s="1"/>
       <c r="B15" s="2"/>
       <c r="E15" s="3"/>
@@ -2160,7 +2223,7 @@
       <c r="G15" s="2"/>
       <c r="H15" s="2"/>
     </row>
-    <row r="16" spans="1:8" ht="15">
+    <row r="16" spans="1:8">
       <c r="A16" s="1"/>
       <c r="B16" s="2"/>
       <c r="E16" s="3"/>
@@ -2168,7 +2231,7 @@
       <c r="G16" s="2"/>
       <c r="H16" s="2"/>
     </row>
-    <row r="17" spans="1:8" ht="15">
+    <row r="17" spans="1:8">
       <c r="A17" s="1"/>
       <c r="B17" s="2"/>
       <c r="E17" s="3"/>
@@ -2176,7 +2239,7 @@
       <c r="G17" s="2"/>
       <c r="H17" s="2"/>
     </row>
-    <row r="18" spans="1:8" ht="15">
+    <row r="18" spans="1:8">
       <c r="A18" s="1"/>
       <c r="B18" s="2"/>
       <c r="E18" s="3"/>
@@ -2184,7 +2247,7 @@
       <c r="G18" s="2"/>
       <c r="H18" s="2"/>
     </row>
-    <row r="19" spans="1:8" ht="15">
+    <row r="19" spans="1:8">
       <c r="A19" s="1"/>
       <c r="B19" s="2"/>
       <c r="E19" s="3"/>
@@ -2192,7 +2255,7 @@
       <c r="G19" s="2"/>
       <c r="H19" s="2"/>
     </row>
-    <row r="20" spans="1:8" ht="15">
+    <row r="20" spans="1:8">
       <c r="A20" s="1"/>
       <c r="B20" s="2"/>
       <c r="E20" s="3"/>
@@ -2200,7 +2263,7 @@
       <c r="G20" s="2"/>
       <c r="H20" s="2"/>
     </row>
-    <row r="21" spans="1:8" ht="15">
+    <row r="21" spans="1:8">
       <c r="A21" s="1"/>
       <c r="B21" s="2"/>
       <c r="E21" s="3"/>
@@ -2208,7 +2271,7 @@
       <c r="G21" s="2"/>
       <c r="H21" s="2"/>
     </row>
-    <row r="22" spans="1:8" ht="15">
+    <row r="22" spans="1:8">
       <c r="A22" s="1"/>
       <c r="B22" s="2"/>
       <c r="E22" s="3"/>
@@ -2216,7 +2279,7 @@
       <c r="G22" s="2"/>
       <c r="H22" s="2"/>
     </row>
-    <row r="23" spans="1:8" ht="15">
+    <row r="23" spans="1:8">
       <c r="A23" s="1"/>
       <c r="B23" s="2"/>
       <c r="E23" s="3"/>
@@ -2224,7 +2287,7 @@
       <c r="G23" s="2"/>
       <c r="H23" s="2"/>
     </row>
-    <row r="24" spans="1:8" ht="15">
+    <row r="24" spans="1:8">
       <c r="A24" s="1"/>
       <c r="B24" s="2"/>
       <c r="E24" s="3"/>
@@ -2232,7 +2295,7 @@
       <c r="G24" s="2"/>
       <c r="H24" s="2"/>
     </row>
-    <row r="25" spans="1:8" ht="15">
+    <row r="25" spans="1:8">
       <c r="A25" s="1"/>
       <c r="B25" s="2"/>
       <c r="E25" s="3"/>
@@ -2240,7 +2303,7 @@
       <c r="G25" s="2"/>
       <c r="H25" s="2"/>
     </row>
-    <row r="26" spans="1:8" ht="15">
+    <row r="26" spans="1:8">
       <c r="A26" s="1"/>
       <c r="B26" s="2"/>
       <c r="E26" s="3"/>
@@ -2248,7 +2311,7 @@
       <c r="G26" s="2"/>
       <c r="H26" s="2"/>
     </row>
-    <row r="27" spans="1:8" ht="15">
+    <row r="27" spans="1:8">
       <c r="A27" s="1"/>
       <c r="B27" s="2"/>
       <c r="E27" s="3"/>
@@ -2256,7 +2319,7 @@
       <c r="G27" s="2"/>
       <c r="H27" s="2"/>
     </row>
-    <row r="28" spans="1:8" ht="15">
+    <row r="28" spans="1:8">
       <c r="A28" s="1"/>
       <c r="B28" s="2"/>
       <c r="E28" s="3"/>
@@ -2264,7 +2327,7 @@
       <c r="G28" s="2"/>
       <c r="H28" s="2"/>
     </row>
-    <row r="29" spans="1:8" ht="15">
+    <row r="29" spans="1:8">
       <c r="A29" s="1"/>
       <c r="B29" s="2"/>
       <c r="E29" s="3"/>
@@ -2272,7 +2335,7 @@
       <c r="G29" s="2"/>
       <c r="H29" s="2"/>
     </row>
-    <row r="30" spans="1:8" ht="15">
+    <row r="30" spans="1:8">
       <c r="A30" s="1"/>
       <c r="B30" s="2"/>
       <c r="E30" s="3"/>
@@ -2280,7 +2343,7 @@
       <c r="G30" s="2"/>
       <c r="H30" s="2"/>
     </row>
-    <row r="31" spans="1:8" ht="15">
+    <row r="31" spans="1:8">
       <c r="A31" s="1"/>
       <c r="B31" s="2"/>
       <c r="E31" s="3"/>
@@ -2288,7 +2351,7 @@
       <c r="G31" s="2"/>
       <c r="H31" s="2"/>
     </row>
-    <row r="32" spans="1:8" ht="15">
+    <row r="32" spans="1:8">
       <c r="A32" s="1"/>
       <c r="B32" s="2"/>
       <c r="E32" s="3"/>
@@ -2296,7 +2359,7 @@
       <c r="G32" s="2"/>
       <c r="H32" s="2"/>
     </row>
-    <row r="33" spans="1:8" ht="15">
+    <row r="33" spans="1:8">
       <c r="A33" s="1"/>
       <c r="B33" s="2"/>
       <c r="E33" s="3"/>
@@ -2304,7 +2367,7 @@
       <c r="G33" s="2"/>
       <c r="H33" s="2"/>
     </row>
-    <row r="34" spans="1:8" ht="15">
+    <row r="34" spans="1:8">
       <c r="A34" s="1"/>
       <c r="B34" s="2"/>
       <c r="E34" s="3"/>
@@ -2312,7 +2375,7 @@
       <c r="G34" s="2"/>
       <c r="H34" s="2"/>
     </row>
-    <row r="35" spans="1:8" ht="15">
+    <row r="35" spans="1:8">
       <c r="A35" s="1"/>
       <c r="B35" s="2"/>
       <c r="E35" s="3"/>
@@ -2320,7 +2383,7 @@
       <c r="G35" s="2"/>
       <c r="H35" s="2"/>
     </row>
-    <row r="36" spans="1:8" ht="15">
+    <row r="36" spans="1:8">
       <c r="A36" s="1"/>
       <c r="B36" s="2"/>
       <c r="E36" s="3"/>
@@ -2328,7 +2391,7 @@
       <c r="G36" s="2"/>
       <c r="H36" s="2"/>
     </row>
-    <row r="37" spans="1:8" ht="15">
+    <row r="37" spans="1:8">
       <c r="A37" s="1"/>
       <c r="B37" s="2"/>
       <c r="E37" s="3"/>
@@ -2336,7 +2399,7 @@
       <c r="G37" s="2"/>
       <c r="H37" s="2"/>
     </row>
-    <row r="38" spans="1:8" ht="15">
+    <row r="38" spans="1:8">
       <c r="A38" s="1"/>
       <c r="B38" s="2"/>
       <c r="E38" s="3"/>
@@ -2344,7 +2407,7 @@
       <c r="G38" s="2"/>
       <c r="H38" s="2"/>
     </row>
-    <row r="39" spans="1:8" ht="15">
+    <row r="39" spans="1:8">
       <c r="A39" s="1"/>
       <c r="B39" s="2"/>
       <c r="E39" s="3"/>
@@ -2352,7 +2415,7 @@
       <c r="G39" s="2"/>
       <c r="H39" s="2"/>
     </row>
-    <row r="40" spans="1:8" ht="15">
+    <row r="40" spans="1:8">
       <c r="A40" s="1"/>
       <c r="B40" s="2"/>
       <c r="E40" s="3"/>
@@ -2360,7 +2423,7 @@
       <c r="G40" s="2"/>
       <c r="H40" s="2"/>
     </row>
-    <row r="41" spans="1:8" ht="15">
+    <row r="41" spans="1:8">
       <c r="A41" s="1"/>
       <c r="B41" s="2"/>
       <c r="E41" s="3"/>
@@ -2368,7 +2431,7 @@
       <c r="G41" s="2"/>
       <c r="H41" s="2"/>
     </row>
-    <row r="42" spans="1:8" ht="15">
+    <row r="42" spans="1:8">
       <c r="A42" s="1"/>
       <c r="B42" s="2"/>
       <c r="E42" s="3"/>
@@ -2376,7 +2439,7 @@
       <c r="G42" s="2"/>
       <c r="H42" s="2"/>
     </row>
-    <row r="43" spans="1:8" ht="15">
+    <row r="43" spans="1:8">
       <c r="A43" s="1"/>
       <c r="B43" s="2"/>
       <c r="E43" s="3"/>
@@ -2384,7 +2447,7 @@
       <c r="G43" s="2"/>
       <c r="H43" s="2"/>
     </row>
-    <row r="44" spans="1:8" ht="15">
+    <row r="44" spans="1:8">
       <c r="A44" s="1"/>
       <c r="B44" s="2"/>
       <c r="E44" s="3"/>
@@ -2392,7 +2455,7 @@
       <c r="G44" s="2"/>
       <c r="H44" s="2"/>
     </row>
-    <row r="45" spans="1:8" ht="15">
+    <row r="45" spans="1:8">
       <c r="A45" s="1"/>
       <c r="B45" s="2"/>
       <c r="E45" s="3"/>
@@ -2400,7 +2463,7 @@
       <c r="G45" s="2"/>
       <c r="H45" s="2"/>
     </row>
-    <row r="46" spans="1:8" ht="15">
+    <row r="46" spans="1:8">
       <c r="A46" s="1"/>
       <c r="B46" s="2"/>
       <c r="E46" s="3"/>
@@ -2408,7 +2471,7 @@
       <c r="G46" s="2"/>
       <c r="H46" s="2"/>
     </row>
-    <row r="47" spans="1:8" ht="15">
+    <row r="47" spans="1:8">
       <c r="A47" s="1"/>
       <c r="B47" s="2"/>
       <c r="E47" s="3"/>
@@ -2416,7 +2479,7 @@
       <c r="G47" s="2"/>
       <c r="H47" s="2"/>
     </row>
-    <row r="48" spans="1:8" ht="15">
+    <row r="48" spans="1:8">
       <c r="A48" s="1"/>
       <c r="B48" s="2"/>
       <c r="E48" s="3"/>
@@ -2424,7 +2487,7 @@
       <c r="G48" s="2"/>
       <c r="H48" s="2"/>
     </row>
-    <row r="49" spans="1:8" ht="15">
+    <row r="49" spans="1:8">
       <c r="A49" s="1"/>
       <c r="B49" s="2"/>
       <c r="E49" s="3"/>
@@ -2432,7 +2495,7 @@
       <c r="G49" s="2"/>
       <c r="H49" s="2"/>
     </row>
-    <row r="50" spans="1:8" ht="15">
+    <row r="50" spans="1:8">
       <c r="A50" s="1"/>
       <c r="B50" s="2"/>
       <c r="E50" s="3"/>
@@ -2440,7 +2503,7 @@
       <c r="G50" s="2"/>
       <c r="H50" s="2"/>
     </row>
-    <row r="51" spans="1:8" ht="15">
+    <row r="51" spans="1:8">
       <c r="A51" s="1"/>
       <c r="B51" s="2"/>
       <c r="E51" s="3"/>
@@ -2448,7 +2511,7 @@
       <c r="G51" s="2"/>
       <c r="H51" s="2"/>
     </row>
-    <row r="52" spans="1:8" ht="15">
+    <row r="52" spans="1:8">
       <c r="A52" s="1"/>
       <c r="B52" s="2"/>
       <c r="E52" s="3"/>
@@ -2456,7 +2519,7 @@
       <c r="G52" s="2"/>
       <c r="H52" s="2"/>
     </row>
-    <row r="53" spans="1:8" ht="15">
+    <row r="53" spans="1:8">
       <c r="A53" s="1"/>
       <c r="B53" s="2"/>
       <c r="E53" s="3"/>
@@ -2464,7 +2527,7 @@
       <c r="G53" s="2"/>
       <c r="H53" s="2"/>
     </row>
-    <row r="54" spans="1:8" ht="15">
+    <row r="54" spans="1:8">
       <c r="A54" s="1"/>
       <c r="B54" s="2"/>
       <c r="E54" s="3"/>
@@ -2472,7 +2535,7 @@
       <c r="G54" s="2"/>
       <c r="H54" s="2"/>
     </row>
-    <row r="55" spans="1:8" ht="15">
+    <row r="55" spans="1:8">
       <c r="A55" s="1"/>
       <c r="B55" s="2"/>
       <c r="E55" s="3"/>
@@ -2480,7 +2543,7 @@
       <c r="G55" s="2"/>
       <c r="H55" s="2"/>
     </row>
-    <row r="56" spans="1:8" ht="15">
+    <row r="56" spans="1:8">
       <c r="A56" s="1"/>
       <c r="B56" s="2"/>
       <c r="E56" s="3"/>
@@ -2488,7 +2551,7 @@
       <c r="G56" s="2"/>
       <c r="H56" s="2"/>
     </row>
-    <row r="57" spans="1:8" ht="15">
+    <row r="57" spans="1:8">
       <c r="A57" s="1"/>
       <c r="B57" s="2"/>
       <c r="E57" s="3"/>
@@ -2496,7 +2559,7 @@
       <c r="G57" s="2"/>
       <c r="H57" s="2"/>
     </row>
-    <row r="58" spans="1:8" ht="15">
+    <row r="58" spans="1:8">
       <c r="A58" s="1"/>
       <c r="B58" s="2"/>
       <c r="E58" s="3"/>
@@ -2504,7 +2567,7 @@
       <c r="G58" s="2"/>
       <c r="H58" s="2"/>
     </row>
-    <row r="59" spans="1:8" ht="15">
+    <row r="59" spans="1:8">
       <c r="A59" s="1"/>
       <c r="B59" s="2"/>
       <c r="E59" s="3"/>
@@ -2512,7 +2575,7 @@
       <c r="G59" s="2"/>
       <c r="H59" s="2"/>
     </row>
-    <row r="60" spans="1:8" ht="15">
+    <row r="60" spans="1:8">
       <c r="A60" s="1"/>
       <c r="B60" s="2"/>
       <c r="E60" s="3"/>
@@ -2520,7 +2583,7 @@
       <c r="G60" s="2"/>
       <c r="H60" s="2"/>
     </row>
-    <row r="61" spans="1:8" ht="15">
+    <row r="61" spans="1:8">
       <c r="A61" s="1"/>
       <c r="B61" s="2"/>
       <c r="E61" s="3"/>
@@ -2528,7 +2591,7 @@
       <c r="G61" s="2"/>
       <c r="H61" s="2"/>
     </row>
-    <row r="62" spans="1:8" ht="15">
+    <row r="62" spans="1:8">
       <c r="A62" s="1"/>
       <c r="B62" s="2"/>
       <c r="E62" s="3"/>
@@ -2536,7 +2599,7 @@
       <c r="G62" s="2"/>
       <c r="H62" s="2"/>
     </row>
-    <row r="63" spans="1:8" ht="15">
+    <row r="63" spans="1:8">
       <c r="A63" s="1"/>
       <c r="B63" s="2"/>
       <c r="E63" s="3"/>
@@ -2544,7 +2607,7 @@
       <c r="G63" s="2"/>
       <c r="H63" s="2"/>
     </row>
-    <row r="64" spans="1:8" ht="15">
+    <row r="64" spans="1:8">
       <c r="A64" s="1"/>
       <c r="B64" s="2"/>
       <c r="E64" s="3"/>
@@ -2552,7 +2615,7 @@
       <c r="G64" s="2"/>
       <c r="H64" s="2"/>
     </row>
-    <row r="65" spans="1:8" ht="15">
+    <row r="65" spans="1:8">
       <c r="A65" s="1"/>
       <c r="B65" s="2"/>
       <c r="E65" s="3"/>
@@ -2560,7 +2623,7 @@
       <c r="G65" s="2"/>
       <c r="H65" s="2"/>
     </row>
-    <row r="66" spans="1:8" ht="15">
+    <row r="66" spans="1:8">
       <c r="A66" s="1"/>
       <c r="B66" s="2"/>
       <c r="E66" s="3"/>
@@ -2568,7 +2631,7 @@
       <c r="G66" s="2"/>
       <c r="H66" s="2"/>
     </row>
-    <row r="67" spans="1:8" ht="15">
+    <row r="67" spans="1:8">
       <c r="A67" s="1"/>
       <c r="B67" s="2"/>
       <c r="E67" s="3"/>
@@ -2576,7 +2639,7 @@
       <c r="G67" s="2"/>
       <c r="H67" s="2"/>
     </row>
-    <row r="68" spans="1:8" ht="15">
+    <row r="68" spans="1:8">
       <c r="A68" s="1"/>
       <c r="B68" s="2"/>
       <c r="E68" s="3"/>
@@ -2584,7 +2647,7 @@
       <c r="G68" s="2"/>
       <c r="H68" s="2"/>
     </row>
-    <row r="69" spans="1:8" ht="15">
+    <row r="69" spans="1:8">
       <c r="A69" s="1"/>
       <c r="B69" s="2"/>
       <c r="E69" s="3"/>
@@ -2592,7 +2655,7 @@
       <c r="G69" s="2"/>
       <c r="H69" s="2"/>
     </row>
-    <row r="70" spans="1:8" ht="15">
+    <row r="70" spans="1:8">
       <c r="A70" s="1"/>
       <c r="B70" s="2"/>
       <c r="E70" s="3"/>
@@ -2600,7 +2663,7 @@
       <c r="G70" s="2"/>
       <c r="H70" s="2"/>
     </row>
-    <row r="71" spans="1:8" ht="15">
+    <row r="71" spans="1:8">
       <c r="A71" s="1"/>
       <c r="B71" s="2"/>
       <c r="E71" s="3"/>
@@ -2608,7 +2671,7 @@
       <c r="G71" s="2"/>
       <c r="H71" s="2"/>
     </row>
-    <row r="72" spans="1:8" ht="15">
+    <row r="72" spans="1:8">
       <c r="A72" s="1"/>
       <c r="B72" s="2"/>
       <c r="E72" s="3"/>
@@ -2616,7 +2679,7 @@
       <c r="G72" s="2"/>
       <c r="H72" s="2"/>
     </row>
-    <row r="73" spans="1:8" ht="15">
+    <row r="73" spans="1:8">
       <c r="A73" s="1"/>
       <c r="B73" s="2"/>
       <c r="E73" s="3"/>
@@ -2624,7 +2687,7 @@
       <c r="G73" s="2"/>
       <c r="H73" s="2"/>
     </row>
-    <row r="74" spans="1:8" ht="15">
+    <row r="74" spans="1:8">
       <c r="A74" s="1"/>
       <c r="B74" s="2"/>
       <c r="E74" s="3"/>
@@ -2632,7 +2695,7 @@
       <c r="G74" s="2"/>
       <c r="H74" s="2"/>
     </row>
-    <row r="75" spans="1:8" ht="15">
+    <row r="75" spans="1:8">
       <c r="A75" s="1"/>
       <c r="B75" s="2"/>
       <c r="E75" s="3"/>
@@ -2640,7 +2703,7 @@
       <c r="G75" s="2"/>
       <c r="H75" s="2"/>
     </row>
-    <row r="76" spans="1:8" ht="15">
+    <row r="76" spans="1:8">
       <c r="A76" s="1"/>
       <c r="B76" s="2"/>
       <c r="E76" s="3"/>
@@ -2648,7 +2711,7 @@
       <c r="G76" s="2"/>
       <c r="H76" s="2"/>
     </row>
-    <row r="77" spans="1:8" ht="15">
+    <row r="77" spans="1:8">
       <c r="A77" s="1"/>
       <c r="B77" s="2"/>
       <c r="E77" s="3"/>
@@ -2656,7 +2719,7 @@
       <c r="G77" s="2"/>
       <c r="H77" s="2"/>
     </row>
-    <row r="78" spans="1:8" ht="15">
+    <row r="78" spans="1:8">
       <c r="A78" s="1"/>
       <c r="B78" s="2"/>
       <c r="E78" s="3"/>
@@ -2664,7 +2727,7 @@
       <c r="G78" s="2"/>
       <c r="H78" s="2"/>
     </row>
-    <row r="79" spans="1:8" ht="15">
+    <row r="79" spans="1:8">
       <c r="A79" s="1"/>
       <c r="B79" s="2"/>
       <c r="E79" s="3"/>
@@ -2672,7 +2735,7 @@
       <c r="G79" s="2"/>
       <c r="H79" s="2"/>
     </row>
-    <row r="80" spans="1:8" ht="15">
+    <row r="80" spans="1:8">
       <c r="A80" s="1"/>
       <c r="B80" s="2"/>
       <c r="E80" s="3"/>
@@ -2680,7 +2743,7 @@
       <c r="G80" s="2"/>
       <c r="H80" s="2"/>
     </row>
-    <row r="81" spans="1:8" ht="15">
+    <row r="81" spans="1:8">
       <c r="A81" s="1"/>
       <c r="B81" s="2"/>
       <c r="E81" s="3"/>
@@ -2688,7 +2751,7 @@
       <c r="G81" s="2"/>
       <c r="H81" s="2"/>
     </row>
-    <row r="82" spans="1:8" ht="15">
+    <row r="82" spans="1:8">
       <c r="A82" s="1"/>
       <c r="B82" s="2"/>
       <c r="E82" s="3"/>
@@ -2696,7 +2759,7 @@
       <c r="G82" s="2"/>
       <c r="H82" s="2"/>
     </row>
-    <row r="83" spans="1:8" ht="15">
+    <row r="83" spans="1:8">
       <c r="A83" s="1"/>
       <c r="B83" s="2"/>
       <c r="E83" s="3"/>
@@ -2704,7 +2767,7 @@
       <c r="G83" s="2"/>
       <c r="H83" s="2"/>
     </row>
-    <row r="84" spans="1:8" ht="15">
+    <row r="84" spans="1:8">
       <c r="A84" s="1"/>
       <c r="B84" s="2"/>
       <c r="E84" s="3"/>
@@ -2712,7 +2775,7 @@
       <c r="G84" s="2"/>
       <c r="H84" s="2"/>
     </row>
-    <row r="85" spans="1:8" ht="15">
+    <row r="85" spans="1:8">
       <c r="A85" s="1"/>
       <c r="B85" s="2"/>
       <c r="E85" s="3"/>
@@ -2720,7 +2783,7 @@
       <c r="G85" s="2"/>
       <c r="H85" s="2"/>
     </row>
-    <row r="86" spans="1:8" ht="15">
+    <row r="86" spans="1:8">
       <c r="A86" s="1"/>
       <c r="B86" s="2"/>
       <c r="E86" s="3"/>
@@ -2728,7 +2791,7 @@
       <c r="G86" s="2"/>
       <c r="H86" s="2"/>
     </row>
-    <row r="87" spans="1:8" ht="15">
+    <row r="87" spans="1:8">
       <c r="A87" s="1"/>
       <c r="B87" s="2"/>
       <c r="E87" s="3"/>
@@ -2842,14 +2905,14 @@
     </row>
   </sheetData>
   <dataValidations count="4">
-    <dataValidation type="list" errorStyle="warning" showInputMessage="1" showErrorMessage="1" errorTitle="Select Status" error="Fill in Status to proccessd " sqref="D2:D16" xr:uid="{E71B4AA3-209B-477E-A06E-31A006A45CD7}">
+    <dataValidation type="list" errorStyle="warning" showInputMessage="1" showErrorMessage="1" errorTitle="Select Status" error="Fill in Status to proccessd " sqref="D3:D16" xr:uid="{E71B4AA3-209B-477E-A06E-31A006A45CD7}">
       <formula1>"To Do,In Progress,Completed,Blocked"</formula1>
     </dataValidation>
-    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F2:F100" xr:uid="{1CA240CB-8CBA-47E0-8CFF-996BD4AF540F}">
+    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F3:F100" xr:uid="{1CA240CB-8CBA-47E0-8CFF-996BD4AF540F}">
       <formula1>1</formula1>
       <formula2>24</formula2>
     </dataValidation>
-    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2:E100" xr:uid="{2CF02A19-ACD0-4709-8E3E-614FB1991DD8}">
+    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E3:E100" xr:uid="{2CF02A19-ACD0-4709-8E3E-614FB1991DD8}">
       <formula1>0</formula1>
       <formula2>100</formula2>
     </dataValidation>
@@ -2859,7 +2922,7 @@
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <ignoredErrors>
-    <ignoredError sqref="D2:D100" listDataValidation="1"/>
+    <ignoredError sqref="D3:D100" listDataValidation="1"/>
   </ignoredErrors>
   <tableParts count="1">
     <tablePart r:id="rId1"/>
@@ -2875,19 +2938,19 @@
       <selection activeCell="D2" sqref="D2:D100"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8"/>
+  <sheetFormatPr defaultRowHeight="14"/>
   <cols>
-    <col min="1" max="1" width="7.69921875" customWidth="1"/>
-    <col min="2" max="2" width="17.296875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.59765625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="7.6640625" customWidth="1"/>
+    <col min="2" max="2" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.58203125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="9" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.8984375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="23.59765625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="13.3984375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="19.09765625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.9140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="23.58203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.4140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="19.08203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="15.75">
+    <row r="1" spans="1:8" ht="15.5">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
@@ -2913,7 +2976,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="15">
+    <row r="2" spans="1:8">
       <c r="A2" s="1"/>
       <c r="B2" s="2"/>
       <c r="E2" s="3"/>
@@ -2921,7 +2984,7 @@
       <c r="G2" s="2"/>
       <c r="H2" s="2"/>
     </row>
-    <row r="3" spans="1:8" ht="15">
+    <row r="3" spans="1:8">
       <c r="A3" s="1"/>
       <c r="B3" s="2"/>
       <c r="E3" s="3"/>
@@ -2929,7 +2992,7 @@
       <c r="G3" s="2"/>
       <c r="H3" s="2"/>
     </row>
-    <row r="4" spans="1:8" ht="15">
+    <row r="4" spans="1:8">
       <c r="A4" s="1"/>
       <c r="B4" s="2"/>
       <c r="E4" s="3"/>
@@ -2937,7 +3000,7 @@
       <c r="G4" s="2"/>
       <c r="H4" s="2"/>
     </row>
-    <row r="5" spans="1:8" ht="15">
+    <row r="5" spans="1:8">
       <c r="A5" s="1"/>
       <c r="B5" s="2"/>
       <c r="E5" s="3"/>
@@ -2945,7 +3008,7 @@
       <c r="G5" s="2"/>
       <c r="H5" s="2"/>
     </row>
-    <row r="6" spans="1:8" ht="15">
+    <row r="6" spans="1:8">
       <c r="A6" s="1"/>
       <c r="B6" s="2"/>
       <c r="E6" s="3"/>
@@ -2953,7 +3016,7 @@
       <c r="G6" s="2"/>
       <c r="H6" s="2"/>
     </row>
-    <row r="7" spans="1:8" ht="15">
+    <row r="7" spans="1:8">
       <c r="A7" s="1"/>
       <c r="B7" s="2"/>
       <c r="E7" s="3"/>
@@ -2961,7 +3024,7 @@
       <c r="G7" s="2"/>
       <c r="H7" s="2"/>
     </row>
-    <row r="8" spans="1:8" ht="15">
+    <row r="8" spans="1:8">
       <c r="A8" s="1"/>
       <c r="B8" s="2"/>
       <c r="E8" s="3"/>
@@ -2969,7 +3032,7 @@
       <c r="G8" s="2"/>
       <c r="H8" s="2"/>
     </row>
-    <row r="9" spans="1:8" ht="15">
+    <row r="9" spans="1:8">
       <c r="A9" s="1"/>
       <c r="B9" s="2"/>
       <c r="E9" s="3"/>
@@ -2977,7 +3040,7 @@
       <c r="G9" s="2"/>
       <c r="H9" s="2"/>
     </row>
-    <row r="10" spans="1:8" ht="15">
+    <row r="10" spans="1:8">
       <c r="A10" s="1"/>
       <c r="B10" s="2"/>
       <c r="E10" s="3"/>
@@ -2985,7 +3048,7 @@
       <c r="G10" s="2"/>
       <c r="H10" s="2"/>
     </row>
-    <row r="11" spans="1:8" ht="15">
+    <row r="11" spans="1:8">
       <c r="A11" s="1"/>
       <c r="B11" s="2"/>
       <c r="E11" s="3"/>
@@ -2993,7 +3056,7 @@
       <c r="G11" s="2"/>
       <c r="H11" s="2"/>
     </row>
-    <row r="12" spans="1:8" ht="15">
+    <row r="12" spans="1:8">
       <c r="A12" s="1"/>
       <c r="B12" s="2"/>
       <c r="E12" s="3"/>
@@ -3001,7 +3064,7 @@
       <c r="G12" s="2"/>
       <c r="H12" s="2"/>
     </row>
-    <row r="13" spans="1:8" ht="15">
+    <row r="13" spans="1:8">
       <c r="A13" s="1"/>
       <c r="B13" s="2"/>
       <c r="E13" s="3"/>
@@ -3009,7 +3072,7 @@
       <c r="G13" s="2"/>
       <c r="H13" s="2"/>
     </row>
-    <row r="14" spans="1:8" ht="15">
+    <row r="14" spans="1:8">
       <c r="A14" s="1"/>
       <c r="B14" s="2"/>
       <c r="E14" s="3"/>
@@ -3017,7 +3080,7 @@
       <c r="G14" s="2"/>
       <c r="H14" s="2"/>
     </row>
-    <row r="15" spans="1:8" ht="15">
+    <row r="15" spans="1:8">
       <c r="A15" s="1"/>
       <c r="B15" s="2"/>
       <c r="E15" s="3"/>
@@ -3025,7 +3088,7 @@
       <c r="G15" s="2"/>
       <c r="H15" s="2"/>
     </row>
-    <row r="16" spans="1:8" ht="15">
+    <row r="16" spans="1:8">
       <c r="A16" s="1"/>
       <c r="B16" s="2"/>
       <c r="E16" s="3"/>
@@ -3033,7 +3096,7 @@
       <c r="G16" s="2"/>
       <c r="H16" s="2"/>
     </row>
-    <row r="17" spans="1:8" ht="15">
+    <row r="17" spans="1:8">
       <c r="A17" s="1"/>
       <c r="B17" s="2"/>
       <c r="E17" s="3"/>
@@ -3041,7 +3104,7 @@
       <c r="G17" s="2"/>
       <c r="H17" s="2"/>
     </row>
-    <row r="18" spans="1:8" ht="15">
+    <row r="18" spans="1:8">
       <c r="A18" s="1"/>
       <c r="B18" s="2"/>
       <c r="E18" s="3"/>
@@ -3049,7 +3112,7 @@
       <c r="G18" s="2"/>
       <c r="H18" s="2"/>
     </row>
-    <row r="19" spans="1:8" ht="15">
+    <row r="19" spans="1:8">
       <c r="A19" s="1"/>
       <c r="B19" s="2"/>
       <c r="E19" s="3"/>
@@ -3057,7 +3120,7 @@
       <c r="G19" s="2"/>
       <c r="H19" s="2"/>
     </row>
-    <row r="20" spans="1:8" ht="15">
+    <row r="20" spans="1:8">
       <c r="A20" s="1"/>
       <c r="B20" s="2"/>
       <c r="E20" s="3"/>
@@ -3065,7 +3128,7 @@
       <c r="G20" s="2"/>
       <c r="H20" s="2"/>
     </row>
-    <row r="21" spans="1:8" ht="15">
+    <row r="21" spans="1:8">
       <c r="A21" s="1"/>
       <c r="B21" s="2"/>
       <c r="E21" s="3"/>
@@ -3073,7 +3136,7 @@
       <c r="G21" s="2"/>
       <c r="H21" s="2"/>
     </row>
-    <row r="22" spans="1:8" ht="15">
+    <row r="22" spans="1:8">
       <c r="A22" s="1"/>
       <c r="B22" s="2"/>
       <c r="E22" s="3"/>
@@ -3081,7 +3144,7 @@
       <c r="G22" s="2"/>
       <c r="H22" s="2"/>
     </row>
-    <row r="23" spans="1:8" ht="15">
+    <row r="23" spans="1:8">
       <c r="A23" s="1"/>
       <c r="B23" s="2"/>
       <c r="E23" s="3"/>
@@ -3089,7 +3152,7 @@
       <c r="G23" s="2"/>
       <c r="H23" s="2"/>
     </row>
-    <row r="24" spans="1:8" ht="15">
+    <row r="24" spans="1:8">
       <c r="A24" s="1"/>
       <c r="B24" s="2"/>
       <c r="E24" s="3"/>
@@ -3097,7 +3160,7 @@
       <c r="G24" s="2"/>
       <c r="H24" s="2"/>
     </row>
-    <row r="25" spans="1:8" ht="15">
+    <row r="25" spans="1:8">
       <c r="A25" s="1"/>
       <c r="B25" s="2"/>
       <c r="E25" s="3"/>
@@ -3105,7 +3168,7 @@
       <c r="G25" s="2"/>
       <c r="H25" s="2"/>
     </row>
-    <row r="26" spans="1:8" ht="15">
+    <row r="26" spans="1:8">
       <c r="A26" s="1"/>
       <c r="B26" s="2"/>
       <c r="E26" s="3"/>
@@ -3113,7 +3176,7 @@
       <c r="G26" s="2"/>
       <c r="H26" s="2"/>
     </row>
-    <row r="27" spans="1:8" ht="15">
+    <row r="27" spans="1:8">
       <c r="A27" s="1"/>
       <c r="B27" s="2"/>
       <c r="E27" s="3"/>
@@ -3121,7 +3184,7 @@
       <c r="G27" s="2"/>
       <c r="H27" s="2"/>
     </row>
-    <row r="28" spans="1:8" ht="15">
+    <row r="28" spans="1:8">
       <c r="A28" s="1"/>
       <c r="B28" s="2"/>
       <c r="E28" s="3"/>
@@ -3129,7 +3192,7 @@
       <c r="G28" s="2"/>
       <c r="H28" s="2"/>
     </row>
-    <row r="29" spans="1:8" ht="15">
+    <row r="29" spans="1:8">
       <c r="A29" s="1"/>
       <c r="B29" s="2"/>
       <c r="E29" s="3"/>
@@ -3137,7 +3200,7 @@
       <c r="G29" s="2"/>
       <c r="H29" s="2"/>
     </row>
-    <row r="30" spans="1:8" ht="15">
+    <row r="30" spans="1:8">
       <c r="A30" s="1"/>
       <c r="B30" s="2"/>
       <c r="E30" s="3"/>
@@ -3145,7 +3208,7 @@
       <c r="G30" s="2"/>
       <c r="H30" s="2"/>
     </row>
-    <row r="31" spans="1:8" ht="15">
+    <row r="31" spans="1:8">
       <c r="A31" s="1"/>
       <c r="B31" s="2"/>
       <c r="E31" s="3"/>
@@ -3153,7 +3216,7 @@
       <c r="G31" s="2"/>
       <c r="H31" s="2"/>
     </row>
-    <row r="32" spans="1:8" ht="15">
+    <row r="32" spans="1:8">
       <c r="A32" s="1"/>
       <c r="B32" s="2"/>
       <c r="E32" s="3"/>
@@ -3161,7 +3224,7 @@
       <c r="G32" s="2"/>
       <c r="H32" s="2"/>
     </row>
-    <row r="33" spans="1:8" ht="15">
+    <row r="33" spans="1:8">
       <c r="A33" s="1"/>
       <c r="B33" s="2"/>
       <c r="E33" s="3"/>
@@ -3169,7 +3232,7 @@
       <c r="G33" s="2"/>
       <c r="H33" s="2"/>
     </row>
-    <row r="34" spans="1:8" ht="15">
+    <row r="34" spans="1:8">
       <c r="A34" s="1"/>
       <c r="B34" s="2"/>
       <c r="E34" s="3"/>
@@ -3177,7 +3240,7 @@
       <c r="G34" s="2"/>
       <c r="H34" s="2"/>
     </row>
-    <row r="35" spans="1:8" ht="15">
+    <row r="35" spans="1:8">
       <c r="A35" s="1"/>
       <c r="B35" s="2"/>
       <c r="E35" s="3"/>
@@ -3185,7 +3248,7 @@
       <c r="G35" s="2"/>
       <c r="H35" s="2"/>
     </row>
-    <row r="36" spans="1:8" ht="15">
+    <row r="36" spans="1:8">
       <c r="A36" s="1"/>
       <c r="B36" s="2"/>
       <c r="E36" s="3"/>
@@ -3193,7 +3256,7 @@
       <c r="G36" s="2"/>
       <c r="H36" s="2"/>
     </row>
-    <row r="37" spans="1:8" ht="15">
+    <row r="37" spans="1:8">
       <c r="A37" s="1"/>
       <c r="B37" s="2"/>
       <c r="E37" s="3"/>
@@ -3201,7 +3264,7 @@
       <c r="G37" s="2"/>
       <c r="H37" s="2"/>
     </row>
-    <row r="38" spans="1:8" ht="15">
+    <row r="38" spans="1:8">
       <c r="A38" s="1"/>
       <c r="B38" s="2"/>
       <c r="E38" s="3"/>
@@ -3209,7 +3272,7 @@
       <c r="G38" s="2"/>
       <c r="H38" s="2"/>
     </row>
-    <row r="39" spans="1:8" ht="15">
+    <row r="39" spans="1:8">
       <c r="A39" s="1"/>
       <c r="B39" s="2"/>
       <c r="E39" s="3"/>
@@ -3217,7 +3280,7 @@
       <c r="G39" s="2"/>
       <c r="H39" s="2"/>
     </row>
-    <row r="40" spans="1:8" ht="15">
+    <row r="40" spans="1:8">
       <c r="A40" s="1"/>
       <c r="B40" s="2"/>
       <c r="E40" s="3"/>
@@ -3225,7 +3288,7 @@
       <c r="G40" s="2"/>
       <c r="H40" s="2"/>
     </row>
-    <row r="41" spans="1:8" ht="15">
+    <row r="41" spans="1:8">
       <c r="A41" s="1"/>
       <c r="B41" s="2"/>
       <c r="E41" s="3"/>
@@ -3233,7 +3296,7 @@
       <c r="G41" s="2"/>
       <c r="H41" s="2"/>
     </row>
-    <row r="42" spans="1:8" ht="15">
+    <row r="42" spans="1:8">
       <c r="A42" s="1"/>
       <c r="B42" s="2"/>
       <c r="E42" s="3"/>
@@ -3241,7 +3304,7 @@
       <c r="G42" s="2"/>
       <c r="H42" s="2"/>
     </row>
-    <row r="43" spans="1:8" ht="15">
+    <row r="43" spans="1:8">
       <c r="A43" s="1"/>
       <c r="B43" s="2"/>
       <c r="E43" s="3"/>
@@ -3249,7 +3312,7 @@
       <c r="G43" s="2"/>
       <c r="H43" s="2"/>
     </row>
-    <row r="44" spans="1:8" ht="15">
+    <row r="44" spans="1:8">
       <c r="A44" s="1"/>
       <c r="B44" s="2"/>
       <c r="E44" s="3"/>
@@ -3257,7 +3320,7 @@
       <c r="G44" s="2"/>
       <c r="H44" s="2"/>
     </row>
-    <row r="45" spans="1:8" ht="15">
+    <row r="45" spans="1:8">
       <c r="A45" s="1"/>
       <c r="B45" s="2"/>
       <c r="E45" s="3"/>
@@ -3265,7 +3328,7 @@
       <c r="G45" s="2"/>
       <c r="H45" s="2"/>
     </row>
-    <row r="46" spans="1:8" ht="15">
+    <row r="46" spans="1:8">
       <c r="A46" s="1"/>
       <c r="B46" s="2"/>
       <c r="E46" s="3"/>
@@ -3273,7 +3336,7 @@
       <c r="G46" s="2"/>
       <c r="H46" s="2"/>
     </row>
-    <row r="47" spans="1:8" ht="15">
+    <row r="47" spans="1:8">
       <c r="A47" s="1"/>
       <c r="B47" s="2"/>
       <c r="E47" s="3"/>
@@ -3281,7 +3344,7 @@
       <c r="G47" s="2"/>
       <c r="H47" s="2"/>
     </row>
-    <row r="48" spans="1:8" ht="15">
+    <row r="48" spans="1:8">
       <c r="A48" s="1"/>
       <c r="B48" s="2"/>
       <c r="E48" s="3"/>
@@ -3289,7 +3352,7 @@
       <c r="G48" s="2"/>
       <c r="H48" s="2"/>
     </row>
-    <row r="49" spans="1:8" ht="15">
+    <row r="49" spans="1:8">
       <c r="A49" s="1"/>
       <c r="B49" s="2"/>
       <c r="E49" s="3"/>
@@ -3297,7 +3360,7 @@
       <c r="G49" s="2"/>
       <c r="H49" s="2"/>
     </row>
-    <row r="50" spans="1:8" ht="15">
+    <row r="50" spans="1:8">
       <c r="A50" s="1"/>
       <c r="B50" s="2"/>
       <c r="E50" s="3"/>
@@ -3305,7 +3368,7 @@
       <c r="G50" s="2"/>
       <c r="H50" s="2"/>
     </row>
-    <row r="51" spans="1:8" ht="15">
+    <row r="51" spans="1:8">
       <c r="A51" s="1"/>
       <c r="B51" s="2"/>
       <c r="E51" s="3"/>
@@ -3313,7 +3376,7 @@
       <c r="G51" s="2"/>
       <c r="H51" s="2"/>
     </row>
-    <row r="52" spans="1:8" ht="15">
+    <row r="52" spans="1:8">
       <c r="A52" s="1"/>
       <c r="B52" s="2"/>
       <c r="E52" s="3"/>
@@ -3321,7 +3384,7 @@
       <c r="G52" s="2"/>
       <c r="H52" s="2"/>
     </row>
-    <row r="53" spans="1:8" ht="15">
+    <row r="53" spans="1:8">
       <c r="A53" s="1"/>
       <c r="B53" s="2"/>
       <c r="E53" s="3"/>
@@ -3329,7 +3392,7 @@
       <c r="G53" s="2"/>
       <c r="H53" s="2"/>
     </row>
-    <row r="54" spans="1:8" ht="15">
+    <row r="54" spans="1:8">
       <c r="A54" s="1"/>
       <c r="B54" s="2"/>
       <c r="E54" s="3"/>
@@ -3337,7 +3400,7 @@
       <c r="G54" s="2"/>
       <c r="H54" s="2"/>
     </row>
-    <row r="55" spans="1:8" ht="15">
+    <row r="55" spans="1:8">
       <c r="A55" s="1"/>
       <c r="B55" s="2"/>
       <c r="E55" s="3"/>
@@ -3345,7 +3408,7 @@
       <c r="G55" s="2"/>
       <c r="H55" s="2"/>
     </row>
-    <row r="56" spans="1:8" ht="15">
+    <row r="56" spans="1:8">
       <c r="A56" s="1"/>
       <c r="B56" s="2"/>
       <c r="E56" s="3"/>
@@ -3353,7 +3416,7 @@
       <c r="G56" s="2"/>
       <c r="H56" s="2"/>
     </row>
-    <row r="57" spans="1:8" ht="15">
+    <row r="57" spans="1:8">
       <c r="A57" s="1"/>
       <c r="B57" s="2"/>
       <c r="E57" s="3"/>
@@ -3361,7 +3424,7 @@
       <c r="G57" s="2"/>
       <c r="H57" s="2"/>
     </row>
-    <row r="58" spans="1:8" ht="15">
+    <row r="58" spans="1:8">
       <c r="A58" s="1"/>
       <c r="B58" s="2"/>
       <c r="E58" s="3"/>
@@ -3369,7 +3432,7 @@
       <c r="G58" s="2"/>
       <c r="H58" s="2"/>
     </row>
-    <row r="59" spans="1:8" ht="15">
+    <row r="59" spans="1:8">
       <c r="A59" s="1"/>
       <c r="B59" s="2"/>
       <c r="E59" s="3"/>
@@ -3377,7 +3440,7 @@
       <c r="G59" s="2"/>
       <c r="H59" s="2"/>
     </row>
-    <row r="60" spans="1:8" ht="15">
+    <row r="60" spans="1:8">
       <c r="A60" s="1"/>
       <c r="B60" s="2"/>
       <c r="E60" s="3"/>
@@ -3385,7 +3448,7 @@
       <c r="G60" s="2"/>
       <c r="H60" s="2"/>
     </row>
-    <row r="61" spans="1:8" ht="15">
+    <row r="61" spans="1:8">
       <c r="A61" s="1"/>
       <c r="B61" s="2"/>
       <c r="E61" s="3"/>
@@ -3393,7 +3456,7 @@
       <c r="G61" s="2"/>
       <c r="H61" s="2"/>
     </row>
-    <row r="62" spans="1:8" ht="15">
+    <row r="62" spans="1:8">
       <c r="A62" s="1"/>
       <c r="B62" s="2"/>
       <c r="E62" s="3"/>
@@ -3401,7 +3464,7 @@
       <c r="G62" s="2"/>
       <c r="H62" s="2"/>
     </row>
-    <row r="63" spans="1:8" ht="15">
+    <row r="63" spans="1:8">
       <c r="A63" s="1"/>
       <c r="B63" s="2"/>
       <c r="E63" s="3"/>
@@ -3409,7 +3472,7 @@
       <c r="G63" s="2"/>
       <c r="H63" s="2"/>
     </row>
-    <row r="64" spans="1:8" ht="15">
+    <row r="64" spans="1:8">
       <c r="A64" s="1"/>
       <c r="B64" s="2"/>
       <c r="E64" s="3"/>
@@ -3417,7 +3480,7 @@
       <c r="G64" s="2"/>
       <c r="H64" s="2"/>
     </row>
-    <row r="65" spans="1:8" ht="15">
+    <row r="65" spans="1:8">
       <c r="A65" s="1"/>
       <c r="B65" s="2"/>
       <c r="E65" s="3"/>
@@ -3425,7 +3488,7 @@
       <c r="G65" s="2"/>
       <c r="H65" s="2"/>
     </row>
-    <row r="66" spans="1:8" ht="15">
+    <row r="66" spans="1:8">
       <c r="A66" s="1"/>
       <c r="B66" s="2"/>
       <c r="E66" s="3"/>
@@ -3433,7 +3496,7 @@
       <c r="G66" s="2"/>
       <c r="H66" s="2"/>
     </row>
-    <row r="67" spans="1:8" ht="15">
+    <row r="67" spans="1:8">
       <c r="A67" s="1"/>
       <c r="B67" s="2"/>
       <c r="E67" s="3"/>
@@ -3441,7 +3504,7 @@
       <c r="G67" s="2"/>
       <c r="H67" s="2"/>
     </row>
-    <row r="68" spans="1:8" ht="15">
+    <row r="68" spans="1:8">
       <c r="A68" s="1"/>
       <c r="B68" s="2"/>
       <c r="E68" s="3"/>
@@ -3449,7 +3512,7 @@
       <c r="G68" s="2"/>
       <c r="H68" s="2"/>
     </row>
-    <row r="69" spans="1:8" ht="15">
+    <row r="69" spans="1:8">
       <c r="A69" s="1"/>
       <c r="B69" s="2"/>
       <c r="E69" s="3"/>
@@ -3457,7 +3520,7 @@
       <c r="G69" s="2"/>
       <c r="H69" s="2"/>
     </row>
-    <row r="70" spans="1:8" ht="15">
+    <row r="70" spans="1:8">
       <c r="A70" s="1"/>
       <c r="B70" s="2"/>
       <c r="E70" s="3"/>
@@ -3465,7 +3528,7 @@
       <c r="G70" s="2"/>
       <c r="H70" s="2"/>
     </row>
-    <row r="71" spans="1:8" ht="15">
+    <row r="71" spans="1:8">
       <c r="A71" s="1"/>
       <c r="B71" s="2"/>
       <c r="E71" s="3"/>
@@ -3473,7 +3536,7 @@
       <c r="G71" s="2"/>
       <c r="H71" s="2"/>
     </row>
-    <row r="72" spans="1:8" ht="15">
+    <row r="72" spans="1:8">
       <c r="A72" s="1"/>
       <c r="B72" s="2"/>
       <c r="E72" s="3"/>
@@ -3481,7 +3544,7 @@
       <c r="G72" s="2"/>
       <c r="H72" s="2"/>
     </row>
-    <row r="73" spans="1:8" ht="15">
+    <row r="73" spans="1:8">
       <c r="A73" s="1"/>
       <c r="B73" s="2"/>
       <c r="E73" s="3"/>
@@ -3489,7 +3552,7 @@
       <c r="G73" s="2"/>
       <c r="H73" s="2"/>
     </row>
-    <row r="74" spans="1:8" ht="15">
+    <row r="74" spans="1:8">
       <c r="A74" s="1"/>
       <c r="B74" s="2"/>
       <c r="E74" s="3"/>
@@ -3497,7 +3560,7 @@
       <c r="G74" s="2"/>
       <c r="H74" s="2"/>
     </row>
-    <row r="75" spans="1:8" ht="15">
+    <row r="75" spans="1:8">
       <c r="A75" s="1"/>
       <c r="B75" s="2"/>
       <c r="E75" s="3"/>
@@ -3505,7 +3568,7 @@
       <c r="G75" s="2"/>
       <c r="H75" s="2"/>
     </row>
-    <row r="76" spans="1:8" ht="15">
+    <row r="76" spans="1:8">
       <c r="A76" s="1"/>
       <c r="B76" s="2"/>
       <c r="E76" s="3"/>
@@ -3513,7 +3576,7 @@
       <c r="G76" s="2"/>
       <c r="H76" s="2"/>
     </row>
-    <row r="77" spans="1:8" ht="15">
+    <row r="77" spans="1:8">
       <c r="A77" s="1"/>
       <c r="B77" s="2"/>
       <c r="E77" s="3"/>
@@ -3521,7 +3584,7 @@
       <c r="G77" s="2"/>
       <c r="H77" s="2"/>
     </row>
-    <row r="78" spans="1:8" ht="15">
+    <row r="78" spans="1:8">
       <c r="A78" s="1"/>
       <c r="B78" s="2"/>
       <c r="E78" s="3"/>
@@ -3529,7 +3592,7 @@
       <c r="G78" s="2"/>
       <c r="H78" s="2"/>
     </row>
-    <row r="79" spans="1:8" ht="15">
+    <row r="79" spans="1:8">
       <c r="A79" s="1"/>
       <c r="B79" s="2"/>
       <c r="E79" s="3"/>
@@ -3537,7 +3600,7 @@
       <c r="G79" s="2"/>
       <c r="H79" s="2"/>
     </row>
-    <row r="80" spans="1:8" ht="15">
+    <row r="80" spans="1:8">
       <c r="A80" s="1"/>
       <c r="B80" s="2"/>
       <c r="E80" s="3"/>
@@ -3545,7 +3608,7 @@
       <c r="G80" s="2"/>
       <c r="H80" s="2"/>
     </row>
-    <row r="81" spans="1:8" ht="15">
+    <row r="81" spans="1:8">
       <c r="A81" s="1"/>
       <c r="B81" s="2"/>
       <c r="E81" s="3"/>
@@ -3553,7 +3616,7 @@
       <c r="G81" s="2"/>
       <c r="H81" s="2"/>
     </row>
-    <row r="82" spans="1:8" ht="15">
+    <row r="82" spans="1:8">
       <c r="A82" s="1"/>
       <c r="B82" s="2"/>
       <c r="E82" s="3"/>
@@ -3561,7 +3624,7 @@
       <c r="G82" s="2"/>
       <c r="H82" s="2"/>
     </row>
-    <row r="83" spans="1:8" ht="15">
+    <row r="83" spans="1:8">
       <c r="A83" s="1"/>
       <c r="B83" s="2"/>
       <c r="E83" s="3"/>
@@ -3569,7 +3632,7 @@
       <c r="G83" s="2"/>
       <c r="H83" s="2"/>
     </row>
-    <row r="84" spans="1:8" ht="15">
+    <row r="84" spans="1:8">
       <c r="A84" s="1"/>
       <c r="B84" s="2"/>
       <c r="E84" s="3"/>
@@ -3577,7 +3640,7 @@
       <c r="G84" s="2"/>
       <c r="H84" s="2"/>
     </row>
-    <row r="85" spans="1:8" ht="15">
+    <row r="85" spans="1:8">
       <c r="A85" s="1"/>
       <c r="B85" s="2"/>
       <c r="E85" s="3"/>
@@ -3585,7 +3648,7 @@
       <c r="G85" s="2"/>
       <c r="H85" s="2"/>
     </row>
-    <row r="86" spans="1:8" ht="15">
+    <row r="86" spans="1:8">
       <c r="A86" s="1"/>
       <c r="B86" s="2"/>
       <c r="E86" s="3"/>
@@ -3593,7 +3656,7 @@
       <c r="G86" s="2"/>
       <c r="H86" s="2"/>
     </row>
-    <row r="87" spans="1:8" ht="15">
+    <row r="87" spans="1:8">
       <c r="A87" s="1"/>
       <c r="B87" s="2"/>
       <c r="E87" s="3"/>
@@ -3740,21 +3803,21 @@
       <selection activeCell="P21" sqref="P21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8"/>
+  <sheetFormatPr defaultRowHeight="14"/>
   <cols>
-    <col min="1" max="1" width="10.09765625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.8984375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.8984375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="19.3984375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.59765625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.59765625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.08203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.9140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.9140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19.4140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.58203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.58203125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="9" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="17.8984375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="17.9140625" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="17" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="19.09765625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="19.08203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="15.75">
+    <row r="1" spans="1:10" ht="15.5">
       <c r="A1" s="7" t="s">
         <v>8</v>
       </c>
@@ -3786,7 +3849,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:10" ht="15">
+    <row r="2" spans="1:10">
       <c r="A2" s="2"/>
       <c r="B2" s="8"/>
       <c r="D2" s="2"/>
@@ -3794,7 +3857,7 @@
       <c r="I2" s="8"/>
       <c r="J2" s="2"/>
     </row>
-    <row r="3" spans="1:10" ht="15">
+    <row r="3" spans="1:10">
       <c r="A3" s="2"/>
       <c r="B3" s="8"/>
       <c r="D3" s="2"/>
@@ -3802,7 +3865,7 @@
       <c r="I3" s="8"/>
       <c r="J3" s="2"/>
     </row>
-    <row r="4" spans="1:10" ht="15">
+    <row r="4" spans="1:10">
       <c r="A4" s="2"/>
       <c r="B4" s="8"/>
       <c r="D4" s="2"/>
@@ -3810,7 +3873,7 @@
       <c r="I4" s="8"/>
       <c r="J4" s="2"/>
     </row>
-    <row r="5" spans="1:10" ht="15">
+    <row r="5" spans="1:10">
       <c r="A5" s="2"/>
       <c r="B5" s="8"/>
       <c r="D5" s="2"/>
@@ -3818,7 +3881,7 @@
       <c r="I5" s="8"/>
       <c r="J5" s="2"/>
     </row>
-    <row r="6" spans="1:10" ht="15">
+    <row r="6" spans="1:10">
       <c r="A6" s="2"/>
       <c r="B6" s="8"/>
       <c r="D6" s="2"/>
@@ -3826,7 +3889,7 @@
       <c r="I6" s="8"/>
       <c r="J6" s="2"/>
     </row>
-    <row r="7" spans="1:10" ht="15">
+    <row r="7" spans="1:10">
       <c r="A7" s="2"/>
       <c r="B7" s="8"/>
       <c r="D7" s="2"/>
@@ -3834,7 +3897,7 @@
       <c r="I7" s="8"/>
       <c r="J7" s="2"/>
     </row>
-    <row r="8" spans="1:10" ht="15">
+    <row r="8" spans="1:10">
       <c r="A8" s="2"/>
       <c r="B8" s="8"/>
       <c r="D8" s="2"/>
@@ -3842,7 +3905,7 @@
       <c r="I8" s="8"/>
       <c r="J8" s="2"/>
     </row>
-    <row r="9" spans="1:10" ht="15">
+    <row r="9" spans="1:10">
       <c r="A9" s="2"/>
       <c r="B9" s="8"/>
       <c r="D9" s="2"/>
@@ -3850,7 +3913,7 @@
       <c r="I9" s="8"/>
       <c r="J9" s="2"/>
     </row>
-    <row r="10" spans="1:10" ht="15">
+    <row r="10" spans="1:10">
       <c r="A10" s="2"/>
       <c r="B10" s="8"/>
       <c r="D10" s="2"/>
@@ -3858,7 +3921,7 @@
       <c r="I10" s="8"/>
       <c r="J10" s="2"/>
     </row>
-    <row r="11" spans="1:10" ht="15">
+    <row r="11" spans="1:10">
       <c r="A11" s="2"/>
       <c r="B11" s="8"/>
       <c r="D11" s="2"/>
@@ -3866,7 +3929,7 @@
       <c r="I11" s="8"/>
       <c r="J11" s="2"/>
     </row>
-    <row r="12" spans="1:10" ht="15">
+    <row r="12" spans="1:10">
       <c r="A12" s="2"/>
       <c r="B12" s="8"/>
       <c r="D12" s="2"/>
@@ -3874,7 +3937,7 @@
       <c r="I12" s="8"/>
       <c r="J12" s="2"/>
     </row>
-    <row r="13" spans="1:10" ht="15">
+    <row r="13" spans="1:10">
       <c r="A13" s="2"/>
       <c r="B13" s="8"/>
       <c r="D13" s="2"/>
@@ -3882,7 +3945,7 @@
       <c r="I13" s="8"/>
       <c r="J13" s="2"/>
     </row>
-    <row r="14" spans="1:10" ht="15">
+    <row r="14" spans="1:10">
       <c r="A14" s="2"/>
       <c r="B14" s="8"/>
       <c r="D14" s="2"/>
@@ -3890,7 +3953,7 @@
       <c r="I14" s="8"/>
       <c r="J14" s="2"/>
     </row>
-    <row r="15" spans="1:10" ht="15">
+    <row r="15" spans="1:10">
       <c r="A15" s="2"/>
       <c r="B15" s="8"/>
       <c r="D15" s="2"/>
@@ -3898,7 +3961,7 @@
       <c r="I15" s="8"/>
       <c r="J15" s="2"/>
     </row>
-    <row r="16" spans="1:10" ht="15">
+    <row r="16" spans="1:10">
       <c r="A16" s="2"/>
       <c r="B16" s="8"/>
       <c r="D16" s="2"/>
@@ -3906,7 +3969,7 @@
       <c r="I16" s="8"/>
       <c r="J16" s="2"/>
     </row>
-    <row r="17" spans="1:10" ht="15">
+    <row r="17" spans="1:10">
       <c r="A17" s="2"/>
       <c r="B17" s="8"/>
       <c r="D17" s="2"/>
@@ -3914,7 +3977,7 @@
       <c r="I17" s="8"/>
       <c r="J17" s="2"/>
     </row>
-    <row r="18" spans="1:10" ht="15">
+    <row r="18" spans="1:10">
       <c r="A18" s="2"/>
       <c r="B18" s="8"/>
       <c r="D18" s="2"/>
@@ -3922,7 +3985,7 @@
       <c r="I18" s="8"/>
       <c r="J18" s="2"/>
     </row>
-    <row r="19" spans="1:10" ht="15">
+    <row r="19" spans="1:10">
       <c r="A19" s="2"/>
       <c r="B19" s="8"/>
       <c r="D19" s="2"/>
@@ -3930,7 +3993,7 @@
       <c r="I19" s="8"/>
       <c r="J19" s="2"/>
     </row>
-    <row r="20" spans="1:10" ht="15">
+    <row r="20" spans="1:10">
       <c r="A20" s="2"/>
       <c r="B20" s="8"/>
       <c r="D20" s="2"/>
@@ -3938,7 +4001,7 @@
       <c r="I20" s="8"/>
       <c r="J20" s="2"/>
     </row>
-    <row r="21" spans="1:10" ht="15">
+    <row r="21" spans="1:10">
       <c r="A21" s="2"/>
       <c r="B21" s="8"/>
       <c r="D21" s="2"/>
@@ -3946,7 +4009,7 @@
       <c r="I21" s="8"/>
       <c r="J21" s="2"/>
     </row>
-    <row r="22" spans="1:10" ht="15">
+    <row r="22" spans="1:10">
       <c r="A22" s="2"/>
       <c r="B22" s="8"/>
       <c r="D22" s="2"/>
@@ -3954,7 +4017,7 @@
       <c r="I22" s="8"/>
       <c r="J22" s="2"/>
     </row>
-    <row r="23" spans="1:10" ht="15">
+    <row r="23" spans="1:10">
       <c r="A23" s="2"/>
       <c r="B23" s="8"/>
       <c r="D23" s="2"/>
@@ -3962,7 +4025,7 @@
       <c r="I23" s="8"/>
       <c r="J23" s="2"/>
     </row>
-    <row r="24" spans="1:10" ht="15">
+    <row r="24" spans="1:10">
       <c r="A24" s="2"/>
       <c r="B24" s="8"/>
       <c r="D24" s="2"/>
@@ -3970,7 +4033,7 @@
       <c r="I24" s="8"/>
       <c r="J24" s="2"/>
     </row>
-    <row r="25" spans="1:10" ht="15">
+    <row r="25" spans="1:10">
       <c r="A25" s="2"/>
       <c r="B25" s="8"/>
       <c r="D25" s="2"/>

</xml_diff>

<commit_message>
Updated progress report for 11/05 + 12/05 Sun + Mon by Avichal
</commit_message>
<xml_diff>
--- a/PR&IR.xlsx
+++ b/PR&IR.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\yashp\Documents\CS415\CS415_A3\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\avichal avneel nath\Documents\Semester 7\CS415\A3\CS415_A3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{12BDB62A-F46C-4707-A947-1DB9D8B92BFE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29E4A58F-3349-45EB-9D46-A150A4875504}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="2" xr2:uid="{BFA1E21A-08FA-4F02-8C25-33C81C8EE970}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{BFA1E21A-08FA-4F02-8C25-33C81C8EE970}"/>
   </bookViews>
   <sheets>
     <sheet name="Avichal" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="29">
   <si>
     <t>Date</t>
   </si>
@@ -126,40 +126,19 @@
     <t>All major issues addressed. Application UI improved and backend setup completed with SQL Server and SSMS installation.</t>
   </si>
   <si>
-    <t>Shivya Kumar</t>
+    <t>Researched: how microservices can use different languages while being under one same system + how python will actually CRUD with SSMS( via Sqlalchemy.</t>
   </si>
   <si>
-    <t>Convert UI for login, homepage and student profile</t>
+    <t>Read Docker Documentation. Watched docker tutorials. Coded for course enrollment Logic</t>
   </si>
   <si>
-    <t>In Progress</t>
+    <t>research backend logic + config</t>
   </si>
   <si>
-    <t>Continue converting UI and setting route</t>
+    <t>research on pulling data from firebase and pushing to sql server</t>
   </si>
   <si>
-    <t>I was unable to run the app locally, so I created a folder named run_main_app.py with the required code Once I did that I was able to start the Flask server successfully</t>
-  </si>
-  <si>
-    <t>Added header and footer to the remaining UIs, and converted UI for enrollment page.</t>
-  </si>
-  <si>
-    <t>Solve my routes and fix UI</t>
-  </si>
-  <si>
-    <t>I added my routes in the same file run_main_app.py</t>
-  </si>
-  <si>
-    <t>YPP</t>
-  </si>
-  <si>
-    <t>Converted all assigned dart-flutter files to html/css/js files respectively.</t>
-  </si>
-  <si>
-    <t>Fix my route error and make my local host runnable.</t>
-  </si>
-  <si>
-    <t>N/A</t>
+    <t>complete pending ToDos</t>
   </si>
 </sst>
 </file>
@@ -170,7 +149,7 @@
     <numFmt numFmtId="164" formatCode="h"/>
     <numFmt numFmtId="165" formatCode="d/mm/yyyy;@"/>
   </numFmts>
-  <fonts count="4">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -190,29 +169,16 @@
       <name val="Arial Unicode MS"/>
       <family val="2"/>
     </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Aptos Narrow"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
-  <fills count="3">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFCAEDFB"/>
-        <bgColor rgb="FFCAEDFB"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="2">
+  <borders count="1">
     <border>
       <left/>
       <right/>
@@ -220,26 +186,11 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF61CBF3"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF61CBF3"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF61CBF3"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF61CBF3"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -252,18 +203,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="14" fontId="3" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="3" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="10" fontId="3" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="3" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -321,7 +261,7 @@
       <numFmt numFmtId="30" formatCode="@"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="19" formatCode="m/d/yyyy"/>
+      <numFmt numFmtId="166" formatCode="m/d/yyyy"/>
     </dxf>
     <dxf>
       <font>
@@ -357,7 +297,7 @@
       <numFmt numFmtId="30" formatCode="@"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="19" formatCode="m/d/yyyy"/>
+      <numFmt numFmtId="166" formatCode="m/d/yyyy"/>
     </dxf>
     <dxf>
       <font>
@@ -429,7 +369,7 @@
       <numFmt numFmtId="30" formatCode="@"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="19" formatCode="m/d/yyyy"/>
+      <numFmt numFmtId="166" formatCode="m/d/yyyy"/>
     </dxf>
     <dxf>
       <font>
@@ -944,30 +884,30 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{37EAA098-74C6-4411-B7E2-26AD2DCBC3F0}">
   <dimension ref="A1:H28"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.4140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.58203125" style="2" customWidth="1"/>
+    <col min="1" max="1" width="10.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.5703125" style="2" customWidth="1"/>
     <col min="3" max="3" width="58" customWidth="1"/>
-    <col min="5" max="5" width="13.08203125" style="3" customWidth="1"/>
-    <col min="6" max="6" width="20.9140625" style="4" customWidth="1"/>
-    <col min="7" max="7" width="34.9140625" style="2" customWidth="1"/>
-    <col min="8" max="8" width="43.4140625" style="2" customWidth="1"/>
-    <col min="11" max="11" width="9.08203125" customWidth="1"/>
-    <col min="12" max="12" width="13.33203125" customWidth="1"/>
-    <col min="13" max="13" width="11.4140625" customWidth="1"/>
-    <col min="14" max="14" width="17.4140625" customWidth="1"/>
-    <col min="16" max="16" width="9.08203125" customWidth="1"/>
-    <col min="18" max="18" width="16.58203125" customWidth="1"/>
-    <col min="19" max="19" width="14.6640625" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="16.9140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.140625" style="3" customWidth="1"/>
+    <col min="6" max="6" width="20.85546875" style="4" customWidth="1"/>
+    <col min="7" max="7" width="34.85546875" style="2" customWidth="1"/>
+    <col min="8" max="8" width="43.42578125" style="2" customWidth="1"/>
+    <col min="11" max="11" width="9.140625" customWidth="1"/>
+    <col min="12" max="12" width="13.28515625" customWidth="1"/>
+    <col min="13" max="13" width="11.42578125" customWidth="1"/>
+    <col min="14" max="14" width="17.42578125" customWidth="1"/>
+    <col min="16" max="16" width="9.140625" customWidth="1"/>
+    <col min="18" max="18" width="16.5703125" customWidth="1"/>
+    <col min="19" max="19" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="16.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="15.5">
+    <row r="1" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
@@ -983,7 +923,7 @@
       <c r="E1" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="10" t="s">
+      <c r="F1" s="7" t="s">
         <v>5</v>
       </c>
       <c r="G1" s="7" t="s">
@@ -993,7 +933,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:8">
+    <row r="2" spans="1:8" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A2" s="1">
         <v>45786</v>
       </c>
@@ -1009,7 +949,7 @@
       <c r="E2" s="3">
         <v>1</v>
       </c>
-      <c r="F2" s="11">
+      <c r="F2">
         <v>4</v>
       </c>
       <c r="G2" t="s">
@@ -1019,7 +959,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="3" spans="1:8" ht="112">
+    <row r="3" spans="1:8" ht="120" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>45787</v>
       </c>
@@ -1029,10 +969,10 @@
       <c r="D3" t="s">
         <v>17</v>
       </c>
-      <c r="E3" s="3">
-        <v>1</v>
-      </c>
-      <c r="F3" s="11">
+      <c r="E3" s="10">
+        <v>100</v>
+      </c>
+      <c r="F3">
         <v>3</v>
       </c>
       <c r="G3" s="2" t="s">
@@ -1042,80 +982,128 @@
         <v>23</v>
       </c>
     </row>
-    <row r="4" spans="1:8">
-      <c r="F4" s="11"/>
-    </row>
-    <row r="5" spans="1:8">
-      <c r="F5" s="11"/>
-    </row>
-    <row r="6" spans="1:8">
-      <c r="F6" s="11"/>
-    </row>
-    <row r="7" spans="1:8">
-      <c r="F7" s="11"/>
-    </row>
-    <row r="8" spans="1:8">
-      <c r="F8" s="11"/>
-    </row>
-    <row r="9" spans="1:8">
-      <c r="F9" s="11"/>
-    </row>
-    <row r="10" spans="1:8">
-      <c r="F10" s="11"/>
-    </row>
-    <row r="11" spans="1:8">
-      <c r="F11" s="11"/>
-    </row>
-    <row r="12" spans="1:8">
-      <c r="F12" s="11"/>
-    </row>
-    <row r="13" spans="1:8">
-      <c r="F13" s="11"/>
-    </row>
-    <row r="14" spans="1:8">
-      <c r="F14" s="11"/>
-    </row>
-    <row r="15" spans="1:8">
-      <c r="F15" s="11"/>
-    </row>
-    <row r="16" spans="1:8">
-      <c r="F16" s="11"/>
-    </row>
-    <row r="17" spans="6:6">
-      <c r="F17" s="11"/>
-    </row>
-    <row r="18" spans="6:6">
-      <c r="F18" s="11"/>
-    </row>
-    <row r="19" spans="6:6">
-      <c r="F19" s="11"/>
-    </row>
-    <row r="20" spans="6:6">
-      <c r="F20" s="11"/>
-    </row>
-    <row r="21" spans="6:6">
-      <c r="F21" s="11"/>
-    </row>
-    <row r="22" spans="6:6">
-      <c r="F22" s="11"/>
-    </row>
-    <row r="23" spans="6:6">
-      <c r="F23" s="11"/>
-    </row>
-    <row r="24" spans="6:6">
-      <c r="F24" s="11"/>
-    </row>
-    <row r="25" spans="6:6">
-      <c r="F25" s="11"/>
-    </row>
-    <row r="26" spans="6:6">
-      <c r="F26" s="11"/>
-    </row>
-    <row r="27" spans="6:6">
-      <c r="F27" s="11"/>
-    </row>
-    <row r="28" spans="6:6">
-      <c r="F28" s="11"/>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4" s="1">
+        <v>45788</v>
+      </c>
+      <c r="C4" t="s">
+        <v>24</v>
+      </c>
+      <c r="D4" t="s">
+        <v>17</v>
+      </c>
+      <c r="E4" s="10">
+        <v>90</v>
+      </c>
+      <c r="F4">
+        <v>2</v>
+      </c>
+      <c r="G4" s="2" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" ht="76.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="1">
+        <v>45789</v>
+      </c>
+      <c r="C5" t="s">
+        <v>25</v>
+      </c>
+      <c r="D5" t="s">
+        <v>17</v>
+      </c>
+      <c r="E5" s="10">
+        <v>100</v>
+      </c>
+      <c r="F5">
+        <v>3</v>
+      </c>
+      <c r="G5" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="H5" s="2" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="E6" s="10"/>
+      <c r="F6"/>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="E7" s="10"/>
+      <c r="F7"/>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="E8" s="10"/>
+      <c r="F8"/>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="E9" s="10"/>
+      <c r="F9"/>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="E10" s="10"/>
+      <c r="F10"/>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="E11" s="10"/>
+      <c r="F11"/>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="E12" s="10"/>
+      <c r="F12"/>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="E13" s="10"/>
+      <c r="F13"/>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="E14" s="10"/>
+      <c r="F14"/>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="E15" s="10"/>
+      <c r="F15"/>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="E16" s="10"/>
+      <c r="F16"/>
+    </row>
+    <row r="17" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F17"/>
+    </row>
+    <row r="18" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F18"/>
+    </row>
+    <row r="19" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F19"/>
+    </row>
+    <row r="20" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F20"/>
+    </row>
+    <row r="21" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F21"/>
+    </row>
+    <row r="22" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F22"/>
+    </row>
+    <row r="23" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F23"/>
+    </row>
+    <row r="24" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F24"/>
+    </row>
+    <row r="25" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F25"/>
+    </row>
+    <row r="26" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F26"/>
+    </row>
+    <row r="27" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F27"/>
+    </row>
+    <row r="28" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F28"/>
     </row>
   </sheetData>
   <dataValidations count="4">
@@ -1137,7 +1125,7 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
   <ignoredErrors>
-    <ignoredError sqref="D4:D6 D7:D16" listDataValidation="1"/>
+    <ignoredError sqref="D7:D16 D6" listDataValidation="1"/>
   </ignoredErrors>
   <tableParts count="1">
     <tablePart r:id="rId2"/>
@@ -1147,25 +1135,25 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3BDA6702-5DDF-42FB-988E-13FBEB26F5C9}">
-  <dimension ref="A1:I100"/>
+  <dimension ref="A1:H100"/>
   <sheetViews>
-    <sheetView topLeftCell="G1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:H3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.9140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="17.33203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="63" customWidth="1"/>
+    <col min="1" max="1" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.5703125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="9" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.9140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="23.58203125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="21.83203125" customWidth="1"/>
-    <col min="8" max="8" width="116.4140625" customWidth="1"/>
+    <col min="5" max="5" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="23.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="19.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="15.5">
+    <row r="1" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
@@ -1191,60 +1179,21 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:9">
-      <c r="A2" s="15">
-        <v>45786</v>
-      </c>
-      <c r="B2" s="13" t="s">
-        <v>24</v>
-      </c>
-      <c r="C2" s="12" t="s">
-        <v>25</v>
-      </c>
-      <c r="D2" s="12" t="s">
-        <v>26</v>
-      </c>
-      <c r="E2" s="14">
-        <v>0.9</v>
-      </c>
-      <c r="F2" s="16">
-        <v>8</v>
-      </c>
-      <c r="G2" s="13" t="s">
-        <v>27</v>
-      </c>
-      <c r="H2" s="12" t="s">
-        <v>28</v>
-      </c>
-      <c r="I2" s="13"/>
-    </row>
-    <row r="3" spans="1:9">
-      <c r="A3" s="8">
-        <v>45787</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="C3" t="s">
-        <v>29</v>
-      </c>
-      <c r="D3" t="s">
-        <v>26</v>
-      </c>
-      <c r="E3" s="16">
-        <v>90</v>
-      </c>
-      <c r="F3" s="16">
-        <v>8</v>
-      </c>
-      <c r="G3" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="H3" s="2" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2" s="8"/>
+      <c r="B2" s="2"/>
+      <c r="E2" s="3"/>
+      <c r="G2" s="2"/>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3" s="8"/>
+      <c r="B3" s="2"/>
+      <c r="E3" s="3"/>
+      <c r="F3" s="4"/>
+      <c r="G3" s="2"/>
+      <c r="H3" s="2"/>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="8"/>
       <c r="B4" s="2"/>
       <c r="E4" s="3"/>
@@ -1252,7 +1201,7 @@
       <c r="G4" s="2"/>
       <c r="H4" s="2"/>
     </row>
-    <row r="5" spans="1:9">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="8"/>
       <c r="B5" s="2"/>
       <c r="E5" s="3"/>
@@ -1260,7 +1209,7 @@
       <c r="G5" s="2"/>
       <c r="H5" s="2"/>
     </row>
-    <row r="6" spans="1:9">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="8"/>
       <c r="B6" s="2"/>
       <c r="E6" s="3"/>
@@ -1268,7 +1217,7 @@
       <c r="G6" s="2"/>
       <c r="H6" s="2"/>
     </row>
-    <row r="7" spans="1:9">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="8"/>
       <c r="B7" s="2"/>
       <c r="E7" s="3"/>
@@ -1276,7 +1225,7 @@
       <c r="G7" s="2"/>
       <c r="H7" s="2"/>
     </row>
-    <row r="8" spans="1:9">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="8"/>
       <c r="B8" s="2"/>
       <c r="E8" s="3"/>
@@ -1284,7 +1233,7 @@
       <c r="G8" s="2"/>
       <c r="H8" s="2"/>
     </row>
-    <row r="9" spans="1:9">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="8"/>
       <c r="B9" s="2"/>
       <c r="E9" s="3"/>
@@ -1292,7 +1241,7 @@
       <c r="G9" s="2"/>
       <c r="H9" s="2"/>
     </row>
-    <row r="10" spans="1:9">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="8"/>
       <c r="B10" s="2"/>
       <c r="E10" s="3"/>
@@ -1300,7 +1249,7 @@
       <c r="G10" s="2"/>
       <c r="H10" s="2"/>
     </row>
-    <row r="11" spans="1:9">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="8"/>
       <c r="B11" s="2"/>
       <c r="E11" s="3"/>
@@ -1308,7 +1257,7 @@
       <c r="G11" s="2"/>
       <c r="H11" s="2"/>
     </row>
-    <row r="12" spans="1:9">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="8"/>
       <c r="B12" s="2"/>
       <c r="E12" s="3"/>
@@ -1316,7 +1265,7 @@
       <c r="G12" s="2"/>
       <c r="H12" s="2"/>
     </row>
-    <row r="13" spans="1:9">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="8"/>
       <c r="B13" s="2"/>
       <c r="E13" s="3"/>
@@ -1324,7 +1273,7 @@
       <c r="G13" s="2"/>
       <c r="H13" s="2"/>
     </row>
-    <row r="14" spans="1:9">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" s="8"/>
       <c r="B14" s="2"/>
       <c r="E14" s="3"/>
@@ -1332,7 +1281,7 @@
       <c r="G14" s="2"/>
       <c r="H14" s="2"/>
     </row>
-    <row r="15" spans="1:9">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" s="8"/>
       <c r="B15" s="2"/>
       <c r="E15" s="3"/>
@@ -1340,7 +1289,7 @@
       <c r="G15" s="2"/>
       <c r="H15" s="2"/>
     </row>
-    <row r="16" spans="1:9">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" s="8"/>
       <c r="B16" s="2"/>
       <c r="E16" s="3"/>
@@ -1348,7 +1297,7 @@
       <c r="G16" s="2"/>
       <c r="H16" s="2"/>
     </row>
-    <row r="17" spans="1:8">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" s="8"/>
       <c r="B17" s="2"/>
       <c r="E17" s="3"/>
@@ -1356,7 +1305,7 @@
       <c r="G17" s="2"/>
       <c r="H17" s="2"/>
     </row>
-    <row r="18" spans="1:8">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" s="8"/>
       <c r="B18" s="2"/>
       <c r="E18" s="3"/>
@@ -1364,7 +1313,7 @@
       <c r="G18" s="2"/>
       <c r="H18" s="2"/>
     </row>
-    <row r="19" spans="1:8">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" s="8"/>
       <c r="B19" s="2"/>
       <c r="E19" s="3"/>
@@ -1372,7 +1321,7 @@
       <c r="G19" s="2"/>
       <c r="H19" s="2"/>
     </row>
-    <row r="20" spans="1:8">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" s="8"/>
       <c r="B20" s="2"/>
       <c r="E20" s="3"/>
@@ -1380,7 +1329,7 @@
       <c r="G20" s="2"/>
       <c r="H20" s="2"/>
     </row>
-    <row r="21" spans="1:8">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" s="8"/>
       <c r="B21" s="2"/>
       <c r="E21" s="3"/>
@@ -1388,7 +1337,7 @@
       <c r="G21" s="2"/>
       <c r="H21" s="2"/>
     </row>
-    <row r="22" spans="1:8">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" s="8"/>
       <c r="B22" s="2"/>
       <c r="E22" s="3"/>
@@ -1396,7 +1345,7 @@
       <c r="G22" s="2"/>
       <c r="H22" s="2"/>
     </row>
-    <row r="23" spans="1:8">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" s="8"/>
       <c r="B23" s="2"/>
       <c r="E23" s="3"/>
@@ -1404,7 +1353,7 @@
       <c r="G23" s="2"/>
       <c r="H23" s="2"/>
     </row>
-    <row r="24" spans="1:8">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24" s="8"/>
       <c r="B24" s="2"/>
       <c r="E24" s="3"/>
@@ -1412,7 +1361,7 @@
       <c r="G24" s="2"/>
       <c r="H24" s="2"/>
     </row>
-    <row r="25" spans="1:8">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25" s="8"/>
       <c r="B25" s="2"/>
       <c r="E25" s="3"/>
@@ -1420,7 +1369,7 @@
       <c r="G25" s="2"/>
       <c r="H25" s="2"/>
     </row>
-    <row r="26" spans="1:8">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26" s="8"/>
       <c r="B26" s="2"/>
       <c r="E26" s="3"/>
@@ -1428,7 +1377,7 @@
       <c r="G26" s="2"/>
       <c r="H26" s="2"/>
     </row>
-    <row r="27" spans="1:8">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A27" s="8"/>
       <c r="B27" s="2"/>
       <c r="E27" s="3"/>
@@ -1436,7 +1385,7 @@
       <c r="G27" s="2"/>
       <c r="H27" s="2"/>
     </row>
-    <row r="28" spans="1:8">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A28" s="8"/>
       <c r="B28" s="2"/>
       <c r="E28" s="3"/>
@@ -1444,7 +1393,7 @@
       <c r="G28" s="2"/>
       <c r="H28" s="2"/>
     </row>
-    <row r="29" spans="1:8">
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A29" s="8"/>
       <c r="B29" s="2"/>
       <c r="E29" s="3"/>
@@ -1452,7 +1401,7 @@
       <c r="G29" s="2"/>
       <c r="H29" s="2"/>
     </row>
-    <row r="30" spans="1:8">
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A30" s="8"/>
       <c r="B30" s="2"/>
       <c r="E30" s="3"/>
@@ -1460,7 +1409,7 @@
       <c r="G30" s="2"/>
       <c r="H30" s="2"/>
     </row>
-    <row r="31" spans="1:8">
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A31" s="8"/>
       <c r="B31" s="2"/>
       <c r="E31" s="3"/>
@@ -1468,7 +1417,7 @@
       <c r="G31" s="2"/>
       <c r="H31" s="2"/>
     </row>
-    <row r="32" spans="1:8">
+    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A32" s="8"/>
       <c r="B32" s="2"/>
       <c r="E32" s="3"/>
@@ -1476,7 +1425,7 @@
       <c r="G32" s="2"/>
       <c r="H32" s="2"/>
     </row>
-    <row r="33" spans="1:8">
+    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A33" s="8"/>
       <c r="B33" s="2"/>
       <c r="E33" s="3"/>
@@ -1484,7 +1433,7 @@
       <c r="G33" s="2"/>
       <c r="H33" s="2"/>
     </row>
-    <row r="34" spans="1:8">
+    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A34" s="8"/>
       <c r="B34" s="2"/>
       <c r="E34" s="3"/>
@@ -1492,7 +1441,7 @@
       <c r="G34" s="2"/>
       <c r="H34" s="2"/>
     </row>
-    <row r="35" spans="1:8">
+    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A35" s="8"/>
       <c r="B35" s="2"/>
       <c r="E35" s="3"/>
@@ -1500,7 +1449,7 @@
       <c r="G35" s="2"/>
       <c r="H35" s="2"/>
     </row>
-    <row r="36" spans="1:8">
+    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A36" s="8"/>
       <c r="B36" s="2"/>
       <c r="E36" s="3"/>
@@ -1508,7 +1457,7 @@
       <c r="G36" s="2"/>
       <c r="H36" s="2"/>
     </row>
-    <row r="37" spans="1:8">
+    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A37" s="8"/>
       <c r="B37" s="2"/>
       <c r="E37" s="3"/>
@@ -1516,7 +1465,7 @@
       <c r="G37" s="2"/>
       <c r="H37" s="2"/>
     </row>
-    <row r="38" spans="1:8">
+    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A38" s="8"/>
       <c r="B38" s="2"/>
       <c r="E38" s="3"/>
@@ -1524,7 +1473,7 @@
       <c r="G38" s="2"/>
       <c r="H38" s="2"/>
     </row>
-    <row r="39" spans="1:8">
+    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A39" s="8"/>
       <c r="B39" s="2"/>
       <c r="E39" s="3"/>
@@ -1532,7 +1481,7 @@
       <c r="G39" s="2"/>
       <c r="H39" s="2"/>
     </row>
-    <row r="40" spans="1:8">
+    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A40" s="8"/>
       <c r="B40" s="2"/>
       <c r="E40" s="3"/>
@@ -1540,7 +1489,7 @@
       <c r="G40" s="2"/>
       <c r="H40" s="2"/>
     </row>
-    <row r="41" spans="1:8">
+    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A41" s="8"/>
       <c r="B41" s="2"/>
       <c r="E41" s="3"/>
@@ -1548,7 +1497,7 @@
       <c r="G41" s="2"/>
       <c r="H41" s="2"/>
     </row>
-    <row r="42" spans="1:8">
+    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A42" s="8"/>
       <c r="B42" s="2"/>
       <c r="E42" s="3"/>
@@ -1556,7 +1505,7 @@
       <c r="G42" s="2"/>
       <c r="H42" s="2"/>
     </row>
-    <row r="43" spans="1:8">
+    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A43" s="8"/>
       <c r="B43" s="2"/>
       <c r="E43" s="3"/>
@@ -1564,7 +1513,7 @@
       <c r="G43" s="2"/>
       <c r="H43" s="2"/>
     </row>
-    <row r="44" spans="1:8">
+    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A44" s="8"/>
       <c r="B44" s="2"/>
       <c r="E44" s="3"/>
@@ -1572,7 +1521,7 @@
       <c r="G44" s="2"/>
       <c r="H44" s="2"/>
     </row>
-    <row r="45" spans="1:8">
+    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A45" s="8"/>
       <c r="B45" s="2"/>
       <c r="E45" s="3"/>
@@ -1580,7 +1529,7 @@
       <c r="G45" s="2"/>
       <c r="H45" s="2"/>
     </row>
-    <row r="46" spans="1:8">
+    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A46" s="8"/>
       <c r="B46" s="2"/>
       <c r="E46" s="3"/>
@@ -1588,7 +1537,7 @@
       <c r="G46" s="2"/>
       <c r="H46" s="2"/>
     </row>
-    <row r="47" spans="1:8">
+    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A47" s="8"/>
       <c r="B47" s="2"/>
       <c r="E47" s="3"/>
@@ -1596,7 +1545,7 @@
       <c r="G47" s="2"/>
       <c r="H47" s="2"/>
     </row>
-    <row r="48" spans="1:8">
+    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A48" s="8"/>
       <c r="B48" s="2"/>
       <c r="E48" s="3"/>
@@ -1604,7 +1553,7 @@
       <c r="G48" s="2"/>
       <c r="H48" s="2"/>
     </row>
-    <row r="49" spans="1:8">
+    <row r="49" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A49" s="8"/>
       <c r="B49" s="2"/>
       <c r="E49" s="3"/>
@@ -1612,7 +1561,7 @@
       <c r="G49" s="2"/>
       <c r="H49" s="2"/>
     </row>
-    <row r="50" spans="1:8">
+    <row r="50" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A50" s="8"/>
       <c r="B50" s="2"/>
       <c r="E50" s="3"/>
@@ -1620,7 +1569,7 @@
       <c r="G50" s="2"/>
       <c r="H50" s="2"/>
     </row>
-    <row r="51" spans="1:8">
+    <row r="51" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A51" s="8"/>
       <c r="B51" s="2"/>
       <c r="E51" s="3"/>
@@ -1628,7 +1577,7 @@
       <c r="G51" s="2"/>
       <c r="H51" s="2"/>
     </row>
-    <row r="52" spans="1:8">
+    <row r="52" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A52" s="8"/>
       <c r="B52" s="2"/>
       <c r="E52" s="3"/>
@@ -1636,7 +1585,7 @@
       <c r="G52" s="2"/>
       <c r="H52" s="2"/>
     </row>
-    <row r="53" spans="1:8">
+    <row r="53" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A53" s="8"/>
       <c r="B53" s="2"/>
       <c r="E53" s="3"/>
@@ -1644,7 +1593,7 @@
       <c r="G53" s="2"/>
       <c r="H53" s="2"/>
     </row>
-    <row r="54" spans="1:8">
+    <row r="54" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A54" s="8"/>
       <c r="B54" s="2"/>
       <c r="E54" s="3"/>
@@ -1652,7 +1601,7 @@
       <c r="G54" s="2"/>
       <c r="H54" s="2"/>
     </row>
-    <row r="55" spans="1:8">
+    <row r="55" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A55" s="8"/>
       <c r="B55" s="2"/>
       <c r="E55" s="3"/>
@@ -1660,7 +1609,7 @@
       <c r="G55" s="2"/>
       <c r="H55" s="2"/>
     </row>
-    <row r="56" spans="1:8">
+    <row r="56" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A56" s="8"/>
       <c r="B56" s="2"/>
       <c r="E56" s="3"/>
@@ -1668,7 +1617,7 @@
       <c r="G56" s="2"/>
       <c r="H56" s="2"/>
     </row>
-    <row r="57" spans="1:8">
+    <row r="57" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A57" s="8"/>
       <c r="B57" s="2"/>
       <c r="E57" s="3"/>
@@ -1676,7 +1625,7 @@
       <c r="G57" s="2"/>
       <c r="H57" s="2"/>
     </row>
-    <row r="58" spans="1:8">
+    <row r="58" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A58" s="8"/>
       <c r="B58" s="2"/>
       <c r="E58" s="3"/>
@@ -1684,7 +1633,7 @@
       <c r="G58" s="2"/>
       <c r="H58" s="2"/>
     </row>
-    <row r="59" spans="1:8">
+    <row r="59" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A59" s="8"/>
       <c r="B59" s="2"/>
       <c r="E59" s="3"/>
@@ -1692,7 +1641,7 @@
       <c r="G59" s="2"/>
       <c r="H59" s="2"/>
     </row>
-    <row r="60" spans="1:8">
+    <row r="60" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A60" s="8"/>
       <c r="B60" s="2"/>
       <c r="E60" s="3"/>
@@ -1700,7 +1649,7 @@
       <c r="G60" s="2"/>
       <c r="H60" s="2"/>
     </row>
-    <row r="61" spans="1:8">
+    <row r="61" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A61" s="8"/>
       <c r="B61" s="2"/>
       <c r="E61" s="3"/>
@@ -1708,7 +1657,7 @@
       <c r="G61" s="2"/>
       <c r="H61" s="2"/>
     </row>
-    <row r="62" spans="1:8">
+    <row r="62" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A62" s="8"/>
       <c r="B62" s="2"/>
       <c r="E62" s="3"/>
@@ -1716,7 +1665,7 @@
       <c r="G62" s="2"/>
       <c r="H62" s="2"/>
     </row>
-    <row r="63" spans="1:8">
+    <row r="63" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A63" s="8"/>
       <c r="B63" s="2"/>
       <c r="E63" s="3"/>
@@ -1724,7 +1673,7 @@
       <c r="G63" s="2"/>
       <c r="H63" s="2"/>
     </row>
-    <row r="64" spans="1:8">
+    <row r="64" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A64" s="8"/>
       <c r="B64" s="2"/>
       <c r="E64" s="3"/>
@@ -1732,7 +1681,7 @@
       <c r="G64" s="2"/>
       <c r="H64" s="2"/>
     </row>
-    <row r="65" spans="1:8">
+    <row r="65" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A65" s="8"/>
       <c r="B65" s="2"/>
       <c r="E65" s="3"/>
@@ -1740,7 +1689,7 @@
       <c r="G65" s="2"/>
       <c r="H65" s="2"/>
     </row>
-    <row r="66" spans="1:8">
+    <row r="66" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A66" s="8"/>
       <c r="B66" s="2"/>
       <c r="E66" s="3"/>
@@ -1748,7 +1697,7 @@
       <c r="G66" s="2"/>
       <c r="H66" s="2"/>
     </row>
-    <row r="67" spans="1:8">
+    <row r="67" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A67" s="8"/>
       <c r="B67" s="2"/>
       <c r="E67" s="3"/>
@@ -1756,7 +1705,7 @@
       <c r="G67" s="2"/>
       <c r="H67" s="2"/>
     </row>
-    <row r="68" spans="1:8">
+    <row r="68" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A68" s="8"/>
       <c r="B68" s="2"/>
       <c r="E68" s="3"/>
@@ -1764,7 +1713,7 @@
       <c r="G68" s="2"/>
       <c r="H68" s="2"/>
     </row>
-    <row r="69" spans="1:8">
+    <row r="69" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A69" s="8"/>
       <c r="B69" s="2"/>
       <c r="E69" s="3"/>
@@ -1772,7 +1721,7 @@
       <c r="G69" s="2"/>
       <c r="H69" s="2"/>
     </row>
-    <row r="70" spans="1:8">
+    <row r="70" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A70" s="8"/>
       <c r="B70" s="2"/>
       <c r="E70" s="3"/>
@@ -1780,7 +1729,7 @@
       <c r="G70" s="2"/>
       <c r="H70" s="2"/>
     </row>
-    <row r="71" spans="1:8">
+    <row r="71" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A71" s="8"/>
       <c r="B71" s="2"/>
       <c r="E71" s="3"/>
@@ -1788,7 +1737,7 @@
       <c r="G71" s="2"/>
       <c r="H71" s="2"/>
     </row>
-    <row r="72" spans="1:8">
+    <row r="72" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A72" s="8"/>
       <c r="B72" s="2"/>
       <c r="E72" s="3"/>
@@ -1796,7 +1745,7 @@
       <c r="G72" s="2"/>
       <c r="H72" s="2"/>
     </row>
-    <row r="73" spans="1:8">
+    <row r="73" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A73" s="8"/>
       <c r="B73" s="2"/>
       <c r="E73" s="3"/>
@@ -1804,7 +1753,7 @@
       <c r="G73" s="2"/>
       <c r="H73" s="2"/>
     </row>
-    <row r="74" spans="1:8">
+    <row r="74" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A74" s="8"/>
       <c r="B74" s="2"/>
       <c r="E74" s="3"/>
@@ -1812,7 +1761,7 @@
       <c r="G74" s="2"/>
       <c r="H74" s="2"/>
     </row>
-    <row r="75" spans="1:8">
+    <row r="75" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A75" s="8"/>
       <c r="B75" s="2"/>
       <c r="E75" s="3"/>
@@ -1820,7 +1769,7 @@
       <c r="G75" s="2"/>
       <c r="H75" s="2"/>
     </row>
-    <row r="76" spans="1:8">
+    <row r="76" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A76" s="8"/>
       <c r="B76" s="2"/>
       <c r="E76" s="3"/>
@@ -1828,7 +1777,7 @@
       <c r="G76" s="2"/>
       <c r="H76" s="2"/>
     </row>
-    <row r="77" spans="1:8">
+    <row r="77" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A77" s="8"/>
       <c r="B77" s="2"/>
       <c r="E77" s="3"/>
@@ -1836,7 +1785,7 @@
       <c r="G77" s="2"/>
       <c r="H77" s="2"/>
     </row>
-    <row r="78" spans="1:8">
+    <row r="78" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A78" s="8"/>
       <c r="B78" s="2"/>
       <c r="E78" s="3"/>
@@ -1844,7 +1793,7 @@
       <c r="G78" s="2"/>
       <c r="H78" s="2"/>
     </row>
-    <row r="79" spans="1:8">
+    <row r="79" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A79" s="8"/>
       <c r="B79" s="2"/>
       <c r="E79" s="3"/>
@@ -1852,7 +1801,7 @@
       <c r="G79" s="2"/>
       <c r="H79" s="2"/>
     </row>
-    <row r="80" spans="1:8">
+    <row r="80" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A80" s="8"/>
       <c r="B80" s="2"/>
       <c r="E80" s="3"/>
@@ -1860,7 +1809,7 @@
       <c r="G80" s="2"/>
       <c r="H80" s="2"/>
     </row>
-    <row r="81" spans="1:8">
+    <row r="81" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A81" s="8"/>
       <c r="B81" s="2"/>
       <c r="E81" s="3"/>
@@ -1868,7 +1817,7 @@
       <c r="G81" s="2"/>
       <c r="H81" s="2"/>
     </row>
-    <row r="82" spans="1:8">
+    <row r="82" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A82" s="8"/>
       <c r="B82" s="2"/>
       <c r="E82" s="3"/>
@@ -1876,7 +1825,7 @@
       <c r="G82" s="2"/>
       <c r="H82" s="2"/>
     </row>
-    <row r="83" spans="1:8">
+    <row r="83" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A83" s="8"/>
       <c r="B83" s="2"/>
       <c r="E83" s="3"/>
@@ -1884,7 +1833,7 @@
       <c r="G83" s="2"/>
       <c r="H83" s="2"/>
     </row>
-    <row r="84" spans="1:8">
+    <row r="84" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A84" s="8"/>
       <c r="B84" s="2"/>
       <c r="E84" s="3"/>
@@ -1892,7 +1841,7 @@
       <c r="G84" s="2"/>
       <c r="H84" s="2"/>
     </row>
-    <row r="85" spans="1:8">
+    <row r="85" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A85" s="8"/>
       <c r="B85" s="2"/>
       <c r="E85" s="3"/>
@@ -1900,7 +1849,7 @@
       <c r="G85" s="2"/>
       <c r="H85" s="2"/>
     </row>
-    <row r="86" spans="1:8">
+    <row r="86" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A86" s="8"/>
       <c r="B86" s="2"/>
       <c r="E86" s="3"/>
@@ -1908,7 +1857,7 @@
       <c r="G86" s="2"/>
       <c r="H86" s="2"/>
     </row>
-    <row r="87" spans="1:8">
+    <row r="87" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A87" s="8"/>
       <c r="B87" s="2"/>
       <c r="E87" s="3"/>
@@ -1916,7 +1865,7 @@
       <c r="G87" s="2"/>
       <c r="H87" s="2"/>
     </row>
-    <row r="88" spans="1:8">
+    <row r="88" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A88" s="8"/>
       <c r="B88" s="2"/>
       <c r="E88" s="3"/>
@@ -1924,7 +1873,7 @@
       <c r="G88" s="2"/>
       <c r="H88" s="2"/>
     </row>
-    <row r="89" spans="1:8">
+    <row r="89" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A89" s="8"/>
       <c r="B89" s="2"/>
       <c r="E89" s="3"/>
@@ -1932,7 +1881,7 @@
       <c r="G89" s="2"/>
       <c r="H89" s="2"/>
     </row>
-    <row r="90" spans="1:8">
+    <row r="90" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A90" s="8"/>
       <c r="B90" s="2"/>
       <c r="E90" s="3"/>
@@ -1940,7 +1889,7 @@
       <c r="G90" s="2"/>
       <c r="H90" s="2"/>
     </row>
-    <row r="91" spans="1:8">
+    <row r="91" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A91" s="8"/>
       <c r="B91" s="2"/>
       <c r="E91" s="3"/>
@@ -1948,7 +1897,7 @@
       <c r="G91" s="2"/>
       <c r="H91" s="2"/>
     </row>
-    <row r="92" spans="1:8">
+    <row r="92" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A92" s="8"/>
       <c r="B92" s="2"/>
       <c r="E92" s="3"/>
@@ -1956,7 +1905,7 @@
       <c r="G92" s="2"/>
       <c r="H92" s="2"/>
     </row>
-    <row r="93" spans="1:8">
+    <row r="93" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A93" s="8"/>
       <c r="B93" s="2"/>
       <c r="E93" s="3"/>
@@ -1964,7 +1913,7 @@
       <c r="G93" s="2"/>
       <c r="H93" s="2"/>
     </row>
-    <row r="94" spans="1:8">
+    <row r="94" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A94" s="8"/>
       <c r="B94" s="2"/>
       <c r="E94" s="3"/>
@@ -1972,7 +1921,7 @@
       <c r="G94" s="2"/>
       <c r="H94" s="2"/>
     </row>
-    <row r="95" spans="1:8">
+    <row r="95" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A95" s="8"/>
       <c r="B95" s="2"/>
       <c r="E95" s="3"/>
@@ -1980,7 +1929,7 @@
       <c r="G95" s="2"/>
       <c r="H95" s="2"/>
     </row>
-    <row r="96" spans="1:8">
+    <row r="96" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A96" s="8"/>
       <c r="B96" s="2"/>
       <c r="E96" s="3"/>
@@ -1988,7 +1937,7 @@
       <c r="G96" s="2"/>
       <c r="H96" s="2"/>
     </row>
-    <row r="97" spans="1:8">
+    <row r="97" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A97" s="8"/>
       <c r="B97" s="2"/>
       <c r="E97" s="3"/>
@@ -1996,7 +1945,7 @@
       <c r="G97" s="2"/>
       <c r="H97" s="2"/>
     </row>
-    <row r="98" spans="1:8">
+    <row r="98" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A98" s="8"/>
       <c r="B98" s="2"/>
       <c r="E98" s="3"/>
@@ -2004,7 +1953,7 @@
       <c r="G98" s="2"/>
       <c r="H98" s="2"/>
     </row>
-    <row r="99" spans="1:8">
+    <row r="99" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A99" s="8"/>
       <c r="B99" s="2"/>
       <c r="E99" s="3"/>
@@ -2012,7 +1961,7 @@
       <c r="G99" s="2"/>
       <c r="H99" s="2"/>
     </row>
-    <row r="100" spans="1:8">
+    <row r="100" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A100" s="8"/>
       <c r="B100" s="2"/>
       <c r="E100" s="3"/>
@@ -2039,7 +1988,7 @@
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <ignoredErrors>
-    <ignoredError sqref="D4:D100" listDataValidation="1"/>
+    <ignoredError sqref="D3:D100" listDataValidation="1"/>
   </ignoredErrors>
   <tableParts count="1">
     <tablePart r:id="rId1"/>
@@ -2051,23 +2000,23 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9FD6A201-8E63-4A9E-A683-19506CB489E3}">
   <dimension ref="A1:H100"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+    <sheetView topLeftCell="A63" workbookViewId="0">
+      <selection activeCell="D2" sqref="D2:D100"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="8.75" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="17.33203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.58203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="7.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.5703125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="9" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.9140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="23.58203125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="13.4140625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="19.08203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="23.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="19.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="15.5">
+    <row r="1" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
@@ -2093,33 +2042,15 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:8">
-      <c r="A2" s="17">
-        <v>45939</v>
-      </c>
-      <c r="B2" s="18" t="s">
-        <v>32</v>
-      </c>
-      <c r="C2" s="19" t="s">
-        <v>33</v>
-      </c>
-      <c r="D2" s="19" t="s">
-        <v>17</v>
-      </c>
-      <c r="E2" s="20">
-        <v>1</v>
-      </c>
-      <c r="F2" s="21">
-        <v>3</v>
-      </c>
-      <c r="G2" s="18" t="s">
-        <v>34</v>
-      </c>
-      <c r="H2" s="18" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2" s="1"/>
+      <c r="B2" s="2"/>
+      <c r="E2" s="3"/>
+      <c r="F2" s="4"/>
+      <c r="G2" s="2"/>
+      <c r="H2" s="2"/>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="1"/>
       <c r="B3" s="2"/>
       <c r="E3" s="3"/>
@@ -2127,7 +2058,7 @@
       <c r="G3" s="2"/>
       <c r="H3" s="2"/>
     </row>
-    <row r="4" spans="1:8">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="1"/>
       <c r="B4" s="2"/>
       <c r="E4" s="3"/>
@@ -2135,7 +2066,7 @@
       <c r="G4" s="2"/>
       <c r="H4" s="2"/>
     </row>
-    <row r="5" spans="1:8">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="1"/>
       <c r="B5" s="2"/>
       <c r="E5" s="3"/>
@@ -2143,7 +2074,7 @@
       <c r="G5" s="2"/>
       <c r="H5" s="2"/>
     </row>
-    <row r="6" spans="1:8">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="1"/>
       <c r="B6" s="2"/>
       <c r="E6" s="3"/>
@@ -2151,7 +2082,7 @@
       <c r="G6" s="2"/>
       <c r="H6" s="2"/>
     </row>
-    <row r="7" spans="1:8">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="1"/>
       <c r="B7" s="2"/>
       <c r="E7" s="3"/>
@@ -2159,7 +2090,7 @@
       <c r="G7" s="2"/>
       <c r="H7" s="2"/>
     </row>
-    <row r="8" spans="1:8">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="1"/>
       <c r="B8" s="2"/>
       <c r="E8" s="3"/>
@@ -2167,7 +2098,7 @@
       <c r="G8" s="2"/>
       <c r="H8" s="2"/>
     </row>
-    <row r="9" spans="1:8">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="1"/>
       <c r="B9" s="2"/>
       <c r="E9" s="3"/>
@@ -2175,7 +2106,7 @@
       <c r="G9" s="2"/>
       <c r="H9" s="2"/>
     </row>
-    <row r="10" spans="1:8">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="1"/>
       <c r="B10" s="2"/>
       <c r="E10" s="3"/>
@@ -2183,7 +2114,7 @@
       <c r="G10" s="2"/>
       <c r="H10" s="2"/>
     </row>
-    <row r="11" spans="1:8">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="1"/>
       <c r="B11" s="2"/>
       <c r="E11" s="3"/>
@@ -2191,7 +2122,7 @@
       <c r="G11" s="2"/>
       <c r="H11" s="2"/>
     </row>
-    <row r="12" spans="1:8">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="1"/>
       <c r="B12" s="2"/>
       <c r="E12" s="3"/>
@@ -2199,7 +2130,7 @@
       <c r="G12" s="2"/>
       <c r="H12" s="2"/>
     </row>
-    <row r="13" spans="1:8">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="1"/>
       <c r="B13" s="2"/>
       <c r="E13" s="3"/>
@@ -2207,7 +2138,7 @@
       <c r="G13" s="2"/>
       <c r="H13" s="2"/>
     </row>
-    <row r="14" spans="1:8">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" s="1"/>
       <c r="B14" s="2"/>
       <c r="E14" s="3"/>
@@ -2215,7 +2146,7 @@
       <c r="G14" s="2"/>
       <c r="H14" s="2"/>
     </row>
-    <row r="15" spans="1:8">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" s="1"/>
       <c r="B15" s="2"/>
       <c r="E15" s="3"/>
@@ -2223,7 +2154,7 @@
       <c r="G15" s="2"/>
       <c r="H15" s="2"/>
     </row>
-    <row r="16" spans="1:8">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" s="1"/>
       <c r="B16" s="2"/>
       <c r="E16" s="3"/>
@@ -2231,7 +2162,7 @@
       <c r="G16" s="2"/>
       <c r="H16" s="2"/>
     </row>
-    <row r="17" spans="1:8">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" s="1"/>
       <c r="B17" s="2"/>
       <c r="E17" s="3"/>
@@ -2239,7 +2170,7 @@
       <c r="G17" s="2"/>
       <c r="H17" s="2"/>
     </row>
-    <row r="18" spans="1:8">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" s="1"/>
       <c r="B18" s="2"/>
       <c r="E18" s="3"/>
@@ -2247,7 +2178,7 @@
       <c r="G18" s="2"/>
       <c r="H18" s="2"/>
     </row>
-    <row r="19" spans="1:8">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" s="1"/>
       <c r="B19" s="2"/>
       <c r="E19" s="3"/>
@@ -2255,7 +2186,7 @@
       <c r="G19" s="2"/>
       <c r="H19" s="2"/>
     </row>
-    <row r="20" spans="1:8">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" s="1"/>
       <c r="B20" s="2"/>
       <c r="E20" s="3"/>
@@ -2263,7 +2194,7 @@
       <c r="G20" s="2"/>
       <c r="H20" s="2"/>
     </row>
-    <row r="21" spans="1:8">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" s="1"/>
       <c r="B21" s="2"/>
       <c r="E21" s="3"/>
@@ -2271,7 +2202,7 @@
       <c r="G21" s="2"/>
       <c r="H21" s="2"/>
     </row>
-    <row r="22" spans="1:8">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" s="1"/>
       <c r="B22" s="2"/>
       <c r="E22" s="3"/>
@@ -2279,7 +2210,7 @@
       <c r="G22" s="2"/>
       <c r="H22" s="2"/>
     </row>
-    <row r="23" spans="1:8">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" s="1"/>
       <c r="B23" s="2"/>
       <c r="E23" s="3"/>
@@ -2287,7 +2218,7 @@
       <c r="G23" s="2"/>
       <c r="H23" s="2"/>
     </row>
-    <row r="24" spans="1:8">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24" s="1"/>
       <c r="B24" s="2"/>
       <c r="E24" s="3"/>
@@ -2295,7 +2226,7 @@
       <c r="G24" s="2"/>
       <c r="H24" s="2"/>
     </row>
-    <row r="25" spans="1:8">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25" s="1"/>
       <c r="B25" s="2"/>
       <c r="E25" s="3"/>
@@ -2303,7 +2234,7 @@
       <c r="G25" s="2"/>
       <c r="H25" s="2"/>
     </row>
-    <row r="26" spans="1:8">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26" s="1"/>
       <c r="B26" s="2"/>
       <c r="E26" s="3"/>
@@ -2311,7 +2242,7 @@
       <c r="G26" s="2"/>
       <c r="H26" s="2"/>
     </row>
-    <row r="27" spans="1:8">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A27" s="1"/>
       <c r="B27" s="2"/>
       <c r="E27" s="3"/>
@@ -2319,7 +2250,7 @@
       <c r="G27" s="2"/>
       <c r="H27" s="2"/>
     </row>
-    <row r="28" spans="1:8">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A28" s="1"/>
       <c r="B28" s="2"/>
       <c r="E28" s="3"/>
@@ -2327,7 +2258,7 @@
       <c r="G28" s="2"/>
       <c r="H28" s="2"/>
     </row>
-    <row r="29" spans="1:8">
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A29" s="1"/>
       <c r="B29" s="2"/>
       <c r="E29" s="3"/>
@@ -2335,7 +2266,7 @@
       <c r="G29" s="2"/>
       <c r="H29" s="2"/>
     </row>
-    <row r="30" spans="1:8">
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A30" s="1"/>
       <c r="B30" s="2"/>
       <c r="E30" s="3"/>
@@ -2343,7 +2274,7 @@
       <c r="G30" s="2"/>
       <c r="H30" s="2"/>
     </row>
-    <row r="31" spans="1:8">
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A31" s="1"/>
       <c r="B31" s="2"/>
       <c r="E31" s="3"/>
@@ -2351,7 +2282,7 @@
       <c r="G31" s="2"/>
       <c r="H31" s="2"/>
     </row>
-    <row r="32" spans="1:8">
+    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A32" s="1"/>
       <c r="B32" s="2"/>
       <c r="E32" s="3"/>
@@ -2359,7 +2290,7 @@
       <c r="G32" s="2"/>
       <c r="H32" s="2"/>
     </row>
-    <row r="33" spans="1:8">
+    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A33" s="1"/>
       <c r="B33" s="2"/>
       <c r="E33" s="3"/>
@@ -2367,7 +2298,7 @@
       <c r="G33" s="2"/>
       <c r="H33" s="2"/>
     </row>
-    <row r="34" spans="1:8">
+    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A34" s="1"/>
       <c r="B34" s="2"/>
       <c r="E34" s="3"/>
@@ -2375,7 +2306,7 @@
       <c r="G34" s="2"/>
       <c r="H34" s="2"/>
     </row>
-    <row r="35" spans="1:8">
+    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A35" s="1"/>
       <c r="B35" s="2"/>
       <c r="E35" s="3"/>
@@ -2383,7 +2314,7 @@
       <c r="G35" s="2"/>
       <c r="H35" s="2"/>
     </row>
-    <row r="36" spans="1:8">
+    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A36" s="1"/>
       <c r="B36" s="2"/>
       <c r="E36" s="3"/>
@@ -2391,7 +2322,7 @@
       <c r="G36" s="2"/>
       <c r="H36" s="2"/>
     </row>
-    <row r="37" spans="1:8">
+    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A37" s="1"/>
       <c r="B37" s="2"/>
       <c r="E37" s="3"/>
@@ -2399,7 +2330,7 @@
       <c r="G37" s="2"/>
       <c r="H37" s="2"/>
     </row>
-    <row r="38" spans="1:8">
+    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A38" s="1"/>
       <c r="B38" s="2"/>
       <c r="E38" s="3"/>
@@ -2407,7 +2338,7 @@
       <c r="G38" s="2"/>
       <c r="H38" s="2"/>
     </row>
-    <row r="39" spans="1:8">
+    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A39" s="1"/>
       <c r="B39" s="2"/>
       <c r="E39" s="3"/>
@@ -2415,7 +2346,7 @@
       <c r="G39" s="2"/>
       <c r="H39" s="2"/>
     </row>
-    <row r="40" spans="1:8">
+    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A40" s="1"/>
       <c r="B40" s="2"/>
       <c r="E40" s="3"/>
@@ -2423,7 +2354,7 @@
       <c r="G40" s="2"/>
       <c r="H40" s="2"/>
     </row>
-    <row r="41" spans="1:8">
+    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A41" s="1"/>
       <c r="B41" s="2"/>
       <c r="E41" s="3"/>
@@ -2431,7 +2362,7 @@
       <c r="G41" s="2"/>
       <c r="H41" s="2"/>
     </row>
-    <row r="42" spans="1:8">
+    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A42" s="1"/>
       <c r="B42" s="2"/>
       <c r="E42" s="3"/>
@@ -2439,7 +2370,7 @@
       <c r="G42" s="2"/>
       <c r="H42" s="2"/>
     </row>
-    <row r="43" spans="1:8">
+    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A43" s="1"/>
       <c r="B43" s="2"/>
       <c r="E43" s="3"/>
@@ -2447,7 +2378,7 @@
       <c r="G43" s="2"/>
       <c r="H43" s="2"/>
     </row>
-    <row r="44" spans="1:8">
+    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A44" s="1"/>
       <c r="B44" s="2"/>
       <c r="E44" s="3"/>
@@ -2455,7 +2386,7 @@
       <c r="G44" s="2"/>
       <c r="H44" s="2"/>
     </row>
-    <row r="45" spans="1:8">
+    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A45" s="1"/>
       <c r="B45" s="2"/>
       <c r="E45" s="3"/>
@@ -2463,7 +2394,7 @@
       <c r="G45" s="2"/>
       <c r="H45" s="2"/>
     </row>
-    <row r="46" spans="1:8">
+    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A46" s="1"/>
       <c r="B46" s="2"/>
       <c r="E46" s="3"/>
@@ -2471,7 +2402,7 @@
       <c r="G46" s="2"/>
       <c r="H46" s="2"/>
     </row>
-    <row r="47" spans="1:8">
+    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A47" s="1"/>
       <c r="B47" s="2"/>
       <c r="E47" s="3"/>
@@ -2479,7 +2410,7 @@
       <c r="G47" s="2"/>
       <c r="H47" s="2"/>
     </row>
-    <row r="48" spans="1:8">
+    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A48" s="1"/>
       <c r="B48" s="2"/>
       <c r="E48" s="3"/>
@@ -2487,7 +2418,7 @@
       <c r="G48" s="2"/>
       <c r="H48" s="2"/>
     </row>
-    <row r="49" spans="1:8">
+    <row r="49" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A49" s="1"/>
       <c r="B49" s="2"/>
       <c r="E49" s="3"/>
@@ -2495,7 +2426,7 @@
       <c r="G49" s="2"/>
       <c r="H49" s="2"/>
     </row>
-    <row r="50" spans="1:8">
+    <row r="50" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A50" s="1"/>
       <c r="B50" s="2"/>
       <c r="E50" s="3"/>
@@ -2503,7 +2434,7 @@
       <c r="G50" s="2"/>
       <c r="H50" s="2"/>
     </row>
-    <row r="51" spans="1:8">
+    <row r="51" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A51" s="1"/>
       <c r="B51" s="2"/>
       <c r="E51" s="3"/>
@@ -2511,7 +2442,7 @@
       <c r="G51" s="2"/>
       <c r="H51" s="2"/>
     </row>
-    <row r="52" spans="1:8">
+    <row r="52" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A52" s="1"/>
       <c r="B52" s="2"/>
       <c r="E52" s="3"/>
@@ -2519,7 +2450,7 @@
       <c r="G52" s="2"/>
       <c r="H52" s="2"/>
     </row>
-    <row r="53" spans="1:8">
+    <row r="53" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A53" s="1"/>
       <c r="B53" s="2"/>
       <c r="E53" s="3"/>
@@ -2527,7 +2458,7 @@
       <c r="G53" s="2"/>
       <c r="H53" s="2"/>
     </row>
-    <row r="54" spans="1:8">
+    <row r="54" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A54" s="1"/>
       <c r="B54" s="2"/>
       <c r="E54" s="3"/>
@@ -2535,7 +2466,7 @@
       <c r="G54" s="2"/>
       <c r="H54" s="2"/>
     </row>
-    <row r="55" spans="1:8">
+    <row r="55" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A55" s="1"/>
       <c r="B55" s="2"/>
       <c r="E55" s="3"/>
@@ -2543,7 +2474,7 @@
       <c r="G55" s="2"/>
       <c r="H55" s="2"/>
     </row>
-    <row r="56" spans="1:8">
+    <row r="56" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A56" s="1"/>
       <c r="B56" s="2"/>
       <c r="E56" s="3"/>
@@ -2551,7 +2482,7 @@
       <c r="G56" s="2"/>
       <c r="H56" s="2"/>
     </row>
-    <row r="57" spans="1:8">
+    <row r="57" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A57" s="1"/>
       <c r="B57" s="2"/>
       <c r="E57" s="3"/>
@@ -2559,7 +2490,7 @@
       <c r="G57" s="2"/>
       <c r="H57" s="2"/>
     </row>
-    <row r="58" spans="1:8">
+    <row r="58" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A58" s="1"/>
       <c r="B58" s="2"/>
       <c r="E58" s="3"/>
@@ -2567,7 +2498,7 @@
       <c r="G58" s="2"/>
       <c r="H58" s="2"/>
     </row>
-    <row r="59" spans="1:8">
+    <row r="59" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A59" s="1"/>
       <c r="B59" s="2"/>
       <c r="E59" s="3"/>
@@ -2575,7 +2506,7 @@
       <c r="G59" s="2"/>
       <c r="H59" s="2"/>
     </row>
-    <row r="60" spans="1:8">
+    <row r="60" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A60" s="1"/>
       <c r="B60" s="2"/>
       <c r="E60" s="3"/>
@@ -2583,7 +2514,7 @@
       <c r="G60" s="2"/>
       <c r="H60" s="2"/>
     </row>
-    <row r="61" spans="1:8">
+    <row r="61" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A61" s="1"/>
       <c r="B61" s="2"/>
       <c r="E61" s="3"/>
@@ -2591,7 +2522,7 @@
       <c r="G61" s="2"/>
       <c r="H61" s="2"/>
     </row>
-    <row r="62" spans="1:8">
+    <row r="62" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A62" s="1"/>
       <c r="B62" s="2"/>
       <c r="E62" s="3"/>
@@ -2599,7 +2530,7 @@
       <c r="G62" s="2"/>
       <c r="H62" s="2"/>
     </row>
-    <row r="63" spans="1:8">
+    <row r="63" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A63" s="1"/>
       <c r="B63" s="2"/>
       <c r="E63" s="3"/>
@@ -2607,7 +2538,7 @@
       <c r="G63" s="2"/>
       <c r="H63" s="2"/>
     </row>
-    <row r="64" spans="1:8">
+    <row r="64" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A64" s="1"/>
       <c r="B64" s="2"/>
       <c r="E64" s="3"/>
@@ -2615,7 +2546,7 @@
       <c r="G64" s="2"/>
       <c r="H64" s="2"/>
     </row>
-    <row r="65" spans="1:8">
+    <row r="65" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A65" s="1"/>
       <c r="B65" s="2"/>
       <c r="E65" s="3"/>
@@ -2623,7 +2554,7 @@
       <c r="G65" s="2"/>
       <c r="H65" s="2"/>
     </row>
-    <row r="66" spans="1:8">
+    <row r="66" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A66" s="1"/>
       <c r="B66" s="2"/>
       <c r="E66" s="3"/>
@@ -2631,7 +2562,7 @@
       <c r="G66" s="2"/>
       <c r="H66" s="2"/>
     </row>
-    <row r="67" spans="1:8">
+    <row r="67" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A67" s="1"/>
       <c r="B67" s="2"/>
       <c r="E67" s="3"/>
@@ -2639,7 +2570,7 @@
       <c r="G67" s="2"/>
       <c r="H67" s="2"/>
     </row>
-    <row r="68" spans="1:8">
+    <row r="68" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A68" s="1"/>
       <c r="B68" s="2"/>
       <c r="E68" s="3"/>
@@ -2647,7 +2578,7 @@
       <c r="G68" s="2"/>
       <c r="H68" s="2"/>
     </row>
-    <row r="69" spans="1:8">
+    <row r="69" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A69" s="1"/>
       <c r="B69" s="2"/>
       <c r="E69" s="3"/>
@@ -2655,7 +2586,7 @@
       <c r="G69" s="2"/>
       <c r="H69" s="2"/>
     </row>
-    <row r="70" spans="1:8">
+    <row r="70" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A70" s="1"/>
       <c r="B70" s="2"/>
       <c r="E70" s="3"/>
@@ -2663,7 +2594,7 @@
       <c r="G70" s="2"/>
       <c r="H70" s="2"/>
     </row>
-    <row r="71" spans="1:8">
+    <row r="71" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A71" s="1"/>
       <c r="B71" s="2"/>
       <c r="E71" s="3"/>
@@ -2671,7 +2602,7 @@
       <c r="G71" s="2"/>
       <c r="H71" s="2"/>
     </row>
-    <row r="72" spans="1:8">
+    <row r="72" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A72" s="1"/>
       <c r="B72" s="2"/>
       <c r="E72" s="3"/>
@@ -2679,7 +2610,7 @@
       <c r="G72" s="2"/>
       <c r="H72" s="2"/>
     </row>
-    <row r="73" spans="1:8">
+    <row r="73" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A73" s="1"/>
       <c r="B73" s="2"/>
       <c r="E73" s="3"/>
@@ -2687,7 +2618,7 @@
       <c r="G73" s="2"/>
       <c r="H73" s="2"/>
     </row>
-    <row r="74" spans="1:8">
+    <row r="74" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A74" s="1"/>
       <c r="B74" s="2"/>
       <c r="E74" s="3"/>
@@ -2695,7 +2626,7 @@
       <c r="G74" s="2"/>
       <c r="H74" s="2"/>
     </row>
-    <row r="75" spans="1:8">
+    <row r="75" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A75" s="1"/>
       <c r="B75" s="2"/>
       <c r="E75" s="3"/>
@@ -2703,7 +2634,7 @@
       <c r="G75" s="2"/>
       <c r="H75" s="2"/>
     </row>
-    <row r="76" spans="1:8">
+    <row r="76" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A76" s="1"/>
       <c r="B76" s="2"/>
       <c r="E76" s="3"/>
@@ -2711,7 +2642,7 @@
       <c r="G76" s="2"/>
       <c r="H76" s="2"/>
     </row>
-    <row r="77" spans="1:8">
+    <row r="77" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A77" s="1"/>
       <c r="B77" s="2"/>
       <c r="E77" s="3"/>
@@ -2719,7 +2650,7 @@
       <c r="G77" s="2"/>
       <c r="H77" s="2"/>
     </row>
-    <row r="78" spans="1:8">
+    <row r="78" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A78" s="1"/>
       <c r="B78" s="2"/>
       <c r="E78" s="3"/>
@@ -2727,7 +2658,7 @@
       <c r="G78" s="2"/>
       <c r="H78" s="2"/>
     </row>
-    <row r="79" spans="1:8">
+    <row r="79" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A79" s="1"/>
       <c r="B79" s="2"/>
       <c r="E79" s="3"/>
@@ -2735,7 +2666,7 @@
       <c r="G79" s="2"/>
       <c r="H79" s="2"/>
     </row>
-    <row r="80" spans="1:8">
+    <row r="80" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A80" s="1"/>
       <c r="B80" s="2"/>
       <c r="E80" s="3"/>
@@ -2743,7 +2674,7 @@
       <c r="G80" s="2"/>
       <c r="H80" s="2"/>
     </row>
-    <row r="81" spans="1:8">
+    <row r="81" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A81" s="1"/>
       <c r="B81" s="2"/>
       <c r="E81" s="3"/>
@@ -2751,7 +2682,7 @@
       <c r="G81" s="2"/>
       <c r="H81" s="2"/>
     </row>
-    <row r="82" spans="1:8">
+    <row r="82" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A82" s="1"/>
       <c r="B82" s="2"/>
       <c r="E82" s="3"/>
@@ -2759,7 +2690,7 @@
       <c r="G82" s="2"/>
       <c r="H82" s="2"/>
     </row>
-    <row r="83" spans="1:8">
+    <row r="83" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A83" s="1"/>
       <c r="B83" s="2"/>
       <c r="E83" s="3"/>
@@ -2767,7 +2698,7 @@
       <c r="G83" s="2"/>
       <c r="H83" s="2"/>
     </row>
-    <row r="84" spans="1:8">
+    <row r="84" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A84" s="1"/>
       <c r="B84" s="2"/>
       <c r="E84" s="3"/>
@@ -2775,7 +2706,7 @@
       <c r="G84" s="2"/>
       <c r="H84" s="2"/>
     </row>
-    <row r="85" spans="1:8">
+    <row r="85" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A85" s="1"/>
       <c r="B85" s="2"/>
       <c r="E85" s="3"/>
@@ -2783,7 +2714,7 @@
       <c r="G85" s="2"/>
       <c r="H85" s="2"/>
     </row>
-    <row r="86" spans="1:8">
+    <row r="86" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A86" s="1"/>
       <c r="B86" s="2"/>
       <c r="E86" s="3"/>
@@ -2791,7 +2722,7 @@
       <c r="G86" s="2"/>
       <c r="H86" s="2"/>
     </row>
-    <row r="87" spans="1:8">
+    <row r="87" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A87" s="1"/>
       <c r="B87" s="2"/>
       <c r="E87" s="3"/>
@@ -2799,7 +2730,7 @@
       <c r="G87" s="2"/>
       <c r="H87" s="2"/>
     </row>
-    <row r="88" spans="1:8">
+    <row r="88" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A88" s="1"/>
       <c r="B88" s="2"/>
       <c r="E88" s="3"/>
@@ -2807,7 +2738,7 @@
       <c r="G88" s="2"/>
       <c r="H88" s="2"/>
     </row>
-    <row r="89" spans="1:8">
+    <row r="89" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A89" s="1"/>
       <c r="B89" s="2"/>
       <c r="E89" s="3"/>
@@ -2815,7 +2746,7 @@
       <c r="G89" s="2"/>
       <c r="H89" s="2"/>
     </row>
-    <row r="90" spans="1:8">
+    <row r="90" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A90" s="1"/>
       <c r="B90" s="2"/>
       <c r="E90" s="3"/>
@@ -2823,7 +2754,7 @@
       <c r="G90" s="2"/>
       <c r="H90" s="2"/>
     </row>
-    <row r="91" spans="1:8">
+    <row r="91" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A91" s="1"/>
       <c r="B91" s="2"/>
       <c r="E91" s="3"/>
@@ -2831,7 +2762,7 @@
       <c r="G91" s="2"/>
       <c r="H91" s="2"/>
     </row>
-    <row r="92" spans="1:8">
+    <row r="92" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A92" s="1"/>
       <c r="B92" s="2"/>
       <c r="E92" s="3"/>
@@ -2839,7 +2770,7 @@
       <c r="G92" s="2"/>
       <c r="H92" s="2"/>
     </row>
-    <row r="93" spans="1:8">
+    <row r="93" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A93" s="1"/>
       <c r="B93" s="2"/>
       <c r="E93" s="3"/>
@@ -2847,7 +2778,7 @@
       <c r="G93" s="2"/>
       <c r="H93" s="2"/>
     </row>
-    <row r="94" spans="1:8">
+    <row r="94" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A94" s="1"/>
       <c r="B94" s="2"/>
       <c r="E94" s="3"/>
@@ -2855,7 +2786,7 @@
       <c r="G94" s="2"/>
       <c r="H94" s="2"/>
     </row>
-    <row r="95" spans="1:8">
+    <row r="95" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A95" s="1"/>
       <c r="B95" s="2"/>
       <c r="E95" s="3"/>
@@ -2863,7 +2794,7 @@
       <c r="G95" s="2"/>
       <c r="H95" s="2"/>
     </row>
-    <row r="96" spans="1:8">
+    <row r="96" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A96" s="1"/>
       <c r="B96" s="2"/>
       <c r="E96" s="3"/>
@@ -2871,7 +2802,7 @@
       <c r="G96" s="2"/>
       <c r="H96" s="2"/>
     </row>
-    <row r="97" spans="1:8">
+    <row r="97" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A97" s="1"/>
       <c r="B97" s="2"/>
       <c r="E97" s="3"/>
@@ -2879,7 +2810,7 @@
       <c r="G97" s="2"/>
       <c r="H97" s="2"/>
     </row>
-    <row r="98" spans="1:8">
+    <row r="98" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A98" s="1"/>
       <c r="B98" s="2"/>
       <c r="E98" s="3"/>
@@ -2887,7 +2818,7 @@
       <c r="G98" s="2"/>
       <c r="H98" s="2"/>
     </row>
-    <row r="99" spans="1:8">
+    <row r="99" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A99" s="1"/>
       <c r="B99" s="2"/>
       <c r="E99" s="3"/>
@@ -2895,7 +2826,7 @@
       <c r="G99" s="2"/>
       <c r="H99" s="2"/>
     </row>
-    <row r="100" spans="1:8">
+    <row r="100" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A100" s="1"/>
       <c r="B100" s="2"/>
       <c r="E100" s="3"/>
@@ -2905,14 +2836,14 @@
     </row>
   </sheetData>
   <dataValidations count="4">
-    <dataValidation type="list" errorStyle="warning" showInputMessage="1" showErrorMessage="1" errorTitle="Select Status" error="Fill in Status to proccessd " sqref="D3:D16" xr:uid="{E71B4AA3-209B-477E-A06E-31A006A45CD7}">
+    <dataValidation type="list" errorStyle="warning" showInputMessage="1" showErrorMessage="1" errorTitle="Select Status" error="Fill in Status to proccessd " sqref="D2:D16" xr:uid="{E71B4AA3-209B-477E-A06E-31A006A45CD7}">
       <formula1>"To Do,In Progress,Completed,Blocked"</formula1>
     </dataValidation>
-    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F3:F100" xr:uid="{1CA240CB-8CBA-47E0-8CFF-996BD4AF540F}">
+    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F2:F100" xr:uid="{1CA240CB-8CBA-47E0-8CFF-996BD4AF540F}">
       <formula1>1</formula1>
       <formula2>24</formula2>
     </dataValidation>
-    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E3:E100" xr:uid="{2CF02A19-ACD0-4709-8E3E-614FB1991DD8}">
+    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2:E100" xr:uid="{2CF02A19-ACD0-4709-8E3E-614FB1991DD8}">
       <formula1>0</formula1>
       <formula2>100</formula2>
     </dataValidation>
@@ -2922,7 +2853,7 @@
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <ignoredErrors>
-    <ignoredError sqref="D3:D100" listDataValidation="1"/>
+    <ignoredError sqref="D2:D100" listDataValidation="1"/>
   </ignoredErrors>
   <tableParts count="1">
     <tablePart r:id="rId1"/>
@@ -2938,19 +2869,19 @@
       <selection activeCell="D2" sqref="D2:D100"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="7.6640625" customWidth="1"/>
-    <col min="2" max="2" width="17.33203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.58203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="7.7109375" customWidth="1"/>
+    <col min="2" max="2" width="17.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.5703125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="9" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.9140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="23.58203125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="13.4140625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="19.08203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="23.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="19.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="15.5">
+    <row r="1" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
@@ -2976,7 +2907,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:8">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="1"/>
       <c r="B2" s="2"/>
       <c r="E2" s="3"/>
@@ -2984,7 +2915,7 @@
       <c r="G2" s="2"/>
       <c r="H2" s="2"/>
     </row>
-    <row r="3" spans="1:8">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="1"/>
       <c r="B3" s="2"/>
       <c r="E3" s="3"/>
@@ -2992,7 +2923,7 @@
       <c r="G3" s="2"/>
       <c r="H3" s="2"/>
     </row>
-    <row r="4" spans="1:8">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="1"/>
       <c r="B4" s="2"/>
       <c r="E4" s="3"/>
@@ -3000,7 +2931,7 @@
       <c r="G4" s="2"/>
       <c r="H4" s="2"/>
     </row>
-    <row r="5" spans="1:8">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="1"/>
       <c r="B5" s="2"/>
       <c r="E5" s="3"/>
@@ -3008,7 +2939,7 @@
       <c r="G5" s="2"/>
       <c r="H5" s="2"/>
     </row>
-    <row r="6" spans="1:8">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="1"/>
       <c r="B6" s="2"/>
       <c r="E6" s="3"/>
@@ -3016,7 +2947,7 @@
       <c r="G6" s="2"/>
       <c r="H6" s="2"/>
     </row>
-    <row r="7" spans="1:8">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="1"/>
       <c r="B7" s="2"/>
       <c r="E7" s="3"/>
@@ -3024,7 +2955,7 @@
       <c r="G7" s="2"/>
       <c r="H7" s="2"/>
     </row>
-    <row r="8" spans="1:8">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="1"/>
       <c r="B8" s="2"/>
       <c r="E8" s="3"/>
@@ -3032,7 +2963,7 @@
       <c r="G8" s="2"/>
       <c r="H8" s="2"/>
     </row>
-    <row r="9" spans="1:8">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="1"/>
       <c r="B9" s="2"/>
       <c r="E9" s="3"/>
@@ -3040,7 +2971,7 @@
       <c r="G9" s="2"/>
       <c r="H9" s="2"/>
     </row>
-    <row r="10" spans="1:8">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="1"/>
       <c r="B10" s="2"/>
       <c r="E10" s="3"/>
@@ -3048,7 +2979,7 @@
       <c r="G10" s="2"/>
       <c r="H10" s="2"/>
     </row>
-    <row r="11" spans="1:8">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="1"/>
       <c r="B11" s="2"/>
       <c r="E11" s="3"/>
@@ -3056,7 +2987,7 @@
       <c r="G11" s="2"/>
       <c r="H11" s="2"/>
     </row>
-    <row r="12" spans="1:8">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="1"/>
       <c r="B12" s="2"/>
       <c r="E12" s="3"/>
@@ -3064,7 +2995,7 @@
       <c r="G12" s="2"/>
       <c r="H12" s="2"/>
     </row>
-    <row r="13" spans="1:8">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="1"/>
       <c r="B13" s="2"/>
       <c r="E13" s="3"/>
@@ -3072,7 +3003,7 @@
       <c r="G13" s="2"/>
       <c r="H13" s="2"/>
     </row>
-    <row r="14" spans="1:8">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" s="1"/>
       <c r="B14" s="2"/>
       <c r="E14" s="3"/>
@@ -3080,7 +3011,7 @@
       <c r="G14" s="2"/>
       <c r="H14" s="2"/>
     </row>
-    <row r="15" spans="1:8">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" s="1"/>
       <c r="B15" s="2"/>
       <c r="E15" s="3"/>
@@ -3088,7 +3019,7 @@
       <c r="G15" s="2"/>
       <c r="H15" s="2"/>
     </row>
-    <row r="16" spans="1:8">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" s="1"/>
       <c r="B16" s="2"/>
       <c r="E16" s="3"/>
@@ -3096,7 +3027,7 @@
       <c r="G16" s="2"/>
       <c r="H16" s="2"/>
     </row>
-    <row r="17" spans="1:8">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" s="1"/>
       <c r="B17" s="2"/>
       <c r="E17" s="3"/>
@@ -3104,7 +3035,7 @@
       <c r="G17" s="2"/>
       <c r="H17" s="2"/>
     </row>
-    <row r="18" spans="1:8">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" s="1"/>
       <c r="B18" s="2"/>
       <c r="E18" s="3"/>
@@ -3112,7 +3043,7 @@
       <c r="G18" s="2"/>
       <c r="H18" s="2"/>
     </row>
-    <row r="19" spans="1:8">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" s="1"/>
       <c r="B19" s="2"/>
       <c r="E19" s="3"/>
@@ -3120,7 +3051,7 @@
       <c r="G19" s="2"/>
       <c r="H19" s="2"/>
     </row>
-    <row r="20" spans="1:8">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" s="1"/>
       <c r="B20" s="2"/>
       <c r="E20" s="3"/>
@@ -3128,7 +3059,7 @@
       <c r="G20" s="2"/>
       <c r="H20" s="2"/>
     </row>
-    <row r="21" spans="1:8">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" s="1"/>
       <c r="B21" s="2"/>
       <c r="E21" s="3"/>
@@ -3136,7 +3067,7 @@
       <c r="G21" s="2"/>
       <c r="H21" s="2"/>
     </row>
-    <row r="22" spans="1:8">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" s="1"/>
       <c r="B22" s="2"/>
       <c r="E22" s="3"/>
@@ -3144,7 +3075,7 @@
       <c r="G22" s="2"/>
       <c r="H22" s="2"/>
     </row>
-    <row r="23" spans="1:8">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" s="1"/>
       <c r="B23" s="2"/>
       <c r="E23" s="3"/>
@@ -3152,7 +3083,7 @@
       <c r="G23" s="2"/>
       <c r="H23" s="2"/>
     </row>
-    <row r="24" spans="1:8">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24" s="1"/>
       <c r="B24" s="2"/>
       <c r="E24" s="3"/>
@@ -3160,7 +3091,7 @@
       <c r="G24" s="2"/>
       <c r="H24" s="2"/>
     </row>
-    <row r="25" spans="1:8">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25" s="1"/>
       <c r="B25" s="2"/>
       <c r="E25" s="3"/>
@@ -3168,7 +3099,7 @@
       <c r="G25" s="2"/>
       <c r="H25" s="2"/>
     </row>
-    <row r="26" spans="1:8">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26" s="1"/>
       <c r="B26" s="2"/>
       <c r="E26" s="3"/>
@@ -3176,7 +3107,7 @@
       <c r="G26" s="2"/>
       <c r="H26" s="2"/>
     </row>
-    <row r="27" spans="1:8">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A27" s="1"/>
       <c r="B27" s="2"/>
       <c r="E27" s="3"/>
@@ -3184,7 +3115,7 @@
       <c r="G27" s="2"/>
       <c r="H27" s="2"/>
     </row>
-    <row r="28" spans="1:8">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A28" s="1"/>
       <c r="B28" s="2"/>
       <c r="E28" s="3"/>
@@ -3192,7 +3123,7 @@
       <c r="G28" s="2"/>
       <c r="H28" s="2"/>
     </row>
-    <row r="29" spans="1:8">
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A29" s="1"/>
       <c r="B29" s="2"/>
       <c r="E29" s="3"/>
@@ -3200,7 +3131,7 @@
       <c r="G29" s="2"/>
       <c r="H29" s="2"/>
     </row>
-    <row r="30" spans="1:8">
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A30" s="1"/>
       <c r="B30" s="2"/>
       <c r="E30" s="3"/>
@@ -3208,7 +3139,7 @@
       <c r="G30" s="2"/>
       <c r="H30" s="2"/>
     </row>
-    <row r="31" spans="1:8">
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A31" s="1"/>
       <c r="B31" s="2"/>
       <c r="E31" s="3"/>
@@ -3216,7 +3147,7 @@
       <c r="G31" s="2"/>
       <c r="H31" s="2"/>
     </row>
-    <row r="32" spans="1:8">
+    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A32" s="1"/>
       <c r="B32" s="2"/>
       <c r="E32" s="3"/>
@@ -3224,7 +3155,7 @@
       <c r="G32" s="2"/>
       <c r="H32" s="2"/>
     </row>
-    <row r="33" spans="1:8">
+    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A33" s="1"/>
       <c r="B33" s="2"/>
       <c r="E33" s="3"/>
@@ -3232,7 +3163,7 @@
       <c r="G33" s="2"/>
       <c r="H33" s="2"/>
     </row>
-    <row r="34" spans="1:8">
+    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A34" s="1"/>
       <c r="B34" s="2"/>
       <c r="E34" s="3"/>
@@ -3240,7 +3171,7 @@
       <c r="G34" s="2"/>
       <c r="H34" s="2"/>
     </row>
-    <row r="35" spans="1:8">
+    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A35" s="1"/>
       <c r="B35" s="2"/>
       <c r="E35" s="3"/>
@@ -3248,7 +3179,7 @@
       <c r="G35" s="2"/>
       <c r="H35" s="2"/>
     </row>
-    <row r="36" spans="1:8">
+    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A36" s="1"/>
       <c r="B36" s="2"/>
       <c r="E36" s="3"/>
@@ -3256,7 +3187,7 @@
       <c r="G36" s="2"/>
       <c r="H36" s="2"/>
     </row>
-    <row r="37" spans="1:8">
+    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A37" s="1"/>
       <c r="B37" s="2"/>
       <c r="E37" s="3"/>
@@ -3264,7 +3195,7 @@
       <c r="G37" s="2"/>
       <c r="H37" s="2"/>
     </row>
-    <row r="38" spans="1:8">
+    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A38" s="1"/>
       <c r="B38" s="2"/>
       <c r="E38" s="3"/>
@@ -3272,7 +3203,7 @@
       <c r="G38" s="2"/>
       <c r="H38" s="2"/>
     </row>
-    <row r="39" spans="1:8">
+    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A39" s="1"/>
       <c r="B39" s="2"/>
       <c r="E39" s="3"/>
@@ -3280,7 +3211,7 @@
       <c r="G39" s="2"/>
       <c r="H39" s="2"/>
     </row>
-    <row r="40" spans="1:8">
+    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A40" s="1"/>
       <c r="B40" s="2"/>
       <c r="E40" s="3"/>
@@ -3288,7 +3219,7 @@
       <c r="G40" s="2"/>
       <c r="H40" s="2"/>
     </row>
-    <row r="41" spans="1:8">
+    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A41" s="1"/>
       <c r="B41" s="2"/>
       <c r="E41" s="3"/>
@@ -3296,7 +3227,7 @@
       <c r="G41" s="2"/>
       <c r="H41" s="2"/>
     </row>
-    <row r="42" spans="1:8">
+    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A42" s="1"/>
       <c r="B42" s="2"/>
       <c r="E42" s="3"/>
@@ -3304,7 +3235,7 @@
       <c r="G42" s="2"/>
       <c r="H42" s="2"/>
     </row>
-    <row r="43" spans="1:8">
+    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A43" s="1"/>
       <c r="B43" s="2"/>
       <c r="E43" s="3"/>
@@ -3312,7 +3243,7 @@
       <c r="G43" s="2"/>
       <c r="H43" s="2"/>
     </row>
-    <row r="44" spans="1:8">
+    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A44" s="1"/>
       <c r="B44" s="2"/>
       <c r="E44" s="3"/>
@@ -3320,7 +3251,7 @@
       <c r="G44" s="2"/>
       <c r="H44" s="2"/>
     </row>
-    <row r="45" spans="1:8">
+    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A45" s="1"/>
       <c r="B45" s="2"/>
       <c r="E45" s="3"/>
@@ -3328,7 +3259,7 @@
       <c r="G45" s="2"/>
       <c r="H45" s="2"/>
     </row>
-    <row r="46" spans="1:8">
+    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A46" s="1"/>
       <c r="B46" s="2"/>
       <c r="E46" s="3"/>
@@ -3336,7 +3267,7 @@
       <c r="G46" s="2"/>
       <c r="H46" s="2"/>
     </row>
-    <row r="47" spans="1:8">
+    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A47" s="1"/>
       <c r="B47" s="2"/>
       <c r="E47" s="3"/>
@@ -3344,7 +3275,7 @@
       <c r="G47" s="2"/>
       <c r="H47" s="2"/>
     </row>
-    <row r="48" spans="1:8">
+    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A48" s="1"/>
       <c r="B48" s="2"/>
       <c r="E48" s="3"/>
@@ -3352,7 +3283,7 @@
       <c r="G48" s="2"/>
       <c r="H48" s="2"/>
     </row>
-    <row r="49" spans="1:8">
+    <row r="49" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A49" s="1"/>
       <c r="B49" s="2"/>
       <c r="E49" s="3"/>
@@ -3360,7 +3291,7 @@
       <c r="G49" s="2"/>
       <c r="H49" s="2"/>
     </row>
-    <row r="50" spans="1:8">
+    <row r="50" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A50" s="1"/>
       <c r="B50" s="2"/>
       <c r="E50" s="3"/>
@@ -3368,7 +3299,7 @@
       <c r="G50" s="2"/>
       <c r="H50" s="2"/>
     </row>
-    <row r="51" spans="1:8">
+    <row r="51" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A51" s="1"/>
       <c r="B51" s="2"/>
       <c r="E51" s="3"/>
@@ -3376,7 +3307,7 @@
       <c r="G51" s="2"/>
       <c r="H51" s="2"/>
     </row>
-    <row r="52" spans="1:8">
+    <row r="52" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A52" s="1"/>
       <c r="B52" s="2"/>
       <c r="E52" s="3"/>
@@ -3384,7 +3315,7 @@
       <c r="G52" s="2"/>
       <c r="H52" s="2"/>
     </row>
-    <row r="53" spans="1:8">
+    <row r="53" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A53" s="1"/>
       <c r="B53" s="2"/>
       <c r="E53" s="3"/>
@@ -3392,7 +3323,7 @@
       <c r="G53" s="2"/>
       <c r="H53" s="2"/>
     </row>
-    <row r="54" spans="1:8">
+    <row r="54" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A54" s="1"/>
       <c r="B54" s="2"/>
       <c r="E54" s="3"/>
@@ -3400,7 +3331,7 @@
       <c r="G54" s="2"/>
       <c r="H54" s="2"/>
     </row>
-    <row r="55" spans="1:8">
+    <row r="55" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A55" s="1"/>
       <c r="B55" s="2"/>
       <c r="E55" s="3"/>
@@ -3408,7 +3339,7 @@
       <c r="G55" s="2"/>
       <c r="H55" s="2"/>
     </row>
-    <row r="56" spans="1:8">
+    <row r="56" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A56" s="1"/>
       <c r="B56" s="2"/>
       <c r="E56" s="3"/>
@@ -3416,7 +3347,7 @@
       <c r="G56" s="2"/>
       <c r="H56" s="2"/>
     </row>
-    <row r="57" spans="1:8">
+    <row r="57" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A57" s="1"/>
       <c r="B57" s="2"/>
       <c r="E57" s="3"/>
@@ -3424,7 +3355,7 @@
       <c r="G57" s="2"/>
       <c r="H57" s="2"/>
     </row>
-    <row r="58" spans="1:8">
+    <row r="58" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A58" s="1"/>
       <c r="B58" s="2"/>
       <c r="E58" s="3"/>
@@ -3432,7 +3363,7 @@
       <c r="G58" s="2"/>
       <c r="H58" s="2"/>
     </row>
-    <row r="59" spans="1:8">
+    <row r="59" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A59" s="1"/>
       <c r="B59" s="2"/>
       <c r="E59" s="3"/>
@@ -3440,7 +3371,7 @@
       <c r="G59" s="2"/>
       <c r="H59" s="2"/>
     </row>
-    <row r="60" spans="1:8">
+    <row r="60" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A60" s="1"/>
       <c r="B60" s="2"/>
       <c r="E60" s="3"/>
@@ -3448,7 +3379,7 @@
       <c r="G60" s="2"/>
       <c r="H60" s="2"/>
     </row>
-    <row r="61" spans="1:8">
+    <row r="61" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A61" s="1"/>
       <c r="B61" s="2"/>
       <c r="E61" s="3"/>
@@ -3456,7 +3387,7 @@
       <c r="G61" s="2"/>
       <c r="H61" s="2"/>
     </row>
-    <row r="62" spans="1:8">
+    <row r="62" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A62" s="1"/>
       <c r="B62" s="2"/>
       <c r="E62" s="3"/>
@@ -3464,7 +3395,7 @@
       <c r="G62" s="2"/>
       <c r="H62" s="2"/>
     </row>
-    <row r="63" spans="1:8">
+    <row r="63" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A63" s="1"/>
       <c r="B63" s="2"/>
       <c r="E63" s="3"/>
@@ -3472,7 +3403,7 @@
       <c r="G63" s="2"/>
       <c r="H63" s="2"/>
     </row>
-    <row r="64" spans="1:8">
+    <row r="64" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A64" s="1"/>
       <c r="B64" s="2"/>
       <c r="E64" s="3"/>
@@ -3480,7 +3411,7 @@
       <c r="G64" s="2"/>
       <c r="H64" s="2"/>
     </row>
-    <row r="65" spans="1:8">
+    <row r="65" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A65" s="1"/>
       <c r="B65" s="2"/>
       <c r="E65" s="3"/>
@@ -3488,7 +3419,7 @@
       <c r="G65" s="2"/>
       <c r="H65" s="2"/>
     </row>
-    <row r="66" spans="1:8">
+    <row r="66" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A66" s="1"/>
       <c r="B66" s="2"/>
       <c r="E66" s="3"/>
@@ -3496,7 +3427,7 @@
       <c r="G66" s="2"/>
       <c r="H66" s="2"/>
     </row>
-    <row r="67" spans="1:8">
+    <row r="67" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A67" s="1"/>
       <c r="B67" s="2"/>
       <c r="E67" s="3"/>
@@ -3504,7 +3435,7 @@
       <c r="G67" s="2"/>
       <c r="H67" s="2"/>
     </row>
-    <row r="68" spans="1:8">
+    <row r="68" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A68" s="1"/>
       <c r="B68" s="2"/>
       <c r="E68" s="3"/>
@@ -3512,7 +3443,7 @@
       <c r="G68" s="2"/>
       <c r="H68" s="2"/>
     </row>
-    <row r="69" spans="1:8">
+    <row r="69" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A69" s="1"/>
       <c r="B69" s="2"/>
       <c r="E69" s="3"/>
@@ -3520,7 +3451,7 @@
       <c r="G69" s="2"/>
       <c r="H69" s="2"/>
     </row>
-    <row r="70" spans="1:8">
+    <row r="70" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A70" s="1"/>
       <c r="B70" s="2"/>
       <c r="E70" s="3"/>
@@ -3528,7 +3459,7 @@
       <c r="G70" s="2"/>
       <c r="H70" s="2"/>
     </row>
-    <row r="71" spans="1:8">
+    <row r="71" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A71" s="1"/>
       <c r="B71" s="2"/>
       <c r="E71" s="3"/>
@@ -3536,7 +3467,7 @@
       <c r="G71" s="2"/>
       <c r="H71" s="2"/>
     </row>
-    <row r="72" spans="1:8">
+    <row r="72" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A72" s="1"/>
       <c r="B72" s="2"/>
       <c r="E72" s="3"/>
@@ -3544,7 +3475,7 @@
       <c r="G72" s="2"/>
       <c r="H72" s="2"/>
     </row>
-    <row r="73" spans="1:8">
+    <row r="73" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A73" s="1"/>
       <c r="B73" s="2"/>
       <c r="E73" s="3"/>
@@ -3552,7 +3483,7 @@
       <c r="G73" s="2"/>
       <c r="H73" s="2"/>
     </row>
-    <row r="74" spans="1:8">
+    <row r="74" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A74" s="1"/>
       <c r="B74" s="2"/>
       <c r="E74" s="3"/>
@@ -3560,7 +3491,7 @@
       <c r="G74" s="2"/>
       <c r="H74" s="2"/>
     </row>
-    <row r="75" spans="1:8">
+    <row r="75" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A75" s="1"/>
       <c r="B75" s="2"/>
       <c r="E75" s="3"/>
@@ -3568,7 +3499,7 @@
       <c r="G75" s="2"/>
       <c r="H75" s="2"/>
     </row>
-    <row r="76" spans="1:8">
+    <row r="76" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A76" s="1"/>
       <c r="B76" s="2"/>
       <c r="E76" s="3"/>
@@ -3576,7 +3507,7 @@
       <c r="G76" s="2"/>
       <c r="H76" s="2"/>
     </row>
-    <row r="77" spans="1:8">
+    <row r="77" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A77" s="1"/>
       <c r="B77" s="2"/>
       <c r="E77" s="3"/>
@@ -3584,7 +3515,7 @@
       <c r="G77" s="2"/>
       <c r="H77" s="2"/>
     </row>
-    <row r="78" spans="1:8">
+    <row r="78" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A78" s="1"/>
       <c r="B78" s="2"/>
       <c r="E78" s="3"/>
@@ -3592,7 +3523,7 @@
       <c r="G78" s="2"/>
       <c r="H78" s="2"/>
     </row>
-    <row r="79" spans="1:8">
+    <row r="79" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A79" s="1"/>
       <c r="B79" s="2"/>
       <c r="E79" s="3"/>
@@ -3600,7 +3531,7 @@
       <c r="G79" s="2"/>
       <c r="H79" s="2"/>
     </row>
-    <row r="80" spans="1:8">
+    <row r="80" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A80" s="1"/>
       <c r="B80" s="2"/>
       <c r="E80" s="3"/>
@@ -3608,7 +3539,7 @@
       <c r="G80" s="2"/>
       <c r="H80" s="2"/>
     </row>
-    <row r="81" spans="1:8">
+    <row r="81" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A81" s="1"/>
       <c r="B81" s="2"/>
       <c r="E81" s="3"/>
@@ -3616,7 +3547,7 @@
       <c r="G81" s="2"/>
       <c r="H81" s="2"/>
     </row>
-    <row r="82" spans="1:8">
+    <row r="82" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A82" s="1"/>
       <c r="B82" s="2"/>
       <c r="E82" s="3"/>
@@ -3624,7 +3555,7 @@
       <c r="G82" s="2"/>
       <c r="H82" s="2"/>
     </row>
-    <row r="83" spans="1:8">
+    <row r="83" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A83" s="1"/>
       <c r="B83" s="2"/>
       <c r="E83" s="3"/>
@@ -3632,7 +3563,7 @@
       <c r="G83" s="2"/>
       <c r="H83" s="2"/>
     </row>
-    <row r="84" spans="1:8">
+    <row r="84" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A84" s="1"/>
       <c r="B84" s="2"/>
       <c r="E84" s="3"/>
@@ -3640,7 +3571,7 @@
       <c r="G84" s="2"/>
       <c r="H84" s="2"/>
     </row>
-    <row r="85" spans="1:8">
+    <row r="85" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A85" s="1"/>
       <c r="B85" s="2"/>
       <c r="E85" s="3"/>
@@ -3648,7 +3579,7 @@
       <c r="G85" s="2"/>
       <c r="H85" s="2"/>
     </row>
-    <row r="86" spans="1:8">
+    <row r="86" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A86" s="1"/>
       <c r="B86" s="2"/>
       <c r="E86" s="3"/>
@@ -3656,7 +3587,7 @@
       <c r="G86" s="2"/>
       <c r="H86" s="2"/>
     </row>
-    <row r="87" spans="1:8">
+    <row r="87" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A87" s="1"/>
       <c r="B87" s="2"/>
       <c r="E87" s="3"/>
@@ -3664,7 +3595,7 @@
       <c r="G87" s="2"/>
       <c r="H87" s="2"/>
     </row>
-    <row r="88" spans="1:8">
+    <row r="88" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A88" s="1"/>
       <c r="B88" s="2"/>
       <c r="E88" s="3"/>
@@ -3672,7 +3603,7 @@
       <c r="G88" s="2"/>
       <c r="H88" s="2"/>
     </row>
-    <row r="89" spans="1:8">
+    <row r="89" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A89" s="1"/>
       <c r="B89" s="2"/>
       <c r="E89" s="3"/>
@@ -3680,7 +3611,7 @@
       <c r="G89" s="2"/>
       <c r="H89" s="2"/>
     </row>
-    <row r="90" spans="1:8">
+    <row r="90" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A90" s="1"/>
       <c r="B90" s="2"/>
       <c r="E90" s="3"/>
@@ -3688,7 +3619,7 @@
       <c r="G90" s="2"/>
       <c r="H90" s="2"/>
     </row>
-    <row r="91" spans="1:8">
+    <row r="91" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A91" s="1"/>
       <c r="B91" s="2"/>
       <c r="E91" s="3"/>
@@ -3696,7 +3627,7 @@
       <c r="G91" s="2"/>
       <c r="H91" s="2"/>
     </row>
-    <row r="92" spans="1:8">
+    <row r="92" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A92" s="1"/>
       <c r="B92" s="2"/>
       <c r="E92" s="3"/>
@@ -3704,7 +3635,7 @@
       <c r="G92" s="2"/>
       <c r="H92" s="2"/>
     </row>
-    <row r="93" spans="1:8">
+    <row r="93" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A93" s="1"/>
       <c r="B93" s="2"/>
       <c r="E93" s="3"/>
@@ -3712,7 +3643,7 @@
       <c r="G93" s="2"/>
       <c r="H93" s="2"/>
     </row>
-    <row r="94" spans="1:8">
+    <row r="94" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A94" s="1"/>
       <c r="B94" s="2"/>
       <c r="E94" s="3"/>
@@ -3720,7 +3651,7 @@
       <c r="G94" s="2"/>
       <c r="H94" s="2"/>
     </row>
-    <row r="95" spans="1:8">
+    <row r="95" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A95" s="1"/>
       <c r="B95" s="2"/>
       <c r="E95" s="3"/>
@@ -3728,7 +3659,7 @@
       <c r="G95" s="2"/>
       <c r="H95" s="2"/>
     </row>
-    <row r="96" spans="1:8">
+    <row r="96" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A96" s="1"/>
       <c r="B96" s="2"/>
       <c r="E96" s="3"/>
@@ -3736,7 +3667,7 @@
       <c r="G96" s="2"/>
       <c r="H96" s="2"/>
     </row>
-    <row r="97" spans="1:8">
+    <row r="97" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A97" s="1"/>
       <c r="B97" s="2"/>
       <c r="E97" s="3"/>
@@ -3744,7 +3675,7 @@
       <c r="G97" s="2"/>
       <c r="H97" s="2"/>
     </row>
-    <row r="98" spans="1:8">
+    <row r="98" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A98" s="1"/>
       <c r="B98" s="2"/>
       <c r="E98" s="3"/>
@@ -3752,7 +3683,7 @@
       <c r="G98" s="2"/>
       <c r="H98" s="2"/>
     </row>
-    <row r="99" spans="1:8">
+    <row r="99" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A99" s="1"/>
       <c r="B99" s="2"/>
       <c r="E99" s="3"/>
@@ -3760,7 +3691,7 @@
       <c r="G99" s="2"/>
       <c r="H99" s="2"/>
     </row>
-    <row r="100" spans="1:8">
+    <row r="100" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A100" s="1"/>
       <c r="B100" s="2"/>
       <c r="E100" s="3"/>
@@ -3803,21 +3734,21 @@
       <selection activeCell="P21" sqref="P21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.08203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.9140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.9140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="19.4140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.58203125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.58203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.5703125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="9" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="17.9140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="17.85546875" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="17" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="19.08203125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="19.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="15.5">
+    <row r="1" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="7" t="s">
         <v>8</v>
       </c>
@@ -3849,7 +3780,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:10">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="2"/>
       <c r="B2" s="8"/>
       <c r="D2" s="2"/>
@@ -3857,7 +3788,7 @@
       <c r="I2" s="8"/>
       <c r="J2" s="2"/>
     </row>
-    <row r="3" spans="1:10">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="2"/>
       <c r="B3" s="8"/>
       <c r="D3" s="2"/>
@@ -3865,7 +3796,7 @@
       <c r="I3" s="8"/>
       <c r="J3" s="2"/>
     </row>
-    <row r="4" spans="1:10">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="2"/>
       <c r="B4" s="8"/>
       <c r="D4" s="2"/>
@@ -3873,7 +3804,7 @@
       <c r="I4" s="8"/>
       <c r="J4" s="2"/>
     </row>
-    <row r="5" spans="1:10">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" s="2"/>
       <c r="B5" s="8"/>
       <c r="D5" s="2"/>
@@ -3881,7 +3812,7 @@
       <c r="I5" s="8"/>
       <c r="J5" s="2"/>
     </row>
-    <row r="6" spans="1:10">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" s="2"/>
       <c r="B6" s="8"/>
       <c r="D6" s="2"/>
@@ -3889,7 +3820,7 @@
       <c r="I6" s="8"/>
       <c r="J6" s="2"/>
     </row>
-    <row r="7" spans="1:10">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" s="2"/>
       <c r="B7" s="8"/>
       <c r="D7" s="2"/>
@@ -3897,7 +3828,7 @@
       <c r="I7" s="8"/>
       <c r="J7" s="2"/>
     </row>
-    <row r="8" spans="1:10">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" s="2"/>
       <c r="B8" s="8"/>
       <c r="D8" s="2"/>
@@ -3905,7 +3836,7 @@
       <c r="I8" s="8"/>
       <c r="J8" s="2"/>
     </row>
-    <row r="9" spans="1:10">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" s="2"/>
       <c r="B9" s="8"/>
       <c r="D9" s="2"/>
@@ -3913,7 +3844,7 @@
       <c r="I9" s="8"/>
       <c r="J9" s="2"/>
     </row>
-    <row r="10" spans="1:10">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" s="2"/>
       <c r="B10" s="8"/>
       <c r="D10" s="2"/>
@@ -3921,7 +3852,7 @@
       <c r="I10" s="8"/>
       <c r="J10" s="2"/>
     </row>
-    <row r="11" spans="1:10">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" s="2"/>
       <c r="B11" s="8"/>
       <c r="D11" s="2"/>
@@ -3929,7 +3860,7 @@
       <c r="I11" s="8"/>
       <c r="J11" s="2"/>
     </row>
-    <row r="12" spans="1:10">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" s="2"/>
       <c r="B12" s="8"/>
       <c r="D12" s="2"/>
@@ -3937,7 +3868,7 @@
       <c r="I12" s="8"/>
       <c r="J12" s="2"/>
     </row>
-    <row r="13" spans="1:10">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" s="2"/>
       <c r="B13" s="8"/>
       <c r="D13" s="2"/>
@@ -3945,7 +3876,7 @@
       <c r="I13" s="8"/>
       <c r="J13" s="2"/>
     </row>
-    <row r="14" spans="1:10">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" s="2"/>
       <c r="B14" s="8"/>
       <c r="D14" s="2"/>
@@ -3953,7 +3884,7 @@
       <c r="I14" s="8"/>
       <c r="J14" s="2"/>
     </row>
-    <row r="15" spans="1:10">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" s="2"/>
       <c r="B15" s="8"/>
       <c r="D15" s="2"/>
@@ -3961,7 +3892,7 @@
       <c r="I15" s="8"/>
       <c r="J15" s="2"/>
     </row>
-    <row r="16" spans="1:10">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" s="2"/>
       <c r="B16" s="8"/>
       <c r="D16" s="2"/>
@@ -3969,7 +3900,7 @@
       <c r="I16" s="8"/>
       <c r="J16" s="2"/>
     </row>
-    <row r="17" spans="1:10">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17" s="2"/>
       <c r="B17" s="8"/>
       <c r="D17" s="2"/>
@@ -3977,7 +3908,7 @@
       <c r="I17" s="8"/>
       <c r="J17" s="2"/>
     </row>
-    <row r="18" spans="1:10">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18" s="2"/>
       <c r="B18" s="8"/>
       <c r="D18" s="2"/>
@@ -3985,7 +3916,7 @@
       <c r="I18" s="8"/>
       <c r="J18" s="2"/>
     </row>
-    <row r="19" spans="1:10">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A19" s="2"/>
       <c r="B19" s="8"/>
       <c r="D19" s="2"/>
@@ -3993,7 +3924,7 @@
       <c r="I19" s="8"/>
       <c r="J19" s="2"/>
     </row>
-    <row r="20" spans="1:10">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A20" s="2"/>
       <c r="B20" s="8"/>
       <c r="D20" s="2"/>
@@ -4001,7 +3932,7 @@
       <c r="I20" s="8"/>
       <c r="J20" s="2"/>
     </row>
-    <row r="21" spans="1:10">
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A21" s="2"/>
       <c r="B21" s="8"/>
       <c r="D21" s="2"/>
@@ -4009,7 +3940,7 @@
       <c r="I21" s="8"/>
       <c r="J21" s="2"/>
     </row>
-    <row r="22" spans="1:10">
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A22" s="2"/>
       <c r="B22" s="8"/>
       <c r="D22" s="2"/>
@@ -4017,7 +3948,7 @@
       <c r="I22" s="8"/>
       <c r="J22" s="2"/>
     </row>
-    <row r="23" spans="1:10">
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A23" s="2"/>
       <c r="B23" s="8"/>
       <c r="D23" s="2"/>
@@ -4025,7 +3956,7 @@
       <c r="I23" s="8"/>
       <c r="J23" s="2"/>
     </row>
-    <row r="24" spans="1:10">
+    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A24" s="2"/>
       <c r="B24" s="8"/>
       <c r="D24" s="2"/>
@@ -4033,7 +3964,7 @@
       <c r="I24" s="8"/>
       <c r="J24" s="2"/>
     </row>
-    <row r="25" spans="1:10">
+    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A25" s="2"/>
       <c r="B25" s="8"/>
       <c r="D25" s="2"/>
@@ -4041,7 +3972,7 @@
       <c r="I25" s="8"/>
       <c r="J25" s="2"/>
     </row>
-    <row r="26" spans="1:10">
+    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A26" s="2"/>
       <c r="B26" s="8"/>
       <c r="D26" s="2"/>
@@ -4049,7 +3980,7 @@
       <c r="I26" s="8"/>
       <c r="J26" s="2"/>
     </row>
-    <row r="27" spans="1:10">
+    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A27" s="2"/>
       <c r="B27" s="8"/>
       <c r="D27" s="2"/>
@@ -4057,7 +3988,7 @@
       <c r="I27" s="8"/>
       <c r="J27" s="2"/>
     </row>
-    <row r="28" spans="1:10">
+    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A28" s="2"/>
       <c r="B28" s="8"/>
       <c r="D28" s="2"/>
@@ -4065,7 +3996,7 @@
       <c r="I28" s="8"/>
       <c r="J28" s="2"/>
     </row>
-    <row r="29" spans="1:10">
+    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A29" s="2"/>
       <c r="B29" s="8"/>
       <c r="D29" s="2"/>
@@ -4073,7 +4004,7 @@
       <c r="I29" s="8"/>
       <c r="J29" s="2"/>
     </row>
-    <row r="30" spans="1:10">
+    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A30" s="2"/>
       <c r="B30" s="8"/>
       <c r="D30" s="2"/>
@@ -4081,7 +4012,7 @@
       <c r="I30" s="8"/>
       <c r="J30" s="2"/>
     </row>
-    <row r="31" spans="1:10">
+    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A31" s="2"/>
       <c r="B31" s="8"/>
       <c r="D31" s="2"/>
@@ -4089,7 +4020,7 @@
       <c r="I31" s="8"/>
       <c r="J31" s="2"/>
     </row>
-    <row r="32" spans="1:10">
+    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A32" s="2"/>
       <c r="B32" s="8"/>
       <c r="D32" s="2"/>
@@ -4097,7 +4028,7 @@
       <c r="I32" s="8"/>
       <c r="J32" s="2"/>
     </row>
-    <row r="33" spans="1:10">
+    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A33" s="2"/>
       <c r="B33" s="8"/>
       <c r="D33" s="2"/>
@@ -4105,7 +4036,7 @@
       <c r="I33" s="8"/>
       <c r="J33" s="2"/>
     </row>
-    <row r="34" spans="1:10">
+    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A34" s="2"/>
       <c r="B34" s="8"/>
       <c r="D34" s="2"/>
@@ -4113,7 +4044,7 @@
       <c r="I34" s="8"/>
       <c r="J34" s="2"/>
     </row>
-    <row r="35" spans="1:10">
+    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A35" s="2"/>
       <c r="B35" s="8"/>
       <c r="D35" s="2"/>
@@ -4121,7 +4052,7 @@
       <c r="I35" s="8"/>
       <c r="J35" s="2"/>
     </row>
-    <row r="36" spans="1:10">
+    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A36" s="2"/>
       <c r="B36" s="8"/>
       <c r="D36" s="2"/>
@@ -4129,7 +4060,7 @@
       <c r="I36" s="8"/>
       <c r="J36" s="2"/>
     </row>
-    <row r="37" spans="1:10">
+    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A37" s="2"/>
       <c r="B37" s="8"/>
       <c r="D37" s="2"/>
@@ -4137,7 +4068,7 @@
       <c r="I37" s="8"/>
       <c r="J37" s="2"/>
     </row>
-    <row r="38" spans="1:10">
+    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A38" s="2"/>
       <c r="B38" s="8"/>
       <c r="D38" s="2"/>
@@ -4145,7 +4076,7 @@
       <c r="I38" s="8"/>
       <c r="J38" s="2"/>
     </row>
-    <row r="39" spans="1:10">
+    <row r="39" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A39" s="2"/>
       <c r="B39" s="8"/>
       <c r="D39" s="2"/>
@@ -4153,7 +4084,7 @@
       <c r="I39" s="8"/>
       <c r="J39" s="2"/>
     </row>
-    <row r="40" spans="1:10">
+    <row r="40" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A40" s="2"/>
       <c r="B40" s="8"/>
       <c r="D40" s="2"/>
@@ -4161,7 +4092,7 @@
       <c r="I40" s="8"/>
       <c r="J40" s="2"/>
     </row>
-    <row r="41" spans="1:10">
+    <row r="41" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A41" s="2"/>
       <c r="B41" s="8"/>
       <c r="D41" s="2"/>
@@ -4169,7 +4100,7 @@
       <c r="I41" s="8"/>
       <c r="J41" s="2"/>
     </row>
-    <row r="42" spans="1:10">
+    <row r="42" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A42" s="2"/>
       <c r="B42" s="8"/>
       <c r="D42" s="2"/>
@@ -4177,7 +4108,7 @@
       <c r="I42" s="8"/>
       <c r="J42" s="2"/>
     </row>
-    <row r="43" spans="1:10">
+    <row r="43" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A43" s="2"/>
       <c r="B43" s="8"/>
       <c r="D43" s="2"/>
@@ -4185,7 +4116,7 @@
       <c r="I43" s="8"/>
       <c r="J43" s="2"/>
     </row>
-    <row r="44" spans="1:10">
+    <row r="44" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A44" s="2"/>
       <c r="B44" s="8"/>
       <c r="D44" s="2"/>
@@ -4193,7 +4124,7 @@
       <c r="I44" s="8"/>
       <c r="J44" s="2"/>
     </row>
-    <row r="45" spans="1:10">
+    <row r="45" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A45" s="2"/>
       <c r="B45" s="8"/>
       <c r="D45" s="2"/>
@@ -4201,7 +4132,7 @@
       <c r="I45" s="8"/>
       <c r="J45" s="2"/>
     </row>
-    <row r="46" spans="1:10">
+    <row r="46" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A46" s="2"/>
       <c r="B46" s="8"/>
       <c r="D46" s="2"/>
@@ -4209,7 +4140,7 @@
       <c r="I46" s="8"/>
       <c r="J46" s="2"/>
     </row>
-    <row r="47" spans="1:10">
+    <row r="47" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A47" s="2"/>
       <c r="B47" s="8"/>
       <c r="D47" s="2"/>
@@ -4217,7 +4148,7 @@
       <c r="I47" s="8"/>
       <c r="J47" s="2"/>
     </row>
-    <row r="48" spans="1:10">
+    <row r="48" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A48" s="2"/>
       <c r="B48" s="8"/>
       <c r="D48" s="2"/>
@@ -4225,7 +4156,7 @@
       <c r="I48" s="8"/>
       <c r="J48" s="2"/>
     </row>
-    <row r="49" spans="1:10">
+    <row r="49" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A49" s="2"/>
       <c r="B49" s="8"/>
       <c r="D49" s="2"/>
@@ -4233,7 +4164,7 @@
       <c r="I49" s="8"/>
       <c r="J49" s="2"/>
     </row>
-    <row r="50" spans="1:10">
+    <row r="50" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A50" s="2"/>
       <c r="B50" s="8"/>
       <c r="D50" s="2"/>
@@ -4241,7 +4172,7 @@
       <c r="I50" s="8"/>
       <c r="J50" s="2"/>
     </row>
-    <row r="51" spans="1:10">
+    <row r="51" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A51" s="2"/>
       <c r="B51" s="8"/>
       <c r="D51" s="2"/>
@@ -4249,7 +4180,7 @@
       <c r="I51" s="8"/>
       <c r="J51" s="2"/>
     </row>
-    <row r="52" spans="1:10">
+    <row r="52" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A52" s="2"/>
       <c r="B52" s="8"/>
       <c r="D52" s="2"/>
@@ -4257,7 +4188,7 @@
       <c r="I52" s="8"/>
       <c r="J52" s="2"/>
     </row>
-    <row r="53" spans="1:10">
+    <row r="53" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A53" s="2"/>
       <c r="B53" s="8"/>
       <c r="D53" s="2"/>
@@ -4265,7 +4196,7 @@
       <c r="I53" s="8"/>
       <c r="J53" s="2"/>
     </row>
-    <row r="54" spans="1:10">
+    <row r="54" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A54" s="2"/>
       <c r="B54" s="8"/>
       <c r="D54" s="2"/>
@@ -4273,7 +4204,7 @@
       <c r="I54" s="8"/>
       <c r="J54" s="2"/>
     </row>
-    <row r="55" spans="1:10">
+    <row r="55" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A55" s="2"/>
       <c r="B55" s="8"/>
       <c r="D55" s="2"/>
@@ -4281,7 +4212,7 @@
       <c r="I55" s="8"/>
       <c r="J55" s="2"/>
     </row>
-    <row r="56" spans="1:10">
+    <row r="56" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A56" s="2"/>
       <c r="B56" s="8"/>
       <c r="D56" s="2"/>
@@ -4289,7 +4220,7 @@
       <c r="I56" s="8"/>
       <c r="J56" s="2"/>
     </row>
-    <row r="57" spans="1:10">
+    <row r="57" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A57" s="2"/>
       <c r="B57" s="8"/>
       <c r="D57" s="2"/>
@@ -4297,7 +4228,7 @@
       <c r="I57" s="8"/>
       <c r="J57" s="2"/>
     </row>
-    <row r="58" spans="1:10">
+    <row r="58" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A58" s="2"/>
       <c r="B58" s="8"/>
       <c r="D58" s="2"/>
@@ -4305,7 +4236,7 @@
       <c r="I58" s="8"/>
       <c r="J58" s="2"/>
     </row>
-    <row r="59" spans="1:10">
+    <row r="59" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A59" s="2"/>
       <c r="B59" s="8"/>
       <c r="D59" s="2"/>
@@ -4313,7 +4244,7 @@
       <c r="I59" s="8"/>
       <c r="J59" s="2"/>
     </row>
-    <row r="60" spans="1:10">
+    <row r="60" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A60" s="2"/>
       <c r="B60" s="8"/>
       <c r="D60" s="2"/>
@@ -4321,7 +4252,7 @@
       <c r="I60" s="8"/>
       <c r="J60" s="2"/>
     </row>
-    <row r="61" spans="1:10">
+    <row r="61" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A61" s="2"/>
       <c r="B61" s="8"/>
       <c r="D61" s="2"/>
@@ -4329,7 +4260,7 @@
       <c r="I61" s="8"/>
       <c r="J61" s="2"/>
     </row>
-    <row r="62" spans="1:10">
+    <row r="62" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A62" s="2"/>
       <c r="B62" s="8"/>
       <c r="D62" s="2"/>
@@ -4337,7 +4268,7 @@
       <c r="I62" s="8"/>
       <c r="J62" s="2"/>
     </row>
-    <row r="63" spans="1:10">
+    <row r="63" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A63" s="2"/>
       <c r="B63" s="8"/>
       <c r="D63" s="2"/>
@@ -4345,7 +4276,7 @@
       <c r="I63" s="8"/>
       <c r="J63" s="2"/>
     </row>
-    <row r="64" spans="1:10">
+    <row r="64" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A64" s="2"/>
       <c r="B64" s="8"/>
       <c r="D64" s="2"/>
@@ -4353,7 +4284,7 @@
       <c r="I64" s="8"/>
       <c r="J64" s="2"/>
     </row>
-    <row r="65" spans="1:10">
+    <row r="65" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A65" s="2"/>
       <c r="B65" s="8"/>
       <c r="D65" s="2"/>
@@ -4361,7 +4292,7 @@
       <c r="I65" s="8"/>
       <c r="J65" s="2"/>
     </row>
-    <row r="66" spans="1:10">
+    <row r="66" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A66" s="2"/>
       <c r="B66" s="8"/>
       <c r="D66" s="2"/>
@@ -4369,7 +4300,7 @@
       <c r="I66" s="8"/>
       <c r="J66" s="2"/>
     </row>
-    <row r="67" spans="1:10">
+    <row r="67" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A67" s="2"/>
       <c r="B67" s="8"/>
       <c r="D67" s="2"/>
@@ -4377,7 +4308,7 @@
       <c r="I67" s="8"/>
       <c r="J67" s="2"/>
     </row>
-    <row r="68" spans="1:10">
+    <row r="68" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A68" s="2"/>
       <c r="B68" s="8"/>
       <c r="D68" s="2"/>
@@ -4385,7 +4316,7 @@
       <c r="I68" s="8"/>
       <c r="J68" s="2"/>
     </row>
-    <row r="69" spans="1:10">
+    <row r="69" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A69" s="2"/>
       <c r="B69" s="8"/>
       <c r="D69" s="2"/>
@@ -4393,7 +4324,7 @@
       <c r="I69" s="8"/>
       <c r="J69" s="2"/>
     </row>
-    <row r="70" spans="1:10">
+    <row r="70" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A70" s="2"/>
       <c r="B70" s="8"/>
       <c r="D70" s="2"/>
@@ -4401,7 +4332,7 @@
       <c r="I70" s="8"/>
       <c r="J70" s="2"/>
     </row>
-    <row r="71" spans="1:10">
+    <row r="71" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A71" s="2"/>
       <c r="B71" s="8"/>
       <c r="D71" s="2"/>
@@ -4409,7 +4340,7 @@
       <c r="I71" s="8"/>
       <c r="J71" s="2"/>
     </row>
-    <row r="72" spans="1:10">
+    <row r="72" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A72" s="2"/>
       <c r="B72" s="8"/>
       <c r="D72" s="2"/>
@@ -4417,7 +4348,7 @@
       <c r="I72" s="8"/>
       <c r="J72" s="2"/>
     </row>
-    <row r="73" spans="1:10">
+    <row r="73" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A73" s="2"/>
       <c r="B73" s="8"/>
       <c r="D73" s="2"/>
@@ -4425,7 +4356,7 @@
       <c r="I73" s="8"/>
       <c r="J73" s="2"/>
     </row>
-    <row r="74" spans="1:10">
+    <row r="74" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A74" s="2"/>
       <c r="B74" s="8"/>
       <c r="D74" s="2"/>
@@ -4433,7 +4364,7 @@
       <c r="I74" s="8"/>
       <c r="J74" s="2"/>
     </row>
-    <row r="75" spans="1:10">
+    <row r="75" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A75" s="2"/>
       <c r="B75" s="8"/>
       <c r="D75" s="2"/>
@@ -4441,7 +4372,7 @@
       <c r="I75" s="8"/>
       <c r="J75" s="2"/>
     </row>
-    <row r="76" spans="1:10">
+    <row r="76" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A76" s="2"/>
       <c r="B76" s="8"/>
       <c r="D76" s="2"/>
@@ -4449,7 +4380,7 @@
       <c r="I76" s="8"/>
       <c r="J76" s="2"/>
     </row>
-    <row r="77" spans="1:10">
+    <row r="77" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A77" s="2"/>
       <c r="B77" s="8"/>
       <c r="D77" s="2"/>
@@ -4457,7 +4388,7 @@
       <c r="I77" s="8"/>
       <c r="J77" s="2"/>
     </row>
-    <row r="78" spans="1:10">
+    <row r="78" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A78" s="2"/>
       <c r="B78" s="8"/>
       <c r="D78" s="2"/>
@@ -4465,7 +4396,7 @@
       <c r="I78" s="8"/>
       <c r="J78" s="2"/>
     </row>
-    <row r="79" spans="1:10">
+    <row r="79" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A79" s="2"/>
       <c r="B79" s="8"/>
       <c r="D79" s="2"/>
@@ -4473,7 +4404,7 @@
       <c r="I79" s="8"/>
       <c r="J79" s="2"/>
     </row>
-    <row r="80" spans="1:10">
+    <row r="80" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A80" s="2"/>
       <c r="B80" s="8"/>
       <c r="D80" s="2"/>
@@ -4481,7 +4412,7 @@
       <c r="I80" s="8"/>
       <c r="J80" s="2"/>
     </row>
-    <row r="81" spans="1:10">
+    <row r="81" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A81" s="2"/>
       <c r="B81" s="8"/>
       <c r="D81" s="2"/>
@@ -4489,7 +4420,7 @@
       <c r="I81" s="8"/>
       <c r="J81" s="2"/>
     </row>
-    <row r="82" spans="1:10">
+    <row r="82" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A82" s="2"/>
       <c r="B82" s="8"/>
       <c r="D82" s="2"/>
@@ -4497,7 +4428,7 @@
       <c r="I82" s="8"/>
       <c r="J82" s="2"/>
     </row>
-    <row r="83" spans="1:10">
+    <row r="83" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A83" s="2"/>
       <c r="B83" s="8"/>
       <c r="D83" s="2"/>
@@ -4505,7 +4436,7 @@
       <c r="I83" s="8"/>
       <c r="J83" s="2"/>
     </row>
-    <row r="84" spans="1:10">
+    <row r="84" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A84" s="2"/>
       <c r="B84" s="8"/>
       <c r="D84" s="2"/>
@@ -4513,7 +4444,7 @@
       <c r="I84" s="8"/>
       <c r="J84" s="2"/>
     </row>
-    <row r="85" spans="1:10">
+    <row r="85" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A85" s="2"/>
       <c r="B85" s="8"/>
       <c r="D85" s="2"/>
@@ -4521,7 +4452,7 @@
       <c r="I85" s="8"/>
       <c r="J85" s="2"/>
     </row>
-    <row r="86" spans="1:10">
+    <row r="86" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A86" s="2"/>
       <c r="B86" s="8"/>
       <c r="D86" s="2"/>
@@ -4529,7 +4460,7 @@
       <c r="I86" s="8"/>
       <c r="J86" s="2"/>
     </row>
-    <row r="87" spans="1:10">
+    <row r="87" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A87" s="2"/>
       <c r="B87" s="8"/>
       <c r="D87" s="2"/>
@@ -4537,7 +4468,7 @@
       <c r="I87" s="8"/>
       <c r="J87" s="2"/>
     </row>
-    <row r="88" spans="1:10">
+    <row r="88" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A88" s="2"/>
       <c r="B88" s="8"/>
       <c r="D88" s="2"/>
@@ -4545,7 +4476,7 @@
       <c r="I88" s="8"/>
       <c r="J88" s="2"/>
     </row>
-    <row r="89" spans="1:10">
+    <row r="89" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A89" s="2"/>
       <c r="B89" s="8"/>
       <c r="D89" s="2"/>
@@ -4553,7 +4484,7 @@
       <c r="I89" s="8"/>
       <c r="J89" s="2"/>
     </row>
-    <row r="90" spans="1:10">
+    <row r="90" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A90" s="2"/>
       <c r="B90" s="8"/>
       <c r="D90" s="2"/>
@@ -4561,7 +4492,7 @@
       <c r="I90" s="8"/>
       <c r="J90" s="2"/>
     </row>
-    <row r="91" spans="1:10">
+    <row r="91" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A91" s="2"/>
       <c r="B91" s="8"/>
       <c r="D91" s="2"/>
@@ -4569,7 +4500,7 @@
       <c r="I91" s="8"/>
       <c r="J91" s="2"/>
     </row>
-    <row r="92" spans="1:10">
+    <row r="92" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A92" s="2"/>
       <c r="B92" s="8"/>
       <c r="D92" s="2"/>
@@ -4577,7 +4508,7 @@
       <c r="I92" s="8"/>
       <c r="J92" s="2"/>
     </row>
-    <row r="93" spans="1:10">
+    <row r="93" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A93" s="2"/>
       <c r="B93" s="8"/>
       <c r="D93" s="2"/>
@@ -4585,7 +4516,7 @@
       <c r="I93" s="8"/>
       <c r="J93" s="2"/>
     </row>
-    <row r="94" spans="1:10">
+    <row r="94" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A94" s="2"/>
       <c r="B94" s="8"/>
       <c r="D94" s="2"/>
@@ -4593,7 +4524,7 @@
       <c r="I94" s="8"/>
       <c r="J94" s="2"/>
     </row>
-    <row r="95" spans="1:10">
+    <row r="95" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A95" s="2"/>
       <c r="B95" s="8"/>
       <c r="D95" s="2"/>
@@ -4601,7 +4532,7 @@
       <c r="I95" s="8"/>
       <c r="J95" s="2"/>
     </row>
-    <row r="96" spans="1:10">
+    <row r="96" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A96" s="2"/>
       <c r="B96" s="8"/>
       <c r="D96" s="2"/>
@@ -4609,7 +4540,7 @@
       <c r="I96" s="8"/>
       <c r="J96" s="2"/>
     </row>
-    <row r="97" spans="1:10">
+    <row r="97" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A97" s="2"/>
       <c r="B97" s="8"/>
       <c r="D97" s="2"/>
@@ -4617,7 +4548,7 @@
       <c r="I97" s="8"/>
       <c r="J97" s="2"/>
     </row>
-    <row r="98" spans="1:10">
+    <row r="98" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A98" s="2"/>
       <c r="B98" s="8"/>
       <c r="D98" s="2"/>
@@ -4625,7 +4556,7 @@
       <c r="I98" s="8"/>
       <c r="J98" s="2"/>
     </row>
-    <row r="99" spans="1:10">
+    <row r="99" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A99" s="2"/>
       <c r="B99" s="8"/>
       <c r="D99" s="2"/>
@@ -4633,7 +4564,7 @@
       <c r="I99" s="8"/>
       <c r="J99" s="2"/>
     </row>
-    <row r="100" spans="1:10">
+    <row r="100" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A100" s="2"/>
       <c r="B100" s="8"/>
       <c r="D100" s="2"/>

</xml_diff>

<commit_message>
Updated progress report for May 13 Tue by Avichal
</commit_message>
<xml_diff>
--- a/PR&IR.xlsx
+++ b/PR&IR.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\avichal avneel nath\Documents\Semester 7\CS415\A3\CS415_A3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29E4A58F-3349-45EB-9D46-A150A4875504}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C2150F46-1E77-4BD6-9AB2-4FBCA6C7B7F4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{BFA1E21A-08FA-4F02-8C25-33C81C8EE970}"/>
   </bookViews>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="33">
   <si>
     <t>Date</t>
   </si>
@@ -140,6 +140,18 @@
   <si>
     <t>complete pending ToDos</t>
   </si>
+  <si>
+    <t>13/0/2025</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Resolved merge conflict and synced with main. Researched on sqlalchemy vs pyodbc. Custom validation for enrollment services. </t>
+  </si>
+  <si>
+    <t>Exception handling for all routes and research on DB</t>
+  </si>
+  <si>
+    <t>Best Wishes w/ Backend.</t>
+  </si>
 </sst>
 </file>
 
@@ -190,7 +202,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -203,7 +215,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -885,7 +896,7 @@
   <dimension ref="A1:H28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+      <selection activeCell="H6" sqref="H6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -969,7 +980,7 @@
       <c r="D3" t="s">
         <v>17</v>
       </c>
-      <c r="E3" s="10">
+      <c r="E3">
         <v>100</v>
       </c>
       <c r="F3">
@@ -992,7 +1003,7 @@
       <c r="D4" t="s">
         <v>17</v>
       </c>
-      <c r="E4" s="10">
+      <c r="E4">
         <v>90</v>
       </c>
       <c r="F4">
@@ -1012,7 +1023,7 @@
       <c r="D5" t="s">
         <v>17</v>
       </c>
-      <c r="E5" s="10">
+      <c r="E5">
         <v>100</v>
       </c>
       <c r="F5">
@@ -1026,47 +1037,66 @@
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="E6" s="10"/>
-      <c r="F6"/>
+      <c r="A6" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C6" t="s">
+        <v>30</v>
+      </c>
+      <c r="D6" t="s">
+        <v>17</v>
+      </c>
+      <c r="E6">
+        <v>100</v>
+      </c>
+      <c r="F6">
+        <v>5</v>
+      </c>
+      <c r="G6" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="H6" s="2" t="s">
+        <v>32</v>
+      </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="E7" s="10"/>
+      <c r="E7"/>
       <c r="F7"/>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="E8" s="10"/>
+      <c r="E8"/>
       <c r="F8"/>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="E9" s="10"/>
+      <c r="E9"/>
       <c r="F9"/>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="E10" s="10"/>
+      <c r="E10"/>
       <c r="F10"/>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="E11" s="10"/>
+      <c r="E11"/>
       <c r="F11"/>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="E12" s="10"/>
+      <c r="E12"/>
       <c r="F12"/>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="E13" s="10"/>
+      <c r="E13"/>
       <c r="F13"/>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="E14" s="10"/>
+      <c r="E14"/>
       <c r="F14"/>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="E15" s="10"/>
+      <c r="E15"/>
       <c r="F15"/>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="E16" s="10"/>
+      <c r="E16"/>
       <c r="F16"/>
     </row>
     <row r="17" spans="6:6" x14ac:dyDescent="0.25">
@@ -1125,7 +1155,7 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
   <ignoredErrors>
-    <ignoredError sqref="D7:D16 D6" listDataValidation="1"/>
+    <ignoredError sqref="D7:D16" listDataValidation="1"/>
   </ignoredErrors>
   <tableParts count="1">
     <tablePart r:id="rId2"/>

</xml_diff>

<commit_message>
Add/update progress report for 13/05/2025 Tue by Shivya
</commit_message>
<xml_diff>
--- a/PR&IR.xlsx
+++ b/PR&IR.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26026"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\avichal avneel nath\Documents\Semester 7\CS415\A3\CS415_A3\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SHIVYA KUMAR\Desktop\new415\CS415_A3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C2150F46-1E77-4BD6-9AB2-4FBCA6C7B7F4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FCBE4524-C6CA-4495-B5C8-C5EC464FB1CD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{BFA1E21A-08FA-4F02-8C25-33C81C8EE970}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{BFA1E21A-08FA-4F02-8C25-33C81C8EE970}"/>
   </bookViews>
   <sheets>
     <sheet name="Avichal" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="46">
   <si>
     <t>Date</t>
   </si>
@@ -152,6 +152,45 @@
   <si>
     <t>Best Wishes w/ Backend.</t>
   </si>
+  <si>
+    <t>Shivya Kumar</t>
+  </si>
+  <si>
+    <t>Convert UI for login, homepage and student profile</t>
+  </si>
+  <si>
+    <t>In Progress</t>
+  </si>
+  <si>
+    <t>Continue converting UI and setting route</t>
+  </si>
+  <si>
+    <t>I was unable to run the app locally, so I created a folder named run_main_app.py with the required code Once I did that I was able to start the Flask server successfully</t>
+  </si>
+  <si>
+    <t>Added header and footer to the remaining UIs, and converted UI for enrollment page.</t>
+  </si>
+  <si>
+    <t>Solve my routes and fix UI</t>
+  </si>
+  <si>
+    <t>Customizing UI and recovered deleted codes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Continue converting UI </t>
+  </si>
+  <si>
+    <t>I added my routes in the same file app.py</t>
+  </si>
+  <si>
+    <t>shivya Kumar</t>
+  </si>
+  <si>
+    <t>continue implementing remaining UI logic based on feedback and custom validation with exception handling for all of her routes</t>
+  </si>
+  <si>
+    <t>Converted all user interface designs into HTML and set up respective routes.</t>
+  </si>
 </sst>
 </file>
 
@@ -161,7 +200,7 @@
     <numFmt numFmtId="164" formatCode="h"/>
     <numFmt numFmtId="165" formatCode="d/mm/yyyy;@"/>
   </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="3">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -202,7 +241,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -215,11 +254,22 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="35">
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
     <dxf>
       <numFmt numFmtId="30" formatCode="@"/>
     </dxf>
@@ -330,15 +380,6 @@
     </dxf>
     <dxf>
       <numFmt numFmtId="30" formatCode="@"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="164" formatCode="h"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="14" formatCode="0.00%"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="30" formatCode="@"/>
@@ -456,17 +497,17 @@
     <tableColumn id="2" xr3:uid="{55A78D6C-890A-4502-A184-DEEFF14BB82E}" name="Member Name" dataDxfId="25"/>
     <tableColumn id="3" xr3:uid="{57B9A516-E930-4C06-A589-24182A37BA85}" name="Task/Activity"/>
     <tableColumn id="4" xr3:uid="{A7CD18E8-808E-43EA-A960-7EDF2D2AB452}" name="Status"/>
-    <tableColumn id="5" xr3:uid="{A9BAB96D-D5FD-4C0D-A277-6E052D27EC3A}" name="% Complete" dataDxfId="24"/>
-    <tableColumn id="6" xr3:uid="{4EBDEBD4-A02D-4266-88BC-5E6088167CE4}" name="Hours Worked Today" dataDxfId="23"/>
-    <tableColumn id="7" xr3:uid="{88484166-6833-4A6B-B292-081E908E7876}" name="Next Steps" dataDxfId="22"/>
-    <tableColumn id="8" xr3:uid="{65034E84-46C0-4115-A351-A3C28C7B9EE1}" name="Notes/Comments" dataDxfId="21"/>
+    <tableColumn id="5" xr3:uid="{A9BAB96D-D5FD-4C0D-A277-6E052D27EC3A}" name="% Complete" dataDxfId="2"/>
+    <tableColumn id="6" xr3:uid="{4EBDEBD4-A02D-4266-88BC-5E6088167CE4}" name="Hours Worked Today" dataDxfId="0"/>
+    <tableColumn id="7" xr3:uid="{88484166-6833-4A6B-B292-081E908E7876}" name="Next Steps" dataDxfId="1"/>
+    <tableColumn id="8" xr3:uid="{65034E84-46C0-4115-A351-A3C28C7B9EE1}" name="Notes/Comments" dataDxfId="24"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium26" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{D9A2FBFA-47C8-4A27-8A35-991BC77E93AD}" name="Table14" displayName="Table14" ref="A1:H100" totalsRowShown="0" headerRowDxfId="20">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{D9A2FBFA-47C8-4A27-8A35-991BC77E93AD}" name="Table14" displayName="Table14" ref="A1:H100" totalsRowShown="0" headerRowDxfId="23">
   <autoFilter ref="A1:H100" xr:uid="{D9A2FBFA-47C8-4A27-8A35-991BC77E93AD}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
@@ -478,21 +519,21 @@
     <filterColumn colId="7" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="8">
-    <tableColumn id="1" xr3:uid="{9DF80C4D-D075-4428-A54F-FD6AD093D08C}" name="Date" dataDxfId="19"/>
-    <tableColumn id="2" xr3:uid="{EBFC72C6-272F-4910-98B7-AD481D68F5CF}" name="Member Name" dataDxfId="18"/>
+    <tableColumn id="1" xr3:uid="{9DF80C4D-D075-4428-A54F-FD6AD093D08C}" name="Date" dataDxfId="22"/>
+    <tableColumn id="2" xr3:uid="{EBFC72C6-272F-4910-98B7-AD481D68F5CF}" name="Member Name" dataDxfId="21"/>
     <tableColumn id="3" xr3:uid="{9F5B3984-7002-4FEA-8B81-D2D8284783D7}" name="Task/Activity"/>
     <tableColumn id="4" xr3:uid="{5F85F44B-886F-440F-9E69-8335A039C2E6}" name="Status"/>
-    <tableColumn id="5" xr3:uid="{AF0043ED-9EF2-470B-9735-7321011714BA}" name="% Complete" dataDxfId="17"/>
-    <tableColumn id="6" xr3:uid="{4F961AD8-B86B-411C-BB04-8D7EE4DD134D}" name="Hours Worked Today" dataDxfId="16"/>
-    <tableColumn id="7" xr3:uid="{34EBB1FC-FFD7-47AB-A959-A220B742401C}" name="Next Steps" dataDxfId="15"/>
-    <tableColumn id="8" xr3:uid="{128DAA9E-15FB-4BB9-B76B-4A920C859038}" name="Notes/Comments" dataDxfId="14"/>
+    <tableColumn id="5" xr3:uid="{AF0043ED-9EF2-470B-9735-7321011714BA}" name="% Complete" dataDxfId="20"/>
+    <tableColumn id="6" xr3:uid="{4F961AD8-B86B-411C-BB04-8D7EE4DD134D}" name="Hours Worked Today" dataDxfId="19"/>
+    <tableColumn id="7" xr3:uid="{34EBB1FC-FFD7-47AB-A959-A220B742401C}" name="Next Steps" dataDxfId="18"/>
+    <tableColumn id="8" xr3:uid="{128DAA9E-15FB-4BB9-B76B-4A920C859038}" name="Notes/Comments" dataDxfId="17"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium26" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{646C4EC7-41A3-4570-9D38-06D55FDE20F6}" name="Table15" displayName="Table15" ref="A1:H100" totalsRowShown="0" headerRowDxfId="13">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{646C4EC7-41A3-4570-9D38-06D55FDE20F6}" name="Table15" displayName="Table15" ref="A1:H100" totalsRowShown="0" headerRowDxfId="16">
   <autoFilter ref="A1:H100" xr:uid="{646C4EC7-41A3-4570-9D38-06D55FDE20F6}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
@@ -504,21 +545,21 @@
     <filterColumn colId="7" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="8">
-    <tableColumn id="1" xr3:uid="{13D6CE41-CF73-478C-B7F6-3B0C25C48DFD}" name="Date" dataDxfId="12"/>
-    <tableColumn id="2" xr3:uid="{E468B109-F9F1-48D8-BECE-0F7015DD8D95}" name="Member Name" dataDxfId="11"/>
+    <tableColumn id="1" xr3:uid="{13D6CE41-CF73-478C-B7F6-3B0C25C48DFD}" name="Date" dataDxfId="15"/>
+    <tableColumn id="2" xr3:uid="{E468B109-F9F1-48D8-BECE-0F7015DD8D95}" name="Member Name" dataDxfId="14"/>
     <tableColumn id="3" xr3:uid="{279E5366-E900-45EE-80D9-5446A85E61AD}" name="Task/Activity"/>
     <tableColumn id="4" xr3:uid="{63D996BE-E8E2-4186-8CD4-49EAB9AA8847}" name="Status"/>
-    <tableColumn id="5" xr3:uid="{2FF82CF3-E17A-4896-9C9C-7339D28CD4A7}" name="% Complete" dataDxfId="10"/>
-    <tableColumn id="6" xr3:uid="{67DCB379-6881-4BBC-A633-BD51853A9B6B}" name="Hours Worked Today" dataDxfId="9"/>
-    <tableColumn id="7" xr3:uid="{91C8F225-F251-45F2-BC41-843547B77A6F}" name="Next Steps" dataDxfId="8"/>
-    <tableColumn id="8" xr3:uid="{EEAB1D68-5668-4B1F-8473-D3A49DA7E015}" name="Notes/Comments" dataDxfId="7"/>
+    <tableColumn id="5" xr3:uid="{2FF82CF3-E17A-4896-9C9C-7339D28CD4A7}" name="% Complete" dataDxfId="13"/>
+    <tableColumn id="6" xr3:uid="{67DCB379-6881-4BBC-A633-BD51853A9B6B}" name="Hours Worked Today" dataDxfId="12"/>
+    <tableColumn id="7" xr3:uid="{91C8F225-F251-45F2-BC41-843547B77A6F}" name="Next Steps" dataDxfId="11"/>
+    <tableColumn id="8" xr3:uid="{EEAB1D68-5668-4B1F-8473-D3A49DA7E015}" name="Notes/Comments" dataDxfId="10"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium26" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{5818BB59-8F2C-4810-A78D-CBC8FA25F524}" name="Table5" displayName="Table5" ref="A1:J100" totalsRowShown="0" headerRowDxfId="6">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{5818BB59-8F2C-4810-A78D-CBC8FA25F524}" name="Table5" displayName="Table5" ref="A1:J100" totalsRowShown="0" headerRowDxfId="9">
   <autoFilter ref="A1:J100" xr:uid="{5818BB59-8F2C-4810-A78D-CBC8FA25F524}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
@@ -532,16 +573,16 @@
     <filterColumn colId="9" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="10">
-    <tableColumn id="1" xr3:uid="{BC250DF1-329E-4733-8702-E009738E43CB}" name="Header" dataDxfId="5"/>
-    <tableColumn id="2" xr3:uid="{F6CCDA73-9A12-472B-A535-0F3DC2A5CF61}" name="Date Raised" dataDxfId="4"/>
+    <tableColumn id="1" xr3:uid="{BC250DF1-329E-4733-8702-E009738E43CB}" name="Header" dataDxfId="8"/>
+    <tableColumn id="2" xr3:uid="{F6CCDA73-9A12-472B-A535-0F3DC2A5CF61}" name="Date Raised" dataDxfId="7"/>
     <tableColumn id="3" xr3:uid="{2E3C7862-32AA-44B8-BCC3-2F9299A8F3DC}" name="Raised By"/>
-    <tableColumn id="4" xr3:uid="{FB9438A9-92FB-4A8D-95A5-F17D6EF9AA82}" name="Issue Description" dataDxfId="3"/>
+    <tableColumn id="4" xr3:uid="{FB9438A9-92FB-4A8D-95A5-F17D6EF9AA82}" name="Issue Description" dataDxfId="6"/>
     <tableColumn id="5" xr3:uid="{48223256-C4C0-467B-9FA7-AA8E7742B58A}" name="Impact"/>
     <tableColumn id="6" xr3:uid="{EEDBAAB2-0361-4BF5-8FDB-3FAD49E87C1B}" name="Priority"/>
     <tableColumn id="7" xr3:uid="{515F6321-7FC0-4B4E-A422-3A0E332B7B97}" name="Status"/>
-    <tableColumn id="8" xr3:uid="{60A704D7-818B-442C-91EF-B82765B2618D}" name="Resolution Plan" dataDxfId="2"/>
-    <tableColumn id="9" xr3:uid="{D95E2A6F-E7D4-4FC5-9AAF-1E3DBEE8D8FC}" name="Date Resolved" dataDxfId="1"/>
-    <tableColumn id="10" xr3:uid="{D43B4A1C-AE3D-43D4-A514-7BAA3E281FD3}" name="Notes/Comments" dataDxfId="0"/>
+    <tableColumn id="8" xr3:uid="{60A704D7-818B-442C-91EF-B82765B2618D}" name="Resolution Plan" dataDxfId="5"/>
+    <tableColumn id="9" xr3:uid="{D95E2A6F-E7D4-4FC5-9AAF-1E3DBEE8D8FC}" name="Date Resolved" dataDxfId="4"/>
+    <tableColumn id="10" xr3:uid="{D43B4A1C-AE3D-43D4-A514-7BAA3E281FD3}" name="Notes/Comments" dataDxfId="3"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight15" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -895,30 +936,30 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{37EAA098-74C6-4411-B7E2-26AD2DCBC3F0}">
   <dimension ref="A1:H28"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H6" sqref="H6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col min="1" max="1" width="10.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.5703125" style="2" customWidth="1"/>
+    <col min="1" max="1" width="10.3984375" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.59765625" style="2" customWidth="1"/>
     <col min="3" max="3" width="58" customWidth="1"/>
-    <col min="5" max="5" width="13.140625" style="3" customWidth="1"/>
-    <col min="6" max="6" width="20.85546875" style="4" customWidth="1"/>
-    <col min="7" max="7" width="34.85546875" style="2" customWidth="1"/>
-    <col min="8" max="8" width="43.42578125" style="2" customWidth="1"/>
-    <col min="11" max="11" width="9.140625" customWidth="1"/>
-    <col min="12" max="12" width="13.28515625" customWidth="1"/>
-    <col min="13" max="13" width="11.42578125" customWidth="1"/>
-    <col min="14" max="14" width="17.42578125" customWidth="1"/>
-    <col min="16" max="16" width="9.140625" customWidth="1"/>
-    <col min="18" max="18" width="16.5703125" customWidth="1"/>
-    <col min="19" max="19" width="14.7109375" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="16.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.09765625" style="3" customWidth="1"/>
+    <col min="6" max="6" width="20.8984375" style="4" customWidth="1"/>
+    <col min="7" max="7" width="34.8984375" style="2" customWidth="1"/>
+    <col min="8" max="8" width="43.3984375" style="2" customWidth="1"/>
+    <col min="11" max="11" width="9.09765625" customWidth="1"/>
+    <col min="12" max="12" width="13.296875" customWidth="1"/>
+    <col min="13" max="13" width="11.3984375" customWidth="1"/>
+    <col min="14" max="14" width="17.3984375" customWidth="1"/>
+    <col min="16" max="16" width="9.09765625" customWidth="1"/>
+    <col min="18" max="18" width="16.59765625" customWidth="1"/>
+    <col min="19" max="19" width="14.69921875" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="16.8984375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" ht="15.75">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
@@ -944,7 +985,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="15.75" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:8" ht="15.75">
       <c r="A2" s="1">
         <v>45786</v>
       </c>
@@ -970,7 +1011,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="3" spans="1:8" ht="120" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" ht="120">
       <c r="A3" s="1">
         <v>45787</v>
       </c>
@@ -993,7 +1034,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" ht="15">
       <c r="A4" s="1">
         <v>45788</v>
       </c>
@@ -1013,7 +1054,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="5" spans="1:8" ht="76.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" ht="76.5" customHeight="1">
       <c r="A5" s="1">
         <v>45789</v>
       </c>
@@ -1036,7 +1077,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" ht="15">
       <c r="A6" s="1" t="s">
         <v>29</v>
       </c>
@@ -1059,80 +1100,80 @@
         <v>32</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" ht="15">
       <c r="E7"/>
       <c r="F7"/>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" ht="15">
       <c r="E8"/>
       <c r="F8"/>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" ht="15">
       <c r="E9"/>
       <c r="F9"/>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" ht="15">
       <c r="E10"/>
       <c r="F10"/>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" ht="15">
       <c r="E11"/>
       <c r="F11"/>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8" ht="15">
       <c r="E12"/>
       <c r="F12"/>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8" ht="15">
       <c r="E13"/>
       <c r="F13"/>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8" ht="15">
       <c r="E14"/>
       <c r="F14"/>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8">
       <c r="E15"/>
       <c r="F15"/>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8">
       <c r="E16"/>
       <c r="F16"/>
     </row>
-    <row r="17" spans="6:6" x14ac:dyDescent="0.25">
+    <row r="17" spans="6:6">
       <c r="F17"/>
     </row>
-    <row r="18" spans="6:6" x14ac:dyDescent="0.25">
+    <row r="18" spans="6:6">
       <c r="F18"/>
     </row>
-    <row r="19" spans="6:6" x14ac:dyDescent="0.25">
+    <row r="19" spans="6:6">
       <c r="F19"/>
     </row>
-    <row r="20" spans="6:6" x14ac:dyDescent="0.25">
+    <row r="20" spans="6:6">
       <c r="F20"/>
     </row>
-    <row r="21" spans="6:6" x14ac:dyDescent="0.25">
+    <row r="21" spans="6:6">
       <c r="F21"/>
     </row>
-    <row r="22" spans="6:6" x14ac:dyDescent="0.25">
+    <row r="22" spans="6:6">
       <c r="F22"/>
     </row>
-    <row r="23" spans="6:6" x14ac:dyDescent="0.25">
+    <row r="23" spans="6:6">
       <c r="F23"/>
     </row>
-    <row r="24" spans="6:6" x14ac:dyDescent="0.25">
+    <row r="24" spans="6:6">
       <c r="F24"/>
     </row>
-    <row r="25" spans="6:6" x14ac:dyDescent="0.25">
+    <row r="25" spans="6:6">
       <c r="F25"/>
     </row>
-    <row r="26" spans="6:6" x14ac:dyDescent="0.25">
+    <row r="26" spans="6:6">
       <c r="F26"/>
     </row>
-    <row r="27" spans="6:6" x14ac:dyDescent="0.25">
+    <row r="27" spans="6:6">
       <c r="F27"/>
     </row>
-    <row r="28" spans="6:6" x14ac:dyDescent="0.25">
+    <row r="28" spans="6:6">
       <c r="F28"/>
     </row>
   </sheetData>
@@ -1167,23 +1208,23 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3BDA6702-5DDF-42FB-988E-13FBEB26F5C9}">
   <dimension ref="A1:H100"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H2" sqref="H2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col min="1" max="1" width="9.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="17.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.85546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="23.5703125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="13.42578125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="19.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.8984375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.296875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="54.69921875" customWidth="1"/>
+    <col min="4" max="4" width="8.8984375" customWidth="1"/>
+    <col min="5" max="5" width="14.8984375" style="11" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="23.59765625" style="11" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="29.19921875" customWidth="1"/>
+    <col min="8" max="8" width="39.69921875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" ht="15.75">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
@@ -1196,10 +1237,10 @@
       <c r="D1" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="7" t="s">
+      <c r="E1" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="7" t="s">
+      <c r="F1" s="10" t="s">
         <v>5</v>
       </c>
       <c r="G1" s="7" t="s">
@@ -1209,793 +1250,673 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A2" s="8"/>
-      <c r="B2" s="2"/>
-      <c r="E2" s="3"/>
-      <c r="G2" s="2"/>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A3" s="8"/>
-      <c r="B3" s="2"/>
-      <c r="E3" s="3"/>
-      <c r="F3" s="4"/>
-      <c r="G3" s="2"/>
-      <c r="H3" s="2"/>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A4" s="8"/>
-      <c r="B4" s="2"/>
-      <c r="E4" s="3"/>
-      <c r="F4" s="4"/>
-      <c r="G4" s="2"/>
+    <row r="2" spans="1:8" ht="15">
+      <c r="A2" s="8">
+        <v>45786</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="C2" t="s">
+        <v>34</v>
+      </c>
+      <c r="D2" t="s">
+        <v>35</v>
+      </c>
+      <c r="E2" s="11">
+        <v>90</v>
+      </c>
+      <c r="F2" s="11">
+        <v>8</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="H2" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" ht="15">
+      <c r="A3" s="8">
+        <v>45787</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="C3" t="s">
+        <v>38</v>
+      </c>
+      <c r="D3" t="s">
+        <v>35</v>
+      </c>
+      <c r="E3" s="11">
+        <v>90</v>
+      </c>
+      <c r="F3" s="11">
+        <v>8</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="H3" s="2" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" ht="15">
+      <c r="A4" s="8">
+        <v>45789</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="C4" t="s">
+        <v>40</v>
+      </c>
+      <c r="D4" t="s">
+        <v>35</v>
+      </c>
+      <c r="E4" s="11">
+        <v>90</v>
+      </c>
+      <c r="F4" s="11">
+        <v>5</v>
+      </c>
+      <c r="G4" s="2" t="s">
+        <v>41</v>
+      </c>
       <c r="H4" s="2"/>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A5" s="8"/>
-      <c r="B5" s="2"/>
-      <c r="E5" s="3"/>
-      <c r="F5" s="4"/>
-      <c r="G5" s="2"/>
+    <row r="5" spans="1:8" ht="15">
+      <c r="A5" s="8">
+        <v>45790</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="C5" t="s">
+        <v>45</v>
+      </c>
+      <c r="D5" t="s">
+        <v>17</v>
+      </c>
+      <c r="E5" s="11">
+        <v>100</v>
+      </c>
+      <c r="F5" s="11">
+        <v>5</v>
+      </c>
+      <c r="G5" s="2" t="s">
+        <v>44</v>
+      </c>
       <c r="H5" s="2"/>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" ht="15">
       <c r="A6" s="8"/>
       <c r="B6" s="2"/>
-      <c r="E6" s="3"/>
-      <c r="F6" s="4"/>
       <c r="G6" s="2"/>
       <c r="H6" s="2"/>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" ht="15">
       <c r="A7" s="8"/>
       <c r="B7" s="2"/>
-      <c r="E7" s="3"/>
-      <c r="F7" s="4"/>
       <c r="G7" s="2"/>
       <c r="H7" s="2"/>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" ht="15">
       <c r="A8" s="8"/>
       <c r="B8" s="2"/>
-      <c r="E8" s="3"/>
-      <c r="F8" s="4"/>
       <c r="G8" s="2"/>
       <c r="H8" s="2"/>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" ht="15">
       <c r="A9" s="8"/>
       <c r="B9" s="2"/>
-      <c r="E9" s="3"/>
-      <c r="F9" s="4"/>
       <c r="G9" s="2"/>
       <c r="H9" s="2"/>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" ht="15">
       <c r="A10" s="8"/>
       <c r="B10" s="2"/>
-      <c r="E10" s="3"/>
-      <c r="F10" s="4"/>
       <c r="G10" s="2"/>
       <c r="H10" s="2"/>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" ht="15">
       <c r="A11" s="8"/>
       <c r="B11" s="2"/>
-      <c r="E11" s="3"/>
-      <c r="F11" s="4"/>
       <c r="G11" s="2"/>
       <c r="H11" s="2"/>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8" ht="15">
       <c r="A12" s="8"/>
       <c r="B12" s="2"/>
-      <c r="E12" s="3"/>
-      <c r="F12" s="4"/>
       <c r="G12" s="2"/>
       <c r="H12" s="2"/>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8" ht="15">
       <c r="A13" s="8"/>
       <c r="B13" s="2"/>
-      <c r="E13" s="3"/>
-      <c r="F13" s="4"/>
       <c r="G13" s="2"/>
       <c r="H13" s="2"/>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8" ht="15">
       <c r="A14" s="8"/>
       <c r="B14" s="2"/>
-      <c r="E14" s="3"/>
-      <c r="F14" s="4"/>
       <c r="G14" s="2"/>
       <c r="H14" s="2"/>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8" ht="15">
       <c r="A15" s="8"/>
       <c r="B15" s="2"/>
-      <c r="E15" s="3"/>
-      <c r="F15" s="4"/>
       <c r="G15" s="2"/>
       <c r="H15" s="2"/>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8" ht="15">
       <c r="A16" s="8"/>
       <c r="B16" s="2"/>
-      <c r="E16" s="3"/>
-      <c r="F16" s="4"/>
       <c r="G16" s="2"/>
       <c r="H16" s="2"/>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:8" ht="15">
       <c r="A17" s="8"/>
       <c r="B17" s="2"/>
-      <c r="E17" s="3"/>
-      <c r="F17" s="4"/>
       <c r="G17" s="2"/>
       <c r="H17" s="2"/>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:8" ht="15">
       <c r="A18" s="8"/>
       <c r="B18" s="2"/>
-      <c r="E18" s="3"/>
-      <c r="F18" s="4"/>
       <c r="G18" s="2"/>
       <c r="H18" s="2"/>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:8" ht="15">
       <c r="A19" s="8"/>
       <c r="B19" s="2"/>
-      <c r="E19" s="3"/>
-      <c r="F19" s="4"/>
       <c r="G19" s="2"/>
       <c r="H19" s="2"/>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:8" ht="15">
       <c r="A20" s="8"/>
       <c r="B20" s="2"/>
-      <c r="E20" s="3"/>
-      <c r="F20" s="4"/>
       <c r="G20" s="2"/>
       <c r="H20" s="2"/>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:8" ht="15">
       <c r="A21" s="8"/>
       <c r="B21" s="2"/>
-      <c r="E21" s="3"/>
-      <c r="F21" s="4"/>
       <c r="G21" s="2"/>
       <c r="H21" s="2"/>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:8" ht="15">
       <c r="A22" s="8"/>
       <c r="B22" s="2"/>
-      <c r="E22" s="3"/>
-      <c r="F22" s="4"/>
       <c r="G22" s="2"/>
       <c r="H22" s="2"/>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:8" ht="15">
       <c r="A23" s="8"/>
       <c r="B23" s="2"/>
-      <c r="E23" s="3"/>
-      <c r="F23" s="4"/>
       <c r="G23" s="2"/>
       <c r="H23" s="2"/>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:8" ht="15">
       <c r="A24" s="8"/>
       <c r="B24" s="2"/>
-      <c r="E24" s="3"/>
-      <c r="F24" s="4"/>
       <c r="G24" s="2"/>
       <c r="H24" s="2"/>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:8" ht="15">
       <c r="A25" s="8"/>
       <c r="B25" s="2"/>
-      <c r="E25" s="3"/>
-      <c r="F25" s="4"/>
       <c r="G25" s="2"/>
       <c r="H25" s="2"/>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:8">
       <c r="A26" s="8"/>
       <c r="B26" s="2"/>
-      <c r="E26" s="3"/>
-      <c r="F26" s="4"/>
       <c r="G26" s="2"/>
       <c r="H26" s="2"/>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:8">
       <c r="A27" s="8"/>
       <c r="B27" s="2"/>
-      <c r="E27" s="3"/>
-      <c r="F27" s="4"/>
       <c r="G27" s="2"/>
       <c r="H27" s="2"/>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:8">
       <c r="A28" s="8"/>
       <c r="B28" s="2"/>
-      <c r="E28" s="3"/>
-      <c r="F28" s="4"/>
       <c r="G28" s="2"/>
       <c r="H28" s="2"/>
     </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:8">
       <c r="A29" s="8"/>
       <c r="B29" s="2"/>
-      <c r="E29" s="3"/>
-      <c r="F29" s="4"/>
       <c r="G29" s="2"/>
       <c r="H29" s="2"/>
     </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:8">
       <c r="A30" s="8"/>
       <c r="B30" s="2"/>
-      <c r="E30" s="3"/>
-      <c r="F30" s="4"/>
       <c r="G30" s="2"/>
       <c r="H30" s="2"/>
     </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:8">
       <c r="A31" s="8"/>
       <c r="B31" s="2"/>
-      <c r="E31" s="3"/>
-      <c r="F31" s="4"/>
       <c r="G31" s="2"/>
       <c r="H31" s="2"/>
     </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:8">
       <c r="A32" s="8"/>
       <c r="B32" s="2"/>
-      <c r="E32" s="3"/>
-      <c r="F32" s="4"/>
       <c r="G32" s="2"/>
       <c r="H32" s="2"/>
     </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:8">
       <c r="A33" s="8"/>
       <c r="B33" s="2"/>
-      <c r="E33" s="3"/>
-      <c r="F33" s="4"/>
       <c r="G33" s="2"/>
       <c r="H33" s="2"/>
     </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:8">
       <c r="A34" s="8"/>
       <c r="B34" s="2"/>
-      <c r="E34" s="3"/>
-      <c r="F34" s="4"/>
       <c r="G34" s="2"/>
       <c r="H34" s="2"/>
     </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:8">
       <c r="A35" s="8"/>
       <c r="B35" s="2"/>
-      <c r="E35" s="3"/>
-      <c r="F35" s="4"/>
       <c r="G35" s="2"/>
       <c r="H35" s="2"/>
     </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:8">
       <c r="A36" s="8"/>
       <c r="B36" s="2"/>
-      <c r="E36" s="3"/>
-      <c r="F36" s="4"/>
       <c r="G36" s="2"/>
       <c r="H36" s="2"/>
     </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:8">
       <c r="A37" s="8"/>
       <c r="B37" s="2"/>
-      <c r="E37" s="3"/>
-      <c r="F37" s="4"/>
       <c r="G37" s="2"/>
       <c r="H37" s="2"/>
     </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:8">
       <c r="A38" s="8"/>
       <c r="B38" s="2"/>
-      <c r="E38" s="3"/>
-      <c r="F38" s="4"/>
       <c r="G38" s="2"/>
       <c r="H38" s="2"/>
     </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:8">
       <c r="A39" s="8"/>
       <c r="B39" s="2"/>
-      <c r="E39" s="3"/>
-      <c r="F39" s="4"/>
       <c r="G39" s="2"/>
       <c r="H39" s="2"/>
     </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:8">
       <c r="A40" s="8"/>
       <c r="B40" s="2"/>
-      <c r="E40" s="3"/>
-      <c r="F40" s="4"/>
       <c r="G40" s="2"/>
       <c r="H40" s="2"/>
     </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:8">
       <c r="A41" s="8"/>
       <c r="B41" s="2"/>
-      <c r="E41" s="3"/>
-      <c r="F41" s="4"/>
       <c r="G41" s="2"/>
       <c r="H41" s="2"/>
     </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:8">
       <c r="A42" s="8"/>
       <c r="B42" s="2"/>
-      <c r="E42" s="3"/>
-      <c r="F42" s="4"/>
       <c r="G42" s="2"/>
       <c r="H42" s="2"/>
     </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:8">
       <c r="A43" s="8"/>
       <c r="B43" s="2"/>
-      <c r="E43" s="3"/>
-      <c r="F43" s="4"/>
       <c r="G43" s="2"/>
       <c r="H43" s="2"/>
     </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:8">
       <c r="A44" s="8"/>
       <c r="B44" s="2"/>
-      <c r="E44" s="3"/>
-      <c r="F44" s="4"/>
       <c r="G44" s="2"/>
       <c r="H44" s="2"/>
     </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:8">
       <c r="A45" s="8"/>
       <c r="B45" s="2"/>
-      <c r="E45" s="3"/>
-      <c r="F45" s="4"/>
       <c r="G45" s="2"/>
       <c r="H45" s="2"/>
     </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:8">
       <c r="A46" s="8"/>
       <c r="B46" s="2"/>
-      <c r="E46" s="3"/>
-      <c r="F46" s="4"/>
       <c r="G46" s="2"/>
       <c r="H46" s="2"/>
     </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:8">
       <c r="A47" s="8"/>
       <c r="B47" s="2"/>
-      <c r="E47" s="3"/>
-      <c r="F47" s="4"/>
       <c r="G47" s="2"/>
       <c r="H47" s="2"/>
     </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:8">
       <c r="A48" s="8"/>
       <c r="B48" s="2"/>
-      <c r="E48" s="3"/>
-      <c r="F48" s="4"/>
       <c r="G48" s="2"/>
       <c r="H48" s="2"/>
     </row>
-    <row r="49" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:8">
       <c r="A49" s="8"/>
       <c r="B49" s="2"/>
-      <c r="E49" s="3"/>
-      <c r="F49" s="4"/>
       <c r="G49" s="2"/>
       <c r="H49" s="2"/>
     </row>
-    <row r="50" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:8">
       <c r="A50" s="8"/>
       <c r="B50" s="2"/>
-      <c r="E50" s="3"/>
-      <c r="F50" s="4"/>
       <c r="G50" s="2"/>
       <c r="H50" s="2"/>
     </row>
-    <row r="51" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:8">
       <c r="A51" s="8"/>
       <c r="B51" s="2"/>
-      <c r="E51" s="3"/>
-      <c r="F51" s="4"/>
       <c r="G51" s="2"/>
       <c r="H51" s="2"/>
     </row>
-    <row r="52" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:8">
       <c r="A52" s="8"/>
       <c r="B52" s="2"/>
-      <c r="E52" s="3"/>
-      <c r="F52" s="4"/>
       <c r="G52" s="2"/>
       <c r="H52" s="2"/>
     </row>
-    <row r="53" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:8">
       <c r="A53" s="8"/>
       <c r="B53" s="2"/>
-      <c r="E53" s="3"/>
-      <c r="F53" s="4"/>
       <c r="G53" s="2"/>
       <c r="H53" s="2"/>
     </row>
-    <row r="54" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:8">
       <c r="A54" s="8"/>
       <c r="B54" s="2"/>
-      <c r="E54" s="3"/>
-      <c r="F54" s="4"/>
       <c r="G54" s="2"/>
       <c r="H54" s="2"/>
     </row>
-    <row r="55" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:8">
       <c r="A55" s="8"/>
       <c r="B55" s="2"/>
-      <c r="E55" s="3"/>
-      <c r="F55" s="4"/>
       <c r="G55" s="2"/>
       <c r="H55" s="2"/>
     </row>
-    <row r="56" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:8">
       <c r="A56" s="8"/>
       <c r="B56" s="2"/>
-      <c r="E56" s="3"/>
-      <c r="F56" s="4"/>
       <c r="G56" s="2"/>
       <c r="H56" s="2"/>
     </row>
-    <row r="57" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:8">
       <c r="A57" s="8"/>
       <c r="B57" s="2"/>
-      <c r="E57" s="3"/>
-      <c r="F57" s="4"/>
       <c r="G57" s="2"/>
       <c r="H57" s="2"/>
     </row>
-    <row r="58" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:8">
       <c r="A58" s="8"/>
       <c r="B58" s="2"/>
-      <c r="E58" s="3"/>
-      <c r="F58" s="4"/>
       <c r="G58" s="2"/>
       <c r="H58" s="2"/>
     </row>
-    <row r="59" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:8">
       <c r="A59" s="8"/>
       <c r="B59" s="2"/>
-      <c r="E59" s="3"/>
-      <c r="F59" s="4"/>
       <c r="G59" s="2"/>
       <c r="H59" s="2"/>
     </row>
-    <row r="60" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:8">
       <c r="A60" s="8"/>
       <c r="B60" s="2"/>
-      <c r="E60" s="3"/>
-      <c r="F60" s="4"/>
       <c r="G60" s="2"/>
       <c r="H60" s="2"/>
     </row>
-    <row r="61" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:8">
       <c r="A61" s="8"/>
       <c r="B61" s="2"/>
-      <c r="E61" s="3"/>
-      <c r="F61" s="4"/>
       <c r="G61" s="2"/>
       <c r="H61" s="2"/>
     </row>
-    <row r="62" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:8">
       <c r="A62" s="8"/>
       <c r="B62" s="2"/>
-      <c r="E62" s="3"/>
-      <c r="F62" s="4"/>
       <c r="G62" s="2"/>
       <c r="H62" s="2"/>
     </row>
-    <row r="63" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:8">
       <c r="A63" s="8"/>
       <c r="B63" s="2"/>
-      <c r="E63" s="3"/>
-      <c r="F63" s="4"/>
       <c r="G63" s="2"/>
       <c r="H63" s="2"/>
     </row>
-    <row r="64" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:8">
       <c r="A64" s="8"/>
       <c r="B64" s="2"/>
-      <c r="E64" s="3"/>
-      <c r="F64" s="4"/>
       <c r="G64" s="2"/>
       <c r="H64" s="2"/>
     </row>
-    <row r="65" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:8">
       <c r="A65" s="8"/>
       <c r="B65" s="2"/>
-      <c r="E65" s="3"/>
-      <c r="F65" s="4"/>
       <c r="G65" s="2"/>
       <c r="H65" s="2"/>
     </row>
-    <row r="66" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:8">
       <c r="A66" s="8"/>
       <c r="B66" s="2"/>
-      <c r="E66" s="3"/>
-      <c r="F66" s="4"/>
       <c r="G66" s="2"/>
       <c r="H66" s="2"/>
     </row>
-    <row r="67" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:8">
       <c r="A67" s="8"/>
       <c r="B67" s="2"/>
-      <c r="E67" s="3"/>
-      <c r="F67" s="4"/>
       <c r="G67" s="2"/>
       <c r="H67" s="2"/>
     </row>
-    <row r="68" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:8">
       <c r="A68" s="8"/>
       <c r="B68" s="2"/>
-      <c r="E68" s="3"/>
-      <c r="F68" s="4"/>
       <c r="G68" s="2"/>
       <c r="H68" s="2"/>
     </row>
-    <row r="69" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:8">
       <c r="A69" s="8"/>
       <c r="B69" s="2"/>
-      <c r="E69" s="3"/>
-      <c r="F69" s="4"/>
       <c r="G69" s="2"/>
       <c r="H69" s="2"/>
     </row>
-    <row r="70" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:8">
       <c r="A70" s="8"/>
       <c r="B70" s="2"/>
-      <c r="E70" s="3"/>
-      <c r="F70" s="4"/>
       <c r="G70" s="2"/>
       <c r="H70" s="2"/>
     </row>
-    <row r="71" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:8">
       <c r="A71" s="8"/>
       <c r="B71" s="2"/>
-      <c r="E71" s="3"/>
-      <c r="F71" s="4"/>
       <c r="G71" s="2"/>
       <c r="H71" s="2"/>
     </row>
-    <row r="72" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:8">
       <c r="A72" s="8"/>
       <c r="B72" s="2"/>
-      <c r="E72" s="3"/>
-      <c r="F72" s="4"/>
       <c r="G72" s="2"/>
       <c r="H72" s="2"/>
     </row>
-    <row r="73" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:8">
       <c r="A73" s="8"/>
       <c r="B73" s="2"/>
-      <c r="E73" s="3"/>
-      <c r="F73" s="4"/>
       <c r="G73" s="2"/>
       <c r="H73" s="2"/>
     </row>
-    <row r="74" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:8">
       <c r="A74" s="8"/>
       <c r="B74" s="2"/>
-      <c r="E74" s="3"/>
-      <c r="F74" s="4"/>
       <c r="G74" s="2"/>
       <c r="H74" s="2"/>
     </row>
-    <row r="75" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:8">
       <c r="A75" s="8"/>
       <c r="B75" s="2"/>
-      <c r="E75" s="3"/>
-      <c r="F75" s="4"/>
       <c r="G75" s="2"/>
       <c r="H75" s="2"/>
     </row>
-    <row r="76" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:8">
       <c r="A76" s="8"/>
       <c r="B76" s="2"/>
-      <c r="E76" s="3"/>
-      <c r="F76" s="4"/>
       <c r="G76" s="2"/>
       <c r="H76" s="2"/>
     </row>
-    <row r="77" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:8">
       <c r="A77" s="8"/>
       <c r="B77" s="2"/>
-      <c r="E77" s="3"/>
-      <c r="F77" s="4"/>
       <c r="G77" s="2"/>
       <c r="H77" s="2"/>
     </row>
-    <row r="78" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:8">
       <c r="A78" s="8"/>
       <c r="B78" s="2"/>
-      <c r="E78" s="3"/>
-      <c r="F78" s="4"/>
       <c r="G78" s="2"/>
       <c r="H78" s="2"/>
     </row>
-    <row r="79" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:8">
       <c r="A79" s="8"/>
       <c r="B79" s="2"/>
-      <c r="E79" s="3"/>
-      <c r="F79" s="4"/>
       <c r="G79" s="2"/>
       <c r="H79" s="2"/>
     </row>
-    <row r="80" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:8">
       <c r="A80" s="8"/>
       <c r="B80" s="2"/>
-      <c r="E80" s="3"/>
-      <c r="F80" s="4"/>
       <c r="G80" s="2"/>
       <c r="H80" s="2"/>
     </row>
-    <row r="81" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:8">
       <c r="A81" s="8"/>
       <c r="B81" s="2"/>
-      <c r="E81" s="3"/>
-      <c r="F81" s="4"/>
       <c r="G81" s="2"/>
       <c r="H81" s="2"/>
     </row>
-    <row r="82" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:8">
       <c r="A82" s="8"/>
       <c r="B82" s="2"/>
-      <c r="E82" s="3"/>
-      <c r="F82" s="4"/>
       <c r="G82" s="2"/>
       <c r="H82" s="2"/>
     </row>
-    <row r="83" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:8">
       <c r="A83" s="8"/>
       <c r="B83" s="2"/>
-      <c r="E83" s="3"/>
-      <c r="F83" s="4"/>
       <c r="G83" s="2"/>
       <c r="H83" s="2"/>
     </row>
-    <row r="84" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:8">
       <c r="A84" s="8"/>
       <c r="B84" s="2"/>
-      <c r="E84" s="3"/>
-      <c r="F84" s="4"/>
       <c r="G84" s="2"/>
       <c r="H84" s="2"/>
     </row>
-    <row r="85" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:8">
       <c r="A85" s="8"/>
       <c r="B85" s="2"/>
-      <c r="E85" s="3"/>
-      <c r="F85" s="4"/>
       <c r="G85" s="2"/>
       <c r="H85" s="2"/>
     </row>
-    <row r="86" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:8">
       <c r="A86" s="8"/>
       <c r="B86" s="2"/>
-      <c r="E86" s="3"/>
-      <c r="F86" s="4"/>
       <c r="G86" s="2"/>
       <c r="H86" s="2"/>
     </row>
-    <row r="87" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:8">
       <c r="A87" s="8"/>
       <c r="B87" s="2"/>
-      <c r="E87" s="3"/>
-      <c r="F87" s="4"/>
       <c r="G87" s="2"/>
       <c r="H87" s="2"/>
     </row>
-    <row r="88" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:8">
       <c r="A88" s="8"/>
       <c r="B88" s="2"/>
-      <c r="E88" s="3"/>
-      <c r="F88" s="4"/>
       <c r="G88" s="2"/>
       <c r="H88" s="2"/>
     </row>
-    <row r="89" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:8">
       <c r="A89" s="8"/>
       <c r="B89" s="2"/>
-      <c r="E89" s="3"/>
-      <c r="F89" s="4"/>
       <c r="G89" s="2"/>
       <c r="H89" s="2"/>
     </row>
-    <row r="90" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:8">
       <c r="A90" s="8"/>
       <c r="B90" s="2"/>
-      <c r="E90" s="3"/>
-      <c r="F90" s="4"/>
       <c r="G90" s="2"/>
       <c r="H90" s="2"/>
     </row>
-    <row r="91" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:8">
       <c r="A91" s="8"/>
       <c r="B91" s="2"/>
-      <c r="E91" s="3"/>
-      <c r="F91" s="4"/>
       <c r="G91" s="2"/>
       <c r="H91" s="2"/>
     </row>
-    <row r="92" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:8">
       <c r="A92" s="8"/>
       <c r="B92" s="2"/>
-      <c r="E92" s="3"/>
-      <c r="F92" s="4"/>
       <c r="G92" s="2"/>
       <c r="H92" s="2"/>
     </row>
-    <row r="93" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:8">
       <c r="A93" s="8"/>
       <c r="B93" s="2"/>
-      <c r="E93" s="3"/>
-      <c r="F93" s="4"/>
       <c r="G93" s="2"/>
       <c r="H93" s="2"/>
     </row>
-    <row r="94" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:8">
       <c r="A94" s="8"/>
       <c r="B94" s="2"/>
-      <c r="E94" s="3"/>
-      <c r="F94" s="4"/>
       <c r="G94" s="2"/>
       <c r="H94" s="2"/>
     </row>
-    <row r="95" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:8">
       <c r="A95" s="8"/>
       <c r="B95" s="2"/>
-      <c r="E95" s="3"/>
-      <c r="F95" s="4"/>
       <c r="G95" s="2"/>
       <c r="H95" s="2"/>
     </row>
-    <row r="96" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:8">
       <c r="A96" s="8"/>
       <c r="B96" s="2"/>
-      <c r="E96" s="3"/>
-      <c r="F96" s="4"/>
       <c r="G96" s="2"/>
       <c r="H96" s="2"/>
     </row>
-    <row r="97" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:8">
       <c r="A97" s="8"/>
       <c r="B97" s="2"/>
-      <c r="E97" s="3"/>
-      <c r="F97" s="4"/>
       <c r="G97" s="2"/>
       <c r="H97" s="2"/>
     </row>
-    <row r="98" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:8">
       <c r="A98" s="8"/>
       <c r="B98" s="2"/>
-      <c r="E98" s="3"/>
-      <c r="F98" s="4"/>
       <c r="G98" s="2"/>
       <c r="H98" s="2"/>
     </row>
-    <row r="99" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:8">
       <c r="A99" s="8"/>
       <c r="B99" s="2"/>
-      <c r="E99" s="3"/>
-      <c r="F99" s="4"/>
       <c r="G99" s="2"/>
       <c r="H99" s="2"/>
     </row>
-    <row r="100" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:8">
       <c r="A100" s="8"/>
       <c r="B100" s="2"/>
-      <c r="E100" s="3"/>
-      <c r="F100" s="4"/>
       <c r="G100" s="2"/>
       <c r="H100" s="2"/>
     </row>
@@ -2018,7 +1939,7 @@
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <ignoredErrors>
-    <ignoredError sqref="D3:D100" listDataValidation="1"/>
+    <ignoredError sqref="D6:D100" listDataValidation="1"/>
   </ignoredErrors>
   <tableParts count="1">
     <tablePart r:id="rId1"/>
@@ -2034,19 +1955,19 @@
       <selection activeCell="D2" sqref="D2:D100"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col min="1" max="1" width="7.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="17.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="7.69921875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.296875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.59765625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="9" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.85546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="23.5703125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="13.42578125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="19.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.8984375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="23.59765625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.3984375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="19.09765625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" ht="15.75">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
@@ -2072,7 +1993,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" ht="15">
       <c r="A2" s="1"/>
       <c r="B2" s="2"/>
       <c r="E2" s="3"/>
@@ -2080,7 +2001,7 @@
       <c r="G2" s="2"/>
       <c r="H2" s="2"/>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" ht="15">
       <c r="A3" s="1"/>
       <c r="B3" s="2"/>
       <c r="E3" s="3"/>
@@ -2088,7 +2009,7 @@
       <c r="G3" s="2"/>
       <c r="H3" s="2"/>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" ht="15">
       <c r="A4" s="1"/>
       <c r="B4" s="2"/>
       <c r="E4" s="3"/>
@@ -2096,7 +2017,7 @@
       <c r="G4" s="2"/>
       <c r="H4" s="2"/>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" ht="15">
       <c r="A5" s="1"/>
       <c r="B5" s="2"/>
       <c r="E5" s="3"/>
@@ -2104,7 +2025,7 @@
       <c r="G5" s="2"/>
       <c r="H5" s="2"/>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" ht="15">
       <c r="A6" s="1"/>
       <c r="B6" s="2"/>
       <c r="E6" s="3"/>
@@ -2112,7 +2033,7 @@
       <c r="G6" s="2"/>
       <c r="H6" s="2"/>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" ht="15">
       <c r="A7" s="1"/>
       <c r="B7" s="2"/>
       <c r="E7" s="3"/>
@@ -2120,7 +2041,7 @@
       <c r="G7" s="2"/>
       <c r="H7" s="2"/>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" ht="15">
       <c r="A8" s="1"/>
       <c r="B8" s="2"/>
       <c r="E8" s="3"/>
@@ -2128,7 +2049,7 @@
       <c r="G8" s="2"/>
       <c r="H8" s="2"/>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" ht="15">
       <c r="A9" s="1"/>
       <c r="B9" s="2"/>
       <c r="E9" s="3"/>
@@ -2136,7 +2057,7 @@
       <c r="G9" s="2"/>
       <c r="H9" s="2"/>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" ht="15">
       <c r="A10" s="1"/>
       <c r="B10" s="2"/>
       <c r="E10" s="3"/>
@@ -2144,7 +2065,7 @@
       <c r="G10" s="2"/>
       <c r="H10" s="2"/>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" ht="15">
       <c r="A11" s="1"/>
       <c r="B11" s="2"/>
       <c r="E11" s="3"/>
@@ -2152,7 +2073,7 @@
       <c r="G11" s="2"/>
       <c r="H11" s="2"/>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8" ht="15">
       <c r="A12" s="1"/>
       <c r="B12" s="2"/>
       <c r="E12" s="3"/>
@@ -2160,7 +2081,7 @@
       <c r="G12" s="2"/>
       <c r="H12" s="2"/>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8" ht="15">
       <c r="A13" s="1"/>
       <c r="B13" s="2"/>
       <c r="E13" s="3"/>
@@ -2168,7 +2089,7 @@
       <c r="G13" s="2"/>
       <c r="H13" s="2"/>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8" ht="15">
       <c r="A14" s="1"/>
       <c r="B14" s="2"/>
       <c r="E14" s="3"/>
@@ -2176,7 +2097,7 @@
       <c r="G14" s="2"/>
       <c r="H14" s="2"/>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8" ht="15">
       <c r="A15" s="1"/>
       <c r="B15" s="2"/>
       <c r="E15" s="3"/>
@@ -2184,7 +2105,7 @@
       <c r="G15" s="2"/>
       <c r="H15" s="2"/>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8" ht="15">
       <c r="A16" s="1"/>
       <c r="B16" s="2"/>
       <c r="E16" s="3"/>
@@ -2192,7 +2113,7 @@
       <c r="G16" s="2"/>
       <c r="H16" s="2"/>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:8" ht="15">
       <c r="A17" s="1"/>
       <c r="B17" s="2"/>
       <c r="E17" s="3"/>
@@ -2200,7 +2121,7 @@
       <c r="G17" s="2"/>
       <c r="H17" s="2"/>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:8" ht="15">
       <c r="A18" s="1"/>
       <c r="B18" s="2"/>
       <c r="E18" s="3"/>
@@ -2208,7 +2129,7 @@
       <c r="G18" s="2"/>
       <c r="H18" s="2"/>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:8" ht="15">
       <c r="A19" s="1"/>
       <c r="B19" s="2"/>
       <c r="E19" s="3"/>
@@ -2216,7 +2137,7 @@
       <c r="G19" s="2"/>
       <c r="H19" s="2"/>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:8" ht="15">
       <c r="A20" s="1"/>
       <c r="B20" s="2"/>
       <c r="E20" s="3"/>
@@ -2224,7 +2145,7 @@
       <c r="G20" s="2"/>
       <c r="H20" s="2"/>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:8" ht="15">
       <c r="A21" s="1"/>
       <c r="B21" s="2"/>
       <c r="E21" s="3"/>
@@ -2232,7 +2153,7 @@
       <c r="G21" s="2"/>
       <c r="H21" s="2"/>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:8" ht="15">
       <c r="A22" s="1"/>
       <c r="B22" s="2"/>
       <c r="E22" s="3"/>
@@ -2240,7 +2161,7 @@
       <c r="G22" s="2"/>
       <c r="H22" s="2"/>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:8" ht="15">
       <c r="A23" s="1"/>
       <c r="B23" s="2"/>
       <c r="E23" s="3"/>
@@ -2248,7 +2169,7 @@
       <c r="G23" s="2"/>
       <c r="H23" s="2"/>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:8" ht="15">
       <c r="A24" s="1"/>
       <c r="B24" s="2"/>
       <c r="E24" s="3"/>
@@ -2256,7 +2177,7 @@
       <c r="G24" s="2"/>
       <c r="H24" s="2"/>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:8" ht="15">
       <c r="A25" s="1"/>
       <c r="B25" s="2"/>
       <c r="E25" s="3"/>
@@ -2264,7 +2185,7 @@
       <c r="G25" s="2"/>
       <c r="H25" s="2"/>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:8" ht="15">
       <c r="A26" s="1"/>
       <c r="B26" s="2"/>
       <c r="E26" s="3"/>
@@ -2272,7 +2193,7 @@
       <c r="G26" s="2"/>
       <c r="H26" s="2"/>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:8" ht="15">
       <c r="A27" s="1"/>
       <c r="B27" s="2"/>
       <c r="E27" s="3"/>
@@ -2280,7 +2201,7 @@
       <c r="G27" s="2"/>
       <c r="H27" s="2"/>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:8" ht="15">
       <c r="A28" s="1"/>
       <c r="B28" s="2"/>
       <c r="E28" s="3"/>
@@ -2288,7 +2209,7 @@
       <c r="G28" s="2"/>
       <c r="H28" s="2"/>
     </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:8" ht="15">
       <c r="A29" s="1"/>
       <c r="B29" s="2"/>
       <c r="E29" s="3"/>
@@ -2296,7 +2217,7 @@
       <c r="G29" s="2"/>
       <c r="H29" s="2"/>
     </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:8" ht="15">
       <c r="A30" s="1"/>
       <c r="B30" s="2"/>
       <c r="E30" s="3"/>
@@ -2304,7 +2225,7 @@
       <c r="G30" s="2"/>
       <c r="H30" s="2"/>
     </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:8" ht="15">
       <c r="A31" s="1"/>
       <c r="B31" s="2"/>
       <c r="E31" s="3"/>
@@ -2312,7 +2233,7 @@
       <c r="G31" s="2"/>
       <c r="H31" s="2"/>
     </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:8" ht="15">
       <c r="A32" s="1"/>
       <c r="B32" s="2"/>
       <c r="E32" s="3"/>
@@ -2320,7 +2241,7 @@
       <c r="G32" s="2"/>
       <c r="H32" s="2"/>
     </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:8" ht="15">
       <c r="A33" s="1"/>
       <c r="B33" s="2"/>
       <c r="E33" s="3"/>
@@ -2328,7 +2249,7 @@
       <c r="G33" s="2"/>
       <c r="H33" s="2"/>
     </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:8" ht="15">
       <c r="A34" s="1"/>
       <c r="B34" s="2"/>
       <c r="E34" s="3"/>
@@ -2336,7 +2257,7 @@
       <c r="G34" s="2"/>
       <c r="H34" s="2"/>
     </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:8" ht="15">
       <c r="A35" s="1"/>
       <c r="B35" s="2"/>
       <c r="E35" s="3"/>
@@ -2344,7 +2265,7 @@
       <c r="G35" s="2"/>
       <c r="H35" s="2"/>
     </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:8" ht="15">
       <c r="A36" s="1"/>
       <c r="B36" s="2"/>
       <c r="E36" s="3"/>
@@ -2352,7 +2273,7 @@
       <c r="G36" s="2"/>
       <c r="H36" s="2"/>
     </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:8" ht="15">
       <c r="A37" s="1"/>
       <c r="B37" s="2"/>
       <c r="E37" s="3"/>
@@ -2360,7 +2281,7 @@
       <c r="G37" s="2"/>
       <c r="H37" s="2"/>
     </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:8" ht="15">
       <c r="A38" s="1"/>
       <c r="B38" s="2"/>
       <c r="E38" s="3"/>
@@ -2368,7 +2289,7 @@
       <c r="G38" s="2"/>
       <c r="H38" s="2"/>
     </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:8" ht="15">
       <c r="A39" s="1"/>
       <c r="B39" s="2"/>
       <c r="E39" s="3"/>
@@ -2376,7 +2297,7 @@
       <c r="G39" s="2"/>
       <c r="H39" s="2"/>
     </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:8" ht="15">
       <c r="A40" s="1"/>
       <c r="B40" s="2"/>
       <c r="E40" s="3"/>
@@ -2384,7 +2305,7 @@
       <c r="G40" s="2"/>
       <c r="H40" s="2"/>
     </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:8" ht="15">
       <c r="A41" s="1"/>
       <c r="B41" s="2"/>
       <c r="E41" s="3"/>
@@ -2392,7 +2313,7 @@
       <c r="G41" s="2"/>
       <c r="H41" s="2"/>
     </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:8" ht="15">
       <c r="A42" s="1"/>
       <c r="B42" s="2"/>
       <c r="E42" s="3"/>
@@ -2400,7 +2321,7 @@
       <c r="G42" s="2"/>
       <c r="H42" s="2"/>
     </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:8" ht="15">
       <c r="A43" s="1"/>
       <c r="B43" s="2"/>
       <c r="E43" s="3"/>
@@ -2408,7 +2329,7 @@
       <c r="G43" s="2"/>
       <c r="H43" s="2"/>
     </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:8" ht="15">
       <c r="A44" s="1"/>
       <c r="B44" s="2"/>
       <c r="E44" s="3"/>
@@ -2416,7 +2337,7 @@
       <c r="G44" s="2"/>
       <c r="H44" s="2"/>
     </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:8" ht="15">
       <c r="A45" s="1"/>
       <c r="B45" s="2"/>
       <c r="E45" s="3"/>
@@ -2424,7 +2345,7 @@
       <c r="G45" s="2"/>
       <c r="H45" s="2"/>
     </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:8" ht="15">
       <c r="A46" s="1"/>
       <c r="B46" s="2"/>
       <c r="E46" s="3"/>
@@ -2432,7 +2353,7 @@
       <c r="G46" s="2"/>
       <c r="H46" s="2"/>
     </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:8" ht="15">
       <c r="A47" s="1"/>
       <c r="B47" s="2"/>
       <c r="E47" s="3"/>
@@ -2440,7 +2361,7 @@
       <c r="G47" s="2"/>
       <c r="H47" s="2"/>
     </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:8" ht="15">
       <c r="A48" s="1"/>
       <c r="B48" s="2"/>
       <c r="E48" s="3"/>
@@ -2448,7 +2369,7 @@
       <c r="G48" s="2"/>
       <c r="H48" s="2"/>
     </row>
-    <row r="49" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:8" ht="15">
       <c r="A49" s="1"/>
       <c r="B49" s="2"/>
       <c r="E49" s="3"/>
@@ -2456,7 +2377,7 @@
       <c r="G49" s="2"/>
       <c r="H49" s="2"/>
     </row>
-    <row r="50" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:8" ht="15">
       <c r="A50" s="1"/>
       <c r="B50" s="2"/>
       <c r="E50" s="3"/>
@@ -2464,7 +2385,7 @@
       <c r="G50" s="2"/>
       <c r="H50" s="2"/>
     </row>
-    <row r="51" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:8" ht="15">
       <c r="A51" s="1"/>
       <c r="B51" s="2"/>
       <c r="E51" s="3"/>
@@ -2472,7 +2393,7 @@
       <c r="G51" s="2"/>
       <c r="H51" s="2"/>
     </row>
-    <row r="52" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:8" ht="15">
       <c r="A52" s="1"/>
       <c r="B52" s="2"/>
       <c r="E52" s="3"/>
@@ -2480,7 +2401,7 @@
       <c r="G52" s="2"/>
       <c r="H52" s="2"/>
     </row>
-    <row r="53" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:8" ht="15">
       <c r="A53" s="1"/>
       <c r="B53" s="2"/>
       <c r="E53" s="3"/>
@@ -2488,7 +2409,7 @@
       <c r="G53" s="2"/>
       <c r="H53" s="2"/>
     </row>
-    <row r="54" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:8" ht="15">
       <c r="A54" s="1"/>
       <c r="B54" s="2"/>
       <c r="E54" s="3"/>
@@ -2496,7 +2417,7 @@
       <c r="G54" s="2"/>
       <c r="H54" s="2"/>
     </row>
-    <row r="55" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:8" ht="15">
       <c r="A55" s="1"/>
       <c r="B55" s="2"/>
       <c r="E55" s="3"/>
@@ -2504,7 +2425,7 @@
       <c r="G55" s="2"/>
       <c r="H55" s="2"/>
     </row>
-    <row r="56" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:8" ht="15">
       <c r="A56" s="1"/>
       <c r="B56" s="2"/>
       <c r="E56" s="3"/>
@@ -2512,7 +2433,7 @@
       <c r="G56" s="2"/>
       <c r="H56" s="2"/>
     </row>
-    <row r="57" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:8" ht="15">
       <c r="A57" s="1"/>
       <c r="B57" s="2"/>
       <c r="E57" s="3"/>
@@ -2520,7 +2441,7 @@
       <c r="G57" s="2"/>
       <c r="H57" s="2"/>
     </row>
-    <row r="58" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:8" ht="15">
       <c r="A58" s="1"/>
       <c r="B58" s="2"/>
       <c r="E58" s="3"/>
@@ -2528,7 +2449,7 @@
       <c r="G58" s="2"/>
       <c r="H58" s="2"/>
     </row>
-    <row r="59" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:8" ht="15">
       <c r="A59" s="1"/>
       <c r="B59" s="2"/>
       <c r="E59" s="3"/>
@@ -2536,7 +2457,7 @@
       <c r="G59" s="2"/>
       <c r="H59" s="2"/>
     </row>
-    <row r="60" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:8" ht="15">
       <c r="A60" s="1"/>
       <c r="B60" s="2"/>
       <c r="E60" s="3"/>
@@ -2544,7 +2465,7 @@
       <c r="G60" s="2"/>
       <c r="H60" s="2"/>
     </row>
-    <row r="61" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:8" ht="15">
       <c r="A61" s="1"/>
       <c r="B61" s="2"/>
       <c r="E61" s="3"/>
@@ -2552,7 +2473,7 @@
       <c r="G61" s="2"/>
       <c r="H61" s="2"/>
     </row>
-    <row r="62" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:8" ht="15">
       <c r="A62" s="1"/>
       <c r="B62" s="2"/>
       <c r="E62" s="3"/>
@@ -2560,7 +2481,7 @@
       <c r="G62" s="2"/>
       <c r="H62" s="2"/>
     </row>
-    <row r="63" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:8" ht="15">
       <c r="A63" s="1"/>
       <c r="B63" s="2"/>
       <c r="E63" s="3"/>
@@ -2568,7 +2489,7 @@
       <c r="G63" s="2"/>
       <c r="H63" s="2"/>
     </row>
-    <row r="64" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:8" ht="15">
       <c r="A64" s="1"/>
       <c r="B64" s="2"/>
       <c r="E64" s="3"/>
@@ -2576,7 +2497,7 @@
       <c r="G64" s="2"/>
       <c r="H64" s="2"/>
     </row>
-    <row r="65" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:8" ht="15">
       <c r="A65" s="1"/>
       <c r="B65" s="2"/>
       <c r="E65" s="3"/>
@@ -2584,7 +2505,7 @@
       <c r="G65" s="2"/>
       <c r="H65" s="2"/>
     </row>
-    <row r="66" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:8" ht="15">
       <c r="A66" s="1"/>
       <c r="B66" s="2"/>
       <c r="E66" s="3"/>
@@ -2592,7 +2513,7 @@
       <c r="G66" s="2"/>
       <c r="H66" s="2"/>
     </row>
-    <row r="67" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:8" ht="15">
       <c r="A67" s="1"/>
       <c r="B67" s="2"/>
       <c r="E67" s="3"/>
@@ -2600,7 +2521,7 @@
       <c r="G67" s="2"/>
       <c r="H67" s="2"/>
     </row>
-    <row r="68" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:8" ht="15">
       <c r="A68" s="1"/>
       <c r="B68" s="2"/>
       <c r="E68" s="3"/>
@@ -2608,7 +2529,7 @@
       <c r="G68" s="2"/>
       <c r="H68" s="2"/>
     </row>
-    <row r="69" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:8" ht="15">
       <c r="A69" s="1"/>
       <c r="B69" s="2"/>
       <c r="E69" s="3"/>
@@ -2616,7 +2537,7 @@
       <c r="G69" s="2"/>
       <c r="H69" s="2"/>
     </row>
-    <row r="70" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:8" ht="15">
       <c r="A70" s="1"/>
       <c r="B70" s="2"/>
       <c r="E70" s="3"/>
@@ -2624,7 +2545,7 @@
       <c r="G70" s="2"/>
       <c r="H70" s="2"/>
     </row>
-    <row r="71" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:8" ht="15">
       <c r="A71" s="1"/>
       <c r="B71" s="2"/>
       <c r="E71" s="3"/>
@@ -2632,7 +2553,7 @@
       <c r="G71" s="2"/>
       <c r="H71" s="2"/>
     </row>
-    <row r="72" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:8" ht="15">
       <c r="A72" s="1"/>
       <c r="B72" s="2"/>
       <c r="E72" s="3"/>
@@ -2640,7 +2561,7 @@
       <c r="G72" s="2"/>
       <c r="H72" s="2"/>
     </row>
-    <row r="73" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:8" ht="15">
       <c r="A73" s="1"/>
       <c r="B73" s="2"/>
       <c r="E73" s="3"/>
@@ -2648,7 +2569,7 @@
       <c r="G73" s="2"/>
       <c r="H73" s="2"/>
     </row>
-    <row r="74" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:8" ht="15">
       <c r="A74" s="1"/>
       <c r="B74" s="2"/>
       <c r="E74" s="3"/>
@@ -2656,7 +2577,7 @@
       <c r="G74" s="2"/>
       <c r="H74" s="2"/>
     </row>
-    <row r="75" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:8" ht="15">
       <c r="A75" s="1"/>
       <c r="B75" s="2"/>
       <c r="E75" s="3"/>
@@ -2664,7 +2585,7 @@
       <c r="G75" s="2"/>
       <c r="H75" s="2"/>
     </row>
-    <row r="76" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:8" ht="15">
       <c r="A76" s="1"/>
       <c r="B76" s="2"/>
       <c r="E76" s="3"/>
@@ -2672,7 +2593,7 @@
       <c r="G76" s="2"/>
       <c r="H76" s="2"/>
     </row>
-    <row r="77" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:8" ht="15">
       <c r="A77" s="1"/>
       <c r="B77" s="2"/>
       <c r="E77" s="3"/>
@@ -2680,7 +2601,7 @@
       <c r="G77" s="2"/>
       <c r="H77" s="2"/>
     </row>
-    <row r="78" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:8" ht="15">
       <c r="A78" s="1"/>
       <c r="B78" s="2"/>
       <c r="E78" s="3"/>
@@ -2688,7 +2609,7 @@
       <c r="G78" s="2"/>
       <c r="H78" s="2"/>
     </row>
-    <row r="79" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:8" ht="15">
       <c r="A79" s="1"/>
       <c r="B79" s="2"/>
       <c r="E79" s="3"/>
@@ -2696,7 +2617,7 @@
       <c r="G79" s="2"/>
       <c r="H79" s="2"/>
     </row>
-    <row r="80" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:8" ht="15">
       <c r="A80" s="1"/>
       <c r="B80" s="2"/>
       <c r="E80" s="3"/>
@@ -2704,7 +2625,7 @@
       <c r="G80" s="2"/>
       <c r="H80" s="2"/>
     </row>
-    <row r="81" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:8" ht="15">
       <c r="A81" s="1"/>
       <c r="B81" s="2"/>
       <c r="E81" s="3"/>
@@ -2712,7 +2633,7 @@
       <c r="G81" s="2"/>
       <c r="H81" s="2"/>
     </row>
-    <row r="82" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:8" ht="15">
       <c r="A82" s="1"/>
       <c r="B82" s="2"/>
       <c r="E82" s="3"/>
@@ -2720,7 +2641,7 @@
       <c r="G82" s="2"/>
       <c r="H82" s="2"/>
     </row>
-    <row r="83" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:8" ht="15">
       <c r="A83" s="1"/>
       <c r="B83" s="2"/>
       <c r="E83" s="3"/>
@@ -2728,7 +2649,7 @@
       <c r="G83" s="2"/>
       <c r="H83" s="2"/>
     </row>
-    <row r="84" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:8" ht="15">
       <c r="A84" s="1"/>
       <c r="B84" s="2"/>
       <c r="E84" s="3"/>
@@ -2736,7 +2657,7 @@
       <c r="G84" s="2"/>
       <c r="H84" s="2"/>
     </row>
-    <row r="85" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:8" ht="15">
       <c r="A85" s="1"/>
       <c r="B85" s="2"/>
       <c r="E85" s="3"/>
@@ -2744,7 +2665,7 @@
       <c r="G85" s="2"/>
       <c r="H85" s="2"/>
     </row>
-    <row r="86" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:8" ht="15">
       <c r="A86" s="1"/>
       <c r="B86" s="2"/>
       <c r="E86" s="3"/>
@@ -2752,7 +2673,7 @@
       <c r="G86" s="2"/>
       <c r="H86" s="2"/>
     </row>
-    <row r="87" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:8" ht="15">
       <c r="A87" s="1"/>
       <c r="B87" s="2"/>
       <c r="E87" s="3"/>
@@ -2760,7 +2681,7 @@
       <c r="G87" s="2"/>
       <c r="H87" s="2"/>
     </row>
-    <row r="88" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:8">
       <c r="A88" s="1"/>
       <c r="B88" s="2"/>
       <c r="E88" s="3"/>
@@ -2768,7 +2689,7 @@
       <c r="G88" s="2"/>
       <c r="H88" s="2"/>
     </row>
-    <row r="89" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:8">
       <c r="A89" s="1"/>
       <c r="B89" s="2"/>
       <c r="E89" s="3"/>
@@ -2776,7 +2697,7 @@
       <c r="G89" s="2"/>
       <c r="H89" s="2"/>
     </row>
-    <row r="90" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:8">
       <c r="A90" s="1"/>
       <c r="B90" s="2"/>
       <c r="E90" s="3"/>
@@ -2784,7 +2705,7 @@
       <c r="G90" s="2"/>
       <c r="H90" s="2"/>
     </row>
-    <row r="91" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:8">
       <c r="A91" s="1"/>
       <c r="B91" s="2"/>
       <c r="E91" s="3"/>
@@ -2792,7 +2713,7 @@
       <c r="G91" s="2"/>
       <c r="H91" s="2"/>
     </row>
-    <row r="92" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:8">
       <c r="A92" s="1"/>
       <c r="B92" s="2"/>
       <c r="E92" s="3"/>
@@ -2800,7 +2721,7 @@
       <c r="G92" s="2"/>
       <c r="H92" s="2"/>
     </row>
-    <row r="93" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:8">
       <c r="A93" s="1"/>
       <c r="B93" s="2"/>
       <c r="E93" s="3"/>
@@ -2808,7 +2729,7 @@
       <c r="G93" s="2"/>
       <c r="H93" s="2"/>
     </row>
-    <row r="94" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:8">
       <c r="A94" s="1"/>
       <c r="B94" s="2"/>
       <c r="E94" s="3"/>
@@ -2816,7 +2737,7 @@
       <c r="G94" s="2"/>
       <c r="H94" s="2"/>
     </row>
-    <row r="95" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:8">
       <c r="A95" s="1"/>
       <c r="B95" s="2"/>
       <c r="E95" s="3"/>
@@ -2824,7 +2745,7 @@
       <c r="G95" s="2"/>
       <c r="H95" s="2"/>
     </row>
-    <row r="96" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:8">
       <c r="A96" s="1"/>
       <c r="B96" s="2"/>
       <c r="E96" s="3"/>
@@ -2832,7 +2753,7 @@
       <c r="G96" s="2"/>
       <c r="H96" s="2"/>
     </row>
-    <row r="97" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:8">
       <c r="A97" s="1"/>
       <c r="B97" s="2"/>
       <c r="E97" s="3"/>
@@ -2840,7 +2761,7 @@
       <c r="G97" s="2"/>
       <c r="H97" s="2"/>
     </row>
-    <row r="98" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:8">
       <c r="A98" s="1"/>
       <c r="B98" s="2"/>
       <c r="E98" s="3"/>
@@ -2848,7 +2769,7 @@
       <c r="G98" s="2"/>
       <c r="H98" s="2"/>
     </row>
-    <row r="99" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:8">
       <c r="A99" s="1"/>
       <c r="B99" s="2"/>
       <c r="E99" s="3"/>
@@ -2856,7 +2777,7 @@
       <c r="G99" s="2"/>
       <c r="H99" s="2"/>
     </row>
-    <row r="100" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:8">
       <c r="A100" s="1"/>
       <c r="B100" s="2"/>
       <c r="E100" s="3"/>
@@ -2899,19 +2820,19 @@
       <selection activeCell="D2" sqref="D2:D100"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col min="1" max="1" width="7.7109375" customWidth="1"/>
-    <col min="2" max="2" width="17.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="7.69921875" customWidth="1"/>
+    <col min="2" max="2" width="17.296875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.59765625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="9" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.85546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="23.5703125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="13.42578125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="19.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.8984375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="23.59765625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.3984375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="19.09765625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" ht="15.75">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
@@ -2937,7 +2858,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" ht="15">
       <c r="A2" s="1"/>
       <c r="B2" s="2"/>
       <c r="E2" s="3"/>
@@ -2945,7 +2866,7 @@
       <c r="G2" s="2"/>
       <c r="H2" s="2"/>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" ht="15">
       <c r="A3" s="1"/>
       <c r="B3" s="2"/>
       <c r="E3" s="3"/>
@@ -2953,7 +2874,7 @@
       <c r="G3" s="2"/>
       <c r="H3" s="2"/>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" ht="15">
       <c r="A4" s="1"/>
       <c r="B4" s="2"/>
       <c r="E4" s="3"/>
@@ -2961,7 +2882,7 @@
       <c r="G4" s="2"/>
       <c r="H4" s="2"/>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" ht="15">
       <c r="A5" s="1"/>
       <c r="B5" s="2"/>
       <c r="E5" s="3"/>
@@ -2969,7 +2890,7 @@
       <c r="G5" s="2"/>
       <c r="H5" s="2"/>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" ht="15">
       <c r="A6" s="1"/>
       <c r="B6" s="2"/>
       <c r="E6" s="3"/>
@@ -2977,7 +2898,7 @@
       <c r="G6" s="2"/>
       <c r="H6" s="2"/>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" ht="15">
       <c r="A7" s="1"/>
       <c r="B7" s="2"/>
       <c r="E7" s="3"/>
@@ -2985,7 +2906,7 @@
       <c r="G7" s="2"/>
       <c r="H7" s="2"/>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" ht="15">
       <c r="A8" s="1"/>
       <c r="B8" s="2"/>
       <c r="E8" s="3"/>
@@ -2993,7 +2914,7 @@
       <c r="G8" s="2"/>
       <c r="H8" s="2"/>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" ht="15">
       <c r="A9" s="1"/>
       <c r="B9" s="2"/>
       <c r="E9" s="3"/>
@@ -3001,7 +2922,7 @@
       <c r="G9" s="2"/>
       <c r="H9" s="2"/>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" ht="15">
       <c r="A10" s="1"/>
       <c r="B10" s="2"/>
       <c r="E10" s="3"/>
@@ -3009,7 +2930,7 @@
       <c r="G10" s="2"/>
       <c r="H10" s="2"/>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" ht="15">
       <c r="A11" s="1"/>
       <c r="B11" s="2"/>
       <c r="E11" s="3"/>
@@ -3017,7 +2938,7 @@
       <c r="G11" s="2"/>
       <c r="H11" s="2"/>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8" ht="15">
       <c r="A12" s="1"/>
       <c r="B12" s="2"/>
       <c r="E12" s="3"/>
@@ -3025,7 +2946,7 @@
       <c r="G12" s="2"/>
       <c r="H12" s="2"/>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8" ht="15">
       <c r="A13" s="1"/>
       <c r="B13" s="2"/>
       <c r="E13" s="3"/>
@@ -3033,7 +2954,7 @@
       <c r="G13" s="2"/>
       <c r="H13" s="2"/>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8" ht="15">
       <c r="A14" s="1"/>
       <c r="B14" s="2"/>
       <c r="E14" s="3"/>
@@ -3041,7 +2962,7 @@
       <c r="G14" s="2"/>
       <c r="H14" s="2"/>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8" ht="15">
       <c r="A15" s="1"/>
       <c r="B15" s="2"/>
       <c r="E15" s="3"/>
@@ -3049,7 +2970,7 @@
       <c r="G15" s="2"/>
       <c r="H15" s="2"/>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8" ht="15">
       <c r="A16" s="1"/>
       <c r="B16" s="2"/>
       <c r="E16" s="3"/>
@@ -3057,7 +2978,7 @@
       <c r="G16" s="2"/>
       <c r="H16" s="2"/>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:8" ht="15">
       <c r="A17" s="1"/>
       <c r="B17" s="2"/>
       <c r="E17" s="3"/>
@@ -3065,7 +2986,7 @@
       <c r="G17" s="2"/>
       <c r="H17" s="2"/>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:8" ht="15">
       <c r="A18" s="1"/>
       <c r="B18" s="2"/>
       <c r="E18" s="3"/>
@@ -3073,7 +2994,7 @@
       <c r="G18" s="2"/>
       <c r="H18" s="2"/>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:8" ht="15">
       <c r="A19" s="1"/>
       <c r="B19" s="2"/>
       <c r="E19" s="3"/>
@@ -3081,7 +3002,7 @@
       <c r="G19" s="2"/>
       <c r="H19" s="2"/>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:8" ht="15">
       <c r="A20" s="1"/>
       <c r="B20" s="2"/>
       <c r="E20" s="3"/>
@@ -3089,7 +3010,7 @@
       <c r="G20" s="2"/>
       <c r="H20" s="2"/>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:8" ht="15">
       <c r="A21" s="1"/>
       <c r="B21" s="2"/>
       <c r="E21" s="3"/>
@@ -3097,7 +3018,7 @@
       <c r="G21" s="2"/>
       <c r="H21" s="2"/>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:8" ht="15">
       <c r="A22" s="1"/>
       <c r="B22" s="2"/>
       <c r="E22" s="3"/>
@@ -3105,7 +3026,7 @@
       <c r="G22" s="2"/>
       <c r="H22" s="2"/>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:8" ht="15">
       <c r="A23" s="1"/>
       <c r="B23" s="2"/>
       <c r="E23" s="3"/>
@@ -3113,7 +3034,7 @@
       <c r="G23" s="2"/>
       <c r="H23" s="2"/>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:8" ht="15">
       <c r="A24" s="1"/>
       <c r="B24" s="2"/>
       <c r="E24" s="3"/>
@@ -3121,7 +3042,7 @@
       <c r="G24" s="2"/>
       <c r="H24" s="2"/>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:8" ht="15">
       <c r="A25" s="1"/>
       <c r="B25" s="2"/>
       <c r="E25" s="3"/>
@@ -3129,7 +3050,7 @@
       <c r="G25" s="2"/>
       <c r="H25" s="2"/>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:8" ht="15">
       <c r="A26" s="1"/>
       <c r="B26" s="2"/>
       <c r="E26" s="3"/>
@@ -3137,7 +3058,7 @@
       <c r="G26" s="2"/>
       <c r="H26" s="2"/>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:8" ht="15">
       <c r="A27" s="1"/>
       <c r="B27" s="2"/>
       <c r="E27" s="3"/>
@@ -3145,7 +3066,7 @@
       <c r="G27" s="2"/>
       <c r="H27" s="2"/>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:8" ht="15">
       <c r="A28" s="1"/>
       <c r="B28" s="2"/>
       <c r="E28" s="3"/>
@@ -3153,7 +3074,7 @@
       <c r="G28" s="2"/>
       <c r="H28" s="2"/>
     </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:8" ht="15">
       <c r="A29" s="1"/>
       <c r="B29" s="2"/>
       <c r="E29" s="3"/>
@@ -3161,7 +3082,7 @@
       <c r="G29" s="2"/>
       <c r="H29" s="2"/>
     </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:8" ht="15">
       <c r="A30" s="1"/>
       <c r="B30" s="2"/>
       <c r="E30" s="3"/>
@@ -3169,7 +3090,7 @@
       <c r="G30" s="2"/>
       <c r="H30" s="2"/>
     </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:8" ht="15">
       <c r="A31" s="1"/>
       <c r="B31" s="2"/>
       <c r="E31" s="3"/>
@@ -3177,7 +3098,7 @@
       <c r="G31" s="2"/>
       <c r="H31" s="2"/>
     </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:8" ht="15">
       <c r="A32" s="1"/>
       <c r="B32" s="2"/>
       <c r="E32" s="3"/>
@@ -3185,7 +3106,7 @@
       <c r="G32" s="2"/>
       <c r="H32" s="2"/>
     </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:8" ht="15">
       <c r="A33" s="1"/>
       <c r="B33" s="2"/>
       <c r="E33" s="3"/>
@@ -3193,7 +3114,7 @@
       <c r="G33" s="2"/>
       <c r="H33" s="2"/>
     </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:8" ht="15">
       <c r="A34" s="1"/>
       <c r="B34" s="2"/>
       <c r="E34" s="3"/>
@@ -3201,7 +3122,7 @@
       <c r="G34" s="2"/>
       <c r="H34" s="2"/>
     </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:8" ht="15">
       <c r="A35" s="1"/>
       <c r="B35" s="2"/>
       <c r="E35" s="3"/>
@@ -3209,7 +3130,7 @@
       <c r="G35" s="2"/>
       <c r="H35" s="2"/>
     </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:8" ht="15">
       <c r="A36" s="1"/>
       <c r="B36" s="2"/>
       <c r="E36" s="3"/>
@@ -3217,7 +3138,7 @@
       <c r="G36" s="2"/>
       <c r="H36" s="2"/>
     </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:8" ht="15">
       <c r="A37" s="1"/>
       <c r="B37" s="2"/>
       <c r="E37" s="3"/>
@@ -3225,7 +3146,7 @@
       <c r="G37" s="2"/>
       <c r="H37" s="2"/>
     </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:8" ht="15">
       <c r="A38" s="1"/>
       <c r="B38" s="2"/>
       <c r="E38" s="3"/>
@@ -3233,7 +3154,7 @@
       <c r="G38" s="2"/>
       <c r="H38" s="2"/>
     </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:8" ht="15">
       <c r="A39" s="1"/>
       <c r="B39" s="2"/>
       <c r="E39" s="3"/>
@@ -3241,7 +3162,7 @@
       <c r="G39" s="2"/>
       <c r="H39" s="2"/>
     </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:8" ht="15">
       <c r="A40" s="1"/>
       <c r="B40" s="2"/>
       <c r="E40" s="3"/>
@@ -3249,7 +3170,7 @@
       <c r="G40" s="2"/>
       <c r="H40" s="2"/>
     </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:8" ht="15">
       <c r="A41" s="1"/>
       <c r="B41" s="2"/>
       <c r="E41" s="3"/>
@@ -3257,7 +3178,7 @@
       <c r="G41" s="2"/>
       <c r="H41" s="2"/>
     </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:8" ht="15">
       <c r="A42" s="1"/>
       <c r="B42" s="2"/>
       <c r="E42" s="3"/>
@@ -3265,7 +3186,7 @@
       <c r="G42" s="2"/>
       <c r="H42" s="2"/>
     </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:8" ht="15">
       <c r="A43" s="1"/>
       <c r="B43" s="2"/>
       <c r="E43" s="3"/>
@@ -3273,7 +3194,7 @@
       <c r="G43" s="2"/>
       <c r="H43" s="2"/>
     </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:8" ht="15">
       <c r="A44" s="1"/>
       <c r="B44" s="2"/>
       <c r="E44" s="3"/>
@@ -3281,7 +3202,7 @@
       <c r="G44" s="2"/>
       <c r="H44" s="2"/>
     </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:8" ht="15">
       <c r="A45" s="1"/>
       <c r="B45" s="2"/>
       <c r="E45" s="3"/>
@@ -3289,7 +3210,7 @@
       <c r="G45" s="2"/>
       <c r="H45" s="2"/>
     </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:8" ht="15">
       <c r="A46" s="1"/>
       <c r="B46" s="2"/>
       <c r="E46" s="3"/>
@@ -3297,7 +3218,7 @@
       <c r="G46" s="2"/>
       <c r="H46" s="2"/>
     </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:8" ht="15">
       <c r="A47" s="1"/>
       <c r="B47" s="2"/>
       <c r="E47" s="3"/>
@@ -3305,7 +3226,7 @@
       <c r="G47" s="2"/>
       <c r="H47" s="2"/>
     </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:8" ht="15">
       <c r="A48" s="1"/>
       <c r="B48" s="2"/>
       <c r="E48" s="3"/>
@@ -3313,7 +3234,7 @@
       <c r="G48" s="2"/>
       <c r="H48" s="2"/>
     </row>
-    <row r="49" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:8" ht="15">
       <c r="A49" s="1"/>
       <c r="B49" s="2"/>
       <c r="E49" s="3"/>
@@ -3321,7 +3242,7 @@
       <c r="G49" s="2"/>
       <c r="H49" s="2"/>
     </row>
-    <row r="50" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:8" ht="15">
       <c r="A50" s="1"/>
       <c r="B50" s="2"/>
       <c r="E50" s="3"/>
@@ -3329,7 +3250,7 @@
       <c r="G50" s="2"/>
       <c r="H50" s="2"/>
     </row>
-    <row r="51" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:8" ht="15">
       <c r="A51" s="1"/>
       <c r="B51" s="2"/>
       <c r="E51" s="3"/>
@@ -3337,7 +3258,7 @@
       <c r="G51" s="2"/>
       <c r="H51" s="2"/>
     </row>
-    <row r="52" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:8" ht="15">
       <c r="A52" s="1"/>
       <c r="B52" s="2"/>
       <c r="E52" s="3"/>
@@ -3345,7 +3266,7 @@
       <c r="G52" s="2"/>
       <c r="H52" s="2"/>
     </row>
-    <row r="53" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:8" ht="15">
       <c r="A53" s="1"/>
       <c r="B53" s="2"/>
       <c r="E53" s="3"/>
@@ -3353,7 +3274,7 @@
       <c r="G53" s="2"/>
       <c r="H53" s="2"/>
     </row>
-    <row r="54" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:8" ht="15">
       <c r="A54" s="1"/>
       <c r="B54" s="2"/>
       <c r="E54" s="3"/>
@@ -3361,7 +3282,7 @@
       <c r="G54" s="2"/>
       <c r="H54" s="2"/>
     </row>
-    <row r="55" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:8" ht="15">
       <c r="A55" s="1"/>
       <c r="B55" s="2"/>
       <c r="E55" s="3"/>
@@ -3369,7 +3290,7 @@
       <c r="G55" s="2"/>
       <c r="H55" s="2"/>
     </row>
-    <row r="56" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:8" ht="15">
       <c r="A56" s="1"/>
       <c r="B56" s="2"/>
       <c r="E56" s="3"/>
@@ -3377,7 +3298,7 @@
       <c r="G56" s="2"/>
       <c r="H56" s="2"/>
     </row>
-    <row r="57" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:8" ht="15">
       <c r="A57" s="1"/>
       <c r="B57" s="2"/>
       <c r="E57" s="3"/>
@@ -3385,7 +3306,7 @@
       <c r="G57" s="2"/>
       <c r="H57" s="2"/>
     </row>
-    <row r="58" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:8" ht="15">
       <c r="A58" s="1"/>
       <c r="B58" s="2"/>
       <c r="E58" s="3"/>
@@ -3393,7 +3314,7 @@
       <c r="G58" s="2"/>
       <c r="H58" s="2"/>
     </row>
-    <row r="59" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:8" ht="15">
       <c r="A59" s="1"/>
       <c r="B59" s="2"/>
       <c r="E59" s="3"/>
@@ -3401,7 +3322,7 @@
       <c r="G59" s="2"/>
       <c r="H59" s="2"/>
     </row>
-    <row r="60" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:8" ht="15">
       <c r="A60" s="1"/>
       <c r="B60" s="2"/>
       <c r="E60" s="3"/>
@@ -3409,7 +3330,7 @@
       <c r="G60" s="2"/>
       <c r="H60" s="2"/>
     </row>
-    <row r="61" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:8" ht="15">
       <c r="A61" s="1"/>
       <c r="B61" s="2"/>
       <c r="E61" s="3"/>
@@ -3417,7 +3338,7 @@
       <c r="G61" s="2"/>
       <c r="H61" s="2"/>
     </row>
-    <row r="62" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:8" ht="15">
       <c r="A62" s="1"/>
       <c r="B62" s="2"/>
       <c r="E62" s="3"/>
@@ -3425,7 +3346,7 @@
       <c r="G62" s="2"/>
       <c r="H62" s="2"/>
     </row>
-    <row r="63" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:8" ht="15">
       <c r="A63" s="1"/>
       <c r="B63" s="2"/>
       <c r="E63" s="3"/>
@@ -3433,7 +3354,7 @@
       <c r="G63" s="2"/>
       <c r="H63" s="2"/>
     </row>
-    <row r="64" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:8" ht="15">
       <c r="A64" s="1"/>
       <c r="B64" s="2"/>
       <c r="E64" s="3"/>
@@ -3441,7 +3362,7 @@
       <c r="G64" s="2"/>
       <c r="H64" s="2"/>
     </row>
-    <row r="65" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:8" ht="15">
       <c r="A65" s="1"/>
       <c r="B65" s="2"/>
       <c r="E65" s="3"/>
@@ -3449,7 +3370,7 @@
       <c r="G65" s="2"/>
       <c r="H65" s="2"/>
     </row>
-    <row r="66" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:8" ht="15">
       <c r="A66" s="1"/>
       <c r="B66" s="2"/>
       <c r="E66" s="3"/>
@@ -3457,7 +3378,7 @@
       <c r="G66" s="2"/>
       <c r="H66" s="2"/>
     </row>
-    <row r="67" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:8" ht="15">
       <c r="A67" s="1"/>
       <c r="B67" s="2"/>
       <c r="E67" s="3"/>
@@ -3465,7 +3386,7 @@
       <c r="G67" s="2"/>
       <c r="H67" s="2"/>
     </row>
-    <row r="68" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:8" ht="15">
       <c r="A68" s="1"/>
       <c r="B68" s="2"/>
       <c r="E68" s="3"/>
@@ -3473,7 +3394,7 @@
       <c r="G68" s="2"/>
       <c r="H68" s="2"/>
     </row>
-    <row r="69" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:8" ht="15">
       <c r="A69" s="1"/>
       <c r="B69" s="2"/>
       <c r="E69" s="3"/>
@@ -3481,7 +3402,7 @@
       <c r="G69" s="2"/>
       <c r="H69" s="2"/>
     </row>
-    <row r="70" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:8" ht="15">
       <c r="A70" s="1"/>
       <c r="B70" s="2"/>
       <c r="E70" s="3"/>
@@ -3489,7 +3410,7 @@
       <c r="G70" s="2"/>
       <c r="H70" s="2"/>
     </row>
-    <row r="71" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:8" ht="15">
       <c r="A71" s="1"/>
       <c r="B71" s="2"/>
       <c r="E71" s="3"/>
@@ -3497,7 +3418,7 @@
       <c r="G71" s="2"/>
       <c r="H71" s="2"/>
     </row>
-    <row r="72" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:8" ht="15">
       <c r="A72" s="1"/>
       <c r="B72" s="2"/>
       <c r="E72" s="3"/>
@@ -3505,7 +3426,7 @@
       <c r="G72" s="2"/>
       <c r="H72" s="2"/>
     </row>
-    <row r="73" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:8" ht="15">
       <c r="A73" s="1"/>
       <c r="B73" s="2"/>
       <c r="E73" s="3"/>
@@ -3513,7 +3434,7 @@
       <c r="G73" s="2"/>
       <c r="H73" s="2"/>
     </row>
-    <row r="74" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:8" ht="15">
       <c r="A74" s="1"/>
       <c r="B74" s="2"/>
       <c r="E74" s="3"/>
@@ -3521,7 +3442,7 @@
       <c r="G74" s="2"/>
       <c r="H74" s="2"/>
     </row>
-    <row r="75" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:8" ht="15">
       <c r="A75" s="1"/>
       <c r="B75" s="2"/>
       <c r="E75" s="3"/>
@@ -3529,7 +3450,7 @@
       <c r="G75" s="2"/>
       <c r="H75" s="2"/>
     </row>
-    <row r="76" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:8" ht="15">
       <c r="A76" s="1"/>
       <c r="B76" s="2"/>
       <c r="E76" s="3"/>
@@ -3537,7 +3458,7 @@
       <c r="G76" s="2"/>
       <c r="H76" s="2"/>
     </row>
-    <row r="77" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:8" ht="15">
       <c r="A77" s="1"/>
       <c r="B77" s="2"/>
       <c r="E77" s="3"/>
@@ -3545,7 +3466,7 @@
       <c r="G77" s="2"/>
       <c r="H77" s="2"/>
     </row>
-    <row r="78" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:8" ht="15">
       <c r="A78" s="1"/>
       <c r="B78" s="2"/>
       <c r="E78" s="3"/>
@@ -3553,7 +3474,7 @@
       <c r="G78" s="2"/>
       <c r="H78" s="2"/>
     </row>
-    <row r="79" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:8" ht="15">
       <c r="A79" s="1"/>
       <c r="B79" s="2"/>
       <c r="E79" s="3"/>
@@ -3561,7 +3482,7 @@
       <c r="G79" s="2"/>
       <c r="H79" s="2"/>
     </row>
-    <row r="80" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:8" ht="15">
       <c r="A80" s="1"/>
       <c r="B80" s="2"/>
       <c r="E80" s="3"/>
@@ -3569,7 +3490,7 @@
       <c r="G80" s="2"/>
       <c r="H80" s="2"/>
     </row>
-    <row r="81" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:8" ht="15">
       <c r="A81" s="1"/>
       <c r="B81" s="2"/>
       <c r="E81" s="3"/>
@@ -3577,7 +3498,7 @@
       <c r="G81" s="2"/>
       <c r="H81" s="2"/>
     </row>
-    <row r="82" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:8" ht="15">
       <c r="A82" s="1"/>
       <c r="B82" s="2"/>
       <c r="E82" s="3"/>
@@ -3585,7 +3506,7 @@
       <c r="G82" s="2"/>
       <c r="H82" s="2"/>
     </row>
-    <row r="83" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:8" ht="15">
       <c r="A83" s="1"/>
       <c r="B83" s="2"/>
       <c r="E83" s="3"/>
@@ -3593,7 +3514,7 @@
       <c r="G83" s="2"/>
       <c r="H83" s="2"/>
     </row>
-    <row r="84" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:8" ht="15">
       <c r="A84" s="1"/>
       <c r="B84" s="2"/>
       <c r="E84" s="3"/>
@@ -3601,7 +3522,7 @@
       <c r="G84" s="2"/>
       <c r="H84" s="2"/>
     </row>
-    <row r="85" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:8" ht="15">
       <c r="A85" s="1"/>
       <c r="B85" s="2"/>
       <c r="E85" s="3"/>
@@ -3609,7 +3530,7 @@
       <c r="G85" s="2"/>
       <c r="H85" s="2"/>
     </row>
-    <row r="86" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:8" ht="15">
       <c r="A86" s="1"/>
       <c r="B86" s="2"/>
       <c r="E86" s="3"/>
@@ -3617,7 +3538,7 @@
       <c r="G86" s="2"/>
       <c r="H86" s="2"/>
     </row>
-    <row r="87" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:8" ht="15">
       <c r="A87" s="1"/>
       <c r="B87" s="2"/>
       <c r="E87" s="3"/>
@@ -3625,7 +3546,7 @@
       <c r="G87" s="2"/>
       <c r="H87" s="2"/>
     </row>
-    <row r="88" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:8">
       <c r="A88" s="1"/>
       <c r="B88" s="2"/>
       <c r="E88" s="3"/>
@@ -3633,7 +3554,7 @@
       <c r="G88" s="2"/>
       <c r="H88" s="2"/>
     </row>
-    <row r="89" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:8">
       <c r="A89" s="1"/>
       <c r="B89" s="2"/>
       <c r="E89" s="3"/>
@@ -3641,7 +3562,7 @@
       <c r="G89" s="2"/>
       <c r="H89" s="2"/>
     </row>
-    <row r="90" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:8">
       <c r="A90" s="1"/>
       <c r="B90" s="2"/>
       <c r="E90" s="3"/>
@@ -3649,7 +3570,7 @@
       <c r="G90" s="2"/>
       <c r="H90" s="2"/>
     </row>
-    <row r="91" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:8">
       <c r="A91" s="1"/>
       <c r="B91" s="2"/>
       <c r="E91" s="3"/>
@@ -3657,7 +3578,7 @@
       <c r="G91" s="2"/>
       <c r="H91" s="2"/>
     </row>
-    <row r="92" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:8">
       <c r="A92" s="1"/>
       <c r="B92" s="2"/>
       <c r="E92" s="3"/>
@@ -3665,7 +3586,7 @@
       <c r="G92" s="2"/>
       <c r="H92" s="2"/>
     </row>
-    <row r="93" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:8">
       <c r="A93" s="1"/>
       <c r="B93" s="2"/>
       <c r="E93" s="3"/>
@@ -3673,7 +3594,7 @@
       <c r="G93" s="2"/>
       <c r="H93" s="2"/>
     </row>
-    <row r="94" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:8">
       <c r="A94" s="1"/>
       <c r="B94" s="2"/>
       <c r="E94" s="3"/>
@@ -3681,7 +3602,7 @@
       <c r="G94" s="2"/>
       <c r="H94" s="2"/>
     </row>
-    <row r="95" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:8">
       <c r="A95" s="1"/>
       <c r="B95" s="2"/>
       <c r="E95" s="3"/>
@@ -3689,7 +3610,7 @@
       <c r="G95" s="2"/>
       <c r="H95" s="2"/>
     </row>
-    <row r="96" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:8">
       <c r="A96" s="1"/>
       <c r="B96" s="2"/>
       <c r="E96" s="3"/>
@@ -3697,7 +3618,7 @@
       <c r="G96" s="2"/>
       <c r="H96" s="2"/>
     </row>
-    <row r="97" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:8">
       <c r="A97" s="1"/>
       <c r="B97" s="2"/>
       <c r="E97" s="3"/>
@@ -3705,7 +3626,7 @@
       <c r="G97" s="2"/>
       <c r="H97" s="2"/>
     </row>
-    <row r="98" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:8">
       <c r="A98" s="1"/>
       <c r="B98" s="2"/>
       <c r="E98" s="3"/>
@@ -3713,7 +3634,7 @@
       <c r="G98" s="2"/>
       <c r="H98" s="2"/>
     </row>
-    <row r="99" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:8">
       <c r="A99" s="1"/>
       <c r="B99" s="2"/>
       <c r="E99" s="3"/>
@@ -3721,7 +3642,7 @@
       <c r="G99" s="2"/>
       <c r="H99" s="2"/>
     </row>
-    <row r="100" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:8">
       <c r="A100" s="1"/>
       <c r="B100" s="2"/>
       <c r="E100" s="3"/>
@@ -3764,21 +3685,21 @@
       <selection activeCell="P21" sqref="P21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col min="1" max="1" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="19.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.5703125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.09765625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.8984375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.8984375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19.3984375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.59765625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.59765625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="9" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="17.85546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="17.8984375" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="17" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="19.140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="19.09765625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" ht="15.75">
       <c r="A1" s="7" t="s">
         <v>8</v>
       </c>
@@ -3810,7 +3731,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" ht="15">
       <c r="A2" s="2"/>
       <c r="B2" s="8"/>
       <c r="D2" s="2"/>
@@ -3818,7 +3739,7 @@
       <c r="I2" s="8"/>
       <c r="J2" s="2"/>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" ht="15">
       <c r="A3" s="2"/>
       <c r="B3" s="8"/>
       <c r="D3" s="2"/>
@@ -3826,7 +3747,7 @@
       <c r="I3" s="8"/>
       <c r="J3" s="2"/>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" ht="15">
       <c r="A4" s="2"/>
       <c r="B4" s="8"/>
       <c r="D4" s="2"/>
@@ -3834,7 +3755,7 @@
       <c r="I4" s="8"/>
       <c r="J4" s="2"/>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" ht="15">
       <c r="A5" s="2"/>
       <c r="B5" s="8"/>
       <c r="D5" s="2"/>
@@ -3842,7 +3763,7 @@
       <c r="I5" s="8"/>
       <c r="J5" s="2"/>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" ht="15">
       <c r="A6" s="2"/>
       <c r="B6" s="8"/>
       <c r="D6" s="2"/>
@@ -3850,7 +3771,7 @@
       <c r="I6" s="8"/>
       <c r="J6" s="2"/>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10" ht="15">
       <c r="A7" s="2"/>
       <c r="B7" s="8"/>
       <c r="D7" s="2"/>
@@ -3858,7 +3779,7 @@
       <c r="I7" s="8"/>
       <c r="J7" s="2"/>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10" ht="15">
       <c r="A8" s="2"/>
       <c r="B8" s="8"/>
       <c r="D8" s="2"/>
@@ -3866,7 +3787,7 @@
       <c r="I8" s="8"/>
       <c r="J8" s="2"/>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10" ht="15">
       <c r="A9" s="2"/>
       <c r="B9" s="8"/>
       <c r="D9" s="2"/>
@@ -3874,7 +3795,7 @@
       <c r="I9" s="8"/>
       <c r="J9" s="2"/>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:10" ht="15">
       <c r="A10" s="2"/>
       <c r="B10" s="8"/>
       <c r="D10" s="2"/>
@@ -3882,7 +3803,7 @@
       <c r="I10" s="8"/>
       <c r="J10" s="2"/>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:10" ht="15">
       <c r="A11" s="2"/>
       <c r="B11" s="8"/>
       <c r="D11" s="2"/>
@@ -3890,7 +3811,7 @@
       <c r="I11" s="8"/>
       <c r="J11" s="2"/>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:10" ht="15">
       <c r="A12" s="2"/>
       <c r="B12" s="8"/>
       <c r="D12" s="2"/>
@@ -3898,7 +3819,7 @@
       <c r="I12" s="8"/>
       <c r="J12" s="2"/>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:10" ht="15">
       <c r="A13" s="2"/>
       <c r="B13" s="8"/>
       <c r="D13" s="2"/>
@@ -3906,7 +3827,7 @@
       <c r="I13" s="8"/>
       <c r="J13" s="2"/>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:10" ht="15">
       <c r="A14" s="2"/>
       <c r="B14" s="8"/>
       <c r="D14" s="2"/>
@@ -3914,7 +3835,7 @@
       <c r="I14" s="8"/>
       <c r="J14" s="2"/>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:10" ht="15">
       <c r="A15" s="2"/>
       <c r="B15" s="8"/>
       <c r="D15" s="2"/>
@@ -3922,7 +3843,7 @@
       <c r="I15" s="8"/>
       <c r="J15" s="2"/>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:10" ht="15">
       <c r="A16" s="2"/>
       <c r="B16" s="8"/>
       <c r="D16" s="2"/>
@@ -3930,7 +3851,7 @@
       <c r="I16" s="8"/>
       <c r="J16" s="2"/>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:10" ht="15">
       <c r="A17" s="2"/>
       <c r="B17" s="8"/>
       <c r="D17" s="2"/>
@@ -3938,7 +3859,7 @@
       <c r="I17" s="8"/>
       <c r="J17" s="2"/>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:10" ht="15">
       <c r="A18" s="2"/>
       <c r="B18" s="8"/>
       <c r="D18" s="2"/>
@@ -3946,7 +3867,7 @@
       <c r="I18" s="8"/>
       <c r="J18" s="2"/>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:10" ht="15">
       <c r="A19" s="2"/>
       <c r="B19" s="8"/>
       <c r="D19" s="2"/>
@@ -3954,7 +3875,7 @@
       <c r="I19" s="8"/>
       <c r="J19" s="2"/>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:10" ht="15">
       <c r="A20" s="2"/>
       <c r="B20" s="8"/>
       <c r="D20" s="2"/>
@@ -3962,7 +3883,7 @@
       <c r="I20" s="8"/>
       <c r="J20" s="2"/>
     </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:10" ht="15">
       <c r="A21" s="2"/>
       <c r="B21" s="8"/>
       <c r="D21" s="2"/>
@@ -3970,7 +3891,7 @@
       <c r="I21" s="8"/>
       <c r="J21" s="2"/>
     </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:10" ht="15">
       <c r="A22" s="2"/>
       <c r="B22" s="8"/>
       <c r="D22" s="2"/>
@@ -3978,7 +3899,7 @@
       <c r="I22" s="8"/>
       <c r="J22" s="2"/>
     </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:10" ht="15">
       <c r="A23" s="2"/>
       <c r="B23" s="8"/>
       <c r="D23" s="2"/>
@@ -3986,7 +3907,7 @@
       <c r="I23" s="8"/>
       <c r="J23" s="2"/>
     </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:10" ht="15">
       <c r="A24" s="2"/>
       <c r="B24" s="8"/>
       <c r="D24" s="2"/>
@@ -3994,7 +3915,7 @@
       <c r="I24" s="8"/>
       <c r="J24" s="2"/>
     </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:10" ht="15">
       <c r="A25" s="2"/>
       <c r="B25" s="8"/>
       <c r="D25" s="2"/>
@@ -4002,7 +3923,7 @@
       <c r="I25" s="8"/>
       <c r="J25" s="2"/>
     </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:10">
       <c r="A26" s="2"/>
       <c r="B26" s="8"/>
       <c r="D26" s="2"/>
@@ -4010,7 +3931,7 @@
       <c r="I26" s="8"/>
       <c r="J26" s="2"/>
     </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:10">
       <c r="A27" s="2"/>
       <c r="B27" s="8"/>
       <c r="D27" s="2"/>
@@ -4018,7 +3939,7 @@
       <c r="I27" s="8"/>
       <c r="J27" s="2"/>
     </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:10">
       <c r="A28" s="2"/>
       <c r="B28" s="8"/>
       <c r="D28" s="2"/>
@@ -4026,7 +3947,7 @@
       <c r="I28" s="8"/>
       <c r="J28" s="2"/>
     </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:10">
       <c r="A29" s="2"/>
       <c r="B29" s="8"/>
       <c r="D29" s="2"/>
@@ -4034,7 +3955,7 @@
       <c r="I29" s="8"/>
       <c r="J29" s="2"/>
     </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:10">
       <c r="A30" s="2"/>
       <c r="B30" s="8"/>
       <c r="D30" s="2"/>
@@ -4042,7 +3963,7 @@
       <c r="I30" s="8"/>
       <c r="J30" s="2"/>
     </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:10">
       <c r="A31" s="2"/>
       <c r="B31" s="8"/>
       <c r="D31" s="2"/>
@@ -4050,7 +3971,7 @@
       <c r="I31" s="8"/>
       <c r="J31" s="2"/>
     </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:10">
       <c r="A32" s="2"/>
       <c r="B32" s="8"/>
       <c r="D32" s="2"/>
@@ -4058,7 +3979,7 @@
       <c r="I32" s="8"/>
       <c r="J32" s="2"/>
     </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:10">
       <c r="A33" s="2"/>
       <c r="B33" s="8"/>
       <c r="D33" s="2"/>
@@ -4066,7 +3987,7 @@
       <c r="I33" s="8"/>
       <c r="J33" s="2"/>
     </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:10">
       <c r="A34" s="2"/>
       <c r="B34" s="8"/>
       <c r="D34" s="2"/>
@@ -4074,7 +3995,7 @@
       <c r="I34" s="8"/>
       <c r="J34" s="2"/>
     </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:10">
       <c r="A35" s="2"/>
       <c r="B35" s="8"/>
       <c r="D35" s="2"/>
@@ -4082,7 +4003,7 @@
       <c r="I35" s="8"/>
       <c r="J35" s="2"/>
     </row>
-    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:10">
       <c r="A36" s="2"/>
       <c r="B36" s="8"/>
       <c r="D36" s="2"/>
@@ -4090,7 +4011,7 @@
       <c r="I36" s="8"/>
       <c r="J36" s="2"/>
     </row>
-    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:10">
       <c r="A37" s="2"/>
       <c r="B37" s="8"/>
       <c r="D37" s="2"/>
@@ -4098,7 +4019,7 @@
       <c r="I37" s="8"/>
       <c r="J37" s="2"/>
     </row>
-    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:10">
       <c r="A38" s="2"/>
       <c r="B38" s="8"/>
       <c r="D38" s="2"/>
@@ -4106,7 +4027,7 @@
       <c r="I38" s="8"/>
       <c r="J38" s="2"/>
     </row>
-    <row r="39" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:10">
       <c r="A39" s="2"/>
       <c r="B39" s="8"/>
       <c r="D39" s="2"/>
@@ -4114,7 +4035,7 @@
       <c r="I39" s="8"/>
       <c r="J39" s="2"/>
     </row>
-    <row r="40" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:10">
       <c r="A40" s="2"/>
       <c r="B40" s="8"/>
       <c r="D40" s="2"/>
@@ -4122,7 +4043,7 @@
       <c r="I40" s="8"/>
       <c r="J40" s="2"/>
     </row>
-    <row r="41" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:10">
       <c r="A41" s="2"/>
       <c r="B41" s="8"/>
       <c r="D41" s="2"/>
@@ -4130,7 +4051,7 @@
       <c r="I41" s="8"/>
       <c r="J41" s="2"/>
     </row>
-    <row r="42" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:10">
       <c r="A42" s="2"/>
       <c r="B42" s="8"/>
       <c r="D42" s="2"/>
@@ -4138,7 +4059,7 @@
       <c r="I42" s="8"/>
       <c r="J42" s="2"/>
     </row>
-    <row r="43" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:10">
       <c r="A43" s="2"/>
       <c r="B43" s="8"/>
       <c r="D43" s="2"/>
@@ -4146,7 +4067,7 @@
       <c r="I43" s="8"/>
       <c r="J43" s="2"/>
     </row>
-    <row r="44" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:10">
       <c r="A44" s="2"/>
       <c r="B44" s="8"/>
       <c r="D44" s="2"/>
@@ -4154,7 +4075,7 @@
       <c r="I44" s="8"/>
       <c r="J44" s="2"/>
     </row>
-    <row r="45" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:10">
       <c r="A45" s="2"/>
       <c r="B45" s="8"/>
       <c r="D45" s="2"/>
@@ -4162,7 +4083,7 @@
       <c r="I45" s="8"/>
       <c r="J45" s="2"/>
     </row>
-    <row r="46" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:10">
       <c r="A46" s="2"/>
       <c r="B46" s="8"/>
       <c r="D46" s="2"/>
@@ -4170,7 +4091,7 @@
       <c r="I46" s="8"/>
       <c r="J46" s="2"/>
     </row>
-    <row r="47" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:10">
       <c r="A47" s="2"/>
       <c r="B47" s="8"/>
       <c r="D47" s="2"/>
@@ -4178,7 +4099,7 @@
       <c r="I47" s="8"/>
       <c r="J47" s="2"/>
     </row>
-    <row r="48" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:10">
       <c r="A48" s="2"/>
       <c r="B48" s="8"/>
       <c r="D48" s="2"/>
@@ -4186,7 +4107,7 @@
       <c r="I48" s="8"/>
       <c r="J48" s="2"/>
     </row>
-    <row r="49" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:10">
       <c r="A49" s="2"/>
       <c r="B49" s="8"/>
       <c r="D49" s="2"/>
@@ -4194,7 +4115,7 @@
       <c r="I49" s="8"/>
       <c r="J49" s="2"/>
     </row>
-    <row r="50" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:10">
       <c r="A50" s="2"/>
       <c r="B50" s="8"/>
       <c r="D50" s="2"/>
@@ -4202,7 +4123,7 @@
       <c r="I50" s="8"/>
       <c r="J50" s="2"/>
     </row>
-    <row r="51" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:10">
       <c r="A51" s="2"/>
       <c r="B51" s="8"/>
       <c r="D51" s="2"/>
@@ -4210,7 +4131,7 @@
       <c r="I51" s="8"/>
       <c r="J51" s="2"/>
     </row>
-    <row r="52" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:10">
       <c r="A52" s="2"/>
       <c r="B52" s="8"/>
       <c r="D52" s="2"/>
@@ -4218,7 +4139,7 @@
       <c r="I52" s="8"/>
       <c r="J52" s="2"/>
     </row>
-    <row r="53" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:10">
       <c r="A53" s="2"/>
       <c r="B53" s="8"/>
       <c r="D53" s="2"/>
@@ -4226,7 +4147,7 @@
       <c r="I53" s="8"/>
       <c r="J53" s="2"/>
     </row>
-    <row r="54" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:10">
       <c r="A54" s="2"/>
       <c r="B54" s="8"/>
       <c r="D54" s="2"/>
@@ -4234,7 +4155,7 @@
       <c r="I54" s="8"/>
       <c r="J54" s="2"/>
     </row>
-    <row r="55" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:10">
       <c r="A55" s="2"/>
       <c r="B55" s="8"/>
       <c r="D55" s="2"/>
@@ -4242,7 +4163,7 @@
       <c r="I55" s="8"/>
       <c r="J55" s="2"/>
     </row>
-    <row r="56" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:10">
       <c r="A56" s="2"/>
       <c r="B56" s="8"/>
       <c r="D56" s="2"/>
@@ -4250,7 +4171,7 @@
       <c r="I56" s="8"/>
       <c r="J56" s="2"/>
     </row>
-    <row r="57" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:10">
       <c r="A57" s="2"/>
       <c r="B57" s="8"/>
       <c r="D57" s="2"/>
@@ -4258,7 +4179,7 @@
       <c r="I57" s="8"/>
       <c r="J57" s="2"/>
     </row>
-    <row r="58" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:10">
       <c r="A58" s="2"/>
       <c r="B58" s="8"/>
       <c r="D58" s="2"/>
@@ -4266,7 +4187,7 @@
       <c r="I58" s="8"/>
       <c r="J58" s="2"/>
     </row>
-    <row r="59" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:10">
       <c r="A59" s="2"/>
       <c r="B59" s="8"/>
       <c r="D59" s="2"/>
@@ -4274,7 +4195,7 @@
       <c r="I59" s="8"/>
       <c r="J59" s="2"/>
     </row>
-    <row r="60" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:10">
       <c r="A60" s="2"/>
       <c r="B60" s="8"/>
       <c r="D60" s="2"/>
@@ -4282,7 +4203,7 @@
       <c r="I60" s="8"/>
       <c r="J60" s="2"/>
     </row>
-    <row r="61" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:10">
       <c r="A61" s="2"/>
       <c r="B61" s="8"/>
       <c r="D61" s="2"/>
@@ -4290,7 +4211,7 @@
       <c r="I61" s="8"/>
       <c r="J61" s="2"/>
     </row>
-    <row r="62" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:10">
       <c r="A62" s="2"/>
       <c r="B62" s="8"/>
       <c r="D62" s="2"/>
@@ -4298,7 +4219,7 @@
       <c r="I62" s="8"/>
       <c r="J62" s="2"/>
     </row>
-    <row r="63" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:10">
       <c r="A63" s="2"/>
       <c r="B63" s="8"/>
       <c r="D63" s="2"/>
@@ -4306,7 +4227,7 @@
       <c r="I63" s="8"/>
       <c r="J63" s="2"/>
     </row>
-    <row r="64" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:10">
       <c r="A64" s="2"/>
       <c r="B64" s="8"/>
       <c r="D64" s="2"/>
@@ -4314,7 +4235,7 @@
       <c r="I64" s="8"/>
       <c r="J64" s="2"/>
     </row>
-    <row r="65" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:10">
       <c r="A65" s="2"/>
       <c r="B65" s="8"/>
       <c r="D65" s="2"/>
@@ -4322,7 +4243,7 @@
       <c r="I65" s="8"/>
       <c r="J65" s="2"/>
     </row>
-    <row r="66" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:10">
       <c r="A66" s="2"/>
       <c r="B66" s="8"/>
       <c r="D66" s="2"/>
@@ -4330,7 +4251,7 @@
       <c r="I66" s="8"/>
       <c r="J66" s="2"/>
     </row>
-    <row r="67" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:10">
       <c r="A67" s="2"/>
       <c r="B67" s="8"/>
       <c r="D67" s="2"/>
@@ -4338,7 +4259,7 @@
       <c r="I67" s="8"/>
       <c r="J67" s="2"/>
     </row>
-    <row r="68" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:10">
       <c r="A68" s="2"/>
       <c r="B68" s="8"/>
       <c r="D68" s="2"/>
@@ -4346,7 +4267,7 @@
       <c r="I68" s="8"/>
       <c r="J68" s="2"/>
     </row>
-    <row r="69" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:10">
       <c r="A69" s="2"/>
       <c r="B69" s="8"/>
       <c r="D69" s="2"/>
@@ -4354,7 +4275,7 @@
       <c r="I69" s="8"/>
       <c r="J69" s="2"/>
     </row>
-    <row r="70" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:10">
       <c r="A70" s="2"/>
       <c r="B70" s="8"/>
       <c r="D70" s="2"/>
@@ -4362,7 +4283,7 @@
       <c r="I70" s="8"/>
       <c r="J70" s="2"/>
     </row>
-    <row r="71" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:10">
       <c r="A71" s="2"/>
       <c r="B71" s="8"/>
       <c r="D71" s="2"/>
@@ -4370,7 +4291,7 @@
       <c r="I71" s="8"/>
       <c r="J71" s="2"/>
     </row>
-    <row r="72" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:10">
       <c r="A72" s="2"/>
       <c r="B72" s="8"/>
       <c r="D72" s="2"/>
@@ -4378,7 +4299,7 @@
       <c r="I72" s="8"/>
       <c r="J72" s="2"/>
     </row>
-    <row r="73" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:10">
       <c r="A73" s="2"/>
       <c r="B73" s="8"/>
       <c r="D73" s="2"/>
@@ -4386,7 +4307,7 @@
       <c r="I73" s="8"/>
       <c r="J73" s="2"/>
     </row>
-    <row r="74" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:10">
       <c r="A74" s="2"/>
       <c r="B74" s="8"/>
       <c r="D74" s="2"/>
@@ -4394,7 +4315,7 @@
       <c r="I74" s="8"/>
       <c r="J74" s="2"/>
     </row>
-    <row r="75" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:10">
       <c r="A75" s="2"/>
       <c r="B75" s="8"/>
       <c r="D75" s="2"/>
@@ -4402,7 +4323,7 @@
       <c r="I75" s="8"/>
       <c r="J75" s="2"/>
     </row>
-    <row r="76" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:10">
       <c r="A76" s="2"/>
       <c r="B76" s="8"/>
       <c r="D76" s="2"/>
@@ -4410,7 +4331,7 @@
       <c r="I76" s="8"/>
       <c r="J76" s="2"/>
     </row>
-    <row r="77" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:10">
       <c r="A77" s="2"/>
       <c r="B77" s="8"/>
       <c r="D77" s="2"/>
@@ -4418,7 +4339,7 @@
       <c r="I77" s="8"/>
       <c r="J77" s="2"/>
     </row>
-    <row r="78" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:10">
       <c r="A78" s="2"/>
       <c r="B78" s="8"/>
       <c r="D78" s="2"/>
@@ -4426,7 +4347,7 @@
       <c r="I78" s="8"/>
       <c r="J78" s="2"/>
     </row>
-    <row r="79" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:10">
       <c r="A79" s="2"/>
       <c r="B79" s="8"/>
       <c r="D79" s="2"/>
@@ -4434,7 +4355,7 @@
       <c r="I79" s="8"/>
       <c r="J79" s="2"/>
     </row>
-    <row r="80" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:10">
       <c r="A80" s="2"/>
       <c r="B80" s="8"/>
       <c r="D80" s="2"/>
@@ -4442,7 +4363,7 @@
       <c r="I80" s="8"/>
       <c r="J80" s="2"/>
     </row>
-    <row r="81" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:10">
       <c r="A81" s="2"/>
       <c r="B81" s="8"/>
       <c r="D81" s="2"/>
@@ -4450,7 +4371,7 @@
       <c r="I81" s="8"/>
       <c r="J81" s="2"/>
     </row>
-    <row r="82" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:10">
       <c r="A82" s="2"/>
       <c r="B82" s="8"/>
       <c r="D82" s="2"/>
@@ -4458,7 +4379,7 @@
       <c r="I82" s="8"/>
       <c r="J82" s="2"/>
     </row>
-    <row r="83" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:10">
       <c r="A83" s="2"/>
       <c r="B83" s="8"/>
       <c r="D83" s="2"/>
@@ -4466,7 +4387,7 @@
       <c r="I83" s="8"/>
       <c r="J83" s="2"/>
     </row>
-    <row r="84" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:10">
       <c r="A84" s="2"/>
       <c r="B84" s="8"/>
       <c r="D84" s="2"/>
@@ -4474,7 +4395,7 @@
       <c r="I84" s="8"/>
       <c r="J84" s="2"/>
     </row>
-    <row r="85" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:10">
       <c r="A85" s="2"/>
       <c r="B85" s="8"/>
       <c r="D85" s="2"/>
@@ -4482,7 +4403,7 @@
       <c r="I85" s="8"/>
       <c r="J85" s="2"/>
     </row>
-    <row r="86" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:10">
       <c r="A86" s="2"/>
       <c r="B86" s="8"/>
       <c r="D86" s="2"/>
@@ -4490,7 +4411,7 @@
       <c r="I86" s="8"/>
       <c r="J86" s="2"/>
     </row>
-    <row r="87" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:10">
       <c r="A87" s="2"/>
       <c r="B87" s="8"/>
       <c r="D87" s="2"/>
@@ -4498,7 +4419,7 @@
       <c r="I87" s="8"/>
       <c r="J87" s="2"/>
     </row>
-    <row r="88" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:10">
       <c r="A88" s="2"/>
       <c r="B88" s="8"/>
       <c r="D88" s="2"/>
@@ -4506,7 +4427,7 @@
       <c r="I88" s="8"/>
       <c r="J88" s="2"/>
     </row>
-    <row r="89" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:10">
       <c r="A89" s="2"/>
       <c r="B89" s="8"/>
       <c r="D89" s="2"/>
@@ -4514,7 +4435,7 @@
       <c r="I89" s="8"/>
       <c r="J89" s="2"/>
     </row>
-    <row r="90" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:10">
       <c r="A90" s="2"/>
       <c r="B90" s="8"/>
       <c r="D90" s="2"/>
@@ -4522,7 +4443,7 @@
       <c r="I90" s="8"/>
       <c r="J90" s="2"/>
     </row>
-    <row r="91" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:10">
       <c r="A91" s="2"/>
       <c r="B91" s="8"/>
       <c r="D91" s="2"/>
@@ -4530,7 +4451,7 @@
       <c r="I91" s="8"/>
       <c r="J91" s="2"/>
     </row>
-    <row r="92" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:10">
       <c r="A92" s="2"/>
       <c r="B92" s="8"/>
       <c r="D92" s="2"/>
@@ -4538,7 +4459,7 @@
       <c r="I92" s="8"/>
       <c r="J92" s="2"/>
     </row>
-    <row r="93" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:10">
       <c r="A93" s="2"/>
       <c r="B93" s="8"/>
       <c r="D93" s="2"/>
@@ -4546,7 +4467,7 @@
       <c r="I93" s="8"/>
       <c r="J93" s="2"/>
     </row>
-    <row r="94" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:10">
       <c r="A94" s="2"/>
       <c r="B94" s="8"/>
       <c r="D94" s="2"/>
@@ -4554,7 +4475,7 @@
       <c r="I94" s="8"/>
       <c r="J94" s="2"/>
     </row>
-    <row r="95" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:10">
       <c r="A95" s="2"/>
       <c r="B95" s="8"/>
       <c r="D95" s="2"/>
@@ -4562,7 +4483,7 @@
       <c r="I95" s="8"/>
       <c r="J95" s="2"/>
     </row>
-    <row r="96" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:10">
       <c r="A96" s="2"/>
       <c r="B96" s="8"/>
       <c r="D96" s="2"/>
@@ -4570,7 +4491,7 @@
       <c r="I96" s="8"/>
       <c r="J96" s="2"/>
     </row>
-    <row r="97" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:10">
       <c r="A97" s="2"/>
       <c r="B97" s="8"/>
       <c r="D97" s="2"/>
@@ -4578,7 +4499,7 @@
       <c r="I97" s="8"/>
       <c r="J97" s="2"/>
     </row>
-    <row r="98" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:10">
       <c r="A98" s="2"/>
       <c r="B98" s="8"/>
       <c r="D98" s="2"/>
@@ -4586,7 +4507,7 @@
       <c r="I98" s="8"/>
       <c r="J98" s="2"/>
     </row>
-    <row r="99" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:10">
       <c r="A99" s="2"/>
       <c r="B99" s="8"/>
       <c r="D99" s="2"/>
@@ -4594,7 +4515,7 @@
       <c r="I99" s="8"/>
       <c r="J99" s="2"/>
     </row>
-    <row r="100" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:10">
       <c r="A100" s="2"/>
       <c r="B100" s="8"/>
       <c r="D100" s="2"/>

</xml_diff>

<commit_message>
Enrollment services - exception handling with custom pages and validations
</commit_message>
<xml_diff>
--- a/PR&IR.xlsx
+++ b/PR&IR.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28730"/>
-  <workbookPr defaultThemeVersion="202300"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jayshil.singh\Desktop\Personal Files\CS415_A3\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\avichal avneel nath\Documents\Semester 7\CS415\A3\CS415_A3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{804CE9A9-4F24-4029-A552-382870E1B724}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{446B9638-145F-47A9-8E17-E54F5F829A5D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{BFA1E21A-08FA-4F02-8C25-33C81C8EE970}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{BFA1E21A-08FA-4F02-8C25-33C81C8EE970}"/>
   </bookViews>
   <sheets>
     <sheet name="Avichal" sheetId="1" r:id="rId1"/>
@@ -24,23 +24,12 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="35">
   <si>
     <t>Date</t>
   </si>
@@ -89,16 +78,96 @@
   <si>
     <t>Date Resolved</t>
   </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Developed core features of Enrollment Services module: course enrollment functionality, enrolled courses view, and course drop with validation. Integrated basic routing and tested module using </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial Unicode MS"/>
+        <family val="2"/>
+      </rPr>
+      <t>run_enrollment_services.py</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>.</t>
+    </r>
+  </si>
+  <si>
+    <t>Completed</t>
+  </si>
+  <si>
+    <t>Connect Enrollment with Fees &amp; Holds and Profile modules</t>
+  </si>
+  <si>
+    <t>Implemented drop course validation logic; routing structure established and tested successfully</t>
+  </si>
+  <si>
+    <t>AAN</t>
+  </si>
+  <si>
+    <t>Resolved TemplateNotFound errors by relocating templates directory to root.
+Integrated Bootstrap and Font Awesome into Fees &amp; Holds UI for improved layout and clarity.
+Installed SQL Server and SQL Server Management Studio (SSMS), verified successful setup</t>
+  </si>
+  <si>
+    <t>setup backend logic for course enrollment</t>
+  </si>
+  <si>
+    <t>All major issues addressed. Application UI improved and backend setup completed with SQL Server and SSMS installation.</t>
+  </si>
+  <si>
+    <t>Researched: how microservices can use different languages while being under one same system + how python will actually CRUD with SSMS( via Sqlalchemy.</t>
+  </si>
+  <si>
+    <t>Read Docker Documentation. Watched docker tutorials. Coded for course enrollment Logic</t>
+  </si>
+  <si>
+    <t>research backend logic + config</t>
+  </si>
+  <si>
+    <t>research on pulling data from firebase and pushing to sql server</t>
+  </si>
+  <si>
+    <t>complete pending ToDos</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Resolved merge conflict and synced with main. Researched on sqlalchemy vs pyodbc. Custom validation for enrollment services. </t>
+  </si>
+  <si>
+    <t>Exception handling for all routes and research on DB</t>
+  </si>
+  <si>
+    <t>Best Wishes w/ Backend.</t>
+  </si>
+  <si>
+    <t>Completed custom exception handling for all routes and custom validtion for enrollment services</t>
+  </si>
+  <si>
+    <t>Fee and Hold services routing exceptions and validations</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Stay Healthy Aviiii. Don’t get sick </t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
-    <numFmt numFmtId="170" formatCode="h"/>
-    <numFmt numFmtId="171" formatCode="d/mm/yyyy;@"/>
+    <numFmt numFmtId="164" formatCode="h"/>
+    <numFmt numFmtId="165" formatCode="d/mm/yyyy;@"/>
   </numFmts>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -111,6 +180,12 @@
       <color theme="1"/>
       <name val="Times New Roman"/>
       <family val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial Unicode MS"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -133,16 +208,19 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="170" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="14" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="171" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -152,7 +230,7 @@
       <numFmt numFmtId="30" formatCode="@"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="171" formatCode="d/mm/yyyy;@"/>
+      <numFmt numFmtId="165" formatCode="d/mm/yyyy;@"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="30" formatCode="@"/>
@@ -161,49 +239,10 @@
       <numFmt numFmtId="30" formatCode="@"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="171" formatCode="d/mm/yyyy;@"/>
+      <numFmt numFmtId="165" formatCode="d/mm/yyyy;@"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="30" formatCode="@"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <name val="Times New Roman"/>
-        <family val="1"/>
-        <scheme val="none"/>
-      </font>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="171" formatCode="d/mm/yyyy;@"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="170" formatCode="h"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="14" formatCode="0.00%"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="19" formatCode="m/d/yyyy"/>
     </dxf>
     <dxf>
       <font>
@@ -230,7 +269,7 @@
       <numFmt numFmtId="30" formatCode="@"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="170" formatCode="h"/>
+      <numFmt numFmtId="164" formatCode="h"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="14" formatCode="0.00%"/>
@@ -239,7 +278,7 @@
       <numFmt numFmtId="30" formatCode="@"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="19" formatCode="m/d/yyyy"/>
+      <numFmt numFmtId="166" formatCode="m/d/yyyy"/>
     </dxf>
     <dxf>
       <font>
@@ -266,7 +305,7 @@
       <numFmt numFmtId="30" formatCode="@"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="170" formatCode="h"/>
+      <numFmt numFmtId="164" formatCode="h"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="14" formatCode="0.00%"/>
@@ -275,22 +314,7 @@
       <numFmt numFmtId="30" formatCode="@"/>
     </dxf>
     <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <name val="Times New Roman"/>
-        <family val="1"/>
-        <scheme val="none"/>
-      </font>
+      <numFmt numFmtId="166" formatCode="m/d/yyyy"/>
     </dxf>
     <dxf>
       <font>
@@ -317,7 +341,7 @@
       <numFmt numFmtId="30" formatCode="@"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="170" formatCode="h"/>
+      <numFmt numFmtId="164" formatCode="h"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="14" formatCode="0.00%"/>
@@ -326,7 +350,61 @@
       <numFmt numFmtId="30" formatCode="@"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="19" formatCode="m/d/yyyy"/>
+      <numFmt numFmtId="165" formatCode="d/mm/yyyy;@"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Times New Roman"/>
+        <family val="1"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="h"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="14" formatCode="0.00%"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="166" formatCode="m/d/yyyy"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Times New Roman"/>
+        <family val="1"/>
+        <scheme val="none"/>
+      </font>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -342,7 +420,7 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{9FACB7F7-F35A-492E-AAF4-C8AD07A65A4F}" name="Table1" displayName="Table1" ref="A1:H100" totalsRowShown="0" headerRowDxfId="28">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{9FACB7F7-F35A-492E-AAF4-C8AD07A65A4F}" name="Table1" displayName="Table1" ref="A1:H100" totalsRowShown="0" headerRowDxfId="34">
   <autoFilter ref="A1:H100" xr:uid="{9FACB7F7-F35A-492E-AAF4-C8AD07A65A4F}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
@@ -354,14 +432,14 @@
     <filterColumn colId="7" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="8">
-    <tableColumn id="1" xr3:uid="{022F0CCA-D3AD-4C41-96AC-23A1F1ACD784}" name="Date" dataDxfId="34"/>
-    <tableColumn id="2" xr3:uid="{37EC747A-FF52-4BB8-9E7B-6658170B560E}" name="Member Name" dataDxfId="33"/>
+    <tableColumn id="1" xr3:uid="{022F0CCA-D3AD-4C41-96AC-23A1F1ACD784}" name="Date" dataDxfId="33"/>
+    <tableColumn id="2" xr3:uid="{37EC747A-FF52-4BB8-9E7B-6658170B560E}" name="Member Name" dataDxfId="32"/>
     <tableColumn id="3" xr3:uid="{595E07A7-B79C-490D-94F8-CC8A9548AAAE}" name="Task/Activity"/>
     <tableColumn id="4" xr3:uid="{399451D6-2EBE-4B51-8C25-09283BEE7B49}" name="Status"/>
-    <tableColumn id="5" xr3:uid="{951691AA-F5B7-4E87-94DD-56C88DDA7F01}" name="% Complete" dataDxfId="32"/>
-    <tableColumn id="6" xr3:uid="{5173E32D-1D51-4EE1-B4EB-015C386C7E1D}" name="Hours Worked Today" dataDxfId="31"/>
-    <tableColumn id="7" xr3:uid="{9793C2C7-1239-4777-8672-318111FFC5D8}" name="Next Steps" dataDxfId="30"/>
-    <tableColumn id="8" xr3:uid="{46550E96-F4E9-4167-888B-2889A1FA646A}" name="Notes/Comments" dataDxfId="29"/>
+    <tableColumn id="5" xr3:uid="{951691AA-F5B7-4E87-94DD-56C88DDA7F01}" name="% Complete" dataDxfId="31"/>
+    <tableColumn id="6" xr3:uid="{5173E32D-1D51-4EE1-B4EB-015C386C7E1D}" name="Hours Worked Today" dataDxfId="30"/>
+    <tableColumn id="7" xr3:uid="{9793C2C7-1239-4777-8672-318111FFC5D8}" name="Next Steps" dataDxfId="29"/>
+    <tableColumn id="8" xr3:uid="{46550E96-F4E9-4167-888B-2889A1FA646A}" name="Notes/Comments" dataDxfId="28"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium26" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -380,21 +458,21 @@
     <filterColumn colId="7" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="8">
-    <tableColumn id="1" xr3:uid="{80182F43-8CEA-4E5A-AE23-4E131CE1B1B1}" name="Date" dataDxfId="7"/>
-    <tableColumn id="2" xr3:uid="{55A78D6C-890A-4502-A184-DEEFF14BB82E}" name="Member Name" dataDxfId="26"/>
+    <tableColumn id="1" xr3:uid="{80182F43-8CEA-4E5A-AE23-4E131CE1B1B1}" name="Date" dataDxfId="26"/>
+    <tableColumn id="2" xr3:uid="{55A78D6C-890A-4502-A184-DEEFF14BB82E}" name="Member Name" dataDxfId="25"/>
     <tableColumn id="3" xr3:uid="{57B9A516-E930-4C06-A589-24182A37BA85}" name="Task/Activity"/>
     <tableColumn id="4" xr3:uid="{A7CD18E8-808E-43EA-A960-7EDF2D2AB452}" name="Status"/>
-    <tableColumn id="5" xr3:uid="{A9BAB96D-D5FD-4C0D-A277-6E052D27EC3A}" name="% Complete" dataDxfId="25"/>
-    <tableColumn id="6" xr3:uid="{4EBDEBD4-A02D-4266-88BC-5E6088167CE4}" name="Hours Worked Today" dataDxfId="24"/>
-    <tableColumn id="7" xr3:uid="{88484166-6833-4A6B-B292-081E908E7876}" name="Next Steps" dataDxfId="23"/>
-    <tableColumn id="8" xr3:uid="{65034E84-46C0-4115-A351-A3C28C7B9EE1}" name="Notes/Comments" dataDxfId="22"/>
+    <tableColumn id="5" xr3:uid="{A9BAB96D-D5FD-4C0D-A277-6E052D27EC3A}" name="% Complete" dataDxfId="24"/>
+    <tableColumn id="6" xr3:uid="{4EBDEBD4-A02D-4266-88BC-5E6088167CE4}" name="Hours Worked Today" dataDxfId="23"/>
+    <tableColumn id="7" xr3:uid="{88484166-6833-4A6B-B292-081E908E7876}" name="Next Steps" dataDxfId="22"/>
+    <tableColumn id="8" xr3:uid="{65034E84-46C0-4115-A351-A3C28C7B9EE1}" name="Notes/Comments" dataDxfId="21"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium26" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{D9A2FBFA-47C8-4A27-8A35-991BC77E93AD}" name="Table14" displayName="Table14" ref="A1:H100" totalsRowShown="0" headerRowDxfId="21">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{D9A2FBFA-47C8-4A27-8A35-991BC77E93AD}" name="Table14" displayName="Table14" ref="A1:H100" totalsRowShown="0" headerRowDxfId="20">
   <autoFilter ref="A1:H100" xr:uid="{D9A2FBFA-47C8-4A27-8A35-991BC77E93AD}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
@@ -406,21 +484,21 @@
     <filterColumn colId="7" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="8">
-    <tableColumn id="1" xr3:uid="{9DF80C4D-D075-4428-A54F-FD6AD093D08C}" name="Date" dataDxfId="20"/>
-    <tableColumn id="2" xr3:uid="{EBFC72C6-272F-4910-98B7-AD481D68F5CF}" name="Member Name" dataDxfId="19"/>
+    <tableColumn id="1" xr3:uid="{9DF80C4D-D075-4428-A54F-FD6AD093D08C}" name="Date" dataDxfId="19"/>
+    <tableColumn id="2" xr3:uid="{EBFC72C6-272F-4910-98B7-AD481D68F5CF}" name="Member Name" dataDxfId="18"/>
     <tableColumn id="3" xr3:uid="{9F5B3984-7002-4FEA-8B81-D2D8284783D7}" name="Task/Activity"/>
     <tableColumn id="4" xr3:uid="{5F85F44B-886F-440F-9E69-8335A039C2E6}" name="Status"/>
-    <tableColumn id="5" xr3:uid="{AF0043ED-9EF2-470B-9735-7321011714BA}" name="% Complete" dataDxfId="18"/>
-    <tableColumn id="6" xr3:uid="{4F961AD8-B86B-411C-BB04-8D7EE4DD134D}" name="Hours Worked Today" dataDxfId="17"/>
-    <tableColumn id="7" xr3:uid="{34EBB1FC-FFD7-47AB-A959-A220B742401C}" name="Next Steps" dataDxfId="16"/>
-    <tableColumn id="8" xr3:uid="{128DAA9E-15FB-4BB9-B76B-4A920C859038}" name="Notes/Comments" dataDxfId="15"/>
+    <tableColumn id="5" xr3:uid="{AF0043ED-9EF2-470B-9735-7321011714BA}" name="% Complete" dataDxfId="17"/>
+    <tableColumn id="6" xr3:uid="{4F961AD8-B86B-411C-BB04-8D7EE4DD134D}" name="Hours Worked Today" dataDxfId="16"/>
+    <tableColumn id="7" xr3:uid="{34EBB1FC-FFD7-47AB-A959-A220B742401C}" name="Next Steps" dataDxfId="15"/>
+    <tableColumn id="8" xr3:uid="{128DAA9E-15FB-4BB9-B76B-4A920C859038}" name="Notes/Comments" dataDxfId="14"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium26" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{646C4EC7-41A3-4570-9D38-06D55FDE20F6}" name="Table15" displayName="Table15" ref="A1:H100" totalsRowShown="0" headerRowDxfId="14">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{646C4EC7-41A3-4570-9D38-06D55FDE20F6}" name="Table15" displayName="Table15" ref="A1:H100" totalsRowShown="0" headerRowDxfId="13">
   <autoFilter ref="A1:H100" xr:uid="{646C4EC7-41A3-4570-9D38-06D55FDE20F6}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
@@ -432,14 +510,14 @@
     <filterColumn colId="7" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="8">
-    <tableColumn id="1" xr3:uid="{13D6CE41-CF73-478C-B7F6-3B0C25C48DFD}" name="Date" dataDxfId="13"/>
-    <tableColumn id="2" xr3:uid="{E468B109-F9F1-48D8-BECE-0F7015DD8D95}" name="Member Name" dataDxfId="12"/>
+    <tableColumn id="1" xr3:uid="{13D6CE41-CF73-478C-B7F6-3B0C25C48DFD}" name="Date" dataDxfId="12"/>
+    <tableColumn id="2" xr3:uid="{E468B109-F9F1-48D8-BECE-0F7015DD8D95}" name="Member Name" dataDxfId="11"/>
     <tableColumn id="3" xr3:uid="{279E5366-E900-45EE-80D9-5446A85E61AD}" name="Task/Activity"/>
     <tableColumn id="4" xr3:uid="{63D996BE-E8E2-4186-8CD4-49EAB9AA8847}" name="Status"/>
-    <tableColumn id="5" xr3:uid="{2FF82CF3-E17A-4896-9C9C-7339D28CD4A7}" name="% Complete" dataDxfId="11"/>
-    <tableColumn id="6" xr3:uid="{67DCB379-6881-4BBC-A633-BD51853A9B6B}" name="Hours Worked Today" dataDxfId="10"/>
-    <tableColumn id="7" xr3:uid="{91C8F225-F251-45F2-BC41-843547B77A6F}" name="Next Steps" dataDxfId="9"/>
-    <tableColumn id="8" xr3:uid="{EEAB1D68-5668-4B1F-8473-D3A49DA7E015}" name="Notes/Comments" dataDxfId="8"/>
+    <tableColumn id="5" xr3:uid="{2FF82CF3-E17A-4896-9C9C-7339D28CD4A7}" name="% Complete" dataDxfId="10"/>
+    <tableColumn id="6" xr3:uid="{67DCB379-6881-4BBC-A633-BD51853A9B6B}" name="Hours Worked Today" dataDxfId="9"/>
+    <tableColumn id="7" xr3:uid="{91C8F225-F251-45F2-BC41-843547B77A6F}" name="Next Steps" dataDxfId="8"/>
+    <tableColumn id="8" xr3:uid="{EEAB1D68-5668-4B1F-8473-D3A49DA7E015}" name="Notes/Comments" dataDxfId="7"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium26" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -821,32 +899,32 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{37EAA098-74C6-4411-B7E2-26AD2DCBC3F0}">
-  <dimension ref="A1:H1"/>
+  <dimension ref="A1:H28"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="K1" sqref="K1:T100"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H7" sqref="H7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="8.7265625" style="1"/>
-    <col min="2" max="2" width="15.54296875" style="2" customWidth="1"/>
-    <col min="3" max="3" width="13.36328125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.08984375" style="3" customWidth="1"/>
-    <col min="6" max="6" width="20.90625" style="4" customWidth="1"/>
-    <col min="7" max="7" width="12.1796875" style="2" customWidth="1"/>
-    <col min="8" max="8" width="17.36328125" style="2" customWidth="1"/>
-    <col min="11" max="11" width="9.1796875" customWidth="1"/>
-    <col min="12" max="12" width="13.26953125" customWidth="1"/>
-    <col min="13" max="13" width="11.453125" customWidth="1"/>
-    <col min="14" max="14" width="17.453125" customWidth="1"/>
-    <col min="16" max="16" width="9.1796875" customWidth="1"/>
-    <col min="18" max="18" width="16.54296875" customWidth="1"/>
-    <col min="19" max="19" width="14.7265625" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="16.90625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.5703125" style="2" customWidth="1"/>
+    <col min="3" max="3" width="58" customWidth="1"/>
+    <col min="5" max="5" width="13.140625" style="3" customWidth="1"/>
+    <col min="6" max="6" width="20.85546875" style="4" customWidth="1"/>
+    <col min="7" max="7" width="34.85546875" style="2" customWidth="1"/>
+    <col min="8" max="8" width="43.42578125" style="2" customWidth="1"/>
+    <col min="11" max="11" width="9.140625" customWidth="1"/>
+    <col min="12" max="12" width="13.28515625" customWidth="1"/>
+    <col min="13" max="13" width="11.42578125" customWidth="1"/>
+    <col min="14" max="14" width="17.42578125" customWidth="1"/>
+    <col min="16" max="16" width="9.140625" customWidth="1"/>
+    <col min="18" max="18" width="16.5703125" customWidth="1"/>
+    <col min="19" max="19" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="16.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
@@ -871,6 +949,216 @@
       <c r="H1" s="7" t="s">
         <v>7</v>
       </c>
+    </row>
+    <row r="2" spans="1:8" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A2" s="1">
+        <v>45786</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="C2" t="s">
+        <v>16</v>
+      </c>
+      <c r="D2" t="s">
+        <v>17</v>
+      </c>
+      <c r="E2" s="3">
+        <v>1</v>
+      </c>
+      <c r="F2">
+        <v>4</v>
+      </c>
+      <c r="G2" t="s">
+        <v>18</v>
+      </c>
+      <c r="H2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" ht="120" x14ac:dyDescent="0.25">
+      <c r="A3" s="1">
+        <v>45787</v>
+      </c>
+      <c r="C3" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="D3" t="s">
+        <v>17</v>
+      </c>
+      <c r="E3">
+        <v>100</v>
+      </c>
+      <c r="F3">
+        <v>3</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="H3" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4" s="1">
+        <v>45788</v>
+      </c>
+      <c r="C4" t="s">
+        <v>24</v>
+      </c>
+      <c r="D4" t="s">
+        <v>17</v>
+      </c>
+      <c r="E4">
+        <v>90</v>
+      </c>
+      <c r="F4">
+        <v>2</v>
+      </c>
+      <c r="G4" s="2" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" ht="76.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="1">
+        <v>45789</v>
+      </c>
+      <c r="C5" t="s">
+        <v>25</v>
+      </c>
+      <c r="D5" t="s">
+        <v>17</v>
+      </c>
+      <c r="E5">
+        <v>100</v>
+      </c>
+      <c r="F5">
+        <v>3</v>
+      </c>
+      <c r="G5" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="H5" s="2" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A6" s="1">
+        <v>45790</v>
+      </c>
+      <c r="C6" t="s">
+        <v>29</v>
+      </c>
+      <c r="D6" t="s">
+        <v>17</v>
+      </c>
+      <c r="E6">
+        <v>100</v>
+      </c>
+      <c r="F6">
+        <v>5</v>
+      </c>
+      <c r="G6" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="H6" s="2" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A7" s="1">
+        <v>45791</v>
+      </c>
+      <c r="C7" t="s">
+        <v>32</v>
+      </c>
+      <c r="D7" t="s">
+        <v>17</v>
+      </c>
+      <c r="E7">
+        <v>100</v>
+      </c>
+      <c r="F7">
+        <v>2</v>
+      </c>
+      <c r="G7" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="H7" s="2" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="E8"/>
+      <c r="F8"/>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="E9"/>
+      <c r="F9"/>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="E10"/>
+      <c r="F10"/>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="E11"/>
+      <c r="F11"/>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="E12"/>
+      <c r="F12"/>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="E13"/>
+      <c r="F13"/>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="E14"/>
+      <c r="F14"/>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="E15"/>
+      <c r="F15"/>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="E16"/>
+      <c r="F16"/>
+    </row>
+    <row r="17" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F17"/>
+    </row>
+    <row r="18" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F18"/>
+    </row>
+    <row r="19" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F19"/>
+    </row>
+    <row r="20" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F20"/>
+    </row>
+    <row r="21" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F21"/>
+    </row>
+    <row r="22" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F22"/>
+    </row>
+    <row r="23" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F23"/>
+    </row>
+    <row r="24" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F24"/>
+    </row>
+    <row r="25" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F25"/>
+    </row>
+    <row r="26" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F26"/>
+    </row>
+    <row r="27" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F27"/>
+    </row>
+    <row r="28" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F28"/>
     </row>
   </sheetData>
   <dataValidations count="4">
@@ -885,16 +1173,17 @@
       <formula1>1</formula1>
       <formula2>24</formula2>
     </dataValidation>
-    <dataValidation type="list" errorStyle="warning" showInputMessage="1" showErrorMessage="1" errorTitle="Select Status" error="Fill in Status to proccessd " sqref="D2:D16" xr:uid="{C06F6745-3BEF-4E36-9959-47AACC93D371}">
+    <dataValidation type="list" errorStyle="warning" showInputMessage="1" showErrorMessage="1" errorTitle="Select Status" error="Fill in Status to proccessd " sqref="D3:D16" xr:uid="{C06F6745-3BEF-4E36-9959-47AACC93D371}">
       <formula1>"To Do,In Progress,Completed,Blocked"</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
   <ignoredErrors>
-    <ignoredError sqref="D2:D6 D7:D16" listDataValidation="1"/>
+    <ignoredError sqref="D8:D16" listDataValidation="1"/>
   </ignoredErrors>
   <tableParts count="1">
-    <tablePart r:id="rId1"/>
+    <tablePart r:id="rId2"/>
   </tableParts>
 </worksheet>
 </file>
@@ -903,23 +1192,23 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3BDA6702-5DDF-42FB-988E-13FBEB26F5C9}">
   <dimension ref="A1:H100"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I34" sqref="I34"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="7.7265625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="17.26953125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.6328125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.5703125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="9" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.81640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="23.6328125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="13.36328125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="19.1796875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="23.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="19.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
@@ -945,15 +1234,13 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="8"/>
       <c r="B2" s="2"/>
       <c r="E2" s="3"/>
-      <c r="F2" s="4"/>
       <c r="G2" s="2"/>
-      <c r="H2" s="2"/>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="8"/>
       <c r="B3" s="2"/>
       <c r="E3" s="3"/>
@@ -961,7 +1248,7 @@
       <c r="G3" s="2"/>
       <c r="H3" s="2"/>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="8"/>
       <c r="B4" s="2"/>
       <c r="E4" s="3"/>
@@ -969,7 +1256,7 @@
       <c r="G4" s="2"/>
       <c r="H4" s="2"/>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="8"/>
       <c r="B5" s="2"/>
       <c r="E5" s="3"/>
@@ -977,7 +1264,7 @@
       <c r="G5" s="2"/>
       <c r="H5" s="2"/>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="8"/>
       <c r="B6" s="2"/>
       <c r="E6" s="3"/>
@@ -985,7 +1272,7 @@
       <c r="G6" s="2"/>
       <c r="H6" s="2"/>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="8"/>
       <c r="B7" s="2"/>
       <c r="E7" s="3"/>
@@ -993,7 +1280,7 @@
       <c r="G7" s="2"/>
       <c r="H7" s="2"/>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="8"/>
       <c r="B8" s="2"/>
       <c r="E8" s="3"/>
@@ -1001,7 +1288,7 @@
       <c r="G8" s="2"/>
       <c r="H8" s="2"/>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="8"/>
       <c r="B9" s="2"/>
       <c r="E9" s="3"/>
@@ -1009,7 +1296,7 @@
       <c r="G9" s="2"/>
       <c r="H9" s="2"/>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="8"/>
       <c r="B10" s="2"/>
       <c r="E10" s="3"/>
@@ -1017,7 +1304,7 @@
       <c r="G10" s="2"/>
       <c r="H10" s="2"/>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="8"/>
       <c r="B11" s="2"/>
       <c r="E11" s="3"/>
@@ -1025,7 +1312,7 @@
       <c r="G11" s="2"/>
       <c r="H11" s="2"/>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="8"/>
       <c r="B12" s="2"/>
       <c r="E12" s="3"/>
@@ -1033,7 +1320,7 @@
       <c r="G12" s="2"/>
       <c r="H12" s="2"/>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="8"/>
       <c r="B13" s="2"/>
       <c r="E13" s="3"/>
@@ -1041,7 +1328,7 @@
       <c r="G13" s="2"/>
       <c r="H13" s="2"/>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" s="8"/>
       <c r="B14" s="2"/>
       <c r="E14" s="3"/>
@@ -1049,7 +1336,7 @@
       <c r="G14" s="2"/>
       <c r="H14" s="2"/>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" s="8"/>
       <c r="B15" s="2"/>
       <c r="E15" s="3"/>
@@ -1057,7 +1344,7 @@
       <c r="G15" s="2"/>
       <c r="H15" s="2"/>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" s="8"/>
       <c r="B16" s="2"/>
       <c r="E16" s="3"/>
@@ -1065,7 +1352,7 @@
       <c r="G16" s="2"/>
       <c r="H16" s="2"/>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" s="8"/>
       <c r="B17" s="2"/>
       <c r="E17" s="3"/>
@@ -1073,7 +1360,7 @@
       <c r="G17" s="2"/>
       <c r="H17" s="2"/>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" s="8"/>
       <c r="B18" s="2"/>
       <c r="E18" s="3"/>
@@ -1081,7 +1368,7 @@
       <c r="G18" s="2"/>
       <c r="H18" s="2"/>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" s="8"/>
       <c r="B19" s="2"/>
       <c r="E19" s="3"/>
@@ -1089,7 +1376,7 @@
       <c r="G19" s="2"/>
       <c r="H19" s="2"/>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" s="8"/>
       <c r="B20" s="2"/>
       <c r="E20" s="3"/>
@@ -1097,7 +1384,7 @@
       <c r="G20" s="2"/>
       <c r="H20" s="2"/>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" s="8"/>
       <c r="B21" s="2"/>
       <c r="E21" s="3"/>
@@ -1105,7 +1392,7 @@
       <c r="G21" s="2"/>
       <c r="H21" s="2"/>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" s="8"/>
       <c r="B22" s="2"/>
       <c r="E22" s="3"/>
@@ -1113,7 +1400,7 @@
       <c r="G22" s="2"/>
       <c r="H22" s="2"/>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" s="8"/>
       <c r="B23" s="2"/>
       <c r="E23" s="3"/>
@@ -1121,7 +1408,7 @@
       <c r="G23" s="2"/>
       <c r="H23" s="2"/>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24" s="8"/>
       <c r="B24" s="2"/>
       <c r="E24" s="3"/>
@@ -1129,7 +1416,7 @@
       <c r="G24" s="2"/>
       <c r="H24" s="2"/>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25" s="8"/>
       <c r="B25" s="2"/>
       <c r="E25" s="3"/>
@@ -1137,7 +1424,7 @@
       <c r="G25" s="2"/>
       <c r="H25" s="2"/>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26" s="8"/>
       <c r="B26" s="2"/>
       <c r="E26" s="3"/>
@@ -1145,7 +1432,7 @@
       <c r="G26" s="2"/>
       <c r="H26" s="2"/>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A27" s="8"/>
       <c r="B27" s="2"/>
       <c r="E27" s="3"/>
@@ -1153,7 +1440,7 @@
       <c r="G27" s="2"/>
       <c r="H27" s="2"/>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A28" s="8"/>
       <c r="B28" s="2"/>
       <c r="E28" s="3"/>
@@ -1161,7 +1448,7 @@
       <c r="G28" s="2"/>
       <c r="H28" s="2"/>
     </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A29" s="8"/>
       <c r="B29" s="2"/>
       <c r="E29" s="3"/>
@@ -1169,7 +1456,7 @@
       <c r="G29" s="2"/>
       <c r="H29" s="2"/>
     </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A30" s="8"/>
       <c r="B30" s="2"/>
       <c r="E30" s="3"/>
@@ -1177,7 +1464,7 @@
       <c r="G30" s="2"/>
       <c r="H30" s="2"/>
     </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A31" s="8"/>
       <c r="B31" s="2"/>
       <c r="E31" s="3"/>
@@ -1185,7 +1472,7 @@
       <c r="G31" s="2"/>
       <c r="H31" s="2"/>
     </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A32" s="8"/>
       <c r="B32" s="2"/>
       <c r="E32" s="3"/>
@@ -1193,7 +1480,7 @@
       <c r="G32" s="2"/>
       <c r="H32" s="2"/>
     </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A33" s="8"/>
       <c r="B33" s="2"/>
       <c r="E33" s="3"/>
@@ -1201,7 +1488,7 @@
       <c r="G33" s="2"/>
       <c r="H33" s="2"/>
     </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A34" s="8"/>
       <c r="B34" s="2"/>
       <c r="E34" s="3"/>
@@ -1209,7 +1496,7 @@
       <c r="G34" s="2"/>
       <c r="H34" s="2"/>
     </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A35" s="8"/>
       <c r="B35" s="2"/>
       <c r="E35" s="3"/>
@@ -1217,7 +1504,7 @@
       <c r="G35" s="2"/>
       <c r="H35" s="2"/>
     </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A36" s="8"/>
       <c r="B36" s="2"/>
       <c r="E36" s="3"/>
@@ -1225,7 +1512,7 @@
       <c r="G36" s="2"/>
       <c r="H36" s="2"/>
     </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A37" s="8"/>
       <c r="B37" s="2"/>
       <c r="E37" s="3"/>
@@ -1233,7 +1520,7 @@
       <c r="G37" s="2"/>
       <c r="H37" s="2"/>
     </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A38" s="8"/>
       <c r="B38" s="2"/>
       <c r="E38" s="3"/>
@@ -1241,7 +1528,7 @@
       <c r="G38" s="2"/>
       <c r="H38" s="2"/>
     </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A39" s="8"/>
       <c r="B39" s="2"/>
       <c r="E39" s="3"/>
@@ -1249,7 +1536,7 @@
       <c r="G39" s="2"/>
       <c r="H39" s="2"/>
     </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A40" s="8"/>
       <c r="B40" s="2"/>
       <c r="E40" s="3"/>
@@ -1257,7 +1544,7 @@
       <c r="G40" s="2"/>
       <c r="H40" s="2"/>
     </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A41" s="8"/>
       <c r="B41" s="2"/>
       <c r="E41" s="3"/>
@@ -1265,7 +1552,7 @@
       <c r="G41" s="2"/>
       <c r="H41" s="2"/>
     </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A42" s="8"/>
       <c r="B42" s="2"/>
       <c r="E42" s="3"/>
@@ -1273,7 +1560,7 @@
       <c r="G42" s="2"/>
       <c r="H42" s="2"/>
     </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A43" s="8"/>
       <c r="B43" s="2"/>
       <c r="E43" s="3"/>
@@ -1281,7 +1568,7 @@
       <c r="G43" s="2"/>
       <c r="H43" s="2"/>
     </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A44" s="8"/>
       <c r="B44" s="2"/>
       <c r="E44" s="3"/>
@@ -1289,7 +1576,7 @@
       <c r="G44" s="2"/>
       <c r="H44" s="2"/>
     </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A45" s="8"/>
       <c r="B45" s="2"/>
       <c r="E45" s="3"/>
@@ -1297,7 +1584,7 @@
       <c r="G45" s="2"/>
       <c r="H45" s="2"/>
     </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A46" s="8"/>
       <c r="B46" s="2"/>
       <c r="E46" s="3"/>
@@ -1305,7 +1592,7 @@
       <c r="G46" s="2"/>
       <c r="H46" s="2"/>
     </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A47" s="8"/>
       <c r="B47" s="2"/>
       <c r="E47" s="3"/>
@@ -1313,7 +1600,7 @@
       <c r="G47" s="2"/>
       <c r="H47" s="2"/>
     </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A48" s="8"/>
       <c r="B48" s="2"/>
       <c r="E48" s="3"/>
@@ -1321,7 +1608,7 @@
       <c r="G48" s="2"/>
       <c r="H48" s="2"/>
     </row>
-    <row r="49" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A49" s="8"/>
       <c r="B49" s="2"/>
       <c r="E49" s="3"/>
@@ -1329,7 +1616,7 @@
       <c r="G49" s="2"/>
       <c r="H49" s="2"/>
     </row>
-    <row r="50" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A50" s="8"/>
       <c r="B50" s="2"/>
       <c r="E50" s="3"/>
@@ -1337,7 +1624,7 @@
       <c r="G50" s="2"/>
       <c r="H50" s="2"/>
     </row>
-    <row r="51" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A51" s="8"/>
       <c r="B51" s="2"/>
       <c r="E51" s="3"/>
@@ -1345,7 +1632,7 @@
       <c r="G51" s="2"/>
       <c r="H51" s="2"/>
     </row>
-    <row r="52" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A52" s="8"/>
       <c r="B52" s="2"/>
       <c r="E52" s="3"/>
@@ -1353,7 +1640,7 @@
       <c r="G52" s="2"/>
       <c r="H52" s="2"/>
     </row>
-    <row r="53" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A53" s="8"/>
       <c r="B53" s="2"/>
       <c r="E53" s="3"/>
@@ -1361,7 +1648,7 @@
       <c r="G53" s="2"/>
       <c r="H53" s="2"/>
     </row>
-    <row r="54" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A54" s="8"/>
       <c r="B54" s="2"/>
       <c r="E54" s="3"/>
@@ -1369,7 +1656,7 @@
       <c r="G54" s="2"/>
       <c r="H54" s="2"/>
     </row>
-    <row r="55" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A55" s="8"/>
       <c r="B55" s="2"/>
       <c r="E55" s="3"/>
@@ -1377,7 +1664,7 @@
       <c r="G55" s="2"/>
       <c r="H55" s="2"/>
     </row>
-    <row r="56" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A56" s="8"/>
       <c r="B56" s="2"/>
       <c r="E56" s="3"/>
@@ -1385,7 +1672,7 @@
       <c r="G56" s="2"/>
       <c r="H56" s="2"/>
     </row>
-    <row r="57" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A57" s="8"/>
       <c r="B57" s="2"/>
       <c r="E57" s="3"/>
@@ -1393,7 +1680,7 @@
       <c r="G57" s="2"/>
       <c r="H57" s="2"/>
     </row>
-    <row r="58" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A58" s="8"/>
       <c r="B58" s="2"/>
       <c r="E58" s="3"/>
@@ -1401,7 +1688,7 @@
       <c r="G58" s="2"/>
       <c r="H58" s="2"/>
     </row>
-    <row r="59" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A59" s="8"/>
       <c r="B59" s="2"/>
       <c r="E59" s="3"/>
@@ -1409,7 +1696,7 @@
       <c r="G59" s="2"/>
       <c r="H59" s="2"/>
     </row>
-    <row r="60" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A60" s="8"/>
       <c r="B60" s="2"/>
       <c r="E60" s="3"/>
@@ -1417,7 +1704,7 @@
       <c r="G60" s="2"/>
       <c r="H60" s="2"/>
     </row>
-    <row r="61" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A61" s="8"/>
       <c r="B61" s="2"/>
       <c r="E61" s="3"/>
@@ -1425,7 +1712,7 @@
       <c r="G61" s="2"/>
       <c r="H61" s="2"/>
     </row>
-    <row r="62" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A62" s="8"/>
       <c r="B62" s="2"/>
       <c r="E62" s="3"/>
@@ -1433,7 +1720,7 @@
       <c r="G62" s="2"/>
       <c r="H62" s="2"/>
     </row>
-    <row r="63" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A63" s="8"/>
       <c r="B63" s="2"/>
       <c r="E63" s="3"/>
@@ -1441,7 +1728,7 @@
       <c r="G63" s="2"/>
       <c r="H63" s="2"/>
     </row>
-    <row r="64" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A64" s="8"/>
       <c r="B64" s="2"/>
       <c r="E64" s="3"/>
@@ -1449,7 +1736,7 @@
       <c r="G64" s="2"/>
       <c r="H64" s="2"/>
     </row>
-    <row r="65" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A65" s="8"/>
       <c r="B65" s="2"/>
       <c r="E65" s="3"/>
@@ -1457,7 +1744,7 @@
       <c r="G65" s="2"/>
       <c r="H65" s="2"/>
     </row>
-    <row r="66" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A66" s="8"/>
       <c r="B66" s="2"/>
       <c r="E66" s="3"/>
@@ -1465,7 +1752,7 @@
       <c r="G66" s="2"/>
       <c r="H66" s="2"/>
     </row>
-    <row r="67" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A67" s="8"/>
       <c r="B67" s="2"/>
       <c r="E67" s="3"/>
@@ -1473,7 +1760,7 @@
       <c r="G67" s="2"/>
       <c r="H67" s="2"/>
     </row>
-    <row r="68" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A68" s="8"/>
       <c r="B68" s="2"/>
       <c r="E68" s="3"/>
@@ -1481,7 +1768,7 @@
       <c r="G68" s="2"/>
       <c r="H68" s="2"/>
     </row>
-    <row r="69" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A69" s="8"/>
       <c r="B69" s="2"/>
       <c r="E69" s="3"/>
@@ -1489,7 +1776,7 @@
       <c r="G69" s="2"/>
       <c r="H69" s="2"/>
     </row>
-    <row r="70" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A70" s="8"/>
       <c r="B70" s="2"/>
       <c r="E70" s="3"/>
@@ -1497,7 +1784,7 @@
       <c r="G70" s="2"/>
       <c r="H70" s="2"/>
     </row>
-    <row r="71" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A71" s="8"/>
       <c r="B71" s="2"/>
       <c r="E71" s="3"/>
@@ -1505,7 +1792,7 @@
       <c r="G71" s="2"/>
       <c r="H71" s="2"/>
     </row>
-    <row r="72" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A72" s="8"/>
       <c r="B72" s="2"/>
       <c r="E72" s="3"/>
@@ -1513,7 +1800,7 @@
       <c r="G72" s="2"/>
       <c r="H72" s="2"/>
     </row>
-    <row r="73" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A73" s="8"/>
       <c r="B73" s="2"/>
       <c r="E73" s="3"/>
@@ -1521,7 +1808,7 @@
       <c r="G73" s="2"/>
       <c r="H73" s="2"/>
     </row>
-    <row r="74" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A74" s="8"/>
       <c r="B74" s="2"/>
       <c r="E74" s="3"/>
@@ -1529,7 +1816,7 @@
       <c r="G74" s="2"/>
       <c r="H74" s="2"/>
     </row>
-    <row r="75" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A75" s="8"/>
       <c r="B75" s="2"/>
       <c r="E75" s="3"/>
@@ -1537,7 +1824,7 @@
       <c r="G75" s="2"/>
       <c r="H75" s="2"/>
     </row>
-    <row r="76" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="76" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A76" s="8"/>
       <c r="B76" s="2"/>
       <c r="E76" s="3"/>
@@ -1545,7 +1832,7 @@
       <c r="G76" s="2"/>
       <c r="H76" s="2"/>
     </row>
-    <row r="77" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="77" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A77" s="8"/>
       <c r="B77" s="2"/>
       <c r="E77" s="3"/>
@@ -1553,7 +1840,7 @@
       <c r="G77" s="2"/>
       <c r="H77" s="2"/>
     </row>
-    <row r="78" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="78" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A78" s="8"/>
       <c r="B78" s="2"/>
       <c r="E78" s="3"/>
@@ -1561,7 +1848,7 @@
       <c r="G78" s="2"/>
       <c r="H78" s="2"/>
     </row>
-    <row r="79" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="79" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A79" s="8"/>
       <c r="B79" s="2"/>
       <c r="E79" s="3"/>
@@ -1569,7 +1856,7 @@
       <c r="G79" s="2"/>
       <c r="H79" s="2"/>
     </row>
-    <row r="80" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="80" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A80" s="8"/>
       <c r="B80" s="2"/>
       <c r="E80" s="3"/>
@@ -1577,7 +1864,7 @@
       <c r="G80" s="2"/>
       <c r="H80" s="2"/>
     </row>
-    <row r="81" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="81" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A81" s="8"/>
       <c r="B81" s="2"/>
       <c r="E81" s="3"/>
@@ -1585,7 +1872,7 @@
       <c r="G81" s="2"/>
       <c r="H81" s="2"/>
     </row>
-    <row r="82" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="82" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A82" s="8"/>
       <c r="B82" s="2"/>
       <c r="E82" s="3"/>
@@ -1593,7 +1880,7 @@
       <c r="G82" s="2"/>
       <c r="H82" s="2"/>
     </row>
-    <row r="83" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="83" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A83" s="8"/>
       <c r="B83" s="2"/>
       <c r="E83" s="3"/>
@@ -1601,7 +1888,7 @@
       <c r="G83" s="2"/>
       <c r="H83" s="2"/>
     </row>
-    <row r="84" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="84" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A84" s="8"/>
       <c r="B84" s="2"/>
       <c r="E84" s="3"/>
@@ -1609,7 +1896,7 @@
       <c r="G84" s="2"/>
       <c r="H84" s="2"/>
     </row>
-    <row r="85" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="85" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A85" s="8"/>
       <c r="B85" s="2"/>
       <c r="E85" s="3"/>
@@ -1617,7 +1904,7 @@
       <c r="G85" s="2"/>
       <c r="H85" s="2"/>
     </row>
-    <row r="86" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="86" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A86" s="8"/>
       <c r="B86" s="2"/>
       <c r="E86" s="3"/>
@@ -1625,7 +1912,7 @@
       <c r="G86" s="2"/>
       <c r="H86" s="2"/>
     </row>
-    <row r="87" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="87" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A87" s="8"/>
       <c r="B87" s="2"/>
       <c r="E87" s="3"/>
@@ -1633,7 +1920,7 @@
       <c r="G87" s="2"/>
       <c r="H87" s="2"/>
     </row>
-    <row r="88" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="88" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A88" s="8"/>
       <c r="B88" s="2"/>
       <c r="E88" s="3"/>
@@ -1641,7 +1928,7 @@
       <c r="G88" s="2"/>
       <c r="H88" s="2"/>
     </row>
-    <row r="89" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="89" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A89" s="8"/>
       <c r="B89" s="2"/>
       <c r="E89" s="3"/>
@@ -1649,7 +1936,7 @@
       <c r="G89" s="2"/>
       <c r="H89" s="2"/>
     </row>
-    <row r="90" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="90" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A90" s="8"/>
       <c r="B90" s="2"/>
       <c r="E90" s="3"/>
@@ -1657,7 +1944,7 @@
       <c r="G90" s="2"/>
       <c r="H90" s="2"/>
     </row>
-    <row r="91" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="91" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A91" s="8"/>
       <c r="B91" s="2"/>
       <c r="E91" s="3"/>
@@ -1665,7 +1952,7 @@
       <c r="G91" s="2"/>
       <c r="H91" s="2"/>
     </row>
-    <row r="92" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="92" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A92" s="8"/>
       <c r="B92" s="2"/>
       <c r="E92" s="3"/>
@@ -1673,7 +1960,7 @@
       <c r="G92" s="2"/>
       <c r="H92" s="2"/>
     </row>
-    <row r="93" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="93" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A93" s="8"/>
       <c r="B93" s="2"/>
       <c r="E93" s="3"/>
@@ -1681,7 +1968,7 @@
       <c r="G93" s="2"/>
       <c r="H93" s="2"/>
     </row>
-    <row r="94" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="94" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A94" s="8"/>
       <c r="B94" s="2"/>
       <c r="E94" s="3"/>
@@ -1689,7 +1976,7 @@
       <c r="G94" s="2"/>
       <c r="H94" s="2"/>
     </row>
-    <row r="95" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="95" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A95" s="8"/>
       <c r="B95" s="2"/>
       <c r="E95" s="3"/>
@@ -1697,7 +1984,7 @@
       <c r="G95" s="2"/>
       <c r="H95" s="2"/>
     </row>
-    <row r="96" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="96" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A96" s="8"/>
       <c r="B96" s="2"/>
       <c r="E96" s="3"/>
@@ -1705,7 +1992,7 @@
       <c r="G96" s="2"/>
       <c r="H96" s="2"/>
     </row>
-    <row r="97" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="97" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A97" s="8"/>
       <c r="B97" s="2"/>
       <c r="E97" s="3"/>
@@ -1713,7 +2000,7 @@
       <c r="G97" s="2"/>
       <c r="H97" s="2"/>
     </row>
-    <row r="98" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="98" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A98" s="8"/>
       <c r="B98" s="2"/>
       <c r="E98" s="3"/>
@@ -1721,7 +2008,7 @@
       <c r="G98" s="2"/>
       <c r="H98" s="2"/>
     </row>
-    <row r="99" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="99" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A99" s="8"/>
       <c r="B99" s="2"/>
       <c r="E99" s="3"/>
@@ -1729,7 +2016,7 @@
       <c r="G99" s="2"/>
       <c r="H99" s="2"/>
     </row>
-    <row r="100" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="100" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A100" s="8"/>
       <c r="B100" s="2"/>
       <c r="E100" s="3"/>
@@ -1739,10 +2026,10 @@
     </row>
   </sheetData>
   <dataValidations count="4">
-    <dataValidation type="list" errorStyle="warning" showInputMessage="1" showErrorMessage="1" errorTitle="Select Status" error="Fill in Status to proccessd " sqref="D2:D16" xr:uid="{45147164-8A29-4CAF-A2DB-395497B89382}">
+    <dataValidation type="list" errorStyle="warning" showInputMessage="1" showErrorMessage="1" errorTitle="Select Status" error="Fill in Status to proccessd " sqref="D3:D16" xr:uid="{45147164-8A29-4CAF-A2DB-395497B89382}">
       <formula1>"To Do,In Progress,Completed,Blocked"</formula1>
     </dataValidation>
-    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F2:F100" xr:uid="{22EE2D3D-9C8A-455C-B524-020B4CD90E60}">
+    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F3:F100" xr:uid="{22EE2D3D-9C8A-455C-B524-020B4CD90E60}">
       <formula1>1</formula1>
       <formula2>24</formula2>
     </dataValidation>
@@ -1756,7 +2043,7 @@
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <ignoredErrors>
-    <ignoredError sqref="D2:D100" listDataValidation="1"/>
+    <ignoredError sqref="D3:D100" listDataValidation="1"/>
   </ignoredErrors>
   <tableParts count="1">
     <tablePart r:id="rId1"/>
@@ -1772,19 +2059,19 @@
       <selection activeCell="D2" sqref="D2:D100"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="7.7265625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="17.26953125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.6328125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="7.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.5703125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="9" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.81640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="23.6328125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="13.36328125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="19.1796875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="23.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="19.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
@@ -1810,7 +2097,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="1"/>
       <c r="B2" s="2"/>
       <c r="E2" s="3"/>
@@ -1818,7 +2105,7 @@
       <c r="G2" s="2"/>
       <c r="H2" s="2"/>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="1"/>
       <c r="B3" s="2"/>
       <c r="E3" s="3"/>
@@ -1826,7 +2113,7 @@
       <c r="G3" s="2"/>
       <c r="H3" s="2"/>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="1"/>
       <c r="B4" s="2"/>
       <c r="E4" s="3"/>
@@ -1834,7 +2121,7 @@
       <c r="G4" s="2"/>
       <c r="H4" s="2"/>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="1"/>
       <c r="B5" s="2"/>
       <c r="E5" s="3"/>
@@ -1842,7 +2129,7 @@
       <c r="G5" s="2"/>
       <c r="H5" s="2"/>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="1"/>
       <c r="B6" s="2"/>
       <c r="E6" s="3"/>
@@ -1850,7 +2137,7 @@
       <c r="G6" s="2"/>
       <c r="H6" s="2"/>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="1"/>
       <c r="B7" s="2"/>
       <c r="E7" s="3"/>
@@ -1858,7 +2145,7 @@
       <c r="G7" s="2"/>
       <c r="H7" s="2"/>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="1"/>
       <c r="B8" s="2"/>
       <c r="E8" s="3"/>
@@ -1866,7 +2153,7 @@
       <c r="G8" s="2"/>
       <c r="H8" s="2"/>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="1"/>
       <c r="B9" s="2"/>
       <c r="E9" s="3"/>
@@ -1874,7 +2161,7 @@
       <c r="G9" s="2"/>
       <c r="H9" s="2"/>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="1"/>
       <c r="B10" s="2"/>
       <c r="E10" s="3"/>
@@ -1882,7 +2169,7 @@
       <c r="G10" s="2"/>
       <c r="H10" s="2"/>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="1"/>
       <c r="B11" s="2"/>
       <c r="E11" s="3"/>
@@ -1890,7 +2177,7 @@
       <c r="G11" s="2"/>
       <c r="H11" s="2"/>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="1"/>
       <c r="B12" s="2"/>
       <c r="E12" s="3"/>
@@ -1898,7 +2185,7 @@
       <c r="G12" s="2"/>
       <c r="H12" s="2"/>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="1"/>
       <c r="B13" s="2"/>
       <c r="E13" s="3"/>
@@ -1906,7 +2193,7 @@
       <c r="G13" s="2"/>
       <c r="H13" s="2"/>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" s="1"/>
       <c r="B14" s="2"/>
       <c r="E14" s="3"/>
@@ -1914,7 +2201,7 @@
       <c r="G14" s="2"/>
       <c r="H14" s="2"/>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" s="1"/>
       <c r="B15" s="2"/>
       <c r="E15" s="3"/>
@@ -1922,7 +2209,7 @@
       <c r="G15" s="2"/>
       <c r="H15" s="2"/>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" s="1"/>
       <c r="B16" s="2"/>
       <c r="E16" s="3"/>
@@ -1930,7 +2217,7 @@
       <c r="G16" s="2"/>
       <c r="H16" s="2"/>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" s="1"/>
       <c r="B17" s="2"/>
       <c r="E17" s="3"/>
@@ -1938,7 +2225,7 @@
       <c r="G17" s="2"/>
       <c r="H17" s="2"/>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" s="1"/>
       <c r="B18" s="2"/>
       <c r="E18" s="3"/>
@@ -1946,7 +2233,7 @@
       <c r="G18" s="2"/>
       <c r="H18" s="2"/>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" s="1"/>
       <c r="B19" s="2"/>
       <c r="E19" s="3"/>
@@ -1954,7 +2241,7 @@
       <c r="G19" s="2"/>
       <c r="H19" s="2"/>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" s="1"/>
       <c r="B20" s="2"/>
       <c r="E20" s="3"/>
@@ -1962,7 +2249,7 @@
       <c r="G20" s="2"/>
       <c r="H20" s="2"/>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" s="1"/>
       <c r="B21" s="2"/>
       <c r="E21" s="3"/>
@@ -1970,7 +2257,7 @@
       <c r="G21" s="2"/>
       <c r="H21" s="2"/>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" s="1"/>
       <c r="B22" s="2"/>
       <c r="E22" s="3"/>
@@ -1978,7 +2265,7 @@
       <c r="G22" s="2"/>
       <c r="H22" s="2"/>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" s="1"/>
       <c r="B23" s="2"/>
       <c r="E23" s="3"/>
@@ -1986,7 +2273,7 @@
       <c r="G23" s="2"/>
       <c r="H23" s="2"/>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24" s="1"/>
       <c r="B24" s="2"/>
       <c r="E24" s="3"/>
@@ -1994,7 +2281,7 @@
       <c r="G24" s="2"/>
       <c r="H24" s="2"/>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25" s="1"/>
       <c r="B25" s="2"/>
       <c r="E25" s="3"/>
@@ -2002,7 +2289,7 @@
       <c r="G25" s="2"/>
       <c r="H25" s="2"/>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26" s="1"/>
       <c r="B26" s="2"/>
       <c r="E26" s="3"/>
@@ -2010,7 +2297,7 @@
       <c r="G26" s="2"/>
       <c r="H26" s="2"/>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A27" s="1"/>
       <c r="B27" s="2"/>
       <c r="E27" s="3"/>
@@ -2018,7 +2305,7 @@
       <c r="G27" s="2"/>
       <c r="H27" s="2"/>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A28" s="1"/>
       <c r="B28" s="2"/>
       <c r="E28" s="3"/>
@@ -2026,7 +2313,7 @@
       <c r="G28" s="2"/>
       <c r="H28" s="2"/>
     </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A29" s="1"/>
       <c r="B29" s="2"/>
       <c r="E29" s="3"/>
@@ -2034,7 +2321,7 @@
       <c r="G29" s="2"/>
       <c r="H29" s="2"/>
     </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A30" s="1"/>
       <c r="B30" s="2"/>
       <c r="E30" s="3"/>
@@ -2042,7 +2329,7 @@
       <c r="G30" s="2"/>
       <c r="H30" s="2"/>
     </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A31" s="1"/>
       <c r="B31" s="2"/>
       <c r="E31" s="3"/>
@@ -2050,7 +2337,7 @@
       <c r="G31" s="2"/>
       <c r="H31" s="2"/>
     </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A32" s="1"/>
       <c r="B32" s="2"/>
       <c r="E32" s="3"/>
@@ -2058,7 +2345,7 @@
       <c r="G32" s="2"/>
       <c r="H32" s="2"/>
     </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A33" s="1"/>
       <c r="B33" s="2"/>
       <c r="E33" s="3"/>
@@ -2066,7 +2353,7 @@
       <c r="G33" s="2"/>
       <c r="H33" s="2"/>
     </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A34" s="1"/>
       <c r="B34" s="2"/>
       <c r="E34" s="3"/>
@@ -2074,7 +2361,7 @@
       <c r="G34" s="2"/>
       <c r="H34" s="2"/>
     </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A35" s="1"/>
       <c r="B35" s="2"/>
       <c r="E35" s="3"/>
@@ -2082,7 +2369,7 @@
       <c r="G35" s="2"/>
       <c r="H35" s="2"/>
     </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A36" s="1"/>
       <c r="B36" s="2"/>
       <c r="E36" s="3"/>
@@ -2090,7 +2377,7 @@
       <c r="G36" s="2"/>
       <c r="H36" s="2"/>
     </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A37" s="1"/>
       <c r="B37" s="2"/>
       <c r="E37" s="3"/>
@@ -2098,7 +2385,7 @@
       <c r="G37" s="2"/>
       <c r="H37" s="2"/>
     </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A38" s="1"/>
       <c r="B38" s="2"/>
       <c r="E38" s="3"/>
@@ -2106,7 +2393,7 @@
       <c r="G38" s="2"/>
       <c r="H38" s="2"/>
     </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A39" s="1"/>
       <c r="B39" s="2"/>
       <c r="E39" s="3"/>
@@ -2114,7 +2401,7 @@
       <c r="G39" s="2"/>
       <c r="H39" s="2"/>
     </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A40" s="1"/>
       <c r="B40" s="2"/>
       <c r="E40" s="3"/>
@@ -2122,7 +2409,7 @@
       <c r="G40" s="2"/>
       <c r="H40" s="2"/>
     </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A41" s="1"/>
       <c r="B41" s="2"/>
       <c r="E41" s="3"/>
@@ -2130,7 +2417,7 @@
       <c r="G41" s="2"/>
       <c r="H41" s="2"/>
     </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A42" s="1"/>
       <c r="B42" s="2"/>
       <c r="E42" s="3"/>
@@ -2138,7 +2425,7 @@
       <c r="G42" s="2"/>
       <c r="H42" s="2"/>
     </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A43" s="1"/>
       <c r="B43" s="2"/>
       <c r="E43" s="3"/>
@@ -2146,7 +2433,7 @@
       <c r="G43" s="2"/>
       <c r="H43" s="2"/>
     </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A44" s="1"/>
       <c r="B44" s="2"/>
       <c r="E44" s="3"/>
@@ -2154,7 +2441,7 @@
       <c r="G44" s="2"/>
       <c r="H44" s="2"/>
     </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A45" s="1"/>
       <c r="B45" s="2"/>
       <c r="E45" s="3"/>
@@ -2162,7 +2449,7 @@
       <c r="G45" s="2"/>
       <c r="H45" s="2"/>
     </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A46" s="1"/>
       <c r="B46" s="2"/>
       <c r="E46" s="3"/>
@@ -2170,7 +2457,7 @@
       <c r="G46" s="2"/>
       <c r="H46" s="2"/>
     </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A47" s="1"/>
       <c r="B47" s="2"/>
       <c r="E47" s="3"/>
@@ -2178,7 +2465,7 @@
       <c r="G47" s="2"/>
       <c r="H47" s="2"/>
     </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A48" s="1"/>
       <c r="B48" s="2"/>
       <c r="E48" s="3"/>
@@ -2186,7 +2473,7 @@
       <c r="G48" s="2"/>
       <c r="H48" s="2"/>
     </row>
-    <row r="49" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A49" s="1"/>
       <c r="B49" s="2"/>
       <c r="E49" s="3"/>
@@ -2194,7 +2481,7 @@
       <c r="G49" s="2"/>
       <c r="H49" s="2"/>
     </row>
-    <row r="50" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A50" s="1"/>
       <c r="B50" s="2"/>
       <c r="E50" s="3"/>
@@ -2202,7 +2489,7 @@
       <c r="G50" s="2"/>
       <c r="H50" s="2"/>
     </row>
-    <row r="51" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A51" s="1"/>
       <c r="B51" s="2"/>
       <c r="E51" s="3"/>
@@ -2210,7 +2497,7 @@
       <c r="G51" s="2"/>
       <c r="H51" s="2"/>
     </row>
-    <row r="52" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A52" s="1"/>
       <c r="B52" s="2"/>
       <c r="E52" s="3"/>
@@ -2218,7 +2505,7 @@
       <c r="G52" s="2"/>
       <c r="H52" s="2"/>
     </row>
-    <row r="53" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A53" s="1"/>
       <c r="B53" s="2"/>
       <c r="E53" s="3"/>
@@ -2226,7 +2513,7 @@
       <c r="G53" s="2"/>
       <c r="H53" s="2"/>
     </row>
-    <row r="54" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A54" s="1"/>
       <c r="B54" s="2"/>
       <c r="E54" s="3"/>
@@ -2234,7 +2521,7 @@
       <c r="G54" s="2"/>
       <c r="H54" s="2"/>
     </row>
-    <row r="55" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A55" s="1"/>
       <c r="B55" s="2"/>
       <c r="E55" s="3"/>
@@ -2242,7 +2529,7 @@
       <c r="G55" s="2"/>
       <c r="H55" s="2"/>
     </row>
-    <row r="56" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A56" s="1"/>
       <c r="B56" s="2"/>
       <c r="E56" s="3"/>
@@ -2250,7 +2537,7 @@
       <c r="G56" s="2"/>
       <c r="H56" s="2"/>
     </row>
-    <row r="57" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A57" s="1"/>
       <c r="B57" s="2"/>
       <c r="E57" s="3"/>
@@ -2258,7 +2545,7 @@
       <c r="G57" s="2"/>
       <c r="H57" s="2"/>
     </row>
-    <row r="58" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A58" s="1"/>
       <c r="B58" s="2"/>
       <c r="E58" s="3"/>
@@ -2266,7 +2553,7 @@
       <c r="G58" s="2"/>
       <c r="H58" s="2"/>
     </row>
-    <row r="59" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A59" s="1"/>
       <c r="B59" s="2"/>
       <c r="E59" s="3"/>
@@ -2274,7 +2561,7 @@
       <c r="G59" s="2"/>
       <c r="H59" s="2"/>
     </row>
-    <row r="60" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A60" s="1"/>
       <c r="B60" s="2"/>
       <c r="E60" s="3"/>
@@ -2282,7 +2569,7 @@
       <c r="G60" s="2"/>
       <c r="H60" s="2"/>
     </row>
-    <row r="61" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A61" s="1"/>
       <c r="B61" s="2"/>
       <c r="E61" s="3"/>
@@ -2290,7 +2577,7 @@
       <c r="G61" s="2"/>
       <c r="H61" s="2"/>
     </row>
-    <row r="62" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A62" s="1"/>
       <c r="B62" s="2"/>
       <c r="E62" s="3"/>
@@ -2298,7 +2585,7 @@
       <c r="G62" s="2"/>
       <c r="H62" s="2"/>
     </row>
-    <row r="63" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A63" s="1"/>
       <c r="B63" s="2"/>
       <c r="E63" s="3"/>
@@ -2306,7 +2593,7 @@
       <c r="G63" s="2"/>
       <c r="H63" s="2"/>
     </row>
-    <row r="64" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A64" s="1"/>
       <c r="B64" s="2"/>
       <c r="E64" s="3"/>
@@ -2314,7 +2601,7 @@
       <c r="G64" s="2"/>
       <c r="H64" s="2"/>
     </row>
-    <row r="65" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A65" s="1"/>
       <c r="B65" s="2"/>
       <c r="E65" s="3"/>
@@ -2322,7 +2609,7 @@
       <c r="G65" s="2"/>
       <c r="H65" s="2"/>
     </row>
-    <row r="66" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A66" s="1"/>
       <c r="B66" s="2"/>
       <c r="E66" s="3"/>
@@ -2330,7 +2617,7 @@
       <c r="G66" s="2"/>
       <c r="H66" s="2"/>
     </row>
-    <row r="67" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A67" s="1"/>
       <c r="B67" s="2"/>
       <c r="E67" s="3"/>
@@ -2338,7 +2625,7 @@
       <c r="G67" s="2"/>
       <c r="H67" s="2"/>
     </row>
-    <row r="68" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A68" s="1"/>
       <c r="B68" s="2"/>
       <c r="E68" s="3"/>
@@ -2346,7 +2633,7 @@
       <c r="G68" s="2"/>
       <c r="H68" s="2"/>
     </row>
-    <row r="69" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A69" s="1"/>
       <c r="B69" s="2"/>
       <c r="E69" s="3"/>
@@ -2354,7 +2641,7 @@
       <c r="G69" s="2"/>
       <c r="H69" s="2"/>
     </row>
-    <row r="70" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A70" s="1"/>
       <c r="B70" s="2"/>
       <c r="E70" s="3"/>
@@ -2362,7 +2649,7 @@
       <c r="G70" s="2"/>
       <c r="H70" s="2"/>
     </row>
-    <row r="71" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A71" s="1"/>
       <c r="B71" s="2"/>
       <c r="E71" s="3"/>
@@ -2370,7 +2657,7 @@
       <c r="G71" s="2"/>
       <c r="H71" s="2"/>
     </row>
-    <row r="72" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A72" s="1"/>
       <c r="B72" s="2"/>
       <c r="E72" s="3"/>
@@ -2378,7 +2665,7 @@
       <c r="G72" s="2"/>
       <c r="H72" s="2"/>
     </row>
-    <row r="73" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A73" s="1"/>
       <c r="B73" s="2"/>
       <c r="E73" s="3"/>
@@ -2386,7 +2673,7 @@
       <c r="G73" s="2"/>
       <c r="H73" s="2"/>
     </row>
-    <row r="74" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A74" s="1"/>
       <c r="B74" s="2"/>
       <c r="E74" s="3"/>
@@ -2394,7 +2681,7 @@
       <c r="G74" s="2"/>
       <c r="H74" s="2"/>
     </row>
-    <row r="75" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A75" s="1"/>
       <c r="B75" s="2"/>
       <c r="E75" s="3"/>
@@ -2402,7 +2689,7 @@
       <c r="G75" s="2"/>
       <c r="H75" s="2"/>
     </row>
-    <row r="76" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="76" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A76" s="1"/>
       <c r="B76" s="2"/>
       <c r="E76" s="3"/>
@@ -2410,7 +2697,7 @@
       <c r="G76" s="2"/>
       <c r="H76" s="2"/>
     </row>
-    <row r="77" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="77" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A77" s="1"/>
       <c r="B77" s="2"/>
       <c r="E77" s="3"/>
@@ -2418,7 +2705,7 @@
       <c r="G77" s="2"/>
       <c r="H77" s="2"/>
     </row>
-    <row r="78" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="78" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A78" s="1"/>
       <c r="B78" s="2"/>
       <c r="E78" s="3"/>
@@ -2426,7 +2713,7 @@
       <c r="G78" s="2"/>
       <c r="H78" s="2"/>
     </row>
-    <row r="79" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="79" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A79" s="1"/>
       <c r="B79" s="2"/>
       <c r="E79" s="3"/>
@@ -2434,7 +2721,7 @@
       <c r="G79" s="2"/>
       <c r="H79" s="2"/>
     </row>
-    <row r="80" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="80" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A80" s="1"/>
       <c r="B80" s="2"/>
       <c r="E80" s="3"/>
@@ -2442,7 +2729,7 @@
       <c r="G80" s="2"/>
       <c r="H80" s="2"/>
     </row>
-    <row r="81" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="81" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A81" s="1"/>
       <c r="B81" s="2"/>
       <c r="E81" s="3"/>
@@ -2450,7 +2737,7 @@
       <c r="G81" s="2"/>
       <c r="H81" s="2"/>
     </row>
-    <row r="82" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="82" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A82" s="1"/>
       <c r="B82" s="2"/>
       <c r="E82" s="3"/>
@@ -2458,7 +2745,7 @@
       <c r="G82" s="2"/>
       <c r="H82" s="2"/>
     </row>
-    <row r="83" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="83" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A83" s="1"/>
       <c r="B83" s="2"/>
       <c r="E83" s="3"/>
@@ -2466,7 +2753,7 @@
       <c r="G83" s="2"/>
       <c r="H83" s="2"/>
     </row>
-    <row r="84" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="84" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A84" s="1"/>
       <c r="B84" s="2"/>
       <c r="E84" s="3"/>
@@ -2474,7 +2761,7 @@
       <c r="G84" s="2"/>
       <c r="H84" s="2"/>
     </row>
-    <row r="85" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="85" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A85" s="1"/>
       <c r="B85" s="2"/>
       <c r="E85" s="3"/>
@@ -2482,7 +2769,7 @@
       <c r="G85" s="2"/>
       <c r="H85" s="2"/>
     </row>
-    <row r="86" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="86" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A86" s="1"/>
       <c r="B86" s="2"/>
       <c r="E86" s="3"/>
@@ -2490,7 +2777,7 @@
       <c r="G86" s="2"/>
       <c r="H86" s="2"/>
     </row>
-    <row r="87" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="87" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A87" s="1"/>
       <c r="B87" s="2"/>
       <c r="E87" s="3"/>
@@ -2498,7 +2785,7 @@
       <c r="G87" s="2"/>
       <c r="H87" s="2"/>
     </row>
-    <row r="88" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="88" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A88" s="1"/>
       <c r="B88" s="2"/>
       <c r="E88" s="3"/>
@@ -2506,7 +2793,7 @@
       <c r="G88" s="2"/>
       <c r="H88" s="2"/>
     </row>
-    <row r="89" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="89" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A89" s="1"/>
       <c r="B89" s="2"/>
       <c r="E89" s="3"/>
@@ -2514,7 +2801,7 @@
       <c r="G89" s="2"/>
       <c r="H89" s="2"/>
     </row>
-    <row r="90" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="90" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A90" s="1"/>
       <c r="B90" s="2"/>
       <c r="E90" s="3"/>
@@ -2522,7 +2809,7 @@
       <c r="G90" s="2"/>
       <c r="H90" s="2"/>
     </row>
-    <row r="91" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="91" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A91" s="1"/>
       <c r="B91" s="2"/>
       <c r="E91" s="3"/>
@@ -2530,7 +2817,7 @@
       <c r="G91" s="2"/>
       <c r="H91" s="2"/>
     </row>
-    <row r="92" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="92" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A92" s="1"/>
       <c r="B92" s="2"/>
       <c r="E92" s="3"/>
@@ -2538,7 +2825,7 @@
       <c r="G92" s="2"/>
       <c r="H92" s="2"/>
     </row>
-    <row r="93" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="93" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A93" s="1"/>
       <c r="B93" s="2"/>
       <c r="E93" s="3"/>
@@ -2546,7 +2833,7 @@
       <c r="G93" s="2"/>
       <c r="H93" s="2"/>
     </row>
-    <row r="94" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="94" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A94" s="1"/>
       <c r="B94" s="2"/>
       <c r="E94" s="3"/>
@@ -2554,7 +2841,7 @@
       <c r="G94" s="2"/>
       <c r="H94" s="2"/>
     </row>
-    <row r="95" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="95" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A95" s="1"/>
       <c r="B95" s="2"/>
       <c r="E95" s="3"/>
@@ -2562,7 +2849,7 @@
       <c r="G95" s="2"/>
       <c r="H95" s="2"/>
     </row>
-    <row r="96" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="96" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A96" s="1"/>
       <c r="B96" s="2"/>
       <c r="E96" s="3"/>
@@ -2570,7 +2857,7 @@
       <c r="G96" s="2"/>
       <c r="H96" s="2"/>
     </row>
-    <row r="97" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="97" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A97" s="1"/>
       <c r="B97" s="2"/>
       <c r="E97" s="3"/>
@@ -2578,7 +2865,7 @@
       <c r="G97" s="2"/>
       <c r="H97" s="2"/>
     </row>
-    <row r="98" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="98" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A98" s="1"/>
       <c r="B98" s="2"/>
       <c r="E98" s="3"/>
@@ -2586,7 +2873,7 @@
       <c r="G98" s="2"/>
       <c r="H98" s="2"/>
     </row>
-    <row r="99" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="99" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A99" s="1"/>
       <c r="B99" s="2"/>
       <c r="E99" s="3"/>
@@ -2594,7 +2881,7 @@
       <c r="G99" s="2"/>
       <c r="H99" s="2"/>
     </row>
-    <row r="100" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="100" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A100" s="1"/>
       <c r="B100" s="2"/>
       <c r="E100" s="3"/>
@@ -2637,19 +2924,19 @@
       <selection activeCell="D2" sqref="D2:D100"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="7.7265625" customWidth="1"/>
-    <col min="2" max="2" width="17.26953125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.6328125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="7.7109375" customWidth="1"/>
+    <col min="2" max="2" width="17.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.5703125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="9" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.81640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="23.6328125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="13.36328125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="19.1796875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="23.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="19.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
@@ -2675,7 +2962,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="1"/>
       <c r="B2" s="2"/>
       <c r="E2" s="3"/>
@@ -2683,7 +2970,7 @@
       <c r="G2" s="2"/>
       <c r="H2" s="2"/>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="1"/>
       <c r="B3" s="2"/>
       <c r="E3" s="3"/>
@@ -2691,7 +2978,7 @@
       <c r="G3" s="2"/>
       <c r="H3" s="2"/>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="1"/>
       <c r="B4" s="2"/>
       <c r="E4" s="3"/>
@@ -2699,7 +2986,7 @@
       <c r="G4" s="2"/>
       <c r="H4" s="2"/>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="1"/>
       <c r="B5" s="2"/>
       <c r="E5" s="3"/>
@@ -2707,7 +2994,7 @@
       <c r="G5" s="2"/>
       <c r="H5" s="2"/>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="1"/>
       <c r="B6" s="2"/>
       <c r="E6" s="3"/>
@@ -2715,7 +3002,7 @@
       <c r="G6" s="2"/>
       <c r="H6" s="2"/>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="1"/>
       <c r="B7" s="2"/>
       <c r="E7" s="3"/>
@@ -2723,7 +3010,7 @@
       <c r="G7" s="2"/>
       <c r="H7" s="2"/>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="1"/>
       <c r="B8" s="2"/>
       <c r="E8" s="3"/>
@@ -2731,7 +3018,7 @@
       <c r="G8" s="2"/>
       <c r="H8" s="2"/>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="1"/>
       <c r="B9" s="2"/>
       <c r="E9" s="3"/>
@@ -2739,7 +3026,7 @@
       <c r="G9" s="2"/>
       <c r="H9" s="2"/>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="1"/>
       <c r="B10" s="2"/>
       <c r="E10" s="3"/>
@@ -2747,7 +3034,7 @@
       <c r="G10" s="2"/>
       <c r="H10" s="2"/>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="1"/>
       <c r="B11" s="2"/>
       <c r="E11" s="3"/>
@@ -2755,7 +3042,7 @@
       <c r="G11" s="2"/>
       <c r="H11" s="2"/>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="1"/>
       <c r="B12" s="2"/>
       <c r="E12" s="3"/>
@@ -2763,7 +3050,7 @@
       <c r="G12" s="2"/>
       <c r="H12" s="2"/>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="1"/>
       <c r="B13" s="2"/>
       <c r="E13" s="3"/>
@@ -2771,7 +3058,7 @@
       <c r="G13" s="2"/>
       <c r="H13" s="2"/>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" s="1"/>
       <c r="B14" s="2"/>
       <c r="E14" s="3"/>
@@ -2779,7 +3066,7 @@
       <c r="G14" s="2"/>
       <c r="H14" s="2"/>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" s="1"/>
       <c r="B15" s="2"/>
       <c r="E15" s="3"/>
@@ -2787,7 +3074,7 @@
       <c r="G15" s="2"/>
       <c r="H15" s="2"/>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" s="1"/>
       <c r="B16" s="2"/>
       <c r="E16" s="3"/>
@@ -2795,7 +3082,7 @@
       <c r="G16" s="2"/>
       <c r="H16" s="2"/>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" s="1"/>
       <c r="B17" s="2"/>
       <c r="E17" s="3"/>
@@ -2803,7 +3090,7 @@
       <c r="G17" s="2"/>
       <c r="H17" s="2"/>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" s="1"/>
       <c r="B18" s="2"/>
       <c r="E18" s="3"/>
@@ -2811,7 +3098,7 @@
       <c r="G18" s="2"/>
       <c r="H18" s="2"/>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" s="1"/>
       <c r="B19" s="2"/>
       <c r="E19" s="3"/>
@@ -2819,7 +3106,7 @@
       <c r="G19" s="2"/>
       <c r="H19" s="2"/>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" s="1"/>
       <c r="B20" s="2"/>
       <c r="E20" s="3"/>
@@ -2827,7 +3114,7 @@
       <c r="G20" s="2"/>
       <c r="H20" s="2"/>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" s="1"/>
       <c r="B21" s="2"/>
       <c r="E21" s="3"/>
@@ -2835,7 +3122,7 @@
       <c r="G21" s="2"/>
       <c r="H21" s="2"/>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" s="1"/>
       <c r="B22" s="2"/>
       <c r="E22" s="3"/>
@@ -2843,7 +3130,7 @@
       <c r="G22" s="2"/>
       <c r="H22" s="2"/>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" s="1"/>
       <c r="B23" s="2"/>
       <c r="E23" s="3"/>
@@ -2851,7 +3138,7 @@
       <c r="G23" s="2"/>
       <c r="H23" s="2"/>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24" s="1"/>
       <c r="B24" s="2"/>
       <c r="E24" s="3"/>
@@ -2859,7 +3146,7 @@
       <c r="G24" s="2"/>
       <c r="H24" s="2"/>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25" s="1"/>
       <c r="B25" s="2"/>
       <c r="E25" s="3"/>
@@ -2867,7 +3154,7 @@
       <c r="G25" s="2"/>
       <c r="H25" s="2"/>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26" s="1"/>
       <c r="B26" s="2"/>
       <c r="E26" s="3"/>
@@ -2875,7 +3162,7 @@
       <c r="G26" s="2"/>
       <c r="H26" s="2"/>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A27" s="1"/>
       <c r="B27" s="2"/>
       <c r="E27" s="3"/>
@@ -2883,7 +3170,7 @@
       <c r="G27" s="2"/>
       <c r="H27" s="2"/>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A28" s="1"/>
       <c r="B28" s="2"/>
       <c r="E28" s="3"/>
@@ -2891,7 +3178,7 @@
       <c r="G28" s="2"/>
       <c r="H28" s="2"/>
     </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A29" s="1"/>
       <c r="B29" s="2"/>
       <c r="E29" s="3"/>
@@ -2899,7 +3186,7 @@
       <c r="G29" s="2"/>
       <c r="H29" s="2"/>
     </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A30" s="1"/>
       <c r="B30" s="2"/>
       <c r="E30" s="3"/>
@@ -2907,7 +3194,7 @@
       <c r="G30" s="2"/>
       <c r="H30" s="2"/>
     </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A31" s="1"/>
       <c r="B31" s="2"/>
       <c r="E31" s="3"/>
@@ -2915,7 +3202,7 @@
       <c r="G31" s="2"/>
       <c r="H31" s="2"/>
     </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A32" s="1"/>
       <c r="B32" s="2"/>
       <c r="E32" s="3"/>
@@ -2923,7 +3210,7 @@
       <c r="G32" s="2"/>
       <c r="H32" s="2"/>
     </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A33" s="1"/>
       <c r="B33" s="2"/>
       <c r="E33" s="3"/>
@@ -2931,7 +3218,7 @@
       <c r="G33" s="2"/>
       <c r="H33" s="2"/>
     </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A34" s="1"/>
       <c r="B34" s="2"/>
       <c r="E34" s="3"/>
@@ -2939,7 +3226,7 @@
       <c r="G34" s="2"/>
       <c r="H34" s="2"/>
     </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A35" s="1"/>
       <c r="B35" s="2"/>
       <c r="E35" s="3"/>
@@ -2947,7 +3234,7 @@
       <c r="G35" s="2"/>
       <c r="H35" s="2"/>
     </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A36" s="1"/>
       <c r="B36" s="2"/>
       <c r="E36" s="3"/>
@@ -2955,7 +3242,7 @@
       <c r="G36" s="2"/>
       <c r="H36" s="2"/>
     </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A37" s="1"/>
       <c r="B37" s="2"/>
       <c r="E37" s="3"/>
@@ -2963,7 +3250,7 @@
       <c r="G37" s="2"/>
       <c r="H37" s="2"/>
     </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A38" s="1"/>
       <c r="B38" s="2"/>
       <c r="E38" s="3"/>
@@ -2971,7 +3258,7 @@
       <c r="G38" s="2"/>
       <c r="H38" s="2"/>
     </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A39" s="1"/>
       <c r="B39" s="2"/>
       <c r="E39" s="3"/>
@@ -2979,7 +3266,7 @@
       <c r="G39" s="2"/>
       <c r="H39" s="2"/>
     </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A40" s="1"/>
       <c r="B40" s="2"/>
       <c r="E40" s="3"/>
@@ -2987,7 +3274,7 @@
       <c r="G40" s="2"/>
       <c r="H40" s="2"/>
     </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A41" s="1"/>
       <c r="B41" s="2"/>
       <c r="E41" s="3"/>
@@ -2995,7 +3282,7 @@
       <c r="G41" s="2"/>
       <c r="H41" s="2"/>
     </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A42" s="1"/>
       <c r="B42" s="2"/>
       <c r="E42" s="3"/>
@@ -3003,7 +3290,7 @@
       <c r="G42" s="2"/>
       <c r="H42" s="2"/>
     </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A43" s="1"/>
       <c r="B43" s="2"/>
       <c r="E43" s="3"/>
@@ -3011,7 +3298,7 @@
       <c r="G43" s="2"/>
       <c r="H43" s="2"/>
     </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A44" s="1"/>
       <c r="B44" s="2"/>
       <c r="E44" s="3"/>
@@ -3019,7 +3306,7 @@
       <c r="G44" s="2"/>
       <c r="H44" s="2"/>
     </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A45" s="1"/>
       <c r="B45" s="2"/>
       <c r="E45" s="3"/>
@@ -3027,7 +3314,7 @@
       <c r="G45" s="2"/>
       <c r="H45" s="2"/>
     </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A46" s="1"/>
       <c r="B46" s="2"/>
       <c r="E46" s="3"/>
@@ -3035,7 +3322,7 @@
       <c r="G46" s="2"/>
       <c r="H46" s="2"/>
     </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A47" s="1"/>
       <c r="B47" s="2"/>
       <c r="E47" s="3"/>
@@ -3043,7 +3330,7 @@
       <c r="G47" s="2"/>
       <c r="H47" s="2"/>
     </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A48" s="1"/>
       <c r="B48" s="2"/>
       <c r="E48" s="3"/>
@@ -3051,7 +3338,7 @@
       <c r="G48" s="2"/>
       <c r="H48" s="2"/>
     </row>
-    <row r="49" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A49" s="1"/>
       <c r="B49" s="2"/>
       <c r="E49" s="3"/>
@@ -3059,7 +3346,7 @@
       <c r="G49" s="2"/>
       <c r="H49" s="2"/>
     </row>
-    <row r="50" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A50" s="1"/>
       <c r="B50" s="2"/>
       <c r="E50" s="3"/>
@@ -3067,7 +3354,7 @@
       <c r="G50" s="2"/>
       <c r="H50" s="2"/>
     </row>
-    <row r="51" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A51" s="1"/>
       <c r="B51" s="2"/>
       <c r="E51" s="3"/>
@@ -3075,7 +3362,7 @@
       <c r="G51" s="2"/>
       <c r="H51" s="2"/>
     </row>
-    <row r="52" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A52" s="1"/>
       <c r="B52" s="2"/>
       <c r="E52" s="3"/>
@@ -3083,7 +3370,7 @@
       <c r="G52" s="2"/>
       <c r="H52" s="2"/>
     </row>
-    <row r="53" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A53" s="1"/>
       <c r="B53" s="2"/>
       <c r="E53" s="3"/>
@@ -3091,7 +3378,7 @@
       <c r="G53" s="2"/>
       <c r="H53" s="2"/>
     </row>
-    <row r="54" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A54" s="1"/>
       <c r="B54" s="2"/>
       <c r="E54" s="3"/>
@@ -3099,7 +3386,7 @@
       <c r="G54" s="2"/>
       <c r="H54" s="2"/>
     </row>
-    <row r="55" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A55" s="1"/>
       <c r="B55" s="2"/>
       <c r="E55" s="3"/>
@@ -3107,7 +3394,7 @@
       <c r="G55" s="2"/>
       <c r="H55" s="2"/>
     </row>
-    <row r="56" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A56" s="1"/>
       <c r="B56" s="2"/>
       <c r="E56" s="3"/>
@@ -3115,7 +3402,7 @@
       <c r="G56" s="2"/>
       <c r="H56" s="2"/>
     </row>
-    <row r="57" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A57" s="1"/>
       <c r="B57" s="2"/>
       <c r="E57" s="3"/>
@@ -3123,7 +3410,7 @@
       <c r="G57" s="2"/>
       <c r="H57" s="2"/>
     </row>
-    <row r="58" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A58" s="1"/>
       <c r="B58" s="2"/>
       <c r="E58" s="3"/>
@@ -3131,7 +3418,7 @@
       <c r="G58" s="2"/>
       <c r="H58" s="2"/>
     </row>
-    <row r="59" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A59" s="1"/>
       <c r="B59" s="2"/>
       <c r="E59" s="3"/>
@@ -3139,7 +3426,7 @@
       <c r="G59" s="2"/>
       <c r="H59" s="2"/>
     </row>
-    <row r="60" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A60" s="1"/>
       <c r="B60" s="2"/>
       <c r="E60" s="3"/>
@@ -3147,7 +3434,7 @@
       <c r="G60" s="2"/>
       <c r="H60" s="2"/>
     </row>
-    <row r="61" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A61" s="1"/>
       <c r="B61" s="2"/>
       <c r="E61" s="3"/>
@@ -3155,7 +3442,7 @@
       <c r="G61" s="2"/>
       <c r="H61" s="2"/>
     </row>
-    <row r="62" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A62" s="1"/>
       <c r="B62" s="2"/>
       <c r="E62" s="3"/>
@@ -3163,7 +3450,7 @@
       <c r="G62" s="2"/>
       <c r="H62" s="2"/>
     </row>
-    <row r="63" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A63" s="1"/>
       <c r="B63" s="2"/>
       <c r="E63" s="3"/>
@@ -3171,7 +3458,7 @@
       <c r="G63" s="2"/>
       <c r="H63" s="2"/>
     </row>
-    <row r="64" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A64" s="1"/>
       <c r="B64" s="2"/>
       <c r="E64" s="3"/>
@@ -3179,7 +3466,7 @@
       <c r="G64" s="2"/>
       <c r="H64" s="2"/>
     </row>
-    <row r="65" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A65" s="1"/>
       <c r="B65" s="2"/>
       <c r="E65" s="3"/>
@@ -3187,7 +3474,7 @@
       <c r="G65" s="2"/>
       <c r="H65" s="2"/>
     </row>
-    <row r="66" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A66" s="1"/>
       <c r="B66" s="2"/>
       <c r="E66" s="3"/>
@@ -3195,7 +3482,7 @@
       <c r="G66" s="2"/>
       <c r="H66" s="2"/>
     </row>
-    <row r="67" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A67" s="1"/>
       <c r="B67" s="2"/>
       <c r="E67" s="3"/>
@@ -3203,7 +3490,7 @@
       <c r="G67" s="2"/>
       <c r="H67" s="2"/>
     </row>
-    <row r="68" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A68" s="1"/>
       <c r="B68" s="2"/>
       <c r="E68" s="3"/>
@@ -3211,7 +3498,7 @@
       <c r="G68" s="2"/>
       <c r="H68" s="2"/>
     </row>
-    <row r="69" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A69" s="1"/>
       <c r="B69" s="2"/>
       <c r="E69" s="3"/>
@@ -3219,7 +3506,7 @@
       <c r="G69" s="2"/>
       <c r="H69" s="2"/>
     </row>
-    <row r="70" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A70" s="1"/>
       <c r="B70" s="2"/>
       <c r="E70" s="3"/>
@@ -3227,7 +3514,7 @@
       <c r="G70" s="2"/>
       <c r="H70" s="2"/>
     </row>
-    <row r="71" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A71" s="1"/>
       <c r="B71" s="2"/>
       <c r="E71" s="3"/>
@@ -3235,7 +3522,7 @@
       <c r="G71" s="2"/>
       <c r="H71" s="2"/>
     </row>
-    <row r="72" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A72" s="1"/>
       <c r="B72" s="2"/>
       <c r="E72" s="3"/>
@@ -3243,7 +3530,7 @@
       <c r="G72" s="2"/>
       <c r="H72" s="2"/>
     </row>
-    <row r="73" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A73" s="1"/>
       <c r="B73" s="2"/>
       <c r="E73" s="3"/>
@@ -3251,7 +3538,7 @@
       <c r="G73" s="2"/>
       <c r="H73" s="2"/>
     </row>
-    <row r="74" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A74" s="1"/>
       <c r="B74" s="2"/>
       <c r="E74" s="3"/>
@@ -3259,7 +3546,7 @@
       <c r="G74" s="2"/>
       <c r="H74" s="2"/>
     </row>
-    <row r="75" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A75" s="1"/>
       <c r="B75" s="2"/>
       <c r="E75" s="3"/>
@@ -3267,7 +3554,7 @@
       <c r="G75" s="2"/>
       <c r="H75" s="2"/>
     </row>
-    <row r="76" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="76" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A76" s="1"/>
       <c r="B76" s="2"/>
       <c r="E76" s="3"/>
@@ -3275,7 +3562,7 @@
       <c r="G76" s="2"/>
       <c r="H76" s="2"/>
     </row>
-    <row r="77" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="77" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A77" s="1"/>
       <c r="B77" s="2"/>
       <c r="E77" s="3"/>
@@ -3283,7 +3570,7 @@
       <c r="G77" s="2"/>
       <c r="H77" s="2"/>
     </row>
-    <row r="78" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="78" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A78" s="1"/>
       <c r="B78" s="2"/>
       <c r="E78" s="3"/>
@@ -3291,7 +3578,7 @@
       <c r="G78" s="2"/>
       <c r="H78" s="2"/>
     </row>
-    <row r="79" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="79" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A79" s="1"/>
       <c r="B79" s="2"/>
       <c r="E79" s="3"/>
@@ -3299,7 +3586,7 @@
       <c r="G79" s="2"/>
       <c r="H79" s="2"/>
     </row>
-    <row r="80" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="80" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A80" s="1"/>
       <c r="B80" s="2"/>
       <c r="E80" s="3"/>
@@ -3307,7 +3594,7 @@
       <c r="G80" s="2"/>
       <c r="H80" s="2"/>
     </row>
-    <row r="81" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="81" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A81" s="1"/>
       <c r="B81" s="2"/>
       <c r="E81" s="3"/>
@@ -3315,7 +3602,7 @@
       <c r="G81" s="2"/>
       <c r="H81" s="2"/>
     </row>
-    <row r="82" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="82" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A82" s="1"/>
       <c r="B82" s="2"/>
       <c r="E82" s="3"/>
@@ -3323,7 +3610,7 @@
       <c r="G82" s="2"/>
       <c r="H82" s="2"/>
     </row>
-    <row r="83" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="83" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A83" s="1"/>
       <c r="B83" s="2"/>
       <c r="E83" s="3"/>
@@ -3331,7 +3618,7 @@
       <c r="G83" s="2"/>
       <c r="H83" s="2"/>
     </row>
-    <row r="84" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="84" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A84" s="1"/>
       <c r="B84" s="2"/>
       <c r="E84" s="3"/>
@@ -3339,7 +3626,7 @@
       <c r="G84" s="2"/>
       <c r="H84" s="2"/>
     </row>
-    <row r="85" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="85" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A85" s="1"/>
       <c r="B85" s="2"/>
       <c r="E85" s="3"/>
@@ -3347,7 +3634,7 @@
       <c r="G85" s="2"/>
       <c r="H85" s="2"/>
     </row>
-    <row r="86" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="86" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A86" s="1"/>
       <c r="B86" s="2"/>
       <c r="E86" s="3"/>
@@ -3355,7 +3642,7 @@
       <c r="G86" s="2"/>
       <c r="H86" s="2"/>
     </row>
-    <row r="87" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="87" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A87" s="1"/>
       <c r="B87" s="2"/>
       <c r="E87" s="3"/>
@@ -3363,7 +3650,7 @@
       <c r="G87" s="2"/>
       <c r="H87" s="2"/>
     </row>
-    <row r="88" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="88" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A88" s="1"/>
       <c r="B88" s="2"/>
       <c r="E88" s="3"/>
@@ -3371,7 +3658,7 @@
       <c r="G88" s="2"/>
       <c r="H88" s="2"/>
     </row>
-    <row r="89" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="89" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A89" s="1"/>
       <c r="B89" s="2"/>
       <c r="E89" s="3"/>
@@ -3379,7 +3666,7 @@
       <c r="G89" s="2"/>
       <c r="H89" s="2"/>
     </row>
-    <row r="90" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="90" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A90" s="1"/>
       <c r="B90" s="2"/>
       <c r="E90" s="3"/>
@@ -3387,7 +3674,7 @@
       <c r="G90" s="2"/>
       <c r="H90" s="2"/>
     </row>
-    <row r="91" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="91" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A91" s="1"/>
       <c r="B91" s="2"/>
       <c r="E91" s="3"/>
@@ -3395,7 +3682,7 @@
       <c r="G91" s="2"/>
       <c r="H91" s="2"/>
     </row>
-    <row r="92" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="92" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A92" s="1"/>
       <c r="B92" s="2"/>
       <c r="E92" s="3"/>
@@ -3403,7 +3690,7 @@
       <c r="G92" s="2"/>
       <c r="H92" s="2"/>
     </row>
-    <row r="93" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="93" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A93" s="1"/>
       <c r="B93" s="2"/>
       <c r="E93" s="3"/>
@@ -3411,7 +3698,7 @@
       <c r="G93" s="2"/>
       <c r="H93" s="2"/>
     </row>
-    <row r="94" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="94" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A94" s="1"/>
       <c r="B94" s="2"/>
       <c r="E94" s="3"/>
@@ -3419,7 +3706,7 @@
       <c r="G94" s="2"/>
       <c r="H94" s="2"/>
     </row>
-    <row r="95" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="95" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A95" s="1"/>
       <c r="B95" s="2"/>
       <c r="E95" s="3"/>
@@ -3427,7 +3714,7 @@
       <c r="G95" s="2"/>
       <c r="H95" s="2"/>
     </row>
-    <row r="96" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="96" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A96" s="1"/>
       <c r="B96" s="2"/>
       <c r="E96" s="3"/>
@@ -3435,7 +3722,7 @@
       <c r="G96" s="2"/>
       <c r="H96" s="2"/>
     </row>
-    <row r="97" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="97" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A97" s="1"/>
       <c r="B97" s="2"/>
       <c r="E97" s="3"/>
@@ -3443,7 +3730,7 @@
       <c r="G97" s="2"/>
       <c r="H97" s="2"/>
     </row>
-    <row r="98" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="98" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A98" s="1"/>
       <c r="B98" s="2"/>
       <c r="E98" s="3"/>
@@ -3451,7 +3738,7 @@
       <c r="G98" s="2"/>
       <c r="H98" s="2"/>
     </row>
-    <row r="99" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="99" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A99" s="1"/>
       <c r="B99" s="2"/>
       <c r="E99" s="3"/>
@@ -3459,7 +3746,7 @@
       <c r="G99" s="2"/>
       <c r="H99" s="2"/>
     </row>
-    <row r="100" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="100" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A100" s="1"/>
       <c r="B100" s="2"/>
       <c r="E100" s="3"/>
@@ -3502,21 +3789,21 @@
       <selection activeCell="P21" sqref="P21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.08984375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.81640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.81640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="19.453125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.6328125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.6328125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.5703125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="9" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="17.90625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="17.85546875" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="17" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="19.1796875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="19.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="7" t="s">
         <v>8</v>
       </c>
@@ -3548,7 +3835,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="2"/>
       <c r="B2" s="8"/>
       <c r="D2" s="2"/>
@@ -3556,7 +3843,7 @@
       <c r="I2" s="8"/>
       <c r="J2" s="2"/>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="2"/>
       <c r="B3" s="8"/>
       <c r="D3" s="2"/>
@@ -3564,7 +3851,7 @@
       <c r="I3" s="8"/>
       <c r="J3" s="2"/>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="2"/>
       <c r="B4" s="8"/>
       <c r="D4" s="2"/>
@@ -3572,7 +3859,7 @@
       <c r="I4" s="8"/>
       <c r="J4" s="2"/>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" s="2"/>
       <c r="B5" s="8"/>
       <c r="D5" s="2"/>
@@ -3580,7 +3867,7 @@
       <c r="I5" s="8"/>
       <c r="J5" s="2"/>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" s="2"/>
       <c r="B6" s="8"/>
       <c r="D6" s="2"/>
@@ -3588,7 +3875,7 @@
       <c r="I6" s="8"/>
       <c r="J6" s="2"/>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" s="2"/>
       <c r="B7" s="8"/>
       <c r="D7" s="2"/>
@@ -3596,7 +3883,7 @@
       <c r="I7" s="8"/>
       <c r="J7" s="2"/>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" s="2"/>
       <c r="B8" s="8"/>
       <c r="D8" s="2"/>
@@ -3604,7 +3891,7 @@
       <c r="I8" s="8"/>
       <c r="J8" s="2"/>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" s="2"/>
       <c r="B9" s="8"/>
       <c r="D9" s="2"/>
@@ -3612,7 +3899,7 @@
       <c r="I9" s="8"/>
       <c r="J9" s="2"/>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" s="2"/>
       <c r="B10" s="8"/>
       <c r="D10" s="2"/>
@@ -3620,7 +3907,7 @@
       <c r="I10" s="8"/>
       <c r="J10" s="2"/>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" s="2"/>
       <c r="B11" s="8"/>
       <c r="D11" s="2"/>
@@ -3628,7 +3915,7 @@
       <c r="I11" s="8"/>
       <c r="J11" s="2"/>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" s="2"/>
       <c r="B12" s="8"/>
       <c r="D12" s="2"/>
@@ -3636,7 +3923,7 @@
       <c r="I12" s="8"/>
       <c r="J12" s="2"/>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" s="2"/>
       <c r="B13" s="8"/>
       <c r="D13" s="2"/>
@@ -3644,7 +3931,7 @@
       <c r="I13" s="8"/>
       <c r="J13" s="2"/>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" s="2"/>
       <c r="B14" s="8"/>
       <c r="D14" s="2"/>
@@ -3652,7 +3939,7 @@
       <c r="I14" s="8"/>
       <c r="J14" s="2"/>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" s="2"/>
       <c r="B15" s="8"/>
       <c r="D15" s="2"/>
@@ -3660,7 +3947,7 @@
       <c r="I15" s="8"/>
       <c r="J15" s="2"/>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" s="2"/>
       <c r="B16" s="8"/>
       <c r="D16" s="2"/>
@@ -3668,7 +3955,7 @@
       <c r="I16" s="8"/>
       <c r="J16" s="2"/>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17" s="2"/>
       <c r="B17" s="8"/>
       <c r="D17" s="2"/>
@@ -3676,7 +3963,7 @@
       <c r="I17" s="8"/>
       <c r="J17" s="2"/>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18" s="2"/>
       <c r="B18" s="8"/>
       <c r="D18" s="2"/>
@@ -3684,7 +3971,7 @@
       <c r="I18" s="8"/>
       <c r="J18" s="2"/>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A19" s="2"/>
       <c r="B19" s="8"/>
       <c r="D19" s="2"/>
@@ -3692,7 +3979,7 @@
       <c r="I19" s="8"/>
       <c r="J19" s="2"/>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A20" s="2"/>
       <c r="B20" s="8"/>
       <c r="D20" s="2"/>
@@ -3700,7 +3987,7 @@
       <c r="I20" s="8"/>
       <c r="J20" s="2"/>
     </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A21" s="2"/>
       <c r="B21" s="8"/>
       <c r="D21" s="2"/>
@@ -3708,7 +3995,7 @@
       <c r="I21" s="8"/>
       <c r="J21" s="2"/>
     </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A22" s="2"/>
       <c r="B22" s="8"/>
       <c r="D22" s="2"/>
@@ -3716,7 +4003,7 @@
       <c r="I22" s="8"/>
       <c r="J22" s="2"/>
     </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A23" s="2"/>
       <c r="B23" s="8"/>
       <c r="D23" s="2"/>
@@ -3724,7 +4011,7 @@
       <c r="I23" s="8"/>
       <c r="J23" s="2"/>
     </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A24" s="2"/>
       <c r="B24" s="8"/>
       <c r="D24" s="2"/>
@@ -3732,7 +4019,7 @@
       <c r="I24" s="8"/>
       <c r="J24" s="2"/>
     </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A25" s="2"/>
       <c r="B25" s="8"/>
       <c r="D25" s="2"/>
@@ -3740,7 +4027,7 @@
       <c r="I25" s="8"/>
       <c r="J25" s="2"/>
     </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A26" s="2"/>
       <c r="B26" s="8"/>
       <c r="D26" s="2"/>
@@ -3748,7 +4035,7 @@
       <c r="I26" s="8"/>
       <c r="J26" s="2"/>
     </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A27" s="2"/>
       <c r="B27" s="8"/>
       <c r="D27" s="2"/>
@@ -3756,7 +4043,7 @@
       <c r="I27" s="8"/>
       <c r="J27" s="2"/>
     </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A28" s="2"/>
       <c r="B28" s="8"/>
       <c r="D28" s="2"/>
@@ -3764,7 +4051,7 @@
       <c r="I28" s="8"/>
       <c r="J28" s="2"/>
     </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A29" s="2"/>
       <c r="B29" s="8"/>
       <c r="D29" s="2"/>
@@ -3772,7 +4059,7 @@
       <c r="I29" s="8"/>
       <c r="J29" s="2"/>
     </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A30" s="2"/>
       <c r="B30" s="8"/>
       <c r="D30" s="2"/>
@@ -3780,7 +4067,7 @@
       <c r="I30" s="8"/>
       <c r="J30" s="2"/>
     </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A31" s="2"/>
       <c r="B31" s="8"/>
       <c r="D31" s="2"/>
@@ -3788,7 +4075,7 @@
       <c r="I31" s="8"/>
       <c r="J31" s="2"/>
     </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A32" s="2"/>
       <c r="B32" s="8"/>
       <c r="D32" s="2"/>
@@ -3796,7 +4083,7 @@
       <c r="I32" s="8"/>
       <c r="J32" s="2"/>
     </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A33" s="2"/>
       <c r="B33" s="8"/>
       <c r="D33" s="2"/>
@@ -3804,7 +4091,7 @@
       <c r="I33" s="8"/>
       <c r="J33" s="2"/>
     </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A34" s="2"/>
       <c r="B34" s="8"/>
       <c r="D34" s="2"/>
@@ -3812,7 +4099,7 @@
       <c r="I34" s="8"/>
       <c r="J34" s="2"/>
     </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A35" s="2"/>
       <c r="B35" s="8"/>
       <c r="D35" s="2"/>
@@ -3820,7 +4107,7 @@
       <c r="I35" s="8"/>
       <c r="J35" s="2"/>
     </row>
-    <row r="36" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A36" s="2"/>
       <c r="B36" s="8"/>
       <c r="D36" s="2"/>
@@ -3828,7 +4115,7 @@
       <c r="I36" s="8"/>
       <c r="J36" s="2"/>
     </row>
-    <row r="37" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A37" s="2"/>
       <c r="B37" s="8"/>
       <c r="D37" s="2"/>
@@ -3836,7 +4123,7 @@
       <c r="I37" s="8"/>
       <c r="J37" s="2"/>
     </row>
-    <row r="38" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A38" s="2"/>
       <c r="B38" s="8"/>
       <c r="D38" s="2"/>
@@ -3844,7 +4131,7 @@
       <c r="I38" s="8"/>
       <c r="J38" s="2"/>
     </row>
-    <row r="39" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A39" s="2"/>
       <c r="B39" s="8"/>
       <c r="D39" s="2"/>
@@ -3852,7 +4139,7 @@
       <c r="I39" s="8"/>
       <c r="J39" s="2"/>
     </row>
-    <row r="40" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A40" s="2"/>
       <c r="B40" s="8"/>
       <c r="D40" s="2"/>
@@ -3860,7 +4147,7 @@
       <c r="I40" s="8"/>
       <c r="J40" s="2"/>
     </row>
-    <row r="41" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A41" s="2"/>
       <c r="B41" s="8"/>
       <c r="D41" s="2"/>
@@ -3868,7 +4155,7 @@
       <c r="I41" s="8"/>
       <c r="J41" s="2"/>
     </row>
-    <row r="42" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A42" s="2"/>
       <c r="B42" s="8"/>
       <c r="D42" s="2"/>
@@ -3876,7 +4163,7 @@
       <c r="I42" s="8"/>
       <c r="J42" s="2"/>
     </row>
-    <row r="43" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A43" s="2"/>
       <c r="B43" s="8"/>
       <c r="D43" s="2"/>
@@ -3884,7 +4171,7 @@
       <c r="I43" s="8"/>
       <c r="J43" s="2"/>
     </row>
-    <row r="44" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A44" s="2"/>
       <c r="B44" s="8"/>
       <c r="D44" s="2"/>
@@ -3892,7 +4179,7 @@
       <c r="I44" s="8"/>
       <c r="J44" s="2"/>
     </row>
-    <row r="45" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A45" s="2"/>
       <c r="B45" s="8"/>
       <c r="D45" s="2"/>
@@ -3900,7 +4187,7 @@
       <c r="I45" s="8"/>
       <c r="J45" s="2"/>
     </row>
-    <row r="46" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A46" s="2"/>
       <c r="B46" s="8"/>
       <c r="D46" s="2"/>
@@ -3908,7 +4195,7 @@
       <c r="I46" s="8"/>
       <c r="J46" s="2"/>
     </row>
-    <row r="47" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A47" s="2"/>
       <c r="B47" s="8"/>
       <c r="D47" s="2"/>
@@ -3916,7 +4203,7 @@
       <c r="I47" s="8"/>
       <c r="J47" s="2"/>
     </row>
-    <row r="48" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A48" s="2"/>
       <c r="B48" s="8"/>
       <c r="D48" s="2"/>
@@ -3924,7 +4211,7 @@
       <c r="I48" s="8"/>
       <c r="J48" s="2"/>
     </row>
-    <row r="49" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A49" s="2"/>
       <c r="B49" s="8"/>
       <c r="D49" s="2"/>
@@ -3932,7 +4219,7 @@
       <c r="I49" s="8"/>
       <c r="J49" s="2"/>
     </row>
-    <row r="50" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A50" s="2"/>
       <c r="B50" s="8"/>
       <c r="D50" s="2"/>
@@ -3940,7 +4227,7 @@
       <c r="I50" s="8"/>
       <c r="J50" s="2"/>
     </row>
-    <row r="51" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A51" s="2"/>
       <c r="B51" s="8"/>
       <c r="D51" s="2"/>
@@ -3948,7 +4235,7 @@
       <c r="I51" s="8"/>
       <c r="J51" s="2"/>
     </row>
-    <row r="52" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A52" s="2"/>
       <c r="B52" s="8"/>
       <c r="D52" s="2"/>
@@ -3956,7 +4243,7 @@
       <c r="I52" s="8"/>
       <c r="J52" s="2"/>
     </row>
-    <row r="53" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A53" s="2"/>
       <c r="B53" s="8"/>
       <c r="D53" s="2"/>
@@ -3964,7 +4251,7 @@
       <c r="I53" s="8"/>
       <c r="J53" s="2"/>
     </row>
-    <row r="54" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A54" s="2"/>
       <c r="B54" s="8"/>
       <c r="D54" s="2"/>
@@ -3972,7 +4259,7 @@
       <c r="I54" s="8"/>
       <c r="J54" s="2"/>
     </row>
-    <row r="55" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A55" s="2"/>
       <c r="B55" s="8"/>
       <c r="D55" s="2"/>
@@ -3980,7 +4267,7 @@
       <c r="I55" s="8"/>
       <c r="J55" s="2"/>
     </row>
-    <row r="56" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A56" s="2"/>
       <c r="B56" s="8"/>
       <c r="D56" s="2"/>
@@ -3988,7 +4275,7 @@
       <c r="I56" s="8"/>
       <c r="J56" s="2"/>
     </row>
-    <row r="57" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A57" s="2"/>
       <c r="B57" s="8"/>
       <c r="D57" s="2"/>
@@ -3996,7 +4283,7 @@
       <c r="I57" s="8"/>
       <c r="J57" s="2"/>
     </row>
-    <row r="58" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A58" s="2"/>
       <c r="B58" s="8"/>
       <c r="D58" s="2"/>
@@ -4004,7 +4291,7 @@
       <c r="I58" s="8"/>
       <c r="J58" s="2"/>
     </row>
-    <row r="59" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A59" s="2"/>
       <c r="B59" s="8"/>
       <c r="D59" s="2"/>
@@ -4012,7 +4299,7 @@
       <c r="I59" s="8"/>
       <c r="J59" s="2"/>
     </row>
-    <row r="60" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A60" s="2"/>
       <c r="B60" s="8"/>
       <c r="D60" s="2"/>
@@ -4020,7 +4307,7 @@
       <c r="I60" s="8"/>
       <c r="J60" s="2"/>
     </row>
-    <row r="61" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A61" s="2"/>
       <c r="B61" s="8"/>
       <c r="D61" s="2"/>
@@ -4028,7 +4315,7 @@
       <c r="I61" s="8"/>
       <c r="J61" s="2"/>
     </row>
-    <row r="62" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A62" s="2"/>
       <c r="B62" s="8"/>
       <c r="D62" s="2"/>
@@ -4036,7 +4323,7 @@
       <c r="I62" s="8"/>
       <c r="J62" s="2"/>
     </row>
-    <row r="63" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A63" s="2"/>
       <c r="B63" s="8"/>
       <c r="D63" s="2"/>
@@ -4044,7 +4331,7 @@
       <c r="I63" s="8"/>
       <c r="J63" s="2"/>
     </row>
-    <row r="64" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A64" s="2"/>
       <c r="B64" s="8"/>
       <c r="D64" s="2"/>
@@ -4052,7 +4339,7 @@
       <c r="I64" s="8"/>
       <c r="J64" s="2"/>
     </row>
-    <row r="65" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A65" s="2"/>
       <c r="B65" s="8"/>
       <c r="D65" s="2"/>
@@ -4060,7 +4347,7 @@
       <c r="I65" s="8"/>
       <c r="J65" s="2"/>
     </row>
-    <row r="66" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A66" s="2"/>
       <c r="B66" s="8"/>
       <c r="D66" s="2"/>
@@ -4068,7 +4355,7 @@
       <c r="I66" s="8"/>
       <c r="J66" s="2"/>
     </row>
-    <row r="67" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A67" s="2"/>
       <c r="B67" s="8"/>
       <c r="D67" s="2"/>
@@ -4076,7 +4363,7 @@
       <c r="I67" s="8"/>
       <c r="J67" s="2"/>
     </row>
-    <row r="68" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A68" s="2"/>
       <c r="B68" s="8"/>
       <c r="D68" s="2"/>
@@ -4084,7 +4371,7 @@
       <c r="I68" s="8"/>
       <c r="J68" s="2"/>
     </row>
-    <row r="69" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A69" s="2"/>
       <c r="B69" s="8"/>
       <c r="D69" s="2"/>
@@ -4092,7 +4379,7 @@
       <c r="I69" s="8"/>
       <c r="J69" s="2"/>
     </row>
-    <row r="70" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A70" s="2"/>
       <c r="B70" s="8"/>
       <c r="D70" s="2"/>
@@ -4100,7 +4387,7 @@
       <c r="I70" s="8"/>
       <c r="J70" s="2"/>
     </row>
-    <row r="71" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A71" s="2"/>
       <c r="B71" s="8"/>
       <c r="D71" s="2"/>
@@ -4108,7 +4395,7 @@
       <c r="I71" s="8"/>
       <c r="J71" s="2"/>
     </row>
-    <row r="72" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A72" s="2"/>
       <c r="B72" s="8"/>
       <c r="D72" s="2"/>
@@ -4116,7 +4403,7 @@
       <c r="I72" s="8"/>
       <c r="J72" s="2"/>
     </row>
-    <row r="73" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A73" s="2"/>
       <c r="B73" s="8"/>
       <c r="D73" s="2"/>
@@ -4124,7 +4411,7 @@
       <c r="I73" s="8"/>
       <c r="J73" s="2"/>
     </row>
-    <row r="74" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A74" s="2"/>
       <c r="B74" s="8"/>
       <c r="D74" s="2"/>
@@ -4132,7 +4419,7 @@
       <c r="I74" s="8"/>
       <c r="J74" s="2"/>
     </row>
-    <row r="75" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A75" s="2"/>
       <c r="B75" s="8"/>
       <c r="D75" s="2"/>
@@ -4140,7 +4427,7 @@
       <c r="I75" s="8"/>
       <c r="J75" s="2"/>
     </row>
-    <row r="76" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="76" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A76" s="2"/>
       <c r="B76" s="8"/>
       <c r="D76" s="2"/>
@@ -4148,7 +4435,7 @@
       <c r="I76" s="8"/>
       <c r="J76" s="2"/>
     </row>
-    <row r="77" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="77" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A77" s="2"/>
       <c r="B77" s="8"/>
       <c r="D77" s="2"/>
@@ -4156,7 +4443,7 @@
       <c r="I77" s="8"/>
       <c r="J77" s="2"/>
     </row>
-    <row r="78" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="78" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A78" s="2"/>
       <c r="B78" s="8"/>
       <c r="D78" s="2"/>
@@ -4164,7 +4451,7 @@
       <c r="I78" s="8"/>
       <c r="J78" s="2"/>
     </row>
-    <row r="79" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="79" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A79" s="2"/>
       <c r="B79" s="8"/>
       <c r="D79" s="2"/>
@@ -4172,7 +4459,7 @@
       <c r="I79" s="8"/>
       <c r="J79" s="2"/>
     </row>
-    <row r="80" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="80" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A80" s="2"/>
       <c r="B80" s="8"/>
       <c r="D80" s="2"/>
@@ -4180,7 +4467,7 @@
       <c r="I80" s="8"/>
       <c r="J80" s="2"/>
     </row>
-    <row r="81" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="81" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A81" s="2"/>
       <c r="B81" s="8"/>
       <c r="D81" s="2"/>
@@ -4188,7 +4475,7 @@
       <c r="I81" s="8"/>
       <c r="J81" s="2"/>
     </row>
-    <row r="82" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="82" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A82" s="2"/>
       <c r="B82" s="8"/>
       <c r="D82" s="2"/>
@@ -4196,7 +4483,7 @@
       <c r="I82" s="8"/>
       <c r="J82" s="2"/>
     </row>
-    <row r="83" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="83" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A83" s="2"/>
       <c r="B83" s="8"/>
       <c r="D83" s="2"/>
@@ -4204,7 +4491,7 @@
       <c r="I83" s="8"/>
       <c r="J83" s="2"/>
     </row>
-    <row r="84" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="84" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A84" s="2"/>
       <c r="B84" s="8"/>
       <c r="D84" s="2"/>
@@ -4212,7 +4499,7 @@
       <c r="I84" s="8"/>
       <c r="J84" s="2"/>
     </row>
-    <row r="85" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="85" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A85" s="2"/>
       <c r="B85" s="8"/>
       <c r="D85" s="2"/>
@@ -4220,7 +4507,7 @@
       <c r="I85" s="8"/>
       <c r="J85" s="2"/>
     </row>
-    <row r="86" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="86" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A86" s="2"/>
       <c r="B86" s="8"/>
       <c r="D86" s="2"/>
@@ -4228,7 +4515,7 @@
       <c r="I86" s="8"/>
       <c r="J86" s="2"/>
     </row>
-    <row r="87" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="87" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A87" s="2"/>
       <c r="B87" s="8"/>
       <c r="D87" s="2"/>
@@ -4236,7 +4523,7 @@
       <c r="I87" s="8"/>
       <c r="J87" s="2"/>
     </row>
-    <row r="88" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="88" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A88" s="2"/>
       <c r="B88" s="8"/>
       <c r="D88" s="2"/>
@@ -4244,7 +4531,7 @@
       <c r="I88" s="8"/>
       <c r="J88" s="2"/>
     </row>
-    <row r="89" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="89" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A89" s="2"/>
       <c r="B89" s="8"/>
       <c r="D89" s="2"/>
@@ -4252,7 +4539,7 @@
       <c r="I89" s="8"/>
       <c r="J89" s="2"/>
     </row>
-    <row r="90" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="90" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A90" s="2"/>
       <c r="B90" s="8"/>
       <c r="D90" s="2"/>
@@ -4260,7 +4547,7 @@
       <c r="I90" s="8"/>
       <c r="J90" s="2"/>
     </row>
-    <row r="91" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="91" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A91" s="2"/>
       <c r="B91" s="8"/>
       <c r="D91" s="2"/>
@@ -4268,7 +4555,7 @@
       <c r="I91" s="8"/>
       <c r="J91" s="2"/>
     </row>
-    <row r="92" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="92" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A92" s="2"/>
       <c r="B92" s="8"/>
       <c r="D92" s="2"/>
@@ -4276,7 +4563,7 @@
       <c r="I92" s="8"/>
       <c r="J92" s="2"/>
     </row>
-    <row r="93" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="93" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A93" s="2"/>
       <c r="B93" s="8"/>
       <c r="D93" s="2"/>
@@ -4284,7 +4571,7 @@
       <c r="I93" s="8"/>
       <c r="J93" s="2"/>
     </row>
-    <row r="94" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="94" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A94" s="2"/>
       <c r="B94" s="8"/>
       <c r="D94" s="2"/>
@@ -4292,7 +4579,7 @@
       <c r="I94" s="8"/>
       <c r="J94" s="2"/>
     </row>
-    <row r="95" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="95" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A95" s="2"/>
       <c r="B95" s="8"/>
       <c r="D95" s="2"/>
@@ -4300,7 +4587,7 @@
       <c r="I95" s="8"/>
       <c r="J95" s="2"/>
     </row>
-    <row r="96" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="96" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A96" s="2"/>
       <c r="B96" s="8"/>
       <c r="D96" s="2"/>
@@ -4308,7 +4595,7 @@
       <c r="I96" s="8"/>
       <c r="J96" s="2"/>
     </row>
-    <row r="97" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="97" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A97" s="2"/>
       <c r="B97" s="8"/>
       <c r="D97" s="2"/>
@@ -4316,7 +4603,7 @@
       <c r="I97" s="8"/>
       <c r="J97" s="2"/>
     </row>
-    <row r="98" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="98" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A98" s="2"/>
       <c r="B98" s="8"/>
       <c r="D98" s="2"/>
@@ -4324,7 +4611,7 @@
       <c r="I98" s="8"/>
       <c r="J98" s="2"/>
     </row>
-    <row r="99" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="99" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A99" s="2"/>
       <c r="B99" s="8"/>
       <c r="D99" s="2"/>
@@ -4332,7 +4619,7 @@
       <c r="I99" s="8"/>
       <c r="J99" s="2"/>
     </row>
-    <row r="100" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="100" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A100" s="2"/>
       <c r="B100" s="8"/>
       <c r="D100" s="2"/>

</xml_diff>

<commit_message>
Updated progress report for May 14 Wed by Avichal
</commit_message>
<xml_diff>
--- a/PR&IR.xlsx
+++ b/PR&IR.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SHIVYA KUMAR\Desktop\new415\CS415_A3\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\avichal avneel nath\Documents\Semester 7\CS415\A3\CS415_A3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FCBE4524-C6CA-4495-B5C8-C5EC464FB1CD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{446B9638-145F-47A9-8E17-E54F5F829A5D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{BFA1E21A-08FA-4F02-8C25-33C81C8EE970}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{BFA1E21A-08FA-4F02-8C25-33C81C8EE970}"/>
   </bookViews>
   <sheets>
     <sheet name="Avichal" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="35">
   <si>
     <t>Date</t>
   </si>
@@ -141,9 +141,6 @@
     <t>complete pending ToDos</t>
   </si>
   <si>
-    <t>13/0/2025</t>
-  </si>
-  <si>
     <t xml:space="preserve">Resolved merge conflict and synced with main. Researched on sqlalchemy vs pyodbc. Custom validation for enrollment services. </t>
   </si>
   <si>
@@ -153,43 +150,13 @@
     <t>Best Wishes w/ Backend.</t>
   </si>
   <si>
-    <t>Shivya Kumar</t>
+    <t>Completed custom exception handling for all routes and custom validtion for enrollment services</t>
   </si>
   <si>
-    <t>Convert UI for login, homepage and student profile</t>
+    <t>Fee and Hold services routing exceptions and validations</t>
   </si>
   <si>
-    <t>In Progress</t>
-  </si>
-  <si>
-    <t>Continue converting UI and setting route</t>
-  </si>
-  <si>
-    <t>I was unable to run the app locally, so I created a folder named run_main_app.py with the required code Once I did that I was able to start the Flask server successfully</t>
-  </si>
-  <si>
-    <t>Added header and footer to the remaining UIs, and converted UI for enrollment page.</t>
-  </si>
-  <si>
-    <t>Solve my routes and fix UI</t>
-  </si>
-  <si>
-    <t>Customizing UI and recovered deleted codes</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Continue converting UI </t>
-  </si>
-  <si>
-    <t>I added my routes in the same file app.py</t>
-  </si>
-  <si>
-    <t>shivya Kumar</t>
-  </si>
-  <si>
-    <t>continue implementing remaining UI logic based on feedback and custom validation with exception handling for all of her routes</t>
-  </si>
-  <si>
-    <t>Converted all user interface designs into HTML and set up respective routes.</t>
+    <t xml:space="preserve">Stay Healthy Aviiii. Don’t get sick </t>
   </si>
 </sst>
 </file>
@@ -200,7 +167,7 @@
     <numFmt numFmtId="164" formatCode="h"/>
     <numFmt numFmtId="165" formatCode="d/mm/yyyy;@"/>
   </numFmts>
-  <fonts count="3">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -241,7 +208,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -254,22 +221,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="35">
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
     <dxf>
       <numFmt numFmtId="30" formatCode="@"/>
     </dxf>
@@ -380,6 +336,15 @@
     </dxf>
     <dxf>
       <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="h"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="14" formatCode="0.00%"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="30" formatCode="@"/>
@@ -497,17 +462,17 @@
     <tableColumn id="2" xr3:uid="{55A78D6C-890A-4502-A184-DEEFF14BB82E}" name="Member Name" dataDxfId="25"/>
     <tableColumn id="3" xr3:uid="{57B9A516-E930-4C06-A589-24182A37BA85}" name="Task/Activity"/>
     <tableColumn id="4" xr3:uid="{A7CD18E8-808E-43EA-A960-7EDF2D2AB452}" name="Status"/>
-    <tableColumn id="5" xr3:uid="{A9BAB96D-D5FD-4C0D-A277-6E052D27EC3A}" name="% Complete" dataDxfId="2"/>
-    <tableColumn id="6" xr3:uid="{4EBDEBD4-A02D-4266-88BC-5E6088167CE4}" name="Hours Worked Today" dataDxfId="0"/>
-    <tableColumn id="7" xr3:uid="{88484166-6833-4A6B-B292-081E908E7876}" name="Next Steps" dataDxfId="1"/>
-    <tableColumn id="8" xr3:uid="{65034E84-46C0-4115-A351-A3C28C7B9EE1}" name="Notes/Comments" dataDxfId="24"/>
+    <tableColumn id="5" xr3:uid="{A9BAB96D-D5FD-4C0D-A277-6E052D27EC3A}" name="% Complete" dataDxfId="24"/>
+    <tableColumn id="6" xr3:uid="{4EBDEBD4-A02D-4266-88BC-5E6088167CE4}" name="Hours Worked Today" dataDxfId="23"/>
+    <tableColumn id="7" xr3:uid="{88484166-6833-4A6B-B292-081E908E7876}" name="Next Steps" dataDxfId="22"/>
+    <tableColumn id="8" xr3:uid="{65034E84-46C0-4115-A351-A3C28C7B9EE1}" name="Notes/Comments" dataDxfId="21"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium26" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{D9A2FBFA-47C8-4A27-8A35-991BC77E93AD}" name="Table14" displayName="Table14" ref="A1:H100" totalsRowShown="0" headerRowDxfId="23">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{D9A2FBFA-47C8-4A27-8A35-991BC77E93AD}" name="Table14" displayName="Table14" ref="A1:H100" totalsRowShown="0" headerRowDxfId="20">
   <autoFilter ref="A1:H100" xr:uid="{D9A2FBFA-47C8-4A27-8A35-991BC77E93AD}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
@@ -519,21 +484,21 @@
     <filterColumn colId="7" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="8">
-    <tableColumn id="1" xr3:uid="{9DF80C4D-D075-4428-A54F-FD6AD093D08C}" name="Date" dataDxfId="22"/>
-    <tableColumn id="2" xr3:uid="{EBFC72C6-272F-4910-98B7-AD481D68F5CF}" name="Member Name" dataDxfId="21"/>
+    <tableColumn id="1" xr3:uid="{9DF80C4D-D075-4428-A54F-FD6AD093D08C}" name="Date" dataDxfId="19"/>
+    <tableColumn id="2" xr3:uid="{EBFC72C6-272F-4910-98B7-AD481D68F5CF}" name="Member Name" dataDxfId="18"/>
     <tableColumn id="3" xr3:uid="{9F5B3984-7002-4FEA-8B81-D2D8284783D7}" name="Task/Activity"/>
     <tableColumn id="4" xr3:uid="{5F85F44B-886F-440F-9E69-8335A039C2E6}" name="Status"/>
-    <tableColumn id="5" xr3:uid="{AF0043ED-9EF2-470B-9735-7321011714BA}" name="% Complete" dataDxfId="20"/>
-    <tableColumn id="6" xr3:uid="{4F961AD8-B86B-411C-BB04-8D7EE4DD134D}" name="Hours Worked Today" dataDxfId="19"/>
-    <tableColumn id="7" xr3:uid="{34EBB1FC-FFD7-47AB-A959-A220B742401C}" name="Next Steps" dataDxfId="18"/>
-    <tableColumn id="8" xr3:uid="{128DAA9E-15FB-4BB9-B76B-4A920C859038}" name="Notes/Comments" dataDxfId="17"/>
+    <tableColumn id="5" xr3:uid="{AF0043ED-9EF2-470B-9735-7321011714BA}" name="% Complete" dataDxfId="17"/>
+    <tableColumn id="6" xr3:uid="{4F961AD8-B86B-411C-BB04-8D7EE4DD134D}" name="Hours Worked Today" dataDxfId="16"/>
+    <tableColumn id="7" xr3:uid="{34EBB1FC-FFD7-47AB-A959-A220B742401C}" name="Next Steps" dataDxfId="15"/>
+    <tableColumn id="8" xr3:uid="{128DAA9E-15FB-4BB9-B76B-4A920C859038}" name="Notes/Comments" dataDxfId="14"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium26" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{646C4EC7-41A3-4570-9D38-06D55FDE20F6}" name="Table15" displayName="Table15" ref="A1:H100" totalsRowShown="0" headerRowDxfId="16">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{646C4EC7-41A3-4570-9D38-06D55FDE20F6}" name="Table15" displayName="Table15" ref="A1:H100" totalsRowShown="0" headerRowDxfId="13">
   <autoFilter ref="A1:H100" xr:uid="{646C4EC7-41A3-4570-9D38-06D55FDE20F6}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
@@ -545,21 +510,21 @@
     <filterColumn colId="7" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="8">
-    <tableColumn id="1" xr3:uid="{13D6CE41-CF73-478C-B7F6-3B0C25C48DFD}" name="Date" dataDxfId="15"/>
-    <tableColumn id="2" xr3:uid="{E468B109-F9F1-48D8-BECE-0F7015DD8D95}" name="Member Name" dataDxfId="14"/>
+    <tableColumn id="1" xr3:uid="{13D6CE41-CF73-478C-B7F6-3B0C25C48DFD}" name="Date" dataDxfId="12"/>
+    <tableColumn id="2" xr3:uid="{E468B109-F9F1-48D8-BECE-0F7015DD8D95}" name="Member Name" dataDxfId="11"/>
     <tableColumn id="3" xr3:uid="{279E5366-E900-45EE-80D9-5446A85E61AD}" name="Task/Activity"/>
     <tableColumn id="4" xr3:uid="{63D996BE-E8E2-4186-8CD4-49EAB9AA8847}" name="Status"/>
-    <tableColumn id="5" xr3:uid="{2FF82CF3-E17A-4896-9C9C-7339D28CD4A7}" name="% Complete" dataDxfId="13"/>
-    <tableColumn id="6" xr3:uid="{67DCB379-6881-4BBC-A633-BD51853A9B6B}" name="Hours Worked Today" dataDxfId="12"/>
-    <tableColumn id="7" xr3:uid="{91C8F225-F251-45F2-BC41-843547B77A6F}" name="Next Steps" dataDxfId="11"/>
-    <tableColumn id="8" xr3:uid="{EEAB1D68-5668-4B1F-8473-D3A49DA7E015}" name="Notes/Comments" dataDxfId="10"/>
+    <tableColumn id="5" xr3:uid="{2FF82CF3-E17A-4896-9C9C-7339D28CD4A7}" name="% Complete" dataDxfId="10"/>
+    <tableColumn id="6" xr3:uid="{67DCB379-6881-4BBC-A633-BD51853A9B6B}" name="Hours Worked Today" dataDxfId="9"/>
+    <tableColumn id="7" xr3:uid="{91C8F225-F251-45F2-BC41-843547B77A6F}" name="Next Steps" dataDxfId="8"/>
+    <tableColumn id="8" xr3:uid="{EEAB1D68-5668-4B1F-8473-D3A49DA7E015}" name="Notes/Comments" dataDxfId="7"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium26" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{5818BB59-8F2C-4810-A78D-CBC8FA25F524}" name="Table5" displayName="Table5" ref="A1:J100" totalsRowShown="0" headerRowDxfId="9">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{5818BB59-8F2C-4810-A78D-CBC8FA25F524}" name="Table5" displayName="Table5" ref="A1:J100" totalsRowShown="0" headerRowDxfId="6">
   <autoFilter ref="A1:J100" xr:uid="{5818BB59-8F2C-4810-A78D-CBC8FA25F524}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
@@ -573,16 +538,16 @@
     <filterColumn colId="9" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="10">
-    <tableColumn id="1" xr3:uid="{BC250DF1-329E-4733-8702-E009738E43CB}" name="Header" dataDxfId="8"/>
-    <tableColumn id="2" xr3:uid="{F6CCDA73-9A12-472B-A535-0F3DC2A5CF61}" name="Date Raised" dataDxfId="7"/>
+    <tableColumn id="1" xr3:uid="{BC250DF1-329E-4733-8702-E009738E43CB}" name="Header" dataDxfId="5"/>
+    <tableColumn id="2" xr3:uid="{F6CCDA73-9A12-472B-A535-0F3DC2A5CF61}" name="Date Raised" dataDxfId="4"/>
     <tableColumn id="3" xr3:uid="{2E3C7862-32AA-44B8-BCC3-2F9299A8F3DC}" name="Raised By"/>
-    <tableColumn id="4" xr3:uid="{FB9438A9-92FB-4A8D-95A5-F17D6EF9AA82}" name="Issue Description" dataDxfId="6"/>
+    <tableColumn id="4" xr3:uid="{FB9438A9-92FB-4A8D-95A5-F17D6EF9AA82}" name="Issue Description" dataDxfId="3"/>
     <tableColumn id="5" xr3:uid="{48223256-C4C0-467B-9FA7-AA8E7742B58A}" name="Impact"/>
     <tableColumn id="6" xr3:uid="{EEDBAAB2-0361-4BF5-8FDB-3FAD49E87C1B}" name="Priority"/>
     <tableColumn id="7" xr3:uid="{515F6321-7FC0-4B4E-A422-3A0E332B7B97}" name="Status"/>
-    <tableColumn id="8" xr3:uid="{60A704D7-818B-442C-91EF-B82765B2618D}" name="Resolution Plan" dataDxfId="5"/>
-    <tableColumn id="9" xr3:uid="{D95E2A6F-E7D4-4FC5-9AAF-1E3DBEE8D8FC}" name="Date Resolved" dataDxfId="4"/>
-    <tableColumn id="10" xr3:uid="{D43B4A1C-AE3D-43D4-A514-7BAA3E281FD3}" name="Notes/Comments" dataDxfId="3"/>
+    <tableColumn id="8" xr3:uid="{60A704D7-818B-442C-91EF-B82765B2618D}" name="Resolution Plan" dataDxfId="2"/>
+    <tableColumn id="9" xr3:uid="{D95E2A6F-E7D4-4FC5-9AAF-1E3DBEE8D8FC}" name="Date Resolved" dataDxfId="1"/>
+    <tableColumn id="10" xr3:uid="{D43B4A1C-AE3D-43D4-A514-7BAA3E281FD3}" name="Notes/Comments" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight15" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -936,30 +901,30 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{37EAA098-74C6-4411-B7E2-26AD2DCBC3F0}">
   <dimension ref="A1:H28"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H6" sqref="H6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H7" sqref="H7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.3984375" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.59765625" style="2" customWidth="1"/>
+    <col min="1" max="1" width="10.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.5703125" style="2" customWidth="1"/>
     <col min="3" max="3" width="58" customWidth="1"/>
-    <col min="5" max="5" width="13.09765625" style="3" customWidth="1"/>
-    <col min="6" max="6" width="20.8984375" style="4" customWidth="1"/>
-    <col min="7" max="7" width="34.8984375" style="2" customWidth="1"/>
-    <col min="8" max="8" width="43.3984375" style="2" customWidth="1"/>
-    <col min="11" max="11" width="9.09765625" customWidth="1"/>
-    <col min="12" max="12" width="13.296875" customWidth="1"/>
-    <col min="13" max="13" width="11.3984375" customWidth="1"/>
-    <col min="14" max="14" width="17.3984375" customWidth="1"/>
-    <col min="16" max="16" width="9.09765625" customWidth="1"/>
-    <col min="18" max="18" width="16.59765625" customWidth="1"/>
-    <col min="19" max="19" width="14.69921875" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="16.8984375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.140625" style="3" customWidth="1"/>
+    <col min="6" max="6" width="20.85546875" style="4" customWidth="1"/>
+    <col min="7" max="7" width="34.85546875" style="2" customWidth="1"/>
+    <col min="8" max="8" width="43.42578125" style="2" customWidth="1"/>
+    <col min="11" max="11" width="9.140625" customWidth="1"/>
+    <col min="12" max="12" width="13.28515625" customWidth="1"/>
+    <col min="13" max="13" width="11.42578125" customWidth="1"/>
+    <col min="14" max="14" width="17.42578125" customWidth="1"/>
+    <col min="16" max="16" width="9.140625" customWidth="1"/>
+    <col min="18" max="18" width="16.5703125" customWidth="1"/>
+    <col min="19" max="19" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="16.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="15.75">
+    <row r="1" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
@@ -985,7 +950,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="15.75">
+    <row r="2" spans="1:8" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A2" s="1">
         <v>45786</v>
       </c>
@@ -1011,7 +976,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="3" spans="1:8" ht="120">
+    <row r="3" spans="1:8" ht="120" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>45787</v>
       </c>
@@ -1034,7 +999,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="4" spans="1:8" ht="15">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>45788</v>
       </c>
@@ -1054,7 +1019,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="5" spans="1:8" ht="76.5" customHeight="1">
+    <row r="5" spans="1:8" ht="76.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>45789</v>
       </c>
@@ -1077,12 +1042,12 @@
         <v>27</v>
       </c>
     </row>
-    <row r="6" spans="1:8" ht="15">
-      <c r="A6" s="1" t="s">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A6" s="1">
+        <v>45790</v>
+      </c>
+      <c r="C6" t="s">
         <v>29</v>
-      </c>
-      <c r="C6" t="s">
-        <v>30</v>
       </c>
       <c r="D6" t="s">
         <v>17</v>
@@ -1094,86 +1059,105 @@
         <v>5</v>
       </c>
       <c r="G6" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="H6" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="H6" s="2" t="s">
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A7" s="1">
+        <v>45791</v>
+      </c>
+      <c r="C7" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="7" spans="1:8" ht="15">
-      <c r="E7"/>
-      <c r="F7"/>
-    </row>
-    <row r="8" spans="1:8" ht="15">
+      <c r="D7" t="s">
+        <v>17</v>
+      </c>
+      <c r="E7">
+        <v>100</v>
+      </c>
+      <c r="F7">
+        <v>2</v>
+      </c>
+      <c r="G7" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="H7" s="2" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="E8"/>
       <c r="F8"/>
     </row>
-    <row r="9" spans="1:8" ht="15">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="E9"/>
       <c r="F9"/>
     </row>
-    <row r="10" spans="1:8" ht="15">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="E10"/>
       <c r="F10"/>
     </row>
-    <row r="11" spans="1:8" ht="15">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="E11"/>
       <c r="F11"/>
     </row>
-    <row r="12" spans="1:8" ht="15">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="E12"/>
       <c r="F12"/>
     </row>
-    <row r="13" spans="1:8" ht="15">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="E13"/>
       <c r="F13"/>
     </row>
-    <row r="14" spans="1:8" ht="15">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="E14"/>
       <c r="F14"/>
     </row>
-    <row r="15" spans="1:8">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="E15"/>
       <c r="F15"/>
     </row>
-    <row r="16" spans="1:8">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="E16"/>
       <c r="F16"/>
     </row>
-    <row r="17" spans="6:6">
+    <row r="17" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F17"/>
     </row>
-    <row r="18" spans="6:6">
+    <row r="18" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F18"/>
     </row>
-    <row r="19" spans="6:6">
+    <row r="19" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F19"/>
     </row>
-    <row r="20" spans="6:6">
+    <row r="20" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F20"/>
     </row>
-    <row r="21" spans="6:6">
+    <row r="21" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F21"/>
     </row>
-    <row r="22" spans="6:6">
+    <row r="22" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F22"/>
     </row>
-    <row r="23" spans="6:6">
+    <row r="23" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F23"/>
     </row>
-    <row r="24" spans="6:6">
+    <row r="24" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F24"/>
     </row>
-    <row r="25" spans="6:6">
+    <row r="25" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F25"/>
     </row>
-    <row r="26" spans="6:6">
+    <row r="26" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F26"/>
     </row>
-    <row r="27" spans="6:6">
+    <row r="27" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F27"/>
     </row>
-    <row r="28" spans="6:6">
+    <row r="28" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F28"/>
     </row>
   </sheetData>
@@ -1196,7 +1180,7 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
   <ignoredErrors>
-    <ignoredError sqref="D7:D16" listDataValidation="1"/>
+    <ignoredError sqref="D8:D16" listDataValidation="1"/>
   </ignoredErrors>
   <tableParts count="1">
     <tablePart r:id="rId2"/>
@@ -1208,23 +1192,23 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3BDA6702-5DDF-42FB-988E-13FBEB26F5C9}">
   <dimension ref="A1:H100"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.8984375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="17.296875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="54.69921875" customWidth="1"/>
-    <col min="4" max="4" width="8.8984375" customWidth="1"/>
-    <col min="5" max="5" width="14.8984375" style="11" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="23.59765625" style="11" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="29.19921875" customWidth="1"/>
-    <col min="8" max="8" width="39.69921875" customWidth="1"/>
+    <col min="1" max="1" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="23.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="19.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="15.75">
+    <row r="1" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
@@ -1237,10 +1221,10 @@
       <c r="D1" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="10" t="s">
+      <c r="E1" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="10" t="s">
+      <c r="F1" s="7" t="s">
         <v>5</v>
       </c>
       <c r="G1" s="7" t="s">
@@ -1250,673 +1234,793 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="15">
-      <c r="A2" s="8">
-        <v>45786</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="C2" t="s">
-        <v>34</v>
-      </c>
-      <c r="D2" t="s">
-        <v>35</v>
-      </c>
-      <c r="E2" s="11">
-        <v>90</v>
-      </c>
-      <c r="F2" s="11">
-        <v>8</v>
-      </c>
-      <c r="G2" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="H2" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" ht="15">
-      <c r="A3" s="8">
-        <v>45787</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="C3" t="s">
-        <v>38</v>
-      </c>
-      <c r="D3" t="s">
-        <v>35</v>
-      </c>
-      <c r="E3" s="11">
-        <v>90</v>
-      </c>
-      <c r="F3" s="11">
-        <v>8</v>
-      </c>
-      <c r="G3" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="H3" s="2" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" ht="15">
-      <c r="A4" s="8">
-        <v>45789</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="C4" t="s">
-        <v>40</v>
-      </c>
-      <c r="D4" t="s">
-        <v>35</v>
-      </c>
-      <c r="E4" s="11">
-        <v>90</v>
-      </c>
-      <c r="F4" s="11">
-        <v>5</v>
-      </c>
-      <c r="G4" s="2" t="s">
-        <v>41</v>
-      </c>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2" s="8"/>
+      <c r="B2" s="2"/>
+      <c r="E2" s="3"/>
+      <c r="G2" s="2"/>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3" s="8"/>
+      <c r="B3" s="2"/>
+      <c r="E3" s="3"/>
+      <c r="F3" s="4"/>
+      <c r="G3" s="2"/>
+      <c r="H3" s="2"/>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4" s="8"/>
+      <c r="B4" s="2"/>
+      <c r="E4" s="3"/>
+      <c r="F4" s="4"/>
+      <c r="G4" s="2"/>
       <c r="H4" s="2"/>
     </row>
-    <row r="5" spans="1:8" ht="15">
-      <c r="A5" s="8">
-        <v>45790</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="C5" t="s">
-        <v>45</v>
-      </c>
-      <c r="D5" t="s">
-        <v>17</v>
-      </c>
-      <c r="E5" s="11">
-        <v>100</v>
-      </c>
-      <c r="F5" s="11">
-        <v>5</v>
-      </c>
-      <c r="G5" s="2" t="s">
-        <v>44</v>
-      </c>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A5" s="8"/>
+      <c r="B5" s="2"/>
+      <c r="E5" s="3"/>
+      <c r="F5" s="4"/>
+      <c r="G5" s="2"/>
       <c r="H5" s="2"/>
     </row>
-    <row r="6" spans="1:8" ht="15">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="8"/>
       <c r="B6" s="2"/>
+      <c r="E6" s="3"/>
+      <c r="F6" s="4"/>
       <c r="G6" s="2"/>
       <c r="H6" s="2"/>
     </row>
-    <row r="7" spans="1:8" ht="15">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="8"/>
       <c r="B7" s="2"/>
+      <c r="E7" s="3"/>
+      <c r="F7" s="4"/>
       <c r="G7" s="2"/>
       <c r="H7" s="2"/>
     </row>
-    <row r="8" spans="1:8" ht="15">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="8"/>
       <c r="B8" s="2"/>
+      <c r="E8" s="3"/>
+      <c r="F8" s="4"/>
       <c r="G8" s="2"/>
       <c r="H8" s="2"/>
     </row>
-    <row r="9" spans="1:8" ht="15">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="8"/>
       <c r="B9" s="2"/>
+      <c r="E9" s="3"/>
+      <c r="F9" s="4"/>
       <c r="G9" s="2"/>
       <c r="H9" s="2"/>
     </row>
-    <row r="10" spans="1:8" ht="15">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="8"/>
       <c r="B10" s="2"/>
+      <c r="E10" s="3"/>
+      <c r="F10" s="4"/>
       <c r="G10" s="2"/>
       <c r="H10" s="2"/>
     </row>
-    <row r="11" spans="1:8" ht="15">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="8"/>
       <c r="B11" s="2"/>
+      <c r="E11" s="3"/>
+      <c r="F11" s="4"/>
       <c r="G11" s="2"/>
       <c r="H11" s="2"/>
     </row>
-    <row r="12" spans="1:8" ht="15">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="8"/>
       <c r="B12" s="2"/>
+      <c r="E12" s="3"/>
+      <c r="F12" s="4"/>
       <c r="G12" s="2"/>
       <c r="H12" s="2"/>
     </row>
-    <row r="13" spans="1:8" ht="15">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="8"/>
       <c r="B13" s="2"/>
+      <c r="E13" s="3"/>
+      <c r="F13" s="4"/>
       <c r="G13" s="2"/>
       <c r="H13" s="2"/>
     </row>
-    <row r="14" spans="1:8" ht="15">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" s="8"/>
       <c r="B14" s="2"/>
+      <c r="E14" s="3"/>
+      <c r="F14" s="4"/>
       <c r="G14" s="2"/>
       <c r="H14" s="2"/>
     </row>
-    <row r="15" spans="1:8" ht="15">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" s="8"/>
       <c r="B15" s="2"/>
+      <c r="E15" s="3"/>
+      <c r="F15" s="4"/>
       <c r="G15" s="2"/>
       <c r="H15" s="2"/>
     </row>
-    <row r="16" spans="1:8" ht="15">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" s="8"/>
       <c r="B16" s="2"/>
+      <c r="E16" s="3"/>
+      <c r="F16" s="4"/>
       <c r="G16" s="2"/>
       <c r="H16" s="2"/>
     </row>
-    <row r="17" spans="1:8" ht="15">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" s="8"/>
       <c r="B17" s="2"/>
+      <c r="E17" s="3"/>
+      <c r="F17" s="4"/>
       <c r="G17" s="2"/>
       <c r="H17" s="2"/>
     </row>
-    <row r="18" spans="1:8" ht="15">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" s="8"/>
       <c r="B18" s="2"/>
+      <c r="E18" s="3"/>
+      <c r="F18" s="4"/>
       <c r="G18" s="2"/>
       <c r="H18" s="2"/>
     </row>
-    <row r="19" spans="1:8" ht="15">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" s="8"/>
       <c r="B19" s="2"/>
+      <c r="E19" s="3"/>
+      <c r="F19" s="4"/>
       <c r="G19" s="2"/>
       <c r="H19" s="2"/>
     </row>
-    <row r="20" spans="1:8" ht="15">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" s="8"/>
       <c r="B20" s="2"/>
+      <c r="E20" s="3"/>
+      <c r="F20" s="4"/>
       <c r="G20" s="2"/>
       <c r="H20" s="2"/>
     </row>
-    <row r="21" spans="1:8" ht="15">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" s="8"/>
       <c r="B21" s="2"/>
+      <c r="E21" s="3"/>
+      <c r="F21" s="4"/>
       <c r="G21" s="2"/>
       <c r="H21" s="2"/>
     </row>
-    <row r="22" spans="1:8" ht="15">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" s="8"/>
       <c r="B22" s="2"/>
+      <c r="E22" s="3"/>
+      <c r="F22" s="4"/>
       <c r="G22" s="2"/>
       <c r="H22" s="2"/>
     </row>
-    <row r="23" spans="1:8" ht="15">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" s="8"/>
       <c r="B23" s="2"/>
+      <c r="E23" s="3"/>
+      <c r="F23" s="4"/>
       <c r="G23" s="2"/>
       <c r="H23" s="2"/>
     </row>
-    <row r="24" spans="1:8" ht="15">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24" s="8"/>
       <c r="B24" s="2"/>
+      <c r="E24" s="3"/>
+      <c r="F24" s="4"/>
       <c r="G24" s="2"/>
       <c r="H24" s="2"/>
     </row>
-    <row r="25" spans="1:8" ht="15">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25" s="8"/>
       <c r="B25" s="2"/>
+      <c r="E25" s="3"/>
+      <c r="F25" s="4"/>
       <c r="G25" s="2"/>
       <c r="H25" s="2"/>
     </row>
-    <row r="26" spans="1:8">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26" s="8"/>
       <c r="B26" s="2"/>
+      <c r="E26" s="3"/>
+      <c r="F26" s="4"/>
       <c r="G26" s="2"/>
       <c r="H26" s="2"/>
     </row>
-    <row r="27" spans="1:8">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A27" s="8"/>
       <c r="B27" s="2"/>
+      <c r="E27" s="3"/>
+      <c r="F27" s="4"/>
       <c r="G27" s="2"/>
       <c r="H27" s="2"/>
     </row>
-    <row r="28" spans="1:8">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A28" s="8"/>
       <c r="B28" s="2"/>
+      <c r="E28" s="3"/>
+      <c r="F28" s="4"/>
       <c r="G28" s="2"/>
       <c r="H28" s="2"/>
     </row>
-    <row r="29" spans="1:8">
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A29" s="8"/>
       <c r="B29" s="2"/>
+      <c r="E29" s="3"/>
+      <c r="F29" s="4"/>
       <c r="G29" s="2"/>
       <c r="H29" s="2"/>
     </row>
-    <row r="30" spans="1:8">
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A30" s="8"/>
       <c r="B30" s="2"/>
+      <c r="E30" s="3"/>
+      <c r="F30" s="4"/>
       <c r="G30" s="2"/>
       <c r="H30" s="2"/>
     </row>
-    <row r="31" spans="1:8">
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A31" s="8"/>
       <c r="B31" s="2"/>
+      <c r="E31" s="3"/>
+      <c r="F31" s="4"/>
       <c r="G31" s="2"/>
       <c r="H31" s="2"/>
     </row>
-    <row r="32" spans="1:8">
+    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A32" s="8"/>
       <c r="B32" s="2"/>
+      <c r="E32" s="3"/>
+      <c r="F32" s="4"/>
       <c r="G32" s="2"/>
       <c r="H32" s="2"/>
     </row>
-    <row r="33" spans="1:8">
+    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A33" s="8"/>
       <c r="B33" s="2"/>
+      <c r="E33" s="3"/>
+      <c r="F33" s="4"/>
       <c r="G33" s="2"/>
       <c r="H33" s="2"/>
     </row>
-    <row r="34" spans="1:8">
+    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A34" s="8"/>
       <c r="B34" s="2"/>
+      <c r="E34" s="3"/>
+      <c r="F34" s="4"/>
       <c r="G34" s="2"/>
       <c r="H34" s="2"/>
     </row>
-    <row r="35" spans="1:8">
+    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A35" s="8"/>
       <c r="B35" s="2"/>
+      <c r="E35" s="3"/>
+      <c r="F35" s="4"/>
       <c r="G35" s="2"/>
       <c r="H35" s="2"/>
     </row>
-    <row r="36" spans="1:8">
+    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A36" s="8"/>
       <c r="B36" s="2"/>
+      <c r="E36" s="3"/>
+      <c r="F36" s="4"/>
       <c r="G36" s="2"/>
       <c r="H36" s="2"/>
     </row>
-    <row r="37" spans="1:8">
+    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A37" s="8"/>
       <c r="B37" s="2"/>
+      <c r="E37" s="3"/>
+      <c r="F37" s="4"/>
       <c r="G37" s="2"/>
       <c r="H37" s="2"/>
     </row>
-    <row r="38" spans="1:8">
+    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A38" s="8"/>
       <c r="B38" s="2"/>
+      <c r="E38" s="3"/>
+      <c r="F38" s="4"/>
       <c r="G38" s="2"/>
       <c r="H38" s="2"/>
     </row>
-    <row r="39" spans="1:8">
+    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A39" s="8"/>
       <c r="B39" s="2"/>
+      <c r="E39" s="3"/>
+      <c r="F39" s="4"/>
       <c r="G39" s="2"/>
       <c r="H39" s="2"/>
     </row>
-    <row r="40" spans="1:8">
+    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A40" s="8"/>
       <c r="B40" s="2"/>
+      <c r="E40" s="3"/>
+      <c r="F40" s="4"/>
       <c r="G40" s="2"/>
       <c r="H40" s="2"/>
     </row>
-    <row r="41" spans="1:8">
+    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A41" s="8"/>
       <c r="B41" s="2"/>
+      <c r="E41" s="3"/>
+      <c r="F41" s="4"/>
       <c r="G41" s="2"/>
       <c r="H41" s="2"/>
     </row>
-    <row r="42" spans="1:8">
+    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A42" s="8"/>
       <c r="B42" s="2"/>
+      <c r="E42" s="3"/>
+      <c r="F42" s="4"/>
       <c r="G42" s="2"/>
       <c r="H42" s="2"/>
     </row>
-    <row r="43" spans="1:8">
+    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A43" s="8"/>
       <c r="B43" s="2"/>
+      <c r="E43" s="3"/>
+      <c r="F43" s="4"/>
       <c r="G43" s="2"/>
       <c r="H43" s="2"/>
     </row>
-    <row r="44" spans="1:8">
+    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A44" s="8"/>
       <c r="B44" s="2"/>
+      <c r="E44" s="3"/>
+      <c r="F44" s="4"/>
       <c r="G44" s="2"/>
       <c r="H44" s="2"/>
     </row>
-    <row r="45" spans="1:8">
+    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A45" s="8"/>
       <c r="B45" s="2"/>
+      <c r="E45" s="3"/>
+      <c r="F45" s="4"/>
       <c r="G45" s="2"/>
       <c r="H45" s="2"/>
     </row>
-    <row r="46" spans="1:8">
+    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A46" s="8"/>
       <c r="B46" s="2"/>
+      <c r="E46" s="3"/>
+      <c r="F46" s="4"/>
       <c r="G46" s="2"/>
       <c r="H46" s="2"/>
     </row>
-    <row r="47" spans="1:8">
+    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A47" s="8"/>
       <c r="B47" s="2"/>
+      <c r="E47" s="3"/>
+      <c r="F47" s="4"/>
       <c r="G47" s="2"/>
       <c r="H47" s="2"/>
     </row>
-    <row r="48" spans="1:8">
+    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A48" s="8"/>
       <c r="B48" s="2"/>
+      <c r="E48" s="3"/>
+      <c r="F48" s="4"/>
       <c r="G48" s="2"/>
       <c r="H48" s="2"/>
     </row>
-    <row r="49" spans="1:8">
+    <row r="49" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A49" s="8"/>
       <c r="B49" s="2"/>
+      <c r="E49" s="3"/>
+      <c r="F49" s="4"/>
       <c r="G49" s="2"/>
       <c r="H49" s="2"/>
     </row>
-    <row r="50" spans="1:8">
+    <row r="50" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A50" s="8"/>
       <c r="B50" s="2"/>
+      <c r="E50" s="3"/>
+      <c r="F50" s="4"/>
       <c r="G50" s="2"/>
       <c r="H50" s="2"/>
     </row>
-    <row r="51" spans="1:8">
+    <row r="51" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A51" s="8"/>
       <c r="B51" s="2"/>
+      <c r="E51" s="3"/>
+      <c r="F51" s="4"/>
       <c r="G51" s="2"/>
       <c r="H51" s="2"/>
     </row>
-    <row r="52" spans="1:8">
+    <row r="52" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A52" s="8"/>
       <c r="B52" s="2"/>
+      <c r="E52" s="3"/>
+      <c r="F52" s="4"/>
       <c r="G52" s="2"/>
       <c r="H52" s="2"/>
     </row>
-    <row r="53" spans="1:8">
+    <row r="53" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A53" s="8"/>
       <c r="B53" s="2"/>
+      <c r="E53" s="3"/>
+      <c r="F53" s="4"/>
       <c r="G53" s="2"/>
       <c r="H53" s="2"/>
     </row>
-    <row r="54" spans="1:8">
+    <row r="54" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A54" s="8"/>
       <c r="B54" s="2"/>
+      <c r="E54" s="3"/>
+      <c r="F54" s="4"/>
       <c r="G54" s="2"/>
       <c r="H54" s="2"/>
     </row>
-    <row r="55" spans="1:8">
+    <row r="55" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A55" s="8"/>
       <c r="B55" s="2"/>
+      <c r="E55" s="3"/>
+      <c r="F55" s="4"/>
       <c r="G55" s="2"/>
       <c r="H55" s="2"/>
     </row>
-    <row r="56" spans="1:8">
+    <row r="56" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A56" s="8"/>
       <c r="B56" s="2"/>
+      <c r="E56" s="3"/>
+      <c r="F56" s="4"/>
       <c r="G56" s="2"/>
       <c r="H56" s="2"/>
     </row>
-    <row r="57" spans="1:8">
+    <row r="57" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A57" s="8"/>
       <c r="B57" s="2"/>
+      <c r="E57" s="3"/>
+      <c r="F57" s="4"/>
       <c r="G57" s="2"/>
       <c r="H57" s="2"/>
     </row>
-    <row r="58" spans="1:8">
+    <row r="58" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A58" s="8"/>
       <c r="B58" s="2"/>
+      <c r="E58" s="3"/>
+      <c r="F58" s="4"/>
       <c r="G58" s="2"/>
       <c r="H58" s="2"/>
     </row>
-    <row r="59" spans="1:8">
+    <row r="59" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A59" s="8"/>
       <c r="B59" s="2"/>
+      <c r="E59" s="3"/>
+      <c r="F59" s="4"/>
       <c r="G59" s="2"/>
       <c r="H59" s="2"/>
     </row>
-    <row r="60" spans="1:8">
+    <row r="60" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A60" s="8"/>
       <c r="B60" s="2"/>
+      <c r="E60" s="3"/>
+      <c r="F60" s="4"/>
       <c r="G60" s="2"/>
       <c r="H60" s="2"/>
     </row>
-    <row r="61" spans="1:8">
+    <row r="61" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A61" s="8"/>
       <c r="B61" s="2"/>
+      <c r="E61" s="3"/>
+      <c r="F61" s="4"/>
       <c r="G61" s="2"/>
       <c r="H61" s="2"/>
     </row>
-    <row r="62" spans="1:8">
+    <row r="62" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A62" s="8"/>
       <c r="B62" s="2"/>
+      <c r="E62" s="3"/>
+      <c r="F62" s="4"/>
       <c r="G62" s="2"/>
       <c r="H62" s="2"/>
     </row>
-    <row r="63" spans="1:8">
+    <row r="63" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A63" s="8"/>
       <c r="B63" s="2"/>
+      <c r="E63" s="3"/>
+      <c r="F63" s="4"/>
       <c r="G63" s="2"/>
       <c r="H63" s="2"/>
     </row>
-    <row r="64" spans="1:8">
+    <row r="64" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A64" s="8"/>
       <c r="B64" s="2"/>
+      <c r="E64" s="3"/>
+      <c r="F64" s="4"/>
       <c r="G64" s="2"/>
       <c r="H64" s="2"/>
     </row>
-    <row r="65" spans="1:8">
+    <row r="65" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A65" s="8"/>
       <c r="B65" s="2"/>
+      <c r="E65" s="3"/>
+      <c r="F65" s="4"/>
       <c r="G65" s="2"/>
       <c r="H65" s="2"/>
     </row>
-    <row r="66" spans="1:8">
+    <row r="66" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A66" s="8"/>
       <c r="B66" s="2"/>
+      <c r="E66" s="3"/>
+      <c r="F66" s="4"/>
       <c r="G66" s="2"/>
       <c r="H66" s="2"/>
     </row>
-    <row r="67" spans="1:8">
+    <row r="67" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A67" s="8"/>
       <c r="B67" s="2"/>
+      <c r="E67" s="3"/>
+      <c r="F67" s="4"/>
       <c r="G67" s="2"/>
       <c r="H67" s="2"/>
     </row>
-    <row r="68" spans="1:8">
+    <row r="68" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A68" s="8"/>
       <c r="B68" s="2"/>
+      <c r="E68" s="3"/>
+      <c r="F68" s="4"/>
       <c r="G68" s="2"/>
       <c r="H68" s="2"/>
     </row>
-    <row r="69" spans="1:8">
+    <row r="69" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A69" s="8"/>
       <c r="B69" s="2"/>
+      <c r="E69" s="3"/>
+      <c r="F69" s="4"/>
       <c r="G69" s="2"/>
       <c r="H69" s="2"/>
     </row>
-    <row r="70" spans="1:8">
+    <row r="70" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A70" s="8"/>
       <c r="B70" s="2"/>
+      <c r="E70" s="3"/>
+      <c r="F70" s="4"/>
       <c r="G70" s="2"/>
       <c r="H70" s="2"/>
     </row>
-    <row r="71" spans="1:8">
+    <row r="71" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A71" s="8"/>
       <c r="B71" s="2"/>
+      <c r="E71" s="3"/>
+      <c r="F71" s="4"/>
       <c r="G71" s="2"/>
       <c r="H71" s="2"/>
     </row>
-    <row r="72" spans="1:8">
+    <row r="72" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A72" s="8"/>
       <c r="B72" s="2"/>
+      <c r="E72" s="3"/>
+      <c r="F72" s="4"/>
       <c r="G72" s="2"/>
       <c r="H72" s="2"/>
     </row>
-    <row r="73" spans="1:8">
+    <row r="73" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A73" s="8"/>
       <c r="B73" s="2"/>
+      <c r="E73" s="3"/>
+      <c r="F73" s="4"/>
       <c r="G73" s="2"/>
       <c r="H73" s="2"/>
     </row>
-    <row r="74" spans="1:8">
+    <row r="74" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A74" s="8"/>
       <c r="B74" s="2"/>
+      <c r="E74" s="3"/>
+      <c r="F74" s="4"/>
       <c r="G74" s="2"/>
       <c r="H74" s="2"/>
     </row>
-    <row r="75" spans="1:8">
+    <row r="75" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A75" s="8"/>
       <c r="B75" s="2"/>
+      <c r="E75" s="3"/>
+      <c r="F75" s="4"/>
       <c r="G75" s="2"/>
       <c r="H75" s="2"/>
     </row>
-    <row r="76" spans="1:8">
+    <row r="76" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A76" s="8"/>
       <c r="B76" s="2"/>
+      <c r="E76" s="3"/>
+      <c r="F76" s="4"/>
       <c r="G76" s="2"/>
       <c r="H76" s="2"/>
     </row>
-    <row r="77" spans="1:8">
+    <row r="77" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A77" s="8"/>
       <c r="B77" s="2"/>
+      <c r="E77" s="3"/>
+      <c r="F77" s="4"/>
       <c r="G77" s="2"/>
       <c r="H77" s="2"/>
     </row>
-    <row r="78" spans="1:8">
+    <row r="78" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A78" s="8"/>
       <c r="B78" s="2"/>
+      <c r="E78" s="3"/>
+      <c r="F78" s="4"/>
       <c r="G78" s="2"/>
       <c r="H78" s="2"/>
     </row>
-    <row r="79" spans="1:8">
+    <row r="79" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A79" s="8"/>
       <c r="B79" s="2"/>
+      <c r="E79" s="3"/>
+      <c r="F79" s="4"/>
       <c r="G79" s="2"/>
       <c r="H79" s="2"/>
     </row>
-    <row r="80" spans="1:8">
+    <row r="80" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A80" s="8"/>
       <c r="B80" s="2"/>
+      <c r="E80" s="3"/>
+      <c r="F80" s="4"/>
       <c r="G80" s="2"/>
       <c r="H80" s="2"/>
     </row>
-    <row r="81" spans="1:8">
+    <row r="81" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A81" s="8"/>
       <c r="B81" s="2"/>
+      <c r="E81" s="3"/>
+      <c r="F81" s="4"/>
       <c r="G81" s="2"/>
       <c r="H81" s="2"/>
     </row>
-    <row r="82" spans="1:8">
+    <row r="82" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A82" s="8"/>
       <c r="B82" s="2"/>
+      <c r="E82" s="3"/>
+      <c r="F82" s="4"/>
       <c r="G82" s="2"/>
       <c r="H82" s="2"/>
     </row>
-    <row r="83" spans="1:8">
+    <row r="83" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A83" s="8"/>
       <c r="B83" s="2"/>
+      <c r="E83" s="3"/>
+      <c r="F83" s="4"/>
       <c r="G83" s="2"/>
       <c r="H83" s="2"/>
     </row>
-    <row r="84" spans="1:8">
+    <row r="84" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A84" s="8"/>
       <c r="B84" s="2"/>
+      <c r="E84" s="3"/>
+      <c r="F84" s="4"/>
       <c r="G84" s="2"/>
       <c r="H84" s="2"/>
     </row>
-    <row r="85" spans="1:8">
+    <row r="85" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A85" s="8"/>
       <c r="B85" s="2"/>
+      <c r="E85" s="3"/>
+      <c r="F85" s="4"/>
       <c r="G85" s="2"/>
       <c r="H85" s="2"/>
     </row>
-    <row r="86" spans="1:8">
+    <row r="86" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A86" s="8"/>
       <c r="B86" s="2"/>
+      <c r="E86" s="3"/>
+      <c r="F86" s="4"/>
       <c r="G86" s="2"/>
       <c r="H86" s="2"/>
     </row>
-    <row r="87" spans="1:8">
+    <row r="87" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A87" s="8"/>
       <c r="B87" s="2"/>
+      <c r="E87" s="3"/>
+      <c r="F87" s="4"/>
       <c r="G87" s="2"/>
       <c r="H87" s="2"/>
     </row>
-    <row r="88" spans="1:8">
+    <row r="88" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A88" s="8"/>
       <c r="B88" s="2"/>
+      <c r="E88" s="3"/>
+      <c r="F88" s="4"/>
       <c r="G88" s="2"/>
       <c r="H88" s="2"/>
     </row>
-    <row r="89" spans="1:8">
+    <row r="89" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A89" s="8"/>
       <c r="B89" s="2"/>
+      <c r="E89" s="3"/>
+      <c r="F89" s="4"/>
       <c r="G89" s="2"/>
       <c r="H89" s="2"/>
     </row>
-    <row r="90" spans="1:8">
+    <row r="90" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A90" s="8"/>
       <c r="B90" s="2"/>
+      <c r="E90" s="3"/>
+      <c r="F90" s="4"/>
       <c r="G90" s="2"/>
       <c r="H90" s="2"/>
     </row>
-    <row r="91" spans="1:8">
+    <row r="91" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A91" s="8"/>
       <c r="B91" s="2"/>
+      <c r="E91" s="3"/>
+      <c r="F91" s="4"/>
       <c r="G91" s="2"/>
       <c r="H91" s="2"/>
     </row>
-    <row r="92" spans="1:8">
+    <row r="92" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A92" s="8"/>
       <c r="B92" s="2"/>
+      <c r="E92" s="3"/>
+      <c r="F92" s="4"/>
       <c r="G92" s="2"/>
       <c r="H92" s="2"/>
     </row>
-    <row r="93" spans="1:8">
+    <row r="93" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A93" s="8"/>
       <c r="B93" s="2"/>
+      <c r="E93" s="3"/>
+      <c r="F93" s="4"/>
       <c r="G93" s="2"/>
       <c r="H93" s="2"/>
     </row>
-    <row r="94" spans="1:8">
+    <row r="94" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A94" s="8"/>
       <c r="B94" s="2"/>
+      <c r="E94" s="3"/>
+      <c r="F94" s="4"/>
       <c r="G94" s="2"/>
       <c r="H94" s="2"/>
     </row>
-    <row r="95" spans="1:8">
+    <row r="95" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A95" s="8"/>
       <c r="B95" s="2"/>
+      <c r="E95" s="3"/>
+      <c r="F95" s="4"/>
       <c r="G95" s="2"/>
       <c r="H95" s="2"/>
     </row>
-    <row r="96" spans="1:8">
+    <row r="96" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A96" s="8"/>
       <c r="B96" s="2"/>
+      <c r="E96" s="3"/>
+      <c r="F96" s="4"/>
       <c r="G96" s="2"/>
       <c r="H96" s="2"/>
     </row>
-    <row r="97" spans="1:8">
+    <row r="97" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A97" s="8"/>
       <c r="B97" s="2"/>
+      <c r="E97" s="3"/>
+      <c r="F97" s="4"/>
       <c r="G97" s="2"/>
       <c r="H97" s="2"/>
     </row>
-    <row r="98" spans="1:8">
+    <row r="98" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A98" s="8"/>
       <c r="B98" s="2"/>
+      <c r="E98" s="3"/>
+      <c r="F98" s="4"/>
       <c r="G98" s="2"/>
       <c r="H98" s="2"/>
     </row>
-    <row r="99" spans="1:8">
+    <row r="99" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A99" s="8"/>
       <c r="B99" s="2"/>
+      <c r="E99" s="3"/>
+      <c r="F99" s="4"/>
       <c r="G99" s="2"/>
       <c r="H99" s="2"/>
     </row>
-    <row r="100" spans="1:8">
+    <row r="100" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A100" s="8"/>
       <c r="B100" s="2"/>
+      <c r="E100" s="3"/>
+      <c r="F100" s="4"/>
       <c r="G100" s="2"/>
       <c r="H100" s="2"/>
     </row>
@@ -1939,7 +2043,7 @@
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <ignoredErrors>
-    <ignoredError sqref="D6:D100" listDataValidation="1"/>
+    <ignoredError sqref="D3:D100" listDataValidation="1"/>
   </ignoredErrors>
   <tableParts count="1">
     <tablePart r:id="rId1"/>
@@ -1955,19 +2059,19 @@
       <selection activeCell="D2" sqref="D2:D100"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="7.69921875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="17.296875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.59765625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="7.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.5703125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="9" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.8984375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="23.59765625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="13.3984375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="19.09765625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="23.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="19.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="15.75">
+    <row r="1" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
@@ -1993,7 +2097,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="15">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="1"/>
       <c r="B2" s="2"/>
       <c r="E2" s="3"/>
@@ -2001,7 +2105,7 @@
       <c r="G2" s="2"/>
       <c r="H2" s="2"/>
     </row>
-    <row r="3" spans="1:8" ht="15">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="1"/>
       <c r="B3" s="2"/>
       <c r="E3" s="3"/>
@@ -2009,7 +2113,7 @@
       <c r="G3" s="2"/>
       <c r="H3" s="2"/>
     </row>
-    <row r="4" spans="1:8" ht="15">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="1"/>
       <c r="B4" s="2"/>
       <c r="E4" s="3"/>
@@ -2017,7 +2121,7 @@
       <c r="G4" s="2"/>
       <c r="H4" s="2"/>
     </row>
-    <row r="5" spans="1:8" ht="15">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="1"/>
       <c r="B5" s="2"/>
       <c r="E5" s="3"/>
@@ -2025,7 +2129,7 @@
       <c r="G5" s="2"/>
       <c r="H5" s="2"/>
     </row>
-    <row r="6" spans="1:8" ht="15">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="1"/>
       <c r="B6" s="2"/>
       <c r="E6" s="3"/>
@@ -2033,7 +2137,7 @@
       <c r="G6" s="2"/>
       <c r="H6" s="2"/>
     </row>
-    <row r="7" spans="1:8" ht="15">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="1"/>
       <c r="B7" s="2"/>
       <c r="E7" s="3"/>
@@ -2041,7 +2145,7 @@
       <c r="G7" s="2"/>
       <c r="H7" s="2"/>
     </row>
-    <row r="8" spans="1:8" ht="15">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="1"/>
       <c r="B8" s="2"/>
       <c r="E8" s="3"/>
@@ -2049,7 +2153,7 @@
       <c r="G8" s="2"/>
       <c r="H8" s="2"/>
     </row>
-    <row r="9" spans="1:8" ht="15">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="1"/>
       <c r="B9" s="2"/>
       <c r="E9" s="3"/>
@@ -2057,7 +2161,7 @@
       <c r="G9" s="2"/>
       <c r="H9" s="2"/>
     </row>
-    <row r="10" spans="1:8" ht="15">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="1"/>
       <c r="B10" s="2"/>
       <c r="E10" s="3"/>
@@ -2065,7 +2169,7 @@
       <c r="G10" s="2"/>
       <c r="H10" s="2"/>
     </row>
-    <row r="11" spans="1:8" ht="15">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="1"/>
       <c r="B11" s="2"/>
       <c r="E11" s="3"/>
@@ -2073,7 +2177,7 @@
       <c r="G11" s="2"/>
       <c r="H11" s="2"/>
     </row>
-    <row r="12" spans="1:8" ht="15">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="1"/>
       <c r="B12" s="2"/>
       <c r="E12" s="3"/>
@@ -2081,7 +2185,7 @@
       <c r="G12" s="2"/>
       <c r="H12" s="2"/>
     </row>
-    <row r="13" spans="1:8" ht="15">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="1"/>
       <c r="B13" s="2"/>
       <c r="E13" s="3"/>
@@ -2089,7 +2193,7 @@
       <c r="G13" s="2"/>
       <c r="H13" s="2"/>
     </row>
-    <row r="14" spans="1:8" ht="15">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" s="1"/>
       <c r="B14" s="2"/>
       <c r="E14" s="3"/>
@@ -2097,7 +2201,7 @@
       <c r="G14" s="2"/>
       <c r="H14" s="2"/>
     </row>
-    <row r="15" spans="1:8" ht="15">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" s="1"/>
       <c r="B15" s="2"/>
       <c r="E15" s="3"/>
@@ -2105,7 +2209,7 @@
       <c r="G15" s="2"/>
       <c r="H15" s="2"/>
     </row>
-    <row r="16" spans="1:8" ht="15">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" s="1"/>
       <c r="B16" s="2"/>
       <c r="E16" s="3"/>
@@ -2113,7 +2217,7 @@
       <c r="G16" s="2"/>
       <c r="H16" s="2"/>
     </row>
-    <row r="17" spans="1:8" ht="15">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" s="1"/>
       <c r="B17" s="2"/>
       <c r="E17" s="3"/>
@@ -2121,7 +2225,7 @@
       <c r="G17" s="2"/>
       <c r="H17" s="2"/>
     </row>
-    <row r="18" spans="1:8" ht="15">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" s="1"/>
       <c r="B18" s="2"/>
       <c r="E18" s="3"/>
@@ -2129,7 +2233,7 @@
       <c r="G18" s="2"/>
       <c r="H18" s="2"/>
     </row>
-    <row r="19" spans="1:8" ht="15">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" s="1"/>
       <c r="B19" s="2"/>
       <c r="E19" s="3"/>
@@ -2137,7 +2241,7 @@
       <c r="G19" s="2"/>
       <c r="H19" s="2"/>
     </row>
-    <row r="20" spans="1:8" ht="15">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" s="1"/>
       <c r="B20" s="2"/>
       <c r="E20" s="3"/>
@@ -2145,7 +2249,7 @@
       <c r="G20" s="2"/>
       <c r="H20" s="2"/>
     </row>
-    <row r="21" spans="1:8" ht="15">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" s="1"/>
       <c r="B21" s="2"/>
       <c r="E21" s="3"/>
@@ -2153,7 +2257,7 @@
       <c r="G21" s="2"/>
       <c r="H21" s="2"/>
     </row>
-    <row r="22" spans="1:8" ht="15">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" s="1"/>
       <c r="B22" s="2"/>
       <c r="E22" s="3"/>
@@ -2161,7 +2265,7 @@
       <c r="G22" s="2"/>
       <c r="H22" s="2"/>
     </row>
-    <row r="23" spans="1:8" ht="15">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" s="1"/>
       <c r="B23" s="2"/>
       <c r="E23" s="3"/>
@@ -2169,7 +2273,7 @@
       <c r="G23" s="2"/>
       <c r="H23" s="2"/>
     </row>
-    <row r="24" spans="1:8" ht="15">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24" s="1"/>
       <c r="B24" s="2"/>
       <c r="E24" s="3"/>
@@ -2177,7 +2281,7 @@
       <c r="G24" s="2"/>
       <c r="H24" s="2"/>
     </row>
-    <row r="25" spans="1:8" ht="15">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25" s="1"/>
       <c r="B25" s="2"/>
       <c r="E25" s="3"/>
@@ -2185,7 +2289,7 @@
       <c r="G25" s="2"/>
       <c r="H25" s="2"/>
     </row>
-    <row r="26" spans="1:8" ht="15">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26" s="1"/>
       <c r="B26" s="2"/>
       <c r="E26" s="3"/>
@@ -2193,7 +2297,7 @@
       <c r="G26" s="2"/>
       <c r="H26" s="2"/>
     </row>
-    <row r="27" spans="1:8" ht="15">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A27" s="1"/>
       <c r="B27" s="2"/>
       <c r="E27" s="3"/>
@@ -2201,7 +2305,7 @@
       <c r="G27" s="2"/>
       <c r="H27" s="2"/>
     </row>
-    <row r="28" spans="1:8" ht="15">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A28" s="1"/>
       <c r="B28" s="2"/>
       <c r="E28" s="3"/>
@@ -2209,7 +2313,7 @@
       <c r="G28" s="2"/>
       <c r="H28" s="2"/>
     </row>
-    <row r="29" spans="1:8" ht="15">
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A29" s="1"/>
       <c r="B29" s="2"/>
       <c r="E29" s="3"/>
@@ -2217,7 +2321,7 @@
       <c r="G29" s="2"/>
       <c r="H29" s="2"/>
     </row>
-    <row r="30" spans="1:8" ht="15">
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A30" s="1"/>
       <c r="B30" s="2"/>
       <c r="E30" s="3"/>
@@ -2225,7 +2329,7 @@
       <c r="G30" s="2"/>
       <c r="H30" s="2"/>
     </row>
-    <row r="31" spans="1:8" ht="15">
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A31" s="1"/>
       <c r="B31" s="2"/>
       <c r="E31" s="3"/>
@@ -2233,7 +2337,7 @@
       <c r="G31" s="2"/>
       <c r="H31" s="2"/>
     </row>
-    <row r="32" spans="1:8" ht="15">
+    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A32" s="1"/>
       <c r="B32" s="2"/>
       <c r="E32" s="3"/>
@@ -2241,7 +2345,7 @@
       <c r="G32" s="2"/>
       <c r="H32" s="2"/>
     </row>
-    <row r="33" spans="1:8" ht="15">
+    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A33" s="1"/>
       <c r="B33" s="2"/>
       <c r="E33" s="3"/>
@@ -2249,7 +2353,7 @@
       <c r="G33" s="2"/>
       <c r="H33" s="2"/>
     </row>
-    <row r="34" spans="1:8" ht="15">
+    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A34" s="1"/>
       <c r="B34" s="2"/>
       <c r="E34" s="3"/>
@@ -2257,7 +2361,7 @@
       <c r="G34" s="2"/>
       <c r="H34" s="2"/>
     </row>
-    <row r="35" spans="1:8" ht="15">
+    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A35" s="1"/>
       <c r="B35" s="2"/>
       <c r="E35" s="3"/>
@@ -2265,7 +2369,7 @@
       <c r="G35" s="2"/>
       <c r="H35" s="2"/>
     </row>
-    <row r="36" spans="1:8" ht="15">
+    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A36" s="1"/>
       <c r="B36" s="2"/>
       <c r="E36" s="3"/>
@@ -2273,7 +2377,7 @@
       <c r="G36" s="2"/>
       <c r="H36" s="2"/>
     </row>
-    <row r="37" spans="1:8" ht="15">
+    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A37" s="1"/>
       <c r="B37" s="2"/>
       <c r="E37" s="3"/>
@@ -2281,7 +2385,7 @@
       <c r="G37" s="2"/>
       <c r="H37" s="2"/>
     </row>
-    <row r="38" spans="1:8" ht="15">
+    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A38" s="1"/>
       <c r="B38" s="2"/>
       <c r="E38" s="3"/>
@@ -2289,7 +2393,7 @@
       <c r="G38" s="2"/>
       <c r="H38" s="2"/>
     </row>
-    <row r="39" spans="1:8" ht="15">
+    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A39" s="1"/>
       <c r="B39" s="2"/>
       <c r="E39" s="3"/>
@@ -2297,7 +2401,7 @@
       <c r="G39" s="2"/>
       <c r="H39" s="2"/>
     </row>
-    <row r="40" spans="1:8" ht="15">
+    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A40" s="1"/>
       <c r="B40" s="2"/>
       <c r="E40" s="3"/>
@@ -2305,7 +2409,7 @@
       <c r="G40" s="2"/>
       <c r="H40" s="2"/>
     </row>
-    <row r="41" spans="1:8" ht="15">
+    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A41" s="1"/>
       <c r="B41" s="2"/>
       <c r="E41" s="3"/>
@@ -2313,7 +2417,7 @@
       <c r="G41" s="2"/>
       <c r="H41" s="2"/>
     </row>
-    <row r="42" spans="1:8" ht="15">
+    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A42" s="1"/>
       <c r="B42" s="2"/>
       <c r="E42" s="3"/>
@@ -2321,7 +2425,7 @@
       <c r="G42" s="2"/>
       <c r="H42" s="2"/>
     </row>
-    <row r="43" spans="1:8" ht="15">
+    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A43" s="1"/>
       <c r="B43" s="2"/>
       <c r="E43" s="3"/>
@@ -2329,7 +2433,7 @@
       <c r="G43" s="2"/>
       <c r="H43" s="2"/>
     </row>
-    <row r="44" spans="1:8" ht="15">
+    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A44" s="1"/>
       <c r="B44" s="2"/>
       <c r="E44" s="3"/>
@@ -2337,7 +2441,7 @@
       <c r="G44" s="2"/>
       <c r="H44" s="2"/>
     </row>
-    <row r="45" spans="1:8" ht="15">
+    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A45" s="1"/>
       <c r="B45" s="2"/>
       <c r="E45" s="3"/>
@@ -2345,7 +2449,7 @@
       <c r="G45" s="2"/>
       <c r="H45" s="2"/>
     </row>
-    <row r="46" spans="1:8" ht="15">
+    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A46" s="1"/>
       <c r="B46" s="2"/>
       <c r="E46" s="3"/>
@@ -2353,7 +2457,7 @@
       <c r="G46" s="2"/>
       <c r="H46" s="2"/>
     </row>
-    <row r="47" spans="1:8" ht="15">
+    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A47" s="1"/>
       <c r="B47" s="2"/>
       <c r="E47" s="3"/>
@@ -2361,7 +2465,7 @@
       <c r="G47" s="2"/>
       <c r="H47" s="2"/>
     </row>
-    <row r="48" spans="1:8" ht="15">
+    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A48" s="1"/>
       <c r="B48" s="2"/>
       <c r="E48" s="3"/>
@@ -2369,7 +2473,7 @@
       <c r="G48" s="2"/>
       <c r="H48" s="2"/>
     </row>
-    <row r="49" spans="1:8" ht="15">
+    <row r="49" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A49" s="1"/>
       <c r="B49" s="2"/>
       <c r="E49" s="3"/>
@@ -2377,7 +2481,7 @@
       <c r="G49" s="2"/>
       <c r="H49" s="2"/>
     </row>
-    <row r="50" spans="1:8" ht="15">
+    <row r="50" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A50" s="1"/>
       <c r="B50" s="2"/>
       <c r="E50" s="3"/>
@@ -2385,7 +2489,7 @@
       <c r="G50" s="2"/>
       <c r="H50" s="2"/>
     </row>
-    <row r="51" spans="1:8" ht="15">
+    <row r="51" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A51" s="1"/>
       <c r="B51" s="2"/>
       <c r="E51" s="3"/>
@@ -2393,7 +2497,7 @@
       <c r="G51" s="2"/>
       <c r="H51" s="2"/>
     </row>
-    <row r="52" spans="1:8" ht="15">
+    <row r="52" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A52" s="1"/>
       <c r="B52" s="2"/>
       <c r="E52" s="3"/>
@@ -2401,7 +2505,7 @@
       <c r="G52" s="2"/>
       <c r="H52" s="2"/>
     </row>
-    <row r="53" spans="1:8" ht="15">
+    <row r="53" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A53" s="1"/>
       <c r="B53" s="2"/>
       <c r="E53" s="3"/>
@@ -2409,7 +2513,7 @@
       <c r="G53" s="2"/>
       <c r="H53" s="2"/>
     </row>
-    <row r="54" spans="1:8" ht="15">
+    <row r="54" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A54" s="1"/>
       <c r="B54" s="2"/>
       <c r="E54" s="3"/>
@@ -2417,7 +2521,7 @@
       <c r="G54" s="2"/>
       <c r="H54" s="2"/>
     </row>
-    <row r="55" spans="1:8" ht="15">
+    <row r="55" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A55" s="1"/>
       <c r="B55" s="2"/>
       <c r="E55" s="3"/>
@@ -2425,7 +2529,7 @@
       <c r="G55" s="2"/>
       <c r="H55" s="2"/>
     </row>
-    <row r="56" spans="1:8" ht="15">
+    <row r="56" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A56" s="1"/>
       <c r="B56" s="2"/>
       <c r="E56" s="3"/>
@@ -2433,7 +2537,7 @@
       <c r="G56" s="2"/>
       <c r="H56" s="2"/>
     </row>
-    <row r="57" spans="1:8" ht="15">
+    <row r="57" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A57" s="1"/>
       <c r="B57" s="2"/>
       <c r="E57" s="3"/>
@@ -2441,7 +2545,7 @@
       <c r="G57" s="2"/>
       <c r="H57" s="2"/>
     </row>
-    <row r="58" spans="1:8" ht="15">
+    <row r="58" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A58" s="1"/>
       <c r="B58" s="2"/>
       <c r="E58" s="3"/>
@@ -2449,7 +2553,7 @@
       <c r="G58" s="2"/>
       <c r="H58" s="2"/>
     </row>
-    <row r="59" spans="1:8" ht="15">
+    <row r="59" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A59" s="1"/>
       <c r="B59" s="2"/>
       <c r="E59" s="3"/>
@@ -2457,7 +2561,7 @@
       <c r="G59" s="2"/>
       <c r="H59" s="2"/>
     </row>
-    <row r="60" spans="1:8" ht="15">
+    <row r="60" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A60" s="1"/>
       <c r="B60" s="2"/>
       <c r="E60" s="3"/>
@@ -2465,7 +2569,7 @@
       <c r="G60" s="2"/>
       <c r="H60" s="2"/>
     </row>
-    <row r="61" spans="1:8" ht="15">
+    <row r="61" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A61" s="1"/>
       <c r="B61" s="2"/>
       <c r="E61" s="3"/>
@@ -2473,7 +2577,7 @@
       <c r="G61" s="2"/>
       <c r="H61" s="2"/>
     </row>
-    <row r="62" spans="1:8" ht="15">
+    <row r="62" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A62" s="1"/>
       <c r="B62" s="2"/>
       <c r="E62" s="3"/>
@@ -2481,7 +2585,7 @@
       <c r="G62" s="2"/>
       <c r="H62" s="2"/>
     </row>
-    <row r="63" spans="1:8" ht="15">
+    <row r="63" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A63" s="1"/>
       <c r="B63" s="2"/>
       <c r="E63" s="3"/>
@@ -2489,7 +2593,7 @@
       <c r="G63" s="2"/>
       <c r="H63" s="2"/>
     </row>
-    <row r="64" spans="1:8" ht="15">
+    <row r="64" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A64" s="1"/>
       <c r="B64" s="2"/>
       <c r="E64" s="3"/>
@@ -2497,7 +2601,7 @@
       <c r="G64" s="2"/>
       <c r="H64" s="2"/>
     </row>
-    <row r="65" spans="1:8" ht="15">
+    <row r="65" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A65" s="1"/>
       <c r="B65" s="2"/>
       <c r="E65" s="3"/>
@@ -2505,7 +2609,7 @@
       <c r="G65" s="2"/>
       <c r="H65" s="2"/>
     </row>
-    <row r="66" spans="1:8" ht="15">
+    <row r="66" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A66" s="1"/>
       <c r="B66" s="2"/>
       <c r="E66" s="3"/>
@@ -2513,7 +2617,7 @@
       <c r="G66" s="2"/>
       <c r="H66" s="2"/>
     </row>
-    <row r="67" spans="1:8" ht="15">
+    <row r="67" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A67" s="1"/>
       <c r="B67" s="2"/>
       <c r="E67" s="3"/>
@@ -2521,7 +2625,7 @@
       <c r="G67" s="2"/>
       <c r="H67" s="2"/>
     </row>
-    <row r="68" spans="1:8" ht="15">
+    <row r="68" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A68" s="1"/>
       <c r="B68" s="2"/>
       <c r="E68" s="3"/>
@@ -2529,7 +2633,7 @@
       <c r="G68" s="2"/>
       <c r="H68" s="2"/>
     </row>
-    <row r="69" spans="1:8" ht="15">
+    <row r="69" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A69" s="1"/>
       <c r="B69" s="2"/>
       <c r="E69" s="3"/>
@@ -2537,7 +2641,7 @@
       <c r="G69" s="2"/>
       <c r="H69" s="2"/>
     </row>
-    <row r="70" spans="1:8" ht="15">
+    <row r="70" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A70" s="1"/>
       <c r="B70" s="2"/>
       <c r="E70" s="3"/>
@@ -2545,7 +2649,7 @@
       <c r="G70" s="2"/>
       <c r="H70" s="2"/>
     </row>
-    <row r="71" spans="1:8" ht="15">
+    <row r="71" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A71" s="1"/>
       <c r="B71" s="2"/>
       <c r="E71" s="3"/>
@@ -2553,7 +2657,7 @@
       <c r="G71" s="2"/>
       <c r="H71" s="2"/>
     </row>
-    <row r="72" spans="1:8" ht="15">
+    <row r="72" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A72" s="1"/>
       <c r="B72" s="2"/>
       <c r="E72" s="3"/>
@@ -2561,7 +2665,7 @@
       <c r="G72" s="2"/>
       <c r="H72" s="2"/>
     </row>
-    <row r="73" spans="1:8" ht="15">
+    <row r="73" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A73" s="1"/>
       <c r="B73" s="2"/>
       <c r="E73" s="3"/>
@@ -2569,7 +2673,7 @@
       <c r="G73" s="2"/>
       <c r="H73" s="2"/>
     </row>
-    <row r="74" spans="1:8" ht="15">
+    <row r="74" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A74" s="1"/>
       <c r="B74" s="2"/>
       <c r="E74" s="3"/>
@@ -2577,7 +2681,7 @@
       <c r="G74" s="2"/>
       <c r="H74" s="2"/>
     </row>
-    <row r="75" spans="1:8" ht="15">
+    <row r="75" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A75" s="1"/>
       <c r="B75" s="2"/>
       <c r="E75" s="3"/>
@@ -2585,7 +2689,7 @@
       <c r="G75" s="2"/>
       <c r="H75" s="2"/>
     </row>
-    <row r="76" spans="1:8" ht="15">
+    <row r="76" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A76" s="1"/>
       <c r="B76" s="2"/>
       <c r="E76" s="3"/>
@@ -2593,7 +2697,7 @@
       <c r="G76" s="2"/>
       <c r="H76" s="2"/>
     </row>
-    <row r="77" spans="1:8" ht="15">
+    <row r="77" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A77" s="1"/>
       <c r="B77" s="2"/>
       <c r="E77" s="3"/>
@@ -2601,7 +2705,7 @@
       <c r="G77" s="2"/>
       <c r="H77" s="2"/>
     </row>
-    <row r="78" spans="1:8" ht="15">
+    <row r="78" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A78" s="1"/>
       <c r="B78" s="2"/>
       <c r="E78" s="3"/>
@@ -2609,7 +2713,7 @@
       <c r="G78" s="2"/>
       <c r="H78" s="2"/>
     </row>
-    <row r="79" spans="1:8" ht="15">
+    <row r="79" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A79" s="1"/>
       <c r="B79" s="2"/>
       <c r="E79" s="3"/>
@@ -2617,7 +2721,7 @@
       <c r="G79" s="2"/>
       <c r="H79" s="2"/>
     </row>
-    <row r="80" spans="1:8" ht="15">
+    <row r="80" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A80" s="1"/>
       <c r="B80" s="2"/>
       <c r="E80" s="3"/>
@@ -2625,7 +2729,7 @@
       <c r="G80" s="2"/>
       <c r="H80" s="2"/>
     </row>
-    <row r="81" spans="1:8" ht="15">
+    <row r="81" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A81" s="1"/>
       <c r="B81" s="2"/>
       <c r="E81" s="3"/>
@@ -2633,7 +2737,7 @@
       <c r="G81" s="2"/>
       <c r="H81" s="2"/>
     </row>
-    <row r="82" spans="1:8" ht="15">
+    <row r="82" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A82" s="1"/>
       <c r="B82" s="2"/>
       <c r="E82" s="3"/>
@@ -2641,7 +2745,7 @@
       <c r="G82" s="2"/>
       <c r="H82" s="2"/>
     </row>
-    <row r="83" spans="1:8" ht="15">
+    <row r="83" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A83" s="1"/>
       <c r="B83" s="2"/>
       <c r="E83" s="3"/>
@@ -2649,7 +2753,7 @@
       <c r="G83" s="2"/>
       <c r="H83" s="2"/>
     </row>
-    <row r="84" spans="1:8" ht="15">
+    <row r="84" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A84" s="1"/>
       <c r="B84" s="2"/>
       <c r="E84" s="3"/>
@@ -2657,7 +2761,7 @@
       <c r="G84" s="2"/>
       <c r="H84" s="2"/>
     </row>
-    <row r="85" spans="1:8" ht="15">
+    <row r="85" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A85" s="1"/>
       <c r="B85" s="2"/>
       <c r="E85" s="3"/>
@@ -2665,7 +2769,7 @@
       <c r="G85" s="2"/>
       <c r="H85" s="2"/>
     </row>
-    <row r="86" spans="1:8" ht="15">
+    <row r="86" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A86" s="1"/>
       <c r="B86" s="2"/>
       <c r="E86" s="3"/>
@@ -2673,7 +2777,7 @@
       <c r="G86" s="2"/>
       <c r="H86" s="2"/>
     </row>
-    <row r="87" spans="1:8" ht="15">
+    <row r="87" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A87" s="1"/>
       <c r="B87" s="2"/>
       <c r="E87" s="3"/>
@@ -2681,7 +2785,7 @@
       <c r="G87" s="2"/>
       <c r="H87" s="2"/>
     </row>
-    <row r="88" spans="1:8">
+    <row r="88" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A88" s="1"/>
       <c r="B88" s="2"/>
       <c r="E88" s="3"/>
@@ -2689,7 +2793,7 @@
       <c r="G88" s="2"/>
       <c r="H88" s="2"/>
     </row>
-    <row r="89" spans="1:8">
+    <row r="89" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A89" s="1"/>
       <c r="B89" s="2"/>
       <c r="E89" s="3"/>
@@ -2697,7 +2801,7 @@
       <c r="G89" s="2"/>
       <c r="H89" s="2"/>
     </row>
-    <row r="90" spans="1:8">
+    <row r="90" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A90" s="1"/>
       <c r="B90" s="2"/>
       <c r="E90" s="3"/>
@@ -2705,7 +2809,7 @@
       <c r="G90" s="2"/>
       <c r="H90" s="2"/>
     </row>
-    <row r="91" spans="1:8">
+    <row r="91" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A91" s="1"/>
       <c r="B91" s="2"/>
       <c r="E91" s="3"/>
@@ -2713,7 +2817,7 @@
       <c r="G91" s="2"/>
       <c r="H91" s="2"/>
     </row>
-    <row r="92" spans="1:8">
+    <row r="92" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A92" s="1"/>
       <c r="B92" s="2"/>
       <c r="E92" s="3"/>
@@ -2721,7 +2825,7 @@
       <c r="G92" s="2"/>
       <c r="H92" s="2"/>
     </row>
-    <row r="93" spans="1:8">
+    <row r="93" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A93" s="1"/>
       <c r="B93" s="2"/>
       <c r="E93" s="3"/>
@@ -2729,7 +2833,7 @@
       <c r="G93" s="2"/>
       <c r="H93" s="2"/>
     </row>
-    <row r="94" spans="1:8">
+    <row r="94" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A94" s="1"/>
       <c r="B94" s="2"/>
       <c r="E94" s="3"/>
@@ -2737,7 +2841,7 @@
       <c r="G94" s="2"/>
       <c r="H94" s="2"/>
     </row>
-    <row r="95" spans="1:8">
+    <row r="95" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A95" s="1"/>
       <c r="B95" s="2"/>
       <c r="E95" s="3"/>
@@ -2745,7 +2849,7 @@
       <c r="G95" s="2"/>
       <c r="H95" s="2"/>
     </row>
-    <row r="96" spans="1:8">
+    <row r="96" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A96" s="1"/>
       <c r="B96" s="2"/>
       <c r="E96" s="3"/>
@@ -2753,7 +2857,7 @@
       <c r="G96" s="2"/>
       <c r="H96" s="2"/>
     </row>
-    <row r="97" spans="1:8">
+    <row r="97" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A97" s="1"/>
       <c r="B97" s="2"/>
       <c r="E97" s="3"/>
@@ -2761,7 +2865,7 @@
       <c r="G97" s="2"/>
       <c r="H97" s="2"/>
     </row>
-    <row r="98" spans="1:8">
+    <row r="98" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A98" s="1"/>
       <c r="B98" s="2"/>
       <c r="E98" s="3"/>
@@ -2769,7 +2873,7 @@
       <c r="G98" s="2"/>
       <c r="H98" s="2"/>
     </row>
-    <row r="99" spans="1:8">
+    <row r="99" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A99" s="1"/>
       <c r="B99" s="2"/>
       <c r="E99" s="3"/>
@@ -2777,7 +2881,7 @@
       <c r="G99" s="2"/>
       <c r="H99" s="2"/>
     </row>
-    <row r="100" spans="1:8">
+    <row r="100" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A100" s="1"/>
       <c r="B100" s="2"/>
       <c r="E100" s="3"/>
@@ -2820,19 +2924,19 @@
       <selection activeCell="D2" sqref="D2:D100"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="7.69921875" customWidth="1"/>
-    <col min="2" max="2" width="17.296875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.59765625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="7.7109375" customWidth="1"/>
+    <col min="2" max="2" width="17.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.5703125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="9" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.8984375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="23.59765625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="13.3984375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="19.09765625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="23.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="19.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="15.75">
+    <row r="1" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
@@ -2858,7 +2962,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="15">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="1"/>
       <c r="B2" s="2"/>
       <c r="E2" s="3"/>
@@ -2866,7 +2970,7 @@
       <c r="G2" s="2"/>
       <c r="H2" s="2"/>
     </row>
-    <row r="3" spans="1:8" ht="15">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="1"/>
       <c r="B3" s="2"/>
       <c r="E3" s="3"/>
@@ -2874,7 +2978,7 @@
       <c r="G3" s="2"/>
       <c r="H3" s="2"/>
     </row>
-    <row r="4" spans="1:8" ht="15">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="1"/>
       <c r="B4" s="2"/>
       <c r="E4" s="3"/>
@@ -2882,7 +2986,7 @@
       <c r="G4" s="2"/>
       <c r="H4" s="2"/>
     </row>
-    <row r="5" spans="1:8" ht="15">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="1"/>
       <c r="B5" s="2"/>
       <c r="E5" s="3"/>
@@ -2890,7 +2994,7 @@
       <c r="G5" s="2"/>
       <c r="H5" s="2"/>
     </row>
-    <row r="6" spans="1:8" ht="15">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="1"/>
       <c r="B6" s="2"/>
       <c r="E6" s="3"/>
@@ -2898,7 +3002,7 @@
       <c r="G6" s="2"/>
       <c r="H6" s="2"/>
     </row>
-    <row r="7" spans="1:8" ht="15">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="1"/>
       <c r="B7" s="2"/>
       <c r="E7" s="3"/>
@@ -2906,7 +3010,7 @@
       <c r="G7" s="2"/>
       <c r="H7" s="2"/>
     </row>
-    <row r="8" spans="1:8" ht="15">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="1"/>
       <c r="B8" s="2"/>
       <c r="E8" s="3"/>
@@ -2914,7 +3018,7 @@
       <c r="G8" s="2"/>
       <c r="H8" s="2"/>
     </row>
-    <row r="9" spans="1:8" ht="15">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="1"/>
       <c r="B9" s="2"/>
       <c r="E9" s="3"/>
@@ -2922,7 +3026,7 @@
       <c r="G9" s="2"/>
       <c r="H9" s="2"/>
     </row>
-    <row r="10" spans="1:8" ht="15">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="1"/>
       <c r="B10" s="2"/>
       <c r="E10" s="3"/>
@@ -2930,7 +3034,7 @@
       <c r="G10" s="2"/>
       <c r="H10" s="2"/>
     </row>
-    <row r="11" spans="1:8" ht="15">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="1"/>
       <c r="B11" s="2"/>
       <c r="E11" s="3"/>
@@ -2938,7 +3042,7 @@
       <c r="G11" s="2"/>
       <c r="H11" s="2"/>
     </row>
-    <row r="12" spans="1:8" ht="15">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="1"/>
       <c r="B12" s="2"/>
       <c r="E12" s="3"/>
@@ -2946,7 +3050,7 @@
       <c r="G12" s="2"/>
       <c r="H12" s="2"/>
     </row>
-    <row r="13" spans="1:8" ht="15">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="1"/>
       <c r="B13" s="2"/>
       <c r="E13" s="3"/>
@@ -2954,7 +3058,7 @@
       <c r="G13" s="2"/>
       <c r="H13" s="2"/>
     </row>
-    <row r="14" spans="1:8" ht="15">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" s="1"/>
       <c r="B14" s="2"/>
       <c r="E14" s="3"/>
@@ -2962,7 +3066,7 @@
       <c r="G14" s="2"/>
       <c r="H14" s="2"/>
     </row>
-    <row r="15" spans="1:8" ht="15">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" s="1"/>
       <c r="B15" s="2"/>
       <c r="E15" s="3"/>
@@ -2970,7 +3074,7 @@
       <c r="G15" s="2"/>
       <c r="H15" s="2"/>
     </row>
-    <row r="16" spans="1:8" ht="15">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" s="1"/>
       <c r="B16" s="2"/>
       <c r="E16" s="3"/>
@@ -2978,7 +3082,7 @@
       <c r="G16" s="2"/>
       <c r="H16" s="2"/>
     </row>
-    <row r="17" spans="1:8" ht="15">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" s="1"/>
       <c r="B17" s="2"/>
       <c r="E17" s="3"/>
@@ -2986,7 +3090,7 @@
       <c r="G17" s="2"/>
       <c r="H17" s="2"/>
     </row>
-    <row r="18" spans="1:8" ht="15">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" s="1"/>
       <c r="B18" s="2"/>
       <c r="E18" s="3"/>
@@ -2994,7 +3098,7 @@
       <c r="G18" s="2"/>
       <c r="H18" s="2"/>
     </row>
-    <row r="19" spans="1:8" ht="15">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" s="1"/>
       <c r="B19" s="2"/>
       <c r="E19" s="3"/>
@@ -3002,7 +3106,7 @@
       <c r="G19" s="2"/>
       <c r="H19" s="2"/>
     </row>
-    <row r="20" spans="1:8" ht="15">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" s="1"/>
       <c r="B20" s="2"/>
       <c r="E20" s="3"/>
@@ -3010,7 +3114,7 @@
       <c r="G20" s="2"/>
       <c r="H20" s="2"/>
     </row>
-    <row r="21" spans="1:8" ht="15">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" s="1"/>
       <c r="B21" s="2"/>
       <c r="E21" s="3"/>
@@ -3018,7 +3122,7 @@
       <c r="G21" s="2"/>
       <c r="H21" s="2"/>
     </row>
-    <row r="22" spans="1:8" ht="15">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" s="1"/>
       <c r="B22" s="2"/>
       <c r="E22" s="3"/>
@@ -3026,7 +3130,7 @@
       <c r="G22" s="2"/>
       <c r="H22" s="2"/>
     </row>
-    <row r="23" spans="1:8" ht="15">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" s="1"/>
       <c r="B23" s="2"/>
       <c r="E23" s="3"/>
@@ -3034,7 +3138,7 @@
       <c r="G23" s="2"/>
       <c r="H23" s="2"/>
     </row>
-    <row r="24" spans="1:8" ht="15">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24" s="1"/>
       <c r="B24" s="2"/>
       <c r="E24" s="3"/>
@@ -3042,7 +3146,7 @@
       <c r="G24" s="2"/>
       <c r="H24" s="2"/>
     </row>
-    <row r="25" spans="1:8" ht="15">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25" s="1"/>
       <c r="B25" s="2"/>
       <c r="E25" s="3"/>
@@ -3050,7 +3154,7 @@
       <c r="G25" s="2"/>
       <c r="H25" s="2"/>
     </row>
-    <row r="26" spans="1:8" ht="15">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26" s="1"/>
       <c r="B26" s="2"/>
       <c r="E26" s="3"/>
@@ -3058,7 +3162,7 @@
       <c r="G26" s="2"/>
       <c r="H26" s="2"/>
     </row>
-    <row r="27" spans="1:8" ht="15">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A27" s="1"/>
       <c r="B27" s="2"/>
       <c r="E27" s="3"/>
@@ -3066,7 +3170,7 @@
       <c r="G27" s="2"/>
       <c r="H27" s="2"/>
     </row>
-    <row r="28" spans="1:8" ht="15">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A28" s="1"/>
       <c r="B28" s="2"/>
       <c r="E28" s="3"/>
@@ -3074,7 +3178,7 @@
       <c r="G28" s="2"/>
       <c r="H28" s="2"/>
     </row>
-    <row r="29" spans="1:8" ht="15">
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A29" s="1"/>
       <c r="B29" s="2"/>
       <c r="E29" s="3"/>
@@ -3082,7 +3186,7 @@
       <c r="G29" s="2"/>
       <c r="H29" s="2"/>
     </row>
-    <row r="30" spans="1:8" ht="15">
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A30" s="1"/>
       <c r="B30" s="2"/>
       <c r="E30" s="3"/>
@@ -3090,7 +3194,7 @@
       <c r="G30" s="2"/>
       <c r="H30" s="2"/>
     </row>
-    <row r="31" spans="1:8" ht="15">
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A31" s="1"/>
       <c r="B31" s="2"/>
       <c r="E31" s="3"/>
@@ -3098,7 +3202,7 @@
       <c r="G31" s="2"/>
       <c r="H31" s="2"/>
     </row>
-    <row r="32" spans="1:8" ht="15">
+    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A32" s="1"/>
       <c r="B32" s="2"/>
       <c r="E32" s="3"/>
@@ -3106,7 +3210,7 @@
       <c r="G32" s="2"/>
       <c r="H32" s="2"/>
     </row>
-    <row r="33" spans="1:8" ht="15">
+    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A33" s="1"/>
       <c r="B33" s="2"/>
       <c r="E33" s="3"/>
@@ -3114,7 +3218,7 @@
       <c r="G33" s="2"/>
       <c r="H33" s="2"/>
     </row>
-    <row r="34" spans="1:8" ht="15">
+    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A34" s="1"/>
       <c r="B34" s="2"/>
       <c r="E34" s="3"/>
@@ -3122,7 +3226,7 @@
       <c r="G34" s="2"/>
       <c r="H34" s="2"/>
     </row>
-    <row r="35" spans="1:8" ht="15">
+    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A35" s="1"/>
       <c r="B35" s="2"/>
       <c r="E35" s="3"/>
@@ -3130,7 +3234,7 @@
       <c r="G35" s="2"/>
       <c r="H35" s="2"/>
     </row>
-    <row r="36" spans="1:8" ht="15">
+    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A36" s="1"/>
       <c r="B36" s="2"/>
       <c r="E36" s="3"/>
@@ -3138,7 +3242,7 @@
       <c r="G36" s="2"/>
       <c r="H36" s="2"/>
     </row>
-    <row r="37" spans="1:8" ht="15">
+    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A37" s="1"/>
       <c r="B37" s="2"/>
       <c r="E37" s="3"/>
@@ -3146,7 +3250,7 @@
       <c r="G37" s="2"/>
       <c r="H37" s="2"/>
     </row>
-    <row r="38" spans="1:8" ht="15">
+    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A38" s="1"/>
       <c r="B38" s="2"/>
       <c r="E38" s="3"/>
@@ -3154,7 +3258,7 @@
       <c r="G38" s="2"/>
       <c r="H38" s="2"/>
     </row>
-    <row r="39" spans="1:8" ht="15">
+    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A39" s="1"/>
       <c r="B39" s="2"/>
       <c r="E39" s="3"/>
@@ -3162,7 +3266,7 @@
       <c r="G39" s="2"/>
       <c r="H39" s="2"/>
     </row>
-    <row r="40" spans="1:8" ht="15">
+    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A40" s="1"/>
       <c r="B40" s="2"/>
       <c r="E40" s="3"/>
@@ -3170,7 +3274,7 @@
       <c r="G40" s="2"/>
       <c r="H40" s="2"/>
     </row>
-    <row r="41" spans="1:8" ht="15">
+    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A41" s="1"/>
       <c r="B41" s="2"/>
       <c r="E41" s="3"/>
@@ -3178,7 +3282,7 @@
       <c r="G41" s="2"/>
       <c r="H41" s="2"/>
     </row>
-    <row r="42" spans="1:8" ht="15">
+    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A42" s="1"/>
       <c r="B42" s="2"/>
       <c r="E42" s="3"/>
@@ -3186,7 +3290,7 @@
       <c r="G42" s="2"/>
       <c r="H42" s="2"/>
     </row>
-    <row r="43" spans="1:8" ht="15">
+    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A43" s="1"/>
       <c r="B43" s="2"/>
       <c r="E43" s="3"/>
@@ -3194,7 +3298,7 @@
       <c r="G43" s="2"/>
       <c r="H43" s="2"/>
     </row>
-    <row r="44" spans="1:8" ht="15">
+    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A44" s="1"/>
       <c r="B44" s="2"/>
       <c r="E44" s="3"/>
@@ -3202,7 +3306,7 @@
       <c r="G44" s="2"/>
       <c r="H44" s="2"/>
     </row>
-    <row r="45" spans="1:8" ht="15">
+    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A45" s="1"/>
       <c r="B45" s="2"/>
       <c r="E45" s="3"/>
@@ -3210,7 +3314,7 @@
       <c r="G45" s="2"/>
       <c r="H45" s="2"/>
     </row>
-    <row r="46" spans="1:8" ht="15">
+    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A46" s="1"/>
       <c r="B46" s="2"/>
       <c r="E46" s="3"/>
@@ -3218,7 +3322,7 @@
       <c r="G46" s="2"/>
       <c r="H46" s="2"/>
     </row>
-    <row r="47" spans="1:8" ht="15">
+    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A47" s="1"/>
       <c r="B47" s="2"/>
       <c r="E47" s="3"/>
@@ -3226,7 +3330,7 @@
       <c r="G47" s="2"/>
       <c r="H47" s="2"/>
     </row>
-    <row r="48" spans="1:8" ht="15">
+    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A48" s="1"/>
       <c r="B48" s="2"/>
       <c r="E48" s="3"/>
@@ -3234,7 +3338,7 @@
       <c r="G48" s="2"/>
       <c r="H48" s="2"/>
     </row>
-    <row r="49" spans="1:8" ht="15">
+    <row r="49" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A49" s="1"/>
       <c r="B49" s="2"/>
       <c r="E49" s="3"/>
@@ -3242,7 +3346,7 @@
       <c r="G49" s="2"/>
       <c r="H49" s="2"/>
     </row>
-    <row r="50" spans="1:8" ht="15">
+    <row r="50" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A50" s="1"/>
       <c r="B50" s="2"/>
       <c r="E50" s="3"/>
@@ -3250,7 +3354,7 @@
       <c r="G50" s="2"/>
       <c r="H50" s="2"/>
     </row>
-    <row r="51" spans="1:8" ht="15">
+    <row r="51" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A51" s="1"/>
       <c r="B51" s="2"/>
       <c r="E51" s="3"/>
@@ -3258,7 +3362,7 @@
       <c r="G51" s="2"/>
       <c r="H51" s="2"/>
     </row>
-    <row r="52" spans="1:8" ht="15">
+    <row r="52" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A52" s="1"/>
       <c r="B52" s="2"/>
       <c r="E52" s="3"/>
@@ -3266,7 +3370,7 @@
       <c r="G52" s="2"/>
       <c r="H52" s="2"/>
     </row>
-    <row r="53" spans="1:8" ht="15">
+    <row r="53" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A53" s="1"/>
       <c r="B53" s="2"/>
       <c r="E53" s="3"/>
@@ -3274,7 +3378,7 @@
       <c r="G53" s="2"/>
       <c r="H53" s="2"/>
     </row>
-    <row r="54" spans="1:8" ht="15">
+    <row r="54" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A54" s="1"/>
       <c r="B54" s="2"/>
       <c r="E54" s="3"/>
@@ -3282,7 +3386,7 @@
       <c r="G54" s="2"/>
       <c r="H54" s="2"/>
     </row>
-    <row r="55" spans="1:8" ht="15">
+    <row r="55" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A55" s="1"/>
       <c r="B55" s="2"/>
       <c r="E55" s="3"/>
@@ -3290,7 +3394,7 @@
       <c r="G55" s="2"/>
       <c r="H55" s="2"/>
     </row>
-    <row r="56" spans="1:8" ht="15">
+    <row r="56" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A56" s="1"/>
       <c r="B56" s="2"/>
       <c r="E56" s="3"/>
@@ -3298,7 +3402,7 @@
       <c r="G56" s="2"/>
       <c r="H56" s="2"/>
     </row>
-    <row r="57" spans="1:8" ht="15">
+    <row r="57" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A57" s="1"/>
       <c r="B57" s="2"/>
       <c r="E57" s="3"/>
@@ -3306,7 +3410,7 @@
       <c r="G57" s="2"/>
       <c r="H57" s="2"/>
     </row>
-    <row r="58" spans="1:8" ht="15">
+    <row r="58" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A58" s="1"/>
       <c r="B58" s="2"/>
       <c r="E58" s="3"/>
@@ -3314,7 +3418,7 @@
       <c r="G58" s="2"/>
       <c r="H58" s="2"/>
     </row>
-    <row r="59" spans="1:8" ht="15">
+    <row r="59" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A59" s="1"/>
       <c r="B59" s="2"/>
       <c r="E59" s="3"/>
@@ -3322,7 +3426,7 @@
       <c r="G59" s="2"/>
       <c r="H59" s="2"/>
     </row>
-    <row r="60" spans="1:8" ht="15">
+    <row r="60" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A60" s="1"/>
       <c r="B60" s="2"/>
       <c r="E60" s="3"/>
@@ -3330,7 +3434,7 @@
       <c r="G60" s="2"/>
       <c r="H60" s="2"/>
     </row>
-    <row r="61" spans="1:8" ht="15">
+    <row r="61" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A61" s="1"/>
       <c r="B61" s="2"/>
       <c r="E61" s="3"/>
@@ -3338,7 +3442,7 @@
       <c r="G61" s="2"/>
       <c r="H61" s="2"/>
     </row>
-    <row r="62" spans="1:8" ht="15">
+    <row r="62" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A62" s="1"/>
       <c r="B62" s="2"/>
       <c r="E62" s="3"/>
@@ -3346,7 +3450,7 @@
       <c r="G62" s="2"/>
       <c r="H62" s="2"/>
     </row>
-    <row r="63" spans="1:8" ht="15">
+    <row r="63" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A63" s="1"/>
       <c r="B63" s="2"/>
       <c r="E63" s="3"/>
@@ -3354,7 +3458,7 @@
       <c r="G63" s="2"/>
       <c r="H63" s="2"/>
     </row>
-    <row r="64" spans="1:8" ht="15">
+    <row r="64" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A64" s="1"/>
       <c r="B64" s="2"/>
       <c r="E64" s="3"/>
@@ -3362,7 +3466,7 @@
       <c r="G64" s="2"/>
       <c r="H64" s="2"/>
     </row>
-    <row r="65" spans="1:8" ht="15">
+    <row r="65" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A65" s="1"/>
       <c r="B65" s="2"/>
       <c r="E65" s="3"/>
@@ -3370,7 +3474,7 @@
       <c r="G65" s="2"/>
       <c r="H65" s="2"/>
     </row>
-    <row r="66" spans="1:8" ht="15">
+    <row r="66" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A66" s="1"/>
       <c r="B66" s="2"/>
       <c r="E66" s="3"/>
@@ -3378,7 +3482,7 @@
       <c r="G66" s="2"/>
       <c r="H66" s="2"/>
     </row>
-    <row r="67" spans="1:8" ht="15">
+    <row r="67" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A67" s="1"/>
       <c r="B67" s="2"/>
       <c r="E67" s="3"/>
@@ -3386,7 +3490,7 @@
       <c r="G67" s="2"/>
       <c r="H67" s="2"/>
     </row>
-    <row r="68" spans="1:8" ht="15">
+    <row r="68" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A68" s="1"/>
       <c r="B68" s="2"/>
       <c r="E68" s="3"/>
@@ -3394,7 +3498,7 @@
       <c r="G68" s="2"/>
       <c r="H68" s="2"/>
     </row>
-    <row r="69" spans="1:8" ht="15">
+    <row r="69" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A69" s="1"/>
       <c r="B69" s="2"/>
       <c r="E69" s="3"/>
@@ -3402,7 +3506,7 @@
       <c r="G69" s="2"/>
       <c r="H69" s="2"/>
     </row>
-    <row r="70" spans="1:8" ht="15">
+    <row r="70" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A70" s="1"/>
       <c r="B70" s="2"/>
       <c r="E70" s="3"/>
@@ -3410,7 +3514,7 @@
       <c r="G70" s="2"/>
       <c r="H70" s="2"/>
     </row>
-    <row r="71" spans="1:8" ht="15">
+    <row r="71" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A71" s="1"/>
       <c r="B71" s="2"/>
       <c r="E71" s="3"/>
@@ -3418,7 +3522,7 @@
       <c r="G71" s="2"/>
       <c r="H71" s="2"/>
     </row>
-    <row r="72" spans="1:8" ht="15">
+    <row r="72" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A72" s="1"/>
       <c r="B72" s="2"/>
       <c r="E72" s="3"/>
@@ -3426,7 +3530,7 @@
       <c r="G72" s="2"/>
       <c r="H72" s="2"/>
     </row>
-    <row r="73" spans="1:8" ht="15">
+    <row r="73" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A73" s="1"/>
       <c r="B73" s="2"/>
       <c r="E73" s="3"/>
@@ -3434,7 +3538,7 @@
       <c r="G73" s="2"/>
       <c r="H73" s="2"/>
     </row>
-    <row r="74" spans="1:8" ht="15">
+    <row r="74" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A74" s="1"/>
       <c r="B74" s="2"/>
       <c r="E74" s="3"/>
@@ -3442,7 +3546,7 @@
       <c r="G74" s="2"/>
       <c r="H74" s="2"/>
     </row>
-    <row r="75" spans="1:8" ht="15">
+    <row r="75" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A75" s="1"/>
       <c r="B75" s="2"/>
       <c r="E75" s="3"/>
@@ -3450,7 +3554,7 @@
       <c r="G75" s="2"/>
       <c r="H75" s="2"/>
     </row>
-    <row r="76" spans="1:8" ht="15">
+    <row r="76" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A76" s="1"/>
       <c r="B76" s="2"/>
       <c r="E76" s="3"/>
@@ -3458,7 +3562,7 @@
       <c r="G76" s="2"/>
       <c r="H76" s="2"/>
     </row>
-    <row r="77" spans="1:8" ht="15">
+    <row r="77" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A77" s="1"/>
       <c r="B77" s="2"/>
       <c r="E77" s="3"/>
@@ -3466,7 +3570,7 @@
       <c r="G77" s="2"/>
       <c r="H77" s="2"/>
     </row>
-    <row r="78" spans="1:8" ht="15">
+    <row r="78" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A78" s="1"/>
       <c r="B78" s="2"/>
       <c r="E78" s="3"/>
@@ -3474,7 +3578,7 @@
       <c r="G78" s="2"/>
       <c r="H78" s="2"/>
     </row>
-    <row r="79" spans="1:8" ht="15">
+    <row r="79" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A79" s="1"/>
       <c r="B79" s="2"/>
       <c r="E79" s="3"/>
@@ -3482,7 +3586,7 @@
       <c r="G79" s="2"/>
       <c r="H79" s="2"/>
     </row>
-    <row r="80" spans="1:8" ht="15">
+    <row r="80" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A80" s="1"/>
       <c r="B80" s="2"/>
       <c r="E80" s="3"/>
@@ -3490,7 +3594,7 @@
       <c r="G80" s="2"/>
       <c r="H80" s="2"/>
     </row>
-    <row r="81" spans="1:8" ht="15">
+    <row r="81" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A81" s="1"/>
       <c r="B81" s="2"/>
       <c r="E81" s="3"/>
@@ -3498,7 +3602,7 @@
       <c r="G81" s="2"/>
       <c r="H81" s="2"/>
     </row>
-    <row r="82" spans="1:8" ht="15">
+    <row r="82" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A82" s="1"/>
       <c r="B82" s="2"/>
       <c r="E82" s="3"/>
@@ -3506,7 +3610,7 @@
       <c r="G82" s="2"/>
       <c r="H82" s="2"/>
     </row>
-    <row r="83" spans="1:8" ht="15">
+    <row r="83" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A83" s="1"/>
       <c r="B83" s="2"/>
       <c r="E83" s="3"/>
@@ -3514,7 +3618,7 @@
       <c r="G83" s="2"/>
       <c r="H83" s="2"/>
     </row>
-    <row r="84" spans="1:8" ht="15">
+    <row r="84" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A84" s="1"/>
       <c r="B84" s="2"/>
       <c r="E84" s="3"/>
@@ -3522,7 +3626,7 @@
       <c r="G84" s="2"/>
       <c r="H84" s="2"/>
     </row>
-    <row r="85" spans="1:8" ht="15">
+    <row r="85" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A85" s="1"/>
       <c r="B85" s="2"/>
       <c r="E85" s="3"/>
@@ -3530,7 +3634,7 @@
       <c r="G85" s="2"/>
       <c r="H85" s="2"/>
     </row>
-    <row r="86" spans="1:8" ht="15">
+    <row r="86" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A86" s="1"/>
       <c r="B86" s="2"/>
       <c r="E86" s="3"/>
@@ -3538,7 +3642,7 @@
       <c r="G86" s="2"/>
       <c r="H86" s="2"/>
     </row>
-    <row r="87" spans="1:8" ht="15">
+    <row r="87" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A87" s="1"/>
       <c r="B87" s="2"/>
       <c r="E87" s="3"/>
@@ -3546,7 +3650,7 @@
       <c r="G87" s="2"/>
       <c r="H87" s="2"/>
     </row>
-    <row r="88" spans="1:8">
+    <row r="88" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A88" s="1"/>
       <c r="B88" s="2"/>
       <c r="E88" s="3"/>
@@ -3554,7 +3658,7 @@
       <c r="G88" s="2"/>
       <c r="H88" s="2"/>
     </row>
-    <row r="89" spans="1:8">
+    <row r="89" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A89" s="1"/>
       <c r="B89" s="2"/>
       <c r="E89" s="3"/>
@@ -3562,7 +3666,7 @@
       <c r="G89" s="2"/>
       <c r="H89" s="2"/>
     </row>
-    <row r="90" spans="1:8">
+    <row r="90" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A90" s="1"/>
       <c r="B90" s="2"/>
       <c r="E90" s="3"/>
@@ -3570,7 +3674,7 @@
       <c r="G90" s="2"/>
       <c r="H90" s="2"/>
     </row>
-    <row r="91" spans="1:8">
+    <row r="91" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A91" s="1"/>
       <c r="B91" s="2"/>
       <c r="E91" s="3"/>
@@ -3578,7 +3682,7 @@
       <c r="G91" s="2"/>
       <c r="H91" s="2"/>
     </row>
-    <row r="92" spans="1:8">
+    <row r="92" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A92" s="1"/>
       <c r="B92" s="2"/>
       <c r="E92" s="3"/>
@@ -3586,7 +3690,7 @@
       <c r="G92" s="2"/>
       <c r="H92" s="2"/>
     </row>
-    <row r="93" spans="1:8">
+    <row r="93" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A93" s="1"/>
       <c r="B93" s="2"/>
       <c r="E93" s="3"/>
@@ -3594,7 +3698,7 @@
       <c r="G93" s="2"/>
       <c r="H93" s="2"/>
     </row>
-    <row r="94" spans="1:8">
+    <row r="94" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A94" s="1"/>
       <c r="B94" s="2"/>
       <c r="E94" s="3"/>
@@ -3602,7 +3706,7 @@
       <c r="G94" s="2"/>
       <c r="H94" s="2"/>
     </row>
-    <row r="95" spans="1:8">
+    <row r="95" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A95" s="1"/>
       <c r="B95" s="2"/>
       <c r="E95" s="3"/>
@@ -3610,7 +3714,7 @@
       <c r="G95" s="2"/>
       <c r="H95" s="2"/>
     </row>
-    <row r="96" spans="1:8">
+    <row r="96" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A96" s="1"/>
       <c r="B96" s="2"/>
       <c r="E96" s="3"/>
@@ -3618,7 +3722,7 @@
       <c r="G96" s="2"/>
       <c r="H96" s="2"/>
     </row>
-    <row r="97" spans="1:8">
+    <row r="97" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A97" s="1"/>
       <c r="B97" s="2"/>
       <c r="E97" s="3"/>
@@ -3626,7 +3730,7 @@
       <c r="G97" s="2"/>
       <c r="H97" s="2"/>
     </row>
-    <row r="98" spans="1:8">
+    <row r="98" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A98" s="1"/>
       <c r="B98" s="2"/>
       <c r="E98" s="3"/>
@@ -3634,7 +3738,7 @@
       <c r="G98" s="2"/>
       <c r="H98" s="2"/>
     </row>
-    <row r="99" spans="1:8">
+    <row r="99" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A99" s="1"/>
       <c r="B99" s="2"/>
       <c r="E99" s="3"/>
@@ -3642,7 +3746,7 @@
       <c r="G99" s="2"/>
       <c r="H99" s="2"/>
     </row>
-    <row r="100" spans="1:8">
+    <row r="100" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A100" s="1"/>
       <c r="B100" s="2"/>
       <c r="E100" s="3"/>
@@ -3685,21 +3789,21 @@
       <selection activeCell="P21" sqref="P21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.09765625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.8984375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.8984375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="19.3984375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.59765625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.59765625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.5703125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="9" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="17.8984375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="17.85546875" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="17" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="19.09765625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="19.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="15.75">
+    <row r="1" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="7" t="s">
         <v>8</v>
       </c>
@@ -3731,7 +3835,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:10" ht="15">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="2"/>
       <c r="B2" s="8"/>
       <c r="D2" s="2"/>
@@ -3739,7 +3843,7 @@
       <c r="I2" s="8"/>
       <c r="J2" s="2"/>
     </row>
-    <row r="3" spans="1:10" ht="15">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="2"/>
       <c r="B3" s="8"/>
       <c r="D3" s="2"/>
@@ -3747,7 +3851,7 @@
       <c r="I3" s="8"/>
       <c r="J3" s="2"/>
     </row>
-    <row r="4" spans="1:10" ht="15">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="2"/>
       <c r="B4" s="8"/>
       <c r="D4" s="2"/>
@@ -3755,7 +3859,7 @@
       <c r="I4" s="8"/>
       <c r="J4" s="2"/>
     </row>
-    <row r="5" spans="1:10" ht="15">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" s="2"/>
       <c r="B5" s="8"/>
       <c r="D5" s="2"/>
@@ -3763,7 +3867,7 @@
       <c r="I5" s="8"/>
       <c r="J5" s="2"/>
     </row>
-    <row r="6" spans="1:10" ht="15">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" s="2"/>
       <c r="B6" s="8"/>
       <c r="D6" s="2"/>
@@ -3771,7 +3875,7 @@
       <c r="I6" s="8"/>
       <c r="J6" s="2"/>
     </row>
-    <row r="7" spans="1:10" ht="15">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" s="2"/>
       <c r="B7" s="8"/>
       <c r="D7" s="2"/>
@@ -3779,7 +3883,7 @@
       <c r="I7" s="8"/>
       <c r="J7" s="2"/>
     </row>
-    <row r="8" spans="1:10" ht="15">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" s="2"/>
       <c r="B8" s="8"/>
       <c r="D8" s="2"/>
@@ -3787,7 +3891,7 @@
       <c r="I8" s="8"/>
       <c r="J8" s="2"/>
     </row>
-    <row r="9" spans="1:10" ht="15">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" s="2"/>
       <c r="B9" s="8"/>
       <c r="D9" s="2"/>
@@ -3795,7 +3899,7 @@
       <c r="I9" s="8"/>
       <c r="J9" s="2"/>
     </row>
-    <row r="10" spans="1:10" ht="15">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" s="2"/>
       <c r="B10" s="8"/>
       <c r="D10" s="2"/>
@@ -3803,7 +3907,7 @@
       <c r="I10" s="8"/>
       <c r="J10" s="2"/>
     </row>
-    <row r="11" spans="1:10" ht="15">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" s="2"/>
       <c r="B11" s="8"/>
       <c r="D11" s="2"/>
@@ -3811,7 +3915,7 @@
       <c r="I11" s="8"/>
       <c r="J11" s="2"/>
     </row>
-    <row r="12" spans="1:10" ht="15">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" s="2"/>
       <c r="B12" s="8"/>
       <c r="D12" s="2"/>
@@ -3819,7 +3923,7 @@
       <c r="I12" s="8"/>
       <c r="J12" s="2"/>
     </row>
-    <row r="13" spans="1:10" ht="15">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" s="2"/>
       <c r="B13" s="8"/>
       <c r="D13" s="2"/>
@@ -3827,7 +3931,7 @@
       <c r="I13" s="8"/>
       <c r="J13" s="2"/>
     </row>
-    <row r="14" spans="1:10" ht="15">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" s="2"/>
       <c r="B14" s="8"/>
       <c r="D14" s="2"/>
@@ -3835,7 +3939,7 @@
       <c r="I14" s="8"/>
       <c r="J14" s="2"/>
     </row>
-    <row r="15" spans="1:10" ht="15">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" s="2"/>
       <c r="B15" s="8"/>
       <c r="D15" s="2"/>
@@ -3843,7 +3947,7 @@
       <c r="I15" s="8"/>
       <c r="J15" s="2"/>
     </row>
-    <row r="16" spans="1:10" ht="15">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" s="2"/>
       <c r="B16" s="8"/>
       <c r="D16" s="2"/>
@@ -3851,7 +3955,7 @@
       <c r="I16" s="8"/>
       <c r="J16" s="2"/>
     </row>
-    <row r="17" spans="1:10" ht="15">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17" s="2"/>
       <c r="B17" s="8"/>
       <c r="D17" s="2"/>
@@ -3859,7 +3963,7 @@
       <c r="I17" s="8"/>
       <c r="J17" s="2"/>
     </row>
-    <row r="18" spans="1:10" ht="15">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18" s="2"/>
       <c r="B18" s="8"/>
       <c r="D18" s="2"/>
@@ -3867,7 +3971,7 @@
       <c r="I18" s="8"/>
       <c r="J18" s="2"/>
     </row>
-    <row r="19" spans="1:10" ht="15">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A19" s="2"/>
       <c r="B19" s="8"/>
       <c r="D19" s="2"/>
@@ -3875,7 +3979,7 @@
       <c r="I19" s="8"/>
       <c r="J19" s="2"/>
     </row>
-    <row r="20" spans="1:10" ht="15">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A20" s="2"/>
       <c r="B20" s="8"/>
       <c r="D20" s="2"/>
@@ -3883,7 +3987,7 @@
       <c r="I20" s="8"/>
       <c r="J20" s="2"/>
     </row>
-    <row r="21" spans="1:10" ht="15">
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A21" s="2"/>
       <c r="B21" s="8"/>
       <c r="D21" s="2"/>
@@ -3891,7 +3995,7 @@
       <c r="I21" s="8"/>
       <c r="J21" s="2"/>
     </row>
-    <row r="22" spans="1:10" ht="15">
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A22" s="2"/>
       <c r="B22" s="8"/>
       <c r="D22" s="2"/>
@@ -3899,7 +4003,7 @@
       <c r="I22" s="8"/>
       <c r="J22" s="2"/>
     </row>
-    <row r="23" spans="1:10" ht="15">
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A23" s="2"/>
       <c r="B23" s="8"/>
       <c r="D23" s="2"/>
@@ -3907,7 +4011,7 @@
       <c r="I23" s="8"/>
       <c r="J23" s="2"/>
     </row>
-    <row r="24" spans="1:10" ht="15">
+    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A24" s="2"/>
       <c r="B24" s="8"/>
       <c r="D24" s="2"/>
@@ -3915,7 +4019,7 @@
       <c r="I24" s="8"/>
       <c r="J24" s="2"/>
     </row>
-    <row r="25" spans="1:10" ht="15">
+    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A25" s="2"/>
       <c r="B25" s="8"/>
       <c r="D25" s="2"/>
@@ -3923,7 +4027,7 @@
       <c r="I25" s="8"/>
       <c r="J25" s="2"/>
     </row>
-    <row r="26" spans="1:10">
+    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A26" s="2"/>
       <c r="B26" s="8"/>
       <c r="D26" s="2"/>
@@ -3931,7 +4035,7 @@
       <c r="I26" s="8"/>
       <c r="J26" s="2"/>
     </row>
-    <row r="27" spans="1:10">
+    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A27" s="2"/>
       <c r="B27" s="8"/>
       <c r="D27" s="2"/>
@@ -3939,7 +4043,7 @@
       <c r="I27" s="8"/>
       <c r="J27" s="2"/>
     </row>
-    <row r="28" spans="1:10">
+    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A28" s="2"/>
       <c r="B28" s="8"/>
       <c r="D28" s="2"/>
@@ -3947,7 +4051,7 @@
       <c r="I28" s="8"/>
       <c r="J28" s="2"/>
     </row>
-    <row r="29" spans="1:10">
+    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A29" s="2"/>
       <c r="B29" s="8"/>
       <c r="D29" s="2"/>
@@ -3955,7 +4059,7 @@
       <c r="I29" s="8"/>
       <c r="J29" s="2"/>
     </row>
-    <row r="30" spans="1:10">
+    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A30" s="2"/>
       <c r="B30" s="8"/>
       <c r="D30" s="2"/>
@@ -3963,7 +4067,7 @@
       <c r="I30" s="8"/>
       <c r="J30" s="2"/>
     </row>
-    <row r="31" spans="1:10">
+    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A31" s="2"/>
       <c r="B31" s="8"/>
       <c r="D31" s="2"/>
@@ -3971,7 +4075,7 @@
       <c r="I31" s="8"/>
       <c r="J31" s="2"/>
     </row>
-    <row r="32" spans="1:10">
+    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A32" s="2"/>
       <c r="B32" s="8"/>
       <c r="D32" s="2"/>
@@ -3979,7 +4083,7 @@
       <c r="I32" s="8"/>
       <c r="J32" s="2"/>
     </row>
-    <row r="33" spans="1:10">
+    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A33" s="2"/>
       <c r="B33" s="8"/>
       <c r="D33" s="2"/>
@@ -3987,7 +4091,7 @@
       <c r="I33" s="8"/>
       <c r="J33" s="2"/>
     </row>
-    <row r="34" spans="1:10">
+    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A34" s="2"/>
       <c r="B34" s="8"/>
       <c r="D34" s="2"/>
@@ -3995,7 +4099,7 @@
       <c r="I34" s="8"/>
       <c r="J34" s="2"/>
     </row>
-    <row r="35" spans="1:10">
+    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A35" s="2"/>
       <c r="B35" s="8"/>
       <c r="D35" s="2"/>
@@ -4003,7 +4107,7 @@
       <c r="I35" s="8"/>
       <c r="J35" s="2"/>
     </row>
-    <row r="36" spans="1:10">
+    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A36" s="2"/>
       <c r="B36" s="8"/>
       <c r="D36" s="2"/>
@@ -4011,7 +4115,7 @@
       <c r="I36" s="8"/>
       <c r="J36" s="2"/>
     </row>
-    <row r="37" spans="1:10">
+    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A37" s="2"/>
       <c r="B37" s="8"/>
       <c r="D37" s="2"/>
@@ -4019,7 +4123,7 @@
       <c r="I37" s="8"/>
       <c r="J37" s="2"/>
     </row>
-    <row r="38" spans="1:10">
+    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A38" s="2"/>
       <c r="B38" s="8"/>
       <c r="D38" s="2"/>
@@ -4027,7 +4131,7 @@
       <c r="I38" s="8"/>
       <c r="J38" s="2"/>
     </row>
-    <row r="39" spans="1:10">
+    <row r="39" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A39" s="2"/>
       <c r="B39" s="8"/>
       <c r="D39" s="2"/>
@@ -4035,7 +4139,7 @@
       <c r="I39" s="8"/>
       <c r="J39" s="2"/>
     </row>
-    <row r="40" spans="1:10">
+    <row r="40" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A40" s="2"/>
       <c r="B40" s="8"/>
       <c r="D40" s="2"/>
@@ -4043,7 +4147,7 @@
       <c r="I40" s="8"/>
       <c r="J40" s="2"/>
     </row>
-    <row r="41" spans="1:10">
+    <row r="41" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A41" s="2"/>
       <c r="B41" s="8"/>
       <c r="D41" s="2"/>
@@ -4051,7 +4155,7 @@
       <c r="I41" s="8"/>
       <c r="J41" s="2"/>
     </row>
-    <row r="42" spans="1:10">
+    <row r="42" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A42" s="2"/>
       <c r="B42" s="8"/>
       <c r="D42" s="2"/>
@@ -4059,7 +4163,7 @@
       <c r="I42" s="8"/>
       <c r="J42" s="2"/>
     </row>
-    <row r="43" spans="1:10">
+    <row r="43" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A43" s="2"/>
       <c r="B43" s="8"/>
       <c r="D43" s="2"/>
@@ -4067,7 +4171,7 @@
       <c r="I43" s="8"/>
       <c r="J43" s="2"/>
     </row>
-    <row r="44" spans="1:10">
+    <row r="44" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A44" s="2"/>
       <c r="B44" s="8"/>
       <c r="D44" s="2"/>
@@ -4075,7 +4179,7 @@
       <c r="I44" s="8"/>
       <c r="J44" s="2"/>
     </row>
-    <row r="45" spans="1:10">
+    <row r="45" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A45" s="2"/>
       <c r="B45" s="8"/>
       <c r="D45" s="2"/>
@@ -4083,7 +4187,7 @@
       <c r="I45" s="8"/>
       <c r="J45" s="2"/>
     </row>
-    <row r="46" spans="1:10">
+    <row r="46" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A46" s="2"/>
       <c r="B46" s="8"/>
       <c r="D46" s="2"/>
@@ -4091,7 +4195,7 @@
       <c r="I46" s="8"/>
       <c r="J46" s="2"/>
     </row>
-    <row r="47" spans="1:10">
+    <row r="47" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A47" s="2"/>
       <c r="B47" s="8"/>
       <c r="D47" s="2"/>
@@ -4099,7 +4203,7 @@
       <c r="I47" s="8"/>
       <c r="J47" s="2"/>
     </row>
-    <row r="48" spans="1:10">
+    <row r="48" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A48" s="2"/>
       <c r="B48" s="8"/>
       <c r="D48" s="2"/>
@@ -4107,7 +4211,7 @@
       <c r="I48" s="8"/>
       <c r="J48" s="2"/>
     </row>
-    <row r="49" spans="1:10">
+    <row r="49" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A49" s="2"/>
       <c r="B49" s="8"/>
       <c r="D49" s="2"/>
@@ -4115,7 +4219,7 @@
       <c r="I49" s="8"/>
       <c r="J49" s="2"/>
     </row>
-    <row r="50" spans="1:10">
+    <row r="50" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A50" s="2"/>
       <c r="B50" s="8"/>
       <c r="D50" s="2"/>
@@ -4123,7 +4227,7 @@
       <c r="I50" s="8"/>
       <c r="J50" s="2"/>
     </row>
-    <row r="51" spans="1:10">
+    <row r="51" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A51" s="2"/>
       <c r="B51" s="8"/>
       <c r="D51" s="2"/>
@@ -4131,7 +4235,7 @@
       <c r="I51" s="8"/>
       <c r="J51" s="2"/>
     </row>
-    <row r="52" spans="1:10">
+    <row r="52" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A52" s="2"/>
       <c r="B52" s="8"/>
       <c r="D52" s="2"/>
@@ -4139,7 +4243,7 @@
       <c r="I52" s="8"/>
       <c r="J52" s="2"/>
     </row>
-    <row r="53" spans="1:10">
+    <row r="53" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A53" s="2"/>
       <c r="B53" s="8"/>
       <c r="D53" s="2"/>
@@ -4147,7 +4251,7 @@
       <c r="I53" s="8"/>
       <c r="J53" s="2"/>
     </row>
-    <row r="54" spans="1:10">
+    <row r="54" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A54" s="2"/>
       <c r="B54" s="8"/>
       <c r="D54" s="2"/>
@@ -4155,7 +4259,7 @@
       <c r="I54" s="8"/>
       <c r="J54" s="2"/>
     </row>
-    <row r="55" spans="1:10">
+    <row r="55" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A55" s="2"/>
       <c r="B55" s="8"/>
       <c r="D55" s="2"/>
@@ -4163,7 +4267,7 @@
       <c r="I55" s="8"/>
       <c r="J55" s="2"/>
     </row>
-    <row r="56" spans="1:10">
+    <row r="56" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A56" s="2"/>
       <c r="B56" s="8"/>
       <c r="D56" s="2"/>
@@ -4171,7 +4275,7 @@
       <c r="I56" s="8"/>
       <c r="J56" s="2"/>
     </row>
-    <row r="57" spans="1:10">
+    <row r="57" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A57" s="2"/>
       <c r="B57" s="8"/>
       <c r="D57" s="2"/>
@@ -4179,7 +4283,7 @@
       <c r="I57" s="8"/>
       <c r="J57" s="2"/>
     </row>
-    <row r="58" spans="1:10">
+    <row r="58" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A58" s="2"/>
       <c r="B58" s="8"/>
       <c r="D58" s="2"/>
@@ -4187,7 +4291,7 @@
       <c r="I58" s="8"/>
       <c r="J58" s="2"/>
     </row>
-    <row r="59" spans="1:10">
+    <row r="59" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A59" s="2"/>
       <c r="B59" s="8"/>
       <c r="D59" s="2"/>
@@ -4195,7 +4299,7 @@
       <c r="I59" s="8"/>
       <c r="J59" s="2"/>
     </row>
-    <row r="60" spans="1:10">
+    <row r="60" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A60" s="2"/>
       <c r="B60" s="8"/>
       <c r="D60" s="2"/>
@@ -4203,7 +4307,7 @@
       <c r="I60" s="8"/>
       <c r="J60" s="2"/>
     </row>
-    <row r="61" spans="1:10">
+    <row r="61" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A61" s="2"/>
       <c r="B61" s="8"/>
       <c r="D61" s="2"/>
@@ -4211,7 +4315,7 @@
       <c r="I61" s="8"/>
       <c r="J61" s="2"/>
     </row>
-    <row r="62" spans="1:10">
+    <row r="62" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A62" s="2"/>
       <c r="B62" s="8"/>
       <c r="D62" s="2"/>
@@ -4219,7 +4323,7 @@
       <c r="I62" s="8"/>
       <c r="J62" s="2"/>
     </row>
-    <row r="63" spans="1:10">
+    <row r="63" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A63" s="2"/>
       <c r="B63" s="8"/>
       <c r="D63" s="2"/>
@@ -4227,7 +4331,7 @@
       <c r="I63" s="8"/>
       <c r="J63" s="2"/>
     </row>
-    <row r="64" spans="1:10">
+    <row r="64" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A64" s="2"/>
       <c r="B64" s="8"/>
       <c r="D64" s="2"/>
@@ -4235,7 +4339,7 @@
       <c r="I64" s="8"/>
       <c r="J64" s="2"/>
     </row>
-    <row r="65" spans="1:10">
+    <row r="65" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A65" s="2"/>
       <c r="B65" s="8"/>
       <c r="D65" s="2"/>
@@ -4243,7 +4347,7 @@
       <c r="I65" s="8"/>
       <c r="J65" s="2"/>
     </row>
-    <row r="66" spans="1:10">
+    <row r="66" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A66" s="2"/>
       <c r="B66" s="8"/>
       <c r="D66" s="2"/>
@@ -4251,7 +4355,7 @@
       <c r="I66" s="8"/>
       <c r="J66" s="2"/>
     </row>
-    <row r="67" spans="1:10">
+    <row r="67" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A67" s="2"/>
       <c r="B67" s="8"/>
       <c r="D67" s="2"/>
@@ -4259,7 +4363,7 @@
       <c r="I67" s="8"/>
       <c r="J67" s="2"/>
     </row>
-    <row r="68" spans="1:10">
+    <row r="68" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A68" s="2"/>
       <c r="B68" s="8"/>
       <c r="D68" s="2"/>
@@ -4267,7 +4371,7 @@
       <c r="I68" s="8"/>
       <c r="J68" s="2"/>
     </row>
-    <row r="69" spans="1:10">
+    <row r="69" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A69" s="2"/>
       <c r="B69" s="8"/>
       <c r="D69" s="2"/>
@@ -4275,7 +4379,7 @@
       <c r="I69" s="8"/>
       <c r="J69" s="2"/>
     </row>
-    <row r="70" spans="1:10">
+    <row r="70" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A70" s="2"/>
       <c r="B70" s="8"/>
       <c r="D70" s="2"/>
@@ -4283,7 +4387,7 @@
       <c r="I70" s="8"/>
       <c r="J70" s="2"/>
     </row>
-    <row r="71" spans="1:10">
+    <row r="71" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A71" s="2"/>
       <c r="B71" s="8"/>
       <c r="D71" s="2"/>
@@ -4291,7 +4395,7 @@
       <c r="I71" s="8"/>
       <c r="J71" s="2"/>
     </row>
-    <row r="72" spans="1:10">
+    <row r="72" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A72" s="2"/>
       <c r="B72" s="8"/>
       <c r="D72" s="2"/>
@@ -4299,7 +4403,7 @@
       <c r="I72" s="8"/>
       <c r="J72" s="2"/>
     </row>
-    <row r="73" spans="1:10">
+    <row r="73" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A73" s="2"/>
       <c r="B73" s="8"/>
       <c r="D73" s="2"/>
@@ -4307,7 +4411,7 @@
       <c r="I73" s="8"/>
       <c r="J73" s="2"/>
     </row>
-    <row r="74" spans="1:10">
+    <row r="74" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A74" s="2"/>
       <c r="B74" s="8"/>
       <c r="D74" s="2"/>
@@ -4315,7 +4419,7 @@
       <c r="I74" s="8"/>
       <c r="J74" s="2"/>
     </row>
-    <row r="75" spans="1:10">
+    <row r="75" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A75" s="2"/>
       <c r="B75" s="8"/>
       <c r="D75" s="2"/>
@@ -4323,7 +4427,7 @@
       <c r="I75" s="8"/>
       <c r="J75" s="2"/>
     </row>
-    <row r="76" spans="1:10">
+    <row r="76" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A76" s="2"/>
       <c r="B76" s="8"/>
       <c r="D76" s="2"/>
@@ -4331,7 +4435,7 @@
       <c r="I76" s="8"/>
       <c r="J76" s="2"/>
     </row>
-    <row r="77" spans="1:10">
+    <row r="77" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A77" s="2"/>
       <c r="B77" s="8"/>
       <c r="D77" s="2"/>
@@ -4339,7 +4443,7 @@
       <c r="I77" s="8"/>
       <c r="J77" s="2"/>
     </row>
-    <row r="78" spans="1:10">
+    <row r="78" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A78" s="2"/>
       <c r="B78" s="8"/>
       <c r="D78" s="2"/>
@@ -4347,7 +4451,7 @@
       <c r="I78" s="8"/>
       <c r="J78" s="2"/>
     </row>
-    <row r="79" spans="1:10">
+    <row r="79" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A79" s="2"/>
       <c r="B79" s="8"/>
       <c r="D79" s="2"/>
@@ -4355,7 +4459,7 @@
       <c r="I79" s="8"/>
       <c r="J79" s="2"/>
     </row>
-    <row r="80" spans="1:10">
+    <row r="80" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A80" s="2"/>
       <c r="B80" s="8"/>
       <c r="D80" s="2"/>
@@ -4363,7 +4467,7 @@
       <c r="I80" s="8"/>
       <c r="J80" s="2"/>
     </row>
-    <row r="81" spans="1:10">
+    <row r="81" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A81" s="2"/>
       <c r="B81" s="8"/>
       <c r="D81" s="2"/>
@@ -4371,7 +4475,7 @@
       <c r="I81" s="8"/>
       <c r="J81" s="2"/>
     </row>
-    <row r="82" spans="1:10">
+    <row r="82" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A82" s="2"/>
       <c r="B82" s="8"/>
       <c r="D82" s="2"/>
@@ -4379,7 +4483,7 @@
       <c r="I82" s="8"/>
       <c r="J82" s="2"/>
     </row>
-    <row r="83" spans="1:10">
+    <row r="83" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A83" s="2"/>
       <c r="B83" s="8"/>
       <c r="D83" s="2"/>
@@ -4387,7 +4491,7 @@
       <c r="I83" s="8"/>
       <c r="J83" s="2"/>
     </row>
-    <row r="84" spans="1:10">
+    <row r="84" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A84" s="2"/>
       <c r="B84" s="8"/>
       <c r="D84" s="2"/>
@@ -4395,7 +4499,7 @@
       <c r="I84" s="8"/>
       <c r="J84" s="2"/>
     </row>
-    <row r="85" spans="1:10">
+    <row r="85" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A85" s="2"/>
       <c r="B85" s="8"/>
       <c r="D85" s="2"/>
@@ -4403,7 +4507,7 @@
       <c r="I85" s="8"/>
       <c r="J85" s="2"/>
     </row>
-    <row r="86" spans="1:10">
+    <row r="86" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A86" s="2"/>
       <c r="B86" s="8"/>
       <c r="D86" s="2"/>
@@ -4411,7 +4515,7 @@
       <c r="I86" s="8"/>
       <c r="J86" s="2"/>
     </row>
-    <row r="87" spans="1:10">
+    <row r="87" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A87" s="2"/>
       <c r="B87" s="8"/>
       <c r="D87" s="2"/>
@@ -4419,7 +4523,7 @@
       <c r="I87" s="8"/>
       <c r="J87" s="2"/>
     </row>
-    <row r="88" spans="1:10">
+    <row r="88" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A88" s="2"/>
       <c r="B88" s="8"/>
       <c r="D88" s="2"/>
@@ -4427,7 +4531,7 @@
       <c r="I88" s="8"/>
       <c r="J88" s="2"/>
     </row>
-    <row r="89" spans="1:10">
+    <row r="89" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A89" s="2"/>
       <c r="B89" s="8"/>
       <c r="D89" s="2"/>
@@ -4435,7 +4539,7 @@
       <c r="I89" s="8"/>
       <c r="J89" s="2"/>
     </row>
-    <row r="90" spans="1:10">
+    <row r="90" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A90" s="2"/>
       <c r="B90" s="8"/>
       <c r="D90" s="2"/>
@@ -4443,7 +4547,7 @@
       <c r="I90" s="8"/>
       <c r="J90" s="2"/>
     </row>
-    <row r="91" spans="1:10">
+    <row r="91" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A91" s="2"/>
       <c r="B91" s="8"/>
       <c r="D91" s="2"/>
@@ -4451,7 +4555,7 @@
       <c r="I91" s="8"/>
       <c r="J91" s="2"/>
     </row>
-    <row r="92" spans="1:10">
+    <row r="92" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A92" s="2"/>
       <c r="B92" s="8"/>
       <c r="D92" s="2"/>
@@ -4459,7 +4563,7 @@
       <c r="I92" s="8"/>
       <c r="J92" s="2"/>
     </row>
-    <row r="93" spans="1:10">
+    <row r="93" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A93" s="2"/>
       <c r="B93" s="8"/>
       <c r="D93" s="2"/>
@@ -4467,7 +4571,7 @@
       <c r="I93" s="8"/>
       <c r="J93" s="2"/>
     </row>
-    <row r="94" spans="1:10">
+    <row r="94" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A94" s="2"/>
       <c r="B94" s="8"/>
       <c r="D94" s="2"/>
@@ -4475,7 +4579,7 @@
       <c r="I94" s="8"/>
       <c r="J94" s="2"/>
     </row>
-    <row r="95" spans="1:10">
+    <row r="95" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A95" s="2"/>
       <c r="B95" s="8"/>
       <c r="D95" s="2"/>
@@ -4483,7 +4587,7 @@
       <c r="I95" s="8"/>
       <c r="J95" s="2"/>
     </row>
-    <row r="96" spans="1:10">
+    <row r="96" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A96" s="2"/>
       <c r="B96" s="8"/>
       <c r="D96" s="2"/>
@@ -4491,7 +4595,7 @@
       <c r="I96" s="8"/>
       <c r="J96" s="2"/>
     </row>
-    <row r="97" spans="1:10">
+    <row r="97" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A97" s="2"/>
       <c r="B97" s="8"/>
       <c r="D97" s="2"/>
@@ -4499,7 +4603,7 @@
       <c r="I97" s="8"/>
       <c r="J97" s="2"/>
     </row>
-    <row r="98" spans="1:10">
+    <row r="98" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A98" s="2"/>
       <c r="B98" s="8"/>
       <c r="D98" s="2"/>
@@ -4507,7 +4611,7 @@
       <c r="I98" s="8"/>
       <c r="J98" s="2"/>
     </row>
-    <row r="99" spans="1:10">
+    <row r="99" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A99" s="2"/>
       <c r="B99" s="8"/>
       <c r="D99" s="2"/>
@@ -4515,7 +4619,7 @@
       <c r="I99" s="8"/>
       <c r="J99" s="2"/>
     </row>
-    <row r="100" spans="1:10">
+    <row r="100" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A100" s="2"/>
       <c r="B100" s="8"/>
       <c r="D100" s="2"/>

</xml_diff>

<commit_message>
Add/update progress report for 15/05/2025 Thurs by Shivya
</commit_message>
<xml_diff>
--- a/PR&IR.xlsx
+++ b/PR&IR.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26026"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\avichal avneel nath\Documents\Semester 7\CS415\A3\CS415_A3\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SHIVYA KUMAR\Desktop\new415\CS415_A3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{446B9638-145F-47A9-8E17-E54F5F829A5D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{17103190-127F-4537-9CCD-D430D1B89B94}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{BFA1E21A-08FA-4F02-8C25-33C81C8EE970}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{BFA1E21A-08FA-4F02-8C25-33C81C8EE970}"/>
   </bookViews>
   <sheets>
     <sheet name="Avichal" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="51">
   <si>
     <t>Date</t>
   </si>
@@ -158,6 +158,54 @@
   <si>
     <t xml:space="preserve">Stay Healthy Aviiii. Don’t get sick </t>
   </si>
+  <si>
+    <t>Shivya Kumar</t>
+  </si>
+  <si>
+    <t>Convert UI for login, homepage and student profile</t>
+  </si>
+  <si>
+    <t>In Progress</t>
+  </si>
+  <si>
+    <t>Continue converting UI and setting route</t>
+  </si>
+  <si>
+    <t>I was unable to run the app locally, so I created a folder named run_main_app.py with the required code Once I did that I was able to start the Flask server successfully</t>
+  </si>
+  <si>
+    <t>Added header and footer to the remaining UIs, and converted UI for enrollment page.</t>
+  </si>
+  <si>
+    <t>Solve my routes and fix UI</t>
+  </si>
+  <si>
+    <t>I added my routes in the same file app.py</t>
+  </si>
+  <si>
+    <t>Customizing UI and recovered deleted codes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Continue converting UI </t>
+  </si>
+  <si>
+    <t>shivya Kumar</t>
+  </si>
+  <si>
+    <t>Converted all user interface designs into HTML and set up respective routes.</t>
+  </si>
+  <si>
+    <t>continue implementing remaining UI logic based on feedback and custom validation with exception handling for all of her routes</t>
+  </si>
+  <si>
+    <t>Added custom validation for logout and exception handling for all routes</t>
+  </si>
+  <si>
+    <t>Not feeling well, assignments are due and short tests are approaching.</t>
+  </si>
+  <si>
+    <t>Start with next workpackage once approved and given by Jayshil Singh</t>
+  </si>
 </sst>
 </file>
 
@@ -167,7 +215,7 @@
     <numFmt numFmtId="164" formatCode="h"/>
     <numFmt numFmtId="165" formatCode="d/mm/yyyy;@"/>
   </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="3">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -208,7 +256,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -221,11 +269,22 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="35">
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
     <dxf>
       <numFmt numFmtId="30" formatCode="@"/>
     </dxf>
@@ -336,15 +395,6 @@
     </dxf>
     <dxf>
       <numFmt numFmtId="30" formatCode="@"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="164" formatCode="h"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="14" formatCode="0.00%"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="30" formatCode="@"/>
@@ -462,17 +512,17 @@
     <tableColumn id="2" xr3:uid="{55A78D6C-890A-4502-A184-DEEFF14BB82E}" name="Member Name" dataDxfId="25"/>
     <tableColumn id="3" xr3:uid="{57B9A516-E930-4C06-A589-24182A37BA85}" name="Task/Activity"/>
     <tableColumn id="4" xr3:uid="{A7CD18E8-808E-43EA-A960-7EDF2D2AB452}" name="Status"/>
-    <tableColumn id="5" xr3:uid="{A9BAB96D-D5FD-4C0D-A277-6E052D27EC3A}" name="% Complete" dataDxfId="24"/>
-    <tableColumn id="6" xr3:uid="{4EBDEBD4-A02D-4266-88BC-5E6088167CE4}" name="Hours Worked Today" dataDxfId="23"/>
-    <tableColumn id="7" xr3:uid="{88484166-6833-4A6B-B292-081E908E7876}" name="Next Steps" dataDxfId="22"/>
-    <tableColumn id="8" xr3:uid="{65034E84-46C0-4115-A351-A3C28C7B9EE1}" name="Notes/Comments" dataDxfId="21"/>
+    <tableColumn id="5" xr3:uid="{A9BAB96D-D5FD-4C0D-A277-6E052D27EC3A}" name="% Complete" dataDxfId="0"/>
+    <tableColumn id="6" xr3:uid="{4EBDEBD4-A02D-4266-88BC-5E6088167CE4}" name="Hours Worked Today" dataDxfId="1"/>
+    <tableColumn id="7" xr3:uid="{88484166-6833-4A6B-B292-081E908E7876}" name="Next Steps" dataDxfId="2"/>
+    <tableColumn id="8" xr3:uid="{65034E84-46C0-4115-A351-A3C28C7B9EE1}" name="Notes/Comments" dataDxfId="24"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium26" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{D9A2FBFA-47C8-4A27-8A35-991BC77E93AD}" name="Table14" displayName="Table14" ref="A1:H100" totalsRowShown="0" headerRowDxfId="20">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{D9A2FBFA-47C8-4A27-8A35-991BC77E93AD}" name="Table14" displayName="Table14" ref="A1:H100" totalsRowShown="0" headerRowDxfId="23">
   <autoFilter ref="A1:H100" xr:uid="{D9A2FBFA-47C8-4A27-8A35-991BC77E93AD}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
@@ -484,21 +534,21 @@
     <filterColumn colId="7" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="8">
-    <tableColumn id="1" xr3:uid="{9DF80C4D-D075-4428-A54F-FD6AD093D08C}" name="Date" dataDxfId="19"/>
-    <tableColumn id="2" xr3:uid="{EBFC72C6-272F-4910-98B7-AD481D68F5CF}" name="Member Name" dataDxfId="18"/>
+    <tableColumn id="1" xr3:uid="{9DF80C4D-D075-4428-A54F-FD6AD093D08C}" name="Date" dataDxfId="22"/>
+    <tableColumn id="2" xr3:uid="{EBFC72C6-272F-4910-98B7-AD481D68F5CF}" name="Member Name" dataDxfId="21"/>
     <tableColumn id="3" xr3:uid="{9F5B3984-7002-4FEA-8B81-D2D8284783D7}" name="Task/Activity"/>
     <tableColumn id="4" xr3:uid="{5F85F44B-886F-440F-9E69-8335A039C2E6}" name="Status"/>
-    <tableColumn id="5" xr3:uid="{AF0043ED-9EF2-470B-9735-7321011714BA}" name="% Complete" dataDxfId="17"/>
-    <tableColumn id="6" xr3:uid="{4F961AD8-B86B-411C-BB04-8D7EE4DD134D}" name="Hours Worked Today" dataDxfId="16"/>
-    <tableColumn id="7" xr3:uid="{34EBB1FC-FFD7-47AB-A959-A220B742401C}" name="Next Steps" dataDxfId="15"/>
-    <tableColumn id="8" xr3:uid="{128DAA9E-15FB-4BB9-B76B-4A920C859038}" name="Notes/Comments" dataDxfId="14"/>
+    <tableColumn id="5" xr3:uid="{AF0043ED-9EF2-470B-9735-7321011714BA}" name="% Complete" dataDxfId="20"/>
+    <tableColumn id="6" xr3:uid="{4F961AD8-B86B-411C-BB04-8D7EE4DD134D}" name="Hours Worked Today" dataDxfId="19"/>
+    <tableColumn id="7" xr3:uid="{34EBB1FC-FFD7-47AB-A959-A220B742401C}" name="Next Steps" dataDxfId="18"/>
+    <tableColumn id="8" xr3:uid="{128DAA9E-15FB-4BB9-B76B-4A920C859038}" name="Notes/Comments" dataDxfId="17"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium26" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{646C4EC7-41A3-4570-9D38-06D55FDE20F6}" name="Table15" displayName="Table15" ref="A1:H100" totalsRowShown="0" headerRowDxfId="13">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{646C4EC7-41A3-4570-9D38-06D55FDE20F6}" name="Table15" displayName="Table15" ref="A1:H100" totalsRowShown="0" headerRowDxfId="16">
   <autoFilter ref="A1:H100" xr:uid="{646C4EC7-41A3-4570-9D38-06D55FDE20F6}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
@@ -510,21 +560,21 @@
     <filterColumn colId="7" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="8">
-    <tableColumn id="1" xr3:uid="{13D6CE41-CF73-478C-B7F6-3B0C25C48DFD}" name="Date" dataDxfId="12"/>
-    <tableColumn id="2" xr3:uid="{E468B109-F9F1-48D8-BECE-0F7015DD8D95}" name="Member Name" dataDxfId="11"/>
+    <tableColumn id="1" xr3:uid="{13D6CE41-CF73-478C-B7F6-3B0C25C48DFD}" name="Date" dataDxfId="15"/>
+    <tableColumn id="2" xr3:uid="{E468B109-F9F1-48D8-BECE-0F7015DD8D95}" name="Member Name" dataDxfId="14"/>
     <tableColumn id="3" xr3:uid="{279E5366-E900-45EE-80D9-5446A85E61AD}" name="Task/Activity"/>
     <tableColumn id="4" xr3:uid="{63D996BE-E8E2-4186-8CD4-49EAB9AA8847}" name="Status"/>
-    <tableColumn id="5" xr3:uid="{2FF82CF3-E17A-4896-9C9C-7339D28CD4A7}" name="% Complete" dataDxfId="10"/>
-    <tableColumn id="6" xr3:uid="{67DCB379-6881-4BBC-A633-BD51853A9B6B}" name="Hours Worked Today" dataDxfId="9"/>
-    <tableColumn id="7" xr3:uid="{91C8F225-F251-45F2-BC41-843547B77A6F}" name="Next Steps" dataDxfId="8"/>
-    <tableColumn id="8" xr3:uid="{EEAB1D68-5668-4B1F-8473-D3A49DA7E015}" name="Notes/Comments" dataDxfId="7"/>
+    <tableColumn id="5" xr3:uid="{2FF82CF3-E17A-4896-9C9C-7339D28CD4A7}" name="% Complete" dataDxfId="13"/>
+    <tableColumn id="6" xr3:uid="{67DCB379-6881-4BBC-A633-BD51853A9B6B}" name="Hours Worked Today" dataDxfId="12"/>
+    <tableColumn id="7" xr3:uid="{91C8F225-F251-45F2-BC41-843547B77A6F}" name="Next Steps" dataDxfId="11"/>
+    <tableColumn id="8" xr3:uid="{EEAB1D68-5668-4B1F-8473-D3A49DA7E015}" name="Notes/Comments" dataDxfId="10"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium26" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{5818BB59-8F2C-4810-A78D-CBC8FA25F524}" name="Table5" displayName="Table5" ref="A1:J100" totalsRowShown="0" headerRowDxfId="6">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{5818BB59-8F2C-4810-A78D-CBC8FA25F524}" name="Table5" displayName="Table5" ref="A1:J100" totalsRowShown="0" headerRowDxfId="9">
   <autoFilter ref="A1:J100" xr:uid="{5818BB59-8F2C-4810-A78D-CBC8FA25F524}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
@@ -538,16 +588,16 @@
     <filterColumn colId="9" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="10">
-    <tableColumn id="1" xr3:uid="{BC250DF1-329E-4733-8702-E009738E43CB}" name="Header" dataDxfId="5"/>
-    <tableColumn id="2" xr3:uid="{F6CCDA73-9A12-472B-A535-0F3DC2A5CF61}" name="Date Raised" dataDxfId="4"/>
+    <tableColumn id="1" xr3:uid="{BC250DF1-329E-4733-8702-E009738E43CB}" name="Header" dataDxfId="8"/>
+    <tableColumn id="2" xr3:uid="{F6CCDA73-9A12-472B-A535-0F3DC2A5CF61}" name="Date Raised" dataDxfId="7"/>
     <tableColumn id="3" xr3:uid="{2E3C7862-32AA-44B8-BCC3-2F9299A8F3DC}" name="Raised By"/>
-    <tableColumn id="4" xr3:uid="{FB9438A9-92FB-4A8D-95A5-F17D6EF9AA82}" name="Issue Description" dataDxfId="3"/>
+    <tableColumn id="4" xr3:uid="{FB9438A9-92FB-4A8D-95A5-F17D6EF9AA82}" name="Issue Description" dataDxfId="6"/>
     <tableColumn id="5" xr3:uid="{48223256-C4C0-467B-9FA7-AA8E7742B58A}" name="Impact"/>
     <tableColumn id="6" xr3:uid="{EEDBAAB2-0361-4BF5-8FDB-3FAD49E87C1B}" name="Priority"/>
     <tableColumn id="7" xr3:uid="{515F6321-7FC0-4B4E-A422-3A0E332B7B97}" name="Status"/>
-    <tableColumn id="8" xr3:uid="{60A704D7-818B-442C-91EF-B82765B2618D}" name="Resolution Plan" dataDxfId="2"/>
-    <tableColumn id="9" xr3:uid="{D95E2A6F-E7D4-4FC5-9AAF-1E3DBEE8D8FC}" name="Date Resolved" dataDxfId="1"/>
-    <tableColumn id="10" xr3:uid="{D43B4A1C-AE3D-43D4-A514-7BAA3E281FD3}" name="Notes/Comments" dataDxfId="0"/>
+    <tableColumn id="8" xr3:uid="{60A704D7-818B-442C-91EF-B82765B2618D}" name="Resolution Plan" dataDxfId="5"/>
+    <tableColumn id="9" xr3:uid="{D95E2A6F-E7D4-4FC5-9AAF-1E3DBEE8D8FC}" name="Date Resolved" dataDxfId="4"/>
+    <tableColumn id="10" xr3:uid="{D43B4A1C-AE3D-43D4-A514-7BAA3E281FD3}" name="Notes/Comments" dataDxfId="3"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight15" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -901,30 +951,30 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{37EAA098-74C6-4411-B7E2-26AD2DCBC3F0}">
   <dimension ref="A1:H28"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H7" sqref="H7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col min="1" max="1" width="10.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.5703125" style="2" customWidth="1"/>
+    <col min="1" max="1" width="10.3984375" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.59765625" style="2" customWidth="1"/>
     <col min="3" max="3" width="58" customWidth="1"/>
-    <col min="5" max="5" width="13.140625" style="3" customWidth="1"/>
-    <col min="6" max="6" width="20.85546875" style="4" customWidth="1"/>
-    <col min="7" max="7" width="34.85546875" style="2" customWidth="1"/>
-    <col min="8" max="8" width="43.42578125" style="2" customWidth="1"/>
-    <col min="11" max="11" width="9.140625" customWidth="1"/>
-    <col min="12" max="12" width="13.28515625" customWidth="1"/>
-    <col min="13" max="13" width="11.42578125" customWidth="1"/>
-    <col min="14" max="14" width="17.42578125" customWidth="1"/>
-    <col min="16" max="16" width="9.140625" customWidth="1"/>
-    <col min="18" max="18" width="16.5703125" customWidth="1"/>
-    <col min="19" max="19" width="14.7109375" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="16.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.09765625" style="3" customWidth="1"/>
+    <col min="6" max="6" width="20.8984375" style="4" customWidth="1"/>
+    <col min="7" max="7" width="34.8984375" style="2" customWidth="1"/>
+    <col min="8" max="8" width="43.3984375" style="2" customWidth="1"/>
+    <col min="11" max="11" width="9.09765625" customWidth="1"/>
+    <col min="12" max="12" width="13.296875" customWidth="1"/>
+    <col min="13" max="13" width="11.3984375" customWidth="1"/>
+    <col min="14" max="14" width="17.3984375" customWidth="1"/>
+    <col min="16" max="16" width="9.09765625" customWidth="1"/>
+    <col min="18" max="18" width="16.59765625" customWidth="1"/>
+    <col min="19" max="19" width="14.69921875" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="16.8984375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" ht="15.75">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
@@ -950,7 +1000,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="15.75" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:8" ht="15.75">
       <c r="A2" s="1">
         <v>45786</v>
       </c>
@@ -976,7 +1026,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="3" spans="1:8" ht="120" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" ht="120">
       <c r="A3" s="1">
         <v>45787</v>
       </c>
@@ -999,7 +1049,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" ht="15">
       <c r="A4" s="1">
         <v>45788</v>
       </c>
@@ -1019,7 +1069,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="5" spans="1:8" ht="76.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" ht="76.5" customHeight="1">
       <c r="A5" s="1">
         <v>45789</v>
       </c>
@@ -1042,7 +1092,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" ht="15">
       <c r="A6" s="1">
         <v>45790</v>
       </c>
@@ -1065,7 +1115,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8">
       <c r="A7" s="1">
         <v>45791</v>
       </c>
@@ -1088,76 +1138,76 @@
         <v>34</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" ht="15">
       <c r="E8"/>
       <c r="F8"/>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" ht="15">
       <c r="E9"/>
       <c r="F9"/>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" ht="15">
       <c r="E10"/>
       <c r="F10"/>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" ht="15">
       <c r="E11"/>
       <c r="F11"/>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8" ht="15">
       <c r="E12"/>
       <c r="F12"/>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8" ht="15">
       <c r="E13"/>
       <c r="F13"/>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8" ht="15">
       <c r="E14"/>
       <c r="F14"/>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8">
       <c r="E15"/>
       <c r="F15"/>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8">
       <c r="E16"/>
       <c r="F16"/>
     </row>
-    <row r="17" spans="6:6" x14ac:dyDescent="0.25">
+    <row r="17" spans="6:6">
       <c r="F17"/>
     </row>
-    <row r="18" spans="6:6" x14ac:dyDescent="0.25">
+    <row r="18" spans="6:6">
       <c r="F18"/>
     </row>
-    <row r="19" spans="6:6" x14ac:dyDescent="0.25">
+    <row r="19" spans="6:6">
       <c r="F19"/>
     </row>
-    <row r="20" spans="6:6" x14ac:dyDescent="0.25">
+    <row r="20" spans="6:6">
       <c r="F20"/>
     </row>
-    <row r="21" spans="6:6" x14ac:dyDescent="0.25">
+    <row r="21" spans="6:6">
       <c r="F21"/>
     </row>
-    <row r="22" spans="6:6" x14ac:dyDescent="0.25">
+    <row r="22" spans="6:6">
       <c r="F22"/>
     </row>
-    <row r="23" spans="6:6" x14ac:dyDescent="0.25">
+    <row r="23" spans="6:6">
       <c r="F23"/>
     </row>
-    <row r="24" spans="6:6" x14ac:dyDescent="0.25">
+    <row r="24" spans="6:6">
       <c r="F24"/>
     </row>
-    <row r="25" spans="6:6" x14ac:dyDescent="0.25">
+    <row r="25" spans="6:6">
       <c r="F25"/>
     </row>
-    <row r="26" spans="6:6" x14ac:dyDescent="0.25">
+    <row r="26" spans="6:6">
       <c r="F26"/>
     </row>
-    <row r="27" spans="6:6" x14ac:dyDescent="0.25">
+    <row r="27" spans="6:6">
       <c r="F27"/>
     </row>
-    <row r="28" spans="6:6" x14ac:dyDescent="0.25">
+    <row r="28" spans="6:6">
       <c r="F28"/>
     </row>
   </sheetData>
@@ -1192,23 +1242,23 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3BDA6702-5DDF-42FB-988E-13FBEB26F5C9}">
   <dimension ref="A1:H100"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H2" sqref="H2"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col min="1" max="1" width="9.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="17.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.85546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="23.5703125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="13.42578125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="19.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.8984375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.296875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="55.59765625" customWidth="1"/>
+    <col min="4" max="4" width="10.59765625" customWidth="1"/>
+    <col min="5" max="5" width="14.8984375" style="11" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.296875" style="11" customWidth="1"/>
+    <col min="7" max="7" width="92.8984375" customWidth="1"/>
+    <col min="8" max="8" width="82.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" ht="15.75">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
@@ -1221,10 +1271,10 @@
       <c r="D1" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="7" t="s">
+      <c r="E1" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="7" t="s">
+      <c r="F1" s="10" t="s">
         <v>5</v>
       </c>
       <c r="G1" s="7" t="s">
@@ -1234,793 +1284,693 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A2" s="8"/>
-      <c r="B2" s="2"/>
-      <c r="E2" s="3"/>
-      <c r="G2" s="2"/>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A3" s="8"/>
-      <c r="B3" s="2"/>
-      <c r="E3" s="3"/>
-      <c r="F3" s="4"/>
-      <c r="G3" s="2"/>
-      <c r="H3" s="2"/>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A4" s="8"/>
-      <c r="B4" s="2"/>
-      <c r="E4" s="3"/>
-      <c r="F4" s="4"/>
-      <c r="G4" s="2"/>
+    <row r="2" spans="1:8" ht="15">
+      <c r="A2" s="8">
+        <v>45786</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="C2" t="s">
+        <v>36</v>
+      </c>
+      <c r="D2" t="s">
+        <v>37</v>
+      </c>
+      <c r="E2" s="11">
+        <v>90</v>
+      </c>
+      <c r="F2" s="11">
+        <v>8</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="H2" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" ht="15">
+      <c r="A3" s="8">
+        <v>45787</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="C3" t="s">
+        <v>40</v>
+      </c>
+      <c r="D3" t="s">
+        <v>37</v>
+      </c>
+      <c r="E3" s="11">
+        <v>90</v>
+      </c>
+      <c r="F3" s="11">
+        <v>8</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="H3" s="2" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" ht="15">
+      <c r="A4" s="8">
+        <v>45789</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="C4" t="s">
+        <v>43</v>
+      </c>
+      <c r="D4" t="s">
+        <v>37</v>
+      </c>
+      <c r="E4" s="11">
+        <v>90</v>
+      </c>
+      <c r="F4" s="11">
+        <v>5</v>
+      </c>
+      <c r="G4" s="2" t="s">
+        <v>44</v>
+      </c>
       <c r="H4" s="2"/>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A5" s="8"/>
-      <c r="B5" s="2"/>
-      <c r="E5" s="3"/>
-      <c r="F5" s="4"/>
-      <c r="G5" s="2"/>
+    <row r="5" spans="1:8" ht="15">
+      <c r="A5" s="8">
+        <v>45790</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="C5" t="s">
+        <v>46</v>
+      </c>
+      <c r="D5" t="s">
+        <v>17</v>
+      </c>
+      <c r="E5" s="11">
+        <v>100</v>
+      </c>
+      <c r="F5" s="11">
+        <v>5</v>
+      </c>
+      <c r="G5" s="2" t="s">
+        <v>47</v>
+      </c>
       <c r="H5" s="2"/>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A6" s="8"/>
-      <c r="B6" s="2"/>
-      <c r="E6" s="3"/>
-      <c r="F6" s="4"/>
-      <c r="G6" s="2"/>
-      <c r="H6" s="2"/>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" ht="15">
+      <c r="A6" s="8">
+        <v>45791</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="C6" t="s">
+        <v>48</v>
+      </c>
+      <c r="D6" t="s">
+        <v>17</v>
+      </c>
+      <c r="E6" s="11">
+        <v>100</v>
+      </c>
+      <c r="F6" s="11">
+        <v>5</v>
+      </c>
+      <c r="G6" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="H6" s="2" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" ht="15">
       <c r="A7" s="8"/>
       <c r="B7" s="2"/>
-      <c r="E7" s="3"/>
-      <c r="F7" s="4"/>
       <c r="G7" s="2"/>
       <c r="H7" s="2"/>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" ht="15">
       <c r="A8" s="8"/>
       <c r="B8" s="2"/>
-      <c r="E8" s="3"/>
-      <c r="F8" s="4"/>
       <c r="G8" s="2"/>
       <c r="H8" s="2"/>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" ht="15">
       <c r="A9" s="8"/>
       <c r="B9" s="2"/>
-      <c r="E9" s="3"/>
-      <c r="F9" s="4"/>
       <c r="G9" s="2"/>
       <c r="H9" s="2"/>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" ht="15">
       <c r="A10" s="8"/>
       <c r="B10" s="2"/>
-      <c r="E10" s="3"/>
-      <c r="F10" s="4"/>
       <c r="G10" s="2"/>
       <c r="H10" s="2"/>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" ht="15">
       <c r="A11" s="8"/>
       <c r="B11" s="2"/>
-      <c r="E11" s="3"/>
-      <c r="F11" s="4"/>
       <c r="G11" s="2"/>
       <c r="H11" s="2"/>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8" ht="15">
       <c r="A12" s="8"/>
       <c r="B12" s="2"/>
-      <c r="E12" s="3"/>
-      <c r="F12" s="4"/>
       <c r="G12" s="2"/>
       <c r="H12" s="2"/>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8" ht="15">
       <c r="A13" s="8"/>
       <c r="B13" s="2"/>
-      <c r="E13" s="3"/>
-      <c r="F13" s="4"/>
       <c r="G13" s="2"/>
       <c r="H13" s="2"/>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8" ht="15">
       <c r="A14" s="8"/>
       <c r="B14" s="2"/>
-      <c r="E14" s="3"/>
-      <c r="F14" s="4"/>
       <c r="G14" s="2"/>
       <c r="H14" s="2"/>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8" ht="15">
       <c r="A15" s="8"/>
       <c r="B15" s="2"/>
-      <c r="E15" s="3"/>
-      <c r="F15" s="4"/>
       <c r="G15" s="2"/>
       <c r="H15" s="2"/>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8" ht="15">
       <c r="A16" s="8"/>
       <c r="B16" s="2"/>
-      <c r="E16" s="3"/>
-      <c r="F16" s="4"/>
       <c r="G16" s="2"/>
       <c r="H16" s="2"/>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:8" ht="15">
       <c r="A17" s="8"/>
       <c r="B17" s="2"/>
-      <c r="E17" s="3"/>
-      <c r="F17" s="4"/>
       <c r="G17" s="2"/>
       <c r="H17" s="2"/>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:8" ht="15">
       <c r="A18" s="8"/>
       <c r="B18" s="2"/>
-      <c r="E18" s="3"/>
-      <c r="F18" s="4"/>
       <c r="G18" s="2"/>
       <c r="H18" s="2"/>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:8" ht="15">
       <c r="A19" s="8"/>
       <c r="B19" s="2"/>
-      <c r="E19" s="3"/>
-      <c r="F19" s="4"/>
       <c r="G19" s="2"/>
       <c r="H19" s="2"/>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:8" ht="15">
       <c r="A20" s="8"/>
       <c r="B20" s="2"/>
-      <c r="E20" s="3"/>
-      <c r="F20" s="4"/>
       <c r="G20" s="2"/>
       <c r="H20" s="2"/>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:8" ht="15">
       <c r="A21" s="8"/>
       <c r="B21" s="2"/>
-      <c r="E21" s="3"/>
-      <c r="F21" s="4"/>
       <c r="G21" s="2"/>
       <c r="H21" s="2"/>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:8" ht="15">
       <c r="A22" s="8"/>
       <c r="B22" s="2"/>
-      <c r="E22" s="3"/>
-      <c r="F22" s="4"/>
       <c r="G22" s="2"/>
       <c r="H22" s="2"/>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:8" ht="15">
       <c r="A23" s="8"/>
       <c r="B23" s="2"/>
-      <c r="E23" s="3"/>
-      <c r="F23" s="4"/>
       <c r="G23" s="2"/>
       <c r="H23" s="2"/>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:8" ht="15">
       <c r="A24" s="8"/>
       <c r="B24" s="2"/>
-      <c r="E24" s="3"/>
-      <c r="F24" s="4"/>
       <c r="G24" s="2"/>
       <c r="H24" s="2"/>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:8" ht="15">
       <c r="A25" s="8"/>
       <c r="B25" s="2"/>
-      <c r="E25" s="3"/>
-      <c r="F25" s="4"/>
       <c r="G25" s="2"/>
       <c r="H25" s="2"/>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:8">
       <c r="A26" s="8"/>
       <c r="B26" s="2"/>
-      <c r="E26" s="3"/>
-      <c r="F26" s="4"/>
       <c r="G26" s="2"/>
       <c r="H26" s="2"/>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:8">
       <c r="A27" s="8"/>
       <c r="B27" s="2"/>
-      <c r="E27" s="3"/>
-      <c r="F27" s="4"/>
       <c r="G27" s="2"/>
       <c r="H27" s="2"/>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:8">
       <c r="A28" s="8"/>
       <c r="B28" s="2"/>
-      <c r="E28" s="3"/>
-      <c r="F28" s="4"/>
       <c r="G28" s="2"/>
       <c r="H28" s="2"/>
     </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:8">
       <c r="A29" s="8"/>
       <c r="B29" s="2"/>
-      <c r="E29" s="3"/>
-      <c r="F29" s="4"/>
       <c r="G29" s="2"/>
       <c r="H29" s="2"/>
     </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:8">
       <c r="A30" s="8"/>
       <c r="B30" s="2"/>
-      <c r="E30" s="3"/>
-      <c r="F30" s="4"/>
       <c r="G30" s="2"/>
       <c r="H30" s="2"/>
     </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:8">
       <c r="A31" s="8"/>
       <c r="B31" s="2"/>
-      <c r="E31" s="3"/>
-      <c r="F31" s="4"/>
       <c r="G31" s="2"/>
       <c r="H31" s="2"/>
     </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:8">
       <c r="A32" s="8"/>
       <c r="B32" s="2"/>
-      <c r="E32" s="3"/>
-      <c r="F32" s="4"/>
       <c r="G32" s="2"/>
       <c r="H32" s="2"/>
     </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:8">
       <c r="A33" s="8"/>
       <c r="B33" s="2"/>
-      <c r="E33" s="3"/>
-      <c r="F33" s="4"/>
       <c r="G33" s="2"/>
       <c r="H33" s="2"/>
     </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:8">
       <c r="A34" s="8"/>
       <c r="B34" s="2"/>
-      <c r="E34" s="3"/>
-      <c r="F34" s="4"/>
       <c r="G34" s="2"/>
       <c r="H34" s="2"/>
     </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:8">
       <c r="A35" s="8"/>
       <c r="B35" s="2"/>
-      <c r="E35" s="3"/>
-      <c r="F35" s="4"/>
       <c r="G35" s="2"/>
       <c r="H35" s="2"/>
     </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:8">
       <c r="A36" s="8"/>
       <c r="B36" s="2"/>
-      <c r="E36" s="3"/>
-      <c r="F36" s="4"/>
       <c r="G36" s="2"/>
       <c r="H36" s="2"/>
     </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:8">
       <c r="A37" s="8"/>
       <c r="B37" s="2"/>
-      <c r="E37" s="3"/>
-      <c r="F37" s="4"/>
       <c r="G37" s="2"/>
       <c r="H37" s="2"/>
     </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:8">
       <c r="A38" s="8"/>
       <c r="B38" s="2"/>
-      <c r="E38" s="3"/>
-      <c r="F38" s="4"/>
       <c r="G38" s="2"/>
       <c r="H38" s="2"/>
     </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:8">
       <c r="A39" s="8"/>
       <c r="B39" s="2"/>
-      <c r="E39" s="3"/>
-      <c r="F39" s="4"/>
       <c r="G39" s="2"/>
       <c r="H39" s="2"/>
     </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:8">
       <c r="A40" s="8"/>
       <c r="B40" s="2"/>
-      <c r="E40" s="3"/>
-      <c r="F40" s="4"/>
       <c r="G40" s="2"/>
       <c r="H40" s="2"/>
     </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:8">
       <c r="A41" s="8"/>
       <c r="B41" s="2"/>
-      <c r="E41" s="3"/>
-      <c r="F41" s="4"/>
       <c r="G41" s="2"/>
       <c r="H41" s="2"/>
     </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:8">
       <c r="A42" s="8"/>
       <c r="B42" s="2"/>
-      <c r="E42" s="3"/>
-      <c r="F42" s="4"/>
       <c r="G42" s="2"/>
       <c r="H42" s="2"/>
     </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:8">
       <c r="A43" s="8"/>
       <c r="B43" s="2"/>
-      <c r="E43" s="3"/>
-      <c r="F43" s="4"/>
       <c r="G43" s="2"/>
       <c r="H43" s="2"/>
     </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:8">
       <c r="A44" s="8"/>
       <c r="B44" s="2"/>
-      <c r="E44" s="3"/>
-      <c r="F44" s="4"/>
       <c r="G44" s="2"/>
       <c r="H44" s="2"/>
     </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:8">
       <c r="A45" s="8"/>
       <c r="B45" s="2"/>
-      <c r="E45" s="3"/>
-      <c r="F45" s="4"/>
       <c r="G45" s="2"/>
       <c r="H45" s="2"/>
     </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:8">
       <c r="A46" s="8"/>
       <c r="B46" s="2"/>
-      <c r="E46" s="3"/>
-      <c r="F46" s="4"/>
       <c r="G46" s="2"/>
       <c r="H46" s="2"/>
     </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:8">
       <c r="A47" s="8"/>
       <c r="B47" s="2"/>
-      <c r="E47" s="3"/>
-      <c r="F47" s="4"/>
       <c r="G47" s="2"/>
       <c r="H47" s="2"/>
     </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:8">
       <c r="A48" s="8"/>
       <c r="B48" s="2"/>
-      <c r="E48" s="3"/>
-      <c r="F48" s="4"/>
       <c r="G48" s="2"/>
       <c r="H48" s="2"/>
     </row>
-    <row r="49" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:8">
       <c r="A49" s="8"/>
       <c r="B49" s="2"/>
-      <c r="E49" s="3"/>
-      <c r="F49" s="4"/>
       <c r="G49" s="2"/>
       <c r="H49" s="2"/>
     </row>
-    <row r="50" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:8">
       <c r="A50" s="8"/>
       <c r="B50" s="2"/>
-      <c r="E50" s="3"/>
-      <c r="F50" s="4"/>
       <c r="G50" s="2"/>
       <c r="H50" s="2"/>
     </row>
-    <row r="51" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:8">
       <c r="A51" s="8"/>
       <c r="B51" s="2"/>
-      <c r="E51" s="3"/>
-      <c r="F51" s="4"/>
       <c r="G51" s="2"/>
       <c r="H51" s="2"/>
     </row>
-    <row r="52" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:8">
       <c r="A52" s="8"/>
       <c r="B52" s="2"/>
-      <c r="E52" s="3"/>
-      <c r="F52" s="4"/>
       <c r="G52" s="2"/>
       <c r="H52" s="2"/>
     </row>
-    <row r="53" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:8">
       <c r="A53" s="8"/>
       <c r="B53" s="2"/>
-      <c r="E53" s="3"/>
-      <c r="F53" s="4"/>
       <c r="G53" s="2"/>
       <c r="H53" s="2"/>
     </row>
-    <row r="54" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:8">
       <c r="A54" s="8"/>
       <c r="B54" s="2"/>
-      <c r="E54" s="3"/>
-      <c r="F54" s="4"/>
       <c r="G54" s="2"/>
       <c r="H54" s="2"/>
     </row>
-    <row r="55" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:8">
       <c r="A55" s="8"/>
       <c r="B55" s="2"/>
-      <c r="E55" s="3"/>
-      <c r="F55" s="4"/>
       <c r="G55" s="2"/>
       <c r="H55" s="2"/>
     </row>
-    <row r="56" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:8">
       <c r="A56" s="8"/>
       <c r="B56" s="2"/>
-      <c r="E56" s="3"/>
-      <c r="F56" s="4"/>
       <c r="G56" s="2"/>
       <c r="H56" s="2"/>
     </row>
-    <row r="57" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:8">
       <c r="A57" s="8"/>
       <c r="B57" s="2"/>
-      <c r="E57" s="3"/>
-      <c r="F57" s="4"/>
       <c r="G57" s="2"/>
       <c r="H57" s="2"/>
     </row>
-    <row r="58" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:8">
       <c r="A58" s="8"/>
       <c r="B58" s="2"/>
-      <c r="E58" s="3"/>
-      <c r="F58" s="4"/>
       <c r="G58" s="2"/>
       <c r="H58" s="2"/>
     </row>
-    <row r="59" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:8">
       <c r="A59" s="8"/>
       <c r="B59" s="2"/>
-      <c r="E59" s="3"/>
-      <c r="F59" s="4"/>
       <c r="G59" s="2"/>
       <c r="H59" s="2"/>
     </row>
-    <row r="60" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:8">
       <c r="A60" s="8"/>
       <c r="B60" s="2"/>
-      <c r="E60" s="3"/>
-      <c r="F60" s="4"/>
       <c r="G60" s="2"/>
       <c r="H60" s="2"/>
     </row>
-    <row r="61" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:8">
       <c r="A61" s="8"/>
       <c r="B61" s="2"/>
-      <c r="E61" s="3"/>
-      <c r="F61" s="4"/>
       <c r="G61" s="2"/>
       <c r="H61" s="2"/>
     </row>
-    <row r="62" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:8">
       <c r="A62" s="8"/>
       <c r="B62" s="2"/>
-      <c r="E62" s="3"/>
-      <c r="F62" s="4"/>
       <c r="G62" s="2"/>
       <c r="H62" s="2"/>
     </row>
-    <row r="63" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:8">
       <c r="A63" s="8"/>
       <c r="B63" s="2"/>
-      <c r="E63" s="3"/>
-      <c r="F63" s="4"/>
       <c r="G63" s="2"/>
       <c r="H63" s="2"/>
     </row>
-    <row r="64" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:8">
       <c r="A64" s="8"/>
       <c r="B64" s="2"/>
-      <c r="E64" s="3"/>
-      <c r="F64" s="4"/>
       <c r="G64" s="2"/>
       <c r="H64" s="2"/>
     </row>
-    <row r="65" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:8">
       <c r="A65" s="8"/>
       <c r="B65" s="2"/>
-      <c r="E65" s="3"/>
-      <c r="F65" s="4"/>
       <c r="G65" s="2"/>
       <c r="H65" s="2"/>
     </row>
-    <row r="66" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:8">
       <c r="A66" s="8"/>
       <c r="B66" s="2"/>
-      <c r="E66" s="3"/>
-      <c r="F66" s="4"/>
       <c r="G66" s="2"/>
       <c r="H66" s="2"/>
     </row>
-    <row r="67" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:8">
       <c r="A67" s="8"/>
       <c r="B67" s="2"/>
-      <c r="E67" s="3"/>
-      <c r="F67" s="4"/>
       <c r="G67" s="2"/>
       <c r="H67" s="2"/>
     </row>
-    <row r="68" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:8">
       <c r="A68" s="8"/>
       <c r="B68" s="2"/>
-      <c r="E68" s="3"/>
-      <c r="F68" s="4"/>
       <c r="G68" s="2"/>
       <c r="H68" s="2"/>
     </row>
-    <row r="69" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:8">
       <c r="A69" s="8"/>
       <c r="B69" s="2"/>
-      <c r="E69" s="3"/>
-      <c r="F69" s="4"/>
       <c r="G69" s="2"/>
       <c r="H69" s="2"/>
     </row>
-    <row r="70" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:8">
       <c r="A70" s="8"/>
       <c r="B70" s="2"/>
-      <c r="E70" s="3"/>
-      <c r="F70" s="4"/>
       <c r="G70" s="2"/>
       <c r="H70" s="2"/>
     </row>
-    <row r="71" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:8">
       <c r="A71" s="8"/>
       <c r="B71" s="2"/>
-      <c r="E71" s="3"/>
-      <c r="F71" s="4"/>
       <c r="G71" s="2"/>
       <c r="H71" s="2"/>
     </row>
-    <row r="72" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:8">
       <c r="A72" s="8"/>
       <c r="B72" s="2"/>
-      <c r="E72" s="3"/>
-      <c r="F72" s="4"/>
       <c r="G72" s="2"/>
       <c r="H72" s="2"/>
     </row>
-    <row r="73" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:8">
       <c r="A73" s="8"/>
       <c r="B73" s="2"/>
-      <c r="E73" s="3"/>
-      <c r="F73" s="4"/>
       <c r="G73" s="2"/>
       <c r="H73" s="2"/>
     </row>
-    <row r="74" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:8">
       <c r="A74" s="8"/>
       <c r="B74" s="2"/>
-      <c r="E74" s="3"/>
-      <c r="F74" s="4"/>
       <c r="G74" s="2"/>
       <c r="H74" s="2"/>
     </row>
-    <row r="75" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:8">
       <c r="A75" s="8"/>
       <c r="B75" s="2"/>
-      <c r="E75" s="3"/>
-      <c r="F75" s="4"/>
       <c r="G75" s="2"/>
       <c r="H75" s="2"/>
     </row>
-    <row r="76" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:8">
       <c r="A76" s="8"/>
       <c r="B76" s="2"/>
-      <c r="E76" s="3"/>
-      <c r="F76" s="4"/>
       <c r="G76" s="2"/>
       <c r="H76" s="2"/>
     </row>
-    <row r="77" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:8">
       <c r="A77" s="8"/>
       <c r="B77" s="2"/>
-      <c r="E77" s="3"/>
-      <c r="F77" s="4"/>
       <c r="G77" s="2"/>
       <c r="H77" s="2"/>
     </row>
-    <row r="78" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:8">
       <c r="A78" s="8"/>
       <c r="B78" s="2"/>
-      <c r="E78" s="3"/>
-      <c r="F78" s="4"/>
       <c r="G78" s="2"/>
       <c r="H78" s="2"/>
     </row>
-    <row r="79" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:8">
       <c r="A79" s="8"/>
       <c r="B79" s="2"/>
-      <c r="E79" s="3"/>
-      <c r="F79" s="4"/>
       <c r="G79" s="2"/>
       <c r="H79" s="2"/>
     </row>
-    <row r="80" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:8">
       <c r="A80" s="8"/>
       <c r="B80" s="2"/>
-      <c r="E80" s="3"/>
-      <c r="F80" s="4"/>
       <c r="G80" s="2"/>
       <c r="H80" s="2"/>
     </row>
-    <row r="81" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:8">
       <c r="A81" s="8"/>
       <c r="B81" s="2"/>
-      <c r="E81" s="3"/>
-      <c r="F81" s="4"/>
       <c r="G81" s="2"/>
       <c r="H81" s="2"/>
     </row>
-    <row r="82" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:8">
       <c r="A82" s="8"/>
       <c r="B82" s="2"/>
-      <c r="E82" s="3"/>
-      <c r="F82" s="4"/>
       <c r="G82" s="2"/>
       <c r="H82" s="2"/>
     </row>
-    <row r="83" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:8">
       <c r="A83" s="8"/>
       <c r="B83" s="2"/>
-      <c r="E83" s="3"/>
-      <c r="F83" s="4"/>
       <c r="G83" s="2"/>
       <c r="H83" s="2"/>
     </row>
-    <row r="84" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:8">
       <c r="A84" s="8"/>
       <c r="B84" s="2"/>
-      <c r="E84" s="3"/>
-      <c r="F84" s="4"/>
       <c r="G84" s="2"/>
       <c r="H84" s="2"/>
     </row>
-    <row r="85" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:8">
       <c r="A85" s="8"/>
       <c r="B85" s="2"/>
-      <c r="E85" s="3"/>
-      <c r="F85" s="4"/>
       <c r="G85" s="2"/>
       <c r="H85" s="2"/>
     </row>
-    <row r="86" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:8">
       <c r="A86" s="8"/>
       <c r="B86" s="2"/>
-      <c r="E86" s="3"/>
-      <c r="F86" s="4"/>
       <c r="G86" s="2"/>
       <c r="H86" s="2"/>
     </row>
-    <row r="87" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:8">
       <c r="A87" s="8"/>
       <c r="B87" s="2"/>
-      <c r="E87" s="3"/>
-      <c r="F87" s="4"/>
       <c r="G87" s="2"/>
       <c r="H87" s="2"/>
     </row>
-    <row r="88" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:8">
       <c r="A88" s="8"/>
       <c r="B88" s="2"/>
-      <c r="E88" s="3"/>
-      <c r="F88" s="4"/>
       <c r="G88" s="2"/>
       <c r="H88" s="2"/>
     </row>
-    <row r="89" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:8">
       <c r="A89" s="8"/>
       <c r="B89" s="2"/>
-      <c r="E89" s="3"/>
-      <c r="F89" s="4"/>
       <c r="G89" s="2"/>
       <c r="H89" s="2"/>
     </row>
-    <row r="90" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:8">
       <c r="A90" s="8"/>
       <c r="B90" s="2"/>
-      <c r="E90" s="3"/>
-      <c r="F90" s="4"/>
       <c r="G90" s="2"/>
       <c r="H90" s="2"/>
     </row>
-    <row r="91" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:8">
       <c r="A91" s="8"/>
       <c r="B91" s="2"/>
-      <c r="E91" s="3"/>
-      <c r="F91" s="4"/>
       <c r="G91" s="2"/>
       <c r="H91" s="2"/>
     </row>
-    <row r="92" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:8">
       <c r="A92" s="8"/>
       <c r="B92" s="2"/>
-      <c r="E92" s="3"/>
-      <c r="F92" s="4"/>
       <c r="G92" s="2"/>
       <c r="H92" s="2"/>
     </row>
-    <row r="93" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:8">
       <c r="A93" s="8"/>
       <c r="B93" s="2"/>
-      <c r="E93" s="3"/>
-      <c r="F93" s="4"/>
       <c r="G93" s="2"/>
       <c r="H93" s="2"/>
     </row>
-    <row r="94" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:8">
       <c r="A94" s="8"/>
       <c r="B94" s="2"/>
-      <c r="E94" s="3"/>
-      <c r="F94" s="4"/>
       <c r="G94" s="2"/>
       <c r="H94" s="2"/>
     </row>
-    <row r="95" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:8">
       <c r="A95" s="8"/>
       <c r="B95" s="2"/>
-      <c r="E95" s="3"/>
-      <c r="F95" s="4"/>
       <c r="G95" s="2"/>
       <c r="H95" s="2"/>
     </row>
-    <row r="96" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:8">
       <c r="A96" s="8"/>
       <c r="B96" s="2"/>
-      <c r="E96" s="3"/>
-      <c r="F96" s="4"/>
       <c r="G96" s="2"/>
       <c r="H96" s="2"/>
     </row>
-    <row r="97" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:8">
       <c r="A97" s="8"/>
       <c r="B97" s="2"/>
-      <c r="E97" s="3"/>
-      <c r="F97" s="4"/>
       <c r="G97" s="2"/>
       <c r="H97" s="2"/>
     </row>
-    <row r="98" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:8">
       <c r="A98" s="8"/>
       <c r="B98" s="2"/>
-      <c r="E98" s="3"/>
-      <c r="F98" s="4"/>
       <c r="G98" s="2"/>
       <c r="H98" s="2"/>
     </row>
-    <row r="99" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:8">
       <c r="A99" s="8"/>
       <c r="B99" s="2"/>
-      <c r="E99" s="3"/>
-      <c r="F99" s="4"/>
       <c r="G99" s="2"/>
       <c r="H99" s="2"/>
     </row>
-    <row r="100" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:8">
       <c r="A100" s="8"/>
       <c r="B100" s="2"/>
-      <c r="E100" s="3"/>
-      <c r="F100" s="4"/>
       <c r="G100" s="2"/>
       <c r="H100" s="2"/>
     </row>
@@ -2043,7 +1993,7 @@
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <ignoredErrors>
-    <ignoredError sqref="D3:D100" listDataValidation="1"/>
+    <ignoredError sqref="D7:D100" listDataValidation="1"/>
   </ignoredErrors>
   <tableParts count="1">
     <tablePart r:id="rId1"/>
@@ -2059,19 +2009,19 @@
       <selection activeCell="D2" sqref="D2:D100"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col min="1" max="1" width="7.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="17.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="7.69921875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.296875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.59765625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="9" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.85546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="23.5703125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="13.42578125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="19.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.8984375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="23.59765625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.3984375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="19.09765625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" ht="15.75">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
@@ -2097,7 +2047,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" ht="15">
       <c r="A2" s="1"/>
       <c r="B2" s="2"/>
       <c r="E2" s="3"/>
@@ -2105,7 +2055,7 @@
       <c r="G2" s="2"/>
       <c r="H2" s="2"/>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" ht="15">
       <c r="A3" s="1"/>
       <c r="B3" s="2"/>
       <c r="E3" s="3"/>
@@ -2113,7 +2063,7 @@
       <c r="G3" s="2"/>
       <c r="H3" s="2"/>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" ht="15">
       <c r="A4" s="1"/>
       <c r="B4" s="2"/>
       <c r="E4" s="3"/>
@@ -2121,7 +2071,7 @@
       <c r="G4" s="2"/>
       <c r="H4" s="2"/>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" ht="15">
       <c r="A5" s="1"/>
       <c r="B5" s="2"/>
       <c r="E5" s="3"/>
@@ -2129,7 +2079,7 @@
       <c r="G5" s="2"/>
       <c r="H5" s="2"/>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" ht="15">
       <c r="A6" s="1"/>
       <c r="B6" s="2"/>
       <c r="E6" s="3"/>
@@ -2137,7 +2087,7 @@
       <c r="G6" s="2"/>
       <c r="H6" s="2"/>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" ht="15">
       <c r="A7" s="1"/>
       <c r="B7" s="2"/>
       <c r="E7" s="3"/>
@@ -2145,7 +2095,7 @@
       <c r="G7" s="2"/>
       <c r="H7" s="2"/>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" ht="15">
       <c r="A8" s="1"/>
       <c r="B8" s="2"/>
       <c r="E8" s="3"/>
@@ -2153,7 +2103,7 @@
       <c r="G8" s="2"/>
       <c r="H8" s="2"/>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" ht="15">
       <c r="A9" s="1"/>
       <c r="B9" s="2"/>
       <c r="E9" s="3"/>
@@ -2161,7 +2111,7 @@
       <c r="G9" s="2"/>
       <c r="H9" s="2"/>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" ht="15">
       <c r="A10" s="1"/>
       <c r="B10" s="2"/>
       <c r="E10" s="3"/>
@@ -2169,7 +2119,7 @@
       <c r="G10" s="2"/>
       <c r="H10" s="2"/>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" ht="15">
       <c r="A11" s="1"/>
       <c r="B11" s="2"/>
       <c r="E11" s="3"/>
@@ -2177,7 +2127,7 @@
       <c r="G11" s="2"/>
       <c r="H11" s="2"/>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8" ht="15">
       <c r="A12" s="1"/>
       <c r="B12" s="2"/>
       <c r="E12" s="3"/>
@@ -2185,7 +2135,7 @@
       <c r="G12" s="2"/>
       <c r="H12" s="2"/>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8" ht="15">
       <c r="A13" s="1"/>
       <c r="B13" s="2"/>
       <c r="E13" s="3"/>
@@ -2193,7 +2143,7 @@
       <c r="G13" s="2"/>
       <c r="H13" s="2"/>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8" ht="15">
       <c r="A14" s="1"/>
       <c r="B14" s="2"/>
       <c r="E14" s="3"/>
@@ -2201,7 +2151,7 @@
       <c r="G14" s="2"/>
       <c r="H14" s="2"/>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8" ht="15">
       <c r="A15" s="1"/>
       <c r="B15" s="2"/>
       <c r="E15" s="3"/>
@@ -2209,7 +2159,7 @@
       <c r="G15" s="2"/>
       <c r="H15" s="2"/>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8" ht="15">
       <c r="A16" s="1"/>
       <c r="B16" s="2"/>
       <c r="E16" s="3"/>
@@ -2217,7 +2167,7 @@
       <c r="G16" s="2"/>
       <c r="H16" s="2"/>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:8" ht="15">
       <c r="A17" s="1"/>
       <c r="B17" s="2"/>
       <c r="E17" s="3"/>
@@ -2225,7 +2175,7 @@
       <c r="G17" s="2"/>
       <c r="H17" s="2"/>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:8" ht="15">
       <c r="A18" s="1"/>
       <c r="B18" s="2"/>
       <c r="E18" s="3"/>
@@ -2233,7 +2183,7 @@
       <c r="G18" s="2"/>
       <c r="H18" s="2"/>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:8" ht="15">
       <c r="A19" s="1"/>
       <c r="B19" s="2"/>
       <c r="E19" s="3"/>
@@ -2241,7 +2191,7 @@
       <c r="G19" s="2"/>
       <c r="H19" s="2"/>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:8" ht="15">
       <c r="A20" s="1"/>
       <c r="B20" s="2"/>
       <c r="E20" s="3"/>
@@ -2249,7 +2199,7 @@
       <c r="G20" s="2"/>
       <c r="H20" s="2"/>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:8" ht="15">
       <c r="A21" s="1"/>
       <c r="B21" s="2"/>
       <c r="E21" s="3"/>
@@ -2257,7 +2207,7 @@
       <c r="G21" s="2"/>
       <c r="H21" s="2"/>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:8" ht="15">
       <c r="A22" s="1"/>
       <c r="B22" s="2"/>
       <c r="E22" s="3"/>
@@ -2265,7 +2215,7 @@
       <c r="G22" s="2"/>
       <c r="H22" s="2"/>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:8" ht="15">
       <c r="A23" s="1"/>
       <c r="B23" s="2"/>
       <c r="E23" s="3"/>
@@ -2273,7 +2223,7 @@
       <c r="G23" s="2"/>
       <c r="H23" s="2"/>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:8" ht="15">
       <c r="A24" s="1"/>
       <c r="B24" s="2"/>
       <c r="E24" s="3"/>
@@ -2281,7 +2231,7 @@
       <c r="G24" s="2"/>
       <c r="H24" s="2"/>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:8" ht="15">
       <c r="A25" s="1"/>
       <c r="B25" s="2"/>
       <c r="E25" s="3"/>
@@ -2289,7 +2239,7 @@
       <c r="G25" s="2"/>
       <c r="H25" s="2"/>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:8" ht="15">
       <c r="A26" s="1"/>
       <c r="B26" s="2"/>
       <c r="E26" s="3"/>
@@ -2297,7 +2247,7 @@
       <c r="G26" s="2"/>
       <c r="H26" s="2"/>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:8" ht="15">
       <c r="A27" s="1"/>
       <c r="B27" s="2"/>
       <c r="E27" s="3"/>
@@ -2305,7 +2255,7 @@
       <c r="G27" s="2"/>
       <c r="H27" s="2"/>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:8" ht="15">
       <c r="A28" s="1"/>
       <c r="B28" s="2"/>
       <c r="E28" s="3"/>
@@ -2313,7 +2263,7 @@
       <c r="G28" s="2"/>
       <c r="H28" s="2"/>
     </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:8" ht="15">
       <c r="A29" s="1"/>
       <c r="B29" s="2"/>
       <c r="E29" s="3"/>
@@ -2321,7 +2271,7 @@
       <c r="G29" s="2"/>
       <c r="H29" s="2"/>
     </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:8" ht="15">
       <c r="A30" s="1"/>
       <c r="B30" s="2"/>
       <c r="E30" s="3"/>
@@ -2329,7 +2279,7 @@
       <c r="G30" s="2"/>
       <c r="H30" s="2"/>
     </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:8" ht="15">
       <c r="A31" s="1"/>
       <c r="B31" s="2"/>
       <c r="E31" s="3"/>
@@ -2337,7 +2287,7 @@
       <c r="G31" s="2"/>
       <c r="H31" s="2"/>
     </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:8" ht="15">
       <c r="A32" s="1"/>
       <c r="B32" s="2"/>
       <c r="E32" s="3"/>
@@ -2345,7 +2295,7 @@
       <c r="G32" s="2"/>
       <c r="H32" s="2"/>
     </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:8" ht="15">
       <c r="A33" s="1"/>
       <c r="B33" s="2"/>
       <c r="E33" s="3"/>
@@ -2353,7 +2303,7 @@
       <c r="G33" s="2"/>
       <c r="H33" s="2"/>
     </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:8" ht="15">
       <c r="A34" s="1"/>
       <c r="B34" s="2"/>
       <c r="E34" s="3"/>
@@ -2361,7 +2311,7 @@
       <c r="G34" s="2"/>
       <c r="H34" s="2"/>
     </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:8" ht="15">
       <c r="A35" s="1"/>
       <c r="B35" s="2"/>
       <c r="E35" s="3"/>
@@ -2369,7 +2319,7 @@
       <c r="G35" s="2"/>
       <c r="H35" s="2"/>
     </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:8" ht="15">
       <c r="A36" s="1"/>
       <c r="B36" s="2"/>
       <c r="E36" s="3"/>
@@ -2377,7 +2327,7 @@
       <c r="G36" s="2"/>
       <c r="H36" s="2"/>
     </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:8" ht="15">
       <c r="A37" s="1"/>
       <c r="B37" s="2"/>
       <c r="E37" s="3"/>
@@ -2385,7 +2335,7 @@
       <c r="G37" s="2"/>
       <c r="H37" s="2"/>
     </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:8" ht="15">
       <c r="A38" s="1"/>
       <c r="B38" s="2"/>
       <c r="E38" s="3"/>
@@ -2393,7 +2343,7 @@
       <c r="G38" s="2"/>
       <c r="H38" s="2"/>
     </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:8" ht="15">
       <c r="A39" s="1"/>
       <c r="B39" s="2"/>
       <c r="E39" s="3"/>
@@ -2401,7 +2351,7 @@
       <c r="G39" s="2"/>
       <c r="H39" s="2"/>
     </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:8" ht="15">
       <c r="A40" s="1"/>
       <c r="B40" s="2"/>
       <c r="E40" s="3"/>
@@ -2409,7 +2359,7 @@
       <c r="G40" s="2"/>
       <c r="H40" s="2"/>
     </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:8" ht="15">
       <c r="A41" s="1"/>
       <c r="B41" s="2"/>
       <c r="E41" s="3"/>
@@ -2417,7 +2367,7 @@
       <c r="G41" s="2"/>
       <c r="H41" s="2"/>
     </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:8" ht="15">
       <c r="A42" s="1"/>
       <c r="B42" s="2"/>
       <c r="E42" s="3"/>
@@ -2425,7 +2375,7 @@
       <c r="G42" s="2"/>
       <c r="H42" s="2"/>
     </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:8" ht="15">
       <c r="A43" s="1"/>
       <c r="B43" s="2"/>
       <c r="E43" s="3"/>
@@ -2433,7 +2383,7 @@
       <c r="G43" s="2"/>
       <c r="H43" s="2"/>
     </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:8" ht="15">
       <c r="A44" s="1"/>
       <c r="B44" s="2"/>
       <c r="E44" s="3"/>
@@ -2441,7 +2391,7 @@
       <c r="G44" s="2"/>
       <c r="H44" s="2"/>
     </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:8" ht="15">
       <c r="A45" s="1"/>
       <c r="B45" s="2"/>
       <c r="E45" s="3"/>
@@ -2449,7 +2399,7 @@
       <c r="G45" s="2"/>
       <c r="H45" s="2"/>
     </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:8" ht="15">
       <c r="A46" s="1"/>
       <c r="B46" s="2"/>
       <c r="E46" s="3"/>
@@ -2457,7 +2407,7 @@
       <c r="G46" s="2"/>
       <c r="H46" s="2"/>
     </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:8" ht="15">
       <c r="A47" s="1"/>
       <c r="B47" s="2"/>
       <c r="E47" s="3"/>
@@ -2465,7 +2415,7 @@
       <c r="G47" s="2"/>
       <c r="H47" s="2"/>
     </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:8" ht="15">
       <c r="A48" s="1"/>
       <c r="B48" s="2"/>
       <c r="E48" s="3"/>
@@ -2473,7 +2423,7 @@
       <c r="G48" s="2"/>
       <c r="H48" s="2"/>
     </row>
-    <row r="49" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:8" ht="15">
       <c r="A49" s="1"/>
       <c r="B49" s="2"/>
       <c r="E49" s="3"/>
@@ -2481,7 +2431,7 @@
       <c r="G49" s="2"/>
       <c r="H49" s="2"/>
     </row>
-    <row r="50" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:8" ht="15">
       <c r="A50" s="1"/>
       <c r="B50" s="2"/>
       <c r="E50" s="3"/>
@@ -2489,7 +2439,7 @@
       <c r="G50" s="2"/>
       <c r="H50" s="2"/>
     </row>
-    <row r="51" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:8" ht="15">
       <c r="A51" s="1"/>
       <c r="B51" s="2"/>
       <c r="E51" s="3"/>
@@ -2497,7 +2447,7 @@
       <c r="G51" s="2"/>
       <c r="H51" s="2"/>
     </row>
-    <row r="52" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:8" ht="15">
       <c r="A52" s="1"/>
       <c r="B52" s="2"/>
       <c r="E52" s="3"/>
@@ -2505,7 +2455,7 @@
       <c r="G52" s="2"/>
       <c r="H52" s="2"/>
     </row>
-    <row r="53" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:8" ht="15">
       <c r="A53" s="1"/>
       <c r="B53" s="2"/>
       <c r="E53" s="3"/>
@@ -2513,7 +2463,7 @@
       <c r="G53" s="2"/>
       <c r="H53" s="2"/>
     </row>
-    <row r="54" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:8" ht="15">
       <c r="A54" s="1"/>
       <c r="B54" s="2"/>
       <c r="E54" s="3"/>
@@ -2521,7 +2471,7 @@
       <c r="G54" s="2"/>
       <c r="H54" s="2"/>
     </row>
-    <row r="55" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:8" ht="15">
       <c r="A55" s="1"/>
       <c r="B55" s="2"/>
       <c r="E55" s="3"/>
@@ -2529,7 +2479,7 @@
       <c r="G55" s="2"/>
       <c r="H55" s="2"/>
     </row>
-    <row r="56" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:8" ht="15">
       <c r="A56" s="1"/>
       <c r="B56" s="2"/>
       <c r="E56" s="3"/>
@@ -2537,7 +2487,7 @@
       <c r="G56" s="2"/>
       <c r="H56" s="2"/>
     </row>
-    <row r="57" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:8" ht="15">
       <c r="A57" s="1"/>
       <c r="B57" s="2"/>
       <c r="E57" s="3"/>
@@ -2545,7 +2495,7 @@
       <c r="G57" s="2"/>
       <c r="H57" s="2"/>
     </row>
-    <row r="58" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:8" ht="15">
       <c r="A58" s="1"/>
       <c r="B58" s="2"/>
       <c r="E58" s="3"/>
@@ -2553,7 +2503,7 @@
       <c r="G58" s="2"/>
       <c r="H58" s="2"/>
     </row>
-    <row r="59" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:8" ht="15">
       <c r="A59" s="1"/>
       <c r="B59" s="2"/>
       <c r="E59" s="3"/>
@@ -2561,7 +2511,7 @@
       <c r="G59" s="2"/>
       <c r="H59" s="2"/>
     </row>
-    <row r="60" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:8" ht="15">
       <c r="A60" s="1"/>
       <c r="B60" s="2"/>
       <c r="E60" s="3"/>
@@ -2569,7 +2519,7 @@
       <c r="G60" s="2"/>
       <c r="H60" s="2"/>
     </row>
-    <row r="61" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:8" ht="15">
       <c r="A61" s="1"/>
       <c r="B61" s="2"/>
       <c r="E61" s="3"/>
@@ -2577,7 +2527,7 @@
       <c r="G61" s="2"/>
       <c r="H61" s="2"/>
     </row>
-    <row r="62" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:8" ht="15">
       <c r="A62" s="1"/>
       <c r="B62" s="2"/>
       <c r="E62" s="3"/>
@@ -2585,7 +2535,7 @@
       <c r="G62" s="2"/>
       <c r="H62" s="2"/>
     </row>
-    <row r="63" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:8" ht="15">
       <c r="A63" s="1"/>
       <c r="B63" s="2"/>
       <c r="E63" s="3"/>
@@ -2593,7 +2543,7 @@
       <c r="G63" s="2"/>
       <c r="H63" s="2"/>
     </row>
-    <row r="64" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:8" ht="15">
       <c r="A64" s="1"/>
       <c r="B64" s="2"/>
       <c r="E64" s="3"/>
@@ -2601,7 +2551,7 @@
       <c r="G64" s="2"/>
       <c r="H64" s="2"/>
     </row>
-    <row r="65" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:8" ht="15">
       <c r="A65" s="1"/>
       <c r="B65" s="2"/>
       <c r="E65" s="3"/>
@@ -2609,7 +2559,7 @@
       <c r="G65" s="2"/>
       <c r="H65" s="2"/>
     </row>
-    <row r="66" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:8" ht="15">
       <c r="A66" s="1"/>
       <c r="B66" s="2"/>
       <c r="E66" s="3"/>
@@ -2617,7 +2567,7 @@
       <c r="G66" s="2"/>
       <c r="H66" s="2"/>
     </row>
-    <row r="67" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:8" ht="15">
       <c r="A67" s="1"/>
       <c r="B67" s="2"/>
       <c r="E67" s="3"/>
@@ -2625,7 +2575,7 @@
       <c r="G67" s="2"/>
       <c r="H67" s="2"/>
     </row>
-    <row r="68" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:8" ht="15">
       <c r="A68" s="1"/>
       <c r="B68" s="2"/>
       <c r="E68" s="3"/>
@@ -2633,7 +2583,7 @@
       <c r="G68" s="2"/>
       <c r="H68" s="2"/>
     </row>
-    <row r="69" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:8" ht="15">
       <c r="A69" s="1"/>
       <c r="B69" s="2"/>
       <c r="E69" s="3"/>
@@ -2641,7 +2591,7 @@
       <c r="G69" s="2"/>
       <c r="H69" s="2"/>
     </row>
-    <row r="70" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:8" ht="15">
       <c r="A70" s="1"/>
       <c r="B70" s="2"/>
       <c r="E70" s="3"/>
@@ -2649,7 +2599,7 @@
       <c r="G70" s="2"/>
       <c r="H70" s="2"/>
     </row>
-    <row r="71" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:8" ht="15">
       <c r="A71" s="1"/>
       <c r="B71" s="2"/>
       <c r="E71" s="3"/>
@@ -2657,7 +2607,7 @@
       <c r="G71" s="2"/>
       <c r="H71" s="2"/>
     </row>
-    <row r="72" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:8" ht="15">
       <c r="A72" s="1"/>
       <c r="B72" s="2"/>
       <c r="E72" s="3"/>
@@ -2665,7 +2615,7 @@
       <c r="G72" s="2"/>
       <c r="H72" s="2"/>
     </row>
-    <row r="73" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:8" ht="15">
       <c r="A73" s="1"/>
       <c r="B73" s="2"/>
       <c r="E73" s="3"/>
@@ -2673,7 +2623,7 @@
       <c r="G73" s="2"/>
       <c r="H73" s="2"/>
     </row>
-    <row r="74" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:8" ht="15">
       <c r="A74" s="1"/>
       <c r="B74" s="2"/>
       <c r="E74" s="3"/>
@@ -2681,7 +2631,7 @@
       <c r="G74" s="2"/>
       <c r="H74" s="2"/>
     </row>
-    <row r="75" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:8" ht="15">
       <c r="A75" s="1"/>
       <c r="B75" s="2"/>
       <c r="E75" s="3"/>
@@ -2689,7 +2639,7 @@
       <c r="G75" s="2"/>
       <c r="H75" s="2"/>
     </row>
-    <row r="76" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:8" ht="15">
       <c r="A76" s="1"/>
       <c r="B76" s="2"/>
       <c r="E76" s="3"/>
@@ -2697,7 +2647,7 @@
       <c r="G76" s="2"/>
       <c r="H76" s="2"/>
     </row>
-    <row r="77" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:8" ht="15">
       <c r="A77" s="1"/>
       <c r="B77" s="2"/>
       <c r="E77" s="3"/>
@@ -2705,7 +2655,7 @@
       <c r="G77" s="2"/>
       <c r="H77" s="2"/>
     </row>
-    <row r="78" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:8" ht="15">
       <c r="A78" s="1"/>
       <c r="B78" s="2"/>
       <c r="E78" s="3"/>
@@ -2713,7 +2663,7 @@
       <c r="G78" s="2"/>
       <c r="H78" s="2"/>
     </row>
-    <row r="79" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:8" ht="15">
       <c r="A79" s="1"/>
       <c r="B79" s="2"/>
       <c r="E79" s="3"/>
@@ -2721,7 +2671,7 @@
       <c r="G79" s="2"/>
       <c r="H79" s="2"/>
     </row>
-    <row r="80" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:8" ht="15">
       <c r="A80" s="1"/>
       <c r="B80" s="2"/>
       <c r="E80" s="3"/>
@@ -2729,7 +2679,7 @@
       <c r="G80" s="2"/>
       <c r="H80" s="2"/>
     </row>
-    <row r="81" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:8" ht="15">
       <c r="A81" s="1"/>
       <c r="B81" s="2"/>
       <c r="E81" s="3"/>
@@ -2737,7 +2687,7 @@
       <c r="G81" s="2"/>
       <c r="H81" s="2"/>
     </row>
-    <row r="82" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:8" ht="15">
       <c r="A82" s="1"/>
       <c r="B82" s="2"/>
       <c r="E82" s="3"/>
@@ -2745,7 +2695,7 @@
       <c r="G82" s="2"/>
       <c r="H82" s="2"/>
     </row>
-    <row r="83" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:8" ht="15">
       <c r="A83" s="1"/>
       <c r="B83" s="2"/>
       <c r="E83" s="3"/>
@@ -2753,7 +2703,7 @@
       <c r="G83" s="2"/>
       <c r="H83" s="2"/>
     </row>
-    <row r="84" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:8" ht="15">
       <c r="A84" s="1"/>
       <c r="B84" s="2"/>
       <c r="E84" s="3"/>
@@ -2761,7 +2711,7 @@
       <c r="G84" s="2"/>
       <c r="H84" s="2"/>
     </row>
-    <row r="85" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:8" ht="15">
       <c r="A85" s="1"/>
       <c r="B85" s="2"/>
       <c r="E85" s="3"/>
@@ -2769,7 +2719,7 @@
       <c r="G85" s="2"/>
       <c r="H85" s="2"/>
     </row>
-    <row r="86" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:8" ht="15">
       <c r="A86" s="1"/>
       <c r="B86" s="2"/>
       <c r="E86" s="3"/>
@@ -2777,7 +2727,7 @@
       <c r="G86" s="2"/>
       <c r="H86" s="2"/>
     </row>
-    <row r="87" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:8" ht="15">
       <c r="A87" s="1"/>
       <c r="B87" s="2"/>
       <c r="E87" s="3"/>
@@ -2785,7 +2735,7 @@
       <c r="G87" s="2"/>
       <c r="H87" s="2"/>
     </row>
-    <row r="88" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:8">
       <c r="A88" s="1"/>
       <c r="B88" s="2"/>
       <c r="E88" s="3"/>
@@ -2793,7 +2743,7 @@
       <c r="G88" s="2"/>
       <c r="H88" s="2"/>
     </row>
-    <row r="89" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:8">
       <c r="A89" s="1"/>
       <c r="B89" s="2"/>
       <c r="E89" s="3"/>
@@ -2801,7 +2751,7 @@
       <c r="G89" s="2"/>
       <c r="H89" s="2"/>
     </row>
-    <row r="90" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:8">
       <c r="A90" s="1"/>
       <c r="B90" s="2"/>
       <c r="E90" s="3"/>
@@ -2809,7 +2759,7 @@
       <c r="G90" s="2"/>
       <c r="H90" s="2"/>
     </row>
-    <row r="91" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:8">
       <c r="A91" s="1"/>
       <c r="B91" s="2"/>
       <c r="E91" s="3"/>
@@ -2817,7 +2767,7 @@
       <c r="G91" s="2"/>
       <c r="H91" s="2"/>
     </row>
-    <row r="92" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:8">
       <c r="A92" s="1"/>
       <c r="B92" s="2"/>
       <c r="E92" s="3"/>
@@ -2825,7 +2775,7 @@
       <c r="G92" s="2"/>
       <c r="H92" s="2"/>
     </row>
-    <row r="93" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:8">
       <c r="A93" s="1"/>
       <c r="B93" s="2"/>
       <c r="E93" s="3"/>
@@ -2833,7 +2783,7 @@
       <c r="G93" s="2"/>
       <c r="H93" s="2"/>
     </row>
-    <row r="94" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:8">
       <c r="A94" s="1"/>
       <c r="B94" s="2"/>
       <c r="E94" s="3"/>
@@ -2841,7 +2791,7 @@
       <c r="G94" s="2"/>
       <c r="H94" s="2"/>
     </row>
-    <row r="95" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:8">
       <c r="A95" s="1"/>
       <c r="B95" s="2"/>
       <c r="E95" s="3"/>
@@ -2849,7 +2799,7 @@
       <c r="G95" s="2"/>
       <c r="H95" s="2"/>
     </row>
-    <row r="96" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:8">
       <c r="A96" s="1"/>
       <c r="B96" s="2"/>
       <c r="E96" s="3"/>
@@ -2857,7 +2807,7 @@
       <c r="G96" s="2"/>
       <c r="H96" s="2"/>
     </row>
-    <row r="97" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:8">
       <c r="A97" s="1"/>
       <c r="B97" s="2"/>
       <c r="E97" s="3"/>
@@ -2865,7 +2815,7 @@
       <c r="G97" s="2"/>
       <c r="H97" s="2"/>
     </row>
-    <row r="98" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:8">
       <c r="A98" s="1"/>
       <c r="B98" s="2"/>
       <c r="E98" s="3"/>
@@ -2873,7 +2823,7 @@
       <c r="G98" s="2"/>
       <c r="H98" s="2"/>
     </row>
-    <row r="99" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:8">
       <c r="A99" s="1"/>
       <c r="B99" s="2"/>
       <c r="E99" s="3"/>
@@ -2881,7 +2831,7 @@
       <c r="G99" s="2"/>
       <c r="H99" s="2"/>
     </row>
-    <row r="100" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:8">
       <c r="A100" s="1"/>
       <c r="B100" s="2"/>
       <c r="E100" s="3"/>
@@ -2924,19 +2874,19 @@
       <selection activeCell="D2" sqref="D2:D100"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col min="1" max="1" width="7.7109375" customWidth="1"/>
-    <col min="2" max="2" width="17.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="7.69921875" customWidth="1"/>
+    <col min="2" max="2" width="17.296875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.59765625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="9" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.85546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="23.5703125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="13.42578125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="19.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.8984375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="23.59765625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.3984375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="19.09765625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" ht="15.75">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
@@ -2962,7 +2912,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" ht="15">
       <c r="A2" s="1"/>
       <c r="B2" s="2"/>
       <c r="E2" s="3"/>
@@ -2970,7 +2920,7 @@
       <c r="G2" s="2"/>
       <c r="H2" s="2"/>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" ht="15">
       <c r="A3" s="1"/>
       <c r="B3" s="2"/>
       <c r="E3" s="3"/>
@@ -2978,7 +2928,7 @@
       <c r="G3" s="2"/>
       <c r="H3" s="2"/>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" ht="15">
       <c r="A4" s="1"/>
       <c r="B4" s="2"/>
       <c r="E4" s="3"/>
@@ -2986,7 +2936,7 @@
       <c r="G4" s="2"/>
       <c r="H4" s="2"/>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" ht="15">
       <c r="A5" s="1"/>
       <c r="B5" s="2"/>
       <c r="E5" s="3"/>
@@ -2994,7 +2944,7 @@
       <c r="G5" s="2"/>
       <c r="H5" s="2"/>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" ht="15">
       <c r="A6" s="1"/>
       <c r="B6" s="2"/>
       <c r="E6" s="3"/>
@@ -3002,7 +2952,7 @@
       <c r="G6" s="2"/>
       <c r="H6" s="2"/>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" ht="15">
       <c r="A7" s="1"/>
       <c r="B7" s="2"/>
       <c r="E7" s="3"/>
@@ -3010,7 +2960,7 @@
       <c r="G7" s="2"/>
       <c r="H7" s="2"/>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" ht="15">
       <c r="A8" s="1"/>
       <c r="B8" s="2"/>
       <c r="E8" s="3"/>
@@ -3018,7 +2968,7 @@
       <c r="G8" s="2"/>
       <c r="H8" s="2"/>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" ht="15">
       <c r="A9" s="1"/>
       <c r="B9" s="2"/>
       <c r="E9" s="3"/>
@@ -3026,7 +2976,7 @@
       <c r="G9" s="2"/>
       <c r="H9" s="2"/>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" ht="15">
       <c r="A10" s="1"/>
       <c r="B10" s="2"/>
       <c r="E10" s="3"/>
@@ -3034,7 +2984,7 @@
       <c r="G10" s="2"/>
       <c r="H10" s="2"/>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" ht="15">
       <c r="A11" s="1"/>
       <c r="B11" s="2"/>
       <c r="E11" s="3"/>
@@ -3042,7 +2992,7 @@
       <c r="G11" s="2"/>
       <c r="H11" s="2"/>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8" ht="15">
       <c r="A12" s="1"/>
       <c r="B12" s="2"/>
       <c r="E12" s="3"/>
@@ -3050,7 +3000,7 @@
       <c r="G12" s="2"/>
       <c r="H12" s="2"/>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8" ht="15">
       <c r="A13" s="1"/>
       <c r="B13" s="2"/>
       <c r="E13" s="3"/>
@@ -3058,7 +3008,7 @@
       <c r="G13" s="2"/>
       <c r="H13" s="2"/>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8" ht="15">
       <c r="A14" s="1"/>
       <c r="B14" s="2"/>
       <c r="E14" s="3"/>
@@ -3066,7 +3016,7 @@
       <c r="G14" s="2"/>
       <c r="H14" s="2"/>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8" ht="15">
       <c r="A15" s="1"/>
       <c r="B15" s="2"/>
       <c r="E15" s="3"/>
@@ -3074,7 +3024,7 @@
       <c r="G15" s="2"/>
       <c r="H15" s="2"/>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8" ht="15">
       <c r="A16" s="1"/>
       <c r="B16" s="2"/>
       <c r="E16" s="3"/>
@@ -3082,7 +3032,7 @@
       <c r="G16" s="2"/>
       <c r="H16" s="2"/>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:8" ht="15">
       <c r="A17" s="1"/>
       <c r="B17" s="2"/>
       <c r="E17" s="3"/>
@@ -3090,7 +3040,7 @@
       <c r="G17" s="2"/>
       <c r="H17" s="2"/>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:8" ht="15">
       <c r="A18" s="1"/>
       <c r="B18" s="2"/>
       <c r="E18" s="3"/>
@@ -3098,7 +3048,7 @@
       <c r="G18" s="2"/>
       <c r="H18" s="2"/>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:8" ht="15">
       <c r="A19" s="1"/>
       <c r="B19" s="2"/>
       <c r="E19" s="3"/>
@@ -3106,7 +3056,7 @@
       <c r="G19" s="2"/>
       <c r="H19" s="2"/>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:8" ht="15">
       <c r="A20" s="1"/>
       <c r="B20" s="2"/>
       <c r="E20" s="3"/>
@@ -3114,7 +3064,7 @@
       <c r="G20" s="2"/>
       <c r="H20" s="2"/>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:8" ht="15">
       <c r="A21" s="1"/>
       <c r="B21" s="2"/>
       <c r="E21" s="3"/>
@@ -3122,7 +3072,7 @@
       <c r="G21" s="2"/>
       <c r="H21" s="2"/>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:8" ht="15">
       <c r="A22" s="1"/>
       <c r="B22" s="2"/>
       <c r="E22" s="3"/>
@@ -3130,7 +3080,7 @@
       <c r="G22" s="2"/>
       <c r="H22" s="2"/>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:8" ht="15">
       <c r="A23" s="1"/>
       <c r="B23" s="2"/>
       <c r="E23" s="3"/>
@@ -3138,7 +3088,7 @@
       <c r="G23" s="2"/>
       <c r="H23" s="2"/>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:8" ht="15">
       <c r="A24" s="1"/>
       <c r="B24" s="2"/>
       <c r="E24" s="3"/>
@@ -3146,7 +3096,7 @@
       <c r="G24" s="2"/>
       <c r="H24" s="2"/>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:8" ht="15">
       <c r="A25" s="1"/>
       <c r="B25" s="2"/>
       <c r="E25" s="3"/>
@@ -3154,7 +3104,7 @@
       <c r="G25" s="2"/>
       <c r="H25" s="2"/>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:8" ht="15">
       <c r="A26" s="1"/>
       <c r="B26" s="2"/>
       <c r="E26" s="3"/>
@@ -3162,7 +3112,7 @@
       <c r="G26" s="2"/>
       <c r="H26" s="2"/>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:8" ht="15">
       <c r="A27" s="1"/>
       <c r="B27" s="2"/>
       <c r="E27" s="3"/>
@@ -3170,7 +3120,7 @@
       <c r="G27" s="2"/>
       <c r="H27" s="2"/>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:8" ht="15">
       <c r="A28" s="1"/>
       <c r="B28" s="2"/>
       <c r="E28" s="3"/>
@@ -3178,7 +3128,7 @@
       <c r="G28" s="2"/>
       <c r="H28" s="2"/>
     </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:8" ht="15">
       <c r="A29" s="1"/>
       <c r="B29" s="2"/>
       <c r="E29" s="3"/>
@@ -3186,7 +3136,7 @@
       <c r="G29" s="2"/>
       <c r="H29" s="2"/>
     </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:8" ht="15">
       <c r="A30" s="1"/>
       <c r="B30" s="2"/>
       <c r="E30" s="3"/>
@@ -3194,7 +3144,7 @@
       <c r="G30" s="2"/>
       <c r="H30" s="2"/>
     </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:8" ht="15">
       <c r="A31" s="1"/>
       <c r="B31" s="2"/>
       <c r="E31" s="3"/>
@@ -3202,7 +3152,7 @@
       <c r="G31" s="2"/>
       <c r="H31" s="2"/>
     </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:8" ht="15">
       <c r="A32" s="1"/>
       <c r="B32" s="2"/>
       <c r="E32" s="3"/>
@@ -3210,7 +3160,7 @@
       <c r="G32" s="2"/>
       <c r="H32" s="2"/>
     </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:8" ht="15">
       <c r="A33" s="1"/>
       <c r="B33" s="2"/>
       <c r="E33" s="3"/>
@@ -3218,7 +3168,7 @@
       <c r="G33" s="2"/>
       <c r="H33" s="2"/>
     </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:8" ht="15">
       <c r="A34" s="1"/>
       <c r="B34" s="2"/>
       <c r="E34" s="3"/>
@@ -3226,7 +3176,7 @@
       <c r="G34" s="2"/>
       <c r="H34" s="2"/>
     </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:8" ht="15">
       <c r="A35" s="1"/>
       <c r="B35" s="2"/>
       <c r="E35" s="3"/>
@@ -3234,7 +3184,7 @@
       <c r="G35" s="2"/>
       <c r="H35" s="2"/>
     </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:8" ht="15">
       <c r="A36" s="1"/>
       <c r="B36" s="2"/>
       <c r="E36" s="3"/>
@@ -3242,7 +3192,7 @@
       <c r="G36" s="2"/>
       <c r="H36" s="2"/>
     </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:8" ht="15">
       <c r="A37" s="1"/>
       <c r="B37" s="2"/>
       <c r="E37" s="3"/>
@@ -3250,7 +3200,7 @@
       <c r="G37" s="2"/>
       <c r="H37" s="2"/>
     </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:8" ht="15">
       <c r="A38" s="1"/>
       <c r="B38" s="2"/>
       <c r="E38" s="3"/>
@@ -3258,7 +3208,7 @@
       <c r="G38" s="2"/>
       <c r="H38" s="2"/>
     </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:8" ht="15">
       <c r="A39" s="1"/>
       <c r="B39" s="2"/>
       <c r="E39" s="3"/>
@@ -3266,7 +3216,7 @@
       <c r="G39" s="2"/>
       <c r="H39" s="2"/>
     </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:8" ht="15">
       <c r="A40" s="1"/>
       <c r="B40" s="2"/>
       <c r="E40" s="3"/>
@@ -3274,7 +3224,7 @@
       <c r="G40" s="2"/>
       <c r="H40" s="2"/>
     </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:8" ht="15">
       <c r="A41" s="1"/>
       <c r="B41" s="2"/>
       <c r="E41" s="3"/>
@@ -3282,7 +3232,7 @@
       <c r="G41" s="2"/>
       <c r="H41" s="2"/>
     </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:8" ht="15">
       <c r="A42" s="1"/>
       <c r="B42" s="2"/>
       <c r="E42" s="3"/>
@@ -3290,7 +3240,7 @@
       <c r="G42" s="2"/>
       <c r="H42" s="2"/>
     </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:8" ht="15">
       <c r="A43" s="1"/>
       <c r="B43" s="2"/>
       <c r="E43" s="3"/>
@@ -3298,7 +3248,7 @@
       <c r="G43" s="2"/>
       <c r="H43" s="2"/>
     </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:8" ht="15">
       <c r="A44" s="1"/>
       <c r="B44" s="2"/>
       <c r="E44" s="3"/>
@@ -3306,7 +3256,7 @@
       <c r="G44" s="2"/>
       <c r="H44" s="2"/>
     </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:8" ht="15">
       <c r="A45" s="1"/>
       <c r="B45" s="2"/>
       <c r="E45" s="3"/>
@@ -3314,7 +3264,7 @@
       <c r="G45" s="2"/>
       <c r="H45" s="2"/>
     </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:8" ht="15">
       <c r="A46" s="1"/>
       <c r="B46" s="2"/>
       <c r="E46" s="3"/>
@@ -3322,7 +3272,7 @@
       <c r="G46" s="2"/>
       <c r="H46" s="2"/>
     </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:8" ht="15">
       <c r="A47" s="1"/>
       <c r="B47" s="2"/>
       <c r="E47" s="3"/>
@@ -3330,7 +3280,7 @@
       <c r="G47" s="2"/>
       <c r="H47" s="2"/>
     </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:8" ht="15">
       <c r="A48" s="1"/>
       <c r="B48" s="2"/>
       <c r="E48" s="3"/>
@@ -3338,7 +3288,7 @@
       <c r="G48" s="2"/>
       <c r="H48" s="2"/>
     </row>
-    <row r="49" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:8" ht="15">
       <c r="A49" s="1"/>
       <c r="B49" s="2"/>
       <c r="E49" s="3"/>
@@ -3346,7 +3296,7 @@
       <c r="G49" s="2"/>
       <c r="H49" s="2"/>
     </row>
-    <row r="50" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:8" ht="15">
       <c r="A50" s="1"/>
       <c r="B50" s="2"/>
       <c r="E50" s="3"/>
@@ -3354,7 +3304,7 @@
       <c r="G50" s="2"/>
       <c r="H50" s="2"/>
     </row>
-    <row r="51" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:8" ht="15">
       <c r="A51" s="1"/>
       <c r="B51" s="2"/>
       <c r="E51" s="3"/>
@@ -3362,7 +3312,7 @@
       <c r="G51" s="2"/>
       <c r="H51" s="2"/>
     </row>
-    <row r="52" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:8" ht="15">
       <c r="A52" s="1"/>
       <c r="B52" s="2"/>
       <c r="E52" s="3"/>
@@ -3370,7 +3320,7 @@
       <c r="G52" s="2"/>
       <c r="H52" s="2"/>
     </row>
-    <row r="53" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:8" ht="15">
       <c r="A53" s="1"/>
       <c r="B53" s="2"/>
       <c r="E53" s="3"/>
@@ -3378,7 +3328,7 @@
       <c r="G53" s="2"/>
       <c r="H53" s="2"/>
     </row>
-    <row r="54" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:8" ht="15">
       <c r="A54" s="1"/>
       <c r="B54" s="2"/>
       <c r="E54" s="3"/>
@@ -3386,7 +3336,7 @@
       <c r="G54" s="2"/>
       <c r="H54" s="2"/>
     </row>
-    <row r="55" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:8" ht="15">
       <c r="A55" s="1"/>
       <c r="B55" s="2"/>
       <c r="E55" s="3"/>
@@ -3394,7 +3344,7 @@
       <c r="G55" s="2"/>
       <c r="H55" s="2"/>
     </row>
-    <row r="56" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:8" ht="15">
       <c r="A56" s="1"/>
       <c r="B56" s="2"/>
       <c r="E56" s="3"/>
@@ -3402,7 +3352,7 @@
       <c r="G56" s="2"/>
       <c r="H56" s="2"/>
     </row>
-    <row r="57" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:8" ht="15">
       <c r="A57" s="1"/>
       <c r="B57" s="2"/>
       <c r="E57" s="3"/>
@@ -3410,7 +3360,7 @@
       <c r="G57" s="2"/>
       <c r="H57" s="2"/>
     </row>
-    <row r="58" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:8" ht="15">
       <c r="A58" s="1"/>
       <c r="B58" s="2"/>
       <c r="E58" s="3"/>
@@ -3418,7 +3368,7 @@
       <c r="G58" s="2"/>
       <c r="H58" s="2"/>
     </row>
-    <row r="59" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:8" ht="15">
       <c r="A59" s="1"/>
       <c r="B59" s="2"/>
       <c r="E59" s="3"/>
@@ -3426,7 +3376,7 @@
       <c r="G59" s="2"/>
       <c r="H59" s="2"/>
     </row>
-    <row r="60" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:8" ht="15">
       <c r="A60" s="1"/>
       <c r="B60" s="2"/>
       <c r="E60" s="3"/>
@@ -3434,7 +3384,7 @@
       <c r="G60" s="2"/>
       <c r="H60" s="2"/>
     </row>
-    <row r="61" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:8" ht="15">
       <c r="A61" s="1"/>
       <c r="B61" s="2"/>
       <c r="E61" s="3"/>
@@ -3442,7 +3392,7 @@
       <c r="G61" s="2"/>
       <c r="H61" s="2"/>
     </row>
-    <row r="62" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:8" ht="15">
       <c r="A62" s="1"/>
       <c r="B62" s="2"/>
       <c r="E62" s="3"/>
@@ -3450,7 +3400,7 @@
       <c r="G62" s="2"/>
       <c r="H62" s="2"/>
     </row>
-    <row r="63" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:8" ht="15">
       <c r="A63" s="1"/>
       <c r="B63" s="2"/>
       <c r="E63" s="3"/>
@@ -3458,7 +3408,7 @@
       <c r="G63" s="2"/>
       <c r="H63" s="2"/>
     </row>
-    <row r="64" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:8" ht="15">
       <c r="A64" s="1"/>
       <c r="B64" s="2"/>
       <c r="E64" s="3"/>
@@ -3466,7 +3416,7 @@
       <c r="G64" s="2"/>
       <c r="H64" s="2"/>
     </row>
-    <row r="65" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:8" ht="15">
       <c r="A65" s="1"/>
       <c r="B65" s="2"/>
       <c r="E65" s="3"/>
@@ -3474,7 +3424,7 @@
       <c r="G65" s="2"/>
       <c r="H65" s="2"/>
     </row>
-    <row r="66" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:8" ht="15">
       <c r="A66" s="1"/>
       <c r="B66" s="2"/>
       <c r="E66" s="3"/>
@@ -3482,7 +3432,7 @@
       <c r="G66" s="2"/>
       <c r="H66" s="2"/>
     </row>
-    <row r="67" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:8" ht="15">
       <c r="A67" s="1"/>
       <c r="B67" s="2"/>
       <c r="E67" s="3"/>
@@ -3490,7 +3440,7 @@
       <c r="G67" s="2"/>
       <c r="H67" s="2"/>
     </row>
-    <row r="68" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:8" ht="15">
       <c r="A68" s="1"/>
       <c r="B68" s="2"/>
       <c r="E68" s="3"/>
@@ -3498,7 +3448,7 @@
       <c r="G68" s="2"/>
       <c r="H68" s="2"/>
     </row>
-    <row r="69" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:8" ht="15">
       <c r="A69" s="1"/>
       <c r="B69" s="2"/>
       <c r="E69" s="3"/>
@@ -3506,7 +3456,7 @@
       <c r="G69" s="2"/>
       <c r="H69" s="2"/>
     </row>
-    <row r="70" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:8" ht="15">
       <c r="A70" s="1"/>
       <c r="B70" s="2"/>
       <c r="E70" s="3"/>
@@ -3514,7 +3464,7 @@
       <c r="G70" s="2"/>
       <c r="H70" s="2"/>
     </row>
-    <row r="71" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:8" ht="15">
       <c r="A71" s="1"/>
       <c r="B71" s="2"/>
       <c r="E71" s="3"/>
@@ -3522,7 +3472,7 @@
       <c r="G71" s="2"/>
       <c r="H71" s="2"/>
     </row>
-    <row r="72" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:8" ht="15">
       <c r="A72" s="1"/>
       <c r="B72" s="2"/>
       <c r="E72" s="3"/>
@@ -3530,7 +3480,7 @@
       <c r="G72" s="2"/>
       <c r="H72" s="2"/>
     </row>
-    <row r="73" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:8" ht="15">
       <c r="A73" s="1"/>
       <c r="B73" s="2"/>
       <c r="E73" s="3"/>
@@ -3538,7 +3488,7 @@
       <c r="G73" s="2"/>
       <c r="H73" s="2"/>
     </row>
-    <row r="74" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:8" ht="15">
       <c r="A74" s="1"/>
       <c r="B74" s="2"/>
       <c r="E74" s="3"/>
@@ -3546,7 +3496,7 @@
       <c r="G74" s="2"/>
       <c r="H74" s="2"/>
     </row>
-    <row r="75" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:8" ht="15">
       <c r="A75" s="1"/>
       <c r="B75" s="2"/>
       <c r="E75" s="3"/>
@@ -3554,7 +3504,7 @@
       <c r="G75" s="2"/>
       <c r="H75" s="2"/>
     </row>
-    <row r="76" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:8" ht="15">
       <c r="A76" s="1"/>
       <c r="B76" s="2"/>
       <c r="E76" s="3"/>
@@ -3562,7 +3512,7 @@
       <c r="G76" s="2"/>
       <c r="H76" s="2"/>
     </row>
-    <row r="77" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:8" ht="15">
       <c r="A77" s="1"/>
       <c r="B77" s="2"/>
       <c r="E77" s="3"/>
@@ -3570,7 +3520,7 @@
       <c r="G77" s="2"/>
       <c r="H77" s="2"/>
     </row>
-    <row r="78" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:8" ht="15">
       <c r="A78" s="1"/>
       <c r="B78" s="2"/>
       <c r="E78" s="3"/>
@@ -3578,7 +3528,7 @@
       <c r="G78" s="2"/>
       <c r="H78" s="2"/>
     </row>
-    <row r="79" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:8" ht="15">
       <c r="A79" s="1"/>
       <c r="B79" s="2"/>
       <c r="E79" s="3"/>
@@ -3586,7 +3536,7 @@
       <c r="G79" s="2"/>
       <c r="H79" s="2"/>
     </row>
-    <row r="80" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:8" ht="15">
       <c r="A80" s="1"/>
       <c r="B80" s="2"/>
       <c r="E80" s="3"/>
@@ -3594,7 +3544,7 @@
       <c r="G80" s="2"/>
       <c r="H80" s="2"/>
     </row>
-    <row r="81" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:8" ht="15">
       <c r="A81" s="1"/>
       <c r="B81" s="2"/>
       <c r="E81" s="3"/>
@@ -3602,7 +3552,7 @@
       <c r="G81" s="2"/>
       <c r="H81" s="2"/>
     </row>
-    <row r="82" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:8" ht="15">
       <c r="A82" s="1"/>
       <c r="B82" s="2"/>
       <c r="E82" s="3"/>
@@ -3610,7 +3560,7 @@
       <c r="G82" s="2"/>
       <c r="H82" s="2"/>
     </row>
-    <row r="83" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:8" ht="15">
       <c r="A83" s="1"/>
       <c r="B83" s="2"/>
       <c r="E83" s="3"/>
@@ -3618,7 +3568,7 @@
       <c r="G83" s="2"/>
       <c r="H83" s="2"/>
     </row>
-    <row r="84" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:8" ht="15">
       <c r="A84" s="1"/>
       <c r="B84" s="2"/>
       <c r="E84" s="3"/>
@@ -3626,7 +3576,7 @@
       <c r="G84" s="2"/>
       <c r="H84" s="2"/>
     </row>
-    <row r="85" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:8" ht="15">
       <c r="A85" s="1"/>
       <c r="B85" s="2"/>
       <c r="E85" s="3"/>
@@ -3634,7 +3584,7 @@
       <c r="G85" s="2"/>
       <c r="H85" s="2"/>
     </row>
-    <row r="86" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:8" ht="15">
       <c r="A86" s="1"/>
       <c r="B86" s="2"/>
       <c r="E86" s="3"/>
@@ -3642,7 +3592,7 @@
       <c r="G86" s="2"/>
       <c r="H86" s="2"/>
     </row>
-    <row r="87" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:8" ht="15">
       <c r="A87" s="1"/>
       <c r="B87" s="2"/>
       <c r="E87" s="3"/>
@@ -3650,7 +3600,7 @@
       <c r="G87" s="2"/>
       <c r="H87" s="2"/>
     </row>
-    <row r="88" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:8">
       <c r="A88" s="1"/>
       <c r="B88" s="2"/>
       <c r="E88" s="3"/>
@@ -3658,7 +3608,7 @@
       <c r="G88" s="2"/>
       <c r="H88" s="2"/>
     </row>
-    <row r="89" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:8">
       <c r="A89" s="1"/>
       <c r="B89" s="2"/>
       <c r="E89" s="3"/>
@@ -3666,7 +3616,7 @@
       <c r="G89" s="2"/>
       <c r="H89" s="2"/>
     </row>
-    <row r="90" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:8">
       <c r="A90" s="1"/>
       <c r="B90" s="2"/>
       <c r="E90" s="3"/>
@@ -3674,7 +3624,7 @@
       <c r="G90" s="2"/>
       <c r="H90" s="2"/>
     </row>
-    <row r="91" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:8">
       <c r="A91" s="1"/>
       <c r="B91" s="2"/>
       <c r="E91" s="3"/>
@@ -3682,7 +3632,7 @@
       <c r="G91" s="2"/>
       <c r="H91" s="2"/>
     </row>
-    <row r="92" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:8">
       <c r="A92" s="1"/>
       <c r="B92" s="2"/>
       <c r="E92" s="3"/>
@@ -3690,7 +3640,7 @@
       <c r="G92" s="2"/>
       <c r="H92" s="2"/>
     </row>
-    <row r="93" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:8">
       <c r="A93" s="1"/>
       <c r="B93" s="2"/>
       <c r="E93" s="3"/>
@@ -3698,7 +3648,7 @@
       <c r="G93" s="2"/>
       <c r="H93" s="2"/>
     </row>
-    <row r="94" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:8">
       <c r="A94" s="1"/>
       <c r="B94" s="2"/>
       <c r="E94" s="3"/>
@@ -3706,7 +3656,7 @@
       <c r="G94" s="2"/>
       <c r="H94" s="2"/>
     </row>
-    <row r="95" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:8">
       <c r="A95" s="1"/>
       <c r="B95" s="2"/>
       <c r="E95" s="3"/>
@@ -3714,7 +3664,7 @@
       <c r="G95" s="2"/>
       <c r="H95" s="2"/>
     </row>
-    <row r="96" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:8">
       <c r="A96" s="1"/>
       <c r="B96" s="2"/>
       <c r="E96" s="3"/>
@@ -3722,7 +3672,7 @@
       <c r="G96" s="2"/>
       <c r="H96" s="2"/>
     </row>
-    <row r="97" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:8">
       <c r="A97" s="1"/>
       <c r="B97" s="2"/>
       <c r="E97" s="3"/>
@@ -3730,7 +3680,7 @@
       <c r="G97" s="2"/>
       <c r="H97" s="2"/>
     </row>
-    <row r="98" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:8">
       <c r="A98" s="1"/>
       <c r="B98" s="2"/>
       <c r="E98" s="3"/>
@@ -3738,7 +3688,7 @@
       <c r="G98" s="2"/>
       <c r="H98" s="2"/>
     </row>
-    <row r="99" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:8">
       <c r="A99" s="1"/>
       <c r="B99" s="2"/>
       <c r="E99" s="3"/>
@@ -3746,7 +3696,7 @@
       <c r="G99" s="2"/>
       <c r="H99" s="2"/>
     </row>
-    <row r="100" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:8">
       <c r="A100" s="1"/>
       <c r="B100" s="2"/>
       <c r="E100" s="3"/>
@@ -3789,21 +3739,21 @@
       <selection activeCell="P21" sqref="P21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col min="1" max="1" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="19.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.5703125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.09765625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.8984375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.8984375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19.3984375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.59765625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.59765625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="9" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="17.85546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="17.8984375" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="17" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="19.140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="19.09765625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" ht="15.75">
       <c r="A1" s="7" t="s">
         <v>8</v>
       </c>
@@ -3835,7 +3785,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" ht="15">
       <c r="A2" s="2"/>
       <c r="B2" s="8"/>
       <c r="D2" s="2"/>
@@ -3843,7 +3793,7 @@
       <c r="I2" s="8"/>
       <c r="J2" s="2"/>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" ht="15">
       <c r="A3" s="2"/>
       <c r="B3" s="8"/>
       <c r="D3" s="2"/>
@@ -3851,7 +3801,7 @@
       <c r="I3" s="8"/>
       <c r="J3" s="2"/>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" ht="15">
       <c r="A4" s="2"/>
       <c r="B4" s="8"/>
       <c r="D4" s="2"/>
@@ -3859,7 +3809,7 @@
       <c r="I4" s="8"/>
       <c r="J4" s="2"/>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" ht="15">
       <c r="A5" s="2"/>
       <c r="B5" s="8"/>
       <c r="D5" s="2"/>
@@ -3867,7 +3817,7 @@
       <c r="I5" s="8"/>
       <c r="J5" s="2"/>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" ht="15">
       <c r="A6" s="2"/>
       <c r="B6" s="8"/>
       <c r="D6" s="2"/>
@@ -3875,7 +3825,7 @@
       <c r="I6" s="8"/>
       <c r="J6" s="2"/>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10" ht="15">
       <c r="A7" s="2"/>
       <c r="B7" s="8"/>
       <c r="D7" s="2"/>
@@ -3883,7 +3833,7 @@
       <c r="I7" s="8"/>
       <c r="J7" s="2"/>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10" ht="15">
       <c r="A8" s="2"/>
       <c r="B8" s="8"/>
       <c r="D8" s="2"/>
@@ -3891,7 +3841,7 @@
       <c r="I8" s="8"/>
       <c r="J8" s="2"/>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10" ht="15">
       <c r="A9" s="2"/>
       <c r="B9" s="8"/>
       <c r="D9" s="2"/>
@@ -3899,7 +3849,7 @@
       <c r="I9" s="8"/>
       <c r="J9" s="2"/>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:10" ht="15">
       <c r="A10" s="2"/>
       <c r="B10" s="8"/>
       <c r="D10" s="2"/>
@@ -3907,7 +3857,7 @@
       <c r="I10" s="8"/>
       <c r="J10" s="2"/>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:10" ht="15">
       <c r="A11" s="2"/>
       <c r="B11" s="8"/>
       <c r="D11" s="2"/>
@@ -3915,7 +3865,7 @@
       <c r="I11" s="8"/>
       <c r="J11" s="2"/>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:10" ht="15">
       <c r="A12" s="2"/>
       <c r="B12" s="8"/>
       <c r="D12" s="2"/>
@@ -3923,7 +3873,7 @@
       <c r="I12" s="8"/>
       <c r="J12" s="2"/>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:10" ht="15">
       <c r="A13" s="2"/>
       <c r="B13" s="8"/>
       <c r="D13" s="2"/>
@@ -3931,7 +3881,7 @@
       <c r="I13" s="8"/>
       <c r="J13" s="2"/>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:10" ht="15">
       <c r="A14" s="2"/>
       <c r="B14" s="8"/>
       <c r="D14" s="2"/>
@@ -3939,7 +3889,7 @@
       <c r="I14" s="8"/>
       <c r="J14" s="2"/>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:10" ht="15">
       <c r="A15" s="2"/>
       <c r="B15" s="8"/>
       <c r="D15" s="2"/>
@@ -3947,7 +3897,7 @@
       <c r="I15" s="8"/>
       <c r="J15" s="2"/>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:10" ht="15">
       <c r="A16" s="2"/>
       <c r="B16" s="8"/>
       <c r="D16" s="2"/>
@@ -3955,7 +3905,7 @@
       <c r="I16" s="8"/>
       <c r="J16" s="2"/>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:10" ht="15">
       <c r="A17" s="2"/>
       <c r="B17" s="8"/>
       <c r="D17" s="2"/>
@@ -3963,7 +3913,7 @@
       <c r="I17" s="8"/>
       <c r="J17" s="2"/>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:10" ht="15">
       <c r="A18" s="2"/>
       <c r="B18" s="8"/>
       <c r="D18" s="2"/>
@@ -3971,7 +3921,7 @@
       <c r="I18" s="8"/>
       <c r="J18" s="2"/>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:10" ht="15">
       <c r="A19" s="2"/>
       <c r="B19" s="8"/>
       <c r="D19" s="2"/>
@@ -3979,7 +3929,7 @@
       <c r="I19" s="8"/>
       <c r="J19" s="2"/>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:10" ht="15">
       <c r="A20" s="2"/>
       <c r="B20" s="8"/>
       <c r="D20" s="2"/>
@@ -3987,7 +3937,7 @@
       <c r="I20" s="8"/>
       <c r="J20" s="2"/>
     </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:10" ht="15">
       <c r="A21" s="2"/>
       <c r="B21" s="8"/>
       <c r="D21" s="2"/>
@@ -3995,7 +3945,7 @@
       <c r="I21" s="8"/>
       <c r="J21" s="2"/>
     </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:10" ht="15">
       <c r="A22" s="2"/>
       <c r="B22" s="8"/>
       <c r="D22" s="2"/>
@@ -4003,7 +3953,7 @@
       <c r="I22" s="8"/>
       <c r="J22" s="2"/>
     </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:10" ht="15">
       <c r="A23" s="2"/>
       <c r="B23" s="8"/>
       <c r="D23" s="2"/>
@@ -4011,7 +3961,7 @@
       <c r="I23" s="8"/>
       <c r="J23" s="2"/>
     </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:10" ht="15">
       <c r="A24" s="2"/>
       <c r="B24" s="8"/>
       <c r="D24" s="2"/>
@@ -4019,7 +3969,7 @@
       <c r="I24" s="8"/>
       <c r="J24" s="2"/>
     </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:10" ht="15">
       <c r="A25" s="2"/>
       <c r="B25" s="8"/>
       <c r="D25" s="2"/>
@@ -4027,7 +3977,7 @@
       <c r="I25" s="8"/>
       <c r="J25" s="2"/>
     </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:10">
       <c r="A26" s="2"/>
       <c r="B26" s="8"/>
       <c r="D26" s="2"/>
@@ -4035,7 +3985,7 @@
       <c r="I26" s="8"/>
       <c r="J26" s="2"/>
     </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:10">
       <c r="A27" s="2"/>
       <c r="B27" s="8"/>
       <c r="D27" s="2"/>
@@ -4043,7 +3993,7 @@
       <c r="I27" s="8"/>
       <c r="J27" s="2"/>
     </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:10">
       <c r="A28" s="2"/>
       <c r="B28" s="8"/>
       <c r="D28" s="2"/>
@@ -4051,7 +4001,7 @@
       <c r="I28" s="8"/>
       <c r="J28" s="2"/>
     </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:10">
       <c r="A29" s="2"/>
       <c r="B29" s="8"/>
       <c r="D29" s="2"/>
@@ -4059,7 +4009,7 @@
       <c r="I29" s="8"/>
       <c r="J29" s="2"/>
     </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:10">
       <c r="A30" s="2"/>
       <c r="B30" s="8"/>
       <c r="D30" s="2"/>
@@ -4067,7 +4017,7 @@
       <c r="I30" s="8"/>
       <c r="J30" s="2"/>
     </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:10">
       <c r="A31" s="2"/>
       <c r="B31" s="8"/>
       <c r="D31" s="2"/>
@@ -4075,7 +4025,7 @@
       <c r="I31" s="8"/>
       <c r="J31" s="2"/>
     </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:10">
       <c r="A32" s="2"/>
       <c r="B32" s="8"/>
       <c r="D32" s="2"/>
@@ -4083,7 +4033,7 @@
       <c r="I32" s="8"/>
       <c r="J32" s="2"/>
     </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:10">
       <c r="A33" s="2"/>
       <c r="B33" s="8"/>
       <c r="D33" s="2"/>
@@ -4091,7 +4041,7 @@
       <c r="I33" s="8"/>
       <c r="J33" s="2"/>
     </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:10">
       <c r="A34" s="2"/>
       <c r="B34" s="8"/>
       <c r="D34" s="2"/>
@@ -4099,7 +4049,7 @@
       <c r="I34" s="8"/>
       <c r="J34" s="2"/>
     </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:10">
       <c r="A35" s="2"/>
       <c r="B35" s="8"/>
       <c r="D35" s="2"/>
@@ -4107,7 +4057,7 @@
       <c r="I35" s="8"/>
       <c r="J35" s="2"/>
     </row>
-    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:10">
       <c r="A36" s="2"/>
       <c r="B36" s="8"/>
       <c r="D36" s="2"/>
@@ -4115,7 +4065,7 @@
       <c r="I36" s="8"/>
       <c r="J36" s="2"/>
     </row>
-    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:10">
       <c r="A37" s="2"/>
       <c r="B37" s="8"/>
       <c r="D37" s="2"/>
@@ -4123,7 +4073,7 @@
       <c r="I37" s="8"/>
       <c r="J37" s="2"/>
     </row>
-    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:10">
       <c r="A38" s="2"/>
       <c r="B38" s="8"/>
       <c r="D38" s="2"/>
@@ -4131,7 +4081,7 @@
       <c r="I38" s="8"/>
       <c r="J38" s="2"/>
     </row>
-    <row r="39" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:10">
       <c r="A39" s="2"/>
       <c r="B39" s="8"/>
       <c r="D39" s="2"/>
@@ -4139,7 +4089,7 @@
       <c r="I39" s="8"/>
       <c r="J39" s="2"/>
     </row>
-    <row r="40" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:10">
       <c r="A40" s="2"/>
       <c r="B40" s="8"/>
       <c r="D40" s="2"/>
@@ -4147,7 +4097,7 @@
       <c r="I40" s="8"/>
       <c r="J40" s="2"/>
     </row>
-    <row r="41" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:10">
       <c r="A41" s="2"/>
       <c r="B41" s="8"/>
       <c r="D41" s="2"/>
@@ -4155,7 +4105,7 @@
       <c r="I41" s="8"/>
       <c r="J41" s="2"/>
     </row>
-    <row r="42" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:10">
       <c r="A42" s="2"/>
       <c r="B42" s="8"/>
       <c r="D42" s="2"/>
@@ -4163,7 +4113,7 @@
       <c r="I42" s="8"/>
       <c r="J42" s="2"/>
     </row>
-    <row r="43" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:10">
       <c r="A43" s="2"/>
       <c r="B43" s="8"/>
       <c r="D43" s="2"/>
@@ -4171,7 +4121,7 @@
       <c r="I43" s="8"/>
       <c r="J43" s="2"/>
     </row>
-    <row r="44" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:10">
       <c r="A44" s="2"/>
       <c r="B44" s="8"/>
       <c r="D44" s="2"/>
@@ -4179,7 +4129,7 @@
       <c r="I44" s="8"/>
       <c r="J44" s="2"/>
     </row>
-    <row r="45" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:10">
       <c r="A45" s="2"/>
       <c r="B45" s="8"/>
       <c r="D45" s="2"/>
@@ -4187,7 +4137,7 @@
       <c r="I45" s="8"/>
       <c r="J45" s="2"/>
     </row>
-    <row r="46" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:10">
       <c r="A46" s="2"/>
       <c r="B46" s="8"/>
       <c r="D46" s="2"/>
@@ -4195,7 +4145,7 @@
       <c r="I46" s="8"/>
       <c r="J46" s="2"/>
     </row>
-    <row r="47" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:10">
       <c r="A47" s="2"/>
       <c r="B47" s="8"/>
       <c r="D47" s="2"/>
@@ -4203,7 +4153,7 @@
       <c r="I47" s="8"/>
       <c r="J47" s="2"/>
     </row>
-    <row r="48" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:10">
       <c r="A48" s="2"/>
       <c r="B48" s="8"/>
       <c r="D48" s="2"/>
@@ -4211,7 +4161,7 @@
       <c r="I48" s="8"/>
       <c r="J48" s="2"/>
     </row>
-    <row r="49" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:10">
       <c r="A49" s="2"/>
       <c r="B49" s="8"/>
       <c r="D49" s="2"/>
@@ -4219,7 +4169,7 @@
       <c r="I49" s="8"/>
       <c r="J49" s="2"/>
     </row>
-    <row r="50" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:10">
       <c r="A50" s="2"/>
       <c r="B50" s="8"/>
       <c r="D50" s="2"/>
@@ -4227,7 +4177,7 @@
       <c r="I50" s="8"/>
       <c r="J50" s="2"/>
     </row>
-    <row r="51" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:10">
       <c r="A51" s="2"/>
       <c r="B51" s="8"/>
       <c r="D51" s="2"/>
@@ -4235,7 +4185,7 @@
       <c r="I51" s="8"/>
       <c r="J51" s="2"/>
     </row>
-    <row r="52" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:10">
       <c r="A52" s="2"/>
       <c r="B52" s="8"/>
       <c r="D52" s="2"/>
@@ -4243,7 +4193,7 @@
       <c r="I52" s="8"/>
       <c r="J52" s="2"/>
     </row>
-    <row r="53" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:10">
       <c r="A53" s="2"/>
       <c r="B53" s="8"/>
       <c r="D53" s="2"/>
@@ -4251,7 +4201,7 @@
       <c r="I53" s="8"/>
       <c r="J53" s="2"/>
     </row>
-    <row r="54" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:10">
       <c r="A54" s="2"/>
       <c r="B54" s="8"/>
       <c r="D54" s="2"/>
@@ -4259,7 +4209,7 @@
       <c r="I54" s="8"/>
       <c r="J54" s="2"/>
     </row>
-    <row r="55" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:10">
       <c r="A55" s="2"/>
       <c r="B55" s="8"/>
       <c r="D55" s="2"/>
@@ -4267,7 +4217,7 @@
       <c r="I55" s="8"/>
       <c r="J55" s="2"/>
     </row>
-    <row r="56" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:10">
       <c r="A56" s="2"/>
       <c r="B56" s="8"/>
       <c r="D56" s="2"/>
@@ -4275,7 +4225,7 @@
       <c r="I56" s="8"/>
       <c r="J56" s="2"/>
     </row>
-    <row r="57" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:10">
       <c r="A57" s="2"/>
       <c r="B57" s="8"/>
       <c r="D57" s="2"/>
@@ -4283,7 +4233,7 @@
       <c r="I57" s="8"/>
       <c r="J57" s="2"/>
     </row>
-    <row r="58" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:10">
       <c r="A58" s="2"/>
       <c r="B58" s="8"/>
       <c r="D58" s="2"/>
@@ -4291,7 +4241,7 @@
       <c r="I58" s="8"/>
       <c r="J58" s="2"/>
     </row>
-    <row r="59" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:10">
       <c r="A59" s="2"/>
       <c r="B59" s="8"/>
       <c r="D59" s="2"/>
@@ -4299,7 +4249,7 @@
       <c r="I59" s="8"/>
       <c r="J59" s="2"/>
     </row>
-    <row r="60" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:10">
       <c r="A60" s="2"/>
       <c r="B60" s="8"/>
       <c r="D60" s="2"/>
@@ -4307,7 +4257,7 @@
       <c r="I60" s="8"/>
       <c r="J60" s="2"/>
     </row>
-    <row r="61" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:10">
       <c r="A61" s="2"/>
       <c r="B61" s="8"/>
       <c r="D61" s="2"/>
@@ -4315,7 +4265,7 @@
       <c r="I61" s="8"/>
       <c r="J61" s="2"/>
     </row>
-    <row r="62" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:10">
       <c r="A62" s="2"/>
       <c r="B62" s="8"/>
       <c r="D62" s="2"/>
@@ -4323,7 +4273,7 @@
       <c r="I62" s="8"/>
       <c r="J62" s="2"/>
     </row>
-    <row r="63" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:10">
       <c r="A63" s="2"/>
       <c r="B63" s="8"/>
       <c r="D63" s="2"/>
@@ -4331,7 +4281,7 @@
       <c r="I63" s="8"/>
       <c r="J63" s="2"/>
     </row>
-    <row r="64" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:10">
       <c r="A64" s="2"/>
       <c r="B64" s="8"/>
       <c r="D64" s="2"/>
@@ -4339,7 +4289,7 @@
       <c r="I64" s="8"/>
       <c r="J64" s="2"/>
     </row>
-    <row r="65" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:10">
       <c r="A65" s="2"/>
       <c r="B65" s="8"/>
       <c r="D65" s="2"/>
@@ -4347,7 +4297,7 @@
       <c r="I65" s="8"/>
       <c r="J65" s="2"/>
     </row>
-    <row r="66" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:10">
       <c r="A66" s="2"/>
       <c r="B66" s="8"/>
       <c r="D66" s="2"/>
@@ -4355,7 +4305,7 @@
       <c r="I66" s="8"/>
       <c r="J66" s="2"/>
     </row>
-    <row r="67" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:10">
       <c r="A67" s="2"/>
       <c r="B67" s="8"/>
       <c r="D67" s="2"/>
@@ -4363,7 +4313,7 @@
       <c r="I67" s="8"/>
       <c r="J67" s="2"/>
     </row>
-    <row r="68" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:10">
       <c r="A68" s="2"/>
       <c r="B68" s="8"/>
       <c r="D68" s="2"/>
@@ -4371,7 +4321,7 @@
       <c r="I68" s="8"/>
       <c r="J68" s="2"/>
     </row>
-    <row r="69" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:10">
       <c r="A69" s="2"/>
       <c r="B69" s="8"/>
       <c r="D69" s="2"/>
@@ -4379,7 +4329,7 @@
       <c r="I69" s="8"/>
       <c r="J69" s="2"/>
     </row>
-    <row r="70" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:10">
       <c r="A70" s="2"/>
       <c r="B70" s="8"/>
       <c r="D70" s="2"/>
@@ -4387,7 +4337,7 @@
       <c r="I70" s="8"/>
       <c r="J70" s="2"/>
     </row>
-    <row r="71" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:10">
       <c r="A71" s="2"/>
       <c r="B71" s="8"/>
       <c r="D71" s="2"/>
@@ -4395,7 +4345,7 @@
       <c r="I71" s="8"/>
       <c r="J71" s="2"/>
     </row>
-    <row r="72" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:10">
       <c r="A72" s="2"/>
       <c r="B72" s="8"/>
       <c r="D72" s="2"/>
@@ -4403,7 +4353,7 @@
       <c r="I72" s="8"/>
       <c r="J72" s="2"/>
     </row>
-    <row r="73" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:10">
       <c r="A73" s="2"/>
       <c r="B73" s="8"/>
       <c r="D73" s="2"/>
@@ -4411,7 +4361,7 @@
       <c r="I73" s="8"/>
       <c r="J73" s="2"/>
     </row>
-    <row r="74" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:10">
       <c r="A74" s="2"/>
       <c r="B74" s="8"/>
       <c r="D74" s="2"/>
@@ -4419,7 +4369,7 @@
       <c r="I74" s="8"/>
       <c r="J74" s="2"/>
     </row>
-    <row r="75" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:10">
       <c r="A75" s="2"/>
       <c r="B75" s="8"/>
       <c r="D75" s="2"/>
@@ -4427,7 +4377,7 @@
       <c r="I75" s="8"/>
       <c r="J75" s="2"/>
     </row>
-    <row r="76" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:10">
       <c r="A76" s="2"/>
       <c r="B76" s="8"/>
       <c r="D76" s="2"/>
@@ -4435,7 +4385,7 @@
       <c r="I76" s="8"/>
       <c r="J76" s="2"/>
     </row>
-    <row r="77" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:10">
       <c r="A77" s="2"/>
       <c r="B77" s="8"/>
       <c r="D77" s="2"/>
@@ -4443,7 +4393,7 @@
       <c r="I77" s="8"/>
       <c r="J77" s="2"/>
     </row>
-    <row r="78" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:10">
       <c r="A78" s="2"/>
       <c r="B78" s="8"/>
       <c r="D78" s="2"/>
@@ -4451,7 +4401,7 @@
       <c r="I78" s="8"/>
       <c r="J78" s="2"/>
     </row>
-    <row r="79" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:10">
       <c r="A79" s="2"/>
       <c r="B79" s="8"/>
       <c r="D79" s="2"/>
@@ -4459,7 +4409,7 @@
       <c r="I79" s="8"/>
       <c r="J79" s="2"/>
     </row>
-    <row r="80" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:10">
       <c r="A80" s="2"/>
       <c r="B80" s="8"/>
       <c r="D80" s="2"/>
@@ -4467,7 +4417,7 @@
       <c r="I80" s="8"/>
       <c r="J80" s="2"/>
     </row>
-    <row r="81" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:10">
       <c r="A81" s="2"/>
       <c r="B81" s="8"/>
       <c r="D81" s="2"/>
@@ -4475,7 +4425,7 @@
       <c r="I81" s="8"/>
       <c r="J81" s="2"/>
     </row>
-    <row r="82" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:10">
       <c r="A82" s="2"/>
       <c r="B82" s="8"/>
       <c r="D82" s="2"/>
@@ -4483,7 +4433,7 @@
       <c r="I82" s="8"/>
       <c r="J82" s="2"/>
     </row>
-    <row r="83" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:10">
       <c r="A83" s="2"/>
       <c r="B83" s="8"/>
       <c r="D83" s="2"/>
@@ -4491,7 +4441,7 @@
       <c r="I83" s="8"/>
       <c r="J83" s="2"/>
     </row>
-    <row r="84" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:10">
       <c r="A84" s="2"/>
       <c r="B84" s="8"/>
       <c r="D84" s="2"/>
@@ -4499,7 +4449,7 @@
       <c r="I84" s="8"/>
       <c r="J84" s="2"/>
     </row>
-    <row r="85" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:10">
       <c r="A85" s="2"/>
       <c r="B85" s="8"/>
       <c r="D85" s="2"/>
@@ -4507,7 +4457,7 @@
       <c r="I85" s="8"/>
       <c r="J85" s="2"/>
     </row>
-    <row r="86" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:10">
       <c r="A86" s="2"/>
       <c r="B86" s="8"/>
       <c r="D86" s="2"/>
@@ -4515,7 +4465,7 @@
       <c r="I86" s="8"/>
       <c r="J86" s="2"/>
     </row>
-    <row r="87" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:10">
       <c r="A87" s="2"/>
       <c r="B87" s="8"/>
       <c r="D87" s="2"/>
@@ -4523,7 +4473,7 @@
       <c r="I87" s="8"/>
       <c r="J87" s="2"/>
     </row>
-    <row r="88" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:10">
       <c r="A88" s="2"/>
       <c r="B88" s="8"/>
       <c r="D88" s="2"/>
@@ -4531,7 +4481,7 @@
       <c r="I88" s="8"/>
       <c r="J88" s="2"/>
     </row>
-    <row r="89" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:10">
       <c r="A89" s="2"/>
       <c r="B89" s="8"/>
       <c r="D89" s="2"/>
@@ -4539,7 +4489,7 @@
       <c r="I89" s="8"/>
       <c r="J89" s="2"/>
     </row>
-    <row r="90" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:10">
       <c r="A90" s="2"/>
       <c r="B90" s="8"/>
       <c r="D90" s="2"/>
@@ -4547,7 +4497,7 @@
       <c r="I90" s="8"/>
       <c r="J90" s="2"/>
     </row>
-    <row r="91" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:10">
       <c r="A91" s="2"/>
       <c r="B91" s="8"/>
       <c r="D91" s="2"/>
@@ -4555,7 +4505,7 @@
       <c r="I91" s="8"/>
       <c r="J91" s="2"/>
     </row>
-    <row r="92" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:10">
       <c r="A92" s="2"/>
       <c r="B92" s="8"/>
       <c r="D92" s="2"/>
@@ -4563,7 +4513,7 @@
       <c r="I92" s="8"/>
       <c r="J92" s="2"/>
     </row>
-    <row r="93" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:10">
       <c r="A93" s="2"/>
       <c r="B93" s="8"/>
       <c r="D93" s="2"/>
@@ -4571,7 +4521,7 @@
       <c r="I93" s="8"/>
       <c r="J93" s="2"/>
     </row>
-    <row r="94" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:10">
       <c r="A94" s="2"/>
       <c r="B94" s="8"/>
       <c r="D94" s="2"/>
@@ -4579,7 +4529,7 @@
       <c r="I94" s="8"/>
       <c r="J94" s="2"/>
     </row>
-    <row r="95" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:10">
       <c r="A95" s="2"/>
       <c r="B95" s="8"/>
       <c r="D95" s="2"/>
@@ -4587,7 +4537,7 @@
       <c r="I95" s="8"/>
       <c r="J95" s="2"/>
     </row>
-    <row r="96" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:10">
       <c r="A96" s="2"/>
       <c r="B96" s="8"/>
       <c r="D96" s="2"/>
@@ -4595,7 +4545,7 @@
       <c r="I96" s="8"/>
       <c r="J96" s="2"/>
     </row>
-    <row r="97" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:10">
       <c r="A97" s="2"/>
       <c r="B97" s="8"/>
       <c r="D97" s="2"/>
@@ -4603,7 +4553,7 @@
       <c r="I97" s="8"/>
       <c r="J97" s="2"/>
     </row>
-    <row r="98" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:10">
       <c r="A98" s="2"/>
       <c r="B98" s="8"/>
       <c r="D98" s="2"/>
@@ -4611,7 +4561,7 @@
       <c r="I98" s="8"/>
       <c r="J98" s="2"/>
     </row>
-    <row r="99" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:10">
       <c r="A99" s="2"/>
       <c r="B99" s="8"/>
       <c r="D99" s="2"/>
@@ -4619,7 +4569,7 @@
       <c r="I99" s="8"/>
       <c r="J99" s="2"/>
     </row>
-    <row r="100" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:10">
       <c r="A100" s="2"/>
       <c r="B100" s="8"/>
       <c r="D100" s="2"/>

</xml_diff>

<commit_message>
Updated PR&IR for Yash
</commit_message>
<xml_diff>
--- a/PR&IR.xlsx
+++ b/PR&IR.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SHIVYA KUMAR\Desktop\new415\CS415_A3\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\yashp\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{17103190-127F-4537-9CCD-D430D1B89B94}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F6DC0729-3852-445A-8D44-750E3FCF7692}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{BFA1E21A-08FA-4F02-8C25-33C81C8EE970}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="2" xr2:uid="{BFA1E21A-08FA-4F02-8C25-33C81C8EE970}"/>
   </bookViews>
   <sheets>
     <sheet name="Avichal" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="64">
   <si>
     <t>Date</t>
   </si>
@@ -205,6 +205,45 @@
   </si>
   <si>
     <t>Start with next workpackage once approved and given by Jayshil Singh</t>
+  </si>
+  <si>
+    <t>YPP</t>
+  </si>
+  <si>
+    <t>Converted Dart files to HTML files</t>
+  </si>
+  <si>
+    <t>Updating JS to render all htmls properly</t>
+  </si>
+  <si>
+    <t>N/A</t>
+  </si>
+  <si>
+    <t>Completed JS modification</t>
+  </si>
+  <si>
+    <t>Patch up any errors and add exception handling</t>
+  </si>
+  <si>
+    <t>13/5/2025</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Added Exception Handling </t>
+  </si>
+  <si>
+    <t>Parse XML's to registration Dropdowns</t>
+  </si>
+  <si>
+    <t>Will work on CS403 so hours worked on CS415 might decrease</t>
+  </si>
+  <si>
+    <t>14/5/2025</t>
+  </si>
+  <si>
+    <t>Parsed XML's Properly</t>
+  </si>
+  <si>
+    <t>Waiting PM's Lead</t>
   </si>
 </sst>
 </file>
@@ -256,7 +295,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -271,19 +310,21 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="2" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="35">
     <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
+      <numFmt numFmtId="2" formatCode="0.00"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="14" formatCode="0.00%"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="30" formatCode="@"/>
@@ -337,7 +378,7 @@
       <numFmt numFmtId="30" formatCode="@"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="166" formatCode="m/d/yyyy"/>
+      <numFmt numFmtId="19" formatCode="m/d/yyyy"/>
     </dxf>
     <dxf>
       <font>
@@ -364,16 +405,7 @@
       <numFmt numFmtId="30" formatCode="@"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="164" formatCode="h"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="14" formatCode="0.00%"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="166" formatCode="m/d/yyyy"/>
+      <numFmt numFmtId="19" formatCode="m/d/yyyy"/>
     </dxf>
     <dxf>
       <font>
@@ -395,6 +427,15 @@
     </dxf>
     <dxf>
       <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="30" formatCode="@"/>
@@ -436,7 +477,7 @@
       <numFmt numFmtId="30" formatCode="@"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="166" formatCode="m/d/yyyy"/>
+      <numFmt numFmtId="19" formatCode="m/d/yyyy"/>
     </dxf>
     <dxf>
       <font>
@@ -512,17 +553,17 @@
     <tableColumn id="2" xr3:uid="{55A78D6C-890A-4502-A184-DEEFF14BB82E}" name="Member Name" dataDxfId="25"/>
     <tableColumn id="3" xr3:uid="{57B9A516-E930-4C06-A589-24182A37BA85}" name="Task/Activity"/>
     <tableColumn id="4" xr3:uid="{A7CD18E8-808E-43EA-A960-7EDF2D2AB452}" name="Status"/>
-    <tableColumn id="5" xr3:uid="{A9BAB96D-D5FD-4C0D-A277-6E052D27EC3A}" name="% Complete" dataDxfId="0"/>
-    <tableColumn id="6" xr3:uid="{4EBDEBD4-A02D-4266-88BC-5E6088167CE4}" name="Hours Worked Today" dataDxfId="1"/>
-    <tableColumn id="7" xr3:uid="{88484166-6833-4A6B-B292-081E908E7876}" name="Next Steps" dataDxfId="2"/>
-    <tableColumn id="8" xr3:uid="{65034E84-46C0-4115-A351-A3C28C7B9EE1}" name="Notes/Comments" dataDxfId="24"/>
+    <tableColumn id="5" xr3:uid="{A9BAB96D-D5FD-4C0D-A277-6E052D27EC3A}" name="% Complete" dataDxfId="24"/>
+    <tableColumn id="6" xr3:uid="{4EBDEBD4-A02D-4266-88BC-5E6088167CE4}" name="Hours Worked Today" dataDxfId="23"/>
+    <tableColumn id="7" xr3:uid="{88484166-6833-4A6B-B292-081E908E7876}" name="Next Steps" dataDxfId="22"/>
+    <tableColumn id="8" xr3:uid="{65034E84-46C0-4115-A351-A3C28C7B9EE1}" name="Notes/Comments" dataDxfId="21"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium26" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{D9A2FBFA-47C8-4A27-8A35-991BC77E93AD}" name="Table14" displayName="Table14" ref="A1:H100" totalsRowShown="0" headerRowDxfId="23">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{D9A2FBFA-47C8-4A27-8A35-991BC77E93AD}" name="Table14" displayName="Table14" ref="A1:H100" totalsRowShown="0" headerRowDxfId="20">
   <autoFilter ref="A1:H100" xr:uid="{D9A2FBFA-47C8-4A27-8A35-991BC77E93AD}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
@@ -534,13 +575,13 @@
     <filterColumn colId="7" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="8">
-    <tableColumn id="1" xr3:uid="{9DF80C4D-D075-4428-A54F-FD6AD093D08C}" name="Date" dataDxfId="22"/>
-    <tableColumn id="2" xr3:uid="{EBFC72C6-272F-4910-98B7-AD481D68F5CF}" name="Member Name" dataDxfId="21"/>
+    <tableColumn id="1" xr3:uid="{9DF80C4D-D075-4428-A54F-FD6AD093D08C}" name="Date" dataDxfId="19"/>
+    <tableColumn id="2" xr3:uid="{EBFC72C6-272F-4910-98B7-AD481D68F5CF}" name="Member Name" dataDxfId="18"/>
     <tableColumn id="3" xr3:uid="{9F5B3984-7002-4FEA-8B81-D2D8284783D7}" name="Task/Activity"/>
     <tableColumn id="4" xr3:uid="{5F85F44B-886F-440F-9E69-8335A039C2E6}" name="Status"/>
-    <tableColumn id="5" xr3:uid="{AF0043ED-9EF2-470B-9735-7321011714BA}" name="% Complete" dataDxfId="20"/>
-    <tableColumn id="6" xr3:uid="{4F961AD8-B86B-411C-BB04-8D7EE4DD134D}" name="Hours Worked Today" dataDxfId="19"/>
-    <tableColumn id="7" xr3:uid="{34EBB1FC-FFD7-47AB-A959-A220B742401C}" name="Next Steps" dataDxfId="18"/>
+    <tableColumn id="5" xr3:uid="{AF0043ED-9EF2-470B-9735-7321011714BA}" name="% Complete" dataDxfId="2"/>
+    <tableColumn id="6" xr3:uid="{4F961AD8-B86B-411C-BB04-8D7EE4DD134D}" name="Hours Worked Today" dataDxfId="0"/>
+    <tableColumn id="7" xr3:uid="{34EBB1FC-FFD7-47AB-A959-A220B742401C}" name="Next Steps" dataDxfId="1"/>
     <tableColumn id="8" xr3:uid="{128DAA9E-15FB-4BB9-B76B-4A920C859038}" name="Notes/Comments" dataDxfId="17"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium26" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -955,26 +996,26 @@
       <selection activeCell="H7" sqref="H7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8"/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="10.3984375" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.59765625" style="2" customWidth="1"/>
+    <col min="1" max="1" width="10.36328125" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.6328125" style="2" customWidth="1"/>
     <col min="3" max="3" width="58" customWidth="1"/>
-    <col min="5" max="5" width="13.09765625" style="3" customWidth="1"/>
-    <col min="6" max="6" width="20.8984375" style="4" customWidth="1"/>
-    <col min="7" max="7" width="34.8984375" style="2" customWidth="1"/>
-    <col min="8" max="8" width="43.3984375" style="2" customWidth="1"/>
-    <col min="11" max="11" width="9.09765625" customWidth="1"/>
-    <col min="12" max="12" width="13.296875" customWidth="1"/>
-    <col min="13" max="13" width="11.3984375" customWidth="1"/>
-    <col min="14" max="14" width="17.3984375" customWidth="1"/>
-    <col min="16" max="16" width="9.09765625" customWidth="1"/>
-    <col min="18" max="18" width="16.59765625" customWidth="1"/>
-    <col min="19" max="19" width="14.69921875" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="16.8984375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.08984375" style="3" customWidth="1"/>
+    <col min="6" max="6" width="20.90625" style="4" customWidth="1"/>
+    <col min="7" max="7" width="34.90625" style="2" customWidth="1"/>
+    <col min="8" max="8" width="43.36328125" style="2" customWidth="1"/>
+    <col min="11" max="11" width="9.08984375" customWidth="1"/>
+    <col min="12" max="12" width="13.26953125" customWidth="1"/>
+    <col min="13" max="13" width="11.36328125" customWidth="1"/>
+    <col min="14" max="14" width="17.36328125" customWidth="1"/>
+    <col min="16" max="16" width="9.08984375" customWidth="1"/>
+    <col min="18" max="18" width="16.6328125" customWidth="1"/>
+    <col min="19" max="19" width="14.7265625" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="16.90625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="15.75">
+    <row r="1" spans="1:8" ht="15.5">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
@@ -1000,7 +1041,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="15.75">
+    <row r="2" spans="1:8">
       <c r="A2" s="1">
         <v>45786</v>
       </c>
@@ -1026,7 +1067,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="3" spans="1:8" ht="120">
+    <row r="3" spans="1:8" ht="116">
       <c r="A3" s="1">
         <v>45787</v>
       </c>
@@ -1049,7 +1090,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="4" spans="1:8" ht="15">
+    <row r="4" spans="1:8">
       <c r="A4" s="1">
         <v>45788</v>
       </c>
@@ -1092,7 +1133,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="6" spans="1:8" ht="15">
+    <row r="6" spans="1:8">
       <c r="A6" s="1">
         <v>45790</v>
       </c>
@@ -1138,31 +1179,31 @@
         <v>34</v>
       </c>
     </row>
-    <row r="8" spans="1:8" ht="15">
+    <row r="8" spans="1:8">
       <c r="E8"/>
       <c r="F8"/>
     </row>
-    <row r="9" spans="1:8" ht="15">
+    <row r="9" spans="1:8">
       <c r="E9"/>
       <c r="F9"/>
     </row>
-    <row r="10" spans="1:8" ht="15">
+    <row r="10" spans="1:8">
       <c r="E10"/>
       <c r="F10"/>
     </row>
-    <row r="11" spans="1:8" ht="15">
+    <row r="11" spans="1:8">
       <c r="E11"/>
       <c r="F11"/>
     </row>
-    <row r="12" spans="1:8" ht="15">
+    <row r="12" spans="1:8">
       <c r="E12"/>
       <c r="F12"/>
     </row>
-    <row r="13" spans="1:8" ht="15">
+    <row r="13" spans="1:8">
       <c r="E13"/>
       <c r="F13"/>
     </row>
-    <row r="14" spans="1:8" ht="15">
+    <row r="14" spans="1:8">
       <c r="E14"/>
       <c r="F14"/>
     </row>
@@ -1242,23 +1283,23 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3BDA6702-5DDF-42FB-988E-13FBEB26F5C9}">
   <dimension ref="A1:H100"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+    <sheetView topLeftCell="D1" workbookViewId="0">
       <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8"/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="9.8984375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="17.296875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="55.59765625" customWidth="1"/>
-    <col min="4" max="4" width="10.59765625" customWidth="1"/>
-    <col min="5" max="5" width="14.8984375" style="11" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14.296875" style="11" customWidth="1"/>
-    <col min="7" max="7" width="92.8984375" customWidth="1"/>
-    <col min="8" max="8" width="82.5" customWidth="1"/>
+    <col min="1" max="1" width="9.90625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.26953125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="55.6328125" customWidth="1"/>
+    <col min="4" max="4" width="10.6328125" customWidth="1"/>
+    <col min="5" max="5" width="14.90625" style="11" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.26953125" style="11" customWidth="1"/>
+    <col min="7" max="7" width="92.90625" customWidth="1"/>
+    <col min="8" max="8" width="82.453125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="15.75">
+    <row r="1" spans="1:8" ht="15.5">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
@@ -1284,7 +1325,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="15">
+    <row r="2" spans="1:8">
       <c r="A2" s="8">
         <v>45786</v>
       </c>
@@ -1310,7 +1351,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="3" spans="1:8" ht="15">
+    <row r="3" spans="1:8">
       <c r="A3" s="8">
         <v>45787</v>
       </c>
@@ -1336,7 +1377,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="4" spans="1:8" ht="15">
+    <row r="4" spans="1:8">
       <c r="A4" s="8">
         <v>45789</v>
       </c>
@@ -1360,7 +1401,7 @@
       </c>
       <c r="H4" s="2"/>
     </row>
-    <row r="5" spans="1:8" ht="15">
+    <row r="5" spans="1:8">
       <c r="A5" s="8">
         <v>45790</v>
       </c>
@@ -1384,7 +1425,7 @@
       </c>
       <c r="H5" s="2"/>
     </row>
-    <row r="6" spans="1:8" ht="15">
+    <row r="6" spans="1:8">
       <c r="A6" s="8">
         <v>45791</v>
       </c>
@@ -1410,115 +1451,115 @@
         <v>49</v>
       </c>
     </row>
-    <row r="7" spans="1:8" ht="15">
+    <row r="7" spans="1:8">
       <c r="A7" s="8"/>
       <c r="B7" s="2"/>
       <c r="G7" s="2"/>
       <c r="H7" s="2"/>
     </row>
-    <row r="8" spans="1:8" ht="15">
+    <row r="8" spans="1:8">
       <c r="A8" s="8"/>
       <c r="B8" s="2"/>
       <c r="G8" s="2"/>
       <c r="H8" s="2"/>
     </row>
-    <row r="9" spans="1:8" ht="15">
+    <row r="9" spans="1:8">
       <c r="A9" s="8"/>
       <c r="B9" s="2"/>
       <c r="G9" s="2"/>
       <c r="H9" s="2"/>
     </row>
-    <row r="10" spans="1:8" ht="15">
+    <row r="10" spans="1:8">
       <c r="A10" s="8"/>
       <c r="B10" s="2"/>
       <c r="G10" s="2"/>
       <c r="H10" s="2"/>
     </row>
-    <row r="11" spans="1:8" ht="15">
+    <row r="11" spans="1:8">
       <c r="A11" s="8"/>
       <c r="B11" s="2"/>
       <c r="G11" s="2"/>
       <c r="H11" s="2"/>
     </row>
-    <row r="12" spans="1:8" ht="15">
+    <row r="12" spans="1:8">
       <c r="A12" s="8"/>
       <c r="B12" s="2"/>
       <c r="G12" s="2"/>
       <c r="H12" s="2"/>
     </row>
-    <row r="13" spans="1:8" ht="15">
+    <row r="13" spans="1:8">
       <c r="A13" s="8"/>
       <c r="B13" s="2"/>
       <c r="G13" s="2"/>
       <c r="H13" s="2"/>
     </row>
-    <row r="14" spans="1:8" ht="15">
+    <row r="14" spans="1:8">
       <c r="A14" s="8"/>
       <c r="B14" s="2"/>
       <c r="G14" s="2"/>
       <c r="H14" s="2"/>
     </row>
-    <row r="15" spans="1:8" ht="15">
+    <row r="15" spans="1:8">
       <c r="A15" s="8"/>
       <c r="B15" s="2"/>
       <c r="G15" s="2"/>
       <c r="H15" s="2"/>
     </row>
-    <row r="16" spans="1:8" ht="15">
+    <row r="16" spans="1:8">
       <c r="A16" s="8"/>
       <c r="B16" s="2"/>
       <c r="G16" s="2"/>
       <c r="H16" s="2"/>
     </row>
-    <row r="17" spans="1:8" ht="15">
+    <row r="17" spans="1:8">
       <c r="A17" s="8"/>
       <c r="B17" s="2"/>
       <c r="G17" s="2"/>
       <c r="H17" s="2"/>
     </row>
-    <row r="18" spans="1:8" ht="15">
+    <row r="18" spans="1:8">
       <c r="A18" s="8"/>
       <c r="B18" s="2"/>
       <c r="G18" s="2"/>
       <c r="H18" s="2"/>
     </row>
-    <row r="19" spans="1:8" ht="15">
+    <row r="19" spans="1:8">
       <c r="A19" s="8"/>
       <c r="B19" s="2"/>
       <c r="G19" s="2"/>
       <c r="H19" s="2"/>
     </row>
-    <row r="20" spans="1:8" ht="15">
+    <row r="20" spans="1:8">
       <c r="A20" s="8"/>
       <c r="B20" s="2"/>
       <c r="G20" s="2"/>
       <c r="H20" s="2"/>
     </row>
-    <row r="21" spans="1:8" ht="15">
+    <row r="21" spans="1:8">
       <c r="A21" s="8"/>
       <c r="B21" s="2"/>
       <c r="G21" s="2"/>
       <c r="H21" s="2"/>
     </row>
-    <row r="22" spans="1:8" ht="15">
+    <row r="22" spans="1:8">
       <c r="A22" s="8"/>
       <c r="B22" s="2"/>
       <c r="G22" s="2"/>
       <c r="H22" s="2"/>
     </row>
-    <row r="23" spans="1:8" ht="15">
+    <row r="23" spans="1:8">
       <c r="A23" s="8"/>
       <c r="B23" s="2"/>
       <c r="G23" s="2"/>
       <c r="H23" s="2"/>
     </row>
-    <row r="24" spans="1:8" ht="15">
+    <row r="24" spans="1:8">
       <c r="A24" s="8"/>
       <c r="B24" s="2"/>
       <c r="G24" s="2"/>
       <c r="H24" s="2"/>
     </row>
-    <row r="25" spans="1:8" ht="15">
+    <row r="25" spans="1:8">
       <c r="A25" s="8"/>
       <c r="B25" s="2"/>
       <c r="G25" s="2"/>
@@ -2005,23 +2046,23 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9FD6A201-8E63-4A9E-A683-19506CB489E3}">
   <dimension ref="A1:H100"/>
   <sheetViews>
-    <sheetView topLeftCell="A63" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2:D100"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8"/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="7.69921875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="17.296875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.59765625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.8984375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="23.59765625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="13.3984375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="19.09765625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.08984375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.26953125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="27.81640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.7265625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.90625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="23.6328125" style="12" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="39.08984375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="51.08984375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="15.75">
+    <row r="1" spans="1:8" ht="15.5">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
@@ -2037,7 +2078,7 @@
       <c r="E1" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="7" t="s">
+      <c r="F1" s="13" t="s">
         <v>5</v>
       </c>
       <c r="G1" s="7" t="s">
@@ -2047,691 +2088,681 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="15">
-      <c r="A2" s="1"/>
-      <c r="B2" s="2"/>
-      <c r="E2" s="3"/>
-      <c r="F2" s="4"/>
-      <c r="G2" s="2"/>
-      <c r="H2" s="2"/>
-    </row>
-    <row r="3" spans="1:8" ht="15">
-      <c r="A3" s="1"/>
-      <c r="B3" s="2"/>
-      <c r="E3" s="3"/>
-      <c r="F3" s="4"/>
-      <c r="G3" s="2"/>
-      <c r="H3" s="2"/>
-    </row>
-    <row r="4" spans="1:8" ht="15">
-      <c r="A4" s="1"/>
-      <c r="B4" s="2"/>
-      <c r="E4" s="3"/>
-      <c r="F4" s="4"/>
-      <c r="G4" s="2"/>
-      <c r="H4" s="2"/>
-    </row>
-    <row r="5" spans="1:8" ht="15">
-      <c r="A5" s="1"/>
-      <c r="B5" s="2"/>
-      <c r="E5" s="3"/>
-      <c r="F5" s="4"/>
-      <c r="G5" s="2"/>
-      <c r="H5" s="2"/>
-    </row>
-    <row r="6" spans="1:8" ht="15">
+    <row r="2" spans="1:8">
+      <c r="A2" s="1">
+        <v>45935</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="C2" t="s">
+        <v>52</v>
+      </c>
+      <c r="D2" t="s">
+        <v>17</v>
+      </c>
+      <c r="E2" s="3">
+        <v>1</v>
+      </c>
+      <c r="F2" s="12">
+        <v>4</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8">
+      <c r="A3" s="1">
+        <v>45996</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="C3" t="s">
+        <v>55</v>
+      </c>
+      <c r="D3" t="s">
+        <v>17</v>
+      </c>
+      <c r="E3" s="3">
+        <v>1</v>
+      </c>
+      <c r="F3" s="12">
+        <v>4</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="H3" s="2" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8">
+      <c r="A4" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="C4" t="s">
+        <v>58</v>
+      </c>
+      <c r="D4" t="s">
+        <v>17</v>
+      </c>
+      <c r="E4" s="3">
+        <v>1</v>
+      </c>
+      <c r="F4" s="12">
+        <v>4</v>
+      </c>
+      <c r="G4" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="H4" s="2" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8">
+      <c r="A5" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="C5" t="s">
+        <v>62</v>
+      </c>
+      <c r="D5" t="s">
+        <v>17</v>
+      </c>
+      <c r="E5" s="3">
+        <v>1</v>
+      </c>
+      <c r="F5" s="12">
+        <v>5</v>
+      </c>
+      <c r="G5" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="H5" s="2" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8">
       <c r="A6" s="1"/>
       <c r="B6" s="2"/>
       <c r="E6" s="3"/>
-      <c r="F6" s="4"/>
       <c r="G6" s="2"/>
       <c r="H6" s="2"/>
     </row>
-    <row r="7" spans="1:8" ht="15">
+    <row r="7" spans="1:8">
       <c r="A7" s="1"/>
       <c r="B7" s="2"/>
       <c r="E7" s="3"/>
-      <c r="F7" s="4"/>
       <c r="G7" s="2"/>
       <c r="H7" s="2"/>
     </row>
-    <row r="8" spans="1:8" ht="15">
+    <row r="8" spans="1:8">
       <c r="A8" s="1"/>
       <c r="B8" s="2"/>
       <c r="E8" s="3"/>
-      <c r="F8" s="4"/>
       <c r="G8" s="2"/>
       <c r="H8" s="2"/>
     </row>
-    <row r="9" spans="1:8" ht="15">
+    <row r="9" spans="1:8">
       <c r="A9" s="1"/>
       <c r="B9" s="2"/>
       <c r="E9" s="3"/>
-      <c r="F9" s="4"/>
       <c r="G9" s="2"/>
       <c r="H9" s="2"/>
     </row>
-    <row r="10" spans="1:8" ht="15">
+    <row r="10" spans="1:8">
       <c r="A10" s="1"/>
       <c r="B10" s="2"/>
       <c r="E10" s="3"/>
-      <c r="F10" s="4"/>
       <c r="G10" s="2"/>
       <c r="H10" s="2"/>
     </row>
-    <row r="11" spans="1:8" ht="15">
+    <row r="11" spans="1:8">
       <c r="A11" s="1"/>
       <c r="B11" s="2"/>
       <c r="E11" s="3"/>
-      <c r="F11" s="4"/>
       <c r="G11" s="2"/>
       <c r="H11" s="2"/>
     </row>
-    <row r="12" spans="1:8" ht="15">
+    <row r="12" spans="1:8">
       <c r="A12" s="1"/>
       <c r="B12" s="2"/>
       <c r="E12" s="3"/>
-      <c r="F12" s="4"/>
       <c r="G12" s="2"/>
       <c r="H12" s="2"/>
     </row>
-    <row r="13" spans="1:8" ht="15">
+    <row r="13" spans="1:8">
       <c r="A13" s="1"/>
       <c r="B13" s="2"/>
       <c r="E13" s="3"/>
-      <c r="F13" s="4"/>
       <c r="G13" s="2"/>
       <c r="H13" s="2"/>
     </row>
-    <row r="14" spans="1:8" ht="15">
+    <row r="14" spans="1:8">
       <c r="A14" s="1"/>
       <c r="B14" s="2"/>
       <c r="E14" s="3"/>
-      <c r="F14" s="4"/>
       <c r="G14" s="2"/>
       <c r="H14" s="2"/>
     </row>
-    <row r="15" spans="1:8" ht="15">
+    <row r="15" spans="1:8">
       <c r="A15" s="1"/>
       <c r="B15" s="2"/>
       <c r="E15" s="3"/>
-      <c r="F15" s="4"/>
       <c r="G15" s="2"/>
       <c r="H15" s="2"/>
     </row>
-    <row r="16" spans="1:8" ht="15">
+    <row r="16" spans="1:8">
       <c r="A16" s="1"/>
       <c r="B16" s="2"/>
       <c r="E16" s="3"/>
-      <c r="F16" s="4"/>
       <c r="G16" s="2"/>
       <c r="H16" s="2"/>
     </row>
-    <row r="17" spans="1:8" ht="15">
+    <row r="17" spans="1:8">
       <c r="A17" s="1"/>
       <c r="B17" s="2"/>
       <c r="E17" s="3"/>
-      <c r="F17" s="4"/>
       <c r="G17" s="2"/>
       <c r="H17" s="2"/>
     </row>
-    <row r="18" spans="1:8" ht="15">
+    <row r="18" spans="1:8">
       <c r="A18" s="1"/>
       <c r="B18" s="2"/>
       <c r="E18" s="3"/>
-      <c r="F18" s="4"/>
       <c r="G18" s="2"/>
       <c r="H18" s="2"/>
     </row>
-    <row r="19" spans="1:8" ht="15">
+    <row r="19" spans="1:8">
       <c r="A19" s="1"/>
       <c r="B19" s="2"/>
       <c r="E19" s="3"/>
-      <c r="F19" s="4"/>
       <c r="G19" s="2"/>
       <c r="H19" s="2"/>
     </row>
-    <row r="20" spans="1:8" ht="15">
+    <row r="20" spans="1:8">
       <c r="A20" s="1"/>
       <c r="B20" s="2"/>
       <c r="E20" s="3"/>
-      <c r="F20" s="4"/>
       <c r="G20" s="2"/>
       <c r="H20" s="2"/>
     </row>
-    <row r="21" spans="1:8" ht="15">
+    <row r="21" spans="1:8">
       <c r="A21" s="1"/>
       <c r="B21" s="2"/>
       <c r="E21" s="3"/>
-      <c r="F21" s="4"/>
       <c r="G21" s="2"/>
       <c r="H21" s="2"/>
     </row>
-    <row r="22" spans="1:8" ht="15">
+    <row r="22" spans="1:8">
       <c r="A22" s="1"/>
       <c r="B22" s="2"/>
       <c r="E22" s="3"/>
-      <c r="F22" s="4"/>
       <c r="G22" s="2"/>
       <c r="H22" s="2"/>
     </row>
-    <row r="23" spans="1:8" ht="15">
+    <row r="23" spans="1:8">
       <c r="A23" s="1"/>
       <c r="B23" s="2"/>
       <c r="E23" s="3"/>
-      <c r="F23" s="4"/>
       <c r="G23" s="2"/>
       <c r="H23" s="2"/>
     </row>
-    <row r="24" spans="1:8" ht="15">
+    <row r="24" spans="1:8">
       <c r="A24" s="1"/>
       <c r="B24" s="2"/>
       <c r="E24" s="3"/>
-      <c r="F24" s="4"/>
       <c r="G24" s="2"/>
       <c r="H24" s="2"/>
     </row>
-    <row r="25" spans="1:8" ht="15">
+    <row r="25" spans="1:8">
       <c r="A25" s="1"/>
       <c r="B25" s="2"/>
       <c r="E25" s="3"/>
-      <c r="F25" s="4"/>
       <c r="G25" s="2"/>
       <c r="H25" s="2"/>
     </row>
-    <row r="26" spans="1:8" ht="15">
+    <row r="26" spans="1:8">
       <c r="A26" s="1"/>
       <c r="B26" s="2"/>
       <c r="E26" s="3"/>
-      <c r="F26" s="4"/>
       <c r="G26" s="2"/>
       <c r="H26" s="2"/>
     </row>
-    <row r="27" spans="1:8" ht="15">
+    <row r="27" spans="1:8">
       <c r="A27" s="1"/>
       <c r="B27" s="2"/>
       <c r="E27" s="3"/>
-      <c r="F27" s="4"/>
       <c r="G27" s="2"/>
       <c r="H27" s="2"/>
     </row>
-    <row r="28" spans="1:8" ht="15">
+    <row r="28" spans="1:8">
       <c r="A28" s="1"/>
       <c r="B28" s="2"/>
       <c r="E28" s="3"/>
-      <c r="F28" s="4"/>
       <c r="G28" s="2"/>
       <c r="H28" s="2"/>
     </row>
-    <row r="29" spans="1:8" ht="15">
+    <row r="29" spans="1:8">
       <c r="A29" s="1"/>
       <c r="B29" s="2"/>
       <c r="E29" s="3"/>
-      <c r="F29" s="4"/>
       <c r="G29" s="2"/>
       <c r="H29" s="2"/>
     </row>
-    <row r="30" spans="1:8" ht="15">
+    <row r="30" spans="1:8">
       <c r="A30" s="1"/>
       <c r="B30" s="2"/>
       <c r="E30" s="3"/>
-      <c r="F30" s="4"/>
       <c r="G30" s="2"/>
       <c r="H30" s="2"/>
     </row>
-    <row r="31" spans="1:8" ht="15">
+    <row r="31" spans="1:8">
       <c r="A31" s="1"/>
       <c r="B31" s="2"/>
       <c r="E31" s="3"/>
-      <c r="F31" s="4"/>
       <c r="G31" s="2"/>
       <c r="H31" s="2"/>
     </row>
-    <row r="32" spans="1:8" ht="15">
+    <row r="32" spans="1:8">
       <c r="A32" s="1"/>
       <c r="B32" s="2"/>
       <c r="E32" s="3"/>
-      <c r="F32" s="4"/>
       <c r="G32" s="2"/>
       <c r="H32" s="2"/>
     </row>
-    <row r="33" spans="1:8" ht="15">
+    <row r="33" spans="1:8">
       <c r="A33" s="1"/>
       <c r="B33" s="2"/>
       <c r="E33" s="3"/>
-      <c r="F33" s="4"/>
       <c r="G33" s="2"/>
       <c r="H33" s="2"/>
     </row>
-    <row r="34" spans="1:8" ht="15">
+    <row r="34" spans="1:8">
       <c r="A34" s="1"/>
       <c r="B34" s="2"/>
       <c r="E34" s="3"/>
-      <c r="F34" s="4"/>
       <c r="G34" s="2"/>
       <c r="H34" s="2"/>
     </row>
-    <row r="35" spans="1:8" ht="15">
+    <row r="35" spans="1:8">
       <c r="A35" s="1"/>
       <c r="B35" s="2"/>
       <c r="E35" s="3"/>
-      <c r="F35" s="4"/>
       <c r="G35" s="2"/>
       <c r="H35" s="2"/>
     </row>
-    <row r="36" spans="1:8" ht="15">
+    <row r="36" spans="1:8">
       <c r="A36" s="1"/>
       <c r="B36" s="2"/>
       <c r="E36" s="3"/>
-      <c r="F36" s="4"/>
       <c r="G36" s="2"/>
       <c r="H36" s="2"/>
     </row>
-    <row r="37" spans="1:8" ht="15">
+    <row r="37" spans="1:8">
       <c r="A37" s="1"/>
       <c r="B37" s="2"/>
       <c r="E37" s="3"/>
-      <c r="F37" s="4"/>
       <c r="G37" s="2"/>
       <c r="H37" s="2"/>
     </row>
-    <row r="38" spans="1:8" ht="15">
+    <row r="38" spans="1:8">
       <c r="A38" s="1"/>
       <c r="B38" s="2"/>
       <c r="E38" s="3"/>
-      <c r="F38" s="4"/>
       <c r="G38" s="2"/>
       <c r="H38" s="2"/>
     </row>
-    <row r="39" spans="1:8" ht="15">
+    <row r="39" spans="1:8">
       <c r="A39" s="1"/>
       <c r="B39" s="2"/>
       <c r="E39" s="3"/>
-      <c r="F39" s="4"/>
       <c r="G39" s="2"/>
       <c r="H39" s="2"/>
     </row>
-    <row r="40" spans="1:8" ht="15">
+    <row r="40" spans="1:8">
       <c r="A40" s="1"/>
       <c r="B40" s="2"/>
       <c r="E40" s="3"/>
-      <c r="F40" s="4"/>
       <c r="G40" s="2"/>
       <c r="H40" s="2"/>
     </row>
-    <row r="41" spans="1:8" ht="15">
+    <row r="41" spans="1:8">
       <c r="A41" s="1"/>
       <c r="B41" s="2"/>
       <c r="E41" s="3"/>
-      <c r="F41" s="4"/>
       <c r="G41" s="2"/>
       <c r="H41" s="2"/>
     </row>
-    <row r="42" spans="1:8" ht="15">
+    <row r="42" spans="1:8">
       <c r="A42" s="1"/>
       <c r="B42" s="2"/>
       <c r="E42" s="3"/>
-      <c r="F42" s="4"/>
       <c r="G42" s="2"/>
       <c r="H42" s="2"/>
     </row>
-    <row r="43" spans="1:8" ht="15">
+    <row r="43" spans="1:8">
       <c r="A43" s="1"/>
       <c r="B43" s="2"/>
       <c r="E43" s="3"/>
-      <c r="F43" s="4"/>
       <c r="G43" s="2"/>
       <c r="H43" s="2"/>
     </row>
-    <row r="44" spans="1:8" ht="15">
+    <row r="44" spans="1:8">
       <c r="A44" s="1"/>
       <c r="B44" s="2"/>
       <c r="E44" s="3"/>
-      <c r="F44" s="4"/>
       <c r="G44" s="2"/>
       <c r="H44" s="2"/>
     </row>
-    <row r="45" spans="1:8" ht="15">
+    <row r="45" spans="1:8">
       <c r="A45" s="1"/>
       <c r="B45" s="2"/>
       <c r="E45" s="3"/>
-      <c r="F45" s="4"/>
       <c r="G45" s="2"/>
       <c r="H45" s="2"/>
     </row>
-    <row r="46" spans="1:8" ht="15">
+    <row r="46" spans="1:8">
       <c r="A46" s="1"/>
       <c r="B46" s="2"/>
       <c r="E46" s="3"/>
-      <c r="F46" s="4"/>
       <c r="G46" s="2"/>
       <c r="H46" s="2"/>
     </row>
-    <row r="47" spans="1:8" ht="15">
+    <row r="47" spans="1:8">
       <c r="A47" s="1"/>
       <c r="B47" s="2"/>
       <c r="E47" s="3"/>
-      <c r="F47" s="4"/>
       <c r="G47" s="2"/>
       <c r="H47" s="2"/>
     </row>
-    <row r="48" spans="1:8" ht="15">
+    <row r="48" spans="1:8">
       <c r="A48" s="1"/>
       <c r="B48" s="2"/>
       <c r="E48" s="3"/>
-      <c r="F48" s="4"/>
       <c r="G48" s="2"/>
       <c r="H48" s="2"/>
     </row>
-    <row r="49" spans="1:8" ht="15">
+    <row r="49" spans="1:8">
       <c r="A49" s="1"/>
       <c r="B49" s="2"/>
       <c r="E49" s="3"/>
-      <c r="F49" s="4"/>
       <c r="G49" s="2"/>
       <c r="H49" s="2"/>
     </row>
-    <row r="50" spans="1:8" ht="15">
+    <row r="50" spans="1:8">
       <c r="A50" s="1"/>
       <c r="B50" s="2"/>
       <c r="E50" s="3"/>
-      <c r="F50" s="4"/>
       <c r="G50" s="2"/>
       <c r="H50" s="2"/>
     </row>
-    <row r="51" spans="1:8" ht="15">
+    <row r="51" spans="1:8">
       <c r="A51" s="1"/>
       <c r="B51" s="2"/>
       <c r="E51" s="3"/>
-      <c r="F51" s="4"/>
       <c r="G51" s="2"/>
       <c r="H51" s="2"/>
     </row>
-    <row r="52" spans="1:8" ht="15">
+    <row r="52" spans="1:8">
       <c r="A52" s="1"/>
       <c r="B52" s="2"/>
       <c r="E52" s="3"/>
-      <c r="F52" s="4"/>
       <c r="G52" s="2"/>
       <c r="H52" s="2"/>
     </row>
-    <row r="53" spans="1:8" ht="15">
+    <row r="53" spans="1:8">
       <c r="A53" s="1"/>
       <c r="B53" s="2"/>
       <c r="E53" s="3"/>
-      <c r="F53" s="4"/>
       <c r="G53" s="2"/>
       <c r="H53" s="2"/>
     </row>
-    <row r="54" spans="1:8" ht="15">
+    <row r="54" spans="1:8">
       <c r="A54" s="1"/>
       <c r="B54" s="2"/>
       <c r="E54" s="3"/>
-      <c r="F54" s="4"/>
       <c r="G54" s="2"/>
       <c r="H54" s="2"/>
     </row>
-    <row r="55" spans="1:8" ht="15">
+    <row r="55" spans="1:8">
       <c r="A55" s="1"/>
       <c r="B55" s="2"/>
       <c r="E55" s="3"/>
-      <c r="F55" s="4"/>
       <c r="G55" s="2"/>
       <c r="H55" s="2"/>
     </row>
-    <row r="56" spans="1:8" ht="15">
+    <row r="56" spans="1:8">
       <c r="A56" s="1"/>
       <c r="B56" s="2"/>
       <c r="E56" s="3"/>
-      <c r="F56" s="4"/>
       <c r="G56" s="2"/>
       <c r="H56" s="2"/>
     </row>
-    <row r="57" spans="1:8" ht="15">
+    <row r="57" spans="1:8">
       <c r="A57" s="1"/>
       <c r="B57" s="2"/>
       <c r="E57" s="3"/>
-      <c r="F57" s="4"/>
       <c r="G57" s="2"/>
       <c r="H57" s="2"/>
     </row>
-    <row r="58" spans="1:8" ht="15">
+    <row r="58" spans="1:8">
       <c r="A58" s="1"/>
       <c r="B58" s="2"/>
       <c r="E58" s="3"/>
-      <c r="F58" s="4"/>
       <c r="G58" s="2"/>
       <c r="H58" s="2"/>
     </row>
-    <row r="59" spans="1:8" ht="15">
+    <row r="59" spans="1:8">
       <c r="A59" s="1"/>
       <c r="B59" s="2"/>
       <c r="E59" s="3"/>
-      <c r="F59" s="4"/>
       <c r="G59" s="2"/>
       <c r="H59" s="2"/>
     </row>
-    <row r="60" spans="1:8" ht="15">
+    <row r="60" spans="1:8">
       <c r="A60" s="1"/>
       <c r="B60" s="2"/>
       <c r="E60" s="3"/>
-      <c r="F60" s="4"/>
       <c r="G60" s="2"/>
       <c r="H60" s="2"/>
     </row>
-    <row r="61" spans="1:8" ht="15">
+    <row r="61" spans="1:8">
       <c r="A61" s="1"/>
       <c r="B61" s="2"/>
       <c r="E61" s="3"/>
-      <c r="F61" s="4"/>
       <c r="G61" s="2"/>
       <c r="H61" s="2"/>
     </row>
-    <row r="62" spans="1:8" ht="15">
+    <row r="62" spans="1:8">
       <c r="A62" s="1"/>
       <c r="B62" s="2"/>
       <c r="E62" s="3"/>
-      <c r="F62" s="4"/>
       <c r="G62" s="2"/>
       <c r="H62" s="2"/>
     </row>
-    <row r="63" spans="1:8" ht="15">
+    <row r="63" spans="1:8">
       <c r="A63" s="1"/>
       <c r="B63" s="2"/>
       <c r="E63" s="3"/>
-      <c r="F63" s="4"/>
       <c r="G63" s="2"/>
       <c r="H63" s="2"/>
     </row>
-    <row r="64" spans="1:8" ht="15">
+    <row r="64" spans="1:8">
       <c r="A64" s="1"/>
       <c r="B64" s="2"/>
       <c r="E64" s="3"/>
-      <c r="F64" s="4"/>
       <c r="G64" s="2"/>
       <c r="H64" s="2"/>
     </row>
-    <row r="65" spans="1:8" ht="15">
+    <row r="65" spans="1:8">
       <c r="A65" s="1"/>
       <c r="B65" s="2"/>
       <c r="E65" s="3"/>
-      <c r="F65" s="4"/>
       <c r="G65" s="2"/>
       <c r="H65" s="2"/>
     </row>
-    <row r="66" spans="1:8" ht="15">
+    <row r="66" spans="1:8">
       <c r="A66" s="1"/>
       <c r="B66" s="2"/>
       <c r="E66" s="3"/>
-      <c r="F66" s="4"/>
       <c r="G66" s="2"/>
       <c r="H66" s="2"/>
     </row>
-    <row r="67" spans="1:8" ht="15">
+    <row r="67" spans="1:8">
       <c r="A67" s="1"/>
       <c r="B67" s="2"/>
       <c r="E67" s="3"/>
-      <c r="F67" s="4"/>
       <c r="G67" s="2"/>
       <c r="H67" s="2"/>
     </row>
-    <row r="68" spans="1:8" ht="15">
+    <row r="68" spans="1:8">
       <c r="A68" s="1"/>
       <c r="B68" s="2"/>
       <c r="E68" s="3"/>
-      <c r="F68" s="4"/>
       <c r="G68" s="2"/>
       <c r="H68" s="2"/>
     </row>
-    <row r="69" spans="1:8" ht="15">
+    <row r="69" spans="1:8">
       <c r="A69" s="1"/>
       <c r="B69" s="2"/>
       <c r="E69" s="3"/>
-      <c r="F69" s="4"/>
       <c r="G69" s="2"/>
       <c r="H69" s="2"/>
     </row>
-    <row r="70" spans="1:8" ht="15">
+    <row r="70" spans="1:8">
       <c r="A70" s="1"/>
       <c r="B70" s="2"/>
       <c r="E70" s="3"/>
-      <c r="F70" s="4"/>
       <c r="G70" s="2"/>
       <c r="H70" s="2"/>
     </row>
-    <row r="71" spans="1:8" ht="15">
+    <row r="71" spans="1:8">
       <c r="A71" s="1"/>
       <c r="B71" s="2"/>
       <c r="E71" s="3"/>
-      <c r="F71" s="4"/>
       <c r="G71" s="2"/>
       <c r="H71" s="2"/>
     </row>
-    <row r="72" spans="1:8" ht="15">
+    <row r="72" spans="1:8">
       <c r="A72" s="1"/>
       <c r="B72" s="2"/>
       <c r="E72" s="3"/>
-      <c r="F72" s="4"/>
       <c r="G72" s="2"/>
       <c r="H72" s="2"/>
     </row>
-    <row r="73" spans="1:8" ht="15">
+    <row r="73" spans="1:8">
       <c r="A73" s="1"/>
       <c r="B73" s="2"/>
       <c r="E73" s="3"/>
-      <c r="F73" s="4"/>
       <c r="G73" s="2"/>
       <c r="H73" s="2"/>
     </row>
-    <row r="74" spans="1:8" ht="15">
+    <row r="74" spans="1:8">
       <c r="A74" s="1"/>
       <c r="B74" s="2"/>
       <c r="E74" s="3"/>
-      <c r="F74" s="4"/>
       <c r="G74" s="2"/>
       <c r="H74" s="2"/>
     </row>
-    <row r="75" spans="1:8" ht="15">
+    <row r="75" spans="1:8">
       <c r="A75" s="1"/>
       <c r="B75" s="2"/>
       <c r="E75" s="3"/>
-      <c r="F75" s="4"/>
       <c r="G75" s="2"/>
       <c r="H75" s="2"/>
     </row>
-    <row r="76" spans="1:8" ht="15">
+    <row r="76" spans="1:8">
       <c r="A76" s="1"/>
       <c r="B76" s="2"/>
       <c r="E76" s="3"/>
-      <c r="F76" s="4"/>
       <c r="G76" s="2"/>
       <c r="H76" s="2"/>
     </row>
-    <row r="77" spans="1:8" ht="15">
+    <row r="77" spans="1:8">
       <c r="A77" s="1"/>
       <c r="B77" s="2"/>
       <c r="E77" s="3"/>
-      <c r="F77" s="4"/>
       <c r="G77" s="2"/>
       <c r="H77" s="2"/>
     </row>
-    <row r="78" spans="1:8" ht="15">
+    <row r="78" spans="1:8">
       <c r="A78" s="1"/>
       <c r="B78" s="2"/>
       <c r="E78" s="3"/>
-      <c r="F78" s="4"/>
       <c r="G78" s="2"/>
       <c r="H78" s="2"/>
     </row>
-    <row r="79" spans="1:8" ht="15">
+    <row r="79" spans="1:8">
       <c r="A79" s="1"/>
       <c r="B79" s="2"/>
       <c r="E79" s="3"/>
-      <c r="F79" s="4"/>
       <c r="G79" s="2"/>
       <c r="H79" s="2"/>
     </row>
-    <row r="80" spans="1:8" ht="15">
+    <row r="80" spans="1:8">
       <c r="A80" s="1"/>
       <c r="B80" s="2"/>
       <c r="E80" s="3"/>
-      <c r="F80" s="4"/>
       <c r="G80" s="2"/>
       <c r="H80" s="2"/>
     </row>
-    <row r="81" spans="1:8" ht="15">
+    <row r="81" spans="1:8">
       <c r="A81" s="1"/>
       <c r="B81" s="2"/>
       <c r="E81" s="3"/>
-      <c r="F81" s="4"/>
       <c r="G81" s="2"/>
       <c r="H81" s="2"/>
     </row>
-    <row r="82" spans="1:8" ht="15">
+    <row r="82" spans="1:8">
       <c r="A82" s="1"/>
       <c r="B82" s="2"/>
       <c r="E82" s="3"/>
-      <c r="F82" s="4"/>
       <c r="G82" s="2"/>
       <c r="H82" s="2"/>
     </row>
-    <row r="83" spans="1:8" ht="15">
+    <row r="83" spans="1:8">
       <c r="A83" s="1"/>
       <c r="B83" s="2"/>
       <c r="E83" s="3"/>
-      <c r="F83" s="4"/>
       <c r="G83" s="2"/>
       <c r="H83" s="2"/>
     </row>
-    <row r="84" spans="1:8" ht="15">
+    <row r="84" spans="1:8">
       <c r="A84" s="1"/>
       <c r="B84" s="2"/>
       <c r="E84" s="3"/>
-      <c r="F84" s="4"/>
       <c r="G84" s="2"/>
       <c r="H84" s="2"/>
     </row>
-    <row r="85" spans="1:8" ht="15">
+    <row r="85" spans="1:8">
       <c r="A85" s="1"/>
       <c r="B85" s="2"/>
       <c r="E85" s="3"/>
-      <c r="F85" s="4"/>
       <c r="G85" s="2"/>
       <c r="H85" s="2"/>
     </row>
-    <row r="86" spans="1:8" ht="15">
+    <row r="86" spans="1:8">
       <c r="A86" s="1"/>
       <c r="B86" s="2"/>
       <c r="E86" s="3"/>
-      <c r="F86" s="4"/>
       <c r="G86" s="2"/>
       <c r="H86" s="2"/>
     </row>
-    <row r="87" spans="1:8" ht="15">
+    <row r="87" spans="1:8">
       <c r="A87" s="1"/>
       <c r="B87" s="2"/>
       <c r="E87" s="3"/>
-      <c r="F87" s="4"/>
       <c r="G87" s="2"/>
       <c r="H87" s="2"/>
     </row>
@@ -2739,7 +2770,6 @@
       <c r="A88" s="1"/>
       <c r="B88" s="2"/>
       <c r="E88" s="3"/>
-      <c r="F88" s="4"/>
       <c r="G88" s="2"/>
       <c r="H88" s="2"/>
     </row>
@@ -2747,7 +2777,6 @@
       <c r="A89" s="1"/>
       <c r="B89" s="2"/>
       <c r="E89" s="3"/>
-      <c r="F89" s="4"/>
       <c r="G89" s="2"/>
       <c r="H89" s="2"/>
     </row>
@@ -2755,7 +2784,6 @@
       <c r="A90" s="1"/>
       <c r="B90" s="2"/>
       <c r="E90" s="3"/>
-      <c r="F90" s="4"/>
       <c r="G90" s="2"/>
       <c r="H90" s="2"/>
     </row>
@@ -2763,7 +2791,6 @@
       <c r="A91" s="1"/>
       <c r="B91" s="2"/>
       <c r="E91" s="3"/>
-      <c r="F91" s="4"/>
       <c r="G91" s="2"/>
       <c r="H91" s="2"/>
     </row>
@@ -2771,7 +2798,6 @@
       <c r="A92" s="1"/>
       <c r="B92" s="2"/>
       <c r="E92" s="3"/>
-      <c r="F92" s="4"/>
       <c r="G92" s="2"/>
       <c r="H92" s="2"/>
     </row>
@@ -2779,7 +2805,6 @@
       <c r="A93" s="1"/>
       <c r="B93" s="2"/>
       <c r="E93" s="3"/>
-      <c r="F93" s="4"/>
       <c r="G93" s="2"/>
       <c r="H93" s="2"/>
     </row>
@@ -2787,7 +2812,6 @@
       <c r="A94" s="1"/>
       <c r="B94" s="2"/>
       <c r="E94" s="3"/>
-      <c r="F94" s="4"/>
       <c r="G94" s="2"/>
       <c r="H94" s="2"/>
     </row>
@@ -2795,7 +2819,6 @@
       <c r="A95" s="1"/>
       <c r="B95" s="2"/>
       <c r="E95" s="3"/>
-      <c r="F95" s="4"/>
       <c r="G95" s="2"/>
       <c r="H95" s="2"/>
     </row>
@@ -2803,7 +2826,6 @@
       <c r="A96" s="1"/>
       <c r="B96" s="2"/>
       <c r="E96" s="3"/>
-      <c r="F96" s="4"/>
       <c r="G96" s="2"/>
       <c r="H96" s="2"/>
     </row>
@@ -2811,7 +2833,6 @@
       <c r="A97" s="1"/>
       <c r="B97" s="2"/>
       <c r="E97" s="3"/>
-      <c r="F97" s="4"/>
       <c r="G97" s="2"/>
       <c r="H97" s="2"/>
     </row>
@@ -2819,7 +2840,6 @@
       <c r="A98" s="1"/>
       <c r="B98" s="2"/>
       <c r="E98" s="3"/>
-      <c r="F98" s="4"/>
       <c r="G98" s="2"/>
       <c r="H98" s="2"/>
     </row>
@@ -2827,7 +2847,6 @@
       <c r="A99" s="1"/>
       <c r="B99" s="2"/>
       <c r="E99" s="3"/>
-      <c r="F99" s="4"/>
       <c r="G99" s="2"/>
       <c r="H99" s="2"/>
     </row>
@@ -2835,7 +2854,6 @@
       <c r="A100" s="1"/>
       <c r="B100" s="2"/>
       <c r="E100" s="3"/>
-      <c r="F100" s="4"/>
       <c r="G100" s="2"/>
       <c r="H100" s="2"/>
     </row>
@@ -2858,7 +2876,7 @@
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <ignoredErrors>
-    <ignoredError sqref="D2:D100" listDataValidation="1"/>
+    <ignoredError sqref="D6:D100" listDataValidation="1"/>
   </ignoredErrors>
   <tableParts count="1">
     <tablePart r:id="rId1"/>
@@ -2874,19 +2892,19 @@
       <selection activeCell="D2" sqref="D2:D100"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8"/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="7.69921875" customWidth="1"/>
-    <col min="2" max="2" width="17.296875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.59765625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="7.7265625" customWidth="1"/>
+    <col min="2" max="2" width="17.26953125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.6328125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="9" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.8984375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="23.59765625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="13.3984375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="19.09765625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.90625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="23.6328125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.36328125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="19.08984375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="15.75">
+    <row r="1" spans="1:8" ht="15.5">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
@@ -2912,7 +2930,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="15">
+    <row r="2" spans="1:8">
       <c r="A2" s="1"/>
       <c r="B2" s="2"/>
       <c r="E2" s="3"/>
@@ -2920,7 +2938,7 @@
       <c r="G2" s="2"/>
       <c r="H2" s="2"/>
     </row>
-    <row r="3" spans="1:8" ht="15">
+    <row r="3" spans="1:8">
       <c r="A3" s="1"/>
       <c r="B3" s="2"/>
       <c r="E3" s="3"/>
@@ -2928,7 +2946,7 @@
       <c r="G3" s="2"/>
       <c r="H3" s="2"/>
     </row>
-    <row r="4" spans="1:8" ht="15">
+    <row r="4" spans="1:8">
       <c r="A4" s="1"/>
       <c r="B4" s="2"/>
       <c r="E4" s="3"/>
@@ -2936,7 +2954,7 @@
       <c r="G4" s="2"/>
       <c r="H4" s="2"/>
     </row>
-    <row r="5" spans="1:8" ht="15">
+    <row r="5" spans="1:8">
       <c r="A5" s="1"/>
       <c r="B5" s="2"/>
       <c r="E5" s="3"/>
@@ -2944,7 +2962,7 @@
       <c r="G5" s="2"/>
       <c r="H5" s="2"/>
     </row>
-    <row r="6" spans="1:8" ht="15">
+    <row r="6" spans="1:8">
       <c r="A6" s="1"/>
       <c r="B6" s="2"/>
       <c r="E6" s="3"/>
@@ -2952,7 +2970,7 @@
       <c r="G6" s="2"/>
       <c r="H6" s="2"/>
     </row>
-    <row r="7" spans="1:8" ht="15">
+    <row r="7" spans="1:8">
       <c r="A7" s="1"/>
       <c r="B7" s="2"/>
       <c r="E7" s="3"/>
@@ -2960,7 +2978,7 @@
       <c r="G7" s="2"/>
       <c r="H7" s="2"/>
     </row>
-    <row r="8" spans="1:8" ht="15">
+    <row r="8" spans="1:8">
       <c r="A8" s="1"/>
       <c r="B8" s="2"/>
       <c r="E8" s="3"/>
@@ -2968,7 +2986,7 @@
       <c r="G8" s="2"/>
       <c r="H8" s="2"/>
     </row>
-    <row r="9" spans="1:8" ht="15">
+    <row r="9" spans="1:8">
       <c r="A9" s="1"/>
       <c r="B9" s="2"/>
       <c r="E9" s="3"/>
@@ -2976,7 +2994,7 @@
       <c r="G9" s="2"/>
       <c r="H9" s="2"/>
     </row>
-    <row r="10" spans="1:8" ht="15">
+    <row r="10" spans="1:8">
       <c r="A10" s="1"/>
       <c r="B10" s="2"/>
       <c r="E10" s="3"/>
@@ -2984,7 +3002,7 @@
       <c r="G10" s="2"/>
       <c r="H10" s="2"/>
     </row>
-    <row r="11" spans="1:8" ht="15">
+    <row r="11" spans="1:8">
       <c r="A11" s="1"/>
       <c r="B11" s="2"/>
       <c r="E11" s="3"/>
@@ -2992,7 +3010,7 @@
       <c r="G11" s="2"/>
       <c r="H11" s="2"/>
     </row>
-    <row r="12" spans="1:8" ht="15">
+    <row r="12" spans="1:8">
       <c r="A12" s="1"/>
       <c r="B12" s="2"/>
       <c r="E12" s="3"/>
@@ -3000,7 +3018,7 @@
       <c r="G12" s="2"/>
       <c r="H12" s="2"/>
     </row>
-    <row r="13" spans="1:8" ht="15">
+    <row r="13" spans="1:8">
       <c r="A13" s="1"/>
       <c r="B13" s="2"/>
       <c r="E13" s="3"/>
@@ -3008,7 +3026,7 @@
       <c r="G13" s="2"/>
       <c r="H13" s="2"/>
     </row>
-    <row r="14" spans="1:8" ht="15">
+    <row r="14" spans="1:8">
       <c r="A14" s="1"/>
       <c r="B14" s="2"/>
       <c r="E14" s="3"/>
@@ -3016,7 +3034,7 @@
       <c r="G14" s="2"/>
       <c r="H14" s="2"/>
     </row>
-    <row r="15" spans="1:8" ht="15">
+    <row r="15" spans="1:8">
       <c r="A15" s="1"/>
       <c r="B15" s="2"/>
       <c r="E15" s="3"/>
@@ -3024,7 +3042,7 @@
       <c r="G15" s="2"/>
       <c r="H15" s="2"/>
     </row>
-    <row r="16" spans="1:8" ht="15">
+    <row r="16" spans="1:8">
       <c r="A16" s="1"/>
       <c r="B16" s="2"/>
       <c r="E16" s="3"/>
@@ -3032,7 +3050,7 @@
       <c r="G16" s="2"/>
       <c r="H16" s="2"/>
     </row>
-    <row r="17" spans="1:8" ht="15">
+    <row r="17" spans="1:8">
       <c r="A17" s="1"/>
       <c r="B17" s="2"/>
       <c r="E17" s="3"/>
@@ -3040,7 +3058,7 @@
       <c r="G17" s="2"/>
       <c r="H17" s="2"/>
     </row>
-    <row r="18" spans="1:8" ht="15">
+    <row r="18" spans="1:8">
       <c r="A18" s="1"/>
       <c r="B18" s="2"/>
       <c r="E18" s="3"/>
@@ -3048,7 +3066,7 @@
       <c r="G18" s="2"/>
       <c r="H18" s="2"/>
     </row>
-    <row r="19" spans="1:8" ht="15">
+    <row r="19" spans="1:8">
       <c r="A19" s="1"/>
       <c r="B19" s="2"/>
       <c r="E19" s="3"/>
@@ -3056,7 +3074,7 @@
       <c r="G19" s="2"/>
       <c r="H19" s="2"/>
     </row>
-    <row r="20" spans="1:8" ht="15">
+    <row r="20" spans="1:8">
       <c r="A20" s="1"/>
       <c r="B20" s="2"/>
       <c r="E20" s="3"/>
@@ -3064,7 +3082,7 @@
       <c r="G20" s="2"/>
       <c r="H20" s="2"/>
     </row>
-    <row r="21" spans="1:8" ht="15">
+    <row r="21" spans="1:8">
       <c r="A21" s="1"/>
       <c r="B21" s="2"/>
       <c r="E21" s="3"/>
@@ -3072,7 +3090,7 @@
       <c r="G21" s="2"/>
       <c r="H21" s="2"/>
     </row>
-    <row r="22" spans="1:8" ht="15">
+    <row r="22" spans="1:8">
       <c r="A22" s="1"/>
       <c r="B22" s="2"/>
       <c r="E22" s="3"/>
@@ -3080,7 +3098,7 @@
       <c r="G22" s="2"/>
       <c r="H22" s="2"/>
     </row>
-    <row r="23" spans="1:8" ht="15">
+    <row r="23" spans="1:8">
       <c r="A23" s="1"/>
       <c r="B23" s="2"/>
       <c r="E23" s="3"/>
@@ -3088,7 +3106,7 @@
       <c r="G23" s="2"/>
       <c r="H23" s="2"/>
     </row>
-    <row r="24" spans="1:8" ht="15">
+    <row r="24" spans="1:8">
       <c r="A24" s="1"/>
       <c r="B24" s="2"/>
       <c r="E24" s="3"/>
@@ -3096,7 +3114,7 @@
       <c r="G24" s="2"/>
       <c r="H24" s="2"/>
     </row>
-    <row r="25" spans="1:8" ht="15">
+    <row r="25" spans="1:8">
       <c r="A25" s="1"/>
       <c r="B25" s="2"/>
       <c r="E25" s="3"/>
@@ -3104,7 +3122,7 @@
       <c r="G25" s="2"/>
       <c r="H25" s="2"/>
     </row>
-    <row r="26" spans="1:8" ht="15">
+    <row r="26" spans="1:8">
       <c r="A26" s="1"/>
       <c r="B26" s="2"/>
       <c r="E26" s="3"/>
@@ -3112,7 +3130,7 @@
       <c r="G26" s="2"/>
       <c r="H26" s="2"/>
     </row>
-    <row r="27" spans="1:8" ht="15">
+    <row r="27" spans="1:8">
       <c r="A27" s="1"/>
       <c r="B27" s="2"/>
       <c r="E27" s="3"/>
@@ -3120,7 +3138,7 @@
       <c r="G27" s="2"/>
       <c r="H27" s="2"/>
     </row>
-    <row r="28" spans="1:8" ht="15">
+    <row r="28" spans="1:8">
       <c r="A28" s="1"/>
       <c r="B28" s="2"/>
       <c r="E28" s="3"/>
@@ -3128,7 +3146,7 @@
       <c r="G28" s="2"/>
       <c r="H28" s="2"/>
     </row>
-    <row r="29" spans="1:8" ht="15">
+    <row r="29" spans="1:8">
       <c r="A29" s="1"/>
       <c r="B29" s="2"/>
       <c r="E29" s="3"/>
@@ -3136,7 +3154,7 @@
       <c r="G29" s="2"/>
       <c r="H29" s="2"/>
     </row>
-    <row r="30" spans="1:8" ht="15">
+    <row r="30" spans="1:8">
       <c r="A30" s="1"/>
       <c r="B30" s="2"/>
       <c r="E30" s="3"/>
@@ -3144,7 +3162,7 @@
       <c r="G30" s="2"/>
       <c r="H30" s="2"/>
     </row>
-    <row r="31" spans="1:8" ht="15">
+    <row r="31" spans="1:8">
       <c r="A31" s="1"/>
       <c r="B31" s="2"/>
       <c r="E31" s="3"/>
@@ -3152,7 +3170,7 @@
       <c r="G31" s="2"/>
       <c r="H31" s="2"/>
     </row>
-    <row r="32" spans="1:8" ht="15">
+    <row r="32" spans="1:8">
       <c r="A32" s="1"/>
       <c r="B32" s="2"/>
       <c r="E32" s="3"/>
@@ -3160,7 +3178,7 @@
       <c r="G32" s="2"/>
       <c r="H32" s="2"/>
     </row>
-    <row r="33" spans="1:8" ht="15">
+    <row r="33" spans="1:8">
       <c r="A33" s="1"/>
       <c r="B33" s="2"/>
       <c r="E33" s="3"/>
@@ -3168,7 +3186,7 @@
       <c r="G33" s="2"/>
       <c r="H33" s="2"/>
     </row>
-    <row r="34" spans="1:8" ht="15">
+    <row r="34" spans="1:8">
       <c r="A34" s="1"/>
       <c r="B34" s="2"/>
       <c r="E34" s="3"/>
@@ -3176,7 +3194,7 @@
       <c r="G34" s="2"/>
       <c r="H34" s="2"/>
     </row>
-    <row r="35" spans="1:8" ht="15">
+    <row r="35" spans="1:8">
       <c r="A35" s="1"/>
       <c r="B35" s="2"/>
       <c r="E35" s="3"/>
@@ -3184,7 +3202,7 @@
       <c r="G35" s="2"/>
       <c r="H35" s="2"/>
     </row>
-    <row r="36" spans="1:8" ht="15">
+    <row r="36" spans="1:8">
       <c r="A36" s="1"/>
       <c r="B36" s="2"/>
       <c r="E36" s="3"/>
@@ -3192,7 +3210,7 @@
       <c r="G36" s="2"/>
       <c r="H36" s="2"/>
     </row>
-    <row r="37" spans="1:8" ht="15">
+    <row r="37" spans="1:8">
       <c r="A37" s="1"/>
       <c r="B37" s="2"/>
       <c r="E37" s="3"/>
@@ -3200,7 +3218,7 @@
       <c r="G37" s="2"/>
       <c r="H37" s="2"/>
     </row>
-    <row r="38" spans="1:8" ht="15">
+    <row r="38" spans="1:8">
       <c r="A38" s="1"/>
       <c r="B38" s="2"/>
       <c r="E38" s="3"/>
@@ -3208,7 +3226,7 @@
       <c r="G38" s="2"/>
       <c r="H38" s="2"/>
     </row>
-    <row r="39" spans="1:8" ht="15">
+    <row r="39" spans="1:8">
       <c r="A39" s="1"/>
       <c r="B39" s="2"/>
       <c r="E39" s="3"/>
@@ -3216,7 +3234,7 @@
       <c r="G39" s="2"/>
       <c r="H39" s="2"/>
     </row>
-    <row r="40" spans="1:8" ht="15">
+    <row r="40" spans="1:8">
       <c r="A40" s="1"/>
       <c r="B40" s="2"/>
       <c r="E40" s="3"/>
@@ -3224,7 +3242,7 @@
       <c r="G40" s="2"/>
       <c r="H40" s="2"/>
     </row>
-    <row r="41" spans="1:8" ht="15">
+    <row r="41" spans="1:8">
       <c r="A41" s="1"/>
       <c r="B41" s="2"/>
       <c r="E41" s="3"/>
@@ -3232,7 +3250,7 @@
       <c r="G41" s="2"/>
       <c r="H41" s="2"/>
     </row>
-    <row r="42" spans="1:8" ht="15">
+    <row r="42" spans="1:8">
       <c r="A42" s="1"/>
       <c r="B42" s="2"/>
       <c r="E42" s="3"/>
@@ -3240,7 +3258,7 @@
       <c r="G42" s="2"/>
       <c r="H42" s="2"/>
     </row>
-    <row r="43" spans="1:8" ht="15">
+    <row r="43" spans="1:8">
       <c r="A43" s="1"/>
       <c r="B43" s="2"/>
       <c r="E43" s="3"/>
@@ -3248,7 +3266,7 @@
       <c r="G43" s="2"/>
       <c r="H43" s="2"/>
     </row>
-    <row r="44" spans="1:8" ht="15">
+    <row r="44" spans="1:8">
       <c r="A44" s="1"/>
       <c r="B44" s="2"/>
       <c r="E44" s="3"/>
@@ -3256,7 +3274,7 @@
       <c r="G44" s="2"/>
       <c r="H44" s="2"/>
     </row>
-    <row r="45" spans="1:8" ht="15">
+    <row r="45" spans="1:8">
       <c r="A45" s="1"/>
       <c r="B45" s="2"/>
       <c r="E45" s="3"/>
@@ -3264,7 +3282,7 @@
       <c r="G45" s="2"/>
       <c r="H45" s="2"/>
     </row>
-    <row r="46" spans="1:8" ht="15">
+    <row r="46" spans="1:8">
       <c r="A46" s="1"/>
       <c r="B46" s="2"/>
       <c r="E46" s="3"/>
@@ -3272,7 +3290,7 @@
       <c r="G46" s="2"/>
       <c r="H46" s="2"/>
     </row>
-    <row r="47" spans="1:8" ht="15">
+    <row r="47" spans="1:8">
       <c r="A47" s="1"/>
       <c r="B47" s="2"/>
       <c r="E47" s="3"/>
@@ -3280,7 +3298,7 @@
       <c r="G47" s="2"/>
       <c r="H47" s="2"/>
     </row>
-    <row r="48" spans="1:8" ht="15">
+    <row r="48" spans="1:8">
       <c r="A48" s="1"/>
       <c r="B48" s="2"/>
       <c r="E48" s="3"/>
@@ -3288,7 +3306,7 @@
       <c r="G48" s="2"/>
       <c r="H48" s="2"/>
     </row>
-    <row r="49" spans="1:8" ht="15">
+    <row r="49" spans="1:8">
       <c r="A49" s="1"/>
       <c r="B49" s="2"/>
       <c r="E49" s="3"/>
@@ -3296,7 +3314,7 @@
       <c r="G49" s="2"/>
       <c r="H49" s="2"/>
     </row>
-    <row r="50" spans="1:8" ht="15">
+    <row r="50" spans="1:8">
       <c r="A50" s="1"/>
       <c r="B50" s="2"/>
       <c r="E50" s="3"/>
@@ -3304,7 +3322,7 @@
       <c r="G50" s="2"/>
       <c r="H50" s="2"/>
     </row>
-    <row r="51" spans="1:8" ht="15">
+    <row r="51" spans="1:8">
       <c r="A51" s="1"/>
       <c r="B51" s="2"/>
       <c r="E51" s="3"/>
@@ -3312,7 +3330,7 @@
       <c r="G51" s="2"/>
       <c r="H51" s="2"/>
     </row>
-    <row r="52" spans="1:8" ht="15">
+    <row r="52" spans="1:8">
       <c r="A52" s="1"/>
       <c r="B52" s="2"/>
       <c r="E52" s="3"/>
@@ -3320,7 +3338,7 @@
       <c r="G52" s="2"/>
       <c r="H52" s="2"/>
     </row>
-    <row r="53" spans="1:8" ht="15">
+    <row r="53" spans="1:8">
       <c r="A53" s="1"/>
       <c r="B53" s="2"/>
       <c r="E53" s="3"/>
@@ -3328,7 +3346,7 @@
       <c r="G53" s="2"/>
       <c r="H53" s="2"/>
     </row>
-    <row r="54" spans="1:8" ht="15">
+    <row r="54" spans="1:8">
       <c r="A54" s="1"/>
       <c r="B54" s="2"/>
       <c r="E54" s="3"/>
@@ -3336,7 +3354,7 @@
       <c r="G54" s="2"/>
       <c r="H54" s="2"/>
     </row>
-    <row r="55" spans="1:8" ht="15">
+    <row r="55" spans="1:8">
       <c r="A55" s="1"/>
       <c r="B55" s="2"/>
       <c r="E55" s="3"/>
@@ -3344,7 +3362,7 @@
       <c r="G55" s="2"/>
       <c r="H55" s="2"/>
     </row>
-    <row r="56" spans="1:8" ht="15">
+    <row r="56" spans="1:8">
       <c r="A56" s="1"/>
       <c r="B56" s="2"/>
       <c r="E56" s="3"/>
@@ -3352,7 +3370,7 @@
       <c r="G56" s="2"/>
       <c r="H56" s="2"/>
     </row>
-    <row r="57" spans="1:8" ht="15">
+    <row r="57" spans="1:8">
       <c r="A57" s="1"/>
       <c r="B57" s="2"/>
       <c r="E57" s="3"/>
@@ -3360,7 +3378,7 @@
       <c r="G57" s="2"/>
       <c r="H57" s="2"/>
     </row>
-    <row r="58" spans="1:8" ht="15">
+    <row r="58" spans="1:8">
       <c r="A58" s="1"/>
       <c r="B58" s="2"/>
       <c r="E58" s="3"/>
@@ -3368,7 +3386,7 @@
       <c r="G58" s="2"/>
       <c r="H58" s="2"/>
     </row>
-    <row r="59" spans="1:8" ht="15">
+    <row r="59" spans="1:8">
       <c r="A59" s="1"/>
       <c r="B59" s="2"/>
       <c r="E59" s="3"/>
@@ -3376,7 +3394,7 @@
       <c r="G59" s="2"/>
       <c r="H59" s="2"/>
     </row>
-    <row r="60" spans="1:8" ht="15">
+    <row r="60" spans="1:8">
       <c r="A60" s="1"/>
       <c r="B60" s="2"/>
       <c r="E60" s="3"/>
@@ -3384,7 +3402,7 @@
       <c r="G60" s="2"/>
       <c r="H60" s="2"/>
     </row>
-    <row r="61" spans="1:8" ht="15">
+    <row r="61" spans="1:8">
       <c r="A61" s="1"/>
       <c r="B61" s="2"/>
       <c r="E61" s="3"/>
@@ -3392,7 +3410,7 @@
       <c r="G61" s="2"/>
       <c r="H61" s="2"/>
     </row>
-    <row r="62" spans="1:8" ht="15">
+    <row r="62" spans="1:8">
       <c r="A62" s="1"/>
       <c r="B62" s="2"/>
       <c r="E62" s="3"/>
@@ -3400,7 +3418,7 @@
       <c r="G62" s="2"/>
       <c r="H62" s="2"/>
     </row>
-    <row r="63" spans="1:8" ht="15">
+    <row r="63" spans="1:8">
       <c r="A63" s="1"/>
       <c r="B63" s="2"/>
       <c r="E63" s="3"/>
@@ -3408,7 +3426,7 @@
       <c r="G63" s="2"/>
       <c r="H63" s="2"/>
     </row>
-    <row r="64" spans="1:8" ht="15">
+    <row r="64" spans="1:8">
       <c r="A64" s="1"/>
       <c r="B64" s="2"/>
       <c r="E64" s="3"/>
@@ -3416,7 +3434,7 @@
       <c r="G64" s="2"/>
       <c r="H64" s="2"/>
     </row>
-    <row r="65" spans="1:8" ht="15">
+    <row r="65" spans="1:8">
       <c r="A65" s="1"/>
       <c r="B65" s="2"/>
       <c r="E65" s="3"/>
@@ -3424,7 +3442,7 @@
       <c r="G65" s="2"/>
       <c r="H65" s="2"/>
     </row>
-    <row r="66" spans="1:8" ht="15">
+    <row r="66" spans="1:8">
       <c r="A66" s="1"/>
       <c r="B66" s="2"/>
       <c r="E66" s="3"/>
@@ -3432,7 +3450,7 @@
       <c r="G66" s="2"/>
       <c r="H66" s="2"/>
     </row>
-    <row r="67" spans="1:8" ht="15">
+    <row r="67" spans="1:8">
       <c r="A67" s="1"/>
       <c r="B67" s="2"/>
       <c r="E67" s="3"/>
@@ -3440,7 +3458,7 @@
       <c r="G67" s="2"/>
       <c r="H67" s="2"/>
     </row>
-    <row r="68" spans="1:8" ht="15">
+    <row r="68" spans="1:8">
       <c r="A68" s="1"/>
       <c r="B68" s="2"/>
       <c r="E68" s="3"/>
@@ -3448,7 +3466,7 @@
       <c r="G68" s="2"/>
       <c r="H68" s="2"/>
     </row>
-    <row r="69" spans="1:8" ht="15">
+    <row r="69" spans="1:8">
       <c r="A69" s="1"/>
       <c r="B69" s="2"/>
       <c r="E69" s="3"/>
@@ -3456,7 +3474,7 @@
       <c r="G69" s="2"/>
       <c r="H69" s="2"/>
     </row>
-    <row r="70" spans="1:8" ht="15">
+    <row r="70" spans="1:8">
       <c r="A70" s="1"/>
       <c r="B70" s="2"/>
       <c r="E70" s="3"/>
@@ -3464,7 +3482,7 @@
       <c r="G70" s="2"/>
       <c r="H70" s="2"/>
     </row>
-    <row r="71" spans="1:8" ht="15">
+    <row r="71" spans="1:8">
       <c r="A71" s="1"/>
       <c r="B71" s="2"/>
       <c r="E71" s="3"/>
@@ -3472,7 +3490,7 @@
       <c r="G71" s="2"/>
       <c r="H71" s="2"/>
     </row>
-    <row r="72" spans="1:8" ht="15">
+    <row r="72" spans="1:8">
       <c r="A72" s="1"/>
       <c r="B72" s="2"/>
       <c r="E72" s="3"/>
@@ -3480,7 +3498,7 @@
       <c r="G72" s="2"/>
       <c r="H72" s="2"/>
     </row>
-    <row r="73" spans="1:8" ht="15">
+    <row r="73" spans="1:8">
       <c r="A73" s="1"/>
       <c r="B73" s="2"/>
       <c r="E73" s="3"/>
@@ -3488,7 +3506,7 @@
       <c r="G73" s="2"/>
       <c r="H73" s="2"/>
     </row>
-    <row r="74" spans="1:8" ht="15">
+    <row r="74" spans="1:8">
       <c r="A74" s="1"/>
       <c r="B74" s="2"/>
       <c r="E74" s="3"/>
@@ -3496,7 +3514,7 @@
       <c r="G74" s="2"/>
       <c r="H74" s="2"/>
     </row>
-    <row r="75" spans="1:8" ht="15">
+    <row r="75" spans="1:8">
       <c r="A75" s="1"/>
       <c r="B75" s="2"/>
       <c r="E75" s="3"/>
@@ -3504,7 +3522,7 @@
       <c r="G75" s="2"/>
       <c r="H75" s="2"/>
     </row>
-    <row r="76" spans="1:8" ht="15">
+    <row r="76" spans="1:8">
       <c r="A76" s="1"/>
       <c r="B76" s="2"/>
       <c r="E76" s="3"/>
@@ -3512,7 +3530,7 @@
       <c r="G76" s="2"/>
       <c r="H76" s="2"/>
     </row>
-    <row r="77" spans="1:8" ht="15">
+    <row r="77" spans="1:8">
       <c r="A77" s="1"/>
       <c r="B77" s="2"/>
       <c r="E77" s="3"/>
@@ -3520,7 +3538,7 @@
       <c r="G77" s="2"/>
       <c r="H77" s="2"/>
     </row>
-    <row r="78" spans="1:8" ht="15">
+    <row r="78" spans="1:8">
       <c r="A78" s="1"/>
       <c r="B78" s="2"/>
       <c r="E78" s="3"/>
@@ -3528,7 +3546,7 @@
       <c r="G78" s="2"/>
       <c r="H78" s="2"/>
     </row>
-    <row r="79" spans="1:8" ht="15">
+    <row r="79" spans="1:8">
       <c r="A79" s="1"/>
       <c r="B79" s="2"/>
       <c r="E79" s="3"/>
@@ -3536,7 +3554,7 @@
       <c r="G79" s="2"/>
       <c r="H79" s="2"/>
     </row>
-    <row r="80" spans="1:8" ht="15">
+    <row r="80" spans="1:8">
       <c r="A80" s="1"/>
       <c r="B80" s="2"/>
       <c r="E80" s="3"/>
@@ -3544,7 +3562,7 @@
       <c r="G80" s="2"/>
       <c r="H80" s="2"/>
     </row>
-    <row r="81" spans="1:8" ht="15">
+    <row r="81" spans="1:8">
       <c r="A81" s="1"/>
       <c r="B81" s="2"/>
       <c r="E81" s="3"/>
@@ -3552,7 +3570,7 @@
       <c r="G81" s="2"/>
       <c r="H81" s="2"/>
     </row>
-    <row r="82" spans="1:8" ht="15">
+    <row r="82" spans="1:8">
       <c r="A82" s="1"/>
       <c r="B82" s="2"/>
       <c r="E82" s="3"/>
@@ -3560,7 +3578,7 @@
       <c r="G82" s="2"/>
       <c r="H82" s="2"/>
     </row>
-    <row r="83" spans="1:8" ht="15">
+    <row r="83" spans="1:8">
       <c r="A83" s="1"/>
       <c r="B83" s="2"/>
       <c r="E83" s="3"/>
@@ -3568,7 +3586,7 @@
       <c r="G83" s="2"/>
       <c r="H83" s="2"/>
     </row>
-    <row r="84" spans="1:8" ht="15">
+    <row r="84" spans="1:8">
       <c r="A84" s="1"/>
       <c r="B84" s="2"/>
       <c r="E84" s="3"/>
@@ -3576,7 +3594,7 @@
       <c r="G84" s="2"/>
       <c r="H84" s="2"/>
     </row>
-    <row r="85" spans="1:8" ht="15">
+    <row r="85" spans="1:8">
       <c r="A85" s="1"/>
       <c r="B85" s="2"/>
       <c r="E85" s="3"/>
@@ -3584,7 +3602,7 @@
       <c r="G85" s="2"/>
       <c r="H85" s="2"/>
     </row>
-    <row r="86" spans="1:8" ht="15">
+    <row r="86" spans="1:8">
       <c r="A86" s="1"/>
       <c r="B86" s="2"/>
       <c r="E86" s="3"/>
@@ -3592,7 +3610,7 @@
       <c r="G86" s="2"/>
       <c r="H86" s="2"/>
     </row>
-    <row r="87" spans="1:8" ht="15">
+    <row r="87" spans="1:8">
       <c r="A87" s="1"/>
       <c r="B87" s="2"/>
       <c r="E87" s="3"/>
@@ -3739,21 +3757,21 @@
       <selection activeCell="P21" sqref="P21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8"/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="10.09765625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.8984375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.8984375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="19.3984375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.59765625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.59765625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.08984375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.90625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.90625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19.36328125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.6328125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.6328125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="9" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="17.8984375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="17.90625" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="17" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="19.09765625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="19.08984375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="15.75">
+    <row r="1" spans="1:10" ht="15.5">
       <c r="A1" s="7" t="s">
         <v>8</v>
       </c>
@@ -3785,7 +3803,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:10" ht="15">
+    <row r="2" spans="1:10">
       <c r="A2" s="2"/>
       <c r="B2" s="8"/>
       <c r="D2" s="2"/>
@@ -3793,7 +3811,7 @@
       <c r="I2" s="8"/>
       <c r="J2" s="2"/>
     </row>
-    <row r="3" spans="1:10" ht="15">
+    <row r="3" spans="1:10">
       <c r="A3" s="2"/>
       <c r="B3" s="8"/>
       <c r="D3" s="2"/>
@@ -3801,7 +3819,7 @@
       <c r="I3" s="8"/>
       <c r="J3" s="2"/>
     </row>
-    <row r="4" spans="1:10" ht="15">
+    <row r="4" spans="1:10">
       <c r="A4" s="2"/>
       <c r="B4" s="8"/>
       <c r="D4" s="2"/>
@@ -3809,7 +3827,7 @@
       <c r="I4" s="8"/>
       <c r="J4" s="2"/>
     </row>
-    <row r="5" spans="1:10" ht="15">
+    <row r="5" spans="1:10">
       <c r="A5" s="2"/>
       <c r="B5" s="8"/>
       <c r="D5" s="2"/>
@@ -3817,7 +3835,7 @@
       <c r="I5" s="8"/>
       <c r="J5" s="2"/>
     </row>
-    <row r="6" spans="1:10" ht="15">
+    <row r="6" spans="1:10">
       <c r="A6" s="2"/>
       <c r="B6" s="8"/>
       <c r="D6" s="2"/>
@@ -3825,7 +3843,7 @@
       <c r="I6" s="8"/>
       <c r="J6" s="2"/>
     </row>
-    <row r="7" spans="1:10" ht="15">
+    <row r="7" spans="1:10">
       <c r="A7" s="2"/>
       <c r="B7" s="8"/>
       <c r="D7" s="2"/>
@@ -3833,7 +3851,7 @@
       <c r="I7" s="8"/>
       <c r="J7" s="2"/>
     </row>
-    <row r="8" spans="1:10" ht="15">
+    <row r="8" spans="1:10">
       <c r="A8" s="2"/>
       <c r="B8" s="8"/>
       <c r="D8" s="2"/>
@@ -3841,7 +3859,7 @@
       <c r="I8" s="8"/>
       <c r="J8" s="2"/>
     </row>
-    <row r="9" spans="1:10" ht="15">
+    <row r="9" spans="1:10">
       <c r="A9" s="2"/>
       <c r="B9" s="8"/>
       <c r="D9" s="2"/>
@@ -3849,7 +3867,7 @@
       <c r="I9" s="8"/>
       <c r="J9" s="2"/>
     </row>
-    <row r="10" spans="1:10" ht="15">
+    <row r="10" spans="1:10">
       <c r="A10" s="2"/>
       <c r="B10" s="8"/>
       <c r="D10" s="2"/>
@@ -3857,7 +3875,7 @@
       <c r="I10" s="8"/>
       <c r="J10" s="2"/>
     </row>
-    <row r="11" spans="1:10" ht="15">
+    <row r="11" spans="1:10">
       <c r="A11" s="2"/>
       <c r="B11" s="8"/>
       <c r="D11" s="2"/>
@@ -3865,7 +3883,7 @@
       <c r="I11" s="8"/>
       <c r="J11" s="2"/>
     </row>
-    <row r="12" spans="1:10" ht="15">
+    <row r="12" spans="1:10">
       <c r="A12" s="2"/>
       <c r="B12" s="8"/>
       <c r="D12" s="2"/>
@@ -3873,7 +3891,7 @@
       <c r="I12" s="8"/>
       <c r="J12" s="2"/>
     </row>
-    <row r="13" spans="1:10" ht="15">
+    <row r="13" spans="1:10">
       <c r="A13" s="2"/>
       <c r="B13" s="8"/>
       <c r="D13" s="2"/>
@@ -3881,7 +3899,7 @@
       <c r="I13" s="8"/>
       <c r="J13" s="2"/>
     </row>
-    <row r="14" spans="1:10" ht="15">
+    <row r="14" spans="1:10">
       <c r="A14" s="2"/>
       <c r="B14" s="8"/>
       <c r="D14" s="2"/>
@@ -3889,7 +3907,7 @@
       <c r="I14" s="8"/>
       <c r="J14" s="2"/>
     </row>
-    <row r="15" spans="1:10" ht="15">
+    <row r="15" spans="1:10">
       <c r="A15" s="2"/>
       <c r="B15" s="8"/>
       <c r="D15" s="2"/>
@@ -3897,7 +3915,7 @@
       <c r="I15" s="8"/>
       <c r="J15" s="2"/>
     </row>
-    <row r="16" spans="1:10" ht="15">
+    <row r="16" spans="1:10">
       <c r="A16" s="2"/>
       <c r="B16" s="8"/>
       <c r="D16" s="2"/>
@@ -3905,7 +3923,7 @@
       <c r="I16" s="8"/>
       <c r="J16" s="2"/>
     </row>
-    <row r="17" spans="1:10" ht="15">
+    <row r="17" spans="1:10">
       <c r="A17" s="2"/>
       <c r="B17" s="8"/>
       <c r="D17" s="2"/>
@@ -3913,7 +3931,7 @@
       <c r="I17" s="8"/>
       <c r="J17" s="2"/>
     </row>
-    <row r="18" spans="1:10" ht="15">
+    <row r="18" spans="1:10">
       <c r="A18" s="2"/>
       <c r="B18" s="8"/>
       <c r="D18" s="2"/>
@@ -3921,7 +3939,7 @@
       <c r="I18" s="8"/>
       <c r="J18" s="2"/>
     </row>
-    <row r="19" spans="1:10" ht="15">
+    <row r="19" spans="1:10">
       <c r="A19" s="2"/>
       <c r="B19" s="8"/>
       <c r="D19" s="2"/>
@@ -3929,7 +3947,7 @@
       <c r="I19" s="8"/>
       <c r="J19" s="2"/>
     </row>
-    <row r="20" spans="1:10" ht="15">
+    <row r="20" spans="1:10">
       <c r="A20" s="2"/>
       <c r="B20" s="8"/>
       <c r="D20" s="2"/>
@@ -3937,7 +3955,7 @@
       <c r="I20" s="8"/>
       <c r="J20" s="2"/>
     </row>
-    <row r="21" spans="1:10" ht="15">
+    <row r="21" spans="1:10">
       <c r="A21" s="2"/>
       <c r="B21" s="8"/>
       <c r="D21" s="2"/>
@@ -3945,7 +3963,7 @@
       <c r="I21" s="8"/>
       <c r="J21" s="2"/>
     </row>
-    <row r="22" spans="1:10" ht="15">
+    <row r="22" spans="1:10">
       <c r="A22" s="2"/>
       <c r="B22" s="8"/>
       <c r="D22" s="2"/>
@@ -3953,7 +3971,7 @@
       <c r="I22" s="8"/>
       <c r="J22" s="2"/>
     </row>
-    <row r="23" spans="1:10" ht="15">
+    <row r="23" spans="1:10">
       <c r="A23" s="2"/>
       <c r="B23" s="8"/>
       <c r="D23" s="2"/>
@@ -3961,7 +3979,7 @@
       <c r="I23" s="8"/>
       <c r="J23" s="2"/>
     </row>
-    <row r="24" spans="1:10" ht="15">
+    <row r="24" spans="1:10">
       <c r="A24" s="2"/>
       <c r="B24" s="8"/>
       <c r="D24" s="2"/>
@@ -3969,7 +3987,7 @@
       <c r="I24" s="8"/>
       <c r="J24" s="2"/>
     </row>
-    <row r="25" spans="1:10" ht="15">
+    <row r="25" spans="1:10">
       <c r="A25" s="2"/>
       <c r="B25" s="8"/>
       <c r="D25" s="2"/>

</xml_diff>

<commit_message>
Updated progress report for May 15 Thurs by Avichal
</commit_message>
<xml_diff>
--- a/PR&IR.xlsx
+++ b/PR&IR.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\yashp\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\avichal avneel nath\Documents\Semester 7\CS415\A3\CS415_A3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F6DC0729-3852-445A-8D44-750E3FCF7692}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C4698082-5310-4F60-BD23-0E98E1F8FAFF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="2" xr2:uid="{BFA1E21A-08FA-4F02-8C25-33C81C8EE970}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{BFA1E21A-08FA-4F02-8C25-33C81C8EE970}"/>
   </bookViews>
   <sheets>
     <sheet name="Avichal" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="67">
   <si>
     <t>Date</t>
   </si>
@@ -245,6 +245,15 @@
   <si>
     <t>Waiting PM's Lead</t>
   </si>
+  <si>
+    <t>Developed an invoice generation feature for a Flask-based enrollment system, starting with the UI in fees.html and linking it to the backend. Initially, used pdfkit to convert an HTML template to a PDF, but encountered wkhtmltopdf setup issues. To simplify, switched to ReportLab, a pure-Python library, and modified the Flask route to generate the PDF programmatically. This involved creating the PDF structure and content directly within the Python code and sending it as a download. Throughout the process, corrected routing in the HTML files to ensure proper navigation within the Flask application.</t>
+  </si>
+  <si>
+    <t>Models for Enrollment N Fees</t>
+  </si>
+  <si>
+    <t>Happy Thurday PM :)</t>
+  </si>
 </sst>
 </file>
 
@@ -254,7 +263,7 @@
     <numFmt numFmtId="164" formatCode="h"/>
     <numFmt numFmtId="165" formatCode="d/mm/yyyy;@"/>
   </numFmts>
-  <fonts count="3">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -295,7 +304,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -308,8 +317,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="2" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
@@ -317,15 +324,6 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="35">
-    <dxf>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="14" formatCode="0.00%"/>
-    </dxf>
     <dxf>
       <numFmt numFmtId="30" formatCode="@"/>
     </dxf>
@@ -378,7 +376,7 @@
       <numFmt numFmtId="30" formatCode="@"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="19" formatCode="m/d/yyyy"/>
+      <numFmt numFmtId="166" formatCode="m/d/yyyy"/>
     </dxf>
     <dxf>
       <font>
@@ -405,7 +403,16 @@
       <numFmt numFmtId="30" formatCode="@"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="19" formatCode="m/d/yyyy"/>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="14" formatCode="0.00%"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="166" formatCode="m/d/yyyy"/>
     </dxf>
     <dxf>
       <font>
@@ -477,7 +484,7 @@
       <numFmt numFmtId="30" formatCode="@"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="19" formatCode="m/d/yyyy"/>
+      <numFmt numFmtId="166" formatCode="m/d/yyyy"/>
     </dxf>
     <dxf>
       <font>
@@ -579,17 +586,17 @@
     <tableColumn id="2" xr3:uid="{EBFC72C6-272F-4910-98B7-AD481D68F5CF}" name="Member Name" dataDxfId="18"/>
     <tableColumn id="3" xr3:uid="{9F5B3984-7002-4FEA-8B81-D2D8284783D7}" name="Task/Activity"/>
     <tableColumn id="4" xr3:uid="{5F85F44B-886F-440F-9E69-8335A039C2E6}" name="Status"/>
-    <tableColumn id="5" xr3:uid="{AF0043ED-9EF2-470B-9735-7321011714BA}" name="% Complete" dataDxfId="2"/>
-    <tableColumn id="6" xr3:uid="{4F961AD8-B86B-411C-BB04-8D7EE4DD134D}" name="Hours Worked Today" dataDxfId="0"/>
-    <tableColumn id="7" xr3:uid="{34EBB1FC-FFD7-47AB-A959-A220B742401C}" name="Next Steps" dataDxfId="1"/>
-    <tableColumn id="8" xr3:uid="{128DAA9E-15FB-4BB9-B76B-4A920C859038}" name="Notes/Comments" dataDxfId="17"/>
+    <tableColumn id="5" xr3:uid="{AF0043ED-9EF2-470B-9735-7321011714BA}" name="% Complete" dataDxfId="17"/>
+    <tableColumn id="6" xr3:uid="{4F961AD8-B86B-411C-BB04-8D7EE4DD134D}" name="Hours Worked Today" dataDxfId="16"/>
+    <tableColumn id="7" xr3:uid="{34EBB1FC-FFD7-47AB-A959-A220B742401C}" name="Next Steps" dataDxfId="15"/>
+    <tableColumn id="8" xr3:uid="{128DAA9E-15FB-4BB9-B76B-4A920C859038}" name="Notes/Comments" dataDxfId="14"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium26" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{646C4EC7-41A3-4570-9D38-06D55FDE20F6}" name="Table15" displayName="Table15" ref="A1:H100" totalsRowShown="0" headerRowDxfId="16">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{646C4EC7-41A3-4570-9D38-06D55FDE20F6}" name="Table15" displayName="Table15" ref="A1:H100" totalsRowShown="0" headerRowDxfId="13">
   <autoFilter ref="A1:H100" xr:uid="{646C4EC7-41A3-4570-9D38-06D55FDE20F6}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
@@ -601,21 +608,21 @@
     <filterColumn colId="7" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="8">
-    <tableColumn id="1" xr3:uid="{13D6CE41-CF73-478C-B7F6-3B0C25C48DFD}" name="Date" dataDxfId="15"/>
-    <tableColumn id="2" xr3:uid="{E468B109-F9F1-48D8-BECE-0F7015DD8D95}" name="Member Name" dataDxfId="14"/>
+    <tableColumn id="1" xr3:uid="{13D6CE41-CF73-478C-B7F6-3B0C25C48DFD}" name="Date" dataDxfId="12"/>
+    <tableColumn id="2" xr3:uid="{E468B109-F9F1-48D8-BECE-0F7015DD8D95}" name="Member Name" dataDxfId="11"/>
     <tableColumn id="3" xr3:uid="{279E5366-E900-45EE-80D9-5446A85E61AD}" name="Task/Activity"/>
     <tableColumn id="4" xr3:uid="{63D996BE-E8E2-4186-8CD4-49EAB9AA8847}" name="Status"/>
-    <tableColumn id="5" xr3:uid="{2FF82CF3-E17A-4896-9C9C-7339D28CD4A7}" name="% Complete" dataDxfId="13"/>
-    <tableColumn id="6" xr3:uid="{67DCB379-6881-4BBC-A633-BD51853A9B6B}" name="Hours Worked Today" dataDxfId="12"/>
-    <tableColumn id="7" xr3:uid="{91C8F225-F251-45F2-BC41-843547B77A6F}" name="Next Steps" dataDxfId="11"/>
-    <tableColumn id="8" xr3:uid="{EEAB1D68-5668-4B1F-8473-D3A49DA7E015}" name="Notes/Comments" dataDxfId="10"/>
+    <tableColumn id="5" xr3:uid="{2FF82CF3-E17A-4896-9C9C-7339D28CD4A7}" name="% Complete" dataDxfId="10"/>
+    <tableColumn id="6" xr3:uid="{67DCB379-6881-4BBC-A633-BD51853A9B6B}" name="Hours Worked Today" dataDxfId="9"/>
+    <tableColumn id="7" xr3:uid="{91C8F225-F251-45F2-BC41-843547B77A6F}" name="Next Steps" dataDxfId="8"/>
+    <tableColumn id="8" xr3:uid="{EEAB1D68-5668-4B1F-8473-D3A49DA7E015}" name="Notes/Comments" dataDxfId="7"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium26" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{5818BB59-8F2C-4810-A78D-CBC8FA25F524}" name="Table5" displayName="Table5" ref="A1:J100" totalsRowShown="0" headerRowDxfId="9">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{5818BB59-8F2C-4810-A78D-CBC8FA25F524}" name="Table5" displayName="Table5" ref="A1:J100" totalsRowShown="0" headerRowDxfId="6">
   <autoFilter ref="A1:J100" xr:uid="{5818BB59-8F2C-4810-A78D-CBC8FA25F524}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
@@ -629,16 +636,16 @@
     <filterColumn colId="9" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="10">
-    <tableColumn id="1" xr3:uid="{BC250DF1-329E-4733-8702-E009738E43CB}" name="Header" dataDxfId="8"/>
-    <tableColumn id="2" xr3:uid="{F6CCDA73-9A12-472B-A535-0F3DC2A5CF61}" name="Date Raised" dataDxfId="7"/>
+    <tableColumn id="1" xr3:uid="{BC250DF1-329E-4733-8702-E009738E43CB}" name="Header" dataDxfId="5"/>
+    <tableColumn id="2" xr3:uid="{F6CCDA73-9A12-472B-A535-0F3DC2A5CF61}" name="Date Raised" dataDxfId="4"/>
     <tableColumn id="3" xr3:uid="{2E3C7862-32AA-44B8-BCC3-2F9299A8F3DC}" name="Raised By"/>
-    <tableColumn id="4" xr3:uid="{FB9438A9-92FB-4A8D-95A5-F17D6EF9AA82}" name="Issue Description" dataDxfId="6"/>
+    <tableColumn id="4" xr3:uid="{FB9438A9-92FB-4A8D-95A5-F17D6EF9AA82}" name="Issue Description" dataDxfId="3"/>
     <tableColumn id="5" xr3:uid="{48223256-C4C0-467B-9FA7-AA8E7742B58A}" name="Impact"/>
     <tableColumn id="6" xr3:uid="{EEDBAAB2-0361-4BF5-8FDB-3FAD49E87C1B}" name="Priority"/>
     <tableColumn id="7" xr3:uid="{515F6321-7FC0-4B4E-A422-3A0E332B7B97}" name="Status"/>
-    <tableColumn id="8" xr3:uid="{60A704D7-818B-442C-91EF-B82765B2618D}" name="Resolution Plan" dataDxfId="5"/>
-    <tableColumn id="9" xr3:uid="{D95E2A6F-E7D4-4FC5-9AAF-1E3DBEE8D8FC}" name="Date Resolved" dataDxfId="4"/>
-    <tableColumn id="10" xr3:uid="{D43B4A1C-AE3D-43D4-A514-7BAA3E281FD3}" name="Notes/Comments" dataDxfId="3"/>
+    <tableColumn id="8" xr3:uid="{60A704D7-818B-442C-91EF-B82765B2618D}" name="Resolution Plan" dataDxfId="2"/>
+    <tableColumn id="9" xr3:uid="{D95E2A6F-E7D4-4FC5-9AAF-1E3DBEE8D8FC}" name="Date Resolved" dataDxfId="1"/>
+    <tableColumn id="10" xr3:uid="{D43B4A1C-AE3D-43D4-A514-7BAA3E281FD3}" name="Notes/Comments" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight15" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -992,30 +999,30 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{37EAA098-74C6-4411-B7E2-26AD2DCBC3F0}">
   <dimension ref="A1:H28"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H7" sqref="H7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.36328125" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.6328125" style="2" customWidth="1"/>
+    <col min="1" max="1" width="10.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.5703125" style="2" customWidth="1"/>
     <col min="3" max="3" width="58" customWidth="1"/>
-    <col min="5" max="5" width="13.08984375" style="3" customWidth="1"/>
-    <col min="6" max="6" width="20.90625" style="4" customWidth="1"/>
-    <col min="7" max="7" width="34.90625" style="2" customWidth="1"/>
-    <col min="8" max="8" width="43.36328125" style="2" customWidth="1"/>
-    <col min="11" max="11" width="9.08984375" customWidth="1"/>
-    <col min="12" max="12" width="13.26953125" customWidth="1"/>
-    <col min="13" max="13" width="11.36328125" customWidth="1"/>
-    <col min="14" max="14" width="17.36328125" customWidth="1"/>
-    <col min="16" max="16" width="9.08984375" customWidth="1"/>
-    <col min="18" max="18" width="16.6328125" customWidth="1"/>
-    <col min="19" max="19" width="14.7265625" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="16.90625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.140625" style="3" customWidth="1"/>
+    <col min="6" max="6" width="20.85546875" style="4" customWidth="1"/>
+    <col min="7" max="7" width="34.85546875" style="2" customWidth="1"/>
+    <col min="8" max="8" width="43.42578125" style="2" customWidth="1"/>
+    <col min="11" max="11" width="9.140625" customWidth="1"/>
+    <col min="12" max="12" width="13.28515625" customWidth="1"/>
+    <col min="13" max="13" width="11.42578125" customWidth="1"/>
+    <col min="14" max="14" width="17.42578125" customWidth="1"/>
+    <col min="16" max="16" width="9.140625" customWidth="1"/>
+    <col min="18" max="18" width="16.5703125" customWidth="1"/>
+    <col min="19" max="19" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="16.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="15.5">
+    <row r="1" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
@@ -1041,7 +1048,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:8">
+    <row r="2" spans="1:8" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A2" s="1">
         <v>45786</v>
       </c>
@@ -1067,7 +1074,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="3" spans="1:8" ht="116">
+    <row r="3" spans="1:8" ht="120" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>45787</v>
       </c>
@@ -1090,7 +1097,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="4" spans="1:8">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>45788</v>
       </c>
@@ -1110,7 +1117,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="5" spans="1:8" ht="76.5" customHeight="1">
+    <row r="5" spans="1:8" ht="76.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>45789</v>
       </c>
@@ -1133,7 +1140,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="6" spans="1:8">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>45790</v>
       </c>
@@ -1156,7 +1163,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="7" spans="1:8">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>45791</v>
       </c>
@@ -1179,76 +1186,95 @@
         <v>34</v>
       </c>
     </row>
-    <row r="8" spans="1:8">
-      <c r="E8"/>
-      <c r="F8"/>
-    </row>
-    <row r="9" spans="1:8">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A8" s="1">
+        <v>45792</v>
+      </c>
+      <c r="C8" t="s">
+        <v>64</v>
+      </c>
+      <c r="D8" t="s">
+        <v>17</v>
+      </c>
+      <c r="E8">
+        <v>100</v>
+      </c>
+      <c r="F8">
+        <v>3</v>
+      </c>
+      <c r="G8" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="H8" s="2" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="E9"/>
       <c r="F9"/>
     </row>
-    <row r="10" spans="1:8">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="E10"/>
       <c r="F10"/>
     </row>
-    <row r="11" spans="1:8">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="E11"/>
       <c r="F11"/>
     </row>
-    <row r="12" spans="1:8">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="E12"/>
       <c r="F12"/>
     </row>
-    <row r="13" spans="1:8">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="E13"/>
       <c r="F13"/>
     </row>
-    <row r="14" spans="1:8">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="E14"/>
       <c r="F14"/>
     </row>
-    <row r="15" spans="1:8">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="E15"/>
       <c r="F15"/>
     </row>
-    <row r="16" spans="1:8">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="E16"/>
       <c r="F16"/>
     </row>
-    <row r="17" spans="6:6">
+    <row r="17" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F17"/>
     </row>
-    <row r="18" spans="6:6">
+    <row r="18" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F18"/>
     </row>
-    <row r="19" spans="6:6">
+    <row r="19" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F19"/>
     </row>
-    <row r="20" spans="6:6">
+    <row r="20" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F20"/>
     </row>
-    <row r="21" spans="6:6">
+    <row r="21" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F21"/>
     </row>
-    <row r="22" spans="6:6">
+    <row r="22" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F22"/>
     </row>
-    <row r="23" spans="6:6">
+    <row r="23" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F23"/>
     </row>
-    <row r="24" spans="6:6">
+    <row r="24" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F24"/>
     </row>
-    <row r="25" spans="6:6">
+    <row r="25" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F25"/>
     </row>
-    <row r="26" spans="6:6">
+    <row r="26" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F26"/>
     </row>
-    <row r="27" spans="6:6">
+    <row r="27" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F27"/>
     </row>
-    <row r="28" spans="6:6">
+    <row r="28" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F28"/>
     </row>
   </sheetData>
@@ -1271,7 +1297,7 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
   <ignoredErrors>
-    <ignoredError sqref="D8:D16" listDataValidation="1"/>
+    <ignoredError sqref="D9:D16" listDataValidation="1"/>
   </ignoredErrors>
   <tableParts count="1">
     <tablePart r:id="rId2"/>
@@ -1287,19 +1313,19 @@
       <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.90625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="17.26953125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="55.6328125" customWidth="1"/>
-    <col min="4" max="4" width="10.6328125" customWidth="1"/>
-    <col min="5" max="5" width="14.90625" style="11" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14.26953125" style="11" customWidth="1"/>
-    <col min="7" max="7" width="92.90625" customWidth="1"/>
-    <col min="8" max="8" width="82.453125" customWidth="1"/>
+    <col min="1" max="1" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="55.5703125" customWidth="1"/>
+    <col min="4" max="4" width="10.5703125" customWidth="1"/>
+    <col min="5" max="5" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.28515625" customWidth="1"/>
+    <col min="7" max="7" width="92.85546875" customWidth="1"/>
+    <col min="8" max="8" width="82.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="15.5">
+    <row r="1" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
@@ -1312,10 +1338,10 @@
       <c r="D1" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="10" t="s">
+      <c r="E1" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="10" t="s">
+      <c r="F1" s="7" t="s">
         <v>5</v>
       </c>
       <c r="G1" s="7" t="s">
@@ -1325,7 +1351,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:8">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="8">
         <v>45786</v>
       </c>
@@ -1338,10 +1364,10 @@
       <c r="D2" t="s">
         <v>37</v>
       </c>
-      <c r="E2" s="11">
+      <c r="E2">
         <v>90</v>
       </c>
-      <c r="F2" s="11">
+      <c r="F2">
         <v>8</v>
       </c>
       <c r="G2" s="2" t="s">
@@ -1351,7 +1377,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="3" spans="1:8">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="8">
         <v>45787</v>
       </c>
@@ -1364,10 +1390,10 @@
       <c r="D3" t="s">
         <v>37</v>
       </c>
-      <c r="E3" s="11">
+      <c r="E3">
         <v>90</v>
       </c>
-      <c r="F3" s="11">
+      <c r="F3">
         <v>8</v>
       </c>
       <c r="G3" s="2" t="s">
@@ -1377,7 +1403,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="4" spans="1:8">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="8">
         <v>45789</v>
       </c>
@@ -1390,10 +1416,10 @@
       <c r="D4" t="s">
         <v>37</v>
       </c>
-      <c r="E4" s="11">
+      <c r="E4">
         <v>90</v>
       </c>
-      <c r="F4" s="11">
+      <c r="F4">
         <v>5</v>
       </c>
       <c r="G4" s="2" t="s">
@@ -1401,7 +1427,7 @@
       </c>
       <c r="H4" s="2"/>
     </row>
-    <row r="5" spans="1:8">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="8">
         <v>45790</v>
       </c>
@@ -1414,10 +1440,10 @@
       <c r="D5" t="s">
         <v>17</v>
       </c>
-      <c r="E5" s="11">
+      <c r="E5">
         <v>100</v>
       </c>
-      <c r="F5" s="11">
+      <c r="F5">
         <v>5</v>
       </c>
       <c r="G5" s="2" t="s">
@@ -1425,7 +1451,7 @@
       </c>
       <c r="H5" s="2"/>
     </row>
-    <row r="6" spans="1:8">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="8">
         <v>45791</v>
       </c>
@@ -1438,10 +1464,10 @@
       <c r="D6" t="s">
         <v>17</v>
       </c>
-      <c r="E6" s="11">
+      <c r="E6">
         <v>100</v>
       </c>
-      <c r="F6" s="11">
+      <c r="F6">
         <v>5</v>
       </c>
       <c r="G6" s="2" t="s">
@@ -1451,565 +1477,565 @@
         <v>49</v>
       </c>
     </row>
-    <row r="7" spans="1:8">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="8"/>
       <c r="B7" s="2"/>
       <c r="G7" s="2"/>
       <c r="H7" s="2"/>
     </row>
-    <row r="8" spans="1:8">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="8"/>
       <c r="B8" s="2"/>
       <c r="G8" s="2"/>
       <c r="H8" s="2"/>
     </row>
-    <row r="9" spans="1:8">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="8"/>
       <c r="B9" s="2"/>
       <c r="G9" s="2"/>
       <c r="H9" s="2"/>
     </row>
-    <row r="10" spans="1:8">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="8"/>
       <c r="B10" s="2"/>
       <c r="G10" s="2"/>
       <c r="H10" s="2"/>
     </row>
-    <row r="11" spans="1:8">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="8"/>
       <c r="B11" s="2"/>
       <c r="G11" s="2"/>
       <c r="H11" s="2"/>
     </row>
-    <row r="12" spans="1:8">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="8"/>
       <c r="B12" s="2"/>
       <c r="G12" s="2"/>
       <c r="H12" s="2"/>
     </row>
-    <row r="13" spans="1:8">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="8"/>
       <c r="B13" s="2"/>
       <c r="G13" s="2"/>
       <c r="H13" s="2"/>
     </row>
-    <row r="14" spans="1:8">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" s="8"/>
       <c r="B14" s="2"/>
       <c r="G14" s="2"/>
       <c r="H14" s="2"/>
     </row>
-    <row r="15" spans="1:8">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" s="8"/>
       <c r="B15" s="2"/>
       <c r="G15" s="2"/>
       <c r="H15" s="2"/>
     </row>
-    <row r="16" spans="1:8">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" s="8"/>
       <c r="B16" s="2"/>
       <c r="G16" s="2"/>
       <c r="H16" s="2"/>
     </row>
-    <row r="17" spans="1:8">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" s="8"/>
       <c r="B17" s="2"/>
       <c r="G17" s="2"/>
       <c r="H17" s="2"/>
     </row>
-    <row r="18" spans="1:8">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" s="8"/>
       <c r="B18" s="2"/>
       <c r="G18" s="2"/>
       <c r="H18" s="2"/>
     </row>
-    <row r="19" spans="1:8">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" s="8"/>
       <c r="B19" s="2"/>
       <c r="G19" s="2"/>
       <c r="H19" s="2"/>
     </row>
-    <row r="20" spans="1:8">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" s="8"/>
       <c r="B20" s="2"/>
       <c r="G20" s="2"/>
       <c r="H20" s="2"/>
     </row>
-    <row r="21" spans="1:8">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" s="8"/>
       <c r="B21" s="2"/>
       <c r="G21" s="2"/>
       <c r="H21" s="2"/>
     </row>
-    <row r="22" spans="1:8">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" s="8"/>
       <c r="B22" s="2"/>
       <c r="G22" s="2"/>
       <c r="H22" s="2"/>
     </row>
-    <row r="23" spans="1:8">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" s="8"/>
       <c r="B23" s="2"/>
       <c r="G23" s="2"/>
       <c r="H23" s="2"/>
     </row>
-    <row r="24" spans="1:8">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24" s="8"/>
       <c r="B24" s="2"/>
       <c r="G24" s="2"/>
       <c r="H24" s="2"/>
     </row>
-    <row r="25" spans="1:8">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25" s="8"/>
       <c r="B25" s="2"/>
       <c r="G25" s="2"/>
       <c r="H25" s="2"/>
     </row>
-    <row r="26" spans="1:8">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26" s="8"/>
       <c r="B26" s="2"/>
       <c r="G26" s="2"/>
       <c r="H26" s="2"/>
     </row>
-    <row r="27" spans="1:8">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A27" s="8"/>
       <c r="B27" s="2"/>
       <c r="G27" s="2"/>
       <c r="H27" s="2"/>
     </row>
-    <row r="28" spans="1:8">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A28" s="8"/>
       <c r="B28" s="2"/>
       <c r="G28" s="2"/>
       <c r="H28" s="2"/>
     </row>
-    <row r="29" spans="1:8">
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A29" s="8"/>
       <c r="B29" s="2"/>
       <c r="G29" s="2"/>
       <c r="H29" s="2"/>
     </row>
-    <row r="30" spans="1:8">
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A30" s="8"/>
       <c r="B30" s="2"/>
       <c r="G30" s="2"/>
       <c r="H30" s="2"/>
     </row>
-    <row r="31" spans="1:8">
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A31" s="8"/>
       <c r="B31" s="2"/>
       <c r="G31" s="2"/>
       <c r="H31" s="2"/>
     </row>
-    <row r="32" spans="1:8">
+    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A32" s="8"/>
       <c r="B32" s="2"/>
       <c r="G32" s="2"/>
       <c r="H32" s="2"/>
     </row>
-    <row r="33" spans="1:8">
+    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A33" s="8"/>
       <c r="B33" s="2"/>
       <c r="G33" s="2"/>
       <c r="H33" s="2"/>
     </row>
-    <row r="34" spans="1:8">
+    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A34" s="8"/>
       <c r="B34" s="2"/>
       <c r="G34" s="2"/>
       <c r="H34" s="2"/>
     </row>
-    <row r="35" spans="1:8">
+    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A35" s="8"/>
       <c r="B35" s="2"/>
       <c r="G35" s="2"/>
       <c r="H35" s="2"/>
     </row>
-    <row r="36" spans="1:8">
+    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A36" s="8"/>
       <c r="B36" s="2"/>
       <c r="G36" s="2"/>
       <c r="H36" s="2"/>
     </row>
-    <row r="37" spans="1:8">
+    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A37" s="8"/>
       <c r="B37" s="2"/>
       <c r="G37" s="2"/>
       <c r="H37" s="2"/>
     </row>
-    <row r="38" spans="1:8">
+    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A38" s="8"/>
       <c r="B38" s="2"/>
       <c r="G38" s="2"/>
       <c r="H38" s="2"/>
     </row>
-    <row r="39" spans="1:8">
+    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A39" s="8"/>
       <c r="B39" s="2"/>
       <c r="G39" s="2"/>
       <c r="H39" s="2"/>
     </row>
-    <row r="40" spans="1:8">
+    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A40" s="8"/>
       <c r="B40" s="2"/>
       <c r="G40" s="2"/>
       <c r="H40" s="2"/>
     </row>
-    <row r="41" spans="1:8">
+    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A41" s="8"/>
       <c r="B41" s="2"/>
       <c r="G41" s="2"/>
       <c r="H41" s="2"/>
     </row>
-    <row r="42" spans="1:8">
+    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A42" s="8"/>
       <c r="B42" s="2"/>
       <c r="G42" s="2"/>
       <c r="H42" s="2"/>
     </row>
-    <row r="43" spans="1:8">
+    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A43" s="8"/>
       <c r="B43" s="2"/>
       <c r="G43" s="2"/>
       <c r="H43" s="2"/>
     </row>
-    <row r="44" spans="1:8">
+    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A44" s="8"/>
       <c r="B44" s="2"/>
       <c r="G44" s="2"/>
       <c r="H44" s="2"/>
     </row>
-    <row r="45" spans="1:8">
+    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A45" s="8"/>
       <c r="B45" s="2"/>
       <c r="G45" s="2"/>
       <c r="H45" s="2"/>
     </row>
-    <row r="46" spans="1:8">
+    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A46" s="8"/>
       <c r="B46" s="2"/>
       <c r="G46" s="2"/>
       <c r="H46" s="2"/>
     </row>
-    <row r="47" spans="1:8">
+    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A47" s="8"/>
       <c r="B47" s="2"/>
       <c r="G47" s="2"/>
       <c r="H47" s="2"/>
     </row>
-    <row r="48" spans="1:8">
+    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A48" s="8"/>
       <c r="B48" s="2"/>
       <c r="G48" s="2"/>
       <c r="H48" s="2"/>
     </row>
-    <row r="49" spans="1:8">
+    <row r="49" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A49" s="8"/>
       <c r="B49" s="2"/>
       <c r="G49" s="2"/>
       <c r="H49" s="2"/>
     </row>
-    <row r="50" spans="1:8">
+    <row r="50" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A50" s="8"/>
       <c r="B50" s="2"/>
       <c r="G50" s="2"/>
       <c r="H50" s="2"/>
     </row>
-    <row r="51" spans="1:8">
+    <row r="51" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A51" s="8"/>
       <c r="B51" s="2"/>
       <c r="G51" s="2"/>
       <c r="H51" s="2"/>
     </row>
-    <row r="52" spans="1:8">
+    <row r="52" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A52" s="8"/>
       <c r="B52" s="2"/>
       <c r="G52" s="2"/>
       <c r="H52" s="2"/>
     </row>
-    <row r="53" spans="1:8">
+    <row r="53" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A53" s="8"/>
       <c r="B53" s="2"/>
       <c r="G53" s="2"/>
       <c r="H53" s="2"/>
     </row>
-    <row r="54" spans="1:8">
+    <row r="54" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A54" s="8"/>
       <c r="B54" s="2"/>
       <c r="G54" s="2"/>
       <c r="H54" s="2"/>
     </row>
-    <row r="55" spans="1:8">
+    <row r="55" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A55" s="8"/>
       <c r="B55" s="2"/>
       <c r="G55" s="2"/>
       <c r="H55" s="2"/>
     </row>
-    <row r="56" spans="1:8">
+    <row r="56" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A56" s="8"/>
       <c r="B56" s="2"/>
       <c r="G56" s="2"/>
       <c r="H56" s="2"/>
     </row>
-    <row r="57" spans="1:8">
+    <row r="57" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A57" s="8"/>
       <c r="B57" s="2"/>
       <c r="G57" s="2"/>
       <c r="H57" s="2"/>
     </row>
-    <row r="58" spans="1:8">
+    <row r="58" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A58" s="8"/>
       <c r="B58" s="2"/>
       <c r="G58" s="2"/>
       <c r="H58" s="2"/>
     </row>
-    <row r="59" spans="1:8">
+    <row r="59" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A59" s="8"/>
       <c r="B59" s="2"/>
       <c r="G59" s="2"/>
       <c r="H59" s="2"/>
     </row>
-    <row r="60" spans="1:8">
+    <row r="60" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A60" s="8"/>
       <c r="B60" s="2"/>
       <c r="G60" s="2"/>
       <c r="H60" s="2"/>
     </row>
-    <row r="61" spans="1:8">
+    <row r="61" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A61" s="8"/>
       <c r="B61" s="2"/>
       <c r="G61" s="2"/>
       <c r="H61" s="2"/>
     </row>
-    <row r="62" spans="1:8">
+    <row r="62" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A62" s="8"/>
       <c r="B62" s="2"/>
       <c r="G62" s="2"/>
       <c r="H62" s="2"/>
     </row>
-    <row r="63" spans="1:8">
+    <row r="63" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A63" s="8"/>
       <c r="B63" s="2"/>
       <c r="G63" s="2"/>
       <c r="H63" s="2"/>
     </row>
-    <row r="64" spans="1:8">
+    <row r="64" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A64" s="8"/>
       <c r="B64" s="2"/>
       <c r="G64" s="2"/>
       <c r="H64" s="2"/>
     </row>
-    <row r="65" spans="1:8">
+    <row r="65" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A65" s="8"/>
       <c r="B65" s="2"/>
       <c r="G65" s="2"/>
       <c r="H65" s="2"/>
     </row>
-    <row r="66" spans="1:8">
+    <row r="66" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A66" s="8"/>
       <c r="B66" s="2"/>
       <c r="G66" s="2"/>
       <c r="H66" s="2"/>
     </row>
-    <row r="67" spans="1:8">
+    <row r="67" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A67" s="8"/>
       <c r="B67" s="2"/>
       <c r="G67" s="2"/>
       <c r="H67" s="2"/>
     </row>
-    <row r="68" spans="1:8">
+    <row r="68" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A68" s="8"/>
       <c r="B68" s="2"/>
       <c r="G68" s="2"/>
       <c r="H68" s="2"/>
     </row>
-    <row r="69" spans="1:8">
+    <row r="69" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A69" s="8"/>
       <c r="B69" s="2"/>
       <c r="G69" s="2"/>
       <c r="H69" s="2"/>
     </row>
-    <row r="70" spans="1:8">
+    <row r="70" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A70" s="8"/>
       <c r="B70" s="2"/>
       <c r="G70" s="2"/>
       <c r="H70" s="2"/>
     </row>
-    <row r="71" spans="1:8">
+    <row r="71" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A71" s="8"/>
       <c r="B71" s="2"/>
       <c r="G71" s="2"/>
       <c r="H71" s="2"/>
     </row>
-    <row r="72" spans="1:8">
+    <row r="72" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A72" s="8"/>
       <c r="B72" s="2"/>
       <c r="G72" s="2"/>
       <c r="H72" s="2"/>
     </row>
-    <row r="73" spans="1:8">
+    <row r="73" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A73" s="8"/>
       <c r="B73" s="2"/>
       <c r="G73" s="2"/>
       <c r="H73" s="2"/>
     </row>
-    <row r="74" spans="1:8">
+    <row r="74" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A74" s="8"/>
       <c r="B74" s="2"/>
       <c r="G74" s="2"/>
       <c r="H74" s="2"/>
     </row>
-    <row r="75" spans="1:8">
+    <row r="75" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A75" s="8"/>
       <c r="B75" s="2"/>
       <c r="G75" s="2"/>
       <c r="H75" s="2"/>
     </row>
-    <row r="76" spans="1:8">
+    <row r="76" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A76" s="8"/>
       <c r="B76" s="2"/>
       <c r="G76" s="2"/>
       <c r="H76" s="2"/>
     </row>
-    <row r="77" spans="1:8">
+    <row r="77" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A77" s="8"/>
       <c r="B77" s="2"/>
       <c r="G77" s="2"/>
       <c r="H77" s="2"/>
     </row>
-    <row r="78" spans="1:8">
+    <row r="78" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A78" s="8"/>
       <c r="B78" s="2"/>
       <c r="G78" s="2"/>
       <c r="H78" s="2"/>
     </row>
-    <row r="79" spans="1:8">
+    <row r="79" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A79" s="8"/>
       <c r="B79" s="2"/>
       <c r="G79" s="2"/>
       <c r="H79" s="2"/>
     </row>
-    <row r="80" spans="1:8">
+    <row r="80" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A80" s="8"/>
       <c r="B80" s="2"/>
       <c r="G80" s="2"/>
       <c r="H80" s="2"/>
     </row>
-    <row r="81" spans="1:8">
+    <row r="81" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A81" s="8"/>
       <c r="B81" s="2"/>
       <c r="G81" s="2"/>
       <c r="H81" s="2"/>
     </row>
-    <row r="82" spans="1:8">
+    <row r="82" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A82" s="8"/>
       <c r="B82" s="2"/>
       <c r="G82" s="2"/>
       <c r="H82" s="2"/>
     </row>
-    <row r="83" spans="1:8">
+    <row r="83" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A83" s="8"/>
       <c r="B83" s="2"/>
       <c r="G83" s="2"/>
       <c r="H83" s="2"/>
     </row>
-    <row r="84" spans="1:8">
+    <row r="84" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A84" s="8"/>
       <c r="B84" s="2"/>
       <c r="G84" s="2"/>
       <c r="H84" s="2"/>
     </row>
-    <row r="85" spans="1:8">
+    <row r="85" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A85" s="8"/>
       <c r="B85" s="2"/>
       <c r="G85" s="2"/>
       <c r="H85" s="2"/>
     </row>
-    <row r="86" spans="1:8">
+    <row r="86" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A86" s="8"/>
       <c r="B86" s="2"/>
       <c r="G86" s="2"/>
       <c r="H86" s="2"/>
     </row>
-    <row r="87" spans="1:8">
+    <row r="87" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A87" s="8"/>
       <c r="B87" s="2"/>
       <c r="G87" s="2"/>
       <c r="H87" s="2"/>
     </row>
-    <row r="88" spans="1:8">
+    <row r="88" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A88" s="8"/>
       <c r="B88" s="2"/>
       <c r="G88" s="2"/>
       <c r="H88" s="2"/>
     </row>
-    <row r="89" spans="1:8">
+    <row r="89" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A89" s="8"/>
       <c r="B89" s="2"/>
       <c r="G89" s="2"/>
       <c r="H89" s="2"/>
     </row>
-    <row r="90" spans="1:8">
+    <row r="90" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A90" s="8"/>
       <c r="B90" s="2"/>
       <c r="G90" s="2"/>
       <c r="H90" s="2"/>
     </row>
-    <row r="91" spans="1:8">
+    <row r="91" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A91" s="8"/>
       <c r="B91" s="2"/>
       <c r="G91" s="2"/>
       <c r="H91" s="2"/>
     </row>
-    <row r="92" spans="1:8">
+    <row r="92" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A92" s="8"/>
       <c r="B92" s="2"/>
       <c r="G92" s="2"/>
       <c r="H92" s="2"/>
     </row>
-    <row r="93" spans="1:8">
+    <row r="93" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A93" s="8"/>
       <c r="B93" s="2"/>
       <c r="G93" s="2"/>
       <c r="H93" s="2"/>
     </row>
-    <row r="94" spans="1:8">
+    <row r="94" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A94" s="8"/>
       <c r="B94" s="2"/>
       <c r="G94" s="2"/>
       <c r="H94" s="2"/>
     </row>
-    <row r="95" spans="1:8">
+    <row r="95" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A95" s="8"/>
       <c r="B95" s="2"/>
       <c r="G95" s="2"/>
       <c r="H95" s="2"/>
     </row>
-    <row r="96" spans="1:8">
+    <row r="96" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A96" s="8"/>
       <c r="B96" s="2"/>
       <c r="G96" s="2"/>
       <c r="H96" s="2"/>
     </row>
-    <row r="97" spans="1:8">
+    <row r="97" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A97" s="8"/>
       <c r="B97" s="2"/>
       <c r="G97" s="2"/>
       <c r="H97" s="2"/>
     </row>
-    <row r="98" spans="1:8">
+    <row r="98" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A98" s="8"/>
       <c r="B98" s="2"/>
       <c r="G98" s="2"/>
       <c r="H98" s="2"/>
     </row>
-    <row r="99" spans="1:8">
+    <row r="99" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A99" s="8"/>
       <c r="B99" s="2"/>
       <c r="G99" s="2"/>
       <c r="H99" s="2"/>
     </row>
-    <row r="100" spans="1:8">
+    <row r="100" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A100" s="8"/>
       <c r="B100" s="2"/>
       <c r="G100" s="2"/>
@@ -2046,23 +2072,23 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9FD6A201-8E63-4A9E-A683-19506CB489E3}">
   <dimension ref="A1:H100"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.08984375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="17.26953125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="27.81640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.7265625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.90625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="23.6328125" style="12" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="39.08984375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="51.08984375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="27.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="23.5703125" style="10" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="39.140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="51.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="15.5">
+    <row r="1" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
@@ -2078,7 +2104,7 @@
       <c r="E1" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="13" t="s">
+      <c r="F1" s="11" t="s">
         <v>5</v>
       </c>
       <c r="G1" s="7" t="s">
@@ -2088,7 +2114,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:8">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>45935</v>
       </c>
@@ -2104,7 +2130,7 @@
       <c r="E2" s="3">
         <v>1</v>
       </c>
-      <c r="F2" s="12">
+      <c r="F2" s="10">
         <v>4</v>
       </c>
       <c r="G2" s="2" t="s">
@@ -2114,7 +2140,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="3" spans="1:8">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>45996</v>
       </c>
@@ -2130,7 +2156,7 @@
       <c r="E3" s="3">
         <v>1</v>
       </c>
-      <c r="F3" s="12">
+      <c r="F3" s="10">
         <v>4</v>
       </c>
       <c r="G3" s="2" t="s">
@@ -2140,7 +2166,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="4" spans="1:8">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>57</v>
       </c>
@@ -2156,7 +2182,7 @@
       <c r="E4" s="3">
         <v>1</v>
       </c>
-      <c r="F4" s="12">
+      <c r="F4" s="10">
         <v>4</v>
       </c>
       <c r="G4" s="2" t="s">
@@ -2166,7 +2192,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="5" spans="1:8">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>61</v>
       </c>
@@ -2182,7 +2208,7 @@
       <c r="E5" s="3">
         <v>1</v>
       </c>
-      <c r="F5" s="12">
+      <c r="F5" s="10">
         <v>5</v>
       </c>
       <c r="G5" s="2" t="s">
@@ -2192,665 +2218,665 @@
         <v>54</v>
       </c>
     </row>
-    <row r="6" spans="1:8">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="1"/>
       <c r="B6" s="2"/>
       <c r="E6" s="3"/>
       <c r="G6" s="2"/>
       <c r="H6" s="2"/>
     </row>
-    <row r="7" spans="1:8">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="1"/>
       <c r="B7" s="2"/>
       <c r="E7" s="3"/>
       <c r="G7" s="2"/>
       <c r="H7" s="2"/>
     </row>
-    <row r="8" spans="1:8">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="1"/>
       <c r="B8" s="2"/>
       <c r="E8" s="3"/>
       <c r="G8" s="2"/>
       <c r="H8" s="2"/>
     </row>
-    <row r="9" spans="1:8">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="1"/>
       <c r="B9" s="2"/>
       <c r="E9" s="3"/>
       <c r="G9" s="2"/>
       <c r="H9" s="2"/>
     </row>
-    <row r="10" spans="1:8">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="1"/>
       <c r="B10" s="2"/>
       <c r="E10" s="3"/>
       <c r="G10" s="2"/>
       <c r="H10" s="2"/>
     </row>
-    <row r="11" spans="1:8">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="1"/>
       <c r="B11" s="2"/>
       <c r="E11" s="3"/>
       <c r="G11" s="2"/>
       <c r="H11" s="2"/>
     </row>
-    <row r="12" spans="1:8">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="1"/>
       <c r="B12" s="2"/>
       <c r="E12" s="3"/>
       <c r="G12" s="2"/>
       <c r="H12" s="2"/>
     </row>
-    <row r="13" spans="1:8">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="1"/>
       <c r="B13" s="2"/>
       <c r="E13" s="3"/>
       <c r="G13" s="2"/>
       <c r="H13" s="2"/>
     </row>
-    <row r="14" spans="1:8">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" s="1"/>
       <c r="B14" s="2"/>
       <c r="E14" s="3"/>
       <c r="G14" s="2"/>
       <c r="H14" s="2"/>
     </row>
-    <row r="15" spans="1:8">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" s="1"/>
       <c r="B15" s="2"/>
       <c r="E15" s="3"/>
       <c r="G15" s="2"/>
       <c r="H15" s="2"/>
     </row>
-    <row r="16" spans="1:8">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" s="1"/>
       <c r="B16" s="2"/>
       <c r="E16" s="3"/>
       <c r="G16" s="2"/>
       <c r="H16" s="2"/>
     </row>
-    <row r="17" spans="1:8">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" s="1"/>
       <c r="B17" s="2"/>
       <c r="E17" s="3"/>
       <c r="G17" s="2"/>
       <c r="H17" s="2"/>
     </row>
-    <row r="18" spans="1:8">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" s="1"/>
       <c r="B18" s="2"/>
       <c r="E18" s="3"/>
       <c r="G18" s="2"/>
       <c r="H18" s="2"/>
     </row>
-    <row r="19" spans="1:8">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" s="1"/>
       <c r="B19" s="2"/>
       <c r="E19" s="3"/>
       <c r="G19" s="2"/>
       <c r="H19" s="2"/>
     </row>
-    <row r="20" spans="1:8">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" s="1"/>
       <c r="B20" s="2"/>
       <c r="E20" s="3"/>
       <c r="G20" s="2"/>
       <c r="H20" s="2"/>
     </row>
-    <row r="21" spans="1:8">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" s="1"/>
       <c r="B21" s="2"/>
       <c r="E21" s="3"/>
       <c r="G21" s="2"/>
       <c r="H21" s="2"/>
     </row>
-    <row r="22" spans="1:8">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" s="1"/>
       <c r="B22" s="2"/>
       <c r="E22" s="3"/>
       <c r="G22" s="2"/>
       <c r="H22" s="2"/>
     </row>
-    <row r="23" spans="1:8">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" s="1"/>
       <c r="B23" s="2"/>
       <c r="E23" s="3"/>
       <c r="G23" s="2"/>
       <c r="H23" s="2"/>
     </row>
-    <row r="24" spans="1:8">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24" s="1"/>
       <c r="B24" s="2"/>
       <c r="E24" s="3"/>
       <c r="G24" s="2"/>
       <c r="H24" s="2"/>
     </row>
-    <row r="25" spans="1:8">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25" s="1"/>
       <c r="B25" s="2"/>
       <c r="E25" s="3"/>
       <c r="G25" s="2"/>
       <c r="H25" s="2"/>
     </row>
-    <row r="26" spans="1:8">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26" s="1"/>
       <c r="B26" s="2"/>
       <c r="E26" s="3"/>
       <c r="G26" s="2"/>
       <c r="H26" s="2"/>
     </row>
-    <row r="27" spans="1:8">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A27" s="1"/>
       <c r="B27" s="2"/>
       <c r="E27" s="3"/>
       <c r="G27" s="2"/>
       <c r="H27" s="2"/>
     </row>
-    <row r="28" spans="1:8">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A28" s="1"/>
       <c r="B28" s="2"/>
       <c r="E28" s="3"/>
       <c r="G28" s="2"/>
       <c r="H28" s="2"/>
     </row>
-    <row r="29" spans="1:8">
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A29" s="1"/>
       <c r="B29" s="2"/>
       <c r="E29" s="3"/>
       <c r="G29" s="2"/>
       <c r="H29" s="2"/>
     </row>
-    <row r="30" spans="1:8">
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A30" s="1"/>
       <c r="B30" s="2"/>
       <c r="E30" s="3"/>
       <c r="G30" s="2"/>
       <c r="H30" s="2"/>
     </row>
-    <row r="31" spans="1:8">
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A31" s="1"/>
       <c r="B31" s="2"/>
       <c r="E31" s="3"/>
       <c r="G31" s="2"/>
       <c r="H31" s="2"/>
     </row>
-    <row r="32" spans="1:8">
+    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A32" s="1"/>
       <c r="B32" s="2"/>
       <c r="E32" s="3"/>
       <c r="G32" s="2"/>
       <c r="H32" s="2"/>
     </row>
-    <row r="33" spans="1:8">
+    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A33" s="1"/>
       <c r="B33" s="2"/>
       <c r="E33" s="3"/>
       <c r="G33" s="2"/>
       <c r="H33" s="2"/>
     </row>
-    <row r="34" spans="1:8">
+    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A34" s="1"/>
       <c r="B34" s="2"/>
       <c r="E34" s="3"/>
       <c r="G34" s="2"/>
       <c r="H34" s="2"/>
     </row>
-    <row r="35" spans="1:8">
+    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A35" s="1"/>
       <c r="B35" s="2"/>
       <c r="E35" s="3"/>
       <c r="G35" s="2"/>
       <c r="H35" s="2"/>
     </row>
-    <row r="36" spans="1:8">
+    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A36" s="1"/>
       <c r="B36" s="2"/>
       <c r="E36" s="3"/>
       <c r="G36" s="2"/>
       <c r="H36" s="2"/>
     </row>
-    <row r="37" spans="1:8">
+    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A37" s="1"/>
       <c r="B37" s="2"/>
       <c r="E37" s="3"/>
       <c r="G37" s="2"/>
       <c r="H37" s="2"/>
     </row>
-    <row r="38" spans="1:8">
+    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A38" s="1"/>
       <c r="B38" s="2"/>
       <c r="E38" s="3"/>
       <c r="G38" s="2"/>
       <c r="H38" s="2"/>
     </row>
-    <row r="39" spans="1:8">
+    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A39" s="1"/>
       <c r="B39" s="2"/>
       <c r="E39" s="3"/>
       <c r="G39" s="2"/>
       <c r="H39" s="2"/>
     </row>
-    <row r="40" spans="1:8">
+    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A40" s="1"/>
       <c r="B40" s="2"/>
       <c r="E40" s="3"/>
       <c r="G40" s="2"/>
       <c r="H40" s="2"/>
     </row>
-    <row r="41" spans="1:8">
+    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A41" s="1"/>
       <c r="B41" s="2"/>
       <c r="E41" s="3"/>
       <c r="G41" s="2"/>
       <c r="H41" s="2"/>
     </row>
-    <row r="42" spans="1:8">
+    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A42" s="1"/>
       <c r="B42" s="2"/>
       <c r="E42" s="3"/>
       <c r="G42" s="2"/>
       <c r="H42" s="2"/>
     </row>
-    <row r="43" spans="1:8">
+    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A43" s="1"/>
       <c r="B43" s="2"/>
       <c r="E43" s="3"/>
       <c r="G43" s="2"/>
       <c r="H43" s="2"/>
     </row>
-    <row r="44" spans="1:8">
+    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A44" s="1"/>
       <c r="B44" s="2"/>
       <c r="E44" s="3"/>
       <c r="G44" s="2"/>
       <c r="H44" s="2"/>
     </row>
-    <row r="45" spans="1:8">
+    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A45" s="1"/>
       <c r="B45" s="2"/>
       <c r="E45" s="3"/>
       <c r="G45" s="2"/>
       <c r="H45" s="2"/>
     </row>
-    <row r="46" spans="1:8">
+    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A46" s="1"/>
       <c r="B46" s="2"/>
       <c r="E46" s="3"/>
       <c r="G46" s="2"/>
       <c r="H46" s="2"/>
     </row>
-    <row r="47" spans="1:8">
+    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A47" s="1"/>
       <c r="B47" s="2"/>
       <c r="E47" s="3"/>
       <c r="G47" s="2"/>
       <c r="H47" s="2"/>
     </row>
-    <row r="48" spans="1:8">
+    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A48" s="1"/>
       <c r="B48" s="2"/>
       <c r="E48" s="3"/>
       <c r="G48" s="2"/>
       <c r="H48" s="2"/>
     </row>
-    <row r="49" spans="1:8">
+    <row r="49" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A49" s="1"/>
       <c r="B49" s="2"/>
       <c r="E49" s="3"/>
       <c r="G49" s="2"/>
       <c r="H49" s="2"/>
     </row>
-    <row r="50" spans="1:8">
+    <row r="50" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A50" s="1"/>
       <c r="B50" s="2"/>
       <c r="E50" s="3"/>
       <c r="G50" s="2"/>
       <c r="H50" s="2"/>
     </row>
-    <row r="51" spans="1:8">
+    <row r="51" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A51" s="1"/>
       <c r="B51" s="2"/>
       <c r="E51" s="3"/>
       <c r="G51" s="2"/>
       <c r="H51" s="2"/>
     </row>
-    <row r="52" spans="1:8">
+    <row r="52" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A52" s="1"/>
       <c r="B52" s="2"/>
       <c r="E52" s="3"/>
       <c r="G52" s="2"/>
       <c r="H52" s="2"/>
     </row>
-    <row r="53" spans="1:8">
+    <row r="53" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A53" s="1"/>
       <c r="B53" s="2"/>
       <c r="E53" s="3"/>
       <c r="G53" s="2"/>
       <c r="H53" s="2"/>
     </row>
-    <row r="54" spans="1:8">
+    <row r="54" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A54" s="1"/>
       <c r="B54" s="2"/>
       <c r="E54" s="3"/>
       <c r="G54" s="2"/>
       <c r="H54" s="2"/>
     </row>
-    <row r="55" spans="1:8">
+    <row r="55" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A55" s="1"/>
       <c r="B55" s="2"/>
       <c r="E55" s="3"/>
       <c r="G55" s="2"/>
       <c r="H55" s="2"/>
     </row>
-    <row r="56" spans="1:8">
+    <row r="56" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A56" s="1"/>
       <c r="B56" s="2"/>
       <c r="E56" s="3"/>
       <c r="G56" s="2"/>
       <c r="H56" s="2"/>
     </row>
-    <row r="57" spans="1:8">
+    <row r="57" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A57" s="1"/>
       <c r="B57" s="2"/>
       <c r="E57" s="3"/>
       <c r="G57" s="2"/>
       <c r="H57" s="2"/>
     </row>
-    <row r="58" spans="1:8">
+    <row r="58" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A58" s="1"/>
       <c r="B58" s="2"/>
       <c r="E58" s="3"/>
       <c r="G58" s="2"/>
       <c r="H58" s="2"/>
     </row>
-    <row r="59" spans="1:8">
+    <row r="59" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A59" s="1"/>
       <c r="B59" s="2"/>
       <c r="E59" s="3"/>
       <c r="G59" s="2"/>
       <c r="H59" s="2"/>
     </row>
-    <row r="60" spans="1:8">
+    <row r="60" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A60" s="1"/>
       <c r="B60" s="2"/>
       <c r="E60" s="3"/>
       <c r="G60" s="2"/>
       <c r="H60" s="2"/>
     </row>
-    <row r="61" spans="1:8">
+    <row r="61" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A61" s="1"/>
       <c r="B61" s="2"/>
       <c r="E61" s="3"/>
       <c r="G61" s="2"/>
       <c r="H61" s="2"/>
     </row>
-    <row r="62" spans="1:8">
+    <row r="62" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A62" s="1"/>
       <c r="B62" s="2"/>
       <c r="E62" s="3"/>
       <c r="G62" s="2"/>
       <c r="H62" s="2"/>
     </row>
-    <row r="63" spans="1:8">
+    <row r="63" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A63" s="1"/>
       <c r="B63" s="2"/>
       <c r="E63" s="3"/>
       <c r="G63" s="2"/>
       <c r="H63" s="2"/>
     </row>
-    <row r="64" spans="1:8">
+    <row r="64" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A64" s="1"/>
       <c r="B64" s="2"/>
       <c r="E64" s="3"/>
       <c r="G64" s="2"/>
       <c r="H64" s="2"/>
     </row>
-    <row r="65" spans="1:8">
+    <row r="65" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A65" s="1"/>
       <c r="B65" s="2"/>
       <c r="E65" s="3"/>
       <c r="G65" s="2"/>
       <c r="H65" s="2"/>
     </row>
-    <row r="66" spans="1:8">
+    <row r="66" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A66" s="1"/>
       <c r="B66" s="2"/>
       <c r="E66" s="3"/>
       <c r="G66" s="2"/>
       <c r="H66" s="2"/>
     </row>
-    <row r="67" spans="1:8">
+    <row r="67" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A67" s="1"/>
       <c r="B67" s="2"/>
       <c r="E67" s="3"/>
       <c r="G67" s="2"/>
       <c r="H67" s="2"/>
     </row>
-    <row r="68" spans="1:8">
+    <row r="68" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A68" s="1"/>
       <c r="B68" s="2"/>
       <c r="E68" s="3"/>
       <c r="G68" s="2"/>
       <c r="H68" s="2"/>
     </row>
-    <row r="69" spans="1:8">
+    <row r="69" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A69" s="1"/>
       <c r="B69" s="2"/>
       <c r="E69" s="3"/>
       <c r="G69" s="2"/>
       <c r="H69" s="2"/>
     </row>
-    <row r="70" spans="1:8">
+    <row r="70" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A70" s="1"/>
       <c r="B70" s="2"/>
       <c r="E70" s="3"/>
       <c r="G70" s="2"/>
       <c r="H70" s="2"/>
     </row>
-    <row r="71" spans="1:8">
+    <row r="71" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A71" s="1"/>
       <c r="B71" s="2"/>
       <c r="E71" s="3"/>
       <c r="G71" s="2"/>
       <c r="H71" s="2"/>
     </row>
-    <row r="72" spans="1:8">
+    <row r="72" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A72" s="1"/>
       <c r="B72" s="2"/>
       <c r="E72" s="3"/>
       <c r="G72" s="2"/>
       <c r="H72" s="2"/>
     </row>
-    <row r="73" spans="1:8">
+    <row r="73" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A73" s="1"/>
       <c r="B73" s="2"/>
       <c r="E73" s="3"/>
       <c r="G73" s="2"/>
       <c r="H73" s="2"/>
     </row>
-    <row r="74" spans="1:8">
+    <row r="74" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A74" s="1"/>
       <c r="B74" s="2"/>
       <c r="E74" s="3"/>
       <c r="G74" s="2"/>
       <c r="H74" s="2"/>
     </row>
-    <row r="75" spans="1:8">
+    <row r="75" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A75" s="1"/>
       <c r="B75" s="2"/>
       <c r="E75" s="3"/>
       <c r="G75" s="2"/>
       <c r="H75" s="2"/>
     </row>
-    <row r="76" spans="1:8">
+    <row r="76" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A76" s="1"/>
       <c r="B76" s="2"/>
       <c r="E76" s="3"/>
       <c r="G76" s="2"/>
       <c r="H76" s="2"/>
     </row>
-    <row r="77" spans="1:8">
+    <row r="77" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A77" s="1"/>
       <c r="B77" s="2"/>
       <c r="E77" s="3"/>
       <c r="G77" s="2"/>
       <c r="H77" s="2"/>
     </row>
-    <row r="78" spans="1:8">
+    <row r="78" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A78" s="1"/>
       <c r="B78" s="2"/>
       <c r="E78" s="3"/>
       <c r="G78" s="2"/>
       <c r="H78" s="2"/>
     </row>
-    <row r="79" spans="1:8">
+    <row r="79" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A79" s="1"/>
       <c r="B79" s="2"/>
       <c r="E79" s="3"/>
       <c r="G79" s="2"/>
       <c r="H79" s="2"/>
     </row>
-    <row r="80" spans="1:8">
+    <row r="80" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A80" s="1"/>
       <c r="B80" s="2"/>
       <c r="E80" s="3"/>
       <c r="G80" s="2"/>
       <c r="H80" s="2"/>
     </row>
-    <row r="81" spans="1:8">
+    <row r="81" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A81" s="1"/>
       <c r="B81" s="2"/>
       <c r="E81" s="3"/>
       <c r="G81" s="2"/>
       <c r="H81" s="2"/>
     </row>
-    <row r="82" spans="1:8">
+    <row r="82" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A82" s="1"/>
       <c r="B82" s="2"/>
       <c r="E82" s="3"/>
       <c r="G82" s="2"/>
       <c r="H82" s="2"/>
     </row>
-    <row r="83" spans="1:8">
+    <row r="83" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A83" s="1"/>
       <c r="B83" s="2"/>
       <c r="E83" s="3"/>
       <c r="G83" s="2"/>
       <c r="H83" s="2"/>
     </row>
-    <row r="84" spans="1:8">
+    <row r="84" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A84" s="1"/>
       <c r="B84" s="2"/>
       <c r="E84" s="3"/>
       <c r="G84" s="2"/>
       <c r="H84" s="2"/>
     </row>
-    <row r="85" spans="1:8">
+    <row r="85" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A85" s="1"/>
       <c r="B85" s="2"/>
       <c r="E85" s="3"/>
       <c r="G85" s="2"/>
       <c r="H85" s="2"/>
     </row>
-    <row r="86" spans="1:8">
+    <row r="86" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A86" s="1"/>
       <c r="B86" s="2"/>
       <c r="E86" s="3"/>
       <c r="G86" s="2"/>
       <c r="H86" s="2"/>
     </row>
-    <row r="87" spans="1:8">
+    <row r="87" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A87" s="1"/>
       <c r="B87" s="2"/>
       <c r="E87" s="3"/>
       <c r="G87" s="2"/>
       <c r="H87" s="2"/>
     </row>
-    <row r="88" spans="1:8">
+    <row r="88" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A88" s="1"/>
       <c r="B88" s="2"/>
       <c r="E88" s="3"/>
       <c r="G88" s="2"/>
       <c r="H88" s="2"/>
     </row>
-    <row r="89" spans="1:8">
+    <row r="89" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A89" s="1"/>
       <c r="B89" s="2"/>
       <c r="E89" s="3"/>
       <c r="G89" s="2"/>
       <c r="H89" s="2"/>
     </row>
-    <row r="90" spans="1:8">
+    <row r="90" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A90" s="1"/>
       <c r="B90" s="2"/>
       <c r="E90" s="3"/>
       <c r="G90" s="2"/>
       <c r="H90" s="2"/>
     </row>
-    <row r="91" spans="1:8">
+    <row r="91" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A91" s="1"/>
       <c r="B91" s="2"/>
       <c r="E91" s="3"/>
       <c r="G91" s="2"/>
       <c r="H91" s="2"/>
     </row>
-    <row r="92" spans="1:8">
+    <row r="92" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A92" s="1"/>
       <c r="B92" s="2"/>
       <c r="E92" s="3"/>
       <c r="G92" s="2"/>
       <c r="H92" s="2"/>
     </row>
-    <row r="93" spans="1:8">
+    <row r="93" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A93" s="1"/>
       <c r="B93" s="2"/>
       <c r="E93" s="3"/>
       <c r="G93" s="2"/>
       <c r="H93" s="2"/>
     </row>
-    <row r="94" spans="1:8">
+    <row r="94" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A94" s="1"/>
       <c r="B94" s="2"/>
       <c r="E94" s="3"/>
       <c r="G94" s="2"/>
       <c r="H94" s="2"/>
     </row>
-    <row r="95" spans="1:8">
+    <row r="95" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A95" s="1"/>
       <c r="B95" s="2"/>
       <c r="E95" s="3"/>
       <c r="G95" s="2"/>
       <c r="H95" s="2"/>
     </row>
-    <row r="96" spans="1:8">
+    <row r="96" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A96" s="1"/>
       <c r="B96" s="2"/>
       <c r="E96" s="3"/>
       <c r="G96" s="2"/>
       <c r="H96" s="2"/>
     </row>
-    <row r="97" spans="1:8">
+    <row r="97" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A97" s="1"/>
       <c r="B97" s="2"/>
       <c r="E97" s="3"/>
       <c r="G97" s="2"/>
       <c r="H97" s="2"/>
     </row>
-    <row r="98" spans="1:8">
+    <row r="98" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A98" s="1"/>
       <c r="B98" s="2"/>
       <c r="E98" s="3"/>
       <c r="G98" s="2"/>
       <c r="H98" s="2"/>
     </row>
-    <row r="99" spans="1:8">
+    <row r="99" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A99" s="1"/>
       <c r="B99" s="2"/>
       <c r="E99" s="3"/>
       <c r="G99" s="2"/>
       <c r="H99" s="2"/>
     </row>
-    <row r="100" spans="1:8">
+    <row r="100" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A100" s="1"/>
       <c r="B100" s="2"/>
       <c r="E100" s="3"/>
@@ -2892,19 +2918,19 @@
       <selection activeCell="D2" sqref="D2:D100"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="7.7265625" customWidth="1"/>
-    <col min="2" max="2" width="17.26953125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.6328125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="7.7109375" customWidth="1"/>
+    <col min="2" max="2" width="17.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.5703125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="9" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.90625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="23.6328125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="13.36328125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="19.08984375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="23.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="19.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="15.5">
+    <row r="1" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
@@ -2930,7 +2956,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:8">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="1"/>
       <c r="B2" s="2"/>
       <c r="E2" s="3"/>
@@ -2938,7 +2964,7 @@
       <c r="G2" s="2"/>
       <c r="H2" s="2"/>
     </row>
-    <row r="3" spans="1:8">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="1"/>
       <c r="B3" s="2"/>
       <c r="E3" s="3"/>
@@ -2946,7 +2972,7 @@
       <c r="G3" s="2"/>
       <c r="H3" s="2"/>
     </row>
-    <row r="4" spans="1:8">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="1"/>
       <c r="B4" s="2"/>
       <c r="E4" s="3"/>
@@ -2954,7 +2980,7 @@
       <c r="G4" s="2"/>
       <c r="H4" s="2"/>
     </row>
-    <row r="5" spans="1:8">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="1"/>
       <c r="B5" s="2"/>
       <c r="E5" s="3"/>
@@ -2962,7 +2988,7 @@
       <c r="G5" s="2"/>
       <c r="H5" s="2"/>
     </row>
-    <row r="6" spans="1:8">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="1"/>
       <c r="B6" s="2"/>
       <c r="E6" s="3"/>
@@ -2970,7 +2996,7 @@
       <c r="G6" s="2"/>
       <c r="H6" s="2"/>
     </row>
-    <row r="7" spans="1:8">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="1"/>
       <c r="B7" s="2"/>
       <c r="E7" s="3"/>
@@ -2978,7 +3004,7 @@
       <c r="G7" s="2"/>
       <c r="H7" s="2"/>
     </row>
-    <row r="8" spans="1:8">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="1"/>
       <c r="B8" s="2"/>
       <c r="E8" s="3"/>
@@ -2986,7 +3012,7 @@
       <c r="G8" s="2"/>
       <c r="H8" s="2"/>
     </row>
-    <row r="9" spans="1:8">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="1"/>
       <c r="B9" s="2"/>
       <c r="E9" s="3"/>
@@ -2994,7 +3020,7 @@
       <c r="G9" s="2"/>
       <c r="H9" s="2"/>
     </row>
-    <row r="10" spans="1:8">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="1"/>
       <c r="B10" s="2"/>
       <c r="E10" s="3"/>
@@ -3002,7 +3028,7 @@
       <c r="G10" s="2"/>
       <c r="H10" s="2"/>
     </row>
-    <row r="11" spans="1:8">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="1"/>
       <c r="B11" s="2"/>
       <c r="E11" s="3"/>
@@ -3010,7 +3036,7 @@
       <c r="G11" s="2"/>
       <c r="H11" s="2"/>
     </row>
-    <row r="12" spans="1:8">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="1"/>
       <c r="B12" s="2"/>
       <c r="E12" s="3"/>
@@ -3018,7 +3044,7 @@
       <c r="G12" s="2"/>
       <c r="H12" s="2"/>
     </row>
-    <row r="13" spans="1:8">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="1"/>
       <c r="B13" s="2"/>
       <c r="E13" s="3"/>
@@ -3026,7 +3052,7 @@
       <c r="G13" s="2"/>
       <c r="H13" s="2"/>
     </row>
-    <row r="14" spans="1:8">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" s="1"/>
       <c r="B14" s="2"/>
       <c r="E14" s="3"/>
@@ -3034,7 +3060,7 @@
       <c r="G14" s="2"/>
       <c r="H14" s="2"/>
     </row>
-    <row r="15" spans="1:8">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" s="1"/>
       <c r="B15" s="2"/>
       <c r="E15" s="3"/>
@@ -3042,7 +3068,7 @@
       <c r="G15" s="2"/>
       <c r="H15" s="2"/>
     </row>
-    <row r="16" spans="1:8">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" s="1"/>
       <c r="B16" s="2"/>
       <c r="E16" s="3"/>
@@ -3050,7 +3076,7 @@
       <c r="G16" s="2"/>
       <c r="H16" s="2"/>
     </row>
-    <row r="17" spans="1:8">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" s="1"/>
       <c r="B17" s="2"/>
       <c r="E17" s="3"/>
@@ -3058,7 +3084,7 @@
       <c r="G17" s="2"/>
       <c r="H17" s="2"/>
     </row>
-    <row r="18" spans="1:8">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" s="1"/>
       <c r="B18" s="2"/>
       <c r="E18" s="3"/>
@@ -3066,7 +3092,7 @@
       <c r="G18" s="2"/>
       <c r="H18" s="2"/>
     </row>
-    <row r="19" spans="1:8">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" s="1"/>
       <c r="B19" s="2"/>
       <c r="E19" s="3"/>
@@ -3074,7 +3100,7 @@
       <c r="G19" s="2"/>
       <c r="H19" s="2"/>
     </row>
-    <row r="20" spans="1:8">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" s="1"/>
       <c r="B20" s="2"/>
       <c r="E20" s="3"/>
@@ -3082,7 +3108,7 @@
       <c r="G20" s="2"/>
       <c r="H20" s="2"/>
     </row>
-    <row r="21" spans="1:8">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" s="1"/>
       <c r="B21" s="2"/>
       <c r="E21" s="3"/>
@@ -3090,7 +3116,7 @@
       <c r="G21" s="2"/>
       <c r="H21" s="2"/>
     </row>
-    <row r="22" spans="1:8">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" s="1"/>
       <c r="B22" s="2"/>
       <c r="E22" s="3"/>
@@ -3098,7 +3124,7 @@
       <c r="G22" s="2"/>
       <c r="H22" s="2"/>
     </row>
-    <row r="23" spans="1:8">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" s="1"/>
       <c r="B23" s="2"/>
       <c r="E23" s="3"/>
@@ -3106,7 +3132,7 @@
       <c r="G23" s="2"/>
       <c r="H23" s="2"/>
     </row>
-    <row r="24" spans="1:8">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24" s="1"/>
       <c r="B24" s="2"/>
       <c r="E24" s="3"/>
@@ -3114,7 +3140,7 @@
       <c r="G24" s="2"/>
       <c r="H24" s="2"/>
     </row>
-    <row r="25" spans="1:8">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25" s="1"/>
       <c r="B25" s="2"/>
       <c r="E25" s="3"/>
@@ -3122,7 +3148,7 @@
       <c r="G25" s="2"/>
       <c r="H25" s="2"/>
     </row>
-    <row r="26" spans="1:8">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26" s="1"/>
       <c r="B26" s="2"/>
       <c r="E26" s="3"/>
@@ -3130,7 +3156,7 @@
       <c r="G26" s="2"/>
       <c r="H26" s="2"/>
     </row>
-    <row r="27" spans="1:8">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A27" s="1"/>
       <c r="B27" s="2"/>
       <c r="E27" s="3"/>
@@ -3138,7 +3164,7 @@
       <c r="G27" s="2"/>
       <c r="H27" s="2"/>
     </row>
-    <row r="28" spans="1:8">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A28" s="1"/>
       <c r="B28" s="2"/>
       <c r="E28" s="3"/>
@@ -3146,7 +3172,7 @@
       <c r="G28" s="2"/>
       <c r="H28" s="2"/>
     </row>
-    <row r="29" spans="1:8">
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A29" s="1"/>
       <c r="B29" s="2"/>
       <c r="E29" s="3"/>
@@ -3154,7 +3180,7 @@
       <c r="G29" s="2"/>
       <c r="H29" s="2"/>
     </row>
-    <row r="30" spans="1:8">
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A30" s="1"/>
       <c r="B30" s="2"/>
       <c r="E30" s="3"/>
@@ -3162,7 +3188,7 @@
       <c r="G30" s="2"/>
       <c r="H30" s="2"/>
     </row>
-    <row r="31" spans="1:8">
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A31" s="1"/>
       <c r="B31" s="2"/>
       <c r="E31" s="3"/>
@@ -3170,7 +3196,7 @@
       <c r="G31" s="2"/>
       <c r="H31" s="2"/>
     </row>
-    <row r="32" spans="1:8">
+    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A32" s="1"/>
       <c r="B32" s="2"/>
       <c r="E32" s="3"/>
@@ -3178,7 +3204,7 @@
       <c r="G32" s="2"/>
       <c r="H32" s="2"/>
     </row>
-    <row r="33" spans="1:8">
+    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A33" s="1"/>
       <c r="B33" s="2"/>
       <c r="E33" s="3"/>
@@ -3186,7 +3212,7 @@
       <c r="G33" s="2"/>
       <c r="H33" s="2"/>
     </row>
-    <row r="34" spans="1:8">
+    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A34" s="1"/>
       <c r="B34" s="2"/>
       <c r="E34" s="3"/>
@@ -3194,7 +3220,7 @@
       <c r="G34" s="2"/>
       <c r="H34" s="2"/>
     </row>
-    <row r="35" spans="1:8">
+    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A35" s="1"/>
       <c r="B35" s="2"/>
       <c r="E35" s="3"/>
@@ -3202,7 +3228,7 @@
       <c r="G35" s="2"/>
       <c r="H35" s="2"/>
     </row>
-    <row r="36" spans="1:8">
+    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A36" s="1"/>
       <c r="B36" s="2"/>
       <c r="E36" s="3"/>
@@ -3210,7 +3236,7 @@
       <c r="G36" s="2"/>
       <c r="H36" s="2"/>
     </row>
-    <row r="37" spans="1:8">
+    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A37" s="1"/>
       <c r="B37" s="2"/>
       <c r="E37" s="3"/>
@@ -3218,7 +3244,7 @@
       <c r="G37" s="2"/>
       <c r="H37" s="2"/>
     </row>
-    <row r="38" spans="1:8">
+    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A38" s="1"/>
       <c r="B38" s="2"/>
       <c r="E38" s="3"/>
@@ -3226,7 +3252,7 @@
       <c r="G38" s="2"/>
       <c r="H38" s="2"/>
     </row>
-    <row r="39" spans="1:8">
+    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A39" s="1"/>
       <c r="B39" s="2"/>
       <c r="E39" s="3"/>
@@ -3234,7 +3260,7 @@
       <c r="G39" s="2"/>
       <c r="H39" s="2"/>
     </row>
-    <row r="40" spans="1:8">
+    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A40" s="1"/>
       <c r="B40" s="2"/>
       <c r="E40" s="3"/>
@@ -3242,7 +3268,7 @@
       <c r="G40" s="2"/>
       <c r="H40" s="2"/>
     </row>
-    <row r="41" spans="1:8">
+    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A41" s="1"/>
       <c r="B41" s="2"/>
       <c r="E41" s="3"/>
@@ -3250,7 +3276,7 @@
       <c r="G41" s="2"/>
       <c r="H41" s="2"/>
     </row>
-    <row r="42" spans="1:8">
+    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A42" s="1"/>
       <c r="B42" s="2"/>
       <c r="E42" s="3"/>
@@ -3258,7 +3284,7 @@
       <c r="G42" s="2"/>
       <c r="H42" s="2"/>
     </row>
-    <row r="43" spans="1:8">
+    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A43" s="1"/>
       <c r="B43" s="2"/>
       <c r="E43" s="3"/>
@@ -3266,7 +3292,7 @@
       <c r="G43" s="2"/>
       <c r="H43" s="2"/>
     </row>
-    <row r="44" spans="1:8">
+    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A44" s="1"/>
       <c r="B44" s="2"/>
       <c r="E44" s="3"/>
@@ -3274,7 +3300,7 @@
       <c r="G44" s="2"/>
       <c r="H44" s="2"/>
     </row>
-    <row r="45" spans="1:8">
+    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A45" s="1"/>
       <c r="B45" s="2"/>
       <c r="E45" s="3"/>
@@ -3282,7 +3308,7 @@
       <c r="G45" s="2"/>
       <c r="H45" s="2"/>
     </row>
-    <row r="46" spans="1:8">
+    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A46" s="1"/>
       <c r="B46" s="2"/>
       <c r="E46" s="3"/>
@@ -3290,7 +3316,7 @@
       <c r="G46" s="2"/>
       <c r="H46" s="2"/>
     </row>
-    <row r="47" spans="1:8">
+    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A47" s="1"/>
       <c r="B47" s="2"/>
       <c r="E47" s="3"/>
@@ -3298,7 +3324,7 @@
       <c r="G47" s="2"/>
       <c r="H47" s="2"/>
     </row>
-    <row r="48" spans="1:8">
+    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A48" s="1"/>
       <c r="B48" s="2"/>
       <c r="E48" s="3"/>
@@ -3306,7 +3332,7 @@
       <c r="G48" s="2"/>
       <c r="H48" s="2"/>
     </row>
-    <row r="49" spans="1:8">
+    <row r="49" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A49" s="1"/>
       <c r="B49" s="2"/>
       <c r="E49" s="3"/>
@@ -3314,7 +3340,7 @@
       <c r="G49" s="2"/>
       <c r="H49" s="2"/>
     </row>
-    <row r="50" spans="1:8">
+    <row r="50" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A50" s="1"/>
       <c r="B50" s="2"/>
       <c r="E50" s="3"/>
@@ -3322,7 +3348,7 @@
       <c r="G50" s="2"/>
       <c r="H50" s="2"/>
     </row>
-    <row r="51" spans="1:8">
+    <row r="51" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A51" s="1"/>
       <c r="B51" s="2"/>
       <c r="E51" s="3"/>
@@ -3330,7 +3356,7 @@
       <c r="G51" s="2"/>
       <c r="H51" s="2"/>
     </row>
-    <row r="52" spans="1:8">
+    <row r="52" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A52" s="1"/>
       <c r="B52" s="2"/>
       <c r="E52" s="3"/>
@@ -3338,7 +3364,7 @@
       <c r="G52" s="2"/>
       <c r="H52" s="2"/>
     </row>
-    <row r="53" spans="1:8">
+    <row r="53" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A53" s="1"/>
       <c r="B53" s="2"/>
       <c r="E53" s="3"/>
@@ -3346,7 +3372,7 @@
       <c r="G53" s="2"/>
       <c r="H53" s="2"/>
     </row>
-    <row r="54" spans="1:8">
+    <row r="54" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A54" s="1"/>
       <c r="B54" s="2"/>
       <c r="E54" s="3"/>
@@ -3354,7 +3380,7 @@
       <c r="G54" s="2"/>
       <c r="H54" s="2"/>
     </row>
-    <row r="55" spans="1:8">
+    <row r="55" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A55" s="1"/>
       <c r="B55" s="2"/>
       <c r="E55" s="3"/>
@@ -3362,7 +3388,7 @@
       <c r="G55" s="2"/>
       <c r="H55" s="2"/>
     </row>
-    <row r="56" spans="1:8">
+    <row r="56" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A56" s="1"/>
       <c r="B56" s="2"/>
       <c r="E56" s="3"/>
@@ -3370,7 +3396,7 @@
       <c r="G56" s="2"/>
       <c r="H56" s="2"/>
     </row>
-    <row r="57" spans="1:8">
+    <row r="57" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A57" s="1"/>
       <c r="B57" s="2"/>
       <c r="E57" s="3"/>
@@ -3378,7 +3404,7 @@
       <c r="G57" s="2"/>
       <c r="H57" s="2"/>
     </row>
-    <row r="58" spans="1:8">
+    <row r="58" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A58" s="1"/>
       <c r="B58" s="2"/>
       <c r="E58" s="3"/>
@@ -3386,7 +3412,7 @@
       <c r="G58" s="2"/>
       <c r="H58" s="2"/>
     </row>
-    <row r="59" spans="1:8">
+    <row r="59" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A59" s="1"/>
       <c r="B59" s="2"/>
       <c r="E59" s="3"/>
@@ -3394,7 +3420,7 @@
       <c r="G59" s="2"/>
       <c r="H59" s="2"/>
     </row>
-    <row r="60" spans="1:8">
+    <row r="60" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A60" s="1"/>
       <c r="B60" s="2"/>
       <c r="E60" s="3"/>
@@ -3402,7 +3428,7 @@
       <c r="G60" s="2"/>
       <c r="H60" s="2"/>
     </row>
-    <row r="61" spans="1:8">
+    <row r="61" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A61" s="1"/>
       <c r="B61" s="2"/>
       <c r="E61" s="3"/>
@@ -3410,7 +3436,7 @@
       <c r="G61" s="2"/>
       <c r="H61" s="2"/>
     </row>
-    <row r="62" spans="1:8">
+    <row r="62" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A62" s="1"/>
       <c r="B62" s="2"/>
       <c r="E62" s="3"/>
@@ -3418,7 +3444,7 @@
       <c r="G62" s="2"/>
       <c r="H62" s="2"/>
     </row>
-    <row r="63" spans="1:8">
+    <row r="63" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A63" s="1"/>
       <c r="B63" s="2"/>
       <c r="E63" s="3"/>
@@ -3426,7 +3452,7 @@
       <c r="G63" s="2"/>
       <c r="H63" s="2"/>
     </row>
-    <row r="64" spans="1:8">
+    <row r="64" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A64" s="1"/>
       <c r="B64" s="2"/>
       <c r="E64" s="3"/>
@@ -3434,7 +3460,7 @@
       <c r="G64" s="2"/>
       <c r="H64" s="2"/>
     </row>
-    <row r="65" spans="1:8">
+    <row r="65" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A65" s="1"/>
       <c r="B65" s="2"/>
       <c r="E65" s="3"/>
@@ -3442,7 +3468,7 @@
       <c r="G65" s="2"/>
       <c r="H65" s="2"/>
     </row>
-    <row r="66" spans="1:8">
+    <row r="66" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A66" s="1"/>
       <c r="B66" s="2"/>
       <c r="E66" s="3"/>
@@ -3450,7 +3476,7 @@
       <c r="G66" s="2"/>
       <c r="H66" s="2"/>
     </row>
-    <row r="67" spans="1:8">
+    <row r="67" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A67" s="1"/>
       <c r="B67" s="2"/>
       <c r="E67" s="3"/>
@@ -3458,7 +3484,7 @@
       <c r="G67" s="2"/>
       <c r="H67" s="2"/>
     </row>
-    <row r="68" spans="1:8">
+    <row r="68" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A68" s="1"/>
       <c r="B68" s="2"/>
       <c r="E68" s="3"/>
@@ -3466,7 +3492,7 @@
       <c r="G68" s="2"/>
       <c r="H68" s="2"/>
     </row>
-    <row r="69" spans="1:8">
+    <row r="69" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A69" s="1"/>
       <c r="B69" s="2"/>
       <c r="E69" s="3"/>
@@ -3474,7 +3500,7 @@
       <c r="G69" s="2"/>
       <c r="H69" s="2"/>
     </row>
-    <row r="70" spans="1:8">
+    <row r="70" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A70" s="1"/>
       <c r="B70" s="2"/>
       <c r="E70" s="3"/>
@@ -3482,7 +3508,7 @@
       <c r="G70" s="2"/>
       <c r="H70" s="2"/>
     </row>
-    <row r="71" spans="1:8">
+    <row r="71" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A71" s="1"/>
       <c r="B71" s="2"/>
       <c r="E71" s="3"/>
@@ -3490,7 +3516,7 @@
       <c r="G71" s="2"/>
       <c r="H71" s="2"/>
     </row>
-    <row r="72" spans="1:8">
+    <row r="72" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A72" s="1"/>
       <c r="B72" s="2"/>
       <c r="E72" s="3"/>
@@ -3498,7 +3524,7 @@
       <c r="G72" s="2"/>
       <c r="H72" s="2"/>
     </row>
-    <row r="73" spans="1:8">
+    <row r="73" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A73" s="1"/>
       <c r="B73" s="2"/>
       <c r="E73" s="3"/>
@@ -3506,7 +3532,7 @@
       <c r="G73" s="2"/>
       <c r="H73" s="2"/>
     </row>
-    <row r="74" spans="1:8">
+    <row r="74" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A74" s="1"/>
       <c r="B74" s="2"/>
       <c r="E74" s="3"/>
@@ -3514,7 +3540,7 @@
       <c r="G74" s="2"/>
       <c r="H74" s="2"/>
     </row>
-    <row r="75" spans="1:8">
+    <row r="75" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A75" s="1"/>
       <c r="B75" s="2"/>
       <c r="E75" s="3"/>
@@ -3522,7 +3548,7 @@
       <c r="G75" s="2"/>
       <c r="H75" s="2"/>
     </row>
-    <row r="76" spans="1:8">
+    <row r="76" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A76" s="1"/>
       <c r="B76" s="2"/>
       <c r="E76" s="3"/>
@@ -3530,7 +3556,7 @@
       <c r="G76" s="2"/>
       <c r="H76" s="2"/>
     </row>
-    <row r="77" spans="1:8">
+    <row r="77" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A77" s="1"/>
       <c r="B77" s="2"/>
       <c r="E77" s="3"/>
@@ -3538,7 +3564,7 @@
       <c r="G77" s="2"/>
       <c r="H77" s="2"/>
     </row>
-    <row r="78" spans="1:8">
+    <row r="78" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A78" s="1"/>
       <c r="B78" s="2"/>
       <c r="E78" s="3"/>
@@ -3546,7 +3572,7 @@
       <c r="G78" s="2"/>
       <c r="H78" s="2"/>
     </row>
-    <row r="79" spans="1:8">
+    <row r="79" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A79" s="1"/>
       <c r="B79" s="2"/>
       <c r="E79" s="3"/>
@@ -3554,7 +3580,7 @@
       <c r="G79" s="2"/>
       <c r="H79" s="2"/>
     </row>
-    <row r="80" spans="1:8">
+    <row r="80" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A80" s="1"/>
       <c r="B80" s="2"/>
       <c r="E80" s="3"/>
@@ -3562,7 +3588,7 @@
       <c r="G80" s="2"/>
       <c r="H80" s="2"/>
     </row>
-    <row r="81" spans="1:8">
+    <row r="81" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A81" s="1"/>
       <c r="B81" s="2"/>
       <c r="E81" s="3"/>
@@ -3570,7 +3596,7 @@
       <c r="G81" s="2"/>
       <c r="H81" s="2"/>
     </row>
-    <row r="82" spans="1:8">
+    <row r="82" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A82" s="1"/>
       <c r="B82" s="2"/>
       <c r="E82" s="3"/>
@@ -3578,7 +3604,7 @@
       <c r="G82" s="2"/>
       <c r="H82" s="2"/>
     </row>
-    <row r="83" spans="1:8">
+    <row r="83" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A83" s="1"/>
       <c r="B83" s="2"/>
       <c r="E83" s="3"/>
@@ -3586,7 +3612,7 @@
       <c r="G83" s="2"/>
       <c r="H83" s="2"/>
     </row>
-    <row r="84" spans="1:8">
+    <row r="84" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A84" s="1"/>
       <c r="B84" s="2"/>
       <c r="E84" s="3"/>
@@ -3594,7 +3620,7 @@
       <c r="G84" s="2"/>
       <c r="H84" s="2"/>
     </row>
-    <row r="85" spans="1:8">
+    <row r="85" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A85" s="1"/>
       <c r="B85" s="2"/>
       <c r="E85" s="3"/>
@@ -3602,7 +3628,7 @@
       <c r="G85" s="2"/>
       <c r="H85" s="2"/>
     </row>
-    <row r="86" spans="1:8">
+    <row r="86" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A86" s="1"/>
       <c r="B86" s="2"/>
       <c r="E86" s="3"/>
@@ -3610,7 +3636,7 @@
       <c r="G86" s="2"/>
       <c r="H86" s="2"/>
     </row>
-    <row r="87" spans="1:8">
+    <row r="87" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A87" s="1"/>
       <c r="B87" s="2"/>
       <c r="E87" s="3"/>
@@ -3618,7 +3644,7 @@
       <c r="G87" s="2"/>
       <c r="H87" s="2"/>
     </row>
-    <row r="88" spans="1:8">
+    <row r="88" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A88" s="1"/>
       <c r="B88" s="2"/>
       <c r="E88" s="3"/>
@@ -3626,7 +3652,7 @@
       <c r="G88" s="2"/>
       <c r="H88" s="2"/>
     </row>
-    <row r="89" spans="1:8">
+    <row r="89" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A89" s="1"/>
       <c r="B89" s="2"/>
       <c r="E89" s="3"/>
@@ -3634,7 +3660,7 @@
       <c r="G89" s="2"/>
       <c r="H89" s="2"/>
     </row>
-    <row r="90" spans="1:8">
+    <row r="90" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A90" s="1"/>
       <c r="B90" s="2"/>
       <c r="E90" s="3"/>
@@ -3642,7 +3668,7 @@
       <c r="G90" s="2"/>
       <c r="H90" s="2"/>
     </row>
-    <row r="91" spans="1:8">
+    <row r="91" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A91" s="1"/>
       <c r="B91" s="2"/>
       <c r="E91" s="3"/>
@@ -3650,7 +3676,7 @@
       <c r="G91" s="2"/>
       <c r="H91" s="2"/>
     </row>
-    <row r="92" spans="1:8">
+    <row r="92" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A92" s="1"/>
       <c r="B92" s="2"/>
       <c r="E92" s="3"/>
@@ -3658,7 +3684,7 @@
       <c r="G92" s="2"/>
       <c r="H92" s="2"/>
     </row>
-    <row r="93" spans="1:8">
+    <row r="93" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A93" s="1"/>
       <c r="B93" s="2"/>
       <c r="E93" s="3"/>
@@ -3666,7 +3692,7 @@
       <c r="G93" s="2"/>
       <c r="H93" s="2"/>
     </row>
-    <row r="94" spans="1:8">
+    <row r="94" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A94" s="1"/>
       <c r="B94" s="2"/>
       <c r="E94" s="3"/>
@@ -3674,7 +3700,7 @@
       <c r="G94" s="2"/>
       <c r="H94" s="2"/>
     </row>
-    <row r="95" spans="1:8">
+    <row r="95" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A95" s="1"/>
       <c r="B95" s="2"/>
       <c r="E95" s="3"/>
@@ -3682,7 +3708,7 @@
       <c r="G95" s="2"/>
       <c r="H95" s="2"/>
     </row>
-    <row r="96" spans="1:8">
+    <row r="96" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A96" s="1"/>
       <c r="B96" s="2"/>
       <c r="E96" s="3"/>
@@ -3690,7 +3716,7 @@
       <c r="G96" s="2"/>
       <c r="H96" s="2"/>
     </row>
-    <row r="97" spans="1:8">
+    <row r="97" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A97" s="1"/>
       <c r="B97" s="2"/>
       <c r="E97" s="3"/>
@@ -3698,7 +3724,7 @@
       <c r="G97" s="2"/>
       <c r="H97" s="2"/>
     </row>
-    <row r="98" spans="1:8">
+    <row r="98" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A98" s="1"/>
       <c r="B98" s="2"/>
       <c r="E98" s="3"/>
@@ -3706,7 +3732,7 @@
       <c r="G98" s="2"/>
       <c r="H98" s="2"/>
     </row>
-    <row r="99" spans="1:8">
+    <row r="99" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A99" s="1"/>
       <c r="B99" s="2"/>
       <c r="E99" s="3"/>
@@ -3714,7 +3740,7 @@
       <c r="G99" s="2"/>
       <c r="H99" s="2"/>
     </row>
-    <row r="100" spans="1:8">
+    <row r="100" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A100" s="1"/>
       <c r="B100" s="2"/>
       <c r="E100" s="3"/>
@@ -3757,21 +3783,21 @@
       <selection activeCell="P21" sqref="P21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.08984375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.90625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.90625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="19.36328125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.6328125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.6328125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.5703125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="9" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="17.90625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="17.85546875" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="17" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="19.08984375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="19.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="15.5">
+    <row r="1" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="7" t="s">
         <v>8</v>
       </c>
@@ -3803,7 +3829,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:10">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="2"/>
       <c r="B2" s="8"/>
       <c r="D2" s="2"/>
@@ -3811,7 +3837,7 @@
       <c r="I2" s="8"/>
       <c r="J2" s="2"/>
     </row>
-    <row r="3" spans="1:10">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="2"/>
       <c r="B3" s="8"/>
       <c r="D3" s="2"/>
@@ -3819,7 +3845,7 @@
       <c r="I3" s="8"/>
       <c r="J3" s="2"/>
     </row>
-    <row r="4" spans="1:10">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="2"/>
       <c r="B4" s="8"/>
       <c r="D4" s="2"/>
@@ -3827,7 +3853,7 @@
       <c r="I4" s="8"/>
       <c r="J4" s="2"/>
     </row>
-    <row r="5" spans="1:10">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" s="2"/>
       <c r="B5" s="8"/>
       <c r="D5" s="2"/>
@@ -3835,7 +3861,7 @@
       <c r="I5" s="8"/>
       <c r="J5" s="2"/>
     </row>
-    <row r="6" spans="1:10">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" s="2"/>
       <c r="B6" s="8"/>
       <c r="D6" s="2"/>
@@ -3843,7 +3869,7 @@
       <c r="I6" s="8"/>
       <c r="J6" s="2"/>
     </row>
-    <row r="7" spans="1:10">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" s="2"/>
       <c r="B7" s="8"/>
       <c r="D7" s="2"/>
@@ -3851,7 +3877,7 @@
       <c r="I7" s="8"/>
       <c r="J7" s="2"/>
     </row>
-    <row r="8" spans="1:10">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" s="2"/>
       <c r="B8" s="8"/>
       <c r="D8" s="2"/>
@@ -3859,7 +3885,7 @@
       <c r="I8" s="8"/>
       <c r="J8" s="2"/>
     </row>
-    <row r="9" spans="1:10">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" s="2"/>
       <c r="B9" s="8"/>
       <c r="D9" s="2"/>
@@ -3867,7 +3893,7 @@
       <c r="I9" s="8"/>
       <c r="J9" s="2"/>
     </row>
-    <row r="10" spans="1:10">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" s="2"/>
       <c r="B10" s="8"/>
       <c r="D10" s="2"/>
@@ -3875,7 +3901,7 @@
       <c r="I10" s="8"/>
       <c r="J10" s="2"/>
     </row>
-    <row r="11" spans="1:10">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" s="2"/>
       <c r="B11" s="8"/>
       <c r="D11" s="2"/>
@@ -3883,7 +3909,7 @@
       <c r="I11" s="8"/>
       <c r="J11" s="2"/>
     </row>
-    <row r="12" spans="1:10">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" s="2"/>
       <c r="B12" s="8"/>
       <c r="D12" s="2"/>
@@ -3891,7 +3917,7 @@
       <c r="I12" s="8"/>
       <c r="J12" s="2"/>
     </row>
-    <row r="13" spans="1:10">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" s="2"/>
       <c r="B13" s="8"/>
       <c r="D13" s="2"/>
@@ -3899,7 +3925,7 @@
       <c r="I13" s="8"/>
       <c r="J13" s="2"/>
     </row>
-    <row r="14" spans="1:10">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" s="2"/>
       <c r="B14" s="8"/>
       <c r="D14" s="2"/>
@@ -3907,7 +3933,7 @@
       <c r="I14" s="8"/>
       <c r="J14" s="2"/>
     </row>
-    <row r="15" spans="1:10">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" s="2"/>
       <c r="B15" s="8"/>
       <c r="D15" s="2"/>
@@ -3915,7 +3941,7 @@
       <c r="I15" s="8"/>
       <c r="J15" s="2"/>
     </row>
-    <row r="16" spans="1:10">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" s="2"/>
       <c r="B16" s="8"/>
       <c r="D16" s="2"/>
@@ -3923,7 +3949,7 @@
       <c r="I16" s="8"/>
       <c r="J16" s="2"/>
     </row>
-    <row r="17" spans="1:10">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17" s="2"/>
       <c r="B17" s="8"/>
       <c r="D17" s="2"/>
@@ -3931,7 +3957,7 @@
       <c r="I17" s="8"/>
       <c r="J17" s="2"/>
     </row>
-    <row r="18" spans="1:10">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18" s="2"/>
       <c r="B18" s="8"/>
       <c r="D18" s="2"/>
@@ -3939,7 +3965,7 @@
       <c r="I18" s="8"/>
       <c r="J18" s="2"/>
     </row>
-    <row r="19" spans="1:10">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A19" s="2"/>
       <c r="B19" s="8"/>
       <c r="D19" s="2"/>
@@ -3947,7 +3973,7 @@
       <c r="I19" s="8"/>
       <c r="J19" s="2"/>
     </row>
-    <row r="20" spans="1:10">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A20" s="2"/>
       <c r="B20" s="8"/>
       <c r="D20" s="2"/>
@@ -3955,7 +3981,7 @@
       <c r="I20" s="8"/>
       <c r="J20" s="2"/>
     </row>
-    <row r="21" spans="1:10">
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A21" s="2"/>
       <c r="B21" s="8"/>
       <c r="D21" s="2"/>
@@ -3963,7 +3989,7 @@
       <c r="I21" s="8"/>
       <c r="J21" s="2"/>
     </row>
-    <row r="22" spans="1:10">
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A22" s="2"/>
       <c r="B22" s="8"/>
       <c r="D22" s="2"/>
@@ -3971,7 +3997,7 @@
       <c r="I22" s="8"/>
       <c r="J22" s="2"/>
     </row>
-    <row r="23" spans="1:10">
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A23" s="2"/>
       <c r="B23" s="8"/>
       <c r="D23" s="2"/>
@@ -3979,7 +4005,7 @@
       <c r="I23" s="8"/>
       <c r="J23" s="2"/>
     </row>
-    <row r="24" spans="1:10">
+    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A24" s="2"/>
       <c r="B24" s="8"/>
       <c r="D24" s="2"/>
@@ -3987,7 +4013,7 @@
       <c r="I24" s="8"/>
       <c r="J24" s="2"/>
     </row>
-    <row r="25" spans="1:10">
+    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A25" s="2"/>
       <c r="B25" s="8"/>
       <c r="D25" s="2"/>
@@ -3995,7 +4021,7 @@
       <c r="I25" s="8"/>
       <c r="J25" s="2"/>
     </row>
-    <row r="26" spans="1:10">
+    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A26" s="2"/>
       <c r="B26" s="8"/>
       <c r="D26" s="2"/>
@@ -4003,7 +4029,7 @@
       <c r="I26" s="8"/>
       <c r="J26" s="2"/>
     </row>
-    <row r="27" spans="1:10">
+    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A27" s="2"/>
       <c r="B27" s="8"/>
       <c r="D27" s="2"/>
@@ -4011,7 +4037,7 @@
       <c r="I27" s="8"/>
       <c r="J27" s="2"/>
     </row>
-    <row r="28" spans="1:10">
+    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A28" s="2"/>
       <c r="B28" s="8"/>
       <c r="D28" s="2"/>
@@ -4019,7 +4045,7 @@
       <c r="I28" s="8"/>
       <c r="J28" s="2"/>
     </row>
-    <row r="29" spans="1:10">
+    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A29" s="2"/>
       <c r="B29" s="8"/>
       <c r="D29" s="2"/>
@@ -4027,7 +4053,7 @@
       <c r="I29" s="8"/>
       <c r="J29" s="2"/>
     </row>
-    <row r="30" spans="1:10">
+    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A30" s="2"/>
       <c r="B30" s="8"/>
       <c r="D30" s="2"/>
@@ -4035,7 +4061,7 @@
       <c r="I30" s="8"/>
       <c r="J30" s="2"/>
     </row>
-    <row r="31" spans="1:10">
+    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A31" s="2"/>
       <c r="B31" s="8"/>
       <c r="D31" s="2"/>
@@ -4043,7 +4069,7 @@
       <c r="I31" s="8"/>
       <c r="J31" s="2"/>
     </row>
-    <row r="32" spans="1:10">
+    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A32" s="2"/>
       <c r="B32" s="8"/>
       <c r="D32" s="2"/>
@@ -4051,7 +4077,7 @@
       <c r="I32" s="8"/>
       <c r="J32" s="2"/>
     </row>
-    <row r="33" spans="1:10">
+    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A33" s="2"/>
       <c r="B33" s="8"/>
       <c r="D33" s="2"/>
@@ -4059,7 +4085,7 @@
       <c r="I33" s="8"/>
       <c r="J33" s="2"/>
     </row>
-    <row r="34" spans="1:10">
+    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A34" s="2"/>
       <c r="B34" s="8"/>
       <c r="D34" s="2"/>
@@ -4067,7 +4093,7 @@
       <c r="I34" s="8"/>
       <c r="J34" s="2"/>
     </row>
-    <row r="35" spans="1:10">
+    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A35" s="2"/>
       <c r="B35" s="8"/>
       <c r="D35" s="2"/>
@@ -4075,7 +4101,7 @@
       <c r="I35" s="8"/>
       <c r="J35" s="2"/>
     </row>
-    <row r="36" spans="1:10">
+    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A36" s="2"/>
       <c r="B36" s="8"/>
       <c r="D36" s="2"/>
@@ -4083,7 +4109,7 @@
       <c r="I36" s="8"/>
       <c r="J36" s="2"/>
     </row>
-    <row r="37" spans="1:10">
+    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A37" s="2"/>
       <c r="B37" s="8"/>
       <c r="D37" s="2"/>
@@ -4091,7 +4117,7 @@
       <c r="I37" s="8"/>
       <c r="J37" s="2"/>
     </row>
-    <row r="38" spans="1:10">
+    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A38" s="2"/>
       <c r="B38" s="8"/>
       <c r="D38" s="2"/>
@@ -4099,7 +4125,7 @@
       <c r="I38" s="8"/>
       <c r="J38" s="2"/>
     </row>
-    <row r="39" spans="1:10">
+    <row r="39" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A39" s="2"/>
       <c r="B39" s="8"/>
       <c r="D39" s="2"/>
@@ -4107,7 +4133,7 @@
       <c r="I39" s="8"/>
       <c r="J39" s="2"/>
     </row>
-    <row r="40" spans="1:10">
+    <row r="40" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A40" s="2"/>
       <c r="B40" s="8"/>
       <c r="D40" s="2"/>
@@ -4115,7 +4141,7 @@
       <c r="I40" s="8"/>
       <c r="J40" s="2"/>
     </row>
-    <row r="41" spans="1:10">
+    <row r="41" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A41" s="2"/>
       <c r="B41" s="8"/>
       <c r="D41" s="2"/>
@@ -4123,7 +4149,7 @@
       <c r="I41" s="8"/>
       <c r="J41" s="2"/>
     </row>
-    <row r="42" spans="1:10">
+    <row r="42" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A42" s="2"/>
       <c r="B42" s="8"/>
       <c r="D42" s="2"/>
@@ -4131,7 +4157,7 @@
       <c r="I42" s="8"/>
       <c r="J42" s="2"/>
     </row>
-    <row r="43" spans="1:10">
+    <row r="43" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A43" s="2"/>
       <c r="B43" s="8"/>
       <c r="D43" s="2"/>
@@ -4139,7 +4165,7 @@
       <c r="I43" s="8"/>
       <c r="J43" s="2"/>
     </row>
-    <row r="44" spans="1:10">
+    <row r="44" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A44" s="2"/>
       <c r="B44" s="8"/>
       <c r="D44" s="2"/>
@@ -4147,7 +4173,7 @@
       <c r="I44" s="8"/>
       <c r="J44" s="2"/>
     </row>
-    <row r="45" spans="1:10">
+    <row r="45" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A45" s="2"/>
       <c r="B45" s="8"/>
       <c r="D45" s="2"/>
@@ -4155,7 +4181,7 @@
       <c r="I45" s="8"/>
       <c r="J45" s="2"/>
     </row>
-    <row r="46" spans="1:10">
+    <row r="46" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A46" s="2"/>
       <c r="B46" s="8"/>
       <c r="D46" s="2"/>
@@ -4163,7 +4189,7 @@
       <c r="I46" s="8"/>
       <c r="J46" s="2"/>
     </row>
-    <row r="47" spans="1:10">
+    <row r="47" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A47" s="2"/>
       <c r="B47" s="8"/>
       <c r="D47" s="2"/>
@@ -4171,7 +4197,7 @@
       <c r="I47" s="8"/>
       <c r="J47" s="2"/>
     </row>
-    <row r="48" spans="1:10">
+    <row r="48" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A48" s="2"/>
       <c r="B48" s="8"/>
       <c r="D48" s="2"/>
@@ -4179,7 +4205,7 @@
       <c r="I48" s="8"/>
       <c r="J48" s="2"/>
     </row>
-    <row r="49" spans="1:10">
+    <row r="49" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A49" s="2"/>
       <c r="B49" s="8"/>
       <c r="D49" s="2"/>
@@ -4187,7 +4213,7 @@
       <c r="I49" s="8"/>
       <c r="J49" s="2"/>
     </row>
-    <row r="50" spans="1:10">
+    <row r="50" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A50" s="2"/>
       <c r="B50" s="8"/>
       <c r="D50" s="2"/>
@@ -4195,7 +4221,7 @@
       <c r="I50" s="8"/>
       <c r="J50" s="2"/>
     </row>
-    <row r="51" spans="1:10">
+    <row r="51" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A51" s="2"/>
       <c r="B51" s="8"/>
       <c r="D51" s="2"/>
@@ -4203,7 +4229,7 @@
       <c r="I51" s="8"/>
       <c r="J51" s="2"/>
     </row>
-    <row r="52" spans="1:10">
+    <row r="52" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A52" s="2"/>
       <c r="B52" s="8"/>
       <c r="D52" s="2"/>
@@ -4211,7 +4237,7 @@
       <c r="I52" s="8"/>
       <c r="J52" s="2"/>
     </row>
-    <row r="53" spans="1:10">
+    <row r="53" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A53" s="2"/>
       <c r="B53" s="8"/>
       <c r="D53" s="2"/>
@@ -4219,7 +4245,7 @@
       <c r="I53" s="8"/>
       <c r="J53" s="2"/>
     </row>
-    <row r="54" spans="1:10">
+    <row r="54" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A54" s="2"/>
       <c r="B54" s="8"/>
       <c r="D54" s="2"/>
@@ -4227,7 +4253,7 @@
       <c r="I54" s="8"/>
       <c r="J54" s="2"/>
     </row>
-    <row r="55" spans="1:10">
+    <row r="55" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A55" s="2"/>
       <c r="B55" s="8"/>
       <c r="D55" s="2"/>
@@ -4235,7 +4261,7 @@
       <c r="I55" s="8"/>
       <c r="J55" s="2"/>
     </row>
-    <row r="56" spans="1:10">
+    <row r="56" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A56" s="2"/>
       <c r="B56" s="8"/>
       <c r="D56" s="2"/>
@@ -4243,7 +4269,7 @@
       <c r="I56" s="8"/>
       <c r="J56" s="2"/>
     </row>
-    <row r="57" spans="1:10">
+    <row r="57" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A57" s="2"/>
       <c r="B57" s="8"/>
       <c r="D57" s="2"/>
@@ -4251,7 +4277,7 @@
       <c r="I57" s="8"/>
       <c r="J57" s="2"/>
     </row>
-    <row r="58" spans="1:10">
+    <row r="58" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A58" s="2"/>
       <c r="B58" s="8"/>
       <c r="D58" s="2"/>
@@ -4259,7 +4285,7 @@
       <c r="I58" s="8"/>
       <c r="J58" s="2"/>
     </row>
-    <row r="59" spans="1:10">
+    <row r="59" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A59" s="2"/>
       <c r="B59" s="8"/>
       <c r="D59" s="2"/>
@@ -4267,7 +4293,7 @@
       <c r="I59" s="8"/>
       <c r="J59" s="2"/>
     </row>
-    <row r="60" spans="1:10">
+    <row r="60" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A60" s="2"/>
       <c r="B60" s="8"/>
       <c r="D60" s="2"/>
@@ -4275,7 +4301,7 @@
       <c r="I60" s="8"/>
       <c r="J60" s="2"/>
     </row>
-    <row r="61" spans="1:10">
+    <row r="61" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A61" s="2"/>
       <c r="B61" s="8"/>
       <c r="D61" s="2"/>
@@ -4283,7 +4309,7 @@
       <c r="I61" s="8"/>
       <c r="J61" s="2"/>
     </row>
-    <row r="62" spans="1:10">
+    <row r="62" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A62" s="2"/>
       <c r="B62" s="8"/>
       <c r="D62" s="2"/>
@@ -4291,7 +4317,7 @@
       <c r="I62" s="8"/>
       <c r="J62" s="2"/>
     </row>
-    <row r="63" spans="1:10">
+    <row r="63" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A63" s="2"/>
       <c r="B63" s="8"/>
       <c r="D63" s="2"/>
@@ -4299,7 +4325,7 @@
       <c r="I63" s="8"/>
       <c r="J63" s="2"/>
     </row>
-    <row r="64" spans="1:10">
+    <row r="64" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A64" s="2"/>
       <c r="B64" s="8"/>
       <c r="D64" s="2"/>
@@ -4307,7 +4333,7 @@
       <c r="I64" s="8"/>
       <c r="J64" s="2"/>
     </row>
-    <row r="65" spans="1:10">
+    <row r="65" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A65" s="2"/>
       <c r="B65" s="8"/>
       <c r="D65" s="2"/>
@@ -4315,7 +4341,7 @@
       <c r="I65" s="8"/>
       <c r="J65" s="2"/>
     </row>
-    <row r="66" spans="1:10">
+    <row r="66" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A66" s="2"/>
       <c r="B66" s="8"/>
       <c r="D66" s="2"/>
@@ -4323,7 +4349,7 @@
       <c r="I66" s="8"/>
       <c r="J66" s="2"/>
     </row>
-    <row r="67" spans="1:10">
+    <row r="67" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A67" s="2"/>
       <c r="B67" s="8"/>
       <c r="D67" s="2"/>
@@ -4331,7 +4357,7 @@
       <c r="I67" s="8"/>
       <c r="J67" s="2"/>
     </row>
-    <row r="68" spans="1:10">
+    <row r="68" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A68" s="2"/>
       <c r="B68" s="8"/>
       <c r="D68" s="2"/>
@@ -4339,7 +4365,7 @@
       <c r="I68" s="8"/>
       <c r="J68" s="2"/>
     </row>
-    <row r="69" spans="1:10">
+    <row r="69" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A69" s="2"/>
       <c r="B69" s="8"/>
       <c r="D69" s="2"/>
@@ -4347,7 +4373,7 @@
       <c r="I69" s="8"/>
       <c r="J69" s="2"/>
     </row>
-    <row r="70" spans="1:10">
+    <row r="70" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A70" s="2"/>
       <c r="B70" s="8"/>
       <c r="D70" s="2"/>
@@ -4355,7 +4381,7 @@
       <c r="I70" s="8"/>
       <c r="J70" s="2"/>
     </row>
-    <row r="71" spans="1:10">
+    <row r="71" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A71" s="2"/>
       <c r="B71" s="8"/>
       <c r="D71" s="2"/>
@@ -4363,7 +4389,7 @@
       <c r="I71" s="8"/>
       <c r="J71" s="2"/>
     </row>
-    <row r="72" spans="1:10">
+    <row r="72" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A72" s="2"/>
       <c r="B72" s="8"/>
       <c r="D72" s="2"/>
@@ -4371,7 +4397,7 @@
       <c r="I72" s="8"/>
       <c r="J72" s="2"/>
     </row>
-    <row r="73" spans="1:10">
+    <row r="73" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A73" s="2"/>
       <c r="B73" s="8"/>
       <c r="D73" s="2"/>
@@ -4379,7 +4405,7 @@
       <c r="I73" s="8"/>
       <c r="J73" s="2"/>
     </row>
-    <row r="74" spans="1:10">
+    <row r="74" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A74" s="2"/>
       <c r="B74" s="8"/>
       <c r="D74" s="2"/>
@@ -4387,7 +4413,7 @@
       <c r="I74" s="8"/>
       <c r="J74" s="2"/>
     </row>
-    <row r="75" spans="1:10">
+    <row r="75" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A75" s="2"/>
       <c r="B75" s="8"/>
       <c r="D75" s="2"/>
@@ -4395,7 +4421,7 @@
       <c r="I75" s="8"/>
       <c r="J75" s="2"/>
     </row>
-    <row r="76" spans="1:10">
+    <row r="76" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A76" s="2"/>
       <c r="B76" s="8"/>
       <c r="D76" s="2"/>
@@ -4403,7 +4429,7 @@
       <c r="I76" s="8"/>
       <c r="J76" s="2"/>
     </row>
-    <row r="77" spans="1:10">
+    <row r="77" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A77" s="2"/>
       <c r="B77" s="8"/>
       <c r="D77" s="2"/>
@@ -4411,7 +4437,7 @@
       <c r="I77" s="8"/>
       <c r="J77" s="2"/>
     </row>
-    <row r="78" spans="1:10">
+    <row r="78" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A78" s="2"/>
       <c r="B78" s="8"/>
       <c r="D78" s="2"/>
@@ -4419,7 +4445,7 @@
       <c r="I78" s="8"/>
       <c r="J78" s="2"/>
     </row>
-    <row r="79" spans="1:10">
+    <row r="79" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A79" s="2"/>
       <c r="B79" s="8"/>
       <c r="D79" s="2"/>
@@ -4427,7 +4453,7 @@
       <c r="I79" s="8"/>
       <c r="J79" s="2"/>
     </row>
-    <row r="80" spans="1:10">
+    <row r="80" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A80" s="2"/>
       <c r="B80" s="8"/>
       <c r="D80" s="2"/>
@@ -4435,7 +4461,7 @@
       <c r="I80" s="8"/>
       <c r="J80" s="2"/>
     </row>
-    <row r="81" spans="1:10">
+    <row r="81" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A81" s="2"/>
       <c r="B81" s="8"/>
       <c r="D81" s="2"/>
@@ -4443,7 +4469,7 @@
       <c r="I81" s="8"/>
       <c r="J81" s="2"/>
     </row>
-    <row r="82" spans="1:10">
+    <row r="82" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A82" s="2"/>
       <c r="B82" s="8"/>
       <c r="D82" s="2"/>
@@ -4451,7 +4477,7 @@
       <c r="I82" s="8"/>
       <c r="J82" s="2"/>
     </row>
-    <row r="83" spans="1:10">
+    <row r="83" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A83" s="2"/>
       <c r="B83" s="8"/>
       <c r="D83" s="2"/>
@@ -4459,7 +4485,7 @@
       <c r="I83" s="8"/>
       <c r="J83" s="2"/>
     </row>
-    <row r="84" spans="1:10">
+    <row r="84" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A84" s="2"/>
       <c r="B84" s="8"/>
       <c r="D84" s="2"/>
@@ -4467,7 +4493,7 @@
       <c r="I84" s="8"/>
       <c r="J84" s="2"/>
     </row>
-    <row r="85" spans="1:10">
+    <row r="85" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A85" s="2"/>
       <c r="B85" s="8"/>
       <c r="D85" s="2"/>
@@ -4475,7 +4501,7 @@
       <c r="I85" s="8"/>
       <c r="J85" s="2"/>
     </row>
-    <row r="86" spans="1:10">
+    <row r="86" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A86" s="2"/>
       <c r="B86" s="8"/>
       <c r="D86" s="2"/>
@@ -4483,7 +4509,7 @@
       <c r="I86" s="8"/>
       <c r="J86" s="2"/>
     </row>
-    <row r="87" spans="1:10">
+    <row r="87" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A87" s="2"/>
       <c r="B87" s="8"/>
       <c r="D87" s="2"/>
@@ -4491,7 +4517,7 @@
       <c r="I87" s="8"/>
       <c r="J87" s="2"/>
     </row>
-    <row r="88" spans="1:10">
+    <row r="88" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A88" s="2"/>
       <c r="B88" s="8"/>
       <c r="D88" s="2"/>
@@ -4499,7 +4525,7 @@
       <c r="I88" s="8"/>
       <c r="J88" s="2"/>
     </row>
-    <row r="89" spans="1:10">
+    <row r="89" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A89" s="2"/>
       <c r="B89" s="8"/>
       <c r="D89" s="2"/>
@@ -4507,7 +4533,7 @@
       <c r="I89" s="8"/>
       <c r="J89" s="2"/>
     </row>
-    <row r="90" spans="1:10">
+    <row r="90" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A90" s="2"/>
       <c r="B90" s="8"/>
       <c r="D90" s="2"/>
@@ -4515,7 +4541,7 @@
       <c r="I90" s="8"/>
       <c r="J90" s="2"/>
     </row>
-    <row r="91" spans="1:10">
+    <row r="91" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A91" s="2"/>
       <c r="B91" s="8"/>
       <c r="D91" s="2"/>
@@ -4523,7 +4549,7 @@
       <c r="I91" s="8"/>
       <c r="J91" s="2"/>
     </row>
-    <row r="92" spans="1:10">
+    <row r="92" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A92" s="2"/>
       <c r="B92" s="8"/>
       <c r="D92" s="2"/>
@@ -4531,7 +4557,7 @@
       <c r="I92" s="8"/>
       <c r="J92" s="2"/>
     </row>
-    <row r="93" spans="1:10">
+    <row r="93" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A93" s="2"/>
       <c r="B93" s="8"/>
       <c r="D93" s="2"/>
@@ -4539,7 +4565,7 @@
       <c r="I93" s="8"/>
       <c r="J93" s="2"/>
     </row>
-    <row r="94" spans="1:10">
+    <row r="94" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A94" s="2"/>
       <c r="B94" s="8"/>
       <c r="D94" s="2"/>
@@ -4547,7 +4573,7 @@
       <c r="I94" s="8"/>
       <c r="J94" s="2"/>
     </row>
-    <row r="95" spans="1:10">
+    <row r="95" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A95" s="2"/>
       <c r="B95" s="8"/>
       <c r="D95" s="2"/>
@@ -4555,7 +4581,7 @@
       <c r="I95" s="8"/>
       <c r="J95" s="2"/>
     </row>
-    <row r="96" spans="1:10">
+    <row r="96" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A96" s="2"/>
       <c r="B96" s="8"/>
       <c r="D96" s="2"/>
@@ -4563,7 +4589,7 @@
       <c r="I96" s="8"/>
       <c r="J96" s="2"/>
     </row>
-    <row r="97" spans="1:10">
+    <row r="97" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A97" s="2"/>
       <c r="B97" s="8"/>
       <c r="D97" s="2"/>
@@ -4571,7 +4597,7 @@
       <c r="I97" s="8"/>
       <c r="J97" s="2"/>
     </row>
-    <row r="98" spans="1:10">
+    <row r="98" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A98" s="2"/>
       <c r="B98" s="8"/>
       <c r="D98" s="2"/>
@@ -4579,7 +4605,7 @@
       <c r="I98" s="8"/>
       <c r="J98" s="2"/>
     </row>
-    <row r="99" spans="1:10">
+    <row r="99" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A99" s="2"/>
       <c r="B99" s="8"/>
       <c r="D99" s="2"/>
@@ -4587,7 +4613,7 @@
       <c r="I99" s="8"/>
       <c r="J99" s="2"/>
     </row>
-    <row r="100" spans="1:10">
+    <row r="100" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A100" s="2"/>
       <c r="B100" s="8"/>
       <c r="D100" s="2"/>

</xml_diff>

<commit_message>
Updated progress report for May 16-19 by Avichal
</commit_message>
<xml_diff>
--- a/PR&IR.xlsx
+++ b/PR&IR.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28623"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\yashp\Downloads\CS415_A3\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\avichal avneel nath\Documents\Semester 7\CS415\A3\CS415_A3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{22F34894-3F54-458B-8CE8-BA08E82FF539}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{265B2D53-2233-42DA-BDE7-A3000AC9A528}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="2" xr2:uid="{BFA1E21A-08FA-4F02-8C25-33C81C8EE970}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{BFA1E21A-08FA-4F02-8C25-33C81C8EE970}"/>
   </bookViews>
   <sheets>
     <sheet name="Avichal" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="81">
   <si>
     <t>Date</t>
   </si>
@@ -272,6 +272,30 @@
   <si>
     <t>Learning how to work with Docker Database</t>
   </si>
+  <si>
+    <t xml:space="preserve">Modified invoice </t>
+  </si>
+  <si>
+    <t>Backend commencement</t>
+  </si>
+  <si>
+    <t>configuring enrollment services to designated port</t>
+  </si>
+  <si>
+    <t>Configure on specified port</t>
+  </si>
+  <si>
+    <t>Successfully run the services on port 5004</t>
+  </si>
+  <si>
+    <t>confgure API</t>
+  </si>
+  <si>
+    <t xml:space="preserve">only read docker documentation </t>
+  </si>
+  <si>
+    <t>Port configuration</t>
+  </si>
 </sst>
 </file>
 
@@ -281,7 +305,7 @@
     <numFmt numFmtId="164" formatCode="h"/>
     <numFmt numFmtId="165" formatCode="d/mm/yyyy;@"/>
   </numFmts>
-  <fonts count="3">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -394,7 +418,7 @@
       <numFmt numFmtId="30" formatCode="@"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="19" formatCode="m/d/yyyy"/>
+      <numFmt numFmtId="166" formatCode="m/d/yyyy"/>
     </dxf>
     <dxf>
       <font>
@@ -430,7 +454,7 @@
       <numFmt numFmtId="30" formatCode="@"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="19" formatCode="m/d/yyyy"/>
+      <numFmt numFmtId="166" formatCode="m/d/yyyy"/>
     </dxf>
     <dxf>
       <font>
@@ -502,7 +526,7 @@
       <numFmt numFmtId="30" formatCode="@"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="19" formatCode="m/d/yyyy"/>
+      <numFmt numFmtId="166" formatCode="m/d/yyyy"/>
     </dxf>
     <dxf>
       <font>
@@ -1017,30 +1041,30 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{37EAA098-74C6-4411-B7E2-26AD2DCBC3F0}">
   <dimension ref="A1:H28"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H8" sqref="H8"/>
+    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.4140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.58203125" style="2" customWidth="1"/>
+    <col min="1" max="1" width="10.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.5703125" style="2" customWidth="1"/>
     <col min="3" max="3" width="58" customWidth="1"/>
-    <col min="5" max="5" width="13.1640625" style="3" customWidth="1"/>
-    <col min="6" max="6" width="20.83203125" style="4" customWidth="1"/>
-    <col min="7" max="7" width="34.83203125" style="2" customWidth="1"/>
-    <col min="8" max="8" width="43.4140625" style="2" customWidth="1"/>
-    <col min="11" max="11" width="9.1640625" customWidth="1"/>
-    <col min="12" max="12" width="13.25" customWidth="1"/>
-    <col min="13" max="13" width="11.4140625" customWidth="1"/>
-    <col min="14" max="14" width="17.4140625" customWidth="1"/>
-    <col min="16" max="16" width="9.1640625" customWidth="1"/>
-    <col min="18" max="18" width="16.58203125" customWidth="1"/>
-    <col min="19" max="19" width="14.75" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="16.83203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.140625" style="3" customWidth="1"/>
+    <col min="6" max="6" width="20.85546875" style="4" customWidth="1"/>
+    <col min="7" max="7" width="34.85546875" style="2" customWidth="1"/>
+    <col min="8" max="8" width="43.42578125" style="2" customWidth="1"/>
+    <col min="11" max="11" width="9.140625" customWidth="1"/>
+    <col min="12" max="12" width="13.28515625" customWidth="1"/>
+    <col min="13" max="13" width="11.42578125" customWidth="1"/>
+    <col min="14" max="14" width="17.42578125" customWidth="1"/>
+    <col min="16" max="16" width="9.140625" customWidth="1"/>
+    <col min="18" max="18" width="16.5703125" customWidth="1"/>
+    <col min="19" max="19" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="16.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="15.5">
+    <row r="1" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
@@ -1066,7 +1090,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:8">
+    <row r="2" spans="1:8" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A2" s="1">
         <v>45786</v>
       </c>
@@ -1092,7 +1116,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="3" spans="1:8" ht="112">
+    <row r="3" spans="1:8" ht="120" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>45787</v>
       </c>
@@ -1115,7 +1139,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="4" spans="1:8">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>45788</v>
       </c>
@@ -1135,7 +1159,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="5" spans="1:8" ht="76.5" customHeight="1">
+    <row r="5" spans="1:8" ht="76.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>45789</v>
       </c>
@@ -1158,7 +1182,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="6" spans="1:8">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>45790</v>
       </c>
@@ -1181,7 +1205,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="7" spans="1:8">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>45791</v>
       </c>
@@ -1204,7 +1228,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="8" spans="1:8">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>45792</v>
       </c>
@@ -1227,72 +1251,136 @@
         <v>66</v>
       </c>
     </row>
-    <row r="9" spans="1:8">
-      <c r="E9"/>
-      <c r="F9"/>
-    </row>
-    <row r="10" spans="1:8">
-      <c r="E10"/>
-      <c r="F10"/>
-    </row>
-    <row r="11" spans="1:8">
-      <c r="E11"/>
-      <c r="F11"/>
-    </row>
-    <row r="12" spans="1:8">
-      <c r="E12"/>
-      <c r="F12"/>
-    </row>
-    <row r="13" spans="1:8">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A9" s="1">
+        <v>45793</v>
+      </c>
+      <c r="C9" t="s">
+        <v>73</v>
+      </c>
+      <c r="D9" t="s">
+        <v>17</v>
+      </c>
+      <c r="E9">
+        <v>100</v>
+      </c>
+      <c r="F9">
+        <v>1</v>
+      </c>
+      <c r="G9" s="2" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A10" s="1">
+        <v>45794</v>
+      </c>
+      <c r="C10" t="s">
+        <v>79</v>
+      </c>
+      <c r="D10" t="s">
+        <v>37</v>
+      </c>
+      <c r="E10">
+        <v>10</v>
+      </c>
+      <c r="F10">
+        <v>1</v>
+      </c>
+      <c r="G10" s="2" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A11" s="1">
+        <v>45795</v>
+      </c>
+      <c r="C11" t="s">
+        <v>75</v>
+      </c>
+      <c r="D11" t="s">
+        <v>37</v>
+      </c>
+      <c r="E11">
+        <v>50</v>
+      </c>
+      <c r="F11">
+        <v>1</v>
+      </c>
+      <c r="G11" s="2" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A12" s="1">
+        <v>45796</v>
+      </c>
+      <c r="C12" t="s">
+        <v>77</v>
+      </c>
+      <c r="D12" t="s">
+        <v>17</v>
+      </c>
+      <c r="E12">
+        <v>100</v>
+      </c>
+      <c r="F12">
+        <v>1</v>
+      </c>
+      <c r="G12" s="2" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="E13"/>
       <c r="F13"/>
     </row>
-    <row r="14" spans="1:8">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="E14"/>
       <c r="F14"/>
     </row>
-    <row r="15" spans="1:8">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="E15"/>
       <c r="F15"/>
     </row>
-    <row r="16" spans="1:8">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="E16"/>
       <c r="F16"/>
     </row>
-    <row r="17" spans="6:6">
+    <row r="17" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F17"/>
     </row>
-    <row r="18" spans="6:6">
+    <row r="18" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F18"/>
     </row>
-    <row r="19" spans="6:6">
+    <row r="19" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F19"/>
     </row>
-    <row r="20" spans="6:6">
+    <row r="20" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F20"/>
     </row>
-    <row r="21" spans="6:6">
+    <row r="21" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F21"/>
     </row>
-    <row r="22" spans="6:6">
+    <row r="22" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F22"/>
     </row>
-    <row r="23" spans="6:6">
+    <row r="23" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F23"/>
     </row>
-    <row r="24" spans="6:6">
+    <row r="24" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F24"/>
     </row>
-    <row r="25" spans="6:6">
+    <row r="25" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F25"/>
     </row>
-    <row r="26" spans="6:6">
+    <row r="26" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F26"/>
     </row>
-    <row r="27" spans="6:6">
+    <row r="27" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F27"/>
     </row>
-    <row r="28" spans="6:6">
+    <row r="28" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F28"/>
     </row>
   </sheetData>
@@ -1315,7 +1403,7 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
   <ignoredErrors>
-    <ignoredError sqref="D9:D16" listDataValidation="1"/>
+    <ignoredError sqref="D13:D16" listDataValidation="1"/>
   </ignoredErrors>
   <tableParts count="1">
     <tablePart r:id="rId2"/>
@@ -1331,19 +1419,19 @@
       <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.83203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="17.25" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="55.58203125" customWidth="1"/>
-    <col min="4" max="4" width="10.58203125" customWidth="1"/>
-    <col min="5" max="5" width="14.83203125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14.25" customWidth="1"/>
-    <col min="7" max="7" width="92.83203125" customWidth="1"/>
-    <col min="8" max="8" width="82.4140625" customWidth="1"/>
+    <col min="1" max="1" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="55.5703125" customWidth="1"/>
+    <col min="4" max="4" width="10.5703125" customWidth="1"/>
+    <col min="5" max="5" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.28515625" customWidth="1"/>
+    <col min="7" max="7" width="92.85546875" customWidth="1"/>
+    <col min="8" max="8" width="82.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="15.5">
+    <row r="1" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
@@ -1369,7 +1457,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:8">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="8">
         <v>45786</v>
       </c>
@@ -1395,7 +1483,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="3" spans="1:8">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="8">
         <v>45787</v>
       </c>
@@ -1421,7 +1509,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="4" spans="1:8">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="8">
         <v>45789</v>
       </c>
@@ -1445,7 +1533,7 @@
       </c>
       <c r="H4" s="2"/>
     </row>
-    <row r="5" spans="1:8">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="8">
         <v>45790</v>
       </c>
@@ -1469,7 +1557,7 @@
       </c>
       <c r="H5" s="2"/>
     </row>
-    <row r="6" spans="1:8">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="8">
         <v>45791</v>
       </c>
@@ -1495,565 +1583,565 @@
         <v>49</v>
       </c>
     </row>
-    <row r="7" spans="1:8">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="8"/>
       <c r="B7" s="2"/>
       <c r="G7" s="2"/>
       <c r="H7" s="2"/>
     </row>
-    <row r="8" spans="1:8">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="8"/>
       <c r="B8" s="2"/>
       <c r="G8" s="2"/>
       <c r="H8" s="2"/>
     </row>
-    <row r="9" spans="1:8">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="8"/>
       <c r="B9" s="2"/>
       <c r="G9" s="2"/>
       <c r="H9" s="2"/>
     </row>
-    <row r="10" spans="1:8">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="8"/>
       <c r="B10" s="2"/>
       <c r="G10" s="2"/>
       <c r="H10" s="2"/>
     </row>
-    <row r="11" spans="1:8">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="8"/>
       <c r="B11" s="2"/>
       <c r="G11" s="2"/>
       <c r="H11" s="2"/>
     </row>
-    <row r="12" spans="1:8">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="8"/>
       <c r="B12" s="2"/>
       <c r="G12" s="2"/>
       <c r="H12" s="2"/>
     </row>
-    <row r="13" spans="1:8">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="8"/>
       <c r="B13" s="2"/>
       <c r="G13" s="2"/>
       <c r="H13" s="2"/>
     </row>
-    <row r="14" spans="1:8">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" s="8"/>
       <c r="B14" s="2"/>
       <c r="G14" s="2"/>
       <c r="H14" s="2"/>
     </row>
-    <row r="15" spans="1:8">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" s="8"/>
       <c r="B15" s="2"/>
       <c r="G15" s="2"/>
       <c r="H15" s="2"/>
     </row>
-    <row r="16" spans="1:8">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" s="8"/>
       <c r="B16" s="2"/>
       <c r="G16" s="2"/>
       <c r="H16" s="2"/>
     </row>
-    <row r="17" spans="1:8">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" s="8"/>
       <c r="B17" s="2"/>
       <c r="G17" s="2"/>
       <c r="H17" s="2"/>
     </row>
-    <row r="18" spans="1:8">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" s="8"/>
       <c r="B18" s="2"/>
       <c r="G18" s="2"/>
       <c r="H18" s="2"/>
     </row>
-    <row r="19" spans="1:8">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" s="8"/>
       <c r="B19" s="2"/>
       <c r="G19" s="2"/>
       <c r="H19" s="2"/>
     </row>
-    <row r="20" spans="1:8">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" s="8"/>
       <c r="B20" s="2"/>
       <c r="G20" s="2"/>
       <c r="H20" s="2"/>
     </row>
-    <row r="21" spans="1:8">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" s="8"/>
       <c r="B21" s="2"/>
       <c r="G21" s="2"/>
       <c r="H21" s="2"/>
     </row>
-    <row r="22" spans="1:8">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" s="8"/>
       <c r="B22" s="2"/>
       <c r="G22" s="2"/>
       <c r="H22" s="2"/>
     </row>
-    <row r="23" spans="1:8">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" s="8"/>
       <c r="B23" s="2"/>
       <c r="G23" s="2"/>
       <c r="H23" s="2"/>
     </row>
-    <row r="24" spans="1:8">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24" s="8"/>
       <c r="B24" s="2"/>
       <c r="G24" s="2"/>
       <c r="H24" s="2"/>
     </row>
-    <row r="25" spans="1:8">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25" s="8"/>
       <c r="B25" s="2"/>
       <c r="G25" s="2"/>
       <c r="H25" s="2"/>
     </row>
-    <row r="26" spans="1:8">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26" s="8"/>
       <c r="B26" s="2"/>
       <c r="G26" s="2"/>
       <c r="H26" s="2"/>
     </row>
-    <row r="27" spans="1:8">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A27" s="8"/>
       <c r="B27" s="2"/>
       <c r="G27" s="2"/>
       <c r="H27" s="2"/>
     </row>
-    <row r="28" spans="1:8">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A28" s="8"/>
       <c r="B28" s="2"/>
       <c r="G28" s="2"/>
       <c r="H28" s="2"/>
     </row>
-    <row r="29" spans="1:8">
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A29" s="8"/>
       <c r="B29" s="2"/>
       <c r="G29" s="2"/>
       <c r="H29" s="2"/>
     </row>
-    <row r="30" spans="1:8">
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A30" s="8"/>
       <c r="B30" s="2"/>
       <c r="G30" s="2"/>
       <c r="H30" s="2"/>
     </row>
-    <row r="31" spans="1:8">
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A31" s="8"/>
       <c r="B31" s="2"/>
       <c r="G31" s="2"/>
       <c r="H31" s="2"/>
     </row>
-    <row r="32" spans="1:8">
+    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A32" s="8"/>
       <c r="B32" s="2"/>
       <c r="G32" s="2"/>
       <c r="H32" s="2"/>
     </row>
-    <row r="33" spans="1:8">
+    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A33" s="8"/>
       <c r="B33" s="2"/>
       <c r="G33" s="2"/>
       <c r="H33" s="2"/>
     </row>
-    <row r="34" spans="1:8">
+    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A34" s="8"/>
       <c r="B34" s="2"/>
       <c r="G34" s="2"/>
       <c r="H34" s="2"/>
     </row>
-    <row r="35" spans="1:8">
+    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A35" s="8"/>
       <c r="B35" s="2"/>
       <c r="G35" s="2"/>
       <c r="H35" s="2"/>
     </row>
-    <row r="36" spans="1:8">
+    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A36" s="8"/>
       <c r="B36" s="2"/>
       <c r="G36" s="2"/>
       <c r="H36" s="2"/>
     </row>
-    <row r="37" spans="1:8">
+    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A37" s="8"/>
       <c r="B37" s="2"/>
       <c r="G37" s="2"/>
       <c r="H37" s="2"/>
     </row>
-    <row r="38" spans="1:8">
+    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A38" s="8"/>
       <c r="B38" s="2"/>
       <c r="G38" s="2"/>
       <c r="H38" s="2"/>
     </row>
-    <row r="39" spans="1:8">
+    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A39" s="8"/>
       <c r="B39" s="2"/>
       <c r="G39" s="2"/>
       <c r="H39" s="2"/>
     </row>
-    <row r="40" spans="1:8">
+    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A40" s="8"/>
       <c r="B40" s="2"/>
       <c r="G40" s="2"/>
       <c r="H40" s="2"/>
     </row>
-    <row r="41" spans="1:8">
+    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A41" s="8"/>
       <c r="B41" s="2"/>
       <c r="G41" s="2"/>
       <c r="H41" s="2"/>
     </row>
-    <row r="42" spans="1:8">
+    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A42" s="8"/>
       <c r="B42" s="2"/>
       <c r="G42" s="2"/>
       <c r="H42" s="2"/>
     </row>
-    <row r="43" spans="1:8">
+    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A43" s="8"/>
       <c r="B43" s="2"/>
       <c r="G43" s="2"/>
       <c r="H43" s="2"/>
     </row>
-    <row r="44" spans="1:8">
+    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A44" s="8"/>
       <c r="B44" s="2"/>
       <c r="G44" s="2"/>
       <c r="H44" s="2"/>
     </row>
-    <row r="45" spans="1:8">
+    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A45" s="8"/>
       <c r="B45" s="2"/>
       <c r="G45" s="2"/>
       <c r="H45" s="2"/>
     </row>
-    <row r="46" spans="1:8">
+    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A46" s="8"/>
       <c r="B46" s="2"/>
       <c r="G46" s="2"/>
       <c r="H46" s="2"/>
     </row>
-    <row r="47" spans="1:8">
+    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A47" s="8"/>
       <c r="B47" s="2"/>
       <c r="G47" s="2"/>
       <c r="H47" s="2"/>
     </row>
-    <row r="48" spans="1:8">
+    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A48" s="8"/>
       <c r="B48" s="2"/>
       <c r="G48" s="2"/>
       <c r="H48" s="2"/>
     </row>
-    <row r="49" spans="1:8">
+    <row r="49" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A49" s="8"/>
       <c r="B49" s="2"/>
       <c r="G49" s="2"/>
       <c r="H49" s="2"/>
     </row>
-    <row r="50" spans="1:8">
+    <row r="50" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A50" s="8"/>
       <c r="B50" s="2"/>
       <c r="G50" s="2"/>
       <c r="H50" s="2"/>
     </row>
-    <row r="51" spans="1:8">
+    <row r="51" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A51" s="8"/>
       <c r="B51" s="2"/>
       <c r="G51" s="2"/>
       <c r="H51" s="2"/>
     </row>
-    <row r="52" spans="1:8">
+    <row r="52" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A52" s="8"/>
       <c r="B52" s="2"/>
       <c r="G52" s="2"/>
       <c r="H52" s="2"/>
     </row>
-    <row r="53" spans="1:8">
+    <row r="53" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A53" s="8"/>
       <c r="B53" s="2"/>
       <c r="G53" s="2"/>
       <c r="H53" s="2"/>
     </row>
-    <row r="54" spans="1:8">
+    <row r="54" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A54" s="8"/>
       <c r="B54" s="2"/>
       <c r="G54" s="2"/>
       <c r="H54" s="2"/>
     </row>
-    <row r="55" spans="1:8">
+    <row r="55" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A55" s="8"/>
       <c r="B55" s="2"/>
       <c r="G55" s="2"/>
       <c r="H55" s="2"/>
     </row>
-    <row r="56" spans="1:8">
+    <row r="56" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A56" s="8"/>
       <c r="B56" s="2"/>
       <c r="G56" s="2"/>
       <c r="H56" s="2"/>
     </row>
-    <row r="57" spans="1:8">
+    <row r="57" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A57" s="8"/>
       <c r="B57" s="2"/>
       <c r="G57" s="2"/>
       <c r="H57" s="2"/>
     </row>
-    <row r="58" spans="1:8">
+    <row r="58" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A58" s="8"/>
       <c r="B58" s="2"/>
       <c r="G58" s="2"/>
       <c r="H58" s="2"/>
     </row>
-    <row r="59" spans="1:8">
+    <row r="59" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A59" s="8"/>
       <c r="B59" s="2"/>
       <c r="G59" s="2"/>
       <c r="H59" s="2"/>
     </row>
-    <row r="60" spans="1:8">
+    <row r="60" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A60" s="8"/>
       <c r="B60" s="2"/>
       <c r="G60" s="2"/>
       <c r="H60" s="2"/>
     </row>
-    <row r="61" spans="1:8">
+    <row r="61" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A61" s="8"/>
       <c r="B61" s="2"/>
       <c r="G61" s="2"/>
       <c r="H61" s="2"/>
     </row>
-    <row r="62" spans="1:8">
+    <row r="62" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A62" s="8"/>
       <c r="B62" s="2"/>
       <c r="G62" s="2"/>
       <c r="H62" s="2"/>
     </row>
-    <row r="63" spans="1:8">
+    <row r="63" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A63" s="8"/>
       <c r="B63" s="2"/>
       <c r="G63" s="2"/>
       <c r="H63" s="2"/>
     </row>
-    <row r="64" spans="1:8">
+    <row r="64" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A64" s="8"/>
       <c r="B64" s="2"/>
       <c r="G64" s="2"/>
       <c r="H64" s="2"/>
     </row>
-    <row r="65" spans="1:8">
+    <row r="65" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A65" s="8"/>
       <c r="B65" s="2"/>
       <c r="G65" s="2"/>
       <c r="H65" s="2"/>
     </row>
-    <row r="66" spans="1:8">
+    <row r="66" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A66" s="8"/>
       <c r="B66" s="2"/>
       <c r="G66" s="2"/>
       <c r="H66" s="2"/>
     </row>
-    <row r="67" spans="1:8">
+    <row r="67" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A67" s="8"/>
       <c r="B67" s="2"/>
       <c r="G67" s="2"/>
       <c r="H67" s="2"/>
     </row>
-    <row r="68" spans="1:8">
+    <row r="68" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A68" s="8"/>
       <c r="B68" s="2"/>
       <c r="G68" s="2"/>
       <c r="H68" s="2"/>
     </row>
-    <row r="69" spans="1:8">
+    <row r="69" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A69" s="8"/>
       <c r="B69" s="2"/>
       <c r="G69" s="2"/>
       <c r="H69" s="2"/>
     </row>
-    <row r="70" spans="1:8">
+    <row r="70" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A70" s="8"/>
       <c r="B70" s="2"/>
       <c r="G70" s="2"/>
       <c r="H70" s="2"/>
     </row>
-    <row r="71" spans="1:8">
+    <row r="71" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A71" s="8"/>
       <c r="B71" s="2"/>
       <c r="G71" s="2"/>
       <c r="H71" s="2"/>
     </row>
-    <row r="72" spans="1:8">
+    <row r="72" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A72" s="8"/>
       <c r="B72" s="2"/>
       <c r="G72" s="2"/>
       <c r="H72" s="2"/>
     </row>
-    <row r="73" spans="1:8">
+    <row r="73" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A73" s="8"/>
       <c r="B73" s="2"/>
       <c r="G73" s="2"/>
       <c r="H73" s="2"/>
     </row>
-    <row r="74" spans="1:8">
+    <row r="74" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A74" s="8"/>
       <c r="B74" s="2"/>
       <c r="G74" s="2"/>
       <c r="H74" s="2"/>
     </row>
-    <row r="75" spans="1:8">
+    <row r="75" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A75" s="8"/>
       <c r="B75" s="2"/>
       <c r="G75" s="2"/>
       <c r="H75" s="2"/>
     </row>
-    <row r="76" spans="1:8">
+    <row r="76" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A76" s="8"/>
       <c r="B76" s="2"/>
       <c r="G76" s="2"/>
       <c r="H76" s="2"/>
     </row>
-    <row r="77" spans="1:8">
+    <row r="77" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A77" s="8"/>
       <c r="B77" s="2"/>
       <c r="G77" s="2"/>
       <c r="H77" s="2"/>
     </row>
-    <row r="78" spans="1:8">
+    <row r="78" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A78" s="8"/>
       <c r="B78" s="2"/>
       <c r="G78" s="2"/>
       <c r="H78" s="2"/>
     </row>
-    <row r="79" spans="1:8">
+    <row r="79" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A79" s="8"/>
       <c r="B79" s="2"/>
       <c r="G79" s="2"/>
       <c r="H79" s="2"/>
     </row>
-    <row r="80" spans="1:8">
+    <row r="80" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A80" s="8"/>
       <c r="B80" s="2"/>
       <c r="G80" s="2"/>
       <c r="H80" s="2"/>
     </row>
-    <row r="81" spans="1:8">
+    <row r="81" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A81" s="8"/>
       <c r="B81" s="2"/>
       <c r="G81" s="2"/>
       <c r="H81" s="2"/>
     </row>
-    <row r="82" spans="1:8">
+    <row r="82" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A82" s="8"/>
       <c r="B82" s="2"/>
       <c r="G82" s="2"/>
       <c r="H82" s="2"/>
     </row>
-    <row r="83" spans="1:8">
+    <row r="83" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A83" s="8"/>
       <c r="B83" s="2"/>
       <c r="G83" s="2"/>
       <c r="H83" s="2"/>
     </row>
-    <row r="84" spans="1:8">
+    <row r="84" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A84" s="8"/>
       <c r="B84" s="2"/>
       <c r="G84" s="2"/>
       <c r="H84" s="2"/>
     </row>
-    <row r="85" spans="1:8">
+    <row r="85" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A85" s="8"/>
       <c r="B85" s="2"/>
       <c r="G85" s="2"/>
       <c r="H85" s="2"/>
     </row>
-    <row r="86" spans="1:8">
+    <row r="86" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A86" s="8"/>
       <c r="B86" s="2"/>
       <c r="G86" s="2"/>
       <c r="H86" s="2"/>
     </row>
-    <row r="87" spans="1:8">
+    <row r="87" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A87" s="8"/>
       <c r="B87" s="2"/>
       <c r="G87" s="2"/>
       <c r="H87" s="2"/>
     </row>
-    <row r="88" spans="1:8">
+    <row r="88" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A88" s="8"/>
       <c r="B88" s="2"/>
       <c r="G88" s="2"/>
       <c r="H88" s="2"/>
     </row>
-    <row r="89" spans="1:8">
+    <row r="89" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A89" s="8"/>
       <c r="B89" s="2"/>
       <c r="G89" s="2"/>
       <c r="H89" s="2"/>
     </row>
-    <row r="90" spans="1:8">
+    <row r="90" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A90" s="8"/>
       <c r="B90" s="2"/>
       <c r="G90" s="2"/>
       <c r="H90" s="2"/>
     </row>
-    <row r="91" spans="1:8">
+    <row r="91" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A91" s="8"/>
       <c r="B91" s="2"/>
       <c r="G91" s="2"/>
       <c r="H91" s="2"/>
     </row>
-    <row r="92" spans="1:8">
+    <row r="92" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A92" s="8"/>
       <c r="B92" s="2"/>
       <c r="G92" s="2"/>
       <c r="H92" s="2"/>
     </row>
-    <row r="93" spans="1:8">
+    <row r="93" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A93" s="8"/>
       <c r="B93" s="2"/>
       <c r="G93" s="2"/>
       <c r="H93" s="2"/>
     </row>
-    <row r="94" spans="1:8">
+    <row r="94" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A94" s="8"/>
       <c r="B94" s="2"/>
       <c r="G94" s="2"/>
       <c r="H94" s="2"/>
     </row>
-    <row r="95" spans="1:8">
+    <row r="95" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A95" s="8"/>
       <c r="B95" s="2"/>
       <c r="G95" s="2"/>
       <c r="H95" s="2"/>
     </row>
-    <row r="96" spans="1:8">
+    <row r="96" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A96" s="8"/>
       <c r="B96" s="2"/>
       <c r="G96" s="2"/>
       <c r="H96" s="2"/>
     </row>
-    <row r="97" spans="1:8">
+    <row r="97" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A97" s="8"/>
       <c r="B97" s="2"/>
       <c r="G97" s="2"/>
       <c r="H97" s="2"/>
     </row>
-    <row r="98" spans="1:8">
+    <row r="98" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A98" s="8"/>
       <c r="B98" s="2"/>
       <c r="G98" s="2"/>
       <c r="H98" s="2"/>
     </row>
-    <row r="99" spans="1:8">
+    <row r="99" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A99" s="8"/>
       <c r="B99" s="2"/>
       <c r="G99" s="2"/>
       <c r="H99" s="2"/>
     </row>
-    <row r="100" spans="1:8">
+    <row r="100" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A100" s="8"/>
       <c r="B100" s="2"/>
       <c r="G100" s="2"/>
@@ -2090,23 +2178,23 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9FD6A201-8E63-4A9E-A683-19506CB489E3}">
   <dimension ref="A1:H100"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.1640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="17.25" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="27.83203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.75" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.83203125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="23.58203125" style="10" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="39.1640625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="51.1640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="27.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="23.5703125" style="10" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="39.140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="51.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="15.5">
+    <row r="1" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
@@ -2132,7 +2220,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:8">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>45935</v>
       </c>
@@ -2158,7 +2246,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="3" spans="1:8">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>45996</v>
       </c>
@@ -2184,7 +2272,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="4" spans="1:8">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>57</v>
       </c>
@@ -2210,7 +2298,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="5" spans="1:8">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>61</v>
       </c>
@@ -2236,7 +2324,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="6" spans="1:8">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>67</v>
       </c>
@@ -2262,7 +2350,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="7" spans="1:8">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>70</v>
       </c>
@@ -2288,651 +2376,651 @@
         <v>54</v>
       </c>
     </row>
-    <row r="8" spans="1:8">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="1"/>
       <c r="B8" s="2"/>
       <c r="E8" s="3"/>
       <c r="G8" s="2"/>
       <c r="H8" s="2"/>
     </row>
-    <row r="9" spans="1:8">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="1"/>
       <c r="B9" s="2"/>
       <c r="E9" s="3"/>
       <c r="G9" s="2"/>
       <c r="H9" s="2"/>
     </row>
-    <row r="10" spans="1:8">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="1"/>
       <c r="B10" s="2"/>
       <c r="E10" s="3"/>
       <c r="G10" s="2"/>
       <c r="H10" s="2"/>
     </row>
-    <row r="11" spans="1:8">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="1"/>
       <c r="B11" s="2"/>
       <c r="E11" s="3"/>
       <c r="G11" s="2"/>
       <c r="H11" s="2"/>
     </row>
-    <row r="12" spans="1:8">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="1"/>
       <c r="B12" s="2"/>
       <c r="E12" s="3"/>
       <c r="G12" s="2"/>
       <c r="H12" s="2"/>
     </row>
-    <row r="13" spans="1:8">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="1"/>
       <c r="B13" s="2"/>
       <c r="E13" s="3"/>
       <c r="G13" s="2"/>
       <c r="H13" s="2"/>
     </row>
-    <row r="14" spans="1:8">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" s="1"/>
       <c r="B14" s="2"/>
       <c r="E14" s="3"/>
       <c r="G14" s="2"/>
       <c r="H14" s="2"/>
     </row>
-    <row r="15" spans="1:8">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" s="1"/>
       <c r="B15" s="2"/>
       <c r="E15" s="3"/>
       <c r="G15" s="2"/>
       <c r="H15" s="2"/>
     </row>
-    <row r="16" spans="1:8">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" s="1"/>
       <c r="B16" s="2"/>
       <c r="E16" s="3"/>
       <c r="G16" s="2"/>
       <c r="H16" s="2"/>
     </row>
-    <row r="17" spans="1:8">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" s="1"/>
       <c r="B17" s="2"/>
       <c r="E17" s="3"/>
       <c r="G17" s="2"/>
       <c r="H17" s="2"/>
     </row>
-    <row r="18" spans="1:8">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" s="1"/>
       <c r="B18" s="2"/>
       <c r="E18" s="3"/>
       <c r="G18" s="2"/>
       <c r="H18" s="2"/>
     </row>
-    <row r="19" spans="1:8">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" s="1"/>
       <c r="B19" s="2"/>
       <c r="E19" s="3"/>
       <c r="G19" s="2"/>
       <c r="H19" s="2"/>
     </row>
-    <row r="20" spans="1:8">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" s="1"/>
       <c r="B20" s="2"/>
       <c r="E20" s="3"/>
       <c r="G20" s="2"/>
       <c r="H20" s="2"/>
     </row>
-    <row r="21" spans="1:8">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" s="1"/>
       <c r="B21" s="2"/>
       <c r="E21" s="3"/>
       <c r="G21" s="2"/>
       <c r="H21" s="2"/>
     </row>
-    <row r="22" spans="1:8">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" s="1"/>
       <c r="B22" s="2"/>
       <c r="E22" s="3"/>
       <c r="G22" s="2"/>
       <c r="H22" s="2"/>
     </row>
-    <row r="23" spans="1:8">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" s="1"/>
       <c r="B23" s="2"/>
       <c r="E23" s="3"/>
       <c r="G23" s="2"/>
       <c r="H23" s="2"/>
     </row>
-    <row r="24" spans="1:8">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24" s="1"/>
       <c r="B24" s="2"/>
       <c r="E24" s="3"/>
       <c r="G24" s="2"/>
       <c r="H24" s="2"/>
     </row>
-    <row r="25" spans="1:8">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25" s="1"/>
       <c r="B25" s="2"/>
       <c r="E25" s="3"/>
       <c r="G25" s="2"/>
       <c r="H25" s="2"/>
     </row>
-    <row r="26" spans="1:8">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26" s="1"/>
       <c r="B26" s="2"/>
       <c r="E26" s="3"/>
       <c r="G26" s="2"/>
       <c r="H26" s="2"/>
     </row>
-    <row r="27" spans="1:8">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A27" s="1"/>
       <c r="B27" s="2"/>
       <c r="E27" s="3"/>
       <c r="G27" s="2"/>
       <c r="H27" s="2"/>
     </row>
-    <row r="28" spans="1:8">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A28" s="1"/>
       <c r="B28" s="2"/>
       <c r="E28" s="3"/>
       <c r="G28" s="2"/>
       <c r="H28" s="2"/>
     </row>
-    <row r="29" spans="1:8">
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A29" s="1"/>
       <c r="B29" s="2"/>
       <c r="E29" s="3"/>
       <c r="G29" s="2"/>
       <c r="H29" s="2"/>
     </row>
-    <row r="30" spans="1:8">
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A30" s="1"/>
       <c r="B30" s="2"/>
       <c r="E30" s="3"/>
       <c r="G30" s="2"/>
       <c r="H30" s="2"/>
     </row>
-    <row r="31" spans="1:8">
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A31" s="1"/>
       <c r="B31" s="2"/>
       <c r="E31" s="3"/>
       <c r="G31" s="2"/>
       <c r="H31" s="2"/>
     </row>
-    <row r="32" spans="1:8">
+    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A32" s="1"/>
       <c r="B32" s="2"/>
       <c r="E32" s="3"/>
       <c r="G32" s="2"/>
       <c r="H32" s="2"/>
     </row>
-    <row r="33" spans="1:8">
+    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A33" s="1"/>
       <c r="B33" s="2"/>
       <c r="E33" s="3"/>
       <c r="G33" s="2"/>
       <c r="H33" s="2"/>
     </row>
-    <row r="34" spans="1:8">
+    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A34" s="1"/>
       <c r="B34" s="2"/>
       <c r="E34" s="3"/>
       <c r="G34" s="2"/>
       <c r="H34" s="2"/>
     </row>
-    <row r="35" spans="1:8">
+    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A35" s="1"/>
       <c r="B35" s="2"/>
       <c r="E35" s="3"/>
       <c r="G35" s="2"/>
       <c r="H35" s="2"/>
     </row>
-    <row r="36" spans="1:8">
+    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A36" s="1"/>
       <c r="B36" s="2"/>
       <c r="E36" s="3"/>
       <c r="G36" s="2"/>
       <c r="H36" s="2"/>
     </row>
-    <row r="37" spans="1:8">
+    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A37" s="1"/>
       <c r="B37" s="2"/>
       <c r="E37" s="3"/>
       <c r="G37" s="2"/>
       <c r="H37" s="2"/>
     </row>
-    <row r="38" spans="1:8">
+    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A38" s="1"/>
       <c r="B38" s="2"/>
       <c r="E38" s="3"/>
       <c r="G38" s="2"/>
       <c r="H38" s="2"/>
     </row>
-    <row r="39" spans="1:8">
+    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A39" s="1"/>
       <c r="B39" s="2"/>
       <c r="E39" s="3"/>
       <c r="G39" s="2"/>
       <c r="H39" s="2"/>
     </row>
-    <row r="40" spans="1:8">
+    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A40" s="1"/>
       <c r="B40" s="2"/>
       <c r="E40" s="3"/>
       <c r="G40" s="2"/>
       <c r="H40" s="2"/>
     </row>
-    <row r="41" spans="1:8">
+    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A41" s="1"/>
       <c r="B41" s="2"/>
       <c r="E41" s="3"/>
       <c r="G41" s="2"/>
       <c r="H41" s="2"/>
     </row>
-    <row r="42" spans="1:8">
+    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A42" s="1"/>
       <c r="B42" s="2"/>
       <c r="E42" s="3"/>
       <c r="G42" s="2"/>
       <c r="H42" s="2"/>
     </row>
-    <row r="43" spans="1:8">
+    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A43" s="1"/>
       <c r="B43" s="2"/>
       <c r="E43" s="3"/>
       <c r="G43" s="2"/>
       <c r="H43" s="2"/>
     </row>
-    <row r="44" spans="1:8">
+    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A44" s="1"/>
       <c r="B44" s="2"/>
       <c r="E44" s="3"/>
       <c r="G44" s="2"/>
       <c r="H44" s="2"/>
     </row>
-    <row r="45" spans="1:8">
+    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A45" s="1"/>
       <c r="B45" s="2"/>
       <c r="E45" s="3"/>
       <c r="G45" s="2"/>
       <c r="H45" s="2"/>
     </row>
-    <row r="46" spans="1:8">
+    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A46" s="1"/>
       <c r="B46" s="2"/>
       <c r="E46" s="3"/>
       <c r="G46" s="2"/>
       <c r="H46" s="2"/>
     </row>
-    <row r="47" spans="1:8">
+    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A47" s="1"/>
       <c r="B47" s="2"/>
       <c r="E47" s="3"/>
       <c r="G47" s="2"/>
       <c r="H47" s="2"/>
     </row>
-    <row r="48" spans="1:8">
+    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A48" s="1"/>
       <c r="B48" s="2"/>
       <c r="E48" s="3"/>
       <c r="G48" s="2"/>
       <c r="H48" s="2"/>
     </row>
-    <row r="49" spans="1:8">
+    <row r="49" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A49" s="1"/>
       <c r="B49" s="2"/>
       <c r="E49" s="3"/>
       <c r="G49" s="2"/>
       <c r="H49" s="2"/>
     </row>
-    <row r="50" spans="1:8">
+    <row r="50" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A50" s="1"/>
       <c r="B50" s="2"/>
       <c r="E50" s="3"/>
       <c r="G50" s="2"/>
       <c r="H50" s="2"/>
     </row>
-    <row r="51" spans="1:8">
+    <row r="51" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A51" s="1"/>
       <c r="B51" s="2"/>
       <c r="E51" s="3"/>
       <c r="G51" s="2"/>
       <c r="H51" s="2"/>
     </row>
-    <row r="52" spans="1:8">
+    <row r="52" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A52" s="1"/>
       <c r="B52" s="2"/>
       <c r="E52" s="3"/>
       <c r="G52" s="2"/>
       <c r="H52" s="2"/>
     </row>
-    <row r="53" spans="1:8">
+    <row r="53" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A53" s="1"/>
       <c r="B53" s="2"/>
       <c r="E53" s="3"/>
       <c r="G53" s="2"/>
       <c r="H53" s="2"/>
     </row>
-    <row r="54" spans="1:8">
+    <row r="54" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A54" s="1"/>
       <c r="B54" s="2"/>
       <c r="E54" s="3"/>
       <c r="G54" s="2"/>
       <c r="H54" s="2"/>
     </row>
-    <row r="55" spans="1:8">
+    <row r="55" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A55" s="1"/>
       <c r="B55" s="2"/>
       <c r="E55" s="3"/>
       <c r="G55" s="2"/>
       <c r="H55" s="2"/>
     </row>
-    <row r="56" spans="1:8">
+    <row r="56" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A56" s="1"/>
       <c r="B56" s="2"/>
       <c r="E56" s="3"/>
       <c r="G56" s="2"/>
       <c r="H56" s="2"/>
     </row>
-    <row r="57" spans="1:8">
+    <row r="57" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A57" s="1"/>
       <c r="B57" s="2"/>
       <c r="E57" s="3"/>
       <c r="G57" s="2"/>
       <c r="H57" s="2"/>
     </row>
-    <row r="58" spans="1:8">
+    <row r="58" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A58" s="1"/>
       <c r="B58" s="2"/>
       <c r="E58" s="3"/>
       <c r="G58" s="2"/>
       <c r="H58" s="2"/>
     </row>
-    <row r="59" spans="1:8">
+    <row r="59" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A59" s="1"/>
       <c r="B59" s="2"/>
       <c r="E59" s="3"/>
       <c r="G59" s="2"/>
       <c r="H59" s="2"/>
     </row>
-    <row r="60" spans="1:8">
+    <row r="60" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A60" s="1"/>
       <c r="B60" s="2"/>
       <c r="E60" s="3"/>
       <c r="G60" s="2"/>
       <c r="H60" s="2"/>
     </row>
-    <row r="61" spans="1:8">
+    <row r="61" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A61" s="1"/>
       <c r="B61" s="2"/>
       <c r="E61" s="3"/>
       <c r="G61" s="2"/>
       <c r="H61" s="2"/>
     </row>
-    <row r="62" spans="1:8">
+    <row r="62" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A62" s="1"/>
       <c r="B62" s="2"/>
       <c r="E62" s="3"/>
       <c r="G62" s="2"/>
       <c r="H62" s="2"/>
     </row>
-    <row r="63" spans="1:8">
+    <row r="63" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A63" s="1"/>
       <c r="B63" s="2"/>
       <c r="E63" s="3"/>
       <c r="G63" s="2"/>
       <c r="H63" s="2"/>
     </row>
-    <row r="64" spans="1:8">
+    <row r="64" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A64" s="1"/>
       <c r="B64" s="2"/>
       <c r="E64" s="3"/>
       <c r="G64" s="2"/>
       <c r="H64" s="2"/>
     </row>
-    <row r="65" spans="1:8">
+    <row r="65" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A65" s="1"/>
       <c r="B65" s="2"/>
       <c r="E65" s="3"/>
       <c r="G65" s="2"/>
       <c r="H65" s="2"/>
     </row>
-    <row r="66" spans="1:8">
+    <row r="66" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A66" s="1"/>
       <c r="B66" s="2"/>
       <c r="E66" s="3"/>
       <c r="G66" s="2"/>
       <c r="H66" s="2"/>
     </row>
-    <row r="67" spans="1:8">
+    <row r="67" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A67" s="1"/>
       <c r="B67" s="2"/>
       <c r="E67" s="3"/>
       <c r="G67" s="2"/>
       <c r="H67" s="2"/>
     </row>
-    <row r="68" spans="1:8">
+    <row r="68" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A68" s="1"/>
       <c r="B68" s="2"/>
       <c r="E68" s="3"/>
       <c r="G68" s="2"/>
       <c r="H68" s="2"/>
     </row>
-    <row r="69" spans="1:8">
+    <row r="69" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A69" s="1"/>
       <c r="B69" s="2"/>
       <c r="E69" s="3"/>
       <c r="G69" s="2"/>
       <c r="H69" s="2"/>
     </row>
-    <row r="70" spans="1:8">
+    <row r="70" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A70" s="1"/>
       <c r="B70" s="2"/>
       <c r="E70" s="3"/>
       <c r="G70" s="2"/>
       <c r="H70" s="2"/>
     </row>
-    <row r="71" spans="1:8">
+    <row r="71" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A71" s="1"/>
       <c r="B71" s="2"/>
       <c r="E71" s="3"/>
       <c r="G71" s="2"/>
       <c r="H71" s="2"/>
     </row>
-    <row r="72" spans="1:8">
+    <row r="72" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A72" s="1"/>
       <c r="B72" s="2"/>
       <c r="E72" s="3"/>
       <c r="G72" s="2"/>
       <c r="H72" s="2"/>
     </row>
-    <row r="73" spans="1:8">
+    <row r="73" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A73" s="1"/>
       <c r="B73" s="2"/>
       <c r="E73" s="3"/>
       <c r="G73" s="2"/>
       <c r="H73" s="2"/>
     </row>
-    <row r="74" spans="1:8">
+    <row r="74" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A74" s="1"/>
       <c r="B74" s="2"/>
       <c r="E74" s="3"/>
       <c r="G74" s="2"/>
       <c r="H74" s="2"/>
     </row>
-    <row r="75" spans="1:8">
+    <row r="75" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A75" s="1"/>
       <c r="B75" s="2"/>
       <c r="E75" s="3"/>
       <c r="G75" s="2"/>
       <c r="H75" s="2"/>
     </row>
-    <row r="76" spans="1:8">
+    <row r="76" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A76" s="1"/>
       <c r="B76" s="2"/>
       <c r="E76" s="3"/>
       <c r="G76" s="2"/>
       <c r="H76" s="2"/>
     </row>
-    <row r="77" spans="1:8">
+    <row r="77" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A77" s="1"/>
       <c r="B77" s="2"/>
       <c r="E77" s="3"/>
       <c r="G77" s="2"/>
       <c r="H77" s="2"/>
     </row>
-    <row r="78" spans="1:8">
+    <row r="78" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A78" s="1"/>
       <c r="B78" s="2"/>
       <c r="E78" s="3"/>
       <c r="G78" s="2"/>
       <c r="H78" s="2"/>
     </row>
-    <row r="79" spans="1:8">
+    <row r="79" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A79" s="1"/>
       <c r="B79" s="2"/>
       <c r="E79" s="3"/>
       <c r="G79" s="2"/>
       <c r="H79" s="2"/>
     </row>
-    <row r="80" spans="1:8">
+    <row r="80" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A80" s="1"/>
       <c r="B80" s="2"/>
       <c r="E80" s="3"/>
       <c r="G80" s="2"/>
       <c r="H80" s="2"/>
     </row>
-    <row r="81" spans="1:8">
+    <row r="81" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A81" s="1"/>
       <c r="B81" s="2"/>
       <c r="E81" s="3"/>
       <c r="G81" s="2"/>
       <c r="H81" s="2"/>
     </row>
-    <row r="82" spans="1:8">
+    <row r="82" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A82" s="1"/>
       <c r="B82" s="2"/>
       <c r="E82" s="3"/>
       <c r="G82" s="2"/>
       <c r="H82" s="2"/>
     </row>
-    <row r="83" spans="1:8">
+    <row r="83" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A83" s="1"/>
       <c r="B83" s="2"/>
       <c r="E83" s="3"/>
       <c r="G83" s="2"/>
       <c r="H83" s="2"/>
     </row>
-    <row r="84" spans="1:8">
+    <row r="84" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A84" s="1"/>
       <c r="B84" s="2"/>
       <c r="E84" s="3"/>
       <c r="G84" s="2"/>
       <c r="H84" s="2"/>
     </row>
-    <row r="85" spans="1:8">
+    <row r="85" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A85" s="1"/>
       <c r="B85" s="2"/>
       <c r="E85" s="3"/>
       <c r="G85" s="2"/>
       <c r="H85" s="2"/>
     </row>
-    <row r="86" spans="1:8">
+    <row r="86" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A86" s="1"/>
       <c r="B86" s="2"/>
       <c r="E86" s="3"/>
       <c r="G86" s="2"/>
       <c r="H86" s="2"/>
     </row>
-    <row r="87" spans="1:8">
+    <row r="87" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A87" s="1"/>
       <c r="B87" s="2"/>
       <c r="E87" s="3"/>
       <c r="G87" s="2"/>
       <c r="H87" s="2"/>
     </row>
-    <row r="88" spans="1:8">
+    <row r="88" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A88" s="1"/>
       <c r="B88" s="2"/>
       <c r="E88" s="3"/>
       <c r="G88" s="2"/>
       <c r="H88" s="2"/>
     </row>
-    <row r="89" spans="1:8">
+    <row r="89" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A89" s="1"/>
       <c r="B89" s="2"/>
       <c r="E89" s="3"/>
       <c r="G89" s="2"/>
       <c r="H89" s="2"/>
     </row>
-    <row r="90" spans="1:8">
+    <row r="90" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A90" s="1"/>
       <c r="B90" s="2"/>
       <c r="E90" s="3"/>
       <c r="G90" s="2"/>
       <c r="H90" s="2"/>
     </row>
-    <row r="91" spans="1:8">
+    <row r="91" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A91" s="1"/>
       <c r="B91" s="2"/>
       <c r="E91" s="3"/>
       <c r="G91" s="2"/>
       <c r="H91" s="2"/>
     </row>
-    <row r="92" spans="1:8">
+    <row r="92" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A92" s="1"/>
       <c r="B92" s="2"/>
       <c r="E92" s="3"/>
       <c r="G92" s="2"/>
       <c r="H92" s="2"/>
     </row>
-    <row r="93" spans="1:8">
+    <row r="93" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A93" s="1"/>
       <c r="B93" s="2"/>
       <c r="E93" s="3"/>
       <c r="G93" s="2"/>
       <c r="H93" s="2"/>
     </row>
-    <row r="94" spans="1:8">
+    <row r="94" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A94" s="1"/>
       <c r="B94" s="2"/>
       <c r="E94" s="3"/>
       <c r="G94" s="2"/>
       <c r="H94" s="2"/>
     </row>
-    <row r="95" spans="1:8">
+    <row r="95" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A95" s="1"/>
       <c r="B95" s="2"/>
       <c r="E95" s="3"/>
       <c r="G95" s="2"/>
       <c r="H95" s="2"/>
     </row>
-    <row r="96" spans="1:8">
+    <row r="96" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A96" s="1"/>
       <c r="B96" s="2"/>
       <c r="E96" s="3"/>
       <c r="G96" s="2"/>
       <c r="H96" s="2"/>
     </row>
-    <row r="97" spans="1:8">
+    <row r="97" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A97" s="1"/>
       <c r="B97" s="2"/>
       <c r="E97" s="3"/>
       <c r="G97" s="2"/>
       <c r="H97" s="2"/>
     </row>
-    <row r="98" spans="1:8">
+    <row r="98" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A98" s="1"/>
       <c r="B98" s="2"/>
       <c r="E98" s="3"/>
       <c r="G98" s="2"/>
       <c r="H98" s="2"/>
     </row>
-    <row r="99" spans="1:8">
+    <row r="99" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A99" s="1"/>
       <c r="B99" s="2"/>
       <c r="E99" s="3"/>
       <c r="G99" s="2"/>
       <c r="H99" s="2"/>
     </row>
-    <row r="100" spans="1:8">
+    <row r="100" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A100" s="1"/>
       <c r="B100" s="2"/>
       <c r="E100" s="3"/>
@@ -2974,19 +3062,19 @@
       <selection activeCell="D2" sqref="D2:D100"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="7.75" customWidth="1"/>
-    <col min="2" max="2" width="17.25" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.58203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="7.7109375" customWidth="1"/>
+    <col min="2" max="2" width="17.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.5703125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="9" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.83203125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="23.58203125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="13.4140625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="19.1640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="23.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="19.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="15.5">
+    <row r="1" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
@@ -3012,7 +3100,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:8">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="1"/>
       <c r="B2" s="2"/>
       <c r="E2" s="3"/>
@@ -3020,7 +3108,7 @@
       <c r="G2" s="2"/>
       <c r="H2" s="2"/>
     </row>
-    <row r="3" spans="1:8">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="1"/>
       <c r="B3" s="2"/>
       <c r="E3" s="3"/>
@@ -3028,7 +3116,7 @@
       <c r="G3" s="2"/>
       <c r="H3" s="2"/>
     </row>
-    <row r="4" spans="1:8">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="1"/>
       <c r="B4" s="2"/>
       <c r="E4" s="3"/>
@@ -3036,7 +3124,7 @@
       <c r="G4" s="2"/>
       <c r="H4" s="2"/>
     </row>
-    <row r="5" spans="1:8">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="1"/>
       <c r="B5" s="2"/>
       <c r="E5" s="3"/>
@@ -3044,7 +3132,7 @@
       <c r="G5" s="2"/>
       <c r="H5" s="2"/>
     </row>
-    <row r="6" spans="1:8">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="1"/>
       <c r="B6" s="2"/>
       <c r="E6" s="3"/>
@@ -3052,7 +3140,7 @@
       <c r="G6" s="2"/>
       <c r="H6" s="2"/>
     </row>
-    <row r="7" spans="1:8">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="1"/>
       <c r="B7" s="2"/>
       <c r="E7" s="3"/>
@@ -3060,7 +3148,7 @@
       <c r="G7" s="2"/>
       <c r="H7" s="2"/>
     </row>
-    <row r="8" spans="1:8">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="1"/>
       <c r="B8" s="2"/>
       <c r="E8" s="3"/>
@@ -3068,7 +3156,7 @@
       <c r="G8" s="2"/>
       <c r="H8" s="2"/>
     </row>
-    <row r="9" spans="1:8">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="1"/>
       <c r="B9" s="2"/>
       <c r="E9" s="3"/>
@@ -3076,7 +3164,7 @@
       <c r="G9" s="2"/>
       <c r="H9" s="2"/>
     </row>
-    <row r="10" spans="1:8">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="1"/>
       <c r="B10" s="2"/>
       <c r="E10" s="3"/>
@@ -3084,7 +3172,7 @@
       <c r="G10" s="2"/>
       <c r="H10" s="2"/>
     </row>
-    <row r="11" spans="1:8">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="1"/>
       <c r="B11" s="2"/>
       <c r="E11" s="3"/>
@@ -3092,7 +3180,7 @@
       <c r="G11" s="2"/>
       <c r="H11" s="2"/>
     </row>
-    <row r="12" spans="1:8">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="1"/>
       <c r="B12" s="2"/>
       <c r="E12" s="3"/>
@@ -3100,7 +3188,7 @@
       <c r="G12" s="2"/>
       <c r="H12" s="2"/>
     </row>
-    <row r="13" spans="1:8">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="1"/>
       <c r="B13" s="2"/>
       <c r="E13" s="3"/>
@@ -3108,7 +3196,7 @@
       <c r="G13" s="2"/>
       <c r="H13" s="2"/>
     </row>
-    <row r="14" spans="1:8">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" s="1"/>
       <c r="B14" s="2"/>
       <c r="E14" s="3"/>
@@ -3116,7 +3204,7 @@
       <c r="G14" s="2"/>
       <c r="H14" s="2"/>
     </row>
-    <row r="15" spans="1:8">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" s="1"/>
       <c r="B15" s="2"/>
       <c r="E15" s="3"/>
@@ -3124,7 +3212,7 @@
       <c r="G15" s="2"/>
       <c r="H15" s="2"/>
     </row>
-    <row r="16" spans="1:8">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" s="1"/>
       <c r="B16" s="2"/>
       <c r="E16" s="3"/>
@@ -3132,7 +3220,7 @@
       <c r="G16" s="2"/>
       <c r="H16" s="2"/>
     </row>
-    <row r="17" spans="1:8">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" s="1"/>
       <c r="B17" s="2"/>
       <c r="E17" s="3"/>
@@ -3140,7 +3228,7 @@
       <c r="G17" s="2"/>
       <c r="H17" s="2"/>
     </row>
-    <row r="18" spans="1:8">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" s="1"/>
       <c r="B18" s="2"/>
       <c r="E18" s="3"/>
@@ -3148,7 +3236,7 @@
       <c r="G18" s="2"/>
       <c r="H18" s="2"/>
     </row>
-    <row r="19" spans="1:8">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" s="1"/>
       <c r="B19" s="2"/>
       <c r="E19" s="3"/>
@@ -3156,7 +3244,7 @@
       <c r="G19" s="2"/>
       <c r="H19" s="2"/>
     </row>
-    <row r="20" spans="1:8">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" s="1"/>
       <c r="B20" s="2"/>
       <c r="E20" s="3"/>
@@ -3164,7 +3252,7 @@
       <c r="G20" s="2"/>
       <c r="H20" s="2"/>
     </row>
-    <row r="21" spans="1:8">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" s="1"/>
       <c r="B21" s="2"/>
       <c r="E21" s="3"/>
@@ -3172,7 +3260,7 @@
       <c r="G21" s="2"/>
       <c r="H21" s="2"/>
     </row>
-    <row r="22" spans="1:8">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" s="1"/>
       <c r="B22" s="2"/>
       <c r="E22" s="3"/>
@@ -3180,7 +3268,7 @@
       <c r="G22" s="2"/>
       <c r="H22" s="2"/>
     </row>
-    <row r="23" spans="1:8">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" s="1"/>
       <c r="B23" s="2"/>
       <c r="E23" s="3"/>
@@ -3188,7 +3276,7 @@
       <c r="G23" s="2"/>
       <c r="H23" s="2"/>
     </row>
-    <row r="24" spans="1:8">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24" s="1"/>
       <c r="B24" s="2"/>
       <c r="E24" s="3"/>
@@ -3196,7 +3284,7 @@
       <c r="G24" s="2"/>
       <c r="H24" s="2"/>
     </row>
-    <row r="25" spans="1:8">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25" s="1"/>
       <c r="B25" s="2"/>
       <c r="E25" s="3"/>
@@ -3204,7 +3292,7 @@
       <c r="G25" s="2"/>
       <c r="H25" s="2"/>
     </row>
-    <row r="26" spans="1:8">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26" s="1"/>
       <c r="B26" s="2"/>
       <c r="E26" s="3"/>
@@ -3212,7 +3300,7 @@
       <c r="G26" s="2"/>
       <c r="H26" s="2"/>
     </row>
-    <row r="27" spans="1:8">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A27" s="1"/>
       <c r="B27" s="2"/>
       <c r="E27" s="3"/>
@@ -3220,7 +3308,7 @@
       <c r="G27" s="2"/>
       <c r="H27" s="2"/>
     </row>
-    <row r="28" spans="1:8">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A28" s="1"/>
       <c r="B28" s="2"/>
       <c r="E28" s="3"/>
@@ -3228,7 +3316,7 @@
       <c r="G28" s="2"/>
       <c r="H28" s="2"/>
     </row>
-    <row r="29" spans="1:8">
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A29" s="1"/>
       <c r="B29" s="2"/>
       <c r="E29" s="3"/>
@@ -3236,7 +3324,7 @@
       <c r="G29" s="2"/>
       <c r="H29" s="2"/>
     </row>
-    <row r="30" spans="1:8">
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A30" s="1"/>
       <c r="B30" s="2"/>
       <c r="E30" s="3"/>
@@ -3244,7 +3332,7 @@
       <c r="G30" s="2"/>
       <c r="H30" s="2"/>
     </row>
-    <row r="31" spans="1:8">
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A31" s="1"/>
       <c r="B31" s="2"/>
       <c r="E31" s="3"/>
@@ -3252,7 +3340,7 @@
       <c r="G31" s="2"/>
       <c r="H31" s="2"/>
     </row>
-    <row r="32" spans="1:8">
+    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A32" s="1"/>
       <c r="B32" s="2"/>
       <c r="E32" s="3"/>
@@ -3260,7 +3348,7 @@
       <c r="G32" s="2"/>
       <c r="H32" s="2"/>
     </row>
-    <row r="33" spans="1:8">
+    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A33" s="1"/>
       <c r="B33" s="2"/>
       <c r="E33" s="3"/>
@@ -3268,7 +3356,7 @@
       <c r="G33" s="2"/>
       <c r="H33" s="2"/>
     </row>
-    <row r="34" spans="1:8">
+    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A34" s="1"/>
       <c r="B34" s="2"/>
       <c r="E34" s="3"/>
@@ -3276,7 +3364,7 @@
       <c r="G34" s="2"/>
       <c r="H34" s="2"/>
     </row>
-    <row r="35" spans="1:8">
+    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A35" s="1"/>
       <c r="B35" s="2"/>
       <c r="E35" s="3"/>
@@ -3284,7 +3372,7 @@
       <c r="G35" s="2"/>
       <c r="H35" s="2"/>
     </row>
-    <row r="36" spans="1:8">
+    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A36" s="1"/>
       <c r="B36" s="2"/>
       <c r="E36" s="3"/>
@@ -3292,7 +3380,7 @@
       <c r="G36" s="2"/>
       <c r="H36" s="2"/>
     </row>
-    <row r="37" spans="1:8">
+    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A37" s="1"/>
       <c r="B37" s="2"/>
       <c r="E37" s="3"/>
@@ -3300,7 +3388,7 @@
       <c r="G37" s="2"/>
       <c r="H37" s="2"/>
     </row>
-    <row r="38" spans="1:8">
+    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A38" s="1"/>
       <c r="B38" s="2"/>
       <c r="E38" s="3"/>
@@ -3308,7 +3396,7 @@
       <c r="G38" s="2"/>
       <c r="H38" s="2"/>
     </row>
-    <row r="39" spans="1:8">
+    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A39" s="1"/>
       <c r="B39" s="2"/>
       <c r="E39" s="3"/>
@@ -3316,7 +3404,7 @@
       <c r="G39" s="2"/>
       <c r="H39" s="2"/>
     </row>
-    <row r="40" spans="1:8">
+    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A40" s="1"/>
       <c r="B40" s="2"/>
       <c r="E40" s="3"/>
@@ -3324,7 +3412,7 @@
       <c r="G40" s="2"/>
       <c r="H40" s="2"/>
     </row>
-    <row r="41" spans="1:8">
+    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A41" s="1"/>
       <c r="B41" s="2"/>
       <c r="E41" s="3"/>
@@ -3332,7 +3420,7 @@
       <c r="G41" s="2"/>
       <c r="H41" s="2"/>
     </row>
-    <row r="42" spans="1:8">
+    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A42" s="1"/>
       <c r="B42" s="2"/>
       <c r="E42" s="3"/>
@@ -3340,7 +3428,7 @@
       <c r="G42" s="2"/>
       <c r="H42" s="2"/>
     </row>
-    <row r="43" spans="1:8">
+    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A43" s="1"/>
       <c r="B43" s="2"/>
       <c r="E43" s="3"/>
@@ -3348,7 +3436,7 @@
       <c r="G43" s="2"/>
       <c r="H43" s="2"/>
     </row>
-    <row r="44" spans="1:8">
+    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A44" s="1"/>
       <c r="B44" s="2"/>
       <c r="E44" s="3"/>
@@ -3356,7 +3444,7 @@
       <c r="G44" s="2"/>
       <c r="H44" s="2"/>
     </row>
-    <row r="45" spans="1:8">
+    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A45" s="1"/>
       <c r="B45" s="2"/>
       <c r="E45" s="3"/>
@@ -3364,7 +3452,7 @@
       <c r="G45" s="2"/>
       <c r="H45" s="2"/>
     </row>
-    <row r="46" spans="1:8">
+    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A46" s="1"/>
       <c r="B46" s="2"/>
       <c r="E46" s="3"/>
@@ -3372,7 +3460,7 @@
       <c r="G46" s="2"/>
       <c r="H46" s="2"/>
     </row>
-    <row r="47" spans="1:8">
+    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A47" s="1"/>
       <c r="B47" s="2"/>
       <c r="E47" s="3"/>
@@ -3380,7 +3468,7 @@
       <c r="G47" s="2"/>
       <c r="H47" s="2"/>
     </row>
-    <row r="48" spans="1:8">
+    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A48" s="1"/>
       <c r="B48" s="2"/>
       <c r="E48" s="3"/>
@@ -3388,7 +3476,7 @@
       <c r="G48" s="2"/>
       <c r="H48" s="2"/>
     </row>
-    <row r="49" spans="1:8">
+    <row r="49" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A49" s="1"/>
       <c r="B49" s="2"/>
       <c r="E49" s="3"/>
@@ -3396,7 +3484,7 @@
       <c r="G49" s="2"/>
       <c r="H49" s="2"/>
     </row>
-    <row r="50" spans="1:8">
+    <row r="50" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A50" s="1"/>
       <c r="B50" s="2"/>
       <c r="E50" s="3"/>
@@ -3404,7 +3492,7 @@
       <c r="G50" s="2"/>
       <c r="H50" s="2"/>
     </row>
-    <row r="51" spans="1:8">
+    <row r="51" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A51" s="1"/>
       <c r="B51" s="2"/>
       <c r="E51" s="3"/>
@@ -3412,7 +3500,7 @@
       <c r="G51" s="2"/>
       <c r="H51" s="2"/>
     </row>
-    <row r="52" spans="1:8">
+    <row r="52" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A52" s="1"/>
       <c r="B52" s="2"/>
       <c r="E52" s="3"/>
@@ -3420,7 +3508,7 @@
       <c r="G52" s="2"/>
       <c r="H52" s="2"/>
     </row>
-    <row r="53" spans="1:8">
+    <row r="53" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A53" s="1"/>
       <c r="B53" s="2"/>
       <c r="E53" s="3"/>
@@ -3428,7 +3516,7 @@
       <c r="G53" s="2"/>
       <c r="H53" s="2"/>
     </row>
-    <row r="54" spans="1:8">
+    <row r="54" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A54" s="1"/>
       <c r="B54" s="2"/>
       <c r="E54" s="3"/>
@@ -3436,7 +3524,7 @@
       <c r="G54" s="2"/>
       <c r="H54" s="2"/>
     </row>
-    <row r="55" spans="1:8">
+    <row r="55" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A55" s="1"/>
       <c r="B55" s="2"/>
       <c r="E55" s="3"/>
@@ -3444,7 +3532,7 @@
       <c r="G55" s="2"/>
       <c r="H55" s="2"/>
     </row>
-    <row r="56" spans="1:8">
+    <row r="56" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A56" s="1"/>
       <c r="B56" s="2"/>
       <c r="E56" s="3"/>
@@ -3452,7 +3540,7 @@
       <c r="G56" s="2"/>
       <c r="H56" s="2"/>
     </row>
-    <row r="57" spans="1:8">
+    <row r="57" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A57" s="1"/>
       <c r="B57" s="2"/>
       <c r="E57" s="3"/>
@@ -3460,7 +3548,7 @@
       <c r="G57" s="2"/>
       <c r="H57" s="2"/>
     </row>
-    <row r="58" spans="1:8">
+    <row r="58" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A58" s="1"/>
       <c r="B58" s="2"/>
       <c r="E58" s="3"/>
@@ -3468,7 +3556,7 @@
       <c r="G58" s="2"/>
       <c r="H58" s="2"/>
     </row>
-    <row r="59" spans="1:8">
+    <row r="59" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A59" s="1"/>
       <c r="B59" s="2"/>
       <c r="E59" s="3"/>
@@ -3476,7 +3564,7 @@
       <c r="G59" s="2"/>
       <c r="H59" s="2"/>
     </row>
-    <row r="60" spans="1:8">
+    <row r="60" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A60" s="1"/>
       <c r="B60" s="2"/>
       <c r="E60" s="3"/>
@@ -3484,7 +3572,7 @@
       <c r="G60" s="2"/>
       <c r="H60" s="2"/>
     </row>
-    <row r="61" spans="1:8">
+    <row r="61" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A61" s="1"/>
       <c r="B61" s="2"/>
       <c r="E61" s="3"/>
@@ -3492,7 +3580,7 @@
       <c r="G61" s="2"/>
       <c r="H61" s="2"/>
     </row>
-    <row r="62" spans="1:8">
+    <row r="62" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A62" s="1"/>
       <c r="B62" s="2"/>
       <c r="E62" s="3"/>
@@ -3500,7 +3588,7 @@
       <c r="G62" s="2"/>
       <c r="H62" s="2"/>
     </row>
-    <row r="63" spans="1:8">
+    <row r="63" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A63" s="1"/>
       <c r="B63" s="2"/>
       <c r="E63" s="3"/>
@@ -3508,7 +3596,7 @@
       <c r="G63" s="2"/>
       <c r="H63" s="2"/>
     </row>
-    <row r="64" spans="1:8">
+    <row r="64" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A64" s="1"/>
       <c r="B64" s="2"/>
       <c r="E64" s="3"/>
@@ -3516,7 +3604,7 @@
       <c r="G64" s="2"/>
       <c r="H64" s="2"/>
     </row>
-    <row r="65" spans="1:8">
+    <row r="65" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A65" s="1"/>
       <c r="B65" s="2"/>
       <c r="E65" s="3"/>
@@ -3524,7 +3612,7 @@
       <c r="G65" s="2"/>
       <c r="H65" s="2"/>
     </row>
-    <row r="66" spans="1:8">
+    <row r="66" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A66" s="1"/>
       <c r="B66" s="2"/>
       <c r="E66" s="3"/>
@@ -3532,7 +3620,7 @@
       <c r="G66" s="2"/>
       <c r="H66" s="2"/>
     </row>
-    <row r="67" spans="1:8">
+    <row r="67" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A67" s="1"/>
       <c r="B67" s="2"/>
       <c r="E67" s="3"/>
@@ -3540,7 +3628,7 @@
       <c r="G67" s="2"/>
       <c r="H67" s="2"/>
     </row>
-    <row r="68" spans="1:8">
+    <row r="68" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A68" s="1"/>
       <c r="B68" s="2"/>
       <c r="E68" s="3"/>
@@ -3548,7 +3636,7 @@
       <c r="G68" s="2"/>
       <c r="H68" s="2"/>
     </row>
-    <row r="69" spans="1:8">
+    <row r="69" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A69" s="1"/>
       <c r="B69" s="2"/>
       <c r="E69" s="3"/>
@@ -3556,7 +3644,7 @@
       <c r="G69" s="2"/>
       <c r="H69" s="2"/>
     </row>
-    <row r="70" spans="1:8">
+    <row r="70" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A70" s="1"/>
       <c r="B70" s="2"/>
       <c r="E70" s="3"/>
@@ -3564,7 +3652,7 @@
       <c r="G70" s="2"/>
       <c r="H70" s="2"/>
     </row>
-    <row r="71" spans="1:8">
+    <row r="71" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A71" s="1"/>
       <c r="B71" s="2"/>
       <c r="E71" s="3"/>
@@ -3572,7 +3660,7 @@
       <c r="G71" s="2"/>
       <c r="H71" s="2"/>
     </row>
-    <row r="72" spans="1:8">
+    <row r="72" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A72" s="1"/>
       <c r="B72" s="2"/>
       <c r="E72" s="3"/>
@@ -3580,7 +3668,7 @@
       <c r="G72" s="2"/>
       <c r="H72" s="2"/>
     </row>
-    <row r="73" spans="1:8">
+    <row r="73" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A73" s="1"/>
       <c r="B73" s="2"/>
       <c r="E73" s="3"/>
@@ -3588,7 +3676,7 @@
       <c r="G73" s="2"/>
       <c r="H73" s="2"/>
     </row>
-    <row r="74" spans="1:8">
+    <row r="74" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A74" s="1"/>
       <c r="B74" s="2"/>
       <c r="E74" s="3"/>
@@ -3596,7 +3684,7 @@
       <c r="G74" s="2"/>
       <c r="H74" s="2"/>
     </row>
-    <row r="75" spans="1:8">
+    <row r="75" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A75" s="1"/>
       <c r="B75" s="2"/>
       <c r="E75" s="3"/>
@@ -3604,7 +3692,7 @@
       <c r="G75" s="2"/>
       <c r="H75" s="2"/>
     </row>
-    <row r="76" spans="1:8">
+    <row r="76" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A76" s="1"/>
       <c r="B76" s="2"/>
       <c r="E76" s="3"/>
@@ -3612,7 +3700,7 @@
       <c r="G76" s="2"/>
       <c r="H76" s="2"/>
     </row>
-    <row r="77" spans="1:8">
+    <row r="77" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A77" s="1"/>
       <c r="B77" s="2"/>
       <c r="E77" s="3"/>
@@ -3620,7 +3708,7 @@
       <c r="G77" s="2"/>
       <c r="H77" s="2"/>
     </row>
-    <row r="78" spans="1:8">
+    <row r="78" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A78" s="1"/>
       <c r="B78" s="2"/>
       <c r="E78" s="3"/>
@@ -3628,7 +3716,7 @@
       <c r="G78" s="2"/>
       <c r="H78" s="2"/>
     </row>
-    <row r="79" spans="1:8">
+    <row r="79" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A79" s="1"/>
       <c r="B79" s="2"/>
       <c r="E79" s="3"/>
@@ -3636,7 +3724,7 @@
       <c r="G79" s="2"/>
       <c r="H79" s="2"/>
     </row>
-    <row r="80" spans="1:8">
+    <row r="80" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A80" s="1"/>
       <c r="B80" s="2"/>
       <c r="E80" s="3"/>
@@ -3644,7 +3732,7 @@
       <c r="G80" s="2"/>
       <c r="H80" s="2"/>
     </row>
-    <row r="81" spans="1:8">
+    <row r="81" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A81" s="1"/>
       <c r="B81" s="2"/>
       <c r="E81" s="3"/>
@@ -3652,7 +3740,7 @@
       <c r="G81" s="2"/>
       <c r="H81" s="2"/>
     </row>
-    <row r="82" spans="1:8">
+    <row r="82" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A82" s="1"/>
       <c r="B82" s="2"/>
       <c r="E82" s="3"/>
@@ -3660,7 +3748,7 @@
       <c r="G82" s="2"/>
       <c r="H82" s="2"/>
     </row>
-    <row r="83" spans="1:8">
+    <row r="83" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A83" s="1"/>
       <c r="B83" s="2"/>
       <c r="E83" s="3"/>
@@ -3668,7 +3756,7 @@
       <c r="G83" s="2"/>
       <c r="H83" s="2"/>
     </row>
-    <row r="84" spans="1:8">
+    <row r="84" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A84" s="1"/>
       <c r="B84" s="2"/>
       <c r="E84" s="3"/>
@@ -3676,7 +3764,7 @@
       <c r="G84" s="2"/>
       <c r="H84" s="2"/>
     </row>
-    <row r="85" spans="1:8">
+    <row r="85" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A85" s="1"/>
       <c r="B85" s="2"/>
       <c r="E85" s="3"/>
@@ -3684,7 +3772,7 @@
       <c r="G85" s="2"/>
       <c r="H85" s="2"/>
     </row>
-    <row r="86" spans="1:8">
+    <row r="86" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A86" s="1"/>
       <c r="B86" s="2"/>
       <c r="E86" s="3"/>
@@ -3692,7 +3780,7 @@
       <c r="G86" s="2"/>
       <c r="H86" s="2"/>
     </row>
-    <row r="87" spans="1:8">
+    <row r="87" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A87" s="1"/>
       <c r="B87" s="2"/>
       <c r="E87" s="3"/>
@@ -3700,7 +3788,7 @@
       <c r="G87" s="2"/>
       <c r="H87" s="2"/>
     </row>
-    <row r="88" spans="1:8">
+    <row r="88" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A88" s="1"/>
       <c r="B88" s="2"/>
       <c r="E88" s="3"/>
@@ -3708,7 +3796,7 @@
       <c r="G88" s="2"/>
       <c r="H88" s="2"/>
     </row>
-    <row r="89" spans="1:8">
+    <row r="89" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A89" s="1"/>
       <c r="B89" s="2"/>
       <c r="E89" s="3"/>
@@ -3716,7 +3804,7 @@
       <c r="G89" s="2"/>
       <c r="H89" s="2"/>
     </row>
-    <row r="90" spans="1:8">
+    <row r="90" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A90" s="1"/>
       <c r="B90" s="2"/>
       <c r="E90" s="3"/>
@@ -3724,7 +3812,7 @@
       <c r="G90" s="2"/>
       <c r="H90" s="2"/>
     </row>
-    <row r="91" spans="1:8">
+    <row r="91" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A91" s="1"/>
       <c r="B91" s="2"/>
       <c r="E91" s="3"/>
@@ -3732,7 +3820,7 @@
       <c r="G91" s="2"/>
       <c r="H91" s="2"/>
     </row>
-    <row r="92" spans="1:8">
+    <row r="92" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A92" s="1"/>
       <c r="B92" s="2"/>
       <c r="E92" s="3"/>
@@ -3740,7 +3828,7 @@
       <c r="G92" s="2"/>
       <c r="H92" s="2"/>
     </row>
-    <row r="93" spans="1:8">
+    <row r="93" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A93" s="1"/>
       <c r="B93" s="2"/>
       <c r="E93" s="3"/>
@@ -3748,7 +3836,7 @@
       <c r="G93" s="2"/>
       <c r="H93" s="2"/>
     </row>
-    <row r="94" spans="1:8">
+    <row r="94" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A94" s="1"/>
       <c r="B94" s="2"/>
       <c r="E94" s="3"/>
@@ -3756,7 +3844,7 @@
       <c r="G94" s="2"/>
       <c r="H94" s="2"/>
     </row>
-    <row r="95" spans="1:8">
+    <row r="95" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A95" s="1"/>
       <c r="B95" s="2"/>
       <c r="E95" s="3"/>
@@ -3764,7 +3852,7 @@
       <c r="G95" s="2"/>
       <c r="H95" s="2"/>
     </row>
-    <row r="96" spans="1:8">
+    <row r="96" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A96" s="1"/>
       <c r="B96" s="2"/>
       <c r="E96" s="3"/>
@@ -3772,7 +3860,7 @@
       <c r="G96" s="2"/>
       <c r="H96" s="2"/>
     </row>
-    <row r="97" spans="1:8">
+    <row r="97" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A97" s="1"/>
       <c r="B97" s="2"/>
       <c r="E97" s="3"/>
@@ -3780,7 +3868,7 @@
       <c r="G97" s="2"/>
       <c r="H97" s="2"/>
     </row>
-    <row r="98" spans="1:8">
+    <row r="98" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A98" s="1"/>
       <c r="B98" s="2"/>
       <c r="E98" s="3"/>
@@ -3788,7 +3876,7 @@
       <c r="G98" s="2"/>
       <c r="H98" s="2"/>
     </row>
-    <row r="99" spans="1:8">
+    <row r="99" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A99" s="1"/>
       <c r="B99" s="2"/>
       <c r="E99" s="3"/>
@@ -3796,7 +3884,7 @@
       <c r="G99" s="2"/>
       <c r="H99" s="2"/>
     </row>
-    <row r="100" spans="1:8">
+    <row r="100" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A100" s="1"/>
       <c r="B100" s="2"/>
       <c r="E100" s="3"/>
@@ -3839,21 +3927,21 @@
       <selection activeCell="P21" sqref="P21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.1640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.83203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.83203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="19.4140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.58203125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.58203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.5703125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="9" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="17.83203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="17.85546875" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="17" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="19.1640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="19.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="15.5">
+    <row r="1" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="7" t="s">
         <v>8</v>
       </c>
@@ -3885,7 +3973,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:10">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="2"/>
       <c r="B2" s="8"/>
       <c r="D2" s="2"/>
@@ -3893,7 +3981,7 @@
       <c r="I2" s="8"/>
       <c r="J2" s="2"/>
     </row>
-    <row r="3" spans="1:10">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="2"/>
       <c r="B3" s="8"/>
       <c r="D3" s="2"/>
@@ -3901,7 +3989,7 @@
       <c r="I3" s="8"/>
       <c r="J3" s="2"/>
     </row>
-    <row r="4" spans="1:10">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="2"/>
       <c r="B4" s="8"/>
       <c r="D4" s="2"/>
@@ -3909,7 +3997,7 @@
       <c r="I4" s="8"/>
       <c r="J4" s="2"/>
     </row>
-    <row r="5" spans="1:10">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" s="2"/>
       <c r="B5" s="8"/>
       <c r="D5" s="2"/>
@@ -3917,7 +4005,7 @@
       <c r="I5" s="8"/>
       <c r="J5" s="2"/>
     </row>
-    <row r="6" spans="1:10">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" s="2"/>
       <c r="B6" s="8"/>
       <c r="D6" s="2"/>
@@ -3925,7 +4013,7 @@
       <c r="I6" s="8"/>
       <c r="J6" s="2"/>
     </row>
-    <row r="7" spans="1:10">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" s="2"/>
       <c r="B7" s="8"/>
       <c r="D7" s="2"/>
@@ -3933,7 +4021,7 @@
       <c r="I7" s="8"/>
       <c r="J7" s="2"/>
     </row>
-    <row r="8" spans="1:10">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" s="2"/>
       <c r="B8" s="8"/>
       <c r="D8" s="2"/>
@@ -3941,7 +4029,7 @@
       <c r="I8" s="8"/>
       <c r="J8" s="2"/>
     </row>
-    <row r="9" spans="1:10">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" s="2"/>
       <c r="B9" s="8"/>
       <c r="D9" s="2"/>
@@ -3949,7 +4037,7 @@
       <c r="I9" s="8"/>
       <c r="J9" s="2"/>
     </row>
-    <row r="10" spans="1:10">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" s="2"/>
       <c r="B10" s="8"/>
       <c r="D10" s="2"/>
@@ -3957,7 +4045,7 @@
       <c r="I10" s="8"/>
       <c r="J10" s="2"/>
     </row>
-    <row r="11" spans="1:10">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" s="2"/>
       <c r="B11" s="8"/>
       <c r="D11" s="2"/>
@@ -3965,7 +4053,7 @@
       <c r="I11" s="8"/>
       <c r="J11" s="2"/>
     </row>
-    <row r="12" spans="1:10">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" s="2"/>
       <c r="B12" s="8"/>
       <c r="D12" s="2"/>
@@ -3973,7 +4061,7 @@
       <c r="I12" s="8"/>
       <c r="J12" s="2"/>
     </row>
-    <row r="13" spans="1:10">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" s="2"/>
       <c r="B13" s="8"/>
       <c r="D13" s="2"/>
@@ -3981,7 +4069,7 @@
       <c r="I13" s="8"/>
       <c r="J13" s="2"/>
     </row>
-    <row r="14" spans="1:10">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" s="2"/>
       <c r="B14" s="8"/>
       <c r="D14" s="2"/>
@@ -3989,7 +4077,7 @@
       <c r="I14" s="8"/>
       <c r="J14" s="2"/>
     </row>
-    <row r="15" spans="1:10">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" s="2"/>
       <c r="B15" s="8"/>
       <c r="D15" s="2"/>
@@ -3997,7 +4085,7 @@
       <c r="I15" s="8"/>
       <c r="J15" s="2"/>
     </row>
-    <row r="16" spans="1:10">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" s="2"/>
       <c r="B16" s="8"/>
       <c r="D16" s="2"/>
@@ -4005,7 +4093,7 @@
       <c r="I16" s="8"/>
       <c r="J16" s="2"/>
     </row>
-    <row r="17" spans="1:10">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17" s="2"/>
       <c r="B17" s="8"/>
       <c r="D17" s="2"/>
@@ -4013,7 +4101,7 @@
       <c r="I17" s="8"/>
       <c r="J17" s="2"/>
     </row>
-    <row r="18" spans="1:10">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18" s="2"/>
       <c r="B18" s="8"/>
       <c r="D18" s="2"/>
@@ -4021,7 +4109,7 @@
       <c r="I18" s="8"/>
       <c r="J18" s="2"/>
     </row>
-    <row r="19" spans="1:10">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A19" s="2"/>
       <c r="B19" s="8"/>
       <c r="D19" s="2"/>
@@ -4029,7 +4117,7 @@
       <c r="I19" s="8"/>
       <c r="J19" s="2"/>
     </row>
-    <row r="20" spans="1:10">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A20" s="2"/>
       <c r="B20" s="8"/>
       <c r="D20" s="2"/>
@@ -4037,7 +4125,7 @@
       <c r="I20" s="8"/>
       <c r="J20" s="2"/>
     </row>
-    <row r="21" spans="1:10">
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A21" s="2"/>
       <c r="B21" s="8"/>
       <c r="D21" s="2"/>
@@ -4045,7 +4133,7 @@
       <c r="I21" s="8"/>
       <c r="J21" s="2"/>
     </row>
-    <row r="22" spans="1:10">
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A22" s="2"/>
       <c r="B22" s="8"/>
       <c r="D22" s="2"/>
@@ -4053,7 +4141,7 @@
       <c r="I22" s="8"/>
       <c r="J22" s="2"/>
     </row>
-    <row r="23" spans="1:10">
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A23" s="2"/>
       <c r="B23" s="8"/>
       <c r="D23" s="2"/>
@@ -4061,7 +4149,7 @@
       <c r="I23" s="8"/>
       <c r="J23" s="2"/>
     </row>
-    <row r="24" spans="1:10">
+    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A24" s="2"/>
       <c r="B24" s="8"/>
       <c r="D24" s="2"/>
@@ -4069,7 +4157,7 @@
       <c r="I24" s="8"/>
       <c r="J24" s="2"/>
     </row>
-    <row r="25" spans="1:10">
+    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A25" s="2"/>
       <c r="B25" s="8"/>
       <c r="D25" s="2"/>
@@ -4077,7 +4165,7 @@
       <c r="I25" s="8"/>
       <c r="J25" s="2"/>
     </row>
-    <row r="26" spans="1:10">
+    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A26" s="2"/>
       <c r="B26" s="8"/>
       <c r="D26" s="2"/>
@@ -4085,7 +4173,7 @@
       <c r="I26" s="8"/>
       <c r="J26" s="2"/>
     </row>
-    <row r="27" spans="1:10">
+    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A27" s="2"/>
       <c r="B27" s="8"/>
       <c r="D27" s="2"/>
@@ -4093,7 +4181,7 @@
       <c r="I27" s="8"/>
       <c r="J27" s="2"/>
     </row>
-    <row r="28" spans="1:10">
+    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A28" s="2"/>
       <c r="B28" s="8"/>
       <c r="D28" s="2"/>
@@ -4101,7 +4189,7 @@
       <c r="I28" s="8"/>
       <c r="J28" s="2"/>
     </row>
-    <row r="29" spans="1:10">
+    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A29" s="2"/>
       <c r="B29" s="8"/>
       <c r="D29" s="2"/>
@@ -4109,7 +4197,7 @@
       <c r="I29" s="8"/>
       <c r="J29" s="2"/>
     </row>
-    <row r="30" spans="1:10">
+    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A30" s="2"/>
       <c r="B30" s="8"/>
       <c r="D30" s="2"/>
@@ -4117,7 +4205,7 @@
       <c r="I30" s="8"/>
       <c r="J30" s="2"/>
     </row>
-    <row r="31" spans="1:10">
+    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A31" s="2"/>
       <c r="B31" s="8"/>
       <c r="D31" s="2"/>
@@ -4125,7 +4213,7 @@
       <c r="I31" s="8"/>
       <c r="J31" s="2"/>
     </row>
-    <row r="32" spans="1:10">
+    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A32" s="2"/>
       <c r="B32" s="8"/>
       <c r="D32" s="2"/>
@@ -4133,7 +4221,7 @@
       <c r="I32" s="8"/>
       <c r="J32" s="2"/>
     </row>
-    <row r="33" spans="1:10">
+    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A33" s="2"/>
       <c r="B33" s="8"/>
       <c r="D33" s="2"/>
@@ -4141,7 +4229,7 @@
       <c r="I33" s="8"/>
       <c r="J33" s="2"/>
     </row>
-    <row r="34" spans="1:10">
+    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A34" s="2"/>
       <c r="B34" s="8"/>
       <c r="D34" s="2"/>
@@ -4149,7 +4237,7 @@
       <c r="I34" s="8"/>
       <c r="J34" s="2"/>
     </row>
-    <row r="35" spans="1:10">
+    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A35" s="2"/>
       <c r="B35" s="8"/>
       <c r="D35" s="2"/>
@@ -4157,7 +4245,7 @@
       <c r="I35" s="8"/>
       <c r="J35" s="2"/>
     </row>
-    <row r="36" spans="1:10">
+    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A36" s="2"/>
       <c r="B36" s="8"/>
       <c r="D36" s="2"/>
@@ -4165,7 +4253,7 @@
       <c r="I36" s="8"/>
       <c r="J36" s="2"/>
     </row>
-    <row r="37" spans="1:10">
+    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A37" s="2"/>
       <c r="B37" s="8"/>
       <c r="D37" s="2"/>
@@ -4173,7 +4261,7 @@
       <c r="I37" s="8"/>
       <c r="J37" s="2"/>
     </row>
-    <row r="38" spans="1:10">
+    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A38" s="2"/>
       <c r="B38" s="8"/>
       <c r="D38" s="2"/>
@@ -4181,7 +4269,7 @@
       <c r="I38" s="8"/>
       <c r="J38" s="2"/>
     </row>
-    <row r="39" spans="1:10">
+    <row r="39" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A39" s="2"/>
       <c r="B39" s="8"/>
       <c r="D39" s="2"/>
@@ -4189,7 +4277,7 @@
       <c r="I39" s="8"/>
       <c r="J39" s="2"/>
     </row>
-    <row r="40" spans="1:10">
+    <row r="40" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A40" s="2"/>
       <c r="B40" s="8"/>
       <c r="D40" s="2"/>
@@ -4197,7 +4285,7 @@
       <c r="I40" s="8"/>
       <c r="J40" s="2"/>
     </row>
-    <row r="41" spans="1:10">
+    <row r="41" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A41" s="2"/>
       <c r="B41" s="8"/>
       <c r="D41" s="2"/>
@@ -4205,7 +4293,7 @@
       <c r="I41" s="8"/>
       <c r="J41" s="2"/>
     </row>
-    <row r="42" spans="1:10">
+    <row r="42" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A42" s="2"/>
       <c r="B42" s="8"/>
       <c r="D42" s="2"/>
@@ -4213,7 +4301,7 @@
       <c r="I42" s="8"/>
       <c r="J42" s="2"/>
     </row>
-    <row r="43" spans="1:10">
+    <row r="43" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A43" s="2"/>
       <c r="B43" s="8"/>
       <c r="D43" s="2"/>
@@ -4221,7 +4309,7 @@
       <c r="I43" s="8"/>
       <c r="J43" s="2"/>
     </row>
-    <row r="44" spans="1:10">
+    <row r="44" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A44" s="2"/>
       <c r="B44" s="8"/>
       <c r="D44" s="2"/>
@@ -4229,7 +4317,7 @@
       <c r="I44" s="8"/>
       <c r="J44" s="2"/>
     </row>
-    <row r="45" spans="1:10">
+    <row r="45" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A45" s="2"/>
       <c r="B45" s="8"/>
       <c r="D45" s="2"/>
@@ -4237,7 +4325,7 @@
       <c r="I45" s="8"/>
       <c r="J45" s="2"/>
     </row>
-    <row r="46" spans="1:10">
+    <row r="46" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A46" s="2"/>
       <c r="B46" s="8"/>
       <c r="D46" s="2"/>
@@ -4245,7 +4333,7 @@
       <c r="I46" s="8"/>
       <c r="J46" s="2"/>
     </row>
-    <row r="47" spans="1:10">
+    <row r="47" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A47" s="2"/>
       <c r="B47" s="8"/>
       <c r="D47" s="2"/>
@@ -4253,7 +4341,7 @@
       <c r="I47" s="8"/>
       <c r="J47" s="2"/>
     </row>
-    <row r="48" spans="1:10">
+    <row r="48" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A48" s="2"/>
       <c r="B48" s="8"/>
       <c r="D48" s="2"/>
@@ -4261,7 +4349,7 @@
       <c r="I48" s="8"/>
       <c r="J48" s="2"/>
     </row>
-    <row r="49" spans="1:10">
+    <row r="49" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A49" s="2"/>
       <c r="B49" s="8"/>
       <c r="D49" s="2"/>
@@ -4269,7 +4357,7 @@
       <c r="I49" s="8"/>
       <c r="J49" s="2"/>
     </row>
-    <row r="50" spans="1:10">
+    <row r="50" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A50" s="2"/>
       <c r="B50" s="8"/>
       <c r="D50" s="2"/>
@@ -4277,7 +4365,7 @@
       <c r="I50" s="8"/>
       <c r="J50" s="2"/>
     </row>
-    <row r="51" spans="1:10">
+    <row r="51" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A51" s="2"/>
       <c r="B51" s="8"/>
       <c r="D51" s="2"/>
@@ -4285,7 +4373,7 @@
       <c r="I51" s="8"/>
       <c r="J51" s="2"/>
     </row>
-    <row r="52" spans="1:10">
+    <row r="52" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A52" s="2"/>
       <c r="B52" s="8"/>
       <c r="D52" s="2"/>
@@ -4293,7 +4381,7 @@
       <c r="I52" s="8"/>
       <c r="J52" s="2"/>
     </row>
-    <row r="53" spans="1:10">
+    <row r="53" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A53" s="2"/>
       <c r="B53" s="8"/>
       <c r="D53" s="2"/>
@@ -4301,7 +4389,7 @@
       <c r="I53" s="8"/>
       <c r="J53" s="2"/>
     </row>
-    <row r="54" spans="1:10">
+    <row r="54" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A54" s="2"/>
       <c r="B54" s="8"/>
       <c r="D54" s="2"/>
@@ -4309,7 +4397,7 @@
       <c r="I54" s="8"/>
       <c r="J54" s="2"/>
     </row>
-    <row r="55" spans="1:10">
+    <row r="55" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A55" s="2"/>
       <c r="B55" s="8"/>
       <c r="D55" s="2"/>
@@ -4317,7 +4405,7 @@
       <c r="I55" s="8"/>
       <c r="J55" s="2"/>
     </row>
-    <row r="56" spans="1:10">
+    <row r="56" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A56" s="2"/>
       <c r="B56" s="8"/>
       <c r="D56" s="2"/>
@@ -4325,7 +4413,7 @@
       <c r="I56" s="8"/>
       <c r="J56" s="2"/>
     </row>
-    <row r="57" spans="1:10">
+    <row r="57" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A57" s="2"/>
       <c r="B57" s="8"/>
       <c r="D57" s="2"/>
@@ -4333,7 +4421,7 @@
       <c r="I57" s="8"/>
       <c r="J57" s="2"/>
     </row>
-    <row r="58" spans="1:10">
+    <row r="58" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A58" s="2"/>
       <c r="B58" s="8"/>
       <c r="D58" s="2"/>
@@ -4341,7 +4429,7 @@
       <c r="I58" s="8"/>
       <c r="J58" s="2"/>
     </row>
-    <row r="59" spans="1:10">
+    <row r="59" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A59" s="2"/>
       <c r="B59" s="8"/>
       <c r="D59" s="2"/>
@@ -4349,7 +4437,7 @@
       <c r="I59" s="8"/>
       <c r="J59" s="2"/>
     </row>
-    <row r="60" spans="1:10">
+    <row r="60" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A60" s="2"/>
       <c r="B60" s="8"/>
       <c r="D60" s="2"/>
@@ -4357,7 +4445,7 @@
       <c r="I60" s="8"/>
       <c r="J60" s="2"/>
     </row>
-    <row r="61" spans="1:10">
+    <row r="61" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A61" s="2"/>
       <c r="B61" s="8"/>
       <c r="D61" s="2"/>
@@ -4365,7 +4453,7 @@
       <c r="I61" s="8"/>
       <c r="J61" s="2"/>
     </row>
-    <row r="62" spans="1:10">
+    <row r="62" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A62" s="2"/>
       <c r="B62" s="8"/>
       <c r="D62" s="2"/>
@@ -4373,7 +4461,7 @@
       <c r="I62" s="8"/>
       <c r="J62" s="2"/>
     </row>
-    <row r="63" spans="1:10">
+    <row r="63" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A63" s="2"/>
       <c r="B63" s="8"/>
       <c r="D63" s="2"/>
@@ -4381,7 +4469,7 @@
       <c r="I63" s="8"/>
       <c r="J63" s="2"/>
     </row>
-    <row r="64" spans="1:10">
+    <row r="64" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A64" s="2"/>
       <c r="B64" s="8"/>
       <c r="D64" s="2"/>
@@ -4389,7 +4477,7 @@
       <c r="I64" s="8"/>
       <c r="J64" s="2"/>
     </row>
-    <row r="65" spans="1:10">
+    <row r="65" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A65" s="2"/>
       <c r="B65" s="8"/>
       <c r="D65" s="2"/>
@@ -4397,7 +4485,7 @@
       <c r="I65" s="8"/>
       <c r="J65" s="2"/>
     </row>
-    <row r="66" spans="1:10">
+    <row r="66" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A66" s="2"/>
       <c r="B66" s="8"/>
       <c r="D66" s="2"/>
@@ -4405,7 +4493,7 @@
       <c r="I66" s="8"/>
       <c r="J66" s="2"/>
     </row>
-    <row r="67" spans="1:10">
+    <row r="67" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A67" s="2"/>
       <c r="B67" s="8"/>
       <c r="D67" s="2"/>
@@ -4413,7 +4501,7 @@
       <c r="I67" s="8"/>
       <c r="J67" s="2"/>
     </row>
-    <row r="68" spans="1:10">
+    <row r="68" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A68" s="2"/>
       <c r="B68" s="8"/>
       <c r="D68" s="2"/>
@@ -4421,7 +4509,7 @@
       <c r="I68" s="8"/>
       <c r="J68" s="2"/>
     </row>
-    <row r="69" spans="1:10">
+    <row r="69" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A69" s="2"/>
       <c r="B69" s="8"/>
       <c r="D69" s="2"/>
@@ -4429,7 +4517,7 @@
       <c r="I69" s="8"/>
       <c r="J69" s="2"/>
     </row>
-    <row r="70" spans="1:10">
+    <row r="70" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A70" s="2"/>
       <c r="B70" s="8"/>
       <c r="D70" s="2"/>
@@ -4437,7 +4525,7 @@
       <c r="I70" s="8"/>
       <c r="J70" s="2"/>
     </row>
-    <row r="71" spans="1:10">
+    <row r="71" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A71" s="2"/>
       <c r="B71" s="8"/>
       <c r="D71" s="2"/>
@@ -4445,7 +4533,7 @@
       <c r="I71" s="8"/>
       <c r="J71" s="2"/>
     </row>
-    <row r="72" spans="1:10">
+    <row r="72" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A72" s="2"/>
       <c r="B72" s="8"/>
       <c r="D72" s="2"/>
@@ -4453,7 +4541,7 @@
       <c r="I72" s="8"/>
       <c r="J72" s="2"/>
     </row>
-    <row r="73" spans="1:10">
+    <row r="73" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A73" s="2"/>
       <c r="B73" s="8"/>
       <c r="D73" s="2"/>
@@ -4461,7 +4549,7 @@
       <c r="I73" s="8"/>
       <c r="J73" s="2"/>
     </row>
-    <row r="74" spans="1:10">
+    <row r="74" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A74" s="2"/>
       <c r="B74" s="8"/>
       <c r="D74" s="2"/>
@@ -4469,7 +4557,7 @@
       <c r="I74" s="8"/>
       <c r="J74" s="2"/>
     </row>
-    <row r="75" spans="1:10">
+    <row r="75" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A75" s="2"/>
       <c r="B75" s="8"/>
       <c r="D75" s="2"/>
@@ -4477,7 +4565,7 @@
       <c r="I75" s="8"/>
       <c r="J75" s="2"/>
     </row>
-    <row r="76" spans="1:10">
+    <row r="76" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A76" s="2"/>
       <c r="B76" s="8"/>
       <c r="D76" s="2"/>
@@ -4485,7 +4573,7 @@
       <c r="I76" s="8"/>
       <c r="J76" s="2"/>
     </row>
-    <row r="77" spans="1:10">
+    <row r="77" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A77" s="2"/>
       <c r="B77" s="8"/>
       <c r="D77" s="2"/>
@@ -4493,7 +4581,7 @@
       <c r="I77" s="8"/>
       <c r="J77" s="2"/>
     </row>
-    <row r="78" spans="1:10">
+    <row r="78" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A78" s="2"/>
       <c r="B78" s="8"/>
       <c r="D78" s="2"/>
@@ -4501,7 +4589,7 @@
       <c r="I78" s="8"/>
       <c r="J78" s="2"/>
     </row>
-    <row r="79" spans="1:10">
+    <row r="79" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A79" s="2"/>
       <c r="B79" s="8"/>
       <c r="D79" s="2"/>
@@ -4509,7 +4597,7 @@
       <c r="I79" s="8"/>
       <c r="J79" s="2"/>
     </row>
-    <row r="80" spans="1:10">
+    <row r="80" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A80" s="2"/>
       <c r="B80" s="8"/>
       <c r="D80" s="2"/>
@@ -4517,7 +4605,7 @@
       <c r="I80" s="8"/>
       <c r="J80" s="2"/>
     </row>
-    <row r="81" spans="1:10">
+    <row r="81" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A81" s="2"/>
       <c r="B81" s="8"/>
       <c r="D81" s="2"/>
@@ -4525,7 +4613,7 @@
       <c r="I81" s="8"/>
       <c r="J81" s="2"/>
     </row>
-    <row r="82" spans="1:10">
+    <row r="82" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A82" s="2"/>
       <c r="B82" s="8"/>
       <c r="D82" s="2"/>
@@ -4533,7 +4621,7 @@
       <c r="I82" s="8"/>
       <c r="J82" s="2"/>
     </row>
-    <row r="83" spans="1:10">
+    <row r="83" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A83" s="2"/>
       <c r="B83" s="8"/>
       <c r="D83" s="2"/>
@@ -4541,7 +4629,7 @@
       <c r="I83" s="8"/>
       <c r="J83" s="2"/>
     </row>
-    <row r="84" spans="1:10">
+    <row r="84" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A84" s="2"/>
       <c r="B84" s="8"/>
       <c r="D84" s="2"/>
@@ -4549,7 +4637,7 @@
       <c r="I84" s="8"/>
       <c r="J84" s="2"/>
     </row>
-    <row r="85" spans="1:10">
+    <row r="85" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A85" s="2"/>
       <c r="B85" s="8"/>
       <c r="D85" s="2"/>
@@ -4557,7 +4645,7 @@
       <c r="I85" s="8"/>
       <c r="J85" s="2"/>
     </row>
-    <row r="86" spans="1:10">
+    <row r="86" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A86" s="2"/>
       <c r="B86" s="8"/>
       <c r="D86" s="2"/>
@@ -4565,7 +4653,7 @@
       <c r="I86" s="8"/>
       <c r="J86" s="2"/>
     </row>
-    <row r="87" spans="1:10">
+    <row r="87" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A87" s="2"/>
       <c r="B87" s="8"/>
       <c r="D87" s="2"/>
@@ -4573,7 +4661,7 @@
       <c r="I87" s="8"/>
       <c r="J87" s="2"/>
     </row>
-    <row r="88" spans="1:10">
+    <row r="88" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A88" s="2"/>
       <c r="B88" s="8"/>
       <c r="D88" s="2"/>
@@ -4581,7 +4669,7 @@
       <c r="I88" s="8"/>
       <c r="J88" s="2"/>
     </row>
-    <row r="89" spans="1:10">
+    <row r="89" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A89" s="2"/>
       <c r="B89" s="8"/>
       <c r="D89" s="2"/>
@@ -4589,7 +4677,7 @@
       <c r="I89" s="8"/>
       <c r="J89" s="2"/>
     </row>
-    <row r="90" spans="1:10">
+    <row r="90" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A90" s="2"/>
       <c r="B90" s="8"/>
       <c r="D90" s="2"/>
@@ -4597,7 +4685,7 @@
       <c r="I90" s="8"/>
       <c r="J90" s="2"/>
     </row>
-    <row r="91" spans="1:10">
+    <row r="91" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A91" s="2"/>
       <c r="B91" s="8"/>
       <c r="D91" s="2"/>
@@ -4605,7 +4693,7 @@
       <c r="I91" s="8"/>
       <c r="J91" s="2"/>
     </row>
-    <row r="92" spans="1:10">
+    <row r="92" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A92" s="2"/>
       <c r="B92" s="8"/>
       <c r="D92" s="2"/>
@@ -4613,7 +4701,7 @@
       <c r="I92" s="8"/>
       <c r="J92" s="2"/>
     </row>
-    <row r="93" spans="1:10">
+    <row r="93" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A93" s="2"/>
       <c r="B93" s="8"/>
       <c r="D93" s="2"/>
@@ -4621,7 +4709,7 @@
       <c r="I93" s="8"/>
       <c r="J93" s="2"/>
     </row>
-    <row r="94" spans="1:10">
+    <row r="94" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A94" s="2"/>
       <c r="B94" s="8"/>
       <c r="D94" s="2"/>
@@ -4629,7 +4717,7 @@
       <c r="I94" s="8"/>
       <c r="J94" s="2"/>
     </row>
-    <row r="95" spans="1:10">
+    <row r="95" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A95" s="2"/>
       <c r="B95" s="8"/>
       <c r="D95" s="2"/>
@@ -4637,7 +4725,7 @@
       <c r="I95" s="8"/>
       <c r="J95" s="2"/>
     </row>
-    <row r="96" spans="1:10">
+    <row r="96" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A96" s="2"/>
       <c r="B96" s="8"/>
       <c r="D96" s="2"/>
@@ -4645,7 +4733,7 @@
       <c r="I96" s="8"/>
       <c r="J96" s="2"/>
     </row>
-    <row r="97" spans="1:10">
+    <row r="97" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A97" s="2"/>
       <c r="B97" s="8"/>
       <c r="D97" s="2"/>
@@ -4653,7 +4741,7 @@
       <c r="I97" s="8"/>
       <c r="J97" s="2"/>
     </row>
-    <row r="98" spans="1:10">
+    <row r="98" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A98" s="2"/>
       <c r="B98" s="8"/>
       <c r="D98" s="2"/>
@@ -4661,7 +4749,7 @@
       <c r="I98" s="8"/>
       <c r="J98" s="2"/>
     </row>
-    <row r="99" spans="1:10">
+    <row r="99" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A99" s="2"/>
       <c r="B99" s="8"/>
       <c r="D99" s="2"/>
@@ -4669,7 +4757,7 @@
       <c r="I99" s="8"/>
       <c r="J99" s="2"/>
     </row>
-    <row r="100" spans="1:10">
+    <row r="100" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A100" s="2"/>
       <c r="B100" s="8"/>
       <c r="D100" s="2"/>

</xml_diff>

<commit_message>
Configured services on port 5004
</commit_message>
<xml_diff>
--- a/PR&IR.xlsx
+++ b/PR&IR.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28623"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\avichal avneel nath\Documents\Semester 7\CS415\A3\CS415_A3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{446B9638-145F-47A9-8E17-E54F5F829A5D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{265B2D53-2233-42DA-BDE7-A3000AC9A528}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{BFA1E21A-08FA-4F02-8C25-33C81C8EE970}"/>
   </bookViews>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="81">
   <si>
     <t>Date</t>
   </si>
@@ -157,6 +157,144 @@
   </si>
   <si>
     <t xml:space="preserve">Stay Healthy Aviiii. Don’t get sick </t>
+  </si>
+  <si>
+    <t>Shivya Kumar</t>
+  </si>
+  <si>
+    <t>Convert UI for login, homepage and student profile</t>
+  </si>
+  <si>
+    <t>In Progress</t>
+  </si>
+  <si>
+    <t>Continue converting UI and setting route</t>
+  </si>
+  <si>
+    <t>I was unable to run the app locally, so I created a folder named run_main_app.py with the required code Once I did that I was able to start the Flask server successfully</t>
+  </si>
+  <si>
+    <t>Added header and footer to the remaining UIs, and converted UI for enrollment page.</t>
+  </si>
+  <si>
+    <t>Solve my routes and fix UI</t>
+  </si>
+  <si>
+    <t>I added my routes in the same file app.py</t>
+  </si>
+  <si>
+    <t>Customizing UI and recovered deleted codes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Continue converting UI </t>
+  </si>
+  <si>
+    <t>shivya Kumar</t>
+  </si>
+  <si>
+    <t>Converted all user interface designs into HTML and set up respective routes.</t>
+  </si>
+  <si>
+    <t>continue implementing remaining UI logic based on feedback and custom validation with exception handling for all of her routes</t>
+  </si>
+  <si>
+    <t>Added custom validation for logout and exception handling for all routes</t>
+  </si>
+  <si>
+    <t>Not feeling well, assignments are due and short tests are approaching.</t>
+  </si>
+  <si>
+    <t>Start with next workpackage once approved and given by Jayshil Singh</t>
+  </si>
+  <si>
+    <t>YPP</t>
+  </si>
+  <si>
+    <t>Converted Dart files to HTML files</t>
+  </si>
+  <si>
+    <t>Updating JS to render all htmls properly</t>
+  </si>
+  <si>
+    <t>N/A</t>
+  </si>
+  <si>
+    <t>Completed JS modification</t>
+  </si>
+  <si>
+    <t>Patch up any errors and add exception handling</t>
+  </si>
+  <si>
+    <t>13/5/2025</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Added Exception Handling </t>
+  </si>
+  <si>
+    <t>Parse XML's to registration Dropdowns</t>
+  </si>
+  <si>
+    <t>Will work on CS403 so hours worked on CS415 might decrease</t>
+  </si>
+  <si>
+    <t>14/5/2025</t>
+  </si>
+  <si>
+    <t>Parsed XML's Properly</t>
+  </si>
+  <si>
+    <t>Waiting PM's Lead</t>
+  </si>
+  <si>
+    <t>Developed an invoice generation feature for a Flask-based enrollment system, starting with the UI in fees.html and linking it to the backend. Initially, used pdfkit to convert an HTML template to a PDF, but encountered wkhtmltopdf setup issues. To simplify, switched to ReportLab, a pure-Python library, and modified the Flask route to generate the PDF programmatically. This involved creating the PDF structure and content directly within the Python code and sending it as a download. Throughout the process, corrected routing in the HTML files to ensure proper navigation within the Flask application.</t>
+  </si>
+  <si>
+    <t>Models for Enrollment N Fees</t>
+  </si>
+  <si>
+    <t>Happy Thurday PM :)</t>
+  </si>
+  <si>
+    <t>16/5/2025</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Implemented the API Key linking </t>
+  </si>
+  <si>
+    <t>Fixing the HTML Pages and the errors that occurred due to restructuring</t>
+  </si>
+  <si>
+    <t>18/5/2025</t>
+  </si>
+  <si>
+    <t>Implementing masterpage in all pages</t>
+  </si>
+  <si>
+    <t>Learning how to work with Docker Database</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Modified invoice </t>
+  </si>
+  <si>
+    <t>Backend commencement</t>
+  </si>
+  <si>
+    <t>configuring enrollment services to designated port</t>
+  </si>
+  <si>
+    <t>Configure on specified port</t>
+  </si>
+  <si>
+    <t>Successfully run the services on port 5004</t>
+  </si>
+  <si>
+    <t>confgure API</t>
+  </si>
+  <si>
+    <t xml:space="preserve">only read docker documentation </t>
+  </si>
+  <si>
+    <t>Port configuration</t>
   </si>
 </sst>
 </file>
@@ -208,7 +346,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -221,6 +359,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="2" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -305,7 +445,7 @@
       <numFmt numFmtId="30" formatCode="@"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="164" formatCode="h"/>
+      <numFmt numFmtId="2" formatCode="0.00"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="14" formatCode="0.00%"/>
@@ -341,10 +481,10 @@
       <numFmt numFmtId="30" formatCode="@"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="164" formatCode="h"/>
+      <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="14" formatCode="0.00%"/>
+      <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="30" formatCode="@"/>
@@ -901,8 +1041,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{37EAA098-74C6-4411-B7E2-26AD2DCBC3F0}">
   <dimension ref="A1:H28"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H7" sqref="H7"/>
+    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1089,24 +1229,107 @@
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="E8"/>
-      <c r="F8"/>
+      <c r="A8" s="1">
+        <v>45792</v>
+      </c>
+      <c r="C8" t="s">
+        <v>64</v>
+      </c>
+      <c r="D8" t="s">
+        <v>17</v>
+      </c>
+      <c r="E8">
+        <v>100</v>
+      </c>
+      <c r="F8">
+        <v>3</v>
+      </c>
+      <c r="G8" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="H8" s="2" t="s">
+        <v>66</v>
+      </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="E9"/>
-      <c r="F9"/>
+      <c r="A9" s="1">
+        <v>45793</v>
+      </c>
+      <c r="C9" t="s">
+        <v>73</v>
+      </c>
+      <c r="D9" t="s">
+        <v>17</v>
+      </c>
+      <c r="E9">
+        <v>100</v>
+      </c>
+      <c r="F9">
+        <v>1</v>
+      </c>
+      <c r="G9" s="2" t="s">
+        <v>74</v>
+      </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="E10"/>
-      <c r="F10"/>
+      <c r="A10" s="1">
+        <v>45794</v>
+      </c>
+      <c r="C10" t="s">
+        <v>79</v>
+      </c>
+      <c r="D10" t="s">
+        <v>37</v>
+      </c>
+      <c r="E10">
+        <v>10</v>
+      </c>
+      <c r="F10">
+        <v>1</v>
+      </c>
+      <c r="G10" s="2" t="s">
+        <v>80</v>
+      </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="E11"/>
-      <c r="F11"/>
+      <c r="A11" s="1">
+        <v>45795</v>
+      </c>
+      <c r="C11" t="s">
+        <v>75</v>
+      </c>
+      <c r="D11" t="s">
+        <v>37</v>
+      </c>
+      <c r="E11">
+        <v>50</v>
+      </c>
+      <c r="F11">
+        <v>1</v>
+      </c>
+      <c r="G11" s="2" t="s">
+        <v>76</v>
+      </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="E12"/>
-      <c r="F12"/>
+      <c r="A12" s="1">
+        <v>45796</v>
+      </c>
+      <c r="C12" t="s">
+        <v>77</v>
+      </c>
+      <c r="D12" t="s">
+        <v>17</v>
+      </c>
+      <c r="E12">
+        <v>100</v>
+      </c>
+      <c r="F12">
+        <v>1</v>
+      </c>
+      <c r="G12" s="2" t="s">
+        <v>78</v>
+      </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="E13"/>
@@ -1180,7 +1403,7 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
   <ignoredErrors>
-    <ignoredError sqref="D8:D16" listDataValidation="1"/>
+    <ignoredError sqref="D13:D16" listDataValidation="1"/>
   </ignoredErrors>
   <tableParts count="1">
     <tablePart r:id="rId2"/>
@@ -1192,20 +1415,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3BDA6702-5DDF-42FB-988E-13FBEB26F5C9}">
   <dimension ref="A1:H100"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H2" sqref="H2"/>
+    <sheetView topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.85546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="17.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="55.5703125" customWidth="1"/>
+    <col min="4" max="4" width="10.5703125" customWidth="1"/>
     <col min="5" max="5" width="14.85546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="23.5703125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="13.42578125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="19.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.28515625" customWidth="1"/>
+    <col min="7" max="7" width="92.85546875" customWidth="1"/>
+    <col min="8" max="8" width="82.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
@@ -1235,792 +1458,692 @@
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A2" s="8"/>
-      <c r="B2" s="2"/>
-      <c r="E2" s="3"/>
-      <c r="G2" s="2"/>
+      <c r="A2" s="8">
+        <v>45786</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="C2" t="s">
+        <v>36</v>
+      </c>
+      <c r="D2" t="s">
+        <v>37</v>
+      </c>
+      <c r="E2">
+        <v>90</v>
+      </c>
+      <c r="F2">
+        <v>8</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="H2" t="s">
+        <v>39</v>
+      </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A3" s="8"/>
-      <c r="B3" s="2"/>
-      <c r="E3" s="3"/>
-      <c r="F3" s="4"/>
-      <c r="G3" s="2"/>
-      <c r="H3" s="2"/>
+      <c r="A3" s="8">
+        <v>45787</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="C3" t="s">
+        <v>40</v>
+      </c>
+      <c r="D3" t="s">
+        <v>37</v>
+      </c>
+      <c r="E3">
+        <v>90</v>
+      </c>
+      <c r="F3">
+        <v>8</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="H3" s="2" t="s">
+        <v>42</v>
+      </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A4" s="8"/>
-      <c r="B4" s="2"/>
-      <c r="E4" s="3"/>
-      <c r="F4" s="4"/>
-      <c r="G4" s="2"/>
+      <c r="A4" s="8">
+        <v>45789</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="C4" t="s">
+        <v>43</v>
+      </c>
+      <c r="D4" t="s">
+        <v>37</v>
+      </c>
+      <c r="E4">
+        <v>90</v>
+      </c>
+      <c r="F4">
+        <v>5</v>
+      </c>
+      <c r="G4" s="2" t="s">
+        <v>44</v>
+      </c>
       <c r="H4" s="2"/>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A5" s="8"/>
-      <c r="B5" s="2"/>
-      <c r="E5" s="3"/>
-      <c r="F5" s="4"/>
-      <c r="G5" s="2"/>
+      <c r="A5" s="8">
+        <v>45790</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="C5" t="s">
+        <v>46</v>
+      </c>
+      <c r="D5" t="s">
+        <v>17</v>
+      </c>
+      <c r="E5">
+        <v>100</v>
+      </c>
+      <c r="F5">
+        <v>5</v>
+      </c>
+      <c r="G5" s="2" t="s">
+        <v>47</v>
+      </c>
       <c r="H5" s="2"/>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A6" s="8"/>
-      <c r="B6" s="2"/>
-      <c r="E6" s="3"/>
-      <c r="F6" s="4"/>
-      <c r="G6" s="2"/>
-      <c r="H6" s="2"/>
+      <c r="A6" s="8">
+        <v>45791</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="C6" t="s">
+        <v>48</v>
+      </c>
+      <c r="D6" t="s">
+        <v>17</v>
+      </c>
+      <c r="E6">
+        <v>100</v>
+      </c>
+      <c r="F6">
+        <v>5</v>
+      </c>
+      <c r="G6" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="H6" s="2" t="s">
+        <v>49</v>
+      </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="8"/>
       <c r="B7" s="2"/>
-      <c r="E7" s="3"/>
-      <c r="F7" s="4"/>
       <c r="G7" s="2"/>
       <c r="H7" s="2"/>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="8"/>
       <c r="B8" s="2"/>
-      <c r="E8" s="3"/>
-      <c r="F8" s="4"/>
       <c r="G8" s="2"/>
       <c r="H8" s="2"/>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="8"/>
       <c r="B9" s="2"/>
-      <c r="E9" s="3"/>
-      <c r="F9" s="4"/>
       <c r="G9" s="2"/>
       <c r="H9" s="2"/>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="8"/>
       <c r="B10" s="2"/>
-      <c r="E10" s="3"/>
-      <c r="F10" s="4"/>
       <c r="G10" s="2"/>
       <c r="H10" s="2"/>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="8"/>
       <c r="B11" s="2"/>
-      <c r="E11" s="3"/>
-      <c r="F11" s="4"/>
       <c r="G11" s="2"/>
       <c r="H11" s="2"/>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="8"/>
       <c r="B12" s="2"/>
-      <c r="E12" s="3"/>
-      <c r="F12" s="4"/>
       <c r="G12" s="2"/>
       <c r="H12" s="2"/>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="8"/>
       <c r="B13" s="2"/>
-      <c r="E13" s="3"/>
-      <c r="F13" s="4"/>
       <c r="G13" s="2"/>
       <c r="H13" s="2"/>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" s="8"/>
       <c r="B14" s="2"/>
-      <c r="E14" s="3"/>
-      <c r="F14" s="4"/>
       <c r="G14" s="2"/>
       <c r="H14" s="2"/>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" s="8"/>
       <c r="B15" s="2"/>
-      <c r="E15" s="3"/>
-      <c r="F15" s="4"/>
       <c r="G15" s="2"/>
       <c r="H15" s="2"/>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" s="8"/>
       <c r="B16" s="2"/>
-      <c r="E16" s="3"/>
-      <c r="F16" s="4"/>
       <c r="G16" s="2"/>
       <c r="H16" s="2"/>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" s="8"/>
       <c r="B17" s="2"/>
-      <c r="E17" s="3"/>
-      <c r="F17" s="4"/>
       <c r="G17" s="2"/>
       <c r="H17" s="2"/>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" s="8"/>
       <c r="B18" s="2"/>
-      <c r="E18" s="3"/>
-      <c r="F18" s="4"/>
       <c r="G18" s="2"/>
       <c r="H18" s="2"/>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" s="8"/>
       <c r="B19" s="2"/>
-      <c r="E19" s="3"/>
-      <c r="F19" s="4"/>
       <c r="G19" s="2"/>
       <c r="H19" s="2"/>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" s="8"/>
       <c r="B20" s="2"/>
-      <c r="E20" s="3"/>
-      <c r="F20" s="4"/>
       <c r="G20" s="2"/>
       <c r="H20" s="2"/>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" s="8"/>
       <c r="B21" s="2"/>
-      <c r="E21" s="3"/>
-      <c r="F21" s="4"/>
       <c r="G21" s="2"/>
       <c r="H21" s="2"/>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" s="8"/>
       <c r="B22" s="2"/>
-      <c r="E22" s="3"/>
-      <c r="F22" s="4"/>
       <c r="G22" s="2"/>
       <c r="H22" s="2"/>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" s="8"/>
       <c r="B23" s="2"/>
-      <c r="E23" s="3"/>
-      <c r="F23" s="4"/>
       <c r="G23" s="2"/>
       <c r="H23" s="2"/>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24" s="8"/>
       <c r="B24" s="2"/>
-      <c r="E24" s="3"/>
-      <c r="F24" s="4"/>
       <c r="G24" s="2"/>
       <c r="H24" s="2"/>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25" s="8"/>
       <c r="B25" s="2"/>
-      <c r="E25" s="3"/>
-      <c r="F25" s="4"/>
       <c r="G25" s="2"/>
       <c r="H25" s="2"/>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26" s="8"/>
       <c r="B26" s="2"/>
-      <c r="E26" s="3"/>
-      <c r="F26" s="4"/>
       <c r="G26" s="2"/>
       <c r="H26" s="2"/>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A27" s="8"/>
       <c r="B27" s="2"/>
-      <c r="E27" s="3"/>
-      <c r="F27" s="4"/>
       <c r="G27" s="2"/>
       <c r="H27" s="2"/>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A28" s="8"/>
       <c r="B28" s="2"/>
-      <c r="E28" s="3"/>
-      <c r="F28" s="4"/>
       <c r="G28" s="2"/>
       <c r="H28" s="2"/>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A29" s="8"/>
       <c r="B29" s="2"/>
-      <c r="E29" s="3"/>
-      <c r="F29" s="4"/>
       <c r="G29" s="2"/>
       <c r="H29" s="2"/>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A30" s="8"/>
       <c r="B30" s="2"/>
-      <c r="E30" s="3"/>
-      <c r="F30" s="4"/>
       <c r="G30" s="2"/>
       <c r="H30" s="2"/>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A31" s="8"/>
       <c r="B31" s="2"/>
-      <c r="E31" s="3"/>
-      <c r="F31" s="4"/>
       <c r="G31" s="2"/>
       <c r="H31" s="2"/>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A32" s="8"/>
       <c r="B32" s="2"/>
-      <c r="E32" s="3"/>
-      <c r="F32" s="4"/>
       <c r="G32" s="2"/>
       <c r="H32" s="2"/>
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A33" s="8"/>
       <c r="B33" s="2"/>
-      <c r="E33" s="3"/>
-      <c r="F33" s="4"/>
       <c r="G33" s="2"/>
       <c r="H33" s="2"/>
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A34" s="8"/>
       <c r="B34" s="2"/>
-      <c r="E34" s="3"/>
-      <c r="F34" s="4"/>
       <c r="G34" s="2"/>
       <c r="H34" s="2"/>
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A35" s="8"/>
       <c r="B35" s="2"/>
-      <c r="E35" s="3"/>
-      <c r="F35" s="4"/>
       <c r="G35" s="2"/>
       <c r="H35" s="2"/>
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A36" s="8"/>
       <c r="B36" s="2"/>
-      <c r="E36" s="3"/>
-      <c r="F36" s="4"/>
       <c r="G36" s="2"/>
       <c r="H36" s="2"/>
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A37" s="8"/>
       <c r="B37" s="2"/>
-      <c r="E37" s="3"/>
-      <c r="F37" s="4"/>
       <c r="G37" s="2"/>
       <c r="H37" s="2"/>
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A38" s="8"/>
       <c r="B38" s="2"/>
-      <c r="E38" s="3"/>
-      <c r="F38" s="4"/>
       <c r="G38" s="2"/>
       <c r="H38" s="2"/>
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A39" s="8"/>
       <c r="B39" s="2"/>
-      <c r="E39" s="3"/>
-      <c r="F39" s="4"/>
       <c r="G39" s="2"/>
       <c r="H39" s="2"/>
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A40" s="8"/>
       <c r="B40" s="2"/>
-      <c r="E40" s="3"/>
-      <c r="F40" s="4"/>
       <c r="G40" s="2"/>
       <c r="H40" s="2"/>
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A41" s="8"/>
       <c r="B41" s="2"/>
-      <c r="E41" s="3"/>
-      <c r="F41" s="4"/>
       <c r="G41" s="2"/>
       <c r="H41" s="2"/>
     </row>
     <row r="42" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A42" s="8"/>
       <c r="B42" s="2"/>
-      <c r="E42" s="3"/>
-      <c r="F42" s="4"/>
       <c r="G42" s="2"/>
       <c r="H42" s="2"/>
     </row>
     <row r="43" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A43" s="8"/>
       <c r="B43" s="2"/>
-      <c r="E43" s="3"/>
-      <c r="F43" s="4"/>
       <c r="G43" s="2"/>
       <c r="H43" s="2"/>
     </row>
     <row r="44" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A44" s="8"/>
       <c r="B44" s="2"/>
-      <c r="E44" s="3"/>
-      <c r="F44" s="4"/>
       <c r="G44" s="2"/>
       <c r="H44" s="2"/>
     </row>
     <row r="45" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A45" s="8"/>
       <c r="B45" s="2"/>
-      <c r="E45" s="3"/>
-      <c r="F45" s="4"/>
       <c r="G45" s="2"/>
       <c r="H45" s="2"/>
     </row>
     <row r="46" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A46" s="8"/>
       <c r="B46" s="2"/>
-      <c r="E46" s="3"/>
-      <c r="F46" s="4"/>
       <c r="G46" s="2"/>
       <c r="H46" s="2"/>
     </row>
     <row r="47" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A47" s="8"/>
       <c r="B47" s="2"/>
-      <c r="E47" s="3"/>
-      <c r="F47" s="4"/>
       <c r="G47" s="2"/>
       <c r="H47" s="2"/>
     </row>
     <row r="48" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A48" s="8"/>
       <c r="B48" s="2"/>
-      <c r="E48" s="3"/>
-      <c r="F48" s="4"/>
       <c r="G48" s="2"/>
       <c r="H48" s="2"/>
     </row>
     <row r="49" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A49" s="8"/>
       <c r="B49" s="2"/>
-      <c r="E49" s="3"/>
-      <c r="F49" s="4"/>
       <c r="G49" s="2"/>
       <c r="H49" s="2"/>
     </row>
     <row r="50" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A50" s="8"/>
       <c r="B50" s="2"/>
-      <c r="E50" s="3"/>
-      <c r="F50" s="4"/>
       <c r="G50" s="2"/>
       <c r="H50" s="2"/>
     </row>
     <row r="51" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A51" s="8"/>
       <c r="B51" s="2"/>
-      <c r="E51" s="3"/>
-      <c r="F51" s="4"/>
       <c r="G51" s="2"/>
       <c r="H51" s="2"/>
     </row>
     <row r="52" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A52" s="8"/>
       <c r="B52" s="2"/>
-      <c r="E52" s="3"/>
-      <c r="F52" s="4"/>
       <c r="G52" s="2"/>
       <c r="H52" s="2"/>
     </row>
     <row r="53" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A53" s="8"/>
       <c r="B53" s="2"/>
-      <c r="E53" s="3"/>
-      <c r="F53" s="4"/>
       <c r="G53" s="2"/>
       <c r="H53" s="2"/>
     </row>
     <row r="54" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A54" s="8"/>
       <c r="B54" s="2"/>
-      <c r="E54" s="3"/>
-      <c r="F54" s="4"/>
       <c r="G54" s="2"/>
       <c r="H54" s="2"/>
     </row>
     <row r="55" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A55" s="8"/>
       <c r="B55" s="2"/>
-      <c r="E55" s="3"/>
-      <c r="F55" s="4"/>
       <c r="G55" s="2"/>
       <c r="H55" s="2"/>
     </row>
     <row r="56" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A56" s="8"/>
       <c r="B56" s="2"/>
-      <c r="E56" s="3"/>
-      <c r="F56" s="4"/>
       <c r="G56" s="2"/>
       <c r="H56" s="2"/>
     </row>
     <row r="57" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A57" s="8"/>
       <c r="B57" s="2"/>
-      <c r="E57" s="3"/>
-      <c r="F57" s="4"/>
       <c r="G57" s="2"/>
       <c r="H57" s="2"/>
     </row>
     <row r="58" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A58" s="8"/>
       <c r="B58" s="2"/>
-      <c r="E58" s="3"/>
-      <c r="F58" s="4"/>
       <c r="G58" s="2"/>
       <c r="H58" s="2"/>
     </row>
     <row r="59" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A59" s="8"/>
       <c r="B59" s="2"/>
-      <c r="E59" s="3"/>
-      <c r="F59" s="4"/>
       <c r="G59" s="2"/>
       <c r="H59" s="2"/>
     </row>
     <row r="60" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A60" s="8"/>
       <c r="B60" s="2"/>
-      <c r="E60" s="3"/>
-      <c r="F60" s="4"/>
       <c r="G60" s="2"/>
       <c r="H60" s="2"/>
     </row>
     <row r="61" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A61" s="8"/>
       <c r="B61" s="2"/>
-      <c r="E61" s="3"/>
-      <c r="F61" s="4"/>
       <c r="G61" s="2"/>
       <c r="H61" s="2"/>
     </row>
     <row r="62" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A62" s="8"/>
       <c r="B62" s="2"/>
-      <c r="E62" s="3"/>
-      <c r="F62" s="4"/>
       <c r="G62" s="2"/>
       <c r="H62" s="2"/>
     </row>
     <row r="63" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A63" s="8"/>
       <c r="B63" s="2"/>
-      <c r="E63" s="3"/>
-      <c r="F63" s="4"/>
       <c r="G63" s="2"/>
       <c r="H63" s="2"/>
     </row>
     <row r="64" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A64" s="8"/>
       <c r="B64" s="2"/>
-      <c r="E64" s="3"/>
-      <c r="F64" s="4"/>
       <c r="G64" s="2"/>
       <c r="H64" s="2"/>
     </row>
     <row r="65" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A65" s="8"/>
       <c r="B65" s="2"/>
-      <c r="E65" s="3"/>
-      <c r="F65" s="4"/>
       <c r="G65" s="2"/>
       <c r="H65" s="2"/>
     </row>
     <row r="66" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A66" s="8"/>
       <c r="B66" s="2"/>
-      <c r="E66" s="3"/>
-      <c r="F66" s="4"/>
       <c r="G66" s="2"/>
       <c r="H66" s="2"/>
     </row>
     <row r="67" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A67" s="8"/>
       <c r="B67" s="2"/>
-      <c r="E67" s="3"/>
-      <c r="F67" s="4"/>
       <c r="G67" s="2"/>
       <c r="H67" s="2"/>
     </row>
     <row r="68" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A68" s="8"/>
       <c r="B68" s="2"/>
-      <c r="E68" s="3"/>
-      <c r="F68" s="4"/>
       <c r="G68" s="2"/>
       <c r="H68" s="2"/>
     </row>
     <row r="69" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A69" s="8"/>
       <c r="B69" s="2"/>
-      <c r="E69" s="3"/>
-      <c r="F69" s="4"/>
       <c r="G69" s="2"/>
       <c r="H69" s="2"/>
     </row>
     <row r="70" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A70" s="8"/>
       <c r="B70" s="2"/>
-      <c r="E70" s="3"/>
-      <c r="F70" s="4"/>
       <c r="G70" s="2"/>
       <c r="H70" s="2"/>
     </row>
     <row r="71" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A71" s="8"/>
       <c r="B71" s="2"/>
-      <c r="E71" s="3"/>
-      <c r="F71" s="4"/>
       <c r="G71" s="2"/>
       <c r="H71" s="2"/>
     </row>
     <row r="72" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A72" s="8"/>
       <c r="B72" s="2"/>
-      <c r="E72" s="3"/>
-      <c r="F72" s="4"/>
       <c r="G72" s="2"/>
       <c r="H72" s="2"/>
     </row>
     <row r="73" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A73" s="8"/>
       <c r="B73" s="2"/>
-      <c r="E73" s="3"/>
-      <c r="F73" s="4"/>
       <c r="G73" s="2"/>
       <c r="H73" s="2"/>
     </row>
     <row r="74" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A74" s="8"/>
       <c r="B74" s="2"/>
-      <c r="E74" s="3"/>
-      <c r="F74" s="4"/>
       <c r="G74" s="2"/>
       <c r="H74" s="2"/>
     </row>
     <row r="75" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A75" s="8"/>
       <c r="B75" s="2"/>
-      <c r="E75" s="3"/>
-      <c r="F75" s="4"/>
       <c r="G75" s="2"/>
       <c r="H75" s="2"/>
     </row>
     <row r="76" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A76" s="8"/>
       <c r="B76" s="2"/>
-      <c r="E76" s="3"/>
-      <c r="F76" s="4"/>
       <c r="G76" s="2"/>
       <c r="H76" s="2"/>
     </row>
     <row r="77" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A77" s="8"/>
       <c r="B77" s="2"/>
-      <c r="E77" s="3"/>
-      <c r="F77" s="4"/>
       <c r="G77" s="2"/>
       <c r="H77" s="2"/>
     </row>
     <row r="78" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A78" s="8"/>
       <c r="B78" s="2"/>
-      <c r="E78" s="3"/>
-      <c r="F78" s="4"/>
       <c r="G78" s="2"/>
       <c r="H78" s="2"/>
     </row>
     <row r="79" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A79" s="8"/>
       <c r="B79" s="2"/>
-      <c r="E79" s="3"/>
-      <c r="F79" s="4"/>
       <c r="G79" s="2"/>
       <c r="H79" s="2"/>
     </row>
     <row r="80" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A80" s="8"/>
       <c r="B80" s="2"/>
-      <c r="E80" s="3"/>
-      <c r="F80" s="4"/>
       <c r="G80" s="2"/>
       <c r="H80" s="2"/>
     </row>
     <row r="81" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A81" s="8"/>
       <c r="B81" s="2"/>
-      <c r="E81" s="3"/>
-      <c r="F81" s="4"/>
       <c r="G81" s="2"/>
       <c r="H81" s="2"/>
     </row>
     <row r="82" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A82" s="8"/>
       <c r="B82" s="2"/>
-      <c r="E82" s="3"/>
-      <c r="F82" s="4"/>
       <c r="G82" s="2"/>
       <c r="H82" s="2"/>
     </row>
     <row r="83" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A83" s="8"/>
       <c r="B83" s="2"/>
-      <c r="E83" s="3"/>
-      <c r="F83" s="4"/>
       <c r="G83" s="2"/>
       <c r="H83" s="2"/>
     </row>
     <row r="84" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A84" s="8"/>
       <c r="B84" s="2"/>
-      <c r="E84" s="3"/>
-      <c r="F84" s="4"/>
       <c r="G84" s="2"/>
       <c r="H84" s="2"/>
     </row>
     <row r="85" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A85" s="8"/>
       <c r="B85" s="2"/>
-      <c r="E85" s="3"/>
-      <c r="F85" s="4"/>
       <c r="G85" s="2"/>
       <c r="H85" s="2"/>
     </row>
     <row r="86" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A86" s="8"/>
       <c r="B86" s="2"/>
-      <c r="E86" s="3"/>
-      <c r="F86" s="4"/>
       <c r="G86" s="2"/>
       <c r="H86" s="2"/>
     </row>
     <row r="87" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A87" s="8"/>
       <c r="B87" s="2"/>
-      <c r="E87" s="3"/>
-      <c r="F87" s="4"/>
       <c r="G87" s="2"/>
       <c r="H87" s="2"/>
     </row>
     <row r="88" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A88" s="8"/>
       <c r="B88" s="2"/>
-      <c r="E88" s="3"/>
-      <c r="F88" s="4"/>
       <c r="G88" s="2"/>
       <c r="H88" s="2"/>
     </row>
     <row r="89" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A89" s="8"/>
       <c r="B89" s="2"/>
-      <c r="E89" s="3"/>
-      <c r="F89" s="4"/>
       <c r="G89" s="2"/>
       <c r="H89" s="2"/>
     </row>
     <row r="90" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A90" s="8"/>
       <c r="B90" s="2"/>
-      <c r="E90" s="3"/>
-      <c r="F90" s="4"/>
       <c r="G90" s="2"/>
       <c r="H90" s="2"/>
     </row>
     <row r="91" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A91" s="8"/>
       <c r="B91" s="2"/>
-      <c r="E91" s="3"/>
-      <c r="F91" s="4"/>
       <c r="G91" s="2"/>
       <c r="H91" s="2"/>
     </row>
     <row r="92" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A92" s="8"/>
       <c r="B92" s="2"/>
-      <c r="E92" s="3"/>
-      <c r="F92" s="4"/>
       <c r="G92" s="2"/>
       <c r="H92" s="2"/>
     </row>
     <row r="93" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A93" s="8"/>
       <c r="B93" s="2"/>
-      <c r="E93" s="3"/>
-      <c r="F93" s="4"/>
       <c r="G93" s="2"/>
       <c r="H93" s="2"/>
     </row>
     <row r="94" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A94" s="8"/>
       <c r="B94" s="2"/>
-      <c r="E94" s="3"/>
-      <c r="F94" s="4"/>
       <c r="G94" s="2"/>
       <c r="H94" s="2"/>
     </row>
     <row r="95" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A95" s="8"/>
       <c r="B95" s="2"/>
-      <c r="E95" s="3"/>
-      <c r="F95" s="4"/>
       <c r="G95" s="2"/>
       <c r="H95" s="2"/>
     </row>
     <row r="96" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A96" s="8"/>
       <c r="B96" s="2"/>
-      <c r="E96" s="3"/>
-      <c r="F96" s="4"/>
       <c r="G96" s="2"/>
       <c r="H96" s="2"/>
     </row>
     <row r="97" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A97" s="8"/>
       <c r="B97" s="2"/>
-      <c r="E97" s="3"/>
-      <c r="F97" s="4"/>
       <c r="G97" s="2"/>
       <c r="H97" s="2"/>
     </row>
     <row r="98" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A98" s="8"/>
       <c r="B98" s="2"/>
-      <c r="E98" s="3"/>
-      <c r="F98" s="4"/>
       <c r="G98" s="2"/>
       <c r="H98" s="2"/>
     </row>
     <row r="99" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A99" s="8"/>
       <c r="B99" s="2"/>
-      <c r="E99" s="3"/>
-      <c r="F99" s="4"/>
       <c r="G99" s="2"/>
       <c r="H99" s="2"/>
     </row>
     <row r="100" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A100" s="8"/>
       <c r="B100" s="2"/>
-      <c r="E100" s="3"/>
-      <c r="F100" s="4"/>
       <c r="G100" s="2"/>
       <c r="H100" s="2"/>
     </row>
@@ -2043,7 +2166,7 @@
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <ignoredErrors>
-    <ignoredError sqref="D3:D100" listDataValidation="1"/>
+    <ignoredError sqref="D7:D100" listDataValidation="1"/>
   </ignoredErrors>
   <tableParts count="1">
     <tablePart r:id="rId1"/>
@@ -2055,20 +2178,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9FD6A201-8E63-4A9E-A683-19506CB489E3}">
   <dimension ref="A1:H100"/>
   <sheetViews>
-    <sheetView topLeftCell="A63" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2:D100"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="7.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.140625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="17.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="27.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.7109375" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="14.85546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="23.5703125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="13.42578125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="19.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="23.5703125" style="10" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="39.140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="51.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
@@ -2087,7 +2210,7 @@
       <c r="E1" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="7" t="s">
+      <c r="F1" s="11" t="s">
         <v>5</v>
       </c>
       <c r="G1" s="7" t="s">
@@ -2098,58 +2221,165 @@
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A2" s="1"/>
-      <c r="B2" s="2"/>
-      <c r="E2" s="3"/>
-      <c r="F2" s="4"/>
-      <c r="G2" s="2"/>
-      <c r="H2" s="2"/>
+      <c r="A2" s="1">
+        <v>45935</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="C2" t="s">
+        <v>52</v>
+      </c>
+      <c r="D2" t="s">
+        <v>17</v>
+      </c>
+      <c r="E2" s="3">
+        <v>1</v>
+      </c>
+      <c r="F2" s="10">
+        <v>4</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>54</v>
+      </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A3" s="1"/>
-      <c r="B3" s="2"/>
-      <c r="E3" s="3"/>
-      <c r="F3" s="4"/>
-      <c r="G3" s="2"/>
-      <c r="H3" s="2"/>
+      <c r="A3" s="1">
+        <v>45996</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="C3" t="s">
+        <v>55</v>
+      </c>
+      <c r="D3" t="s">
+        <v>17</v>
+      </c>
+      <c r="E3" s="3">
+        <v>1</v>
+      </c>
+      <c r="F3" s="10">
+        <v>4</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="H3" s="2" t="s">
+        <v>54</v>
+      </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A4" s="1"/>
-      <c r="B4" s="2"/>
-      <c r="E4" s="3"/>
-      <c r="F4" s="4"/>
-      <c r="G4" s="2"/>
-      <c r="H4" s="2"/>
+      <c r="A4" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="C4" t="s">
+        <v>58</v>
+      </c>
+      <c r="D4" t="s">
+        <v>17</v>
+      </c>
+      <c r="E4" s="3">
+        <v>1</v>
+      </c>
+      <c r="F4" s="10">
+        <v>4</v>
+      </c>
+      <c r="G4" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="H4" s="2" t="s">
+        <v>60</v>
+      </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A5" s="1"/>
-      <c r="B5" s="2"/>
-      <c r="E5" s="3"/>
-      <c r="F5" s="4"/>
-      <c r="G5" s="2"/>
-      <c r="H5" s="2"/>
+      <c r="A5" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="C5" t="s">
+        <v>62</v>
+      </c>
+      <c r="D5" t="s">
+        <v>17</v>
+      </c>
+      <c r="E5" s="3">
+        <v>1</v>
+      </c>
+      <c r="F5" s="10">
+        <v>5</v>
+      </c>
+      <c r="G5" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="H5" s="2" t="s">
+        <v>54</v>
+      </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A6" s="1"/>
-      <c r="B6" s="2"/>
-      <c r="E6" s="3"/>
-      <c r="F6" s="4"/>
-      <c r="G6" s="2"/>
-      <c r="H6" s="2"/>
+      <c r="A6" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="C6" t="s">
+        <v>68</v>
+      </c>
+      <c r="D6" t="s">
+        <v>17</v>
+      </c>
+      <c r="E6" s="3">
+        <v>1</v>
+      </c>
+      <c r="F6" s="10">
+        <v>3</v>
+      </c>
+      <c r="G6" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="H6" s="2" t="s">
+        <v>54</v>
+      </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A7" s="1"/>
-      <c r="B7" s="2"/>
-      <c r="E7" s="3"/>
-      <c r="F7" s="4"/>
-      <c r="G7" s="2"/>
-      <c r="H7" s="2"/>
+      <c r="A7" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="C7" t="s">
+        <v>71</v>
+      </c>
+      <c r="D7" t="s">
+        <v>17</v>
+      </c>
+      <c r="E7" s="3">
+        <v>1</v>
+      </c>
+      <c r="F7" s="10">
+        <v>5</v>
+      </c>
+      <c r="G7" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="H7" s="2" t="s">
+        <v>54</v>
+      </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="1"/>
       <c r="B8" s="2"/>
       <c r="E8" s="3"/>
-      <c r="F8" s="4"/>
       <c r="G8" s="2"/>
       <c r="H8" s="2"/>
     </row>
@@ -2157,7 +2387,6 @@
       <c r="A9" s="1"/>
       <c r="B9" s="2"/>
       <c r="E9" s="3"/>
-      <c r="F9" s="4"/>
       <c r="G9" s="2"/>
       <c r="H9" s="2"/>
     </row>
@@ -2165,7 +2394,6 @@
       <c r="A10" s="1"/>
       <c r="B10" s="2"/>
       <c r="E10" s="3"/>
-      <c r="F10" s="4"/>
       <c r="G10" s="2"/>
       <c r="H10" s="2"/>
     </row>
@@ -2173,7 +2401,6 @@
       <c r="A11" s="1"/>
       <c r="B11" s="2"/>
       <c r="E11" s="3"/>
-      <c r="F11" s="4"/>
       <c r="G11" s="2"/>
       <c r="H11" s="2"/>
     </row>
@@ -2181,7 +2408,6 @@
       <c r="A12" s="1"/>
       <c r="B12" s="2"/>
       <c r="E12" s="3"/>
-      <c r="F12" s="4"/>
       <c r="G12" s="2"/>
       <c r="H12" s="2"/>
     </row>
@@ -2189,7 +2415,6 @@
       <c r="A13" s="1"/>
       <c r="B13" s="2"/>
       <c r="E13" s="3"/>
-      <c r="F13" s="4"/>
       <c r="G13" s="2"/>
       <c r="H13" s="2"/>
     </row>
@@ -2197,7 +2422,6 @@
       <c r="A14" s="1"/>
       <c r="B14" s="2"/>
       <c r="E14" s="3"/>
-      <c r="F14" s="4"/>
       <c r="G14" s="2"/>
       <c r="H14" s="2"/>
     </row>
@@ -2205,7 +2429,6 @@
       <c r="A15" s="1"/>
       <c r="B15" s="2"/>
       <c r="E15" s="3"/>
-      <c r="F15" s="4"/>
       <c r="G15" s="2"/>
       <c r="H15" s="2"/>
     </row>
@@ -2213,7 +2436,6 @@
       <c r="A16" s="1"/>
       <c r="B16" s="2"/>
       <c r="E16" s="3"/>
-      <c r="F16" s="4"/>
       <c r="G16" s="2"/>
       <c r="H16" s="2"/>
     </row>
@@ -2221,7 +2443,6 @@
       <c r="A17" s="1"/>
       <c r="B17" s="2"/>
       <c r="E17" s="3"/>
-      <c r="F17" s="4"/>
       <c r="G17" s="2"/>
       <c r="H17" s="2"/>
     </row>
@@ -2229,7 +2450,6 @@
       <c r="A18" s="1"/>
       <c r="B18" s="2"/>
       <c r="E18" s="3"/>
-      <c r="F18" s="4"/>
       <c r="G18" s="2"/>
       <c r="H18" s="2"/>
     </row>
@@ -2237,7 +2457,6 @@
       <c r="A19" s="1"/>
       <c r="B19" s="2"/>
       <c r="E19" s="3"/>
-      <c r="F19" s="4"/>
       <c r="G19" s="2"/>
       <c r="H19" s="2"/>
     </row>
@@ -2245,7 +2464,6 @@
       <c r="A20" s="1"/>
       <c r="B20" s="2"/>
       <c r="E20" s="3"/>
-      <c r="F20" s="4"/>
       <c r="G20" s="2"/>
       <c r="H20" s="2"/>
     </row>
@@ -2253,7 +2471,6 @@
       <c r="A21" s="1"/>
       <c r="B21" s="2"/>
       <c r="E21" s="3"/>
-      <c r="F21" s="4"/>
       <c r="G21" s="2"/>
       <c r="H21" s="2"/>
     </row>
@@ -2261,7 +2478,6 @@
       <c r="A22" s="1"/>
       <c r="B22" s="2"/>
       <c r="E22" s="3"/>
-      <c r="F22" s="4"/>
       <c r="G22" s="2"/>
       <c r="H22" s="2"/>
     </row>
@@ -2269,7 +2485,6 @@
       <c r="A23" s="1"/>
       <c r="B23" s="2"/>
       <c r="E23" s="3"/>
-      <c r="F23" s="4"/>
       <c r="G23" s="2"/>
       <c r="H23" s="2"/>
     </row>
@@ -2277,7 +2492,6 @@
       <c r="A24" s="1"/>
       <c r="B24" s="2"/>
       <c r="E24" s="3"/>
-      <c r="F24" s="4"/>
       <c r="G24" s="2"/>
       <c r="H24" s="2"/>
     </row>
@@ -2285,7 +2499,6 @@
       <c r="A25" s="1"/>
       <c r="B25" s="2"/>
       <c r="E25" s="3"/>
-      <c r="F25" s="4"/>
       <c r="G25" s="2"/>
       <c r="H25" s="2"/>
     </row>
@@ -2293,7 +2506,6 @@
       <c r="A26" s="1"/>
       <c r="B26" s="2"/>
       <c r="E26" s="3"/>
-      <c r="F26" s="4"/>
       <c r="G26" s="2"/>
       <c r="H26" s="2"/>
     </row>
@@ -2301,7 +2513,6 @@
       <c r="A27" s="1"/>
       <c r="B27" s="2"/>
       <c r="E27" s="3"/>
-      <c r="F27" s="4"/>
       <c r="G27" s="2"/>
       <c r="H27" s="2"/>
     </row>
@@ -2309,7 +2520,6 @@
       <c r="A28" s="1"/>
       <c r="B28" s="2"/>
       <c r="E28" s="3"/>
-      <c r="F28" s="4"/>
       <c r="G28" s="2"/>
       <c r="H28" s="2"/>
     </row>
@@ -2317,7 +2527,6 @@
       <c r="A29" s="1"/>
       <c r="B29" s="2"/>
       <c r="E29" s="3"/>
-      <c r="F29" s="4"/>
       <c r="G29" s="2"/>
       <c r="H29" s="2"/>
     </row>
@@ -2325,7 +2534,6 @@
       <c r="A30" s="1"/>
       <c r="B30" s="2"/>
       <c r="E30" s="3"/>
-      <c r="F30" s="4"/>
       <c r="G30" s="2"/>
       <c r="H30" s="2"/>
     </row>
@@ -2333,7 +2541,6 @@
       <c r="A31" s="1"/>
       <c r="B31" s="2"/>
       <c r="E31" s="3"/>
-      <c r="F31" s="4"/>
       <c r="G31" s="2"/>
       <c r="H31" s="2"/>
     </row>
@@ -2341,7 +2548,6 @@
       <c r="A32" s="1"/>
       <c r="B32" s="2"/>
       <c r="E32" s="3"/>
-      <c r="F32" s="4"/>
       <c r="G32" s="2"/>
       <c r="H32" s="2"/>
     </row>
@@ -2349,7 +2555,6 @@
       <c r="A33" s="1"/>
       <c r="B33" s="2"/>
       <c r="E33" s="3"/>
-      <c r="F33" s="4"/>
       <c r="G33" s="2"/>
       <c r="H33" s="2"/>
     </row>
@@ -2357,7 +2562,6 @@
       <c r="A34" s="1"/>
       <c r="B34" s="2"/>
       <c r="E34" s="3"/>
-      <c r="F34" s="4"/>
       <c r="G34" s="2"/>
       <c r="H34" s="2"/>
     </row>
@@ -2365,7 +2569,6 @@
       <c r="A35" s="1"/>
       <c r="B35" s="2"/>
       <c r="E35" s="3"/>
-      <c r="F35" s="4"/>
       <c r="G35" s="2"/>
       <c r="H35" s="2"/>
     </row>
@@ -2373,7 +2576,6 @@
       <c r="A36" s="1"/>
       <c r="B36" s="2"/>
       <c r="E36" s="3"/>
-      <c r="F36" s="4"/>
       <c r="G36" s="2"/>
       <c r="H36" s="2"/>
     </row>
@@ -2381,7 +2583,6 @@
       <c r="A37" s="1"/>
       <c r="B37" s="2"/>
       <c r="E37" s="3"/>
-      <c r="F37" s="4"/>
       <c r="G37" s="2"/>
       <c r="H37" s="2"/>
     </row>
@@ -2389,7 +2590,6 @@
       <c r="A38" s="1"/>
       <c r="B38" s="2"/>
       <c r="E38" s="3"/>
-      <c r="F38" s="4"/>
       <c r="G38" s="2"/>
       <c r="H38" s="2"/>
     </row>
@@ -2397,7 +2597,6 @@
       <c r="A39" s="1"/>
       <c r="B39" s="2"/>
       <c r="E39" s="3"/>
-      <c r="F39" s="4"/>
       <c r="G39" s="2"/>
       <c r="H39" s="2"/>
     </row>
@@ -2405,7 +2604,6 @@
       <c r="A40" s="1"/>
       <c r="B40" s="2"/>
       <c r="E40" s="3"/>
-      <c r="F40" s="4"/>
       <c r="G40" s="2"/>
       <c r="H40" s="2"/>
     </row>
@@ -2413,7 +2611,6 @@
       <c r="A41" s="1"/>
       <c r="B41" s="2"/>
       <c r="E41" s="3"/>
-      <c r="F41" s="4"/>
       <c r="G41" s="2"/>
       <c r="H41" s="2"/>
     </row>
@@ -2421,7 +2618,6 @@
       <c r="A42" s="1"/>
       <c r="B42" s="2"/>
       <c r="E42" s="3"/>
-      <c r="F42" s="4"/>
       <c r="G42" s="2"/>
       <c r="H42" s="2"/>
     </row>
@@ -2429,7 +2625,6 @@
       <c r="A43" s="1"/>
       <c r="B43" s="2"/>
       <c r="E43" s="3"/>
-      <c r="F43" s="4"/>
       <c r="G43" s="2"/>
       <c r="H43" s="2"/>
     </row>
@@ -2437,7 +2632,6 @@
       <c r="A44" s="1"/>
       <c r="B44" s="2"/>
       <c r="E44" s="3"/>
-      <c r="F44" s="4"/>
       <c r="G44" s="2"/>
       <c r="H44" s="2"/>
     </row>
@@ -2445,7 +2639,6 @@
       <c r="A45" s="1"/>
       <c r="B45" s="2"/>
       <c r="E45" s="3"/>
-      <c r="F45" s="4"/>
       <c r="G45" s="2"/>
       <c r="H45" s="2"/>
     </row>
@@ -2453,7 +2646,6 @@
       <c r="A46" s="1"/>
       <c r="B46" s="2"/>
       <c r="E46" s="3"/>
-      <c r="F46" s="4"/>
       <c r="G46" s="2"/>
       <c r="H46" s="2"/>
     </row>
@@ -2461,7 +2653,6 @@
       <c r="A47" s="1"/>
       <c r="B47" s="2"/>
       <c r="E47" s="3"/>
-      <c r="F47" s="4"/>
       <c r="G47" s="2"/>
       <c r="H47" s="2"/>
     </row>
@@ -2469,7 +2660,6 @@
       <c r="A48" s="1"/>
       <c r="B48" s="2"/>
       <c r="E48" s="3"/>
-      <c r="F48" s="4"/>
       <c r="G48" s="2"/>
       <c r="H48" s="2"/>
     </row>
@@ -2477,7 +2667,6 @@
       <c r="A49" s="1"/>
       <c r="B49" s="2"/>
       <c r="E49" s="3"/>
-      <c r="F49" s="4"/>
       <c r="G49" s="2"/>
       <c r="H49" s="2"/>
     </row>
@@ -2485,7 +2674,6 @@
       <c r="A50" s="1"/>
       <c r="B50" s="2"/>
       <c r="E50" s="3"/>
-      <c r="F50" s="4"/>
       <c r="G50" s="2"/>
       <c r="H50" s="2"/>
     </row>
@@ -2493,7 +2681,6 @@
       <c r="A51" s="1"/>
       <c r="B51" s="2"/>
       <c r="E51" s="3"/>
-      <c r="F51" s="4"/>
       <c r="G51" s="2"/>
       <c r="H51" s="2"/>
     </row>
@@ -2501,7 +2688,6 @@
       <c r="A52" s="1"/>
       <c r="B52" s="2"/>
       <c r="E52" s="3"/>
-      <c r="F52" s="4"/>
       <c r="G52" s="2"/>
       <c r="H52" s="2"/>
     </row>
@@ -2509,7 +2695,6 @@
       <c r="A53" s="1"/>
       <c r="B53" s="2"/>
       <c r="E53" s="3"/>
-      <c r="F53" s="4"/>
       <c r="G53" s="2"/>
       <c r="H53" s="2"/>
     </row>
@@ -2517,7 +2702,6 @@
       <c r="A54" s="1"/>
       <c r="B54" s="2"/>
       <c r="E54" s="3"/>
-      <c r="F54" s="4"/>
       <c r="G54" s="2"/>
       <c r="H54" s="2"/>
     </row>
@@ -2525,7 +2709,6 @@
       <c r="A55" s="1"/>
       <c r="B55" s="2"/>
       <c r="E55" s="3"/>
-      <c r="F55" s="4"/>
       <c r="G55" s="2"/>
       <c r="H55" s="2"/>
     </row>
@@ -2533,7 +2716,6 @@
       <c r="A56" s="1"/>
       <c r="B56" s="2"/>
       <c r="E56" s="3"/>
-      <c r="F56" s="4"/>
       <c r="G56" s="2"/>
       <c r="H56" s="2"/>
     </row>
@@ -2541,7 +2723,6 @@
       <c r="A57" s="1"/>
       <c r="B57" s="2"/>
       <c r="E57" s="3"/>
-      <c r="F57" s="4"/>
       <c r="G57" s="2"/>
       <c r="H57" s="2"/>
     </row>
@@ -2549,7 +2730,6 @@
       <c r="A58" s="1"/>
       <c r="B58" s="2"/>
       <c r="E58" s="3"/>
-      <c r="F58" s="4"/>
       <c r="G58" s="2"/>
       <c r="H58" s="2"/>
     </row>
@@ -2557,7 +2737,6 @@
       <c r="A59" s="1"/>
       <c r="B59" s="2"/>
       <c r="E59" s="3"/>
-      <c r="F59" s="4"/>
       <c r="G59" s="2"/>
       <c r="H59" s="2"/>
     </row>
@@ -2565,7 +2744,6 @@
       <c r="A60" s="1"/>
       <c r="B60" s="2"/>
       <c r="E60" s="3"/>
-      <c r="F60" s="4"/>
       <c r="G60" s="2"/>
       <c r="H60" s="2"/>
     </row>
@@ -2573,7 +2751,6 @@
       <c r="A61" s="1"/>
       <c r="B61" s="2"/>
       <c r="E61" s="3"/>
-      <c r="F61" s="4"/>
       <c r="G61" s="2"/>
       <c r="H61" s="2"/>
     </row>
@@ -2581,7 +2758,6 @@
       <c r="A62" s="1"/>
       <c r="B62" s="2"/>
       <c r="E62" s="3"/>
-      <c r="F62" s="4"/>
       <c r="G62" s="2"/>
       <c r="H62" s="2"/>
     </row>
@@ -2589,7 +2765,6 @@
       <c r="A63" s="1"/>
       <c r="B63" s="2"/>
       <c r="E63" s="3"/>
-      <c r="F63" s="4"/>
       <c r="G63" s="2"/>
       <c r="H63" s="2"/>
     </row>
@@ -2597,7 +2772,6 @@
       <c r="A64" s="1"/>
       <c r="B64" s="2"/>
       <c r="E64" s="3"/>
-      <c r="F64" s="4"/>
       <c r="G64" s="2"/>
       <c r="H64" s="2"/>
     </row>
@@ -2605,7 +2779,6 @@
       <c r="A65" s="1"/>
       <c r="B65" s="2"/>
       <c r="E65" s="3"/>
-      <c r="F65" s="4"/>
       <c r="G65" s="2"/>
       <c r="H65" s="2"/>
     </row>
@@ -2613,7 +2786,6 @@
       <c r="A66" s="1"/>
       <c r="B66" s="2"/>
       <c r="E66" s="3"/>
-      <c r="F66" s="4"/>
       <c r="G66" s="2"/>
       <c r="H66" s="2"/>
     </row>
@@ -2621,7 +2793,6 @@
       <c r="A67" s="1"/>
       <c r="B67" s="2"/>
       <c r="E67" s="3"/>
-      <c r="F67" s="4"/>
       <c r="G67" s="2"/>
       <c r="H67" s="2"/>
     </row>
@@ -2629,7 +2800,6 @@
       <c r="A68" s="1"/>
       <c r="B68" s="2"/>
       <c r="E68" s="3"/>
-      <c r="F68" s="4"/>
       <c r="G68" s="2"/>
       <c r="H68" s="2"/>
     </row>
@@ -2637,7 +2807,6 @@
       <c r="A69" s="1"/>
       <c r="B69" s="2"/>
       <c r="E69" s="3"/>
-      <c r="F69" s="4"/>
       <c r="G69" s="2"/>
       <c r="H69" s="2"/>
     </row>
@@ -2645,7 +2814,6 @@
       <c r="A70" s="1"/>
       <c r="B70" s="2"/>
       <c r="E70" s="3"/>
-      <c r="F70" s="4"/>
       <c r="G70" s="2"/>
       <c r="H70" s="2"/>
     </row>
@@ -2653,7 +2821,6 @@
       <c r="A71" s="1"/>
       <c r="B71" s="2"/>
       <c r="E71" s="3"/>
-      <c r="F71" s="4"/>
       <c r="G71" s="2"/>
       <c r="H71" s="2"/>
     </row>
@@ -2661,7 +2828,6 @@
       <c r="A72" s="1"/>
       <c r="B72" s="2"/>
       <c r="E72" s="3"/>
-      <c r="F72" s="4"/>
       <c r="G72" s="2"/>
       <c r="H72" s="2"/>
     </row>
@@ -2669,7 +2835,6 @@
       <c r="A73" s="1"/>
       <c r="B73" s="2"/>
       <c r="E73" s="3"/>
-      <c r="F73" s="4"/>
       <c r="G73" s="2"/>
       <c r="H73" s="2"/>
     </row>
@@ -2677,7 +2842,6 @@
       <c r="A74" s="1"/>
       <c r="B74" s="2"/>
       <c r="E74" s="3"/>
-      <c r="F74" s="4"/>
       <c r="G74" s="2"/>
       <c r="H74" s="2"/>
     </row>
@@ -2685,7 +2849,6 @@
       <c r="A75" s="1"/>
       <c r="B75" s="2"/>
       <c r="E75" s="3"/>
-      <c r="F75" s="4"/>
       <c r="G75" s="2"/>
       <c r="H75" s="2"/>
     </row>
@@ -2693,7 +2856,6 @@
       <c r="A76" s="1"/>
       <c r="B76" s="2"/>
       <c r="E76" s="3"/>
-      <c r="F76" s="4"/>
       <c r="G76" s="2"/>
       <c r="H76" s="2"/>
     </row>
@@ -2701,7 +2863,6 @@
       <c r="A77" s="1"/>
       <c r="B77" s="2"/>
       <c r="E77" s="3"/>
-      <c r="F77" s="4"/>
       <c r="G77" s="2"/>
       <c r="H77" s="2"/>
     </row>
@@ -2709,7 +2870,6 @@
       <c r="A78" s="1"/>
       <c r="B78" s="2"/>
       <c r="E78" s="3"/>
-      <c r="F78" s="4"/>
       <c r="G78" s="2"/>
       <c r="H78" s="2"/>
     </row>
@@ -2717,7 +2877,6 @@
       <c r="A79" s="1"/>
       <c r="B79" s="2"/>
       <c r="E79" s="3"/>
-      <c r="F79" s="4"/>
       <c r="G79" s="2"/>
       <c r="H79" s="2"/>
     </row>
@@ -2725,7 +2884,6 @@
       <c r="A80" s="1"/>
       <c r="B80" s="2"/>
       <c r="E80" s="3"/>
-      <c r="F80" s="4"/>
       <c r="G80" s="2"/>
       <c r="H80" s="2"/>
     </row>
@@ -2733,7 +2891,6 @@
       <c r="A81" s="1"/>
       <c r="B81" s="2"/>
       <c r="E81" s="3"/>
-      <c r="F81" s="4"/>
       <c r="G81" s="2"/>
       <c r="H81" s="2"/>
     </row>
@@ -2741,7 +2898,6 @@
       <c r="A82" s="1"/>
       <c r="B82" s="2"/>
       <c r="E82" s="3"/>
-      <c r="F82" s="4"/>
       <c r="G82" s="2"/>
       <c r="H82" s="2"/>
     </row>
@@ -2749,7 +2905,6 @@
       <c r="A83" s="1"/>
       <c r="B83" s="2"/>
       <c r="E83" s="3"/>
-      <c r="F83" s="4"/>
       <c r="G83" s="2"/>
       <c r="H83" s="2"/>
     </row>
@@ -2757,7 +2912,6 @@
       <c r="A84" s="1"/>
       <c r="B84" s="2"/>
       <c r="E84" s="3"/>
-      <c r="F84" s="4"/>
       <c r="G84" s="2"/>
       <c r="H84" s="2"/>
     </row>
@@ -2765,7 +2919,6 @@
       <c r="A85" s="1"/>
       <c r="B85" s="2"/>
       <c r="E85" s="3"/>
-      <c r="F85" s="4"/>
       <c r="G85" s="2"/>
       <c r="H85" s="2"/>
     </row>
@@ -2773,7 +2926,6 @@
       <c r="A86" s="1"/>
       <c r="B86" s="2"/>
       <c r="E86" s="3"/>
-      <c r="F86" s="4"/>
       <c r="G86" s="2"/>
       <c r="H86" s="2"/>
     </row>
@@ -2781,7 +2933,6 @@
       <c r="A87" s="1"/>
       <c r="B87" s="2"/>
       <c r="E87" s="3"/>
-      <c r="F87" s="4"/>
       <c r="G87" s="2"/>
       <c r="H87" s="2"/>
     </row>
@@ -2789,7 +2940,6 @@
       <c r="A88" s="1"/>
       <c r="B88" s="2"/>
       <c r="E88" s="3"/>
-      <c r="F88" s="4"/>
       <c r="G88" s="2"/>
       <c r="H88" s="2"/>
     </row>
@@ -2797,7 +2947,6 @@
       <c r="A89" s="1"/>
       <c r="B89" s="2"/>
       <c r="E89" s="3"/>
-      <c r="F89" s="4"/>
       <c r="G89" s="2"/>
       <c r="H89" s="2"/>
     </row>
@@ -2805,7 +2954,6 @@
       <c r="A90" s="1"/>
       <c r="B90" s="2"/>
       <c r="E90" s="3"/>
-      <c r="F90" s="4"/>
       <c r="G90" s="2"/>
       <c r="H90" s="2"/>
     </row>
@@ -2813,7 +2961,6 @@
       <c r="A91" s="1"/>
       <c r="B91" s="2"/>
       <c r="E91" s="3"/>
-      <c r="F91" s="4"/>
       <c r="G91" s="2"/>
       <c r="H91" s="2"/>
     </row>
@@ -2821,7 +2968,6 @@
       <c r="A92" s="1"/>
       <c r="B92" s="2"/>
       <c r="E92" s="3"/>
-      <c r="F92" s="4"/>
       <c r="G92" s="2"/>
       <c r="H92" s="2"/>
     </row>
@@ -2829,7 +2975,6 @@
       <c r="A93" s="1"/>
       <c r="B93" s="2"/>
       <c r="E93" s="3"/>
-      <c r="F93" s="4"/>
       <c r="G93" s="2"/>
       <c r="H93" s="2"/>
     </row>
@@ -2837,7 +2982,6 @@
       <c r="A94" s="1"/>
       <c r="B94" s="2"/>
       <c r="E94" s="3"/>
-      <c r="F94" s="4"/>
       <c r="G94" s="2"/>
       <c r="H94" s="2"/>
     </row>
@@ -2845,7 +2989,6 @@
       <c r="A95" s="1"/>
       <c r="B95" s="2"/>
       <c r="E95" s="3"/>
-      <c r="F95" s="4"/>
       <c r="G95" s="2"/>
       <c r="H95" s="2"/>
     </row>
@@ -2853,7 +2996,6 @@
       <c r="A96" s="1"/>
       <c r="B96" s="2"/>
       <c r="E96" s="3"/>
-      <c r="F96" s="4"/>
       <c r="G96" s="2"/>
       <c r="H96" s="2"/>
     </row>
@@ -2861,7 +3003,6 @@
       <c r="A97" s="1"/>
       <c r="B97" s="2"/>
       <c r="E97" s="3"/>
-      <c r="F97" s="4"/>
       <c r="G97" s="2"/>
       <c r="H97" s="2"/>
     </row>
@@ -2869,7 +3010,6 @@
       <c r="A98" s="1"/>
       <c r="B98" s="2"/>
       <c r="E98" s="3"/>
-      <c r="F98" s="4"/>
       <c r="G98" s="2"/>
       <c r="H98" s="2"/>
     </row>
@@ -2877,7 +3017,6 @@
       <c r="A99" s="1"/>
       <c r="B99" s="2"/>
       <c r="E99" s="3"/>
-      <c r="F99" s="4"/>
       <c r="G99" s="2"/>
       <c r="H99" s="2"/>
     </row>
@@ -2885,7 +3024,6 @@
       <c r="A100" s="1"/>
       <c r="B100" s="2"/>
       <c r="E100" s="3"/>
-      <c r="F100" s="4"/>
       <c r="G100" s="2"/>
       <c r="H100" s="2"/>
     </row>
@@ -2908,7 +3046,7 @@
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <ignoredErrors>
-    <ignoredError sqref="D2:D100" listDataValidation="1"/>
+    <ignoredError sqref="D8:D100" listDataValidation="1"/>
   </ignoredErrors>
   <tableParts count="1">
     <tablePart r:id="rId1"/>

</xml_diff>

<commit_message>
Add/update progress report for 19/05/2025 Mon by Shivya
</commit_message>
<xml_diff>
--- a/PR&IR.xlsx
+++ b/PR&IR.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28623"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26026"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\avichal avneel nath\Documents\Semester 7\CS415\A3\CS415_A3\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SHIVYA KUMAR\Desktop\new415\CS415_A3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{265B2D53-2233-42DA-BDE7-A3000AC9A528}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D10B44C-54A7-4F21-8F22-614AAAF0B8A7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{BFA1E21A-08FA-4F02-8C25-33C81C8EE970}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{BFA1E21A-08FA-4F02-8C25-33C81C8EE970}"/>
   </bookViews>
   <sheets>
     <sheet name="Avichal" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="83">
   <si>
     <t>Date</t>
   </si>
@@ -296,6 +296,12 @@
   <si>
     <t>Port configuration</t>
   </si>
+  <si>
+    <t>Initiated my microservice</t>
+  </si>
+  <si>
+    <t>Sick, too much workloads in other units</t>
+  </si>
 </sst>
 </file>
 
@@ -305,7 +311,7 @@
     <numFmt numFmtId="164" formatCode="h"/>
     <numFmt numFmtId="165" formatCode="d/mm/yyyy;@"/>
   </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="3">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1041,30 +1047,30 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{37EAA098-74C6-4411-B7E2-26AD2DCBC3F0}">
   <dimension ref="A1:H28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
+    <sheetView topLeftCell="A5" workbookViewId="0">
       <selection activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="10.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.5703125" style="2" customWidth="1"/>
+    <col min="1" max="1" width="10.44140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.5546875" style="2" customWidth="1"/>
     <col min="3" max="3" width="58" customWidth="1"/>
-    <col min="5" max="5" width="13.140625" style="3" customWidth="1"/>
-    <col min="6" max="6" width="20.85546875" style="4" customWidth="1"/>
-    <col min="7" max="7" width="34.85546875" style="2" customWidth="1"/>
-    <col min="8" max="8" width="43.42578125" style="2" customWidth="1"/>
-    <col min="11" max="11" width="9.140625" customWidth="1"/>
-    <col min="12" max="12" width="13.28515625" customWidth="1"/>
-    <col min="13" max="13" width="11.42578125" customWidth="1"/>
-    <col min="14" max="14" width="17.42578125" customWidth="1"/>
-    <col min="16" max="16" width="9.140625" customWidth="1"/>
-    <col min="18" max="18" width="16.5703125" customWidth="1"/>
-    <col min="19" max="19" width="14.7109375" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="16.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.109375" style="3" customWidth="1"/>
+    <col min="6" max="6" width="20.88671875" style="4" customWidth="1"/>
+    <col min="7" max="7" width="34.88671875" style="2" customWidth="1"/>
+    <col min="8" max="8" width="43.44140625" style="2" customWidth="1"/>
+    <col min="11" max="11" width="9.109375" customWidth="1"/>
+    <col min="12" max="12" width="13.33203125" customWidth="1"/>
+    <col min="13" max="13" width="11.44140625" customWidth="1"/>
+    <col min="14" max="14" width="17.44140625" customWidth="1"/>
+    <col min="16" max="16" width="9.109375" customWidth="1"/>
+    <col min="18" max="18" width="16.5546875" customWidth="1"/>
+    <col min="19" max="19" width="14.6640625" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="16.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" ht="15.6">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
@@ -1090,7 +1096,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="15.75" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:8">
       <c r="A2" s="1">
         <v>45786</v>
       </c>
@@ -1116,7 +1122,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="3" spans="1:8" ht="120" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" ht="115.2">
       <c r="A3" s="1">
         <v>45787</v>
       </c>
@@ -1139,7 +1145,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8">
       <c r="A4" s="1">
         <v>45788</v>
       </c>
@@ -1159,7 +1165,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="5" spans="1:8" ht="76.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" ht="76.5" customHeight="1">
       <c r="A5" s="1">
         <v>45789</v>
       </c>
@@ -1182,7 +1188,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8">
       <c r="A6" s="1">
         <v>45790</v>
       </c>
@@ -1205,7 +1211,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8">
       <c r="A7" s="1">
         <v>45791</v>
       </c>
@@ -1228,7 +1234,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8">
       <c r="A8" s="1">
         <v>45792</v>
       </c>
@@ -1251,7 +1257,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8">
       <c r="A9" s="1">
         <v>45793</v>
       </c>
@@ -1271,7 +1277,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8">
       <c r="A10" s="1">
         <v>45794</v>
       </c>
@@ -1291,7 +1297,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8">
       <c r="A11" s="1">
         <v>45795</v>
       </c>
@@ -1311,7 +1317,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8">
       <c r="A12" s="1">
         <v>45796</v>
       </c>
@@ -1331,56 +1337,56 @@
         <v>78</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8">
       <c r="E13"/>
       <c r="F13"/>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8">
       <c r="E14"/>
       <c r="F14"/>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8">
       <c r="E15"/>
       <c r="F15"/>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8">
       <c r="E16"/>
       <c r="F16"/>
     </row>
-    <row r="17" spans="6:6" x14ac:dyDescent="0.25">
+    <row r="17" spans="6:6">
       <c r="F17"/>
     </row>
-    <row r="18" spans="6:6" x14ac:dyDescent="0.25">
+    <row r="18" spans="6:6">
       <c r="F18"/>
     </row>
-    <row r="19" spans="6:6" x14ac:dyDescent="0.25">
+    <row r="19" spans="6:6">
       <c r="F19"/>
     </row>
-    <row r="20" spans="6:6" x14ac:dyDescent="0.25">
+    <row r="20" spans="6:6">
       <c r="F20"/>
     </row>
-    <row r="21" spans="6:6" x14ac:dyDescent="0.25">
+    <row r="21" spans="6:6">
       <c r="F21"/>
     </row>
-    <row r="22" spans="6:6" x14ac:dyDescent="0.25">
+    <row r="22" spans="6:6">
       <c r="F22"/>
     </row>
-    <row r="23" spans="6:6" x14ac:dyDescent="0.25">
+    <row r="23" spans="6:6">
       <c r="F23"/>
     </row>
-    <row r="24" spans="6:6" x14ac:dyDescent="0.25">
+    <row r="24" spans="6:6">
       <c r="F24"/>
     </row>
-    <row r="25" spans="6:6" x14ac:dyDescent="0.25">
+    <row r="25" spans="6:6">
       <c r="F25"/>
     </row>
-    <row r="26" spans="6:6" x14ac:dyDescent="0.25">
+    <row r="26" spans="6:6">
       <c r="F26"/>
     </row>
-    <row r="27" spans="6:6" x14ac:dyDescent="0.25">
+    <row r="27" spans="6:6">
       <c r="F27"/>
     </row>
-    <row r="28" spans="6:6" x14ac:dyDescent="0.25">
+    <row r="28" spans="6:6">
       <c r="F28"/>
     </row>
   </sheetData>
@@ -1415,23 +1421,23 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3BDA6702-5DDF-42FB-988E-13FBEB26F5C9}">
   <dimension ref="A1:H100"/>
   <sheetViews>
-    <sheetView topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H7" sqref="H7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="9.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="17.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="55.5703125" customWidth="1"/>
-    <col min="4" max="4" width="10.5703125" customWidth="1"/>
-    <col min="5" max="5" width="14.85546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14.28515625" customWidth="1"/>
-    <col min="7" max="7" width="92.85546875" customWidth="1"/>
-    <col min="8" max="8" width="82.42578125" customWidth="1"/>
+    <col min="1" max="1" width="10.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="55.5546875" customWidth="1"/>
+    <col min="4" max="4" width="10.5546875" customWidth="1"/>
+    <col min="5" max="5" width="14.88671875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.33203125" customWidth="1"/>
+    <col min="7" max="7" width="92.88671875" customWidth="1"/>
+    <col min="8" max="8" width="82.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" ht="15.6">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
@@ -1457,7 +1463,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8">
       <c r="A2" s="8">
         <v>45786</v>
       </c>
@@ -1483,7 +1489,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8">
       <c r="A3" s="8">
         <v>45787</v>
       </c>
@@ -1509,7 +1515,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8">
       <c r="A4" s="8">
         <v>45789</v>
       </c>
@@ -1533,7 +1539,7 @@
       </c>
       <c r="H4" s="2"/>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8">
       <c r="A5" s="8">
         <v>45790</v>
       </c>
@@ -1557,7 +1563,7 @@
       </c>
       <c r="H5" s="2"/>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8">
       <c r="A6" s="8">
         <v>45791</v>
       </c>
@@ -1583,565 +1589,583 @@
         <v>49</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A7" s="8"/>
-      <c r="B7" s="2"/>
+    <row r="7" spans="1:8">
+      <c r="A7" s="8">
+        <v>45795</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="C7" t="s">
+        <v>81</v>
+      </c>
+      <c r="D7" t="s">
+        <v>17</v>
+      </c>
+      <c r="E7">
+        <v>100</v>
+      </c>
+      <c r="F7">
+        <v>5</v>
+      </c>
       <c r="G7" s="2"/>
-      <c r="H7" s="2"/>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H7" s="2" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8">
       <c r="A8" s="8"/>
       <c r="B8" s="2"/>
       <c r="G8" s="2"/>
       <c r="H8" s="2"/>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8">
       <c r="A9" s="8"/>
       <c r="B9" s="2"/>
       <c r="G9" s="2"/>
       <c r="H9" s="2"/>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8">
       <c r="A10" s="8"/>
       <c r="B10" s="2"/>
       <c r="G10" s="2"/>
       <c r="H10" s="2"/>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8">
       <c r="A11" s="8"/>
       <c r="B11" s="2"/>
       <c r="G11" s="2"/>
       <c r="H11" s="2"/>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8">
       <c r="A12" s="8"/>
       <c r="B12" s="2"/>
       <c r="G12" s="2"/>
       <c r="H12" s="2"/>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8">
       <c r="A13" s="8"/>
       <c r="B13" s="2"/>
       <c r="G13" s="2"/>
       <c r="H13" s="2"/>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8">
       <c r="A14" s="8"/>
       <c r="B14" s="2"/>
       <c r="G14" s="2"/>
       <c r="H14" s="2"/>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8">
       <c r="A15" s="8"/>
       <c r="B15" s="2"/>
       <c r="G15" s="2"/>
       <c r="H15" s="2"/>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8">
       <c r="A16" s="8"/>
       <c r="B16" s="2"/>
       <c r="G16" s="2"/>
       <c r="H16" s="2"/>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:8">
       <c r="A17" s="8"/>
       <c r="B17" s="2"/>
       <c r="G17" s="2"/>
       <c r="H17" s="2"/>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:8">
       <c r="A18" s="8"/>
       <c r="B18" s="2"/>
       <c r="G18" s="2"/>
       <c r="H18" s="2"/>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:8">
       <c r="A19" s="8"/>
       <c r="B19" s="2"/>
       <c r="G19" s="2"/>
       <c r="H19" s="2"/>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:8">
       <c r="A20" s="8"/>
       <c r="B20" s="2"/>
       <c r="G20" s="2"/>
       <c r="H20" s="2"/>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:8">
       <c r="A21" s="8"/>
       <c r="B21" s="2"/>
       <c r="G21" s="2"/>
       <c r="H21" s="2"/>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:8">
       <c r="A22" s="8"/>
       <c r="B22" s="2"/>
       <c r="G22" s="2"/>
       <c r="H22" s="2"/>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:8">
       <c r="A23" s="8"/>
       <c r="B23" s="2"/>
       <c r="G23" s="2"/>
       <c r="H23" s="2"/>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:8">
       <c r="A24" s="8"/>
       <c r="B24" s="2"/>
       <c r="G24" s="2"/>
       <c r="H24" s="2"/>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:8">
       <c r="A25" s="8"/>
       <c r="B25" s="2"/>
       <c r="G25" s="2"/>
       <c r="H25" s="2"/>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:8">
       <c r="A26" s="8"/>
       <c r="B26" s="2"/>
       <c r="G26" s="2"/>
       <c r="H26" s="2"/>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:8">
       <c r="A27" s="8"/>
       <c r="B27" s="2"/>
       <c r="G27" s="2"/>
       <c r="H27" s="2"/>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:8">
       <c r="A28" s="8"/>
       <c r="B28" s="2"/>
       <c r="G28" s="2"/>
       <c r="H28" s="2"/>
     </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:8">
       <c r="A29" s="8"/>
       <c r="B29" s="2"/>
       <c r="G29" s="2"/>
       <c r="H29" s="2"/>
     </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:8">
       <c r="A30" s="8"/>
       <c r="B30" s="2"/>
       <c r="G30" s="2"/>
       <c r="H30" s="2"/>
     </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:8">
       <c r="A31" s="8"/>
       <c r="B31" s="2"/>
       <c r="G31" s="2"/>
       <c r="H31" s="2"/>
     </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:8">
       <c r="A32" s="8"/>
       <c r="B32" s="2"/>
       <c r="G32" s="2"/>
       <c r="H32" s="2"/>
     </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:8">
       <c r="A33" s="8"/>
       <c r="B33" s="2"/>
       <c r="G33" s="2"/>
       <c r="H33" s="2"/>
     </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:8">
       <c r="A34" s="8"/>
       <c r="B34" s="2"/>
       <c r="G34" s="2"/>
       <c r="H34" s="2"/>
     </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:8">
       <c r="A35" s="8"/>
       <c r="B35" s="2"/>
       <c r="G35" s="2"/>
       <c r="H35" s="2"/>
     </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:8">
       <c r="A36" s="8"/>
       <c r="B36" s="2"/>
       <c r="G36" s="2"/>
       <c r="H36" s="2"/>
     </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:8">
       <c r="A37" s="8"/>
       <c r="B37" s="2"/>
       <c r="G37" s="2"/>
       <c r="H37" s="2"/>
     </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:8">
       <c r="A38" s="8"/>
       <c r="B38" s="2"/>
       <c r="G38" s="2"/>
       <c r="H38" s="2"/>
     </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:8">
       <c r="A39" s="8"/>
       <c r="B39" s="2"/>
       <c r="G39" s="2"/>
       <c r="H39" s="2"/>
     </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:8">
       <c r="A40" s="8"/>
       <c r="B40" s="2"/>
       <c r="G40" s="2"/>
       <c r="H40" s="2"/>
     </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:8">
       <c r="A41" s="8"/>
       <c r="B41" s="2"/>
       <c r="G41" s="2"/>
       <c r="H41" s="2"/>
     </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:8">
       <c r="A42" s="8"/>
       <c r="B42" s="2"/>
       <c r="G42" s="2"/>
       <c r="H42" s="2"/>
     </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:8">
       <c r="A43" s="8"/>
       <c r="B43" s="2"/>
       <c r="G43" s="2"/>
       <c r="H43" s="2"/>
     </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:8">
       <c r="A44" s="8"/>
       <c r="B44" s="2"/>
       <c r="G44" s="2"/>
       <c r="H44" s="2"/>
     </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:8">
       <c r="A45" s="8"/>
       <c r="B45" s="2"/>
       <c r="G45" s="2"/>
       <c r="H45" s="2"/>
     </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:8">
       <c r="A46" s="8"/>
       <c r="B46" s="2"/>
       <c r="G46" s="2"/>
       <c r="H46" s="2"/>
     </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:8">
       <c r="A47" s="8"/>
       <c r="B47" s="2"/>
       <c r="G47" s="2"/>
       <c r="H47" s="2"/>
     </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:8">
       <c r="A48" s="8"/>
       <c r="B48" s="2"/>
       <c r="G48" s="2"/>
       <c r="H48" s="2"/>
     </row>
-    <row r="49" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:8">
       <c r="A49" s="8"/>
       <c r="B49" s="2"/>
       <c r="G49" s="2"/>
       <c r="H49" s="2"/>
     </row>
-    <row r="50" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:8">
       <c r="A50" s="8"/>
       <c r="B50" s="2"/>
       <c r="G50" s="2"/>
       <c r="H50" s="2"/>
     </row>
-    <row r="51" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:8">
       <c r="A51" s="8"/>
       <c r="B51" s="2"/>
       <c r="G51" s="2"/>
       <c r="H51" s="2"/>
     </row>
-    <row r="52" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:8">
       <c r="A52" s="8"/>
       <c r="B52" s="2"/>
       <c r="G52" s="2"/>
       <c r="H52" s="2"/>
     </row>
-    <row r="53" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:8">
       <c r="A53" s="8"/>
       <c r="B53" s="2"/>
       <c r="G53" s="2"/>
       <c r="H53" s="2"/>
     </row>
-    <row r="54" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:8">
       <c r="A54" s="8"/>
       <c r="B54" s="2"/>
       <c r="G54" s="2"/>
       <c r="H54" s="2"/>
     </row>
-    <row r="55" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:8">
       <c r="A55" s="8"/>
       <c r="B55" s="2"/>
       <c r="G55" s="2"/>
       <c r="H55" s="2"/>
     </row>
-    <row r="56" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:8">
       <c r="A56" s="8"/>
       <c r="B56" s="2"/>
       <c r="G56" s="2"/>
       <c r="H56" s="2"/>
     </row>
-    <row r="57" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:8">
       <c r="A57" s="8"/>
       <c r="B57" s="2"/>
       <c r="G57" s="2"/>
       <c r="H57" s="2"/>
     </row>
-    <row r="58" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:8">
       <c r="A58" s="8"/>
       <c r="B58" s="2"/>
       <c r="G58" s="2"/>
       <c r="H58" s="2"/>
     </row>
-    <row r="59" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:8">
       <c r="A59" s="8"/>
       <c r="B59" s="2"/>
       <c r="G59" s="2"/>
       <c r="H59" s="2"/>
     </row>
-    <row r="60" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:8">
       <c r="A60" s="8"/>
       <c r="B60" s="2"/>
       <c r="G60" s="2"/>
       <c r="H60" s="2"/>
     </row>
-    <row r="61" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:8">
       <c r="A61" s="8"/>
       <c r="B61" s="2"/>
       <c r="G61" s="2"/>
       <c r="H61" s="2"/>
     </row>
-    <row r="62" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:8">
       <c r="A62" s="8"/>
       <c r="B62" s="2"/>
       <c r="G62" s="2"/>
       <c r="H62" s="2"/>
     </row>
-    <row r="63" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:8">
       <c r="A63" s="8"/>
       <c r="B63" s="2"/>
       <c r="G63" s="2"/>
       <c r="H63" s="2"/>
     </row>
-    <row r="64" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:8">
       <c r="A64" s="8"/>
       <c r="B64" s="2"/>
       <c r="G64" s="2"/>
       <c r="H64" s="2"/>
     </row>
-    <row r="65" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:8">
       <c r="A65" s="8"/>
       <c r="B65" s="2"/>
       <c r="G65" s="2"/>
       <c r="H65" s="2"/>
     </row>
-    <row r="66" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:8">
       <c r="A66" s="8"/>
       <c r="B66" s="2"/>
       <c r="G66" s="2"/>
       <c r="H66" s="2"/>
     </row>
-    <row r="67" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:8">
       <c r="A67" s="8"/>
       <c r="B67" s="2"/>
       <c r="G67" s="2"/>
       <c r="H67" s="2"/>
     </row>
-    <row r="68" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:8">
       <c r="A68" s="8"/>
       <c r="B68" s="2"/>
       <c r="G68" s="2"/>
       <c r="H68" s="2"/>
     </row>
-    <row r="69" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:8">
       <c r="A69" s="8"/>
       <c r="B69" s="2"/>
       <c r="G69" s="2"/>
       <c r="H69" s="2"/>
     </row>
-    <row r="70" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:8">
       <c r="A70" s="8"/>
       <c r="B70" s="2"/>
       <c r="G70" s="2"/>
       <c r="H70" s="2"/>
     </row>
-    <row r="71" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:8">
       <c r="A71" s="8"/>
       <c r="B71" s="2"/>
       <c r="G71" s="2"/>
       <c r="H71" s="2"/>
     </row>
-    <row r="72" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:8">
       <c r="A72" s="8"/>
       <c r="B72" s="2"/>
       <c r="G72" s="2"/>
       <c r="H72" s="2"/>
     </row>
-    <row r="73" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:8">
       <c r="A73" s="8"/>
       <c r="B73" s="2"/>
       <c r="G73" s="2"/>
       <c r="H73" s="2"/>
     </row>
-    <row r="74" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:8">
       <c r="A74" s="8"/>
       <c r="B74" s="2"/>
       <c r="G74" s="2"/>
       <c r="H74" s="2"/>
     </row>
-    <row r="75" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:8">
       <c r="A75" s="8"/>
       <c r="B75" s="2"/>
       <c r="G75" s="2"/>
       <c r="H75" s="2"/>
     </row>
-    <row r="76" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:8">
       <c r="A76" s="8"/>
       <c r="B76" s="2"/>
       <c r="G76" s="2"/>
       <c r="H76" s="2"/>
     </row>
-    <row r="77" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:8">
       <c r="A77" s="8"/>
       <c r="B77" s="2"/>
       <c r="G77" s="2"/>
       <c r="H77" s="2"/>
     </row>
-    <row r="78" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:8">
       <c r="A78" s="8"/>
       <c r="B78" s="2"/>
       <c r="G78" s="2"/>
       <c r="H78" s="2"/>
     </row>
-    <row r="79" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:8">
       <c r="A79" s="8"/>
       <c r="B79" s="2"/>
       <c r="G79" s="2"/>
       <c r="H79" s="2"/>
     </row>
-    <row r="80" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:8">
       <c r="A80" s="8"/>
       <c r="B80" s="2"/>
       <c r="G80" s="2"/>
       <c r="H80" s="2"/>
     </row>
-    <row r="81" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:8">
       <c r="A81" s="8"/>
       <c r="B81" s="2"/>
       <c r="G81" s="2"/>
       <c r="H81" s="2"/>
     </row>
-    <row r="82" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:8">
       <c r="A82" s="8"/>
       <c r="B82" s="2"/>
       <c r="G82" s="2"/>
       <c r="H82" s="2"/>
     </row>
-    <row r="83" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:8">
       <c r="A83" s="8"/>
       <c r="B83" s="2"/>
       <c r="G83" s="2"/>
       <c r="H83" s="2"/>
     </row>
-    <row r="84" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:8">
       <c r="A84" s="8"/>
       <c r="B84" s="2"/>
       <c r="G84" s="2"/>
       <c r="H84" s="2"/>
     </row>
-    <row r="85" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:8">
       <c r="A85" s="8"/>
       <c r="B85" s="2"/>
       <c r="G85" s="2"/>
       <c r="H85" s="2"/>
     </row>
-    <row r="86" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:8">
       <c r="A86" s="8"/>
       <c r="B86" s="2"/>
       <c r="G86" s="2"/>
       <c r="H86" s="2"/>
     </row>
-    <row r="87" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:8">
       <c r="A87" s="8"/>
       <c r="B87" s="2"/>
       <c r="G87" s="2"/>
       <c r="H87" s="2"/>
     </row>
-    <row r="88" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:8">
       <c r="A88" s="8"/>
       <c r="B88" s="2"/>
       <c r="G88" s="2"/>
       <c r="H88" s="2"/>
     </row>
-    <row r="89" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:8">
       <c r="A89" s="8"/>
       <c r="B89" s="2"/>
       <c r="G89" s="2"/>
       <c r="H89" s="2"/>
     </row>
-    <row r="90" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:8">
       <c r="A90" s="8"/>
       <c r="B90" s="2"/>
       <c r="G90" s="2"/>
       <c r="H90" s="2"/>
     </row>
-    <row r="91" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:8">
       <c r="A91" s="8"/>
       <c r="B91" s="2"/>
       <c r="G91" s="2"/>
       <c r="H91" s="2"/>
     </row>
-    <row r="92" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:8">
       <c r="A92" s="8"/>
       <c r="B92" s="2"/>
       <c r="G92" s="2"/>
       <c r="H92" s="2"/>
     </row>
-    <row r="93" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:8">
       <c r="A93" s="8"/>
       <c r="B93" s="2"/>
       <c r="G93" s="2"/>
       <c r="H93" s="2"/>
     </row>
-    <row r="94" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:8">
       <c r="A94" s="8"/>
       <c r="B94" s="2"/>
       <c r="G94" s="2"/>
       <c r="H94" s="2"/>
     </row>
-    <row r="95" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:8">
       <c r="A95" s="8"/>
       <c r="B95" s="2"/>
       <c r="G95" s="2"/>
       <c r="H95" s="2"/>
     </row>
-    <row r="96" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:8">
       <c r="A96" s="8"/>
       <c r="B96" s="2"/>
       <c r="G96" s="2"/>
       <c r="H96" s="2"/>
     </row>
-    <row r="97" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:8">
       <c r="A97" s="8"/>
       <c r="B97" s="2"/>
       <c r="G97" s="2"/>
       <c r="H97" s="2"/>
     </row>
-    <row r="98" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:8">
       <c r="A98" s="8"/>
       <c r="B98" s="2"/>
       <c r="G98" s="2"/>
       <c r="H98" s="2"/>
     </row>
-    <row r="99" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:8">
       <c r="A99" s="8"/>
       <c r="B99" s="2"/>
       <c r="G99" s="2"/>
       <c r="H99" s="2"/>
     </row>
-    <row r="100" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:8">
       <c r="A100" s="8"/>
       <c r="B100" s="2"/>
       <c r="G100" s="2"/>
@@ -2166,7 +2190,7 @@
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <ignoredErrors>
-    <ignoredError sqref="D7:D100" listDataValidation="1"/>
+    <ignoredError sqref="D8:D100" listDataValidation="1"/>
   </ignoredErrors>
   <tableParts count="1">
     <tablePart r:id="rId1"/>
@@ -2182,19 +2206,19 @@
       <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="9.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="17.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="27.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.85546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="23.5703125" style="10" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="39.140625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="51.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="27.88671875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.88671875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="23.5546875" style="10" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="39.109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="51.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" ht="15.6">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
@@ -2220,7 +2244,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8">
       <c r="A2" s="1">
         <v>45935</v>
       </c>
@@ -2246,7 +2270,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8">
       <c r="A3" s="1">
         <v>45996</v>
       </c>
@@ -2272,7 +2296,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8">
       <c r="A4" s="1" t="s">
         <v>57</v>
       </c>
@@ -2298,7 +2322,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8">
       <c r="A5" s="1" t="s">
         <v>61</v>
       </c>
@@ -2324,7 +2348,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8">
       <c r="A6" s="1" t="s">
         <v>67</v>
       </c>
@@ -2350,7 +2374,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8">
       <c r="A7" s="1" t="s">
         <v>70</v>
       </c>
@@ -2376,651 +2400,651 @@
         <v>54</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8">
       <c r="A8" s="1"/>
       <c r="B8" s="2"/>
       <c r="E8" s="3"/>
       <c r="G8" s="2"/>
       <c r="H8" s="2"/>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8">
       <c r="A9" s="1"/>
       <c r="B9" s="2"/>
       <c r="E9" s="3"/>
       <c r="G9" s="2"/>
       <c r="H9" s="2"/>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8">
       <c r="A10" s="1"/>
       <c r="B10" s="2"/>
       <c r="E10" s="3"/>
       <c r="G10" s="2"/>
       <c r="H10" s="2"/>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8">
       <c r="A11" s="1"/>
       <c r="B11" s="2"/>
       <c r="E11" s="3"/>
       <c r="G11" s="2"/>
       <c r="H11" s="2"/>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8">
       <c r="A12" s="1"/>
       <c r="B12" s="2"/>
       <c r="E12" s="3"/>
       <c r="G12" s="2"/>
       <c r="H12" s="2"/>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8">
       <c r="A13" s="1"/>
       <c r="B13" s="2"/>
       <c r="E13" s="3"/>
       <c r="G13" s="2"/>
       <c r="H13" s="2"/>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8">
       <c r="A14" s="1"/>
       <c r="B14" s="2"/>
       <c r="E14" s="3"/>
       <c r="G14" s="2"/>
       <c r="H14" s="2"/>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8">
       <c r="A15" s="1"/>
       <c r="B15" s="2"/>
       <c r="E15" s="3"/>
       <c r="G15" s="2"/>
       <c r="H15" s="2"/>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8">
       <c r="A16" s="1"/>
       <c r="B16" s="2"/>
       <c r="E16" s="3"/>
       <c r="G16" s="2"/>
       <c r="H16" s="2"/>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:8">
       <c r="A17" s="1"/>
       <c r="B17" s="2"/>
       <c r="E17" s="3"/>
       <c r="G17" s="2"/>
       <c r="H17" s="2"/>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:8">
       <c r="A18" s="1"/>
       <c r="B18" s="2"/>
       <c r="E18" s="3"/>
       <c r="G18" s="2"/>
       <c r="H18" s="2"/>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:8">
       <c r="A19" s="1"/>
       <c r="B19" s="2"/>
       <c r="E19" s="3"/>
       <c r="G19" s="2"/>
       <c r="H19" s="2"/>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:8">
       <c r="A20" s="1"/>
       <c r="B20" s="2"/>
       <c r="E20" s="3"/>
       <c r="G20" s="2"/>
       <c r="H20" s="2"/>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:8">
       <c r="A21" s="1"/>
       <c r="B21" s="2"/>
       <c r="E21" s="3"/>
       <c r="G21" s="2"/>
       <c r="H21" s="2"/>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:8">
       <c r="A22" s="1"/>
       <c r="B22" s="2"/>
       <c r="E22" s="3"/>
       <c r="G22" s="2"/>
       <c r="H22" s="2"/>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:8">
       <c r="A23" s="1"/>
       <c r="B23" s="2"/>
       <c r="E23" s="3"/>
       <c r="G23" s="2"/>
       <c r="H23" s="2"/>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:8">
       <c r="A24" s="1"/>
       <c r="B24" s="2"/>
       <c r="E24" s="3"/>
       <c r="G24" s="2"/>
       <c r="H24" s="2"/>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:8">
       <c r="A25" s="1"/>
       <c r="B25" s="2"/>
       <c r="E25" s="3"/>
       <c r="G25" s="2"/>
       <c r="H25" s="2"/>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:8">
       <c r="A26" s="1"/>
       <c r="B26" s="2"/>
       <c r="E26" s="3"/>
       <c r="G26" s="2"/>
       <c r="H26" s="2"/>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:8">
       <c r="A27" s="1"/>
       <c r="B27" s="2"/>
       <c r="E27" s="3"/>
       <c r="G27" s="2"/>
       <c r="H27" s="2"/>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:8">
       <c r="A28" s="1"/>
       <c r="B28" s="2"/>
       <c r="E28" s="3"/>
       <c r="G28" s="2"/>
       <c r="H28" s="2"/>
     </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:8">
       <c r="A29" s="1"/>
       <c r="B29" s="2"/>
       <c r="E29" s="3"/>
       <c r="G29" s="2"/>
       <c r="H29" s="2"/>
     </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:8">
       <c r="A30" s="1"/>
       <c r="B30" s="2"/>
       <c r="E30" s="3"/>
       <c r="G30" s="2"/>
       <c r="H30" s="2"/>
     </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:8">
       <c r="A31" s="1"/>
       <c r="B31" s="2"/>
       <c r="E31" s="3"/>
       <c r="G31" s="2"/>
       <c r="H31" s="2"/>
     </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:8">
       <c r="A32" s="1"/>
       <c r="B32" s="2"/>
       <c r="E32" s="3"/>
       <c r="G32" s="2"/>
       <c r="H32" s="2"/>
     </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:8">
       <c r="A33" s="1"/>
       <c r="B33" s="2"/>
       <c r="E33" s="3"/>
       <c r="G33" s="2"/>
       <c r="H33" s="2"/>
     </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:8">
       <c r="A34" s="1"/>
       <c r="B34" s="2"/>
       <c r="E34" s="3"/>
       <c r="G34" s="2"/>
       <c r="H34" s="2"/>
     </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:8">
       <c r="A35" s="1"/>
       <c r="B35" s="2"/>
       <c r="E35" s="3"/>
       <c r="G35" s="2"/>
       <c r="H35" s="2"/>
     </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:8">
       <c r="A36" s="1"/>
       <c r="B36" s="2"/>
       <c r="E36" s="3"/>
       <c r="G36" s="2"/>
       <c r="H36" s="2"/>
     </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:8">
       <c r="A37" s="1"/>
       <c r="B37" s="2"/>
       <c r="E37" s="3"/>
       <c r="G37" s="2"/>
       <c r="H37" s="2"/>
     </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:8">
       <c r="A38" s="1"/>
       <c r="B38" s="2"/>
       <c r="E38" s="3"/>
       <c r="G38" s="2"/>
       <c r="H38" s="2"/>
     </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:8">
       <c r="A39" s="1"/>
       <c r="B39" s="2"/>
       <c r="E39" s="3"/>
       <c r="G39" s="2"/>
       <c r="H39" s="2"/>
     </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:8">
       <c r="A40" s="1"/>
       <c r="B40" s="2"/>
       <c r="E40" s="3"/>
       <c r="G40" s="2"/>
       <c r="H40" s="2"/>
     </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:8">
       <c r="A41" s="1"/>
       <c r="B41" s="2"/>
       <c r="E41" s="3"/>
       <c r="G41" s="2"/>
       <c r="H41" s="2"/>
     </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:8">
       <c r="A42" s="1"/>
       <c r="B42" s="2"/>
       <c r="E42" s="3"/>
       <c r="G42" s="2"/>
       <c r="H42" s="2"/>
     </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:8">
       <c r="A43" s="1"/>
       <c r="B43" s="2"/>
       <c r="E43" s="3"/>
       <c r="G43" s="2"/>
       <c r="H43" s="2"/>
     </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:8">
       <c r="A44" s="1"/>
       <c r="B44" s="2"/>
       <c r="E44" s="3"/>
       <c r="G44" s="2"/>
       <c r="H44" s="2"/>
     </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:8">
       <c r="A45" s="1"/>
       <c r="B45" s="2"/>
       <c r="E45" s="3"/>
       <c r="G45" s="2"/>
       <c r="H45" s="2"/>
     </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:8">
       <c r="A46" s="1"/>
       <c r="B46" s="2"/>
       <c r="E46" s="3"/>
       <c r="G46" s="2"/>
       <c r="H46" s="2"/>
     </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:8">
       <c r="A47" s="1"/>
       <c r="B47" s="2"/>
       <c r="E47" s="3"/>
       <c r="G47" s="2"/>
       <c r="H47" s="2"/>
     </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:8">
       <c r="A48" s="1"/>
       <c r="B48" s="2"/>
       <c r="E48" s="3"/>
       <c r="G48" s="2"/>
       <c r="H48" s="2"/>
     </row>
-    <row r="49" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:8">
       <c r="A49" s="1"/>
       <c r="B49" s="2"/>
       <c r="E49" s="3"/>
       <c r="G49" s="2"/>
       <c r="H49" s="2"/>
     </row>
-    <row r="50" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:8">
       <c r="A50" s="1"/>
       <c r="B50" s="2"/>
       <c r="E50" s="3"/>
       <c r="G50" s="2"/>
       <c r="H50" s="2"/>
     </row>
-    <row r="51" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:8">
       <c r="A51" s="1"/>
       <c r="B51" s="2"/>
       <c r="E51" s="3"/>
       <c r="G51" s="2"/>
       <c r="H51" s="2"/>
     </row>
-    <row r="52" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:8">
       <c r="A52" s="1"/>
       <c r="B52" s="2"/>
       <c r="E52" s="3"/>
       <c r="G52" s="2"/>
       <c r="H52" s="2"/>
     </row>
-    <row r="53" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:8">
       <c r="A53" s="1"/>
       <c r="B53" s="2"/>
       <c r="E53" s="3"/>
       <c r="G53" s="2"/>
       <c r="H53" s="2"/>
     </row>
-    <row r="54" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:8">
       <c r="A54" s="1"/>
       <c r="B54" s="2"/>
       <c r="E54" s="3"/>
       <c r="G54" s="2"/>
       <c r="H54" s="2"/>
     </row>
-    <row r="55" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:8">
       <c r="A55" s="1"/>
       <c r="B55" s="2"/>
       <c r="E55" s="3"/>
       <c r="G55" s="2"/>
       <c r="H55" s="2"/>
     </row>
-    <row r="56" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:8">
       <c r="A56" s="1"/>
       <c r="B56" s="2"/>
       <c r="E56" s="3"/>
       <c r="G56" s="2"/>
       <c r="H56" s="2"/>
     </row>
-    <row r="57" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:8">
       <c r="A57" s="1"/>
       <c r="B57" s="2"/>
       <c r="E57" s="3"/>
       <c r="G57" s="2"/>
       <c r="H57" s="2"/>
     </row>
-    <row r="58" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:8">
       <c r="A58" s="1"/>
       <c r="B58" s="2"/>
       <c r="E58" s="3"/>
       <c r="G58" s="2"/>
       <c r="H58" s="2"/>
     </row>
-    <row r="59" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:8">
       <c r="A59" s="1"/>
       <c r="B59" s="2"/>
       <c r="E59" s="3"/>
       <c r="G59" s="2"/>
       <c r="H59" s="2"/>
     </row>
-    <row r="60" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:8">
       <c r="A60" s="1"/>
       <c r="B60" s="2"/>
       <c r="E60" s="3"/>
       <c r="G60" s="2"/>
       <c r="H60" s="2"/>
     </row>
-    <row r="61" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:8">
       <c r="A61" s="1"/>
       <c r="B61" s="2"/>
       <c r="E61" s="3"/>
       <c r="G61" s="2"/>
       <c r="H61" s="2"/>
     </row>
-    <row r="62" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:8">
       <c r="A62" s="1"/>
       <c r="B62" s="2"/>
       <c r="E62" s="3"/>
       <c r="G62" s="2"/>
       <c r="H62" s="2"/>
     </row>
-    <row r="63" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:8">
       <c r="A63" s="1"/>
       <c r="B63" s="2"/>
       <c r="E63" s="3"/>
       <c r="G63" s="2"/>
       <c r="H63" s="2"/>
     </row>
-    <row r="64" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:8">
       <c r="A64" s="1"/>
       <c r="B64" s="2"/>
       <c r="E64" s="3"/>
       <c r="G64" s="2"/>
       <c r="H64" s="2"/>
     </row>
-    <row r="65" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:8">
       <c r="A65" s="1"/>
       <c r="B65" s="2"/>
       <c r="E65" s="3"/>
       <c r="G65" s="2"/>
       <c r="H65" s="2"/>
     </row>
-    <row r="66" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:8">
       <c r="A66" s="1"/>
       <c r="B66" s="2"/>
       <c r="E66" s="3"/>
       <c r="G66" s="2"/>
       <c r="H66" s="2"/>
     </row>
-    <row r="67" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:8">
       <c r="A67" s="1"/>
       <c r="B67" s="2"/>
       <c r="E67" s="3"/>
       <c r="G67" s="2"/>
       <c r="H67" s="2"/>
     </row>
-    <row r="68" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:8">
       <c r="A68" s="1"/>
       <c r="B68" s="2"/>
       <c r="E68" s="3"/>
       <c r="G68" s="2"/>
       <c r="H68" s="2"/>
     </row>
-    <row r="69" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:8">
       <c r="A69" s="1"/>
       <c r="B69" s="2"/>
       <c r="E69" s="3"/>
       <c r="G69" s="2"/>
       <c r="H69" s="2"/>
     </row>
-    <row r="70" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:8">
       <c r="A70" s="1"/>
       <c r="B70" s="2"/>
       <c r="E70" s="3"/>
       <c r="G70" s="2"/>
       <c r="H70" s="2"/>
     </row>
-    <row r="71" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:8">
       <c r="A71" s="1"/>
       <c r="B71" s="2"/>
       <c r="E71" s="3"/>
       <c r="G71" s="2"/>
       <c r="H71" s="2"/>
     </row>
-    <row r="72" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:8">
       <c r="A72" s="1"/>
       <c r="B72" s="2"/>
       <c r="E72" s="3"/>
       <c r="G72" s="2"/>
       <c r="H72" s="2"/>
     </row>
-    <row r="73" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:8">
       <c r="A73" s="1"/>
       <c r="B73" s="2"/>
       <c r="E73" s="3"/>
       <c r="G73" s="2"/>
       <c r="H73" s="2"/>
     </row>
-    <row r="74" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:8">
       <c r="A74" s="1"/>
       <c r="B74" s="2"/>
       <c r="E74" s="3"/>
       <c r="G74" s="2"/>
       <c r="H74" s="2"/>
     </row>
-    <row r="75" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:8">
       <c r="A75" s="1"/>
       <c r="B75" s="2"/>
       <c r="E75" s="3"/>
       <c r="G75" s="2"/>
       <c r="H75" s="2"/>
     </row>
-    <row r="76" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:8">
       <c r="A76" s="1"/>
       <c r="B76" s="2"/>
       <c r="E76" s="3"/>
       <c r="G76" s="2"/>
       <c r="H76" s="2"/>
     </row>
-    <row r="77" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:8">
       <c r="A77" s="1"/>
       <c r="B77" s="2"/>
       <c r="E77" s="3"/>
       <c r="G77" s="2"/>
       <c r="H77" s="2"/>
     </row>
-    <row r="78" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:8">
       <c r="A78" s="1"/>
       <c r="B78" s="2"/>
       <c r="E78" s="3"/>
       <c r="G78" s="2"/>
       <c r="H78" s="2"/>
     </row>
-    <row r="79" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:8">
       <c r="A79" s="1"/>
       <c r="B79" s="2"/>
       <c r="E79" s="3"/>
       <c r="G79" s="2"/>
       <c r="H79" s="2"/>
     </row>
-    <row r="80" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:8">
       <c r="A80" s="1"/>
       <c r="B80" s="2"/>
       <c r="E80" s="3"/>
       <c r="G80" s="2"/>
       <c r="H80" s="2"/>
     </row>
-    <row r="81" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:8">
       <c r="A81" s="1"/>
       <c r="B81" s="2"/>
       <c r="E81" s="3"/>
       <c r="G81" s="2"/>
       <c r="H81" s="2"/>
     </row>
-    <row r="82" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:8">
       <c r="A82" s="1"/>
       <c r="B82" s="2"/>
       <c r="E82" s="3"/>
       <c r="G82" s="2"/>
       <c r="H82" s="2"/>
     </row>
-    <row r="83" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:8">
       <c r="A83" s="1"/>
       <c r="B83" s="2"/>
       <c r="E83" s="3"/>
       <c r="G83" s="2"/>
       <c r="H83" s="2"/>
     </row>
-    <row r="84" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:8">
       <c r="A84" s="1"/>
       <c r="B84" s="2"/>
       <c r="E84" s="3"/>
       <c r="G84" s="2"/>
       <c r="H84" s="2"/>
     </row>
-    <row r="85" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:8">
       <c r="A85" s="1"/>
       <c r="B85" s="2"/>
       <c r="E85" s="3"/>
       <c r="G85" s="2"/>
       <c r="H85" s="2"/>
     </row>
-    <row r="86" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:8">
       <c r="A86" s="1"/>
       <c r="B86" s="2"/>
       <c r="E86" s="3"/>
       <c r="G86" s="2"/>
       <c r="H86" s="2"/>
     </row>
-    <row r="87" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:8">
       <c r="A87" s="1"/>
       <c r="B87" s="2"/>
       <c r="E87" s="3"/>
       <c r="G87" s="2"/>
       <c r="H87" s="2"/>
     </row>
-    <row r="88" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:8">
       <c r="A88" s="1"/>
       <c r="B88" s="2"/>
       <c r="E88" s="3"/>
       <c r="G88" s="2"/>
       <c r="H88" s="2"/>
     </row>
-    <row r="89" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:8">
       <c r="A89" s="1"/>
       <c r="B89" s="2"/>
       <c r="E89" s="3"/>
       <c r="G89" s="2"/>
       <c r="H89" s="2"/>
     </row>
-    <row r="90" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:8">
       <c r="A90" s="1"/>
       <c r="B90" s="2"/>
       <c r="E90" s="3"/>
       <c r="G90" s="2"/>
       <c r="H90" s="2"/>
     </row>
-    <row r="91" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:8">
       <c r="A91" s="1"/>
       <c r="B91" s="2"/>
       <c r="E91" s="3"/>
       <c r="G91" s="2"/>
       <c r="H91" s="2"/>
     </row>
-    <row r="92" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:8">
       <c r="A92" s="1"/>
       <c r="B92" s="2"/>
       <c r="E92" s="3"/>
       <c r="G92" s="2"/>
       <c r="H92" s="2"/>
     </row>
-    <row r="93" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:8">
       <c r="A93" s="1"/>
       <c r="B93" s="2"/>
       <c r="E93" s="3"/>
       <c r="G93" s="2"/>
       <c r="H93" s="2"/>
     </row>
-    <row r="94" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:8">
       <c r="A94" s="1"/>
       <c r="B94" s="2"/>
       <c r="E94" s="3"/>
       <c r="G94" s="2"/>
       <c r="H94" s="2"/>
     </row>
-    <row r="95" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:8">
       <c r="A95" s="1"/>
       <c r="B95" s="2"/>
       <c r="E95" s="3"/>
       <c r="G95" s="2"/>
       <c r="H95" s="2"/>
     </row>
-    <row r="96" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:8">
       <c r="A96" s="1"/>
       <c r="B96" s="2"/>
       <c r="E96" s="3"/>
       <c r="G96" s="2"/>
       <c r="H96" s="2"/>
     </row>
-    <row r="97" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:8">
       <c r="A97" s="1"/>
       <c r="B97" s="2"/>
       <c r="E97" s="3"/>
       <c r="G97" s="2"/>
       <c r="H97" s="2"/>
     </row>
-    <row r="98" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:8">
       <c r="A98" s="1"/>
       <c r="B98" s="2"/>
       <c r="E98" s="3"/>
       <c r="G98" s="2"/>
       <c r="H98" s="2"/>
     </row>
-    <row r="99" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:8">
       <c r="A99" s="1"/>
       <c r="B99" s="2"/>
       <c r="E99" s="3"/>
       <c r="G99" s="2"/>
       <c r="H99" s="2"/>
     </row>
-    <row r="100" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:8">
       <c r="A100" s="1"/>
       <c r="B100" s="2"/>
       <c r="E100" s="3"/>
@@ -3062,19 +3086,19 @@
       <selection activeCell="D2" sqref="D2:D100"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="7.7109375" customWidth="1"/>
-    <col min="2" max="2" width="17.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="7.6640625" customWidth="1"/>
+    <col min="2" max="2" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.5546875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="9" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.85546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="23.5703125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="13.42578125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="19.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.88671875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="23.5546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.44140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="19.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" ht="15.6">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
@@ -3100,7 +3124,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8">
       <c r="A2" s="1"/>
       <c r="B2" s="2"/>
       <c r="E2" s="3"/>
@@ -3108,7 +3132,7 @@
       <c r="G2" s="2"/>
       <c r="H2" s="2"/>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8">
       <c r="A3" s="1"/>
       <c r="B3" s="2"/>
       <c r="E3" s="3"/>
@@ -3116,7 +3140,7 @@
       <c r="G3" s="2"/>
       <c r="H3" s="2"/>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8">
       <c r="A4" s="1"/>
       <c r="B4" s="2"/>
       <c r="E4" s="3"/>
@@ -3124,7 +3148,7 @@
       <c r="G4" s="2"/>
       <c r="H4" s="2"/>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8">
       <c r="A5" s="1"/>
       <c r="B5" s="2"/>
       <c r="E5" s="3"/>
@@ -3132,7 +3156,7 @@
       <c r="G5" s="2"/>
       <c r="H5" s="2"/>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8">
       <c r="A6" s="1"/>
       <c r="B6" s="2"/>
       <c r="E6" s="3"/>
@@ -3140,7 +3164,7 @@
       <c r="G6" s="2"/>
       <c r="H6" s="2"/>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8">
       <c r="A7" s="1"/>
       <c r="B7" s="2"/>
       <c r="E7" s="3"/>
@@ -3148,7 +3172,7 @@
       <c r="G7" s="2"/>
       <c r="H7" s="2"/>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8">
       <c r="A8" s="1"/>
       <c r="B8" s="2"/>
       <c r="E8" s="3"/>
@@ -3156,7 +3180,7 @@
       <c r="G8" s="2"/>
       <c r="H8" s="2"/>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8">
       <c r="A9" s="1"/>
       <c r="B9" s="2"/>
       <c r="E9" s="3"/>
@@ -3164,7 +3188,7 @@
       <c r="G9" s="2"/>
       <c r="H9" s="2"/>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8">
       <c r="A10" s="1"/>
       <c r="B10" s="2"/>
       <c r="E10" s="3"/>
@@ -3172,7 +3196,7 @@
       <c r="G10" s="2"/>
       <c r="H10" s="2"/>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8">
       <c r="A11" s="1"/>
       <c r="B11" s="2"/>
       <c r="E11" s="3"/>
@@ -3180,7 +3204,7 @@
       <c r="G11" s="2"/>
       <c r="H11" s="2"/>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8">
       <c r="A12" s="1"/>
       <c r="B12" s="2"/>
       <c r="E12" s="3"/>
@@ -3188,7 +3212,7 @@
       <c r="G12" s="2"/>
       <c r="H12" s="2"/>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8">
       <c r="A13" s="1"/>
       <c r="B13" s="2"/>
       <c r="E13" s="3"/>
@@ -3196,7 +3220,7 @@
       <c r="G13" s="2"/>
       <c r="H13" s="2"/>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8">
       <c r="A14" s="1"/>
       <c r="B14" s="2"/>
       <c r="E14" s="3"/>
@@ -3204,7 +3228,7 @@
       <c r="G14" s="2"/>
       <c r="H14" s="2"/>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8">
       <c r="A15" s="1"/>
       <c r="B15" s="2"/>
       <c r="E15" s="3"/>
@@ -3212,7 +3236,7 @@
       <c r="G15" s="2"/>
       <c r="H15" s="2"/>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8">
       <c r="A16" s="1"/>
       <c r="B16" s="2"/>
       <c r="E16" s="3"/>
@@ -3220,7 +3244,7 @@
       <c r="G16" s="2"/>
       <c r="H16" s="2"/>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:8">
       <c r="A17" s="1"/>
       <c r="B17" s="2"/>
       <c r="E17" s="3"/>
@@ -3228,7 +3252,7 @@
       <c r="G17" s="2"/>
       <c r="H17" s="2"/>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:8">
       <c r="A18" s="1"/>
       <c r="B18" s="2"/>
       <c r="E18" s="3"/>
@@ -3236,7 +3260,7 @@
       <c r="G18" s="2"/>
       <c r="H18" s="2"/>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:8">
       <c r="A19" s="1"/>
       <c r="B19" s="2"/>
       <c r="E19" s="3"/>
@@ -3244,7 +3268,7 @@
       <c r="G19" s="2"/>
       <c r="H19" s="2"/>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:8">
       <c r="A20" s="1"/>
       <c r="B20" s="2"/>
       <c r="E20" s="3"/>
@@ -3252,7 +3276,7 @@
       <c r="G20" s="2"/>
       <c r="H20" s="2"/>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:8">
       <c r="A21" s="1"/>
       <c r="B21" s="2"/>
       <c r="E21" s="3"/>
@@ -3260,7 +3284,7 @@
       <c r="G21" s="2"/>
       <c r="H21" s="2"/>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:8">
       <c r="A22" s="1"/>
       <c r="B22" s="2"/>
       <c r="E22" s="3"/>
@@ -3268,7 +3292,7 @@
       <c r="G22" s="2"/>
       <c r="H22" s="2"/>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:8">
       <c r="A23" s="1"/>
       <c r="B23" s="2"/>
       <c r="E23" s="3"/>
@@ -3276,7 +3300,7 @@
       <c r="G23" s="2"/>
       <c r="H23" s="2"/>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:8">
       <c r="A24" s="1"/>
       <c r="B24" s="2"/>
       <c r="E24" s="3"/>
@@ -3284,7 +3308,7 @@
       <c r="G24" s="2"/>
       <c r="H24" s="2"/>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:8">
       <c r="A25" s="1"/>
       <c r="B25" s="2"/>
       <c r="E25" s="3"/>
@@ -3292,7 +3316,7 @@
       <c r="G25" s="2"/>
       <c r="H25" s="2"/>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:8">
       <c r="A26" s="1"/>
       <c r="B26" s="2"/>
       <c r="E26" s="3"/>
@@ -3300,7 +3324,7 @@
       <c r="G26" s="2"/>
       <c r="H26" s="2"/>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:8">
       <c r="A27" s="1"/>
       <c r="B27" s="2"/>
       <c r="E27" s="3"/>
@@ -3308,7 +3332,7 @@
       <c r="G27" s="2"/>
       <c r="H27" s="2"/>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:8">
       <c r="A28" s="1"/>
       <c r="B28" s="2"/>
       <c r="E28" s="3"/>
@@ -3316,7 +3340,7 @@
       <c r="G28" s="2"/>
       <c r="H28" s="2"/>
     </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:8">
       <c r="A29" s="1"/>
       <c r="B29" s="2"/>
       <c r="E29" s="3"/>
@@ -3324,7 +3348,7 @@
       <c r="G29" s="2"/>
       <c r="H29" s="2"/>
     </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:8">
       <c r="A30" s="1"/>
       <c r="B30" s="2"/>
       <c r="E30" s="3"/>
@@ -3332,7 +3356,7 @@
       <c r="G30" s="2"/>
       <c r="H30" s="2"/>
     </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:8">
       <c r="A31" s="1"/>
       <c r="B31" s="2"/>
       <c r="E31" s="3"/>
@@ -3340,7 +3364,7 @@
       <c r="G31" s="2"/>
       <c r="H31" s="2"/>
     </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:8">
       <c r="A32" s="1"/>
       <c r="B32" s="2"/>
       <c r="E32" s="3"/>
@@ -3348,7 +3372,7 @@
       <c r="G32" s="2"/>
       <c r="H32" s="2"/>
     </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:8">
       <c r="A33" s="1"/>
       <c r="B33" s="2"/>
       <c r="E33" s="3"/>
@@ -3356,7 +3380,7 @@
       <c r="G33" s="2"/>
       <c r="H33" s="2"/>
     </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:8">
       <c r="A34" s="1"/>
       <c r="B34" s="2"/>
       <c r="E34" s="3"/>
@@ -3364,7 +3388,7 @@
       <c r="G34" s="2"/>
       <c r="H34" s="2"/>
     </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:8">
       <c r="A35" s="1"/>
       <c r="B35" s="2"/>
       <c r="E35" s="3"/>
@@ -3372,7 +3396,7 @@
       <c r="G35" s="2"/>
       <c r="H35" s="2"/>
     </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:8">
       <c r="A36" s="1"/>
       <c r="B36" s="2"/>
       <c r="E36" s="3"/>
@@ -3380,7 +3404,7 @@
       <c r="G36" s="2"/>
       <c r="H36" s="2"/>
     </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:8">
       <c r="A37" s="1"/>
       <c r="B37" s="2"/>
       <c r="E37" s="3"/>
@@ -3388,7 +3412,7 @@
       <c r="G37" s="2"/>
       <c r="H37" s="2"/>
     </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:8">
       <c r="A38" s="1"/>
       <c r="B38" s="2"/>
       <c r="E38" s="3"/>
@@ -3396,7 +3420,7 @@
       <c r="G38" s="2"/>
       <c r="H38" s="2"/>
     </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:8">
       <c r="A39" s="1"/>
       <c r="B39" s="2"/>
       <c r="E39" s="3"/>
@@ -3404,7 +3428,7 @@
       <c r="G39" s="2"/>
       <c r="H39" s="2"/>
     </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:8">
       <c r="A40" s="1"/>
       <c r="B40" s="2"/>
       <c r="E40" s="3"/>
@@ -3412,7 +3436,7 @@
       <c r="G40" s="2"/>
       <c r="H40" s="2"/>
     </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:8">
       <c r="A41" s="1"/>
       <c r="B41" s="2"/>
       <c r="E41" s="3"/>
@@ -3420,7 +3444,7 @@
       <c r="G41" s="2"/>
       <c r="H41" s="2"/>
     </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:8">
       <c r="A42" s="1"/>
       <c r="B42" s="2"/>
       <c r="E42" s="3"/>
@@ -3428,7 +3452,7 @@
       <c r="G42" s="2"/>
       <c r="H42" s="2"/>
     </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:8">
       <c r="A43" s="1"/>
       <c r="B43" s="2"/>
       <c r="E43" s="3"/>
@@ -3436,7 +3460,7 @@
       <c r="G43" s="2"/>
       <c r="H43" s="2"/>
     </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:8">
       <c r="A44" s="1"/>
       <c r="B44" s="2"/>
       <c r="E44" s="3"/>
@@ -3444,7 +3468,7 @@
       <c r="G44" s="2"/>
       <c r="H44" s="2"/>
     </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:8">
       <c r="A45" s="1"/>
       <c r="B45" s="2"/>
       <c r="E45" s="3"/>
@@ -3452,7 +3476,7 @@
       <c r="G45" s="2"/>
       <c r="H45" s="2"/>
     </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:8">
       <c r="A46" s="1"/>
       <c r="B46" s="2"/>
       <c r="E46" s="3"/>
@@ -3460,7 +3484,7 @@
       <c r="G46" s="2"/>
       <c r="H46" s="2"/>
     </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:8">
       <c r="A47" s="1"/>
       <c r="B47" s="2"/>
       <c r="E47" s="3"/>
@@ -3468,7 +3492,7 @@
       <c r="G47" s="2"/>
       <c r="H47" s="2"/>
     </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:8">
       <c r="A48" s="1"/>
       <c r="B48" s="2"/>
       <c r="E48" s="3"/>
@@ -3476,7 +3500,7 @@
       <c r="G48" s="2"/>
       <c r="H48" s="2"/>
     </row>
-    <row r="49" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:8">
       <c r="A49" s="1"/>
       <c r="B49" s="2"/>
       <c r="E49" s="3"/>
@@ -3484,7 +3508,7 @@
       <c r="G49" s="2"/>
       <c r="H49" s="2"/>
     </row>
-    <row r="50" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:8">
       <c r="A50" s="1"/>
       <c r="B50" s="2"/>
       <c r="E50" s="3"/>
@@ -3492,7 +3516,7 @@
       <c r="G50" s="2"/>
       <c r="H50" s="2"/>
     </row>
-    <row r="51" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:8">
       <c r="A51" s="1"/>
       <c r="B51" s="2"/>
       <c r="E51" s="3"/>
@@ -3500,7 +3524,7 @@
       <c r="G51" s="2"/>
       <c r="H51" s="2"/>
     </row>
-    <row r="52" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:8">
       <c r="A52" s="1"/>
       <c r="B52" s="2"/>
       <c r="E52" s="3"/>
@@ -3508,7 +3532,7 @@
       <c r="G52" s="2"/>
       <c r="H52" s="2"/>
     </row>
-    <row r="53" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:8">
       <c r="A53" s="1"/>
       <c r="B53" s="2"/>
       <c r="E53" s="3"/>
@@ -3516,7 +3540,7 @@
       <c r="G53" s="2"/>
       <c r="H53" s="2"/>
     </row>
-    <row r="54" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:8">
       <c r="A54" s="1"/>
       <c r="B54" s="2"/>
       <c r="E54" s="3"/>
@@ -3524,7 +3548,7 @@
       <c r="G54" s="2"/>
       <c r="H54" s="2"/>
     </row>
-    <row r="55" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:8">
       <c r="A55" s="1"/>
       <c r="B55" s="2"/>
       <c r="E55" s="3"/>
@@ -3532,7 +3556,7 @@
       <c r="G55" s="2"/>
       <c r="H55" s="2"/>
     </row>
-    <row r="56" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:8">
       <c r="A56" s="1"/>
       <c r="B56" s="2"/>
       <c r="E56" s="3"/>
@@ -3540,7 +3564,7 @@
       <c r="G56" s="2"/>
       <c r="H56" s="2"/>
     </row>
-    <row r="57" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:8">
       <c r="A57" s="1"/>
       <c r="B57" s="2"/>
       <c r="E57" s="3"/>
@@ -3548,7 +3572,7 @@
       <c r="G57" s="2"/>
       <c r="H57" s="2"/>
     </row>
-    <row r="58" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:8">
       <c r="A58" s="1"/>
       <c r="B58" s="2"/>
       <c r="E58" s="3"/>
@@ -3556,7 +3580,7 @@
       <c r="G58" s="2"/>
       <c r="H58" s="2"/>
     </row>
-    <row r="59" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:8">
       <c r="A59" s="1"/>
       <c r="B59" s="2"/>
       <c r="E59" s="3"/>
@@ -3564,7 +3588,7 @@
       <c r="G59" s="2"/>
       <c r="H59" s="2"/>
     </row>
-    <row r="60" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:8">
       <c r="A60" s="1"/>
       <c r="B60" s="2"/>
       <c r="E60" s="3"/>
@@ -3572,7 +3596,7 @@
       <c r="G60" s="2"/>
       <c r="H60" s="2"/>
     </row>
-    <row r="61" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:8">
       <c r="A61" s="1"/>
       <c r="B61" s="2"/>
       <c r="E61" s="3"/>
@@ -3580,7 +3604,7 @@
       <c r="G61" s="2"/>
       <c r="H61" s="2"/>
     </row>
-    <row r="62" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:8">
       <c r="A62" s="1"/>
       <c r="B62" s="2"/>
       <c r="E62" s="3"/>
@@ -3588,7 +3612,7 @@
       <c r="G62" s="2"/>
       <c r="H62" s="2"/>
     </row>
-    <row r="63" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:8">
       <c r="A63" s="1"/>
       <c r="B63" s="2"/>
       <c r="E63" s="3"/>
@@ -3596,7 +3620,7 @@
       <c r="G63" s="2"/>
       <c r="H63" s="2"/>
     </row>
-    <row r="64" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:8">
       <c r="A64" s="1"/>
       <c r="B64" s="2"/>
       <c r="E64" s="3"/>
@@ -3604,7 +3628,7 @@
       <c r="G64" s="2"/>
       <c r="H64" s="2"/>
     </row>
-    <row r="65" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:8">
       <c r="A65" s="1"/>
       <c r="B65" s="2"/>
       <c r="E65" s="3"/>
@@ -3612,7 +3636,7 @@
       <c r="G65" s="2"/>
       <c r="H65" s="2"/>
     </row>
-    <row r="66" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:8">
       <c r="A66" s="1"/>
       <c r="B66" s="2"/>
       <c r="E66" s="3"/>
@@ -3620,7 +3644,7 @@
       <c r="G66" s="2"/>
       <c r="H66" s="2"/>
     </row>
-    <row r="67" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:8">
       <c r="A67" s="1"/>
       <c r="B67" s="2"/>
       <c r="E67" s="3"/>
@@ -3628,7 +3652,7 @@
       <c r="G67" s="2"/>
       <c r="H67" s="2"/>
     </row>
-    <row r="68" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:8">
       <c r="A68" s="1"/>
       <c r="B68" s="2"/>
       <c r="E68" s="3"/>
@@ -3636,7 +3660,7 @@
       <c r="G68" s="2"/>
       <c r="H68" s="2"/>
     </row>
-    <row r="69" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:8">
       <c r="A69" s="1"/>
       <c r="B69" s="2"/>
       <c r="E69" s="3"/>
@@ -3644,7 +3668,7 @@
       <c r="G69" s="2"/>
       <c r="H69" s="2"/>
     </row>
-    <row r="70" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:8">
       <c r="A70" s="1"/>
       <c r="B70" s="2"/>
       <c r="E70" s="3"/>
@@ -3652,7 +3676,7 @@
       <c r="G70" s="2"/>
       <c r="H70" s="2"/>
     </row>
-    <row r="71" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:8">
       <c r="A71" s="1"/>
       <c r="B71" s="2"/>
       <c r="E71" s="3"/>
@@ -3660,7 +3684,7 @@
       <c r="G71" s="2"/>
       <c r="H71" s="2"/>
     </row>
-    <row r="72" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:8">
       <c r="A72" s="1"/>
       <c r="B72" s="2"/>
       <c r="E72" s="3"/>
@@ -3668,7 +3692,7 @@
       <c r="G72" s="2"/>
       <c r="H72" s="2"/>
     </row>
-    <row r="73" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:8">
       <c r="A73" s="1"/>
       <c r="B73" s="2"/>
       <c r="E73" s="3"/>
@@ -3676,7 +3700,7 @@
       <c r="G73" s="2"/>
       <c r="H73" s="2"/>
     </row>
-    <row r="74" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:8">
       <c r="A74" s="1"/>
       <c r="B74" s="2"/>
       <c r="E74" s="3"/>
@@ -3684,7 +3708,7 @@
       <c r="G74" s="2"/>
       <c r="H74" s="2"/>
     </row>
-    <row r="75" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:8">
       <c r="A75" s="1"/>
       <c r="B75" s="2"/>
       <c r="E75" s="3"/>
@@ -3692,7 +3716,7 @@
       <c r="G75" s="2"/>
       <c r="H75" s="2"/>
     </row>
-    <row r="76" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:8">
       <c r="A76" s="1"/>
       <c r="B76" s="2"/>
       <c r="E76" s="3"/>
@@ -3700,7 +3724,7 @@
       <c r="G76" s="2"/>
       <c r="H76" s="2"/>
     </row>
-    <row r="77" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:8">
       <c r="A77" s="1"/>
       <c r="B77" s="2"/>
       <c r="E77" s="3"/>
@@ -3708,7 +3732,7 @@
       <c r="G77" s="2"/>
       <c r="H77" s="2"/>
     </row>
-    <row r="78" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:8">
       <c r="A78" s="1"/>
       <c r="B78" s="2"/>
       <c r="E78" s="3"/>
@@ -3716,7 +3740,7 @@
       <c r="G78" s="2"/>
       <c r="H78" s="2"/>
     </row>
-    <row r="79" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:8">
       <c r="A79" s="1"/>
       <c r="B79" s="2"/>
       <c r="E79" s="3"/>
@@ -3724,7 +3748,7 @@
       <c r="G79" s="2"/>
       <c r="H79" s="2"/>
     </row>
-    <row r="80" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:8">
       <c r="A80" s="1"/>
       <c r="B80" s="2"/>
       <c r="E80" s="3"/>
@@ -3732,7 +3756,7 @@
       <c r="G80" s="2"/>
       <c r="H80" s="2"/>
     </row>
-    <row r="81" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:8">
       <c r="A81" s="1"/>
       <c r="B81" s="2"/>
       <c r="E81" s="3"/>
@@ -3740,7 +3764,7 @@
       <c r="G81" s="2"/>
       <c r="H81" s="2"/>
     </row>
-    <row r="82" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:8">
       <c r="A82" s="1"/>
       <c r="B82" s="2"/>
       <c r="E82" s="3"/>
@@ -3748,7 +3772,7 @@
       <c r="G82" s="2"/>
       <c r="H82" s="2"/>
     </row>
-    <row r="83" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:8">
       <c r="A83" s="1"/>
       <c r="B83" s="2"/>
       <c r="E83" s="3"/>
@@ -3756,7 +3780,7 @@
       <c r="G83" s="2"/>
       <c r="H83" s="2"/>
     </row>
-    <row r="84" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:8">
       <c r="A84" s="1"/>
       <c r="B84" s="2"/>
       <c r="E84" s="3"/>
@@ -3764,7 +3788,7 @@
       <c r="G84" s="2"/>
       <c r="H84" s="2"/>
     </row>
-    <row r="85" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:8">
       <c r="A85" s="1"/>
       <c r="B85" s="2"/>
       <c r="E85" s="3"/>
@@ -3772,7 +3796,7 @@
       <c r="G85" s="2"/>
       <c r="H85" s="2"/>
     </row>
-    <row r="86" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:8">
       <c r="A86" s="1"/>
       <c r="B86" s="2"/>
       <c r="E86" s="3"/>
@@ -3780,7 +3804,7 @@
       <c r="G86" s="2"/>
       <c r="H86" s="2"/>
     </row>
-    <row r="87" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:8">
       <c r="A87" s="1"/>
       <c r="B87" s="2"/>
       <c r="E87" s="3"/>
@@ -3788,7 +3812,7 @@
       <c r="G87" s="2"/>
       <c r="H87" s="2"/>
     </row>
-    <row r="88" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:8">
       <c r="A88" s="1"/>
       <c r="B88" s="2"/>
       <c r="E88" s="3"/>
@@ -3796,7 +3820,7 @@
       <c r="G88" s="2"/>
       <c r="H88" s="2"/>
     </row>
-    <row r="89" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:8">
       <c r="A89" s="1"/>
       <c r="B89" s="2"/>
       <c r="E89" s="3"/>
@@ -3804,7 +3828,7 @@
       <c r="G89" s="2"/>
       <c r="H89" s="2"/>
     </row>
-    <row r="90" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:8">
       <c r="A90" s="1"/>
       <c r="B90" s="2"/>
       <c r="E90" s="3"/>
@@ -3812,7 +3836,7 @@
       <c r="G90" s="2"/>
       <c r="H90" s="2"/>
     </row>
-    <row r="91" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:8">
       <c r="A91" s="1"/>
       <c r="B91" s="2"/>
       <c r="E91" s="3"/>
@@ -3820,7 +3844,7 @@
       <c r="G91" s="2"/>
       <c r="H91" s="2"/>
     </row>
-    <row r="92" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:8">
       <c r="A92" s="1"/>
       <c r="B92" s="2"/>
       <c r="E92" s="3"/>
@@ -3828,7 +3852,7 @@
       <c r="G92" s="2"/>
       <c r="H92" s="2"/>
     </row>
-    <row r="93" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:8">
       <c r="A93" s="1"/>
       <c r="B93" s="2"/>
       <c r="E93" s="3"/>
@@ -3836,7 +3860,7 @@
       <c r="G93" s="2"/>
       <c r="H93" s="2"/>
     </row>
-    <row r="94" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:8">
       <c r="A94" s="1"/>
       <c r="B94" s="2"/>
       <c r="E94" s="3"/>
@@ -3844,7 +3868,7 @@
       <c r="G94" s="2"/>
       <c r="H94" s="2"/>
     </row>
-    <row r="95" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:8">
       <c r="A95" s="1"/>
       <c r="B95" s="2"/>
       <c r="E95" s="3"/>
@@ -3852,7 +3876,7 @@
       <c r="G95" s="2"/>
       <c r="H95" s="2"/>
     </row>
-    <row r="96" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:8">
       <c r="A96" s="1"/>
       <c r="B96" s="2"/>
       <c r="E96" s="3"/>
@@ -3860,7 +3884,7 @@
       <c r="G96" s="2"/>
       <c r="H96" s="2"/>
     </row>
-    <row r="97" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:8">
       <c r="A97" s="1"/>
       <c r="B97" s="2"/>
       <c r="E97" s="3"/>
@@ -3868,7 +3892,7 @@
       <c r="G97" s="2"/>
       <c r="H97" s="2"/>
     </row>
-    <row r="98" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:8">
       <c r="A98" s="1"/>
       <c r="B98" s="2"/>
       <c r="E98" s="3"/>
@@ -3876,7 +3900,7 @@
       <c r="G98" s="2"/>
       <c r="H98" s="2"/>
     </row>
-    <row r="99" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:8">
       <c r="A99" s="1"/>
       <c r="B99" s="2"/>
       <c r="E99" s="3"/>
@@ -3884,7 +3908,7 @@
       <c r="G99" s="2"/>
       <c r="H99" s="2"/>
     </row>
-    <row r="100" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:8">
       <c r="A100" s="1"/>
       <c r="B100" s="2"/>
       <c r="E100" s="3"/>
@@ -3927,21 +3951,21 @@
       <selection activeCell="P21" sqref="P21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="19.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.5703125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.88671875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.88671875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19.44140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.5546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.5546875" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="9" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="17.85546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="17.88671875" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="17" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="19.140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="19.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" ht="15.6">
       <c r="A1" s="7" t="s">
         <v>8</v>
       </c>
@@ -3973,7 +3997,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10">
       <c r="A2" s="2"/>
       <c r="B2" s="8"/>
       <c r="D2" s="2"/>
@@ -3981,7 +4005,7 @@
       <c r="I2" s="8"/>
       <c r="J2" s="2"/>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10">
       <c r="A3" s="2"/>
       <c r="B3" s="8"/>
       <c r="D3" s="2"/>
@@ -3989,7 +4013,7 @@
       <c r="I3" s="8"/>
       <c r="J3" s="2"/>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10">
       <c r="A4" s="2"/>
       <c r="B4" s="8"/>
       <c r="D4" s="2"/>
@@ -3997,7 +4021,7 @@
       <c r="I4" s="8"/>
       <c r="J4" s="2"/>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10">
       <c r="A5" s="2"/>
       <c r="B5" s="8"/>
       <c r="D5" s="2"/>
@@ -4005,7 +4029,7 @@
       <c r="I5" s="8"/>
       <c r="J5" s="2"/>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10">
       <c r="A6" s="2"/>
       <c r="B6" s="8"/>
       <c r="D6" s="2"/>
@@ -4013,7 +4037,7 @@
       <c r="I6" s="8"/>
       <c r="J6" s="2"/>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10">
       <c r="A7" s="2"/>
       <c r="B7" s="8"/>
       <c r="D7" s="2"/>
@@ -4021,7 +4045,7 @@
       <c r="I7" s="8"/>
       <c r="J7" s="2"/>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10">
       <c r="A8" s="2"/>
       <c r="B8" s="8"/>
       <c r="D8" s="2"/>
@@ -4029,7 +4053,7 @@
       <c r="I8" s="8"/>
       <c r="J8" s="2"/>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10">
       <c r="A9" s="2"/>
       <c r="B9" s="8"/>
       <c r="D9" s="2"/>
@@ -4037,7 +4061,7 @@
       <c r="I9" s="8"/>
       <c r="J9" s="2"/>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:10">
       <c r="A10" s="2"/>
       <c r="B10" s="8"/>
       <c r="D10" s="2"/>
@@ -4045,7 +4069,7 @@
       <c r="I10" s="8"/>
       <c r="J10" s="2"/>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:10">
       <c r="A11" s="2"/>
       <c r="B11" s="8"/>
       <c r="D11" s="2"/>
@@ -4053,7 +4077,7 @@
       <c r="I11" s="8"/>
       <c r="J11" s="2"/>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:10">
       <c r="A12" s="2"/>
       <c r="B12" s="8"/>
       <c r="D12" s="2"/>
@@ -4061,7 +4085,7 @@
       <c r="I12" s="8"/>
       <c r="J12" s="2"/>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:10">
       <c r="A13" s="2"/>
       <c r="B13" s="8"/>
       <c r="D13" s="2"/>
@@ -4069,7 +4093,7 @@
       <c r="I13" s="8"/>
       <c r="J13" s="2"/>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:10">
       <c r="A14" s="2"/>
       <c r="B14" s="8"/>
       <c r="D14" s="2"/>
@@ -4077,7 +4101,7 @@
       <c r="I14" s="8"/>
       <c r="J14" s="2"/>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:10">
       <c r="A15" s="2"/>
       <c r="B15" s="8"/>
       <c r="D15" s="2"/>
@@ -4085,7 +4109,7 @@
       <c r="I15" s="8"/>
       <c r="J15" s="2"/>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:10">
       <c r="A16" s="2"/>
       <c r="B16" s="8"/>
       <c r="D16" s="2"/>
@@ -4093,7 +4117,7 @@
       <c r="I16" s="8"/>
       <c r="J16" s="2"/>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:10">
       <c r="A17" s="2"/>
       <c r="B17" s="8"/>
       <c r="D17" s="2"/>
@@ -4101,7 +4125,7 @@
       <c r="I17" s="8"/>
       <c r="J17" s="2"/>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:10">
       <c r="A18" s="2"/>
       <c r="B18" s="8"/>
       <c r="D18" s="2"/>
@@ -4109,7 +4133,7 @@
       <c r="I18" s="8"/>
       <c r="J18" s="2"/>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:10">
       <c r="A19" s="2"/>
       <c r="B19" s="8"/>
       <c r="D19" s="2"/>
@@ -4117,7 +4141,7 @@
       <c r="I19" s="8"/>
       <c r="J19" s="2"/>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:10">
       <c r="A20" s="2"/>
       <c r="B20" s="8"/>
       <c r="D20" s="2"/>
@@ -4125,7 +4149,7 @@
       <c r="I20" s="8"/>
       <c r="J20" s="2"/>
     </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:10">
       <c r="A21" s="2"/>
       <c r="B21" s="8"/>
       <c r="D21" s="2"/>
@@ -4133,7 +4157,7 @@
       <c r="I21" s="8"/>
       <c r="J21" s="2"/>
     </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:10">
       <c r="A22" s="2"/>
       <c r="B22" s="8"/>
       <c r="D22" s="2"/>
@@ -4141,7 +4165,7 @@
       <c r="I22" s="8"/>
       <c r="J22" s="2"/>
     </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:10">
       <c r="A23" s="2"/>
       <c r="B23" s="8"/>
       <c r="D23" s="2"/>
@@ -4149,7 +4173,7 @@
       <c r="I23" s="8"/>
       <c r="J23" s="2"/>
     </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:10">
       <c r="A24" s="2"/>
       <c r="B24" s="8"/>
       <c r="D24" s="2"/>
@@ -4157,7 +4181,7 @@
       <c r="I24" s="8"/>
       <c r="J24" s="2"/>
     </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:10">
       <c r="A25" s="2"/>
       <c r="B25" s="8"/>
       <c r="D25" s="2"/>
@@ -4165,7 +4189,7 @@
       <c r="I25" s="8"/>
       <c r="J25" s="2"/>
     </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:10">
       <c r="A26" s="2"/>
       <c r="B26" s="8"/>
       <c r="D26" s="2"/>
@@ -4173,7 +4197,7 @@
       <c r="I26" s="8"/>
       <c r="J26" s="2"/>
     </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:10">
       <c r="A27" s="2"/>
       <c r="B27" s="8"/>
       <c r="D27" s="2"/>
@@ -4181,7 +4205,7 @@
       <c r="I27" s="8"/>
       <c r="J27" s="2"/>
     </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:10">
       <c r="A28" s="2"/>
       <c r="B28" s="8"/>
       <c r="D28" s="2"/>
@@ -4189,7 +4213,7 @@
       <c r="I28" s="8"/>
       <c r="J28" s="2"/>
     </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:10">
       <c r="A29" s="2"/>
       <c r="B29" s="8"/>
       <c r="D29" s="2"/>
@@ -4197,7 +4221,7 @@
       <c r="I29" s="8"/>
       <c r="J29" s="2"/>
     </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:10">
       <c r="A30" s="2"/>
       <c r="B30" s="8"/>
       <c r="D30" s="2"/>
@@ -4205,7 +4229,7 @@
       <c r="I30" s="8"/>
       <c r="J30" s="2"/>
     </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:10">
       <c r="A31" s="2"/>
       <c r="B31" s="8"/>
       <c r="D31" s="2"/>
@@ -4213,7 +4237,7 @@
       <c r="I31" s="8"/>
       <c r="J31" s="2"/>
     </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:10">
       <c r="A32" s="2"/>
       <c r="B32" s="8"/>
       <c r="D32" s="2"/>
@@ -4221,7 +4245,7 @@
       <c r="I32" s="8"/>
       <c r="J32" s="2"/>
     </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:10">
       <c r="A33" s="2"/>
       <c r="B33" s="8"/>
       <c r="D33" s="2"/>
@@ -4229,7 +4253,7 @@
       <c r="I33" s="8"/>
       <c r="J33" s="2"/>
     </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:10">
       <c r="A34" s="2"/>
       <c r="B34" s="8"/>
       <c r="D34" s="2"/>
@@ -4237,7 +4261,7 @@
       <c r="I34" s="8"/>
       <c r="J34" s="2"/>
     </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:10">
       <c r="A35" s="2"/>
       <c r="B35" s="8"/>
       <c r="D35" s="2"/>
@@ -4245,7 +4269,7 @@
       <c r="I35" s="8"/>
       <c r="J35" s="2"/>
     </row>
-    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:10">
       <c r="A36" s="2"/>
       <c r="B36" s="8"/>
       <c r="D36" s="2"/>
@@ -4253,7 +4277,7 @@
       <c r="I36" s="8"/>
       <c r="J36" s="2"/>
     </row>
-    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:10">
       <c r="A37" s="2"/>
       <c r="B37" s="8"/>
       <c r="D37" s="2"/>
@@ -4261,7 +4285,7 @@
       <c r="I37" s="8"/>
       <c r="J37" s="2"/>
     </row>
-    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:10">
       <c r="A38" s="2"/>
       <c r="B38" s="8"/>
       <c r="D38" s="2"/>
@@ -4269,7 +4293,7 @@
       <c r="I38" s="8"/>
       <c r="J38" s="2"/>
     </row>
-    <row r="39" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:10">
       <c r="A39" s="2"/>
       <c r="B39" s="8"/>
       <c r="D39" s="2"/>
@@ -4277,7 +4301,7 @@
       <c r="I39" s="8"/>
       <c r="J39" s="2"/>
     </row>
-    <row r="40" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:10">
       <c r="A40" s="2"/>
       <c r="B40" s="8"/>
       <c r="D40" s="2"/>
@@ -4285,7 +4309,7 @@
       <c r="I40" s="8"/>
       <c r="J40" s="2"/>
     </row>
-    <row r="41" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:10">
       <c r="A41" s="2"/>
       <c r="B41" s="8"/>
       <c r="D41" s="2"/>
@@ -4293,7 +4317,7 @@
       <c r="I41" s="8"/>
       <c r="J41" s="2"/>
     </row>
-    <row r="42" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:10">
       <c r="A42" s="2"/>
       <c r="B42" s="8"/>
       <c r="D42" s="2"/>
@@ -4301,7 +4325,7 @@
       <c r="I42" s="8"/>
       <c r="J42" s="2"/>
     </row>
-    <row r="43" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:10">
       <c r="A43" s="2"/>
       <c r="B43" s="8"/>
       <c r="D43" s="2"/>
@@ -4309,7 +4333,7 @@
       <c r="I43" s="8"/>
       <c r="J43" s="2"/>
     </row>
-    <row r="44" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:10">
       <c r="A44" s="2"/>
       <c r="B44" s="8"/>
       <c r="D44" s="2"/>
@@ -4317,7 +4341,7 @@
       <c r="I44" s="8"/>
       <c r="J44" s="2"/>
     </row>
-    <row r="45" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:10">
       <c r="A45" s="2"/>
       <c r="B45" s="8"/>
       <c r="D45" s="2"/>
@@ -4325,7 +4349,7 @@
       <c r="I45" s="8"/>
       <c r="J45" s="2"/>
     </row>
-    <row r="46" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:10">
       <c r="A46" s="2"/>
       <c r="B46" s="8"/>
       <c r="D46" s="2"/>
@@ -4333,7 +4357,7 @@
       <c r="I46" s="8"/>
       <c r="J46" s="2"/>
     </row>
-    <row r="47" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:10">
       <c r="A47" s="2"/>
       <c r="B47" s="8"/>
       <c r="D47" s="2"/>
@@ -4341,7 +4365,7 @@
       <c r="I47" s="8"/>
       <c r="J47" s="2"/>
     </row>
-    <row r="48" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:10">
       <c r="A48" s="2"/>
       <c r="B48" s="8"/>
       <c r="D48" s="2"/>
@@ -4349,7 +4373,7 @@
       <c r="I48" s="8"/>
       <c r="J48" s="2"/>
     </row>
-    <row r="49" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:10">
       <c r="A49" s="2"/>
       <c r="B49" s="8"/>
       <c r="D49" s="2"/>
@@ -4357,7 +4381,7 @@
       <c r="I49" s="8"/>
       <c r="J49" s="2"/>
     </row>
-    <row r="50" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:10">
       <c r="A50" s="2"/>
       <c r="B50" s="8"/>
       <c r="D50" s="2"/>
@@ -4365,7 +4389,7 @@
       <c r="I50" s="8"/>
       <c r="J50" s="2"/>
     </row>
-    <row r="51" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:10">
       <c r="A51" s="2"/>
       <c r="B51" s="8"/>
       <c r="D51" s="2"/>
@@ -4373,7 +4397,7 @@
       <c r="I51" s="8"/>
       <c r="J51" s="2"/>
     </row>
-    <row r="52" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:10">
       <c r="A52" s="2"/>
       <c r="B52" s="8"/>
       <c r="D52" s="2"/>
@@ -4381,7 +4405,7 @@
       <c r="I52" s="8"/>
       <c r="J52" s="2"/>
     </row>
-    <row r="53" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:10">
       <c r="A53" s="2"/>
       <c r="B53" s="8"/>
       <c r="D53" s="2"/>
@@ -4389,7 +4413,7 @@
       <c r="I53" s="8"/>
       <c r="J53" s="2"/>
     </row>
-    <row r="54" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:10">
       <c r="A54" s="2"/>
       <c r="B54" s="8"/>
       <c r="D54" s="2"/>
@@ -4397,7 +4421,7 @@
       <c r="I54" s="8"/>
       <c r="J54" s="2"/>
     </row>
-    <row r="55" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:10">
       <c r="A55" s="2"/>
       <c r="B55" s="8"/>
       <c r="D55" s="2"/>
@@ -4405,7 +4429,7 @@
       <c r="I55" s="8"/>
       <c r="J55" s="2"/>
     </row>
-    <row r="56" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:10">
       <c r="A56" s="2"/>
       <c r="B56" s="8"/>
       <c r="D56" s="2"/>
@@ -4413,7 +4437,7 @@
       <c r="I56" s="8"/>
       <c r="J56" s="2"/>
     </row>
-    <row r="57" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:10">
       <c r="A57" s="2"/>
       <c r="B57" s="8"/>
       <c r="D57" s="2"/>
@@ -4421,7 +4445,7 @@
       <c r="I57" s="8"/>
       <c r="J57" s="2"/>
     </row>
-    <row r="58" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:10">
       <c r="A58" s="2"/>
       <c r="B58" s="8"/>
       <c r="D58" s="2"/>
@@ -4429,7 +4453,7 @@
       <c r="I58" s="8"/>
       <c r="J58" s="2"/>
     </row>
-    <row r="59" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:10">
       <c r="A59" s="2"/>
       <c r="B59" s="8"/>
       <c r="D59" s="2"/>
@@ -4437,7 +4461,7 @@
       <c r="I59" s="8"/>
       <c r="J59" s="2"/>
     </row>
-    <row r="60" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:10">
       <c r="A60" s="2"/>
       <c r="B60" s="8"/>
       <c r="D60" s="2"/>
@@ -4445,7 +4469,7 @@
       <c r="I60" s="8"/>
       <c r="J60" s="2"/>
     </row>
-    <row r="61" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:10">
       <c r="A61" s="2"/>
       <c r="B61" s="8"/>
       <c r="D61" s="2"/>
@@ -4453,7 +4477,7 @@
       <c r="I61" s="8"/>
       <c r="J61" s="2"/>
     </row>
-    <row r="62" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:10">
       <c r="A62" s="2"/>
       <c r="B62" s="8"/>
       <c r="D62" s="2"/>
@@ -4461,7 +4485,7 @@
       <c r="I62" s="8"/>
       <c r="J62" s="2"/>
     </row>
-    <row r="63" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:10">
       <c r="A63" s="2"/>
       <c r="B63" s="8"/>
       <c r="D63" s="2"/>
@@ -4469,7 +4493,7 @@
       <c r="I63" s="8"/>
       <c r="J63" s="2"/>
     </row>
-    <row r="64" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:10">
       <c r="A64" s="2"/>
       <c r="B64" s="8"/>
       <c r="D64" s="2"/>
@@ -4477,7 +4501,7 @@
       <c r="I64" s="8"/>
       <c r="J64" s="2"/>
     </row>
-    <row r="65" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:10">
       <c r="A65" s="2"/>
       <c r="B65" s="8"/>
       <c r="D65" s="2"/>
@@ -4485,7 +4509,7 @@
       <c r="I65" s="8"/>
       <c r="J65" s="2"/>
     </row>
-    <row r="66" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:10">
       <c r="A66" s="2"/>
       <c r="B66" s="8"/>
       <c r="D66" s="2"/>
@@ -4493,7 +4517,7 @@
       <c r="I66" s="8"/>
       <c r="J66" s="2"/>
     </row>
-    <row r="67" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:10">
       <c r="A67" s="2"/>
       <c r="B67" s="8"/>
       <c r="D67" s="2"/>
@@ -4501,7 +4525,7 @@
       <c r="I67" s="8"/>
       <c r="J67" s="2"/>
     </row>
-    <row r="68" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:10">
       <c r="A68" s="2"/>
       <c r="B68" s="8"/>
       <c r="D68" s="2"/>
@@ -4509,7 +4533,7 @@
       <c r="I68" s="8"/>
       <c r="J68" s="2"/>
     </row>
-    <row r="69" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:10">
       <c r="A69" s="2"/>
       <c r="B69" s="8"/>
       <c r="D69" s="2"/>
@@ -4517,7 +4541,7 @@
       <c r="I69" s="8"/>
       <c r="J69" s="2"/>
     </row>
-    <row r="70" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:10">
       <c r="A70" s="2"/>
       <c r="B70" s="8"/>
       <c r="D70" s="2"/>
@@ -4525,7 +4549,7 @@
       <c r="I70" s="8"/>
       <c r="J70" s="2"/>
     </row>
-    <row r="71" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:10">
       <c r="A71" s="2"/>
       <c r="B71" s="8"/>
       <c r="D71" s="2"/>
@@ -4533,7 +4557,7 @@
       <c r="I71" s="8"/>
       <c r="J71" s="2"/>
     </row>
-    <row r="72" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:10">
       <c r="A72" s="2"/>
       <c r="B72" s="8"/>
       <c r="D72" s="2"/>
@@ -4541,7 +4565,7 @@
       <c r="I72" s="8"/>
       <c r="J72" s="2"/>
     </row>
-    <row r="73" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:10">
       <c r="A73" s="2"/>
       <c r="B73" s="8"/>
       <c r="D73" s="2"/>
@@ -4549,7 +4573,7 @@
       <c r="I73" s="8"/>
       <c r="J73" s="2"/>
     </row>
-    <row r="74" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:10">
       <c r="A74" s="2"/>
       <c r="B74" s="8"/>
       <c r="D74" s="2"/>
@@ -4557,7 +4581,7 @@
       <c r="I74" s="8"/>
       <c r="J74" s="2"/>
     </row>
-    <row r="75" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:10">
       <c r="A75" s="2"/>
       <c r="B75" s="8"/>
       <c r="D75" s="2"/>
@@ -4565,7 +4589,7 @@
       <c r="I75" s="8"/>
       <c r="J75" s="2"/>
     </row>
-    <row r="76" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:10">
       <c r="A76" s="2"/>
       <c r="B76" s="8"/>
       <c r="D76" s="2"/>
@@ -4573,7 +4597,7 @@
       <c r="I76" s="8"/>
       <c r="J76" s="2"/>
     </row>
-    <row r="77" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:10">
       <c r="A77" s="2"/>
       <c r="B77" s="8"/>
       <c r="D77" s="2"/>
@@ -4581,7 +4605,7 @@
       <c r="I77" s="8"/>
       <c r="J77" s="2"/>
     </row>
-    <row r="78" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:10">
       <c r="A78" s="2"/>
       <c r="B78" s="8"/>
       <c r="D78" s="2"/>
@@ -4589,7 +4613,7 @@
       <c r="I78" s="8"/>
       <c r="J78" s="2"/>
     </row>
-    <row r="79" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:10">
       <c r="A79" s="2"/>
       <c r="B79" s="8"/>
       <c r="D79" s="2"/>
@@ -4597,7 +4621,7 @@
       <c r="I79" s="8"/>
       <c r="J79" s="2"/>
     </row>
-    <row r="80" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:10">
       <c r="A80" s="2"/>
       <c r="B80" s="8"/>
       <c r="D80" s="2"/>
@@ -4605,7 +4629,7 @@
       <c r="I80" s="8"/>
       <c r="J80" s="2"/>
     </row>
-    <row r="81" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:10">
       <c r="A81" s="2"/>
       <c r="B81" s="8"/>
       <c r="D81" s="2"/>
@@ -4613,7 +4637,7 @@
       <c r="I81" s="8"/>
       <c r="J81" s="2"/>
     </row>
-    <row r="82" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:10">
       <c r="A82" s="2"/>
       <c r="B82" s="8"/>
       <c r="D82" s="2"/>
@@ -4621,7 +4645,7 @@
       <c r="I82" s="8"/>
       <c r="J82" s="2"/>
     </row>
-    <row r="83" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:10">
       <c r="A83" s="2"/>
       <c r="B83" s="8"/>
       <c r="D83" s="2"/>
@@ -4629,7 +4653,7 @@
       <c r="I83" s="8"/>
       <c r="J83" s="2"/>
     </row>
-    <row r="84" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:10">
       <c r="A84" s="2"/>
       <c r="B84" s="8"/>
       <c r="D84" s="2"/>
@@ -4637,7 +4661,7 @@
       <c r="I84" s="8"/>
       <c r="J84" s="2"/>
     </row>
-    <row r="85" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:10">
       <c r="A85" s="2"/>
       <c r="B85" s="8"/>
       <c r="D85" s="2"/>
@@ -4645,7 +4669,7 @@
       <c r="I85" s="8"/>
       <c r="J85" s="2"/>
     </row>
-    <row r="86" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:10">
       <c r="A86" s="2"/>
       <c r="B86" s="8"/>
       <c r="D86" s="2"/>
@@ -4653,7 +4677,7 @@
       <c r="I86" s="8"/>
       <c r="J86" s="2"/>
     </row>
-    <row r="87" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:10">
       <c r="A87" s="2"/>
       <c r="B87" s="8"/>
       <c r="D87" s="2"/>
@@ -4661,7 +4685,7 @@
       <c r="I87" s="8"/>
       <c r="J87" s="2"/>
     </row>
-    <row r="88" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:10">
       <c r="A88" s="2"/>
       <c r="B88" s="8"/>
       <c r="D88" s="2"/>
@@ -4669,7 +4693,7 @@
       <c r="I88" s="8"/>
       <c r="J88" s="2"/>
     </row>
-    <row r="89" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:10">
       <c r="A89" s="2"/>
       <c r="B89" s="8"/>
       <c r="D89" s="2"/>
@@ -4677,7 +4701,7 @@
       <c r="I89" s="8"/>
       <c r="J89" s="2"/>
     </row>
-    <row r="90" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:10">
       <c r="A90" s="2"/>
       <c r="B90" s="8"/>
       <c r="D90" s="2"/>
@@ -4685,7 +4709,7 @@
       <c r="I90" s="8"/>
       <c r="J90" s="2"/>
     </row>
-    <row r="91" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:10">
       <c r="A91" s="2"/>
       <c r="B91" s="8"/>
       <c r="D91" s="2"/>
@@ -4693,7 +4717,7 @@
       <c r="I91" s="8"/>
       <c r="J91" s="2"/>
     </row>
-    <row r="92" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:10">
       <c r="A92" s="2"/>
       <c r="B92" s="8"/>
       <c r="D92" s="2"/>
@@ -4701,7 +4725,7 @@
       <c r="I92" s="8"/>
       <c r="J92" s="2"/>
     </row>
-    <row r="93" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:10">
       <c r="A93" s="2"/>
       <c r="B93" s="8"/>
       <c r="D93" s="2"/>
@@ -4709,7 +4733,7 @@
       <c r="I93" s="8"/>
       <c r="J93" s="2"/>
     </row>
-    <row r="94" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:10">
       <c r="A94" s="2"/>
       <c r="B94" s="8"/>
       <c r="D94" s="2"/>
@@ -4717,7 +4741,7 @@
       <c r="I94" s="8"/>
       <c r="J94" s="2"/>
     </row>
-    <row r="95" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:10">
       <c r="A95" s="2"/>
       <c r="B95" s="8"/>
       <c r="D95" s="2"/>
@@ -4725,7 +4749,7 @@
       <c r="I95" s="8"/>
       <c r="J95" s="2"/>
     </row>
-    <row r="96" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:10">
       <c r="A96" s="2"/>
       <c r="B96" s="8"/>
       <c r="D96" s="2"/>
@@ -4733,7 +4757,7 @@
       <c r="I96" s="8"/>
       <c r="J96" s="2"/>
     </row>
-    <row r="97" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:10">
       <c r="A97" s="2"/>
       <c r="B97" s="8"/>
       <c r="D97" s="2"/>
@@ -4741,7 +4765,7 @@
       <c r="I97" s="8"/>
       <c r="J97" s="2"/>
     </row>
-    <row r="98" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:10">
       <c r="A98" s="2"/>
       <c r="B98" s="8"/>
       <c r="D98" s="2"/>
@@ -4749,7 +4773,7 @@
       <c r="I98" s="8"/>
       <c r="J98" s="2"/>
     </row>
-    <row r="99" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:10">
       <c r="A99" s="2"/>
       <c r="B99" s="8"/>
       <c r="D99" s="2"/>
@@ -4757,7 +4781,7 @@
       <c r="I99" s="8"/>
       <c r="J99" s="2"/>
     </row>
-    <row r="100" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:10">
       <c r="A100" s="2"/>
       <c r="B100" s="8"/>
       <c r="D100" s="2"/>

</xml_diff>

<commit_message>
Updated StudentService module and styles
</commit_message>
<xml_diff>
--- a/PR&IR.xlsx
+++ b/PR&IR.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SHIVYA KUMAR\Desktop\new415\CS415_A3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FCBE4524-C6CA-4495-B5C8-C5EC464FB1CD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D10B44C-54A7-4F21-8F22-614AAAF0B8A7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{BFA1E21A-08FA-4F02-8C25-33C81C8EE970}"/>
   </bookViews>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="83">
   <si>
     <t>Date</t>
   </si>
@@ -141,9 +141,6 @@
     <t>complete pending ToDos</t>
   </si>
   <si>
-    <t>13/0/2025</t>
-  </si>
-  <si>
     <t xml:space="preserve">Resolved merge conflict and synced with main. Researched on sqlalchemy vs pyodbc. Custom validation for enrollment services. </t>
   </si>
   <si>
@@ -153,6 +150,15 @@
     <t>Best Wishes w/ Backend.</t>
   </si>
   <si>
+    <t>Completed custom exception handling for all routes and custom validtion for enrollment services</t>
+  </si>
+  <si>
+    <t>Fee and Hold services routing exceptions and validations</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Stay Healthy Aviiii. Don’t get sick </t>
+  </si>
+  <si>
     <t>Shivya Kumar</t>
   </si>
   <si>
@@ -174,22 +180,127 @@
     <t>Solve my routes and fix UI</t>
   </si>
   <si>
+    <t>I added my routes in the same file app.py</t>
+  </si>
+  <si>
     <t>Customizing UI and recovered deleted codes</t>
   </si>
   <si>
     <t xml:space="preserve">Continue converting UI </t>
   </si>
   <si>
-    <t>I added my routes in the same file app.py</t>
-  </si>
-  <si>
     <t>shivya Kumar</t>
   </si>
   <si>
+    <t>Converted all user interface designs into HTML and set up respective routes.</t>
+  </si>
+  <si>
     <t>continue implementing remaining UI logic based on feedback and custom validation with exception handling for all of her routes</t>
   </si>
   <si>
-    <t>Converted all user interface designs into HTML and set up respective routes.</t>
+    <t>Added custom validation for logout and exception handling for all routes</t>
+  </si>
+  <si>
+    <t>Not feeling well, assignments are due and short tests are approaching.</t>
+  </si>
+  <si>
+    <t>Start with next workpackage once approved and given by Jayshil Singh</t>
+  </si>
+  <si>
+    <t>YPP</t>
+  </si>
+  <si>
+    <t>Converted Dart files to HTML files</t>
+  </si>
+  <si>
+    <t>Updating JS to render all htmls properly</t>
+  </si>
+  <si>
+    <t>N/A</t>
+  </si>
+  <si>
+    <t>Completed JS modification</t>
+  </si>
+  <si>
+    <t>Patch up any errors and add exception handling</t>
+  </si>
+  <si>
+    <t>13/5/2025</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Added Exception Handling </t>
+  </si>
+  <si>
+    <t>Parse XML's to registration Dropdowns</t>
+  </si>
+  <si>
+    <t>Will work on CS403 so hours worked on CS415 might decrease</t>
+  </si>
+  <si>
+    <t>14/5/2025</t>
+  </si>
+  <si>
+    <t>Parsed XML's Properly</t>
+  </si>
+  <si>
+    <t>Waiting PM's Lead</t>
+  </si>
+  <si>
+    <t>Developed an invoice generation feature for a Flask-based enrollment system, starting with the UI in fees.html and linking it to the backend. Initially, used pdfkit to convert an HTML template to a PDF, but encountered wkhtmltopdf setup issues. To simplify, switched to ReportLab, a pure-Python library, and modified the Flask route to generate the PDF programmatically. This involved creating the PDF structure and content directly within the Python code and sending it as a download. Throughout the process, corrected routing in the HTML files to ensure proper navigation within the Flask application.</t>
+  </si>
+  <si>
+    <t>Models for Enrollment N Fees</t>
+  </si>
+  <si>
+    <t>Happy Thurday PM :)</t>
+  </si>
+  <si>
+    <t>16/5/2025</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Implemented the API Key linking </t>
+  </si>
+  <si>
+    <t>Fixing the HTML Pages and the errors that occurred due to restructuring</t>
+  </si>
+  <si>
+    <t>18/5/2025</t>
+  </si>
+  <si>
+    <t>Implementing masterpage in all pages</t>
+  </si>
+  <si>
+    <t>Learning how to work with Docker Database</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Modified invoice </t>
+  </si>
+  <si>
+    <t>Backend commencement</t>
+  </si>
+  <si>
+    <t>configuring enrollment services to designated port</t>
+  </si>
+  <si>
+    <t>Configure on specified port</t>
+  </si>
+  <si>
+    <t>Successfully run the services on port 5004</t>
+  </si>
+  <si>
+    <t>confgure API</t>
+  </si>
+  <si>
+    <t xml:space="preserve">only read docker documentation </t>
+  </si>
+  <si>
+    <t>Port configuration</t>
+  </si>
+  <si>
+    <t>Initiated my microservice</t>
+  </si>
+  <si>
+    <t>Sick, too much workloads in other units</t>
   </si>
 </sst>
 </file>
@@ -254,22 +365,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="2" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="35">
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
     <dxf>
       <numFmt numFmtId="30" formatCode="@"/>
     </dxf>
@@ -349,7 +451,7 @@
       <numFmt numFmtId="30" formatCode="@"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="164" formatCode="h"/>
+      <numFmt numFmtId="2" formatCode="0.00"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="14" formatCode="0.00%"/>
@@ -380,6 +482,15 @@
     </dxf>
     <dxf>
       <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="30" formatCode="@"/>
@@ -497,17 +608,17 @@
     <tableColumn id="2" xr3:uid="{55A78D6C-890A-4502-A184-DEEFF14BB82E}" name="Member Name" dataDxfId="25"/>
     <tableColumn id="3" xr3:uid="{57B9A516-E930-4C06-A589-24182A37BA85}" name="Task/Activity"/>
     <tableColumn id="4" xr3:uid="{A7CD18E8-808E-43EA-A960-7EDF2D2AB452}" name="Status"/>
-    <tableColumn id="5" xr3:uid="{A9BAB96D-D5FD-4C0D-A277-6E052D27EC3A}" name="% Complete" dataDxfId="2"/>
-    <tableColumn id="6" xr3:uid="{4EBDEBD4-A02D-4266-88BC-5E6088167CE4}" name="Hours Worked Today" dataDxfId="0"/>
-    <tableColumn id="7" xr3:uid="{88484166-6833-4A6B-B292-081E908E7876}" name="Next Steps" dataDxfId="1"/>
-    <tableColumn id="8" xr3:uid="{65034E84-46C0-4115-A351-A3C28C7B9EE1}" name="Notes/Comments" dataDxfId="24"/>
+    <tableColumn id="5" xr3:uid="{A9BAB96D-D5FD-4C0D-A277-6E052D27EC3A}" name="% Complete" dataDxfId="24"/>
+    <tableColumn id="6" xr3:uid="{4EBDEBD4-A02D-4266-88BC-5E6088167CE4}" name="Hours Worked Today" dataDxfId="23"/>
+    <tableColumn id="7" xr3:uid="{88484166-6833-4A6B-B292-081E908E7876}" name="Next Steps" dataDxfId="22"/>
+    <tableColumn id="8" xr3:uid="{65034E84-46C0-4115-A351-A3C28C7B9EE1}" name="Notes/Comments" dataDxfId="21"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium26" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{D9A2FBFA-47C8-4A27-8A35-991BC77E93AD}" name="Table14" displayName="Table14" ref="A1:H100" totalsRowShown="0" headerRowDxfId="23">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{D9A2FBFA-47C8-4A27-8A35-991BC77E93AD}" name="Table14" displayName="Table14" ref="A1:H100" totalsRowShown="0" headerRowDxfId="20">
   <autoFilter ref="A1:H100" xr:uid="{D9A2FBFA-47C8-4A27-8A35-991BC77E93AD}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
@@ -519,21 +630,21 @@
     <filterColumn colId="7" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="8">
-    <tableColumn id="1" xr3:uid="{9DF80C4D-D075-4428-A54F-FD6AD093D08C}" name="Date" dataDxfId="22"/>
-    <tableColumn id="2" xr3:uid="{EBFC72C6-272F-4910-98B7-AD481D68F5CF}" name="Member Name" dataDxfId="21"/>
+    <tableColumn id="1" xr3:uid="{9DF80C4D-D075-4428-A54F-FD6AD093D08C}" name="Date" dataDxfId="19"/>
+    <tableColumn id="2" xr3:uid="{EBFC72C6-272F-4910-98B7-AD481D68F5CF}" name="Member Name" dataDxfId="18"/>
     <tableColumn id="3" xr3:uid="{9F5B3984-7002-4FEA-8B81-D2D8284783D7}" name="Task/Activity"/>
     <tableColumn id="4" xr3:uid="{5F85F44B-886F-440F-9E69-8335A039C2E6}" name="Status"/>
-    <tableColumn id="5" xr3:uid="{AF0043ED-9EF2-470B-9735-7321011714BA}" name="% Complete" dataDxfId="20"/>
-    <tableColumn id="6" xr3:uid="{4F961AD8-B86B-411C-BB04-8D7EE4DD134D}" name="Hours Worked Today" dataDxfId="19"/>
-    <tableColumn id="7" xr3:uid="{34EBB1FC-FFD7-47AB-A959-A220B742401C}" name="Next Steps" dataDxfId="18"/>
-    <tableColumn id="8" xr3:uid="{128DAA9E-15FB-4BB9-B76B-4A920C859038}" name="Notes/Comments" dataDxfId="17"/>
+    <tableColumn id="5" xr3:uid="{AF0043ED-9EF2-470B-9735-7321011714BA}" name="% Complete" dataDxfId="17"/>
+    <tableColumn id="6" xr3:uid="{4F961AD8-B86B-411C-BB04-8D7EE4DD134D}" name="Hours Worked Today" dataDxfId="16"/>
+    <tableColumn id="7" xr3:uid="{34EBB1FC-FFD7-47AB-A959-A220B742401C}" name="Next Steps" dataDxfId="15"/>
+    <tableColumn id="8" xr3:uid="{128DAA9E-15FB-4BB9-B76B-4A920C859038}" name="Notes/Comments" dataDxfId="14"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium26" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{646C4EC7-41A3-4570-9D38-06D55FDE20F6}" name="Table15" displayName="Table15" ref="A1:H100" totalsRowShown="0" headerRowDxfId="16">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{646C4EC7-41A3-4570-9D38-06D55FDE20F6}" name="Table15" displayName="Table15" ref="A1:H100" totalsRowShown="0" headerRowDxfId="13">
   <autoFilter ref="A1:H100" xr:uid="{646C4EC7-41A3-4570-9D38-06D55FDE20F6}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
@@ -545,21 +656,21 @@
     <filterColumn colId="7" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="8">
-    <tableColumn id="1" xr3:uid="{13D6CE41-CF73-478C-B7F6-3B0C25C48DFD}" name="Date" dataDxfId="15"/>
-    <tableColumn id="2" xr3:uid="{E468B109-F9F1-48D8-BECE-0F7015DD8D95}" name="Member Name" dataDxfId="14"/>
+    <tableColumn id="1" xr3:uid="{13D6CE41-CF73-478C-B7F6-3B0C25C48DFD}" name="Date" dataDxfId="12"/>
+    <tableColumn id="2" xr3:uid="{E468B109-F9F1-48D8-BECE-0F7015DD8D95}" name="Member Name" dataDxfId="11"/>
     <tableColumn id="3" xr3:uid="{279E5366-E900-45EE-80D9-5446A85E61AD}" name="Task/Activity"/>
     <tableColumn id="4" xr3:uid="{63D996BE-E8E2-4186-8CD4-49EAB9AA8847}" name="Status"/>
-    <tableColumn id="5" xr3:uid="{2FF82CF3-E17A-4896-9C9C-7339D28CD4A7}" name="% Complete" dataDxfId="13"/>
-    <tableColumn id="6" xr3:uid="{67DCB379-6881-4BBC-A633-BD51853A9B6B}" name="Hours Worked Today" dataDxfId="12"/>
-    <tableColumn id="7" xr3:uid="{91C8F225-F251-45F2-BC41-843547B77A6F}" name="Next Steps" dataDxfId="11"/>
-    <tableColumn id="8" xr3:uid="{EEAB1D68-5668-4B1F-8473-D3A49DA7E015}" name="Notes/Comments" dataDxfId="10"/>
+    <tableColumn id="5" xr3:uid="{2FF82CF3-E17A-4896-9C9C-7339D28CD4A7}" name="% Complete" dataDxfId="10"/>
+    <tableColumn id="6" xr3:uid="{67DCB379-6881-4BBC-A633-BD51853A9B6B}" name="Hours Worked Today" dataDxfId="9"/>
+    <tableColumn id="7" xr3:uid="{91C8F225-F251-45F2-BC41-843547B77A6F}" name="Next Steps" dataDxfId="8"/>
+    <tableColumn id="8" xr3:uid="{EEAB1D68-5668-4B1F-8473-D3A49DA7E015}" name="Notes/Comments" dataDxfId="7"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium26" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{5818BB59-8F2C-4810-A78D-CBC8FA25F524}" name="Table5" displayName="Table5" ref="A1:J100" totalsRowShown="0" headerRowDxfId="9">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{5818BB59-8F2C-4810-A78D-CBC8FA25F524}" name="Table5" displayName="Table5" ref="A1:J100" totalsRowShown="0" headerRowDxfId="6">
   <autoFilter ref="A1:J100" xr:uid="{5818BB59-8F2C-4810-A78D-CBC8FA25F524}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
@@ -573,16 +684,16 @@
     <filterColumn colId="9" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="10">
-    <tableColumn id="1" xr3:uid="{BC250DF1-329E-4733-8702-E009738E43CB}" name="Header" dataDxfId="8"/>
-    <tableColumn id="2" xr3:uid="{F6CCDA73-9A12-472B-A535-0F3DC2A5CF61}" name="Date Raised" dataDxfId="7"/>
+    <tableColumn id="1" xr3:uid="{BC250DF1-329E-4733-8702-E009738E43CB}" name="Header" dataDxfId="5"/>
+    <tableColumn id="2" xr3:uid="{F6CCDA73-9A12-472B-A535-0F3DC2A5CF61}" name="Date Raised" dataDxfId="4"/>
     <tableColumn id="3" xr3:uid="{2E3C7862-32AA-44B8-BCC3-2F9299A8F3DC}" name="Raised By"/>
-    <tableColumn id="4" xr3:uid="{FB9438A9-92FB-4A8D-95A5-F17D6EF9AA82}" name="Issue Description" dataDxfId="6"/>
+    <tableColumn id="4" xr3:uid="{FB9438A9-92FB-4A8D-95A5-F17D6EF9AA82}" name="Issue Description" dataDxfId="3"/>
     <tableColumn id="5" xr3:uid="{48223256-C4C0-467B-9FA7-AA8E7742B58A}" name="Impact"/>
     <tableColumn id="6" xr3:uid="{EEDBAAB2-0361-4BF5-8FDB-3FAD49E87C1B}" name="Priority"/>
     <tableColumn id="7" xr3:uid="{515F6321-7FC0-4B4E-A422-3A0E332B7B97}" name="Status"/>
-    <tableColumn id="8" xr3:uid="{60A704D7-818B-442C-91EF-B82765B2618D}" name="Resolution Plan" dataDxfId="5"/>
-    <tableColumn id="9" xr3:uid="{D95E2A6F-E7D4-4FC5-9AAF-1E3DBEE8D8FC}" name="Date Resolved" dataDxfId="4"/>
-    <tableColumn id="10" xr3:uid="{D43B4A1C-AE3D-43D4-A514-7BAA3E281FD3}" name="Notes/Comments" dataDxfId="3"/>
+    <tableColumn id="8" xr3:uid="{60A704D7-818B-442C-91EF-B82765B2618D}" name="Resolution Plan" dataDxfId="2"/>
+    <tableColumn id="9" xr3:uid="{D95E2A6F-E7D4-4FC5-9AAF-1E3DBEE8D8FC}" name="Date Resolved" dataDxfId="1"/>
+    <tableColumn id="10" xr3:uid="{D43B4A1C-AE3D-43D4-A514-7BAA3E281FD3}" name="Notes/Comments" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight15" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -936,30 +1047,30 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{37EAA098-74C6-4411-B7E2-26AD2DCBC3F0}">
   <dimension ref="A1:H28"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H6" sqref="H6"/>
+    <sheetView topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="10.3984375" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.59765625" style="2" customWidth="1"/>
+    <col min="1" max="1" width="10.44140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.5546875" style="2" customWidth="1"/>
     <col min="3" max="3" width="58" customWidth="1"/>
-    <col min="5" max="5" width="13.09765625" style="3" customWidth="1"/>
-    <col min="6" max="6" width="20.8984375" style="4" customWidth="1"/>
-    <col min="7" max="7" width="34.8984375" style="2" customWidth="1"/>
-    <col min="8" max="8" width="43.3984375" style="2" customWidth="1"/>
-    <col min="11" max="11" width="9.09765625" customWidth="1"/>
-    <col min="12" max="12" width="13.296875" customWidth="1"/>
-    <col min="13" max="13" width="11.3984375" customWidth="1"/>
-    <col min="14" max="14" width="17.3984375" customWidth="1"/>
-    <col min="16" max="16" width="9.09765625" customWidth="1"/>
-    <col min="18" max="18" width="16.59765625" customWidth="1"/>
-    <col min="19" max="19" width="14.69921875" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="16.8984375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.109375" style="3" customWidth="1"/>
+    <col min="6" max="6" width="20.88671875" style="4" customWidth="1"/>
+    <col min="7" max="7" width="34.88671875" style="2" customWidth="1"/>
+    <col min="8" max="8" width="43.44140625" style="2" customWidth="1"/>
+    <col min="11" max="11" width="9.109375" customWidth="1"/>
+    <col min="12" max="12" width="13.33203125" customWidth="1"/>
+    <col min="13" max="13" width="11.44140625" customWidth="1"/>
+    <col min="14" max="14" width="17.44140625" customWidth="1"/>
+    <col min="16" max="16" width="9.109375" customWidth="1"/>
+    <col min="18" max="18" width="16.5546875" customWidth="1"/>
+    <col min="19" max="19" width="14.6640625" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="16.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="15.75">
+    <row r="1" spans="1:8" ht="15.6">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
@@ -985,7 +1096,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="15.75">
+    <row r="2" spans="1:8">
       <c r="A2" s="1">
         <v>45786</v>
       </c>
@@ -1011,7 +1122,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="3" spans="1:8" ht="120">
+    <row r="3" spans="1:8" ht="115.2">
       <c r="A3" s="1">
         <v>45787</v>
       </c>
@@ -1034,7 +1145,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="4" spans="1:8" ht="15">
+    <row r="4" spans="1:8">
       <c r="A4" s="1">
         <v>45788</v>
       </c>
@@ -1077,12 +1188,12 @@
         <v>27</v>
       </c>
     </row>
-    <row r="6" spans="1:8" ht="15">
-      <c r="A6" s="1" t="s">
+    <row r="6" spans="1:8">
+      <c r="A6" s="1">
+        <v>45790</v>
+      </c>
+      <c r="C6" t="s">
         <v>29</v>
-      </c>
-      <c r="C6" t="s">
-        <v>30</v>
       </c>
       <c r="D6" t="s">
         <v>17</v>
@@ -1094,41 +1205,143 @@
         <v>5</v>
       </c>
       <c r="G6" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="H6" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="H6" s="2" t="s">
+    </row>
+    <row r="7" spans="1:8">
+      <c r="A7" s="1">
+        <v>45791</v>
+      </c>
+      <c r="C7" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="7" spans="1:8" ht="15">
-      <c r="E7"/>
-      <c r="F7"/>
-    </row>
-    <row r="8" spans="1:8" ht="15">
-      <c r="E8"/>
-      <c r="F8"/>
-    </row>
-    <row r="9" spans="1:8" ht="15">
-      <c r="E9"/>
-      <c r="F9"/>
-    </row>
-    <row r="10" spans="1:8" ht="15">
-      <c r="E10"/>
-      <c r="F10"/>
-    </row>
-    <row r="11" spans="1:8" ht="15">
-      <c r="E11"/>
-      <c r="F11"/>
-    </row>
-    <row r="12" spans="1:8" ht="15">
-      <c r="E12"/>
-      <c r="F12"/>
-    </row>
-    <row r="13" spans="1:8" ht="15">
+      <c r="D7" t="s">
+        <v>17</v>
+      </c>
+      <c r="E7">
+        <v>100</v>
+      </c>
+      <c r="F7">
+        <v>2</v>
+      </c>
+      <c r="G7" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="H7" s="2" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8">
+      <c r="A8" s="1">
+        <v>45792</v>
+      </c>
+      <c r="C8" t="s">
+        <v>64</v>
+      </c>
+      <c r="D8" t="s">
+        <v>17</v>
+      </c>
+      <c r="E8">
+        <v>100</v>
+      </c>
+      <c r="F8">
+        <v>3</v>
+      </c>
+      <c r="G8" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="H8" s="2" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8">
+      <c r="A9" s="1">
+        <v>45793</v>
+      </c>
+      <c r="C9" t="s">
+        <v>73</v>
+      </c>
+      <c r="D9" t="s">
+        <v>17</v>
+      </c>
+      <c r="E9">
+        <v>100</v>
+      </c>
+      <c r="F9">
+        <v>1</v>
+      </c>
+      <c r="G9" s="2" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8">
+      <c r="A10" s="1">
+        <v>45794</v>
+      </c>
+      <c r="C10" t="s">
+        <v>79</v>
+      </c>
+      <c r="D10" t="s">
+        <v>37</v>
+      </c>
+      <c r="E10">
+        <v>10</v>
+      </c>
+      <c r="F10">
+        <v>1</v>
+      </c>
+      <c r="G10" s="2" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8">
+      <c r="A11" s="1">
+        <v>45795</v>
+      </c>
+      <c r="C11" t="s">
+        <v>75</v>
+      </c>
+      <c r="D11" t="s">
+        <v>37</v>
+      </c>
+      <c r="E11">
+        <v>50</v>
+      </c>
+      <c r="F11">
+        <v>1</v>
+      </c>
+      <c r="G11" s="2" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8">
+      <c r="A12" s="1">
+        <v>45796</v>
+      </c>
+      <c r="C12" t="s">
+        <v>77</v>
+      </c>
+      <c r="D12" t="s">
+        <v>17</v>
+      </c>
+      <c r="E12">
+        <v>100</v>
+      </c>
+      <c r="F12">
+        <v>1</v>
+      </c>
+      <c r="G12" s="2" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8">
       <c r="E13"/>
       <c r="F13"/>
     </row>
-    <row r="14" spans="1:8" ht="15">
+    <row r="14" spans="1:8">
       <c r="E14"/>
       <c r="F14"/>
     </row>
@@ -1196,7 +1409,7 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
   <ignoredErrors>
-    <ignoredError sqref="D7:D16" listDataValidation="1"/>
+    <ignoredError sqref="D13:D16" listDataValidation="1"/>
   </ignoredErrors>
   <tableParts count="1">
     <tablePart r:id="rId2"/>
@@ -1209,22 +1422,22 @@
   <dimension ref="A1:H100"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="H7" sqref="H7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="9.8984375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="17.296875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="54.69921875" customWidth="1"/>
-    <col min="4" max="4" width="8.8984375" customWidth="1"/>
-    <col min="5" max="5" width="14.8984375" style="11" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="23.59765625" style="11" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="29.19921875" customWidth="1"/>
-    <col min="8" max="8" width="39.69921875" customWidth="1"/>
+    <col min="1" max="1" width="10.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="55.5546875" customWidth="1"/>
+    <col min="4" max="4" width="10.5546875" customWidth="1"/>
+    <col min="5" max="5" width="14.88671875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.33203125" customWidth="1"/>
+    <col min="7" max="7" width="92.88671875" customWidth="1"/>
+    <col min="8" max="8" width="82.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="15.75">
+    <row r="1" spans="1:8" ht="15.6">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
@@ -1237,10 +1450,10 @@
       <c r="D1" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="10" t="s">
+      <c r="E1" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="10" t="s">
+      <c r="F1" s="7" t="s">
         <v>5</v>
       </c>
       <c r="G1" s="7" t="s">
@@ -1250,221 +1463,259 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="15">
+    <row r="2" spans="1:8">
       <c r="A2" s="8">
         <v>45786</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="C2" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="D2" t="s">
-        <v>35</v>
-      </c>
-      <c r="E2" s="11">
+        <v>37</v>
+      </c>
+      <c r="E2">
         <v>90</v>
       </c>
-      <c r="F2" s="11">
+      <c r="F2">
         <v>8</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="H2" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" ht="15">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8">
       <c r="A3" s="8">
         <v>45787</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="C3" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="D3" t="s">
-        <v>35</v>
-      </c>
-      <c r="E3" s="11">
+        <v>37</v>
+      </c>
+      <c r="E3">
         <v>90</v>
       </c>
-      <c r="F3" s="11">
+      <c r="F3">
         <v>8</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="H3" s="2" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="4" spans="1:8" ht="15">
+    <row r="4" spans="1:8">
       <c r="A4" s="8">
         <v>45789</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="C4" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="D4" t="s">
-        <v>35</v>
-      </c>
-      <c r="E4" s="11">
+        <v>37</v>
+      </c>
+      <c r="E4">
         <v>90</v>
       </c>
-      <c r="F4" s="11">
+      <c r="F4">
         <v>5</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="H4" s="2"/>
     </row>
-    <row r="5" spans="1:8" ht="15">
+    <row r="5" spans="1:8">
       <c r="A5" s="8">
         <v>45790</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="C5" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="D5" t="s">
         <v>17</v>
       </c>
-      <c r="E5" s="11">
+      <c r="E5">
         <v>100</v>
       </c>
-      <c r="F5" s="11">
+      <c r="F5">
         <v>5</v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="H5" s="2"/>
     </row>
-    <row r="6" spans="1:8" ht="15">
-      <c r="A6" s="8"/>
-      <c r="B6" s="2"/>
-      <c r="G6" s="2"/>
-      <c r="H6" s="2"/>
-    </row>
-    <row r="7" spans="1:8" ht="15">
-      <c r="A7" s="8"/>
-      <c r="B7" s="2"/>
+    <row r="6" spans="1:8">
+      <c r="A6" s="8">
+        <v>45791</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="C6" t="s">
+        <v>48</v>
+      </c>
+      <c r="D6" t="s">
+        <v>17</v>
+      </c>
+      <c r="E6">
+        <v>100</v>
+      </c>
+      <c r="F6">
+        <v>5</v>
+      </c>
+      <c r="G6" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="H6" s="2" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8">
+      <c r="A7" s="8">
+        <v>45795</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="C7" t="s">
+        <v>81</v>
+      </c>
+      <c r="D7" t="s">
+        <v>17</v>
+      </c>
+      <c r="E7">
+        <v>100</v>
+      </c>
+      <c r="F7">
+        <v>5</v>
+      </c>
       <c r="G7" s="2"/>
-      <c r="H7" s="2"/>
-    </row>
-    <row r="8" spans="1:8" ht="15">
+      <c r="H7" s="2" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8">
       <c r="A8" s="8"/>
       <c r="B8" s="2"/>
       <c r="G8" s="2"/>
       <c r="H8" s="2"/>
     </row>
-    <row r="9" spans="1:8" ht="15">
+    <row r="9" spans="1:8">
       <c r="A9" s="8"/>
       <c r="B9" s="2"/>
       <c r="G9" s="2"/>
       <c r="H9" s="2"/>
     </row>
-    <row r="10" spans="1:8" ht="15">
+    <row r="10" spans="1:8">
       <c r="A10" s="8"/>
       <c r="B10" s="2"/>
       <c r="G10" s="2"/>
       <c r="H10" s="2"/>
     </row>
-    <row r="11" spans="1:8" ht="15">
+    <row r="11" spans="1:8">
       <c r="A11" s="8"/>
       <c r="B11" s="2"/>
       <c r="G11" s="2"/>
       <c r="H11" s="2"/>
     </row>
-    <row r="12" spans="1:8" ht="15">
+    <row r="12" spans="1:8">
       <c r="A12" s="8"/>
       <c r="B12" s="2"/>
       <c r="G12" s="2"/>
       <c r="H12" s="2"/>
     </row>
-    <row r="13" spans="1:8" ht="15">
+    <row r="13" spans="1:8">
       <c r="A13" s="8"/>
       <c r="B13" s="2"/>
       <c r="G13" s="2"/>
       <c r="H13" s="2"/>
     </row>
-    <row r="14" spans="1:8" ht="15">
+    <row r="14" spans="1:8">
       <c r="A14" s="8"/>
       <c r="B14" s="2"/>
       <c r="G14" s="2"/>
       <c r="H14" s="2"/>
     </row>
-    <row r="15" spans="1:8" ht="15">
+    <row r="15" spans="1:8">
       <c r="A15" s="8"/>
       <c r="B15" s="2"/>
       <c r="G15" s="2"/>
       <c r="H15" s="2"/>
     </row>
-    <row r="16" spans="1:8" ht="15">
+    <row r="16" spans="1:8">
       <c r="A16" s="8"/>
       <c r="B16" s="2"/>
       <c r="G16" s="2"/>
       <c r="H16" s="2"/>
     </row>
-    <row r="17" spans="1:8" ht="15">
+    <row r="17" spans="1:8">
       <c r="A17" s="8"/>
       <c r="B17" s="2"/>
       <c r="G17" s="2"/>
       <c r="H17" s="2"/>
     </row>
-    <row r="18" spans="1:8" ht="15">
+    <row r="18" spans="1:8">
       <c r="A18" s="8"/>
       <c r="B18" s="2"/>
       <c r="G18" s="2"/>
       <c r="H18" s="2"/>
     </row>
-    <row r="19" spans="1:8" ht="15">
+    <row r="19" spans="1:8">
       <c r="A19" s="8"/>
       <c r="B19" s="2"/>
       <c r="G19" s="2"/>
       <c r="H19" s="2"/>
     </row>
-    <row r="20" spans="1:8" ht="15">
+    <row r="20" spans="1:8">
       <c r="A20" s="8"/>
       <c r="B20" s="2"/>
       <c r="G20" s="2"/>
       <c r="H20" s="2"/>
     </row>
-    <row r="21" spans="1:8" ht="15">
+    <row r="21" spans="1:8">
       <c r="A21" s="8"/>
       <c r="B21" s="2"/>
       <c r="G21" s="2"/>
       <c r="H21" s="2"/>
     </row>
-    <row r="22" spans="1:8" ht="15">
+    <row r="22" spans="1:8">
       <c r="A22" s="8"/>
       <c r="B22" s="2"/>
       <c r="G22" s="2"/>
       <c r="H22" s="2"/>
     </row>
-    <row r="23" spans="1:8" ht="15">
+    <row r="23" spans="1:8">
       <c r="A23" s="8"/>
       <c r="B23" s="2"/>
       <c r="G23" s="2"/>
       <c r="H23" s="2"/>
     </row>
-    <row r="24" spans="1:8" ht="15">
+    <row r="24" spans="1:8">
       <c r="A24" s="8"/>
       <c r="B24" s="2"/>
       <c r="G24" s="2"/>
       <c r="H24" s="2"/>
     </row>
-    <row r="25" spans="1:8" ht="15">
+    <row r="25" spans="1:8">
       <c r="A25" s="8"/>
       <c r="B25" s="2"/>
       <c r="G25" s="2"/>
@@ -1939,7 +2190,7 @@
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <ignoredErrors>
-    <ignoredError sqref="D6:D100" listDataValidation="1"/>
+    <ignoredError sqref="D8:D100" listDataValidation="1"/>
   </ignoredErrors>
   <tableParts count="1">
     <tablePart r:id="rId1"/>
@@ -1951,23 +2202,23 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9FD6A201-8E63-4A9E-A683-19506CB489E3}">
   <dimension ref="A1:H100"/>
   <sheetViews>
-    <sheetView topLeftCell="A63" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2:D100"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="7.69921875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="17.296875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.59765625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.8984375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="23.59765625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="13.3984375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="19.09765625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="27.88671875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.88671875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="23.5546875" style="10" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="39.109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="51.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="15.75">
+    <row r="1" spans="1:8" ht="15.6">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
@@ -1983,7 +2234,7 @@
       <c r="E1" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="7" t="s">
+      <c r="F1" s="11" t="s">
         <v>5</v>
       </c>
       <c r="G1" s="7" t="s">
@@ -1993,691 +2244,719 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="15">
-      <c r="A2" s="1"/>
-      <c r="B2" s="2"/>
-      <c r="E2" s="3"/>
-      <c r="F2" s="4"/>
-      <c r="G2" s="2"/>
-      <c r="H2" s="2"/>
-    </row>
-    <row r="3" spans="1:8" ht="15">
-      <c r="A3" s="1"/>
-      <c r="B3" s="2"/>
-      <c r="E3" s="3"/>
-      <c r="F3" s="4"/>
-      <c r="G3" s="2"/>
-      <c r="H3" s="2"/>
-    </row>
-    <row r="4" spans="1:8" ht="15">
-      <c r="A4" s="1"/>
-      <c r="B4" s="2"/>
-      <c r="E4" s="3"/>
-      <c r="F4" s="4"/>
-      <c r="G4" s="2"/>
-      <c r="H4" s="2"/>
-    </row>
-    <row r="5" spans="1:8" ht="15">
-      <c r="A5" s="1"/>
-      <c r="B5" s="2"/>
-      <c r="E5" s="3"/>
-      <c r="F5" s="4"/>
-      <c r="G5" s="2"/>
-      <c r="H5" s="2"/>
-    </row>
-    <row r="6" spans="1:8" ht="15">
-      <c r="A6" s="1"/>
-      <c r="B6" s="2"/>
-      <c r="E6" s="3"/>
-      <c r="F6" s="4"/>
-      <c r="G6" s="2"/>
-      <c r="H6" s="2"/>
-    </row>
-    <row r="7" spans="1:8" ht="15">
-      <c r="A7" s="1"/>
-      <c r="B7" s="2"/>
-      <c r="E7" s="3"/>
-      <c r="F7" s="4"/>
-      <c r="G7" s="2"/>
-      <c r="H7" s="2"/>
-    </row>
-    <row r="8" spans="1:8" ht="15">
+    <row r="2" spans="1:8">
+      <c r="A2" s="1">
+        <v>45935</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="C2" t="s">
+        <v>52</v>
+      </c>
+      <c r="D2" t="s">
+        <v>17</v>
+      </c>
+      <c r="E2" s="3">
+        <v>1</v>
+      </c>
+      <c r="F2" s="10">
+        <v>4</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8">
+      <c r="A3" s="1">
+        <v>45996</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="C3" t="s">
+        <v>55</v>
+      </c>
+      <c r="D3" t="s">
+        <v>17</v>
+      </c>
+      <c r="E3" s="3">
+        <v>1</v>
+      </c>
+      <c r="F3" s="10">
+        <v>4</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="H3" s="2" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8">
+      <c r="A4" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="C4" t="s">
+        <v>58</v>
+      </c>
+      <c r="D4" t="s">
+        <v>17</v>
+      </c>
+      <c r="E4" s="3">
+        <v>1</v>
+      </c>
+      <c r="F4" s="10">
+        <v>4</v>
+      </c>
+      <c r="G4" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="H4" s="2" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8">
+      <c r="A5" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="C5" t="s">
+        <v>62</v>
+      </c>
+      <c r="D5" t="s">
+        <v>17</v>
+      </c>
+      <c r="E5" s="3">
+        <v>1</v>
+      </c>
+      <c r="F5" s="10">
+        <v>5</v>
+      </c>
+      <c r="G5" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="H5" s="2" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8">
+      <c r="A6" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="C6" t="s">
+        <v>68</v>
+      </c>
+      <c r="D6" t="s">
+        <v>17</v>
+      </c>
+      <c r="E6" s="3">
+        <v>1</v>
+      </c>
+      <c r="F6" s="10">
+        <v>3</v>
+      </c>
+      <c r="G6" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="H6" s="2" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8">
+      <c r="A7" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="C7" t="s">
+        <v>71</v>
+      </c>
+      <c r="D7" t="s">
+        <v>17</v>
+      </c>
+      <c r="E7" s="3">
+        <v>1</v>
+      </c>
+      <c r="F7" s="10">
+        <v>5</v>
+      </c>
+      <c r="G7" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="H7" s="2" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8">
       <c r="A8" s="1"/>
       <c r="B8" s="2"/>
       <c r="E8" s="3"/>
-      <c r="F8" s="4"/>
       <c r="G8" s="2"/>
       <c r="H8" s="2"/>
     </row>
-    <row r="9" spans="1:8" ht="15">
+    <row r="9" spans="1:8">
       <c r="A9" s="1"/>
       <c r="B9" s="2"/>
       <c r="E9" s="3"/>
-      <c r="F9" s="4"/>
       <c r="G9" s="2"/>
       <c r="H9" s="2"/>
     </row>
-    <row r="10" spans="1:8" ht="15">
+    <row r="10" spans="1:8">
       <c r="A10" s="1"/>
       <c r="B10" s="2"/>
       <c r="E10" s="3"/>
-      <c r="F10" s="4"/>
       <c r="G10" s="2"/>
       <c r="H10" s="2"/>
     </row>
-    <row r="11" spans="1:8" ht="15">
+    <row r="11" spans="1:8">
       <c r="A11" s="1"/>
       <c r="B11" s="2"/>
       <c r="E11" s="3"/>
-      <c r="F11" s="4"/>
       <c r="G11" s="2"/>
       <c r="H11" s="2"/>
     </row>
-    <row r="12" spans="1:8" ht="15">
+    <row r="12" spans="1:8">
       <c r="A12" s="1"/>
       <c r="B12" s="2"/>
       <c r="E12" s="3"/>
-      <c r="F12" s="4"/>
       <c r="G12" s="2"/>
       <c r="H12" s="2"/>
     </row>
-    <row r="13" spans="1:8" ht="15">
+    <row r="13" spans="1:8">
       <c r="A13" s="1"/>
       <c r="B13" s="2"/>
       <c r="E13" s="3"/>
-      <c r="F13" s="4"/>
       <c r="G13" s="2"/>
       <c r="H13" s="2"/>
     </row>
-    <row r="14" spans="1:8" ht="15">
+    <row r="14" spans="1:8">
       <c r="A14" s="1"/>
       <c r="B14" s="2"/>
       <c r="E14" s="3"/>
-      <c r="F14" s="4"/>
       <c r="G14" s="2"/>
       <c r="H14" s="2"/>
     </row>
-    <row r="15" spans="1:8" ht="15">
+    <row r="15" spans="1:8">
       <c r="A15" s="1"/>
       <c r="B15" s="2"/>
       <c r="E15" s="3"/>
-      <c r="F15" s="4"/>
       <c r="G15" s="2"/>
       <c r="H15" s="2"/>
     </row>
-    <row r="16" spans="1:8" ht="15">
+    <row r="16" spans="1:8">
       <c r="A16" s="1"/>
       <c r="B16" s="2"/>
       <c r="E16" s="3"/>
-      <c r="F16" s="4"/>
       <c r="G16" s="2"/>
       <c r="H16" s="2"/>
     </row>
-    <row r="17" spans="1:8" ht="15">
+    <row r="17" spans="1:8">
       <c r="A17" s="1"/>
       <c r="B17" s="2"/>
       <c r="E17" s="3"/>
-      <c r="F17" s="4"/>
       <c r="G17" s="2"/>
       <c r="H17" s="2"/>
     </row>
-    <row r="18" spans="1:8" ht="15">
+    <row r="18" spans="1:8">
       <c r="A18" s="1"/>
       <c r="B18" s="2"/>
       <c r="E18" s="3"/>
-      <c r="F18" s="4"/>
       <c r="G18" s="2"/>
       <c r="H18" s="2"/>
     </row>
-    <row r="19" spans="1:8" ht="15">
+    <row r="19" spans="1:8">
       <c r="A19" s="1"/>
       <c r="B19" s="2"/>
       <c r="E19" s="3"/>
-      <c r="F19" s="4"/>
       <c r="G19" s="2"/>
       <c r="H19" s="2"/>
     </row>
-    <row r="20" spans="1:8" ht="15">
+    <row r="20" spans="1:8">
       <c r="A20" s="1"/>
       <c r="B20" s="2"/>
       <c r="E20" s="3"/>
-      <c r="F20" s="4"/>
       <c r="G20" s="2"/>
       <c r="H20" s="2"/>
     </row>
-    <row r="21" spans="1:8" ht="15">
+    <row r="21" spans="1:8">
       <c r="A21" s="1"/>
       <c r="B21" s="2"/>
       <c r="E21" s="3"/>
-      <c r="F21" s="4"/>
       <c r="G21" s="2"/>
       <c r="H21" s="2"/>
     </row>
-    <row r="22" spans="1:8" ht="15">
+    <row r="22" spans="1:8">
       <c r="A22" s="1"/>
       <c r="B22" s="2"/>
       <c r="E22" s="3"/>
-      <c r="F22" s="4"/>
       <c r="G22" s="2"/>
       <c r="H22" s="2"/>
     </row>
-    <row r="23" spans="1:8" ht="15">
+    <row r="23" spans="1:8">
       <c r="A23" s="1"/>
       <c r="B23" s="2"/>
       <c r="E23" s="3"/>
-      <c r="F23" s="4"/>
       <c r="G23" s="2"/>
       <c r="H23" s="2"/>
     </row>
-    <row r="24" spans="1:8" ht="15">
+    <row r="24" spans="1:8">
       <c r="A24" s="1"/>
       <c r="B24" s="2"/>
       <c r="E24" s="3"/>
-      <c r="F24" s="4"/>
       <c r="G24" s="2"/>
       <c r="H24" s="2"/>
     </row>
-    <row r="25" spans="1:8" ht="15">
+    <row r="25" spans="1:8">
       <c r="A25" s="1"/>
       <c r="B25" s="2"/>
       <c r="E25" s="3"/>
-      <c r="F25" s="4"/>
       <c r="G25" s="2"/>
       <c r="H25" s="2"/>
     </row>
-    <row r="26" spans="1:8" ht="15">
+    <row r="26" spans="1:8">
       <c r="A26" s="1"/>
       <c r="B26" s="2"/>
       <c r="E26" s="3"/>
-      <c r="F26" s="4"/>
       <c r="G26" s="2"/>
       <c r="H26" s="2"/>
     </row>
-    <row r="27" spans="1:8" ht="15">
+    <row r="27" spans="1:8">
       <c r="A27" s="1"/>
       <c r="B27" s="2"/>
       <c r="E27" s="3"/>
-      <c r="F27" s="4"/>
       <c r="G27" s="2"/>
       <c r="H27" s="2"/>
     </row>
-    <row r="28" spans="1:8" ht="15">
+    <row r="28" spans="1:8">
       <c r="A28" s="1"/>
       <c r="B28" s="2"/>
       <c r="E28" s="3"/>
-      <c r="F28" s="4"/>
       <c r="G28" s="2"/>
       <c r="H28" s="2"/>
     </row>
-    <row r="29" spans="1:8" ht="15">
+    <row r="29" spans="1:8">
       <c r="A29" s="1"/>
       <c r="B29" s="2"/>
       <c r="E29" s="3"/>
-      <c r="F29" s="4"/>
       <c r="G29" s="2"/>
       <c r="H29" s="2"/>
     </row>
-    <row r="30" spans="1:8" ht="15">
+    <row r="30" spans="1:8">
       <c r="A30" s="1"/>
       <c r="B30" s="2"/>
       <c r="E30" s="3"/>
-      <c r="F30" s="4"/>
       <c r="G30" s="2"/>
       <c r="H30" s="2"/>
     </row>
-    <row r="31" spans="1:8" ht="15">
+    <row r="31" spans="1:8">
       <c r="A31" s="1"/>
       <c r="B31" s="2"/>
       <c r="E31" s="3"/>
-      <c r="F31" s="4"/>
       <c r="G31" s="2"/>
       <c r="H31" s="2"/>
     </row>
-    <row r="32" spans="1:8" ht="15">
+    <row r="32" spans="1:8">
       <c r="A32" s="1"/>
       <c r="B32" s="2"/>
       <c r="E32" s="3"/>
-      <c r="F32" s="4"/>
       <c r="G32" s="2"/>
       <c r="H32" s="2"/>
     </row>
-    <row r="33" spans="1:8" ht="15">
+    <row r="33" spans="1:8">
       <c r="A33" s="1"/>
       <c r="B33" s="2"/>
       <c r="E33" s="3"/>
-      <c r="F33" s="4"/>
       <c r="G33" s="2"/>
       <c r="H33" s="2"/>
     </row>
-    <row r="34" spans="1:8" ht="15">
+    <row r="34" spans="1:8">
       <c r="A34" s="1"/>
       <c r="B34" s="2"/>
       <c r="E34" s="3"/>
-      <c r="F34" s="4"/>
       <c r="G34" s="2"/>
       <c r="H34" s="2"/>
     </row>
-    <row r="35" spans="1:8" ht="15">
+    <row r="35" spans="1:8">
       <c r="A35" s="1"/>
       <c r="B35" s="2"/>
       <c r="E35" s="3"/>
-      <c r="F35" s="4"/>
       <c r="G35" s="2"/>
       <c r="H35" s="2"/>
     </row>
-    <row r="36" spans="1:8" ht="15">
+    <row r="36" spans="1:8">
       <c r="A36" s="1"/>
       <c r="B36" s="2"/>
       <c r="E36" s="3"/>
-      <c r="F36" s="4"/>
       <c r="G36" s="2"/>
       <c r="H36" s="2"/>
     </row>
-    <row r="37" spans="1:8" ht="15">
+    <row r="37" spans="1:8">
       <c r="A37" s="1"/>
       <c r="B37" s="2"/>
       <c r="E37" s="3"/>
-      <c r="F37" s="4"/>
       <c r="G37" s="2"/>
       <c r="H37" s="2"/>
     </row>
-    <row r="38" spans="1:8" ht="15">
+    <row r="38" spans="1:8">
       <c r="A38" s="1"/>
       <c r="B38" s="2"/>
       <c r="E38" s="3"/>
-      <c r="F38" s="4"/>
       <c r="G38" s="2"/>
       <c r="H38" s="2"/>
     </row>
-    <row r="39" spans="1:8" ht="15">
+    <row r="39" spans="1:8">
       <c r="A39" s="1"/>
       <c r="B39" s="2"/>
       <c r="E39" s="3"/>
-      <c r="F39" s="4"/>
       <c r="G39" s="2"/>
       <c r="H39" s="2"/>
     </row>
-    <row r="40" spans="1:8" ht="15">
+    <row r="40" spans="1:8">
       <c r="A40" s="1"/>
       <c r="B40" s="2"/>
       <c r="E40" s="3"/>
-      <c r="F40" s="4"/>
       <c r="G40" s="2"/>
       <c r="H40" s="2"/>
     </row>
-    <row r="41" spans="1:8" ht="15">
+    <row r="41" spans="1:8">
       <c r="A41" s="1"/>
       <c r="B41" s="2"/>
       <c r="E41" s="3"/>
-      <c r="F41" s="4"/>
       <c r="G41" s="2"/>
       <c r="H41" s="2"/>
     </row>
-    <row r="42" spans="1:8" ht="15">
+    <row r="42" spans="1:8">
       <c r="A42" s="1"/>
       <c r="B42" s="2"/>
       <c r="E42" s="3"/>
-      <c r="F42" s="4"/>
       <c r="G42" s="2"/>
       <c r="H42" s="2"/>
     </row>
-    <row r="43" spans="1:8" ht="15">
+    <row r="43" spans="1:8">
       <c r="A43" s="1"/>
       <c r="B43" s="2"/>
       <c r="E43" s="3"/>
-      <c r="F43" s="4"/>
       <c r="G43" s="2"/>
       <c r="H43" s="2"/>
     </row>
-    <row r="44" spans="1:8" ht="15">
+    <row r="44" spans="1:8">
       <c r="A44" s="1"/>
       <c r="B44" s="2"/>
       <c r="E44" s="3"/>
-      <c r="F44" s="4"/>
       <c r="G44" s="2"/>
       <c r="H44" s="2"/>
     </row>
-    <row r="45" spans="1:8" ht="15">
+    <row r="45" spans="1:8">
       <c r="A45" s="1"/>
       <c r="B45" s="2"/>
       <c r="E45" s="3"/>
-      <c r="F45" s="4"/>
       <c r="G45" s="2"/>
       <c r="H45" s="2"/>
     </row>
-    <row r="46" spans="1:8" ht="15">
+    <row r="46" spans="1:8">
       <c r="A46" s="1"/>
       <c r="B46" s="2"/>
       <c r="E46" s="3"/>
-      <c r="F46" s="4"/>
       <c r="G46" s="2"/>
       <c r="H46" s="2"/>
     </row>
-    <row r="47" spans="1:8" ht="15">
+    <row r="47" spans="1:8">
       <c r="A47" s="1"/>
       <c r="B47" s="2"/>
       <c r="E47" s="3"/>
-      <c r="F47" s="4"/>
       <c r="G47" s="2"/>
       <c r="H47" s="2"/>
     </row>
-    <row r="48" spans="1:8" ht="15">
+    <row r="48" spans="1:8">
       <c r="A48" s="1"/>
       <c r="B48" s="2"/>
       <c r="E48" s="3"/>
-      <c r="F48" s="4"/>
       <c r="G48" s="2"/>
       <c r="H48" s="2"/>
     </row>
-    <row r="49" spans="1:8" ht="15">
+    <row r="49" spans="1:8">
       <c r="A49" s="1"/>
       <c r="B49" s="2"/>
       <c r="E49" s="3"/>
-      <c r="F49" s="4"/>
       <c r="G49" s="2"/>
       <c r="H49" s="2"/>
     </row>
-    <row r="50" spans="1:8" ht="15">
+    <row r="50" spans="1:8">
       <c r="A50" s="1"/>
       <c r="B50" s="2"/>
       <c r="E50" s="3"/>
-      <c r="F50" s="4"/>
       <c r="G50" s="2"/>
       <c r="H50" s="2"/>
     </row>
-    <row r="51" spans="1:8" ht="15">
+    <row r="51" spans="1:8">
       <c r="A51" s="1"/>
       <c r="B51" s="2"/>
       <c r="E51" s="3"/>
-      <c r="F51" s="4"/>
       <c r="G51" s="2"/>
       <c r="H51" s="2"/>
     </row>
-    <row r="52" spans="1:8" ht="15">
+    <row r="52" spans="1:8">
       <c r="A52" s="1"/>
       <c r="B52" s="2"/>
       <c r="E52" s="3"/>
-      <c r="F52" s="4"/>
       <c r="G52" s="2"/>
       <c r="H52" s="2"/>
     </row>
-    <row r="53" spans="1:8" ht="15">
+    <row r="53" spans="1:8">
       <c r="A53" s="1"/>
       <c r="B53" s="2"/>
       <c r="E53" s="3"/>
-      <c r="F53" s="4"/>
       <c r="G53" s="2"/>
       <c r="H53" s="2"/>
     </row>
-    <row r="54" spans="1:8" ht="15">
+    <row r="54" spans="1:8">
       <c r="A54" s="1"/>
       <c r="B54" s="2"/>
       <c r="E54" s="3"/>
-      <c r="F54" s="4"/>
       <c r="G54" s="2"/>
       <c r="H54" s="2"/>
     </row>
-    <row r="55" spans="1:8" ht="15">
+    <row r="55" spans="1:8">
       <c r="A55" s="1"/>
       <c r="B55" s="2"/>
       <c r="E55" s="3"/>
-      <c r="F55" s="4"/>
       <c r="G55" s="2"/>
       <c r="H55" s="2"/>
     </row>
-    <row r="56" spans="1:8" ht="15">
+    <row r="56" spans="1:8">
       <c r="A56" s="1"/>
       <c r="B56" s="2"/>
       <c r="E56" s="3"/>
-      <c r="F56" s="4"/>
       <c r="G56" s="2"/>
       <c r="H56" s="2"/>
     </row>
-    <row r="57" spans="1:8" ht="15">
+    <row r="57" spans="1:8">
       <c r="A57" s="1"/>
       <c r="B57" s="2"/>
       <c r="E57" s="3"/>
-      <c r="F57" s="4"/>
       <c r="G57" s="2"/>
       <c r="H57" s="2"/>
     </row>
-    <row r="58" spans="1:8" ht="15">
+    <row r="58" spans="1:8">
       <c r="A58" s="1"/>
       <c r="B58" s="2"/>
       <c r="E58" s="3"/>
-      <c r="F58" s="4"/>
       <c r="G58" s="2"/>
       <c r="H58" s="2"/>
     </row>
-    <row r="59" spans="1:8" ht="15">
+    <row r="59" spans="1:8">
       <c r="A59" s="1"/>
       <c r="B59" s="2"/>
       <c r="E59" s="3"/>
-      <c r="F59" s="4"/>
       <c r="G59" s="2"/>
       <c r="H59" s="2"/>
     </row>
-    <row r="60" spans="1:8" ht="15">
+    <row r="60" spans="1:8">
       <c r="A60" s="1"/>
       <c r="B60" s="2"/>
       <c r="E60" s="3"/>
-      <c r="F60" s="4"/>
       <c r="G60" s="2"/>
       <c r="H60" s="2"/>
     </row>
-    <row r="61" spans="1:8" ht="15">
+    <row r="61" spans="1:8">
       <c r="A61" s="1"/>
       <c r="B61" s="2"/>
       <c r="E61" s="3"/>
-      <c r="F61" s="4"/>
       <c r="G61" s="2"/>
       <c r="H61" s="2"/>
     </row>
-    <row r="62" spans="1:8" ht="15">
+    <row r="62" spans="1:8">
       <c r="A62" s="1"/>
       <c r="B62" s="2"/>
       <c r="E62" s="3"/>
-      <c r="F62" s="4"/>
       <c r="G62" s="2"/>
       <c r="H62" s="2"/>
     </row>
-    <row r="63" spans="1:8" ht="15">
+    <row r="63" spans="1:8">
       <c r="A63" s="1"/>
       <c r="B63" s="2"/>
       <c r="E63" s="3"/>
-      <c r="F63" s="4"/>
       <c r="G63" s="2"/>
       <c r="H63" s="2"/>
     </row>
-    <row r="64" spans="1:8" ht="15">
+    <row r="64" spans="1:8">
       <c r="A64" s="1"/>
       <c r="B64" s="2"/>
       <c r="E64" s="3"/>
-      <c r="F64" s="4"/>
       <c r="G64" s="2"/>
       <c r="H64" s="2"/>
     </row>
-    <row r="65" spans="1:8" ht="15">
+    <row r="65" spans="1:8">
       <c r="A65" s="1"/>
       <c r="B65" s="2"/>
       <c r="E65" s="3"/>
-      <c r="F65" s="4"/>
       <c r="G65" s="2"/>
       <c r="H65" s="2"/>
     </row>
-    <row r="66" spans="1:8" ht="15">
+    <row r="66" spans="1:8">
       <c r="A66" s="1"/>
       <c r="B66" s="2"/>
       <c r="E66" s="3"/>
-      <c r="F66" s="4"/>
       <c r="G66" s="2"/>
       <c r="H66" s="2"/>
     </row>
-    <row r="67" spans="1:8" ht="15">
+    <row r="67" spans="1:8">
       <c r="A67" s="1"/>
       <c r="B67" s="2"/>
       <c r="E67" s="3"/>
-      <c r="F67" s="4"/>
       <c r="G67" s="2"/>
       <c r="H67" s="2"/>
     </row>
-    <row r="68" spans="1:8" ht="15">
+    <row r="68" spans="1:8">
       <c r="A68" s="1"/>
       <c r="B68" s="2"/>
       <c r="E68" s="3"/>
-      <c r="F68" s="4"/>
       <c r="G68" s="2"/>
       <c r="H68" s="2"/>
     </row>
-    <row r="69" spans="1:8" ht="15">
+    <row r="69" spans="1:8">
       <c r="A69" s="1"/>
       <c r="B69" s="2"/>
       <c r="E69" s="3"/>
-      <c r="F69" s="4"/>
       <c r="G69" s="2"/>
       <c r="H69" s="2"/>
     </row>
-    <row r="70" spans="1:8" ht="15">
+    <row r="70" spans="1:8">
       <c r="A70" s="1"/>
       <c r="B70" s="2"/>
       <c r="E70" s="3"/>
-      <c r="F70" s="4"/>
       <c r="G70" s="2"/>
       <c r="H70" s="2"/>
     </row>
-    <row r="71" spans="1:8" ht="15">
+    <row r="71" spans="1:8">
       <c r="A71" s="1"/>
       <c r="B71" s="2"/>
       <c r="E71" s="3"/>
-      <c r="F71" s="4"/>
       <c r="G71" s="2"/>
       <c r="H71" s="2"/>
     </row>
-    <row r="72" spans="1:8" ht="15">
+    <row r="72" spans="1:8">
       <c r="A72" s="1"/>
       <c r="B72" s="2"/>
       <c r="E72" s="3"/>
-      <c r="F72" s="4"/>
       <c r="G72" s="2"/>
       <c r="H72" s="2"/>
     </row>
-    <row r="73" spans="1:8" ht="15">
+    <row r="73" spans="1:8">
       <c r="A73" s="1"/>
       <c r="B73" s="2"/>
       <c r="E73" s="3"/>
-      <c r="F73" s="4"/>
       <c r="G73" s="2"/>
       <c r="H73" s="2"/>
     </row>
-    <row r="74" spans="1:8" ht="15">
+    <row r="74" spans="1:8">
       <c r="A74" s="1"/>
       <c r="B74" s="2"/>
       <c r="E74" s="3"/>
-      <c r="F74" s="4"/>
       <c r="G74" s="2"/>
       <c r="H74" s="2"/>
     </row>
-    <row r="75" spans="1:8" ht="15">
+    <row r="75" spans="1:8">
       <c r="A75" s="1"/>
       <c r="B75" s="2"/>
       <c r="E75" s="3"/>
-      <c r="F75" s="4"/>
       <c r="G75" s="2"/>
       <c r="H75" s="2"/>
     </row>
-    <row r="76" spans="1:8" ht="15">
+    <row r="76" spans="1:8">
       <c r="A76" s="1"/>
       <c r="B76" s="2"/>
       <c r="E76" s="3"/>
-      <c r="F76" s="4"/>
       <c r="G76" s="2"/>
       <c r="H76" s="2"/>
     </row>
-    <row r="77" spans="1:8" ht="15">
+    <row r="77" spans="1:8">
       <c r="A77" s="1"/>
       <c r="B77" s="2"/>
       <c r="E77" s="3"/>
-      <c r="F77" s="4"/>
       <c r="G77" s="2"/>
       <c r="H77" s="2"/>
     </row>
-    <row r="78" spans="1:8" ht="15">
+    <row r="78" spans="1:8">
       <c r="A78" s="1"/>
       <c r="B78" s="2"/>
       <c r="E78" s="3"/>
-      <c r="F78" s="4"/>
       <c r="G78" s="2"/>
       <c r="H78" s="2"/>
     </row>
-    <row r="79" spans="1:8" ht="15">
+    <row r="79" spans="1:8">
       <c r="A79" s="1"/>
       <c r="B79" s="2"/>
       <c r="E79" s="3"/>
-      <c r="F79" s="4"/>
       <c r="G79" s="2"/>
       <c r="H79" s="2"/>
     </row>
-    <row r="80" spans="1:8" ht="15">
+    <row r="80" spans="1:8">
       <c r="A80" s="1"/>
       <c r="B80" s="2"/>
       <c r="E80" s="3"/>
-      <c r="F80" s="4"/>
       <c r="G80" s="2"/>
       <c r="H80" s="2"/>
     </row>
-    <row r="81" spans="1:8" ht="15">
+    <row r="81" spans="1:8">
       <c r="A81" s="1"/>
       <c r="B81" s="2"/>
       <c r="E81" s="3"/>
-      <c r="F81" s="4"/>
       <c r="G81" s="2"/>
       <c r="H81" s="2"/>
     </row>
-    <row r="82" spans="1:8" ht="15">
+    <row r="82" spans="1:8">
       <c r="A82" s="1"/>
       <c r="B82" s="2"/>
       <c r="E82" s="3"/>
-      <c r="F82" s="4"/>
       <c r="G82" s="2"/>
       <c r="H82" s="2"/>
     </row>
-    <row r="83" spans="1:8" ht="15">
+    <row r="83" spans="1:8">
       <c r="A83" s="1"/>
       <c r="B83" s="2"/>
       <c r="E83" s="3"/>
-      <c r="F83" s="4"/>
       <c r="G83" s="2"/>
       <c r="H83" s="2"/>
     </row>
-    <row r="84" spans="1:8" ht="15">
+    <row r="84" spans="1:8">
       <c r="A84" s="1"/>
       <c r="B84" s="2"/>
       <c r="E84" s="3"/>
-      <c r="F84" s="4"/>
       <c r="G84" s="2"/>
       <c r="H84" s="2"/>
     </row>
-    <row r="85" spans="1:8" ht="15">
+    <row r="85" spans="1:8">
       <c r="A85" s="1"/>
       <c r="B85" s="2"/>
       <c r="E85" s="3"/>
-      <c r="F85" s="4"/>
       <c r="G85" s="2"/>
       <c r="H85" s="2"/>
     </row>
-    <row r="86" spans="1:8" ht="15">
+    <row r="86" spans="1:8">
       <c r="A86" s="1"/>
       <c r="B86" s="2"/>
       <c r="E86" s="3"/>
-      <c r="F86" s="4"/>
       <c r="G86" s="2"/>
       <c r="H86" s="2"/>
     </row>
-    <row r="87" spans="1:8" ht="15">
+    <row r="87" spans="1:8">
       <c r="A87" s="1"/>
       <c r="B87" s="2"/>
       <c r="E87" s="3"/>
-      <c r="F87" s="4"/>
       <c r="G87" s="2"/>
       <c r="H87" s="2"/>
     </row>
@@ -2685,7 +2964,6 @@
       <c r="A88" s="1"/>
       <c r="B88" s="2"/>
       <c r="E88" s="3"/>
-      <c r="F88" s="4"/>
       <c r="G88" s="2"/>
       <c r="H88" s="2"/>
     </row>
@@ -2693,7 +2971,6 @@
       <c r="A89" s="1"/>
       <c r="B89" s="2"/>
       <c r="E89" s="3"/>
-      <c r="F89" s="4"/>
       <c r="G89" s="2"/>
       <c r="H89" s="2"/>
     </row>
@@ -2701,7 +2978,6 @@
       <c r="A90" s="1"/>
       <c r="B90" s="2"/>
       <c r="E90" s="3"/>
-      <c r="F90" s="4"/>
       <c r="G90" s="2"/>
       <c r="H90" s="2"/>
     </row>
@@ -2709,7 +2985,6 @@
       <c r="A91" s="1"/>
       <c r="B91" s="2"/>
       <c r="E91" s="3"/>
-      <c r="F91" s="4"/>
       <c r="G91" s="2"/>
       <c r="H91" s="2"/>
     </row>
@@ -2717,7 +2992,6 @@
       <c r="A92" s="1"/>
       <c r="B92" s="2"/>
       <c r="E92" s="3"/>
-      <c r="F92" s="4"/>
       <c r="G92" s="2"/>
       <c r="H92" s="2"/>
     </row>
@@ -2725,7 +2999,6 @@
       <c r="A93" s="1"/>
       <c r="B93" s="2"/>
       <c r="E93" s="3"/>
-      <c r="F93" s="4"/>
       <c r="G93" s="2"/>
       <c r="H93" s="2"/>
     </row>
@@ -2733,7 +3006,6 @@
       <c r="A94" s="1"/>
       <c r="B94" s="2"/>
       <c r="E94" s="3"/>
-      <c r="F94" s="4"/>
       <c r="G94" s="2"/>
       <c r="H94" s="2"/>
     </row>
@@ -2741,7 +3013,6 @@
       <c r="A95" s="1"/>
       <c r="B95" s="2"/>
       <c r="E95" s="3"/>
-      <c r="F95" s="4"/>
       <c r="G95" s="2"/>
       <c r="H95" s="2"/>
     </row>
@@ -2749,7 +3020,6 @@
       <c r="A96" s="1"/>
       <c r="B96" s="2"/>
       <c r="E96" s="3"/>
-      <c r="F96" s="4"/>
       <c r="G96" s="2"/>
       <c r="H96" s="2"/>
     </row>
@@ -2757,7 +3027,6 @@
       <c r="A97" s="1"/>
       <c r="B97" s="2"/>
       <c r="E97" s="3"/>
-      <c r="F97" s="4"/>
       <c r="G97" s="2"/>
       <c r="H97" s="2"/>
     </row>
@@ -2765,7 +3034,6 @@
       <c r="A98" s="1"/>
       <c r="B98" s="2"/>
       <c r="E98" s="3"/>
-      <c r="F98" s="4"/>
       <c r="G98" s="2"/>
       <c r="H98" s="2"/>
     </row>
@@ -2773,7 +3041,6 @@
       <c r="A99" s="1"/>
       <c r="B99" s="2"/>
       <c r="E99" s="3"/>
-      <c r="F99" s="4"/>
       <c r="G99" s="2"/>
       <c r="H99" s="2"/>
     </row>
@@ -2781,7 +3048,6 @@
       <c r="A100" s="1"/>
       <c r="B100" s="2"/>
       <c r="E100" s="3"/>
-      <c r="F100" s="4"/>
       <c r="G100" s="2"/>
       <c r="H100" s="2"/>
     </row>
@@ -2804,7 +3070,7 @@
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <ignoredErrors>
-    <ignoredError sqref="D2:D100" listDataValidation="1"/>
+    <ignoredError sqref="D8:D100" listDataValidation="1"/>
   </ignoredErrors>
   <tableParts count="1">
     <tablePart r:id="rId1"/>
@@ -2820,19 +3086,19 @@
       <selection activeCell="D2" sqref="D2:D100"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="7.69921875" customWidth="1"/>
-    <col min="2" max="2" width="17.296875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.59765625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="7.6640625" customWidth="1"/>
+    <col min="2" max="2" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.5546875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="9" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.8984375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="23.59765625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="13.3984375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="19.09765625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.88671875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="23.5546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.44140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="19.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="15.75">
+    <row r="1" spans="1:8" ht="15.6">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
@@ -2858,7 +3124,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="15">
+    <row r="2" spans="1:8">
       <c r="A2" s="1"/>
       <c r="B2" s="2"/>
       <c r="E2" s="3"/>
@@ -2866,7 +3132,7 @@
       <c r="G2" s="2"/>
       <c r="H2" s="2"/>
     </row>
-    <row r="3" spans="1:8" ht="15">
+    <row r="3" spans="1:8">
       <c r="A3" s="1"/>
       <c r="B3" s="2"/>
       <c r="E3" s="3"/>
@@ -2874,7 +3140,7 @@
       <c r="G3" s="2"/>
       <c r="H3" s="2"/>
     </row>
-    <row r="4" spans="1:8" ht="15">
+    <row r="4" spans="1:8">
       <c r="A4" s="1"/>
       <c r="B4" s="2"/>
       <c r="E4" s="3"/>
@@ -2882,7 +3148,7 @@
       <c r="G4" s="2"/>
       <c r="H4" s="2"/>
     </row>
-    <row r="5" spans="1:8" ht="15">
+    <row r="5" spans="1:8">
       <c r="A5" s="1"/>
       <c r="B5" s="2"/>
       <c r="E5" s="3"/>
@@ -2890,7 +3156,7 @@
       <c r="G5" s="2"/>
       <c r="H5" s="2"/>
     </row>
-    <row r="6" spans="1:8" ht="15">
+    <row r="6" spans="1:8">
       <c r="A6" s="1"/>
       <c r="B6" s="2"/>
       <c r="E6" s="3"/>
@@ -2898,7 +3164,7 @@
       <c r="G6" s="2"/>
       <c r="H6" s="2"/>
     </row>
-    <row r="7" spans="1:8" ht="15">
+    <row r="7" spans="1:8">
       <c r="A7" s="1"/>
       <c r="B7" s="2"/>
       <c r="E7" s="3"/>
@@ -2906,7 +3172,7 @@
       <c r="G7" s="2"/>
       <c r="H7" s="2"/>
     </row>
-    <row r="8" spans="1:8" ht="15">
+    <row r="8" spans="1:8">
       <c r="A8" s="1"/>
       <c r="B8" s="2"/>
       <c r="E8" s="3"/>
@@ -2914,7 +3180,7 @@
       <c r="G8" s="2"/>
       <c r="H8" s="2"/>
     </row>
-    <row r="9" spans="1:8" ht="15">
+    <row r="9" spans="1:8">
       <c r="A9" s="1"/>
       <c r="B9" s="2"/>
       <c r="E9" s="3"/>
@@ -2922,7 +3188,7 @@
       <c r="G9" s="2"/>
       <c r="H9" s="2"/>
     </row>
-    <row r="10" spans="1:8" ht="15">
+    <row r="10" spans="1:8">
       <c r="A10" s="1"/>
       <c r="B10" s="2"/>
       <c r="E10" s="3"/>
@@ -2930,7 +3196,7 @@
       <c r="G10" s="2"/>
       <c r="H10" s="2"/>
     </row>
-    <row r="11" spans="1:8" ht="15">
+    <row r="11" spans="1:8">
       <c r="A11" s="1"/>
       <c r="B11" s="2"/>
       <c r="E11" s="3"/>
@@ -2938,7 +3204,7 @@
       <c r="G11" s="2"/>
       <c r="H11" s="2"/>
     </row>
-    <row r="12" spans="1:8" ht="15">
+    <row r="12" spans="1:8">
       <c r="A12" s="1"/>
       <c r="B12" s="2"/>
       <c r="E12" s="3"/>
@@ -2946,7 +3212,7 @@
       <c r="G12" s="2"/>
       <c r="H12" s="2"/>
     </row>
-    <row r="13" spans="1:8" ht="15">
+    <row r="13" spans="1:8">
       <c r="A13" s="1"/>
       <c r="B13" s="2"/>
       <c r="E13" s="3"/>
@@ -2954,7 +3220,7 @@
       <c r="G13" s="2"/>
       <c r="H13" s="2"/>
     </row>
-    <row r="14" spans="1:8" ht="15">
+    <row r="14" spans="1:8">
       <c r="A14" s="1"/>
       <c r="B14" s="2"/>
       <c r="E14" s="3"/>
@@ -2962,7 +3228,7 @@
       <c r="G14" s="2"/>
       <c r="H14" s="2"/>
     </row>
-    <row r="15" spans="1:8" ht="15">
+    <row r="15" spans="1:8">
       <c r="A15" s="1"/>
       <c r="B15" s="2"/>
       <c r="E15" s="3"/>
@@ -2970,7 +3236,7 @@
       <c r="G15" s="2"/>
       <c r="H15" s="2"/>
     </row>
-    <row r="16" spans="1:8" ht="15">
+    <row r="16" spans="1:8">
       <c r="A16" s="1"/>
       <c r="B16" s="2"/>
       <c r="E16" s="3"/>
@@ -2978,7 +3244,7 @@
       <c r="G16" s="2"/>
       <c r="H16" s="2"/>
     </row>
-    <row r="17" spans="1:8" ht="15">
+    <row r="17" spans="1:8">
       <c r="A17" s="1"/>
       <c r="B17" s="2"/>
       <c r="E17" s="3"/>
@@ -2986,7 +3252,7 @@
       <c r="G17" s="2"/>
       <c r="H17" s="2"/>
     </row>
-    <row r="18" spans="1:8" ht="15">
+    <row r="18" spans="1:8">
       <c r="A18" s="1"/>
       <c r="B18" s="2"/>
       <c r="E18" s="3"/>
@@ -2994,7 +3260,7 @@
       <c r="G18" s="2"/>
       <c r="H18" s="2"/>
     </row>
-    <row r="19" spans="1:8" ht="15">
+    <row r="19" spans="1:8">
       <c r="A19" s="1"/>
       <c r="B19" s="2"/>
       <c r="E19" s="3"/>
@@ -3002,7 +3268,7 @@
       <c r="G19" s="2"/>
       <c r="H19" s="2"/>
     </row>
-    <row r="20" spans="1:8" ht="15">
+    <row r="20" spans="1:8">
       <c r="A20" s="1"/>
       <c r="B20" s="2"/>
       <c r="E20" s="3"/>
@@ -3010,7 +3276,7 @@
       <c r="G20" s="2"/>
       <c r="H20" s="2"/>
     </row>
-    <row r="21" spans="1:8" ht="15">
+    <row r="21" spans="1:8">
       <c r="A21" s="1"/>
       <c r="B21" s="2"/>
       <c r="E21" s="3"/>
@@ -3018,7 +3284,7 @@
       <c r="G21" s="2"/>
       <c r="H21" s="2"/>
     </row>
-    <row r="22" spans="1:8" ht="15">
+    <row r="22" spans="1:8">
       <c r="A22" s="1"/>
       <c r="B22" s="2"/>
       <c r="E22" s="3"/>
@@ -3026,7 +3292,7 @@
       <c r="G22" s="2"/>
       <c r="H22" s="2"/>
     </row>
-    <row r="23" spans="1:8" ht="15">
+    <row r="23" spans="1:8">
       <c r="A23" s="1"/>
       <c r="B23" s="2"/>
       <c r="E23" s="3"/>
@@ -3034,7 +3300,7 @@
       <c r="G23" s="2"/>
       <c r="H23" s="2"/>
     </row>
-    <row r="24" spans="1:8" ht="15">
+    <row r="24" spans="1:8">
       <c r="A24" s="1"/>
       <c r="B24" s="2"/>
       <c r="E24" s="3"/>
@@ -3042,7 +3308,7 @@
       <c r="G24" s="2"/>
       <c r="H24" s="2"/>
     </row>
-    <row r="25" spans="1:8" ht="15">
+    <row r="25" spans="1:8">
       <c r="A25" s="1"/>
       <c r="B25" s="2"/>
       <c r="E25" s="3"/>
@@ -3050,7 +3316,7 @@
       <c r="G25" s="2"/>
       <c r="H25" s="2"/>
     </row>
-    <row r="26" spans="1:8" ht="15">
+    <row r="26" spans="1:8">
       <c r="A26" s="1"/>
       <c r="B26" s="2"/>
       <c r="E26" s="3"/>
@@ -3058,7 +3324,7 @@
       <c r="G26" s="2"/>
       <c r="H26" s="2"/>
     </row>
-    <row r="27" spans="1:8" ht="15">
+    <row r="27" spans="1:8">
       <c r="A27" s="1"/>
       <c r="B27" s="2"/>
       <c r="E27" s="3"/>
@@ -3066,7 +3332,7 @@
       <c r="G27" s="2"/>
       <c r="H27" s="2"/>
     </row>
-    <row r="28" spans="1:8" ht="15">
+    <row r="28" spans="1:8">
       <c r="A28" s="1"/>
       <c r="B28" s="2"/>
       <c r="E28" s="3"/>
@@ -3074,7 +3340,7 @@
       <c r="G28" s="2"/>
       <c r="H28" s="2"/>
     </row>
-    <row r="29" spans="1:8" ht="15">
+    <row r="29" spans="1:8">
       <c r="A29" s="1"/>
       <c r="B29" s="2"/>
       <c r="E29" s="3"/>
@@ -3082,7 +3348,7 @@
       <c r="G29" s="2"/>
       <c r="H29" s="2"/>
     </row>
-    <row r="30" spans="1:8" ht="15">
+    <row r="30" spans="1:8">
       <c r="A30" s="1"/>
       <c r="B30" s="2"/>
       <c r="E30" s="3"/>
@@ -3090,7 +3356,7 @@
       <c r="G30" s="2"/>
       <c r="H30" s="2"/>
     </row>
-    <row r="31" spans="1:8" ht="15">
+    <row r="31" spans="1:8">
       <c r="A31" s="1"/>
       <c r="B31" s="2"/>
       <c r="E31" s="3"/>
@@ -3098,7 +3364,7 @@
       <c r="G31" s="2"/>
       <c r="H31" s="2"/>
     </row>
-    <row r="32" spans="1:8" ht="15">
+    <row r="32" spans="1:8">
       <c r="A32" s="1"/>
       <c r="B32" s="2"/>
       <c r="E32" s="3"/>
@@ -3106,7 +3372,7 @@
       <c r="G32" s="2"/>
       <c r="H32" s="2"/>
     </row>
-    <row r="33" spans="1:8" ht="15">
+    <row r="33" spans="1:8">
       <c r="A33" s="1"/>
       <c r="B33" s="2"/>
       <c r="E33" s="3"/>
@@ -3114,7 +3380,7 @@
       <c r="G33" s="2"/>
       <c r="H33" s="2"/>
     </row>
-    <row r="34" spans="1:8" ht="15">
+    <row r="34" spans="1:8">
       <c r="A34" s="1"/>
       <c r="B34" s="2"/>
       <c r="E34" s="3"/>
@@ -3122,7 +3388,7 @@
       <c r="G34" s="2"/>
       <c r="H34" s="2"/>
     </row>
-    <row r="35" spans="1:8" ht="15">
+    <row r="35" spans="1:8">
       <c r="A35" s="1"/>
       <c r="B35" s="2"/>
       <c r="E35" s="3"/>
@@ -3130,7 +3396,7 @@
       <c r="G35" s="2"/>
       <c r="H35" s="2"/>
     </row>
-    <row r="36" spans="1:8" ht="15">
+    <row r="36" spans="1:8">
       <c r="A36" s="1"/>
       <c r="B36" s="2"/>
       <c r="E36" s="3"/>
@@ -3138,7 +3404,7 @@
       <c r="G36" s="2"/>
       <c r="H36" s="2"/>
     </row>
-    <row r="37" spans="1:8" ht="15">
+    <row r="37" spans="1:8">
       <c r="A37" s="1"/>
       <c r="B37" s="2"/>
       <c r="E37" s="3"/>
@@ -3146,7 +3412,7 @@
       <c r="G37" s="2"/>
       <c r="H37" s="2"/>
     </row>
-    <row r="38" spans="1:8" ht="15">
+    <row r="38" spans="1:8">
       <c r="A38" s="1"/>
       <c r="B38" s="2"/>
       <c r="E38" s="3"/>
@@ -3154,7 +3420,7 @@
       <c r="G38" s="2"/>
       <c r="H38" s="2"/>
     </row>
-    <row r="39" spans="1:8" ht="15">
+    <row r="39" spans="1:8">
       <c r="A39" s="1"/>
       <c r="B39" s="2"/>
       <c r="E39" s="3"/>
@@ -3162,7 +3428,7 @@
       <c r="G39" s="2"/>
       <c r="H39" s="2"/>
     </row>
-    <row r="40" spans="1:8" ht="15">
+    <row r="40" spans="1:8">
       <c r="A40" s="1"/>
       <c r="B40" s="2"/>
       <c r="E40" s="3"/>
@@ -3170,7 +3436,7 @@
       <c r="G40" s="2"/>
       <c r="H40" s="2"/>
     </row>
-    <row r="41" spans="1:8" ht="15">
+    <row r="41" spans="1:8">
       <c r="A41" s="1"/>
       <c r="B41" s="2"/>
       <c r="E41" s="3"/>
@@ -3178,7 +3444,7 @@
       <c r="G41" s="2"/>
       <c r="H41" s="2"/>
     </row>
-    <row r="42" spans="1:8" ht="15">
+    <row r="42" spans="1:8">
       <c r="A42" s="1"/>
       <c r="B42" s="2"/>
       <c r="E42" s="3"/>
@@ -3186,7 +3452,7 @@
       <c r="G42" s="2"/>
       <c r="H42" s="2"/>
     </row>
-    <row r="43" spans="1:8" ht="15">
+    <row r="43" spans="1:8">
       <c r="A43" s="1"/>
       <c r="B43" s="2"/>
       <c r="E43" s="3"/>
@@ -3194,7 +3460,7 @@
       <c r="G43" s="2"/>
       <c r="H43" s="2"/>
     </row>
-    <row r="44" spans="1:8" ht="15">
+    <row r="44" spans="1:8">
       <c r="A44" s="1"/>
       <c r="B44" s="2"/>
       <c r="E44" s="3"/>
@@ -3202,7 +3468,7 @@
       <c r="G44" s="2"/>
       <c r="H44" s="2"/>
     </row>
-    <row r="45" spans="1:8" ht="15">
+    <row r="45" spans="1:8">
       <c r="A45" s="1"/>
       <c r="B45" s="2"/>
       <c r="E45" s="3"/>
@@ -3210,7 +3476,7 @@
       <c r="G45" s="2"/>
       <c r="H45" s="2"/>
     </row>
-    <row r="46" spans="1:8" ht="15">
+    <row r="46" spans="1:8">
       <c r="A46" s="1"/>
       <c r="B46" s="2"/>
       <c r="E46" s="3"/>
@@ -3218,7 +3484,7 @@
       <c r="G46" s="2"/>
       <c r="H46" s="2"/>
     </row>
-    <row r="47" spans="1:8" ht="15">
+    <row r="47" spans="1:8">
       <c r="A47" s="1"/>
       <c r="B47" s="2"/>
       <c r="E47" s="3"/>
@@ -3226,7 +3492,7 @@
       <c r="G47" s="2"/>
       <c r="H47" s="2"/>
     </row>
-    <row r="48" spans="1:8" ht="15">
+    <row r="48" spans="1:8">
       <c r="A48" s="1"/>
       <c r="B48" s="2"/>
       <c r="E48" s="3"/>
@@ -3234,7 +3500,7 @@
       <c r="G48" s="2"/>
       <c r="H48" s="2"/>
     </row>
-    <row r="49" spans="1:8" ht="15">
+    <row r="49" spans="1:8">
       <c r="A49" s="1"/>
       <c r="B49" s="2"/>
       <c r="E49" s="3"/>
@@ -3242,7 +3508,7 @@
       <c r="G49" s="2"/>
       <c r="H49" s="2"/>
     </row>
-    <row r="50" spans="1:8" ht="15">
+    <row r="50" spans="1:8">
       <c r="A50" s="1"/>
       <c r="B50" s="2"/>
       <c r="E50" s="3"/>
@@ -3250,7 +3516,7 @@
       <c r="G50" s="2"/>
       <c r="H50" s="2"/>
     </row>
-    <row r="51" spans="1:8" ht="15">
+    <row r="51" spans="1:8">
       <c r="A51" s="1"/>
       <c r="B51" s="2"/>
       <c r="E51" s="3"/>
@@ -3258,7 +3524,7 @@
       <c r="G51" s="2"/>
       <c r="H51" s="2"/>
     </row>
-    <row r="52" spans="1:8" ht="15">
+    <row r="52" spans="1:8">
       <c r="A52" s="1"/>
       <c r="B52" s="2"/>
       <c r="E52" s="3"/>
@@ -3266,7 +3532,7 @@
       <c r="G52" s="2"/>
       <c r="H52" s="2"/>
     </row>
-    <row r="53" spans="1:8" ht="15">
+    <row r="53" spans="1:8">
       <c r="A53" s="1"/>
       <c r="B53" s="2"/>
       <c r="E53" s="3"/>
@@ -3274,7 +3540,7 @@
       <c r="G53" s="2"/>
       <c r="H53" s="2"/>
     </row>
-    <row r="54" spans="1:8" ht="15">
+    <row r="54" spans="1:8">
       <c r="A54" s="1"/>
       <c r="B54" s="2"/>
       <c r="E54" s="3"/>
@@ -3282,7 +3548,7 @@
       <c r="G54" s="2"/>
       <c r="H54" s="2"/>
     </row>
-    <row r="55" spans="1:8" ht="15">
+    <row r="55" spans="1:8">
       <c r="A55" s="1"/>
       <c r="B55" s="2"/>
       <c r="E55" s="3"/>
@@ -3290,7 +3556,7 @@
       <c r="G55" s="2"/>
       <c r="H55" s="2"/>
     </row>
-    <row r="56" spans="1:8" ht="15">
+    <row r="56" spans="1:8">
       <c r="A56" s="1"/>
       <c r="B56" s="2"/>
       <c r="E56" s="3"/>
@@ -3298,7 +3564,7 @@
       <c r="G56" s="2"/>
       <c r="H56" s="2"/>
     </row>
-    <row r="57" spans="1:8" ht="15">
+    <row r="57" spans="1:8">
       <c r="A57" s="1"/>
       <c r="B57" s="2"/>
       <c r="E57" s="3"/>
@@ -3306,7 +3572,7 @@
       <c r="G57" s="2"/>
       <c r="H57" s="2"/>
     </row>
-    <row r="58" spans="1:8" ht="15">
+    <row r="58" spans="1:8">
       <c r="A58" s="1"/>
       <c r="B58" s="2"/>
       <c r="E58" s="3"/>
@@ -3314,7 +3580,7 @@
       <c r="G58" s="2"/>
       <c r="H58" s="2"/>
     </row>
-    <row r="59" spans="1:8" ht="15">
+    <row r="59" spans="1:8">
       <c r="A59" s="1"/>
       <c r="B59" s="2"/>
       <c r="E59" s="3"/>
@@ -3322,7 +3588,7 @@
       <c r="G59" s="2"/>
       <c r="H59" s="2"/>
     </row>
-    <row r="60" spans="1:8" ht="15">
+    <row r="60" spans="1:8">
       <c r="A60" s="1"/>
       <c r="B60" s="2"/>
       <c r="E60" s="3"/>
@@ -3330,7 +3596,7 @@
       <c r="G60" s="2"/>
       <c r="H60" s="2"/>
     </row>
-    <row r="61" spans="1:8" ht="15">
+    <row r="61" spans="1:8">
       <c r="A61" s="1"/>
       <c r="B61" s="2"/>
       <c r="E61" s="3"/>
@@ -3338,7 +3604,7 @@
       <c r="G61" s="2"/>
       <c r="H61" s="2"/>
     </row>
-    <row r="62" spans="1:8" ht="15">
+    <row r="62" spans="1:8">
       <c r="A62" s="1"/>
       <c r="B62" s="2"/>
       <c r="E62" s="3"/>
@@ -3346,7 +3612,7 @@
       <c r="G62" s="2"/>
       <c r="H62" s="2"/>
     </row>
-    <row r="63" spans="1:8" ht="15">
+    <row r="63" spans="1:8">
       <c r="A63" s="1"/>
       <c r="B63" s="2"/>
       <c r="E63" s="3"/>
@@ -3354,7 +3620,7 @@
       <c r="G63" s="2"/>
       <c r="H63" s="2"/>
     </row>
-    <row r="64" spans="1:8" ht="15">
+    <row r="64" spans="1:8">
       <c r="A64" s="1"/>
       <c r="B64" s="2"/>
       <c r="E64" s="3"/>
@@ -3362,7 +3628,7 @@
       <c r="G64" s="2"/>
       <c r="H64" s="2"/>
     </row>
-    <row r="65" spans="1:8" ht="15">
+    <row r="65" spans="1:8">
       <c r="A65" s="1"/>
       <c r="B65" s="2"/>
       <c r="E65" s="3"/>
@@ -3370,7 +3636,7 @@
       <c r="G65" s="2"/>
       <c r="H65" s="2"/>
     </row>
-    <row r="66" spans="1:8" ht="15">
+    <row r="66" spans="1:8">
       <c r="A66" s="1"/>
       <c r="B66" s="2"/>
       <c r="E66" s="3"/>
@@ -3378,7 +3644,7 @@
       <c r="G66" s="2"/>
       <c r="H66" s="2"/>
     </row>
-    <row r="67" spans="1:8" ht="15">
+    <row r="67" spans="1:8">
       <c r="A67" s="1"/>
       <c r="B67" s="2"/>
       <c r="E67" s="3"/>
@@ -3386,7 +3652,7 @@
       <c r="G67" s="2"/>
       <c r="H67" s="2"/>
     </row>
-    <row r="68" spans="1:8" ht="15">
+    <row r="68" spans="1:8">
       <c r="A68" s="1"/>
       <c r="B68" s="2"/>
       <c r="E68" s="3"/>
@@ -3394,7 +3660,7 @@
       <c r="G68" s="2"/>
       <c r="H68" s="2"/>
     </row>
-    <row r="69" spans="1:8" ht="15">
+    <row r="69" spans="1:8">
       <c r="A69" s="1"/>
       <c r="B69" s="2"/>
       <c r="E69" s="3"/>
@@ -3402,7 +3668,7 @@
       <c r="G69" s="2"/>
       <c r="H69" s="2"/>
     </row>
-    <row r="70" spans="1:8" ht="15">
+    <row r="70" spans="1:8">
       <c r="A70" s="1"/>
       <c r="B70" s="2"/>
       <c r="E70" s="3"/>
@@ -3410,7 +3676,7 @@
       <c r="G70" s="2"/>
       <c r="H70" s="2"/>
     </row>
-    <row r="71" spans="1:8" ht="15">
+    <row r="71" spans="1:8">
       <c r="A71" s="1"/>
       <c r="B71" s="2"/>
       <c r="E71" s="3"/>
@@ -3418,7 +3684,7 @@
       <c r="G71" s="2"/>
       <c r="H71" s="2"/>
     </row>
-    <row r="72" spans="1:8" ht="15">
+    <row r="72" spans="1:8">
       <c r="A72" s="1"/>
       <c r="B72" s="2"/>
       <c r="E72" s="3"/>
@@ -3426,7 +3692,7 @@
       <c r="G72" s="2"/>
       <c r="H72" s="2"/>
     </row>
-    <row r="73" spans="1:8" ht="15">
+    <row r="73" spans="1:8">
       <c r="A73" s="1"/>
       <c r="B73" s="2"/>
       <c r="E73" s="3"/>
@@ -3434,7 +3700,7 @@
       <c r="G73" s="2"/>
       <c r="H73" s="2"/>
     </row>
-    <row r="74" spans="1:8" ht="15">
+    <row r="74" spans="1:8">
       <c r="A74" s="1"/>
       <c r="B74" s="2"/>
       <c r="E74" s="3"/>
@@ -3442,7 +3708,7 @@
       <c r="G74" s="2"/>
       <c r="H74" s="2"/>
     </row>
-    <row r="75" spans="1:8" ht="15">
+    <row r="75" spans="1:8">
       <c r="A75" s="1"/>
       <c r="B75" s="2"/>
       <c r="E75" s="3"/>
@@ -3450,7 +3716,7 @@
       <c r="G75" s="2"/>
       <c r="H75" s="2"/>
     </row>
-    <row r="76" spans="1:8" ht="15">
+    <row r="76" spans="1:8">
       <c r="A76" s="1"/>
       <c r="B76" s="2"/>
       <c r="E76" s="3"/>
@@ -3458,7 +3724,7 @@
       <c r="G76" s="2"/>
       <c r="H76" s="2"/>
     </row>
-    <row r="77" spans="1:8" ht="15">
+    <row r="77" spans="1:8">
       <c r="A77" s="1"/>
       <c r="B77" s="2"/>
       <c r="E77" s="3"/>
@@ -3466,7 +3732,7 @@
       <c r="G77" s="2"/>
       <c r="H77" s="2"/>
     </row>
-    <row r="78" spans="1:8" ht="15">
+    <row r="78" spans="1:8">
       <c r="A78" s="1"/>
       <c r="B78" s="2"/>
       <c r="E78" s="3"/>
@@ -3474,7 +3740,7 @@
       <c r="G78" s="2"/>
       <c r="H78" s="2"/>
     </row>
-    <row r="79" spans="1:8" ht="15">
+    <row r="79" spans="1:8">
       <c r="A79" s="1"/>
       <c r="B79" s="2"/>
       <c r="E79" s="3"/>
@@ -3482,7 +3748,7 @@
       <c r="G79" s="2"/>
       <c r="H79" s="2"/>
     </row>
-    <row r="80" spans="1:8" ht="15">
+    <row r="80" spans="1:8">
       <c r="A80" s="1"/>
       <c r="B80" s="2"/>
       <c r="E80" s="3"/>
@@ -3490,7 +3756,7 @@
       <c r="G80" s="2"/>
       <c r="H80" s="2"/>
     </row>
-    <row r="81" spans="1:8" ht="15">
+    <row r="81" spans="1:8">
       <c r="A81" s="1"/>
       <c r="B81" s="2"/>
       <c r="E81" s="3"/>
@@ -3498,7 +3764,7 @@
       <c r="G81" s="2"/>
       <c r="H81" s="2"/>
     </row>
-    <row r="82" spans="1:8" ht="15">
+    <row r="82" spans="1:8">
       <c r="A82" s="1"/>
       <c r="B82" s="2"/>
       <c r="E82" s="3"/>
@@ -3506,7 +3772,7 @@
       <c r="G82" s="2"/>
       <c r="H82" s="2"/>
     </row>
-    <row r="83" spans="1:8" ht="15">
+    <row r="83" spans="1:8">
       <c r="A83" s="1"/>
       <c r="B83" s="2"/>
       <c r="E83" s="3"/>
@@ -3514,7 +3780,7 @@
       <c r="G83" s="2"/>
       <c r="H83" s="2"/>
     </row>
-    <row r="84" spans="1:8" ht="15">
+    <row r="84" spans="1:8">
       <c r="A84" s="1"/>
       <c r="B84" s="2"/>
       <c r="E84" s="3"/>
@@ -3522,7 +3788,7 @@
       <c r="G84" s="2"/>
       <c r="H84" s="2"/>
     </row>
-    <row r="85" spans="1:8" ht="15">
+    <row r="85" spans="1:8">
       <c r="A85" s="1"/>
       <c r="B85" s="2"/>
       <c r="E85" s="3"/>
@@ -3530,7 +3796,7 @@
       <c r="G85" s="2"/>
       <c r="H85" s="2"/>
     </row>
-    <row r="86" spans="1:8" ht="15">
+    <row r="86" spans="1:8">
       <c r="A86" s="1"/>
       <c r="B86" s="2"/>
       <c r="E86" s="3"/>
@@ -3538,7 +3804,7 @@
       <c r="G86" s="2"/>
       <c r="H86" s="2"/>
     </row>
-    <row r="87" spans="1:8" ht="15">
+    <row r="87" spans="1:8">
       <c r="A87" s="1"/>
       <c r="B87" s="2"/>
       <c r="E87" s="3"/>
@@ -3685,21 +3951,21 @@
       <selection activeCell="P21" sqref="P21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="10.09765625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.8984375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.8984375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="19.3984375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.59765625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.59765625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.88671875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.88671875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19.44140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.5546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.5546875" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="9" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="17.8984375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="17.88671875" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="17" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="19.09765625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="19.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="15.75">
+    <row r="1" spans="1:10" ht="15.6">
       <c r="A1" s="7" t="s">
         <v>8</v>
       </c>
@@ -3731,7 +3997,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:10" ht="15">
+    <row r="2" spans="1:10">
       <c r="A2" s="2"/>
       <c r="B2" s="8"/>
       <c r="D2" s="2"/>
@@ -3739,7 +4005,7 @@
       <c r="I2" s="8"/>
       <c r="J2" s="2"/>
     </row>
-    <row r="3" spans="1:10" ht="15">
+    <row r="3" spans="1:10">
       <c r="A3" s="2"/>
       <c r="B3" s="8"/>
       <c r="D3" s="2"/>
@@ -3747,7 +4013,7 @@
       <c r="I3" s="8"/>
       <c r="J3" s="2"/>
     </row>
-    <row r="4" spans="1:10" ht="15">
+    <row r="4" spans="1:10">
       <c r="A4" s="2"/>
       <c r="B4" s="8"/>
       <c r="D4" s="2"/>
@@ -3755,7 +4021,7 @@
       <c r="I4" s="8"/>
       <c r="J4" s="2"/>
     </row>
-    <row r="5" spans="1:10" ht="15">
+    <row r="5" spans="1:10">
       <c r="A5" s="2"/>
       <c r="B5" s="8"/>
       <c r="D5" s="2"/>
@@ -3763,7 +4029,7 @@
       <c r="I5" s="8"/>
       <c r="J5" s="2"/>
     </row>
-    <row r="6" spans="1:10" ht="15">
+    <row r="6" spans="1:10">
       <c r="A6" s="2"/>
       <c r="B6" s="8"/>
       <c r="D6" s="2"/>
@@ -3771,7 +4037,7 @@
       <c r="I6" s="8"/>
       <c r="J6" s="2"/>
     </row>
-    <row r="7" spans="1:10" ht="15">
+    <row r="7" spans="1:10">
       <c r="A7" s="2"/>
       <c r="B7" s="8"/>
       <c r="D7" s="2"/>
@@ -3779,7 +4045,7 @@
       <c r="I7" s="8"/>
       <c r="J7" s="2"/>
     </row>
-    <row r="8" spans="1:10" ht="15">
+    <row r="8" spans="1:10">
       <c r="A8" s="2"/>
       <c r="B8" s="8"/>
       <c r="D8" s="2"/>
@@ -3787,7 +4053,7 @@
       <c r="I8" s="8"/>
       <c r="J8" s="2"/>
     </row>
-    <row r="9" spans="1:10" ht="15">
+    <row r="9" spans="1:10">
       <c r="A9" s="2"/>
       <c r="B9" s="8"/>
       <c r="D9" s="2"/>
@@ -3795,7 +4061,7 @@
       <c r="I9" s="8"/>
       <c r="J9" s="2"/>
     </row>
-    <row r="10" spans="1:10" ht="15">
+    <row r="10" spans="1:10">
       <c r="A10" s="2"/>
       <c r="B10" s="8"/>
       <c r="D10" s="2"/>
@@ -3803,7 +4069,7 @@
       <c r="I10" s="8"/>
       <c r="J10" s="2"/>
     </row>
-    <row r="11" spans="1:10" ht="15">
+    <row r="11" spans="1:10">
       <c r="A11" s="2"/>
       <c r="B11" s="8"/>
       <c r="D11" s="2"/>
@@ -3811,7 +4077,7 @@
       <c r="I11" s="8"/>
       <c r="J11" s="2"/>
     </row>
-    <row r="12" spans="1:10" ht="15">
+    <row r="12" spans="1:10">
       <c r="A12" s="2"/>
       <c r="B12" s="8"/>
       <c r="D12" s="2"/>
@@ -3819,7 +4085,7 @@
       <c r="I12" s="8"/>
       <c r="J12" s="2"/>
     </row>
-    <row r="13" spans="1:10" ht="15">
+    <row r="13" spans="1:10">
       <c r="A13" s="2"/>
       <c r="B13" s="8"/>
       <c r="D13" s="2"/>
@@ -3827,7 +4093,7 @@
       <c r="I13" s="8"/>
       <c r="J13" s="2"/>
     </row>
-    <row r="14" spans="1:10" ht="15">
+    <row r="14" spans="1:10">
       <c r="A14" s="2"/>
       <c r="B14" s="8"/>
       <c r="D14" s="2"/>
@@ -3835,7 +4101,7 @@
       <c r="I14" s="8"/>
       <c r="J14" s="2"/>
     </row>
-    <row r="15" spans="1:10" ht="15">
+    <row r="15" spans="1:10">
       <c r="A15" s="2"/>
       <c r="B15" s="8"/>
       <c r="D15" s="2"/>
@@ -3843,7 +4109,7 @@
       <c r="I15" s="8"/>
       <c r="J15" s="2"/>
     </row>
-    <row r="16" spans="1:10" ht="15">
+    <row r="16" spans="1:10">
       <c r="A16" s="2"/>
       <c r="B16" s="8"/>
       <c r="D16" s="2"/>
@@ -3851,7 +4117,7 @@
       <c r="I16" s="8"/>
       <c r="J16" s="2"/>
     </row>
-    <row r="17" spans="1:10" ht="15">
+    <row r="17" spans="1:10">
       <c r="A17" s="2"/>
       <c r="B17" s="8"/>
       <c r="D17" s="2"/>
@@ -3859,7 +4125,7 @@
       <c r="I17" s="8"/>
       <c r="J17" s="2"/>
     </row>
-    <row r="18" spans="1:10" ht="15">
+    <row r="18" spans="1:10">
       <c r="A18" s="2"/>
       <c r="B18" s="8"/>
       <c r="D18" s="2"/>
@@ -3867,7 +4133,7 @@
       <c r="I18" s="8"/>
       <c r="J18" s="2"/>
     </row>
-    <row r="19" spans="1:10" ht="15">
+    <row r="19" spans="1:10">
       <c r="A19" s="2"/>
       <c r="B19" s="8"/>
       <c r="D19" s="2"/>
@@ -3875,7 +4141,7 @@
       <c r="I19" s="8"/>
       <c r="J19" s="2"/>
     </row>
-    <row r="20" spans="1:10" ht="15">
+    <row r="20" spans="1:10">
       <c r="A20" s="2"/>
       <c r="B20" s="8"/>
       <c r="D20" s="2"/>
@@ -3883,7 +4149,7 @@
       <c r="I20" s="8"/>
       <c r="J20" s="2"/>
     </row>
-    <row r="21" spans="1:10" ht="15">
+    <row r="21" spans="1:10">
       <c r="A21" s="2"/>
       <c r="B21" s="8"/>
       <c r="D21" s="2"/>
@@ -3891,7 +4157,7 @@
       <c r="I21" s="8"/>
       <c r="J21" s="2"/>
     </row>
-    <row r="22" spans="1:10" ht="15">
+    <row r="22" spans="1:10">
       <c r="A22" s="2"/>
       <c r="B22" s="8"/>
       <c r="D22" s="2"/>
@@ -3899,7 +4165,7 @@
       <c r="I22" s="8"/>
       <c r="J22" s="2"/>
     </row>
-    <row r="23" spans="1:10" ht="15">
+    <row r="23" spans="1:10">
       <c r="A23" s="2"/>
       <c r="B23" s="8"/>
       <c r="D23" s="2"/>
@@ -3907,7 +4173,7 @@
       <c r="I23" s="8"/>
       <c r="J23" s="2"/>
     </row>
-    <row r="24" spans="1:10" ht="15">
+    <row r="24" spans="1:10">
       <c r="A24" s="2"/>
       <c r="B24" s="8"/>
       <c r="D24" s="2"/>
@@ -3915,7 +4181,7 @@
       <c r="I24" s="8"/>
       <c r="J24" s="2"/>
     </row>
-    <row r="25" spans="1:10" ht="15">
+    <row r="25" spans="1:10">
       <c r="A25" s="2"/>
       <c r="B25" s="8"/>
       <c r="D25" s="2"/>

</xml_diff>

<commit_message>
Updated progress report for May 20-21 by Avichal
</commit_message>
<xml_diff>
--- a/PR&IR.xlsx
+++ b/PR&IR.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28623"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SHIVYA KUMAR\Desktop\new415\CS415_A3\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\avichal avneel nath\Documents\Semester 7\CS415\A3\CS415_A3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D10B44C-54A7-4F21-8F22-614AAAF0B8A7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E40B6A96-FAF6-4C15-B5A0-E2C969B71FD7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{BFA1E21A-08FA-4F02-8C25-33C81C8EE970}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{BFA1E21A-08FA-4F02-8C25-33C81C8EE970}"/>
   </bookViews>
   <sheets>
     <sheet name="Avichal" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="149" uniqueCount="87">
   <si>
     <t>Date</t>
   </si>
@@ -302,6 +302,31 @@
   <si>
     <t>Sick, too much workloads in other units</t>
   </si>
+  <si>
+    <t>Backend Setup:
+Flask application factory pattern implemented in run_es.py.
+Database initialization (db.py) configured for SQLite.
+Flask-SQLAlchemy models (model.py) defined for all key entities from the ER diagram (Program, SubProgram, Semester, Course, CourseAvailability, Student, StudentLevel, Hold, Enrollment, CourseFee, StudentCourseFee).</t>
+  </si>
+  <si>
+    <t>Routing and API Development:</t>
+  </si>
+  <si>
+    <t>Routing and API Development:
+Single Flask Blueprint (enrollment_bp) established for all service routes.
+HTML rendering routes (/dashboard, /enroll, /display_courses, /fees, /download_invoice_pdf) implemented.
+Comprehensive JSON API endpoints (GET, POST, PUT, DELETE) created for all major entities.
+Correct url_for usage (enrollment.endpoint_name) enforced across routes.py and HTML templates.
+Error Resolution &amp; Stability:
+jinja2.exceptions.TemplateNotFound error resolved by correct template_folder configuration and template placement.
+sqlalchemy.exc.AmbiguousForeignKeysError addressed in model.py by explicitly defining foreign_keys in Program and SubProgram relationships.
+Importance of deleting enrollment.db for schema updates highlighted and executed.
+Application now successfully runs and serves the dashboard and other HTML page</t>
+  </si>
+  <si>
+    <t>Database seeding (populating with initial data).
+Replacing mock data in frontend routes with actual database queries.</t>
+  </si>
 </sst>
 </file>
 
@@ -311,7 +336,7 @@
     <numFmt numFmtId="164" formatCode="h"/>
     <numFmt numFmtId="165" formatCode="d/mm/yyyy;@"/>
   </numFmts>
-  <fonts count="3">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -352,7 +377,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -367,6 +392,10 @@
     </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="2" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1047,30 +1076,30 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{37EAA098-74C6-4411-B7E2-26AD2DCBC3F0}">
   <dimension ref="A1:H28"/>
   <sheetViews>
-    <sheetView topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="F16" sqref="F16"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="H14" sqref="H14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.44140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.5546875" style="2" customWidth="1"/>
+    <col min="1" max="1" width="10.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.5703125" style="2" customWidth="1"/>
     <col min="3" max="3" width="58" customWidth="1"/>
-    <col min="5" max="5" width="13.109375" style="3" customWidth="1"/>
-    <col min="6" max="6" width="20.88671875" style="4" customWidth="1"/>
-    <col min="7" max="7" width="34.88671875" style="2" customWidth="1"/>
-    <col min="8" max="8" width="43.44140625" style="2" customWidth="1"/>
-    <col min="11" max="11" width="9.109375" customWidth="1"/>
-    <col min="12" max="12" width="13.33203125" customWidth="1"/>
-    <col min="13" max="13" width="11.44140625" customWidth="1"/>
-    <col min="14" max="14" width="17.44140625" customWidth="1"/>
-    <col min="16" max="16" width="9.109375" customWidth="1"/>
-    <col min="18" max="18" width="16.5546875" customWidth="1"/>
-    <col min="19" max="19" width="14.6640625" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="16.88671875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.140625" style="3" customWidth="1"/>
+    <col min="6" max="6" width="20.85546875" style="4" customWidth="1"/>
+    <col min="7" max="7" width="34.85546875" style="2" customWidth="1"/>
+    <col min="8" max="8" width="43.42578125" style="2" customWidth="1"/>
+    <col min="11" max="11" width="9.140625" customWidth="1"/>
+    <col min="12" max="12" width="13.28515625" customWidth="1"/>
+    <col min="13" max="13" width="11.42578125" customWidth="1"/>
+    <col min="14" max="14" width="17.42578125" customWidth="1"/>
+    <col min="16" max="16" width="9.140625" customWidth="1"/>
+    <col min="18" max="18" width="16.5703125" customWidth="1"/>
+    <col min="19" max="19" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="16.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="15.6">
+    <row r="1" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
@@ -1096,7 +1125,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:8">
+    <row r="2" spans="1:8" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A2" s="1">
         <v>45786</v>
       </c>
@@ -1122,7 +1151,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="3" spans="1:8" ht="115.2">
+    <row r="3" spans="1:8" ht="120" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>45787</v>
       </c>
@@ -1145,7 +1174,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="4" spans="1:8">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>45788</v>
       </c>
@@ -1165,7 +1194,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="5" spans="1:8" ht="76.5" customHeight="1">
+    <row r="5" spans="1:8" ht="76.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>45789</v>
       </c>
@@ -1188,7 +1217,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="6" spans="1:8">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>45790</v>
       </c>
@@ -1211,7 +1240,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="7" spans="1:8">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>45791</v>
       </c>
@@ -1234,7 +1263,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="8" spans="1:8">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>45792</v>
       </c>
@@ -1257,7 +1286,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="9" spans="1:8">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>45793</v>
       </c>
@@ -1277,7 +1306,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="10" spans="1:8">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>45794</v>
       </c>
@@ -1297,7 +1326,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="11" spans="1:8">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>45795</v>
       </c>
@@ -1317,7 +1346,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="12" spans="1:8">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <v>45796</v>
       </c>
@@ -1337,56 +1366,88 @@
         <v>78</v>
       </c>
     </row>
-    <row r="13" spans="1:8">
-      <c r="E13"/>
-      <c r="F13"/>
-    </row>
-    <row r="14" spans="1:8">
-      <c r="E14"/>
-      <c r="F14"/>
-    </row>
-    <row r="15" spans="1:8">
+    <row r="13" spans="1:8" ht="68.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="1">
+        <v>45797</v>
+      </c>
+      <c r="C13" s="9" t="s">
+        <v>83</v>
+      </c>
+      <c r="D13" t="s">
+        <v>37</v>
+      </c>
+      <c r="E13">
+        <v>80</v>
+      </c>
+      <c r="F13">
+        <v>2</v>
+      </c>
+      <c r="G13" s="12" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" ht="60" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="1">
+        <v>45798</v>
+      </c>
+      <c r="C14" s="9" t="s">
+        <v>85</v>
+      </c>
+      <c r="D14" t="s">
+        <v>17</v>
+      </c>
+      <c r="E14">
+        <v>100</v>
+      </c>
+      <c r="F14">
+        <v>4</v>
+      </c>
+      <c r="G14" s="13" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="E15"/>
       <c r="F15"/>
     </row>
-    <row r="16" spans="1:8">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="E16"/>
       <c r="F16"/>
     </row>
-    <row r="17" spans="6:6">
+    <row r="17" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F17"/>
     </row>
-    <row r="18" spans="6:6">
+    <row r="18" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F18"/>
     </row>
-    <row r="19" spans="6:6">
+    <row r="19" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F19"/>
     </row>
-    <row r="20" spans="6:6">
+    <row r="20" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F20"/>
     </row>
-    <row r="21" spans="6:6">
+    <row r="21" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F21"/>
     </row>
-    <row r="22" spans="6:6">
+    <row r="22" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F22"/>
     </row>
-    <row r="23" spans="6:6">
+    <row r="23" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F23"/>
     </row>
-    <row r="24" spans="6:6">
+    <row r="24" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F24"/>
     </row>
-    <row r="25" spans="6:6">
+    <row r="25" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F25"/>
     </row>
-    <row r="26" spans="6:6">
+    <row r="26" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F26"/>
     </row>
-    <row r="27" spans="6:6">
+    <row r="27" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F27"/>
     </row>
-    <row r="28" spans="6:6">
+    <row r="28" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F28"/>
     </row>
   </sheetData>
@@ -1409,7 +1470,7 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
   <ignoredErrors>
-    <ignoredError sqref="D13:D16" listDataValidation="1"/>
+    <ignoredError sqref="D15:D16" listDataValidation="1"/>
   </ignoredErrors>
   <tableParts count="1">
     <tablePart r:id="rId2"/>
@@ -1421,23 +1482,23 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3BDA6702-5DDF-42FB-988E-13FBEB26F5C9}">
   <dimension ref="A1:H100"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H7" sqref="H7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="17.33203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="55.5546875" customWidth="1"/>
-    <col min="4" max="4" width="10.5546875" customWidth="1"/>
-    <col min="5" max="5" width="14.88671875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14.33203125" customWidth="1"/>
-    <col min="7" max="7" width="92.88671875" customWidth="1"/>
-    <col min="8" max="8" width="82.44140625" customWidth="1"/>
+    <col min="1" max="1" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="55.5703125" customWidth="1"/>
+    <col min="4" max="4" width="10.5703125" customWidth="1"/>
+    <col min="5" max="5" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.28515625" customWidth="1"/>
+    <col min="7" max="7" width="92.85546875" customWidth="1"/>
+    <col min="8" max="8" width="82.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="15.6">
+    <row r="1" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
@@ -1463,7 +1524,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:8">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="8">
         <v>45786</v>
       </c>
@@ -1489,7 +1550,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="3" spans="1:8">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="8">
         <v>45787</v>
       </c>
@@ -1515,7 +1576,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="4" spans="1:8">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="8">
         <v>45789</v>
       </c>
@@ -1539,7 +1600,7 @@
       </c>
       <c r="H4" s="2"/>
     </row>
-    <row r="5" spans="1:8">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="8">
         <v>45790</v>
       </c>
@@ -1563,7 +1624,7 @@
       </c>
       <c r="H5" s="2"/>
     </row>
-    <row r="6" spans="1:8">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="8">
         <v>45791</v>
       </c>
@@ -1589,7 +1650,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="7" spans="1:8">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="8">
         <v>45795</v>
       </c>
@@ -1613,559 +1674,559 @@
         <v>82</v>
       </c>
     </row>
-    <row r="8" spans="1:8">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="8"/>
       <c r="B8" s="2"/>
       <c r="G8" s="2"/>
       <c r="H8" s="2"/>
     </row>
-    <row r="9" spans="1:8">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="8"/>
       <c r="B9" s="2"/>
       <c r="G9" s="2"/>
       <c r="H9" s="2"/>
     </row>
-    <row r="10" spans="1:8">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="8"/>
       <c r="B10" s="2"/>
       <c r="G10" s="2"/>
       <c r="H10" s="2"/>
     </row>
-    <row r="11" spans="1:8">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="8"/>
       <c r="B11" s="2"/>
       <c r="G11" s="2"/>
       <c r="H11" s="2"/>
     </row>
-    <row r="12" spans="1:8">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="8"/>
       <c r="B12" s="2"/>
       <c r="G12" s="2"/>
       <c r="H12" s="2"/>
     </row>
-    <row r="13" spans="1:8">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="8"/>
       <c r="B13" s="2"/>
       <c r="G13" s="2"/>
       <c r="H13" s="2"/>
     </row>
-    <row r="14" spans="1:8">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" s="8"/>
       <c r="B14" s="2"/>
       <c r="G14" s="2"/>
       <c r="H14" s="2"/>
     </row>
-    <row r="15" spans="1:8">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" s="8"/>
       <c r="B15" s="2"/>
       <c r="G15" s="2"/>
       <c r="H15" s="2"/>
     </row>
-    <row r="16" spans="1:8">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" s="8"/>
       <c r="B16" s="2"/>
       <c r="G16" s="2"/>
       <c r="H16" s="2"/>
     </row>
-    <row r="17" spans="1:8">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" s="8"/>
       <c r="B17" s="2"/>
       <c r="G17" s="2"/>
       <c r="H17" s="2"/>
     </row>
-    <row r="18" spans="1:8">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" s="8"/>
       <c r="B18" s="2"/>
       <c r="G18" s="2"/>
       <c r="H18" s="2"/>
     </row>
-    <row r="19" spans="1:8">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" s="8"/>
       <c r="B19" s="2"/>
       <c r="G19" s="2"/>
       <c r="H19" s="2"/>
     </row>
-    <row r="20" spans="1:8">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" s="8"/>
       <c r="B20" s="2"/>
       <c r="G20" s="2"/>
       <c r="H20" s="2"/>
     </row>
-    <row r="21" spans="1:8">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" s="8"/>
       <c r="B21" s="2"/>
       <c r="G21" s="2"/>
       <c r="H21" s="2"/>
     </row>
-    <row r="22" spans="1:8">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" s="8"/>
       <c r="B22" s="2"/>
       <c r="G22" s="2"/>
       <c r="H22" s="2"/>
     </row>
-    <row r="23" spans="1:8">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" s="8"/>
       <c r="B23" s="2"/>
       <c r="G23" s="2"/>
       <c r="H23" s="2"/>
     </row>
-    <row r="24" spans="1:8">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24" s="8"/>
       <c r="B24" s="2"/>
       <c r="G24" s="2"/>
       <c r="H24" s="2"/>
     </row>
-    <row r="25" spans="1:8">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25" s="8"/>
       <c r="B25" s="2"/>
       <c r="G25" s="2"/>
       <c r="H25" s="2"/>
     </row>
-    <row r="26" spans="1:8">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26" s="8"/>
       <c r="B26" s="2"/>
       <c r="G26" s="2"/>
       <c r="H26" s="2"/>
     </row>
-    <row r="27" spans="1:8">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A27" s="8"/>
       <c r="B27" s="2"/>
       <c r="G27" s="2"/>
       <c r="H27" s="2"/>
     </row>
-    <row r="28" spans="1:8">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A28" s="8"/>
       <c r="B28" s="2"/>
       <c r="G28" s="2"/>
       <c r="H28" s="2"/>
     </row>
-    <row r="29" spans="1:8">
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A29" s="8"/>
       <c r="B29" s="2"/>
       <c r="G29" s="2"/>
       <c r="H29" s="2"/>
     </row>
-    <row r="30" spans="1:8">
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A30" s="8"/>
       <c r="B30" s="2"/>
       <c r="G30" s="2"/>
       <c r="H30" s="2"/>
     </row>
-    <row r="31" spans="1:8">
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A31" s="8"/>
       <c r="B31" s="2"/>
       <c r="G31" s="2"/>
       <c r="H31" s="2"/>
     </row>
-    <row r="32" spans="1:8">
+    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A32" s="8"/>
       <c r="B32" s="2"/>
       <c r="G32" s="2"/>
       <c r="H32" s="2"/>
     </row>
-    <row r="33" spans="1:8">
+    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A33" s="8"/>
       <c r="B33" s="2"/>
       <c r="G33" s="2"/>
       <c r="H33" s="2"/>
     </row>
-    <row r="34" spans="1:8">
+    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A34" s="8"/>
       <c r="B34" s="2"/>
       <c r="G34" s="2"/>
       <c r="H34" s="2"/>
     </row>
-    <row r="35" spans="1:8">
+    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A35" s="8"/>
       <c r="B35" s="2"/>
       <c r="G35" s="2"/>
       <c r="H35" s="2"/>
     </row>
-    <row r="36" spans="1:8">
+    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A36" s="8"/>
       <c r="B36" s="2"/>
       <c r="G36" s="2"/>
       <c r="H36" s="2"/>
     </row>
-    <row r="37" spans="1:8">
+    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A37" s="8"/>
       <c r="B37" s="2"/>
       <c r="G37" s="2"/>
       <c r="H37" s="2"/>
     </row>
-    <row r="38" spans="1:8">
+    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A38" s="8"/>
       <c r="B38" s="2"/>
       <c r="G38" s="2"/>
       <c r="H38" s="2"/>
     </row>
-    <row r="39" spans="1:8">
+    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A39" s="8"/>
       <c r="B39" s="2"/>
       <c r="G39" s="2"/>
       <c r="H39" s="2"/>
     </row>
-    <row r="40" spans="1:8">
+    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A40" s="8"/>
       <c r="B40" s="2"/>
       <c r="G40" s="2"/>
       <c r="H40" s="2"/>
     </row>
-    <row r="41" spans="1:8">
+    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A41" s="8"/>
       <c r="B41" s="2"/>
       <c r="G41" s="2"/>
       <c r="H41" s="2"/>
     </row>
-    <row r="42" spans="1:8">
+    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A42" s="8"/>
       <c r="B42" s="2"/>
       <c r="G42" s="2"/>
       <c r="H42" s="2"/>
     </row>
-    <row r="43" spans="1:8">
+    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A43" s="8"/>
       <c r="B43" s="2"/>
       <c r="G43" s="2"/>
       <c r="H43" s="2"/>
     </row>
-    <row r="44" spans="1:8">
+    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A44" s="8"/>
       <c r="B44" s="2"/>
       <c r="G44" s="2"/>
       <c r="H44" s="2"/>
     </row>
-    <row r="45" spans="1:8">
+    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A45" s="8"/>
       <c r="B45" s="2"/>
       <c r="G45" s="2"/>
       <c r="H45" s="2"/>
     </row>
-    <row r="46" spans="1:8">
+    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A46" s="8"/>
       <c r="B46" s="2"/>
       <c r="G46" s="2"/>
       <c r="H46" s="2"/>
     </row>
-    <row r="47" spans="1:8">
+    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A47" s="8"/>
       <c r="B47" s="2"/>
       <c r="G47" s="2"/>
       <c r="H47" s="2"/>
     </row>
-    <row r="48" spans="1:8">
+    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A48" s="8"/>
       <c r="B48" s="2"/>
       <c r="G48" s="2"/>
       <c r="H48" s="2"/>
     </row>
-    <row r="49" spans="1:8">
+    <row r="49" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A49" s="8"/>
       <c r="B49" s="2"/>
       <c r="G49" s="2"/>
       <c r="H49" s="2"/>
     </row>
-    <row r="50" spans="1:8">
+    <row r="50" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A50" s="8"/>
       <c r="B50" s="2"/>
       <c r="G50" s="2"/>
       <c r="H50" s="2"/>
     </row>
-    <row r="51" spans="1:8">
+    <row r="51" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A51" s="8"/>
       <c r="B51" s="2"/>
       <c r="G51" s="2"/>
       <c r="H51" s="2"/>
     </row>
-    <row r="52" spans="1:8">
+    <row r="52" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A52" s="8"/>
       <c r="B52" s="2"/>
       <c r="G52" s="2"/>
       <c r="H52" s="2"/>
     </row>
-    <row r="53" spans="1:8">
+    <row r="53" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A53" s="8"/>
       <c r="B53" s="2"/>
       <c r="G53" s="2"/>
       <c r="H53" s="2"/>
     </row>
-    <row r="54" spans="1:8">
+    <row r="54" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A54" s="8"/>
       <c r="B54" s="2"/>
       <c r="G54" s="2"/>
       <c r="H54" s="2"/>
     </row>
-    <row r="55" spans="1:8">
+    <row r="55" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A55" s="8"/>
       <c r="B55" s="2"/>
       <c r="G55" s="2"/>
       <c r="H55" s="2"/>
     </row>
-    <row r="56" spans="1:8">
+    <row r="56" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A56" s="8"/>
       <c r="B56" s="2"/>
       <c r="G56" s="2"/>
       <c r="H56" s="2"/>
     </row>
-    <row r="57" spans="1:8">
+    <row r="57" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A57" s="8"/>
       <c r="B57" s="2"/>
       <c r="G57" s="2"/>
       <c r="H57" s="2"/>
     </row>
-    <row r="58" spans="1:8">
+    <row r="58" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A58" s="8"/>
       <c r="B58" s="2"/>
       <c r="G58" s="2"/>
       <c r="H58" s="2"/>
     </row>
-    <row r="59" spans="1:8">
+    <row r="59" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A59" s="8"/>
       <c r="B59" s="2"/>
       <c r="G59" s="2"/>
       <c r="H59" s="2"/>
     </row>
-    <row r="60" spans="1:8">
+    <row r="60" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A60" s="8"/>
       <c r="B60" s="2"/>
       <c r="G60" s="2"/>
       <c r="H60" s="2"/>
     </row>
-    <row r="61" spans="1:8">
+    <row r="61" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A61" s="8"/>
       <c r="B61" s="2"/>
       <c r="G61" s="2"/>
       <c r="H61" s="2"/>
     </row>
-    <row r="62" spans="1:8">
+    <row r="62" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A62" s="8"/>
       <c r="B62" s="2"/>
       <c r="G62" s="2"/>
       <c r="H62" s="2"/>
     </row>
-    <row r="63" spans="1:8">
+    <row r="63" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A63" s="8"/>
       <c r="B63" s="2"/>
       <c r="G63" s="2"/>
       <c r="H63" s="2"/>
     </row>
-    <row r="64" spans="1:8">
+    <row r="64" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A64" s="8"/>
       <c r="B64" s="2"/>
       <c r="G64" s="2"/>
       <c r="H64" s="2"/>
     </row>
-    <row r="65" spans="1:8">
+    <row r="65" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A65" s="8"/>
       <c r="B65" s="2"/>
       <c r="G65" s="2"/>
       <c r="H65" s="2"/>
     </row>
-    <row r="66" spans="1:8">
+    <row r="66" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A66" s="8"/>
       <c r="B66" s="2"/>
       <c r="G66" s="2"/>
       <c r="H66" s="2"/>
     </row>
-    <row r="67" spans="1:8">
+    <row r="67" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A67" s="8"/>
       <c r="B67" s="2"/>
       <c r="G67" s="2"/>
       <c r="H67" s="2"/>
     </row>
-    <row r="68" spans="1:8">
+    <row r="68" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A68" s="8"/>
       <c r="B68" s="2"/>
       <c r="G68" s="2"/>
       <c r="H68" s="2"/>
     </row>
-    <row r="69" spans="1:8">
+    <row r="69" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A69" s="8"/>
       <c r="B69" s="2"/>
       <c r="G69" s="2"/>
       <c r="H69" s="2"/>
     </row>
-    <row r="70" spans="1:8">
+    <row r="70" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A70" s="8"/>
       <c r="B70" s="2"/>
       <c r="G70" s="2"/>
       <c r="H70" s="2"/>
     </row>
-    <row r="71" spans="1:8">
+    <row r="71" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A71" s="8"/>
       <c r="B71" s="2"/>
       <c r="G71" s="2"/>
       <c r="H71" s="2"/>
     </row>
-    <row r="72" spans="1:8">
+    <row r="72" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A72" s="8"/>
       <c r="B72" s="2"/>
       <c r="G72" s="2"/>
       <c r="H72" s="2"/>
     </row>
-    <row r="73" spans="1:8">
+    <row r="73" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A73" s="8"/>
       <c r="B73" s="2"/>
       <c r="G73" s="2"/>
       <c r="H73" s="2"/>
     </row>
-    <row r="74" spans="1:8">
+    <row r="74" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A74" s="8"/>
       <c r="B74" s="2"/>
       <c r="G74" s="2"/>
       <c r="H74" s="2"/>
     </row>
-    <row r="75" spans="1:8">
+    <row r="75" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A75" s="8"/>
       <c r="B75" s="2"/>
       <c r="G75" s="2"/>
       <c r="H75" s="2"/>
     </row>
-    <row r="76" spans="1:8">
+    <row r="76" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A76" s="8"/>
       <c r="B76" s="2"/>
       <c r="G76" s="2"/>
       <c r="H76" s="2"/>
     </row>
-    <row r="77" spans="1:8">
+    <row r="77" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A77" s="8"/>
       <c r="B77" s="2"/>
       <c r="G77" s="2"/>
       <c r="H77" s="2"/>
     </row>
-    <row r="78" spans="1:8">
+    <row r="78" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A78" s="8"/>
       <c r="B78" s="2"/>
       <c r="G78" s="2"/>
       <c r="H78" s="2"/>
     </row>
-    <row r="79" spans="1:8">
+    <row r="79" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A79" s="8"/>
       <c r="B79" s="2"/>
       <c r="G79" s="2"/>
       <c r="H79" s="2"/>
     </row>
-    <row r="80" spans="1:8">
+    <row r="80" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A80" s="8"/>
       <c r="B80" s="2"/>
       <c r="G80" s="2"/>
       <c r="H80" s="2"/>
     </row>
-    <row r="81" spans="1:8">
+    <row r="81" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A81" s="8"/>
       <c r="B81" s="2"/>
       <c r="G81" s="2"/>
       <c r="H81" s="2"/>
     </row>
-    <row r="82" spans="1:8">
+    <row r="82" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A82" s="8"/>
       <c r="B82" s="2"/>
       <c r="G82" s="2"/>
       <c r="H82" s="2"/>
     </row>
-    <row r="83" spans="1:8">
+    <row r="83" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A83" s="8"/>
       <c r="B83" s="2"/>
       <c r="G83" s="2"/>
       <c r="H83" s="2"/>
     </row>
-    <row r="84" spans="1:8">
+    <row r="84" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A84" s="8"/>
       <c r="B84" s="2"/>
       <c r="G84" s="2"/>
       <c r="H84" s="2"/>
     </row>
-    <row r="85" spans="1:8">
+    <row r="85" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A85" s="8"/>
       <c r="B85" s="2"/>
       <c r="G85" s="2"/>
       <c r="H85" s="2"/>
     </row>
-    <row r="86" spans="1:8">
+    <row r="86" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A86" s="8"/>
       <c r="B86" s="2"/>
       <c r="G86" s="2"/>
       <c r="H86" s="2"/>
     </row>
-    <row r="87" spans="1:8">
+    <row r="87" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A87" s="8"/>
       <c r="B87" s="2"/>
       <c r="G87" s="2"/>
       <c r="H87" s="2"/>
     </row>
-    <row r="88" spans="1:8">
+    <row r="88" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A88" s="8"/>
       <c r="B88" s="2"/>
       <c r="G88" s="2"/>
       <c r="H88" s="2"/>
     </row>
-    <row r="89" spans="1:8">
+    <row r="89" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A89" s="8"/>
       <c r="B89" s="2"/>
       <c r="G89" s="2"/>
       <c r="H89" s="2"/>
     </row>
-    <row r="90" spans="1:8">
+    <row r="90" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A90" s="8"/>
       <c r="B90" s="2"/>
       <c r="G90" s="2"/>
       <c r="H90" s="2"/>
     </row>
-    <row r="91" spans="1:8">
+    <row r="91" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A91" s="8"/>
       <c r="B91" s="2"/>
       <c r="G91" s="2"/>
       <c r="H91" s="2"/>
     </row>
-    <row r="92" spans="1:8">
+    <row r="92" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A92" s="8"/>
       <c r="B92" s="2"/>
       <c r="G92" s="2"/>
       <c r="H92" s="2"/>
     </row>
-    <row r="93" spans="1:8">
+    <row r="93" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A93" s="8"/>
       <c r="B93" s="2"/>
       <c r="G93" s="2"/>
       <c r="H93" s="2"/>
     </row>
-    <row r="94" spans="1:8">
+    <row r="94" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A94" s="8"/>
       <c r="B94" s="2"/>
       <c r="G94" s="2"/>
       <c r="H94" s="2"/>
     </row>
-    <row r="95" spans="1:8">
+    <row r="95" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A95" s="8"/>
       <c r="B95" s="2"/>
       <c r="G95" s="2"/>
       <c r="H95" s="2"/>
     </row>
-    <row r="96" spans="1:8">
+    <row r="96" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A96" s="8"/>
       <c r="B96" s="2"/>
       <c r="G96" s="2"/>
       <c r="H96" s="2"/>
     </row>
-    <row r="97" spans="1:8">
+    <row r="97" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A97" s="8"/>
       <c r="B97" s="2"/>
       <c r="G97" s="2"/>
       <c r="H97" s="2"/>
     </row>
-    <row r="98" spans="1:8">
+    <row r="98" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A98" s="8"/>
       <c r="B98" s="2"/>
       <c r="G98" s="2"/>
       <c r="H98" s="2"/>
     </row>
-    <row r="99" spans="1:8">
+    <row r="99" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A99" s="8"/>
       <c r="B99" s="2"/>
       <c r="G99" s="2"/>
       <c r="H99" s="2"/>
     </row>
-    <row r="100" spans="1:8">
+    <row r="100" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A100" s="8"/>
       <c r="B100" s="2"/>
       <c r="G100" s="2"/>
@@ -2206,19 +2267,19 @@
       <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="17.33203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="27.88671875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.6640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.88671875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="23.5546875" style="10" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="39.109375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="51.109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="27.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="23.5703125" style="10" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="39.140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="51.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="15.6">
+    <row r="1" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
@@ -2244,7 +2305,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:8">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>45935</v>
       </c>
@@ -2270,7 +2331,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="3" spans="1:8">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>45996</v>
       </c>
@@ -2296,7 +2357,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="4" spans="1:8">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>57</v>
       </c>
@@ -2322,7 +2383,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="5" spans="1:8">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>61</v>
       </c>
@@ -2348,7 +2409,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="6" spans="1:8">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>67</v>
       </c>
@@ -2374,7 +2435,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="7" spans="1:8">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>70</v>
       </c>
@@ -2400,651 +2461,651 @@
         <v>54</v>
       </c>
     </row>
-    <row r="8" spans="1:8">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="1"/>
       <c r="B8" s="2"/>
       <c r="E8" s="3"/>
       <c r="G8" s="2"/>
       <c r="H8" s="2"/>
     </row>
-    <row r="9" spans="1:8">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="1"/>
       <c r="B9" s="2"/>
       <c r="E9" s="3"/>
       <c r="G9" s="2"/>
       <c r="H9" s="2"/>
     </row>
-    <row r="10" spans="1:8">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="1"/>
       <c r="B10" s="2"/>
       <c r="E10" s="3"/>
       <c r="G10" s="2"/>
       <c r="H10" s="2"/>
     </row>
-    <row r="11" spans="1:8">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="1"/>
       <c r="B11" s="2"/>
       <c r="E11" s="3"/>
       <c r="G11" s="2"/>
       <c r="H11" s="2"/>
     </row>
-    <row r="12" spans="1:8">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="1"/>
       <c r="B12" s="2"/>
       <c r="E12" s="3"/>
       <c r="G12" s="2"/>
       <c r="H12" s="2"/>
     </row>
-    <row r="13" spans="1:8">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="1"/>
       <c r="B13" s="2"/>
       <c r="E13" s="3"/>
       <c r="G13" s="2"/>
       <c r="H13" s="2"/>
     </row>
-    <row r="14" spans="1:8">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" s="1"/>
       <c r="B14" s="2"/>
       <c r="E14" s="3"/>
       <c r="G14" s="2"/>
       <c r="H14" s="2"/>
     </row>
-    <row r="15" spans="1:8">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" s="1"/>
       <c r="B15" s="2"/>
       <c r="E15" s="3"/>
       <c r="G15" s="2"/>
       <c r="H15" s="2"/>
     </row>
-    <row r="16" spans="1:8">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" s="1"/>
       <c r="B16" s="2"/>
       <c r="E16" s="3"/>
       <c r="G16" s="2"/>
       <c r="H16" s="2"/>
     </row>
-    <row r="17" spans="1:8">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" s="1"/>
       <c r="B17" s="2"/>
       <c r="E17" s="3"/>
       <c r="G17" s="2"/>
       <c r="H17" s="2"/>
     </row>
-    <row r="18" spans="1:8">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" s="1"/>
       <c r="B18" s="2"/>
       <c r="E18" s="3"/>
       <c r="G18" s="2"/>
       <c r="H18" s="2"/>
     </row>
-    <row r="19" spans="1:8">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" s="1"/>
       <c r="B19" s="2"/>
       <c r="E19" s="3"/>
       <c r="G19" s="2"/>
       <c r="H19" s="2"/>
     </row>
-    <row r="20" spans="1:8">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" s="1"/>
       <c r="B20" s="2"/>
       <c r="E20" s="3"/>
       <c r="G20" s="2"/>
       <c r="H20" s="2"/>
     </row>
-    <row r="21" spans="1:8">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" s="1"/>
       <c r="B21" s="2"/>
       <c r="E21" s="3"/>
       <c r="G21" s="2"/>
       <c r="H21" s="2"/>
     </row>
-    <row r="22" spans="1:8">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" s="1"/>
       <c r="B22" s="2"/>
       <c r="E22" s="3"/>
       <c r="G22" s="2"/>
       <c r="H22" s="2"/>
     </row>
-    <row r="23" spans="1:8">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" s="1"/>
       <c r="B23" s="2"/>
       <c r="E23" s="3"/>
       <c r="G23" s="2"/>
       <c r="H23" s="2"/>
     </row>
-    <row r="24" spans="1:8">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24" s="1"/>
       <c r="B24" s="2"/>
       <c r="E24" s="3"/>
       <c r="G24" s="2"/>
       <c r="H24" s="2"/>
     </row>
-    <row r="25" spans="1:8">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25" s="1"/>
       <c r="B25" s="2"/>
       <c r="E25" s="3"/>
       <c r="G25" s="2"/>
       <c r="H25" s="2"/>
     </row>
-    <row r="26" spans="1:8">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26" s="1"/>
       <c r="B26" s="2"/>
       <c r="E26" s="3"/>
       <c r="G26" s="2"/>
       <c r="H26" s="2"/>
     </row>
-    <row r="27" spans="1:8">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A27" s="1"/>
       <c r="B27" s="2"/>
       <c r="E27" s="3"/>
       <c r="G27" s="2"/>
       <c r="H27" s="2"/>
     </row>
-    <row r="28" spans="1:8">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A28" s="1"/>
       <c r="B28" s="2"/>
       <c r="E28" s="3"/>
       <c r="G28" s="2"/>
       <c r="H28" s="2"/>
     </row>
-    <row r="29" spans="1:8">
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A29" s="1"/>
       <c r="B29" s="2"/>
       <c r="E29" s="3"/>
       <c r="G29" s="2"/>
       <c r="H29" s="2"/>
     </row>
-    <row r="30" spans="1:8">
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A30" s="1"/>
       <c r="B30" s="2"/>
       <c r="E30" s="3"/>
       <c r="G30" s="2"/>
       <c r="H30" s="2"/>
     </row>
-    <row r="31" spans="1:8">
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A31" s="1"/>
       <c r="B31" s="2"/>
       <c r="E31" s="3"/>
       <c r="G31" s="2"/>
       <c r="H31" s="2"/>
     </row>
-    <row r="32" spans="1:8">
+    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A32" s="1"/>
       <c r="B32" s="2"/>
       <c r="E32" s="3"/>
       <c r="G32" s="2"/>
       <c r="H32" s="2"/>
     </row>
-    <row r="33" spans="1:8">
+    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A33" s="1"/>
       <c r="B33" s="2"/>
       <c r="E33" s="3"/>
       <c r="G33" s="2"/>
       <c r="H33" s="2"/>
     </row>
-    <row r="34" spans="1:8">
+    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A34" s="1"/>
       <c r="B34" s="2"/>
       <c r="E34" s="3"/>
       <c r="G34" s="2"/>
       <c r="H34" s="2"/>
     </row>
-    <row r="35" spans="1:8">
+    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A35" s="1"/>
       <c r="B35" s="2"/>
       <c r="E35" s="3"/>
       <c r="G35" s="2"/>
       <c r="H35" s="2"/>
     </row>
-    <row r="36" spans="1:8">
+    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A36" s="1"/>
       <c r="B36" s="2"/>
       <c r="E36" s="3"/>
       <c r="G36" s="2"/>
       <c r="H36" s="2"/>
     </row>
-    <row r="37" spans="1:8">
+    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A37" s="1"/>
       <c r="B37" s="2"/>
       <c r="E37" s="3"/>
       <c r="G37" s="2"/>
       <c r="H37" s="2"/>
     </row>
-    <row r="38" spans="1:8">
+    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A38" s="1"/>
       <c r="B38" s="2"/>
       <c r="E38" s="3"/>
       <c r="G38" s="2"/>
       <c r="H38" s="2"/>
     </row>
-    <row r="39" spans="1:8">
+    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A39" s="1"/>
       <c r="B39" s="2"/>
       <c r="E39" s="3"/>
       <c r="G39" s="2"/>
       <c r="H39" s="2"/>
     </row>
-    <row r="40" spans="1:8">
+    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A40" s="1"/>
       <c r="B40" s="2"/>
       <c r="E40" s="3"/>
       <c r="G40" s="2"/>
       <c r="H40" s="2"/>
     </row>
-    <row r="41" spans="1:8">
+    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A41" s="1"/>
       <c r="B41" s="2"/>
       <c r="E41" s="3"/>
       <c r="G41" s="2"/>
       <c r="H41" s="2"/>
     </row>
-    <row r="42" spans="1:8">
+    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A42" s="1"/>
       <c r="B42" s="2"/>
       <c r="E42" s="3"/>
       <c r="G42" s="2"/>
       <c r="H42" s="2"/>
     </row>
-    <row r="43" spans="1:8">
+    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A43" s="1"/>
       <c r="B43" s="2"/>
       <c r="E43" s="3"/>
       <c r="G43" s="2"/>
       <c r="H43" s="2"/>
     </row>
-    <row r="44" spans="1:8">
+    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A44" s="1"/>
       <c r="B44" s="2"/>
       <c r="E44" s="3"/>
       <c r="G44" s="2"/>
       <c r="H44" s="2"/>
     </row>
-    <row r="45" spans="1:8">
+    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A45" s="1"/>
       <c r="B45" s="2"/>
       <c r="E45" s="3"/>
       <c r="G45" s="2"/>
       <c r="H45" s="2"/>
     </row>
-    <row r="46" spans="1:8">
+    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A46" s="1"/>
       <c r="B46" s="2"/>
       <c r="E46" s="3"/>
       <c r="G46" s="2"/>
       <c r="H46" s="2"/>
     </row>
-    <row r="47" spans="1:8">
+    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A47" s="1"/>
       <c r="B47" s="2"/>
       <c r="E47" s="3"/>
       <c r="G47" s="2"/>
       <c r="H47" s="2"/>
     </row>
-    <row r="48" spans="1:8">
+    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A48" s="1"/>
       <c r="B48" s="2"/>
       <c r="E48" s="3"/>
       <c r="G48" s="2"/>
       <c r="H48" s="2"/>
     </row>
-    <row r="49" spans="1:8">
+    <row r="49" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A49" s="1"/>
       <c r="B49" s="2"/>
       <c r="E49" s="3"/>
       <c r="G49" s="2"/>
       <c r="H49" s="2"/>
     </row>
-    <row r="50" spans="1:8">
+    <row r="50" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A50" s="1"/>
       <c r="B50" s="2"/>
       <c r="E50" s="3"/>
       <c r="G50" s="2"/>
       <c r="H50" s="2"/>
     </row>
-    <row r="51" spans="1:8">
+    <row r="51" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A51" s="1"/>
       <c r="B51" s="2"/>
       <c r="E51" s="3"/>
       <c r="G51" s="2"/>
       <c r="H51" s="2"/>
     </row>
-    <row r="52" spans="1:8">
+    <row r="52" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A52" s="1"/>
       <c r="B52" s="2"/>
       <c r="E52" s="3"/>
       <c r="G52" s="2"/>
       <c r="H52" s="2"/>
     </row>
-    <row r="53" spans="1:8">
+    <row r="53" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A53" s="1"/>
       <c r="B53" s="2"/>
       <c r="E53" s="3"/>
       <c r="G53" s="2"/>
       <c r="H53" s="2"/>
     </row>
-    <row r="54" spans="1:8">
+    <row r="54" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A54" s="1"/>
       <c r="B54" s="2"/>
       <c r="E54" s="3"/>
       <c r="G54" s="2"/>
       <c r="H54" s="2"/>
     </row>
-    <row r="55" spans="1:8">
+    <row r="55" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A55" s="1"/>
       <c r="B55" s="2"/>
       <c r="E55" s="3"/>
       <c r="G55" s="2"/>
       <c r="H55" s="2"/>
     </row>
-    <row r="56" spans="1:8">
+    <row r="56" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A56" s="1"/>
       <c r="B56" s="2"/>
       <c r="E56" s="3"/>
       <c r="G56" s="2"/>
       <c r="H56" s="2"/>
     </row>
-    <row r="57" spans="1:8">
+    <row r="57" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A57" s="1"/>
       <c r="B57" s="2"/>
       <c r="E57" s="3"/>
       <c r="G57" s="2"/>
       <c r="H57" s="2"/>
     </row>
-    <row r="58" spans="1:8">
+    <row r="58" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A58" s="1"/>
       <c r="B58" s="2"/>
       <c r="E58" s="3"/>
       <c r="G58" s="2"/>
       <c r="H58" s="2"/>
     </row>
-    <row r="59" spans="1:8">
+    <row r="59" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A59" s="1"/>
       <c r="B59" s="2"/>
       <c r="E59" s="3"/>
       <c r="G59" s="2"/>
       <c r="H59" s="2"/>
     </row>
-    <row r="60" spans="1:8">
+    <row r="60" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A60" s="1"/>
       <c r="B60" s="2"/>
       <c r="E60" s="3"/>
       <c r="G60" s="2"/>
       <c r="H60" s="2"/>
     </row>
-    <row r="61" spans="1:8">
+    <row r="61" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A61" s="1"/>
       <c r="B61" s="2"/>
       <c r="E61" s="3"/>
       <c r="G61" s="2"/>
       <c r="H61" s="2"/>
     </row>
-    <row r="62" spans="1:8">
+    <row r="62" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A62" s="1"/>
       <c r="B62" s="2"/>
       <c r="E62" s="3"/>
       <c r="G62" s="2"/>
       <c r="H62" s="2"/>
     </row>
-    <row r="63" spans="1:8">
+    <row r="63" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A63" s="1"/>
       <c r="B63" s="2"/>
       <c r="E63" s="3"/>
       <c r="G63" s="2"/>
       <c r="H63" s="2"/>
     </row>
-    <row r="64" spans="1:8">
+    <row r="64" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A64" s="1"/>
       <c r="B64" s="2"/>
       <c r="E64" s="3"/>
       <c r="G64" s="2"/>
       <c r="H64" s="2"/>
     </row>
-    <row r="65" spans="1:8">
+    <row r="65" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A65" s="1"/>
       <c r="B65" s="2"/>
       <c r="E65" s="3"/>
       <c r="G65" s="2"/>
       <c r="H65" s="2"/>
     </row>
-    <row r="66" spans="1:8">
+    <row r="66" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A66" s="1"/>
       <c r="B66" s="2"/>
       <c r="E66" s="3"/>
       <c r="G66" s="2"/>
       <c r="H66" s="2"/>
     </row>
-    <row r="67" spans="1:8">
+    <row r="67" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A67" s="1"/>
       <c r="B67" s="2"/>
       <c r="E67" s="3"/>
       <c r="G67" s="2"/>
       <c r="H67" s="2"/>
     </row>
-    <row r="68" spans="1:8">
+    <row r="68" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A68" s="1"/>
       <c r="B68" s="2"/>
       <c r="E68" s="3"/>
       <c r="G68" s="2"/>
       <c r="H68" s="2"/>
     </row>
-    <row r="69" spans="1:8">
+    <row r="69" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A69" s="1"/>
       <c r="B69" s="2"/>
       <c r="E69" s="3"/>
       <c r="G69" s="2"/>
       <c r="H69" s="2"/>
     </row>
-    <row r="70" spans="1:8">
+    <row r="70" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A70" s="1"/>
       <c r="B70" s="2"/>
       <c r="E70" s="3"/>
       <c r="G70" s="2"/>
       <c r="H70" s="2"/>
     </row>
-    <row r="71" spans="1:8">
+    <row r="71" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A71" s="1"/>
       <c r="B71" s="2"/>
       <c r="E71" s="3"/>
       <c r="G71" s="2"/>
       <c r="H71" s="2"/>
     </row>
-    <row r="72" spans="1:8">
+    <row r="72" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A72" s="1"/>
       <c r="B72" s="2"/>
       <c r="E72" s="3"/>
       <c r="G72" s="2"/>
       <c r="H72" s="2"/>
     </row>
-    <row r="73" spans="1:8">
+    <row r="73" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A73" s="1"/>
       <c r="B73" s="2"/>
       <c r="E73" s="3"/>
       <c r="G73" s="2"/>
       <c r="H73" s="2"/>
     </row>
-    <row r="74" spans="1:8">
+    <row r="74" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A74" s="1"/>
       <c r="B74" s="2"/>
       <c r="E74" s="3"/>
       <c r="G74" s="2"/>
       <c r="H74" s="2"/>
     </row>
-    <row r="75" spans="1:8">
+    <row r="75" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A75" s="1"/>
       <c r="B75" s="2"/>
       <c r="E75" s="3"/>
       <c r="G75" s="2"/>
       <c r="H75" s="2"/>
     </row>
-    <row r="76" spans="1:8">
+    <row r="76" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A76" s="1"/>
       <c r="B76" s="2"/>
       <c r="E76" s="3"/>
       <c r="G76" s="2"/>
       <c r="H76" s="2"/>
     </row>
-    <row r="77" spans="1:8">
+    <row r="77" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A77" s="1"/>
       <c r="B77" s="2"/>
       <c r="E77" s="3"/>
       <c r="G77" s="2"/>
       <c r="H77" s="2"/>
     </row>
-    <row r="78" spans="1:8">
+    <row r="78" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A78" s="1"/>
       <c r="B78" s="2"/>
       <c r="E78" s="3"/>
       <c r="G78" s="2"/>
       <c r="H78" s="2"/>
     </row>
-    <row r="79" spans="1:8">
+    <row r="79" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A79" s="1"/>
       <c r="B79" s="2"/>
       <c r="E79" s="3"/>
       <c r="G79" s="2"/>
       <c r="H79" s="2"/>
     </row>
-    <row r="80" spans="1:8">
+    <row r="80" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A80" s="1"/>
       <c r="B80" s="2"/>
       <c r="E80" s="3"/>
       <c r="G80" s="2"/>
       <c r="H80" s="2"/>
     </row>
-    <row r="81" spans="1:8">
+    <row r="81" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A81" s="1"/>
       <c r="B81" s="2"/>
       <c r="E81" s="3"/>
       <c r="G81" s="2"/>
       <c r="H81" s="2"/>
     </row>
-    <row r="82" spans="1:8">
+    <row r="82" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A82" s="1"/>
       <c r="B82" s="2"/>
       <c r="E82" s="3"/>
       <c r="G82" s="2"/>
       <c r="H82" s="2"/>
     </row>
-    <row r="83" spans="1:8">
+    <row r="83" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A83" s="1"/>
       <c r="B83" s="2"/>
       <c r="E83" s="3"/>
       <c r="G83" s="2"/>
       <c r="H83" s="2"/>
     </row>
-    <row r="84" spans="1:8">
+    <row r="84" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A84" s="1"/>
       <c r="B84" s="2"/>
       <c r="E84" s="3"/>
       <c r="G84" s="2"/>
       <c r="H84" s="2"/>
     </row>
-    <row r="85" spans="1:8">
+    <row r="85" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A85" s="1"/>
       <c r="B85" s="2"/>
       <c r="E85" s="3"/>
       <c r="G85" s="2"/>
       <c r="H85" s="2"/>
     </row>
-    <row r="86" spans="1:8">
+    <row r="86" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A86" s="1"/>
       <c r="B86" s="2"/>
       <c r="E86" s="3"/>
       <c r="G86" s="2"/>
       <c r="H86" s="2"/>
     </row>
-    <row r="87" spans="1:8">
+    <row r="87" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A87" s="1"/>
       <c r="B87" s="2"/>
       <c r="E87" s="3"/>
       <c r="G87" s="2"/>
       <c r="H87" s="2"/>
     </row>
-    <row r="88" spans="1:8">
+    <row r="88" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A88" s="1"/>
       <c r="B88" s="2"/>
       <c r="E88" s="3"/>
       <c r="G88" s="2"/>
       <c r="H88" s="2"/>
     </row>
-    <row r="89" spans="1:8">
+    <row r="89" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A89" s="1"/>
       <c r="B89" s="2"/>
       <c r="E89" s="3"/>
       <c r="G89" s="2"/>
       <c r="H89" s="2"/>
     </row>
-    <row r="90" spans="1:8">
+    <row r="90" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A90" s="1"/>
       <c r="B90" s="2"/>
       <c r="E90" s="3"/>
       <c r="G90" s="2"/>
       <c r="H90" s="2"/>
     </row>
-    <row r="91" spans="1:8">
+    <row r="91" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A91" s="1"/>
       <c r="B91" s="2"/>
       <c r="E91" s="3"/>
       <c r="G91" s="2"/>
       <c r="H91" s="2"/>
     </row>
-    <row r="92" spans="1:8">
+    <row r="92" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A92" s="1"/>
       <c r="B92" s="2"/>
       <c r="E92" s="3"/>
       <c r="G92" s="2"/>
       <c r="H92" s="2"/>
     </row>
-    <row r="93" spans="1:8">
+    <row r="93" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A93" s="1"/>
       <c r="B93" s="2"/>
       <c r="E93" s="3"/>
       <c r="G93" s="2"/>
       <c r="H93" s="2"/>
     </row>
-    <row r="94" spans="1:8">
+    <row r="94" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A94" s="1"/>
       <c r="B94" s="2"/>
       <c r="E94" s="3"/>
       <c r="G94" s="2"/>
       <c r="H94" s="2"/>
     </row>
-    <row r="95" spans="1:8">
+    <row r="95" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A95" s="1"/>
       <c r="B95" s="2"/>
       <c r="E95" s="3"/>
       <c r="G95" s="2"/>
       <c r="H95" s="2"/>
     </row>
-    <row r="96" spans="1:8">
+    <row r="96" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A96" s="1"/>
       <c r="B96" s="2"/>
       <c r="E96" s="3"/>
       <c r="G96" s="2"/>
       <c r="H96" s="2"/>
     </row>
-    <row r="97" spans="1:8">
+    <row r="97" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A97" s="1"/>
       <c r="B97" s="2"/>
       <c r="E97" s="3"/>
       <c r="G97" s="2"/>
       <c r="H97" s="2"/>
     </row>
-    <row r="98" spans="1:8">
+    <row r="98" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A98" s="1"/>
       <c r="B98" s="2"/>
       <c r="E98" s="3"/>
       <c r="G98" s="2"/>
       <c r="H98" s="2"/>
     </row>
-    <row r="99" spans="1:8">
+    <row r="99" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A99" s="1"/>
       <c r="B99" s="2"/>
       <c r="E99" s="3"/>
       <c r="G99" s="2"/>
       <c r="H99" s="2"/>
     </row>
-    <row r="100" spans="1:8">
+    <row r="100" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A100" s="1"/>
       <c r="B100" s="2"/>
       <c r="E100" s="3"/>
@@ -3086,19 +3147,19 @@
       <selection activeCell="D2" sqref="D2:D100"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="7.6640625" customWidth="1"/>
-    <col min="2" max="2" width="17.33203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.5546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="7.7109375" customWidth="1"/>
+    <col min="2" max="2" width="17.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.5703125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="9" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.88671875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="23.5546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="13.44140625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="19.109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="23.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="19.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="15.6">
+    <row r="1" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
@@ -3124,7 +3185,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:8">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="1"/>
       <c r="B2" s="2"/>
       <c r="E2" s="3"/>
@@ -3132,7 +3193,7 @@
       <c r="G2" s="2"/>
       <c r="H2" s="2"/>
     </row>
-    <row r="3" spans="1:8">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="1"/>
       <c r="B3" s="2"/>
       <c r="E3" s="3"/>
@@ -3140,7 +3201,7 @@
       <c r="G3" s="2"/>
       <c r="H3" s="2"/>
     </row>
-    <row r="4" spans="1:8">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="1"/>
       <c r="B4" s="2"/>
       <c r="E4" s="3"/>
@@ -3148,7 +3209,7 @@
       <c r="G4" s="2"/>
       <c r="H4" s="2"/>
     </row>
-    <row r="5" spans="1:8">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="1"/>
       <c r="B5" s="2"/>
       <c r="E5" s="3"/>
@@ -3156,7 +3217,7 @@
       <c r="G5" s="2"/>
       <c r="H5" s="2"/>
     </row>
-    <row r="6" spans="1:8">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="1"/>
       <c r="B6" s="2"/>
       <c r="E6" s="3"/>
@@ -3164,7 +3225,7 @@
       <c r="G6" s="2"/>
       <c r="H6" s="2"/>
     </row>
-    <row r="7" spans="1:8">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="1"/>
       <c r="B7" s="2"/>
       <c r="E7" s="3"/>
@@ -3172,7 +3233,7 @@
       <c r="G7" s="2"/>
       <c r="H7" s="2"/>
     </row>
-    <row r="8" spans="1:8">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="1"/>
       <c r="B8" s="2"/>
       <c r="E8" s="3"/>
@@ -3180,7 +3241,7 @@
       <c r="G8" s="2"/>
       <c r="H8" s="2"/>
     </row>
-    <row r="9" spans="1:8">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="1"/>
       <c r="B9" s="2"/>
       <c r="E9" s="3"/>
@@ -3188,7 +3249,7 @@
       <c r="G9" s="2"/>
       <c r="H9" s="2"/>
     </row>
-    <row r="10" spans="1:8">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="1"/>
       <c r="B10" s="2"/>
       <c r="E10" s="3"/>
@@ -3196,7 +3257,7 @@
       <c r="G10" s="2"/>
       <c r="H10" s="2"/>
     </row>
-    <row r="11" spans="1:8">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="1"/>
       <c r="B11" s="2"/>
       <c r="E11" s="3"/>
@@ -3204,7 +3265,7 @@
       <c r="G11" s="2"/>
       <c r="H11" s="2"/>
     </row>
-    <row r="12" spans="1:8">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="1"/>
       <c r="B12" s="2"/>
       <c r="E12" s="3"/>
@@ -3212,7 +3273,7 @@
       <c r="G12" s="2"/>
       <c r="H12" s="2"/>
     </row>
-    <row r="13" spans="1:8">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="1"/>
       <c r="B13" s="2"/>
       <c r="E13" s="3"/>
@@ -3220,7 +3281,7 @@
       <c r="G13" s="2"/>
       <c r="H13" s="2"/>
     </row>
-    <row r="14" spans="1:8">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" s="1"/>
       <c r="B14" s="2"/>
       <c r="E14" s="3"/>
@@ -3228,7 +3289,7 @@
       <c r="G14" s="2"/>
       <c r="H14" s="2"/>
     </row>
-    <row r="15" spans="1:8">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" s="1"/>
       <c r="B15" s="2"/>
       <c r="E15" s="3"/>
@@ -3236,7 +3297,7 @@
       <c r="G15" s="2"/>
       <c r="H15" s="2"/>
     </row>
-    <row r="16" spans="1:8">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" s="1"/>
       <c r="B16" s="2"/>
       <c r="E16" s="3"/>
@@ -3244,7 +3305,7 @@
       <c r="G16" s="2"/>
       <c r="H16" s="2"/>
     </row>
-    <row r="17" spans="1:8">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" s="1"/>
       <c r="B17" s="2"/>
       <c r="E17" s="3"/>
@@ -3252,7 +3313,7 @@
       <c r="G17" s="2"/>
       <c r="H17" s="2"/>
     </row>
-    <row r="18" spans="1:8">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" s="1"/>
       <c r="B18" s="2"/>
       <c r="E18" s="3"/>
@@ -3260,7 +3321,7 @@
       <c r="G18" s="2"/>
       <c r="H18" s="2"/>
     </row>
-    <row r="19" spans="1:8">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" s="1"/>
       <c r="B19" s="2"/>
       <c r="E19" s="3"/>
@@ -3268,7 +3329,7 @@
       <c r="G19" s="2"/>
       <c r="H19" s="2"/>
     </row>
-    <row r="20" spans="1:8">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" s="1"/>
       <c r="B20" s="2"/>
       <c r="E20" s="3"/>
@@ -3276,7 +3337,7 @@
       <c r="G20" s="2"/>
       <c r="H20" s="2"/>
     </row>
-    <row r="21" spans="1:8">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" s="1"/>
       <c r="B21" s="2"/>
       <c r="E21" s="3"/>
@@ -3284,7 +3345,7 @@
       <c r="G21" s="2"/>
       <c r="H21" s="2"/>
     </row>
-    <row r="22" spans="1:8">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" s="1"/>
       <c r="B22" s="2"/>
       <c r="E22" s="3"/>
@@ -3292,7 +3353,7 @@
       <c r="G22" s="2"/>
       <c r="H22" s="2"/>
     </row>
-    <row r="23" spans="1:8">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" s="1"/>
       <c r="B23" s="2"/>
       <c r="E23" s="3"/>
@@ -3300,7 +3361,7 @@
       <c r="G23" s="2"/>
       <c r="H23" s="2"/>
     </row>
-    <row r="24" spans="1:8">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24" s="1"/>
       <c r="B24" s="2"/>
       <c r="E24" s="3"/>
@@ -3308,7 +3369,7 @@
       <c r="G24" s="2"/>
       <c r="H24" s="2"/>
     </row>
-    <row r="25" spans="1:8">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25" s="1"/>
       <c r="B25" s="2"/>
       <c r="E25" s="3"/>
@@ -3316,7 +3377,7 @@
       <c r="G25" s="2"/>
       <c r="H25" s="2"/>
     </row>
-    <row r="26" spans="1:8">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26" s="1"/>
       <c r="B26" s="2"/>
       <c r="E26" s="3"/>
@@ -3324,7 +3385,7 @@
       <c r="G26" s="2"/>
       <c r="H26" s="2"/>
     </row>
-    <row r="27" spans="1:8">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A27" s="1"/>
       <c r="B27" s="2"/>
       <c r="E27" s="3"/>
@@ -3332,7 +3393,7 @@
       <c r="G27" s="2"/>
       <c r="H27" s="2"/>
     </row>
-    <row r="28" spans="1:8">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A28" s="1"/>
       <c r="B28" s="2"/>
       <c r="E28" s="3"/>
@@ -3340,7 +3401,7 @@
       <c r="G28" s="2"/>
       <c r="H28" s="2"/>
     </row>
-    <row r="29" spans="1:8">
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A29" s="1"/>
       <c r="B29" s="2"/>
       <c r="E29" s="3"/>
@@ -3348,7 +3409,7 @@
       <c r="G29" s="2"/>
       <c r="H29" s="2"/>
     </row>
-    <row r="30" spans="1:8">
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A30" s="1"/>
       <c r="B30" s="2"/>
       <c r="E30" s="3"/>
@@ -3356,7 +3417,7 @@
       <c r="G30" s="2"/>
       <c r="H30" s="2"/>
     </row>
-    <row r="31" spans="1:8">
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A31" s="1"/>
       <c r="B31" s="2"/>
       <c r="E31" s="3"/>
@@ -3364,7 +3425,7 @@
       <c r="G31" s="2"/>
       <c r="H31" s="2"/>
     </row>
-    <row r="32" spans="1:8">
+    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A32" s="1"/>
       <c r="B32" s="2"/>
       <c r="E32" s="3"/>
@@ -3372,7 +3433,7 @@
       <c r="G32" s="2"/>
       <c r="H32" s="2"/>
     </row>
-    <row r="33" spans="1:8">
+    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A33" s="1"/>
       <c r="B33" s="2"/>
       <c r="E33" s="3"/>
@@ -3380,7 +3441,7 @@
       <c r="G33" s="2"/>
       <c r="H33" s="2"/>
     </row>
-    <row r="34" spans="1:8">
+    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A34" s="1"/>
       <c r="B34" s="2"/>
       <c r="E34" s="3"/>
@@ -3388,7 +3449,7 @@
       <c r="G34" s="2"/>
       <c r="H34" s="2"/>
     </row>
-    <row r="35" spans="1:8">
+    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A35" s="1"/>
       <c r="B35" s="2"/>
       <c r="E35" s="3"/>
@@ -3396,7 +3457,7 @@
       <c r="G35" s="2"/>
       <c r="H35" s="2"/>
     </row>
-    <row r="36" spans="1:8">
+    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A36" s="1"/>
       <c r="B36" s="2"/>
       <c r="E36" s="3"/>
@@ -3404,7 +3465,7 @@
       <c r="G36" s="2"/>
       <c r="H36" s="2"/>
     </row>
-    <row r="37" spans="1:8">
+    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A37" s="1"/>
       <c r="B37" s="2"/>
       <c r="E37" s="3"/>
@@ -3412,7 +3473,7 @@
       <c r="G37" s="2"/>
       <c r="H37" s="2"/>
     </row>
-    <row r="38" spans="1:8">
+    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A38" s="1"/>
       <c r="B38" s="2"/>
       <c r="E38" s="3"/>
@@ -3420,7 +3481,7 @@
       <c r="G38" s="2"/>
       <c r="H38" s="2"/>
     </row>
-    <row r="39" spans="1:8">
+    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A39" s="1"/>
       <c r="B39" s="2"/>
       <c r="E39" s="3"/>
@@ -3428,7 +3489,7 @@
       <c r="G39" s="2"/>
       <c r="H39" s="2"/>
     </row>
-    <row r="40" spans="1:8">
+    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A40" s="1"/>
       <c r="B40" s="2"/>
       <c r="E40" s="3"/>
@@ -3436,7 +3497,7 @@
       <c r="G40" s="2"/>
       <c r="H40" s="2"/>
     </row>
-    <row r="41" spans="1:8">
+    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A41" s="1"/>
       <c r="B41" s="2"/>
       <c r="E41" s="3"/>
@@ -3444,7 +3505,7 @@
       <c r="G41" s="2"/>
       <c r="H41" s="2"/>
     </row>
-    <row r="42" spans="1:8">
+    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A42" s="1"/>
       <c r="B42" s="2"/>
       <c r="E42" s="3"/>
@@ -3452,7 +3513,7 @@
       <c r="G42" s="2"/>
       <c r="H42" s="2"/>
     </row>
-    <row r="43" spans="1:8">
+    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A43" s="1"/>
       <c r="B43" s="2"/>
       <c r="E43" s="3"/>
@@ -3460,7 +3521,7 @@
       <c r="G43" s="2"/>
       <c r="H43" s="2"/>
     </row>
-    <row r="44" spans="1:8">
+    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A44" s="1"/>
       <c r="B44" s="2"/>
       <c r="E44" s="3"/>
@@ -3468,7 +3529,7 @@
       <c r="G44" s="2"/>
       <c r="H44" s="2"/>
     </row>
-    <row r="45" spans="1:8">
+    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A45" s="1"/>
       <c r="B45" s="2"/>
       <c r="E45" s="3"/>
@@ -3476,7 +3537,7 @@
       <c r="G45" s="2"/>
       <c r="H45" s="2"/>
     </row>
-    <row r="46" spans="1:8">
+    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A46" s="1"/>
       <c r="B46" s="2"/>
       <c r="E46" s="3"/>
@@ -3484,7 +3545,7 @@
       <c r="G46" s="2"/>
       <c r="H46" s="2"/>
     </row>
-    <row r="47" spans="1:8">
+    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A47" s="1"/>
       <c r="B47" s="2"/>
       <c r="E47" s="3"/>
@@ -3492,7 +3553,7 @@
       <c r="G47" s="2"/>
       <c r="H47" s="2"/>
     </row>
-    <row r="48" spans="1:8">
+    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A48" s="1"/>
       <c r="B48" s="2"/>
       <c r="E48" s="3"/>
@@ -3500,7 +3561,7 @@
       <c r="G48" s="2"/>
       <c r="H48" s="2"/>
     </row>
-    <row r="49" spans="1:8">
+    <row r="49" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A49" s="1"/>
       <c r="B49" s="2"/>
       <c r="E49" s="3"/>
@@ -3508,7 +3569,7 @@
       <c r="G49" s="2"/>
       <c r="H49" s="2"/>
     </row>
-    <row r="50" spans="1:8">
+    <row r="50" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A50" s="1"/>
       <c r="B50" s="2"/>
       <c r="E50" s="3"/>
@@ -3516,7 +3577,7 @@
       <c r="G50" s="2"/>
       <c r="H50" s="2"/>
     </row>
-    <row r="51" spans="1:8">
+    <row r="51" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A51" s="1"/>
       <c r="B51" s="2"/>
       <c r="E51" s="3"/>
@@ -3524,7 +3585,7 @@
       <c r="G51" s="2"/>
       <c r="H51" s="2"/>
     </row>
-    <row r="52" spans="1:8">
+    <row r="52" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A52" s="1"/>
       <c r="B52" s="2"/>
       <c r="E52" s="3"/>
@@ -3532,7 +3593,7 @@
       <c r="G52" s="2"/>
       <c r="H52" s="2"/>
     </row>
-    <row r="53" spans="1:8">
+    <row r="53" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A53" s="1"/>
       <c r="B53" s="2"/>
       <c r="E53" s="3"/>
@@ -3540,7 +3601,7 @@
       <c r="G53" s="2"/>
       <c r="H53" s="2"/>
     </row>
-    <row r="54" spans="1:8">
+    <row r="54" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A54" s="1"/>
       <c r="B54" s="2"/>
       <c r="E54" s="3"/>
@@ -3548,7 +3609,7 @@
       <c r="G54" s="2"/>
       <c r="H54" s="2"/>
     </row>
-    <row r="55" spans="1:8">
+    <row r="55" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A55" s="1"/>
       <c r="B55" s="2"/>
       <c r="E55" s="3"/>
@@ -3556,7 +3617,7 @@
       <c r="G55" s="2"/>
       <c r="H55" s="2"/>
     </row>
-    <row r="56" spans="1:8">
+    <row r="56" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A56" s="1"/>
       <c r="B56" s="2"/>
       <c r="E56" s="3"/>
@@ -3564,7 +3625,7 @@
       <c r="G56" s="2"/>
       <c r="H56" s="2"/>
     </row>
-    <row r="57" spans="1:8">
+    <row r="57" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A57" s="1"/>
       <c r="B57" s="2"/>
       <c r="E57" s="3"/>
@@ -3572,7 +3633,7 @@
       <c r="G57" s="2"/>
       <c r="H57" s="2"/>
     </row>
-    <row r="58" spans="1:8">
+    <row r="58" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A58" s="1"/>
       <c r="B58" s="2"/>
       <c r="E58" s="3"/>
@@ -3580,7 +3641,7 @@
       <c r="G58" s="2"/>
       <c r="H58" s="2"/>
     </row>
-    <row r="59" spans="1:8">
+    <row r="59" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A59" s="1"/>
       <c r="B59" s="2"/>
       <c r="E59" s="3"/>
@@ -3588,7 +3649,7 @@
       <c r="G59" s="2"/>
       <c r="H59" s="2"/>
     </row>
-    <row r="60" spans="1:8">
+    <row r="60" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A60" s="1"/>
       <c r="B60" s="2"/>
       <c r="E60" s="3"/>
@@ -3596,7 +3657,7 @@
       <c r="G60" s="2"/>
       <c r="H60" s="2"/>
     </row>
-    <row r="61" spans="1:8">
+    <row r="61" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A61" s="1"/>
       <c r="B61" s="2"/>
       <c r="E61" s="3"/>
@@ -3604,7 +3665,7 @@
       <c r="G61" s="2"/>
       <c r="H61" s="2"/>
     </row>
-    <row r="62" spans="1:8">
+    <row r="62" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A62" s="1"/>
       <c r="B62" s="2"/>
       <c r="E62" s="3"/>
@@ -3612,7 +3673,7 @@
       <c r="G62" s="2"/>
       <c r="H62" s="2"/>
     </row>
-    <row r="63" spans="1:8">
+    <row r="63" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A63" s="1"/>
       <c r="B63" s="2"/>
       <c r="E63" s="3"/>
@@ -3620,7 +3681,7 @@
       <c r="G63" s="2"/>
       <c r="H63" s="2"/>
     </row>
-    <row r="64" spans="1:8">
+    <row r="64" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A64" s="1"/>
       <c r="B64" s="2"/>
       <c r="E64" s="3"/>
@@ -3628,7 +3689,7 @@
       <c r="G64" s="2"/>
       <c r="H64" s="2"/>
     </row>
-    <row r="65" spans="1:8">
+    <row r="65" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A65" s="1"/>
       <c r="B65" s="2"/>
       <c r="E65" s="3"/>
@@ -3636,7 +3697,7 @@
       <c r="G65" s="2"/>
       <c r="H65" s="2"/>
     </row>
-    <row r="66" spans="1:8">
+    <row r="66" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A66" s="1"/>
       <c r="B66" s="2"/>
       <c r="E66" s="3"/>
@@ -3644,7 +3705,7 @@
       <c r="G66" s="2"/>
       <c r="H66" s="2"/>
     </row>
-    <row r="67" spans="1:8">
+    <row r="67" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A67" s="1"/>
       <c r="B67" s="2"/>
       <c r="E67" s="3"/>
@@ -3652,7 +3713,7 @@
       <c r="G67" s="2"/>
       <c r="H67" s="2"/>
     </row>
-    <row r="68" spans="1:8">
+    <row r="68" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A68" s="1"/>
       <c r="B68" s="2"/>
       <c r="E68" s="3"/>
@@ -3660,7 +3721,7 @@
       <c r="G68" s="2"/>
       <c r="H68" s="2"/>
     </row>
-    <row r="69" spans="1:8">
+    <row r="69" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A69" s="1"/>
       <c r="B69" s="2"/>
       <c r="E69" s="3"/>
@@ -3668,7 +3729,7 @@
       <c r="G69" s="2"/>
       <c r="H69" s="2"/>
     </row>
-    <row r="70" spans="1:8">
+    <row r="70" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A70" s="1"/>
       <c r="B70" s="2"/>
       <c r="E70" s="3"/>
@@ -3676,7 +3737,7 @@
       <c r="G70" s="2"/>
       <c r="H70" s="2"/>
     </row>
-    <row r="71" spans="1:8">
+    <row r="71" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A71" s="1"/>
       <c r="B71" s="2"/>
       <c r="E71" s="3"/>
@@ -3684,7 +3745,7 @@
       <c r="G71" s="2"/>
       <c r="H71" s="2"/>
     </row>
-    <row r="72" spans="1:8">
+    <row r="72" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A72" s="1"/>
       <c r="B72" s="2"/>
       <c r="E72" s="3"/>
@@ -3692,7 +3753,7 @@
       <c r="G72" s="2"/>
       <c r="H72" s="2"/>
     </row>
-    <row r="73" spans="1:8">
+    <row r="73" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A73" s="1"/>
       <c r="B73" s="2"/>
       <c r="E73" s="3"/>
@@ -3700,7 +3761,7 @@
       <c r="G73" s="2"/>
       <c r="H73" s="2"/>
     </row>
-    <row r="74" spans="1:8">
+    <row r="74" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A74" s="1"/>
       <c r="B74" s="2"/>
       <c r="E74" s="3"/>
@@ -3708,7 +3769,7 @@
       <c r="G74" s="2"/>
       <c r="H74" s="2"/>
     </row>
-    <row r="75" spans="1:8">
+    <row r="75" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A75" s="1"/>
       <c r="B75" s="2"/>
       <c r="E75" s="3"/>
@@ -3716,7 +3777,7 @@
       <c r="G75" s="2"/>
       <c r="H75" s="2"/>
     </row>
-    <row r="76" spans="1:8">
+    <row r="76" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A76" s="1"/>
       <c r="B76" s="2"/>
       <c r="E76" s="3"/>
@@ -3724,7 +3785,7 @@
       <c r="G76" s="2"/>
       <c r="H76" s="2"/>
     </row>
-    <row r="77" spans="1:8">
+    <row r="77" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A77" s="1"/>
       <c r="B77" s="2"/>
       <c r="E77" s="3"/>
@@ -3732,7 +3793,7 @@
       <c r="G77" s="2"/>
       <c r="H77" s="2"/>
     </row>
-    <row r="78" spans="1:8">
+    <row r="78" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A78" s="1"/>
       <c r="B78" s="2"/>
       <c r="E78" s="3"/>
@@ -3740,7 +3801,7 @@
       <c r="G78" s="2"/>
       <c r="H78" s="2"/>
     </row>
-    <row r="79" spans="1:8">
+    <row r="79" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A79" s="1"/>
       <c r="B79" s="2"/>
       <c r="E79" s="3"/>
@@ -3748,7 +3809,7 @@
       <c r="G79" s="2"/>
       <c r="H79" s="2"/>
     </row>
-    <row r="80" spans="1:8">
+    <row r="80" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A80" s="1"/>
       <c r="B80" s="2"/>
       <c r="E80" s="3"/>
@@ -3756,7 +3817,7 @@
       <c r="G80" s="2"/>
       <c r="H80" s="2"/>
     </row>
-    <row r="81" spans="1:8">
+    <row r="81" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A81" s="1"/>
       <c r="B81" s="2"/>
       <c r="E81" s="3"/>
@@ -3764,7 +3825,7 @@
       <c r="G81" s="2"/>
       <c r="H81" s="2"/>
     </row>
-    <row r="82" spans="1:8">
+    <row r="82" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A82" s="1"/>
       <c r="B82" s="2"/>
       <c r="E82" s="3"/>
@@ -3772,7 +3833,7 @@
       <c r="G82" s="2"/>
       <c r="H82" s="2"/>
     </row>
-    <row r="83" spans="1:8">
+    <row r="83" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A83" s="1"/>
       <c r="B83" s="2"/>
       <c r="E83" s="3"/>
@@ -3780,7 +3841,7 @@
       <c r="G83" s="2"/>
       <c r="H83" s="2"/>
     </row>
-    <row r="84" spans="1:8">
+    <row r="84" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A84" s="1"/>
       <c r="B84" s="2"/>
       <c r="E84" s="3"/>
@@ -3788,7 +3849,7 @@
       <c r="G84" s="2"/>
       <c r="H84" s="2"/>
     </row>
-    <row r="85" spans="1:8">
+    <row r="85" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A85" s="1"/>
       <c r="B85" s="2"/>
       <c r="E85" s="3"/>
@@ -3796,7 +3857,7 @@
       <c r="G85" s="2"/>
       <c r="H85" s="2"/>
     </row>
-    <row r="86" spans="1:8">
+    <row r="86" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A86" s="1"/>
       <c r="B86" s="2"/>
       <c r="E86" s="3"/>
@@ -3804,7 +3865,7 @@
       <c r="G86" s="2"/>
       <c r="H86" s="2"/>
     </row>
-    <row r="87" spans="1:8">
+    <row r="87" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A87" s="1"/>
       <c r="B87" s="2"/>
       <c r="E87" s="3"/>
@@ -3812,7 +3873,7 @@
       <c r="G87" s="2"/>
       <c r="H87" s="2"/>
     </row>
-    <row r="88" spans="1:8">
+    <row r="88" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A88" s="1"/>
       <c r="B88" s="2"/>
       <c r="E88" s="3"/>
@@ -3820,7 +3881,7 @@
       <c r="G88" s="2"/>
       <c r="H88" s="2"/>
     </row>
-    <row r="89" spans="1:8">
+    <row r="89" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A89" s="1"/>
       <c r="B89" s="2"/>
       <c r="E89" s="3"/>
@@ -3828,7 +3889,7 @@
       <c r="G89" s="2"/>
       <c r="H89" s="2"/>
     </row>
-    <row r="90" spans="1:8">
+    <row r="90" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A90" s="1"/>
       <c r="B90" s="2"/>
       <c r="E90" s="3"/>
@@ -3836,7 +3897,7 @@
       <c r="G90" s="2"/>
       <c r="H90" s="2"/>
     </row>
-    <row r="91" spans="1:8">
+    <row r="91" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A91" s="1"/>
       <c r="B91" s="2"/>
       <c r="E91" s="3"/>
@@ -3844,7 +3905,7 @@
       <c r="G91" s="2"/>
       <c r="H91" s="2"/>
     </row>
-    <row r="92" spans="1:8">
+    <row r="92" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A92" s="1"/>
       <c r="B92" s="2"/>
       <c r="E92" s="3"/>
@@ -3852,7 +3913,7 @@
       <c r="G92" s="2"/>
       <c r="H92" s="2"/>
     </row>
-    <row r="93" spans="1:8">
+    <row r="93" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A93" s="1"/>
       <c r="B93" s="2"/>
       <c r="E93" s="3"/>
@@ -3860,7 +3921,7 @@
       <c r="G93" s="2"/>
       <c r="H93" s="2"/>
     </row>
-    <row r="94" spans="1:8">
+    <row r="94" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A94" s="1"/>
       <c r="B94" s="2"/>
       <c r="E94" s="3"/>
@@ -3868,7 +3929,7 @@
       <c r="G94" s="2"/>
       <c r="H94" s="2"/>
     </row>
-    <row r="95" spans="1:8">
+    <row r="95" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A95" s="1"/>
       <c r="B95" s="2"/>
       <c r="E95" s="3"/>
@@ -3876,7 +3937,7 @@
       <c r="G95" s="2"/>
       <c r="H95" s="2"/>
     </row>
-    <row r="96" spans="1:8">
+    <row r="96" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A96" s="1"/>
       <c r="B96" s="2"/>
       <c r="E96" s="3"/>
@@ -3884,7 +3945,7 @@
       <c r="G96" s="2"/>
       <c r="H96" s="2"/>
     </row>
-    <row r="97" spans="1:8">
+    <row r="97" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A97" s="1"/>
       <c r="B97" s="2"/>
       <c r="E97" s="3"/>
@@ -3892,7 +3953,7 @@
       <c r="G97" s="2"/>
       <c r="H97" s="2"/>
     </row>
-    <row r="98" spans="1:8">
+    <row r="98" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A98" s="1"/>
       <c r="B98" s="2"/>
       <c r="E98" s="3"/>
@@ -3900,7 +3961,7 @@
       <c r="G98" s="2"/>
       <c r="H98" s="2"/>
     </row>
-    <row r="99" spans="1:8">
+    <row r="99" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A99" s="1"/>
       <c r="B99" s="2"/>
       <c r="E99" s="3"/>
@@ -3908,7 +3969,7 @@
       <c r="G99" s="2"/>
       <c r="H99" s="2"/>
     </row>
-    <row r="100" spans="1:8">
+    <row r="100" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A100" s="1"/>
       <c r="B100" s="2"/>
       <c r="E100" s="3"/>
@@ -3951,21 +4012,21 @@
       <selection activeCell="P21" sqref="P21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.88671875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.88671875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="19.44140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.5546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.5546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.5703125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="9" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="17.88671875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="17.85546875" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="17" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="19.109375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="19.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="15.6">
+    <row r="1" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="7" t="s">
         <v>8</v>
       </c>
@@ -3997,7 +4058,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:10">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="2"/>
       <c r="B2" s="8"/>
       <c r="D2" s="2"/>
@@ -4005,7 +4066,7 @@
       <c r="I2" s="8"/>
       <c r="J2" s="2"/>
     </row>
-    <row r="3" spans="1:10">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="2"/>
       <c r="B3" s="8"/>
       <c r="D3" s="2"/>
@@ -4013,7 +4074,7 @@
       <c r="I3" s="8"/>
       <c r="J3" s="2"/>
     </row>
-    <row r="4" spans="1:10">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="2"/>
       <c r="B4" s="8"/>
       <c r="D4" s="2"/>
@@ -4021,7 +4082,7 @@
       <c r="I4" s="8"/>
       <c r="J4" s="2"/>
     </row>
-    <row r="5" spans="1:10">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" s="2"/>
       <c r="B5" s="8"/>
       <c r="D5" s="2"/>
@@ -4029,7 +4090,7 @@
       <c r="I5" s="8"/>
       <c r="J5" s="2"/>
     </row>
-    <row r="6" spans="1:10">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" s="2"/>
       <c r="B6" s="8"/>
       <c r="D6" s="2"/>
@@ -4037,7 +4098,7 @@
       <c r="I6" s="8"/>
       <c r="J6" s="2"/>
     </row>
-    <row r="7" spans="1:10">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" s="2"/>
       <c r="B7" s="8"/>
       <c r="D7" s="2"/>
@@ -4045,7 +4106,7 @@
       <c r="I7" s="8"/>
       <c r="J7" s="2"/>
     </row>
-    <row r="8" spans="1:10">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" s="2"/>
       <c r="B8" s="8"/>
       <c r="D8" s="2"/>
@@ -4053,7 +4114,7 @@
       <c r="I8" s="8"/>
       <c r="J8" s="2"/>
     </row>
-    <row r="9" spans="1:10">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" s="2"/>
       <c r="B9" s="8"/>
       <c r="D9" s="2"/>
@@ -4061,7 +4122,7 @@
       <c r="I9" s="8"/>
       <c r="J9" s="2"/>
     </row>
-    <row r="10" spans="1:10">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" s="2"/>
       <c r="B10" s="8"/>
       <c r="D10" s="2"/>
@@ -4069,7 +4130,7 @@
       <c r="I10" s="8"/>
       <c r="J10" s="2"/>
     </row>
-    <row r="11" spans="1:10">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" s="2"/>
       <c r="B11" s="8"/>
       <c r="D11" s="2"/>
@@ -4077,7 +4138,7 @@
       <c r="I11" s="8"/>
       <c r="J11" s="2"/>
     </row>
-    <row r="12" spans="1:10">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" s="2"/>
       <c r="B12" s="8"/>
       <c r="D12" s="2"/>
@@ -4085,7 +4146,7 @@
       <c r="I12" s="8"/>
       <c r="J12" s="2"/>
     </row>
-    <row r="13" spans="1:10">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" s="2"/>
       <c r="B13" s="8"/>
       <c r="D13" s="2"/>
@@ -4093,7 +4154,7 @@
       <c r="I13" s="8"/>
       <c r="J13" s="2"/>
     </row>
-    <row r="14" spans="1:10">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" s="2"/>
       <c r="B14" s="8"/>
       <c r="D14" s="2"/>
@@ -4101,7 +4162,7 @@
       <c r="I14" s="8"/>
       <c r="J14" s="2"/>
     </row>
-    <row r="15" spans="1:10">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" s="2"/>
       <c r="B15" s="8"/>
       <c r="D15" s="2"/>
@@ -4109,7 +4170,7 @@
       <c r="I15" s="8"/>
       <c r="J15" s="2"/>
     </row>
-    <row r="16" spans="1:10">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" s="2"/>
       <c r="B16" s="8"/>
       <c r="D16" s="2"/>
@@ -4117,7 +4178,7 @@
       <c r="I16" s="8"/>
       <c r="J16" s="2"/>
     </row>
-    <row r="17" spans="1:10">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17" s="2"/>
       <c r="B17" s="8"/>
       <c r="D17" s="2"/>
@@ -4125,7 +4186,7 @@
       <c r="I17" s="8"/>
       <c r="J17" s="2"/>
     </row>
-    <row r="18" spans="1:10">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18" s="2"/>
       <c r="B18" s="8"/>
       <c r="D18" s="2"/>
@@ -4133,7 +4194,7 @@
       <c r="I18" s="8"/>
       <c r="J18" s="2"/>
     </row>
-    <row r="19" spans="1:10">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A19" s="2"/>
       <c r="B19" s="8"/>
       <c r="D19" s="2"/>
@@ -4141,7 +4202,7 @@
       <c r="I19" s="8"/>
       <c r="J19" s="2"/>
     </row>
-    <row r="20" spans="1:10">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A20" s="2"/>
       <c r="B20" s="8"/>
       <c r="D20" s="2"/>
@@ -4149,7 +4210,7 @@
       <c r="I20" s="8"/>
       <c r="J20" s="2"/>
     </row>
-    <row r="21" spans="1:10">
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A21" s="2"/>
       <c r="B21" s="8"/>
       <c r="D21" s="2"/>
@@ -4157,7 +4218,7 @@
       <c r="I21" s="8"/>
       <c r="J21" s="2"/>
     </row>
-    <row r="22" spans="1:10">
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A22" s="2"/>
       <c r="B22" s="8"/>
       <c r="D22" s="2"/>
@@ -4165,7 +4226,7 @@
       <c r="I22" s="8"/>
       <c r="J22" s="2"/>
     </row>
-    <row r="23" spans="1:10">
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A23" s="2"/>
       <c r="B23" s="8"/>
       <c r="D23" s="2"/>
@@ -4173,7 +4234,7 @@
       <c r="I23" s="8"/>
       <c r="J23" s="2"/>
     </row>
-    <row r="24" spans="1:10">
+    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A24" s="2"/>
       <c r="B24" s="8"/>
       <c r="D24" s="2"/>
@@ -4181,7 +4242,7 @@
       <c r="I24" s="8"/>
       <c r="J24" s="2"/>
     </row>
-    <row r="25" spans="1:10">
+    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A25" s="2"/>
       <c r="B25" s="8"/>
       <c r="D25" s="2"/>
@@ -4189,7 +4250,7 @@
       <c r="I25" s="8"/>
       <c r="J25" s="2"/>
     </row>
-    <row r="26" spans="1:10">
+    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A26" s="2"/>
       <c r="B26" s="8"/>
       <c r="D26" s="2"/>
@@ -4197,7 +4258,7 @@
       <c r="I26" s="8"/>
       <c r="J26" s="2"/>
     </row>
-    <row r="27" spans="1:10">
+    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A27" s="2"/>
       <c r="B27" s="8"/>
       <c r="D27" s="2"/>
@@ -4205,7 +4266,7 @@
       <c r="I27" s="8"/>
       <c r="J27" s="2"/>
     </row>
-    <row r="28" spans="1:10">
+    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A28" s="2"/>
       <c r="B28" s="8"/>
       <c r="D28" s="2"/>
@@ -4213,7 +4274,7 @@
       <c r="I28" s="8"/>
       <c r="J28" s="2"/>
     </row>
-    <row r="29" spans="1:10">
+    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A29" s="2"/>
       <c r="B29" s="8"/>
       <c r="D29" s="2"/>
@@ -4221,7 +4282,7 @@
       <c r="I29" s="8"/>
       <c r="J29" s="2"/>
     </row>
-    <row r="30" spans="1:10">
+    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A30" s="2"/>
       <c r="B30" s="8"/>
       <c r="D30" s="2"/>
@@ -4229,7 +4290,7 @@
       <c r="I30" s="8"/>
       <c r="J30" s="2"/>
     </row>
-    <row r="31" spans="1:10">
+    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A31" s="2"/>
       <c r="B31" s="8"/>
       <c r="D31" s="2"/>
@@ -4237,7 +4298,7 @@
       <c r="I31" s="8"/>
       <c r="J31" s="2"/>
     </row>
-    <row r="32" spans="1:10">
+    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A32" s="2"/>
       <c r="B32" s="8"/>
       <c r="D32" s="2"/>
@@ -4245,7 +4306,7 @@
       <c r="I32" s="8"/>
       <c r="J32" s="2"/>
     </row>
-    <row r="33" spans="1:10">
+    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A33" s="2"/>
       <c r="B33" s="8"/>
       <c r="D33" s="2"/>
@@ -4253,7 +4314,7 @@
       <c r="I33" s="8"/>
       <c r="J33" s="2"/>
     </row>
-    <row r="34" spans="1:10">
+    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A34" s="2"/>
       <c r="B34" s="8"/>
       <c r="D34" s="2"/>
@@ -4261,7 +4322,7 @@
       <c r="I34" s="8"/>
       <c r="J34" s="2"/>
     </row>
-    <row r="35" spans="1:10">
+    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A35" s="2"/>
       <c r="B35" s="8"/>
       <c r="D35" s="2"/>
@@ -4269,7 +4330,7 @@
       <c r="I35" s="8"/>
       <c r="J35" s="2"/>
     </row>
-    <row r="36" spans="1:10">
+    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A36" s="2"/>
       <c r="B36" s="8"/>
       <c r="D36" s="2"/>
@@ -4277,7 +4338,7 @@
       <c r="I36" s="8"/>
       <c r="J36" s="2"/>
     </row>
-    <row r="37" spans="1:10">
+    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A37" s="2"/>
       <c r="B37" s="8"/>
       <c r="D37" s="2"/>
@@ -4285,7 +4346,7 @@
       <c r="I37" s="8"/>
       <c r="J37" s="2"/>
     </row>
-    <row r="38" spans="1:10">
+    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A38" s="2"/>
       <c r="B38" s="8"/>
       <c r="D38" s="2"/>
@@ -4293,7 +4354,7 @@
       <c r="I38" s="8"/>
       <c r="J38" s="2"/>
     </row>
-    <row r="39" spans="1:10">
+    <row r="39" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A39" s="2"/>
       <c r="B39" s="8"/>
       <c r="D39" s="2"/>
@@ -4301,7 +4362,7 @@
       <c r="I39" s="8"/>
       <c r="J39" s="2"/>
     </row>
-    <row r="40" spans="1:10">
+    <row r="40" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A40" s="2"/>
       <c r="B40" s="8"/>
       <c r="D40" s="2"/>
@@ -4309,7 +4370,7 @@
       <c r="I40" s="8"/>
       <c r="J40" s="2"/>
     </row>
-    <row r="41" spans="1:10">
+    <row r="41" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A41" s="2"/>
       <c r="B41" s="8"/>
       <c r="D41" s="2"/>
@@ -4317,7 +4378,7 @@
       <c r="I41" s="8"/>
       <c r="J41" s="2"/>
     </row>
-    <row r="42" spans="1:10">
+    <row r="42" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A42" s="2"/>
       <c r="B42" s="8"/>
       <c r="D42" s="2"/>
@@ -4325,7 +4386,7 @@
       <c r="I42" s="8"/>
       <c r="J42" s="2"/>
     </row>
-    <row r="43" spans="1:10">
+    <row r="43" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A43" s="2"/>
       <c r="B43" s="8"/>
       <c r="D43" s="2"/>
@@ -4333,7 +4394,7 @@
       <c r="I43" s="8"/>
       <c r="J43" s="2"/>
     </row>
-    <row r="44" spans="1:10">
+    <row r="44" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A44" s="2"/>
       <c r="B44" s="8"/>
       <c r="D44" s="2"/>
@@ -4341,7 +4402,7 @@
       <c r="I44" s="8"/>
       <c r="J44" s="2"/>
     </row>
-    <row r="45" spans="1:10">
+    <row r="45" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A45" s="2"/>
       <c r="B45" s="8"/>
       <c r="D45" s="2"/>
@@ -4349,7 +4410,7 @@
       <c r="I45" s="8"/>
       <c r="J45" s="2"/>
     </row>
-    <row r="46" spans="1:10">
+    <row r="46" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A46" s="2"/>
       <c r="B46" s="8"/>
       <c r="D46" s="2"/>
@@ -4357,7 +4418,7 @@
       <c r="I46" s="8"/>
       <c r="J46" s="2"/>
     </row>
-    <row r="47" spans="1:10">
+    <row r="47" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A47" s="2"/>
       <c r="B47" s="8"/>
       <c r="D47" s="2"/>
@@ -4365,7 +4426,7 @@
       <c r="I47" s="8"/>
       <c r="J47" s="2"/>
     </row>
-    <row r="48" spans="1:10">
+    <row r="48" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A48" s="2"/>
       <c r="B48" s="8"/>
       <c r="D48" s="2"/>
@@ -4373,7 +4434,7 @@
       <c r="I48" s="8"/>
       <c r="J48" s="2"/>
     </row>
-    <row r="49" spans="1:10">
+    <row r="49" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A49" s="2"/>
       <c r="B49" s="8"/>
       <c r="D49" s="2"/>
@@ -4381,7 +4442,7 @@
       <c r="I49" s="8"/>
       <c r="J49" s="2"/>
     </row>
-    <row r="50" spans="1:10">
+    <row r="50" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A50" s="2"/>
       <c r="B50" s="8"/>
       <c r="D50" s="2"/>
@@ -4389,7 +4450,7 @@
       <c r="I50" s="8"/>
       <c r="J50" s="2"/>
     </row>
-    <row r="51" spans="1:10">
+    <row r="51" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A51" s="2"/>
       <c r="B51" s="8"/>
       <c r="D51" s="2"/>
@@ -4397,7 +4458,7 @@
       <c r="I51" s="8"/>
       <c r="J51" s="2"/>
     </row>
-    <row r="52" spans="1:10">
+    <row r="52" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A52" s="2"/>
       <c r="B52" s="8"/>
       <c r="D52" s="2"/>
@@ -4405,7 +4466,7 @@
       <c r="I52" s="8"/>
       <c r="J52" s="2"/>
     </row>
-    <row r="53" spans="1:10">
+    <row r="53" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A53" s="2"/>
       <c r="B53" s="8"/>
       <c r="D53" s="2"/>
@@ -4413,7 +4474,7 @@
       <c r="I53" s="8"/>
       <c r="J53" s="2"/>
     </row>
-    <row r="54" spans="1:10">
+    <row r="54" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A54" s="2"/>
       <c r="B54" s="8"/>
       <c r="D54" s="2"/>
@@ -4421,7 +4482,7 @@
       <c r="I54" s="8"/>
       <c r="J54" s="2"/>
     </row>
-    <row r="55" spans="1:10">
+    <row r="55" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A55" s="2"/>
       <c r="B55" s="8"/>
       <c r="D55" s="2"/>
@@ -4429,7 +4490,7 @@
       <c r="I55" s="8"/>
       <c r="J55" s="2"/>
     </row>
-    <row r="56" spans="1:10">
+    <row r="56" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A56" s="2"/>
       <c r="B56" s="8"/>
       <c r="D56" s="2"/>
@@ -4437,7 +4498,7 @@
       <c r="I56" s="8"/>
       <c r="J56" s="2"/>
     </row>
-    <row r="57" spans="1:10">
+    <row r="57" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A57" s="2"/>
       <c r="B57" s="8"/>
       <c r="D57" s="2"/>
@@ -4445,7 +4506,7 @@
       <c r="I57" s="8"/>
       <c r="J57" s="2"/>
     </row>
-    <row r="58" spans="1:10">
+    <row r="58" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A58" s="2"/>
       <c r="B58" s="8"/>
       <c r="D58" s="2"/>
@@ -4453,7 +4514,7 @@
       <c r="I58" s="8"/>
       <c r="J58" s="2"/>
     </row>
-    <row r="59" spans="1:10">
+    <row r="59" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A59" s="2"/>
       <c r="B59" s="8"/>
       <c r="D59" s="2"/>
@@ -4461,7 +4522,7 @@
       <c r="I59" s="8"/>
       <c r="J59" s="2"/>
     </row>
-    <row r="60" spans="1:10">
+    <row r="60" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A60" s="2"/>
       <c r="B60" s="8"/>
       <c r="D60" s="2"/>
@@ -4469,7 +4530,7 @@
       <c r="I60" s="8"/>
       <c r="J60" s="2"/>
     </row>
-    <row r="61" spans="1:10">
+    <row r="61" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A61" s="2"/>
       <c r="B61" s="8"/>
       <c r="D61" s="2"/>
@@ -4477,7 +4538,7 @@
       <c r="I61" s="8"/>
       <c r="J61" s="2"/>
     </row>
-    <row r="62" spans="1:10">
+    <row r="62" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A62" s="2"/>
       <c r="B62" s="8"/>
       <c r="D62" s="2"/>
@@ -4485,7 +4546,7 @@
       <c r="I62" s="8"/>
       <c r="J62" s="2"/>
     </row>
-    <row r="63" spans="1:10">
+    <row r="63" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A63" s="2"/>
       <c r="B63" s="8"/>
       <c r="D63" s="2"/>
@@ -4493,7 +4554,7 @@
       <c r="I63" s="8"/>
       <c r="J63" s="2"/>
     </row>
-    <row r="64" spans="1:10">
+    <row r="64" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A64" s="2"/>
       <c r="B64" s="8"/>
       <c r="D64" s="2"/>
@@ -4501,7 +4562,7 @@
       <c r="I64" s="8"/>
       <c r="J64" s="2"/>
     </row>
-    <row r="65" spans="1:10">
+    <row r="65" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A65" s="2"/>
       <c r="B65" s="8"/>
       <c r="D65" s="2"/>
@@ -4509,7 +4570,7 @@
       <c r="I65" s="8"/>
       <c r="J65" s="2"/>
     </row>
-    <row r="66" spans="1:10">
+    <row r="66" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A66" s="2"/>
       <c r="B66" s="8"/>
       <c r="D66" s="2"/>
@@ -4517,7 +4578,7 @@
       <c r="I66" s="8"/>
       <c r="J66" s="2"/>
     </row>
-    <row r="67" spans="1:10">
+    <row r="67" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A67" s="2"/>
       <c r="B67" s="8"/>
       <c r="D67" s="2"/>
@@ -4525,7 +4586,7 @@
       <c r="I67" s="8"/>
       <c r="J67" s="2"/>
     </row>
-    <row r="68" spans="1:10">
+    <row r="68" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A68" s="2"/>
       <c r="B68" s="8"/>
       <c r="D68" s="2"/>
@@ -4533,7 +4594,7 @@
       <c r="I68" s="8"/>
       <c r="J68" s="2"/>
     </row>
-    <row r="69" spans="1:10">
+    <row r="69" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A69" s="2"/>
       <c r="B69" s="8"/>
       <c r="D69" s="2"/>
@@ -4541,7 +4602,7 @@
       <c r="I69" s="8"/>
       <c r="J69" s="2"/>
     </row>
-    <row r="70" spans="1:10">
+    <row r="70" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A70" s="2"/>
       <c r="B70" s="8"/>
       <c r="D70" s="2"/>
@@ -4549,7 +4610,7 @@
       <c r="I70" s="8"/>
       <c r="J70" s="2"/>
     </row>
-    <row r="71" spans="1:10">
+    <row r="71" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A71" s="2"/>
       <c r="B71" s="8"/>
       <c r="D71" s="2"/>
@@ -4557,7 +4618,7 @@
       <c r="I71" s="8"/>
       <c r="J71" s="2"/>
     </row>
-    <row r="72" spans="1:10">
+    <row r="72" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A72" s="2"/>
       <c r="B72" s="8"/>
       <c r="D72" s="2"/>
@@ -4565,7 +4626,7 @@
       <c r="I72" s="8"/>
       <c r="J72" s="2"/>
     </row>
-    <row r="73" spans="1:10">
+    <row r="73" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A73" s="2"/>
       <c r="B73" s="8"/>
       <c r="D73" s="2"/>
@@ -4573,7 +4634,7 @@
       <c r="I73" s="8"/>
       <c r="J73" s="2"/>
     </row>
-    <row r="74" spans="1:10">
+    <row r="74" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A74" s="2"/>
       <c r="B74" s="8"/>
       <c r="D74" s="2"/>
@@ -4581,7 +4642,7 @@
       <c r="I74" s="8"/>
       <c r="J74" s="2"/>
     </row>
-    <row r="75" spans="1:10">
+    <row r="75" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A75" s="2"/>
       <c r="B75" s="8"/>
       <c r="D75" s="2"/>
@@ -4589,7 +4650,7 @@
       <c r="I75" s="8"/>
       <c r="J75" s="2"/>
     </row>
-    <row r="76" spans="1:10">
+    <row r="76" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A76" s="2"/>
       <c r="B76" s="8"/>
       <c r="D76" s="2"/>
@@ -4597,7 +4658,7 @@
       <c r="I76" s="8"/>
       <c r="J76" s="2"/>
     </row>
-    <row r="77" spans="1:10">
+    <row r="77" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A77" s="2"/>
       <c r="B77" s="8"/>
       <c r="D77" s="2"/>
@@ -4605,7 +4666,7 @@
       <c r="I77" s="8"/>
       <c r="J77" s="2"/>
     </row>
-    <row r="78" spans="1:10">
+    <row r="78" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A78" s="2"/>
       <c r="B78" s="8"/>
       <c r="D78" s="2"/>
@@ -4613,7 +4674,7 @@
       <c r="I78" s="8"/>
       <c r="J78" s="2"/>
     </row>
-    <row r="79" spans="1:10">
+    <row r="79" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A79" s="2"/>
       <c r="B79" s="8"/>
       <c r="D79" s="2"/>
@@ -4621,7 +4682,7 @@
       <c r="I79" s="8"/>
       <c r="J79" s="2"/>
     </row>
-    <row r="80" spans="1:10">
+    <row r="80" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A80" s="2"/>
       <c r="B80" s="8"/>
       <c r="D80" s="2"/>
@@ -4629,7 +4690,7 @@
       <c r="I80" s="8"/>
       <c r="J80" s="2"/>
     </row>
-    <row r="81" spans="1:10">
+    <row r="81" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A81" s="2"/>
       <c r="B81" s="8"/>
       <c r="D81" s="2"/>
@@ -4637,7 +4698,7 @@
       <c r="I81" s="8"/>
       <c r="J81" s="2"/>
     </row>
-    <row r="82" spans="1:10">
+    <row r="82" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A82" s="2"/>
       <c r="B82" s="8"/>
       <c r="D82" s="2"/>
@@ -4645,7 +4706,7 @@
       <c r="I82" s="8"/>
       <c r="J82" s="2"/>
     </row>
-    <row r="83" spans="1:10">
+    <row r="83" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A83" s="2"/>
       <c r="B83" s="8"/>
       <c r="D83" s="2"/>
@@ -4653,7 +4714,7 @@
       <c r="I83" s="8"/>
       <c r="J83" s="2"/>
     </row>
-    <row r="84" spans="1:10">
+    <row r="84" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A84" s="2"/>
       <c r="B84" s="8"/>
       <c r="D84" s="2"/>
@@ -4661,7 +4722,7 @@
       <c r="I84" s="8"/>
       <c r="J84" s="2"/>
     </row>
-    <row r="85" spans="1:10">
+    <row r="85" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A85" s="2"/>
       <c r="B85" s="8"/>
       <c r="D85" s="2"/>
@@ -4669,7 +4730,7 @@
       <c r="I85" s="8"/>
       <c r="J85" s="2"/>
     </row>
-    <row r="86" spans="1:10">
+    <row r="86" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A86" s="2"/>
       <c r="B86" s="8"/>
       <c r="D86" s="2"/>
@@ -4677,7 +4738,7 @@
       <c r="I86" s="8"/>
       <c r="J86" s="2"/>
     </row>
-    <row r="87" spans="1:10">
+    <row r="87" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A87" s="2"/>
       <c r="B87" s="8"/>
       <c r="D87" s="2"/>
@@ -4685,7 +4746,7 @@
       <c r="I87" s="8"/>
       <c r="J87" s="2"/>
     </row>
-    <row r="88" spans="1:10">
+    <row r="88" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A88" s="2"/>
       <c r="B88" s="8"/>
       <c r="D88" s="2"/>
@@ -4693,7 +4754,7 @@
       <c r="I88" s="8"/>
       <c r="J88" s="2"/>
     </row>
-    <row r="89" spans="1:10">
+    <row r="89" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A89" s="2"/>
       <c r="B89" s="8"/>
       <c r="D89" s="2"/>
@@ -4701,7 +4762,7 @@
       <c r="I89" s="8"/>
       <c r="J89" s="2"/>
     </row>
-    <row r="90" spans="1:10">
+    <row r="90" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A90" s="2"/>
       <c r="B90" s="8"/>
       <c r="D90" s="2"/>
@@ -4709,7 +4770,7 @@
       <c r="I90" s="8"/>
       <c r="J90" s="2"/>
     </row>
-    <row r="91" spans="1:10">
+    <row r="91" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A91" s="2"/>
       <c r="B91" s="8"/>
       <c r="D91" s="2"/>
@@ -4717,7 +4778,7 @@
       <c r="I91" s="8"/>
       <c r="J91" s="2"/>
     </row>
-    <row r="92" spans="1:10">
+    <row r="92" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A92" s="2"/>
       <c r="B92" s="8"/>
       <c r="D92" s="2"/>
@@ -4725,7 +4786,7 @@
       <c r="I92" s="8"/>
       <c r="J92" s="2"/>
     </row>
-    <row r="93" spans="1:10">
+    <row r="93" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A93" s="2"/>
       <c r="B93" s="8"/>
       <c r="D93" s="2"/>
@@ -4733,7 +4794,7 @@
       <c r="I93" s="8"/>
       <c r="J93" s="2"/>
     </row>
-    <row r="94" spans="1:10">
+    <row r="94" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A94" s="2"/>
       <c r="B94" s="8"/>
       <c r="D94" s="2"/>
@@ -4741,7 +4802,7 @@
       <c r="I94" s="8"/>
       <c r="J94" s="2"/>
     </row>
-    <row r="95" spans="1:10">
+    <row r="95" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A95" s="2"/>
       <c r="B95" s="8"/>
       <c r="D95" s="2"/>
@@ -4749,7 +4810,7 @@
       <c r="I95" s="8"/>
       <c r="J95" s="2"/>
     </row>
-    <row r="96" spans="1:10">
+    <row r="96" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A96" s="2"/>
       <c r="B96" s="8"/>
       <c r="D96" s="2"/>
@@ -4757,7 +4818,7 @@
       <c r="I96" s="8"/>
       <c r="J96" s="2"/>
     </row>
-    <row r="97" spans="1:10">
+    <row r="97" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A97" s="2"/>
       <c r="B97" s="8"/>
       <c r="D97" s="2"/>
@@ -4765,7 +4826,7 @@
       <c r="I97" s="8"/>
       <c r="J97" s="2"/>
     </row>
-    <row r="98" spans="1:10">
+    <row r="98" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A98" s="2"/>
       <c r="B98" s="8"/>
       <c r="D98" s="2"/>
@@ -4773,7 +4834,7 @@
       <c r="I98" s="8"/>
       <c r="J98" s="2"/>
     </row>
-    <row r="99" spans="1:10">
+    <row r="99" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A99" s="2"/>
       <c r="B99" s="8"/>
       <c r="D99" s="2"/>
@@ -4781,7 +4842,7 @@
       <c r="I99" s="8"/>
       <c r="J99" s="2"/>
     </row>
-    <row r="100" spans="1:10">
+    <row r="100" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A100" s="2"/>
       <c r="B100" s="8"/>
       <c r="D100" s="2"/>

</xml_diff>

<commit_message>
Successfully initialized and debugged the Flask backend for the Course Enrollment and Fees Microservice, resolving routing, template loading, and SQLAlchemy relationship ambiguities to enable core page viewing and API functionality
</commit_message>
<xml_diff>
--- a/PR&IR.xlsx
+++ b/PR&IR.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\avichal avneel nath\Documents\Semester 7\CS415\A3\CS415_A3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{265B2D53-2233-42DA-BDE7-A3000AC9A528}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E40B6A96-FAF6-4C15-B5A0-E2C969B71FD7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{BFA1E21A-08FA-4F02-8C25-33C81C8EE970}"/>
   </bookViews>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="149" uniqueCount="87">
   <si>
     <t>Date</t>
   </si>
@@ -295,6 +295,37 @@
   </si>
   <si>
     <t>Port configuration</t>
+  </si>
+  <si>
+    <t>Initiated my microservice</t>
+  </si>
+  <si>
+    <t>Sick, too much workloads in other units</t>
+  </si>
+  <si>
+    <t>Backend Setup:
+Flask application factory pattern implemented in run_es.py.
+Database initialization (db.py) configured for SQLite.
+Flask-SQLAlchemy models (model.py) defined for all key entities from the ER diagram (Program, SubProgram, Semester, Course, CourseAvailability, Student, StudentLevel, Hold, Enrollment, CourseFee, StudentCourseFee).</t>
+  </si>
+  <si>
+    <t>Routing and API Development:</t>
+  </si>
+  <si>
+    <t>Routing and API Development:
+Single Flask Blueprint (enrollment_bp) established for all service routes.
+HTML rendering routes (/dashboard, /enroll, /display_courses, /fees, /download_invoice_pdf) implemented.
+Comprehensive JSON API endpoints (GET, POST, PUT, DELETE) created for all major entities.
+Correct url_for usage (enrollment.endpoint_name) enforced across routes.py and HTML templates.
+Error Resolution &amp; Stability:
+jinja2.exceptions.TemplateNotFound error resolved by correct template_folder configuration and template placement.
+sqlalchemy.exc.AmbiguousForeignKeysError addressed in model.py by explicitly defining foreign_keys in Program and SubProgram relationships.
+Importance of deleting enrollment.db for schema updates highlighted and executed.
+Application now successfully runs and serves the dashboard and other HTML page</t>
+  </si>
+  <si>
+    <t>Database seeding (populating with initial data).
+Replacing mock data in frontend routes with actual database queries.</t>
   </si>
 </sst>
 </file>
@@ -346,7 +377,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -361,6 +392,10 @@
     </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="2" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1041,8 +1076,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{37EAA098-74C6-4411-B7E2-26AD2DCBC3F0}">
   <dimension ref="A1:H28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="F16" sqref="F16"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="H14" sqref="H14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1331,13 +1366,45 @@
         <v>78</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="E13"/>
-      <c r="F13"/>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="E14"/>
-      <c r="F14"/>
+    <row r="13" spans="1:8" ht="68.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="1">
+        <v>45797</v>
+      </c>
+      <c r="C13" s="9" t="s">
+        <v>83</v>
+      </c>
+      <c r="D13" t="s">
+        <v>37</v>
+      </c>
+      <c r="E13">
+        <v>80</v>
+      </c>
+      <c r="F13">
+        <v>2</v>
+      </c>
+      <c r="G13" s="12" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" ht="60" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="1">
+        <v>45798</v>
+      </c>
+      <c r="C14" s="9" t="s">
+        <v>85</v>
+      </c>
+      <c r="D14" t="s">
+        <v>17</v>
+      </c>
+      <c r="E14">
+        <v>100</v>
+      </c>
+      <c r="F14">
+        <v>4</v>
+      </c>
+      <c r="G14" s="13" t="s">
+        <v>86</v>
+      </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="E15"/>
@@ -1403,7 +1470,7 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
   <ignoredErrors>
-    <ignoredError sqref="D13:D16" listDataValidation="1"/>
+    <ignoredError sqref="D15:D16" listDataValidation="1"/>
   </ignoredErrors>
   <tableParts count="1">
     <tablePart r:id="rId2"/>
@@ -1415,13 +1482,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3BDA6702-5DDF-42FB-988E-13FBEB26F5C9}">
   <dimension ref="A1:H100"/>
   <sheetViews>
-    <sheetView topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H7" sqref="H7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.28515625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="17.28515625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="55.5703125" customWidth="1"/>
     <col min="4" max="4" width="10.5703125" customWidth="1"/>
@@ -1584,10 +1651,28 @@
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A7" s="8"/>
-      <c r="B7" s="2"/>
+      <c r="A7" s="8">
+        <v>45795</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="C7" t="s">
+        <v>81</v>
+      </c>
+      <c r="D7" t="s">
+        <v>17</v>
+      </c>
+      <c r="E7">
+        <v>100</v>
+      </c>
+      <c r="F7">
+        <v>5</v>
+      </c>
       <c r="G7" s="2"/>
-      <c r="H7" s="2"/>
+      <c r="H7" s="2" t="s">
+        <v>82</v>
+      </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="8"/>
@@ -2166,7 +2251,7 @@
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <ignoredErrors>
-    <ignoredError sqref="D7:D100" listDataValidation="1"/>
+    <ignoredError sqref="D8:D100" listDataValidation="1"/>
   </ignoredErrors>
   <tableParts count="1">
     <tablePart r:id="rId1"/>

</xml_diff>

<commit_message>
Updated progress report for May 21 for Yash
</commit_message>
<xml_diff>
--- a/PR&IR.xlsx
+++ b/PR&IR.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\avichal avneel nath\Documents\Semester 7\CS415\A3\CS415_A3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E40B6A96-FAF6-4C15-B5A0-E2C969B71FD7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A802E3D7-B080-462F-A4F1-67E43BEBAA16}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{BFA1E21A-08FA-4F02-8C25-33C81C8EE970}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="2" xr2:uid="{BFA1E21A-08FA-4F02-8C25-33C81C8EE970}"/>
   </bookViews>
   <sheets>
     <sheet name="Avichal" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="149" uniqueCount="87">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="153" uniqueCount="90">
   <si>
     <t>Date</t>
   </si>
@@ -326,6 +326,17 @@
   <si>
     <t>Database seeding (populating with initial data).
 Replacing mock data in frontend routes with actual database queries.</t>
+  </si>
+  <si>
+    <t>Added grade recheck pages.
+Added students page that displays their enrollment with add and change grade and search functionalities.
+Added grade change and add new grade pages.</t>
+  </si>
+  <si>
+    <t>Continue docker and doing backend</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Not interested </t>
   </si>
 </sst>
 </file>
@@ -377,7 +388,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -392,7 +403,6 @@
     </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="2" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -1076,7 +1086,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{37EAA098-74C6-4411-B7E2-26AD2DCBC3F0}">
   <dimension ref="A1:H28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+    <sheetView topLeftCell="A7" workbookViewId="0">
       <selection activeCell="H14" sqref="H14"/>
     </sheetView>
   </sheetViews>
@@ -1382,7 +1392,7 @@
       <c r="F13">
         <v>2</v>
       </c>
-      <c r="G13" s="12" t="s">
+      <c r="G13" t="s">
         <v>84</v>
       </c>
     </row>
@@ -1402,7 +1412,7 @@
       <c r="F14">
         <v>4</v>
       </c>
-      <c r="G14" s="13" t="s">
+      <c r="G14" s="12" t="s">
         <v>86</v>
       </c>
     </row>
@@ -2263,13 +2273,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9FD6A201-8E63-4A9E-A683-19506CB489E3}">
   <dimension ref="A1:H100"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.42578125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="17.28515625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="27.85546875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="9.7109375" bestFit="1" customWidth="1"/>
@@ -2461,12 +2471,29 @@
         <v>54</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A8" s="1"/>
+    <row r="8" spans="1:8" ht="105" x14ac:dyDescent="0.25">
+      <c r="A8" s="1">
+        <v>45798</v>
+      </c>
       <c r="B8" s="2"/>
-      <c r="E8" s="3"/>
-      <c r="G8" s="2"/>
-      <c r="H8" s="2"/>
+      <c r="C8" s="9" t="s">
+        <v>87</v>
+      </c>
+      <c r="D8" t="s">
+        <v>17</v>
+      </c>
+      <c r="E8" s="3">
+        <v>1</v>
+      </c>
+      <c r="F8" s="10">
+        <v>4</v>
+      </c>
+      <c r="G8" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="H8" s="2" t="s">
+        <v>89</v>
+      </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="1"/>
@@ -3131,7 +3158,7 @@
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <ignoredErrors>
-    <ignoredError sqref="D8:D100" listDataValidation="1"/>
+    <ignoredError sqref="D9:D100" listDataValidation="1"/>
   </ignoredErrors>
   <tableParts count="1">
     <tablePart r:id="rId1"/>

</xml_diff>

<commit_message>
Add/update progress report for 21/05/2025 Wed by Shivya
</commit_message>
<xml_diff>
--- a/PR&IR.xlsx
+++ b/PR&IR.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28623"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26026"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\avichal avneel nath\Documents\Semester 7\CS415\A3\CS415_A3\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SHIVYA KUMAR\Desktop\new415\CS415_A3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A802E3D7-B080-462F-A4F1-67E43BEBAA16}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A5A0D8D-6F80-4613-809E-3598F48933D6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="2" xr2:uid="{BFA1E21A-08FA-4F02-8C25-33C81C8EE970}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{BFA1E21A-08FA-4F02-8C25-33C81C8EE970}"/>
   </bookViews>
   <sheets>
     <sheet name="Avichal" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="153" uniqueCount="90">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="91">
   <si>
     <t>Date</t>
   </si>
@@ -338,6 +338,9 @@
   <si>
     <t xml:space="preserve">Not interested </t>
   </si>
+  <si>
+    <t>interated jayshils feild code for student profile with mine. Added photo icon in the student profile page. Pulled jayshils code.</t>
+  </si>
 </sst>
 </file>
 
@@ -347,7 +350,7 @@
     <numFmt numFmtId="164" formatCode="h"/>
     <numFmt numFmtId="165" formatCode="d/mm/yyyy;@"/>
   </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="3">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1090,26 +1093,26 @@
       <selection activeCell="H14" sqref="H14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="10.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.5703125" style="2" customWidth="1"/>
+    <col min="1" max="1" width="10.44140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.5546875" style="2" customWidth="1"/>
     <col min="3" max="3" width="58" customWidth="1"/>
-    <col min="5" max="5" width="13.140625" style="3" customWidth="1"/>
-    <col min="6" max="6" width="20.85546875" style="4" customWidth="1"/>
-    <col min="7" max="7" width="34.85546875" style="2" customWidth="1"/>
-    <col min="8" max="8" width="43.42578125" style="2" customWidth="1"/>
-    <col min="11" max="11" width="9.140625" customWidth="1"/>
-    <col min="12" max="12" width="13.28515625" customWidth="1"/>
-    <col min="13" max="13" width="11.42578125" customWidth="1"/>
-    <col min="14" max="14" width="17.42578125" customWidth="1"/>
-    <col min="16" max="16" width="9.140625" customWidth="1"/>
-    <col min="18" max="18" width="16.5703125" customWidth="1"/>
-    <col min="19" max="19" width="14.7109375" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="16.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.109375" style="3" customWidth="1"/>
+    <col min="6" max="6" width="20.88671875" style="4" customWidth="1"/>
+    <col min="7" max="7" width="34.88671875" style="2" customWidth="1"/>
+    <col min="8" max="8" width="43.44140625" style="2" customWidth="1"/>
+    <col min="11" max="11" width="9.109375" customWidth="1"/>
+    <col min="12" max="12" width="13.33203125" customWidth="1"/>
+    <col min="13" max="13" width="11.44140625" customWidth="1"/>
+    <col min="14" max="14" width="17.44140625" customWidth="1"/>
+    <col min="16" max="16" width="9.109375" customWidth="1"/>
+    <col min="18" max="18" width="16.5546875" customWidth="1"/>
+    <col min="19" max="19" width="14.6640625" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="16.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" ht="15.6">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
@@ -1135,7 +1138,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="15.75" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:8">
       <c r="A2" s="1">
         <v>45786</v>
       </c>
@@ -1161,7 +1164,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="3" spans="1:8" ht="120" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" ht="115.2">
       <c r="A3" s="1">
         <v>45787</v>
       </c>
@@ -1184,7 +1187,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8">
       <c r="A4" s="1">
         <v>45788</v>
       </c>
@@ -1204,7 +1207,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="5" spans="1:8" ht="76.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" ht="76.5" customHeight="1">
       <c r="A5" s="1">
         <v>45789</v>
       </c>
@@ -1227,7 +1230,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8">
       <c r="A6" s="1">
         <v>45790</v>
       </c>
@@ -1250,7 +1253,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8">
       <c r="A7" s="1">
         <v>45791</v>
       </c>
@@ -1273,7 +1276,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8">
       <c r="A8" s="1">
         <v>45792</v>
       </c>
@@ -1296,7 +1299,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8">
       <c r="A9" s="1">
         <v>45793</v>
       </c>
@@ -1316,7 +1319,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8">
       <c r="A10" s="1">
         <v>45794</v>
       </c>
@@ -1336,7 +1339,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8">
       <c r="A11" s="1">
         <v>45795</v>
       </c>
@@ -1356,7 +1359,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8">
       <c r="A12" s="1">
         <v>45796</v>
       </c>
@@ -1376,7 +1379,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="13" spans="1:8" ht="68.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8" ht="68.25" customHeight="1">
       <c r="A13" s="1">
         <v>45797</v>
       </c>
@@ -1396,7 +1399,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="14" spans="1:8" ht="60" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8" ht="60" customHeight="1">
       <c r="A14" s="1">
         <v>45798</v>
       </c>
@@ -1416,48 +1419,48 @@
         <v>86</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8">
       <c r="E15"/>
       <c r="F15"/>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8">
       <c r="E16"/>
       <c r="F16"/>
     </row>
-    <row r="17" spans="6:6" x14ac:dyDescent="0.25">
+    <row r="17" spans="6:6">
       <c r="F17"/>
     </row>
-    <row r="18" spans="6:6" x14ac:dyDescent="0.25">
+    <row r="18" spans="6:6">
       <c r="F18"/>
     </row>
-    <row r="19" spans="6:6" x14ac:dyDescent="0.25">
+    <row r="19" spans="6:6">
       <c r="F19"/>
     </row>
-    <row r="20" spans="6:6" x14ac:dyDescent="0.25">
+    <row r="20" spans="6:6">
       <c r="F20"/>
     </row>
-    <row r="21" spans="6:6" x14ac:dyDescent="0.25">
+    <row r="21" spans="6:6">
       <c r="F21"/>
     </row>
-    <row r="22" spans="6:6" x14ac:dyDescent="0.25">
+    <row r="22" spans="6:6">
       <c r="F22"/>
     </row>
-    <row r="23" spans="6:6" x14ac:dyDescent="0.25">
+    <row r="23" spans="6:6">
       <c r="F23"/>
     </row>
-    <row r="24" spans="6:6" x14ac:dyDescent="0.25">
+    <row r="24" spans="6:6">
       <c r="F24"/>
     </row>
-    <row r="25" spans="6:6" x14ac:dyDescent="0.25">
+    <row r="25" spans="6:6">
       <c r="F25"/>
     </row>
-    <row r="26" spans="6:6" x14ac:dyDescent="0.25">
+    <row r="26" spans="6:6">
       <c r="F26"/>
     </row>
-    <row r="27" spans="6:6" x14ac:dyDescent="0.25">
+    <row r="27" spans="6:6">
       <c r="F27"/>
     </row>
-    <row r="28" spans="6:6" x14ac:dyDescent="0.25">
+    <row r="28" spans="6:6">
       <c r="F28"/>
     </row>
   </sheetData>
@@ -1492,23 +1495,23 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3BDA6702-5DDF-42FB-988E-13FBEB26F5C9}">
   <dimension ref="A1:H100"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H7" sqref="H7"/>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="10.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="17.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="55.5703125" customWidth="1"/>
-    <col min="4" max="4" width="10.5703125" customWidth="1"/>
-    <col min="5" max="5" width="14.85546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14.28515625" customWidth="1"/>
-    <col min="7" max="7" width="92.85546875" customWidth="1"/>
-    <col min="8" max="8" width="82.42578125" customWidth="1"/>
+    <col min="1" max="1" width="10.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="93.109375" customWidth="1"/>
+    <col min="4" max="4" width="10.5546875" customWidth="1"/>
+    <col min="5" max="5" width="14.88671875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.33203125" customWidth="1"/>
+    <col min="7" max="7" width="92.88671875" customWidth="1"/>
+    <col min="8" max="8" width="82.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" ht="15.6">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
@@ -1534,7 +1537,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8">
       <c r="A2" s="8">
         <v>45786</v>
       </c>
@@ -1560,7 +1563,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8">
       <c r="A3" s="8">
         <v>45787</v>
       </c>
@@ -1586,7 +1589,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8">
       <c r="A4" s="8">
         <v>45789</v>
       </c>
@@ -1610,7 +1613,7 @@
       </c>
       <c r="H4" s="2"/>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8">
       <c r="A5" s="8">
         <v>45790</v>
       </c>
@@ -1634,7 +1637,7 @@
       </c>
       <c r="H5" s="2"/>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8">
       <c r="A6" s="8">
         <v>45791</v>
       </c>
@@ -1660,7 +1663,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8">
       <c r="A7" s="8">
         <v>45795</v>
       </c>
@@ -1684,559 +1687,575 @@
         <v>82</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A8" s="8"/>
-      <c r="B8" s="2"/>
+    <row r="8" spans="1:8">
+      <c r="A8" s="8">
+        <v>45798</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="C8" t="s">
+        <v>90</v>
+      </c>
+      <c r="D8" t="s">
+        <v>17</v>
+      </c>
+      <c r="E8">
+        <v>100</v>
+      </c>
+      <c r="F8">
+        <v>8</v>
+      </c>
       <c r="G8" s="2"/>
       <c r="H8" s="2"/>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8">
       <c r="A9" s="8"/>
       <c r="B9" s="2"/>
       <c r="G9" s="2"/>
       <c r="H9" s="2"/>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8">
       <c r="A10" s="8"/>
       <c r="B10" s="2"/>
       <c r="G10" s="2"/>
       <c r="H10" s="2"/>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8">
       <c r="A11" s="8"/>
       <c r="B11" s="2"/>
       <c r="G11" s="2"/>
       <c r="H11" s="2"/>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8">
       <c r="A12" s="8"/>
       <c r="B12" s="2"/>
       <c r="G12" s="2"/>
       <c r="H12" s="2"/>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8">
       <c r="A13" s="8"/>
       <c r="B13" s="2"/>
       <c r="G13" s="2"/>
       <c r="H13" s="2"/>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8">
       <c r="A14" s="8"/>
       <c r="B14" s="2"/>
       <c r="G14" s="2"/>
       <c r="H14" s="2"/>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8">
       <c r="A15" s="8"/>
       <c r="B15" s="2"/>
       <c r="G15" s="2"/>
       <c r="H15" s="2"/>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8">
       <c r="A16" s="8"/>
       <c r="B16" s="2"/>
       <c r="G16" s="2"/>
       <c r="H16" s="2"/>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:8">
       <c r="A17" s="8"/>
       <c r="B17" s="2"/>
       <c r="G17" s="2"/>
       <c r="H17" s="2"/>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:8">
       <c r="A18" s="8"/>
       <c r="B18" s="2"/>
       <c r="G18" s="2"/>
       <c r="H18" s="2"/>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:8">
       <c r="A19" s="8"/>
       <c r="B19" s="2"/>
       <c r="G19" s="2"/>
       <c r="H19" s="2"/>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:8">
       <c r="A20" s="8"/>
       <c r="B20" s="2"/>
       <c r="G20" s="2"/>
       <c r="H20" s="2"/>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:8">
       <c r="A21" s="8"/>
       <c r="B21" s="2"/>
       <c r="G21" s="2"/>
       <c r="H21" s="2"/>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:8">
       <c r="A22" s="8"/>
       <c r="B22" s="2"/>
       <c r="G22" s="2"/>
       <c r="H22" s="2"/>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:8">
       <c r="A23" s="8"/>
       <c r="B23" s="2"/>
       <c r="G23" s="2"/>
       <c r="H23" s="2"/>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:8">
       <c r="A24" s="8"/>
       <c r="B24" s="2"/>
       <c r="G24" s="2"/>
       <c r="H24" s="2"/>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:8">
       <c r="A25" s="8"/>
       <c r="B25" s="2"/>
       <c r="G25" s="2"/>
       <c r="H25" s="2"/>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:8">
       <c r="A26" s="8"/>
       <c r="B26" s="2"/>
       <c r="G26" s="2"/>
       <c r="H26" s="2"/>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:8">
       <c r="A27" s="8"/>
       <c r="B27" s="2"/>
       <c r="G27" s="2"/>
       <c r="H27" s="2"/>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:8">
       <c r="A28" s="8"/>
       <c r="B28" s="2"/>
       <c r="G28" s="2"/>
       <c r="H28" s="2"/>
     </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:8">
       <c r="A29" s="8"/>
       <c r="B29" s="2"/>
       <c r="G29" s="2"/>
       <c r="H29" s="2"/>
     </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:8">
       <c r="A30" s="8"/>
       <c r="B30" s="2"/>
       <c r="G30" s="2"/>
       <c r="H30" s="2"/>
     </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:8">
       <c r="A31" s="8"/>
       <c r="B31" s="2"/>
       <c r="G31" s="2"/>
       <c r="H31" s="2"/>
     </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:8">
       <c r="A32" s="8"/>
       <c r="B32" s="2"/>
       <c r="G32" s="2"/>
       <c r="H32" s="2"/>
     </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:8">
       <c r="A33" s="8"/>
       <c r="B33" s="2"/>
       <c r="G33" s="2"/>
       <c r="H33" s="2"/>
     </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:8">
       <c r="A34" s="8"/>
       <c r="B34" s="2"/>
       <c r="G34" s="2"/>
       <c r="H34" s="2"/>
     </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:8">
       <c r="A35" s="8"/>
       <c r="B35" s="2"/>
       <c r="G35" s="2"/>
       <c r="H35" s="2"/>
     </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:8">
       <c r="A36" s="8"/>
       <c r="B36" s="2"/>
       <c r="G36" s="2"/>
       <c r="H36" s="2"/>
     </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:8">
       <c r="A37" s="8"/>
       <c r="B37" s="2"/>
       <c r="G37" s="2"/>
       <c r="H37" s="2"/>
     </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:8">
       <c r="A38" s="8"/>
       <c r="B38" s="2"/>
       <c r="G38" s="2"/>
       <c r="H38" s="2"/>
     </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:8">
       <c r="A39" s="8"/>
       <c r="B39" s="2"/>
       <c r="G39" s="2"/>
       <c r="H39" s="2"/>
     </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:8">
       <c r="A40" s="8"/>
       <c r="B40" s="2"/>
       <c r="G40" s="2"/>
       <c r="H40" s="2"/>
     </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:8">
       <c r="A41" s="8"/>
       <c r="B41" s="2"/>
       <c r="G41" s="2"/>
       <c r="H41" s="2"/>
     </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:8">
       <c r="A42" s="8"/>
       <c r="B42" s="2"/>
       <c r="G42" s="2"/>
       <c r="H42" s="2"/>
     </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:8">
       <c r="A43" s="8"/>
       <c r="B43" s="2"/>
       <c r="G43" s="2"/>
       <c r="H43" s="2"/>
     </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:8">
       <c r="A44" s="8"/>
       <c r="B44" s="2"/>
       <c r="G44" s="2"/>
       <c r="H44" s="2"/>
     </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:8">
       <c r="A45" s="8"/>
       <c r="B45" s="2"/>
       <c r="G45" s="2"/>
       <c r="H45" s="2"/>
     </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:8">
       <c r="A46" s="8"/>
       <c r="B46" s="2"/>
       <c r="G46" s="2"/>
       <c r="H46" s="2"/>
     </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:8">
       <c r="A47" s="8"/>
       <c r="B47" s="2"/>
       <c r="G47" s="2"/>
       <c r="H47" s="2"/>
     </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:8">
       <c r="A48" s="8"/>
       <c r="B48" s="2"/>
       <c r="G48" s="2"/>
       <c r="H48" s="2"/>
     </row>
-    <row r="49" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:8">
       <c r="A49" s="8"/>
       <c r="B49" s="2"/>
       <c r="G49" s="2"/>
       <c r="H49" s="2"/>
     </row>
-    <row r="50" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:8">
       <c r="A50" s="8"/>
       <c r="B50" s="2"/>
       <c r="G50" s="2"/>
       <c r="H50" s="2"/>
     </row>
-    <row r="51" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:8">
       <c r="A51" s="8"/>
       <c r="B51" s="2"/>
       <c r="G51" s="2"/>
       <c r="H51" s="2"/>
     </row>
-    <row r="52" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:8">
       <c r="A52" s="8"/>
       <c r="B52" s="2"/>
       <c r="G52" s="2"/>
       <c r="H52" s="2"/>
     </row>
-    <row r="53" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:8">
       <c r="A53" s="8"/>
       <c r="B53" s="2"/>
       <c r="G53" s="2"/>
       <c r="H53" s="2"/>
     </row>
-    <row r="54" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:8">
       <c r="A54" s="8"/>
       <c r="B54" s="2"/>
       <c r="G54" s="2"/>
       <c r="H54" s="2"/>
     </row>
-    <row r="55" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:8">
       <c r="A55" s="8"/>
       <c r="B55" s="2"/>
       <c r="G55" s="2"/>
       <c r="H55" s="2"/>
     </row>
-    <row r="56" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:8">
       <c r="A56" s="8"/>
       <c r="B56" s="2"/>
       <c r="G56" s="2"/>
       <c r="H56" s="2"/>
     </row>
-    <row r="57" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:8">
       <c r="A57" s="8"/>
       <c r="B57" s="2"/>
       <c r="G57" s="2"/>
       <c r="H57" s="2"/>
     </row>
-    <row r="58" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:8">
       <c r="A58" s="8"/>
       <c r="B58" s="2"/>
       <c r="G58" s="2"/>
       <c r="H58" s="2"/>
     </row>
-    <row r="59" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:8">
       <c r="A59" s="8"/>
       <c r="B59" s="2"/>
       <c r="G59" s="2"/>
       <c r="H59" s="2"/>
     </row>
-    <row r="60" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:8">
       <c r="A60" s="8"/>
       <c r="B60" s="2"/>
       <c r="G60" s="2"/>
       <c r="H60" s="2"/>
     </row>
-    <row r="61" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:8">
       <c r="A61" s="8"/>
       <c r="B61" s="2"/>
       <c r="G61" s="2"/>
       <c r="H61" s="2"/>
     </row>
-    <row r="62" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:8">
       <c r="A62" s="8"/>
       <c r="B62" s="2"/>
       <c r="G62" s="2"/>
       <c r="H62" s="2"/>
     </row>
-    <row r="63" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:8">
       <c r="A63" s="8"/>
       <c r="B63" s="2"/>
       <c r="G63" s="2"/>
       <c r="H63" s="2"/>
     </row>
-    <row r="64" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:8">
       <c r="A64" s="8"/>
       <c r="B64" s="2"/>
       <c r="G64" s="2"/>
       <c r="H64" s="2"/>
     </row>
-    <row r="65" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:8">
       <c r="A65" s="8"/>
       <c r="B65" s="2"/>
       <c r="G65" s="2"/>
       <c r="H65" s="2"/>
     </row>
-    <row r="66" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:8">
       <c r="A66" s="8"/>
       <c r="B66" s="2"/>
       <c r="G66" s="2"/>
       <c r="H66" s="2"/>
     </row>
-    <row r="67" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:8">
       <c r="A67" s="8"/>
       <c r="B67" s="2"/>
       <c r="G67" s="2"/>
       <c r="H67" s="2"/>
     </row>
-    <row r="68" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:8">
       <c r="A68" s="8"/>
       <c r="B68" s="2"/>
       <c r="G68" s="2"/>
       <c r="H68" s="2"/>
     </row>
-    <row r="69" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:8">
       <c r="A69" s="8"/>
       <c r="B69" s="2"/>
       <c r="G69" s="2"/>
       <c r="H69" s="2"/>
     </row>
-    <row r="70" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:8">
       <c r="A70" s="8"/>
       <c r="B70" s="2"/>
       <c r="G70" s="2"/>
       <c r="H70" s="2"/>
     </row>
-    <row r="71" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:8">
       <c r="A71" s="8"/>
       <c r="B71" s="2"/>
       <c r="G71" s="2"/>
       <c r="H71" s="2"/>
     </row>
-    <row r="72" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:8">
       <c r="A72" s="8"/>
       <c r="B72" s="2"/>
       <c r="G72" s="2"/>
       <c r="H72" s="2"/>
     </row>
-    <row r="73" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:8">
       <c r="A73" s="8"/>
       <c r="B73" s="2"/>
       <c r="G73" s="2"/>
       <c r="H73" s="2"/>
     </row>
-    <row r="74" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:8">
       <c r="A74" s="8"/>
       <c r="B74" s="2"/>
       <c r="G74" s="2"/>
       <c r="H74" s="2"/>
     </row>
-    <row r="75" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:8">
       <c r="A75" s="8"/>
       <c r="B75" s="2"/>
       <c r="G75" s="2"/>
       <c r="H75" s="2"/>
     </row>
-    <row r="76" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:8">
       <c r="A76" s="8"/>
       <c r="B76" s="2"/>
       <c r="G76" s="2"/>
       <c r="H76" s="2"/>
     </row>
-    <row r="77" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:8">
       <c r="A77" s="8"/>
       <c r="B77" s="2"/>
       <c r="G77" s="2"/>
       <c r="H77" s="2"/>
     </row>
-    <row r="78" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:8">
       <c r="A78" s="8"/>
       <c r="B78" s="2"/>
       <c r="G78" s="2"/>
       <c r="H78" s="2"/>
     </row>
-    <row r="79" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:8">
       <c r="A79" s="8"/>
       <c r="B79" s="2"/>
       <c r="G79" s="2"/>
       <c r="H79" s="2"/>
     </row>
-    <row r="80" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:8">
       <c r="A80" s="8"/>
       <c r="B80" s="2"/>
       <c r="G80" s="2"/>
       <c r="H80" s="2"/>
     </row>
-    <row r="81" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:8">
       <c r="A81" s="8"/>
       <c r="B81" s="2"/>
       <c r="G81" s="2"/>
       <c r="H81" s="2"/>
     </row>
-    <row r="82" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:8">
       <c r="A82" s="8"/>
       <c r="B82" s="2"/>
       <c r="G82" s="2"/>
       <c r="H82" s="2"/>
     </row>
-    <row r="83" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:8">
       <c r="A83" s="8"/>
       <c r="B83" s="2"/>
       <c r="G83" s="2"/>
       <c r="H83" s="2"/>
     </row>
-    <row r="84" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:8">
       <c r="A84" s="8"/>
       <c r="B84" s="2"/>
       <c r="G84" s="2"/>
       <c r="H84" s="2"/>
     </row>
-    <row r="85" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:8">
       <c r="A85" s="8"/>
       <c r="B85" s="2"/>
       <c r="G85" s="2"/>
       <c r="H85" s="2"/>
     </row>
-    <row r="86" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:8">
       <c r="A86" s="8"/>
       <c r="B86" s="2"/>
       <c r="G86" s="2"/>
       <c r="H86" s="2"/>
     </row>
-    <row r="87" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:8">
       <c r="A87" s="8"/>
       <c r="B87" s="2"/>
       <c r="G87" s="2"/>
       <c r="H87" s="2"/>
     </row>
-    <row r="88" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:8">
       <c r="A88" s="8"/>
       <c r="B88" s="2"/>
       <c r="G88" s="2"/>
       <c r="H88" s="2"/>
     </row>
-    <row r="89" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:8">
       <c r="A89" s="8"/>
       <c r="B89" s="2"/>
       <c r="G89" s="2"/>
       <c r="H89" s="2"/>
     </row>
-    <row r="90" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:8">
       <c r="A90" s="8"/>
       <c r="B90" s="2"/>
       <c r="G90" s="2"/>
       <c r="H90" s="2"/>
     </row>
-    <row r="91" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:8">
       <c r="A91" s="8"/>
       <c r="B91" s="2"/>
       <c r="G91" s="2"/>
       <c r="H91" s="2"/>
     </row>
-    <row r="92" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:8">
       <c r="A92" s="8"/>
       <c r="B92" s="2"/>
       <c r="G92" s="2"/>
       <c r="H92" s="2"/>
     </row>
-    <row r="93" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:8">
       <c r="A93" s="8"/>
       <c r="B93" s="2"/>
       <c r="G93" s="2"/>
       <c r="H93" s="2"/>
     </row>
-    <row r="94" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:8">
       <c r="A94" s="8"/>
       <c r="B94" s="2"/>
       <c r="G94" s="2"/>
       <c r="H94" s="2"/>
     </row>
-    <row r="95" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:8">
       <c r="A95" s="8"/>
       <c r="B95" s="2"/>
       <c r="G95" s="2"/>
       <c r="H95" s="2"/>
     </row>
-    <row r="96" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:8">
       <c r="A96" s="8"/>
       <c r="B96" s="2"/>
       <c r="G96" s="2"/>
       <c r="H96" s="2"/>
     </row>
-    <row r="97" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:8">
       <c r="A97" s="8"/>
       <c r="B97" s="2"/>
       <c r="G97" s="2"/>
       <c r="H97" s="2"/>
     </row>
-    <row r="98" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:8">
       <c r="A98" s="8"/>
       <c r="B98" s="2"/>
       <c r="G98" s="2"/>
       <c r="H98" s="2"/>
     </row>
-    <row r="99" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:8">
       <c r="A99" s="8"/>
       <c r="B99" s="2"/>
       <c r="G99" s="2"/>
       <c r="H99" s="2"/>
     </row>
-    <row r="100" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:8">
       <c r="A100" s="8"/>
       <c r="B100" s="2"/>
       <c r="G100" s="2"/>
@@ -2261,7 +2280,7 @@
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <ignoredErrors>
-    <ignoredError sqref="D8:D100" listDataValidation="1"/>
+    <ignoredError sqref="D9:D100" listDataValidation="1"/>
   </ignoredErrors>
   <tableParts count="1">
     <tablePart r:id="rId1"/>
@@ -2273,23 +2292,23 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9FD6A201-8E63-4A9E-A683-19506CB489E3}">
   <dimension ref="A1:H100"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="10.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="17.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="27.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.85546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="23.5703125" style="10" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="39.140625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="51.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.44140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="27.88671875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.88671875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="23.5546875" style="10" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="39.109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="51.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" ht="15.6">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
@@ -2315,7 +2334,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8">
       <c r="A2" s="1">
         <v>45935</v>
       </c>
@@ -2341,7 +2360,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8">
       <c r="A3" s="1">
         <v>45996</v>
       </c>
@@ -2367,7 +2386,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8">
       <c r="A4" s="1" t="s">
         <v>57</v>
       </c>
@@ -2393,7 +2412,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8">
       <c r="A5" s="1" t="s">
         <v>61</v>
       </c>
@@ -2419,7 +2438,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8">
       <c r="A6" s="1" t="s">
         <v>67</v>
       </c>
@@ -2445,7 +2464,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8">
       <c r="A7" s="1" t="s">
         <v>70</v>
       </c>
@@ -2471,7 +2490,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="8" spans="1:8" ht="105" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" ht="100.8">
       <c r="A8" s="1">
         <v>45798</v>
       </c>
@@ -2495,644 +2514,644 @@
         <v>89</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8">
       <c r="A9" s="1"/>
       <c r="B9" s="2"/>
       <c r="E9" s="3"/>
       <c r="G9" s="2"/>
       <c r="H9" s="2"/>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8">
       <c r="A10" s="1"/>
       <c r="B10" s="2"/>
       <c r="E10" s="3"/>
       <c r="G10" s="2"/>
       <c r="H10" s="2"/>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8">
       <c r="A11" s="1"/>
       <c r="B11" s="2"/>
       <c r="E11" s="3"/>
       <c r="G11" s="2"/>
       <c r="H11" s="2"/>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8">
       <c r="A12" s="1"/>
       <c r="B12" s="2"/>
       <c r="E12" s="3"/>
       <c r="G12" s="2"/>
       <c r="H12" s="2"/>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8">
       <c r="A13" s="1"/>
       <c r="B13" s="2"/>
       <c r="E13" s="3"/>
       <c r="G13" s="2"/>
       <c r="H13" s="2"/>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8">
       <c r="A14" s="1"/>
       <c r="B14" s="2"/>
       <c r="E14" s="3"/>
       <c r="G14" s="2"/>
       <c r="H14" s="2"/>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8">
       <c r="A15" s="1"/>
       <c r="B15" s="2"/>
       <c r="E15" s="3"/>
       <c r="G15" s="2"/>
       <c r="H15" s="2"/>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8">
       <c r="A16" s="1"/>
       <c r="B16" s="2"/>
       <c r="E16" s="3"/>
       <c r="G16" s="2"/>
       <c r="H16" s="2"/>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:8">
       <c r="A17" s="1"/>
       <c r="B17" s="2"/>
       <c r="E17" s="3"/>
       <c r="G17" s="2"/>
       <c r="H17" s="2"/>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:8">
       <c r="A18" s="1"/>
       <c r="B18" s="2"/>
       <c r="E18" s="3"/>
       <c r="G18" s="2"/>
       <c r="H18" s="2"/>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:8">
       <c r="A19" s="1"/>
       <c r="B19" s="2"/>
       <c r="E19" s="3"/>
       <c r="G19" s="2"/>
       <c r="H19" s="2"/>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:8">
       <c r="A20" s="1"/>
       <c r="B20" s="2"/>
       <c r="E20" s="3"/>
       <c r="G20" s="2"/>
       <c r="H20" s="2"/>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:8">
       <c r="A21" s="1"/>
       <c r="B21" s="2"/>
       <c r="E21" s="3"/>
       <c r="G21" s="2"/>
       <c r="H21" s="2"/>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:8">
       <c r="A22" s="1"/>
       <c r="B22" s="2"/>
       <c r="E22" s="3"/>
       <c r="G22" s="2"/>
       <c r="H22" s="2"/>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:8">
       <c r="A23" s="1"/>
       <c r="B23" s="2"/>
       <c r="E23" s="3"/>
       <c r="G23" s="2"/>
       <c r="H23" s="2"/>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:8">
       <c r="A24" s="1"/>
       <c r="B24" s="2"/>
       <c r="E24" s="3"/>
       <c r="G24" s="2"/>
       <c r="H24" s="2"/>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:8">
       <c r="A25" s="1"/>
       <c r="B25" s="2"/>
       <c r="E25" s="3"/>
       <c r="G25" s="2"/>
       <c r="H25" s="2"/>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:8">
       <c r="A26" s="1"/>
       <c r="B26" s="2"/>
       <c r="E26" s="3"/>
       <c r="G26" s="2"/>
       <c r="H26" s="2"/>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:8">
       <c r="A27" s="1"/>
       <c r="B27" s="2"/>
       <c r="E27" s="3"/>
       <c r="G27" s="2"/>
       <c r="H27" s="2"/>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:8">
       <c r="A28" s="1"/>
       <c r="B28" s="2"/>
       <c r="E28" s="3"/>
       <c r="G28" s="2"/>
       <c r="H28" s="2"/>
     </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:8">
       <c r="A29" s="1"/>
       <c r="B29" s="2"/>
       <c r="E29" s="3"/>
       <c r="G29" s="2"/>
       <c r="H29" s="2"/>
     </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:8">
       <c r="A30" s="1"/>
       <c r="B30" s="2"/>
       <c r="E30" s="3"/>
       <c r="G30" s="2"/>
       <c r="H30" s="2"/>
     </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:8">
       <c r="A31" s="1"/>
       <c r="B31" s="2"/>
       <c r="E31" s="3"/>
       <c r="G31" s="2"/>
       <c r="H31" s="2"/>
     </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:8">
       <c r="A32" s="1"/>
       <c r="B32" s="2"/>
       <c r="E32" s="3"/>
       <c r="G32" s="2"/>
       <c r="H32" s="2"/>
     </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:8">
       <c r="A33" s="1"/>
       <c r="B33" s="2"/>
       <c r="E33" s="3"/>
       <c r="G33" s="2"/>
       <c r="H33" s="2"/>
     </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:8">
       <c r="A34" s="1"/>
       <c r="B34" s="2"/>
       <c r="E34" s="3"/>
       <c r="G34" s="2"/>
       <c r="H34" s="2"/>
     </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:8">
       <c r="A35" s="1"/>
       <c r="B35" s="2"/>
       <c r="E35" s="3"/>
       <c r="G35" s="2"/>
       <c r="H35" s="2"/>
     </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:8">
       <c r="A36" s="1"/>
       <c r="B36" s="2"/>
       <c r="E36" s="3"/>
       <c r="G36" s="2"/>
       <c r="H36" s="2"/>
     </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:8">
       <c r="A37" s="1"/>
       <c r="B37" s="2"/>
       <c r="E37" s="3"/>
       <c r="G37" s="2"/>
       <c r="H37" s="2"/>
     </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:8">
       <c r="A38" s="1"/>
       <c r="B38" s="2"/>
       <c r="E38" s="3"/>
       <c r="G38" s="2"/>
       <c r="H38" s="2"/>
     </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:8">
       <c r="A39" s="1"/>
       <c r="B39" s="2"/>
       <c r="E39" s="3"/>
       <c r="G39" s="2"/>
       <c r="H39" s="2"/>
     </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:8">
       <c r="A40" s="1"/>
       <c r="B40" s="2"/>
       <c r="E40" s="3"/>
       <c r="G40" s="2"/>
       <c r="H40" s="2"/>
     </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:8">
       <c r="A41" s="1"/>
       <c r="B41" s="2"/>
       <c r="E41" s="3"/>
       <c r="G41" s="2"/>
       <c r="H41" s="2"/>
     </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:8">
       <c r="A42" s="1"/>
       <c r="B42" s="2"/>
       <c r="E42" s="3"/>
       <c r="G42" s="2"/>
       <c r="H42" s="2"/>
     </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:8">
       <c r="A43" s="1"/>
       <c r="B43" s="2"/>
       <c r="E43" s="3"/>
       <c r="G43" s="2"/>
       <c r="H43" s="2"/>
     </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:8">
       <c r="A44" s="1"/>
       <c r="B44" s="2"/>
       <c r="E44" s="3"/>
       <c r="G44" s="2"/>
       <c r="H44" s="2"/>
     </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:8">
       <c r="A45" s="1"/>
       <c r="B45" s="2"/>
       <c r="E45" s="3"/>
       <c r="G45" s="2"/>
       <c r="H45" s="2"/>
     </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:8">
       <c r="A46" s="1"/>
       <c r="B46" s="2"/>
       <c r="E46" s="3"/>
       <c r="G46" s="2"/>
       <c r="H46" s="2"/>
     </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:8">
       <c r="A47" s="1"/>
       <c r="B47" s="2"/>
       <c r="E47" s="3"/>
       <c r="G47" s="2"/>
       <c r="H47" s="2"/>
     </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:8">
       <c r="A48" s="1"/>
       <c r="B48" s="2"/>
       <c r="E48" s="3"/>
       <c r="G48" s="2"/>
       <c r="H48" s="2"/>
     </row>
-    <row r="49" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:8">
       <c r="A49" s="1"/>
       <c r="B49" s="2"/>
       <c r="E49" s="3"/>
       <c r="G49" s="2"/>
       <c r="H49" s="2"/>
     </row>
-    <row r="50" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:8">
       <c r="A50" s="1"/>
       <c r="B50" s="2"/>
       <c r="E50" s="3"/>
       <c r="G50" s="2"/>
       <c r="H50" s="2"/>
     </row>
-    <row r="51" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:8">
       <c r="A51" s="1"/>
       <c r="B51" s="2"/>
       <c r="E51" s="3"/>
       <c r="G51" s="2"/>
       <c r="H51" s="2"/>
     </row>
-    <row r="52" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:8">
       <c r="A52" s="1"/>
       <c r="B52" s="2"/>
       <c r="E52" s="3"/>
       <c r="G52" s="2"/>
       <c r="H52" s="2"/>
     </row>
-    <row r="53" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:8">
       <c r="A53" s="1"/>
       <c r="B53" s="2"/>
       <c r="E53" s="3"/>
       <c r="G53" s="2"/>
       <c r="H53" s="2"/>
     </row>
-    <row r="54" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:8">
       <c r="A54" s="1"/>
       <c r="B54" s="2"/>
       <c r="E54" s="3"/>
       <c r="G54" s="2"/>
       <c r="H54" s="2"/>
     </row>
-    <row r="55" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:8">
       <c r="A55" s="1"/>
       <c r="B55" s="2"/>
       <c r="E55" s="3"/>
       <c r="G55" s="2"/>
       <c r="H55" s="2"/>
     </row>
-    <row r="56" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:8">
       <c r="A56" s="1"/>
       <c r="B56" s="2"/>
       <c r="E56" s="3"/>
       <c r="G56" s="2"/>
       <c r="H56" s="2"/>
     </row>
-    <row r="57" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:8">
       <c r="A57" s="1"/>
       <c r="B57" s="2"/>
       <c r="E57" s="3"/>
       <c r="G57" s="2"/>
       <c r="H57" s="2"/>
     </row>
-    <row r="58" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:8">
       <c r="A58" s="1"/>
       <c r="B58" s="2"/>
       <c r="E58" s="3"/>
       <c r="G58" s="2"/>
       <c r="H58" s="2"/>
     </row>
-    <row r="59" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:8">
       <c r="A59" s="1"/>
       <c r="B59" s="2"/>
       <c r="E59" s="3"/>
       <c r="G59" s="2"/>
       <c r="H59" s="2"/>
     </row>
-    <row r="60" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:8">
       <c r="A60" s="1"/>
       <c r="B60" s="2"/>
       <c r="E60" s="3"/>
       <c r="G60" s="2"/>
       <c r="H60" s="2"/>
     </row>
-    <row r="61" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:8">
       <c r="A61" s="1"/>
       <c r="B61" s="2"/>
       <c r="E61" s="3"/>
       <c r="G61" s="2"/>
       <c r="H61" s="2"/>
     </row>
-    <row r="62" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:8">
       <c r="A62" s="1"/>
       <c r="B62" s="2"/>
       <c r="E62" s="3"/>
       <c r="G62" s="2"/>
       <c r="H62" s="2"/>
     </row>
-    <row r="63" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:8">
       <c r="A63" s="1"/>
       <c r="B63" s="2"/>
       <c r="E63" s="3"/>
       <c r="G63" s="2"/>
       <c r="H63" s="2"/>
     </row>
-    <row r="64" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:8">
       <c r="A64" s="1"/>
       <c r="B64" s="2"/>
       <c r="E64" s="3"/>
       <c r="G64" s="2"/>
       <c r="H64" s="2"/>
     </row>
-    <row r="65" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:8">
       <c r="A65" s="1"/>
       <c r="B65" s="2"/>
       <c r="E65" s="3"/>
       <c r="G65" s="2"/>
       <c r="H65" s="2"/>
     </row>
-    <row r="66" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:8">
       <c r="A66" s="1"/>
       <c r="B66" s="2"/>
       <c r="E66" s="3"/>
       <c r="G66" s="2"/>
       <c r="H66" s="2"/>
     </row>
-    <row r="67" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:8">
       <c r="A67" s="1"/>
       <c r="B67" s="2"/>
       <c r="E67" s="3"/>
       <c r="G67" s="2"/>
       <c r="H67" s="2"/>
     </row>
-    <row r="68" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:8">
       <c r="A68" s="1"/>
       <c r="B68" s="2"/>
       <c r="E68" s="3"/>
       <c r="G68" s="2"/>
       <c r="H68" s="2"/>
     </row>
-    <row r="69" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:8">
       <c r="A69" s="1"/>
       <c r="B69" s="2"/>
       <c r="E69" s="3"/>
       <c r="G69" s="2"/>
       <c r="H69" s="2"/>
     </row>
-    <row r="70" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:8">
       <c r="A70" s="1"/>
       <c r="B70" s="2"/>
       <c r="E70" s="3"/>
       <c r="G70" s="2"/>
       <c r="H70" s="2"/>
     </row>
-    <row r="71" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:8">
       <c r="A71" s="1"/>
       <c r="B71" s="2"/>
       <c r="E71" s="3"/>
       <c r="G71" s="2"/>
       <c r="H71" s="2"/>
     </row>
-    <row r="72" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:8">
       <c r="A72" s="1"/>
       <c r="B72" s="2"/>
       <c r="E72" s="3"/>
       <c r="G72" s="2"/>
       <c r="H72" s="2"/>
     </row>
-    <row r="73" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:8">
       <c r="A73" s="1"/>
       <c r="B73" s="2"/>
       <c r="E73" s="3"/>
       <c r="G73" s="2"/>
       <c r="H73" s="2"/>
     </row>
-    <row r="74" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:8">
       <c r="A74" s="1"/>
       <c r="B74" s="2"/>
       <c r="E74" s="3"/>
       <c r="G74" s="2"/>
       <c r="H74" s="2"/>
     </row>
-    <row r="75" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:8">
       <c r="A75" s="1"/>
       <c r="B75" s="2"/>
       <c r="E75" s="3"/>
       <c r="G75" s="2"/>
       <c r="H75" s="2"/>
     </row>
-    <row r="76" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:8">
       <c r="A76" s="1"/>
       <c r="B76" s="2"/>
       <c r="E76" s="3"/>
       <c r="G76" s="2"/>
       <c r="H76" s="2"/>
     </row>
-    <row r="77" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:8">
       <c r="A77" s="1"/>
       <c r="B77" s="2"/>
       <c r="E77" s="3"/>
       <c r="G77" s="2"/>
       <c r="H77" s="2"/>
     </row>
-    <row r="78" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:8">
       <c r="A78" s="1"/>
       <c r="B78" s="2"/>
       <c r="E78" s="3"/>
       <c r="G78" s="2"/>
       <c r="H78" s="2"/>
     </row>
-    <row r="79" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:8">
       <c r="A79" s="1"/>
       <c r="B79" s="2"/>
       <c r="E79" s="3"/>
       <c r="G79" s="2"/>
       <c r="H79" s="2"/>
     </row>
-    <row r="80" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:8">
       <c r="A80" s="1"/>
       <c r="B80" s="2"/>
       <c r="E80" s="3"/>
       <c r="G80" s="2"/>
       <c r="H80" s="2"/>
     </row>
-    <row r="81" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:8">
       <c r="A81" s="1"/>
       <c r="B81" s="2"/>
       <c r="E81" s="3"/>
       <c r="G81" s="2"/>
       <c r="H81" s="2"/>
     </row>
-    <row r="82" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:8">
       <c r="A82" s="1"/>
       <c r="B82" s="2"/>
       <c r="E82" s="3"/>
       <c r="G82" s="2"/>
       <c r="H82" s="2"/>
     </row>
-    <row r="83" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:8">
       <c r="A83" s="1"/>
       <c r="B83" s="2"/>
       <c r="E83" s="3"/>
       <c r="G83" s="2"/>
       <c r="H83" s="2"/>
     </row>
-    <row r="84" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:8">
       <c r="A84" s="1"/>
       <c r="B84" s="2"/>
       <c r="E84" s="3"/>
       <c r="G84" s="2"/>
       <c r="H84" s="2"/>
     </row>
-    <row r="85" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:8">
       <c r="A85" s="1"/>
       <c r="B85" s="2"/>
       <c r="E85" s="3"/>
       <c r="G85" s="2"/>
       <c r="H85" s="2"/>
     </row>
-    <row r="86" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:8">
       <c r="A86" s="1"/>
       <c r="B86" s="2"/>
       <c r="E86" s="3"/>
       <c r="G86" s="2"/>
       <c r="H86" s="2"/>
     </row>
-    <row r="87" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:8">
       <c r="A87" s="1"/>
       <c r="B87" s="2"/>
       <c r="E87" s="3"/>
       <c r="G87" s="2"/>
       <c r="H87" s="2"/>
     </row>
-    <row r="88" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:8">
       <c r="A88" s="1"/>
       <c r="B88" s="2"/>
       <c r="E88" s="3"/>
       <c r="G88" s="2"/>
       <c r="H88" s="2"/>
     </row>
-    <row r="89" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:8">
       <c r="A89" s="1"/>
       <c r="B89" s="2"/>
       <c r="E89" s="3"/>
       <c r="G89" s="2"/>
       <c r="H89" s="2"/>
     </row>
-    <row r="90" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:8">
       <c r="A90" s="1"/>
       <c r="B90" s="2"/>
       <c r="E90" s="3"/>
       <c r="G90" s="2"/>
       <c r="H90" s="2"/>
     </row>
-    <row r="91" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:8">
       <c r="A91" s="1"/>
       <c r="B91" s="2"/>
       <c r="E91" s="3"/>
       <c r="G91" s="2"/>
       <c r="H91" s="2"/>
     </row>
-    <row r="92" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:8">
       <c r="A92" s="1"/>
       <c r="B92" s="2"/>
       <c r="E92" s="3"/>
       <c r="G92" s="2"/>
       <c r="H92" s="2"/>
     </row>
-    <row r="93" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:8">
       <c r="A93" s="1"/>
       <c r="B93" s="2"/>
       <c r="E93" s="3"/>
       <c r="G93" s="2"/>
       <c r="H93" s="2"/>
     </row>
-    <row r="94" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:8">
       <c r="A94" s="1"/>
       <c r="B94" s="2"/>
       <c r="E94" s="3"/>
       <c r="G94" s="2"/>
       <c r="H94" s="2"/>
     </row>
-    <row r="95" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:8">
       <c r="A95" s="1"/>
       <c r="B95" s="2"/>
       <c r="E95" s="3"/>
       <c r="G95" s="2"/>
       <c r="H95" s="2"/>
     </row>
-    <row r="96" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:8">
       <c r="A96" s="1"/>
       <c r="B96" s="2"/>
       <c r="E96" s="3"/>
       <c r="G96" s="2"/>
       <c r="H96" s="2"/>
     </row>
-    <row r="97" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:8">
       <c r="A97" s="1"/>
       <c r="B97" s="2"/>
       <c r="E97" s="3"/>
       <c r="G97" s="2"/>
       <c r="H97" s="2"/>
     </row>
-    <row r="98" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:8">
       <c r="A98" s="1"/>
       <c r="B98" s="2"/>
       <c r="E98" s="3"/>
       <c r="G98" s="2"/>
       <c r="H98" s="2"/>
     </row>
-    <row r="99" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:8">
       <c r="A99" s="1"/>
       <c r="B99" s="2"/>
       <c r="E99" s="3"/>
       <c r="G99" s="2"/>
       <c r="H99" s="2"/>
     </row>
-    <row r="100" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:8">
       <c r="A100" s="1"/>
       <c r="B100" s="2"/>
       <c r="E100" s="3"/>
@@ -3174,19 +3193,19 @@
       <selection activeCell="D2" sqref="D2:D100"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="7.7109375" customWidth="1"/>
-    <col min="2" max="2" width="17.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="7.6640625" customWidth="1"/>
+    <col min="2" max="2" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.5546875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="9" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.85546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="23.5703125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="13.42578125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="19.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.88671875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="23.5546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.44140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="19.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" ht="15.6">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
@@ -3212,7 +3231,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8">
       <c r="A2" s="1"/>
       <c r="B2" s="2"/>
       <c r="E2" s="3"/>
@@ -3220,7 +3239,7 @@
       <c r="G2" s="2"/>
       <c r="H2" s="2"/>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8">
       <c r="A3" s="1"/>
       <c r="B3" s="2"/>
       <c r="E3" s="3"/>
@@ -3228,7 +3247,7 @@
       <c r="G3" s="2"/>
       <c r="H3" s="2"/>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8">
       <c r="A4" s="1"/>
       <c r="B4" s="2"/>
       <c r="E4" s="3"/>
@@ -3236,7 +3255,7 @@
       <c r="G4" s="2"/>
       <c r="H4" s="2"/>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8">
       <c r="A5" s="1"/>
       <c r="B5" s="2"/>
       <c r="E5" s="3"/>
@@ -3244,7 +3263,7 @@
       <c r="G5" s="2"/>
       <c r="H5" s="2"/>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8">
       <c r="A6" s="1"/>
       <c r="B6" s="2"/>
       <c r="E6" s="3"/>
@@ -3252,7 +3271,7 @@
       <c r="G6" s="2"/>
       <c r="H6" s="2"/>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8">
       <c r="A7" s="1"/>
       <c r="B7" s="2"/>
       <c r="E7" s="3"/>
@@ -3260,7 +3279,7 @@
       <c r="G7" s="2"/>
       <c r="H7" s="2"/>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8">
       <c r="A8" s="1"/>
       <c r="B8" s="2"/>
       <c r="E8" s="3"/>
@@ -3268,7 +3287,7 @@
       <c r="G8" s="2"/>
       <c r="H8" s="2"/>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8">
       <c r="A9" s="1"/>
       <c r="B9" s="2"/>
       <c r="E9" s="3"/>
@@ -3276,7 +3295,7 @@
       <c r="G9" s="2"/>
       <c r="H9" s="2"/>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8">
       <c r="A10" s="1"/>
       <c r="B10" s="2"/>
       <c r="E10" s="3"/>
@@ -3284,7 +3303,7 @@
       <c r="G10" s="2"/>
       <c r="H10" s="2"/>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8">
       <c r="A11" s="1"/>
       <c r="B11" s="2"/>
       <c r="E11" s="3"/>
@@ -3292,7 +3311,7 @@
       <c r="G11" s="2"/>
       <c r="H11" s="2"/>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8">
       <c r="A12" s="1"/>
       <c r="B12" s="2"/>
       <c r="E12" s="3"/>
@@ -3300,7 +3319,7 @@
       <c r="G12" s="2"/>
       <c r="H12" s="2"/>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8">
       <c r="A13" s="1"/>
       <c r="B13" s="2"/>
       <c r="E13" s="3"/>
@@ -3308,7 +3327,7 @@
       <c r="G13" s="2"/>
       <c r="H13" s="2"/>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8">
       <c r="A14" s="1"/>
       <c r="B14" s="2"/>
       <c r="E14" s="3"/>
@@ -3316,7 +3335,7 @@
       <c r="G14" s="2"/>
       <c r="H14" s="2"/>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8">
       <c r="A15" s="1"/>
       <c r="B15" s="2"/>
       <c r="E15" s="3"/>
@@ -3324,7 +3343,7 @@
       <c r="G15" s="2"/>
       <c r="H15" s="2"/>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8">
       <c r="A16" s="1"/>
       <c r="B16" s="2"/>
       <c r="E16" s="3"/>
@@ -3332,7 +3351,7 @@
       <c r="G16" s="2"/>
       <c r="H16" s="2"/>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:8">
       <c r="A17" s="1"/>
       <c r="B17" s="2"/>
       <c r="E17" s="3"/>
@@ -3340,7 +3359,7 @@
       <c r="G17" s="2"/>
       <c r="H17" s="2"/>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:8">
       <c r="A18" s="1"/>
       <c r="B18" s="2"/>
       <c r="E18" s="3"/>
@@ -3348,7 +3367,7 @@
       <c r="G18" s="2"/>
       <c r="H18" s="2"/>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:8">
       <c r="A19" s="1"/>
       <c r="B19" s="2"/>
       <c r="E19" s="3"/>
@@ -3356,7 +3375,7 @@
       <c r="G19" s="2"/>
       <c r="H19" s="2"/>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:8">
       <c r="A20" s="1"/>
       <c r="B20" s="2"/>
       <c r="E20" s="3"/>
@@ -3364,7 +3383,7 @@
       <c r="G20" s="2"/>
       <c r="H20" s="2"/>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:8">
       <c r="A21" s="1"/>
       <c r="B21" s="2"/>
       <c r="E21" s="3"/>
@@ -3372,7 +3391,7 @@
       <c r="G21" s="2"/>
       <c r="H21" s="2"/>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:8">
       <c r="A22" s="1"/>
       <c r="B22" s="2"/>
       <c r="E22" s="3"/>
@@ -3380,7 +3399,7 @@
       <c r="G22" s="2"/>
       <c r="H22" s="2"/>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:8">
       <c r="A23" s="1"/>
       <c r="B23" s="2"/>
       <c r="E23" s="3"/>
@@ -3388,7 +3407,7 @@
       <c r="G23" s="2"/>
       <c r="H23" s="2"/>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:8">
       <c r="A24" s="1"/>
       <c r="B24" s="2"/>
       <c r="E24" s="3"/>
@@ -3396,7 +3415,7 @@
       <c r="G24" s="2"/>
       <c r="H24" s="2"/>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:8">
       <c r="A25" s="1"/>
       <c r="B25" s="2"/>
       <c r="E25" s="3"/>
@@ -3404,7 +3423,7 @@
       <c r="G25" s="2"/>
       <c r="H25" s="2"/>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:8">
       <c r="A26" s="1"/>
       <c r="B26" s="2"/>
       <c r="E26" s="3"/>
@@ -3412,7 +3431,7 @@
       <c r="G26" s="2"/>
       <c r="H26" s="2"/>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:8">
       <c r="A27" s="1"/>
       <c r="B27" s="2"/>
       <c r="E27" s="3"/>
@@ -3420,7 +3439,7 @@
       <c r="G27" s="2"/>
       <c r="H27" s="2"/>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:8">
       <c r="A28" s="1"/>
       <c r="B28" s="2"/>
       <c r="E28" s="3"/>
@@ -3428,7 +3447,7 @@
       <c r="G28" s="2"/>
       <c r="H28" s="2"/>
     </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:8">
       <c r="A29" s="1"/>
       <c r="B29" s="2"/>
       <c r="E29" s="3"/>
@@ -3436,7 +3455,7 @@
       <c r="G29" s="2"/>
       <c r="H29" s="2"/>
     </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:8">
       <c r="A30" s="1"/>
       <c r="B30" s="2"/>
       <c r="E30" s="3"/>
@@ -3444,7 +3463,7 @@
       <c r="G30" s="2"/>
       <c r="H30" s="2"/>
     </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:8">
       <c r="A31" s="1"/>
       <c r="B31" s="2"/>
       <c r="E31" s="3"/>
@@ -3452,7 +3471,7 @@
       <c r="G31" s="2"/>
       <c r="H31" s="2"/>
     </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:8">
       <c r="A32" s="1"/>
       <c r="B32" s="2"/>
       <c r="E32" s="3"/>
@@ -3460,7 +3479,7 @@
       <c r="G32" s="2"/>
       <c r="H32" s="2"/>
     </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:8">
       <c r="A33" s="1"/>
       <c r="B33" s="2"/>
       <c r="E33" s="3"/>
@@ -3468,7 +3487,7 @@
       <c r="G33" s="2"/>
       <c r="H33" s="2"/>
     </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:8">
       <c r="A34" s="1"/>
       <c r="B34" s="2"/>
       <c r="E34" s="3"/>
@@ -3476,7 +3495,7 @@
       <c r="G34" s="2"/>
       <c r="H34" s="2"/>
     </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:8">
       <c r="A35" s="1"/>
       <c r="B35" s="2"/>
       <c r="E35" s="3"/>
@@ -3484,7 +3503,7 @@
       <c r="G35" s="2"/>
       <c r="H35" s="2"/>
     </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:8">
       <c r="A36" s="1"/>
       <c r="B36" s="2"/>
       <c r="E36" s="3"/>
@@ -3492,7 +3511,7 @@
       <c r="G36" s="2"/>
       <c r="H36" s="2"/>
     </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:8">
       <c r="A37" s="1"/>
       <c r="B37" s="2"/>
       <c r="E37" s="3"/>
@@ -3500,7 +3519,7 @@
       <c r="G37" s="2"/>
       <c r="H37" s="2"/>
     </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:8">
       <c r="A38" s="1"/>
       <c r="B38" s="2"/>
       <c r="E38" s="3"/>
@@ -3508,7 +3527,7 @@
       <c r="G38" s="2"/>
       <c r="H38" s="2"/>
     </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:8">
       <c r="A39" s="1"/>
       <c r="B39" s="2"/>
       <c r="E39" s="3"/>
@@ -3516,7 +3535,7 @@
       <c r="G39" s="2"/>
       <c r="H39" s="2"/>
     </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:8">
       <c r="A40" s="1"/>
       <c r="B40" s="2"/>
       <c r="E40" s="3"/>
@@ -3524,7 +3543,7 @@
       <c r="G40" s="2"/>
       <c r="H40" s="2"/>
     </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:8">
       <c r="A41" s="1"/>
       <c r="B41" s="2"/>
       <c r="E41" s="3"/>
@@ -3532,7 +3551,7 @@
       <c r="G41" s="2"/>
       <c r="H41" s="2"/>
     </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:8">
       <c r="A42" s="1"/>
       <c r="B42" s="2"/>
       <c r="E42" s="3"/>
@@ -3540,7 +3559,7 @@
       <c r="G42" s="2"/>
       <c r="H42" s="2"/>
     </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:8">
       <c r="A43" s="1"/>
       <c r="B43" s="2"/>
       <c r="E43" s="3"/>
@@ -3548,7 +3567,7 @@
       <c r="G43" s="2"/>
       <c r="H43" s="2"/>
     </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:8">
       <c r="A44" s="1"/>
       <c r="B44" s="2"/>
       <c r="E44" s="3"/>
@@ -3556,7 +3575,7 @@
       <c r="G44" s="2"/>
       <c r="H44" s="2"/>
     </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:8">
       <c r="A45" s="1"/>
       <c r="B45" s="2"/>
       <c r="E45" s="3"/>
@@ -3564,7 +3583,7 @@
       <c r="G45" s="2"/>
       <c r="H45" s="2"/>
     </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:8">
       <c r="A46" s="1"/>
       <c r="B46" s="2"/>
       <c r="E46" s="3"/>
@@ -3572,7 +3591,7 @@
       <c r="G46" s="2"/>
       <c r="H46" s="2"/>
     </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:8">
       <c r="A47" s="1"/>
       <c r="B47" s="2"/>
       <c r="E47" s="3"/>
@@ -3580,7 +3599,7 @@
       <c r="G47" s="2"/>
       <c r="H47" s="2"/>
     </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:8">
       <c r="A48" s="1"/>
       <c r="B48" s="2"/>
       <c r="E48" s="3"/>
@@ -3588,7 +3607,7 @@
       <c r="G48" s="2"/>
       <c r="H48" s="2"/>
     </row>
-    <row r="49" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:8">
       <c r="A49" s="1"/>
       <c r="B49" s="2"/>
       <c r="E49" s="3"/>
@@ -3596,7 +3615,7 @@
       <c r="G49" s="2"/>
       <c r="H49" s="2"/>
     </row>
-    <row r="50" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:8">
       <c r="A50" s="1"/>
       <c r="B50" s="2"/>
       <c r="E50" s="3"/>
@@ -3604,7 +3623,7 @@
       <c r="G50" s="2"/>
       <c r="H50" s="2"/>
     </row>
-    <row r="51" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:8">
       <c r="A51" s="1"/>
       <c r="B51" s="2"/>
       <c r="E51" s="3"/>
@@ -3612,7 +3631,7 @@
       <c r="G51" s="2"/>
       <c r="H51" s="2"/>
     </row>
-    <row r="52" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:8">
       <c r="A52" s="1"/>
       <c r="B52" s="2"/>
       <c r="E52" s="3"/>
@@ -3620,7 +3639,7 @@
       <c r="G52" s="2"/>
       <c r="H52" s="2"/>
     </row>
-    <row r="53" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:8">
       <c r="A53" s="1"/>
       <c r="B53" s="2"/>
       <c r="E53" s="3"/>
@@ -3628,7 +3647,7 @@
       <c r="G53" s="2"/>
       <c r="H53" s="2"/>
     </row>
-    <row r="54" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:8">
       <c r="A54" s="1"/>
       <c r="B54" s="2"/>
       <c r="E54" s="3"/>
@@ -3636,7 +3655,7 @@
       <c r="G54" s="2"/>
       <c r="H54" s="2"/>
     </row>
-    <row r="55" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:8">
       <c r="A55" s="1"/>
       <c r="B55" s="2"/>
       <c r="E55" s="3"/>
@@ -3644,7 +3663,7 @@
       <c r="G55" s="2"/>
       <c r="H55" s="2"/>
     </row>
-    <row r="56" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:8">
       <c r="A56" s="1"/>
       <c r="B56" s="2"/>
       <c r="E56" s="3"/>
@@ -3652,7 +3671,7 @@
       <c r="G56" s="2"/>
       <c r="H56" s="2"/>
     </row>
-    <row r="57" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:8">
       <c r="A57" s="1"/>
       <c r="B57" s="2"/>
       <c r="E57" s="3"/>
@@ -3660,7 +3679,7 @@
       <c r="G57" s="2"/>
       <c r="H57" s="2"/>
     </row>
-    <row r="58" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:8">
       <c r="A58" s="1"/>
       <c r="B58" s="2"/>
       <c r="E58" s="3"/>
@@ -3668,7 +3687,7 @@
       <c r="G58" s="2"/>
       <c r="H58" s="2"/>
     </row>
-    <row r="59" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:8">
       <c r="A59" s="1"/>
       <c r="B59" s="2"/>
       <c r="E59" s="3"/>
@@ -3676,7 +3695,7 @@
       <c r="G59" s="2"/>
       <c r="H59" s="2"/>
     </row>
-    <row r="60" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:8">
       <c r="A60" s="1"/>
       <c r="B60" s="2"/>
       <c r="E60" s="3"/>
@@ -3684,7 +3703,7 @@
       <c r="G60" s="2"/>
       <c r="H60" s="2"/>
     </row>
-    <row r="61" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:8">
       <c r="A61" s="1"/>
       <c r="B61" s="2"/>
       <c r="E61" s="3"/>
@@ -3692,7 +3711,7 @@
       <c r="G61" s="2"/>
       <c r="H61" s="2"/>
     </row>
-    <row r="62" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:8">
       <c r="A62" s="1"/>
       <c r="B62" s="2"/>
       <c r="E62" s="3"/>
@@ -3700,7 +3719,7 @@
       <c r="G62" s="2"/>
       <c r="H62" s="2"/>
     </row>
-    <row r="63" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:8">
       <c r="A63" s="1"/>
       <c r="B63" s="2"/>
       <c r="E63" s="3"/>
@@ -3708,7 +3727,7 @@
       <c r="G63" s="2"/>
       <c r="H63" s="2"/>
     </row>
-    <row r="64" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:8">
       <c r="A64" s="1"/>
       <c r="B64" s="2"/>
       <c r="E64" s="3"/>
@@ -3716,7 +3735,7 @@
       <c r="G64" s="2"/>
       <c r="H64" s="2"/>
     </row>
-    <row r="65" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:8">
       <c r="A65" s="1"/>
       <c r="B65" s="2"/>
       <c r="E65" s="3"/>
@@ -3724,7 +3743,7 @@
       <c r="G65" s="2"/>
       <c r="H65" s="2"/>
     </row>
-    <row r="66" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:8">
       <c r="A66" s="1"/>
       <c r="B66" s="2"/>
       <c r="E66" s="3"/>
@@ -3732,7 +3751,7 @@
       <c r="G66" s="2"/>
       <c r="H66" s="2"/>
     </row>
-    <row r="67" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:8">
       <c r="A67" s="1"/>
       <c r="B67" s="2"/>
       <c r="E67" s="3"/>
@@ -3740,7 +3759,7 @@
       <c r="G67" s="2"/>
       <c r="H67" s="2"/>
     </row>
-    <row r="68" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:8">
       <c r="A68" s="1"/>
       <c r="B68" s="2"/>
       <c r="E68" s="3"/>
@@ -3748,7 +3767,7 @@
       <c r="G68" s="2"/>
       <c r="H68" s="2"/>
     </row>
-    <row r="69" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:8">
       <c r="A69" s="1"/>
       <c r="B69" s="2"/>
       <c r="E69" s="3"/>
@@ -3756,7 +3775,7 @@
       <c r="G69" s="2"/>
       <c r="H69" s="2"/>
     </row>
-    <row r="70" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:8">
       <c r="A70" s="1"/>
       <c r="B70" s="2"/>
       <c r="E70" s="3"/>
@@ -3764,7 +3783,7 @@
       <c r="G70" s="2"/>
       <c r="H70" s="2"/>
     </row>
-    <row r="71" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:8">
       <c r="A71" s="1"/>
       <c r="B71" s="2"/>
       <c r="E71" s="3"/>
@@ -3772,7 +3791,7 @@
       <c r="G71" s="2"/>
       <c r="H71" s="2"/>
     </row>
-    <row r="72" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:8">
       <c r="A72" s="1"/>
       <c r="B72" s="2"/>
       <c r="E72" s="3"/>
@@ -3780,7 +3799,7 @@
       <c r="G72" s="2"/>
       <c r="H72" s="2"/>
     </row>
-    <row r="73" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:8">
       <c r="A73" s="1"/>
       <c r="B73" s="2"/>
       <c r="E73" s="3"/>
@@ -3788,7 +3807,7 @@
       <c r="G73" s="2"/>
       <c r="H73" s="2"/>
     </row>
-    <row r="74" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:8">
       <c r="A74" s="1"/>
       <c r="B74" s="2"/>
       <c r="E74" s="3"/>
@@ -3796,7 +3815,7 @@
       <c r="G74" s="2"/>
       <c r="H74" s="2"/>
     </row>
-    <row r="75" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:8">
       <c r="A75" s="1"/>
       <c r="B75" s="2"/>
       <c r="E75" s="3"/>
@@ -3804,7 +3823,7 @@
       <c r="G75" s="2"/>
       <c r="H75" s="2"/>
     </row>
-    <row r="76" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:8">
       <c r="A76" s="1"/>
       <c r="B76" s="2"/>
       <c r="E76" s="3"/>
@@ -3812,7 +3831,7 @@
       <c r="G76" s="2"/>
       <c r="H76" s="2"/>
     </row>
-    <row r="77" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:8">
       <c r="A77" s="1"/>
       <c r="B77" s="2"/>
       <c r="E77" s="3"/>
@@ -3820,7 +3839,7 @@
       <c r="G77" s="2"/>
       <c r="H77" s="2"/>
     </row>
-    <row r="78" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:8">
       <c r="A78" s="1"/>
       <c r="B78" s="2"/>
       <c r="E78" s="3"/>
@@ -3828,7 +3847,7 @@
       <c r="G78" s="2"/>
       <c r="H78" s="2"/>
     </row>
-    <row r="79" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:8">
       <c r="A79" s="1"/>
       <c r="B79" s="2"/>
       <c r="E79" s="3"/>
@@ -3836,7 +3855,7 @@
       <c r="G79" s="2"/>
       <c r="H79" s="2"/>
     </row>
-    <row r="80" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:8">
       <c r="A80" s="1"/>
       <c r="B80" s="2"/>
       <c r="E80" s="3"/>
@@ -3844,7 +3863,7 @@
       <c r="G80" s="2"/>
       <c r="H80" s="2"/>
     </row>
-    <row r="81" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:8">
       <c r="A81" s="1"/>
       <c r="B81" s="2"/>
       <c r="E81" s="3"/>
@@ -3852,7 +3871,7 @@
       <c r="G81" s="2"/>
       <c r="H81" s="2"/>
     </row>
-    <row r="82" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:8">
       <c r="A82" s="1"/>
       <c r="B82" s="2"/>
       <c r="E82" s="3"/>
@@ -3860,7 +3879,7 @@
       <c r="G82" s="2"/>
       <c r="H82" s="2"/>
     </row>
-    <row r="83" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:8">
       <c r="A83" s="1"/>
       <c r="B83" s="2"/>
       <c r="E83" s="3"/>
@@ -3868,7 +3887,7 @@
       <c r="G83" s="2"/>
       <c r="H83" s="2"/>
     </row>
-    <row r="84" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:8">
       <c r="A84" s="1"/>
       <c r="B84" s="2"/>
       <c r="E84" s="3"/>
@@ -3876,7 +3895,7 @@
       <c r="G84" s="2"/>
       <c r="H84" s="2"/>
     </row>
-    <row r="85" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:8">
       <c r="A85" s="1"/>
       <c r="B85" s="2"/>
       <c r="E85" s="3"/>
@@ -3884,7 +3903,7 @@
       <c r="G85" s="2"/>
       <c r="H85" s="2"/>
     </row>
-    <row r="86" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:8">
       <c r="A86" s="1"/>
       <c r="B86" s="2"/>
       <c r="E86" s="3"/>
@@ -3892,7 +3911,7 @@
       <c r="G86" s="2"/>
       <c r="H86" s="2"/>
     </row>
-    <row r="87" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:8">
       <c r="A87" s="1"/>
       <c r="B87" s="2"/>
       <c r="E87" s="3"/>
@@ -3900,7 +3919,7 @@
       <c r="G87" s="2"/>
       <c r="H87" s="2"/>
     </row>
-    <row r="88" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:8">
       <c r="A88" s="1"/>
       <c r="B88" s="2"/>
       <c r="E88" s="3"/>
@@ -3908,7 +3927,7 @@
       <c r="G88" s="2"/>
       <c r="H88" s="2"/>
     </row>
-    <row r="89" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:8">
       <c r="A89" s="1"/>
       <c r="B89" s="2"/>
       <c r="E89" s="3"/>
@@ -3916,7 +3935,7 @@
       <c r="G89" s="2"/>
       <c r="H89" s="2"/>
     </row>
-    <row r="90" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:8">
       <c r="A90" s="1"/>
       <c r="B90" s="2"/>
       <c r="E90" s="3"/>
@@ -3924,7 +3943,7 @@
       <c r="G90" s="2"/>
       <c r="H90" s="2"/>
     </row>
-    <row r="91" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:8">
       <c r="A91" s="1"/>
       <c r="B91" s="2"/>
       <c r="E91" s="3"/>
@@ -3932,7 +3951,7 @@
       <c r="G91" s="2"/>
       <c r="H91" s="2"/>
     </row>
-    <row r="92" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:8">
       <c r="A92" s="1"/>
       <c r="B92" s="2"/>
       <c r="E92" s="3"/>
@@ -3940,7 +3959,7 @@
       <c r="G92" s="2"/>
       <c r="H92" s="2"/>
     </row>
-    <row r="93" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:8">
       <c r="A93" s="1"/>
       <c r="B93" s="2"/>
       <c r="E93" s="3"/>
@@ -3948,7 +3967,7 @@
       <c r="G93" s="2"/>
       <c r="H93" s="2"/>
     </row>
-    <row r="94" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:8">
       <c r="A94" s="1"/>
       <c r="B94" s="2"/>
       <c r="E94" s="3"/>
@@ -3956,7 +3975,7 @@
       <c r="G94" s="2"/>
       <c r="H94" s="2"/>
     </row>
-    <row r="95" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:8">
       <c r="A95" s="1"/>
       <c r="B95" s="2"/>
       <c r="E95" s="3"/>
@@ -3964,7 +3983,7 @@
       <c r="G95" s="2"/>
       <c r="H95" s="2"/>
     </row>
-    <row r="96" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:8">
       <c r="A96" s="1"/>
       <c r="B96" s="2"/>
       <c r="E96" s="3"/>
@@ -3972,7 +3991,7 @@
       <c r="G96" s="2"/>
       <c r="H96" s="2"/>
     </row>
-    <row r="97" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:8">
       <c r="A97" s="1"/>
       <c r="B97" s="2"/>
       <c r="E97" s="3"/>
@@ -3980,7 +3999,7 @@
       <c r="G97" s="2"/>
       <c r="H97" s="2"/>
     </row>
-    <row r="98" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:8">
       <c r="A98" s="1"/>
       <c r="B98" s="2"/>
       <c r="E98" s="3"/>
@@ -3988,7 +4007,7 @@
       <c r="G98" s="2"/>
       <c r="H98" s="2"/>
     </row>
-    <row r="99" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:8">
       <c r="A99" s="1"/>
       <c r="B99" s="2"/>
       <c r="E99" s="3"/>
@@ -3996,7 +4015,7 @@
       <c r="G99" s="2"/>
       <c r="H99" s="2"/>
     </row>
-    <row r="100" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:8">
       <c r="A100" s="1"/>
       <c r="B100" s="2"/>
       <c r="E100" s="3"/>
@@ -4039,21 +4058,21 @@
       <selection activeCell="P21" sqref="P21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="19.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.5703125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.88671875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.88671875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19.44140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.5546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.5546875" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="9" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="17.85546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="17.88671875" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="17" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="19.140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="19.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" ht="15.6">
       <c r="A1" s="7" t="s">
         <v>8</v>
       </c>
@@ -4085,7 +4104,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10">
       <c r="A2" s="2"/>
       <c r="B2" s="8"/>
       <c r="D2" s="2"/>
@@ -4093,7 +4112,7 @@
       <c r="I2" s="8"/>
       <c r="J2" s="2"/>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10">
       <c r="A3" s="2"/>
       <c r="B3" s="8"/>
       <c r="D3" s="2"/>
@@ -4101,7 +4120,7 @@
       <c r="I3" s="8"/>
       <c r="J3" s="2"/>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10">
       <c r="A4" s="2"/>
       <c r="B4" s="8"/>
       <c r="D4" s="2"/>
@@ -4109,7 +4128,7 @@
       <c r="I4" s="8"/>
       <c r="J4" s="2"/>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10">
       <c r="A5" s="2"/>
       <c r="B5" s="8"/>
       <c r="D5" s="2"/>
@@ -4117,7 +4136,7 @@
       <c r="I5" s="8"/>
       <c r="J5" s="2"/>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10">
       <c r="A6" s="2"/>
       <c r="B6" s="8"/>
       <c r="D6" s="2"/>
@@ -4125,7 +4144,7 @@
       <c r="I6" s="8"/>
       <c r="J6" s="2"/>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10">
       <c r="A7" s="2"/>
       <c r="B7" s="8"/>
       <c r="D7" s="2"/>
@@ -4133,7 +4152,7 @@
       <c r="I7" s="8"/>
       <c r="J7" s="2"/>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10">
       <c r="A8" s="2"/>
       <c r="B8" s="8"/>
       <c r="D8" s="2"/>
@@ -4141,7 +4160,7 @@
       <c r="I8" s="8"/>
       <c r="J8" s="2"/>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10">
       <c r="A9" s="2"/>
       <c r="B9" s="8"/>
       <c r="D9" s="2"/>
@@ -4149,7 +4168,7 @@
       <c r="I9" s="8"/>
       <c r="J9" s="2"/>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:10">
       <c r="A10" s="2"/>
       <c r="B10" s="8"/>
       <c r="D10" s="2"/>
@@ -4157,7 +4176,7 @@
       <c r="I10" s="8"/>
       <c r="J10" s="2"/>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:10">
       <c r="A11" s="2"/>
       <c r="B11" s="8"/>
       <c r="D11" s="2"/>
@@ -4165,7 +4184,7 @@
       <c r="I11" s="8"/>
       <c r="J11" s="2"/>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:10">
       <c r="A12" s="2"/>
       <c r="B12" s="8"/>
       <c r="D12" s="2"/>
@@ -4173,7 +4192,7 @@
       <c r="I12" s="8"/>
       <c r="J12" s="2"/>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:10">
       <c r="A13" s="2"/>
       <c r="B13" s="8"/>
       <c r="D13" s="2"/>
@@ -4181,7 +4200,7 @@
       <c r="I13" s="8"/>
       <c r="J13" s="2"/>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:10">
       <c r="A14" s="2"/>
       <c r="B14" s="8"/>
       <c r="D14" s="2"/>
@@ -4189,7 +4208,7 @@
       <c r="I14" s="8"/>
       <c r="J14" s="2"/>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:10">
       <c r="A15" s="2"/>
       <c r="B15" s="8"/>
       <c r="D15" s="2"/>
@@ -4197,7 +4216,7 @@
       <c r="I15" s="8"/>
       <c r="J15" s="2"/>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:10">
       <c r="A16" s="2"/>
       <c r="B16" s="8"/>
       <c r="D16" s="2"/>
@@ -4205,7 +4224,7 @@
       <c r="I16" s="8"/>
       <c r="J16" s="2"/>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:10">
       <c r="A17" s="2"/>
       <c r="B17" s="8"/>
       <c r="D17" s="2"/>
@@ -4213,7 +4232,7 @@
       <c r="I17" s="8"/>
       <c r="J17" s="2"/>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:10">
       <c r="A18" s="2"/>
       <c r="B18" s="8"/>
       <c r="D18" s="2"/>
@@ -4221,7 +4240,7 @@
       <c r="I18" s="8"/>
       <c r="J18" s="2"/>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:10">
       <c r="A19" s="2"/>
       <c r="B19" s="8"/>
       <c r="D19" s="2"/>
@@ -4229,7 +4248,7 @@
       <c r="I19" s="8"/>
       <c r="J19" s="2"/>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:10">
       <c r="A20" s="2"/>
       <c r="B20" s="8"/>
       <c r="D20" s="2"/>
@@ -4237,7 +4256,7 @@
       <c r="I20" s="8"/>
       <c r="J20" s="2"/>
     </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:10">
       <c r="A21" s="2"/>
       <c r="B21" s="8"/>
       <c r="D21" s="2"/>
@@ -4245,7 +4264,7 @@
       <c r="I21" s="8"/>
       <c r="J21" s="2"/>
     </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:10">
       <c r="A22" s="2"/>
       <c r="B22" s="8"/>
       <c r="D22" s="2"/>
@@ -4253,7 +4272,7 @@
       <c r="I22" s="8"/>
       <c r="J22" s="2"/>
     </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:10">
       <c r="A23" s="2"/>
       <c r="B23" s="8"/>
       <c r="D23" s="2"/>
@@ -4261,7 +4280,7 @@
       <c r="I23" s="8"/>
       <c r="J23" s="2"/>
     </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:10">
       <c r="A24" s="2"/>
       <c r="B24" s="8"/>
       <c r="D24" s="2"/>
@@ -4269,7 +4288,7 @@
       <c r="I24" s="8"/>
       <c r="J24" s="2"/>
     </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:10">
       <c r="A25" s="2"/>
       <c r="B25" s="8"/>
       <c r="D25" s="2"/>
@@ -4277,7 +4296,7 @@
       <c r="I25" s="8"/>
       <c r="J25" s="2"/>
     </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:10">
       <c r="A26" s="2"/>
       <c r="B26" s="8"/>
       <c r="D26" s="2"/>
@@ -4285,7 +4304,7 @@
       <c r="I26" s="8"/>
       <c r="J26" s="2"/>
     </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:10">
       <c r="A27" s="2"/>
       <c r="B27" s="8"/>
       <c r="D27" s="2"/>
@@ -4293,7 +4312,7 @@
       <c r="I27" s="8"/>
       <c r="J27" s="2"/>
     </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:10">
       <c r="A28" s="2"/>
       <c r="B28" s="8"/>
       <c r="D28" s="2"/>
@@ -4301,7 +4320,7 @@
       <c r="I28" s="8"/>
       <c r="J28" s="2"/>
     </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:10">
       <c r="A29" s="2"/>
       <c r="B29" s="8"/>
       <c r="D29" s="2"/>
@@ -4309,7 +4328,7 @@
       <c r="I29" s="8"/>
       <c r="J29" s="2"/>
     </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:10">
       <c r="A30" s="2"/>
       <c r="B30" s="8"/>
       <c r="D30" s="2"/>
@@ -4317,7 +4336,7 @@
       <c r="I30" s="8"/>
       <c r="J30" s="2"/>
     </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:10">
       <c r="A31" s="2"/>
       <c r="B31" s="8"/>
       <c r="D31" s="2"/>
@@ -4325,7 +4344,7 @@
       <c r="I31" s="8"/>
       <c r="J31" s="2"/>
     </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:10">
       <c r="A32" s="2"/>
       <c r="B32" s="8"/>
       <c r="D32" s="2"/>
@@ -4333,7 +4352,7 @@
       <c r="I32" s="8"/>
       <c r="J32" s="2"/>
     </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:10">
       <c r="A33" s="2"/>
       <c r="B33" s="8"/>
       <c r="D33" s="2"/>
@@ -4341,7 +4360,7 @@
       <c r="I33" s="8"/>
       <c r="J33" s="2"/>
     </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:10">
       <c r="A34" s="2"/>
       <c r="B34" s="8"/>
       <c r="D34" s="2"/>
@@ -4349,7 +4368,7 @@
       <c r="I34" s="8"/>
       <c r="J34" s="2"/>
     </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:10">
       <c r="A35" s="2"/>
       <c r="B35" s="8"/>
       <c r="D35" s="2"/>
@@ -4357,7 +4376,7 @@
       <c r="I35" s="8"/>
       <c r="J35" s="2"/>
     </row>
-    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:10">
       <c r="A36" s="2"/>
       <c r="B36" s="8"/>
       <c r="D36" s="2"/>
@@ -4365,7 +4384,7 @@
       <c r="I36" s="8"/>
       <c r="J36" s="2"/>
     </row>
-    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:10">
       <c r="A37" s="2"/>
       <c r="B37" s="8"/>
       <c r="D37" s="2"/>
@@ -4373,7 +4392,7 @@
       <c r="I37" s="8"/>
       <c r="J37" s="2"/>
     </row>
-    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:10">
       <c r="A38" s="2"/>
       <c r="B38" s="8"/>
       <c r="D38" s="2"/>
@@ -4381,7 +4400,7 @@
       <c r="I38" s="8"/>
       <c r="J38" s="2"/>
     </row>
-    <row r="39" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:10">
       <c r="A39" s="2"/>
       <c r="B39" s="8"/>
       <c r="D39" s="2"/>
@@ -4389,7 +4408,7 @@
       <c r="I39" s="8"/>
       <c r="J39" s="2"/>
     </row>
-    <row r="40" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:10">
       <c r="A40" s="2"/>
       <c r="B40" s="8"/>
       <c r="D40" s="2"/>
@@ -4397,7 +4416,7 @@
       <c r="I40" s="8"/>
       <c r="J40" s="2"/>
     </row>
-    <row r="41" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:10">
       <c r="A41" s="2"/>
       <c r="B41" s="8"/>
       <c r="D41" s="2"/>
@@ -4405,7 +4424,7 @@
       <c r="I41" s="8"/>
       <c r="J41" s="2"/>
     </row>
-    <row r="42" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:10">
       <c r="A42" s="2"/>
       <c r="B42" s="8"/>
       <c r="D42" s="2"/>
@@ -4413,7 +4432,7 @@
       <c r="I42" s="8"/>
       <c r="J42" s="2"/>
     </row>
-    <row r="43" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:10">
       <c r="A43" s="2"/>
       <c r="B43" s="8"/>
       <c r="D43" s="2"/>
@@ -4421,7 +4440,7 @@
       <c r="I43" s="8"/>
       <c r="J43" s="2"/>
     </row>
-    <row r="44" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:10">
       <c r="A44" s="2"/>
       <c r="B44" s="8"/>
       <c r="D44" s="2"/>
@@ -4429,7 +4448,7 @@
       <c r="I44" s="8"/>
       <c r="J44" s="2"/>
     </row>
-    <row r="45" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:10">
       <c r="A45" s="2"/>
       <c r="B45" s="8"/>
       <c r="D45" s="2"/>
@@ -4437,7 +4456,7 @@
       <c r="I45" s="8"/>
       <c r="J45" s="2"/>
     </row>
-    <row r="46" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:10">
       <c r="A46" s="2"/>
       <c r="B46" s="8"/>
       <c r="D46" s="2"/>
@@ -4445,7 +4464,7 @@
       <c r="I46" s="8"/>
       <c r="J46" s="2"/>
     </row>
-    <row r="47" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:10">
       <c r="A47" s="2"/>
       <c r="B47" s="8"/>
       <c r="D47" s="2"/>
@@ -4453,7 +4472,7 @@
       <c r="I47" s="8"/>
       <c r="J47" s="2"/>
     </row>
-    <row r="48" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:10">
       <c r="A48" s="2"/>
       <c r="B48" s="8"/>
       <c r="D48" s="2"/>
@@ -4461,7 +4480,7 @@
       <c r="I48" s="8"/>
       <c r="J48" s="2"/>
     </row>
-    <row r="49" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:10">
       <c r="A49" s="2"/>
       <c r="B49" s="8"/>
       <c r="D49" s="2"/>
@@ -4469,7 +4488,7 @@
       <c r="I49" s="8"/>
       <c r="J49" s="2"/>
     </row>
-    <row r="50" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:10">
       <c r="A50" s="2"/>
       <c r="B50" s="8"/>
       <c r="D50" s="2"/>
@@ -4477,7 +4496,7 @@
       <c r="I50" s="8"/>
       <c r="J50" s="2"/>
     </row>
-    <row r="51" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:10">
       <c r="A51" s="2"/>
       <c r="B51" s="8"/>
       <c r="D51" s="2"/>
@@ -4485,7 +4504,7 @@
       <c r="I51" s="8"/>
       <c r="J51" s="2"/>
     </row>
-    <row r="52" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:10">
       <c r="A52" s="2"/>
       <c r="B52" s="8"/>
       <c r="D52" s="2"/>
@@ -4493,7 +4512,7 @@
       <c r="I52" s="8"/>
       <c r="J52" s="2"/>
     </row>
-    <row r="53" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:10">
       <c r="A53" s="2"/>
       <c r="B53" s="8"/>
       <c r="D53" s="2"/>
@@ -4501,7 +4520,7 @@
       <c r="I53" s="8"/>
       <c r="J53" s="2"/>
     </row>
-    <row r="54" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:10">
       <c r="A54" s="2"/>
       <c r="B54" s="8"/>
       <c r="D54" s="2"/>
@@ -4509,7 +4528,7 @@
       <c r="I54" s="8"/>
       <c r="J54" s="2"/>
     </row>
-    <row r="55" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:10">
       <c r="A55" s="2"/>
       <c r="B55" s="8"/>
       <c r="D55" s="2"/>
@@ -4517,7 +4536,7 @@
       <c r="I55" s="8"/>
       <c r="J55" s="2"/>
     </row>
-    <row r="56" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:10">
       <c r="A56" s="2"/>
       <c r="B56" s="8"/>
       <c r="D56" s="2"/>
@@ -4525,7 +4544,7 @@
       <c r="I56" s="8"/>
       <c r="J56" s="2"/>
     </row>
-    <row r="57" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:10">
       <c r="A57" s="2"/>
       <c r="B57" s="8"/>
       <c r="D57" s="2"/>
@@ -4533,7 +4552,7 @@
       <c r="I57" s="8"/>
       <c r="J57" s="2"/>
     </row>
-    <row r="58" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:10">
       <c r="A58" s="2"/>
       <c r="B58" s="8"/>
       <c r="D58" s="2"/>
@@ -4541,7 +4560,7 @@
       <c r="I58" s="8"/>
       <c r="J58" s="2"/>
     </row>
-    <row r="59" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:10">
       <c r="A59" s="2"/>
       <c r="B59" s="8"/>
       <c r="D59" s="2"/>
@@ -4549,7 +4568,7 @@
       <c r="I59" s="8"/>
       <c r="J59" s="2"/>
     </row>
-    <row r="60" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:10">
       <c r="A60" s="2"/>
       <c r="B60" s="8"/>
       <c r="D60" s="2"/>
@@ -4557,7 +4576,7 @@
       <c r="I60" s="8"/>
       <c r="J60" s="2"/>
     </row>
-    <row r="61" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:10">
       <c r="A61" s="2"/>
       <c r="B61" s="8"/>
       <c r="D61" s="2"/>
@@ -4565,7 +4584,7 @@
       <c r="I61" s="8"/>
       <c r="J61" s="2"/>
     </row>
-    <row r="62" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:10">
       <c r="A62" s="2"/>
       <c r="B62" s="8"/>
       <c r="D62" s="2"/>
@@ -4573,7 +4592,7 @@
       <c r="I62" s="8"/>
       <c r="J62" s="2"/>
     </row>
-    <row r="63" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:10">
       <c r="A63" s="2"/>
       <c r="B63" s="8"/>
       <c r="D63" s="2"/>
@@ -4581,7 +4600,7 @@
       <c r="I63" s="8"/>
       <c r="J63" s="2"/>
     </row>
-    <row r="64" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:10">
       <c r="A64" s="2"/>
       <c r="B64" s="8"/>
       <c r="D64" s="2"/>
@@ -4589,7 +4608,7 @@
       <c r="I64" s="8"/>
       <c r="J64" s="2"/>
     </row>
-    <row r="65" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:10">
       <c r="A65" s="2"/>
       <c r="B65" s="8"/>
       <c r="D65" s="2"/>
@@ -4597,7 +4616,7 @@
       <c r="I65" s="8"/>
       <c r="J65" s="2"/>
     </row>
-    <row r="66" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:10">
       <c r="A66" s="2"/>
       <c r="B66" s="8"/>
       <c r="D66" s="2"/>
@@ -4605,7 +4624,7 @@
       <c r="I66" s="8"/>
       <c r="J66" s="2"/>
     </row>
-    <row r="67" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:10">
       <c r="A67" s="2"/>
       <c r="B67" s="8"/>
       <c r="D67" s="2"/>
@@ -4613,7 +4632,7 @@
       <c r="I67" s="8"/>
       <c r="J67" s="2"/>
     </row>
-    <row r="68" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:10">
       <c r="A68" s="2"/>
       <c r="B68" s="8"/>
       <c r="D68" s="2"/>
@@ -4621,7 +4640,7 @@
       <c r="I68" s="8"/>
       <c r="J68" s="2"/>
     </row>
-    <row r="69" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:10">
       <c r="A69" s="2"/>
       <c r="B69" s="8"/>
       <c r="D69" s="2"/>
@@ -4629,7 +4648,7 @@
       <c r="I69" s="8"/>
       <c r="J69" s="2"/>
     </row>
-    <row r="70" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:10">
       <c r="A70" s="2"/>
       <c r="B70" s="8"/>
       <c r="D70" s="2"/>
@@ -4637,7 +4656,7 @@
       <c r="I70" s="8"/>
       <c r="J70" s="2"/>
     </row>
-    <row r="71" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:10">
       <c r="A71" s="2"/>
       <c r="B71" s="8"/>
       <c r="D71" s="2"/>
@@ -4645,7 +4664,7 @@
       <c r="I71" s="8"/>
       <c r="J71" s="2"/>
     </row>
-    <row r="72" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:10">
       <c r="A72" s="2"/>
       <c r="B72" s="8"/>
       <c r="D72" s="2"/>
@@ -4653,7 +4672,7 @@
       <c r="I72" s="8"/>
       <c r="J72" s="2"/>
     </row>
-    <row r="73" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:10">
       <c r="A73" s="2"/>
       <c r="B73" s="8"/>
       <c r="D73" s="2"/>
@@ -4661,7 +4680,7 @@
       <c r="I73" s="8"/>
       <c r="J73" s="2"/>
     </row>
-    <row r="74" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:10">
       <c r="A74" s="2"/>
       <c r="B74" s="8"/>
       <c r="D74" s="2"/>
@@ -4669,7 +4688,7 @@
       <c r="I74" s="8"/>
       <c r="J74" s="2"/>
     </row>
-    <row r="75" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:10">
       <c r="A75" s="2"/>
       <c r="B75" s="8"/>
       <c r="D75" s="2"/>
@@ -4677,7 +4696,7 @@
       <c r="I75" s="8"/>
       <c r="J75" s="2"/>
     </row>
-    <row r="76" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:10">
       <c r="A76" s="2"/>
       <c r="B76" s="8"/>
       <c r="D76" s="2"/>
@@ -4685,7 +4704,7 @@
       <c r="I76" s="8"/>
       <c r="J76" s="2"/>
     </row>
-    <row r="77" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:10">
       <c r="A77" s="2"/>
       <c r="B77" s="8"/>
       <c r="D77" s="2"/>
@@ -4693,7 +4712,7 @@
       <c r="I77" s="8"/>
       <c r="J77" s="2"/>
     </row>
-    <row r="78" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:10">
       <c r="A78" s="2"/>
       <c r="B78" s="8"/>
       <c r="D78" s="2"/>
@@ -4701,7 +4720,7 @@
       <c r="I78" s="8"/>
       <c r="J78" s="2"/>
     </row>
-    <row r="79" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:10">
       <c r="A79" s="2"/>
       <c r="B79" s="8"/>
       <c r="D79" s="2"/>
@@ -4709,7 +4728,7 @@
       <c r="I79" s="8"/>
       <c r="J79" s="2"/>
     </row>
-    <row r="80" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:10">
       <c r="A80" s="2"/>
       <c r="B80" s="8"/>
       <c r="D80" s="2"/>
@@ -4717,7 +4736,7 @@
       <c r="I80" s="8"/>
       <c r="J80" s="2"/>
     </row>
-    <row r="81" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:10">
       <c r="A81" s="2"/>
       <c r="B81" s="8"/>
       <c r="D81" s="2"/>
@@ -4725,7 +4744,7 @@
       <c r="I81" s="8"/>
       <c r="J81" s="2"/>
     </row>
-    <row r="82" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:10">
       <c r="A82" s="2"/>
       <c r="B82" s="8"/>
       <c r="D82" s="2"/>
@@ -4733,7 +4752,7 @@
       <c r="I82" s="8"/>
       <c r="J82" s="2"/>
     </row>
-    <row r="83" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:10">
       <c r="A83" s="2"/>
       <c r="B83" s="8"/>
       <c r="D83" s="2"/>
@@ -4741,7 +4760,7 @@
       <c r="I83" s="8"/>
       <c r="J83" s="2"/>
     </row>
-    <row r="84" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:10">
       <c r="A84" s="2"/>
       <c r="B84" s="8"/>
       <c r="D84" s="2"/>
@@ -4749,7 +4768,7 @@
       <c r="I84" s="8"/>
       <c r="J84" s="2"/>
     </row>
-    <row r="85" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:10">
       <c r="A85" s="2"/>
       <c r="B85" s="8"/>
       <c r="D85" s="2"/>
@@ -4757,7 +4776,7 @@
       <c r="I85" s="8"/>
       <c r="J85" s="2"/>
     </row>
-    <row r="86" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:10">
       <c r="A86" s="2"/>
       <c r="B86" s="8"/>
       <c r="D86" s="2"/>
@@ -4765,7 +4784,7 @@
       <c r="I86" s="8"/>
       <c r="J86" s="2"/>
     </row>
-    <row r="87" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:10">
       <c r="A87" s="2"/>
       <c r="B87" s="8"/>
       <c r="D87" s="2"/>
@@ -4773,7 +4792,7 @@
       <c r="I87" s="8"/>
       <c r="J87" s="2"/>
     </row>
-    <row r="88" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:10">
       <c r="A88" s="2"/>
       <c r="B88" s="8"/>
       <c r="D88" s="2"/>
@@ -4781,7 +4800,7 @@
       <c r="I88" s="8"/>
       <c r="J88" s="2"/>
     </row>
-    <row r="89" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:10">
       <c r="A89" s="2"/>
       <c r="B89" s="8"/>
       <c r="D89" s="2"/>
@@ -4789,7 +4808,7 @@
       <c r="I89" s="8"/>
       <c r="J89" s="2"/>
     </row>
-    <row r="90" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:10">
       <c r="A90" s="2"/>
       <c r="B90" s="8"/>
       <c r="D90" s="2"/>
@@ -4797,7 +4816,7 @@
       <c r="I90" s="8"/>
       <c r="J90" s="2"/>
     </row>
-    <row r="91" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:10">
       <c r="A91" s="2"/>
       <c r="B91" s="8"/>
       <c r="D91" s="2"/>
@@ -4805,7 +4824,7 @@
       <c r="I91" s="8"/>
       <c r="J91" s="2"/>
     </row>
-    <row r="92" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:10">
       <c r="A92" s="2"/>
       <c r="B92" s="8"/>
       <c r="D92" s="2"/>
@@ -4813,7 +4832,7 @@
       <c r="I92" s="8"/>
       <c r="J92" s="2"/>
     </row>
-    <row r="93" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:10">
       <c r="A93" s="2"/>
       <c r="B93" s="8"/>
       <c r="D93" s="2"/>
@@ -4821,7 +4840,7 @@
       <c r="I93" s="8"/>
       <c r="J93" s="2"/>
     </row>
-    <row r="94" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:10">
       <c r="A94" s="2"/>
       <c r="B94" s="8"/>
       <c r="D94" s="2"/>
@@ -4829,7 +4848,7 @@
       <c r="I94" s="8"/>
       <c r="J94" s="2"/>
     </row>
-    <row r="95" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:10">
       <c r="A95" s="2"/>
       <c r="B95" s="8"/>
       <c r="D95" s="2"/>
@@ -4837,7 +4856,7 @@
       <c r="I95" s="8"/>
       <c r="J95" s="2"/>
     </row>
-    <row r="96" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:10">
       <c r="A96" s="2"/>
       <c r="B96" s="8"/>
       <c r="D96" s="2"/>
@@ -4845,7 +4864,7 @@
       <c r="I96" s="8"/>
       <c r="J96" s="2"/>
     </row>
-    <row r="97" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:10">
       <c r="A97" s="2"/>
       <c r="B97" s="8"/>
       <c r="D97" s="2"/>
@@ -4853,7 +4872,7 @@
       <c r="I97" s="8"/>
       <c r="J97" s="2"/>
     </row>
-    <row r="98" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:10">
       <c r="A98" s="2"/>
       <c r="B98" s="8"/>
       <c r="D98" s="2"/>
@@ -4861,7 +4880,7 @@
       <c r="I98" s="8"/>
       <c r="J98" s="2"/>
     </row>
-    <row r="99" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:10">
       <c r="A99" s="2"/>
       <c r="B99" s="8"/>
       <c r="D99" s="2"/>
@@ -4869,7 +4888,7 @@
       <c r="I99" s="8"/>
       <c r="J99" s="2"/>
     </row>
-    <row r="100" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:10">
       <c r="A100" s="2"/>
       <c r="B100" s="8"/>
       <c r="D100" s="2"/>

</xml_diff>

<commit_message>
Login implemented with DB
</commit_message>
<xml_diff>
--- a/PR&IR.xlsx
+++ b/PR&IR.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\avichal avneel nath\Documents\Semester 7\CS415\A3\CS415_A3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E40B6A96-FAF6-4C15-B5A0-E2C969B71FD7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B56B9EB-9104-48BD-945A-B6FAC90D9711}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{BFA1E21A-08FA-4F02-8C25-33C81C8EE970}"/>
   </bookViews>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="149" uniqueCount="87">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="153" uniqueCount="90">
   <si>
     <t>Date</t>
   </si>
@@ -326,6 +326,17 @@
   <si>
     <t>Database seeding (populating with initial data).
 Replacing mock data in frontend routes with actual database queries.</t>
+  </si>
+  <si>
+    <t>Added grade recheck pages.
+Added students page that displays their enrollment with add and change grade and search functionalities.
+Added grade change and add new grade pages.</t>
+  </si>
+  <si>
+    <t>Continue docker and doing backend</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Not interested </t>
   </si>
 </sst>
 </file>
@@ -377,7 +388,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -392,7 +403,6 @@
     </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="2" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -1077,7 +1087,7 @@
   <dimension ref="A1:H28"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="H14" sqref="H14"/>
+      <selection activeCell="F18" sqref="F18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1382,7 +1392,7 @@
       <c r="F13">
         <v>2</v>
       </c>
-      <c r="G13" s="12" t="s">
+      <c r="G13" t="s">
         <v>84</v>
       </c>
     </row>
@@ -1402,7 +1412,7 @@
       <c r="F14">
         <v>4</v>
       </c>
-      <c r="G14" s="13" t="s">
+      <c r="G14" s="12" t="s">
         <v>86</v>
       </c>
     </row>
@@ -2264,12 +2274,12 @@
   <dimension ref="A1:H100"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.42578125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="17.28515625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="27.85546875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="9.7109375" bestFit="1" customWidth="1"/>
@@ -2461,12 +2471,29 @@
         <v>54</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A8" s="1"/>
+    <row r="8" spans="1:8" ht="105" x14ac:dyDescent="0.25">
+      <c r="A8" s="1">
+        <v>45798</v>
+      </c>
       <c r="B8" s="2"/>
-      <c r="E8" s="3"/>
-      <c r="G8" s="2"/>
-      <c r="H8" s="2"/>
+      <c r="C8" s="9" t="s">
+        <v>87</v>
+      </c>
+      <c r="D8" t="s">
+        <v>17</v>
+      </c>
+      <c r="E8" s="3">
+        <v>1</v>
+      </c>
+      <c r="F8" s="10">
+        <v>4</v>
+      </c>
+      <c r="G8" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="H8" s="2" t="s">
+        <v>89</v>
+      </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="1"/>
@@ -3131,7 +3158,7 @@
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <ignoredErrors>
-    <ignoredError sqref="D8:D100" listDataValidation="1"/>
+    <ignoredError sqref="D9:D100" listDataValidation="1"/>
   </ignoredErrors>
   <tableParts count="1">
     <tablePart r:id="rId1"/>

</xml_diff>

<commit_message>
Add/update progress report for 22/05/2025 Thur by Shivya
</commit_message>
<xml_diff>
--- a/PR&IR.xlsx
+++ b/PR&IR.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SHIVYA KUMAR\Desktop\new415\CS415_A3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A5A0D8D-6F80-4613-809E-3598F48933D6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7011CDF0-3654-4B83-A767-067FCF770A1C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{BFA1E21A-08FA-4F02-8C25-33C81C8EE970}"/>
   </bookViews>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="160" uniqueCount="93">
   <si>
     <t>Date</t>
   </si>
@@ -340,6 +340,12 @@
   </si>
   <si>
     <t>interated jayshils feild code for student profile with mine. Added photo icon in the student profile page. Pulled jayshils code.</t>
+  </si>
+  <si>
+    <t>Integrated jayshils login code in my StudentService</t>
+  </si>
+  <si>
+    <t>Need 2 days time to study for cs310 PLEASEEEEEEEEEEEEEEEEEEEEE</t>
   </si>
 </sst>
 </file>
@@ -1495,13 +1501,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3BDA6702-5DDF-42FB-988E-13FBEB26F5C9}">
   <dimension ref="A1:H100"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="G8" sqref="G8"/>
+    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="102" zoomScaleNormal="102" workbookViewId="0">
+      <selection activeCell="H10" sqref="H10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="10.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16.109375" customWidth="1"/>
     <col min="2" max="2" width="17.33203125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="93.109375" customWidth="1"/>
     <col min="4" max="4" width="10.5546875" customWidth="1"/>
@@ -1710,10 +1716,28 @@
       <c r="H8" s="2"/>
     </row>
     <row r="9" spans="1:8">
-      <c r="A9" s="8"/>
-      <c r="B9" s="2"/>
+      <c r="A9" s="8">
+        <v>45799</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="C9" t="s">
+        <v>91</v>
+      </c>
+      <c r="D9" t="s">
+        <v>17</v>
+      </c>
+      <c r="E9">
+        <v>100</v>
+      </c>
+      <c r="F9">
+        <v>8</v>
+      </c>
       <c r="G9" s="2"/>
-      <c r="H9" s="2"/>
+      <c r="H9" s="2" t="s">
+        <v>92</v>
+      </c>
     </row>
     <row r="10" spans="1:8">
       <c r="A10" s="8"/>
@@ -2280,7 +2304,7 @@
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <ignoredErrors>
-    <ignoredError sqref="D9:D100" listDataValidation="1"/>
+    <ignoredError sqref="D10:D100" listDataValidation="1"/>
   </ignoredErrors>
   <tableParts count="1">
     <tablePart r:id="rId1"/>

</xml_diff>

<commit_message>
Updated progress report for May 22 for Avichal
</commit_message>
<xml_diff>
--- a/PR&IR.xlsx
+++ b/PR&IR.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28623"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SHIVYA KUMAR\Desktop\new415\CS415_A3\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\avichal avneel nath\Documents\Semester 7\CS415\A3\CS415_A3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7011CDF0-3654-4B83-A767-067FCF770A1C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF4C5E19-B462-46FA-9470-AAC7E0CCEE8D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{BFA1E21A-08FA-4F02-8C25-33C81C8EE970}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{BFA1E21A-08FA-4F02-8C25-33C81C8EE970}"/>
   </bookViews>
   <sheets>
     <sheet name="Avichal" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="160" uniqueCount="93">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="163" uniqueCount="95">
   <si>
     <t>Date</t>
   </si>
@@ -347,6 +347,12 @@
   <si>
     <t>Need 2 days time to study for cs310 PLEASEEEEEEEEEEEEEEEEEEEEE</t>
   </si>
+  <si>
+    <t>fixed the Program model's primary key and adjusted relationships in model.py. The seed_db.py script was updated to ensure correct program and subprogram seeding order and linkage. Database pathing was made robust, creating necessary directories. Unicode errors were resolved by specifying UTF-8 encoding for the JSON file. Finally, data loading for all entities improved with better ID handling and fallbacks.</t>
+  </si>
+  <si>
+    <t>Link fronted with Backend</t>
+  </si>
 </sst>
 </file>
 
@@ -356,7 +362,7 @@
     <numFmt numFmtId="164" formatCode="h"/>
     <numFmt numFmtId="165" formatCode="d/mm/yyyy;@"/>
   </numFmts>
-  <fonts count="3">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1095,30 +1101,30 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{37EAA098-74C6-4411-B7E2-26AD2DCBC3F0}">
   <dimension ref="A1:H28"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="H14" sqref="H14"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.44140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.5546875" style="2" customWidth="1"/>
+    <col min="1" max="1" width="10.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.5703125" style="2" customWidth="1"/>
     <col min="3" max="3" width="58" customWidth="1"/>
-    <col min="5" max="5" width="13.109375" style="3" customWidth="1"/>
-    <col min="6" max="6" width="20.88671875" style="4" customWidth="1"/>
-    <col min="7" max="7" width="34.88671875" style="2" customWidth="1"/>
-    <col min="8" max="8" width="43.44140625" style="2" customWidth="1"/>
-    <col min="11" max="11" width="9.109375" customWidth="1"/>
-    <col min="12" max="12" width="13.33203125" customWidth="1"/>
-    <col min="13" max="13" width="11.44140625" customWidth="1"/>
-    <col min="14" max="14" width="17.44140625" customWidth="1"/>
-    <col min="16" max="16" width="9.109375" customWidth="1"/>
-    <col min="18" max="18" width="16.5546875" customWidth="1"/>
-    <col min="19" max="19" width="14.6640625" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="16.88671875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.140625" style="3" customWidth="1"/>
+    <col min="6" max="6" width="20.85546875" style="4" customWidth="1"/>
+    <col min="7" max="7" width="34.85546875" style="2" customWidth="1"/>
+    <col min="8" max="8" width="43.42578125" style="2" customWidth="1"/>
+    <col min="11" max="11" width="9.140625" customWidth="1"/>
+    <col min="12" max="12" width="13.28515625" customWidth="1"/>
+    <col min="13" max="13" width="11.42578125" customWidth="1"/>
+    <col min="14" max="14" width="17.42578125" customWidth="1"/>
+    <col min="16" max="16" width="9.140625" customWidth="1"/>
+    <col min="18" max="18" width="16.5703125" customWidth="1"/>
+    <col min="19" max="19" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="16.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="15.6">
+    <row r="1" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
@@ -1144,7 +1150,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:8">
+    <row r="2" spans="1:8" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A2" s="1">
         <v>45786</v>
       </c>
@@ -1170,7 +1176,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="3" spans="1:8" ht="115.2">
+    <row r="3" spans="1:8" ht="120" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>45787</v>
       </c>
@@ -1193,7 +1199,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="4" spans="1:8">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>45788</v>
       </c>
@@ -1213,7 +1219,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="5" spans="1:8" ht="76.5" customHeight="1">
+    <row r="5" spans="1:8" ht="76.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>45789</v>
       </c>
@@ -1236,7 +1242,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="6" spans="1:8">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>45790</v>
       </c>
@@ -1259,7 +1265,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="7" spans="1:8">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>45791</v>
       </c>
@@ -1282,7 +1288,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="8" spans="1:8">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>45792</v>
       </c>
@@ -1305,7 +1311,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="9" spans="1:8">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>45793</v>
       </c>
@@ -1325,7 +1331,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="10" spans="1:8">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>45794</v>
       </c>
@@ -1345,7 +1351,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="11" spans="1:8">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>45795</v>
       </c>
@@ -1365,7 +1371,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="12" spans="1:8">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <v>45796</v>
       </c>
@@ -1385,7 +1391,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="13" spans="1:8" ht="68.25" customHeight="1">
+    <row r="13" spans="1:8" ht="68.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <v>45797</v>
       </c>
@@ -1405,7 +1411,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="14" spans="1:8" ht="60" customHeight="1">
+    <row r="14" spans="1:8" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
         <v>45798</v>
       </c>
@@ -1425,48 +1431,64 @@
         <v>86</v>
       </c>
     </row>
-    <row r="15" spans="1:8">
-      <c r="E15"/>
-      <c r="F15"/>
-    </row>
-    <row r="16" spans="1:8">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A15" s="1">
+        <v>45799</v>
+      </c>
+      <c r="C15" t="s">
+        <v>93</v>
+      </c>
+      <c r="D15" t="s">
+        <v>17</v>
+      </c>
+      <c r="E15">
+        <v>100</v>
+      </c>
+      <c r="F15">
+        <v>3</v>
+      </c>
+      <c r="G15" s="2" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="E16"/>
       <c r="F16"/>
     </row>
-    <row r="17" spans="6:6">
+    <row r="17" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F17"/>
     </row>
-    <row r="18" spans="6:6">
+    <row r="18" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F18"/>
     </row>
-    <row r="19" spans="6:6">
+    <row r="19" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F19"/>
     </row>
-    <row r="20" spans="6:6">
+    <row r="20" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F20"/>
     </row>
-    <row r="21" spans="6:6">
+    <row r="21" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F21"/>
     </row>
-    <row r="22" spans="6:6">
+    <row r="22" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F22"/>
     </row>
-    <row r="23" spans="6:6">
+    <row r="23" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F23"/>
     </row>
-    <row r="24" spans="6:6">
+    <row r="24" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F24"/>
     </row>
-    <row r="25" spans="6:6">
+    <row r="25" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F25"/>
     </row>
-    <row r="26" spans="6:6">
+    <row r="26" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F26"/>
     </row>
-    <row r="27" spans="6:6">
+    <row r="27" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F27"/>
     </row>
-    <row r="28" spans="6:6">
+    <row r="28" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F28"/>
     </row>
   </sheetData>
@@ -1489,7 +1511,7 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
   <ignoredErrors>
-    <ignoredError sqref="D15:D16" listDataValidation="1"/>
+    <ignoredError sqref="D16" listDataValidation="1"/>
   </ignoredErrors>
   <tableParts count="1">
     <tablePart r:id="rId2"/>
@@ -1501,23 +1523,23 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3BDA6702-5DDF-42FB-988E-13FBEB26F5C9}">
   <dimension ref="A1:H100"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="102" zoomScaleNormal="102" workbookViewId="0">
+    <sheetView topLeftCell="A2" zoomScale="102" zoomScaleNormal="102" workbookViewId="0">
       <selection activeCell="H10" sqref="H10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="16.109375" customWidth="1"/>
-    <col min="2" max="2" width="17.33203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="93.109375" customWidth="1"/>
-    <col min="4" max="4" width="10.5546875" customWidth="1"/>
-    <col min="5" max="5" width="14.88671875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14.33203125" customWidth="1"/>
-    <col min="7" max="7" width="92.88671875" customWidth="1"/>
-    <col min="8" max="8" width="82.44140625" customWidth="1"/>
+    <col min="1" max="1" width="16.140625" customWidth="1"/>
+    <col min="2" max="2" width="17.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="93.140625" customWidth="1"/>
+    <col min="4" max="4" width="10.5703125" customWidth="1"/>
+    <col min="5" max="5" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.28515625" customWidth="1"/>
+    <col min="7" max="7" width="92.85546875" customWidth="1"/>
+    <col min="8" max="8" width="82.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="15.6">
+    <row r="1" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
@@ -1543,7 +1565,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:8">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="8">
         <v>45786</v>
       </c>
@@ -1569,7 +1591,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="3" spans="1:8">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="8">
         <v>45787</v>
       </c>
@@ -1595,7 +1617,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="4" spans="1:8">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="8">
         <v>45789</v>
       </c>
@@ -1619,7 +1641,7 @@
       </c>
       <c r="H4" s="2"/>
     </row>
-    <row r="5" spans="1:8">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="8">
         <v>45790</v>
       </c>
@@ -1643,7 +1665,7 @@
       </c>
       <c r="H5" s="2"/>
     </row>
-    <row r="6" spans="1:8">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="8">
         <v>45791</v>
       </c>
@@ -1669,7 +1691,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="7" spans="1:8">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="8">
         <v>45795</v>
       </c>
@@ -1693,7 +1715,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="8" spans="1:8">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="8">
         <v>45798</v>
       </c>
@@ -1715,7 +1737,7 @@
       <c r="G8" s="2"/>
       <c r="H8" s="2"/>
     </row>
-    <row r="9" spans="1:8">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="8">
         <v>45799</v>
       </c>
@@ -1739,547 +1761,547 @@
         <v>92</v>
       </c>
     </row>
-    <row r="10" spans="1:8">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="8"/>
       <c r="B10" s="2"/>
       <c r="G10" s="2"/>
       <c r="H10" s="2"/>
     </row>
-    <row r="11" spans="1:8">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="8"/>
       <c r="B11" s="2"/>
       <c r="G11" s="2"/>
       <c r="H11" s="2"/>
     </row>
-    <row r="12" spans="1:8">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="8"/>
       <c r="B12" s="2"/>
       <c r="G12" s="2"/>
       <c r="H12" s="2"/>
     </row>
-    <row r="13" spans="1:8">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="8"/>
       <c r="B13" s="2"/>
       <c r="G13" s="2"/>
       <c r="H13" s="2"/>
     </row>
-    <row r="14" spans="1:8">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" s="8"/>
       <c r="B14" s="2"/>
       <c r="G14" s="2"/>
       <c r="H14" s="2"/>
     </row>
-    <row r="15" spans="1:8">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" s="8"/>
       <c r="B15" s="2"/>
       <c r="G15" s="2"/>
       <c r="H15" s="2"/>
     </row>
-    <row r="16" spans="1:8">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" s="8"/>
       <c r="B16" s="2"/>
       <c r="G16" s="2"/>
       <c r="H16" s="2"/>
     </row>
-    <row r="17" spans="1:8">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" s="8"/>
       <c r="B17" s="2"/>
       <c r="G17" s="2"/>
       <c r="H17" s="2"/>
     </row>
-    <row r="18" spans="1:8">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" s="8"/>
       <c r="B18" s="2"/>
       <c r="G18" s="2"/>
       <c r="H18" s="2"/>
     </row>
-    <row r="19" spans="1:8">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" s="8"/>
       <c r="B19" s="2"/>
       <c r="G19" s="2"/>
       <c r="H19" s="2"/>
     </row>
-    <row r="20" spans="1:8">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" s="8"/>
       <c r="B20" s="2"/>
       <c r="G20" s="2"/>
       <c r="H20" s="2"/>
     </row>
-    <row r="21" spans="1:8">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" s="8"/>
       <c r="B21" s="2"/>
       <c r="G21" s="2"/>
       <c r="H21" s="2"/>
     </row>
-    <row r="22" spans="1:8">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" s="8"/>
       <c r="B22" s="2"/>
       <c r="G22" s="2"/>
       <c r="H22" s="2"/>
     </row>
-    <row r="23" spans="1:8">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" s="8"/>
       <c r="B23" s="2"/>
       <c r="G23" s="2"/>
       <c r="H23" s="2"/>
     </row>
-    <row r="24" spans="1:8">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24" s="8"/>
       <c r="B24" s="2"/>
       <c r="G24" s="2"/>
       <c r="H24" s="2"/>
     </row>
-    <row r="25" spans="1:8">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25" s="8"/>
       <c r="B25" s="2"/>
       <c r="G25" s="2"/>
       <c r="H25" s="2"/>
     </row>
-    <row r="26" spans="1:8">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26" s="8"/>
       <c r="B26" s="2"/>
       <c r="G26" s="2"/>
       <c r="H26" s="2"/>
     </row>
-    <row r="27" spans="1:8">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A27" s="8"/>
       <c r="B27" s="2"/>
       <c r="G27" s="2"/>
       <c r="H27" s="2"/>
     </row>
-    <row r="28" spans="1:8">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A28" s="8"/>
       <c r="B28" s="2"/>
       <c r="G28" s="2"/>
       <c r="H28" s="2"/>
     </row>
-    <row r="29" spans="1:8">
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A29" s="8"/>
       <c r="B29" s="2"/>
       <c r="G29" s="2"/>
       <c r="H29" s="2"/>
     </row>
-    <row r="30" spans="1:8">
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A30" s="8"/>
       <c r="B30" s="2"/>
       <c r="G30" s="2"/>
       <c r="H30" s="2"/>
     </row>
-    <row r="31" spans="1:8">
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A31" s="8"/>
       <c r="B31" s="2"/>
       <c r="G31" s="2"/>
       <c r="H31" s="2"/>
     </row>
-    <row r="32" spans="1:8">
+    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A32" s="8"/>
       <c r="B32" s="2"/>
       <c r="G32" s="2"/>
       <c r="H32" s="2"/>
     </row>
-    <row r="33" spans="1:8">
+    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A33" s="8"/>
       <c r="B33" s="2"/>
       <c r="G33" s="2"/>
       <c r="H33" s="2"/>
     </row>
-    <row r="34" spans="1:8">
+    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A34" s="8"/>
       <c r="B34" s="2"/>
       <c r="G34" s="2"/>
       <c r="H34" s="2"/>
     </row>
-    <row r="35" spans="1:8">
+    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A35" s="8"/>
       <c r="B35" s="2"/>
       <c r="G35" s="2"/>
       <c r="H35" s="2"/>
     </row>
-    <row r="36" spans="1:8">
+    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A36" s="8"/>
       <c r="B36" s="2"/>
       <c r="G36" s="2"/>
       <c r="H36" s="2"/>
     </row>
-    <row r="37" spans="1:8">
+    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A37" s="8"/>
       <c r="B37" s="2"/>
       <c r="G37" s="2"/>
       <c r="H37" s="2"/>
     </row>
-    <row r="38" spans="1:8">
+    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A38" s="8"/>
       <c r="B38" s="2"/>
       <c r="G38" s="2"/>
       <c r="H38" s="2"/>
     </row>
-    <row r="39" spans="1:8">
+    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A39" s="8"/>
       <c r="B39" s="2"/>
       <c r="G39" s="2"/>
       <c r="H39" s="2"/>
     </row>
-    <row r="40" spans="1:8">
+    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A40" s="8"/>
       <c r="B40" s="2"/>
       <c r="G40" s="2"/>
       <c r="H40" s="2"/>
     </row>
-    <row r="41" spans="1:8">
+    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A41" s="8"/>
       <c r="B41" s="2"/>
       <c r="G41" s="2"/>
       <c r="H41" s="2"/>
     </row>
-    <row r="42" spans="1:8">
+    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A42" s="8"/>
       <c r="B42" s="2"/>
       <c r="G42" s="2"/>
       <c r="H42" s="2"/>
     </row>
-    <row r="43" spans="1:8">
+    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A43" s="8"/>
       <c r="B43" s="2"/>
       <c r="G43" s="2"/>
       <c r="H43" s="2"/>
     </row>
-    <row r="44" spans="1:8">
+    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A44" s="8"/>
       <c r="B44" s="2"/>
       <c r="G44" s="2"/>
       <c r="H44" s="2"/>
     </row>
-    <row r="45" spans="1:8">
+    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A45" s="8"/>
       <c r="B45" s="2"/>
       <c r="G45" s="2"/>
       <c r="H45" s="2"/>
     </row>
-    <row r="46" spans="1:8">
+    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A46" s="8"/>
       <c r="B46" s="2"/>
       <c r="G46" s="2"/>
       <c r="H46" s="2"/>
     </row>
-    <row r="47" spans="1:8">
+    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A47" s="8"/>
       <c r="B47" s="2"/>
       <c r="G47" s="2"/>
       <c r="H47" s="2"/>
     </row>
-    <row r="48" spans="1:8">
+    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A48" s="8"/>
       <c r="B48" s="2"/>
       <c r="G48" s="2"/>
       <c r="H48" s="2"/>
     </row>
-    <row r="49" spans="1:8">
+    <row r="49" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A49" s="8"/>
       <c r="B49" s="2"/>
       <c r="G49" s="2"/>
       <c r="H49" s="2"/>
     </row>
-    <row r="50" spans="1:8">
+    <row r="50" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A50" s="8"/>
       <c r="B50" s="2"/>
       <c r="G50" s="2"/>
       <c r="H50" s="2"/>
     </row>
-    <row r="51" spans="1:8">
+    <row r="51" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A51" s="8"/>
       <c r="B51" s="2"/>
       <c r="G51" s="2"/>
       <c r="H51" s="2"/>
     </row>
-    <row r="52" spans="1:8">
+    <row r="52" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A52" s="8"/>
       <c r="B52" s="2"/>
       <c r="G52" s="2"/>
       <c r="H52" s="2"/>
     </row>
-    <row r="53" spans="1:8">
+    <row r="53" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A53" s="8"/>
       <c r="B53" s="2"/>
       <c r="G53" s="2"/>
       <c r="H53" s="2"/>
     </row>
-    <row r="54" spans="1:8">
+    <row r="54" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A54" s="8"/>
       <c r="B54" s="2"/>
       <c r="G54" s="2"/>
       <c r="H54" s="2"/>
     </row>
-    <row r="55" spans="1:8">
+    <row r="55" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A55" s="8"/>
       <c r="B55" s="2"/>
       <c r="G55" s="2"/>
       <c r="H55" s="2"/>
     </row>
-    <row r="56" spans="1:8">
+    <row r="56" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A56" s="8"/>
       <c r="B56" s="2"/>
       <c r="G56" s="2"/>
       <c r="H56" s="2"/>
     </row>
-    <row r="57" spans="1:8">
+    <row r="57" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A57" s="8"/>
       <c r="B57" s="2"/>
       <c r="G57" s="2"/>
       <c r="H57" s="2"/>
     </row>
-    <row r="58" spans="1:8">
+    <row r="58" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A58" s="8"/>
       <c r="B58" s="2"/>
       <c r="G58" s="2"/>
       <c r="H58" s="2"/>
     </row>
-    <row r="59" spans="1:8">
+    <row r="59" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A59" s="8"/>
       <c r="B59" s="2"/>
       <c r="G59" s="2"/>
       <c r="H59" s="2"/>
     </row>
-    <row r="60" spans="1:8">
+    <row r="60" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A60" s="8"/>
       <c r="B60" s="2"/>
       <c r="G60" s="2"/>
       <c r="H60" s="2"/>
     </row>
-    <row r="61" spans="1:8">
+    <row r="61" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A61" s="8"/>
       <c r="B61" s="2"/>
       <c r="G61" s="2"/>
       <c r="H61" s="2"/>
     </row>
-    <row r="62" spans="1:8">
+    <row r="62" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A62" s="8"/>
       <c r="B62" s="2"/>
       <c r="G62" s="2"/>
       <c r="H62" s="2"/>
     </row>
-    <row r="63" spans="1:8">
+    <row r="63" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A63" s="8"/>
       <c r="B63" s="2"/>
       <c r="G63" s="2"/>
       <c r="H63" s="2"/>
     </row>
-    <row r="64" spans="1:8">
+    <row r="64" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A64" s="8"/>
       <c r="B64" s="2"/>
       <c r="G64" s="2"/>
       <c r="H64" s="2"/>
     </row>
-    <row r="65" spans="1:8">
+    <row r="65" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A65" s="8"/>
       <c r="B65" s="2"/>
       <c r="G65" s="2"/>
       <c r="H65" s="2"/>
     </row>
-    <row r="66" spans="1:8">
+    <row r="66" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A66" s="8"/>
       <c r="B66" s="2"/>
       <c r="G66" s="2"/>
       <c r="H66" s="2"/>
     </row>
-    <row r="67" spans="1:8">
+    <row r="67" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A67" s="8"/>
       <c r="B67" s="2"/>
       <c r="G67" s="2"/>
       <c r="H67" s="2"/>
     </row>
-    <row r="68" spans="1:8">
+    <row r="68" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A68" s="8"/>
       <c r="B68" s="2"/>
       <c r="G68" s="2"/>
       <c r="H68" s="2"/>
     </row>
-    <row r="69" spans="1:8">
+    <row r="69" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A69" s="8"/>
       <c r="B69" s="2"/>
       <c r="G69" s="2"/>
       <c r="H69" s="2"/>
     </row>
-    <row r="70" spans="1:8">
+    <row r="70" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A70" s="8"/>
       <c r="B70" s="2"/>
       <c r="G70" s="2"/>
       <c r="H70" s="2"/>
     </row>
-    <row r="71" spans="1:8">
+    <row r="71" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A71" s="8"/>
       <c r="B71" s="2"/>
       <c r="G71" s="2"/>
       <c r="H71" s="2"/>
     </row>
-    <row r="72" spans="1:8">
+    <row r="72" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A72" s="8"/>
       <c r="B72" s="2"/>
       <c r="G72" s="2"/>
       <c r="H72" s="2"/>
     </row>
-    <row r="73" spans="1:8">
+    <row r="73" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A73" s="8"/>
       <c r="B73" s="2"/>
       <c r="G73" s="2"/>
       <c r="H73" s="2"/>
     </row>
-    <row r="74" spans="1:8">
+    <row r="74" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A74" s="8"/>
       <c r="B74" s="2"/>
       <c r="G74" s="2"/>
       <c r="H74" s="2"/>
     </row>
-    <row r="75" spans="1:8">
+    <row r="75" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A75" s="8"/>
       <c r="B75" s="2"/>
       <c r="G75" s="2"/>
       <c r="H75" s="2"/>
     </row>
-    <row r="76" spans="1:8">
+    <row r="76" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A76" s="8"/>
       <c r="B76" s="2"/>
       <c r="G76" s="2"/>
       <c r="H76" s="2"/>
     </row>
-    <row r="77" spans="1:8">
+    <row r="77" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A77" s="8"/>
       <c r="B77" s="2"/>
       <c r="G77" s="2"/>
       <c r="H77" s="2"/>
     </row>
-    <row r="78" spans="1:8">
+    <row r="78" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A78" s="8"/>
       <c r="B78" s="2"/>
       <c r="G78" s="2"/>
       <c r="H78" s="2"/>
     </row>
-    <row r="79" spans="1:8">
+    <row r="79" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A79" s="8"/>
       <c r="B79" s="2"/>
       <c r="G79" s="2"/>
       <c r="H79" s="2"/>
     </row>
-    <row r="80" spans="1:8">
+    <row r="80" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A80" s="8"/>
       <c r="B80" s="2"/>
       <c r="G80" s="2"/>
       <c r="H80" s="2"/>
     </row>
-    <row r="81" spans="1:8">
+    <row r="81" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A81" s="8"/>
       <c r="B81" s="2"/>
       <c r="G81" s="2"/>
       <c r="H81" s="2"/>
     </row>
-    <row r="82" spans="1:8">
+    <row r="82" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A82" s="8"/>
       <c r="B82" s="2"/>
       <c r="G82" s="2"/>
       <c r="H82" s="2"/>
     </row>
-    <row r="83" spans="1:8">
+    <row r="83" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A83" s="8"/>
       <c r="B83" s="2"/>
       <c r="G83" s="2"/>
       <c r="H83" s="2"/>
     </row>
-    <row r="84" spans="1:8">
+    <row r="84" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A84" s="8"/>
       <c r="B84" s="2"/>
       <c r="G84" s="2"/>
       <c r="H84" s="2"/>
     </row>
-    <row r="85" spans="1:8">
+    <row r="85" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A85" s="8"/>
       <c r="B85" s="2"/>
       <c r="G85" s="2"/>
       <c r="H85" s="2"/>
     </row>
-    <row r="86" spans="1:8">
+    <row r="86" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A86" s="8"/>
       <c r="B86" s="2"/>
       <c r="G86" s="2"/>
       <c r="H86" s="2"/>
     </row>
-    <row r="87" spans="1:8">
+    <row r="87" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A87" s="8"/>
       <c r="B87" s="2"/>
       <c r="G87" s="2"/>
       <c r="H87" s="2"/>
     </row>
-    <row r="88" spans="1:8">
+    <row r="88" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A88" s="8"/>
       <c r="B88" s="2"/>
       <c r="G88" s="2"/>
       <c r="H88" s="2"/>
     </row>
-    <row r="89" spans="1:8">
+    <row r="89" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A89" s="8"/>
       <c r="B89" s="2"/>
       <c r="G89" s="2"/>
       <c r="H89" s="2"/>
     </row>
-    <row r="90" spans="1:8">
+    <row r="90" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A90" s="8"/>
       <c r="B90" s="2"/>
       <c r="G90" s="2"/>
       <c r="H90" s="2"/>
     </row>
-    <row r="91" spans="1:8">
+    <row r="91" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A91" s="8"/>
       <c r="B91" s="2"/>
       <c r="G91" s="2"/>
       <c r="H91" s="2"/>
     </row>
-    <row r="92" spans="1:8">
+    <row r="92" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A92" s="8"/>
       <c r="B92" s="2"/>
       <c r="G92" s="2"/>
       <c r="H92" s="2"/>
     </row>
-    <row r="93" spans="1:8">
+    <row r="93" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A93" s="8"/>
       <c r="B93" s="2"/>
       <c r="G93" s="2"/>
       <c r="H93" s="2"/>
     </row>
-    <row r="94" spans="1:8">
+    <row r="94" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A94" s="8"/>
       <c r="B94" s="2"/>
       <c r="G94" s="2"/>
       <c r="H94" s="2"/>
     </row>
-    <row r="95" spans="1:8">
+    <row r="95" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A95" s="8"/>
       <c r="B95" s="2"/>
       <c r="G95" s="2"/>
       <c r="H95" s="2"/>
     </row>
-    <row r="96" spans="1:8">
+    <row r="96" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A96" s="8"/>
       <c r="B96" s="2"/>
       <c r="G96" s="2"/>
       <c r="H96" s="2"/>
     </row>
-    <row r="97" spans="1:8">
+    <row r="97" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A97" s="8"/>
       <c r="B97" s="2"/>
       <c r="G97" s="2"/>
       <c r="H97" s="2"/>
     </row>
-    <row r="98" spans="1:8">
+    <row r="98" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A98" s="8"/>
       <c r="B98" s="2"/>
       <c r="G98" s="2"/>
       <c r="H98" s="2"/>
     </row>
-    <row r="99" spans="1:8">
+    <row r="99" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A99" s="8"/>
       <c r="B99" s="2"/>
       <c r="G99" s="2"/>
       <c r="H99" s="2"/>
     </row>
-    <row r="100" spans="1:8">
+    <row r="100" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A100" s="8"/>
       <c r="B100" s="2"/>
       <c r="G100" s="2"/>
@@ -2320,19 +2342,19 @@
       <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.44140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="17.33203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="27.88671875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.6640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.88671875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="23.5546875" style="10" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="39.109375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="51.109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="27.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="23.5703125" style="10" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="39.140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="51.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="15.6">
+    <row r="1" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
@@ -2358,7 +2380,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:8">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>45935</v>
       </c>
@@ -2384,7 +2406,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="3" spans="1:8">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>45996</v>
       </c>
@@ -2410,7 +2432,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="4" spans="1:8">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>57</v>
       </c>
@@ -2436,7 +2458,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="5" spans="1:8">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>61</v>
       </c>
@@ -2462,7 +2484,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="6" spans="1:8">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>67</v>
       </c>
@@ -2488,7 +2510,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="7" spans="1:8">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>70</v>
       </c>
@@ -2514,7 +2536,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="8" spans="1:8" ht="100.8">
+    <row r="8" spans="1:8" ht="105" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>45798</v>
       </c>
@@ -2538,644 +2560,644 @@
         <v>89</v>
       </c>
     </row>
-    <row r="9" spans="1:8">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="1"/>
       <c r="B9" s="2"/>
       <c r="E9" s="3"/>
       <c r="G9" s="2"/>
       <c r="H9" s="2"/>
     </row>
-    <row r="10" spans="1:8">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="1"/>
       <c r="B10" s="2"/>
       <c r="E10" s="3"/>
       <c r="G10" s="2"/>
       <c r="H10" s="2"/>
     </row>
-    <row r="11" spans="1:8">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="1"/>
       <c r="B11" s="2"/>
       <c r="E11" s="3"/>
       <c r="G11" s="2"/>
       <c r="H11" s="2"/>
     </row>
-    <row r="12" spans="1:8">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="1"/>
       <c r="B12" s="2"/>
       <c r="E12" s="3"/>
       <c r="G12" s="2"/>
       <c r="H12" s="2"/>
     </row>
-    <row r="13" spans="1:8">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="1"/>
       <c r="B13" s="2"/>
       <c r="E13" s="3"/>
       <c r="G13" s="2"/>
       <c r="H13" s="2"/>
     </row>
-    <row r="14" spans="1:8">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" s="1"/>
       <c r="B14" s="2"/>
       <c r="E14" s="3"/>
       <c r="G14" s="2"/>
       <c r="H14" s="2"/>
     </row>
-    <row r="15" spans="1:8">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" s="1"/>
       <c r="B15" s="2"/>
       <c r="E15" s="3"/>
       <c r="G15" s="2"/>
       <c r="H15" s="2"/>
     </row>
-    <row r="16" spans="1:8">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" s="1"/>
       <c r="B16" s="2"/>
       <c r="E16" s="3"/>
       <c r="G16" s="2"/>
       <c r="H16" s="2"/>
     </row>
-    <row r="17" spans="1:8">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" s="1"/>
       <c r="B17" s="2"/>
       <c r="E17" s="3"/>
       <c r="G17" s="2"/>
       <c r="H17" s="2"/>
     </row>
-    <row r="18" spans="1:8">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" s="1"/>
       <c r="B18" s="2"/>
       <c r="E18" s="3"/>
       <c r="G18" s="2"/>
       <c r="H18" s="2"/>
     </row>
-    <row r="19" spans="1:8">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" s="1"/>
       <c r="B19" s="2"/>
       <c r="E19" s="3"/>
       <c r="G19" s="2"/>
       <c r="H19" s="2"/>
     </row>
-    <row r="20" spans="1:8">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" s="1"/>
       <c r="B20" s="2"/>
       <c r="E20" s="3"/>
       <c r="G20" s="2"/>
       <c r="H20" s="2"/>
     </row>
-    <row r="21" spans="1:8">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" s="1"/>
       <c r="B21" s="2"/>
       <c r="E21" s="3"/>
       <c r="G21" s="2"/>
       <c r="H21" s="2"/>
     </row>
-    <row r="22" spans="1:8">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" s="1"/>
       <c r="B22" s="2"/>
       <c r="E22" s="3"/>
       <c r="G22" s="2"/>
       <c r="H22" s="2"/>
     </row>
-    <row r="23" spans="1:8">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" s="1"/>
       <c r="B23" s="2"/>
       <c r="E23" s="3"/>
       <c r="G23" s="2"/>
       <c r="H23" s="2"/>
     </row>
-    <row r="24" spans="1:8">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24" s="1"/>
       <c r="B24" s="2"/>
       <c r="E24" s="3"/>
       <c r="G24" s="2"/>
       <c r="H24" s="2"/>
     </row>
-    <row r="25" spans="1:8">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25" s="1"/>
       <c r="B25" s="2"/>
       <c r="E25" s="3"/>
       <c r="G25" s="2"/>
       <c r="H25" s="2"/>
     </row>
-    <row r="26" spans="1:8">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26" s="1"/>
       <c r="B26" s="2"/>
       <c r="E26" s="3"/>
       <c r="G26" s="2"/>
       <c r="H26" s="2"/>
     </row>
-    <row r="27" spans="1:8">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A27" s="1"/>
       <c r="B27" s="2"/>
       <c r="E27" s="3"/>
       <c r="G27" s="2"/>
       <c r="H27" s="2"/>
     </row>
-    <row r="28" spans="1:8">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A28" s="1"/>
       <c r="B28" s="2"/>
       <c r="E28" s="3"/>
       <c r="G28" s="2"/>
       <c r="H28" s="2"/>
     </row>
-    <row r="29" spans="1:8">
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A29" s="1"/>
       <c r="B29" s="2"/>
       <c r="E29" s="3"/>
       <c r="G29" s="2"/>
       <c r="H29" s="2"/>
     </row>
-    <row r="30" spans="1:8">
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A30" s="1"/>
       <c r="B30" s="2"/>
       <c r="E30" s="3"/>
       <c r="G30" s="2"/>
       <c r="H30" s="2"/>
     </row>
-    <row r="31" spans="1:8">
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A31" s="1"/>
       <c r="B31" s="2"/>
       <c r="E31" s="3"/>
       <c r="G31" s="2"/>
       <c r="H31" s="2"/>
     </row>
-    <row r="32" spans="1:8">
+    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A32" s="1"/>
       <c r="B32" s="2"/>
       <c r="E32" s="3"/>
       <c r="G32" s="2"/>
       <c r="H32" s="2"/>
     </row>
-    <row r="33" spans="1:8">
+    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A33" s="1"/>
       <c r="B33" s="2"/>
       <c r="E33" s="3"/>
       <c r="G33" s="2"/>
       <c r="H33" s="2"/>
     </row>
-    <row r="34" spans="1:8">
+    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A34" s="1"/>
       <c r="B34" s="2"/>
       <c r="E34" s="3"/>
       <c r="G34" s="2"/>
       <c r="H34" s="2"/>
     </row>
-    <row r="35" spans="1:8">
+    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A35" s="1"/>
       <c r="B35" s="2"/>
       <c r="E35" s="3"/>
       <c r="G35" s="2"/>
       <c r="H35" s="2"/>
     </row>
-    <row r="36" spans="1:8">
+    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A36" s="1"/>
       <c r="B36" s="2"/>
       <c r="E36" s="3"/>
       <c r="G36" s="2"/>
       <c r="H36" s="2"/>
     </row>
-    <row r="37" spans="1:8">
+    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A37" s="1"/>
       <c r="B37" s="2"/>
       <c r="E37" s="3"/>
       <c r="G37" s="2"/>
       <c r="H37" s="2"/>
     </row>
-    <row r="38" spans="1:8">
+    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A38" s="1"/>
       <c r="B38" s="2"/>
       <c r="E38" s="3"/>
       <c r="G38" s="2"/>
       <c r="H38" s="2"/>
     </row>
-    <row r="39" spans="1:8">
+    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A39" s="1"/>
       <c r="B39" s="2"/>
       <c r="E39" s="3"/>
       <c r="G39" s="2"/>
       <c r="H39" s="2"/>
     </row>
-    <row r="40" spans="1:8">
+    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A40" s="1"/>
       <c r="B40" s="2"/>
       <c r="E40" s="3"/>
       <c r="G40" s="2"/>
       <c r="H40" s="2"/>
     </row>
-    <row r="41" spans="1:8">
+    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A41" s="1"/>
       <c r="B41" s="2"/>
       <c r="E41" s="3"/>
       <c r="G41" s="2"/>
       <c r="H41" s="2"/>
     </row>
-    <row r="42" spans="1:8">
+    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A42" s="1"/>
       <c r="B42" s="2"/>
       <c r="E42" s="3"/>
       <c r="G42" s="2"/>
       <c r="H42" s="2"/>
     </row>
-    <row r="43" spans="1:8">
+    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A43" s="1"/>
       <c r="B43" s="2"/>
       <c r="E43" s="3"/>
       <c r="G43" s="2"/>
       <c r="H43" s="2"/>
     </row>
-    <row r="44" spans="1:8">
+    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A44" s="1"/>
       <c r="B44" s="2"/>
       <c r="E44" s="3"/>
       <c r="G44" s="2"/>
       <c r="H44" s="2"/>
     </row>
-    <row r="45" spans="1:8">
+    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A45" s="1"/>
       <c r="B45" s="2"/>
       <c r="E45" s="3"/>
       <c r="G45" s="2"/>
       <c r="H45" s="2"/>
     </row>
-    <row r="46" spans="1:8">
+    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A46" s="1"/>
       <c r="B46" s="2"/>
       <c r="E46" s="3"/>
       <c r="G46" s="2"/>
       <c r="H46" s="2"/>
     </row>
-    <row r="47" spans="1:8">
+    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A47" s="1"/>
       <c r="B47" s="2"/>
       <c r="E47" s="3"/>
       <c r="G47" s="2"/>
       <c r="H47" s="2"/>
     </row>
-    <row r="48" spans="1:8">
+    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A48" s="1"/>
       <c r="B48" s="2"/>
       <c r="E48" s="3"/>
       <c r="G48" s="2"/>
       <c r="H48" s="2"/>
     </row>
-    <row r="49" spans="1:8">
+    <row r="49" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A49" s="1"/>
       <c r="B49" s="2"/>
       <c r="E49" s="3"/>
       <c r="G49" s="2"/>
       <c r="H49" s="2"/>
     </row>
-    <row r="50" spans="1:8">
+    <row r="50" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A50" s="1"/>
       <c r="B50" s="2"/>
       <c r="E50" s="3"/>
       <c r="G50" s="2"/>
       <c r="H50" s="2"/>
     </row>
-    <row r="51" spans="1:8">
+    <row r="51" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A51" s="1"/>
       <c r="B51" s="2"/>
       <c r="E51" s="3"/>
       <c r="G51" s="2"/>
       <c r="H51" s="2"/>
     </row>
-    <row r="52" spans="1:8">
+    <row r="52" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A52" s="1"/>
       <c r="B52" s="2"/>
       <c r="E52" s="3"/>
       <c r="G52" s="2"/>
       <c r="H52" s="2"/>
     </row>
-    <row r="53" spans="1:8">
+    <row r="53" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A53" s="1"/>
       <c r="B53" s="2"/>
       <c r="E53" s="3"/>
       <c r="G53" s="2"/>
       <c r="H53" s="2"/>
     </row>
-    <row r="54" spans="1:8">
+    <row r="54" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A54" s="1"/>
       <c r="B54" s="2"/>
       <c r="E54" s="3"/>
       <c r="G54" s="2"/>
       <c r="H54" s="2"/>
     </row>
-    <row r="55" spans="1:8">
+    <row r="55" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A55" s="1"/>
       <c r="B55" s="2"/>
       <c r="E55" s="3"/>
       <c r="G55" s="2"/>
       <c r="H55" s="2"/>
     </row>
-    <row r="56" spans="1:8">
+    <row r="56" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A56" s="1"/>
       <c r="B56" s="2"/>
       <c r="E56" s="3"/>
       <c r="G56" s="2"/>
       <c r="H56" s="2"/>
     </row>
-    <row r="57" spans="1:8">
+    <row r="57" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A57" s="1"/>
       <c r="B57" s="2"/>
       <c r="E57" s="3"/>
       <c r="G57" s="2"/>
       <c r="H57" s="2"/>
     </row>
-    <row r="58" spans="1:8">
+    <row r="58" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A58" s="1"/>
       <c r="B58" s="2"/>
       <c r="E58" s="3"/>
       <c r="G58" s="2"/>
       <c r="H58" s="2"/>
     </row>
-    <row r="59" spans="1:8">
+    <row r="59" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A59" s="1"/>
       <c r="B59" s="2"/>
       <c r="E59" s="3"/>
       <c r="G59" s="2"/>
       <c r="H59" s="2"/>
     </row>
-    <row r="60" spans="1:8">
+    <row r="60" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A60" s="1"/>
       <c r="B60" s="2"/>
       <c r="E60" s="3"/>
       <c r="G60" s="2"/>
       <c r="H60" s="2"/>
     </row>
-    <row r="61" spans="1:8">
+    <row r="61" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A61" s="1"/>
       <c r="B61" s="2"/>
       <c r="E61" s="3"/>
       <c r="G61" s="2"/>
       <c r="H61" s="2"/>
     </row>
-    <row r="62" spans="1:8">
+    <row r="62" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A62" s="1"/>
       <c r="B62" s="2"/>
       <c r="E62" s="3"/>
       <c r="G62" s="2"/>
       <c r="H62" s="2"/>
     </row>
-    <row r="63" spans="1:8">
+    <row r="63" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A63" s="1"/>
       <c r="B63" s="2"/>
       <c r="E63" s="3"/>
       <c r="G63" s="2"/>
       <c r="H63" s="2"/>
     </row>
-    <row r="64" spans="1:8">
+    <row r="64" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A64" s="1"/>
       <c r="B64" s="2"/>
       <c r="E64" s="3"/>
       <c r="G64" s="2"/>
       <c r="H64" s="2"/>
     </row>
-    <row r="65" spans="1:8">
+    <row r="65" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A65" s="1"/>
       <c r="B65" s="2"/>
       <c r="E65" s="3"/>
       <c r="G65" s="2"/>
       <c r="H65" s="2"/>
     </row>
-    <row r="66" spans="1:8">
+    <row r="66" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A66" s="1"/>
       <c r="B66" s="2"/>
       <c r="E66" s="3"/>
       <c r="G66" s="2"/>
       <c r="H66" s="2"/>
     </row>
-    <row r="67" spans="1:8">
+    <row r="67" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A67" s="1"/>
       <c r="B67" s="2"/>
       <c r="E67" s="3"/>
       <c r="G67" s="2"/>
       <c r="H67" s="2"/>
     </row>
-    <row r="68" spans="1:8">
+    <row r="68" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A68" s="1"/>
       <c r="B68" s="2"/>
       <c r="E68" s="3"/>
       <c r="G68" s="2"/>
       <c r="H68" s="2"/>
     </row>
-    <row r="69" spans="1:8">
+    <row r="69" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A69" s="1"/>
       <c r="B69" s="2"/>
       <c r="E69" s="3"/>
       <c r="G69" s="2"/>
       <c r="H69" s="2"/>
     </row>
-    <row r="70" spans="1:8">
+    <row r="70" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A70" s="1"/>
       <c r="B70" s="2"/>
       <c r="E70" s="3"/>
       <c r="G70" s="2"/>
       <c r="H70" s="2"/>
     </row>
-    <row r="71" spans="1:8">
+    <row r="71" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A71" s="1"/>
       <c r="B71" s="2"/>
       <c r="E71" s="3"/>
       <c r="G71" s="2"/>
       <c r="H71" s="2"/>
     </row>
-    <row r="72" spans="1:8">
+    <row r="72" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A72" s="1"/>
       <c r="B72" s="2"/>
       <c r="E72" s="3"/>
       <c r="G72" s="2"/>
       <c r="H72" s="2"/>
     </row>
-    <row r="73" spans="1:8">
+    <row r="73" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A73" s="1"/>
       <c r="B73" s="2"/>
       <c r="E73" s="3"/>
       <c r="G73" s="2"/>
       <c r="H73" s="2"/>
     </row>
-    <row r="74" spans="1:8">
+    <row r="74" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A74" s="1"/>
       <c r="B74" s="2"/>
       <c r="E74" s="3"/>
       <c r="G74" s="2"/>
       <c r="H74" s="2"/>
     </row>
-    <row r="75" spans="1:8">
+    <row r="75" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A75" s="1"/>
       <c r="B75" s="2"/>
       <c r="E75" s="3"/>
       <c r="G75" s="2"/>
       <c r="H75" s="2"/>
     </row>
-    <row r="76" spans="1:8">
+    <row r="76" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A76" s="1"/>
       <c r="B76" s="2"/>
       <c r="E76" s="3"/>
       <c r="G76" s="2"/>
       <c r="H76" s="2"/>
     </row>
-    <row r="77" spans="1:8">
+    <row r="77" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A77" s="1"/>
       <c r="B77" s="2"/>
       <c r="E77" s="3"/>
       <c r="G77" s="2"/>
       <c r="H77" s="2"/>
     </row>
-    <row r="78" spans="1:8">
+    <row r="78" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A78" s="1"/>
       <c r="B78" s="2"/>
       <c r="E78" s="3"/>
       <c r="G78" s="2"/>
       <c r="H78" s="2"/>
     </row>
-    <row r="79" spans="1:8">
+    <row r="79" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A79" s="1"/>
       <c r="B79" s="2"/>
       <c r="E79" s="3"/>
       <c r="G79" s="2"/>
       <c r="H79" s="2"/>
     </row>
-    <row r="80" spans="1:8">
+    <row r="80" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A80" s="1"/>
       <c r="B80" s="2"/>
       <c r="E80" s="3"/>
       <c r="G80" s="2"/>
       <c r="H80" s="2"/>
     </row>
-    <row r="81" spans="1:8">
+    <row r="81" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A81" s="1"/>
       <c r="B81" s="2"/>
       <c r="E81" s="3"/>
       <c r="G81" s="2"/>
       <c r="H81" s="2"/>
     </row>
-    <row r="82" spans="1:8">
+    <row r="82" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A82" s="1"/>
       <c r="B82" s="2"/>
       <c r="E82" s="3"/>
       <c r="G82" s="2"/>
       <c r="H82" s="2"/>
     </row>
-    <row r="83" spans="1:8">
+    <row r="83" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A83" s="1"/>
       <c r="B83" s="2"/>
       <c r="E83" s="3"/>
       <c r="G83" s="2"/>
       <c r="H83" s="2"/>
     </row>
-    <row r="84" spans="1:8">
+    <row r="84" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A84" s="1"/>
       <c r="B84" s="2"/>
       <c r="E84" s="3"/>
       <c r="G84" s="2"/>
       <c r="H84" s="2"/>
     </row>
-    <row r="85" spans="1:8">
+    <row r="85" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A85" s="1"/>
       <c r="B85" s="2"/>
       <c r="E85" s="3"/>
       <c r="G85" s="2"/>
       <c r="H85" s="2"/>
     </row>
-    <row r="86" spans="1:8">
+    <row r="86" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A86" s="1"/>
       <c r="B86" s="2"/>
       <c r="E86" s="3"/>
       <c r="G86" s="2"/>
       <c r="H86" s="2"/>
     </row>
-    <row r="87" spans="1:8">
+    <row r="87" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A87" s="1"/>
       <c r="B87" s="2"/>
       <c r="E87" s="3"/>
       <c r="G87" s="2"/>
       <c r="H87" s="2"/>
     </row>
-    <row r="88" spans="1:8">
+    <row r="88" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A88" s="1"/>
       <c r="B88" s="2"/>
       <c r="E88" s="3"/>
       <c r="G88" s="2"/>
       <c r="H88" s="2"/>
     </row>
-    <row r="89" spans="1:8">
+    <row r="89" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A89" s="1"/>
       <c r="B89" s="2"/>
       <c r="E89" s="3"/>
       <c r="G89" s="2"/>
       <c r="H89" s="2"/>
     </row>
-    <row r="90" spans="1:8">
+    <row r="90" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A90" s="1"/>
       <c r="B90" s="2"/>
       <c r="E90" s="3"/>
       <c r="G90" s="2"/>
       <c r="H90" s="2"/>
     </row>
-    <row r="91" spans="1:8">
+    <row r="91" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A91" s="1"/>
       <c r="B91" s="2"/>
       <c r="E91" s="3"/>
       <c r="G91" s="2"/>
       <c r="H91" s="2"/>
     </row>
-    <row r="92" spans="1:8">
+    <row r="92" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A92" s="1"/>
       <c r="B92" s="2"/>
       <c r="E92" s="3"/>
       <c r="G92" s="2"/>
       <c r="H92" s="2"/>
     </row>
-    <row r="93" spans="1:8">
+    <row r="93" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A93" s="1"/>
       <c r="B93" s="2"/>
       <c r="E93" s="3"/>
       <c r="G93" s="2"/>
       <c r="H93" s="2"/>
     </row>
-    <row r="94" spans="1:8">
+    <row r="94" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A94" s="1"/>
       <c r="B94" s="2"/>
       <c r="E94" s="3"/>
       <c r="G94" s="2"/>
       <c r="H94" s="2"/>
     </row>
-    <row r="95" spans="1:8">
+    <row r="95" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A95" s="1"/>
       <c r="B95" s="2"/>
       <c r="E95" s="3"/>
       <c r="G95" s="2"/>
       <c r="H95" s="2"/>
     </row>
-    <row r="96" spans="1:8">
+    <row r="96" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A96" s="1"/>
       <c r="B96" s="2"/>
       <c r="E96" s="3"/>
       <c r="G96" s="2"/>
       <c r="H96" s="2"/>
     </row>
-    <row r="97" spans="1:8">
+    <row r="97" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A97" s="1"/>
       <c r="B97" s="2"/>
       <c r="E97" s="3"/>
       <c r="G97" s="2"/>
       <c r="H97" s="2"/>
     </row>
-    <row r="98" spans="1:8">
+    <row r="98" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A98" s="1"/>
       <c r="B98" s="2"/>
       <c r="E98" s="3"/>
       <c r="G98" s="2"/>
       <c r="H98" s="2"/>
     </row>
-    <row r="99" spans="1:8">
+    <row r="99" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A99" s="1"/>
       <c r="B99" s="2"/>
       <c r="E99" s="3"/>
       <c r="G99" s="2"/>
       <c r="H99" s="2"/>
     </row>
-    <row r="100" spans="1:8">
+    <row r="100" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A100" s="1"/>
       <c r="B100" s="2"/>
       <c r="E100" s="3"/>
@@ -3217,19 +3239,19 @@
       <selection activeCell="D2" sqref="D2:D100"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="7.6640625" customWidth="1"/>
-    <col min="2" max="2" width="17.33203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.5546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="7.7109375" customWidth="1"/>
+    <col min="2" max="2" width="17.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.5703125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="9" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.88671875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="23.5546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="13.44140625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="19.109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="23.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="19.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="15.6">
+    <row r="1" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
@@ -3255,7 +3277,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:8">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="1"/>
       <c r="B2" s="2"/>
       <c r="E2" s="3"/>
@@ -3263,7 +3285,7 @@
       <c r="G2" s="2"/>
       <c r="H2" s="2"/>
     </row>
-    <row r="3" spans="1:8">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="1"/>
       <c r="B3" s="2"/>
       <c r="E3" s="3"/>
@@ -3271,7 +3293,7 @@
       <c r="G3" s="2"/>
       <c r="H3" s="2"/>
     </row>
-    <row r="4" spans="1:8">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="1"/>
       <c r="B4" s="2"/>
       <c r="E4" s="3"/>
@@ -3279,7 +3301,7 @@
       <c r="G4" s="2"/>
       <c r="H4" s="2"/>
     </row>
-    <row r="5" spans="1:8">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="1"/>
       <c r="B5" s="2"/>
       <c r="E5" s="3"/>
@@ -3287,7 +3309,7 @@
       <c r="G5" s="2"/>
       <c r="H5" s="2"/>
     </row>
-    <row r="6" spans="1:8">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="1"/>
       <c r="B6" s="2"/>
       <c r="E6" s="3"/>
@@ -3295,7 +3317,7 @@
       <c r="G6" s="2"/>
       <c r="H6" s="2"/>
     </row>
-    <row r="7" spans="1:8">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="1"/>
       <c r="B7" s="2"/>
       <c r="E7" s="3"/>
@@ -3303,7 +3325,7 @@
       <c r="G7" s="2"/>
       <c r="H7" s="2"/>
     </row>
-    <row r="8" spans="1:8">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="1"/>
       <c r="B8" s="2"/>
       <c r="E8" s="3"/>
@@ -3311,7 +3333,7 @@
       <c r="G8" s="2"/>
       <c r="H8" s="2"/>
     </row>
-    <row r="9" spans="1:8">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="1"/>
       <c r="B9" s="2"/>
       <c r="E9" s="3"/>
@@ -3319,7 +3341,7 @@
       <c r="G9" s="2"/>
       <c r="H9" s="2"/>
     </row>
-    <row r="10" spans="1:8">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="1"/>
       <c r="B10" s="2"/>
       <c r="E10" s="3"/>
@@ -3327,7 +3349,7 @@
       <c r="G10" s="2"/>
       <c r="H10" s="2"/>
     </row>
-    <row r="11" spans="1:8">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="1"/>
       <c r="B11" s="2"/>
       <c r="E11" s="3"/>
@@ -3335,7 +3357,7 @@
       <c r="G11" s="2"/>
       <c r="H11" s="2"/>
     </row>
-    <row r="12" spans="1:8">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="1"/>
       <c r="B12" s="2"/>
       <c r="E12" s="3"/>
@@ -3343,7 +3365,7 @@
       <c r="G12" s="2"/>
       <c r="H12" s="2"/>
     </row>
-    <row r="13" spans="1:8">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="1"/>
       <c r="B13" s="2"/>
       <c r="E13" s="3"/>
@@ -3351,7 +3373,7 @@
       <c r="G13" s="2"/>
       <c r="H13" s="2"/>
     </row>
-    <row r="14" spans="1:8">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" s="1"/>
       <c r="B14" s="2"/>
       <c r="E14" s="3"/>
@@ -3359,7 +3381,7 @@
       <c r="G14" s="2"/>
       <c r="H14" s="2"/>
     </row>
-    <row r="15" spans="1:8">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" s="1"/>
       <c r="B15" s="2"/>
       <c r="E15" s="3"/>
@@ -3367,7 +3389,7 @@
       <c r="G15" s="2"/>
       <c r="H15" s="2"/>
     </row>
-    <row r="16" spans="1:8">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" s="1"/>
       <c r="B16" s="2"/>
       <c r="E16" s="3"/>
@@ -3375,7 +3397,7 @@
       <c r="G16" s="2"/>
       <c r="H16" s="2"/>
     </row>
-    <row r="17" spans="1:8">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" s="1"/>
       <c r="B17" s="2"/>
       <c r="E17" s="3"/>
@@ -3383,7 +3405,7 @@
       <c r="G17" s="2"/>
       <c r="H17" s="2"/>
     </row>
-    <row r="18" spans="1:8">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" s="1"/>
       <c r="B18" s="2"/>
       <c r="E18" s="3"/>
@@ -3391,7 +3413,7 @@
       <c r="G18" s="2"/>
       <c r="H18" s="2"/>
     </row>
-    <row r="19" spans="1:8">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" s="1"/>
       <c r="B19" s="2"/>
       <c r="E19" s="3"/>
@@ -3399,7 +3421,7 @@
       <c r="G19" s="2"/>
       <c r="H19" s="2"/>
     </row>
-    <row r="20" spans="1:8">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" s="1"/>
       <c r="B20" s="2"/>
       <c r="E20" s="3"/>
@@ -3407,7 +3429,7 @@
       <c r="G20" s="2"/>
       <c r="H20" s="2"/>
     </row>
-    <row r="21" spans="1:8">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" s="1"/>
       <c r="B21" s="2"/>
       <c r="E21" s="3"/>
@@ -3415,7 +3437,7 @@
       <c r="G21" s="2"/>
       <c r="H21" s="2"/>
     </row>
-    <row r="22" spans="1:8">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" s="1"/>
       <c r="B22" s="2"/>
       <c r="E22" s="3"/>
@@ -3423,7 +3445,7 @@
       <c r="G22" s="2"/>
       <c r="H22" s="2"/>
     </row>
-    <row r="23" spans="1:8">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" s="1"/>
       <c r="B23" s="2"/>
       <c r="E23" s="3"/>
@@ -3431,7 +3453,7 @@
       <c r="G23" s="2"/>
       <c r="H23" s="2"/>
     </row>
-    <row r="24" spans="1:8">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24" s="1"/>
       <c r="B24" s="2"/>
       <c r="E24" s="3"/>
@@ -3439,7 +3461,7 @@
       <c r="G24" s="2"/>
       <c r="H24" s="2"/>
     </row>
-    <row r="25" spans="1:8">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25" s="1"/>
       <c r="B25" s="2"/>
       <c r="E25" s="3"/>
@@ -3447,7 +3469,7 @@
       <c r="G25" s="2"/>
       <c r="H25" s="2"/>
     </row>
-    <row r="26" spans="1:8">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26" s="1"/>
       <c r="B26" s="2"/>
       <c r="E26" s="3"/>
@@ -3455,7 +3477,7 @@
       <c r="G26" s="2"/>
       <c r="H26" s="2"/>
     </row>
-    <row r="27" spans="1:8">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A27" s="1"/>
       <c r="B27" s="2"/>
       <c r="E27" s="3"/>
@@ -3463,7 +3485,7 @@
       <c r="G27" s="2"/>
       <c r="H27" s="2"/>
     </row>
-    <row r="28" spans="1:8">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A28" s="1"/>
       <c r="B28" s="2"/>
       <c r="E28" s="3"/>
@@ -3471,7 +3493,7 @@
       <c r="G28" s="2"/>
       <c r="H28" s="2"/>
     </row>
-    <row r="29" spans="1:8">
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A29" s="1"/>
       <c r="B29" s="2"/>
       <c r="E29" s="3"/>
@@ -3479,7 +3501,7 @@
       <c r="G29" s="2"/>
       <c r="H29" s="2"/>
     </row>
-    <row r="30" spans="1:8">
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A30" s="1"/>
       <c r="B30" s="2"/>
       <c r="E30" s="3"/>
@@ -3487,7 +3509,7 @@
       <c r="G30" s="2"/>
       <c r="H30" s="2"/>
     </row>
-    <row r="31" spans="1:8">
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A31" s="1"/>
       <c r="B31" s="2"/>
       <c r="E31" s="3"/>
@@ -3495,7 +3517,7 @@
       <c r="G31" s="2"/>
       <c r="H31" s="2"/>
     </row>
-    <row r="32" spans="1:8">
+    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A32" s="1"/>
       <c r="B32" s="2"/>
       <c r="E32" s="3"/>
@@ -3503,7 +3525,7 @@
       <c r="G32" s="2"/>
       <c r="H32" s="2"/>
     </row>
-    <row r="33" spans="1:8">
+    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A33" s="1"/>
       <c r="B33" s="2"/>
       <c r="E33" s="3"/>
@@ -3511,7 +3533,7 @@
       <c r="G33" s="2"/>
       <c r="H33" s="2"/>
     </row>
-    <row r="34" spans="1:8">
+    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A34" s="1"/>
       <c r="B34" s="2"/>
       <c r="E34" s="3"/>
@@ -3519,7 +3541,7 @@
       <c r="G34" s="2"/>
       <c r="H34" s="2"/>
     </row>
-    <row r="35" spans="1:8">
+    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A35" s="1"/>
       <c r="B35" s="2"/>
       <c r="E35" s="3"/>
@@ -3527,7 +3549,7 @@
       <c r="G35" s="2"/>
       <c r="H35" s="2"/>
     </row>
-    <row r="36" spans="1:8">
+    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A36" s="1"/>
       <c r="B36" s="2"/>
       <c r="E36" s="3"/>
@@ -3535,7 +3557,7 @@
       <c r="G36" s="2"/>
       <c r="H36" s="2"/>
     </row>
-    <row r="37" spans="1:8">
+    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A37" s="1"/>
       <c r="B37" s="2"/>
       <c r="E37" s="3"/>
@@ -3543,7 +3565,7 @@
       <c r="G37" s="2"/>
       <c r="H37" s="2"/>
     </row>
-    <row r="38" spans="1:8">
+    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A38" s="1"/>
       <c r="B38" s="2"/>
       <c r="E38" s="3"/>
@@ -3551,7 +3573,7 @@
       <c r="G38" s="2"/>
       <c r="H38" s="2"/>
     </row>
-    <row r="39" spans="1:8">
+    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A39" s="1"/>
       <c r="B39" s="2"/>
       <c r="E39" s="3"/>
@@ -3559,7 +3581,7 @@
       <c r="G39" s="2"/>
       <c r="H39" s="2"/>
     </row>
-    <row r="40" spans="1:8">
+    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A40" s="1"/>
       <c r="B40" s="2"/>
       <c r="E40" s="3"/>
@@ -3567,7 +3589,7 @@
       <c r="G40" s="2"/>
       <c r="H40" s="2"/>
     </row>
-    <row r="41" spans="1:8">
+    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A41" s="1"/>
       <c r="B41" s="2"/>
       <c r="E41" s="3"/>
@@ -3575,7 +3597,7 @@
       <c r="G41" s="2"/>
       <c r="H41" s="2"/>
     </row>
-    <row r="42" spans="1:8">
+    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A42" s="1"/>
       <c r="B42" s="2"/>
       <c r="E42" s="3"/>
@@ -3583,7 +3605,7 @@
       <c r="G42" s="2"/>
       <c r="H42" s="2"/>
     </row>
-    <row r="43" spans="1:8">
+    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A43" s="1"/>
       <c r="B43" s="2"/>
       <c r="E43" s="3"/>
@@ -3591,7 +3613,7 @@
       <c r="G43" s="2"/>
       <c r="H43" s="2"/>
     </row>
-    <row r="44" spans="1:8">
+    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A44" s="1"/>
       <c r="B44" s="2"/>
       <c r="E44" s="3"/>
@@ -3599,7 +3621,7 @@
       <c r="G44" s="2"/>
       <c r="H44" s="2"/>
     </row>
-    <row r="45" spans="1:8">
+    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A45" s="1"/>
       <c r="B45" s="2"/>
       <c r="E45" s="3"/>
@@ -3607,7 +3629,7 @@
       <c r="G45" s="2"/>
       <c r="H45" s="2"/>
     </row>
-    <row r="46" spans="1:8">
+    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A46" s="1"/>
       <c r="B46" s="2"/>
       <c r="E46" s="3"/>
@@ -3615,7 +3637,7 @@
       <c r="G46" s="2"/>
       <c r="H46" s="2"/>
     </row>
-    <row r="47" spans="1:8">
+    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A47" s="1"/>
       <c r="B47" s="2"/>
       <c r="E47" s="3"/>
@@ -3623,7 +3645,7 @@
       <c r="G47" s="2"/>
       <c r="H47" s="2"/>
     </row>
-    <row r="48" spans="1:8">
+    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A48" s="1"/>
       <c r="B48" s="2"/>
       <c r="E48" s="3"/>
@@ -3631,7 +3653,7 @@
       <c r="G48" s="2"/>
       <c r="H48" s="2"/>
     </row>
-    <row r="49" spans="1:8">
+    <row r="49" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A49" s="1"/>
       <c r="B49" s="2"/>
       <c r="E49" s="3"/>
@@ -3639,7 +3661,7 @@
       <c r="G49" s="2"/>
       <c r="H49" s="2"/>
     </row>
-    <row r="50" spans="1:8">
+    <row r="50" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A50" s="1"/>
       <c r="B50" s="2"/>
       <c r="E50" s="3"/>
@@ -3647,7 +3669,7 @@
       <c r="G50" s="2"/>
       <c r="H50" s="2"/>
     </row>
-    <row r="51" spans="1:8">
+    <row r="51" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A51" s="1"/>
       <c r="B51" s="2"/>
       <c r="E51" s="3"/>
@@ -3655,7 +3677,7 @@
       <c r="G51" s="2"/>
       <c r="H51" s="2"/>
     </row>
-    <row r="52" spans="1:8">
+    <row r="52" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A52" s="1"/>
       <c r="B52" s="2"/>
       <c r="E52" s="3"/>
@@ -3663,7 +3685,7 @@
       <c r="G52" s="2"/>
       <c r="H52" s="2"/>
     </row>
-    <row r="53" spans="1:8">
+    <row r="53" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A53" s="1"/>
       <c r="B53" s="2"/>
       <c r="E53" s="3"/>
@@ -3671,7 +3693,7 @@
       <c r="G53" s="2"/>
       <c r="H53" s="2"/>
     </row>
-    <row r="54" spans="1:8">
+    <row r="54" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A54" s="1"/>
       <c r="B54" s="2"/>
       <c r="E54" s="3"/>
@@ -3679,7 +3701,7 @@
       <c r="G54" s="2"/>
       <c r="H54" s="2"/>
     </row>
-    <row r="55" spans="1:8">
+    <row r="55" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A55" s="1"/>
       <c r="B55" s="2"/>
       <c r="E55" s="3"/>
@@ -3687,7 +3709,7 @@
       <c r="G55" s="2"/>
       <c r="H55" s="2"/>
     </row>
-    <row r="56" spans="1:8">
+    <row r="56" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A56" s="1"/>
       <c r="B56" s="2"/>
       <c r="E56" s="3"/>
@@ -3695,7 +3717,7 @@
       <c r="G56" s="2"/>
       <c r="H56" s="2"/>
     </row>
-    <row r="57" spans="1:8">
+    <row r="57" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A57" s="1"/>
       <c r="B57" s="2"/>
       <c r="E57" s="3"/>
@@ -3703,7 +3725,7 @@
       <c r="G57" s="2"/>
       <c r="H57" s="2"/>
     </row>
-    <row r="58" spans="1:8">
+    <row r="58" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A58" s="1"/>
       <c r="B58" s="2"/>
       <c r="E58" s="3"/>
@@ -3711,7 +3733,7 @@
       <c r="G58" s="2"/>
       <c r="H58" s="2"/>
     </row>
-    <row r="59" spans="1:8">
+    <row r="59" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A59" s="1"/>
       <c r="B59" s="2"/>
       <c r="E59" s="3"/>
@@ -3719,7 +3741,7 @@
       <c r="G59" s="2"/>
       <c r="H59" s="2"/>
     </row>
-    <row r="60" spans="1:8">
+    <row r="60" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A60" s="1"/>
       <c r="B60" s="2"/>
       <c r="E60" s="3"/>
@@ -3727,7 +3749,7 @@
       <c r="G60" s="2"/>
       <c r="H60" s="2"/>
     </row>
-    <row r="61" spans="1:8">
+    <row r="61" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A61" s="1"/>
       <c r="B61" s="2"/>
       <c r="E61" s="3"/>
@@ -3735,7 +3757,7 @@
       <c r="G61" s="2"/>
       <c r="H61" s="2"/>
     </row>
-    <row r="62" spans="1:8">
+    <row r="62" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A62" s="1"/>
       <c r="B62" s="2"/>
       <c r="E62" s="3"/>
@@ -3743,7 +3765,7 @@
       <c r="G62" s="2"/>
       <c r="H62" s="2"/>
     </row>
-    <row r="63" spans="1:8">
+    <row r="63" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A63" s="1"/>
       <c r="B63" s="2"/>
       <c r="E63" s="3"/>
@@ -3751,7 +3773,7 @@
       <c r="G63" s="2"/>
       <c r="H63" s="2"/>
     </row>
-    <row r="64" spans="1:8">
+    <row r="64" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A64" s="1"/>
       <c r="B64" s="2"/>
       <c r="E64" s="3"/>
@@ -3759,7 +3781,7 @@
       <c r="G64" s="2"/>
       <c r="H64" s="2"/>
     </row>
-    <row r="65" spans="1:8">
+    <row r="65" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A65" s="1"/>
       <c r="B65" s="2"/>
       <c r="E65" s="3"/>
@@ -3767,7 +3789,7 @@
       <c r="G65" s="2"/>
       <c r="H65" s="2"/>
     </row>
-    <row r="66" spans="1:8">
+    <row r="66" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A66" s="1"/>
       <c r="B66" s="2"/>
       <c r="E66" s="3"/>
@@ -3775,7 +3797,7 @@
       <c r="G66" s="2"/>
       <c r="H66" s="2"/>
     </row>
-    <row r="67" spans="1:8">
+    <row r="67" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A67" s="1"/>
       <c r="B67" s="2"/>
       <c r="E67" s="3"/>
@@ -3783,7 +3805,7 @@
       <c r="G67" s="2"/>
       <c r="H67" s="2"/>
     </row>
-    <row r="68" spans="1:8">
+    <row r="68" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A68" s="1"/>
       <c r="B68" s="2"/>
       <c r="E68" s="3"/>
@@ -3791,7 +3813,7 @@
       <c r="G68" s="2"/>
       <c r="H68" s="2"/>
     </row>
-    <row r="69" spans="1:8">
+    <row r="69" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A69" s="1"/>
       <c r="B69" s="2"/>
       <c r="E69" s="3"/>
@@ -3799,7 +3821,7 @@
       <c r="G69" s="2"/>
       <c r="H69" s="2"/>
     </row>
-    <row r="70" spans="1:8">
+    <row r="70" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A70" s="1"/>
       <c r="B70" s="2"/>
       <c r="E70" s="3"/>
@@ -3807,7 +3829,7 @@
       <c r="G70" s="2"/>
       <c r="H70" s="2"/>
     </row>
-    <row r="71" spans="1:8">
+    <row r="71" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A71" s="1"/>
       <c r="B71" s="2"/>
       <c r="E71" s="3"/>
@@ -3815,7 +3837,7 @@
       <c r="G71" s="2"/>
       <c r="H71" s="2"/>
     </row>
-    <row r="72" spans="1:8">
+    <row r="72" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A72" s="1"/>
       <c r="B72" s="2"/>
       <c r="E72" s="3"/>
@@ -3823,7 +3845,7 @@
       <c r="G72" s="2"/>
       <c r="H72" s="2"/>
     </row>
-    <row r="73" spans="1:8">
+    <row r="73" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A73" s="1"/>
       <c r="B73" s="2"/>
       <c r="E73" s="3"/>
@@ -3831,7 +3853,7 @@
       <c r="G73" s="2"/>
       <c r="H73" s="2"/>
     </row>
-    <row r="74" spans="1:8">
+    <row r="74" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A74" s="1"/>
       <c r="B74" s="2"/>
       <c r="E74" s="3"/>
@@ -3839,7 +3861,7 @@
       <c r="G74" s="2"/>
       <c r="H74" s="2"/>
     </row>
-    <row r="75" spans="1:8">
+    <row r="75" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A75" s="1"/>
       <c r="B75" s="2"/>
       <c r="E75" s="3"/>
@@ -3847,7 +3869,7 @@
       <c r="G75" s="2"/>
       <c r="H75" s="2"/>
     </row>
-    <row r="76" spans="1:8">
+    <row r="76" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A76" s="1"/>
       <c r="B76" s="2"/>
       <c r="E76" s="3"/>
@@ -3855,7 +3877,7 @@
       <c r="G76" s="2"/>
       <c r="H76" s="2"/>
     </row>
-    <row r="77" spans="1:8">
+    <row r="77" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A77" s="1"/>
       <c r="B77" s="2"/>
       <c r="E77" s="3"/>
@@ -3863,7 +3885,7 @@
       <c r="G77" s="2"/>
       <c r="H77" s="2"/>
     </row>
-    <row r="78" spans="1:8">
+    <row r="78" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A78" s="1"/>
       <c r="B78" s="2"/>
       <c r="E78" s="3"/>
@@ -3871,7 +3893,7 @@
       <c r="G78" s="2"/>
       <c r="H78" s="2"/>
     </row>
-    <row r="79" spans="1:8">
+    <row r="79" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A79" s="1"/>
       <c r="B79" s="2"/>
       <c r="E79" s="3"/>
@@ -3879,7 +3901,7 @@
       <c r="G79" s="2"/>
       <c r="H79" s="2"/>
     </row>
-    <row r="80" spans="1:8">
+    <row r="80" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A80" s="1"/>
       <c r="B80" s="2"/>
       <c r="E80" s="3"/>
@@ -3887,7 +3909,7 @@
       <c r="G80" s="2"/>
       <c r="H80" s="2"/>
     </row>
-    <row r="81" spans="1:8">
+    <row r="81" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A81" s="1"/>
       <c r="B81" s="2"/>
       <c r="E81" s="3"/>
@@ -3895,7 +3917,7 @@
       <c r="G81" s="2"/>
       <c r="H81" s="2"/>
     </row>
-    <row r="82" spans="1:8">
+    <row r="82" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A82" s="1"/>
       <c r="B82" s="2"/>
       <c r="E82" s="3"/>
@@ -3903,7 +3925,7 @@
       <c r="G82" s="2"/>
       <c r="H82" s="2"/>
     </row>
-    <row r="83" spans="1:8">
+    <row r="83" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A83" s="1"/>
       <c r="B83" s="2"/>
       <c r="E83" s="3"/>
@@ -3911,7 +3933,7 @@
       <c r="G83" s="2"/>
       <c r="H83" s="2"/>
     </row>
-    <row r="84" spans="1:8">
+    <row r="84" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A84" s="1"/>
       <c r="B84" s="2"/>
       <c r="E84" s="3"/>
@@ -3919,7 +3941,7 @@
       <c r="G84" s="2"/>
       <c r="H84" s="2"/>
     </row>
-    <row r="85" spans="1:8">
+    <row r="85" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A85" s="1"/>
       <c r="B85" s="2"/>
       <c r="E85" s="3"/>
@@ -3927,7 +3949,7 @@
       <c r="G85" s="2"/>
       <c r="H85" s="2"/>
     </row>
-    <row r="86" spans="1:8">
+    <row r="86" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A86" s="1"/>
       <c r="B86" s="2"/>
       <c r="E86" s="3"/>
@@ -3935,7 +3957,7 @@
       <c r="G86" s="2"/>
       <c r="H86" s="2"/>
     </row>
-    <row r="87" spans="1:8">
+    <row r="87" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A87" s="1"/>
       <c r="B87" s="2"/>
       <c r="E87" s="3"/>
@@ -3943,7 +3965,7 @@
       <c r="G87" s="2"/>
       <c r="H87" s="2"/>
     </row>
-    <row r="88" spans="1:8">
+    <row r="88" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A88" s="1"/>
       <c r="B88" s="2"/>
       <c r="E88" s="3"/>
@@ -3951,7 +3973,7 @@
       <c r="G88" s="2"/>
       <c r="H88" s="2"/>
     </row>
-    <row r="89" spans="1:8">
+    <row r="89" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A89" s="1"/>
       <c r="B89" s="2"/>
       <c r="E89" s="3"/>
@@ -3959,7 +3981,7 @@
       <c r="G89" s="2"/>
       <c r="H89" s="2"/>
     </row>
-    <row r="90" spans="1:8">
+    <row r="90" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A90" s="1"/>
       <c r="B90" s="2"/>
       <c r="E90" s="3"/>
@@ -3967,7 +3989,7 @@
       <c r="G90" s="2"/>
       <c r="H90" s="2"/>
     </row>
-    <row r="91" spans="1:8">
+    <row r="91" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A91" s="1"/>
       <c r="B91" s="2"/>
       <c r="E91" s="3"/>
@@ -3975,7 +3997,7 @@
       <c r="G91" s="2"/>
       <c r="H91" s="2"/>
     </row>
-    <row r="92" spans="1:8">
+    <row r="92" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A92" s="1"/>
       <c r="B92" s="2"/>
       <c r="E92" s="3"/>
@@ -3983,7 +4005,7 @@
       <c r="G92" s="2"/>
       <c r="H92" s="2"/>
     </row>
-    <row r="93" spans="1:8">
+    <row r="93" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A93" s="1"/>
       <c r="B93" s="2"/>
       <c r="E93" s="3"/>
@@ -3991,7 +4013,7 @@
       <c r="G93" s="2"/>
       <c r="H93" s="2"/>
     </row>
-    <row r="94" spans="1:8">
+    <row r="94" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A94" s="1"/>
       <c r="B94" s="2"/>
       <c r="E94" s="3"/>
@@ -3999,7 +4021,7 @@
       <c r="G94" s="2"/>
       <c r="H94" s="2"/>
     </row>
-    <row r="95" spans="1:8">
+    <row r="95" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A95" s="1"/>
       <c r="B95" s="2"/>
       <c r="E95" s="3"/>
@@ -4007,7 +4029,7 @@
       <c r="G95" s="2"/>
       <c r="H95" s="2"/>
     </row>
-    <row r="96" spans="1:8">
+    <row r="96" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A96" s="1"/>
       <c r="B96" s="2"/>
       <c r="E96" s="3"/>
@@ -4015,7 +4037,7 @@
       <c r="G96" s="2"/>
       <c r="H96" s="2"/>
     </row>
-    <row r="97" spans="1:8">
+    <row r="97" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A97" s="1"/>
       <c r="B97" s="2"/>
       <c r="E97" s="3"/>
@@ -4023,7 +4045,7 @@
       <c r="G97" s="2"/>
       <c r="H97" s="2"/>
     </row>
-    <row r="98" spans="1:8">
+    <row r="98" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A98" s="1"/>
       <c r="B98" s="2"/>
       <c r="E98" s="3"/>
@@ -4031,7 +4053,7 @@
       <c r="G98" s="2"/>
       <c r="H98" s="2"/>
     </row>
-    <row r="99" spans="1:8">
+    <row r="99" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A99" s="1"/>
       <c r="B99" s="2"/>
       <c r="E99" s="3"/>
@@ -4039,7 +4061,7 @@
       <c r="G99" s="2"/>
       <c r="H99" s="2"/>
     </row>
-    <row r="100" spans="1:8">
+    <row r="100" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A100" s="1"/>
       <c r="B100" s="2"/>
       <c r="E100" s="3"/>
@@ -4082,21 +4104,21 @@
       <selection activeCell="P21" sqref="P21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.88671875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.88671875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="19.44140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.5546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.5546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.5703125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="9" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="17.88671875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="17.85546875" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="17" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="19.109375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="19.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="15.6">
+    <row r="1" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="7" t="s">
         <v>8</v>
       </c>
@@ -4128,7 +4150,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:10">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="2"/>
       <c r="B2" s="8"/>
       <c r="D2" s="2"/>
@@ -4136,7 +4158,7 @@
       <c r="I2" s="8"/>
       <c r="J2" s="2"/>
     </row>
-    <row r="3" spans="1:10">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="2"/>
       <c r="B3" s="8"/>
       <c r="D3" s="2"/>
@@ -4144,7 +4166,7 @@
       <c r="I3" s="8"/>
       <c r="J3" s="2"/>
     </row>
-    <row r="4" spans="1:10">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="2"/>
       <c r="B4" s="8"/>
       <c r="D4" s="2"/>
@@ -4152,7 +4174,7 @@
       <c r="I4" s="8"/>
       <c r="J4" s="2"/>
     </row>
-    <row r="5" spans="1:10">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" s="2"/>
       <c r="B5" s="8"/>
       <c r="D5" s="2"/>
@@ -4160,7 +4182,7 @@
       <c r="I5" s="8"/>
       <c r="J5" s="2"/>
     </row>
-    <row r="6" spans="1:10">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" s="2"/>
       <c r="B6" s="8"/>
       <c r="D6" s="2"/>
@@ -4168,7 +4190,7 @@
       <c r="I6" s="8"/>
       <c r="J6" s="2"/>
     </row>
-    <row r="7" spans="1:10">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" s="2"/>
       <c r="B7" s="8"/>
       <c r="D7" s="2"/>
@@ -4176,7 +4198,7 @@
       <c r="I7" s="8"/>
       <c r="J7" s="2"/>
     </row>
-    <row r="8" spans="1:10">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" s="2"/>
       <c r="B8" s="8"/>
       <c r="D8" s="2"/>
@@ -4184,7 +4206,7 @@
       <c r="I8" s="8"/>
       <c r="J8" s="2"/>
     </row>
-    <row r="9" spans="1:10">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" s="2"/>
       <c r="B9" s="8"/>
       <c r="D9" s="2"/>
@@ -4192,7 +4214,7 @@
       <c r="I9" s="8"/>
       <c r="J9" s="2"/>
     </row>
-    <row r="10" spans="1:10">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" s="2"/>
       <c r="B10" s="8"/>
       <c r="D10" s="2"/>
@@ -4200,7 +4222,7 @@
       <c r="I10" s="8"/>
       <c r="J10" s="2"/>
     </row>
-    <row r="11" spans="1:10">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" s="2"/>
       <c r="B11" s="8"/>
       <c r="D11" s="2"/>
@@ -4208,7 +4230,7 @@
       <c r="I11" s="8"/>
       <c r="J11" s="2"/>
     </row>
-    <row r="12" spans="1:10">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" s="2"/>
       <c r="B12" s="8"/>
       <c r="D12" s="2"/>
@@ -4216,7 +4238,7 @@
       <c r="I12" s="8"/>
       <c r="J12" s="2"/>
     </row>
-    <row r="13" spans="1:10">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" s="2"/>
       <c r="B13" s="8"/>
       <c r="D13" s="2"/>
@@ -4224,7 +4246,7 @@
       <c r="I13" s="8"/>
       <c r="J13" s="2"/>
     </row>
-    <row r="14" spans="1:10">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" s="2"/>
       <c r="B14" s="8"/>
       <c r="D14" s="2"/>
@@ -4232,7 +4254,7 @@
       <c r="I14" s="8"/>
       <c r="J14" s="2"/>
     </row>
-    <row r="15" spans="1:10">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" s="2"/>
       <c r="B15" s="8"/>
       <c r="D15" s="2"/>
@@ -4240,7 +4262,7 @@
       <c r="I15" s="8"/>
       <c r="J15" s="2"/>
     </row>
-    <row r="16" spans="1:10">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" s="2"/>
       <c r="B16" s="8"/>
       <c r="D16" s="2"/>
@@ -4248,7 +4270,7 @@
       <c r="I16" s="8"/>
       <c r="J16" s="2"/>
     </row>
-    <row r="17" spans="1:10">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17" s="2"/>
       <c r="B17" s="8"/>
       <c r="D17" s="2"/>
@@ -4256,7 +4278,7 @@
       <c r="I17" s="8"/>
       <c r="J17" s="2"/>
     </row>
-    <row r="18" spans="1:10">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18" s="2"/>
       <c r="B18" s="8"/>
       <c r="D18" s="2"/>
@@ -4264,7 +4286,7 @@
       <c r="I18" s="8"/>
       <c r="J18" s="2"/>
     </row>
-    <row r="19" spans="1:10">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A19" s="2"/>
       <c r="B19" s="8"/>
       <c r="D19" s="2"/>
@@ -4272,7 +4294,7 @@
       <c r="I19" s="8"/>
       <c r="J19" s="2"/>
     </row>
-    <row r="20" spans="1:10">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A20" s="2"/>
       <c r="B20" s="8"/>
       <c r="D20" s="2"/>
@@ -4280,7 +4302,7 @@
       <c r="I20" s="8"/>
       <c r="J20" s="2"/>
     </row>
-    <row r="21" spans="1:10">
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A21" s="2"/>
       <c r="B21" s="8"/>
       <c r="D21" s="2"/>
@@ -4288,7 +4310,7 @@
       <c r="I21" s="8"/>
       <c r="J21" s="2"/>
     </row>
-    <row r="22" spans="1:10">
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A22" s="2"/>
       <c r="B22" s="8"/>
       <c r="D22" s="2"/>
@@ -4296,7 +4318,7 @@
       <c r="I22" s="8"/>
       <c r="J22" s="2"/>
     </row>
-    <row r="23" spans="1:10">
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A23" s="2"/>
       <c r="B23" s="8"/>
       <c r="D23" s="2"/>
@@ -4304,7 +4326,7 @@
       <c r="I23" s="8"/>
       <c r="J23" s="2"/>
     </row>
-    <row r="24" spans="1:10">
+    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A24" s="2"/>
       <c r="B24" s="8"/>
       <c r="D24" s="2"/>
@@ -4312,7 +4334,7 @@
       <c r="I24" s="8"/>
       <c r="J24" s="2"/>
     </row>
-    <row r="25" spans="1:10">
+    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A25" s="2"/>
       <c r="B25" s="8"/>
       <c r="D25" s="2"/>
@@ -4320,7 +4342,7 @@
       <c r="I25" s="8"/>
       <c r="J25" s="2"/>
     </row>
-    <row r="26" spans="1:10">
+    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A26" s="2"/>
       <c r="B26" s="8"/>
       <c r="D26" s="2"/>
@@ -4328,7 +4350,7 @@
       <c r="I26" s="8"/>
       <c r="J26" s="2"/>
     </row>
-    <row r="27" spans="1:10">
+    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A27" s="2"/>
       <c r="B27" s="8"/>
       <c r="D27" s="2"/>
@@ -4336,7 +4358,7 @@
       <c r="I27" s="8"/>
       <c r="J27" s="2"/>
     </row>
-    <row r="28" spans="1:10">
+    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A28" s="2"/>
       <c r="B28" s="8"/>
       <c r="D28" s="2"/>
@@ -4344,7 +4366,7 @@
       <c r="I28" s="8"/>
       <c r="J28" s="2"/>
     </row>
-    <row r="29" spans="1:10">
+    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A29" s="2"/>
       <c r="B29" s="8"/>
       <c r="D29" s="2"/>
@@ -4352,7 +4374,7 @@
       <c r="I29" s="8"/>
       <c r="J29" s="2"/>
     </row>
-    <row r="30" spans="1:10">
+    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A30" s="2"/>
       <c r="B30" s="8"/>
       <c r="D30" s="2"/>
@@ -4360,7 +4382,7 @@
       <c r="I30" s="8"/>
       <c r="J30" s="2"/>
     </row>
-    <row r="31" spans="1:10">
+    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A31" s="2"/>
       <c r="B31" s="8"/>
       <c r="D31" s="2"/>
@@ -4368,7 +4390,7 @@
       <c r="I31" s="8"/>
       <c r="J31" s="2"/>
     </row>
-    <row r="32" spans="1:10">
+    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A32" s="2"/>
       <c r="B32" s="8"/>
       <c r="D32" s="2"/>
@@ -4376,7 +4398,7 @@
       <c r="I32" s="8"/>
       <c r="J32" s="2"/>
     </row>
-    <row r="33" spans="1:10">
+    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A33" s="2"/>
       <c r="B33" s="8"/>
       <c r="D33" s="2"/>
@@ -4384,7 +4406,7 @@
       <c r="I33" s="8"/>
       <c r="J33" s="2"/>
     </row>
-    <row r="34" spans="1:10">
+    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A34" s="2"/>
       <c r="B34" s="8"/>
       <c r="D34" s="2"/>
@@ -4392,7 +4414,7 @@
       <c r="I34" s="8"/>
       <c r="J34" s="2"/>
     </row>
-    <row r="35" spans="1:10">
+    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A35" s="2"/>
       <c r="B35" s="8"/>
       <c r="D35" s="2"/>
@@ -4400,7 +4422,7 @@
       <c r="I35" s="8"/>
       <c r="J35" s="2"/>
     </row>
-    <row r="36" spans="1:10">
+    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A36" s="2"/>
       <c r="B36" s="8"/>
       <c r="D36" s="2"/>
@@ -4408,7 +4430,7 @@
       <c r="I36" s="8"/>
       <c r="J36" s="2"/>
     </row>
-    <row r="37" spans="1:10">
+    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A37" s="2"/>
       <c r="B37" s="8"/>
       <c r="D37" s="2"/>
@@ -4416,7 +4438,7 @@
       <c r="I37" s="8"/>
       <c r="J37" s="2"/>
     </row>
-    <row r="38" spans="1:10">
+    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A38" s="2"/>
       <c r="B38" s="8"/>
       <c r="D38" s="2"/>
@@ -4424,7 +4446,7 @@
       <c r="I38" s="8"/>
       <c r="J38" s="2"/>
     </row>
-    <row r="39" spans="1:10">
+    <row r="39" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A39" s="2"/>
       <c r="B39" s="8"/>
       <c r="D39" s="2"/>
@@ -4432,7 +4454,7 @@
       <c r="I39" s="8"/>
       <c r="J39" s="2"/>
     </row>
-    <row r="40" spans="1:10">
+    <row r="40" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A40" s="2"/>
       <c r="B40" s="8"/>
       <c r="D40" s="2"/>
@@ -4440,7 +4462,7 @@
       <c r="I40" s="8"/>
       <c r="J40" s="2"/>
     </row>
-    <row r="41" spans="1:10">
+    <row r="41" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A41" s="2"/>
       <c r="B41" s="8"/>
       <c r="D41" s="2"/>
@@ -4448,7 +4470,7 @@
       <c r="I41" s="8"/>
       <c r="J41" s="2"/>
     </row>
-    <row r="42" spans="1:10">
+    <row r="42" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A42" s="2"/>
       <c r="B42" s="8"/>
       <c r="D42" s="2"/>
@@ -4456,7 +4478,7 @@
       <c r="I42" s="8"/>
       <c r="J42" s="2"/>
     </row>
-    <row r="43" spans="1:10">
+    <row r="43" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A43" s="2"/>
       <c r="B43" s="8"/>
       <c r="D43" s="2"/>
@@ -4464,7 +4486,7 @@
       <c r="I43" s="8"/>
       <c r="J43" s="2"/>
     </row>
-    <row r="44" spans="1:10">
+    <row r="44" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A44" s="2"/>
       <c r="B44" s="8"/>
       <c r="D44" s="2"/>
@@ -4472,7 +4494,7 @@
       <c r="I44" s="8"/>
       <c r="J44" s="2"/>
     </row>
-    <row r="45" spans="1:10">
+    <row r="45" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A45" s="2"/>
       <c r="B45" s="8"/>
       <c r="D45" s="2"/>
@@ -4480,7 +4502,7 @@
       <c r="I45" s="8"/>
       <c r="J45" s="2"/>
     </row>
-    <row r="46" spans="1:10">
+    <row r="46" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A46" s="2"/>
       <c r="B46" s="8"/>
       <c r="D46" s="2"/>
@@ -4488,7 +4510,7 @@
       <c r="I46" s="8"/>
       <c r="J46" s="2"/>
     </row>
-    <row r="47" spans="1:10">
+    <row r="47" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A47" s="2"/>
       <c r="B47" s="8"/>
       <c r="D47" s="2"/>
@@ -4496,7 +4518,7 @@
       <c r="I47" s="8"/>
       <c r="J47" s="2"/>
     </row>
-    <row r="48" spans="1:10">
+    <row r="48" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A48" s="2"/>
       <c r="B48" s="8"/>
       <c r="D48" s="2"/>
@@ -4504,7 +4526,7 @@
       <c r="I48" s="8"/>
       <c r="J48" s="2"/>
     </row>
-    <row r="49" spans="1:10">
+    <row r="49" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A49" s="2"/>
       <c r="B49" s="8"/>
       <c r="D49" s="2"/>
@@ -4512,7 +4534,7 @@
       <c r="I49" s="8"/>
       <c r="J49" s="2"/>
     </row>
-    <row r="50" spans="1:10">
+    <row r="50" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A50" s="2"/>
       <c r="B50" s="8"/>
       <c r="D50" s="2"/>
@@ -4520,7 +4542,7 @@
       <c r="I50" s="8"/>
       <c r="J50" s="2"/>
     </row>
-    <row r="51" spans="1:10">
+    <row r="51" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A51" s="2"/>
       <c r="B51" s="8"/>
       <c r="D51" s="2"/>
@@ -4528,7 +4550,7 @@
       <c r="I51" s="8"/>
       <c r="J51" s="2"/>
     </row>
-    <row r="52" spans="1:10">
+    <row r="52" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A52" s="2"/>
       <c r="B52" s="8"/>
       <c r="D52" s="2"/>
@@ -4536,7 +4558,7 @@
       <c r="I52" s="8"/>
       <c r="J52" s="2"/>
     </row>
-    <row r="53" spans="1:10">
+    <row r="53" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A53" s="2"/>
       <c r="B53" s="8"/>
       <c r="D53" s="2"/>
@@ -4544,7 +4566,7 @@
       <c r="I53" s="8"/>
       <c r="J53" s="2"/>
     </row>
-    <row r="54" spans="1:10">
+    <row r="54" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A54" s="2"/>
       <c r="B54" s="8"/>
       <c r="D54" s="2"/>
@@ -4552,7 +4574,7 @@
       <c r="I54" s="8"/>
       <c r="J54" s="2"/>
     </row>
-    <row r="55" spans="1:10">
+    <row r="55" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A55" s="2"/>
       <c r="B55" s="8"/>
       <c r="D55" s="2"/>
@@ -4560,7 +4582,7 @@
       <c r="I55" s="8"/>
       <c r="J55" s="2"/>
     </row>
-    <row r="56" spans="1:10">
+    <row r="56" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A56" s="2"/>
       <c r="B56" s="8"/>
       <c r="D56" s="2"/>
@@ -4568,7 +4590,7 @@
       <c r="I56" s="8"/>
       <c r="J56" s="2"/>
     </row>
-    <row r="57" spans="1:10">
+    <row r="57" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A57" s="2"/>
       <c r="B57" s="8"/>
       <c r="D57" s="2"/>
@@ -4576,7 +4598,7 @@
       <c r="I57" s="8"/>
       <c r="J57" s="2"/>
     </row>
-    <row r="58" spans="1:10">
+    <row r="58" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A58" s="2"/>
       <c r="B58" s="8"/>
       <c r="D58" s="2"/>
@@ -4584,7 +4606,7 @@
       <c r="I58" s="8"/>
       <c r="J58" s="2"/>
     </row>
-    <row r="59" spans="1:10">
+    <row r="59" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A59" s="2"/>
       <c r="B59" s="8"/>
       <c r="D59" s="2"/>
@@ -4592,7 +4614,7 @@
       <c r="I59" s="8"/>
       <c r="J59" s="2"/>
     </row>
-    <row r="60" spans="1:10">
+    <row r="60" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A60" s="2"/>
       <c r="B60" s="8"/>
       <c r="D60" s="2"/>
@@ -4600,7 +4622,7 @@
       <c r="I60" s="8"/>
       <c r="J60" s="2"/>
     </row>
-    <row r="61" spans="1:10">
+    <row r="61" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A61" s="2"/>
       <c r="B61" s="8"/>
       <c r="D61" s="2"/>
@@ -4608,7 +4630,7 @@
       <c r="I61" s="8"/>
       <c r="J61" s="2"/>
     </row>
-    <row r="62" spans="1:10">
+    <row r="62" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A62" s="2"/>
       <c r="B62" s="8"/>
       <c r="D62" s="2"/>
@@ -4616,7 +4638,7 @@
       <c r="I62" s="8"/>
       <c r="J62" s="2"/>
     </row>
-    <row r="63" spans="1:10">
+    <row r="63" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A63" s="2"/>
       <c r="B63" s="8"/>
       <c r="D63" s="2"/>
@@ -4624,7 +4646,7 @@
       <c r="I63" s="8"/>
       <c r="J63" s="2"/>
     </row>
-    <row r="64" spans="1:10">
+    <row r="64" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A64" s="2"/>
       <c r="B64" s="8"/>
       <c r="D64" s="2"/>
@@ -4632,7 +4654,7 @@
       <c r="I64" s="8"/>
       <c r="J64" s="2"/>
     </row>
-    <row r="65" spans="1:10">
+    <row r="65" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A65" s="2"/>
       <c r="B65" s="8"/>
       <c r="D65" s="2"/>
@@ -4640,7 +4662,7 @@
       <c r="I65" s="8"/>
       <c r="J65" s="2"/>
     </row>
-    <row r="66" spans="1:10">
+    <row r="66" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A66" s="2"/>
       <c r="B66" s="8"/>
       <c r="D66" s="2"/>
@@ -4648,7 +4670,7 @@
       <c r="I66" s="8"/>
       <c r="J66" s="2"/>
     </row>
-    <row r="67" spans="1:10">
+    <row r="67" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A67" s="2"/>
       <c r="B67" s="8"/>
       <c r="D67" s="2"/>
@@ -4656,7 +4678,7 @@
       <c r="I67" s="8"/>
       <c r="J67" s="2"/>
     </row>
-    <row r="68" spans="1:10">
+    <row r="68" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A68" s="2"/>
       <c r="B68" s="8"/>
       <c r="D68" s="2"/>
@@ -4664,7 +4686,7 @@
       <c r="I68" s="8"/>
       <c r="J68" s="2"/>
     </row>
-    <row r="69" spans="1:10">
+    <row r="69" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A69" s="2"/>
       <c r="B69" s="8"/>
       <c r="D69" s="2"/>
@@ -4672,7 +4694,7 @@
       <c r="I69" s="8"/>
       <c r="J69" s="2"/>
     </row>
-    <row r="70" spans="1:10">
+    <row r="70" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A70" s="2"/>
       <c r="B70" s="8"/>
       <c r="D70" s="2"/>
@@ -4680,7 +4702,7 @@
       <c r="I70" s="8"/>
       <c r="J70" s="2"/>
     </row>
-    <row r="71" spans="1:10">
+    <row r="71" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A71" s="2"/>
       <c r="B71" s="8"/>
       <c r="D71" s="2"/>
@@ -4688,7 +4710,7 @@
       <c r="I71" s="8"/>
       <c r="J71" s="2"/>
     </row>
-    <row r="72" spans="1:10">
+    <row r="72" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A72" s="2"/>
       <c r="B72" s="8"/>
       <c r="D72" s="2"/>
@@ -4696,7 +4718,7 @@
       <c r="I72" s="8"/>
       <c r="J72" s="2"/>
     </row>
-    <row r="73" spans="1:10">
+    <row r="73" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A73" s="2"/>
       <c r="B73" s="8"/>
       <c r="D73" s="2"/>
@@ -4704,7 +4726,7 @@
       <c r="I73" s="8"/>
       <c r="J73" s="2"/>
     </row>
-    <row r="74" spans="1:10">
+    <row r="74" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A74" s="2"/>
       <c r="B74" s="8"/>
       <c r="D74" s="2"/>
@@ -4712,7 +4734,7 @@
       <c r="I74" s="8"/>
       <c r="J74" s="2"/>
     </row>
-    <row r="75" spans="1:10">
+    <row r="75" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A75" s="2"/>
       <c r="B75" s="8"/>
       <c r="D75" s="2"/>
@@ -4720,7 +4742,7 @@
       <c r="I75" s="8"/>
       <c r="J75" s="2"/>
     </row>
-    <row r="76" spans="1:10">
+    <row r="76" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A76" s="2"/>
       <c r="B76" s="8"/>
       <c r="D76" s="2"/>
@@ -4728,7 +4750,7 @@
       <c r="I76" s="8"/>
       <c r="J76" s="2"/>
     </row>
-    <row r="77" spans="1:10">
+    <row r="77" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A77" s="2"/>
       <c r="B77" s="8"/>
       <c r="D77" s="2"/>
@@ -4736,7 +4758,7 @@
       <c r="I77" s="8"/>
       <c r="J77" s="2"/>
     </row>
-    <row r="78" spans="1:10">
+    <row r="78" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A78" s="2"/>
       <c r="B78" s="8"/>
       <c r="D78" s="2"/>
@@ -4744,7 +4766,7 @@
       <c r="I78" s="8"/>
       <c r="J78" s="2"/>
     </row>
-    <row r="79" spans="1:10">
+    <row r="79" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A79" s="2"/>
       <c r="B79" s="8"/>
       <c r="D79" s="2"/>
@@ -4752,7 +4774,7 @@
       <c r="I79" s="8"/>
       <c r="J79" s="2"/>
     </row>
-    <row r="80" spans="1:10">
+    <row r="80" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A80" s="2"/>
       <c r="B80" s="8"/>
       <c r="D80" s="2"/>
@@ -4760,7 +4782,7 @@
       <c r="I80" s="8"/>
       <c r="J80" s="2"/>
     </row>
-    <row r="81" spans="1:10">
+    <row r="81" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A81" s="2"/>
       <c r="B81" s="8"/>
       <c r="D81" s="2"/>
@@ -4768,7 +4790,7 @@
       <c r="I81" s="8"/>
       <c r="J81" s="2"/>
     </row>
-    <row r="82" spans="1:10">
+    <row r="82" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A82" s="2"/>
       <c r="B82" s="8"/>
       <c r="D82" s="2"/>
@@ -4776,7 +4798,7 @@
       <c r="I82" s="8"/>
       <c r="J82" s="2"/>
     </row>
-    <row r="83" spans="1:10">
+    <row r="83" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A83" s="2"/>
       <c r="B83" s="8"/>
       <c r="D83" s="2"/>
@@ -4784,7 +4806,7 @@
       <c r="I83" s="8"/>
       <c r="J83" s="2"/>
     </row>
-    <row r="84" spans="1:10">
+    <row r="84" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A84" s="2"/>
       <c r="B84" s="8"/>
       <c r="D84" s="2"/>
@@ -4792,7 +4814,7 @@
       <c r="I84" s="8"/>
       <c r="J84" s="2"/>
     </row>
-    <row r="85" spans="1:10">
+    <row r="85" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A85" s="2"/>
       <c r="B85" s="8"/>
       <c r="D85" s="2"/>
@@ -4800,7 +4822,7 @@
       <c r="I85" s="8"/>
       <c r="J85" s="2"/>
     </row>
-    <row r="86" spans="1:10">
+    <row r="86" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A86" s="2"/>
       <c r="B86" s="8"/>
       <c r="D86" s="2"/>
@@ -4808,7 +4830,7 @@
       <c r="I86" s="8"/>
       <c r="J86" s="2"/>
     </row>
-    <row r="87" spans="1:10">
+    <row r="87" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A87" s="2"/>
       <c r="B87" s="8"/>
       <c r="D87" s="2"/>
@@ -4816,7 +4838,7 @@
       <c r="I87" s="8"/>
       <c r="J87" s="2"/>
     </row>
-    <row r="88" spans="1:10">
+    <row r="88" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A88" s="2"/>
       <c r="B88" s="8"/>
       <c r="D88" s="2"/>
@@ -4824,7 +4846,7 @@
       <c r="I88" s="8"/>
       <c r="J88" s="2"/>
     </row>
-    <row r="89" spans="1:10">
+    <row r="89" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A89" s="2"/>
       <c r="B89" s="8"/>
       <c r="D89" s="2"/>
@@ -4832,7 +4854,7 @@
       <c r="I89" s="8"/>
       <c r="J89" s="2"/>
     </row>
-    <row r="90" spans="1:10">
+    <row r="90" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A90" s="2"/>
       <c r="B90" s="8"/>
       <c r="D90" s="2"/>
@@ -4840,7 +4862,7 @@
       <c r="I90" s="8"/>
       <c r="J90" s="2"/>
     </row>
-    <row r="91" spans="1:10">
+    <row r="91" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A91" s="2"/>
       <c r="B91" s="8"/>
       <c r="D91" s="2"/>
@@ -4848,7 +4870,7 @@
       <c r="I91" s="8"/>
       <c r="J91" s="2"/>
     </row>
-    <row r="92" spans="1:10">
+    <row r="92" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A92" s="2"/>
       <c r="B92" s="8"/>
       <c r="D92" s="2"/>
@@ -4856,7 +4878,7 @@
       <c r="I92" s="8"/>
       <c r="J92" s="2"/>
     </row>
-    <row r="93" spans="1:10">
+    <row r="93" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A93" s="2"/>
       <c r="B93" s="8"/>
       <c r="D93" s="2"/>
@@ -4864,7 +4886,7 @@
       <c r="I93" s="8"/>
       <c r="J93" s="2"/>
     </row>
-    <row r="94" spans="1:10">
+    <row r="94" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A94" s="2"/>
       <c r="B94" s="8"/>
       <c r="D94" s="2"/>
@@ -4872,7 +4894,7 @@
       <c r="I94" s="8"/>
       <c r="J94" s="2"/>
     </row>
-    <row r="95" spans="1:10">
+    <row r="95" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A95" s="2"/>
       <c r="B95" s="8"/>
       <c r="D95" s="2"/>
@@ -4880,7 +4902,7 @@
       <c r="I95" s="8"/>
       <c r="J95" s="2"/>
     </row>
-    <row r="96" spans="1:10">
+    <row r="96" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A96" s="2"/>
       <c r="B96" s="8"/>
       <c r="D96" s="2"/>
@@ -4888,7 +4910,7 @@
       <c r="I96" s="8"/>
       <c r="J96" s="2"/>
     </row>
-    <row r="97" spans="1:10">
+    <row r="97" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A97" s="2"/>
       <c r="B97" s="8"/>
       <c r="D97" s="2"/>
@@ -4896,7 +4918,7 @@
       <c r="I97" s="8"/>
       <c r="J97" s="2"/>
     </row>
-    <row r="98" spans="1:10">
+    <row r="98" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A98" s="2"/>
       <c r="B98" s="8"/>
       <c r="D98" s="2"/>
@@ -4904,7 +4926,7 @@
       <c r="I98" s="8"/>
       <c r="J98" s="2"/>
     </row>
-    <row r="99" spans="1:10">
+    <row r="99" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A99" s="2"/>
       <c r="B99" s="8"/>
       <c r="D99" s="2"/>
@@ -4912,7 +4934,7 @@
       <c r="I99" s="8"/>
       <c r="J99" s="2"/>
     </row>
-    <row r="100" spans="1:10">
+    <row r="100" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A100" s="2"/>
       <c r="B100" s="8"/>
       <c r="D100" s="2"/>

</xml_diff>

<commit_message>
Corrected database model primary keys and improved seeding script robustness for program/subprogram relationships, file encoding, and entity creation order.
</commit_message>
<xml_diff>
--- a/PR&IR.xlsx
+++ b/PR&IR.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\avichal avneel nath\Documents\Semester 7\CS415\A3\CS415_A3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B56B9EB-9104-48BD-945A-B6FAC90D9711}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF4C5E19-B462-46FA-9470-AAC7E0CCEE8D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{BFA1E21A-08FA-4F02-8C25-33C81C8EE970}"/>
   </bookViews>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="153" uniqueCount="90">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="163" uniqueCount="95">
   <si>
     <t>Date</t>
   </si>
@@ -337,6 +337,21 @@
   </si>
   <si>
     <t xml:space="preserve">Not interested </t>
+  </si>
+  <si>
+    <t>interated jayshils feild code for student profile with mine. Added photo icon in the student profile page. Pulled jayshils code.</t>
+  </si>
+  <si>
+    <t>Integrated jayshils login code in my StudentService</t>
+  </si>
+  <si>
+    <t>Need 2 days time to study for cs310 PLEASEEEEEEEEEEEEEEEEEEEEE</t>
+  </si>
+  <si>
+    <t>fixed the Program model's primary key and adjusted relationships in model.py. The seed_db.py script was updated to ensure correct program and subprogram seeding order and linkage. Database pathing was made robust, creating necessary directories. Unicode errors were resolved by specifying UTF-8 encoding for the JSON file. Finally, data loading for all entities improved with better ID handling and fallbacks.</t>
+  </si>
+  <si>
+    <t>Link fronted with Backend</t>
   </si>
 </sst>
 </file>
@@ -1087,7 +1102,7 @@
   <dimension ref="A1:H28"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="F18" sqref="F18"/>
+      <selection activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1417,8 +1432,24 @@
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="E15"/>
-      <c r="F15"/>
+      <c r="A15" s="1">
+        <v>45799</v>
+      </c>
+      <c r="C15" t="s">
+        <v>93</v>
+      </c>
+      <c r="D15" t="s">
+        <v>17</v>
+      </c>
+      <c r="E15">
+        <v>100</v>
+      </c>
+      <c r="F15">
+        <v>3</v>
+      </c>
+      <c r="G15" s="2" t="s">
+        <v>94</v>
+      </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="E16"/>
@@ -1480,7 +1511,7 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
   <ignoredErrors>
-    <ignoredError sqref="D15:D16" listDataValidation="1"/>
+    <ignoredError sqref="D16" listDataValidation="1"/>
   </ignoredErrors>
   <tableParts count="1">
     <tablePart r:id="rId2"/>
@@ -1492,15 +1523,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3BDA6702-5DDF-42FB-988E-13FBEB26F5C9}">
   <dimension ref="A1:H100"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H7" sqref="H7"/>
+    <sheetView topLeftCell="A2" zoomScale="102" zoomScaleNormal="102" workbookViewId="0">
+      <selection activeCell="H10" sqref="H10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16.140625" customWidth="1"/>
     <col min="2" max="2" width="17.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="55.5703125" customWidth="1"/>
+    <col min="3" max="3" width="93.140625" customWidth="1"/>
     <col min="4" max="4" width="10.5703125" customWidth="1"/>
     <col min="5" max="5" width="14.85546875" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="14.28515625" customWidth="1"/>
@@ -1685,16 +1716,50 @@
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A8" s="8"/>
-      <c r="B8" s="2"/>
+      <c r="A8" s="8">
+        <v>45798</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="C8" t="s">
+        <v>90</v>
+      </c>
+      <c r="D8" t="s">
+        <v>17</v>
+      </c>
+      <c r="E8">
+        <v>100</v>
+      </c>
+      <c r="F8">
+        <v>8</v>
+      </c>
       <c r="G8" s="2"/>
       <c r="H8" s="2"/>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A9" s="8"/>
-      <c r="B9" s="2"/>
+      <c r="A9" s="8">
+        <v>45799</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="C9" t="s">
+        <v>91</v>
+      </c>
+      <c r="D9" t="s">
+        <v>17</v>
+      </c>
+      <c r="E9">
+        <v>100</v>
+      </c>
+      <c r="F9">
+        <v>8</v>
+      </c>
       <c r="G9" s="2"/>
-      <c r="H9" s="2"/>
+      <c r="H9" s="2" t="s">
+        <v>92</v>
+      </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="8"/>
@@ -2261,7 +2326,7 @@
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <ignoredErrors>
-    <ignoredError sqref="D8:D100" listDataValidation="1"/>
+    <ignoredError sqref="D10:D100" listDataValidation="1"/>
   </ignoredErrors>
   <tableParts count="1">
     <tablePart r:id="rId1"/>
@@ -2274,7 +2339,7 @@
   <dimension ref="A1:H100"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Add/update progress report for 23/05/2025 Fri by Shivya
</commit_message>
<xml_diff>
--- a/PR&IR.xlsx
+++ b/PR&IR.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28623"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26026"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\avichal avneel nath\Documents\Semester 7\CS415\A3\CS415_A3\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SHIVYA KUMAR\Desktop\new415\CS415_A3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF4C5E19-B462-46FA-9470-AAC7E0CCEE8D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{86D61A9A-B9C4-47B4-A459-F33798A920ED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{BFA1E21A-08FA-4F02-8C25-33C81C8EE970}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{BFA1E21A-08FA-4F02-8C25-33C81C8EE970}"/>
   </bookViews>
   <sheets>
     <sheet name="Avichal" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="163" uniqueCount="95">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="167" uniqueCount="97">
   <si>
     <t>Date</t>
   </si>
@@ -353,6 +353,12 @@
   <si>
     <t>Link fronted with Backend</t>
   </si>
+  <si>
+    <t>Changed the UI of the finance page from the dropdowns lists into card formats. Added copyright and contact us page</t>
+  </si>
+  <si>
+    <t>Need time for revision, too much work loads due to others units</t>
+  </si>
 </sst>
 </file>
 
@@ -362,7 +368,7 @@
     <numFmt numFmtId="164" formatCode="h"/>
     <numFmt numFmtId="165" formatCode="d/mm/yyyy;@"/>
   </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="3">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1101,30 +1107,30 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{37EAA098-74C6-4411-B7E2-26AD2DCBC3F0}">
   <dimension ref="A1:H28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+    <sheetView topLeftCell="A7" workbookViewId="0">
       <selection activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="10.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.5703125" style="2" customWidth="1"/>
+    <col min="1" max="1" width="10.44140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.5546875" style="2" customWidth="1"/>
     <col min="3" max="3" width="58" customWidth="1"/>
-    <col min="5" max="5" width="13.140625" style="3" customWidth="1"/>
-    <col min="6" max="6" width="20.85546875" style="4" customWidth="1"/>
-    <col min="7" max="7" width="34.85546875" style="2" customWidth="1"/>
-    <col min="8" max="8" width="43.42578125" style="2" customWidth="1"/>
-    <col min="11" max="11" width="9.140625" customWidth="1"/>
-    <col min="12" max="12" width="13.28515625" customWidth="1"/>
-    <col min="13" max="13" width="11.42578125" customWidth="1"/>
-    <col min="14" max="14" width="17.42578125" customWidth="1"/>
-    <col min="16" max="16" width="9.140625" customWidth="1"/>
-    <col min="18" max="18" width="16.5703125" customWidth="1"/>
-    <col min="19" max="19" width="14.7109375" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="16.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.109375" style="3" customWidth="1"/>
+    <col min="6" max="6" width="20.88671875" style="4" customWidth="1"/>
+    <col min="7" max="7" width="34.88671875" style="2" customWidth="1"/>
+    <col min="8" max="8" width="43.44140625" style="2" customWidth="1"/>
+    <col min="11" max="11" width="9.109375" customWidth="1"/>
+    <col min="12" max="12" width="13.33203125" customWidth="1"/>
+    <col min="13" max="13" width="11.44140625" customWidth="1"/>
+    <col min="14" max="14" width="17.44140625" customWidth="1"/>
+    <col min="16" max="16" width="9.109375" customWidth="1"/>
+    <col min="18" max="18" width="16.5546875" customWidth="1"/>
+    <col min="19" max="19" width="14.6640625" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="16.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" ht="15.6">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
@@ -1150,7 +1156,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="15.75" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:8">
       <c r="A2" s="1">
         <v>45786</v>
       </c>
@@ -1176,7 +1182,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="3" spans="1:8" ht="120" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" ht="115.2">
       <c r="A3" s="1">
         <v>45787</v>
       </c>
@@ -1199,7 +1205,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8">
       <c r="A4" s="1">
         <v>45788</v>
       </c>
@@ -1219,7 +1225,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="5" spans="1:8" ht="76.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" ht="76.5" customHeight="1">
       <c r="A5" s="1">
         <v>45789</v>
       </c>
@@ -1242,7 +1248,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8">
       <c r="A6" s="1">
         <v>45790</v>
       </c>
@@ -1265,7 +1271,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8">
       <c r="A7" s="1">
         <v>45791</v>
       </c>
@@ -1288,7 +1294,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8">
       <c r="A8" s="1">
         <v>45792</v>
       </c>
@@ -1311,7 +1317,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8">
       <c r="A9" s="1">
         <v>45793</v>
       </c>
@@ -1331,7 +1337,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8">
       <c r="A10" s="1">
         <v>45794</v>
       </c>
@@ -1351,7 +1357,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8">
       <c r="A11" s="1">
         <v>45795</v>
       </c>
@@ -1371,7 +1377,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8">
       <c r="A12" s="1">
         <v>45796</v>
       </c>
@@ -1391,7 +1397,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="13" spans="1:8" ht="68.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8" ht="68.25" customHeight="1">
       <c r="A13" s="1">
         <v>45797</v>
       </c>
@@ -1411,7 +1417,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="14" spans="1:8" ht="60" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8" ht="60" customHeight="1">
       <c r="A14" s="1">
         <v>45798</v>
       </c>
@@ -1431,7 +1437,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8">
       <c r="A15" s="1">
         <v>45799</v>
       </c>
@@ -1451,44 +1457,44 @@
         <v>94</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8">
       <c r="E16"/>
       <c r="F16"/>
     </row>
-    <row r="17" spans="6:6" x14ac:dyDescent="0.25">
+    <row r="17" spans="6:6">
       <c r="F17"/>
     </row>
-    <row r="18" spans="6:6" x14ac:dyDescent="0.25">
+    <row r="18" spans="6:6">
       <c r="F18"/>
     </row>
-    <row r="19" spans="6:6" x14ac:dyDescent="0.25">
+    <row r="19" spans="6:6">
       <c r="F19"/>
     </row>
-    <row r="20" spans="6:6" x14ac:dyDescent="0.25">
+    <row r="20" spans="6:6">
       <c r="F20"/>
     </row>
-    <row r="21" spans="6:6" x14ac:dyDescent="0.25">
+    <row r="21" spans="6:6">
       <c r="F21"/>
     </row>
-    <row r="22" spans="6:6" x14ac:dyDescent="0.25">
+    <row r="22" spans="6:6">
       <c r="F22"/>
     </row>
-    <row r="23" spans="6:6" x14ac:dyDescent="0.25">
+    <row r="23" spans="6:6">
       <c r="F23"/>
     </row>
-    <row r="24" spans="6:6" x14ac:dyDescent="0.25">
+    <row r="24" spans="6:6">
       <c r="F24"/>
     </row>
-    <row r="25" spans="6:6" x14ac:dyDescent="0.25">
+    <row r="25" spans="6:6">
       <c r="F25"/>
     </row>
-    <row r="26" spans="6:6" x14ac:dyDescent="0.25">
+    <row r="26" spans="6:6">
       <c r="F26"/>
     </row>
-    <row r="27" spans="6:6" x14ac:dyDescent="0.25">
+    <row r="27" spans="6:6">
       <c r="F27"/>
     </row>
-    <row r="28" spans="6:6" x14ac:dyDescent="0.25">
+    <row r="28" spans="6:6">
       <c r="F28"/>
     </row>
   </sheetData>
@@ -1523,23 +1529,23 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3BDA6702-5DDF-42FB-988E-13FBEB26F5C9}">
   <dimension ref="A1:H100"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" zoomScale="102" zoomScaleNormal="102" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="102" zoomScaleNormal="102" workbookViewId="0">
       <selection activeCell="H10" sqref="H10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="16.140625" customWidth="1"/>
-    <col min="2" max="2" width="17.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="93.140625" customWidth="1"/>
-    <col min="4" max="4" width="10.5703125" customWidth="1"/>
-    <col min="5" max="5" width="14.85546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14.28515625" customWidth="1"/>
-    <col min="7" max="7" width="92.85546875" customWidth="1"/>
-    <col min="8" max="8" width="82.42578125" customWidth="1"/>
+    <col min="1" max="1" width="16.109375" customWidth="1"/>
+    <col min="2" max="2" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="98.44140625" customWidth="1"/>
+    <col min="4" max="4" width="10.5546875" customWidth="1"/>
+    <col min="5" max="5" width="14.88671875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.33203125" customWidth="1"/>
+    <col min="7" max="7" width="92.88671875" customWidth="1"/>
+    <col min="8" max="8" width="82.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" ht="15.6">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
@@ -1565,7 +1571,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8">
       <c r="A2" s="8">
         <v>45786</v>
       </c>
@@ -1591,7 +1597,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8">
       <c r="A3" s="8">
         <v>45787</v>
       </c>
@@ -1617,7 +1623,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8">
       <c r="A4" s="8">
         <v>45789</v>
       </c>
@@ -1641,7 +1647,7 @@
       </c>
       <c r="H4" s="2"/>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8">
       <c r="A5" s="8">
         <v>45790</v>
       </c>
@@ -1665,7 +1671,7 @@
       </c>
       <c r="H5" s="2"/>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8">
       <c r="A6" s="8">
         <v>45791</v>
       </c>
@@ -1691,7 +1697,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8">
       <c r="A7" s="8">
         <v>45795</v>
       </c>
@@ -1715,7 +1721,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8">
       <c r="A8" s="8">
         <v>45798</v>
       </c>
@@ -1737,7 +1743,7 @@
       <c r="G8" s="2"/>
       <c r="H8" s="2"/>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8">
       <c r="A9" s="8">
         <v>45799</v>
       </c>
@@ -1761,547 +1767,565 @@
         <v>92</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A10" s="8"/>
-      <c r="B10" s="2"/>
+    <row r="10" spans="1:8">
+      <c r="A10" s="8">
+        <v>45800</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="C10" t="s">
+        <v>95</v>
+      </c>
+      <c r="D10" t="s">
+        <v>17</v>
+      </c>
+      <c r="E10">
+        <v>100</v>
+      </c>
+      <c r="F10">
+        <v>5</v>
+      </c>
       <c r="G10" s="2"/>
-      <c r="H10" s="2"/>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H10" s="2" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8">
       <c r="A11" s="8"/>
       <c r="B11" s="2"/>
       <c r="G11" s="2"/>
       <c r="H11" s="2"/>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8">
       <c r="A12" s="8"/>
       <c r="B12" s="2"/>
       <c r="G12" s="2"/>
       <c r="H12" s="2"/>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8">
       <c r="A13" s="8"/>
       <c r="B13" s="2"/>
       <c r="G13" s="2"/>
       <c r="H13" s="2"/>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8">
       <c r="A14" s="8"/>
       <c r="B14" s="2"/>
       <c r="G14" s="2"/>
       <c r="H14" s="2"/>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8">
       <c r="A15" s="8"/>
       <c r="B15" s="2"/>
       <c r="G15" s="2"/>
       <c r="H15" s="2"/>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8">
       <c r="A16" s="8"/>
       <c r="B16" s="2"/>
       <c r="G16" s="2"/>
       <c r="H16" s="2"/>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:8">
       <c r="A17" s="8"/>
       <c r="B17" s="2"/>
       <c r="G17" s="2"/>
       <c r="H17" s="2"/>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:8">
       <c r="A18" s="8"/>
       <c r="B18" s="2"/>
       <c r="G18" s="2"/>
       <c r="H18" s="2"/>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:8">
       <c r="A19" s="8"/>
       <c r="B19" s="2"/>
       <c r="G19" s="2"/>
       <c r="H19" s="2"/>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:8">
       <c r="A20" s="8"/>
       <c r="B20" s="2"/>
       <c r="G20" s="2"/>
       <c r="H20" s="2"/>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:8">
       <c r="A21" s="8"/>
       <c r="B21" s="2"/>
       <c r="G21" s="2"/>
       <c r="H21" s="2"/>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:8">
       <c r="A22" s="8"/>
       <c r="B22" s="2"/>
       <c r="G22" s="2"/>
       <c r="H22" s="2"/>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:8">
       <c r="A23" s="8"/>
       <c r="B23" s="2"/>
       <c r="G23" s="2"/>
       <c r="H23" s="2"/>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:8">
       <c r="A24" s="8"/>
       <c r="B24" s="2"/>
       <c r="G24" s="2"/>
       <c r="H24" s="2"/>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:8">
       <c r="A25" s="8"/>
       <c r="B25" s="2"/>
       <c r="G25" s="2"/>
       <c r="H25" s="2"/>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:8">
       <c r="A26" s="8"/>
       <c r="B26" s="2"/>
       <c r="G26" s="2"/>
       <c r="H26" s="2"/>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:8">
       <c r="A27" s="8"/>
       <c r="B27" s="2"/>
       <c r="G27" s="2"/>
       <c r="H27" s="2"/>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:8">
       <c r="A28" s="8"/>
       <c r="B28" s="2"/>
       <c r="G28" s="2"/>
       <c r="H28" s="2"/>
     </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:8">
       <c r="A29" s="8"/>
       <c r="B29" s="2"/>
       <c r="G29" s="2"/>
       <c r="H29" s="2"/>
     </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:8">
       <c r="A30" s="8"/>
       <c r="B30" s="2"/>
       <c r="G30" s="2"/>
       <c r="H30" s="2"/>
     </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:8">
       <c r="A31" s="8"/>
       <c r="B31" s="2"/>
       <c r="G31" s="2"/>
       <c r="H31" s="2"/>
     </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:8">
       <c r="A32" s="8"/>
       <c r="B32" s="2"/>
       <c r="G32" s="2"/>
       <c r="H32" s="2"/>
     </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:8">
       <c r="A33" s="8"/>
       <c r="B33" s="2"/>
       <c r="G33" s="2"/>
       <c r="H33" s="2"/>
     </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:8">
       <c r="A34" s="8"/>
       <c r="B34" s="2"/>
       <c r="G34" s="2"/>
       <c r="H34" s="2"/>
     </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:8">
       <c r="A35" s="8"/>
       <c r="B35" s="2"/>
       <c r="G35" s="2"/>
       <c r="H35" s="2"/>
     </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:8">
       <c r="A36" s="8"/>
       <c r="B36" s="2"/>
       <c r="G36" s="2"/>
       <c r="H36" s="2"/>
     </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:8">
       <c r="A37" s="8"/>
       <c r="B37" s="2"/>
       <c r="G37" s="2"/>
       <c r="H37" s="2"/>
     </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:8">
       <c r="A38" s="8"/>
       <c r="B38" s="2"/>
       <c r="G38" s="2"/>
       <c r="H38" s="2"/>
     </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:8">
       <c r="A39" s="8"/>
       <c r="B39" s="2"/>
       <c r="G39" s="2"/>
       <c r="H39" s="2"/>
     </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:8">
       <c r="A40" s="8"/>
       <c r="B40" s="2"/>
       <c r="G40" s="2"/>
       <c r="H40" s="2"/>
     </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:8">
       <c r="A41" s="8"/>
       <c r="B41" s="2"/>
       <c r="G41" s="2"/>
       <c r="H41" s="2"/>
     </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:8">
       <c r="A42" s="8"/>
       <c r="B42" s="2"/>
       <c r="G42" s="2"/>
       <c r="H42" s="2"/>
     </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:8">
       <c r="A43" s="8"/>
       <c r="B43" s="2"/>
       <c r="G43" s="2"/>
       <c r="H43" s="2"/>
     </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:8">
       <c r="A44" s="8"/>
       <c r="B44" s="2"/>
       <c r="G44" s="2"/>
       <c r="H44" s="2"/>
     </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:8">
       <c r="A45" s="8"/>
       <c r="B45" s="2"/>
       <c r="G45" s="2"/>
       <c r="H45" s="2"/>
     </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:8">
       <c r="A46" s="8"/>
       <c r="B46" s="2"/>
       <c r="G46" s="2"/>
       <c r="H46" s="2"/>
     </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:8">
       <c r="A47" s="8"/>
       <c r="B47" s="2"/>
       <c r="G47" s="2"/>
       <c r="H47" s="2"/>
     </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:8">
       <c r="A48" s="8"/>
       <c r="B48" s="2"/>
       <c r="G48" s="2"/>
       <c r="H48" s="2"/>
     </row>
-    <row r="49" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:8">
       <c r="A49" s="8"/>
       <c r="B49" s="2"/>
       <c r="G49" s="2"/>
       <c r="H49" s="2"/>
     </row>
-    <row r="50" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:8">
       <c r="A50" s="8"/>
       <c r="B50" s="2"/>
       <c r="G50" s="2"/>
       <c r="H50" s="2"/>
     </row>
-    <row r="51" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:8">
       <c r="A51" s="8"/>
       <c r="B51" s="2"/>
       <c r="G51" s="2"/>
       <c r="H51" s="2"/>
     </row>
-    <row r="52" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:8">
       <c r="A52" s="8"/>
       <c r="B52" s="2"/>
       <c r="G52" s="2"/>
       <c r="H52" s="2"/>
     </row>
-    <row r="53" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:8">
       <c r="A53" s="8"/>
       <c r="B53" s="2"/>
       <c r="G53" s="2"/>
       <c r="H53" s="2"/>
     </row>
-    <row r="54" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:8">
       <c r="A54" s="8"/>
       <c r="B54" s="2"/>
       <c r="G54" s="2"/>
       <c r="H54" s="2"/>
     </row>
-    <row r="55" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:8">
       <c r="A55" s="8"/>
       <c r="B55" s="2"/>
       <c r="G55" s="2"/>
       <c r="H55" s="2"/>
     </row>
-    <row r="56" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:8">
       <c r="A56" s="8"/>
       <c r="B56" s="2"/>
       <c r="G56" s="2"/>
       <c r="H56" s="2"/>
     </row>
-    <row r="57" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:8">
       <c r="A57" s="8"/>
       <c r="B57" s="2"/>
       <c r="G57" s="2"/>
       <c r="H57" s="2"/>
     </row>
-    <row r="58" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:8">
       <c r="A58" s="8"/>
       <c r="B58" s="2"/>
       <c r="G58" s="2"/>
       <c r="H58" s="2"/>
     </row>
-    <row r="59" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:8">
       <c r="A59" s="8"/>
       <c r="B59" s="2"/>
       <c r="G59" s="2"/>
       <c r="H59" s="2"/>
     </row>
-    <row r="60" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:8">
       <c r="A60" s="8"/>
       <c r="B60" s="2"/>
       <c r="G60" s="2"/>
       <c r="H60" s="2"/>
     </row>
-    <row r="61" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:8">
       <c r="A61" s="8"/>
       <c r="B61" s="2"/>
       <c r="G61" s="2"/>
       <c r="H61" s="2"/>
     </row>
-    <row r="62" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:8">
       <c r="A62" s="8"/>
       <c r="B62" s="2"/>
       <c r="G62" s="2"/>
       <c r="H62" s="2"/>
     </row>
-    <row r="63" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:8">
       <c r="A63" s="8"/>
       <c r="B63" s="2"/>
       <c r="G63" s="2"/>
       <c r="H63" s="2"/>
     </row>
-    <row r="64" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:8">
       <c r="A64" s="8"/>
       <c r="B64" s="2"/>
       <c r="G64" s="2"/>
       <c r="H64" s="2"/>
     </row>
-    <row r="65" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:8">
       <c r="A65" s="8"/>
       <c r="B65" s="2"/>
       <c r="G65" s="2"/>
       <c r="H65" s="2"/>
     </row>
-    <row r="66" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:8">
       <c r="A66" s="8"/>
       <c r="B66" s="2"/>
       <c r="G66" s="2"/>
       <c r="H66" s="2"/>
     </row>
-    <row r="67" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:8">
       <c r="A67" s="8"/>
       <c r="B67" s="2"/>
       <c r="G67" s="2"/>
       <c r="H67" s="2"/>
     </row>
-    <row r="68" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:8">
       <c r="A68" s="8"/>
       <c r="B68" s="2"/>
       <c r="G68" s="2"/>
       <c r="H68" s="2"/>
     </row>
-    <row r="69" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:8">
       <c r="A69" s="8"/>
       <c r="B69" s="2"/>
       <c r="G69" s="2"/>
       <c r="H69" s="2"/>
     </row>
-    <row r="70" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:8">
       <c r="A70" s="8"/>
       <c r="B70" s="2"/>
       <c r="G70" s="2"/>
       <c r="H70" s="2"/>
     </row>
-    <row r="71" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:8">
       <c r="A71" s="8"/>
       <c r="B71" s="2"/>
       <c r="G71" s="2"/>
       <c r="H71" s="2"/>
     </row>
-    <row r="72" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:8">
       <c r="A72" s="8"/>
       <c r="B72" s="2"/>
       <c r="G72" s="2"/>
       <c r="H72" s="2"/>
     </row>
-    <row r="73" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:8">
       <c r="A73" s="8"/>
       <c r="B73" s="2"/>
       <c r="G73" s="2"/>
       <c r="H73" s="2"/>
     </row>
-    <row r="74" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:8">
       <c r="A74" s="8"/>
       <c r="B74" s="2"/>
       <c r="G74" s="2"/>
       <c r="H74" s="2"/>
     </row>
-    <row r="75" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:8">
       <c r="A75" s="8"/>
       <c r="B75" s="2"/>
       <c r="G75" s="2"/>
       <c r="H75" s="2"/>
     </row>
-    <row r="76" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:8">
       <c r="A76" s="8"/>
       <c r="B76" s="2"/>
       <c r="G76" s="2"/>
       <c r="H76" s="2"/>
     </row>
-    <row r="77" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:8">
       <c r="A77" s="8"/>
       <c r="B77" s="2"/>
       <c r="G77" s="2"/>
       <c r="H77" s="2"/>
     </row>
-    <row r="78" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:8">
       <c r="A78" s="8"/>
       <c r="B78" s="2"/>
       <c r="G78" s="2"/>
       <c r="H78" s="2"/>
     </row>
-    <row r="79" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:8">
       <c r="A79" s="8"/>
       <c r="B79" s="2"/>
       <c r="G79" s="2"/>
       <c r="H79" s="2"/>
     </row>
-    <row r="80" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:8">
       <c r="A80" s="8"/>
       <c r="B80" s="2"/>
       <c r="G80" s="2"/>
       <c r="H80" s="2"/>
     </row>
-    <row r="81" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:8">
       <c r="A81" s="8"/>
       <c r="B81" s="2"/>
       <c r="G81" s="2"/>
       <c r="H81" s="2"/>
     </row>
-    <row r="82" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:8">
       <c r="A82" s="8"/>
       <c r="B82" s="2"/>
       <c r="G82" s="2"/>
       <c r="H82" s="2"/>
     </row>
-    <row r="83" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:8">
       <c r="A83" s="8"/>
       <c r="B83" s="2"/>
       <c r="G83" s="2"/>
       <c r="H83" s="2"/>
     </row>
-    <row r="84" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:8">
       <c r="A84" s="8"/>
       <c r="B84" s="2"/>
       <c r="G84" s="2"/>
       <c r="H84" s="2"/>
     </row>
-    <row r="85" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:8">
       <c r="A85" s="8"/>
       <c r="B85" s="2"/>
       <c r="G85" s="2"/>
       <c r="H85" s="2"/>
     </row>
-    <row r="86" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:8">
       <c r="A86" s="8"/>
       <c r="B86" s="2"/>
       <c r="G86" s="2"/>
       <c r="H86" s="2"/>
     </row>
-    <row r="87" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:8">
       <c r="A87" s="8"/>
       <c r="B87" s="2"/>
       <c r="G87" s="2"/>
       <c r="H87" s="2"/>
     </row>
-    <row r="88" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:8">
       <c r="A88" s="8"/>
       <c r="B88" s="2"/>
       <c r="G88" s="2"/>
       <c r="H88" s="2"/>
     </row>
-    <row r="89" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:8">
       <c r="A89" s="8"/>
       <c r="B89" s="2"/>
       <c r="G89" s="2"/>
       <c r="H89" s="2"/>
     </row>
-    <row r="90" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:8">
       <c r="A90" s="8"/>
       <c r="B90" s="2"/>
       <c r="G90" s="2"/>
       <c r="H90" s="2"/>
     </row>
-    <row r="91" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:8">
       <c r="A91" s="8"/>
       <c r="B91" s="2"/>
       <c r="G91" s="2"/>
       <c r="H91" s="2"/>
     </row>
-    <row r="92" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:8">
       <c r="A92" s="8"/>
       <c r="B92" s="2"/>
       <c r="G92" s="2"/>
       <c r="H92" s="2"/>
     </row>
-    <row r="93" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:8">
       <c r="A93" s="8"/>
       <c r="B93" s="2"/>
       <c r="G93" s="2"/>
       <c r="H93" s="2"/>
     </row>
-    <row r="94" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:8">
       <c r="A94" s="8"/>
       <c r="B94" s="2"/>
       <c r="G94" s="2"/>
       <c r="H94" s="2"/>
     </row>
-    <row r="95" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:8">
       <c r="A95" s="8"/>
       <c r="B95" s="2"/>
       <c r="G95" s="2"/>
       <c r="H95" s="2"/>
     </row>
-    <row r="96" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:8">
       <c r="A96" s="8"/>
       <c r="B96" s="2"/>
       <c r="G96" s="2"/>
       <c r="H96" s="2"/>
     </row>
-    <row r="97" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:8">
       <c r="A97" s="8"/>
       <c r="B97" s="2"/>
       <c r="G97" s="2"/>
       <c r="H97" s="2"/>
     </row>
-    <row r="98" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:8">
       <c r="A98" s="8"/>
       <c r="B98" s="2"/>
       <c r="G98" s="2"/>
       <c r="H98" s="2"/>
     </row>
-    <row r="99" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:8">
       <c r="A99" s="8"/>
       <c r="B99" s="2"/>
       <c r="G99" s="2"/>
       <c r="H99" s="2"/>
     </row>
-    <row r="100" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:8">
       <c r="A100" s="8"/>
       <c r="B100" s="2"/>
       <c r="G100" s="2"/>
@@ -2326,7 +2350,7 @@
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <ignoredErrors>
-    <ignoredError sqref="D10:D100" listDataValidation="1"/>
+    <ignoredError sqref="D11:D100" listDataValidation="1"/>
   </ignoredErrors>
   <tableParts count="1">
     <tablePart r:id="rId1"/>
@@ -2342,19 +2366,19 @@
       <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="10.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="17.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="27.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.85546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="23.5703125" style="10" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="39.140625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="51.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.44140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="27.88671875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.88671875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="23.5546875" style="10" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="39.109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="51.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" ht="15.6">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
@@ -2380,7 +2404,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8">
       <c r="A2" s="1">
         <v>45935</v>
       </c>
@@ -2406,7 +2430,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8">
       <c r="A3" s="1">
         <v>45996</v>
       </c>
@@ -2432,7 +2456,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8">
       <c r="A4" s="1" t="s">
         <v>57</v>
       </c>
@@ -2458,7 +2482,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8">
       <c r="A5" s="1" t="s">
         <v>61</v>
       </c>
@@ -2484,7 +2508,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8">
       <c r="A6" s="1" t="s">
         <v>67</v>
       </c>
@@ -2510,7 +2534,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8">
       <c r="A7" s="1" t="s">
         <v>70</v>
       </c>
@@ -2536,7 +2560,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="8" spans="1:8" ht="105" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" ht="100.8">
       <c r="A8" s="1">
         <v>45798</v>